<commit_message>
Tempo - first version of the boss done.  God I hope we can find a way to make it look better than this!  Need to figure out how to manipulate the falling head.  That should save a lot of time if it can be grabbed after the boss is defeated.
</commit_message>
<xml_diff>
--- a/trunk/Tempo/Tempo.xlsx
+++ b/trunk/Tempo/Tempo.xlsx
@@ -2128,29 +2128,29 @@
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -2186,20 +2186,34 @@
     <xf numFmtId="0" fontId="47" fillId="22" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="41" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="4"/>
     </xf>
@@ -2209,20 +2223,6 @@
     <xf numFmtId="0" fontId="42" fillId="0" borderId="33" xfId="3" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" indent="4"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Accent1" xfId="2" builtinId="29"/>
@@ -2533,8 +2533,8 @@
   <dimension ref="A1:K150"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C25" sqref="C25"/>
+      <pane ySplit="6" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" outlineLevelRow="2"/>
@@ -3024,13 +3024,15 @@
       <c r="B30" s="149" t="s">
         <v>223</v>
       </c>
-      <c r="C30" s="101"/>
+      <c r="C30" s="101">
+        <v>8961</v>
+      </c>
       <c r="D30" s="101">
         <v>9931</v>
       </c>
       <c r="E30" s="123">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>970</v>
       </c>
       <c r="F30" s="105"/>
     </row>
@@ -4716,6 +4718,11 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="A135:A149"/>
+    <mergeCell ref="A106:A115"/>
+    <mergeCell ref="A76:A90"/>
+    <mergeCell ref="A118:A132"/>
+    <mergeCell ref="A93:A103"/>
     <mergeCell ref="A37:A57"/>
     <mergeCell ref="A60:A73"/>
     <mergeCell ref="C5:D5"/>
@@ -4725,11 +4732,6 @@
     <mergeCell ref="A8:A18"/>
     <mergeCell ref="A21:A34"/>
     <mergeCell ref="C4:E4"/>
-    <mergeCell ref="A135:A149"/>
-    <mergeCell ref="A106:A115"/>
-    <mergeCell ref="A76:A90"/>
-    <mergeCell ref="A118:A132"/>
-    <mergeCell ref="A93:A103"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4761,13 +4763,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="26.25" customHeight="1">
-      <c r="A1" s="182" t="s">
+      <c r="A1" s="164" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="182"/>
-      <c r="C1" s="182"/>
-      <c r="D1" s="182"/>
-      <c r="E1" s="182"/>
+      <c r="B1" s="164"/>
+      <c r="C1" s="164"/>
+      <c r="D1" s="164"/>
+      <c r="E1" s="164"/>
       <c r="F1" s="7"/>
       <c r="G1" s="5"/>
       <c r="H1" s="5"/>
@@ -4797,18 +4799,18 @@
         <v>8</v>
       </c>
       <c r="B3" s="36"/>
-      <c r="C3" s="183"/>
-      <c r="D3" s="184"/>
-      <c r="E3" s="184"/>
+      <c r="C3" s="165"/>
+      <c r="D3" s="166"/>
+      <c r="E3" s="166"/>
     </row>
     <row r="4" spans="1:8" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A4" s="46" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="87"/>
-      <c r="C4" s="164"/>
-      <c r="D4" s="165"/>
-      <c r="E4" s="165"/>
+      <c r="C4" s="167"/>
+      <c r="D4" s="168"/>
+      <c r="E4" s="168"/>
       <c r="F4" s="6"/>
     </row>
     <row r="5" spans="1:8" hidden="1" outlineLevel="2">
@@ -4960,9 +4962,9 @@
         <v>9</v>
       </c>
       <c r="B21" s="90"/>
-      <c r="C21" s="166"/>
-      <c r="D21" s="167"/>
-      <c r="E21" s="167"/>
+      <c r="C21" s="169"/>
+      <c r="D21" s="170"/>
+      <c r="E21" s="170"/>
     </row>
     <row r="22" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A22" s="47">
@@ -5113,9 +5115,9 @@
         <v>10</v>
       </c>
       <c r="B38" s="87"/>
-      <c r="C38" s="164"/>
-      <c r="D38" s="165"/>
-      <c r="E38" s="165"/>
+      <c r="C38" s="167"/>
+      <c r="D38" s="168"/>
+      <c r="E38" s="168"/>
     </row>
     <row r="39" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A39" s="47">
@@ -5266,9 +5268,9 @@
         <v>11</v>
       </c>
       <c r="B55" s="87"/>
-      <c r="C55" s="164"/>
-      <c r="D55" s="165"/>
-      <c r="E55" s="165"/>
+      <c r="C55" s="167"/>
+      <c r="D55" s="168"/>
+      <c r="E55" s="168"/>
     </row>
     <row r="56" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A56" s="47">
@@ -5419,9 +5421,9 @@
         <v>12</v>
       </c>
       <c r="B72" s="87"/>
-      <c r="C72" s="164"/>
-      <c r="D72" s="165"/>
-      <c r="E72" s="165"/>
+      <c r="C72" s="167"/>
+      <c r="D72" s="168"/>
+      <c r="E72" s="168"/>
     </row>
     <row r="73" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A73" s="47">
@@ -5572,9 +5574,9 @@
         <v>13</v>
       </c>
       <c r="B89" s="87"/>
-      <c r="C89" s="164"/>
-      <c r="D89" s="165"/>
-      <c r="E89" s="165"/>
+      <c r="C89" s="167"/>
+      <c r="D89" s="168"/>
+      <c r="E89" s="168"/>
     </row>
     <row r="90" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A90" s="47">
@@ -5725,9 +5727,9 @@
         <v>14</v>
       </c>
       <c r="B106" s="87"/>
-      <c r="C106" s="164"/>
-      <c r="D106" s="165"/>
-      <c r="E106" s="165"/>
+      <c r="C106" s="167"/>
+      <c r="D106" s="168"/>
+      <c r="E106" s="168"/>
     </row>
     <row r="107" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A107" s="47">
@@ -5878,9 +5880,9 @@
         <v>15</v>
       </c>
       <c r="B123" s="87"/>
-      <c r="C123" s="164"/>
-      <c r="D123" s="165"/>
-      <c r="E123" s="165"/>
+      <c r="C123" s="167"/>
+      <c r="D123" s="168"/>
+      <c r="E123" s="168"/>
     </row>
     <row r="124" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A124" s="47">
@@ -6031,9 +6033,9 @@
         <v>16</v>
       </c>
       <c r="B140" s="87"/>
-      <c r="C140" s="164"/>
-      <c r="D140" s="165"/>
-      <c r="E140" s="165"/>
+      <c r="C140" s="167"/>
+      <c r="D140" s="168"/>
+      <c r="E140" s="168"/>
     </row>
     <row r="141" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A141" s="47">
@@ -6184,9 +6186,9 @@
         <v>17</v>
       </c>
       <c r="B157" s="87"/>
-      <c r="C157" s="164"/>
-      <c r="D157" s="165"/>
-      <c r="E157" s="165"/>
+      <c r="C157" s="167"/>
+      <c r="D157" s="168"/>
+      <c r="E157" s="168"/>
     </row>
     <row r="158" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A158" s="47">
@@ -6337,9 +6339,9 @@
         <v>18</v>
       </c>
       <c r="B174" s="87"/>
-      <c r="C174" s="164"/>
-      <c r="D174" s="165"/>
-      <c r="E174" s="165"/>
+      <c r="C174" s="167"/>
+      <c r="D174" s="168"/>
+      <c r="E174" s="168"/>
     </row>
     <row r="175" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A175" s="47">
@@ -6490,9 +6492,9 @@
         <v>19</v>
       </c>
       <c r="B191" s="87"/>
-      <c r="C191" s="164"/>
-      <c r="D191" s="165"/>
-      <c r="E191" s="165"/>
+      <c r="C191" s="167"/>
+      <c r="D191" s="168"/>
+      <c r="E191" s="168"/>
     </row>
     <row r="192" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A192" s="47">
@@ -6643,9 +6645,9 @@
         <v>20</v>
       </c>
       <c r="B208" s="87"/>
-      <c r="C208" s="164"/>
-      <c r="D208" s="165"/>
-      <c r="E208" s="165"/>
+      <c r="C208" s="167"/>
+      <c r="D208" s="168"/>
+      <c r="E208" s="168"/>
     </row>
     <row r="209" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A209" s="47">
@@ -6796,9 +6798,9 @@
         <v>21</v>
       </c>
       <c r="B225" s="87"/>
-      <c r="C225" s="164"/>
-      <c r="D225" s="165"/>
-      <c r="E225" s="165"/>
+      <c r="C225" s="167"/>
+      <c r="D225" s="168"/>
+      <c r="E225" s="168"/>
     </row>
     <row r="226" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A226" s="47">
@@ -6949,9 +6951,9 @@
         <v>22</v>
       </c>
       <c r="B242" s="87"/>
-      <c r="C242" s="164"/>
-      <c r="D242" s="165"/>
-      <c r="E242" s="165"/>
+      <c r="C242" s="167"/>
+      <c r="D242" s="168"/>
+      <c r="E242" s="168"/>
     </row>
     <row r="243" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A243" s="47">
@@ -7102,9 +7104,9 @@
         <v>23</v>
       </c>
       <c r="B259" s="87"/>
-      <c r="C259" s="164"/>
-      <c r="D259" s="165"/>
-      <c r="E259" s="165"/>
+      <c r="C259" s="167"/>
+      <c r="D259" s="168"/>
+      <c r="E259" s="168"/>
     </row>
     <row r="260" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A260" s="47">
@@ -7255,18 +7257,18 @@
         <v>24</v>
       </c>
       <c r="B276" s="37"/>
-      <c r="C276" s="180"/>
-      <c r="D276" s="181"/>
-      <c r="E276" s="181"/>
+      <c r="C276" s="171"/>
+      <c r="D276" s="172"/>
+      <c r="E276" s="172"/>
     </row>
     <row r="277" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A277" s="51" t="s">
         <v>25</v>
       </c>
       <c r="B277" s="87"/>
-      <c r="C277" s="164"/>
-      <c r="D277" s="165"/>
-      <c r="E277" s="165"/>
+      <c r="C277" s="167"/>
+      <c r="D277" s="168"/>
+      <c r="E277" s="168"/>
     </row>
     <row r="278" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A278" s="52">
@@ -7417,9 +7419,9 @@
         <v>26</v>
       </c>
       <c r="B294" s="90"/>
-      <c r="C294" s="166"/>
-      <c r="D294" s="167"/>
-      <c r="E294" s="167"/>
+      <c r="C294" s="169"/>
+      <c r="D294" s="170"/>
+      <c r="E294" s="170"/>
     </row>
     <row r="295" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A295" s="52">
@@ -7570,9 +7572,9 @@
         <v>27</v>
       </c>
       <c r="B311" s="87"/>
-      <c r="C311" s="164"/>
-      <c r="D311" s="165"/>
-      <c r="E311" s="165"/>
+      <c r="C311" s="167"/>
+      <c r="D311" s="168"/>
+      <c r="E311" s="168"/>
     </row>
     <row r="312" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A312" s="52">
@@ -7723,9 +7725,9 @@
         <v>28</v>
       </c>
       <c r="B328" s="87"/>
-      <c r="C328" s="164"/>
-      <c r="D328" s="165"/>
-      <c r="E328" s="165"/>
+      <c r="C328" s="167"/>
+      <c r="D328" s="168"/>
+      <c r="E328" s="168"/>
     </row>
     <row r="329" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A329" s="52">
@@ -7876,9 +7878,9 @@
         <v>29</v>
       </c>
       <c r="B345" s="87"/>
-      <c r="C345" s="164"/>
-      <c r="D345" s="165"/>
-      <c r="E345" s="165"/>
+      <c r="C345" s="167"/>
+      <c r="D345" s="168"/>
+      <c r="E345" s="168"/>
     </row>
     <row r="346" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A346" s="52">
@@ -8029,9 +8031,9 @@
         <v>30</v>
       </c>
       <c r="B362" s="87"/>
-      <c r="C362" s="164"/>
-      <c r="D362" s="165"/>
-      <c r="E362" s="165"/>
+      <c r="C362" s="167"/>
+      <c r="D362" s="168"/>
+      <c r="E362" s="168"/>
     </row>
     <row r="363" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A363" s="52">
@@ -8182,9 +8184,9 @@
         <v>31</v>
       </c>
       <c r="B379" s="87"/>
-      <c r="C379" s="164"/>
-      <c r="D379" s="165"/>
-      <c r="E379" s="165"/>
+      <c r="C379" s="167"/>
+      <c r="D379" s="168"/>
+      <c r="E379" s="168"/>
     </row>
     <row r="380" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A380" s="52">
@@ -8335,9 +8337,9 @@
         <v>32</v>
       </c>
       <c r="B396" s="87"/>
-      <c r="C396" s="164"/>
-      <c r="D396" s="165"/>
-      <c r="E396" s="165"/>
+      <c r="C396" s="167"/>
+      <c r="D396" s="168"/>
+      <c r="E396" s="168"/>
     </row>
     <row r="397" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A397" s="52">
@@ -8488,9 +8490,9 @@
         <v>33</v>
       </c>
       <c r="B413" s="87"/>
-      <c r="C413" s="164"/>
-      <c r="D413" s="165"/>
-      <c r="E413" s="165"/>
+      <c r="C413" s="167"/>
+      <c r="D413" s="168"/>
+      <c r="E413" s="168"/>
     </row>
     <row r="414" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A414" s="52">
@@ -8641,9 +8643,9 @@
         <v>34</v>
       </c>
       <c r="B430" s="87"/>
-      <c r="C430" s="164"/>
-      <c r="D430" s="165"/>
-      <c r="E430" s="165"/>
+      <c r="C430" s="167"/>
+      <c r="D430" s="168"/>
+      <c r="E430" s="168"/>
     </row>
     <row r="431" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A431" s="52">
@@ -8794,9 +8796,9 @@
         <v>35</v>
       </c>
       <c r="B447" s="87"/>
-      <c r="C447" s="164"/>
-      <c r="D447" s="165"/>
-      <c r="E447" s="165"/>
+      <c r="C447" s="167"/>
+      <c r="D447" s="168"/>
+      <c r="E447" s="168"/>
     </row>
     <row r="448" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A448" s="52">
@@ -8947,9 +8949,9 @@
         <v>36</v>
       </c>
       <c r="B464" s="87"/>
-      <c r="C464" s="164"/>
-      <c r="D464" s="165"/>
-      <c r="E464" s="165"/>
+      <c r="C464" s="167"/>
+      <c r="D464" s="168"/>
+      <c r="E464" s="168"/>
     </row>
     <row r="465" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A465" s="52">
@@ -9100,9 +9102,9 @@
         <v>37</v>
       </c>
       <c r="B481" s="87"/>
-      <c r="C481" s="164"/>
-      <c r="D481" s="165"/>
-      <c r="E481" s="165"/>
+      <c r="C481" s="167"/>
+      <c r="D481" s="168"/>
+      <c r="E481" s="168"/>
     </row>
     <row r="482" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A482" s="52">
@@ -9253,9 +9255,9 @@
         <v>38</v>
       </c>
       <c r="B498" s="87"/>
-      <c r="C498" s="164"/>
-      <c r="D498" s="165"/>
-      <c r="E498" s="165"/>
+      <c r="C498" s="167"/>
+      <c r="D498" s="168"/>
+      <c r="E498" s="168"/>
     </row>
     <row r="499" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A499" s="52">
@@ -9406,9 +9408,9 @@
         <v>39</v>
       </c>
       <c r="B515" s="87"/>
-      <c r="C515" s="164"/>
-      <c r="D515" s="165"/>
-      <c r="E515" s="165"/>
+      <c r="C515" s="167"/>
+      <c r="D515" s="168"/>
+      <c r="E515" s="168"/>
     </row>
     <row r="516" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A516" s="52">
@@ -9559,9 +9561,9 @@
         <v>40</v>
       </c>
       <c r="B532" s="87"/>
-      <c r="C532" s="164"/>
-      <c r="D532" s="165"/>
-      <c r="E532" s="165"/>
+      <c r="C532" s="167"/>
+      <c r="D532" s="168"/>
+      <c r="E532" s="168"/>
     </row>
     <row r="533" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A533" s="55">
@@ -9712,18 +9714,18 @@
         <v>50</v>
       </c>
       <c r="B549" s="38"/>
-      <c r="C549" s="178"/>
-      <c r="D549" s="179"/>
-      <c r="E549" s="179"/>
+      <c r="C549" s="173"/>
+      <c r="D549" s="174"/>
+      <c r="E549" s="174"/>
     </row>
     <row r="550" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A550" s="58" t="s">
         <v>51</v>
       </c>
       <c r="B550" s="87"/>
-      <c r="C550" s="164"/>
-      <c r="D550" s="165"/>
-      <c r="E550" s="165"/>
+      <c r="C550" s="167"/>
+      <c r="D550" s="168"/>
+      <c r="E550" s="168"/>
     </row>
     <row r="551" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A551" s="59">
@@ -9874,9 +9876,9 @@
         <v>52</v>
       </c>
       <c r="B567" s="90"/>
-      <c r="C567" s="166"/>
-      <c r="D567" s="167"/>
-      <c r="E567" s="167"/>
+      <c r="C567" s="169"/>
+      <c r="D567" s="170"/>
+      <c r="E567" s="170"/>
     </row>
     <row r="568" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A568" s="59">
@@ -10027,9 +10029,9 @@
         <v>53</v>
       </c>
       <c r="B584" s="87"/>
-      <c r="C584" s="164"/>
-      <c r="D584" s="165"/>
-      <c r="E584" s="165"/>
+      <c r="C584" s="167"/>
+      <c r="D584" s="168"/>
+      <c r="E584" s="168"/>
     </row>
     <row r="585" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A585" s="59">
@@ -10180,9 +10182,9 @@
         <v>54</v>
       </c>
       <c r="B601" s="87"/>
-      <c r="C601" s="164"/>
-      <c r="D601" s="165"/>
-      <c r="E601" s="165"/>
+      <c r="C601" s="167"/>
+      <c r="D601" s="168"/>
+      <c r="E601" s="168"/>
     </row>
     <row r="602" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A602" s="59">
@@ -10333,9 +10335,9 @@
         <v>55</v>
       </c>
       <c r="B618" s="87"/>
-      <c r="C618" s="164"/>
-      <c r="D618" s="165"/>
-      <c r="E618" s="165"/>
+      <c r="C618" s="167"/>
+      <c r="D618" s="168"/>
+      <c r="E618" s="168"/>
     </row>
     <row r="619" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A619" s="59">
@@ -10486,9 +10488,9 @@
         <v>56</v>
       </c>
       <c r="B635" s="87"/>
-      <c r="C635" s="164"/>
-      <c r="D635" s="165"/>
-      <c r="E635" s="165"/>
+      <c r="C635" s="167"/>
+      <c r="D635" s="168"/>
+      <c r="E635" s="168"/>
     </row>
     <row r="636" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A636" s="59">
@@ -10639,9 +10641,9 @@
         <v>57</v>
       </c>
       <c r="B652" s="87"/>
-      <c r="C652" s="164"/>
-      <c r="D652" s="165"/>
-      <c r="E652" s="165"/>
+      <c r="C652" s="167"/>
+      <c r="D652" s="168"/>
+      <c r="E652" s="168"/>
     </row>
     <row r="653" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A653" s="59">
@@ -10792,9 +10794,9 @@
         <v>58</v>
       </c>
       <c r="B669" s="87"/>
-      <c r="C669" s="164"/>
-      <c r="D669" s="165"/>
-      <c r="E669" s="165"/>
+      <c r="C669" s="167"/>
+      <c r="D669" s="168"/>
+      <c r="E669" s="168"/>
     </row>
     <row r="670" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A670" s="59">
@@ -10945,9 +10947,9 @@
         <v>59</v>
       </c>
       <c r="B686" s="87"/>
-      <c r="C686" s="164"/>
-      <c r="D686" s="165"/>
-      <c r="E686" s="165"/>
+      <c r="C686" s="167"/>
+      <c r="D686" s="168"/>
+      <c r="E686" s="168"/>
     </row>
     <row r="687" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A687" s="59">
@@ -11098,9 +11100,9 @@
         <v>60</v>
       </c>
       <c r="B703" s="87"/>
-      <c r="C703" s="164"/>
-      <c r="D703" s="165"/>
-      <c r="E703" s="165"/>
+      <c r="C703" s="167"/>
+      <c r="D703" s="168"/>
+      <c r="E703" s="168"/>
     </row>
     <row r="704" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A704" s="59">
@@ -11251,9 +11253,9 @@
         <v>61</v>
       </c>
       <c r="B720" s="87"/>
-      <c r="C720" s="164"/>
-      <c r="D720" s="165"/>
-      <c r="E720" s="165"/>
+      <c r="C720" s="167"/>
+      <c r="D720" s="168"/>
+      <c r="E720" s="168"/>
     </row>
     <row r="721" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A721" s="59">
@@ -11404,9 +11406,9 @@
         <v>62</v>
       </c>
       <c r="B737" s="87"/>
-      <c r="C737" s="164"/>
-      <c r="D737" s="165"/>
-      <c r="E737" s="165"/>
+      <c r="C737" s="167"/>
+      <c r="D737" s="168"/>
+      <c r="E737" s="168"/>
     </row>
     <row r="738" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A738" s="59">
@@ -11557,9 +11559,9 @@
         <v>63</v>
       </c>
       <c r="B754" s="87"/>
-      <c r="C754" s="164"/>
-      <c r="D754" s="165"/>
-      <c r="E754" s="165"/>
+      <c r="C754" s="167"/>
+      <c r="D754" s="168"/>
+      <c r="E754" s="168"/>
     </row>
     <row r="755" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A755" s="59">
@@ -11710,9 +11712,9 @@
         <v>64</v>
       </c>
       <c r="B771" s="87"/>
-      <c r="C771" s="164"/>
-      <c r="D771" s="165"/>
-      <c r="E771" s="165"/>
+      <c r="C771" s="167"/>
+      <c r="D771" s="168"/>
+      <c r="E771" s="168"/>
     </row>
     <row r="772" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A772" s="59">
@@ -11863,9 +11865,9 @@
         <v>65</v>
       </c>
       <c r="B788" s="87"/>
-      <c r="C788" s="164"/>
-      <c r="D788" s="165"/>
-      <c r="E788" s="165"/>
+      <c r="C788" s="167"/>
+      <c r="D788" s="168"/>
+      <c r="E788" s="168"/>
     </row>
     <row r="789" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A789" s="59">
@@ -12016,9 +12018,9 @@
         <v>66</v>
       </c>
       <c r="B805" s="87"/>
-      <c r="C805" s="164"/>
-      <c r="D805" s="165"/>
-      <c r="E805" s="165"/>
+      <c r="C805" s="167"/>
+      <c r="D805" s="168"/>
+      <c r="E805" s="168"/>
     </row>
     <row r="806" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A806" s="59">
@@ -12169,18 +12171,18 @@
         <v>67</v>
       </c>
       <c r="B822" s="39"/>
-      <c r="C822" s="176"/>
-      <c r="D822" s="177"/>
-      <c r="E822" s="177"/>
+      <c r="C822" s="175"/>
+      <c r="D822" s="176"/>
+      <c r="E822" s="176"/>
     </row>
     <row r="823" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A823" s="63" t="s">
         <v>68</v>
       </c>
       <c r="B823" s="87"/>
-      <c r="C823" s="164"/>
-      <c r="D823" s="165"/>
-      <c r="E823" s="165"/>
+      <c r="C823" s="167"/>
+      <c r="D823" s="168"/>
+      <c r="E823" s="168"/>
     </row>
     <row r="824" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A824" s="64">
@@ -12331,9 +12333,9 @@
         <v>69</v>
       </c>
       <c r="B840" s="90"/>
-      <c r="C840" s="166"/>
-      <c r="D840" s="167"/>
-      <c r="E840" s="167"/>
+      <c r="C840" s="169"/>
+      <c r="D840" s="170"/>
+      <c r="E840" s="170"/>
     </row>
     <row r="841" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A841" s="64">
@@ -12484,9 +12486,9 @@
         <v>70</v>
       </c>
       <c r="B857" s="87"/>
-      <c r="C857" s="164"/>
-      <c r="D857" s="165"/>
-      <c r="E857" s="165"/>
+      <c r="C857" s="167"/>
+      <c r="D857" s="168"/>
+      <c r="E857" s="168"/>
     </row>
     <row r="858" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A858" s="64">
@@ -12637,9 +12639,9 @@
         <v>71</v>
       </c>
       <c r="B874" s="87"/>
-      <c r="C874" s="164"/>
-      <c r="D874" s="165"/>
-      <c r="E874" s="165"/>
+      <c r="C874" s="167"/>
+      <c r="D874" s="168"/>
+      <c r="E874" s="168"/>
     </row>
     <row r="875" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A875" s="64">
@@ -12790,9 +12792,9 @@
         <v>72</v>
       </c>
       <c r="B891" s="87"/>
-      <c r="C891" s="164"/>
-      <c r="D891" s="165"/>
-      <c r="E891" s="165"/>
+      <c r="C891" s="167"/>
+      <c r="D891" s="168"/>
+      <c r="E891" s="168"/>
     </row>
     <row r="892" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A892" s="64">
@@ -12943,9 +12945,9 @@
         <v>73</v>
       </c>
       <c r="B908" s="87"/>
-      <c r="C908" s="164"/>
-      <c r="D908" s="165"/>
-      <c r="E908" s="165"/>
+      <c r="C908" s="167"/>
+      <c r="D908" s="168"/>
+      <c r="E908" s="168"/>
     </row>
     <row r="909" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A909" s="64">
@@ -13096,9 +13098,9 @@
         <v>74</v>
       </c>
       <c r="B925" s="87"/>
-      <c r="C925" s="164"/>
-      <c r="D925" s="165"/>
-      <c r="E925" s="165"/>
+      <c r="C925" s="167"/>
+      <c r="D925" s="168"/>
+      <c r="E925" s="168"/>
     </row>
     <row r="926" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A926" s="64">
@@ -13249,9 +13251,9 @@
         <v>75</v>
       </c>
       <c r="B942" s="87"/>
-      <c r="C942" s="164"/>
-      <c r="D942" s="165"/>
-      <c r="E942" s="165"/>
+      <c r="C942" s="167"/>
+      <c r="D942" s="168"/>
+      <c r="E942" s="168"/>
     </row>
     <row r="943" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A943" s="64">
@@ -13402,9 +13404,9 @@
         <v>76</v>
       </c>
       <c r="B959" s="87"/>
-      <c r="C959" s="164"/>
-      <c r="D959" s="165"/>
-      <c r="E959" s="165"/>
+      <c r="C959" s="167"/>
+      <c r="D959" s="168"/>
+      <c r="E959" s="168"/>
     </row>
     <row r="960" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A960" s="64">
@@ -13555,9 +13557,9 @@
         <v>77</v>
       </c>
       <c r="B976" s="87"/>
-      <c r="C976" s="164"/>
-      <c r="D976" s="165"/>
-      <c r="E976" s="165"/>
+      <c r="C976" s="167"/>
+      <c r="D976" s="168"/>
+      <c r="E976" s="168"/>
     </row>
     <row r="977" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A977" s="64">
@@ -13708,9 +13710,9 @@
         <v>78</v>
       </c>
       <c r="B993" s="87"/>
-      <c r="C993" s="164"/>
-      <c r="D993" s="165"/>
-      <c r="E993" s="165"/>
+      <c r="C993" s="167"/>
+      <c r="D993" s="168"/>
+      <c r="E993" s="168"/>
     </row>
     <row r="994" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A994" s="64">
@@ -13861,9 +13863,9 @@
         <v>79</v>
       </c>
       <c r="B1010" s="87"/>
-      <c r="C1010" s="164"/>
-      <c r="D1010" s="165"/>
-      <c r="E1010" s="165"/>
+      <c r="C1010" s="167"/>
+      <c r="D1010" s="168"/>
+      <c r="E1010" s="168"/>
     </row>
     <row r="1011" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1011" s="64">
@@ -14014,9 +14016,9 @@
         <v>80</v>
       </c>
       <c r="B1027" s="87"/>
-      <c r="C1027" s="164"/>
-      <c r="D1027" s="165"/>
-      <c r="E1027" s="165"/>
+      <c r="C1027" s="167"/>
+      <c r="D1027" s="168"/>
+      <c r="E1027" s="168"/>
     </row>
     <row r="1028" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1028" s="64">
@@ -14167,9 +14169,9 @@
         <v>83</v>
       </c>
       <c r="B1044" s="87"/>
-      <c r="C1044" s="164"/>
-      <c r="D1044" s="165"/>
-      <c r="E1044" s="165"/>
+      <c r="C1044" s="167"/>
+      <c r="D1044" s="168"/>
+      <c r="E1044" s="168"/>
     </row>
     <row r="1045" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1045" s="64">
@@ -14320,9 +14322,9 @@
         <v>82</v>
       </c>
       <c r="B1061" s="87"/>
-      <c r="C1061" s="164"/>
-      <c r="D1061" s="165"/>
-      <c r="E1061" s="165"/>
+      <c r="C1061" s="167"/>
+      <c r="D1061" s="168"/>
+      <c r="E1061" s="168"/>
     </row>
     <row r="1062" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1062" s="64">
@@ -14473,9 +14475,9 @@
         <v>84</v>
       </c>
       <c r="B1078" s="87"/>
-      <c r="C1078" s="164"/>
-      <c r="D1078" s="165"/>
-      <c r="E1078" s="165"/>
+      <c r="C1078" s="167"/>
+      <c r="D1078" s="168"/>
+      <c r="E1078" s="168"/>
     </row>
     <row r="1079" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1079" s="64">
@@ -14626,18 +14628,18 @@
         <v>104</v>
       </c>
       <c r="B1095" s="40"/>
-      <c r="C1095" s="174"/>
-      <c r="D1095" s="175"/>
-      <c r="E1095" s="175"/>
+      <c r="C1095" s="177"/>
+      <c r="D1095" s="178"/>
+      <c r="E1095" s="178"/>
     </row>
     <row r="1096" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A1096" s="68" t="s">
         <v>85</v>
       </c>
       <c r="B1096" s="87"/>
-      <c r="C1096" s="164"/>
-      <c r="D1096" s="165"/>
-      <c r="E1096" s="165"/>
+      <c r="C1096" s="167"/>
+      <c r="D1096" s="168"/>
+      <c r="E1096" s="168"/>
     </row>
     <row r="1097" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1097" s="69">
@@ -14788,9 +14790,9 @@
         <v>86</v>
       </c>
       <c r="B1113" s="90"/>
-      <c r="C1113" s="166"/>
-      <c r="D1113" s="167"/>
-      <c r="E1113" s="167"/>
+      <c r="C1113" s="169"/>
+      <c r="D1113" s="170"/>
+      <c r="E1113" s="170"/>
     </row>
     <row r="1114" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1114" s="69">
@@ -14941,9 +14943,9 @@
         <v>87</v>
       </c>
       <c r="B1130" s="87"/>
-      <c r="C1130" s="164"/>
-      <c r="D1130" s="165"/>
-      <c r="E1130" s="165"/>
+      <c r="C1130" s="167"/>
+      <c r="D1130" s="168"/>
+      <c r="E1130" s="168"/>
     </row>
     <row r="1131" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1131" s="69">
@@ -15094,9 +15096,9 @@
         <v>88</v>
       </c>
       <c r="B1147" s="87"/>
-      <c r="C1147" s="164"/>
-      <c r="D1147" s="165"/>
-      <c r="E1147" s="165"/>
+      <c r="C1147" s="167"/>
+      <c r="D1147" s="168"/>
+      <c r="E1147" s="168"/>
     </row>
     <row r="1148" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1148" s="69">
@@ -15247,9 +15249,9 @@
         <v>89</v>
       </c>
       <c r="B1164" s="87"/>
-      <c r="C1164" s="164"/>
-      <c r="D1164" s="165"/>
-      <c r="E1164" s="165"/>
+      <c r="C1164" s="167"/>
+      <c r="D1164" s="168"/>
+      <c r="E1164" s="168"/>
     </row>
     <row r="1165" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1165" s="69">
@@ -15400,9 +15402,9 @@
         <v>90</v>
       </c>
       <c r="B1181" s="87"/>
-      <c r="C1181" s="164"/>
-      <c r="D1181" s="165"/>
-      <c r="E1181" s="165"/>
+      <c r="C1181" s="167"/>
+      <c r="D1181" s="168"/>
+      <c r="E1181" s="168"/>
     </row>
     <row r="1182" spans="1:5" hidden="1" outlineLevel="3">
       <c r="A1182" s="69">
@@ -15553,9 +15555,9 @@
         <v>91</v>
       </c>
       <c r="B1198" s="87"/>
-      <c r="C1198" s="164"/>
-      <c r="D1198" s="165"/>
-      <c r="E1198" s="165"/>
+      <c r="C1198" s="167"/>
+      <c r="D1198" s="168"/>
+      <c r="E1198" s="168"/>
     </row>
     <row r="1199" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1199" s="69">
@@ -15706,9 +15708,9 @@
         <v>92</v>
       </c>
       <c r="B1215" s="87"/>
-      <c r="C1215" s="164"/>
-      <c r="D1215" s="165"/>
-      <c r="E1215" s="165"/>
+      <c r="C1215" s="167"/>
+      <c r="D1215" s="168"/>
+      <c r="E1215" s="168"/>
     </row>
     <row r="1216" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1216" s="69">
@@ -15859,9 +15861,9 @@
         <v>93</v>
       </c>
       <c r="B1232" s="87"/>
-      <c r="C1232" s="164"/>
-      <c r="D1232" s="165"/>
-      <c r="E1232" s="165"/>
+      <c r="C1232" s="167"/>
+      <c r="D1232" s="168"/>
+      <c r="E1232" s="168"/>
     </row>
     <row r="1233" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1233" s="69">
@@ -16012,9 +16014,9 @@
         <v>94</v>
       </c>
       <c r="B1249" s="87"/>
-      <c r="C1249" s="164"/>
-      <c r="D1249" s="165"/>
-      <c r="E1249" s="165"/>
+      <c r="C1249" s="167"/>
+      <c r="D1249" s="168"/>
+      <c r="E1249" s="168"/>
     </row>
     <row r="1250" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1250" s="69">
@@ -16165,9 +16167,9 @@
         <v>99</v>
       </c>
       <c r="B1266" s="87"/>
-      <c r="C1266" s="164"/>
-      <c r="D1266" s="165"/>
-      <c r="E1266" s="165"/>
+      <c r="C1266" s="167"/>
+      <c r="D1266" s="168"/>
+      <c r="E1266" s="168"/>
     </row>
     <row r="1267" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1267" s="69">
@@ -16318,9 +16320,9 @@
         <v>100</v>
       </c>
       <c r="B1283" s="87"/>
-      <c r="C1283" s="164"/>
-      <c r="D1283" s="165"/>
-      <c r="E1283" s="165"/>
+      <c r="C1283" s="167"/>
+      <c r="D1283" s="168"/>
+      <c r="E1283" s="168"/>
     </row>
     <row r="1284" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1284" s="69">
@@ -16471,9 +16473,9 @@
         <v>101</v>
       </c>
       <c r="B1300" s="87"/>
-      <c r="C1300" s="164"/>
-      <c r="D1300" s="165"/>
-      <c r="E1300" s="165"/>
+      <c r="C1300" s="167"/>
+      <c r="D1300" s="168"/>
+      <c r="E1300" s="168"/>
     </row>
     <row r="1301" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1301" s="69">
@@ -16624,9 +16626,9 @@
         <v>81</v>
       </c>
       <c r="B1317" s="87"/>
-      <c r="C1317" s="164"/>
-      <c r="D1317" s="165"/>
-      <c r="E1317" s="165"/>
+      <c r="C1317" s="167"/>
+      <c r="D1317" s="168"/>
+      <c r="E1317" s="168"/>
     </row>
     <row r="1318" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1318" s="69">
@@ -16777,9 +16779,9 @@
         <v>102</v>
       </c>
       <c r="B1334" s="87"/>
-      <c r="C1334" s="164"/>
-      <c r="D1334" s="165"/>
-      <c r="E1334" s="165"/>
+      <c r="C1334" s="167"/>
+      <c r="D1334" s="168"/>
+      <c r="E1334" s="168"/>
     </row>
     <row r="1335" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1335" s="69">
@@ -16930,9 +16932,9 @@
         <v>98</v>
       </c>
       <c r="B1351" s="87"/>
-      <c r="C1351" s="164"/>
-      <c r="D1351" s="165"/>
-      <c r="E1351" s="165"/>
+      <c r="C1351" s="167"/>
+      <c r="D1351" s="168"/>
+      <c r="E1351" s="168"/>
     </row>
     <row r="1352" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1352" s="69">
@@ -17083,18 +17085,18 @@
         <v>103</v>
       </c>
       <c r="B1368" s="41"/>
-      <c r="C1368" s="172"/>
-      <c r="D1368" s="173"/>
-      <c r="E1368" s="173"/>
+      <c r="C1368" s="179"/>
+      <c r="D1368" s="180"/>
+      <c r="E1368" s="180"/>
     </row>
     <row r="1369" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A1369" s="73" t="s">
         <v>105</v>
       </c>
       <c r="B1369" s="87"/>
-      <c r="C1369" s="164"/>
-      <c r="D1369" s="165"/>
-      <c r="E1369" s="165"/>
+      <c r="C1369" s="167"/>
+      <c r="D1369" s="168"/>
+      <c r="E1369" s="168"/>
     </row>
     <row r="1370" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1370" s="74">
@@ -17245,9 +17247,9 @@
         <v>106</v>
       </c>
       <c r="B1386" s="90"/>
-      <c r="C1386" s="166"/>
-      <c r="D1386" s="167"/>
-      <c r="E1386" s="167"/>
+      <c r="C1386" s="169"/>
+      <c r="D1386" s="170"/>
+      <c r="E1386" s="170"/>
     </row>
     <row r="1387" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1387" s="74">
@@ -17398,9 +17400,9 @@
         <v>107</v>
       </c>
       <c r="B1403" s="87"/>
-      <c r="C1403" s="164"/>
-      <c r="D1403" s="165"/>
-      <c r="E1403" s="165"/>
+      <c r="C1403" s="167"/>
+      <c r="D1403" s="168"/>
+      <c r="E1403" s="168"/>
     </row>
     <row r="1404" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1404" s="74">
@@ -17551,9 +17553,9 @@
         <v>108</v>
       </c>
       <c r="B1420" s="87"/>
-      <c r="C1420" s="164"/>
-      <c r="D1420" s="165"/>
-      <c r="E1420" s="165"/>
+      <c r="C1420" s="167"/>
+      <c r="D1420" s="168"/>
+      <c r="E1420" s="168"/>
     </row>
     <row r="1421" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1421" s="74">
@@ -17704,9 +17706,9 @@
         <v>109</v>
       </c>
       <c r="B1437" s="87"/>
-      <c r="C1437" s="164"/>
-      <c r="D1437" s="165"/>
-      <c r="E1437" s="165"/>
+      <c r="C1437" s="167"/>
+      <c r="D1437" s="168"/>
+      <c r="E1437" s="168"/>
     </row>
     <row r="1438" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1438" s="74">
@@ -17857,9 +17859,9 @@
         <v>110</v>
       </c>
       <c r="B1454" s="87"/>
-      <c r="C1454" s="164"/>
-      <c r="D1454" s="165"/>
-      <c r="E1454" s="165"/>
+      <c r="C1454" s="167"/>
+      <c r="D1454" s="168"/>
+      <c r="E1454" s="168"/>
     </row>
     <row r="1455" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1455" s="74">
@@ -18010,9 +18012,9 @@
         <v>111</v>
       </c>
       <c r="B1471" s="87"/>
-      <c r="C1471" s="164"/>
-      <c r="D1471" s="165"/>
-      <c r="E1471" s="165"/>
+      <c r="C1471" s="167"/>
+      <c r="D1471" s="168"/>
+      <c r="E1471" s="168"/>
     </row>
     <row r="1472" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1472" s="74">
@@ -18163,9 +18165,9 @@
         <v>112</v>
       </c>
       <c r="B1488" s="87"/>
-      <c r="C1488" s="164"/>
-      <c r="D1488" s="165"/>
-      <c r="E1488" s="165"/>
+      <c r="C1488" s="167"/>
+      <c r="D1488" s="168"/>
+      <c r="E1488" s="168"/>
     </row>
     <row r="1489" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1489" s="74">
@@ -18316,9 +18318,9 @@
         <v>113</v>
       </c>
       <c r="B1505" s="87"/>
-      <c r="C1505" s="164"/>
-      <c r="D1505" s="165"/>
-      <c r="E1505" s="165"/>
+      <c r="C1505" s="167"/>
+      <c r="D1505" s="168"/>
+      <c r="E1505" s="168"/>
     </row>
     <row r="1506" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1506" s="74">
@@ -18469,9 +18471,9 @@
         <v>114</v>
       </c>
       <c r="B1522" s="87"/>
-      <c r="C1522" s="164"/>
-      <c r="D1522" s="165"/>
-      <c r="E1522" s="165"/>
+      <c r="C1522" s="167"/>
+      <c r="D1522" s="168"/>
+      <c r="E1522" s="168"/>
     </row>
     <row r="1523" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1523" s="74">
@@ -18622,9 +18624,9 @@
         <v>95</v>
       </c>
       <c r="B1539" s="87"/>
-      <c r="C1539" s="164"/>
-      <c r="D1539" s="165"/>
-      <c r="E1539" s="165"/>
+      <c r="C1539" s="167"/>
+      <c r="D1539" s="168"/>
+      <c r="E1539" s="168"/>
     </row>
     <row r="1540" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1540" s="74">
@@ -18775,9 +18777,9 @@
         <v>115</v>
       </c>
       <c r="B1556" s="87"/>
-      <c r="C1556" s="164"/>
-      <c r="D1556" s="165"/>
-      <c r="E1556" s="165"/>
+      <c r="C1556" s="167"/>
+      <c r="D1556" s="168"/>
+      <c r="E1556" s="168"/>
     </row>
     <row r="1557" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1557" s="74">
@@ -18928,9 +18930,9 @@
         <v>116</v>
       </c>
       <c r="B1573" s="87"/>
-      <c r="C1573" s="164"/>
-      <c r="D1573" s="165"/>
-      <c r="E1573" s="165"/>
+      <c r="C1573" s="167"/>
+      <c r="D1573" s="168"/>
+      <c r="E1573" s="168"/>
     </row>
     <row r="1574" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1574" s="74">
@@ -19081,9 +19083,9 @@
         <v>117</v>
       </c>
       <c r="B1590" s="87"/>
-      <c r="C1590" s="164"/>
-      <c r="D1590" s="165"/>
-      <c r="E1590" s="165"/>
+      <c r="C1590" s="167"/>
+      <c r="D1590" s="168"/>
+      <c r="E1590" s="168"/>
     </row>
     <row r="1591" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1591" s="74">
@@ -19234,9 +19236,9 @@
         <v>118</v>
       </c>
       <c r="B1607" s="87"/>
-      <c r="C1607" s="164"/>
-      <c r="D1607" s="165"/>
-      <c r="E1607" s="165"/>
+      <c r="C1607" s="167"/>
+      <c r="D1607" s="168"/>
+      <c r="E1607" s="168"/>
     </row>
     <row r="1608" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1608" s="74">
@@ -19387,9 +19389,9 @@
         <v>119</v>
       </c>
       <c r="B1624" s="87"/>
-      <c r="C1624" s="164"/>
-      <c r="D1624" s="165"/>
-      <c r="E1624" s="165"/>
+      <c r="C1624" s="167"/>
+      <c r="D1624" s="168"/>
+      <c r="E1624" s="168"/>
     </row>
     <row r="1625" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1625" s="74">
@@ -19540,18 +19542,18 @@
         <v>120</v>
       </c>
       <c r="B1641" s="42"/>
-      <c r="C1641" s="170"/>
-      <c r="D1641" s="171"/>
-      <c r="E1641" s="171"/>
+      <c r="C1641" s="181"/>
+      <c r="D1641" s="182"/>
+      <c r="E1641" s="182"/>
     </row>
     <row r="1642" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A1642" s="78" t="s">
         <v>121</v>
       </c>
       <c r="B1642" s="87"/>
-      <c r="C1642" s="164"/>
-      <c r="D1642" s="165"/>
-      <c r="E1642" s="165"/>
+      <c r="C1642" s="167"/>
+      <c r="D1642" s="168"/>
+      <c r="E1642" s="168"/>
     </row>
     <row r="1643" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1643" s="79">
@@ -19702,9 +19704,9 @@
         <v>122</v>
       </c>
       <c r="B1659" s="90"/>
-      <c r="C1659" s="166"/>
-      <c r="D1659" s="167"/>
-      <c r="E1659" s="167"/>
+      <c r="C1659" s="169"/>
+      <c r="D1659" s="170"/>
+      <c r="E1659" s="170"/>
     </row>
     <row r="1660" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1660" s="79">
@@ -19855,9 +19857,9 @@
         <v>123</v>
       </c>
       <c r="B1676" s="87"/>
-      <c r="C1676" s="164"/>
-      <c r="D1676" s="165"/>
-      <c r="E1676" s="165"/>
+      <c r="C1676" s="167"/>
+      <c r="D1676" s="168"/>
+      <c r="E1676" s="168"/>
     </row>
     <row r="1677" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1677" s="79">
@@ -20008,9 +20010,9 @@
         <v>124</v>
       </c>
       <c r="B1693" s="87"/>
-      <c r="C1693" s="164"/>
-      <c r="D1693" s="165"/>
-      <c r="E1693" s="165"/>
+      <c r="C1693" s="167"/>
+      <c r="D1693" s="168"/>
+      <c r="E1693" s="168"/>
     </row>
     <row r="1694" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1694" s="79">
@@ -20161,9 +20163,9 @@
         <v>125</v>
       </c>
       <c r="B1710" s="87"/>
-      <c r="C1710" s="164"/>
-      <c r="D1710" s="165"/>
-      <c r="E1710" s="165"/>
+      <c r="C1710" s="167"/>
+      <c r="D1710" s="168"/>
+      <c r="E1710" s="168"/>
     </row>
     <row r="1711" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1711" s="79">
@@ -20314,9 +20316,9 @@
         <v>126</v>
       </c>
       <c r="B1727" s="87"/>
-      <c r="C1727" s="164"/>
-      <c r="D1727" s="165"/>
-      <c r="E1727" s="165"/>
+      <c r="C1727" s="167"/>
+      <c r="D1727" s="168"/>
+      <c r="E1727" s="168"/>
     </row>
     <row r="1728" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1728" s="79">
@@ -20467,9 +20469,9 @@
         <v>127</v>
       </c>
       <c r="B1744" s="87"/>
-      <c r="C1744" s="164"/>
-      <c r="D1744" s="165"/>
-      <c r="E1744" s="165"/>
+      <c r="C1744" s="167"/>
+      <c r="D1744" s="168"/>
+      <c r="E1744" s="168"/>
     </row>
     <row r="1745" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1745" s="79">
@@ -20620,9 +20622,9 @@
         <v>128</v>
       </c>
       <c r="B1761" s="87"/>
-      <c r="C1761" s="164"/>
-      <c r="D1761" s="165"/>
-      <c r="E1761" s="165"/>
+      <c r="C1761" s="167"/>
+      <c r="D1761" s="168"/>
+      <c r="E1761" s="168"/>
     </row>
     <row r="1762" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1762" s="79">
@@ -20773,9 +20775,9 @@
         <v>129</v>
       </c>
       <c r="B1778" s="87"/>
-      <c r="C1778" s="164"/>
-      <c r="D1778" s="165"/>
-      <c r="E1778" s="165"/>
+      <c r="C1778" s="167"/>
+      <c r="D1778" s="168"/>
+      <c r="E1778" s="168"/>
     </row>
     <row r="1779" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1779" s="79">
@@ -20926,9 +20928,9 @@
         <v>130</v>
       </c>
       <c r="B1795" s="87"/>
-      <c r="C1795" s="164"/>
-      <c r="D1795" s="165"/>
-      <c r="E1795" s="165"/>
+      <c r="C1795" s="167"/>
+      <c r="D1795" s="168"/>
+      <c r="E1795" s="168"/>
     </row>
     <row r="1796" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1796" s="79">
@@ -21079,9 +21081,9 @@
         <v>131</v>
       </c>
       <c r="B1812" s="87"/>
-      <c r="C1812" s="164"/>
-      <c r="D1812" s="165"/>
-      <c r="E1812" s="165"/>
+      <c r="C1812" s="167"/>
+      <c r="D1812" s="168"/>
+      <c r="E1812" s="168"/>
     </row>
     <row r="1813" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1813" s="79">
@@ -21232,9 +21234,9 @@
         <v>96</v>
       </c>
       <c r="B1829" s="87"/>
-      <c r="C1829" s="164"/>
-      <c r="D1829" s="165"/>
-      <c r="E1829" s="165"/>
+      <c r="C1829" s="167"/>
+      <c r="D1829" s="168"/>
+      <c r="E1829" s="168"/>
     </row>
     <row r="1830" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1830" s="79">
@@ -21385,9 +21387,9 @@
         <v>132</v>
       </c>
       <c r="B1846" s="87"/>
-      <c r="C1846" s="164"/>
-      <c r="D1846" s="165"/>
-      <c r="E1846" s="165"/>
+      <c r="C1846" s="167"/>
+      <c r="D1846" s="168"/>
+      <c r="E1846" s="168"/>
     </row>
     <row r="1847" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1847" s="79">
@@ -21538,9 +21540,9 @@
         <v>133</v>
       </c>
       <c r="B1863" s="87"/>
-      <c r="C1863" s="164"/>
-      <c r="D1863" s="165"/>
-      <c r="E1863" s="165"/>
+      <c r="C1863" s="167"/>
+      <c r="D1863" s="168"/>
+      <c r="E1863" s="168"/>
     </row>
     <row r="1864" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1864" s="79">
@@ -21691,9 +21693,9 @@
         <v>134</v>
       </c>
       <c r="B1880" s="87"/>
-      <c r="C1880" s="164"/>
-      <c r="D1880" s="165"/>
-      <c r="E1880" s="165"/>
+      <c r="C1880" s="167"/>
+      <c r="D1880" s="168"/>
+      <c r="E1880" s="168"/>
     </row>
     <row r="1881" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1881" s="79">
@@ -21844,9 +21846,9 @@
         <v>135</v>
       </c>
       <c r="B1897" s="87"/>
-      <c r="C1897" s="164"/>
-      <c r="D1897" s="165"/>
-      <c r="E1897" s="165"/>
+      <c r="C1897" s="167"/>
+      <c r="D1897" s="168"/>
+      <c r="E1897" s="168"/>
     </row>
     <row r="1898" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1898" s="79">
@@ -21997,18 +21999,18 @@
         <v>136</v>
       </c>
       <c r="B1914" s="43"/>
-      <c r="C1914" s="168"/>
-      <c r="D1914" s="169"/>
-      <c r="E1914" s="169"/>
+      <c r="C1914" s="183"/>
+      <c r="D1914" s="184"/>
+      <c r="E1914" s="184"/>
     </row>
     <row r="1915" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A1915" s="83" t="s">
         <v>137</v>
       </c>
       <c r="B1915" s="87"/>
-      <c r="C1915" s="164"/>
-      <c r="D1915" s="165"/>
-      <c r="E1915" s="165"/>
+      <c r="C1915" s="167"/>
+      <c r="D1915" s="168"/>
+      <c r="E1915" s="168"/>
     </row>
     <row r="1916" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1916" s="84">
@@ -22159,9 +22161,9 @@
         <v>138</v>
       </c>
       <c r="B1932" s="90"/>
-      <c r="C1932" s="166"/>
-      <c r="D1932" s="167"/>
-      <c r="E1932" s="167"/>
+      <c r="C1932" s="169"/>
+      <c r="D1932" s="170"/>
+      <c r="E1932" s="170"/>
     </row>
     <row r="1933" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1933" s="84">
@@ -22312,9 +22314,9 @@
         <v>139</v>
       </c>
       <c r="B1949" s="87"/>
-      <c r="C1949" s="164"/>
-      <c r="D1949" s="165"/>
-      <c r="E1949" s="165"/>
+      <c r="C1949" s="167"/>
+      <c r="D1949" s="168"/>
+      <c r="E1949" s="168"/>
     </row>
     <row r="1950" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1950" s="84">
@@ -22465,9 +22467,9 @@
         <v>140</v>
       </c>
       <c r="B1966" s="87"/>
-      <c r="C1966" s="164"/>
-      <c r="D1966" s="165"/>
-      <c r="E1966" s="165"/>
+      <c r="C1966" s="167"/>
+      <c r="D1966" s="168"/>
+      <c r="E1966" s="168"/>
     </row>
     <row r="1967" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1967" s="84">
@@ -22618,9 +22620,9 @@
         <v>141</v>
       </c>
       <c r="B1983" s="87"/>
-      <c r="C1983" s="164"/>
-      <c r="D1983" s="165"/>
-      <c r="E1983" s="165"/>
+      <c r="C1983" s="167"/>
+      <c r="D1983" s="168"/>
+      <c r="E1983" s="168"/>
     </row>
     <row r="1984" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1984" s="84">
@@ -22771,9 +22773,9 @@
         <v>142</v>
       </c>
       <c r="B2000" s="87"/>
-      <c r="C2000" s="164"/>
-      <c r="D2000" s="165"/>
-      <c r="E2000" s="165"/>
+      <c r="C2000" s="167"/>
+      <c r="D2000" s="168"/>
+      <c r="E2000" s="168"/>
     </row>
     <row r="2001" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2001" s="84">
@@ -22924,9 +22926,9 @@
         <v>143</v>
       </c>
       <c r="B2017" s="87"/>
-      <c r="C2017" s="164"/>
-      <c r="D2017" s="165"/>
-      <c r="E2017" s="165"/>
+      <c r="C2017" s="167"/>
+      <c r="D2017" s="168"/>
+      <c r="E2017" s="168"/>
     </row>
     <row r="2018" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2018" s="84">
@@ -23077,9 +23079,9 @@
         <v>144</v>
       </c>
       <c r="B2034" s="87"/>
-      <c r="C2034" s="164"/>
-      <c r="D2034" s="165"/>
-      <c r="E2034" s="165"/>
+      <c r="C2034" s="167"/>
+      <c r="D2034" s="168"/>
+      <c r="E2034" s="168"/>
     </row>
     <row r="2035" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2035" s="84">
@@ -23230,9 +23232,9 @@
         <v>145</v>
       </c>
       <c r="B2051" s="87"/>
-      <c r="C2051" s="164"/>
-      <c r="D2051" s="165"/>
-      <c r="E2051" s="165"/>
+      <c r="C2051" s="167"/>
+      <c r="D2051" s="168"/>
+      <c r="E2051" s="168"/>
     </row>
     <row r="2052" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2052" s="84">
@@ -23383,9 +23385,9 @@
         <v>146</v>
       </c>
       <c r="B2068" s="87"/>
-      <c r="C2068" s="164"/>
-      <c r="D2068" s="165"/>
-      <c r="E2068" s="165"/>
+      <c r="C2068" s="167"/>
+      <c r="D2068" s="168"/>
+      <c r="E2068" s="168"/>
     </row>
     <row r="2069" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2069" s="84">
@@ -23536,9 +23538,9 @@
         <v>147</v>
       </c>
       <c r="B2085" s="87"/>
-      <c r="C2085" s="164"/>
-      <c r="D2085" s="165"/>
-      <c r="E2085" s="165"/>
+      <c r="C2085" s="167"/>
+      <c r="D2085" s="168"/>
+      <c r="E2085" s="168"/>
     </row>
     <row r="2086" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2086" s="84">
@@ -23689,9 +23691,9 @@
         <v>148</v>
       </c>
       <c r="B2102" s="87"/>
-      <c r="C2102" s="164"/>
-      <c r="D2102" s="165"/>
-      <c r="E2102" s="165"/>
+      <c r="C2102" s="167"/>
+      <c r="D2102" s="168"/>
+      <c r="E2102" s="168"/>
     </row>
     <row r="2103" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2103" s="84">
@@ -23842,9 +23844,9 @@
         <v>97</v>
       </c>
       <c r="B2119" s="87"/>
-      <c r="C2119" s="164"/>
-      <c r="D2119" s="165"/>
-      <c r="E2119" s="165"/>
+      <c r="C2119" s="167"/>
+      <c r="D2119" s="168"/>
+      <c r="E2119" s="168"/>
     </row>
     <row r="2120" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2120" s="84">
@@ -23995,9 +23997,9 @@
         <v>149</v>
       </c>
       <c r="B2136" s="87"/>
-      <c r="C2136" s="164"/>
-      <c r="D2136" s="165"/>
-      <c r="E2136" s="165"/>
+      <c r="C2136" s="167"/>
+      <c r="D2136" s="168"/>
+      <c r="E2136" s="168"/>
     </row>
     <row r="2137" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2137" s="84">
@@ -24148,9 +24150,9 @@
         <v>150</v>
       </c>
       <c r="B2153" s="87"/>
-      <c r="C2153" s="164"/>
-      <c r="D2153" s="165"/>
-      <c r="E2153" s="165"/>
+      <c r="C2153" s="167"/>
+      <c r="D2153" s="168"/>
+      <c r="E2153" s="168"/>
     </row>
     <row r="2154" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2154" s="84">
@@ -24301,9 +24303,9 @@
         <v>151</v>
       </c>
       <c r="B2170" s="87"/>
-      <c r="C2170" s="164"/>
-      <c r="D2170" s="165"/>
-      <c r="E2170" s="165"/>
+      <c r="C2170" s="167"/>
+      <c r="D2170" s="168"/>
+      <c r="E2170" s="168"/>
     </row>
     <row r="2171" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2171" s="84">
@@ -24451,26 +24453,111 @@
     </row>
   </sheetData>
   <mergeCells count="137">
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="C89:E89"/>
-    <mergeCell ref="C21:E21"/>
-    <mergeCell ref="C38:E38"/>
-    <mergeCell ref="C55:E55"/>
-    <mergeCell ref="C72:E72"/>
-    <mergeCell ref="C208:E208"/>
-    <mergeCell ref="C225:E225"/>
-    <mergeCell ref="C242:E242"/>
-    <mergeCell ref="C259:E259"/>
-    <mergeCell ref="C276:E276"/>
-    <mergeCell ref="C277:E277"/>
-    <mergeCell ref="C106:E106"/>
-    <mergeCell ref="C123:E123"/>
-    <mergeCell ref="C140:E140"/>
-    <mergeCell ref="C157:E157"/>
-    <mergeCell ref="C174:E174"/>
-    <mergeCell ref="C191:E191"/>
+    <mergeCell ref="C2034:E2034"/>
+    <mergeCell ref="C2051:E2051"/>
+    <mergeCell ref="C2068:E2068"/>
+    <mergeCell ref="C2085:E2085"/>
+    <mergeCell ref="C2170:E2170"/>
+    <mergeCell ref="C2102:E2102"/>
+    <mergeCell ref="C2119:E2119"/>
+    <mergeCell ref="C2136:E2136"/>
+    <mergeCell ref="C2153:E2153"/>
+    <mergeCell ref="C1932:E1932"/>
+    <mergeCell ref="C1949:E1949"/>
+    <mergeCell ref="C1966:E1966"/>
+    <mergeCell ref="C1983:E1983"/>
+    <mergeCell ref="C2000:E2000"/>
+    <mergeCell ref="C2017:E2017"/>
+    <mergeCell ref="C1846:E1846"/>
+    <mergeCell ref="C1863:E1863"/>
+    <mergeCell ref="C1880:E1880"/>
+    <mergeCell ref="C1897:E1897"/>
+    <mergeCell ref="C1914:E1914"/>
+    <mergeCell ref="C1915:E1915"/>
+    <mergeCell ref="C1744:E1744"/>
+    <mergeCell ref="C1761:E1761"/>
+    <mergeCell ref="C1778:E1778"/>
+    <mergeCell ref="C1795:E1795"/>
+    <mergeCell ref="C1812:E1812"/>
+    <mergeCell ref="C1829:E1829"/>
+    <mergeCell ref="C1642:E1642"/>
+    <mergeCell ref="C1659:E1659"/>
+    <mergeCell ref="C1676:E1676"/>
+    <mergeCell ref="C1693:E1693"/>
+    <mergeCell ref="C1710:E1710"/>
+    <mergeCell ref="C1727:E1727"/>
+    <mergeCell ref="C1556:E1556"/>
+    <mergeCell ref="C1573:E1573"/>
+    <mergeCell ref="C1590:E1590"/>
+    <mergeCell ref="C1607:E1607"/>
+    <mergeCell ref="C1624:E1624"/>
+    <mergeCell ref="C1641:E1641"/>
+    <mergeCell ref="C1454:E1454"/>
+    <mergeCell ref="C1471:E1471"/>
+    <mergeCell ref="C1488:E1488"/>
+    <mergeCell ref="C1505:E1505"/>
+    <mergeCell ref="C1522:E1522"/>
+    <mergeCell ref="C1539:E1539"/>
+    <mergeCell ref="C1368:E1368"/>
+    <mergeCell ref="C1369:E1369"/>
+    <mergeCell ref="C1386:E1386"/>
+    <mergeCell ref="C1403:E1403"/>
+    <mergeCell ref="C1420:E1420"/>
+    <mergeCell ref="C1437:E1437"/>
+    <mergeCell ref="C1266:E1266"/>
+    <mergeCell ref="C1283:E1283"/>
+    <mergeCell ref="C1300:E1300"/>
+    <mergeCell ref="C1317:E1317"/>
+    <mergeCell ref="C1334:E1334"/>
+    <mergeCell ref="C1351:E1351"/>
+    <mergeCell ref="C1164:E1164"/>
+    <mergeCell ref="C1181:E1181"/>
+    <mergeCell ref="C1198:E1198"/>
+    <mergeCell ref="C1215:E1215"/>
+    <mergeCell ref="C1232:E1232"/>
+    <mergeCell ref="C1249:E1249"/>
+    <mergeCell ref="C1078:E1078"/>
+    <mergeCell ref="C1095:E1095"/>
+    <mergeCell ref="C1096:E1096"/>
+    <mergeCell ref="C1113:E1113"/>
+    <mergeCell ref="C1130:E1130"/>
+    <mergeCell ref="C1147:E1147"/>
+    <mergeCell ref="C976:E976"/>
+    <mergeCell ref="C993:E993"/>
+    <mergeCell ref="C1010:E1010"/>
+    <mergeCell ref="C1027:E1027"/>
+    <mergeCell ref="C1044:E1044"/>
+    <mergeCell ref="C1061:E1061"/>
+    <mergeCell ref="C874:E874"/>
+    <mergeCell ref="C891:E891"/>
+    <mergeCell ref="C908:E908"/>
+    <mergeCell ref="C925:E925"/>
+    <mergeCell ref="C942:E942"/>
+    <mergeCell ref="C959:E959"/>
+    <mergeCell ref="C788:E788"/>
+    <mergeCell ref="C805:E805"/>
+    <mergeCell ref="C822:E822"/>
+    <mergeCell ref="C823:E823"/>
+    <mergeCell ref="C840:E840"/>
+    <mergeCell ref="C857:E857"/>
+    <mergeCell ref="C686:E686"/>
+    <mergeCell ref="C703:E703"/>
+    <mergeCell ref="C720:E720"/>
+    <mergeCell ref="C737:E737"/>
+    <mergeCell ref="C754:E754"/>
+    <mergeCell ref="C771:E771"/>
+    <mergeCell ref="C584:E584"/>
+    <mergeCell ref="C601:E601"/>
+    <mergeCell ref="C618:E618"/>
+    <mergeCell ref="C635:E635"/>
+    <mergeCell ref="C652:E652"/>
+    <mergeCell ref="C669:E669"/>
+    <mergeCell ref="C498:E498"/>
+    <mergeCell ref="C515:E515"/>
+    <mergeCell ref="C532:E532"/>
+    <mergeCell ref="C549:E549"/>
+    <mergeCell ref="C550:E550"/>
+    <mergeCell ref="C567:E567"/>
     <mergeCell ref="C396:E396"/>
     <mergeCell ref="C413:E413"/>
     <mergeCell ref="C430:E430"/>
@@ -24483,111 +24570,26 @@
     <mergeCell ref="C345:E345"/>
     <mergeCell ref="C362:E362"/>
     <mergeCell ref="C379:E379"/>
-    <mergeCell ref="C584:E584"/>
-    <mergeCell ref="C601:E601"/>
-    <mergeCell ref="C618:E618"/>
-    <mergeCell ref="C635:E635"/>
-    <mergeCell ref="C652:E652"/>
-    <mergeCell ref="C669:E669"/>
-    <mergeCell ref="C498:E498"/>
-    <mergeCell ref="C515:E515"/>
-    <mergeCell ref="C532:E532"/>
-    <mergeCell ref="C549:E549"/>
-    <mergeCell ref="C550:E550"/>
-    <mergeCell ref="C567:E567"/>
-    <mergeCell ref="C788:E788"/>
-    <mergeCell ref="C805:E805"/>
-    <mergeCell ref="C822:E822"/>
-    <mergeCell ref="C823:E823"/>
-    <mergeCell ref="C840:E840"/>
-    <mergeCell ref="C857:E857"/>
-    <mergeCell ref="C686:E686"/>
-    <mergeCell ref="C703:E703"/>
-    <mergeCell ref="C720:E720"/>
-    <mergeCell ref="C737:E737"/>
-    <mergeCell ref="C754:E754"/>
-    <mergeCell ref="C771:E771"/>
-    <mergeCell ref="C976:E976"/>
-    <mergeCell ref="C993:E993"/>
-    <mergeCell ref="C1010:E1010"/>
-    <mergeCell ref="C1027:E1027"/>
-    <mergeCell ref="C1044:E1044"/>
-    <mergeCell ref="C1061:E1061"/>
-    <mergeCell ref="C874:E874"/>
-    <mergeCell ref="C891:E891"/>
-    <mergeCell ref="C908:E908"/>
-    <mergeCell ref="C925:E925"/>
-    <mergeCell ref="C942:E942"/>
-    <mergeCell ref="C959:E959"/>
-    <mergeCell ref="C1164:E1164"/>
-    <mergeCell ref="C1181:E1181"/>
-    <mergeCell ref="C1198:E1198"/>
-    <mergeCell ref="C1215:E1215"/>
-    <mergeCell ref="C1232:E1232"/>
-    <mergeCell ref="C1249:E1249"/>
-    <mergeCell ref="C1078:E1078"/>
-    <mergeCell ref="C1095:E1095"/>
-    <mergeCell ref="C1096:E1096"/>
-    <mergeCell ref="C1113:E1113"/>
-    <mergeCell ref="C1130:E1130"/>
-    <mergeCell ref="C1147:E1147"/>
-    <mergeCell ref="C1368:E1368"/>
-    <mergeCell ref="C1369:E1369"/>
-    <mergeCell ref="C1386:E1386"/>
-    <mergeCell ref="C1403:E1403"/>
-    <mergeCell ref="C1420:E1420"/>
-    <mergeCell ref="C1437:E1437"/>
-    <mergeCell ref="C1266:E1266"/>
-    <mergeCell ref="C1283:E1283"/>
-    <mergeCell ref="C1300:E1300"/>
-    <mergeCell ref="C1317:E1317"/>
-    <mergeCell ref="C1334:E1334"/>
-    <mergeCell ref="C1351:E1351"/>
-    <mergeCell ref="C1556:E1556"/>
-    <mergeCell ref="C1573:E1573"/>
-    <mergeCell ref="C1590:E1590"/>
-    <mergeCell ref="C1607:E1607"/>
-    <mergeCell ref="C1624:E1624"/>
-    <mergeCell ref="C1641:E1641"/>
-    <mergeCell ref="C1454:E1454"/>
-    <mergeCell ref="C1471:E1471"/>
-    <mergeCell ref="C1488:E1488"/>
-    <mergeCell ref="C1505:E1505"/>
-    <mergeCell ref="C1522:E1522"/>
-    <mergeCell ref="C1539:E1539"/>
-    <mergeCell ref="C1744:E1744"/>
-    <mergeCell ref="C1761:E1761"/>
-    <mergeCell ref="C1778:E1778"/>
-    <mergeCell ref="C1795:E1795"/>
-    <mergeCell ref="C1812:E1812"/>
-    <mergeCell ref="C1829:E1829"/>
-    <mergeCell ref="C1642:E1642"/>
-    <mergeCell ref="C1659:E1659"/>
-    <mergeCell ref="C1676:E1676"/>
-    <mergeCell ref="C1693:E1693"/>
-    <mergeCell ref="C1710:E1710"/>
-    <mergeCell ref="C1727:E1727"/>
-    <mergeCell ref="C1932:E1932"/>
-    <mergeCell ref="C1949:E1949"/>
-    <mergeCell ref="C1966:E1966"/>
-    <mergeCell ref="C1983:E1983"/>
-    <mergeCell ref="C2000:E2000"/>
-    <mergeCell ref="C2017:E2017"/>
-    <mergeCell ref="C1846:E1846"/>
-    <mergeCell ref="C1863:E1863"/>
-    <mergeCell ref="C1880:E1880"/>
-    <mergeCell ref="C1897:E1897"/>
-    <mergeCell ref="C1914:E1914"/>
-    <mergeCell ref="C1915:E1915"/>
-    <mergeCell ref="C2034:E2034"/>
-    <mergeCell ref="C2051:E2051"/>
-    <mergeCell ref="C2068:E2068"/>
-    <mergeCell ref="C2085:E2085"/>
-    <mergeCell ref="C2170:E2170"/>
-    <mergeCell ref="C2102:E2102"/>
-    <mergeCell ref="C2119:E2119"/>
-    <mergeCell ref="C2136:E2136"/>
-    <mergeCell ref="C2153:E2153"/>
+    <mergeCell ref="C225:E225"/>
+    <mergeCell ref="C242:E242"/>
+    <mergeCell ref="C259:E259"/>
+    <mergeCell ref="C276:E276"/>
+    <mergeCell ref="C277:E277"/>
+    <mergeCell ref="C106:E106"/>
+    <mergeCell ref="C123:E123"/>
+    <mergeCell ref="C140:E140"/>
+    <mergeCell ref="C157:E157"/>
+    <mergeCell ref="C174:E174"/>
+    <mergeCell ref="C191:E191"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="C89:E89"/>
+    <mergeCell ref="C21:E21"/>
+    <mergeCell ref="C38:E38"/>
+    <mergeCell ref="C55:E55"/>
+    <mergeCell ref="C72:E72"/>
+    <mergeCell ref="C208:E208"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -25846,163 +25848,150 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="33">
-      <c r="A1" s="209" t="s">
+      <c r="A1" s="210" t="s">
         <v>184</v>
       </c>
-      <c r="B1" s="210"/>
+      <c r="B1" s="211"/>
       <c r="C1" s="118"/>
       <c r="D1" s="5"/>
       <c r="E1" s="5"/>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="206" t="s">
+      <c r="A2" s="216" t="s">
         <v>183</v>
       </c>
-      <c r="B2" s="207"/>
+      <c r="B2" s="217"/>
       <c r="C2" s="120"/>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="208" t="s">
+      <c r="A3" s="218" t="s">
         <v>185</v>
       </c>
-      <c r="B3" s="207"/>
+      <c r="B3" s="217"/>
       <c r="C3" s="120"/>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="213"/>
-      <c r="B4" s="214"/>
+      <c r="A4" s="214"/>
+      <c r="B4" s="215"/>
       <c r="C4" s="120"/>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="211" t="s">
+      <c r="A5" s="212" t="s">
         <v>194</v>
       </c>
-      <c r="B5" s="212"/>
+      <c r="B5" s="213"/>
       <c r="C5" s="120"/>
     </row>
     <row r="7" spans="1:5" ht="18.75">
-      <c r="A7" s="217" t="s">
+      <c r="A7" s="204" t="s">
         <v>186</v>
       </c>
-      <c r="B7" s="218"/>
+      <c r="B7" s="205"/>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="120"/>
       <c r="B8" s="9"/>
     </row>
     <row r="9" spans="1:5" ht="39" customHeight="1">
-      <c r="A9" s="215" t="s">
+      <c r="A9" s="206" t="s">
         <v>187</v>
       </c>
-      <c r="B9" s="216"/>
+      <c r="B9" s="207"/>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="202"/>
-      <c r="B10" s="203"/>
+      <c r="A10" s="208"/>
+      <c r="B10" s="209"/>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="204" t="s">
+      <c r="A11" s="200" t="s">
         <v>188</v>
       </c>
-      <c r="B11" s="205"/>
+      <c r="B11" s="201"/>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="204" t="s">
+      <c r="A12" s="200" t="s">
         <v>189</v>
       </c>
-      <c r="B12" s="205"/>
+      <c r="B12" s="201"/>
     </row>
     <row r="13" spans="1:5" ht="43.5" customHeight="1">
-      <c r="A13" s="204" t="s">
+      <c r="A13" s="200" t="s">
         <v>190</v>
       </c>
-      <c r="B13" s="205"/>
+      <c r="B13" s="201"/>
     </row>
     <row r="14" spans="1:5" ht="19.5" customHeight="1">
-      <c r="A14" s="204" t="s">
+      <c r="A14" s="200" t="s">
         <v>191</v>
       </c>
-      <c r="B14" s="205"/>
+      <c r="B14" s="201"/>
     </row>
     <row r="15" spans="1:5" ht="18" customHeight="1">
-      <c r="A15" s="204" t="s">
+      <c r="A15" s="200" t="s">
         <v>192</v>
       </c>
-      <c r="B15" s="205"/>
+      <c r="B15" s="201"/>
     </row>
     <row r="16" spans="1:5" ht="21" customHeight="1">
-      <c r="A16" s="204" t="s">
+      <c r="A16" s="200" t="s">
         <v>193</v>
       </c>
-      <c r="B16" s="205"/>
+      <c r="B16" s="201"/>
     </row>
     <row r="17" spans="1:2" ht="48.75" customHeight="1">
-      <c r="A17" s="200" t="s">
+      <c r="A17" s="202" t="s">
         <v>195</v>
       </c>
-      <c r="B17" s="201"/>
+      <c r="B17" s="203"/>
     </row>
     <row r="19" spans="1:2" ht="18.75">
-      <c r="A19" s="217" t="s">
+      <c r="A19" s="204" t="s">
         <v>197</v>
       </c>
-      <c r="B19" s="218"/>
+      <c r="B19" s="205"/>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="120"/>
       <c r="B20" s="9"/>
     </row>
     <row r="21" spans="1:2">
-      <c r="A21" s="215" t="s">
+      <c r="A21" s="206" t="s">
         <v>198</v>
       </c>
-      <c r="B21" s="216"/>
+      <c r="B21" s="207"/>
     </row>
     <row r="22" spans="1:2">
-      <c r="A22" s="202"/>
-      <c r="B22" s="203"/>
+      <c r="A22" s="208"/>
+      <c r="B22" s="209"/>
     </row>
     <row r="23" spans="1:2">
-      <c r="A23" s="204" t="s">
+      <c r="A23" s="200" t="s">
         <v>199</v>
       </c>
-      <c r="B23" s="205"/>
+      <c r="B23" s="201"/>
     </row>
     <row r="24" spans="1:2">
-      <c r="A24" s="204"/>
-      <c r="B24" s="205"/>
+      <c r="A24" s="200"/>
+      <c r="B24" s="201"/>
     </row>
     <row r="25" spans="1:2">
-      <c r="A25" s="204" t="s">
+      <c r="A25" s="200" t="s">
         <v>200</v>
       </c>
-      <c r="B25" s="205"/>
+      <c r="B25" s="201"/>
     </row>
     <row r="26" spans="1:2">
-      <c r="A26" s="204" t="s">
+      <c r="A26" s="200" t="s">
         <v>201</v>
       </c>
-      <c r="B26" s="205"/>
+      <c r="B26" s="201"/>
     </row>
     <row r="27" spans="1:2">
-      <c r="A27" s="200"/>
-      <c r="B27" s="201"/>
+      <c r="A27" s="202"/>
+      <c r="B27" s="203"/>
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A7:B7"/>
     <mergeCell ref="A17:B17"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
@@ -26013,6 +26002,19 @@
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="A14:B14"/>
     <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A24:B24"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A3" r:id="rId1"/>

</xml_diff>

<commit_message>
Tempo - 1-1 15 frames faster.  Plus some clean up of the spreadsheet.
</commit_message>
<xml_diff>
--- a/trunk/Tempo/Tempo.xlsx
+++ b/trunk/Tempo/Tempo.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="60" windowWidth="11340" windowHeight="8580"/>
@@ -14,12 +14,12 @@
     <sheet name="About Versions" sheetId="9" r:id="rId5"/>
     <sheet name="Documentation" sheetId="11" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1140" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1141" uniqueCount="264">
   <si>
     <t>Notes</t>
   </si>
@@ -848,6 +848,9 @@
   </si>
   <si>
     <t>Enter Final Boss</t>
+  </si>
+  <si>
+    <t>4160 = cardboard attempt</t>
   </si>
 </sst>
 </file>
@@ -2128,29 +2131,29 @@
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -2186,34 +2189,20 @@
     <xf numFmtId="0" fontId="47" fillId="22" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="41" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="4"/>
     </xf>
@@ -2223,6 +2212,20 @@
     <xf numFmtId="0" fontId="42" fillId="0" borderId="33" xfId="3" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" indent="4"/>
     </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Accent1" xfId="2" builtinId="29"/>
@@ -2533,13 +2536,13 @@
   <dimension ref="A1:K150"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C31" sqref="C31"/>
+      <pane ySplit="6" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" outlineLevelRow="2"/>
   <cols>
-    <col min="2" max="2" width="26.140625" customWidth="1"/>
+    <col min="2" max="2" width="30" bestFit="1" customWidth="1"/>
     <col min="3" max="5" width="7.28515625" customWidth="1"/>
     <col min="6" max="6" width="11.140625" customWidth="1"/>
     <col min="7" max="7" width="9.140625" hidden="1" customWidth="1"/>
@@ -2735,9 +2738,11 @@
       <c r="B10" s="149" t="s">
         <v>208</v>
       </c>
-      <c r="C10" s="101"/>
+      <c r="C10" s="101">
+        <v>512</v>
+      </c>
       <c r="D10" s="101">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="E10" s="101">
         <f t="shared" ref="E10:E18" si="0">IF(AND(C10&gt;0,D10&gt;0), D10-C10, 0)</f>
@@ -2750,9 +2755,11 @@
       <c r="B11" s="149" t="s">
         <v>214</v>
       </c>
-      <c r="C11" s="101"/>
+      <c r="C11" s="101">
+        <v>1046</v>
+      </c>
       <c r="D11" s="101">
-        <v>1052</v>
+        <v>1046</v>
       </c>
       <c r="E11" s="101">
         <f t="shared" si="0"/>
@@ -2765,7 +2772,9 @@
       <c r="B12" s="149" t="s">
         <v>209</v>
       </c>
-      <c r="C12" s="101"/>
+      <c r="C12" s="101">
+        <v>1118</v>
+      </c>
       <c r="D12" s="101">
         <v>1118</v>
       </c>
@@ -2780,7 +2789,9 @@
       <c r="B13" s="149" t="s">
         <v>213</v>
       </c>
-      <c r="C13" s="101"/>
+      <c r="C13" s="101">
+        <v>1306</v>
+      </c>
       <c r="D13" s="101">
         <v>1306</v>
       </c>
@@ -2795,9 +2806,11 @@
       <c r="B14" s="149" t="s">
         <v>214</v>
       </c>
-      <c r="C14" s="101"/>
+      <c r="C14" s="101">
+        <v>1842</v>
+      </c>
       <c r="D14" s="101">
-        <v>1848</v>
+        <v>1842</v>
       </c>
       <c r="E14" s="101">
         <f t="shared" si="0"/>
@@ -2810,7 +2823,9 @@
       <c r="B15" s="149" t="s">
         <v>215</v>
       </c>
-      <c r="C15" s="101"/>
+      <c r="C15" s="101">
+        <v>1910</v>
+      </c>
       <c r="D15" s="101">
         <v>1910</v>
       </c>
@@ -2825,7 +2840,9 @@
       <c r="B16" s="149" t="s">
         <v>216</v>
       </c>
-      <c r="C16" s="101"/>
+      <c r="C16" s="101">
+        <v>2494</v>
+      </c>
       <c r="D16" s="101">
         <v>2494</v>
       </c>
@@ -2835,14 +2852,16 @@
       </c>
       <c r="F16" s="105"/>
     </row>
-    <row r="17" spans="1:7" ht="15" outlineLevel="1">
+    <row r="17" spans="1:8" ht="15" outlineLevel="1">
       <c r="A17" s="155"/>
       <c r="B17" s="149" t="s">
         <v>217</v>
       </c>
-      <c r="C17" s="101"/>
+      <c r="C17" s="101">
+        <v>2873</v>
+      </c>
       <c r="D17" s="101">
-        <v>2875</v>
+        <v>2873</v>
       </c>
       <c r="E17" s="121">
         <f t="shared" si="0"/>
@@ -2850,16 +2869,16 @@
       </c>
       <c r="F17" s="105"/>
     </row>
-    <row r="18" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1">
+    <row r="18" spans="1:8" ht="15.75" outlineLevel="1" thickBot="1">
       <c r="A18" s="155"/>
       <c r="B18" s="98" t="s">
         <v>179</v>
       </c>
       <c r="C18" s="99">
-        <v>0</v>
+        <v>2932</v>
       </c>
       <c r="D18" s="99">
-        <v>2930</v>
+        <v>2932</v>
       </c>
       <c r="E18" s="101">
         <f t="shared" si="0"/>
@@ -2867,7 +2886,7 @@
       </c>
       <c r="F18" s="104"/>
     </row>
-    <row r="19" spans="1:7" ht="17.25" thickTop="1" thickBot="1">
+    <row r="19" spans="1:8" ht="17.25" thickTop="1" thickBot="1">
       <c r="A19" s="116" t="s">
         <v>182</v>
       </c>
@@ -2876,11 +2895,11 @@
       </c>
       <c r="C19" s="103">
         <f>C18-C9</f>
-        <v>0</v>
+        <v>2932</v>
       </c>
       <c r="D19" s="103">
         <f>D18-D9</f>
-        <v>2930</v>
+        <v>2932</v>
       </c>
       <c r="E19" s="122">
         <f>E18-E9</f>
@@ -2892,8 +2911,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="13.5" thickBot="1"/>
-    <row r="21" spans="1:7" ht="15" customHeight="1" outlineLevel="1">
+    <row r="20" spans="1:8" ht="13.5" thickBot="1"/>
+    <row r="21" spans="1:8" ht="15" customHeight="1" outlineLevel="1">
       <c r="A21" s="156" t="s">
         <v>219</v>
       </c>
@@ -2913,14 +2932,16 @@
         <v>176</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1">
+    <row r="22" spans="1:8" ht="15.75" outlineLevel="1" thickBot="1">
       <c r="A22" s="155"/>
       <c r="B22" s="98" t="s">
         <v>177</v>
       </c>
-      <c r="C22" s="99"/>
+      <c r="C22" s="99">
+        <v>2932</v>
+      </c>
       <c r="D22" s="99">
-        <v>2930</v>
+        <v>2932</v>
       </c>
       <c r="E22" s="123">
         <f t="shared" ref="E22:E34" si="1">IF(AND(C22&gt;0,D22&gt;0), D22-C22, 0)</f>
@@ -2928,7 +2949,7 @@
       </c>
       <c r="F22" s="104"/>
     </row>
-    <row r="23" spans="1:7" ht="15.75" outlineLevel="1" thickTop="1">
+    <row r="23" spans="1:8" ht="15.75" outlineLevel="1" thickTop="1">
       <c r="A23" s="155"/>
       <c r="B23" s="149" t="s">
         <v>175</v>
@@ -2941,24 +2962,27 @@
       </c>
       <c r="F23" s="105"/>
     </row>
-    <row r="24" spans="1:7" ht="15" outlineLevel="1">
+    <row r="24" spans="1:8" ht="15" outlineLevel="1">
       <c r="A24" s="155"/>
       <c r="B24" s="149" t="s">
         <v>221</v>
       </c>
       <c r="C24" s="101">
-        <v>4160</v>
+        <v>4145</v>
       </c>
       <c r="D24" s="101">
         <v>4612</v>
       </c>
       <c r="E24" s="123">
         <f t="shared" si="1"/>
-        <v>452</v>
+        <v>467</v>
       </c>
       <c r="F24" s="105"/>
-    </row>
-    <row r="25" spans="1:7" ht="15" outlineLevel="1">
+      <c r="H24" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="15" outlineLevel="1">
       <c r="A25" s="155"/>
       <c r="B25" s="149"/>
       <c r="C25" s="101"/>
@@ -2969,7 +2993,7 @@
       </c>
       <c r="F25" s="105"/>
     </row>
-    <row r="26" spans="1:7" ht="15" outlineLevel="1">
+    <row r="26" spans="1:8" ht="15" outlineLevel="1">
       <c r="A26" s="155"/>
       <c r="B26" s="100"/>
       <c r="C26" s="101"/>
@@ -2980,7 +3004,7 @@
       </c>
       <c r="F26" s="105"/>
     </row>
-    <row r="27" spans="1:7" ht="15" outlineLevel="1">
+    <row r="27" spans="1:8" ht="15" outlineLevel="1">
       <c r="A27" s="155"/>
       <c r="B27" s="100"/>
       <c r="C27" s="101"/>
@@ -2991,7 +3015,7 @@
       </c>
       <c r="F27" s="105"/>
     </row>
-    <row r="28" spans="1:7" ht="15" outlineLevel="1">
+    <row r="28" spans="1:8" ht="15" outlineLevel="1">
       <c r="A28" s="155"/>
       <c r="B28" s="149" t="s">
         <v>222</v>
@@ -3008,7 +3032,7 @@
       </c>
       <c r="F28" s="105"/>
     </row>
-    <row r="29" spans="1:7" ht="15" outlineLevel="1">
+    <row r="29" spans="1:8" ht="15" outlineLevel="1">
       <c r="A29" s="155"/>
       <c r="B29" s="100"/>
       <c r="C29" s="101"/>
@@ -3019,7 +3043,7 @@
       </c>
       <c r="F29" s="105"/>
     </row>
-    <row r="30" spans="1:7" ht="15" outlineLevel="1">
+    <row r="30" spans="1:8" ht="15" outlineLevel="1">
       <c r="A30" s="155"/>
       <c r="B30" s="149" t="s">
         <v>223</v>
@@ -3036,7 +3060,7 @@
       </c>
       <c r="F30" s="105"/>
     </row>
-    <row r="31" spans="1:7" ht="15" outlineLevel="1">
+    <row r="31" spans="1:8" ht="15" outlineLevel="1">
       <c r="A31" s="155"/>
       <c r="B31" s="149" t="s">
         <v>224</v>
@@ -3051,7 +3075,7 @@
       </c>
       <c r="F31" s="105"/>
     </row>
-    <row r="32" spans="1:7" ht="15" outlineLevel="1">
+    <row r="32" spans="1:8" ht="15" outlineLevel="1">
       <c r="A32" s="155"/>
       <c r="B32" s="149" t="s">
         <v>225</v>
@@ -3103,11 +3127,11 @@
       </c>
       <c r="C35" s="103">
         <f>C34-C22</f>
-        <v>0</v>
+        <v>-2932</v>
       </c>
       <c r="D35" s="103">
         <f>D34-D22</f>
-        <v>-2930</v>
+        <v>-2932</v>
       </c>
       <c r="E35" s="126">
         <f>E34-E22</f>
@@ -4718,11 +4742,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="A135:A149"/>
-    <mergeCell ref="A106:A115"/>
-    <mergeCell ref="A76:A90"/>
-    <mergeCell ref="A118:A132"/>
-    <mergeCell ref="A93:A103"/>
     <mergeCell ref="A37:A57"/>
     <mergeCell ref="A60:A73"/>
     <mergeCell ref="C5:D5"/>
@@ -4732,6 +4751,11 @@
     <mergeCell ref="A8:A18"/>
     <mergeCell ref="A21:A34"/>
     <mergeCell ref="C4:E4"/>
+    <mergeCell ref="A135:A149"/>
+    <mergeCell ref="A106:A115"/>
+    <mergeCell ref="A76:A90"/>
+    <mergeCell ref="A118:A132"/>
+    <mergeCell ref="A93:A103"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4763,13 +4787,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="26.25" customHeight="1">
-      <c r="A1" s="164" t="s">
+      <c r="A1" s="182" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="164"/>
-      <c r="C1" s="164"/>
-      <c r="D1" s="164"/>
-      <c r="E1" s="164"/>
+      <c r="B1" s="182"/>
+      <c r="C1" s="182"/>
+      <c r="D1" s="182"/>
+      <c r="E1" s="182"/>
       <c r="F1" s="7"/>
       <c r="G1" s="5"/>
       <c r="H1" s="5"/>
@@ -4799,18 +4823,18 @@
         <v>8</v>
       </c>
       <c r="B3" s="36"/>
-      <c r="C3" s="165"/>
-      <c r="D3" s="166"/>
-      <c r="E3" s="166"/>
+      <c r="C3" s="183"/>
+      <c r="D3" s="184"/>
+      <c r="E3" s="184"/>
     </row>
     <row r="4" spans="1:8" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A4" s="46" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="87"/>
-      <c r="C4" s="167"/>
-      <c r="D4" s="168"/>
-      <c r="E4" s="168"/>
+      <c r="C4" s="164"/>
+      <c r="D4" s="165"/>
+      <c r="E4" s="165"/>
       <c r="F4" s="6"/>
     </row>
     <row r="5" spans="1:8" hidden="1" outlineLevel="2">
@@ -4962,9 +4986,9 @@
         <v>9</v>
       </c>
       <c r="B21" s="90"/>
-      <c r="C21" s="169"/>
-      <c r="D21" s="170"/>
-      <c r="E21" s="170"/>
+      <c r="C21" s="166"/>
+      <c r="D21" s="167"/>
+      <c r="E21" s="167"/>
     </row>
     <row r="22" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A22" s="47">
@@ -5115,9 +5139,9 @@
         <v>10</v>
       </c>
       <c r="B38" s="87"/>
-      <c r="C38" s="167"/>
-      <c r="D38" s="168"/>
-      <c r="E38" s="168"/>
+      <c r="C38" s="164"/>
+      <c r="D38" s="165"/>
+      <c r="E38" s="165"/>
     </row>
     <row r="39" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A39" s="47">
@@ -5268,9 +5292,9 @@
         <v>11</v>
       </c>
       <c r="B55" s="87"/>
-      <c r="C55" s="167"/>
-      <c r="D55" s="168"/>
-      <c r="E55" s="168"/>
+      <c r="C55" s="164"/>
+      <c r="D55" s="165"/>
+      <c r="E55" s="165"/>
     </row>
     <row r="56" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A56" s="47">
@@ -5421,9 +5445,9 @@
         <v>12</v>
       </c>
       <c r="B72" s="87"/>
-      <c r="C72" s="167"/>
-      <c r="D72" s="168"/>
-      <c r="E72" s="168"/>
+      <c r="C72" s="164"/>
+      <c r="D72" s="165"/>
+      <c r="E72" s="165"/>
     </row>
     <row r="73" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A73" s="47">
@@ -5574,9 +5598,9 @@
         <v>13</v>
       </c>
       <c r="B89" s="87"/>
-      <c r="C89" s="167"/>
-      <c r="D89" s="168"/>
-      <c r="E89" s="168"/>
+      <c r="C89" s="164"/>
+      <c r="D89" s="165"/>
+      <c r="E89" s="165"/>
     </row>
     <row r="90" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A90" s="47">
@@ -5727,9 +5751,9 @@
         <v>14</v>
       </c>
       <c r="B106" s="87"/>
-      <c r="C106" s="167"/>
-      <c r="D106" s="168"/>
-      <c r="E106" s="168"/>
+      <c r="C106" s="164"/>
+      <c r="D106" s="165"/>
+      <c r="E106" s="165"/>
     </row>
     <row r="107" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A107" s="47">
@@ -5880,9 +5904,9 @@
         <v>15</v>
       </c>
       <c r="B123" s="87"/>
-      <c r="C123" s="167"/>
-      <c r="D123" s="168"/>
-      <c r="E123" s="168"/>
+      <c r="C123" s="164"/>
+      <c r="D123" s="165"/>
+      <c r="E123" s="165"/>
     </row>
     <row r="124" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A124" s="47">
@@ -6033,9 +6057,9 @@
         <v>16</v>
       </c>
       <c r="B140" s="87"/>
-      <c r="C140" s="167"/>
-      <c r="D140" s="168"/>
-      <c r="E140" s="168"/>
+      <c r="C140" s="164"/>
+      <c r="D140" s="165"/>
+      <c r="E140" s="165"/>
     </row>
     <row r="141" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A141" s="47">
@@ -6186,9 +6210,9 @@
         <v>17</v>
       </c>
       <c r="B157" s="87"/>
-      <c r="C157" s="167"/>
-      <c r="D157" s="168"/>
-      <c r="E157" s="168"/>
+      <c r="C157" s="164"/>
+      <c r="D157" s="165"/>
+      <c r="E157" s="165"/>
     </row>
     <row r="158" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A158" s="47">
@@ -6339,9 +6363,9 @@
         <v>18</v>
       </c>
       <c r="B174" s="87"/>
-      <c r="C174" s="167"/>
-      <c r="D174" s="168"/>
-      <c r="E174" s="168"/>
+      <c r="C174" s="164"/>
+      <c r="D174" s="165"/>
+      <c r="E174" s="165"/>
     </row>
     <row r="175" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A175" s="47">
@@ -6492,9 +6516,9 @@
         <v>19</v>
       </c>
       <c r="B191" s="87"/>
-      <c r="C191" s="167"/>
-      <c r="D191" s="168"/>
-      <c r="E191" s="168"/>
+      <c r="C191" s="164"/>
+      <c r="D191" s="165"/>
+      <c r="E191" s="165"/>
     </row>
     <row r="192" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A192" s="47">
@@ -6645,9 +6669,9 @@
         <v>20</v>
       </c>
       <c r="B208" s="87"/>
-      <c r="C208" s="167"/>
-      <c r="D208" s="168"/>
-      <c r="E208" s="168"/>
+      <c r="C208" s="164"/>
+      <c r="D208" s="165"/>
+      <c r="E208" s="165"/>
     </row>
     <row r="209" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A209" s="47">
@@ -6798,9 +6822,9 @@
         <v>21</v>
       </c>
       <c r="B225" s="87"/>
-      <c r="C225" s="167"/>
-      <c r="D225" s="168"/>
-      <c r="E225" s="168"/>
+      <c r="C225" s="164"/>
+      <c r="D225" s="165"/>
+      <c r="E225" s="165"/>
     </row>
     <row r="226" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A226" s="47">
@@ -6951,9 +6975,9 @@
         <v>22</v>
       </c>
       <c r="B242" s="87"/>
-      <c r="C242" s="167"/>
-      <c r="D242" s="168"/>
-      <c r="E242" s="168"/>
+      <c r="C242" s="164"/>
+      <c r="D242" s="165"/>
+      <c r="E242" s="165"/>
     </row>
     <row r="243" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A243" s="47">
@@ -7104,9 +7128,9 @@
         <v>23</v>
       </c>
       <c r="B259" s="87"/>
-      <c r="C259" s="167"/>
-      <c r="D259" s="168"/>
-      <c r="E259" s="168"/>
+      <c r="C259" s="164"/>
+      <c r="D259" s="165"/>
+      <c r="E259" s="165"/>
     </row>
     <row r="260" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A260" s="47">
@@ -7257,18 +7281,18 @@
         <v>24</v>
       </c>
       <c r="B276" s="37"/>
-      <c r="C276" s="171"/>
-      <c r="D276" s="172"/>
-      <c r="E276" s="172"/>
+      <c r="C276" s="180"/>
+      <c r="D276" s="181"/>
+      <c r="E276" s="181"/>
     </row>
     <row r="277" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A277" s="51" t="s">
         <v>25</v>
       </c>
       <c r="B277" s="87"/>
-      <c r="C277" s="167"/>
-      <c r="D277" s="168"/>
-      <c r="E277" s="168"/>
+      <c r="C277" s="164"/>
+      <c r="D277" s="165"/>
+      <c r="E277" s="165"/>
     </row>
     <row r="278" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A278" s="52">
@@ -7419,9 +7443,9 @@
         <v>26</v>
       </c>
       <c r="B294" s="90"/>
-      <c r="C294" s="169"/>
-      <c r="D294" s="170"/>
-      <c r="E294" s="170"/>
+      <c r="C294" s="166"/>
+      <c r="D294" s="167"/>
+      <c r="E294" s="167"/>
     </row>
     <row r="295" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A295" s="52">
@@ -7572,9 +7596,9 @@
         <v>27</v>
       </c>
       <c r="B311" s="87"/>
-      <c r="C311" s="167"/>
-      <c r="D311" s="168"/>
-      <c r="E311" s="168"/>
+      <c r="C311" s="164"/>
+      <c r="D311" s="165"/>
+      <c r="E311" s="165"/>
     </row>
     <row r="312" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A312" s="52">
@@ -7725,9 +7749,9 @@
         <v>28</v>
       </c>
       <c r="B328" s="87"/>
-      <c r="C328" s="167"/>
-      <c r="D328" s="168"/>
-      <c r="E328" s="168"/>
+      <c r="C328" s="164"/>
+      <c r="D328" s="165"/>
+      <c r="E328" s="165"/>
     </row>
     <row r="329" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A329" s="52">
@@ -7878,9 +7902,9 @@
         <v>29</v>
       </c>
       <c r="B345" s="87"/>
-      <c r="C345" s="167"/>
-      <c r="D345" s="168"/>
-      <c r="E345" s="168"/>
+      <c r="C345" s="164"/>
+      <c r="D345" s="165"/>
+      <c r="E345" s="165"/>
     </row>
     <row r="346" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A346" s="52">
@@ -8031,9 +8055,9 @@
         <v>30</v>
       </c>
       <c r="B362" s="87"/>
-      <c r="C362" s="167"/>
-      <c r="D362" s="168"/>
-      <c r="E362" s="168"/>
+      <c r="C362" s="164"/>
+      <c r="D362" s="165"/>
+      <c r="E362" s="165"/>
     </row>
     <row r="363" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A363" s="52">
@@ -8184,9 +8208,9 @@
         <v>31</v>
       </c>
       <c r="B379" s="87"/>
-      <c r="C379" s="167"/>
-      <c r="D379" s="168"/>
-      <c r="E379" s="168"/>
+      <c r="C379" s="164"/>
+      <c r="D379" s="165"/>
+      <c r="E379" s="165"/>
     </row>
     <row r="380" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A380" s="52">
@@ -8337,9 +8361,9 @@
         <v>32</v>
       </c>
       <c r="B396" s="87"/>
-      <c r="C396" s="167"/>
-      <c r="D396" s="168"/>
-      <c r="E396" s="168"/>
+      <c r="C396" s="164"/>
+      <c r="D396" s="165"/>
+      <c r="E396" s="165"/>
     </row>
     <row r="397" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A397" s="52">
@@ -8490,9 +8514,9 @@
         <v>33</v>
       </c>
       <c r="B413" s="87"/>
-      <c r="C413" s="167"/>
-      <c r="D413" s="168"/>
-      <c r="E413" s="168"/>
+      <c r="C413" s="164"/>
+      <c r="D413" s="165"/>
+      <c r="E413" s="165"/>
     </row>
     <row r="414" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A414" s="52">
@@ -8643,9 +8667,9 @@
         <v>34</v>
       </c>
       <c r="B430" s="87"/>
-      <c r="C430" s="167"/>
-      <c r="D430" s="168"/>
-      <c r="E430" s="168"/>
+      <c r="C430" s="164"/>
+      <c r="D430" s="165"/>
+      <c r="E430" s="165"/>
     </row>
     <row r="431" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A431" s="52">
@@ -8796,9 +8820,9 @@
         <v>35</v>
       </c>
       <c r="B447" s="87"/>
-      <c r="C447" s="167"/>
-      <c r="D447" s="168"/>
-      <c r="E447" s="168"/>
+      <c r="C447" s="164"/>
+      <c r="D447" s="165"/>
+      <c r="E447" s="165"/>
     </row>
     <row r="448" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A448" s="52">
@@ -8949,9 +8973,9 @@
         <v>36</v>
       </c>
       <c r="B464" s="87"/>
-      <c r="C464" s="167"/>
-      <c r="D464" s="168"/>
-      <c r="E464" s="168"/>
+      <c r="C464" s="164"/>
+      <c r="D464" s="165"/>
+      <c r="E464" s="165"/>
     </row>
     <row r="465" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A465" s="52">
@@ -9102,9 +9126,9 @@
         <v>37</v>
       </c>
       <c r="B481" s="87"/>
-      <c r="C481" s="167"/>
-      <c r="D481" s="168"/>
-      <c r="E481" s="168"/>
+      <c r="C481" s="164"/>
+      <c r="D481" s="165"/>
+      <c r="E481" s="165"/>
     </row>
     <row r="482" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A482" s="52">
@@ -9255,9 +9279,9 @@
         <v>38</v>
       </c>
       <c r="B498" s="87"/>
-      <c r="C498" s="167"/>
-      <c r="D498" s="168"/>
-      <c r="E498" s="168"/>
+      <c r="C498" s="164"/>
+      <c r="D498" s="165"/>
+      <c r="E498" s="165"/>
     </row>
     <row r="499" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A499" s="52">
@@ -9408,9 +9432,9 @@
         <v>39</v>
       </c>
       <c r="B515" s="87"/>
-      <c r="C515" s="167"/>
-      <c r="D515" s="168"/>
-      <c r="E515" s="168"/>
+      <c r="C515" s="164"/>
+      <c r="D515" s="165"/>
+      <c r="E515" s="165"/>
     </row>
     <row r="516" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A516" s="52">
@@ -9561,9 +9585,9 @@
         <v>40</v>
       </c>
       <c r="B532" s="87"/>
-      <c r="C532" s="167"/>
-      <c r="D532" s="168"/>
-      <c r="E532" s="168"/>
+      <c r="C532" s="164"/>
+      <c r="D532" s="165"/>
+      <c r="E532" s="165"/>
     </row>
     <row r="533" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A533" s="55">
@@ -9714,18 +9738,18 @@
         <v>50</v>
       </c>
       <c r="B549" s="38"/>
-      <c r="C549" s="173"/>
-      <c r="D549" s="174"/>
-      <c r="E549" s="174"/>
+      <c r="C549" s="178"/>
+      <c r="D549" s="179"/>
+      <c r="E549" s="179"/>
     </row>
     <row r="550" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A550" s="58" t="s">
         <v>51</v>
       </c>
       <c r="B550" s="87"/>
-      <c r="C550" s="167"/>
-      <c r="D550" s="168"/>
-      <c r="E550" s="168"/>
+      <c r="C550" s="164"/>
+      <c r="D550" s="165"/>
+      <c r="E550" s="165"/>
     </row>
     <row r="551" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A551" s="59">
@@ -9876,9 +9900,9 @@
         <v>52</v>
       </c>
       <c r="B567" s="90"/>
-      <c r="C567" s="169"/>
-      <c r="D567" s="170"/>
-      <c r="E567" s="170"/>
+      <c r="C567" s="166"/>
+      <c r="D567" s="167"/>
+      <c r="E567" s="167"/>
     </row>
     <row r="568" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A568" s="59">
@@ -10029,9 +10053,9 @@
         <v>53</v>
       </c>
       <c r="B584" s="87"/>
-      <c r="C584" s="167"/>
-      <c r="D584" s="168"/>
-      <c r="E584" s="168"/>
+      <c r="C584" s="164"/>
+      <c r="D584" s="165"/>
+      <c r="E584" s="165"/>
     </row>
     <row r="585" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A585" s="59">
@@ -10182,9 +10206,9 @@
         <v>54</v>
       </c>
       <c r="B601" s="87"/>
-      <c r="C601" s="167"/>
-      <c r="D601" s="168"/>
-      <c r="E601" s="168"/>
+      <c r="C601" s="164"/>
+      <c r="D601" s="165"/>
+      <c r="E601" s="165"/>
     </row>
     <row r="602" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A602" s="59">
@@ -10335,9 +10359,9 @@
         <v>55</v>
       </c>
       <c r="B618" s="87"/>
-      <c r="C618" s="167"/>
-      <c r="D618" s="168"/>
-      <c r="E618" s="168"/>
+      <c r="C618" s="164"/>
+      <c r="D618" s="165"/>
+      <c r="E618" s="165"/>
     </row>
     <row r="619" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A619" s="59">
@@ -10488,9 +10512,9 @@
         <v>56</v>
       </c>
       <c r="B635" s="87"/>
-      <c r="C635" s="167"/>
-      <c r="D635" s="168"/>
-      <c r="E635" s="168"/>
+      <c r="C635" s="164"/>
+      <c r="D635" s="165"/>
+      <c r="E635" s="165"/>
     </row>
     <row r="636" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A636" s="59">
@@ -10641,9 +10665,9 @@
         <v>57</v>
       </c>
       <c r="B652" s="87"/>
-      <c r="C652" s="167"/>
-      <c r="D652" s="168"/>
-      <c r="E652" s="168"/>
+      <c r="C652" s="164"/>
+      <c r="D652" s="165"/>
+      <c r="E652" s="165"/>
     </row>
     <row r="653" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A653" s="59">
@@ -10794,9 +10818,9 @@
         <v>58</v>
       </c>
       <c r="B669" s="87"/>
-      <c r="C669" s="167"/>
-      <c r="D669" s="168"/>
-      <c r="E669" s="168"/>
+      <c r="C669" s="164"/>
+      <c r="D669" s="165"/>
+      <c r="E669" s="165"/>
     </row>
     <row r="670" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A670" s="59">
@@ -10947,9 +10971,9 @@
         <v>59</v>
       </c>
       <c r="B686" s="87"/>
-      <c r="C686" s="167"/>
-      <c r="D686" s="168"/>
-      <c r="E686" s="168"/>
+      <c r="C686" s="164"/>
+      <c r="D686" s="165"/>
+      <c r="E686" s="165"/>
     </row>
     <row r="687" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A687" s="59">
@@ -11100,9 +11124,9 @@
         <v>60</v>
       </c>
       <c r="B703" s="87"/>
-      <c r="C703" s="167"/>
-      <c r="D703" s="168"/>
-      <c r="E703" s="168"/>
+      <c r="C703" s="164"/>
+      <c r="D703" s="165"/>
+      <c r="E703" s="165"/>
     </row>
     <row r="704" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A704" s="59">
@@ -11253,9 +11277,9 @@
         <v>61</v>
       </c>
       <c r="B720" s="87"/>
-      <c r="C720" s="167"/>
-      <c r="D720" s="168"/>
-      <c r="E720" s="168"/>
+      <c r="C720" s="164"/>
+      <c r="D720" s="165"/>
+      <c r="E720" s="165"/>
     </row>
     <row r="721" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A721" s="59">
@@ -11406,9 +11430,9 @@
         <v>62</v>
       </c>
       <c r="B737" s="87"/>
-      <c r="C737" s="167"/>
-      <c r="D737" s="168"/>
-      <c r="E737" s="168"/>
+      <c r="C737" s="164"/>
+      <c r="D737" s="165"/>
+      <c r="E737" s="165"/>
     </row>
     <row r="738" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A738" s="59">
@@ -11559,9 +11583,9 @@
         <v>63</v>
       </c>
       <c r="B754" s="87"/>
-      <c r="C754" s="167"/>
-      <c r="D754" s="168"/>
-      <c r="E754" s="168"/>
+      <c r="C754" s="164"/>
+      <c r="D754" s="165"/>
+      <c r="E754" s="165"/>
     </row>
     <row r="755" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A755" s="59">
@@ -11712,9 +11736,9 @@
         <v>64</v>
       </c>
       <c r="B771" s="87"/>
-      <c r="C771" s="167"/>
-      <c r="D771" s="168"/>
-      <c r="E771" s="168"/>
+      <c r="C771" s="164"/>
+      <c r="D771" s="165"/>
+      <c r="E771" s="165"/>
     </row>
     <row r="772" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A772" s="59">
@@ -11865,9 +11889,9 @@
         <v>65</v>
       </c>
       <c r="B788" s="87"/>
-      <c r="C788" s="167"/>
-      <c r="D788" s="168"/>
-      <c r="E788" s="168"/>
+      <c r="C788" s="164"/>
+      <c r="D788" s="165"/>
+      <c r="E788" s="165"/>
     </row>
     <row r="789" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A789" s="59">
@@ -12018,9 +12042,9 @@
         <v>66</v>
       </c>
       <c r="B805" s="87"/>
-      <c r="C805" s="167"/>
-      <c r="D805" s="168"/>
-      <c r="E805" s="168"/>
+      <c r="C805" s="164"/>
+      <c r="D805" s="165"/>
+      <c r="E805" s="165"/>
     </row>
     <row r="806" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A806" s="59">
@@ -12171,18 +12195,18 @@
         <v>67</v>
       </c>
       <c r="B822" s="39"/>
-      <c r="C822" s="175"/>
-      <c r="D822" s="176"/>
-      <c r="E822" s="176"/>
+      <c r="C822" s="176"/>
+      <c r="D822" s="177"/>
+      <c r="E822" s="177"/>
     </row>
     <row r="823" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A823" s="63" t="s">
         <v>68</v>
       </c>
       <c r="B823" s="87"/>
-      <c r="C823" s="167"/>
-      <c r="D823" s="168"/>
-      <c r="E823" s="168"/>
+      <c r="C823" s="164"/>
+      <c r="D823" s="165"/>
+      <c r="E823" s="165"/>
     </row>
     <row r="824" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A824" s="64">
@@ -12333,9 +12357,9 @@
         <v>69</v>
       </c>
       <c r="B840" s="90"/>
-      <c r="C840" s="169"/>
-      <c r="D840" s="170"/>
-      <c r="E840" s="170"/>
+      <c r="C840" s="166"/>
+      <c r="D840" s="167"/>
+      <c r="E840" s="167"/>
     </row>
     <row r="841" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A841" s="64">
@@ -12486,9 +12510,9 @@
         <v>70</v>
       </c>
       <c r="B857" s="87"/>
-      <c r="C857" s="167"/>
-      <c r="D857" s="168"/>
-      <c r="E857" s="168"/>
+      <c r="C857" s="164"/>
+      <c r="D857" s="165"/>
+      <c r="E857" s="165"/>
     </row>
     <row r="858" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A858" s="64">
@@ -12639,9 +12663,9 @@
         <v>71</v>
       </c>
       <c r="B874" s="87"/>
-      <c r="C874" s="167"/>
-      <c r="D874" s="168"/>
-      <c r="E874" s="168"/>
+      <c r="C874" s="164"/>
+      <c r="D874" s="165"/>
+      <c r="E874" s="165"/>
     </row>
     <row r="875" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A875" s="64">
@@ -12792,9 +12816,9 @@
         <v>72</v>
       </c>
       <c r="B891" s="87"/>
-      <c r="C891" s="167"/>
-      <c r="D891" s="168"/>
-      <c r="E891" s="168"/>
+      <c r="C891" s="164"/>
+      <c r="D891" s="165"/>
+      <c r="E891" s="165"/>
     </row>
     <row r="892" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A892" s="64">
@@ -12945,9 +12969,9 @@
         <v>73</v>
       </c>
       <c r="B908" s="87"/>
-      <c r="C908" s="167"/>
-      <c r="D908" s="168"/>
-      <c r="E908" s="168"/>
+      <c r="C908" s="164"/>
+      <c r="D908" s="165"/>
+      <c r="E908" s="165"/>
     </row>
     <row r="909" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A909" s="64">
@@ -13098,9 +13122,9 @@
         <v>74</v>
       </c>
       <c r="B925" s="87"/>
-      <c r="C925" s="167"/>
-      <c r="D925" s="168"/>
-      <c r="E925" s="168"/>
+      <c r="C925" s="164"/>
+      <c r="D925" s="165"/>
+      <c r="E925" s="165"/>
     </row>
     <row r="926" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A926" s="64">
@@ -13251,9 +13275,9 @@
         <v>75</v>
       </c>
       <c r="B942" s="87"/>
-      <c r="C942" s="167"/>
-      <c r="D942" s="168"/>
-      <c r="E942" s="168"/>
+      <c r="C942" s="164"/>
+      <c r="D942" s="165"/>
+      <c r="E942" s="165"/>
     </row>
     <row r="943" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A943" s="64">
@@ -13404,9 +13428,9 @@
         <v>76</v>
       </c>
       <c r="B959" s="87"/>
-      <c r="C959" s="167"/>
-      <c r="D959" s="168"/>
-      <c r="E959" s="168"/>
+      <c r="C959" s="164"/>
+      <c r="D959" s="165"/>
+      <c r="E959" s="165"/>
     </row>
     <row r="960" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A960" s="64">
@@ -13557,9 +13581,9 @@
         <v>77</v>
       </c>
       <c r="B976" s="87"/>
-      <c r="C976" s="167"/>
-      <c r="D976" s="168"/>
-      <c r="E976" s="168"/>
+      <c r="C976" s="164"/>
+      <c r="D976" s="165"/>
+      <c r="E976" s="165"/>
     </row>
     <row r="977" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A977" s="64">
@@ -13710,9 +13734,9 @@
         <v>78</v>
       </c>
       <c r="B993" s="87"/>
-      <c r="C993" s="167"/>
-      <c r="D993" s="168"/>
-      <c r="E993" s="168"/>
+      <c r="C993" s="164"/>
+      <c r="D993" s="165"/>
+      <c r="E993" s="165"/>
     </row>
     <row r="994" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A994" s="64">
@@ -13863,9 +13887,9 @@
         <v>79</v>
       </c>
       <c r="B1010" s="87"/>
-      <c r="C1010" s="167"/>
-      <c r="D1010" s="168"/>
-      <c r="E1010" s="168"/>
+      <c r="C1010" s="164"/>
+      <c r="D1010" s="165"/>
+      <c r="E1010" s="165"/>
     </row>
     <row r="1011" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1011" s="64">
@@ -14016,9 +14040,9 @@
         <v>80</v>
       </c>
       <c r="B1027" s="87"/>
-      <c r="C1027" s="167"/>
-      <c r="D1027" s="168"/>
-      <c r="E1027" s="168"/>
+      <c r="C1027" s="164"/>
+      <c r="D1027" s="165"/>
+      <c r="E1027" s="165"/>
     </row>
     <row r="1028" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1028" s="64">
@@ -14169,9 +14193,9 @@
         <v>83</v>
       </c>
       <c r="B1044" s="87"/>
-      <c r="C1044" s="167"/>
-      <c r="D1044" s="168"/>
-      <c r="E1044" s="168"/>
+      <c r="C1044" s="164"/>
+      <c r="D1044" s="165"/>
+      <c r="E1044" s="165"/>
     </row>
     <row r="1045" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1045" s="64">
@@ -14322,9 +14346,9 @@
         <v>82</v>
       </c>
       <c r="B1061" s="87"/>
-      <c r="C1061" s="167"/>
-      <c r="D1061" s="168"/>
-      <c r="E1061" s="168"/>
+      <c r="C1061" s="164"/>
+      <c r="D1061" s="165"/>
+      <c r="E1061" s="165"/>
     </row>
     <row r="1062" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1062" s="64">
@@ -14475,9 +14499,9 @@
         <v>84</v>
       </c>
       <c r="B1078" s="87"/>
-      <c r="C1078" s="167"/>
-      <c r="D1078" s="168"/>
-      <c r="E1078" s="168"/>
+      <c r="C1078" s="164"/>
+      <c r="D1078" s="165"/>
+      <c r="E1078" s="165"/>
     </row>
     <row r="1079" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1079" s="64">
@@ -14628,18 +14652,18 @@
         <v>104</v>
       </c>
       <c r="B1095" s="40"/>
-      <c r="C1095" s="177"/>
-      <c r="D1095" s="178"/>
-      <c r="E1095" s="178"/>
+      <c r="C1095" s="174"/>
+      <c r="D1095" s="175"/>
+      <c r="E1095" s="175"/>
     </row>
     <row r="1096" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A1096" s="68" t="s">
         <v>85</v>
       </c>
       <c r="B1096" s="87"/>
-      <c r="C1096" s="167"/>
-      <c r="D1096" s="168"/>
-      <c r="E1096" s="168"/>
+      <c r="C1096" s="164"/>
+      <c r="D1096" s="165"/>
+      <c r="E1096" s="165"/>
     </row>
     <row r="1097" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1097" s="69">
@@ -14790,9 +14814,9 @@
         <v>86</v>
       </c>
       <c r="B1113" s="90"/>
-      <c r="C1113" s="169"/>
-      <c r="D1113" s="170"/>
-      <c r="E1113" s="170"/>
+      <c r="C1113" s="166"/>
+      <c r="D1113" s="167"/>
+      <c r="E1113" s="167"/>
     </row>
     <row r="1114" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1114" s="69">
@@ -14943,9 +14967,9 @@
         <v>87</v>
       </c>
       <c r="B1130" s="87"/>
-      <c r="C1130" s="167"/>
-      <c r="D1130" s="168"/>
-      <c r="E1130" s="168"/>
+      <c r="C1130" s="164"/>
+      <c r="D1130" s="165"/>
+      <c r="E1130" s="165"/>
     </row>
     <row r="1131" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1131" s="69">
@@ -15096,9 +15120,9 @@
         <v>88</v>
       </c>
       <c r="B1147" s="87"/>
-      <c r="C1147" s="167"/>
-      <c r="D1147" s="168"/>
-      <c r="E1147" s="168"/>
+      <c r="C1147" s="164"/>
+      <c r="D1147" s="165"/>
+      <c r="E1147" s="165"/>
     </row>
     <row r="1148" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1148" s="69">
@@ -15249,9 +15273,9 @@
         <v>89</v>
       </c>
       <c r="B1164" s="87"/>
-      <c r="C1164" s="167"/>
-      <c r="D1164" s="168"/>
-      <c r="E1164" s="168"/>
+      <c r="C1164" s="164"/>
+      <c r="D1164" s="165"/>
+      <c r="E1164" s="165"/>
     </row>
     <row r="1165" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1165" s="69">
@@ -15402,9 +15426,9 @@
         <v>90</v>
       </c>
       <c r="B1181" s="87"/>
-      <c r="C1181" s="167"/>
-      <c r="D1181" s="168"/>
-      <c r="E1181" s="168"/>
+      <c r="C1181" s="164"/>
+      <c r="D1181" s="165"/>
+      <c r="E1181" s="165"/>
     </row>
     <row r="1182" spans="1:5" hidden="1" outlineLevel="3">
       <c r="A1182" s="69">
@@ -15555,9 +15579,9 @@
         <v>91</v>
       </c>
       <c r="B1198" s="87"/>
-      <c r="C1198" s="167"/>
-      <c r="D1198" s="168"/>
-      <c r="E1198" s="168"/>
+      <c r="C1198" s="164"/>
+      <c r="D1198" s="165"/>
+      <c r="E1198" s="165"/>
     </row>
     <row r="1199" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1199" s="69">
@@ -15708,9 +15732,9 @@
         <v>92</v>
       </c>
       <c r="B1215" s="87"/>
-      <c r="C1215" s="167"/>
-      <c r="D1215" s="168"/>
-      <c r="E1215" s="168"/>
+      <c r="C1215" s="164"/>
+      <c r="D1215" s="165"/>
+      <c r="E1215" s="165"/>
     </row>
     <row r="1216" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1216" s="69">
@@ -15861,9 +15885,9 @@
         <v>93</v>
       </c>
       <c r="B1232" s="87"/>
-      <c r="C1232" s="167"/>
-      <c r="D1232" s="168"/>
-      <c r="E1232" s="168"/>
+      <c r="C1232" s="164"/>
+      <c r="D1232" s="165"/>
+      <c r="E1232" s="165"/>
     </row>
     <row r="1233" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1233" s="69">
@@ -16014,9 +16038,9 @@
         <v>94</v>
       </c>
       <c r="B1249" s="87"/>
-      <c r="C1249" s="167"/>
-      <c r="D1249" s="168"/>
-      <c r="E1249" s="168"/>
+      <c r="C1249" s="164"/>
+      <c r="D1249" s="165"/>
+      <c r="E1249" s="165"/>
     </row>
     <row r="1250" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1250" s="69">
@@ -16167,9 +16191,9 @@
         <v>99</v>
       </c>
       <c r="B1266" s="87"/>
-      <c r="C1266" s="167"/>
-      <c r="D1266" s="168"/>
-      <c r="E1266" s="168"/>
+      <c r="C1266" s="164"/>
+      <c r="D1266" s="165"/>
+      <c r="E1266" s="165"/>
     </row>
     <row r="1267" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1267" s="69">
@@ -16320,9 +16344,9 @@
         <v>100</v>
       </c>
       <c r="B1283" s="87"/>
-      <c r="C1283" s="167"/>
-      <c r="D1283" s="168"/>
-      <c r="E1283" s="168"/>
+      <c r="C1283" s="164"/>
+      <c r="D1283" s="165"/>
+      <c r="E1283" s="165"/>
     </row>
     <row r="1284" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1284" s="69">
@@ -16473,9 +16497,9 @@
         <v>101</v>
       </c>
       <c r="B1300" s="87"/>
-      <c r="C1300" s="167"/>
-      <c r="D1300" s="168"/>
-      <c r="E1300" s="168"/>
+      <c r="C1300" s="164"/>
+      <c r="D1300" s="165"/>
+      <c r="E1300" s="165"/>
     </row>
     <row r="1301" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1301" s="69">
@@ -16626,9 +16650,9 @@
         <v>81</v>
       </c>
       <c r="B1317" s="87"/>
-      <c r="C1317" s="167"/>
-      <c r="D1317" s="168"/>
-      <c r="E1317" s="168"/>
+      <c r="C1317" s="164"/>
+      <c r="D1317" s="165"/>
+      <c r="E1317" s="165"/>
     </row>
     <row r="1318" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1318" s="69">
@@ -16779,9 +16803,9 @@
         <v>102</v>
       </c>
       <c r="B1334" s="87"/>
-      <c r="C1334" s="167"/>
-      <c r="D1334" s="168"/>
-      <c r="E1334" s="168"/>
+      <c r="C1334" s="164"/>
+      <c r="D1334" s="165"/>
+      <c r="E1334" s="165"/>
     </row>
     <row r="1335" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1335" s="69">
@@ -16932,9 +16956,9 @@
         <v>98</v>
       </c>
       <c r="B1351" s="87"/>
-      <c r="C1351" s="167"/>
-      <c r="D1351" s="168"/>
-      <c r="E1351" s="168"/>
+      <c r="C1351" s="164"/>
+      <c r="D1351" s="165"/>
+      <c r="E1351" s="165"/>
     </row>
     <row r="1352" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1352" s="69">
@@ -17085,18 +17109,18 @@
         <v>103</v>
       </c>
       <c r="B1368" s="41"/>
-      <c r="C1368" s="179"/>
-      <c r="D1368" s="180"/>
-      <c r="E1368" s="180"/>
+      <c r="C1368" s="172"/>
+      <c r="D1368" s="173"/>
+      <c r="E1368" s="173"/>
     </row>
     <row r="1369" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A1369" s="73" t="s">
         <v>105</v>
       </c>
       <c r="B1369" s="87"/>
-      <c r="C1369" s="167"/>
-      <c r="D1369" s="168"/>
-      <c r="E1369" s="168"/>
+      <c r="C1369" s="164"/>
+      <c r="D1369" s="165"/>
+      <c r="E1369" s="165"/>
     </row>
     <row r="1370" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1370" s="74">
@@ -17247,9 +17271,9 @@
         <v>106</v>
       </c>
       <c r="B1386" s="90"/>
-      <c r="C1386" s="169"/>
-      <c r="D1386" s="170"/>
-      <c r="E1386" s="170"/>
+      <c r="C1386" s="166"/>
+      <c r="D1386" s="167"/>
+      <c r="E1386" s="167"/>
     </row>
     <row r="1387" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1387" s="74">
@@ -17400,9 +17424,9 @@
         <v>107</v>
       </c>
       <c r="B1403" s="87"/>
-      <c r="C1403" s="167"/>
-      <c r="D1403" s="168"/>
-      <c r="E1403" s="168"/>
+      <c r="C1403" s="164"/>
+      <c r="D1403" s="165"/>
+      <c r="E1403" s="165"/>
     </row>
     <row r="1404" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1404" s="74">
@@ -17553,9 +17577,9 @@
         <v>108</v>
       </c>
       <c r="B1420" s="87"/>
-      <c r="C1420" s="167"/>
-      <c r="D1420" s="168"/>
-      <c r="E1420" s="168"/>
+      <c r="C1420" s="164"/>
+      <c r="D1420" s="165"/>
+      <c r="E1420" s="165"/>
     </row>
     <row r="1421" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1421" s="74">
@@ -17706,9 +17730,9 @@
         <v>109</v>
       </c>
       <c r="B1437" s="87"/>
-      <c r="C1437" s="167"/>
-      <c r="D1437" s="168"/>
-      <c r="E1437" s="168"/>
+      <c r="C1437" s="164"/>
+      <c r="D1437" s="165"/>
+      <c r="E1437" s="165"/>
     </row>
     <row r="1438" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1438" s="74">
@@ -17859,9 +17883,9 @@
         <v>110</v>
       </c>
       <c r="B1454" s="87"/>
-      <c r="C1454" s="167"/>
-      <c r="D1454" s="168"/>
-      <c r="E1454" s="168"/>
+      <c r="C1454" s="164"/>
+      <c r="D1454" s="165"/>
+      <c r="E1454" s="165"/>
     </row>
     <row r="1455" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1455" s="74">
@@ -18012,9 +18036,9 @@
         <v>111</v>
       </c>
       <c r="B1471" s="87"/>
-      <c r="C1471" s="167"/>
-      <c r="D1471" s="168"/>
-      <c r="E1471" s="168"/>
+      <c r="C1471" s="164"/>
+      <c r="D1471" s="165"/>
+      <c r="E1471" s="165"/>
     </row>
     <row r="1472" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1472" s="74">
@@ -18165,9 +18189,9 @@
         <v>112</v>
       </c>
       <c r="B1488" s="87"/>
-      <c r="C1488" s="167"/>
-      <c r="D1488" s="168"/>
-      <c r="E1488" s="168"/>
+      <c r="C1488" s="164"/>
+      <c r="D1488" s="165"/>
+      <c r="E1488" s="165"/>
     </row>
     <row r="1489" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1489" s="74">
@@ -18318,9 +18342,9 @@
         <v>113</v>
       </c>
       <c r="B1505" s="87"/>
-      <c r="C1505" s="167"/>
-      <c r="D1505" s="168"/>
-      <c r="E1505" s="168"/>
+      <c r="C1505" s="164"/>
+      <c r="D1505" s="165"/>
+      <c r="E1505" s="165"/>
     </row>
     <row r="1506" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1506" s="74">
@@ -18471,9 +18495,9 @@
         <v>114</v>
       </c>
       <c r="B1522" s="87"/>
-      <c r="C1522" s="167"/>
-      <c r="D1522" s="168"/>
-      <c r="E1522" s="168"/>
+      <c r="C1522" s="164"/>
+      <c r="D1522" s="165"/>
+      <c r="E1522" s="165"/>
     </row>
     <row r="1523" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1523" s="74">
@@ -18624,9 +18648,9 @@
         <v>95</v>
       </c>
       <c r="B1539" s="87"/>
-      <c r="C1539" s="167"/>
-      <c r="D1539" s="168"/>
-      <c r="E1539" s="168"/>
+      <c r="C1539" s="164"/>
+      <c r="D1539" s="165"/>
+      <c r="E1539" s="165"/>
     </row>
     <row r="1540" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1540" s="74">
@@ -18777,9 +18801,9 @@
         <v>115</v>
       </c>
       <c r="B1556" s="87"/>
-      <c r="C1556" s="167"/>
-      <c r="D1556" s="168"/>
-      <c r="E1556" s="168"/>
+      <c r="C1556" s="164"/>
+      <c r="D1556" s="165"/>
+      <c r="E1556" s="165"/>
     </row>
     <row r="1557" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1557" s="74">
@@ -18930,9 +18954,9 @@
         <v>116</v>
       </c>
       <c r="B1573" s="87"/>
-      <c r="C1573" s="167"/>
-      <c r="D1573" s="168"/>
-      <c r="E1573" s="168"/>
+      <c r="C1573" s="164"/>
+      <c r="D1573" s="165"/>
+      <c r="E1573" s="165"/>
     </row>
     <row r="1574" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1574" s="74">
@@ -19083,9 +19107,9 @@
         <v>117</v>
       </c>
       <c r="B1590" s="87"/>
-      <c r="C1590" s="167"/>
-      <c r="D1590" s="168"/>
-      <c r="E1590" s="168"/>
+      <c r="C1590" s="164"/>
+      <c r="D1590" s="165"/>
+      <c r="E1590" s="165"/>
     </row>
     <row r="1591" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1591" s="74">
@@ -19236,9 +19260,9 @@
         <v>118</v>
       </c>
       <c r="B1607" s="87"/>
-      <c r="C1607" s="167"/>
-      <c r="D1607" s="168"/>
-      <c r="E1607" s="168"/>
+      <c r="C1607" s="164"/>
+      <c r="D1607" s="165"/>
+      <c r="E1607" s="165"/>
     </row>
     <row r="1608" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1608" s="74">
@@ -19389,9 +19413,9 @@
         <v>119</v>
       </c>
       <c r="B1624" s="87"/>
-      <c r="C1624" s="167"/>
-      <c r="D1624" s="168"/>
-      <c r="E1624" s="168"/>
+      <c r="C1624" s="164"/>
+      <c r="D1624" s="165"/>
+      <c r="E1624" s="165"/>
     </row>
     <row r="1625" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1625" s="74">
@@ -19542,18 +19566,18 @@
         <v>120</v>
       </c>
       <c r="B1641" s="42"/>
-      <c r="C1641" s="181"/>
-      <c r="D1641" s="182"/>
-      <c r="E1641" s="182"/>
+      <c r="C1641" s="170"/>
+      <c r="D1641" s="171"/>
+      <c r="E1641" s="171"/>
     </row>
     <row r="1642" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A1642" s="78" t="s">
         <v>121</v>
       </c>
       <c r="B1642" s="87"/>
-      <c r="C1642" s="167"/>
-      <c r="D1642" s="168"/>
-      <c r="E1642" s="168"/>
+      <c r="C1642" s="164"/>
+      <c r="D1642" s="165"/>
+      <c r="E1642" s="165"/>
     </row>
     <row r="1643" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1643" s="79">
@@ -19704,9 +19728,9 @@
         <v>122</v>
       </c>
       <c r="B1659" s="90"/>
-      <c r="C1659" s="169"/>
-      <c r="D1659" s="170"/>
-      <c r="E1659" s="170"/>
+      <c r="C1659" s="166"/>
+      <c r="D1659" s="167"/>
+      <c r="E1659" s="167"/>
     </row>
     <row r="1660" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1660" s="79">
@@ -19857,9 +19881,9 @@
         <v>123</v>
       </c>
       <c r="B1676" s="87"/>
-      <c r="C1676" s="167"/>
-      <c r="D1676" s="168"/>
-      <c r="E1676" s="168"/>
+      <c r="C1676" s="164"/>
+      <c r="D1676" s="165"/>
+      <c r="E1676" s="165"/>
     </row>
     <row r="1677" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1677" s="79">
@@ -20010,9 +20034,9 @@
         <v>124</v>
       </c>
       <c r="B1693" s="87"/>
-      <c r="C1693" s="167"/>
-      <c r="D1693" s="168"/>
-      <c r="E1693" s="168"/>
+      <c r="C1693" s="164"/>
+      <c r="D1693" s="165"/>
+      <c r="E1693" s="165"/>
     </row>
     <row r="1694" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1694" s="79">
@@ -20163,9 +20187,9 @@
         <v>125</v>
       </c>
       <c r="B1710" s="87"/>
-      <c r="C1710" s="167"/>
-      <c r="D1710" s="168"/>
-      <c r="E1710" s="168"/>
+      <c r="C1710" s="164"/>
+      <c r="D1710" s="165"/>
+      <c r="E1710" s="165"/>
     </row>
     <row r="1711" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1711" s="79">
@@ -20316,9 +20340,9 @@
         <v>126</v>
       </c>
       <c r="B1727" s="87"/>
-      <c r="C1727" s="167"/>
-      <c r="D1727" s="168"/>
-      <c r="E1727" s="168"/>
+      <c r="C1727" s="164"/>
+      <c r="D1727" s="165"/>
+      <c r="E1727" s="165"/>
     </row>
     <row r="1728" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1728" s="79">
@@ -20469,9 +20493,9 @@
         <v>127</v>
       </c>
       <c r="B1744" s="87"/>
-      <c r="C1744" s="167"/>
-      <c r="D1744" s="168"/>
-      <c r="E1744" s="168"/>
+      <c r="C1744" s="164"/>
+      <c r="D1744" s="165"/>
+      <c r="E1744" s="165"/>
     </row>
     <row r="1745" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1745" s="79">
@@ -20622,9 +20646,9 @@
         <v>128</v>
       </c>
       <c r="B1761" s="87"/>
-      <c r="C1761" s="167"/>
-      <c r="D1761" s="168"/>
-      <c r="E1761" s="168"/>
+      <c r="C1761" s="164"/>
+      <c r="D1761" s="165"/>
+      <c r="E1761" s="165"/>
     </row>
     <row r="1762" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1762" s="79">
@@ -20775,9 +20799,9 @@
         <v>129</v>
       </c>
       <c r="B1778" s="87"/>
-      <c r="C1778" s="167"/>
-      <c r="D1778" s="168"/>
-      <c r="E1778" s="168"/>
+      <c r="C1778" s="164"/>
+      <c r="D1778" s="165"/>
+      <c r="E1778" s="165"/>
     </row>
     <row r="1779" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1779" s="79">
@@ -20928,9 +20952,9 @@
         <v>130</v>
       </c>
       <c r="B1795" s="87"/>
-      <c r="C1795" s="167"/>
-      <c r="D1795" s="168"/>
-      <c r="E1795" s="168"/>
+      <c r="C1795" s="164"/>
+      <c r="D1795" s="165"/>
+      <c r="E1795" s="165"/>
     </row>
     <row r="1796" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1796" s="79">
@@ -21081,9 +21105,9 @@
         <v>131</v>
       </c>
       <c r="B1812" s="87"/>
-      <c r="C1812" s="167"/>
-      <c r="D1812" s="168"/>
-      <c r="E1812" s="168"/>
+      <c r="C1812" s="164"/>
+      <c r="D1812" s="165"/>
+      <c r="E1812" s="165"/>
     </row>
     <row r="1813" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1813" s="79">
@@ -21234,9 +21258,9 @@
         <v>96</v>
       </c>
       <c r="B1829" s="87"/>
-      <c r="C1829" s="167"/>
-      <c r="D1829" s="168"/>
-      <c r="E1829" s="168"/>
+      <c r="C1829" s="164"/>
+      <c r="D1829" s="165"/>
+      <c r="E1829" s="165"/>
     </row>
     <row r="1830" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1830" s="79">
@@ -21387,9 +21411,9 @@
         <v>132</v>
       </c>
       <c r="B1846" s="87"/>
-      <c r="C1846" s="167"/>
-      <c r="D1846" s="168"/>
-      <c r="E1846" s="168"/>
+      <c r="C1846" s="164"/>
+      <c r="D1846" s="165"/>
+      <c r="E1846" s="165"/>
     </row>
     <row r="1847" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1847" s="79">
@@ -21540,9 +21564,9 @@
         <v>133</v>
       </c>
       <c r="B1863" s="87"/>
-      <c r="C1863" s="167"/>
-      <c r="D1863" s="168"/>
-      <c r="E1863" s="168"/>
+      <c r="C1863" s="164"/>
+      <c r="D1863" s="165"/>
+      <c r="E1863" s="165"/>
     </row>
     <row r="1864" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1864" s="79">
@@ -21693,9 +21717,9 @@
         <v>134</v>
       </c>
       <c r="B1880" s="87"/>
-      <c r="C1880" s="167"/>
-      <c r="D1880" s="168"/>
-      <c r="E1880" s="168"/>
+      <c r="C1880" s="164"/>
+      <c r="D1880" s="165"/>
+      <c r="E1880" s="165"/>
     </row>
     <row r="1881" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1881" s="79">
@@ -21846,9 +21870,9 @@
         <v>135</v>
       </c>
       <c r="B1897" s="87"/>
-      <c r="C1897" s="167"/>
-      <c r="D1897" s="168"/>
-      <c r="E1897" s="168"/>
+      <c r="C1897" s="164"/>
+      <c r="D1897" s="165"/>
+      <c r="E1897" s="165"/>
     </row>
     <row r="1898" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1898" s="79">
@@ -21999,18 +22023,18 @@
         <v>136</v>
       </c>
       <c r="B1914" s="43"/>
-      <c r="C1914" s="183"/>
-      <c r="D1914" s="184"/>
-      <c r="E1914" s="184"/>
+      <c r="C1914" s="168"/>
+      <c r="D1914" s="169"/>
+      <c r="E1914" s="169"/>
     </row>
     <row r="1915" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A1915" s="83" t="s">
         <v>137</v>
       </c>
       <c r="B1915" s="87"/>
-      <c r="C1915" s="167"/>
-      <c r="D1915" s="168"/>
-      <c r="E1915" s="168"/>
+      <c r="C1915" s="164"/>
+      <c r="D1915" s="165"/>
+      <c r="E1915" s="165"/>
     </row>
     <row r="1916" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1916" s="84">
@@ -22161,9 +22185,9 @@
         <v>138</v>
       </c>
       <c r="B1932" s="90"/>
-      <c r="C1932" s="169"/>
-      <c r="D1932" s="170"/>
-      <c r="E1932" s="170"/>
+      <c r="C1932" s="166"/>
+      <c r="D1932" s="167"/>
+      <c r="E1932" s="167"/>
     </row>
     <row r="1933" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1933" s="84">
@@ -22314,9 +22338,9 @@
         <v>139</v>
       </c>
       <c r="B1949" s="87"/>
-      <c r="C1949" s="167"/>
-      <c r="D1949" s="168"/>
-      <c r="E1949" s="168"/>
+      <c r="C1949" s="164"/>
+      <c r="D1949" s="165"/>
+      <c r="E1949" s="165"/>
     </row>
     <row r="1950" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1950" s="84">
@@ -22467,9 +22491,9 @@
         <v>140</v>
       </c>
       <c r="B1966" s="87"/>
-      <c r="C1966" s="167"/>
-      <c r="D1966" s="168"/>
-      <c r="E1966" s="168"/>
+      <c r="C1966" s="164"/>
+      <c r="D1966" s="165"/>
+      <c r="E1966" s="165"/>
     </row>
     <row r="1967" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1967" s="84">
@@ -22620,9 +22644,9 @@
         <v>141</v>
       </c>
       <c r="B1983" s="87"/>
-      <c r="C1983" s="167"/>
-      <c r="D1983" s="168"/>
-      <c r="E1983" s="168"/>
+      <c r="C1983" s="164"/>
+      <c r="D1983" s="165"/>
+      <c r="E1983" s="165"/>
     </row>
     <row r="1984" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1984" s="84">
@@ -22773,9 +22797,9 @@
         <v>142</v>
       </c>
       <c r="B2000" s="87"/>
-      <c r="C2000" s="167"/>
-      <c r="D2000" s="168"/>
-      <c r="E2000" s="168"/>
+      <c r="C2000" s="164"/>
+      <c r="D2000" s="165"/>
+      <c r="E2000" s="165"/>
     </row>
     <row r="2001" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2001" s="84">
@@ -22926,9 +22950,9 @@
         <v>143</v>
       </c>
       <c r="B2017" s="87"/>
-      <c r="C2017" s="167"/>
-      <c r="D2017" s="168"/>
-      <c r="E2017" s="168"/>
+      <c r="C2017" s="164"/>
+      <c r="D2017" s="165"/>
+      <c r="E2017" s="165"/>
     </row>
     <row r="2018" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2018" s="84">
@@ -23079,9 +23103,9 @@
         <v>144</v>
       </c>
       <c r="B2034" s="87"/>
-      <c r="C2034" s="167"/>
-      <c r="D2034" s="168"/>
-      <c r="E2034" s="168"/>
+      <c r="C2034" s="164"/>
+      <c r="D2034" s="165"/>
+      <c r="E2034" s="165"/>
     </row>
     <row r="2035" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2035" s="84">
@@ -23232,9 +23256,9 @@
         <v>145</v>
       </c>
       <c r="B2051" s="87"/>
-      <c r="C2051" s="167"/>
-      <c r="D2051" s="168"/>
-      <c r="E2051" s="168"/>
+      <c r="C2051" s="164"/>
+      <c r="D2051" s="165"/>
+      <c r="E2051" s="165"/>
     </row>
     <row r="2052" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2052" s="84">
@@ -23385,9 +23409,9 @@
         <v>146</v>
       </c>
       <c r="B2068" s="87"/>
-      <c r="C2068" s="167"/>
-      <c r="D2068" s="168"/>
-      <c r="E2068" s="168"/>
+      <c r="C2068" s="164"/>
+      <c r="D2068" s="165"/>
+      <c r="E2068" s="165"/>
     </row>
     <row r="2069" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2069" s="84">
@@ -23538,9 +23562,9 @@
         <v>147</v>
       </c>
       <c r="B2085" s="87"/>
-      <c r="C2085" s="167"/>
-      <c r="D2085" s="168"/>
-      <c r="E2085" s="168"/>
+      <c r="C2085" s="164"/>
+      <c r="D2085" s="165"/>
+      <c r="E2085" s="165"/>
     </row>
     <row r="2086" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2086" s="84">
@@ -23691,9 +23715,9 @@
         <v>148</v>
       </c>
       <c r="B2102" s="87"/>
-      <c r="C2102" s="167"/>
-      <c r="D2102" s="168"/>
-      <c r="E2102" s="168"/>
+      <c r="C2102" s="164"/>
+      <c r="D2102" s="165"/>
+      <c r="E2102" s="165"/>
     </row>
     <row r="2103" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2103" s="84">
@@ -23844,9 +23868,9 @@
         <v>97</v>
       </c>
       <c r="B2119" s="87"/>
-      <c r="C2119" s="167"/>
-      <c r="D2119" s="168"/>
-      <c r="E2119" s="168"/>
+      <c r="C2119" s="164"/>
+      <c r="D2119" s="165"/>
+      <c r="E2119" s="165"/>
     </row>
     <row r="2120" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2120" s="84">
@@ -23997,9 +24021,9 @@
         <v>149</v>
       </c>
       <c r="B2136" s="87"/>
-      <c r="C2136" s="167"/>
-      <c r="D2136" s="168"/>
-      <c r="E2136" s="168"/>
+      <c r="C2136" s="164"/>
+      <c r="D2136" s="165"/>
+      <c r="E2136" s="165"/>
     </row>
     <row r="2137" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2137" s="84">
@@ -24150,9 +24174,9 @@
         <v>150</v>
       </c>
       <c r="B2153" s="87"/>
-      <c r="C2153" s="167"/>
-      <c r="D2153" s="168"/>
-      <c r="E2153" s="168"/>
+      <c r="C2153" s="164"/>
+      <c r="D2153" s="165"/>
+      <c r="E2153" s="165"/>
     </row>
     <row r="2154" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2154" s="84">
@@ -24303,9 +24327,9 @@
         <v>151</v>
       </c>
       <c r="B2170" s="87"/>
-      <c r="C2170" s="167"/>
-      <c r="D2170" s="168"/>
-      <c r="E2170" s="168"/>
+      <c r="C2170" s="164"/>
+      <c r="D2170" s="165"/>
+      <c r="E2170" s="165"/>
     </row>
     <row r="2171" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2171" s="84">
@@ -24453,15 +24477,122 @@
     </row>
   </sheetData>
   <mergeCells count="137">
-    <mergeCell ref="C2034:E2034"/>
-    <mergeCell ref="C2051:E2051"/>
-    <mergeCell ref="C2068:E2068"/>
-    <mergeCell ref="C2085:E2085"/>
-    <mergeCell ref="C2170:E2170"/>
-    <mergeCell ref="C2102:E2102"/>
-    <mergeCell ref="C2119:E2119"/>
-    <mergeCell ref="C2136:E2136"/>
-    <mergeCell ref="C2153:E2153"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="C89:E89"/>
+    <mergeCell ref="C21:E21"/>
+    <mergeCell ref="C38:E38"/>
+    <mergeCell ref="C55:E55"/>
+    <mergeCell ref="C72:E72"/>
+    <mergeCell ref="C208:E208"/>
+    <mergeCell ref="C225:E225"/>
+    <mergeCell ref="C242:E242"/>
+    <mergeCell ref="C259:E259"/>
+    <mergeCell ref="C276:E276"/>
+    <mergeCell ref="C277:E277"/>
+    <mergeCell ref="C106:E106"/>
+    <mergeCell ref="C123:E123"/>
+    <mergeCell ref="C140:E140"/>
+    <mergeCell ref="C157:E157"/>
+    <mergeCell ref="C174:E174"/>
+    <mergeCell ref="C191:E191"/>
+    <mergeCell ref="C396:E396"/>
+    <mergeCell ref="C413:E413"/>
+    <mergeCell ref="C430:E430"/>
+    <mergeCell ref="C447:E447"/>
+    <mergeCell ref="C464:E464"/>
+    <mergeCell ref="C481:E481"/>
+    <mergeCell ref="C294:E294"/>
+    <mergeCell ref="C311:E311"/>
+    <mergeCell ref="C328:E328"/>
+    <mergeCell ref="C345:E345"/>
+    <mergeCell ref="C362:E362"/>
+    <mergeCell ref="C379:E379"/>
+    <mergeCell ref="C584:E584"/>
+    <mergeCell ref="C601:E601"/>
+    <mergeCell ref="C618:E618"/>
+    <mergeCell ref="C635:E635"/>
+    <mergeCell ref="C652:E652"/>
+    <mergeCell ref="C669:E669"/>
+    <mergeCell ref="C498:E498"/>
+    <mergeCell ref="C515:E515"/>
+    <mergeCell ref="C532:E532"/>
+    <mergeCell ref="C549:E549"/>
+    <mergeCell ref="C550:E550"/>
+    <mergeCell ref="C567:E567"/>
+    <mergeCell ref="C788:E788"/>
+    <mergeCell ref="C805:E805"/>
+    <mergeCell ref="C822:E822"/>
+    <mergeCell ref="C823:E823"/>
+    <mergeCell ref="C840:E840"/>
+    <mergeCell ref="C857:E857"/>
+    <mergeCell ref="C686:E686"/>
+    <mergeCell ref="C703:E703"/>
+    <mergeCell ref="C720:E720"/>
+    <mergeCell ref="C737:E737"/>
+    <mergeCell ref="C754:E754"/>
+    <mergeCell ref="C771:E771"/>
+    <mergeCell ref="C976:E976"/>
+    <mergeCell ref="C993:E993"/>
+    <mergeCell ref="C1010:E1010"/>
+    <mergeCell ref="C1027:E1027"/>
+    <mergeCell ref="C1044:E1044"/>
+    <mergeCell ref="C1061:E1061"/>
+    <mergeCell ref="C874:E874"/>
+    <mergeCell ref="C891:E891"/>
+    <mergeCell ref="C908:E908"/>
+    <mergeCell ref="C925:E925"/>
+    <mergeCell ref="C942:E942"/>
+    <mergeCell ref="C959:E959"/>
+    <mergeCell ref="C1164:E1164"/>
+    <mergeCell ref="C1181:E1181"/>
+    <mergeCell ref="C1198:E1198"/>
+    <mergeCell ref="C1215:E1215"/>
+    <mergeCell ref="C1232:E1232"/>
+    <mergeCell ref="C1249:E1249"/>
+    <mergeCell ref="C1078:E1078"/>
+    <mergeCell ref="C1095:E1095"/>
+    <mergeCell ref="C1096:E1096"/>
+    <mergeCell ref="C1113:E1113"/>
+    <mergeCell ref="C1130:E1130"/>
+    <mergeCell ref="C1147:E1147"/>
+    <mergeCell ref="C1368:E1368"/>
+    <mergeCell ref="C1369:E1369"/>
+    <mergeCell ref="C1386:E1386"/>
+    <mergeCell ref="C1403:E1403"/>
+    <mergeCell ref="C1420:E1420"/>
+    <mergeCell ref="C1437:E1437"/>
+    <mergeCell ref="C1266:E1266"/>
+    <mergeCell ref="C1283:E1283"/>
+    <mergeCell ref="C1300:E1300"/>
+    <mergeCell ref="C1317:E1317"/>
+    <mergeCell ref="C1334:E1334"/>
+    <mergeCell ref="C1351:E1351"/>
+    <mergeCell ref="C1556:E1556"/>
+    <mergeCell ref="C1573:E1573"/>
+    <mergeCell ref="C1590:E1590"/>
+    <mergeCell ref="C1607:E1607"/>
+    <mergeCell ref="C1624:E1624"/>
+    <mergeCell ref="C1641:E1641"/>
+    <mergeCell ref="C1454:E1454"/>
+    <mergeCell ref="C1471:E1471"/>
+    <mergeCell ref="C1488:E1488"/>
+    <mergeCell ref="C1505:E1505"/>
+    <mergeCell ref="C1522:E1522"/>
+    <mergeCell ref="C1539:E1539"/>
+    <mergeCell ref="C1744:E1744"/>
+    <mergeCell ref="C1761:E1761"/>
+    <mergeCell ref="C1778:E1778"/>
+    <mergeCell ref="C1795:E1795"/>
+    <mergeCell ref="C1812:E1812"/>
+    <mergeCell ref="C1829:E1829"/>
+    <mergeCell ref="C1642:E1642"/>
+    <mergeCell ref="C1659:E1659"/>
+    <mergeCell ref="C1676:E1676"/>
+    <mergeCell ref="C1693:E1693"/>
+    <mergeCell ref="C1710:E1710"/>
+    <mergeCell ref="C1727:E1727"/>
     <mergeCell ref="C1932:E1932"/>
     <mergeCell ref="C1949:E1949"/>
     <mergeCell ref="C1966:E1966"/>
@@ -24474,122 +24605,15 @@
     <mergeCell ref="C1897:E1897"/>
     <mergeCell ref="C1914:E1914"/>
     <mergeCell ref="C1915:E1915"/>
-    <mergeCell ref="C1744:E1744"/>
-    <mergeCell ref="C1761:E1761"/>
-    <mergeCell ref="C1778:E1778"/>
-    <mergeCell ref="C1795:E1795"/>
-    <mergeCell ref="C1812:E1812"/>
-    <mergeCell ref="C1829:E1829"/>
-    <mergeCell ref="C1642:E1642"/>
-    <mergeCell ref="C1659:E1659"/>
-    <mergeCell ref="C1676:E1676"/>
-    <mergeCell ref="C1693:E1693"/>
-    <mergeCell ref="C1710:E1710"/>
-    <mergeCell ref="C1727:E1727"/>
-    <mergeCell ref="C1556:E1556"/>
-    <mergeCell ref="C1573:E1573"/>
-    <mergeCell ref="C1590:E1590"/>
-    <mergeCell ref="C1607:E1607"/>
-    <mergeCell ref="C1624:E1624"/>
-    <mergeCell ref="C1641:E1641"/>
-    <mergeCell ref="C1454:E1454"/>
-    <mergeCell ref="C1471:E1471"/>
-    <mergeCell ref="C1488:E1488"/>
-    <mergeCell ref="C1505:E1505"/>
-    <mergeCell ref="C1522:E1522"/>
-    <mergeCell ref="C1539:E1539"/>
-    <mergeCell ref="C1368:E1368"/>
-    <mergeCell ref="C1369:E1369"/>
-    <mergeCell ref="C1386:E1386"/>
-    <mergeCell ref="C1403:E1403"/>
-    <mergeCell ref="C1420:E1420"/>
-    <mergeCell ref="C1437:E1437"/>
-    <mergeCell ref="C1266:E1266"/>
-    <mergeCell ref="C1283:E1283"/>
-    <mergeCell ref="C1300:E1300"/>
-    <mergeCell ref="C1317:E1317"/>
-    <mergeCell ref="C1334:E1334"/>
-    <mergeCell ref="C1351:E1351"/>
-    <mergeCell ref="C1164:E1164"/>
-    <mergeCell ref="C1181:E1181"/>
-    <mergeCell ref="C1198:E1198"/>
-    <mergeCell ref="C1215:E1215"/>
-    <mergeCell ref="C1232:E1232"/>
-    <mergeCell ref="C1249:E1249"/>
-    <mergeCell ref="C1078:E1078"/>
-    <mergeCell ref="C1095:E1095"/>
-    <mergeCell ref="C1096:E1096"/>
-    <mergeCell ref="C1113:E1113"/>
-    <mergeCell ref="C1130:E1130"/>
-    <mergeCell ref="C1147:E1147"/>
-    <mergeCell ref="C976:E976"/>
-    <mergeCell ref="C993:E993"/>
-    <mergeCell ref="C1010:E1010"/>
-    <mergeCell ref="C1027:E1027"/>
-    <mergeCell ref="C1044:E1044"/>
-    <mergeCell ref="C1061:E1061"/>
-    <mergeCell ref="C874:E874"/>
-    <mergeCell ref="C891:E891"/>
-    <mergeCell ref="C908:E908"/>
-    <mergeCell ref="C925:E925"/>
-    <mergeCell ref="C942:E942"/>
-    <mergeCell ref="C959:E959"/>
-    <mergeCell ref="C788:E788"/>
-    <mergeCell ref="C805:E805"/>
-    <mergeCell ref="C822:E822"/>
-    <mergeCell ref="C823:E823"/>
-    <mergeCell ref="C840:E840"/>
-    <mergeCell ref="C857:E857"/>
-    <mergeCell ref="C686:E686"/>
-    <mergeCell ref="C703:E703"/>
-    <mergeCell ref="C720:E720"/>
-    <mergeCell ref="C737:E737"/>
-    <mergeCell ref="C754:E754"/>
-    <mergeCell ref="C771:E771"/>
-    <mergeCell ref="C584:E584"/>
-    <mergeCell ref="C601:E601"/>
-    <mergeCell ref="C618:E618"/>
-    <mergeCell ref="C635:E635"/>
-    <mergeCell ref="C652:E652"/>
-    <mergeCell ref="C669:E669"/>
-    <mergeCell ref="C498:E498"/>
-    <mergeCell ref="C515:E515"/>
-    <mergeCell ref="C532:E532"/>
-    <mergeCell ref="C549:E549"/>
-    <mergeCell ref="C550:E550"/>
-    <mergeCell ref="C567:E567"/>
-    <mergeCell ref="C396:E396"/>
-    <mergeCell ref="C413:E413"/>
-    <mergeCell ref="C430:E430"/>
-    <mergeCell ref="C447:E447"/>
-    <mergeCell ref="C464:E464"/>
-    <mergeCell ref="C481:E481"/>
-    <mergeCell ref="C294:E294"/>
-    <mergeCell ref="C311:E311"/>
-    <mergeCell ref="C328:E328"/>
-    <mergeCell ref="C345:E345"/>
-    <mergeCell ref="C362:E362"/>
-    <mergeCell ref="C379:E379"/>
-    <mergeCell ref="C225:E225"/>
-    <mergeCell ref="C242:E242"/>
-    <mergeCell ref="C259:E259"/>
-    <mergeCell ref="C276:E276"/>
-    <mergeCell ref="C277:E277"/>
-    <mergeCell ref="C106:E106"/>
-    <mergeCell ref="C123:E123"/>
-    <mergeCell ref="C140:E140"/>
-    <mergeCell ref="C157:E157"/>
-    <mergeCell ref="C174:E174"/>
-    <mergeCell ref="C191:E191"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="C89:E89"/>
-    <mergeCell ref="C21:E21"/>
-    <mergeCell ref="C38:E38"/>
-    <mergeCell ref="C55:E55"/>
-    <mergeCell ref="C72:E72"/>
-    <mergeCell ref="C208:E208"/>
+    <mergeCell ref="C2034:E2034"/>
+    <mergeCell ref="C2051:E2051"/>
+    <mergeCell ref="C2068:E2068"/>
+    <mergeCell ref="C2085:E2085"/>
+    <mergeCell ref="C2170:E2170"/>
+    <mergeCell ref="C2102:E2102"/>
+    <mergeCell ref="C2119:E2119"/>
+    <mergeCell ref="C2136:E2136"/>
+    <mergeCell ref="C2153:E2153"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -25357,7 +25381,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>
+      <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -25848,150 +25872,163 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="33">
-      <c r="A1" s="210" t="s">
+      <c r="A1" s="209" t="s">
         <v>184</v>
       </c>
-      <c r="B1" s="211"/>
+      <c r="B1" s="210"/>
       <c r="C1" s="118"/>
       <c r="D1" s="5"/>
       <c r="E1" s="5"/>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="216" t="s">
+      <c r="A2" s="206" t="s">
         <v>183</v>
       </c>
-      <c r="B2" s="217"/>
+      <c r="B2" s="207"/>
       <c r="C2" s="120"/>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="218" t="s">
+      <c r="A3" s="208" t="s">
         <v>185</v>
       </c>
-      <c r="B3" s="217"/>
+      <c r="B3" s="207"/>
       <c r="C3" s="120"/>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="214"/>
-      <c r="B4" s="215"/>
+      <c r="A4" s="213"/>
+      <c r="B4" s="214"/>
       <c r="C4" s="120"/>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="212" t="s">
+      <c r="A5" s="211" t="s">
         <v>194</v>
       </c>
-      <c r="B5" s="213"/>
+      <c r="B5" s="212"/>
       <c r="C5" s="120"/>
     </row>
     <row r="7" spans="1:5" ht="18.75">
-      <c r="A7" s="204" t="s">
+      <c r="A7" s="217" t="s">
         <v>186</v>
       </c>
-      <c r="B7" s="205"/>
+      <c r="B7" s="218"/>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="120"/>
       <c r="B8" s="9"/>
     </row>
     <row r="9" spans="1:5" ht="39" customHeight="1">
-      <c r="A9" s="206" t="s">
+      <c r="A9" s="215" t="s">
         <v>187</v>
       </c>
-      <c r="B9" s="207"/>
+      <c r="B9" s="216"/>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="208"/>
-      <c r="B10" s="209"/>
+      <c r="A10" s="202"/>
+      <c r="B10" s="203"/>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="200" t="s">
+      <c r="A11" s="204" t="s">
         <v>188</v>
       </c>
-      <c r="B11" s="201"/>
+      <c r="B11" s="205"/>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="200" t="s">
+      <c r="A12" s="204" t="s">
         <v>189</v>
       </c>
-      <c r="B12" s="201"/>
+      <c r="B12" s="205"/>
     </row>
     <row r="13" spans="1:5" ht="43.5" customHeight="1">
-      <c r="A13" s="200" t="s">
+      <c r="A13" s="204" t="s">
         <v>190</v>
       </c>
-      <c r="B13" s="201"/>
+      <c r="B13" s="205"/>
     </row>
     <row r="14" spans="1:5" ht="19.5" customHeight="1">
-      <c r="A14" s="200" t="s">
+      <c r="A14" s="204" t="s">
         <v>191</v>
       </c>
-      <c r="B14" s="201"/>
+      <c r="B14" s="205"/>
     </row>
     <row r="15" spans="1:5" ht="18" customHeight="1">
-      <c r="A15" s="200" t="s">
+      <c r="A15" s="204" t="s">
         <v>192</v>
       </c>
-      <c r="B15" s="201"/>
+      <c r="B15" s="205"/>
     </row>
     <row r="16" spans="1:5" ht="21" customHeight="1">
-      <c r="A16" s="200" t="s">
+      <c r="A16" s="204" t="s">
         <v>193</v>
       </c>
-      <c r="B16" s="201"/>
+      <c r="B16" s="205"/>
     </row>
     <row r="17" spans="1:2" ht="48.75" customHeight="1">
-      <c r="A17" s="202" t="s">
+      <c r="A17" s="200" t="s">
         <v>195</v>
       </c>
-      <c r="B17" s="203"/>
+      <c r="B17" s="201"/>
     </row>
     <row r="19" spans="1:2" ht="18.75">
-      <c r="A19" s="204" t="s">
+      <c r="A19" s="217" t="s">
         <v>197</v>
       </c>
-      <c r="B19" s="205"/>
+      <c r="B19" s="218"/>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="120"/>
       <c r="B20" s="9"/>
     </row>
     <row r="21" spans="1:2">
-      <c r="A21" s="206" t="s">
+      <c r="A21" s="215" t="s">
         <v>198</v>
       </c>
-      <c r="B21" s="207"/>
+      <c r="B21" s="216"/>
     </row>
     <row r="22" spans="1:2">
-      <c r="A22" s="208"/>
-      <c r="B22" s="209"/>
+      <c r="A22" s="202"/>
+      <c r="B22" s="203"/>
     </row>
     <row r="23" spans="1:2">
-      <c r="A23" s="200" t="s">
+      <c r="A23" s="204" t="s">
         <v>199</v>
       </c>
-      <c r="B23" s="201"/>
+      <c r="B23" s="205"/>
     </row>
     <row r="24" spans="1:2">
-      <c r="A24" s="200"/>
-      <c r="B24" s="201"/>
+      <c r="A24" s="204"/>
+      <c r="B24" s="205"/>
     </row>
     <row r="25" spans="1:2">
-      <c r="A25" s="200" t="s">
+      <c r="A25" s="204" t="s">
         <v>200</v>
       </c>
-      <c r="B25" s="201"/>
+      <c r="B25" s="205"/>
     </row>
     <row r="26" spans="1:2">
-      <c r="A26" s="200" t="s">
+      <c r="A26" s="204" t="s">
         <v>201</v>
       </c>
-      <c r="B26" s="201"/>
+      <c r="B26" s="205"/>
     </row>
     <row r="27" spans="1:2">
-      <c r="A27" s="202"/>
-      <c r="B27" s="203"/>
+      <c r="A27" s="200"/>
+      <c r="B27" s="201"/>
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A7:B7"/>
     <mergeCell ref="A17:B17"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
@@ -26002,19 +26039,6 @@
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="A14:B14"/>
     <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A24:B24"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A3" r:id="rId1"/>

</xml_diff>

<commit_message>
Tempo - 1-2 done, 15 frames saved from 1-1 lost due to having to still wait for the ...elevators?  1 frame saved at the end of the level woot.
</commit_message>
<xml_diff>
--- a/trunk/Tempo/Tempo.xlsx
+++ b/trunk/Tempo/Tempo.xlsx
@@ -2131,29 +2131,29 @@
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -2189,20 +2189,34 @@
     <xf numFmtId="0" fontId="47" fillId="22" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="41" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="4"/>
     </xf>
@@ -2212,20 +2226,6 @@
     <xf numFmtId="0" fontId="42" fillId="0" borderId="33" xfId="3" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" indent="4"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Accent1" xfId="2" builtinId="29"/>
@@ -2537,7 +2537,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C25" sqref="C25"/>
+      <selection pane="bottomLeft" activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" outlineLevelRow="2"/>
@@ -3021,16 +3021,19 @@
         <v>222</v>
       </c>
       <c r="C28" s="101">
-        <v>5822</v>
+        <v>5821</v>
       </c>
       <c r="D28" s="101">
         <v>6576</v>
       </c>
       <c r="E28" s="123">
         <f t="shared" si="1"/>
-        <v>754</v>
+        <v>755</v>
       </c>
       <c r="F28" s="105"/>
+      <c r="H28">
+        <v>5822</v>
+      </c>
     </row>
     <row r="29" spans="1:8" ht="15" outlineLevel="1">
       <c r="A29" s="155"/>
@@ -4742,6 +4745,11 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="A135:A149"/>
+    <mergeCell ref="A106:A115"/>
+    <mergeCell ref="A76:A90"/>
+    <mergeCell ref="A118:A132"/>
+    <mergeCell ref="A93:A103"/>
     <mergeCell ref="A37:A57"/>
     <mergeCell ref="A60:A73"/>
     <mergeCell ref="C5:D5"/>
@@ -4751,11 +4759,6 @@
     <mergeCell ref="A8:A18"/>
     <mergeCell ref="A21:A34"/>
     <mergeCell ref="C4:E4"/>
-    <mergeCell ref="A135:A149"/>
-    <mergeCell ref="A106:A115"/>
-    <mergeCell ref="A76:A90"/>
-    <mergeCell ref="A118:A132"/>
-    <mergeCell ref="A93:A103"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4787,13 +4790,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="26.25" customHeight="1">
-      <c r="A1" s="182" t="s">
+      <c r="A1" s="164" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="182"/>
-      <c r="C1" s="182"/>
-      <c r="D1" s="182"/>
-      <c r="E1" s="182"/>
+      <c r="B1" s="164"/>
+      <c r="C1" s="164"/>
+      <c r="D1" s="164"/>
+      <c r="E1" s="164"/>
       <c r="F1" s="7"/>
       <c r="G1" s="5"/>
       <c r="H1" s="5"/>
@@ -4823,18 +4826,18 @@
         <v>8</v>
       </c>
       <c r="B3" s="36"/>
-      <c r="C3" s="183"/>
-      <c r="D3" s="184"/>
-      <c r="E3" s="184"/>
+      <c r="C3" s="165"/>
+      <c r="D3" s="166"/>
+      <c r="E3" s="166"/>
     </row>
     <row r="4" spans="1:8" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A4" s="46" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="87"/>
-      <c r="C4" s="164"/>
-      <c r="D4" s="165"/>
-      <c r="E4" s="165"/>
+      <c r="C4" s="167"/>
+      <c r="D4" s="168"/>
+      <c r="E4" s="168"/>
       <c r="F4" s="6"/>
     </row>
     <row r="5" spans="1:8" hidden="1" outlineLevel="2">
@@ -4986,9 +4989,9 @@
         <v>9</v>
       </c>
       <c r="B21" s="90"/>
-      <c r="C21" s="166"/>
-      <c r="D21" s="167"/>
-      <c r="E21" s="167"/>
+      <c r="C21" s="169"/>
+      <c r="D21" s="170"/>
+      <c r="E21" s="170"/>
     </row>
     <row r="22" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A22" s="47">
@@ -5139,9 +5142,9 @@
         <v>10</v>
       </c>
       <c r="B38" s="87"/>
-      <c r="C38" s="164"/>
-      <c r="D38" s="165"/>
-      <c r="E38" s="165"/>
+      <c r="C38" s="167"/>
+      <c r="D38" s="168"/>
+      <c r="E38" s="168"/>
     </row>
     <row r="39" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A39" s="47">
@@ -5292,9 +5295,9 @@
         <v>11</v>
       </c>
       <c r="B55" s="87"/>
-      <c r="C55" s="164"/>
-      <c r="D55" s="165"/>
-      <c r="E55" s="165"/>
+      <c r="C55" s="167"/>
+      <c r="D55" s="168"/>
+      <c r="E55" s="168"/>
     </row>
     <row r="56" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A56" s="47">
@@ -5445,9 +5448,9 @@
         <v>12</v>
       </c>
       <c r="B72" s="87"/>
-      <c r="C72" s="164"/>
-      <c r="D72" s="165"/>
-      <c r="E72" s="165"/>
+      <c r="C72" s="167"/>
+      <c r="D72" s="168"/>
+      <c r="E72" s="168"/>
     </row>
     <row r="73" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A73" s="47">
@@ -5598,9 +5601,9 @@
         <v>13</v>
       </c>
       <c r="B89" s="87"/>
-      <c r="C89" s="164"/>
-      <c r="D89" s="165"/>
-      <c r="E89" s="165"/>
+      <c r="C89" s="167"/>
+      <c r="D89" s="168"/>
+      <c r="E89" s="168"/>
     </row>
     <row r="90" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A90" s="47">
@@ -5751,9 +5754,9 @@
         <v>14</v>
       </c>
       <c r="B106" s="87"/>
-      <c r="C106" s="164"/>
-      <c r="D106" s="165"/>
-      <c r="E106" s="165"/>
+      <c r="C106" s="167"/>
+      <c r="D106" s="168"/>
+      <c r="E106" s="168"/>
     </row>
     <row r="107" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A107" s="47">
@@ -5904,9 +5907,9 @@
         <v>15</v>
       </c>
       <c r="B123" s="87"/>
-      <c r="C123" s="164"/>
-      <c r="D123" s="165"/>
-      <c r="E123" s="165"/>
+      <c r="C123" s="167"/>
+      <c r="D123" s="168"/>
+      <c r="E123" s="168"/>
     </row>
     <row r="124" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A124" s="47">
@@ -6057,9 +6060,9 @@
         <v>16</v>
       </c>
       <c r="B140" s="87"/>
-      <c r="C140" s="164"/>
-      <c r="D140" s="165"/>
-      <c r="E140" s="165"/>
+      <c r="C140" s="167"/>
+      <c r="D140" s="168"/>
+      <c r="E140" s="168"/>
     </row>
     <row r="141" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A141" s="47">
@@ -6210,9 +6213,9 @@
         <v>17</v>
       </c>
       <c r="B157" s="87"/>
-      <c r="C157" s="164"/>
-      <c r="D157" s="165"/>
-      <c r="E157" s="165"/>
+      <c r="C157" s="167"/>
+      <c r="D157" s="168"/>
+      <c r="E157" s="168"/>
     </row>
     <row r="158" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A158" s="47">
@@ -6363,9 +6366,9 @@
         <v>18</v>
       </c>
       <c r="B174" s="87"/>
-      <c r="C174" s="164"/>
-      <c r="D174" s="165"/>
-      <c r="E174" s="165"/>
+      <c r="C174" s="167"/>
+      <c r="D174" s="168"/>
+      <c r="E174" s="168"/>
     </row>
     <row r="175" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A175" s="47">
@@ -6516,9 +6519,9 @@
         <v>19</v>
       </c>
       <c r="B191" s="87"/>
-      <c r="C191" s="164"/>
-      <c r="D191" s="165"/>
-      <c r="E191" s="165"/>
+      <c r="C191" s="167"/>
+      <c r="D191" s="168"/>
+      <c r="E191" s="168"/>
     </row>
     <row r="192" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A192" s="47">
@@ -6669,9 +6672,9 @@
         <v>20</v>
       </c>
       <c r="B208" s="87"/>
-      <c r="C208" s="164"/>
-      <c r="D208" s="165"/>
-      <c r="E208" s="165"/>
+      <c r="C208" s="167"/>
+      <c r="D208" s="168"/>
+      <c r="E208" s="168"/>
     </row>
     <row r="209" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A209" s="47">
@@ -6822,9 +6825,9 @@
         <v>21</v>
       </c>
       <c r="B225" s="87"/>
-      <c r="C225" s="164"/>
-      <c r="D225" s="165"/>
-      <c r="E225" s="165"/>
+      <c r="C225" s="167"/>
+      <c r="D225" s="168"/>
+      <c r="E225" s="168"/>
     </row>
     <row r="226" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A226" s="47">
@@ -6975,9 +6978,9 @@
         <v>22</v>
       </c>
       <c r="B242" s="87"/>
-      <c r="C242" s="164"/>
-      <c r="D242" s="165"/>
-      <c r="E242" s="165"/>
+      <c r="C242" s="167"/>
+      <c r="D242" s="168"/>
+      <c r="E242" s="168"/>
     </row>
     <row r="243" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A243" s="47">
@@ -7128,9 +7131,9 @@
         <v>23</v>
       </c>
       <c r="B259" s="87"/>
-      <c r="C259" s="164"/>
-      <c r="D259" s="165"/>
-      <c r="E259" s="165"/>
+      <c r="C259" s="167"/>
+      <c r="D259" s="168"/>
+      <c r="E259" s="168"/>
     </row>
     <row r="260" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A260" s="47">
@@ -7281,18 +7284,18 @@
         <v>24</v>
       </c>
       <c r="B276" s="37"/>
-      <c r="C276" s="180"/>
-      <c r="D276" s="181"/>
-      <c r="E276" s="181"/>
+      <c r="C276" s="171"/>
+      <c r="D276" s="172"/>
+      <c r="E276" s="172"/>
     </row>
     <row r="277" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A277" s="51" t="s">
         <v>25</v>
       </c>
       <c r="B277" s="87"/>
-      <c r="C277" s="164"/>
-      <c r="D277" s="165"/>
-      <c r="E277" s="165"/>
+      <c r="C277" s="167"/>
+      <c r="D277" s="168"/>
+      <c r="E277" s="168"/>
     </row>
     <row r="278" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A278" s="52">
@@ -7443,9 +7446,9 @@
         <v>26</v>
       </c>
       <c r="B294" s="90"/>
-      <c r="C294" s="166"/>
-      <c r="D294" s="167"/>
-      <c r="E294" s="167"/>
+      <c r="C294" s="169"/>
+      <c r="D294" s="170"/>
+      <c r="E294" s="170"/>
     </row>
     <row r="295" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A295" s="52">
@@ -7596,9 +7599,9 @@
         <v>27</v>
       </c>
       <c r="B311" s="87"/>
-      <c r="C311" s="164"/>
-      <c r="D311" s="165"/>
-      <c r="E311" s="165"/>
+      <c r="C311" s="167"/>
+      <c r="D311" s="168"/>
+      <c r="E311" s="168"/>
     </row>
     <row r="312" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A312" s="52">
@@ -7749,9 +7752,9 @@
         <v>28</v>
       </c>
       <c r="B328" s="87"/>
-      <c r="C328" s="164"/>
-      <c r="D328" s="165"/>
-      <c r="E328" s="165"/>
+      <c r="C328" s="167"/>
+      <c r="D328" s="168"/>
+      <c r="E328" s="168"/>
     </row>
     <row r="329" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A329" s="52">
@@ -7902,9 +7905,9 @@
         <v>29</v>
       </c>
       <c r="B345" s="87"/>
-      <c r="C345" s="164"/>
-      <c r="D345" s="165"/>
-      <c r="E345" s="165"/>
+      <c r="C345" s="167"/>
+      <c r="D345" s="168"/>
+      <c r="E345" s="168"/>
     </row>
     <row r="346" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A346" s="52">
@@ -8055,9 +8058,9 @@
         <v>30</v>
       </c>
       <c r="B362" s="87"/>
-      <c r="C362" s="164"/>
-      <c r="D362" s="165"/>
-      <c r="E362" s="165"/>
+      <c r="C362" s="167"/>
+      <c r="D362" s="168"/>
+      <c r="E362" s="168"/>
     </row>
     <row r="363" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A363" s="52">
@@ -8208,9 +8211,9 @@
         <v>31</v>
       </c>
       <c r="B379" s="87"/>
-      <c r="C379" s="164"/>
-      <c r="D379" s="165"/>
-      <c r="E379" s="165"/>
+      <c r="C379" s="167"/>
+      <c r="D379" s="168"/>
+      <c r="E379" s="168"/>
     </row>
     <row r="380" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A380" s="52">
@@ -8361,9 +8364,9 @@
         <v>32</v>
       </c>
       <c r="B396" s="87"/>
-      <c r="C396" s="164"/>
-      <c r="D396" s="165"/>
-      <c r="E396" s="165"/>
+      <c r="C396" s="167"/>
+      <c r="D396" s="168"/>
+      <c r="E396" s="168"/>
     </row>
     <row r="397" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A397" s="52">
@@ -8514,9 +8517,9 @@
         <v>33</v>
       </c>
       <c r="B413" s="87"/>
-      <c r="C413" s="164"/>
-      <c r="D413" s="165"/>
-      <c r="E413" s="165"/>
+      <c r="C413" s="167"/>
+      <c r="D413" s="168"/>
+      <c r="E413" s="168"/>
     </row>
     <row r="414" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A414" s="52">
@@ -8667,9 +8670,9 @@
         <v>34</v>
       </c>
       <c r="B430" s="87"/>
-      <c r="C430" s="164"/>
-      <c r="D430" s="165"/>
-      <c r="E430" s="165"/>
+      <c r="C430" s="167"/>
+      <c r="D430" s="168"/>
+      <c r="E430" s="168"/>
     </row>
     <row r="431" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A431" s="52">
@@ -8820,9 +8823,9 @@
         <v>35</v>
       </c>
       <c r="B447" s="87"/>
-      <c r="C447" s="164"/>
-      <c r="D447" s="165"/>
-      <c r="E447" s="165"/>
+      <c r="C447" s="167"/>
+      <c r="D447" s="168"/>
+      <c r="E447" s="168"/>
     </row>
     <row r="448" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A448" s="52">
@@ -8973,9 +8976,9 @@
         <v>36</v>
       </c>
       <c r="B464" s="87"/>
-      <c r="C464" s="164"/>
-      <c r="D464" s="165"/>
-      <c r="E464" s="165"/>
+      <c r="C464" s="167"/>
+      <c r="D464" s="168"/>
+      <c r="E464" s="168"/>
     </row>
     <row r="465" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A465" s="52">
@@ -9126,9 +9129,9 @@
         <v>37</v>
       </c>
       <c r="B481" s="87"/>
-      <c r="C481" s="164"/>
-      <c r="D481" s="165"/>
-      <c r="E481" s="165"/>
+      <c r="C481" s="167"/>
+      <c r="D481" s="168"/>
+      <c r="E481" s="168"/>
     </row>
     <row r="482" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A482" s="52">
@@ -9279,9 +9282,9 @@
         <v>38</v>
       </c>
       <c r="B498" s="87"/>
-      <c r="C498" s="164"/>
-      <c r="D498" s="165"/>
-      <c r="E498" s="165"/>
+      <c r="C498" s="167"/>
+      <c r="D498" s="168"/>
+      <c r="E498" s="168"/>
     </row>
     <row r="499" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A499" s="52">
@@ -9432,9 +9435,9 @@
         <v>39</v>
       </c>
       <c r="B515" s="87"/>
-      <c r="C515" s="164"/>
-      <c r="D515" s="165"/>
-      <c r="E515" s="165"/>
+      <c r="C515" s="167"/>
+      <c r="D515" s="168"/>
+      <c r="E515" s="168"/>
     </row>
     <row r="516" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A516" s="52">
@@ -9585,9 +9588,9 @@
         <v>40</v>
       </c>
       <c r="B532" s="87"/>
-      <c r="C532" s="164"/>
-      <c r="D532" s="165"/>
-      <c r="E532" s="165"/>
+      <c r="C532" s="167"/>
+      <c r="D532" s="168"/>
+      <c r="E532" s="168"/>
     </row>
     <row r="533" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A533" s="55">
@@ -9738,18 +9741,18 @@
         <v>50</v>
       </c>
       <c r="B549" s="38"/>
-      <c r="C549" s="178"/>
-      <c r="D549" s="179"/>
-      <c r="E549" s="179"/>
+      <c r="C549" s="173"/>
+      <c r="D549" s="174"/>
+      <c r="E549" s="174"/>
     </row>
     <row r="550" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A550" s="58" t="s">
         <v>51</v>
       </c>
       <c r="B550" s="87"/>
-      <c r="C550" s="164"/>
-      <c r="D550" s="165"/>
-      <c r="E550" s="165"/>
+      <c r="C550" s="167"/>
+      <c r="D550" s="168"/>
+      <c r="E550" s="168"/>
     </row>
     <row r="551" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A551" s="59">
@@ -9900,9 +9903,9 @@
         <v>52</v>
       </c>
       <c r="B567" s="90"/>
-      <c r="C567" s="166"/>
-      <c r="D567" s="167"/>
-      <c r="E567" s="167"/>
+      <c r="C567" s="169"/>
+      <c r="D567" s="170"/>
+      <c r="E567" s="170"/>
     </row>
     <row r="568" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A568" s="59">
@@ -10053,9 +10056,9 @@
         <v>53</v>
       </c>
       <c r="B584" s="87"/>
-      <c r="C584" s="164"/>
-      <c r="D584" s="165"/>
-      <c r="E584" s="165"/>
+      <c r="C584" s="167"/>
+      <c r="D584" s="168"/>
+      <c r="E584" s="168"/>
     </row>
     <row r="585" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A585" s="59">
@@ -10206,9 +10209,9 @@
         <v>54</v>
       </c>
       <c r="B601" s="87"/>
-      <c r="C601" s="164"/>
-      <c r="D601" s="165"/>
-      <c r="E601" s="165"/>
+      <c r="C601" s="167"/>
+      <c r="D601" s="168"/>
+      <c r="E601" s="168"/>
     </row>
     <row r="602" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A602" s="59">
@@ -10359,9 +10362,9 @@
         <v>55</v>
       </c>
       <c r="B618" s="87"/>
-      <c r="C618" s="164"/>
-      <c r="D618" s="165"/>
-      <c r="E618" s="165"/>
+      <c r="C618" s="167"/>
+      <c r="D618" s="168"/>
+      <c r="E618" s="168"/>
     </row>
     <row r="619" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A619" s="59">
@@ -10512,9 +10515,9 @@
         <v>56</v>
       </c>
       <c r="B635" s="87"/>
-      <c r="C635" s="164"/>
-      <c r="D635" s="165"/>
-      <c r="E635" s="165"/>
+      <c r="C635" s="167"/>
+      <c r="D635" s="168"/>
+      <c r="E635" s="168"/>
     </row>
     <row r="636" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A636" s="59">
@@ -10665,9 +10668,9 @@
         <v>57</v>
       </c>
       <c r="B652" s="87"/>
-      <c r="C652" s="164"/>
-      <c r="D652" s="165"/>
-      <c r="E652" s="165"/>
+      <c r="C652" s="167"/>
+      <c r="D652" s="168"/>
+      <c r="E652" s="168"/>
     </row>
     <row r="653" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A653" s="59">
@@ -10818,9 +10821,9 @@
         <v>58</v>
       </c>
       <c r="B669" s="87"/>
-      <c r="C669" s="164"/>
-      <c r="D669" s="165"/>
-      <c r="E669" s="165"/>
+      <c r="C669" s="167"/>
+      <c r="D669" s="168"/>
+      <c r="E669" s="168"/>
     </row>
     <row r="670" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A670" s="59">
@@ -10971,9 +10974,9 @@
         <v>59</v>
       </c>
       <c r="B686" s="87"/>
-      <c r="C686" s="164"/>
-      <c r="D686" s="165"/>
-      <c r="E686" s="165"/>
+      <c r="C686" s="167"/>
+      <c r="D686" s="168"/>
+      <c r="E686" s="168"/>
     </row>
     <row r="687" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A687" s="59">
@@ -11124,9 +11127,9 @@
         <v>60</v>
       </c>
       <c r="B703" s="87"/>
-      <c r="C703" s="164"/>
-      <c r="D703" s="165"/>
-      <c r="E703" s="165"/>
+      <c r="C703" s="167"/>
+      <c r="D703" s="168"/>
+      <c r="E703" s="168"/>
     </row>
     <row r="704" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A704" s="59">
@@ -11277,9 +11280,9 @@
         <v>61</v>
       </c>
       <c r="B720" s="87"/>
-      <c r="C720" s="164"/>
-      <c r="D720" s="165"/>
-      <c r="E720" s="165"/>
+      <c r="C720" s="167"/>
+      <c r="D720" s="168"/>
+      <c r="E720" s="168"/>
     </row>
     <row r="721" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A721" s="59">
@@ -11430,9 +11433,9 @@
         <v>62</v>
       </c>
       <c r="B737" s="87"/>
-      <c r="C737" s="164"/>
-      <c r="D737" s="165"/>
-      <c r="E737" s="165"/>
+      <c r="C737" s="167"/>
+      <c r="D737" s="168"/>
+      <c r="E737" s="168"/>
     </row>
     <row r="738" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A738" s="59">
@@ -11583,9 +11586,9 @@
         <v>63</v>
       </c>
       <c r="B754" s="87"/>
-      <c r="C754" s="164"/>
-      <c r="D754" s="165"/>
-      <c r="E754" s="165"/>
+      <c r="C754" s="167"/>
+      <c r="D754" s="168"/>
+      <c r="E754" s="168"/>
     </row>
     <row r="755" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A755" s="59">
@@ -11736,9 +11739,9 @@
         <v>64</v>
       </c>
       <c r="B771" s="87"/>
-      <c r="C771" s="164"/>
-      <c r="D771" s="165"/>
-      <c r="E771" s="165"/>
+      <c r="C771" s="167"/>
+      <c r="D771" s="168"/>
+      <c r="E771" s="168"/>
     </row>
     <row r="772" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A772" s="59">
@@ -11889,9 +11892,9 @@
         <v>65</v>
       </c>
       <c r="B788" s="87"/>
-      <c r="C788" s="164"/>
-      <c r="D788" s="165"/>
-      <c r="E788" s="165"/>
+      <c r="C788" s="167"/>
+      <c r="D788" s="168"/>
+      <c r="E788" s="168"/>
     </row>
     <row r="789" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A789" s="59">
@@ -12042,9 +12045,9 @@
         <v>66</v>
       </c>
       <c r="B805" s="87"/>
-      <c r="C805" s="164"/>
-      <c r="D805" s="165"/>
-      <c r="E805" s="165"/>
+      <c r="C805" s="167"/>
+      <c r="D805" s="168"/>
+      <c r="E805" s="168"/>
     </row>
     <row r="806" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A806" s="59">
@@ -12195,18 +12198,18 @@
         <v>67</v>
       </c>
       <c r="B822" s="39"/>
-      <c r="C822" s="176"/>
-      <c r="D822" s="177"/>
-      <c r="E822" s="177"/>
+      <c r="C822" s="175"/>
+      <c r="D822" s="176"/>
+      <c r="E822" s="176"/>
     </row>
     <row r="823" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A823" s="63" t="s">
         <v>68</v>
       </c>
       <c r="B823" s="87"/>
-      <c r="C823" s="164"/>
-      <c r="D823" s="165"/>
-      <c r="E823" s="165"/>
+      <c r="C823" s="167"/>
+      <c r="D823" s="168"/>
+      <c r="E823" s="168"/>
     </row>
     <row r="824" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A824" s="64">
@@ -12357,9 +12360,9 @@
         <v>69</v>
       </c>
       <c r="B840" s="90"/>
-      <c r="C840" s="166"/>
-      <c r="D840" s="167"/>
-      <c r="E840" s="167"/>
+      <c r="C840" s="169"/>
+      <c r="D840" s="170"/>
+      <c r="E840" s="170"/>
     </row>
     <row r="841" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A841" s="64">
@@ -12510,9 +12513,9 @@
         <v>70</v>
       </c>
       <c r="B857" s="87"/>
-      <c r="C857" s="164"/>
-      <c r="D857" s="165"/>
-      <c r="E857" s="165"/>
+      <c r="C857" s="167"/>
+      <c r="D857" s="168"/>
+      <c r="E857" s="168"/>
     </row>
     <row r="858" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A858" s="64">
@@ -12663,9 +12666,9 @@
         <v>71</v>
       </c>
       <c r="B874" s="87"/>
-      <c r="C874" s="164"/>
-      <c r="D874" s="165"/>
-      <c r="E874" s="165"/>
+      <c r="C874" s="167"/>
+      <c r="D874" s="168"/>
+      <c r="E874" s="168"/>
     </row>
     <row r="875" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A875" s="64">
@@ -12816,9 +12819,9 @@
         <v>72</v>
       </c>
       <c r="B891" s="87"/>
-      <c r="C891" s="164"/>
-      <c r="D891" s="165"/>
-      <c r="E891" s="165"/>
+      <c r="C891" s="167"/>
+      <c r="D891" s="168"/>
+      <c r="E891" s="168"/>
     </row>
     <row r="892" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A892" s="64">
@@ -12969,9 +12972,9 @@
         <v>73</v>
       </c>
       <c r="B908" s="87"/>
-      <c r="C908" s="164"/>
-      <c r="D908" s="165"/>
-      <c r="E908" s="165"/>
+      <c r="C908" s="167"/>
+      <c r="D908" s="168"/>
+      <c r="E908" s="168"/>
     </row>
     <row r="909" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A909" s="64">
@@ -13122,9 +13125,9 @@
         <v>74</v>
       </c>
       <c r="B925" s="87"/>
-      <c r="C925" s="164"/>
-      <c r="D925" s="165"/>
-      <c r="E925" s="165"/>
+      <c r="C925" s="167"/>
+      <c r="D925" s="168"/>
+      <c r="E925" s="168"/>
     </row>
     <row r="926" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A926" s="64">
@@ -13275,9 +13278,9 @@
         <v>75</v>
       </c>
       <c r="B942" s="87"/>
-      <c r="C942" s="164"/>
-      <c r="D942" s="165"/>
-      <c r="E942" s="165"/>
+      <c r="C942" s="167"/>
+      <c r="D942" s="168"/>
+      <c r="E942" s="168"/>
     </row>
     <row r="943" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A943" s="64">
@@ -13428,9 +13431,9 @@
         <v>76</v>
       </c>
       <c r="B959" s="87"/>
-      <c r="C959" s="164"/>
-      <c r="D959" s="165"/>
-      <c r="E959" s="165"/>
+      <c r="C959" s="167"/>
+      <c r="D959" s="168"/>
+      <c r="E959" s="168"/>
     </row>
     <row r="960" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A960" s="64">
@@ -13581,9 +13584,9 @@
         <v>77</v>
       </c>
       <c r="B976" s="87"/>
-      <c r="C976" s="164"/>
-      <c r="D976" s="165"/>
-      <c r="E976" s="165"/>
+      <c r="C976" s="167"/>
+      <c r="D976" s="168"/>
+      <c r="E976" s="168"/>
     </row>
     <row r="977" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A977" s="64">
@@ -13734,9 +13737,9 @@
         <v>78</v>
       </c>
       <c r="B993" s="87"/>
-      <c r="C993" s="164"/>
-      <c r="D993" s="165"/>
-      <c r="E993" s="165"/>
+      <c r="C993" s="167"/>
+      <c r="D993" s="168"/>
+      <c r="E993" s="168"/>
     </row>
     <row r="994" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A994" s="64">
@@ -13887,9 +13890,9 @@
         <v>79</v>
       </c>
       <c r="B1010" s="87"/>
-      <c r="C1010" s="164"/>
-      <c r="D1010" s="165"/>
-      <c r="E1010" s="165"/>
+      <c r="C1010" s="167"/>
+      <c r="D1010" s="168"/>
+      <c r="E1010" s="168"/>
     </row>
     <row r="1011" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1011" s="64">
@@ -14040,9 +14043,9 @@
         <v>80</v>
       </c>
       <c r="B1027" s="87"/>
-      <c r="C1027" s="164"/>
-      <c r="D1027" s="165"/>
-      <c r="E1027" s="165"/>
+      <c r="C1027" s="167"/>
+      <c r="D1027" s="168"/>
+      <c r="E1027" s="168"/>
     </row>
     <row r="1028" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1028" s="64">
@@ -14193,9 +14196,9 @@
         <v>83</v>
       </c>
       <c r="B1044" s="87"/>
-      <c r="C1044" s="164"/>
-      <c r="D1044" s="165"/>
-      <c r="E1044" s="165"/>
+      <c r="C1044" s="167"/>
+      <c r="D1044" s="168"/>
+      <c r="E1044" s="168"/>
     </row>
     <row r="1045" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1045" s="64">
@@ -14346,9 +14349,9 @@
         <v>82</v>
       </c>
       <c r="B1061" s="87"/>
-      <c r="C1061" s="164"/>
-      <c r="D1061" s="165"/>
-      <c r="E1061" s="165"/>
+      <c r="C1061" s="167"/>
+      <c r="D1061" s="168"/>
+      <c r="E1061" s="168"/>
     </row>
     <row r="1062" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1062" s="64">
@@ -14499,9 +14502,9 @@
         <v>84</v>
       </c>
       <c r="B1078" s="87"/>
-      <c r="C1078" s="164"/>
-      <c r="D1078" s="165"/>
-      <c r="E1078" s="165"/>
+      <c r="C1078" s="167"/>
+      <c r="D1078" s="168"/>
+      <c r="E1078" s="168"/>
     </row>
     <row r="1079" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1079" s="64">
@@ -14652,18 +14655,18 @@
         <v>104</v>
       </c>
       <c r="B1095" s="40"/>
-      <c r="C1095" s="174"/>
-      <c r="D1095" s="175"/>
-      <c r="E1095" s="175"/>
+      <c r="C1095" s="177"/>
+      <c r="D1095" s="178"/>
+      <c r="E1095" s="178"/>
     </row>
     <row r="1096" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A1096" s="68" t="s">
         <v>85</v>
       </c>
       <c r="B1096" s="87"/>
-      <c r="C1096" s="164"/>
-      <c r="D1096" s="165"/>
-      <c r="E1096" s="165"/>
+      <c r="C1096" s="167"/>
+      <c r="D1096" s="168"/>
+      <c r="E1096" s="168"/>
     </row>
     <row r="1097" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1097" s="69">
@@ -14814,9 +14817,9 @@
         <v>86</v>
       </c>
       <c r="B1113" s="90"/>
-      <c r="C1113" s="166"/>
-      <c r="D1113" s="167"/>
-      <c r="E1113" s="167"/>
+      <c r="C1113" s="169"/>
+      <c r="D1113" s="170"/>
+      <c r="E1113" s="170"/>
     </row>
     <row r="1114" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1114" s="69">
@@ -14967,9 +14970,9 @@
         <v>87</v>
       </c>
       <c r="B1130" s="87"/>
-      <c r="C1130" s="164"/>
-      <c r="D1130" s="165"/>
-      <c r="E1130" s="165"/>
+      <c r="C1130" s="167"/>
+      <c r="D1130" s="168"/>
+      <c r="E1130" s="168"/>
     </row>
     <row r="1131" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1131" s="69">
@@ -15120,9 +15123,9 @@
         <v>88</v>
       </c>
       <c r="B1147" s="87"/>
-      <c r="C1147" s="164"/>
-      <c r="D1147" s="165"/>
-      <c r="E1147" s="165"/>
+      <c r="C1147" s="167"/>
+      <c r="D1147" s="168"/>
+      <c r="E1147" s="168"/>
     </row>
     <row r="1148" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1148" s="69">
@@ -15273,9 +15276,9 @@
         <v>89</v>
       </c>
       <c r="B1164" s="87"/>
-      <c r="C1164" s="164"/>
-      <c r="D1164" s="165"/>
-      <c r="E1164" s="165"/>
+      <c r="C1164" s="167"/>
+      <c r="D1164" s="168"/>
+      <c r="E1164" s="168"/>
     </row>
     <row r="1165" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1165" s="69">
@@ -15426,9 +15429,9 @@
         <v>90</v>
       </c>
       <c r="B1181" s="87"/>
-      <c r="C1181" s="164"/>
-      <c r="D1181" s="165"/>
-      <c r="E1181" s="165"/>
+      <c r="C1181" s="167"/>
+      <c r="D1181" s="168"/>
+      <c r="E1181" s="168"/>
     </row>
     <row r="1182" spans="1:5" hidden="1" outlineLevel="3">
       <c r="A1182" s="69">
@@ -15579,9 +15582,9 @@
         <v>91</v>
       </c>
       <c r="B1198" s="87"/>
-      <c r="C1198" s="164"/>
-      <c r="D1198" s="165"/>
-      <c r="E1198" s="165"/>
+      <c r="C1198" s="167"/>
+      <c r="D1198" s="168"/>
+      <c r="E1198" s="168"/>
     </row>
     <row r="1199" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1199" s="69">
@@ -15732,9 +15735,9 @@
         <v>92</v>
       </c>
       <c r="B1215" s="87"/>
-      <c r="C1215" s="164"/>
-      <c r="D1215" s="165"/>
-      <c r="E1215" s="165"/>
+      <c r="C1215" s="167"/>
+      <c r="D1215" s="168"/>
+      <c r="E1215" s="168"/>
     </row>
     <row r="1216" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1216" s="69">
@@ -15885,9 +15888,9 @@
         <v>93</v>
       </c>
       <c r="B1232" s="87"/>
-      <c r="C1232" s="164"/>
-      <c r="D1232" s="165"/>
-      <c r="E1232" s="165"/>
+      <c r="C1232" s="167"/>
+      <c r="D1232" s="168"/>
+      <c r="E1232" s="168"/>
     </row>
     <row r="1233" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1233" s="69">
@@ -16038,9 +16041,9 @@
         <v>94</v>
       </c>
       <c r="B1249" s="87"/>
-      <c r="C1249" s="164"/>
-      <c r="D1249" s="165"/>
-      <c r="E1249" s="165"/>
+      <c r="C1249" s="167"/>
+      <c r="D1249" s="168"/>
+      <c r="E1249" s="168"/>
     </row>
     <row r="1250" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1250" s="69">
@@ -16191,9 +16194,9 @@
         <v>99</v>
       </c>
       <c r="B1266" s="87"/>
-      <c r="C1266" s="164"/>
-      <c r="D1266" s="165"/>
-      <c r="E1266" s="165"/>
+      <c r="C1266" s="167"/>
+      <c r="D1266" s="168"/>
+      <c r="E1266" s="168"/>
     </row>
     <row r="1267" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1267" s="69">
@@ -16344,9 +16347,9 @@
         <v>100</v>
       </c>
       <c r="B1283" s="87"/>
-      <c r="C1283" s="164"/>
-      <c r="D1283" s="165"/>
-      <c r="E1283" s="165"/>
+      <c r="C1283" s="167"/>
+      <c r="D1283" s="168"/>
+      <c r="E1283" s="168"/>
     </row>
     <row r="1284" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1284" s="69">
@@ -16497,9 +16500,9 @@
         <v>101</v>
       </c>
       <c r="B1300" s="87"/>
-      <c r="C1300" s="164"/>
-      <c r="D1300" s="165"/>
-      <c r="E1300" s="165"/>
+      <c r="C1300" s="167"/>
+      <c r="D1300" s="168"/>
+      <c r="E1300" s="168"/>
     </row>
     <row r="1301" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1301" s="69">
@@ -16650,9 +16653,9 @@
         <v>81</v>
       </c>
       <c r="B1317" s="87"/>
-      <c r="C1317" s="164"/>
-      <c r="D1317" s="165"/>
-      <c r="E1317" s="165"/>
+      <c r="C1317" s="167"/>
+      <c r="D1317" s="168"/>
+      <c r="E1317" s="168"/>
     </row>
     <row r="1318" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1318" s="69">
@@ -16803,9 +16806,9 @@
         <v>102</v>
       </c>
       <c r="B1334" s="87"/>
-      <c r="C1334" s="164"/>
-      <c r="D1334" s="165"/>
-      <c r="E1334" s="165"/>
+      <c r="C1334" s="167"/>
+      <c r="D1334" s="168"/>
+      <c r="E1334" s="168"/>
     </row>
     <row r="1335" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1335" s="69">
@@ -16956,9 +16959,9 @@
         <v>98</v>
       </c>
       <c r="B1351" s="87"/>
-      <c r="C1351" s="164"/>
-      <c r="D1351" s="165"/>
-      <c r="E1351" s="165"/>
+      <c r="C1351" s="167"/>
+      <c r="D1351" s="168"/>
+      <c r="E1351" s="168"/>
     </row>
     <row r="1352" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1352" s="69">
@@ -17109,18 +17112,18 @@
         <v>103</v>
       </c>
       <c r="B1368" s="41"/>
-      <c r="C1368" s="172"/>
-      <c r="D1368" s="173"/>
-      <c r="E1368" s="173"/>
+      <c r="C1368" s="179"/>
+      <c r="D1368" s="180"/>
+      <c r="E1368" s="180"/>
     </row>
     <row r="1369" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A1369" s="73" t="s">
         <v>105</v>
       </c>
       <c r="B1369" s="87"/>
-      <c r="C1369" s="164"/>
-      <c r="D1369" s="165"/>
-      <c r="E1369" s="165"/>
+      <c r="C1369" s="167"/>
+      <c r="D1369" s="168"/>
+      <c r="E1369" s="168"/>
     </row>
     <row r="1370" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1370" s="74">
@@ -17271,9 +17274,9 @@
         <v>106</v>
       </c>
       <c r="B1386" s="90"/>
-      <c r="C1386" s="166"/>
-      <c r="D1386" s="167"/>
-      <c r="E1386" s="167"/>
+      <c r="C1386" s="169"/>
+      <c r="D1386" s="170"/>
+      <c r="E1386" s="170"/>
     </row>
     <row r="1387" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1387" s="74">
@@ -17424,9 +17427,9 @@
         <v>107</v>
       </c>
       <c r="B1403" s="87"/>
-      <c r="C1403" s="164"/>
-      <c r="D1403" s="165"/>
-      <c r="E1403" s="165"/>
+      <c r="C1403" s="167"/>
+      <c r="D1403" s="168"/>
+      <c r="E1403" s="168"/>
     </row>
     <row r="1404" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1404" s="74">
@@ -17577,9 +17580,9 @@
         <v>108</v>
       </c>
       <c r="B1420" s="87"/>
-      <c r="C1420" s="164"/>
-      <c r="D1420" s="165"/>
-      <c r="E1420" s="165"/>
+      <c r="C1420" s="167"/>
+      <c r="D1420" s="168"/>
+      <c r="E1420" s="168"/>
     </row>
     <row r="1421" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1421" s="74">
@@ -17730,9 +17733,9 @@
         <v>109</v>
       </c>
       <c r="B1437" s="87"/>
-      <c r="C1437" s="164"/>
-      <c r="D1437" s="165"/>
-      <c r="E1437" s="165"/>
+      <c r="C1437" s="167"/>
+      <c r="D1437" s="168"/>
+      <c r="E1437" s="168"/>
     </row>
     <row r="1438" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1438" s="74">
@@ -17883,9 +17886,9 @@
         <v>110</v>
       </c>
       <c r="B1454" s="87"/>
-      <c r="C1454" s="164"/>
-      <c r="D1454" s="165"/>
-      <c r="E1454" s="165"/>
+      <c r="C1454" s="167"/>
+      <c r="D1454" s="168"/>
+      <c r="E1454" s="168"/>
     </row>
     <row r="1455" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1455" s="74">
@@ -18036,9 +18039,9 @@
         <v>111</v>
       </c>
       <c r="B1471" s="87"/>
-      <c r="C1471" s="164"/>
-      <c r="D1471" s="165"/>
-      <c r="E1471" s="165"/>
+      <c r="C1471" s="167"/>
+      <c r="D1471" s="168"/>
+      <c r="E1471" s="168"/>
     </row>
     <row r="1472" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1472" s="74">
@@ -18189,9 +18192,9 @@
         <v>112</v>
       </c>
       <c r="B1488" s="87"/>
-      <c r="C1488" s="164"/>
-      <c r="D1488" s="165"/>
-      <c r="E1488" s="165"/>
+      <c r="C1488" s="167"/>
+      <c r="D1488" s="168"/>
+      <c r="E1488" s="168"/>
     </row>
     <row r="1489" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1489" s="74">
@@ -18342,9 +18345,9 @@
         <v>113</v>
       </c>
       <c r="B1505" s="87"/>
-      <c r="C1505" s="164"/>
-      <c r="D1505" s="165"/>
-      <c r="E1505" s="165"/>
+      <c r="C1505" s="167"/>
+      <c r="D1505" s="168"/>
+      <c r="E1505" s="168"/>
     </row>
     <row r="1506" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1506" s="74">
@@ -18495,9 +18498,9 @@
         <v>114</v>
       </c>
       <c r="B1522" s="87"/>
-      <c r="C1522" s="164"/>
-      <c r="D1522" s="165"/>
-      <c r="E1522" s="165"/>
+      <c r="C1522" s="167"/>
+      <c r="D1522" s="168"/>
+      <c r="E1522" s="168"/>
     </row>
     <row r="1523" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1523" s="74">
@@ -18648,9 +18651,9 @@
         <v>95</v>
       </c>
       <c r="B1539" s="87"/>
-      <c r="C1539" s="164"/>
-      <c r="D1539" s="165"/>
-      <c r="E1539" s="165"/>
+      <c r="C1539" s="167"/>
+      <c r="D1539" s="168"/>
+      <c r="E1539" s="168"/>
     </row>
     <row r="1540" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1540" s="74">
@@ -18801,9 +18804,9 @@
         <v>115</v>
       </c>
       <c r="B1556" s="87"/>
-      <c r="C1556" s="164"/>
-      <c r="D1556" s="165"/>
-      <c r="E1556" s="165"/>
+      <c r="C1556" s="167"/>
+      <c r="D1556" s="168"/>
+      <c r="E1556" s="168"/>
     </row>
     <row r="1557" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1557" s="74">
@@ -18954,9 +18957,9 @@
         <v>116</v>
       </c>
       <c r="B1573" s="87"/>
-      <c r="C1573" s="164"/>
-      <c r="D1573" s="165"/>
-      <c r="E1573" s="165"/>
+      <c r="C1573" s="167"/>
+      <c r="D1573" s="168"/>
+      <c r="E1573" s="168"/>
     </row>
     <row r="1574" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1574" s="74">
@@ -19107,9 +19110,9 @@
         <v>117</v>
       </c>
       <c r="B1590" s="87"/>
-      <c r="C1590" s="164"/>
-      <c r="D1590" s="165"/>
-      <c r="E1590" s="165"/>
+      <c r="C1590" s="167"/>
+      <c r="D1590" s="168"/>
+      <c r="E1590" s="168"/>
     </row>
     <row r="1591" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1591" s="74">
@@ -19260,9 +19263,9 @@
         <v>118</v>
       </c>
       <c r="B1607" s="87"/>
-      <c r="C1607" s="164"/>
-      <c r="D1607" s="165"/>
-      <c r="E1607" s="165"/>
+      <c r="C1607" s="167"/>
+      <c r="D1607" s="168"/>
+      <c r="E1607" s="168"/>
     </row>
     <row r="1608" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1608" s="74">
@@ -19413,9 +19416,9 @@
         <v>119</v>
       </c>
       <c r="B1624" s="87"/>
-      <c r="C1624" s="164"/>
-      <c r="D1624" s="165"/>
-      <c r="E1624" s="165"/>
+      <c r="C1624" s="167"/>
+      <c r="D1624" s="168"/>
+      <c r="E1624" s="168"/>
     </row>
     <row r="1625" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1625" s="74">
@@ -19566,18 +19569,18 @@
         <v>120</v>
       </c>
       <c r="B1641" s="42"/>
-      <c r="C1641" s="170"/>
-      <c r="D1641" s="171"/>
-      <c r="E1641" s="171"/>
+      <c r="C1641" s="181"/>
+      <c r="D1641" s="182"/>
+      <c r="E1641" s="182"/>
     </row>
     <row r="1642" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A1642" s="78" t="s">
         <v>121</v>
       </c>
       <c r="B1642" s="87"/>
-      <c r="C1642" s="164"/>
-      <c r="D1642" s="165"/>
-      <c r="E1642" s="165"/>
+      <c r="C1642" s="167"/>
+      <c r="D1642" s="168"/>
+      <c r="E1642" s="168"/>
     </row>
     <row r="1643" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1643" s="79">
@@ -19728,9 +19731,9 @@
         <v>122</v>
       </c>
       <c r="B1659" s="90"/>
-      <c r="C1659" s="166"/>
-      <c r="D1659" s="167"/>
-      <c r="E1659" s="167"/>
+      <c r="C1659" s="169"/>
+      <c r="D1659" s="170"/>
+      <c r="E1659" s="170"/>
     </row>
     <row r="1660" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1660" s="79">
@@ -19881,9 +19884,9 @@
         <v>123</v>
       </c>
       <c r="B1676" s="87"/>
-      <c r="C1676" s="164"/>
-      <c r="D1676" s="165"/>
-      <c r="E1676" s="165"/>
+      <c r="C1676" s="167"/>
+      <c r="D1676" s="168"/>
+      <c r="E1676" s="168"/>
     </row>
     <row r="1677" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1677" s="79">
@@ -20034,9 +20037,9 @@
         <v>124</v>
       </c>
       <c r="B1693" s="87"/>
-      <c r="C1693" s="164"/>
-      <c r="D1693" s="165"/>
-      <c r="E1693" s="165"/>
+      <c r="C1693" s="167"/>
+      <c r="D1693" s="168"/>
+      <c r="E1693" s="168"/>
     </row>
     <row r="1694" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1694" s="79">
@@ -20187,9 +20190,9 @@
         <v>125</v>
       </c>
       <c r="B1710" s="87"/>
-      <c r="C1710" s="164"/>
-      <c r="D1710" s="165"/>
-      <c r="E1710" s="165"/>
+      <c r="C1710" s="167"/>
+      <c r="D1710" s="168"/>
+      <c r="E1710" s="168"/>
     </row>
     <row r="1711" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1711" s="79">
@@ -20340,9 +20343,9 @@
         <v>126</v>
       </c>
       <c r="B1727" s="87"/>
-      <c r="C1727" s="164"/>
-      <c r="D1727" s="165"/>
-      <c r="E1727" s="165"/>
+      <c r="C1727" s="167"/>
+      <c r="D1727" s="168"/>
+      <c r="E1727" s="168"/>
     </row>
     <row r="1728" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1728" s="79">
@@ -20493,9 +20496,9 @@
         <v>127</v>
       </c>
       <c r="B1744" s="87"/>
-      <c r="C1744" s="164"/>
-      <c r="D1744" s="165"/>
-      <c r="E1744" s="165"/>
+      <c r="C1744" s="167"/>
+      <c r="D1744" s="168"/>
+      <c r="E1744" s="168"/>
     </row>
     <row r="1745" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1745" s="79">
@@ -20646,9 +20649,9 @@
         <v>128</v>
       </c>
       <c r="B1761" s="87"/>
-      <c r="C1761" s="164"/>
-      <c r="D1761" s="165"/>
-      <c r="E1761" s="165"/>
+      <c r="C1761" s="167"/>
+      <c r="D1761" s="168"/>
+      <c r="E1761" s="168"/>
     </row>
     <row r="1762" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1762" s="79">
@@ -20799,9 +20802,9 @@
         <v>129</v>
       </c>
       <c r="B1778" s="87"/>
-      <c r="C1778" s="164"/>
-      <c r="D1778" s="165"/>
-      <c r="E1778" s="165"/>
+      <c r="C1778" s="167"/>
+      <c r="D1778" s="168"/>
+      <c r="E1778" s="168"/>
     </row>
     <row r="1779" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1779" s="79">
@@ -20952,9 +20955,9 @@
         <v>130</v>
       </c>
       <c r="B1795" s="87"/>
-      <c r="C1795" s="164"/>
-      <c r="D1795" s="165"/>
-      <c r="E1795" s="165"/>
+      <c r="C1795" s="167"/>
+      <c r="D1795" s="168"/>
+      <c r="E1795" s="168"/>
     </row>
     <row r="1796" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1796" s="79">
@@ -21105,9 +21108,9 @@
         <v>131</v>
       </c>
       <c r="B1812" s="87"/>
-      <c r="C1812" s="164"/>
-      <c r="D1812" s="165"/>
-      <c r="E1812" s="165"/>
+      <c r="C1812" s="167"/>
+      <c r="D1812" s="168"/>
+      <c r="E1812" s="168"/>
     </row>
     <row r="1813" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1813" s="79">
@@ -21258,9 +21261,9 @@
         <v>96</v>
       </c>
       <c r="B1829" s="87"/>
-      <c r="C1829" s="164"/>
-      <c r="D1829" s="165"/>
-      <c r="E1829" s="165"/>
+      <c r="C1829" s="167"/>
+      <c r="D1829" s="168"/>
+      <c r="E1829" s="168"/>
     </row>
     <row r="1830" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1830" s="79">
@@ -21411,9 +21414,9 @@
         <v>132</v>
       </c>
       <c r="B1846" s="87"/>
-      <c r="C1846" s="164"/>
-      <c r="D1846" s="165"/>
-      <c r="E1846" s="165"/>
+      <c r="C1846" s="167"/>
+      <c r="D1846" s="168"/>
+      <c r="E1846" s="168"/>
     </row>
     <row r="1847" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1847" s="79">
@@ -21564,9 +21567,9 @@
         <v>133</v>
       </c>
       <c r="B1863" s="87"/>
-      <c r="C1863" s="164"/>
-      <c r="D1863" s="165"/>
-      <c r="E1863" s="165"/>
+      <c r="C1863" s="167"/>
+      <c r="D1863" s="168"/>
+      <c r="E1863" s="168"/>
     </row>
     <row r="1864" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1864" s="79">
@@ -21717,9 +21720,9 @@
         <v>134</v>
       </c>
       <c r="B1880" s="87"/>
-      <c r="C1880" s="164"/>
-      <c r="D1880" s="165"/>
-      <c r="E1880" s="165"/>
+      <c r="C1880" s="167"/>
+      <c r="D1880" s="168"/>
+      <c r="E1880" s="168"/>
     </row>
     <row r="1881" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1881" s="79">
@@ -21870,9 +21873,9 @@
         <v>135</v>
       </c>
       <c r="B1897" s="87"/>
-      <c r="C1897" s="164"/>
-      <c r="D1897" s="165"/>
-      <c r="E1897" s="165"/>
+      <c r="C1897" s="167"/>
+      <c r="D1897" s="168"/>
+      <c r="E1897" s="168"/>
     </row>
     <row r="1898" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1898" s="79">
@@ -22023,18 +22026,18 @@
         <v>136</v>
       </c>
       <c r="B1914" s="43"/>
-      <c r="C1914" s="168"/>
-      <c r="D1914" s="169"/>
-      <c r="E1914" s="169"/>
+      <c r="C1914" s="183"/>
+      <c r="D1914" s="184"/>
+      <c r="E1914" s="184"/>
     </row>
     <row r="1915" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A1915" s="83" t="s">
         <v>137</v>
       </c>
       <c r="B1915" s="87"/>
-      <c r="C1915" s="164"/>
-      <c r="D1915" s="165"/>
-      <c r="E1915" s="165"/>
+      <c r="C1915" s="167"/>
+      <c r="D1915" s="168"/>
+      <c r="E1915" s="168"/>
     </row>
     <row r="1916" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1916" s="84">
@@ -22185,9 +22188,9 @@
         <v>138</v>
       </c>
       <c r="B1932" s="90"/>
-      <c r="C1932" s="166"/>
-      <c r="D1932" s="167"/>
-      <c r="E1932" s="167"/>
+      <c r="C1932" s="169"/>
+      <c r="D1932" s="170"/>
+      <c r="E1932" s="170"/>
     </row>
     <row r="1933" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1933" s="84">
@@ -22338,9 +22341,9 @@
         <v>139</v>
       </c>
       <c r="B1949" s="87"/>
-      <c r="C1949" s="164"/>
-      <c r="D1949" s="165"/>
-      <c r="E1949" s="165"/>
+      <c r="C1949" s="167"/>
+      <c r="D1949" s="168"/>
+      <c r="E1949" s="168"/>
     </row>
     <row r="1950" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1950" s="84">
@@ -22491,9 +22494,9 @@
         <v>140</v>
       </c>
       <c r="B1966" s="87"/>
-      <c r="C1966" s="164"/>
-      <c r="D1966" s="165"/>
-      <c r="E1966" s="165"/>
+      <c r="C1966" s="167"/>
+      <c r="D1966" s="168"/>
+      <c r="E1966" s="168"/>
     </row>
     <row r="1967" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1967" s="84">
@@ -22644,9 +22647,9 @@
         <v>141</v>
       </c>
       <c r="B1983" s="87"/>
-      <c r="C1983" s="164"/>
-      <c r="D1983" s="165"/>
-      <c r="E1983" s="165"/>
+      <c r="C1983" s="167"/>
+      <c r="D1983" s="168"/>
+      <c r="E1983" s="168"/>
     </row>
     <row r="1984" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1984" s="84">
@@ -22797,9 +22800,9 @@
         <v>142</v>
       </c>
       <c r="B2000" s="87"/>
-      <c r="C2000" s="164"/>
-      <c r="D2000" s="165"/>
-      <c r="E2000" s="165"/>
+      <c r="C2000" s="167"/>
+      <c r="D2000" s="168"/>
+      <c r="E2000" s="168"/>
     </row>
     <row r="2001" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2001" s="84">
@@ -22950,9 +22953,9 @@
         <v>143</v>
       </c>
       <c r="B2017" s="87"/>
-      <c r="C2017" s="164"/>
-      <c r="D2017" s="165"/>
-      <c r="E2017" s="165"/>
+      <c r="C2017" s="167"/>
+      <c r="D2017" s="168"/>
+      <c r="E2017" s="168"/>
     </row>
     <row r="2018" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2018" s="84">
@@ -23103,9 +23106,9 @@
         <v>144</v>
       </c>
       <c r="B2034" s="87"/>
-      <c r="C2034" s="164"/>
-      <c r="D2034" s="165"/>
-      <c r="E2034" s="165"/>
+      <c r="C2034" s="167"/>
+      <c r="D2034" s="168"/>
+      <c r="E2034" s="168"/>
     </row>
     <row r="2035" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2035" s="84">
@@ -23256,9 +23259,9 @@
         <v>145</v>
       </c>
       <c r="B2051" s="87"/>
-      <c r="C2051" s="164"/>
-      <c r="D2051" s="165"/>
-      <c r="E2051" s="165"/>
+      <c r="C2051" s="167"/>
+      <c r="D2051" s="168"/>
+      <c r="E2051" s="168"/>
     </row>
     <row r="2052" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2052" s="84">
@@ -23409,9 +23412,9 @@
         <v>146</v>
       </c>
       <c r="B2068" s="87"/>
-      <c r="C2068" s="164"/>
-      <c r="D2068" s="165"/>
-      <c r="E2068" s="165"/>
+      <c r="C2068" s="167"/>
+      <c r="D2068" s="168"/>
+      <c r="E2068" s="168"/>
     </row>
     <row r="2069" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2069" s="84">
@@ -23562,9 +23565,9 @@
         <v>147</v>
       </c>
       <c r="B2085" s="87"/>
-      <c r="C2085" s="164"/>
-      <c r="D2085" s="165"/>
-      <c r="E2085" s="165"/>
+      <c r="C2085" s="167"/>
+      <c r="D2085" s="168"/>
+      <c r="E2085" s="168"/>
     </row>
     <row r="2086" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2086" s="84">
@@ -23715,9 +23718,9 @@
         <v>148</v>
       </c>
       <c r="B2102" s="87"/>
-      <c r="C2102" s="164"/>
-      <c r="D2102" s="165"/>
-      <c r="E2102" s="165"/>
+      <c r="C2102" s="167"/>
+      <c r="D2102" s="168"/>
+      <c r="E2102" s="168"/>
     </row>
     <row r="2103" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2103" s="84">
@@ -23868,9 +23871,9 @@
         <v>97</v>
       </c>
       <c r="B2119" s="87"/>
-      <c r="C2119" s="164"/>
-      <c r="D2119" s="165"/>
-      <c r="E2119" s="165"/>
+      <c r="C2119" s="167"/>
+      <c r="D2119" s="168"/>
+      <c r="E2119" s="168"/>
     </row>
     <row r="2120" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2120" s="84">
@@ -24021,9 +24024,9 @@
         <v>149</v>
       </c>
       <c r="B2136" s="87"/>
-      <c r="C2136" s="164"/>
-      <c r="D2136" s="165"/>
-      <c r="E2136" s="165"/>
+      <c r="C2136" s="167"/>
+      <c r="D2136" s="168"/>
+      <c r="E2136" s="168"/>
     </row>
     <row r="2137" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2137" s="84">
@@ -24174,9 +24177,9 @@
         <v>150</v>
       </c>
       <c r="B2153" s="87"/>
-      <c r="C2153" s="164"/>
-      <c r="D2153" s="165"/>
-      <c r="E2153" s="165"/>
+      <c r="C2153" s="167"/>
+      <c r="D2153" s="168"/>
+      <c r="E2153" s="168"/>
     </row>
     <row r="2154" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2154" s="84">
@@ -24327,9 +24330,9 @@
         <v>151</v>
       </c>
       <c r="B2170" s="87"/>
-      <c r="C2170" s="164"/>
-      <c r="D2170" s="165"/>
-      <c r="E2170" s="165"/>
+      <c r="C2170" s="167"/>
+      <c r="D2170" s="168"/>
+      <c r="E2170" s="168"/>
     </row>
     <row r="2171" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2171" s="84">
@@ -24477,26 +24480,111 @@
     </row>
   </sheetData>
   <mergeCells count="137">
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="C89:E89"/>
-    <mergeCell ref="C21:E21"/>
-    <mergeCell ref="C38:E38"/>
-    <mergeCell ref="C55:E55"/>
-    <mergeCell ref="C72:E72"/>
-    <mergeCell ref="C208:E208"/>
-    <mergeCell ref="C225:E225"/>
-    <mergeCell ref="C242:E242"/>
-    <mergeCell ref="C259:E259"/>
-    <mergeCell ref="C276:E276"/>
-    <mergeCell ref="C277:E277"/>
-    <mergeCell ref="C106:E106"/>
-    <mergeCell ref="C123:E123"/>
-    <mergeCell ref="C140:E140"/>
-    <mergeCell ref="C157:E157"/>
-    <mergeCell ref="C174:E174"/>
-    <mergeCell ref="C191:E191"/>
+    <mergeCell ref="C2034:E2034"/>
+    <mergeCell ref="C2051:E2051"/>
+    <mergeCell ref="C2068:E2068"/>
+    <mergeCell ref="C2085:E2085"/>
+    <mergeCell ref="C2170:E2170"/>
+    <mergeCell ref="C2102:E2102"/>
+    <mergeCell ref="C2119:E2119"/>
+    <mergeCell ref="C2136:E2136"/>
+    <mergeCell ref="C2153:E2153"/>
+    <mergeCell ref="C1932:E1932"/>
+    <mergeCell ref="C1949:E1949"/>
+    <mergeCell ref="C1966:E1966"/>
+    <mergeCell ref="C1983:E1983"/>
+    <mergeCell ref="C2000:E2000"/>
+    <mergeCell ref="C2017:E2017"/>
+    <mergeCell ref="C1846:E1846"/>
+    <mergeCell ref="C1863:E1863"/>
+    <mergeCell ref="C1880:E1880"/>
+    <mergeCell ref="C1897:E1897"/>
+    <mergeCell ref="C1914:E1914"/>
+    <mergeCell ref="C1915:E1915"/>
+    <mergeCell ref="C1744:E1744"/>
+    <mergeCell ref="C1761:E1761"/>
+    <mergeCell ref="C1778:E1778"/>
+    <mergeCell ref="C1795:E1795"/>
+    <mergeCell ref="C1812:E1812"/>
+    <mergeCell ref="C1829:E1829"/>
+    <mergeCell ref="C1642:E1642"/>
+    <mergeCell ref="C1659:E1659"/>
+    <mergeCell ref="C1676:E1676"/>
+    <mergeCell ref="C1693:E1693"/>
+    <mergeCell ref="C1710:E1710"/>
+    <mergeCell ref="C1727:E1727"/>
+    <mergeCell ref="C1556:E1556"/>
+    <mergeCell ref="C1573:E1573"/>
+    <mergeCell ref="C1590:E1590"/>
+    <mergeCell ref="C1607:E1607"/>
+    <mergeCell ref="C1624:E1624"/>
+    <mergeCell ref="C1641:E1641"/>
+    <mergeCell ref="C1454:E1454"/>
+    <mergeCell ref="C1471:E1471"/>
+    <mergeCell ref="C1488:E1488"/>
+    <mergeCell ref="C1505:E1505"/>
+    <mergeCell ref="C1522:E1522"/>
+    <mergeCell ref="C1539:E1539"/>
+    <mergeCell ref="C1368:E1368"/>
+    <mergeCell ref="C1369:E1369"/>
+    <mergeCell ref="C1386:E1386"/>
+    <mergeCell ref="C1403:E1403"/>
+    <mergeCell ref="C1420:E1420"/>
+    <mergeCell ref="C1437:E1437"/>
+    <mergeCell ref="C1266:E1266"/>
+    <mergeCell ref="C1283:E1283"/>
+    <mergeCell ref="C1300:E1300"/>
+    <mergeCell ref="C1317:E1317"/>
+    <mergeCell ref="C1334:E1334"/>
+    <mergeCell ref="C1351:E1351"/>
+    <mergeCell ref="C1164:E1164"/>
+    <mergeCell ref="C1181:E1181"/>
+    <mergeCell ref="C1198:E1198"/>
+    <mergeCell ref="C1215:E1215"/>
+    <mergeCell ref="C1232:E1232"/>
+    <mergeCell ref="C1249:E1249"/>
+    <mergeCell ref="C1078:E1078"/>
+    <mergeCell ref="C1095:E1095"/>
+    <mergeCell ref="C1096:E1096"/>
+    <mergeCell ref="C1113:E1113"/>
+    <mergeCell ref="C1130:E1130"/>
+    <mergeCell ref="C1147:E1147"/>
+    <mergeCell ref="C976:E976"/>
+    <mergeCell ref="C993:E993"/>
+    <mergeCell ref="C1010:E1010"/>
+    <mergeCell ref="C1027:E1027"/>
+    <mergeCell ref="C1044:E1044"/>
+    <mergeCell ref="C1061:E1061"/>
+    <mergeCell ref="C874:E874"/>
+    <mergeCell ref="C891:E891"/>
+    <mergeCell ref="C908:E908"/>
+    <mergeCell ref="C925:E925"/>
+    <mergeCell ref="C942:E942"/>
+    <mergeCell ref="C959:E959"/>
+    <mergeCell ref="C788:E788"/>
+    <mergeCell ref="C805:E805"/>
+    <mergeCell ref="C822:E822"/>
+    <mergeCell ref="C823:E823"/>
+    <mergeCell ref="C840:E840"/>
+    <mergeCell ref="C857:E857"/>
+    <mergeCell ref="C686:E686"/>
+    <mergeCell ref="C703:E703"/>
+    <mergeCell ref="C720:E720"/>
+    <mergeCell ref="C737:E737"/>
+    <mergeCell ref="C754:E754"/>
+    <mergeCell ref="C771:E771"/>
+    <mergeCell ref="C584:E584"/>
+    <mergeCell ref="C601:E601"/>
+    <mergeCell ref="C618:E618"/>
+    <mergeCell ref="C635:E635"/>
+    <mergeCell ref="C652:E652"/>
+    <mergeCell ref="C669:E669"/>
+    <mergeCell ref="C498:E498"/>
+    <mergeCell ref="C515:E515"/>
+    <mergeCell ref="C532:E532"/>
+    <mergeCell ref="C549:E549"/>
+    <mergeCell ref="C550:E550"/>
+    <mergeCell ref="C567:E567"/>
     <mergeCell ref="C396:E396"/>
     <mergeCell ref="C413:E413"/>
     <mergeCell ref="C430:E430"/>
@@ -24509,111 +24597,26 @@
     <mergeCell ref="C345:E345"/>
     <mergeCell ref="C362:E362"/>
     <mergeCell ref="C379:E379"/>
-    <mergeCell ref="C584:E584"/>
-    <mergeCell ref="C601:E601"/>
-    <mergeCell ref="C618:E618"/>
-    <mergeCell ref="C635:E635"/>
-    <mergeCell ref="C652:E652"/>
-    <mergeCell ref="C669:E669"/>
-    <mergeCell ref="C498:E498"/>
-    <mergeCell ref="C515:E515"/>
-    <mergeCell ref="C532:E532"/>
-    <mergeCell ref="C549:E549"/>
-    <mergeCell ref="C550:E550"/>
-    <mergeCell ref="C567:E567"/>
-    <mergeCell ref="C788:E788"/>
-    <mergeCell ref="C805:E805"/>
-    <mergeCell ref="C822:E822"/>
-    <mergeCell ref="C823:E823"/>
-    <mergeCell ref="C840:E840"/>
-    <mergeCell ref="C857:E857"/>
-    <mergeCell ref="C686:E686"/>
-    <mergeCell ref="C703:E703"/>
-    <mergeCell ref="C720:E720"/>
-    <mergeCell ref="C737:E737"/>
-    <mergeCell ref="C754:E754"/>
-    <mergeCell ref="C771:E771"/>
-    <mergeCell ref="C976:E976"/>
-    <mergeCell ref="C993:E993"/>
-    <mergeCell ref="C1010:E1010"/>
-    <mergeCell ref="C1027:E1027"/>
-    <mergeCell ref="C1044:E1044"/>
-    <mergeCell ref="C1061:E1061"/>
-    <mergeCell ref="C874:E874"/>
-    <mergeCell ref="C891:E891"/>
-    <mergeCell ref="C908:E908"/>
-    <mergeCell ref="C925:E925"/>
-    <mergeCell ref="C942:E942"/>
-    <mergeCell ref="C959:E959"/>
-    <mergeCell ref="C1164:E1164"/>
-    <mergeCell ref="C1181:E1181"/>
-    <mergeCell ref="C1198:E1198"/>
-    <mergeCell ref="C1215:E1215"/>
-    <mergeCell ref="C1232:E1232"/>
-    <mergeCell ref="C1249:E1249"/>
-    <mergeCell ref="C1078:E1078"/>
-    <mergeCell ref="C1095:E1095"/>
-    <mergeCell ref="C1096:E1096"/>
-    <mergeCell ref="C1113:E1113"/>
-    <mergeCell ref="C1130:E1130"/>
-    <mergeCell ref="C1147:E1147"/>
-    <mergeCell ref="C1368:E1368"/>
-    <mergeCell ref="C1369:E1369"/>
-    <mergeCell ref="C1386:E1386"/>
-    <mergeCell ref="C1403:E1403"/>
-    <mergeCell ref="C1420:E1420"/>
-    <mergeCell ref="C1437:E1437"/>
-    <mergeCell ref="C1266:E1266"/>
-    <mergeCell ref="C1283:E1283"/>
-    <mergeCell ref="C1300:E1300"/>
-    <mergeCell ref="C1317:E1317"/>
-    <mergeCell ref="C1334:E1334"/>
-    <mergeCell ref="C1351:E1351"/>
-    <mergeCell ref="C1556:E1556"/>
-    <mergeCell ref="C1573:E1573"/>
-    <mergeCell ref="C1590:E1590"/>
-    <mergeCell ref="C1607:E1607"/>
-    <mergeCell ref="C1624:E1624"/>
-    <mergeCell ref="C1641:E1641"/>
-    <mergeCell ref="C1454:E1454"/>
-    <mergeCell ref="C1471:E1471"/>
-    <mergeCell ref="C1488:E1488"/>
-    <mergeCell ref="C1505:E1505"/>
-    <mergeCell ref="C1522:E1522"/>
-    <mergeCell ref="C1539:E1539"/>
-    <mergeCell ref="C1744:E1744"/>
-    <mergeCell ref="C1761:E1761"/>
-    <mergeCell ref="C1778:E1778"/>
-    <mergeCell ref="C1795:E1795"/>
-    <mergeCell ref="C1812:E1812"/>
-    <mergeCell ref="C1829:E1829"/>
-    <mergeCell ref="C1642:E1642"/>
-    <mergeCell ref="C1659:E1659"/>
-    <mergeCell ref="C1676:E1676"/>
-    <mergeCell ref="C1693:E1693"/>
-    <mergeCell ref="C1710:E1710"/>
-    <mergeCell ref="C1727:E1727"/>
-    <mergeCell ref="C1932:E1932"/>
-    <mergeCell ref="C1949:E1949"/>
-    <mergeCell ref="C1966:E1966"/>
-    <mergeCell ref="C1983:E1983"/>
-    <mergeCell ref="C2000:E2000"/>
-    <mergeCell ref="C2017:E2017"/>
-    <mergeCell ref="C1846:E1846"/>
-    <mergeCell ref="C1863:E1863"/>
-    <mergeCell ref="C1880:E1880"/>
-    <mergeCell ref="C1897:E1897"/>
-    <mergeCell ref="C1914:E1914"/>
-    <mergeCell ref="C1915:E1915"/>
-    <mergeCell ref="C2034:E2034"/>
-    <mergeCell ref="C2051:E2051"/>
-    <mergeCell ref="C2068:E2068"/>
-    <mergeCell ref="C2085:E2085"/>
-    <mergeCell ref="C2170:E2170"/>
-    <mergeCell ref="C2102:E2102"/>
-    <mergeCell ref="C2119:E2119"/>
-    <mergeCell ref="C2136:E2136"/>
-    <mergeCell ref="C2153:E2153"/>
+    <mergeCell ref="C225:E225"/>
+    <mergeCell ref="C242:E242"/>
+    <mergeCell ref="C259:E259"/>
+    <mergeCell ref="C276:E276"/>
+    <mergeCell ref="C277:E277"/>
+    <mergeCell ref="C106:E106"/>
+    <mergeCell ref="C123:E123"/>
+    <mergeCell ref="C140:E140"/>
+    <mergeCell ref="C157:E157"/>
+    <mergeCell ref="C174:E174"/>
+    <mergeCell ref="C191:E191"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="C89:E89"/>
+    <mergeCell ref="C21:E21"/>
+    <mergeCell ref="C38:E38"/>
+    <mergeCell ref="C55:E55"/>
+    <mergeCell ref="C72:E72"/>
+    <mergeCell ref="C208:E208"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -25872,163 +25875,150 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="33">
-      <c r="A1" s="209" t="s">
+      <c r="A1" s="210" t="s">
         <v>184</v>
       </c>
-      <c r="B1" s="210"/>
+      <c r="B1" s="211"/>
       <c r="C1" s="118"/>
       <c r="D1" s="5"/>
       <c r="E1" s="5"/>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="206" t="s">
+      <c r="A2" s="216" t="s">
         <v>183</v>
       </c>
-      <c r="B2" s="207"/>
+      <c r="B2" s="217"/>
       <c r="C2" s="120"/>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="208" t="s">
+      <c r="A3" s="218" t="s">
         <v>185</v>
       </c>
-      <c r="B3" s="207"/>
+      <c r="B3" s="217"/>
       <c r="C3" s="120"/>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="213"/>
-      <c r="B4" s="214"/>
+      <c r="A4" s="214"/>
+      <c r="B4" s="215"/>
       <c r="C4" s="120"/>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="211" t="s">
+      <c r="A5" s="212" t="s">
         <v>194</v>
       </c>
-      <c r="B5" s="212"/>
+      <c r="B5" s="213"/>
       <c r="C5" s="120"/>
     </row>
     <row r="7" spans="1:5" ht="18.75">
-      <c r="A7" s="217" t="s">
+      <c r="A7" s="204" t="s">
         <v>186</v>
       </c>
-      <c r="B7" s="218"/>
+      <c r="B7" s="205"/>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="120"/>
       <c r="B8" s="9"/>
     </row>
     <row r="9" spans="1:5" ht="39" customHeight="1">
-      <c r="A9" s="215" t="s">
+      <c r="A9" s="206" t="s">
         <v>187</v>
       </c>
-      <c r="B9" s="216"/>
+      <c r="B9" s="207"/>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="202"/>
-      <c r="B10" s="203"/>
+      <c r="A10" s="208"/>
+      <c r="B10" s="209"/>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="204" t="s">
+      <c r="A11" s="200" t="s">
         <v>188</v>
       </c>
-      <c r="B11" s="205"/>
+      <c r="B11" s="201"/>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="204" t="s">
+      <c r="A12" s="200" t="s">
         <v>189</v>
       </c>
-      <c r="B12" s="205"/>
+      <c r="B12" s="201"/>
     </row>
     <row r="13" spans="1:5" ht="43.5" customHeight="1">
-      <c r="A13" s="204" t="s">
+      <c r="A13" s="200" t="s">
         <v>190</v>
       </c>
-      <c r="B13" s="205"/>
+      <c r="B13" s="201"/>
     </row>
     <row r="14" spans="1:5" ht="19.5" customHeight="1">
-      <c r="A14" s="204" t="s">
+      <c r="A14" s="200" t="s">
         <v>191</v>
       </c>
-      <c r="B14" s="205"/>
+      <c r="B14" s="201"/>
     </row>
     <row r="15" spans="1:5" ht="18" customHeight="1">
-      <c r="A15" s="204" t="s">
+      <c r="A15" s="200" t="s">
         <v>192</v>
       </c>
-      <c r="B15" s="205"/>
+      <c r="B15" s="201"/>
     </row>
     <row r="16" spans="1:5" ht="21" customHeight="1">
-      <c r="A16" s="204" t="s">
+      <c r="A16" s="200" t="s">
         <v>193</v>
       </c>
-      <c r="B16" s="205"/>
+      <c r="B16" s="201"/>
     </row>
     <row r="17" spans="1:2" ht="48.75" customHeight="1">
-      <c r="A17" s="200" t="s">
+      <c r="A17" s="202" t="s">
         <v>195</v>
       </c>
-      <c r="B17" s="201"/>
+      <c r="B17" s="203"/>
     </row>
     <row r="19" spans="1:2" ht="18.75">
-      <c r="A19" s="217" t="s">
+      <c r="A19" s="204" t="s">
         <v>197</v>
       </c>
-      <c r="B19" s="218"/>
+      <c r="B19" s="205"/>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="120"/>
       <c r="B20" s="9"/>
     </row>
     <row r="21" spans="1:2">
-      <c r="A21" s="215" t="s">
+      <c r="A21" s="206" t="s">
         <v>198</v>
       </c>
-      <c r="B21" s="216"/>
+      <c r="B21" s="207"/>
     </row>
     <row r="22" spans="1:2">
-      <c r="A22" s="202"/>
-      <c r="B22" s="203"/>
+      <c r="A22" s="208"/>
+      <c r="B22" s="209"/>
     </row>
     <row r="23" spans="1:2">
-      <c r="A23" s="204" t="s">
+      <c r="A23" s="200" t="s">
         <v>199</v>
       </c>
-      <c r="B23" s="205"/>
+      <c r="B23" s="201"/>
     </row>
     <row r="24" spans="1:2">
-      <c r="A24" s="204"/>
-      <c r="B24" s="205"/>
+      <c r="A24" s="200"/>
+      <c r="B24" s="201"/>
     </row>
     <row r="25" spans="1:2">
-      <c r="A25" s="204" t="s">
+      <c r="A25" s="200" t="s">
         <v>200</v>
       </c>
-      <c r="B25" s="205"/>
+      <c r="B25" s="201"/>
     </row>
     <row r="26" spans="1:2">
-      <c r="A26" s="204" t="s">
+      <c r="A26" s="200" t="s">
         <v>201</v>
       </c>
-      <c r="B26" s="205"/>
+      <c r="B26" s="201"/>
     </row>
     <row r="27" spans="1:2">
-      <c r="A27" s="200"/>
-      <c r="B27" s="201"/>
+      <c r="A27" s="202"/>
+      <c r="B27" s="203"/>
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A7:B7"/>
     <mergeCell ref="A17:B17"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
@@ -26039,6 +26029,19 @@
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="A14:B14"/>
     <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A24:B24"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A3" r:id="rId1"/>

</xml_diff>

<commit_message>
Tempo - some of Hi Fi stage done.
</commit_message>
<xml_diff>
--- a/trunk/Tempo/Tempo.xlsx
+++ b/trunk/Tempo/Tempo.xlsx
@@ -2146,6 +2146,9 @@
       <alignment horizontal="left" indent="1"/>
     </xf>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="34" fillId="21" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -2168,29 +2171,29 @@
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -2226,20 +2229,34 @@
     <xf numFmtId="0" fontId="48" fillId="22" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="46" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="46" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="42" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="4"/>
     </xf>
@@ -2248,23 +2265,6 @@
     </xf>
     <xf numFmtId="0" fontId="43" fillId="0" borderId="33" xfId="3" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" indent="4"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="46" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="46" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -2576,8 +2576,8 @@
   <dimension ref="A1:K156"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C37" sqref="C37"/>
+      <pane ySplit="6" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" outlineLevelRow="2"/>
@@ -2593,16 +2593,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="33">
-      <c r="A1" s="159" t="s">
+      <c r="A1" s="160" t="s">
         <v>205</v>
       </c>
-      <c r="B1" s="158"/>
-      <c r="C1" s="160" t="s">
+      <c r="B1" s="159"/>
+      <c r="C1" s="161" t="s">
         <v>170</v>
       </c>
-      <c r="D1" s="160"/>
-      <c r="E1" s="160"/>
-      <c r="F1" s="161"/>
+      <c r="D1" s="161"/>
+      <c r="E1" s="161"/>
+      <c r="F1" s="162"/>
       <c r="G1" s="140"/>
       <c r="H1" s="141">
         <f>SUM(G1:G65538)</f>
@@ -2667,11 +2667,11 @@
       <c r="B4" s="146" t="s">
         <v>228</v>
       </c>
-      <c r="C4" s="157" t="s">
+      <c r="C4" s="158" t="s">
         <v>232</v>
       </c>
-      <c r="D4" s="157"/>
-      <c r="E4" s="163"/>
+      <c r="D4" s="158"/>
+      <c r="E4" s="164"/>
       <c r="F4" s="143"/>
       <c r="G4" s="140"/>
       <c r="H4" s="140"/>
@@ -2686,10 +2686,10 @@
       <c r="B5" s="147" t="s">
         <v>177</v>
       </c>
-      <c r="C5" s="157" t="s">
+      <c r="C5" s="158" t="s">
         <v>218</v>
       </c>
-      <c r="D5" s="157"/>
+      <c r="D5" s="158"/>
       <c r="E5" s="147"/>
       <c r="F5" s="147"/>
       <c r="G5" s="148" t="s">
@@ -2713,10 +2713,10 @@
       <c r="B6" s="147" t="s">
         <v>179</v>
       </c>
-      <c r="C6" s="157" t="s">
+      <c r="C6" s="158" t="s">
         <v>168</v>
       </c>
-      <c r="D6" s="158"/>
+      <c r="D6" s="159"/>
       <c r="E6" s="147"/>
       <c r="F6" s="143"/>
       <c r="G6" s="140"/>
@@ -2740,7 +2740,7 @@
       <c r="F7" s="93"/>
     </row>
     <row r="8" spans="1:11" ht="15" customHeight="1" outlineLevel="1">
-      <c r="A8" s="162" t="s">
+      <c r="A8" s="163" t="s">
         <v>180</v>
       </c>
       <c r="B8" s="95" t="s">
@@ -2760,7 +2760,7 @@
       </c>
     </row>
     <row r="9" spans="1:11" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="A9" s="155"/>
+      <c r="A9" s="156"/>
       <c r="B9" s="98" t="s">
         <v>177</v>
       </c>
@@ -2774,7 +2774,7 @@
       <c r="F9" s="104"/>
     </row>
     <row r="10" spans="1:11" ht="15.75" outlineLevel="1" thickTop="1">
-      <c r="A10" s="155"/>
+      <c r="A10" s="156"/>
       <c r="B10" s="149" t="s">
         <v>208</v>
       </c>
@@ -2791,7 +2791,7 @@
       <c r="F10" s="105"/>
     </row>
     <row r="11" spans="1:11" ht="15" outlineLevel="1">
-      <c r="A11" s="155"/>
+      <c r="A11" s="156"/>
       <c r="B11" s="149" t="s">
         <v>214</v>
       </c>
@@ -2808,7 +2808,7 @@
       <c r="F11" s="105"/>
     </row>
     <row r="12" spans="1:11" ht="15" outlineLevel="1">
-      <c r="A12" s="155"/>
+      <c r="A12" s="156"/>
       <c r="B12" s="149" t="s">
         <v>209</v>
       </c>
@@ -2825,7 +2825,7 @@
       <c r="F12" s="105"/>
     </row>
     <row r="13" spans="1:11" ht="15" outlineLevel="1">
-      <c r="A13" s="155"/>
+      <c r="A13" s="156"/>
       <c r="B13" s="149" t="s">
         <v>213</v>
       </c>
@@ -2842,7 +2842,7 @@
       <c r="F13" s="105"/>
     </row>
     <row r="14" spans="1:11" ht="15" outlineLevel="1">
-      <c r="A14" s="155"/>
+      <c r="A14" s="156"/>
       <c r="B14" s="149" t="s">
         <v>214</v>
       </c>
@@ -2859,7 +2859,7 @@
       <c r="F14" s="105"/>
     </row>
     <row r="15" spans="1:11" ht="15" outlineLevel="1">
-      <c r="A15" s="155"/>
+      <c r="A15" s="156"/>
       <c r="B15" s="149" t="s">
         <v>215</v>
       </c>
@@ -2876,7 +2876,7 @@
       <c r="F15" s="105"/>
     </row>
     <row r="16" spans="1:11" ht="15" outlineLevel="1">
-      <c r="A16" s="155"/>
+      <c r="A16" s="156"/>
       <c r="B16" s="149" t="s">
         <v>216</v>
       </c>
@@ -2893,7 +2893,7 @@
       <c r="F16" s="105"/>
     </row>
     <row r="17" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A17" s="155"/>
+      <c r="A17" s="156"/>
       <c r="B17" s="149" t="s">
         <v>217</v>
       </c>
@@ -2910,7 +2910,7 @@
       <c r="F17" s="105"/>
     </row>
     <row r="18" spans="1:8" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="A18" s="155"/>
+      <c r="A18" s="156"/>
       <c r="B18" s="98" t="s">
         <v>179</v>
       </c>
@@ -2953,7 +2953,7 @@
     </row>
     <row r="20" spans="1:8" ht="13.5" thickBot="1"/>
     <row r="21" spans="1:8" ht="15" customHeight="1" outlineLevel="1">
-      <c r="A21" s="156" t="s">
+      <c r="A21" s="157" t="s">
         <v>219</v>
       </c>
       <c r="B21" s="109" t="s">
@@ -2973,7 +2973,7 @@
       </c>
     </row>
     <row r="22" spans="1:8" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="A22" s="155"/>
+      <c r="A22" s="156"/>
       <c r="B22" s="98" t="s">
         <v>177</v>
       </c>
@@ -2990,7 +2990,7 @@
       <c r="F22" s="104"/>
     </row>
     <row r="23" spans="1:8" ht="15.75" outlineLevel="1" thickTop="1">
-      <c r="A23" s="155"/>
+      <c r="A23" s="156"/>
       <c r="B23" s="149" t="s">
         <v>175</v>
       </c>
@@ -3003,7 +3003,7 @@
       <c r="F23" s="105"/>
     </row>
     <row r="24" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A24" s="155"/>
+      <c r="A24" s="156"/>
       <c r="B24" s="149" t="s">
         <v>221</v>
       </c>
@@ -3023,7 +3023,7 @@
       </c>
     </row>
     <row r="25" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A25" s="155"/>
+      <c r="A25" s="156"/>
       <c r="B25" s="149"/>
       <c r="C25" s="101"/>
       <c r="D25" s="101"/>
@@ -3034,7 +3034,7 @@
       <c r="F25" s="105"/>
     </row>
     <row r="26" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A26" s="155"/>
+      <c r="A26" s="156"/>
       <c r="B26" s="100"/>
       <c r="C26" s="101"/>
       <c r="D26" s="101"/>
@@ -3045,7 +3045,7 @@
       <c r="F26" s="105"/>
     </row>
     <row r="27" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A27" s="155"/>
+      <c r="A27" s="156"/>
       <c r="B27" s="100"/>
       <c r="C27" s="101"/>
       <c r="D27" s="101"/>
@@ -3056,7 +3056,7 @@
       <c r="F27" s="105"/>
     </row>
     <row r="28" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A28" s="155"/>
+      <c r="A28" s="156"/>
       <c r="B28" s="149" t="s">
         <v>222</v>
       </c>
@@ -3076,8 +3076,8 @@
       </c>
     </row>
     <row r="29" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A29" s="155"/>
-      <c r="B29" s="219" t="s">
+      <c r="A29" s="156"/>
+      <c r="B29" s="154" t="s">
         <v>264</v>
       </c>
       <c r="C29" s="101">
@@ -3094,8 +3094,8 @@
       </c>
     </row>
     <row r="30" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A30" s="155"/>
-      <c r="B30" s="219" t="s">
+      <c r="A30" s="156"/>
+      <c r="B30" s="154" t="s">
         <v>265</v>
       </c>
       <c r="C30" s="101">
@@ -3105,13 +3105,13 @@
       <c r="E30" s="123"/>
       <c r="F30" s="105"/>
       <c r="H30" s="112">
-        <f>C30-C29</f>
+        <f t="shared" ref="H30:H35" si="2">C30-C29</f>
         <v>135</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A31" s="155"/>
-      <c r="B31" s="219" t="s">
+      <c r="A31" s="156"/>
+      <c r="B31" s="154" t="s">
         <v>266</v>
       </c>
       <c r="C31" s="101">
@@ -3121,13 +3121,13 @@
       <c r="E31" s="123"/>
       <c r="F31" s="105"/>
       <c r="H31" s="112">
-        <f>C31-C30</f>
+        <f t="shared" si="2"/>
         <v>135</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A32" s="155"/>
-      <c r="B32" s="219" t="s">
+      <c r="A32" s="156"/>
+      <c r="B32" s="154" t="s">
         <v>267</v>
       </c>
       <c r="C32" s="101">
@@ -3137,13 +3137,13 @@
       <c r="E32" s="123"/>
       <c r="F32" s="105"/>
       <c r="H32" s="112">
-        <f>C32-C31</f>
+        <f t="shared" si="2"/>
         <v>135</v>
       </c>
     </row>
     <row r="33" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A33" s="155"/>
-      <c r="B33" s="219" t="s">
+      <c r="A33" s="156"/>
+      <c r="B33" s="154" t="s">
         <v>269</v>
       </c>
       <c r="C33" s="101">
@@ -3153,13 +3153,13 @@
       <c r="E33" s="123"/>
       <c r="F33" s="105"/>
       <c r="H33" s="112">
-        <f>C33-C32</f>
+        <f t="shared" si="2"/>
         <v>135</v>
       </c>
     </row>
     <row r="34" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A34" s="155"/>
-      <c r="B34" s="219" t="s">
+      <c r="A34" s="156"/>
+      <c r="B34" s="154" t="s">
         <v>270</v>
       </c>
       <c r="C34" s="101">
@@ -3169,13 +3169,13 @@
       <c r="E34" s="123"/>
       <c r="F34" s="105"/>
       <c r="H34" s="112">
-        <f>C34-C33</f>
+        <f t="shared" si="2"/>
         <v>287</v>
       </c>
     </row>
     <row r="35" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A35" s="155"/>
-      <c r="B35" s="219" t="s">
+      <c r="A35" s="156"/>
+      <c r="B35" s="154" t="s">
         <v>271</v>
       </c>
       <c r="C35" s="101">
@@ -3185,7 +3185,7 @@
       <c r="E35" s="123"/>
       <c r="F35" s="105"/>
       <c r="H35" s="112">
-        <f>C35-C34</f>
+        <f t="shared" si="2"/>
         <v>284</v>
       </c>
       <c r="I35" t="s">
@@ -3193,7 +3193,7 @@
       </c>
     </row>
     <row r="36" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A36" s="155"/>
+      <c r="A36" s="156"/>
       <c r="B36" s="149" t="s">
         <v>223</v>
       </c>
@@ -3213,52 +3213,58 @@
       </c>
     </row>
     <row r="37" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A37" s="155"/>
+      <c r="A37" s="156"/>
       <c r="B37" s="149" t="s">
         <v>224</v>
       </c>
-      <c r="C37" s="101"/>
+      <c r="C37" s="101">
+        <v>9164</v>
+      </c>
       <c r="D37" s="101">
         <v>10169</v>
       </c>
       <c r="E37" s="123">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1005</v>
       </c>
       <c r="F37" s="105"/>
     </row>
     <row r="38" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A38" s="155"/>
+      <c r="A38" s="156"/>
       <c r="B38" s="149" t="s">
         <v>225</v>
       </c>
-      <c r="C38" s="101"/>
+      <c r="C38" s="101">
+        <v>9785</v>
+      </c>
       <c r="D38" s="101">
         <v>10783</v>
       </c>
       <c r="E38" s="123">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>998</v>
       </c>
       <c r="F38" s="105"/>
     </row>
     <row r="39" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A39" s="155"/>
+      <c r="A39" s="156"/>
       <c r="B39" s="149" t="s">
         <v>217</v>
       </c>
-      <c r="C39" s="101"/>
+      <c r="C39" s="101">
+        <v>10197</v>
+      </c>
       <c r="D39" s="101">
         <v>11195</v>
       </c>
       <c r="E39" s="123">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>998</v>
       </c>
       <c r="F39" s="105"/>
     </row>
     <row r="40" spans="1:9" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="A40" s="155"/>
+      <c r="A40" s="156"/>
       <c r="B40" s="98" t="s">
         <v>179</v>
       </c>
@@ -3297,7 +3303,7 @@
     </row>
     <row r="42" spans="1:9" ht="13.5" thickBot="1"/>
     <row r="43" spans="1:9" ht="15" customHeight="1" outlineLevel="1">
-      <c r="A43" s="154" t="s">
+      <c r="A43" s="155" t="s">
         <v>226</v>
       </c>
       <c r="B43" s="113" t="s">
@@ -3317,7 +3323,7 @@
       </c>
     </row>
     <row r="44" spans="1:9" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="A44" s="155"/>
+      <c r="A44" s="156"/>
       <c r="B44" s="98" t="s">
         <v>177</v>
       </c>
@@ -3326,7 +3332,7 @@
         <v>11282</v>
       </c>
       <c r="E44" s="123">
-        <f t="shared" ref="E44:E63" si="2">IF(AND(C44&gt;0,D44&gt;0), D44-C44, 0)</f>
+        <f t="shared" ref="E44:E63" si="3">IF(AND(C44&gt;0,D44&gt;0), D44-C44, 0)</f>
         <v>0</v>
       </c>
       <c r="F44" s="104"/>
@@ -3335,18 +3341,18 @@
       </c>
     </row>
     <row r="45" spans="1:9" ht="15.75" outlineLevel="1" thickTop="1">
-      <c r="A45" s="155"/>
+      <c r="A45" s="156"/>
       <c r="B45" s="100"/>
       <c r="C45" s="101"/>
       <c r="D45" s="101"/>
       <c r="E45" s="124">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="F45" s="105"/>
     </row>
     <row r="46" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A46" s="155"/>
+      <c r="A46" s="156"/>
       <c r="B46" s="149" t="s">
         <v>221</v>
       </c>
@@ -3355,13 +3361,13 @@
         <v>13979</v>
       </c>
       <c r="E46" s="123">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="F46" s="105"/>
     </row>
     <row r="47" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A47" s="155"/>
+      <c r="A47" s="156"/>
       <c r="B47" s="150" t="s">
         <v>228</v>
       </c>
@@ -3370,13 +3376,13 @@
         <v>15531</v>
       </c>
       <c r="E47" s="123">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="F47" s="105"/>
     </row>
     <row r="48" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A48" s="155"/>
+      <c r="A48" s="156"/>
       <c r="B48" s="149" t="s">
         <v>222</v>
       </c>
@@ -3385,13 +3391,13 @@
         <v>17009</v>
       </c>
       <c r="E48" s="123">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="F48" s="105"/>
     </row>
     <row r="49" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A49" s="155"/>
+      <c r="A49" s="156"/>
       <c r="B49" s="150" t="s">
         <v>229</v>
       </c>
@@ -3400,13 +3406,13 @@
         <v>17390</v>
       </c>
       <c r="E49" s="123">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="F49" s="105"/>
     </row>
     <row r="50" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A50" s="155"/>
+      <c r="A50" s="156"/>
       <c r="B50" s="150" t="s">
         <v>230</v>
       </c>
@@ -3415,13 +3421,13 @@
         <v>17856</v>
       </c>
       <c r="E50" s="123">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="F50" s="105"/>
     </row>
     <row r="51" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A51" s="155"/>
+      <c r="A51" s="156"/>
       <c r="B51" s="150" t="s">
         <v>231</v>
       </c>
@@ -3430,13 +3436,13 @@
         <v>18332</v>
       </c>
       <c r="E51" s="123">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="F51" s="105"/>
     </row>
     <row r="52" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A52" s="155"/>
+      <c r="A52" s="156"/>
       <c r="B52" s="150" t="s">
         <v>233</v>
       </c>
@@ -3445,13 +3451,13 @@
         <v>18738</v>
       </c>
       <c r="E52" s="123">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="F52" s="105"/>
     </row>
     <row r="53" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A53" s="155"/>
+      <c r="A53" s="156"/>
       <c r="B53" s="150" t="s">
         <v>234</v>
       </c>
@@ -3460,13 +3466,13 @@
         <v>19757</v>
       </c>
       <c r="E53" s="123">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="F53" s="105"/>
     </row>
     <row r="54" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A54" s="155"/>
+      <c r="A54" s="156"/>
       <c r="B54" s="150" t="s">
         <v>235</v>
       </c>
@@ -3475,13 +3481,13 @@
         <v>20174</v>
       </c>
       <c r="E54" s="123">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="F54" s="105"/>
     </row>
     <row r="55" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A55" s="155"/>
+      <c r="A55" s="156"/>
       <c r="B55" s="150" t="s">
         <v>236</v>
       </c>
@@ -3490,48 +3496,48 @@
         <v>20965</v>
       </c>
       <c r="E55" s="123">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="F55" s="105"/>
     </row>
     <row r="56" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A56" s="155"/>
+      <c r="A56" s="156"/>
       <c r="B56" s="100"/>
       <c r="C56" s="101"/>
       <c r="D56" s="101"/>
       <c r="E56" s="123">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="F56" s="105"/>
     </row>
     <row r="57" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A57" s="155"/>
+      <c r="A57" s="156"/>
       <c r="B57" s="100"/>
       <c r="C57" s="101"/>
       <c r="D57" s="101"/>
       <c r="E57" s="123">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="F57" s="105"/>
     </row>
     <row r="58" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A58" s="155"/>
+      <c r="A58" s="156"/>
       <c r="B58" s="150" t="s">
         <v>237</v>
       </c>
       <c r="C58" s="101"/>
       <c r="D58" s="101"/>
       <c r="E58" s="123">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="F58" s="105"/>
     </row>
     <row r="59" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A59" s="155"/>
+      <c r="A59" s="156"/>
       <c r="B59" s="150" t="s">
         <v>223</v>
       </c>
@@ -3540,13 +3546,13 @@
         <v>23906</v>
       </c>
       <c r="E59" s="123">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="F59" s="105"/>
     </row>
     <row r="60" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A60" s="155"/>
+      <c r="A60" s="156"/>
       <c r="B60" s="150" t="s">
         <v>238</v>
       </c>
@@ -3555,13 +3561,13 @@
         <v>24132</v>
       </c>
       <c r="E60" s="123">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="F60" s="105"/>
     </row>
     <row r="61" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A61" s="155"/>
+      <c r="A61" s="156"/>
       <c r="B61" s="150" t="s">
         <v>239</v>
       </c>
@@ -3573,7 +3579,7 @@
       <c r="F61" s="105"/>
     </row>
     <row r="62" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A62" s="155"/>
+      <c r="A62" s="156"/>
       <c r="B62" s="150" t="s">
         <v>217</v>
       </c>
@@ -3582,13 +3588,13 @@
         <v>25129</v>
       </c>
       <c r="E62" s="123">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="F62" s="105"/>
     </row>
     <row r="63" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="A63" s="155"/>
+      <c r="A63" s="156"/>
       <c r="B63" s="98" t="s">
         <v>179</v>
       </c>
@@ -3597,7 +3603,7 @@
         <v>25174</v>
       </c>
       <c r="E63" s="125">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="F63" s="104"/>
@@ -3629,7 +3635,7 @@
     </row>
     <row r="65" spans="1:8" ht="13.5" thickBot="1"/>
     <row r="66" spans="1:8" ht="15" customHeight="1" outlineLevel="1">
-      <c r="A66" s="156" t="s">
+      <c r="A66" s="157" t="s">
         <v>240</v>
       </c>
       <c r="B66" s="109" t="s">
@@ -3649,7 +3655,7 @@
       </c>
     </row>
     <row r="67" spans="1:8" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="A67" s="155"/>
+      <c r="A67" s="156"/>
       <c r="B67" s="98" t="s">
         <v>177</v>
       </c>
@@ -3658,7 +3664,7 @@
         <v>25174</v>
       </c>
       <c r="E67" s="123">
-        <f t="shared" ref="E67:E79" si="3">IF(AND(C67&gt;0,D67&gt;0), D67-C67, 0)</f>
+        <f t="shared" ref="E67:E79" si="4">IF(AND(C67&gt;0,D67&gt;0), D67-C67, 0)</f>
         <v>0</v>
       </c>
       <c r="F67" s="104"/>
@@ -3667,18 +3673,18 @@
       </c>
     </row>
     <row r="68" spans="1:8" ht="15.75" outlineLevel="1" thickTop="1">
-      <c r="A68" s="155"/>
+      <c r="A68" s="156"/>
       <c r="B68" s="100"/>
       <c r="C68" s="101"/>
       <c r="D68" s="101"/>
       <c r="E68" s="124">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="F68" s="105"/>
     </row>
     <row r="69" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A69" s="155"/>
+      <c r="A69" s="156"/>
       <c r="B69" s="151" t="s">
         <v>242</v>
       </c>
@@ -3687,24 +3693,24 @@
         <v>26754</v>
       </c>
       <c r="E69" s="123">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="F69" s="105"/>
     </row>
     <row r="70" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A70" s="155"/>
+      <c r="A70" s="156"/>
       <c r="B70" s="100"/>
       <c r="C70" s="101"/>
       <c r="D70" s="101"/>
       <c r="E70" s="123">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="F70" s="105"/>
     </row>
     <row r="71" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A71" s="155"/>
+      <c r="A71" s="156"/>
       <c r="B71" s="151" t="s">
         <v>243</v>
       </c>
@@ -3713,24 +3719,24 @@
         <v>27765</v>
       </c>
       <c r="E71" s="123">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="F71" s="105"/>
     </row>
     <row r="72" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A72" s="155"/>
+      <c r="A72" s="156"/>
       <c r="B72" s="100"/>
       <c r="C72" s="101"/>
       <c r="D72" s="101"/>
       <c r="E72" s="123">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="F72" s="105"/>
     </row>
     <row r="73" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A73" s="155"/>
+      <c r="A73" s="156"/>
       <c r="B73" s="151" t="s">
         <v>244</v>
       </c>
@@ -3739,24 +3745,24 @@
         <v>30127</v>
       </c>
       <c r="E73" s="123">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="F73" s="105"/>
     </row>
     <row r="74" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A74" s="155"/>
+      <c r="A74" s="156"/>
       <c r="B74" s="100"/>
       <c r="C74" s="101"/>
       <c r="D74" s="101"/>
       <c r="E74" s="123">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="F74" s="105"/>
     </row>
     <row r="75" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A75" s="155"/>
+      <c r="A75" s="156"/>
       <c r="B75" s="151" t="s">
         <v>245</v>
       </c>
@@ -3765,13 +3771,13 @@
         <v>33299</v>
       </c>
       <c r="E75" s="123">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="F75" s="105"/>
     </row>
     <row r="76" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A76" s="155"/>
+      <c r="A76" s="156"/>
       <c r="B76" s="151" t="s">
         <v>238</v>
       </c>
@@ -3780,13 +3786,13 @@
         <v>33527</v>
       </c>
       <c r="E76" s="123">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="F76" s="105"/>
     </row>
     <row r="77" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A77" s="155"/>
+      <c r="A77" s="156"/>
       <c r="B77" s="151" t="s">
         <v>246</v>
       </c>
@@ -3795,13 +3801,13 @@
         <v>34309</v>
       </c>
       <c r="E77" s="123">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="F77" s="105"/>
     </row>
     <row r="78" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A78" s="155"/>
+      <c r="A78" s="156"/>
       <c r="B78" s="151" t="s">
         <v>217</v>
       </c>
@@ -3810,13 +3816,13 @@
         <v>34727</v>
       </c>
       <c r="E78" s="123">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="F78" s="105"/>
     </row>
     <row r="79" spans="1:8" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="A79" s="155"/>
+      <c r="A79" s="156"/>
       <c r="B79" s="98" t="s">
         <v>179</v>
       </c>
@@ -3825,7 +3831,7 @@
         <v>34795</v>
       </c>
       <c r="E79" s="125">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="F79" s="104"/>
@@ -3857,7 +3863,7 @@
     </row>
     <row r="81" spans="1:8" ht="13.5" thickBot="1"/>
     <row r="82" spans="1:8" ht="15" customHeight="1" outlineLevel="1">
-      <c r="A82" s="154" t="s">
+      <c r="A82" s="155" t="s">
         <v>247</v>
       </c>
       <c r="B82" s="113" t="s">
@@ -3877,7 +3883,7 @@
       </c>
     </row>
     <row r="83" spans="1:8" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="A83" s="155"/>
+      <c r="A83" s="156"/>
       <c r="B83" s="98" t="s">
         <v>177</v>
       </c>
@@ -3886,7 +3892,7 @@
         <v>34795</v>
       </c>
       <c r="E83" s="123">
-        <f t="shared" ref="E83:E96" si="4">IF(AND(C83&gt;0,D83&gt;0), D83-C83, 0)</f>
+        <f t="shared" ref="E83:E96" si="5">IF(AND(C83&gt;0,D83&gt;0), D83-C83, 0)</f>
         <v>0</v>
       </c>
       <c r="F83" s="104"/>
@@ -3895,7 +3901,7 @@
       </c>
     </row>
     <row r="84" spans="1:8" ht="15.75" outlineLevel="1" thickTop="1">
-      <c r="A84" s="155"/>
+      <c r="A84" s="156"/>
       <c r="B84" s="151" t="s">
         <v>228</v>
       </c>
@@ -3904,13 +3910,13 @@
         <v>36326</v>
       </c>
       <c r="E84" s="124">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F84" s="105"/>
     </row>
     <row r="85" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A85" s="155"/>
+      <c r="A85" s="156"/>
       <c r="B85" s="151" t="s">
         <v>221</v>
       </c>
@@ -3919,24 +3925,24 @@
         <v>37764</v>
       </c>
       <c r="E85" s="123">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F85" s="105"/>
     </row>
     <row r="86" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A86" s="155"/>
+      <c r="A86" s="156"/>
       <c r="B86" s="100"/>
       <c r="C86" s="101"/>
       <c r="D86" s="101"/>
       <c r="E86" s="123">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F86" s="105"/>
     </row>
     <row r="87" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A87" s="155"/>
+      <c r="A87" s="156"/>
       <c r="B87" s="151" t="s">
         <v>222</v>
       </c>
@@ -3945,24 +3951,24 @@
         <v>43241</v>
       </c>
       <c r="E87" s="123">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F87" s="105"/>
     </row>
     <row r="88" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A88" s="155"/>
+      <c r="A88" s="156"/>
       <c r="B88" s="100"/>
       <c r="C88" s="101"/>
       <c r="D88" s="101"/>
       <c r="E88" s="123">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F88" s="105"/>
     </row>
     <row r="89" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A89" s="155"/>
+      <c r="A89" s="156"/>
       <c r="B89" s="152" t="s">
         <v>236</v>
       </c>
@@ -3971,35 +3977,35 @@
         <v>45890</v>
       </c>
       <c r="E89" s="123">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F89" s="105"/>
     </row>
     <row r="90" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A90" s="155"/>
+      <c r="A90" s="156"/>
       <c r="B90" s="100"/>
       <c r="C90" s="101"/>
       <c r="D90" s="101"/>
       <c r="E90" s="123">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F90" s="105"/>
     </row>
     <row r="91" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A91" s="155"/>
+      <c r="A91" s="156"/>
       <c r="B91" s="100"/>
       <c r="C91" s="101"/>
       <c r="D91" s="101"/>
       <c r="E91" s="123">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F91" s="105"/>
     </row>
     <row r="92" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A92" s="155"/>
+      <c r="A92" s="156"/>
       <c r="B92" s="152" t="s">
         <v>223</v>
       </c>
@@ -4008,13 +4014,13 @@
         <v>49269</v>
       </c>
       <c r="E92" s="123">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F92" s="105"/>
     </row>
     <row r="93" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A93" s="155"/>
+      <c r="A93" s="156"/>
       <c r="B93" s="152" t="s">
         <v>249</v>
       </c>
@@ -4023,13 +4029,13 @@
         <v>49505</v>
       </c>
       <c r="E93" s="123">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F93" s="105"/>
     </row>
     <row r="94" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A94" s="155"/>
+      <c r="A94" s="156"/>
       <c r="B94" s="152" t="s">
         <v>250</v>
       </c>
@@ -4038,13 +4044,13 @@
         <v>50134</v>
       </c>
       <c r="E94" s="123">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F94" s="105"/>
     </row>
     <row r="95" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A95" s="155"/>
+      <c r="A95" s="156"/>
       <c r="B95" s="152" t="s">
         <v>251</v>
       </c>
@@ -4053,13 +4059,13 @@
         <v>50516</v>
       </c>
       <c r="E95" s="123">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F95" s="105"/>
     </row>
     <row r="96" spans="1:8" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="A96" s="155"/>
+      <c r="A96" s="156"/>
       <c r="B96" s="98" t="s">
         <v>179</v>
       </c>
@@ -4068,7 +4074,7 @@
         <v>50574</v>
       </c>
       <c r="E96" s="125">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F96" s="104"/>
@@ -4100,7 +4106,7 @@
     </row>
     <row r="98" spans="1:8" ht="13.5" thickBot="1"/>
     <row r="99" spans="1:8" ht="15" customHeight="1" outlineLevel="1">
-      <c r="A99" s="156" t="s">
+      <c r="A99" s="157" t="s">
         <v>252</v>
       </c>
       <c r="B99" s="109" t="s">
@@ -4120,7 +4126,7 @@
       </c>
     </row>
     <row r="100" spans="1:8" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="A100" s="155"/>
+      <c r="A100" s="156"/>
       <c r="B100" s="98" t="s">
         <v>177</v>
       </c>
@@ -4129,7 +4135,7 @@
         <v>50574</v>
       </c>
       <c r="E100" s="123">
-        <f t="shared" ref="E100:E109" si="5">IF(AND(C100&gt;0,D100&gt;0), D100-C100, 0)</f>
+        <f t="shared" ref="E100:E109" si="6">IF(AND(C100&gt;0,D100&gt;0), D100-C100, 0)</f>
         <v>0</v>
       </c>
       <c r="F100" s="104"/>
@@ -4138,18 +4144,18 @@
       </c>
     </row>
     <row r="101" spans="1:8" ht="15.75" outlineLevel="1" thickTop="1">
-      <c r="A101" s="155"/>
+      <c r="A101" s="156"/>
       <c r="B101" s="100"/>
       <c r="C101" s="101"/>
       <c r="D101" s="101"/>
       <c r="E101" s="124">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="F101" s="105"/>
     </row>
     <row r="102" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A102" s="155"/>
+      <c r="A102" s="156"/>
       <c r="B102" s="152" t="s">
         <v>254</v>
       </c>
@@ -4158,24 +4164,24 @@
         <v>52785</v>
       </c>
       <c r="E102" s="123">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="F102" s="105"/>
     </row>
     <row r="103" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A103" s="155"/>
+      <c r="A103" s="156"/>
       <c r="B103" s="100"/>
       <c r="C103" s="101"/>
       <c r="D103" s="101"/>
       <c r="E103" s="123">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="F103" s="105"/>
     </row>
     <row r="104" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A104" s="155"/>
+      <c r="A104" s="156"/>
       <c r="B104" s="152" t="s">
         <v>255</v>
       </c>
@@ -4184,24 +4190,24 @@
         <v>53409</v>
       </c>
       <c r="E104" s="123">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="F104" s="105"/>
     </row>
     <row r="105" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A105" s="155"/>
+      <c r="A105" s="156"/>
       <c r="B105" s="100"/>
       <c r="C105" s="101"/>
       <c r="D105" s="101"/>
       <c r="E105" s="123">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="F105" s="105"/>
     </row>
     <row r="106" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A106" s="155"/>
+      <c r="A106" s="156"/>
       <c r="B106" s="152" t="s">
         <v>223</v>
       </c>
@@ -4210,13 +4216,13 @@
         <v>55728</v>
       </c>
       <c r="E106" s="123">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="F106" s="105"/>
     </row>
     <row r="107" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A107" s="155"/>
+      <c r="A107" s="156"/>
       <c r="B107" s="152" t="s">
         <v>249</v>
       </c>
@@ -4225,13 +4231,13 @@
         <v>55956</v>
       </c>
       <c r="E107" s="123">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="F107" s="105"/>
     </row>
     <row r="108" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A108" s="155"/>
+      <c r="A108" s="156"/>
       <c r="B108" s="152" t="s">
         <v>256</v>
       </c>
@@ -4240,13 +4246,13 @@
         <v>56314</v>
       </c>
       <c r="E108" s="123">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="F108" s="105"/>
     </row>
     <row r="109" spans="1:8" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="A109" s="155"/>
+      <c r="A109" s="156"/>
       <c r="B109" s="98" t="s">
         <v>179</v>
       </c>
@@ -4255,7 +4261,7 @@
         <v>56373</v>
       </c>
       <c r="E109" s="125">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="F109" s="104"/>
@@ -4287,7 +4293,7 @@
     </row>
     <row r="111" spans="1:8" ht="13.5" thickBot="1"/>
     <row r="112" spans="1:8" ht="15" customHeight="1" outlineLevel="1">
-      <c r="A112" s="154" t="s">
+      <c r="A112" s="155" t="s">
         <v>257</v>
       </c>
       <c r="B112" s="113" t="s">
@@ -4307,7 +4313,7 @@
       </c>
     </row>
     <row r="113" spans="1:9" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="A113" s="155"/>
+      <c r="A113" s="156"/>
       <c r="B113" s="98" t="s">
         <v>177</v>
       </c>
@@ -4316,7 +4322,7 @@
         <v>56373</v>
       </c>
       <c r="E113" s="123">
-        <f t="shared" ref="E113:E121" si="6">IF(AND(C113&gt;0,D113&gt;0), D113-C113, 0)</f>
+        <f t="shared" ref="E113:E121" si="7">IF(AND(C113&gt;0,D113&gt;0), D113-C113, 0)</f>
         <v>0</v>
       </c>
       <c r="F113" s="104"/>
@@ -4329,18 +4335,18 @@
       </c>
     </row>
     <row r="114" spans="1:9" ht="15.75" outlineLevel="1" thickTop="1">
-      <c r="A114" s="155"/>
+      <c r="A114" s="156"/>
       <c r="B114" s="100"/>
       <c r="C114" s="101"/>
       <c r="D114" s="101"/>
       <c r="E114" s="124">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="F114" s="105"/>
     </row>
     <row r="115" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A115" s="155"/>
+      <c r="A115" s="156"/>
       <c r="B115" s="152" t="s">
         <v>221</v>
       </c>
@@ -4349,24 +4355,24 @@
         <v>58041</v>
       </c>
       <c r="E115" s="123">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="F115" s="105"/>
     </row>
     <row r="116" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A116" s="155"/>
+      <c r="A116" s="156"/>
       <c r="B116" s="100"/>
       <c r="C116" s="101"/>
       <c r="D116" s="101"/>
       <c r="E116" s="123">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="F116" s="105"/>
     </row>
     <row r="117" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A117" s="155"/>
+      <c r="A117" s="156"/>
       <c r="B117" s="152" t="s">
         <v>222</v>
       </c>
@@ -4375,13 +4381,13 @@
         <v>60301</v>
       </c>
       <c r="E117" s="123">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="F117" s="105"/>
     </row>
     <row r="118" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A118" s="155"/>
+      <c r="A118" s="156"/>
       <c r="B118" s="152" t="s">
         <v>249</v>
       </c>
@@ -4390,13 +4396,13 @@
         <v>60529</v>
       </c>
       <c r="E118" s="123">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="F118" s="105"/>
     </row>
     <row r="119" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A119" s="155"/>
+      <c r="A119" s="156"/>
       <c r="B119" s="152" t="s">
         <v>259</v>
       </c>
@@ -4405,13 +4411,13 @@
         <v>61068</v>
       </c>
       <c r="E119" s="123">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="F119" s="105"/>
     </row>
     <row r="120" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A120" s="155"/>
+      <c r="A120" s="156"/>
       <c r="B120" s="152" t="s">
         <v>224</v>
       </c>
@@ -4420,13 +4426,13 @@
         <v>61391</v>
       </c>
       <c r="E120" s="123">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="F120" s="105"/>
     </row>
     <row r="121" spans="1:9" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="A121" s="155"/>
+      <c r="A121" s="156"/>
       <c r="B121" s="98" t="s">
         <v>179</v>
       </c>
@@ -4435,7 +4441,7 @@
         <v>61438</v>
       </c>
       <c r="E121" s="125">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="F121" s="104"/>
@@ -4467,7 +4473,7 @@
     </row>
     <row r="123" spans="1:9" ht="13.5" thickBot="1"/>
     <row r="124" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A124" s="156" t="s">
+      <c r="A124" s="157" t="s">
         <v>260</v>
       </c>
       <c r="B124" s="109" t="s">
@@ -4487,7 +4493,7 @@
       </c>
     </row>
     <row r="125" spans="1:9" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="A125" s="155"/>
+      <c r="A125" s="156"/>
       <c r="B125" s="98" t="s">
         <v>177</v>
       </c>
@@ -4496,7 +4502,7 @@
         <v>61438</v>
       </c>
       <c r="E125" s="123">
-        <f t="shared" ref="E125:E138" si="7">IF(AND(C125&gt;0,D125&gt;0), D125-C125, 0)</f>
+        <f t="shared" ref="E125:E138" si="8">IF(AND(C125&gt;0,D125&gt;0), D125-C125, 0)</f>
         <v>0</v>
       </c>
       <c r="F125" s="104"/>
@@ -4509,95 +4515,95 @@
       </c>
     </row>
     <row r="126" spans="1:9" ht="15.75" outlineLevel="1" thickTop="1">
-      <c r="A126" s="155"/>
+      <c r="A126" s="156"/>
       <c r="B126" s="100"/>
       <c r="C126" s="101"/>
       <c r="D126" s="101"/>
       <c r="E126" s="124">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="F126" s="105"/>
     </row>
     <row r="127" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A127" s="155"/>
+      <c r="A127" s="156"/>
       <c r="B127" s="100"/>
       <c r="C127" s="101"/>
       <c r="D127" s="101"/>
       <c r="E127" s="123">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="F127" s="105"/>
     </row>
     <row r="128" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A128" s="155"/>
+      <c r="A128" s="156"/>
       <c r="B128" s="100"/>
       <c r="C128" s="101"/>
       <c r="D128" s="101"/>
       <c r="E128" s="123">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="F128" s="105"/>
     </row>
     <row r="129" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A129" s="155"/>
+      <c r="A129" s="156"/>
       <c r="B129" s="100"/>
       <c r="C129" s="101"/>
       <c r="D129" s="101"/>
       <c r="E129" s="123">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="F129" s="105"/>
     </row>
     <row r="130" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A130" s="155"/>
+      <c r="A130" s="156"/>
       <c r="B130" s="100"/>
       <c r="C130" s="101"/>
       <c r="D130" s="101"/>
       <c r="E130" s="123">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="F130" s="105"/>
     </row>
     <row r="131" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A131" s="155"/>
+      <c r="A131" s="156"/>
       <c r="B131" s="100"/>
       <c r="C131" s="101"/>
       <c r="D131" s="101"/>
       <c r="E131" s="123">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="F131" s="105"/>
     </row>
     <row r="132" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A132" s="155"/>
+      <c r="A132" s="156"/>
       <c r="B132" s="100"/>
       <c r="C132" s="101"/>
       <c r="D132" s="101"/>
       <c r="E132" s="123">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="F132" s="105"/>
     </row>
     <row r="133" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A133" s="155"/>
+      <c r="A133" s="156"/>
       <c r="B133" s="100"/>
       <c r="C133" s="101"/>
       <c r="D133" s="101"/>
       <c r="E133" s="123">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="F133" s="105"/>
     </row>
     <row r="134" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A134" s="155"/>
+      <c r="A134" s="156"/>
       <c r="B134" s="152" t="s">
         <v>262</v>
       </c>
@@ -4606,7 +4612,7 @@
         <v>66926</v>
       </c>
       <c r="E134" s="123">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="F134" s="105"/>
@@ -4619,47 +4625,47 @@
       </c>
     </row>
     <row r="135" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A135" s="155"/>
+      <c r="A135" s="156"/>
       <c r="B135" s="100"/>
       <c r="C135" s="101"/>
       <c r="D135" s="101"/>
       <c r="E135" s="123">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="F135" s="105"/>
     </row>
     <row r="136" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A136" s="155"/>
+      <c r="A136" s="156"/>
       <c r="B136" s="100"/>
       <c r="C136" s="101"/>
       <c r="D136" s="101"/>
       <c r="E136" s="123">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="F136" s="105"/>
     </row>
     <row r="137" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A137" s="155"/>
+      <c r="A137" s="156"/>
       <c r="B137" s="100"/>
       <c r="C137" s="101"/>
       <c r="D137" s="101"/>
       <c r="E137" s="123">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="F137" s="105"/>
     </row>
     <row r="138" spans="1:9" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="A138" s="155"/>
+      <c r="A138" s="156"/>
       <c r="B138" s="98" t="s">
         <v>179</v>
       </c>
       <c r="C138" s="99"/>
       <c r="D138" s="99"/>
       <c r="E138" s="125">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="F138" s="104"/>
@@ -4690,7 +4696,7 @@
       </c>
     </row>
     <row r="141" spans="1:9" ht="15" hidden="1" outlineLevel="2">
-      <c r="A141" s="154" t="s">
+      <c r="A141" s="155" t="s">
         <v>169</v>
       </c>
       <c r="B141" s="113" t="s">
@@ -4710,159 +4716,159 @@
       </c>
     </row>
     <row r="142" spans="1:9" ht="15.75" hidden="1" outlineLevel="2" thickBot="1">
-      <c r="A142" s="155"/>
+      <c r="A142" s="156"/>
       <c r="B142" s="98" t="s">
         <v>177</v>
       </c>
       <c r="C142" s="99"/>
       <c r="D142" s="99"/>
       <c r="E142" s="123">
-        <f t="shared" ref="E142:E155" si="8">IF(AND(C142&gt;0,D142&gt;0), D142-C142, 0)</f>
+        <f t="shared" ref="E142:E155" si="9">IF(AND(C142&gt;0,D142&gt;0), D142-C142, 0)</f>
         <v>0</v>
       </c>
       <c r="F142" s="104"/>
     </row>
     <row r="143" spans="1:9" ht="15.75" hidden="1" outlineLevel="2" thickTop="1">
-      <c r="A143" s="155"/>
+      <c r="A143" s="156"/>
       <c r="B143" s="100"/>
       <c r="C143" s="101"/>
       <c r="D143" s="101"/>
       <c r="E143" s="124">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="F143" s="105"/>
     </row>
     <row r="144" spans="1:9" ht="15" hidden="1" outlineLevel="2">
-      <c r="A144" s="155"/>
+      <c r="A144" s="156"/>
       <c r="B144" s="100"/>
       <c r="C144" s="101"/>
       <c r="D144" s="101"/>
       <c r="E144" s="123">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="F144" s="105"/>
     </row>
     <row r="145" spans="1:7" ht="15" hidden="1" outlineLevel="2">
-      <c r="A145" s="155"/>
+      <c r="A145" s="156"/>
       <c r="B145" s="100"/>
       <c r="C145" s="101"/>
       <c r="D145" s="101"/>
       <c r="E145" s="123">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="F145" s="105"/>
     </row>
     <row r="146" spans="1:7" ht="15" hidden="1" outlineLevel="2">
-      <c r="A146" s="155"/>
+      <c r="A146" s="156"/>
       <c r="B146" s="100"/>
       <c r="C146" s="101"/>
       <c r="D146" s="101"/>
       <c r="E146" s="123">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="F146" s="105"/>
     </row>
     <row r="147" spans="1:7" ht="15" hidden="1" outlineLevel="2">
-      <c r="A147" s="155"/>
+      <c r="A147" s="156"/>
       <c r="B147" s="100"/>
       <c r="C147" s="101"/>
       <c r="D147" s="101"/>
       <c r="E147" s="123">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="F147" s="105"/>
     </row>
     <row r="148" spans="1:7" ht="15" hidden="1" outlineLevel="2">
-      <c r="A148" s="155"/>
+      <c r="A148" s="156"/>
       <c r="B148" s="100"/>
       <c r="C148" s="101"/>
       <c r="D148" s="101"/>
       <c r="E148" s="123">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="F148" s="105"/>
     </row>
     <row r="149" spans="1:7" ht="15" hidden="1" outlineLevel="2">
-      <c r="A149" s="155"/>
+      <c r="A149" s="156"/>
       <c r="B149" s="100"/>
       <c r="C149" s="101"/>
       <c r="D149" s="101"/>
       <c r="E149" s="123">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="F149" s="105"/>
     </row>
     <row r="150" spans="1:7" ht="15" hidden="1" outlineLevel="2">
-      <c r="A150" s="155"/>
+      <c r="A150" s="156"/>
       <c r="B150" s="100"/>
       <c r="C150" s="101"/>
       <c r="D150" s="101"/>
       <c r="E150" s="123">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="F150" s="105"/>
     </row>
     <row r="151" spans="1:7" ht="15" hidden="1" outlineLevel="2">
-      <c r="A151" s="155"/>
+      <c r="A151" s="156"/>
       <c r="B151" s="100"/>
       <c r="C151" s="101"/>
       <c r="D151" s="101"/>
       <c r="E151" s="123">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="F151" s="105"/>
     </row>
     <row r="152" spans="1:7" ht="15" hidden="1" outlineLevel="2">
-      <c r="A152" s="155"/>
+      <c r="A152" s="156"/>
       <c r="B152" s="100"/>
       <c r="C152" s="101"/>
       <c r="D152" s="101"/>
       <c r="E152" s="123">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="F152" s="105"/>
     </row>
     <row r="153" spans="1:7" ht="15" hidden="1" outlineLevel="2">
-      <c r="A153" s="155"/>
+      <c r="A153" s="156"/>
       <c r="B153" s="100"/>
       <c r="C153" s="101"/>
       <c r="D153" s="101"/>
       <c r="E153" s="123">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="F153" s="105"/>
     </row>
     <row r="154" spans="1:7" ht="15" hidden="1" outlineLevel="2">
-      <c r="A154" s="155"/>
+      <c r="A154" s="156"/>
       <c r="B154" s="100"/>
       <c r="C154" s="101"/>
       <c r="D154" s="101"/>
       <c r="E154" s="123">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="F154" s="105"/>
     </row>
     <row r="155" spans="1:7" ht="15.75" hidden="1" outlineLevel="2" thickBot="1">
-      <c r="A155" s="155"/>
+      <c r="A155" s="156"/>
       <c r="B155" s="98" t="s">
         <v>179</v>
       </c>
       <c r="C155" s="99"/>
       <c r="D155" s="99"/>
       <c r="E155" s="125">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="F155" s="104"/>
@@ -4894,6 +4900,11 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="A141:A155"/>
+    <mergeCell ref="A112:A121"/>
+    <mergeCell ref="A82:A96"/>
+    <mergeCell ref="A124:A138"/>
+    <mergeCell ref="A99:A109"/>
     <mergeCell ref="A43:A63"/>
     <mergeCell ref="A66:A79"/>
     <mergeCell ref="C5:D5"/>
@@ -4903,11 +4914,6 @@
     <mergeCell ref="A8:A18"/>
     <mergeCell ref="A21:A40"/>
     <mergeCell ref="C4:E4"/>
-    <mergeCell ref="A141:A155"/>
-    <mergeCell ref="A112:A121"/>
-    <mergeCell ref="A82:A96"/>
-    <mergeCell ref="A124:A138"/>
-    <mergeCell ref="A99:A109"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4939,13 +4945,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="26.25" customHeight="1">
-      <c r="A1" s="182" t="s">
+      <c r="A1" s="165" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="182"/>
-      <c r="C1" s="182"/>
-      <c r="D1" s="182"/>
-      <c r="E1" s="182"/>
+      <c r="B1" s="165"/>
+      <c r="C1" s="165"/>
+      <c r="D1" s="165"/>
+      <c r="E1" s="165"/>
       <c r="F1" s="7"/>
       <c r="G1" s="5"/>
       <c r="H1" s="5"/>
@@ -4975,18 +4981,18 @@
         <v>8</v>
       </c>
       <c r="B3" s="36"/>
-      <c r="C3" s="183"/>
-      <c r="D3" s="184"/>
-      <c r="E3" s="184"/>
+      <c r="C3" s="166"/>
+      <c r="D3" s="167"/>
+      <c r="E3" s="167"/>
     </row>
     <row r="4" spans="1:8" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A4" s="46" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="87"/>
-      <c r="C4" s="164"/>
-      <c r="D4" s="165"/>
-      <c r="E4" s="165"/>
+      <c r="C4" s="168"/>
+      <c r="D4" s="169"/>
+      <c r="E4" s="169"/>
       <c r="F4" s="6"/>
     </row>
     <row r="5" spans="1:8" hidden="1" outlineLevel="2">
@@ -5138,9 +5144,9 @@
         <v>9</v>
       </c>
       <c r="B21" s="90"/>
-      <c r="C21" s="166"/>
-      <c r="D21" s="167"/>
-      <c r="E21" s="167"/>
+      <c r="C21" s="170"/>
+      <c r="D21" s="171"/>
+      <c r="E21" s="171"/>
     </row>
     <row r="22" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A22" s="47">
@@ -5291,9 +5297,9 @@
         <v>10</v>
       </c>
       <c r="B38" s="87"/>
-      <c r="C38" s="164"/>
-      <c r="D38" s="165"/>
-      <c r="E38" s="165"/>
+      <c r="C38" s="168"/>
+      <c r="D38" s="169"/>
+      <c r="E38" s="169"/>
     </row>
     <row r="39" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A39" s="47">
@@ -5444,9 +5450,9 @@
         <v>11</v>
       </c>
       <c r="B55" s="87"/>
-      <c r="C55" s="164"/>
-      <c r="D55" s="165"/>
-      <c r="E55" s="165"/>
+      <c r="C55" s="168"/>
+      <c r="D55" s="169"/>
+      <c r="E55" s="169"/>
     </row>
     <row r="56" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A56" s="47">
@@ -5597,9 +5603,9 @@
         <v>12</v>
       </c>
       <c r="B72" s="87"/>
-      <c r="C72" s="164"/>
-      <c r="D72" s="165"/>
-      <c r="E72" s="165"/>
+      <c r="C72" s="168"/>
+      <c r="D72" s="169"/>
+      <c r="E72" s="169"/>
     </row>
     <row r="73" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A73" s="47">
@@ -5750,9 +5756,9 @@
         <v>13</v>
       </c>
       <c r="B89" s="87"/>
-      <c r="C89" s="164"/>
-      <c r="D89" s="165"/>
-      <c r="E89" s="165"/>
+      <c r="C89" s="168"/>
+      <c r="D89" s="169"/>
+      <c r="E89" s="169"/>
     </row>
     <row r="90" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A90" s="47">
@@ -5903,9 +5909,9 @@
         <v>14</v>
       </c>
       <c r="B106" s="87"/>
-      <c r="C106" s="164"/>
-      <c r="D106" s="165"/>
-      <c r="E106" s="165"/>
+      <c r="C106" s="168"/>
+      <c r="D106" s="169"/>
+      <c r="E106" s="169"/>
     </row>
     <row r="107" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A107" s="47">
@@ -6056,9 +6062,9 @@
         <v>15</v>
       </c>
       <c r="B123" s="87"/>
-      <c r="C123" s="164"/>
-      <c r="D123" s="165"/>
-      <c r="E123" s="165"/>
+      <c r="C123" s="168"/>
+      <c r="D123" s="169"/>
+      <c r="E123" s="169"/>
     </row>
     <row r="124" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A124" s="47">
@@ -6209,9 +6215,9 @@
         <v>16</v>
       </c>
       <c r="B140" s="87"/>
-      <c r="C140" s="164"/>
-      <c r="D140" s="165"/>
-      <c r="E140" s="165"/>
+      <c r="C140" s="168"/>
+      <c r="D140" s="169"/>
+      <c r="E140" s="169"/>
     </row>
     <row r="141" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A141" s="47">
@@ -6362,9 +6368,9 @@
         <v>17</v>
       </c>
       <c r="B157" s="87"/>
-      <c r="C157" s="164"/>
-      <c r="D157" s="165"/>
-      <c r="E157" s="165"/>
+      <c r="C157" s="168"/>
+      <c r="D157" s="169"/>
+      <c r="E157" s="169"/>
     </row>
     <row r="158" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A158" s="47">
@@ -6515,9 +6521,9 @@
         <v>18</v>
       </c>
       <c r="B174" s="87"/>
-      <c r="C174" s="164"/>
-      <c r="D174" s="165"/>
-      <c r="E174" s="165"/>
+      <c r="C174" s="168"/>
+      <c r="D174" s="169"/>
+      <c r="E174" s="169"/>
     </row>
     <row r="175" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A175" s="47">
@@ -6668,9 +6674,9 @@
         <v>19</v>
       </c>
       <c r="B191" s="87"/>
-      <c r="C191" s="164"/>
-      <c r="D191" s="165"/>
-      <c r="E191" s="165"/>
+      <c r="C191" s="168"/>
+      <c r="D191" s="169"/>
+      <c r="E191" s="169"/>
     </row>
     <row r="192" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A192" s="47">
@@ -6821,9 +6827,9 @@
         <v>20</v>
       </c>
       <c r="B208" s="87"/>
-      <c r="C208" s="164"/>
-      <c r="D208" s="165"/>
-      <c r="E208" s="165"/>
+      <c r="C208" s="168"/>
+      <c r="D208" s="169"/>
+      <c r="E208" s="169"/>
     </row>
     <row r="209" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A209" s="47">
@@ -6974,9 +6980,9 @@
         <v>21</v>
       </c>
       <c r="B225" s="87"/>
-      <c r="C225" s="164"/>
-      <c r="D225" s="165"/>
-      <c r="E225" s="165"/>
+      <c r="C225" s="168"/>
+      <c r="D225" s="169"/>
+      <c r="E225" s="169"/>
     </row>
     <row r="226" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A226" s="47">
@@ -7127,9 +7133,9 @@
         <v>22</v>
       </c>
       <c r="B242" s="87"/>
-      <c r="C242" s="164"/>
-      <c r="D242" s="165"/>
-      <c r="E242" s="165"/>
+      <c r="C242" s="168"/>
+      <c r="D242" s="169"/>
+      <c r="E242" s="169"/>
     </row>
     <row r="243" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A243" s="47">
@@ -7280,9 +7286,9 @@
         <v>23</v>
       </c>
       <c r="B259" s="87"/>
-      <c r="C259" s="164"/>
-      <c r="D259" s="165"/>
-      <c r="E259" s="165"/>
+      <c r="C259" s="168"/>
+      <c r="D259" s="169"/>
+      <c r="E259" s="169"/>
     </row>
     <row r="260" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A260" s="47">
@@ -7433,18 +7439,18 @@
         <v>24</v>
       </c>
       <c r="B276" s="37"/>
-      <c r="C276" s="180"/>
-      <c r="D276" s="181"/>
-      <c r="E276" s="181"/>
+      <c r="C276" s="172"/>
+      <c r="D276" s="173"/>
+      <c r="E276" s="173"/>
     </row>
     <row r="277" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A277" s="51" t="s">
         <v>25</v>
       </c>
       <c r="B277" s="87"/>
-      <c r="C277" s="164"/>
-      <c r="D277" s="165"/>
-      <c r="E277" s="165"/>
+      <c r="C277" s="168"/>
+      <c r="D277" s="169"/>
+      <c r="E277" s="169"/>
     </row>
     <row r="278" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A278" s="52">
@@ -7595,9 +7601,9 @@
         <v>26</v>
       </c>
       <c r="B294" s="90"/>
-      <c r="C294" s="166"/>
-      <c r="D294" s="167"/>
-      <c r="E294" s="167"/>
+      <c r="C294" s="170"/>
+      <c r="D294" s="171"/>
+      <c r="E294" s="171"/>
     </row>
     <row r="295" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A295" s="52">
@@ -7748,9 +7754,9 @@
         <v>27</v>
       </c>
       <c r="B311" s="87"/>
-      <c r="C311" s="164"/>
-      <c r="D311" s="165"/>
-      <c r="E311" s="165"/>
+      <c r="C311" s="168"/>
+      <c r="D311" s="169"/>
+      <c r="E311" s="169"/>
     </row>
     <row r="312" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A312" s="52">
@@ -7901,9 +7907,9 @@
         <v>28</v>
       </c>
       <c r="B328" s="87"/>
-      <c r="C328" s="164"/>
-      <c r="D328" s="165"/>
-      <c r="E328" s="165"/>
+      <c r="C328" s="168"/>
+      <c r="D328" s="169"/>
+      <c r="E328" s="169"/>
     </row>
     <row r="329" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A329" s="52">
@@ -8054,9 +8060,9 @@
         <v>29</v>
       </c>
       <c r="B345" s="87"/>
-      <c r="C345" s="164"/>
-      <c r="D345" s="165"/>
-      <c r="E345" s="165"/>
+      <c r="C345" s="168"/>
+      <c r="D345" s="169"/>
+      <c r="E345" s="169"/>
     </row>
     <row r="346" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A346" s="52">
@@ -8207,9 +8213,9 @@
         <v>30</v>
       </c>
       <c r="B362" s="87"/>
-      <c r="C362" s="164"/>
-      <c r="D362" s="165"/>
-      <c r="E362" s="165"/>
+      <c r="C362" s="168"/>
+      <c r="D362" s="169"/>
+      <c r="E362" s="169"/>
     </row>
     <row r="363" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A363" s="52">
@@ -8360,9 +8366,9 @@
         <v>31</v>
       </c>
       <c r="B379" s="87"/>
-      <c r="C379" s="164"/>
-      <c r="D379" s="165"/>
-      <c r="E379" s="165"/>
+      <c r="C379" s="168"/>
+      <c r="D379" s="169"/>
+      <c r="E379" s="169"/>
     </row>
     <row r="380" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A380" s="52">
@@ -8513,9 +8519,9 @@
         <v>32</v>
       </c>
       <c r="B396" s="87"/>
-      <c r="C396" s="164"/>
-      <c r="D396" s="165"/>
-      <c r="E396" s="165"/>
+      <c r="C396" s="168"/>
+      <c r="D396" s="169"/>
+      <c r="E396" s="169"/>
     </row>
     <row r="397" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A397" s="52">
@@ -8666,9 +8672,9 @@
         <v>33</v>
       </c>
       <c r="B413" s="87"/>
-      <c r="C413" s="164"/>
-      <c r="D413" s="165"/>
-      <c r="E413" s="165"/>
+      <c r="C413" s="168"/>
+      <c r="D413" s="169"/>
+      <c r="E413" s="169"/>
     </row>
     <row r="414" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A414" s="52">
@@ -8819,9 +8825,9 @@
         <v>34</v>
       </c>
       <c r="B430" s="87"/>
-      <c r="C430" s="164"/>
-      <c r="D430" s="165"/>
-      <c r="E430" s="165"/>
+      <c r="C430" s="168"/>
+      <c r="D430" s="169"/>
+      <c r="E430" s="169"/>
     </row>
     <row r="431" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A431" s="52">
@@ -8972,9 +8978,9 @@
         <v>35</v>
       </c>
       <c r="B447" s="87"/>
-      <c r="C447" s="164"/>
-      <c r="D447" s="165"/>
-      <c r="E447" s="165"/>
+      <c r="C447" s="168"/>
+      <c r="D447" s="169"/>
+      <c r="E447" s="169"/>
     </row>
     <row r="448" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A448" s="52">
@@ -9125,9 +9131,9 @@
         <v>36</v>
       </c>
       <c r="B464" s="87"/>
-      <c r="C464" s="164"/>
-      <c r="D464" s="165"/>
-      <c r="E464" s="165"/>
+      <c r="C464" s="168"/>
+      <c r="D464" s="169"/>
+      <c r="E464" s="169"/>
     </row>
     <row r="465" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A465" s="52">
@@ -9278,9 +9284,9 @@
         <v>37</v>
       </c>
       <c r="B481" s="87"/>
-      <c r="C481" s="164"/>
-      <c r="D481" s="165"/>
-      <c r="E481" s="165"/>
+      <c r="C481" s="168"/>
+      <c r="D481" s="169"/>
+      <c r="E481" s="169"/>
     </row>
     <row r="482" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A482" s="52">
@@ -9431,9 +9437,9 @@
         <v>38</v>
       </c>
       <c r="B498" s="87"/>
-      <c r="C498" s="164"/>
-      <c r="D498" s="165"/>
-      <c r="E498" s="165"/>
+      <c r="C498" s="168"/>
+      <c r="D498" s="169"/>
+      <c r="E498" s="169"/>
     </row>
     <row r="499" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A499" s="52">
@@ -9584,9 +9590,9 @@
         <v>39</v>
       </c>
       <c r="B515" s="87"/>
-      <c r="C515" s="164"/>
-      <c r="D515" s="165"/>
-      <c r="E515" s="165"/>
+      <c r="C515" s="168"/>
+      <c r="D515" s="169"/>
+      <c r="E515" s="169"/>
     </row>
     <row r="516" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A516" s="52">
@@ -9737,9 +9743,9 @@
         <v>40</v>
       </c>
       <c r="B532" s="87"/>
-      <c r="C532" s="164"/>
-      <c r="D532" s="165"/>
-      <c r="E532" s="165"/>
+      <c r="C532" s="168"/>
+      <c r="D532" s="169"/>
+      <c r="E532" s="169"/>
     </row>
     <row r="533" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A533" s="55">
@@ -9890,18 +9896,18 @@
         <v>50</v>
       </c>
       <c r="B549" s="38"/>
-      <c r="C549" s="178"/>
-      <c r="D549" s="179"/>
-      <c r="E549" s="179"/>
+      <c r="C549" s="174"/>
+      <c r="D549" s="175"/>
+      <c r="E549" s="175"/>
     </row>
     <row r="550" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A550" s="58" t="s">
         <v>51</v>
       </c>
       <c r="B550" s="87"/>
-      <c r="C550" s="164"/>
-      <c r="D550" s="165"/>
-      <c r="E550" s="165"/>
+      <c r="C550" s="168"/>
+      <c r="D550" s="169"/>
+      <c r="E550" s="169"/>
     </row>
     <row r="551" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A551" s="59">
@@ -10052,9 +10058,9 @@
         <v>52</v>
       </c>
       <c r="B567" s="90"/>
-      <c r="C567" s="166"/>
-      <c r="D567" s="167"/>
-      <c r="E567" s="167"/>
+      <c r="C567" s="170"/>
+      <c r="D567" s="171"/>
+      <c r="E567" s="171"/>
     </row>
     <row r="568" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A568" s="59">
@@ -10205,9 +10211,9 @@
         <v>53</v>
       </c>
       <c r="B584" s="87"/>
-      <c r="C584" s="164"/>
-      <c r="D584" s="165"/>
-      <c r="E584" s="165"/>
+      <c r="C584" s="168"/>
+      <c r="D584" s="169"/>
+      <c r="E584" s="169"/>
     </row>
     <row r="585" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A585" s="59">
@@ -10358,9 +10364,9 @@
         <v>54</v>
       </c>
       <c r="B601" s="87"/>
-      <c r="C601" s="164"/>
-      <c r="D601" s="165"/>
-      <c r="E601" s="165"/>
+      <c r="C601" s="168"/>
+      <c r="D601" s="169"/>
+      <c r="E601" s="169"/>
     </row>
     <row r="602" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A602" s="59">
@@ -10511,9 +10517,9 @@
         <v>55</v>
       </c>
       <c r="B618" s="87"/>
-      <c r="C618" s="164"/>
-      <c r="D618" s="165"/>
-      <c r="E618" s="165"/>
+      <c r="C618" s="168"/>
+      <c r="D618" s="169"/>
+      <c r="E618" s="169"/>
     </row>
     <row r="619" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A619" s="59">
@@ -10664,9 +10670,9 @@
         <v>56</v>
       </c>
       <c r="B635" s="87"/>
-      <c r="C635" s="164"/>
-      <c r="D635" s="165"/>
-      <c r="E635" s="165"/>
+      <c r="C635" s="168"/>
+      <c r="D635" s="169"/>
+      <c r="E635" s="169"/>
     </row>
     <row r="636" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A636" s="59">
@@ -10817,9 +10823,9 @@
         <v>57</v>
       </c>
       <c r="B652" s="87"/>
-      <c r="C652" s="164"/>
-      <c r="D652" s="165"/>
-      <c r="E652" s="165"/>
+      <c r="C652" s="168"/>
+      <c r="D652" s="169"/>
+      <c r="E652" s="169"/>
     </row>
     <row r="653" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A653" s="59">
@@ -10970,9 +10976,9 @@
         <v>58</v>
       </c>
       <c r="B669" s="87"/>
-      <c r="C669" s="164"/>
-      <c r="D669" s="165"/>
-      <c r="E669" s="165"/>
+      <c r="C669" s="168"/>
+      <c r="D669" s="169"/>
+      <c r="E669" s="169"/>
     </row>
     <row r="670" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A670" s="59">
@@ -11123,9 +11129,9 @@
         <v>59</v>
       </c>
       <c r="B686" s="87"/>
-      <c r="C686" s="164"/>
-      <c r="D686" s="165"/>
-      <c r="E686" s="165"/>
+      <c r="C686" s="168"/>
+      <c r="D686" s="169"/>
+      <c r="E686" s="169"/>
     </row>
     <row r="687" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A687" s="59">
@@ -11276,9 +11282,9 @@
         <v>60</v>
       </c>
       <c r="B703" s="87"/>
-      <c r="C703" s="164"/>
-      <c r="D703" s="165"/>
-      <c r="E703" s="165"/>
+      <c r="C703" s="168"/>
+      <c r="D703" s="169"/>
+      <c r="E703" s="169"/>
     </row>
     <row r="704" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A704" s="59">
@@ -11429,9 +11435,9 @@
         <v>61</v>
       </c>
       <c r="B720" s="87"/>
-      <c r="C720" s="164"/>
-      <c r="D720" s="165"/>
-      <c r="E720" s="165"/>
+      <c r="C720" s="168"/>
+      <c r="D720" s="169"/>
+      <c r="E720" s="169"/>
     </row>
     <row r="721" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A721" s="59">
@@ -11582,9 +11588,9 @@
         <v>62</v>
       </c>
       <c r="B737" s="87"/>
-      <c r="C737" s="164"/>
-      <c r="D737" s="165"/>
-      <c r="E737" s="165"/>
+      <c r="C737" s="168"/>
+      <c r="D737" s="169"/>
+      <c r="E737" s="169"/>
     </row>
     <row r="738" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A738" s="59">
@@ -11735,9 +11741,9 @@
         <v>63</v>
       </c>
       <c r="B754" s="87"/>
-      <c r="C754" s="164"/>
-      <c r="D754" s="165"/>
-      <c r="E754" s="165"/>
+      <c r="C754" s="168"/>
+      <c r="D754" s="169"/>
+      <c r="E754" s="169"/>
     </row>
     <row r="755" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A755" s="59">
@@ -11888,9 +11894,9 @@
         <v>64</v>
       </c>
       <c r="B771" s="87"/>
-      <c r="C771" s="164"/>
-      <c r="D771" s="165"/>
-      <c r="E771" s="165"/>
+      <c r="C771" s="168"/>
+      <c r="D771" s="169"/>
+      <c r="E771" s="169"/>
     </row>
     <row r="772" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A772" s="59">
@@ -12041,9 +12047,9 @@
         <v>65</v>
       </c>
       <c r="B788" s="87"/>
-      <c r="C788" s="164"/>
-      <c r="D788" s="165"/>
-      <c r="E788" s="165"/>
+      <c r="C788" s="168"/>
+      <c r="D788" s="169"/>
+      <c r="E788" s="169"/>
     </row>
     <row r="789" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A789" s="59">
@@ -12194,9 +12200,9 @@
         <v>66</v>
       </c>
       <c r="B805" s="87"/>
-      <c r="C805" s="164"/>
-      <c r="D805" s="165"/>
-      <c r="E805" s="165"/>
+      <c r="C805" s="168"/>
+      <c r="D805" s="169"/>
+      <c r="E805" s="169"/>
     </row>
     <row r="806" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A806" s="59">
@@ -12356,9 +12362,9 @@
         <v>68</v>
       </c>
       <c r="B823" s="87"/>
-      <c r="C823" s="164"/>
-      <c r="D823" s="165"/>
-      <c r="E823" s="165"/>
+      <c r="C823" s="168"/>
+      <c r="D823" s="169"/>
+      <c r="E823" s="169"/>
     </row>
     <row r="824" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A824" s="64">
@@ -12509,9 +12515,9 @@
         <v>69</v>
       </c>
       <c r="B840" s="90"/>
-      <c r="C840" s="166"/>
-      <c r="D840" s="167"/>
-      <c r="E840" s="167"/>
+      <c r="C840" s="170"/>
+      <c r="D840" s="171"/>
+      <c r="E840" s="171"/>
     </row>
     <row r="841" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A841" s="64">
@@ -12662,9 +12668,9 @@
         <v>70</v>
       </c>
       <c r="B857" s="87"/>
-      <c r="C857" s="164"/>
-      <c r="D857" s="165"/>
-      <c r="E857" s="165"/>
+      <c r="C857" s="168"/>
+      <c r="D857" s="169"/>
+      <c r="E857" s="169"/>
     </row>
     <row r="858" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A858" s="64">
@@ -12815,9 +12821,9 @@
         <v>71</v>
       </c>
       <c r="B874" s="87"/>
-      <c r="C874" s="164"/>
-      <c r="D874" s="165"/>
-      <c r="E874" s="165"/>
+      <c r="C874" s="168"/>
+      <c r="D874" s="169"/>
+      <c r="E874" s="169"/>
     </row>
     <row r="875" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A875" s="64">
@@ -12968,9 +12974,9 @@
         <v>72</v>
       </c>
       <c r="B891" s="87"/>
-      <c r="C891" s="164"/>
-      <c r="D891" s="165"/>
-      <c r="E891" s="165"/>
+      <c r="C891" s="168"/>
+      <c r="D891" s="169"/>
+      <c r="E891" s="169"/>
     </row>
     <row r="892" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A892" s="64">
@@ -13121,9 +13127,9 @@
         <v>73</v>
       </c>
       <c r="B908" s="87"/>
-      <c r="C908" s="164"/>
-      <c r="D908" s="165"/>
-      <c r="E908" s="165"/>
+      <c r="C908" s="168"/>
+      <c r="D908" s="169"/>
+      <c r="E908" s="169"/>
     </row>
     <row r="909" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A909" s="64">
@@ -13274,9 +13280,9 @@
         <v>74</v>
       </c>
       <c r="B925" s="87"/>
-      <c r="C925" s="164"/>
-      <c r="D925" s="165"/>
-      <c r="E925" s="165"/>
+      <c r="C925" s="168"/>
+      <c r="D925" s="169"/>
+      <c r="E925" s="169"/>
     </row>
     <row r="926" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A926" s="64">
@@ -13427,9 +13433,9 @@
         <v>75</v>
       </c>
       <c r="B942" s="87"/>
-      <c r="C942" s="164"/>
-      <c r="D942" s="165"/>
-      <c r="E942" s="165"/>
+      <c r="C942" s="168"/>
+      <c r="D942" s="169"/>
+      <c r="E942" s="169"/>
     </row>
     <row r="943" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A943" s="64">
@@ -13580,9 +13586,9 @@
         <v>76</v>
       </c>
       <c r="B959" s="87"/>
-      <c r="C959" s="164"/>
-      <c r="D959" s="165"/>
-      <c r="E959" s="165"/>
+      <c r="C959" s="168"/>
+      <c r="D959" s="169"/>
+      <c r="E959" s="169"/>
     </row>
     <row r="960" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A960" s="64">
@@ -13733,9 +13739,9 @@
         <v>77</v>
       </c>
       <c r="B976" s="87"/>
-      <c r="C976" s="164"/>
-      <c r="D976" s="165"/>
-      <c r="E976" s="165"/>
+      <c r="C976" s="168"/>
+      <c r="D976" s="169"/>
+      <c r="E976" s="169"/>
     </row>
     <row r="977" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A977" s="64">
@@ -13886,9 +13892,9 @@
         <v>78</v>
       </c>
       <c r="B993" s="87"/>
-      <c r="C993" s="164"/>
-      <c r="D993" s="165"/>
-      <c r="E993" s="165"/>
+      <c r="C993" s="168"/>
+      <c r="D993" s="169"/>
+      <c r="E993" s="169"/>
     </row>
     <row r="994" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A994" s="64">
@@ -14039,9 +14045,9 @@
         <v>79</v>
       </c>
       <c r="B1010" s="87"/>
-      <c r="C1010" s="164"/>
-      <c r="D1010" s="165"/>
-      <c r="E1010" s="165"/>
+      <c r="C1010" s="168"/>
+      <c r="D1010" s="169"/>
+      <c r="E1010" s="169"/>
     </row>
     <row r="1011" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1011" s="64">
@@ -14192,9 +14198,9 @@
         <v>80</v>
       </c>
       <c r="B1027" s="87"/>
-      <c r="C1027" s="164"/>
-      <c r="D1027" s="165"/>
-      <c r="E1027" s="165"/>
+      <c r="C1027" s="168"/>
+      <c r="D1027" s="169"/>
+      <c r="E1027" s="169"/>
     </row>
     <row r="1028" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1028" s="64">
@@ -14345,9 +14351,9 @@
         <v>83</v>
       </c>
       <c r="B1044" s="87"/>
-      <c r="C1044" s="164"/>
-      <c r="D1044" s="165"/>
-      <c r="E1044" s="165"/>
+      <c r="C1044" s="168"/>
+      <c r="D1044" s="169"/>
+      <c r="E1044" s="169"/>
     </row>
     <row r="1045" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1045" s="64">
@@ -14498,9 +14504,9 @@
         <v>82</v>
       </c>
       <c r="B1061" s="87"/>
-      <c r="C1061" s="164"/>
-      <c r="D1061" s="165"/>
-      <c r="E1061" s="165"/>
+      <c r="C1061" s="168"/>
+      <c r="D1061" s="169"/>
+      <c r="E1061" s="169"/>
     </row>
     <row r="1062" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1062" s="64">
@@ -14651,9 +14657,9 @@
         <v>84</v>
       </c>
       <c r="B1078" s="87"/>
-      <c r="C1078" s="164"/>
-      <c r="D1078" s="165"/>
-      <c r="E1078" s="165"/>
+      <c r="C1078" s="168"/>
+      <c r="D1078" s="169"/>
+      <c r="E1078" s="169"/>
     </row>
     <row r="1079" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1079" s="64">
@@ -14804,18 +14810,18 @@
         <v>104</v>
       </c>
       <c r="B1095" s="40"/>
-      <c r="C1095" s="174"/>
-      <c r="D1095" s="175"/>
-      <c r="E1095" s="175"/>
+      <c r="C1095" s="178"/>
+      <c r="D1095" s="179"/>
+      <c r="E1095" s="179"/>
     </row>
     <row r="1096" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A1096" s="68" t="s">
         <v>85</v>
       </c>
       <c r="B1096" s="87"/>
-      <c r="C1096" s="164"/>
-      <c r="D1096" s="165"/>
-      <c r="E1096" s="165"/>
+      <c r="C1096" s="168"/>
+      <c r="D1096" s="169"/>
+      <c r="E1096" s="169"/>
     </row>
     <row r="1097" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1097" s="69">
@@ -14966,9 +14972,9 @@
         <v>86</v>
       </c>
       <c r="B1113" s="90"/>
-      <c r="C1113" s="166"/>
-      <c r="D1113" s="167"/>
-      <c r="E1113" s="167"/>
+      <c r="C1113" s="170"/>
+      <c r="D1113" s="171"/>
+      <c r="E1113" s="171"/>
     </row>
     <row r="1114" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1114" s="69">
@@ -15119,9 +15125,9 @@
         <v>87</v>
       </c>
       <c r="B1130" s="87"/>
-      <c r="C1130" s="164"/>
-      <c r="D1130" s="165"/>
-      <c r="E1130" s="165"/>
+      <c r="C1130" s="168"/>
+      <c r="D1130" s="169"/>
+      <c r="E1130" s="169"/>
     </row>
     <row r="1131" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1131" s="69">
@@ -15272,9 +15278,9 @@
         <v>88</v>
       </c>
       <c r="B1147" s="87"/>
-      <c r="C1147" s="164"/>
-      <c r="D1147" s="165"/>
-      <c r="E1147" s="165"/>
+      <c r="C1147" s="168"/>
+      <c r="D1147" s="169"/>
+      <c r="E1147" s="169"/>
     </row>
     <row r="1148" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1148" s="69">
@@ -15425,9 +15431,9 @@
         <v>89</v>
       </c>
       <c r="B1164" s="87"/>
-      <c r="C1164" s="164"/>
-      <c r="D1164" s="165"/>
-      <c r="E1164" s="165"/>
+      <c r="C1164" s="168"/>
+      <c r="D1164" s="169"/>
+      <c r="E1164" s="169"/>
     </row>
     <row r="1165" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1165" s="69">
@@ -15578,9 +15584,9 @@
         <v>90</v>
       </c>
       <c r="B1181" s="87"/>
-      <c r="C1181" s="164"/>
-      <c r="D1181" s="165"/>
-      <c r="E1181" s="165"/>
+      <c r="C1181" s="168"/>
+      <c r="D1181" s="169"/>
+      <c r="E1181" s="169"/>
     </row>
     <row r="1182" spans="1:5" hidden="1" outlineLevel="3">
       <c r="A1182" s="69">
@@ -15731,9 +15737,9 @@
         <v>91</v>
       </c>
       <c r="B1198" s="87"/>
-      <c r="C1198" s="164"/>
-      <c r="D1198" s="165"/>
-      <c r="E1198" s="165"/>
+      <c r="C1198" s="168"/>
+      <c r="D1198" s="169"/>
+      <c r="E1198" s="169"/>
     </row>
     <row r="1199" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1199" s="69">
@@ -15884,9 +15890,9 @@
         <v>92</v>
       </c>
       <c r="B1215" s="87"/>
-      <c r="C1215" s="164"/>
-      <c r="D1215" s="165"/>
-      <c r="E1215" s="165"/>
+      <c r="C1215" s="168"/>
+      <c r="D1215" s="169"/>
+      <c r="E1215" s="169"/>
     </row>
     <row r="1216" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1216" s="69">
@@ -16037,9 +16043,9 @@
         <v>93</v>
       </c>
       <c r="B1232" s="87"/>
-      <c r="C1232" s="164"/>
-      <c r="D1232" s="165"/>
-      <c r="E1232" s="165"/>
+      <c r="C1232" s="168"/>
+      <c r="D1232" s="169"/>
+      <c r="E1232" s="169"/>
     </row>
     <row r="1233" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1233" s="69">
@@ -16190,9 +16196,9 @@
         <v>94</v>
       </c>
       <c r="B1249" s="87"/>
-      <c r="C1249" s="164"/>
-      <c r="D1249" s="165"/>
-      <c r="E1249" s="165"/>
+      <c r="C1249" s="168"/>
+      <c r="D1249" s="169"/>
+      <c r="E1249" s="169"/>
     </row>
     <row r="1250" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1250" s="69">
@@ -16343,9 +16349,9 @@
         <v>99</v>
       </c>
       <c r="B1266" s="87"/>
-      <c r="C1266" s="164"/>
-      <c r="D1266" s="165"/>
-      <c r="E1266" s="165"/>
+      <c r="C1266" s="168"/>
+      <c r="D1266" s="169"/>
+      <c r="E1266" s="169"/>
     </row>
     <row r="1267" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1267" s="69">
@@ -16496,9 +16502,9 @@
         <v>100</v>
       </c>
       <c r="B1283" s="87"/>
-      <c r="C1283" s="164"/>
-      <c r="D1283" s="165"/>
-      <c r="E1283" s="165"/>
+      <c r="C1283" s="168"/>
+      <c r="D1283" s="169"/>
+      <c r="E1283" s="169"/>
     </row>
     <row r="1284" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1284" s="69">
@@ -16649,9 +16655,9 @@
         <v>101</v>
       </c>
       <c r="B1300" s="87"/>
-      <c r="C1300" s="164"/>
-      <c r="D1300" s="165"/>
-      <c r="E1300" s="165"/>
+      <c r="C1300" s="168"/>
+      <c r="D1300" s="169"/>
+      <c r="E1300" s="169"/>
     </row>
     <row r="1301" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1301" s="69">
@@ -16802,9 +16808,9 @@
         <v>81</v>
       </c>
       <c r="B1317" s="87"/>
-      <c r="C1317" s="164"/>
-      <c r="D1317" s="165"/>
-      <c r="E1317" s="165"/>
+      <c r="C1317" s="168"/>
+      <c r="D1317" s="169"/>
+      <c r="E1317" s="169"/>
     </row>
     <row r="1318" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1318" s="69">
@@ -16955,9 +16961,9 @@
         <v>102</v>
       </c>
       <c r="B1334" s="87"/>
-      <c r="C1334" s="164"/>
-      <c r="D1334" s="165"/>
-      <c r="E1334" s="165"/>
+      <c r="C1334" s="168"/>
+      <c r="D1334" s="169"/>
+      <c r="E1334" s="169"/>
     </row>
     <row r="1335" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1335" s="69">
@@ -17108,9 +17114,9 @@
         <v>98</v>
       </c>
       <c r="B1351" s="87"/>
-      <c r="C1351" s="164"/>
-      <c r="D1351" s="165"/>
-      <c r="E1351" s="165"/>
+      <c r="C1351" s="168"/>
+      <c r="D1351" s="169"/>
+      <c r="E1351" s="169"/>
     </row>
     <row r="1352" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1352" s="69">
@@ -17261,18 +17267,18 @@
         <v>103</v>
       </c>
       <c r="B1368" s="41"/>
-      <c r="C1368" s="172"/>
-      <c r="D1368" s="173"/>
-      <c r="E1368" s="173"/>
+      <c r="C1368" s="180"/>
+      <c r="D1368" s="181"/>
+      <c r="E1368" s="181"/>
     </row>
     <row r="1369" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A1369" s="73" t="s">
         <v>105</v>
       </c>
       <c r="B1369" s="87"/>
-      <c r="C1369" s="164"/>
-      <c r="D1369" s="165"/>
-      <c r="E1369" s="165"/>
+      <c r="C1369" s="168"/>
+      <c r="D1369" s="169"/>
+      <c r="E1369" s="169"/>
     </row>
     <row r="1370" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1370" s="74">
@@ -17423,9 +17429,9 @@
         <v>106</v>
       </c>
       <c r="B1386" s="90"/>
-      <c r="C1386" s="166"/>
-      <c r="D1386" s="167"/>
-      <c r="E1386" s="167"/>
+      <c r="C1386" s="170"/>
+      <c r="D1386" s="171"/>
+      <c r="E1386" s="171"/>
     </row>
     <row r="1387" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1387" s="74">
@@ -17576,9 +17582,9 @@
         <v>107</v>
       </c>
       <c r="B1403" s="87"/>
-      <c r="C1403" s="164"/>
-      <c r="D1403" s="165"/>
-      <c r="E1403" s="165"/>
+      <c r="C1403" s="168"/>
+      <c r="D1403" s="169"/>
+      <c r="E1403" s="169"/>
     </row>
     <row r="1404" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1404" s="74">
@@ -17729,9 +17735,9 @@
         <v>108</v>
       </c>
       <c r="B1420" s="87"/>
-      <c r="C1420" s="164"/>
-      <c r="D1420" s="165"/>
-      <c r="E1420" s="165"/>
+      <c r="C1420" s="168"/>
+      <c r="D1420" s="169"/>
+      <c r="E1420" s="169"/>
     </row>
     <row r="1421" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1421" s="74">
@@ -17882,9 +17888,9 @@
         <v>109</v>
       </c>
       <c r="B1437" s="87"/>
-      <c r="C1437" s="164"/>
-      <c r="D1437" s="165"/>
-      <c r="E1437" s="165"/>
+      <c r="C1437" s="168"/>
+      <c r="D1437" s="169"/>
+      <c r="E1437" s="169"/>
     </row>
     <row r="1438" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1438" s="74">
@@ -18035,9 +18041,9 @@
         <v>110</v>
       </c>
       <c r="B1454" s="87"/>
-      <c r="C1454" s="164"/>
-      <c r="D1454" s="165"/>
-      <c r="E1454" s="165"/>
+      <c r="C1454" s="168"/>
+      <c r="D1454" s="169"/>
+      <c r="E1454" s="169"/>
     </row>
     <row r="1455" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1455" s="74">
@@ -18188,9 +18194,9 @@
         <v>111</v>
       </c>
       <c r="B1471" s="87"/>
-      <c r="C1471" s="164"/>
-      <c r="D1471" s="165"/>
-      <c r="E1471" s="165"/>
+      <c r="C1471" s="168"/>
+      <c r="D1471" s="169"/>
+      <c r="E1471" s="169"/>
     </row>
     <row r="1472" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1472" s="74">
@@ -18341,9 +18347,9 @@
         <v>112</v>
       </c>
       <c r="B1488" s="87"/>
-      <c r="C1488" s="164"/>
-      <c r="D1488" s="165"/>
-      <c r="E1488" s="165"/>
+      <c r="C1488" s="168"/>
+      <c r="D1488" s="169"/>
+      <c r="E1488" s="169"/>
     </row>
     <row r="1489" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1489" s="74">
@@ -18494,9 +18500,9 @@
         <v>113</v>
       </c>
       <c r="B1505" s="87"/>
-      <c r="C1505" s="164"/>
-      <c r="D1505" s="165"/>
-      <c r="E1505" s="165"/>
+      <c r="C1505" s="168"/>
+      <c r="D1505" s="169"/>
+      <c r="E1505" s="169"/>
     </row>
     <row r="1506" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1506" s="74">
@@ -18647,9 +18653,9 @@
         <v>114</v>
       </c>
       <c r="B1522" s="87"/>
-      <c r="C1522" s="164"/>
-      <c r="D1522" s="165"/>
-      <c r="E1522" s="165"/>
+      <c r="C1522" s="168"/>
+      <c r="D1522" s="169"/>
+      <c r="E1522" s="169"/>
     </row>
     <row r="1523" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1523" s="74">
@@ -18800,9 +18806,9 @@
         <v>95</v>
       </c>
       <c r="B1539" s="87"/>
-      <c r="C1539" s="164"/>
-      <c r="D1539" s="165"/>
-      <c r="E1539" s="165"/>
+      <c r="C1539" s="168"/>
+      <c r="D1539" s="169"/>
+      <c r="E1539" s="169"/>
     </row>
     <row r="1540" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1540" s="74">
@@ -18953,9 +18959,9 @@
         <v>115</v>
       </c>
       <c r="B1556" s="87"/>
-      <c r="C1556" s="164"/>
-      <c r="D1556" s="165"/>
-      <c r="E1556" s="165"/>
+      <c r="C1556" s="168"/>
+      <c r="D1556" s="169"/>
+      <c r="E1556" s="169"/>
     </row>
     <row r="1557" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1557" s="74">
@@ -19106,9 +19112,9 @@
         <v>116</v>
       </c>
       <c r="B1573" s="87"/>
-      <c r="C1573" s="164"/>
-      <c r="D1573" s="165"/>
-      <c r="E1573" s="165"/>
+      <c r="C1573" s="168"/>
+      <c r="D1573" s="169"/>
+      <c r="E1573" s="169"/>
     </row>
     <row r="1574" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1574" s="74">
@@ -19259,9 +19265,9 @@
         <v>117</v>
       </c>
       <c r="B1590" s="87"/>
-      <c r="C1590" s="164"/>
-      <c r="D1590" s="165"/>
-      <c r="E1590" s="165"/>
+      <c r="C1590" s="168"/>
+      <c r="D1590" s="169"/>
+      <c r="E1590" s="169"/>
     </row>
     <row r="1591" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1591" s="74">
@@ -19412,9 +19418,9 @@
         <v>118</v>
       </c>
       <c r="B1607" s="87"/>
-      <c r="C1607" s="164"/>
-      <c r="D1607" s="165"/>
-      <c r="E1607" s="165"/>
+      <c r="C1607" s="168"/>
+      <c r="D1607" s="169"/>
+      <c r="E1607" s="169"/>
     </row>
     <row r="1608" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1608" s="74">
@@ -19565,9 +19571,9 @@
         <v>119</v>
       </c>
       <c r="B1624" s="87"/>
-      <c r="C1624" s="164"/>
-      <c r="D1624" s="165"/>
-      <c r="E1624" s="165"/>
+      <c r="C1624" s="168"/>
+      <c r="D1624" s="169"/>
+      <c r="E1624" s="169"/>
     </row>
     <row r="1625" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1625" s="74">
@@ -19718,18 +19724,18 @@
         <v>120</v>
       </c>
       <c r="B1641" s="42"/>
-      <c r="C1641" s="170"/>
-      <c r="D1641" s="171"/>
-      <c r="E1641" s="171"/>
+      <c r="C1641" s="182"/>
+      <c r="D1641" s="183"/>
+      <c r="E1641" s="183"/>
     </row>
     <row r="1642" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A1642" s="78" t="s">
         <v>121</v>
       </c>
       <c r="B1642" s="87"/>
-      <c r="C1642" s="164"/>
-      <c r="D1642" s="165"/>
-      <c r="E1642" s="165"/>
+      <c r="C1642" s="168"/>
+      <c r="D1642" s="169"/>
+      <c r="E1642" s="169"/>
     </row>
     <row r="1643" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1643" s="79">
@@ -19880,9 +19886,9 @@
         <v>122</v>
       </c>
       <c r="B1659" s="90"/>
-      <c r="C1659" s="166"/>
-      <c r="D1659" s="167"/>
-      <c r="E1659" s="167"/>
+      <c r="C1659" s="170"/>
+      <c r="D1659" s="171"/>
+      <c r="E1659" s="171"/>
     </row>
     <row r="1660" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1660" s="79">
@@ -20033,9 +20039,9 @@
         <v>123</v>
       </c>
       <c r="B1676" s="87"/>
-      <c r="C1676" s="164"/>
-      <c r="D1676" s="165"/>
-      <c r="E1676" s="165"/>
+      <c r="C1676" s="168"/>
+      <c r="D1676" s="169"/>
+      <c r="E1676" s="169"/>
     </row>
     <row r="1677" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1677" s="79">
@@ -20186,9 +20192,9 @@
         <v>124</v>
       </c>
       <c r="B1693" s="87"/>
-      <c r="C1693" s="164"/>
-      <c r="D1693" s="165"/>
-      <c r="E1693" s="165"/>
+      <c r="C1693" s="168"/>
+      <c r="D1693" s="169"/>
+      <c r="E1693" s="169"/>
     </row>
     <row r="1694" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1694" s="79">
@@ -20339,9 +20345,9 @@
         <v>125</v>
       </c>
       <c r="B1710" s="87"/>
-      <c r="C1710" s="164"/>
-      <c r="D1710" s="165"/>
-      <c r="E1710" s="165"/>
+      <c r="C1710" s="168"/>
+      <c r="D1710" s="169"/>
+      <c r="E1710" s="169"/>
     </row>
     <row r="1711" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1711" s="79">
@@ -20492,9 +20498,9 @@
         <v>126</v>
       </c>
       <c r="B1727" s="87"/>
-      <c r="C1727" s="164"/>
-      <c r="D1727" s="165"/>
-      <c r="E1727" s="165"/>
+      <c r="C1727" s="168"/>
+      <c r="D1727" s="169"/>
+      <c r="E1727" s="169"/>
     </row>
     <row r="1728" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1728" s="79">
@@ -20645,9 +20651,9 @@
         <v>127</v>
       </c>
       <c r="B1744" s="87"/>
-      <c r="C1744" s="164"/>
-      <c r="D1744" s="165"/>
-      <c r="E1744" s="165"/>
+      <c r="C1744" s="168"/>
+      <c r="D1744" s="169"/>
+      <c r="E1744" s="169"/>
     </row>
     <row r="1745" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1745" s="79">
@@ -20798,9 +20804,9 @@
         <v>128</v>
       </c>
       <c r="B1761" s="87"/>
-      <c r="C1761" s="164"/>
-      <c r="D1761" s="165"/>
-      <c r="E1761" s="165"/>
+      <c r="C1761" s="168"/>
+      <c r="D1761" s="169"/>
+      <c r="E1761" s="169"/>
     </row>
     <row r="1762" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1762" s="79">
@@ -20951,9 +20957,9 @@
         <v>129</v>
       </c>
       <c r="B1778" s="87"/>
-      <c r="C1778" s="164"/>
-      <c r="D1778" s="165"/>
-      <c r="E1778" s="165"/>
+      <c r="C1778" s="168"/>
+      <c r="D1778" s="169"/>
+      <c r="E1778" s="169"/>
     </row>
     <row r="1779" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1779" s="79">
@@ -21104,9 +21110,9 @@
         <v>130</v>
       </c>
       <c r="B1795" s="87"/>
-      <c r="C1795" s="164"/>
-      <c r="D1795" s="165"/>
-      <c r="E1795" s="165"/>
+      <c r="C1795" s="168"/>
+      <c r="D1795" s="169"/>
+      <c r="E1795" s="169"/>
     </row>
     <row r="1796" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1796" s="79">
@@ -21257,9 +21263,9 @@
         <v>131</v>
       </c>
       <c r="B1812" s="87"/>
-      <c r="C1812" s="164"/>
-      <c r="D1812" s="165"/>
-      <c r="E1812" s="165"/>
+      <c r="C1812" s="168"/>
+      <c r="D1812" s="169"/>
+      <c r="E1812" s="169"/>
     </row>
     <row r="1813" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1813" s="79">
@@ -21410,9 +21416,9 @@
         <v>96</v>
       </c>
       <c r="B1829" s="87"/>
-      <c r="C1829" s="164"/>
-      <c r="D1829" s="165"/>
-      <c r="E1829" s="165"/>
+      <c r="C1829" s="168"/>
+      <c r="D1829" s="169"/>
+      <c r="E1829" s="169"/>
     </row>
     <row r="1830" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1830" s="79">
@@ -21563,9 +21569,9 @@
         <v>132</v>
       </c>
       <c r="B1846" s="87"/>
-      <c r="C1846" s="164"/>
-      <c r="D1846" s="165"/>
-      <c r="E1846" s="165"/>
+      <c r="C1846" s="168"/>
+      <c r="D1846" s="169"/>
+      <c r="E1846" s="169"/>
     </row>
     <row r="1847" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1847" s="79">
@@ -21716,9 +21722,9 @@
         <v>133</v>
       </c>
       <c r="B1863" s="87"/>
-      <c r="C1863" s="164"/>
-      <c r="D1863" s="165"/>
-      <c r="E1863" s="165"/>
+      <c r="C1863" s="168"/>
+      <c r="D1863" s="169"/>
+      <c r="E1863" s="169"/>
     </row>
     <row r="1864" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1864" s="79">
@@ -21869,9 +21875,9 @@
         <v>134</v>
       </c>
       <c r="B1880" s="87"/>
-      <c r="C1880" s="164"/>
-      <c r="D1880" s="165"/>
-      <c r="E1880" s="165"/>
+      <c r="C1880" s="168"/>
+      <c r="D1880" s="169"/>
+      <c r="E1880" s="169"/>
     </row>
     <row r="1881" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1881" s="79">
@@ -22022,9 +22028,9 @@
         <v>135</v>
       </c>
       <c r="B1897" s="87"/>
-      <c r="C1897" s="164"/>
-      <c r="D1897" s="165"/>
-      <c r="E1897" s="165"/>
+      <c r="C1897" s="168"/>
+      <c r="D1897" s="169"/>
+      <c r="E1897" s="169"/>
     </row>
     <row r="1898" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1898" s="79">
@@ -22175,18 +22181,18 @@
         <v>136</v>
       </c>
       <c r="B1914" s="43"/>
-      <c r="C1914" s="168"/>
-      <c r="D1914" s="169"/>
-      <c r="E1914" s="169"/>
+      <c r="C1914" s="184"/>
+      <c r="D1914" s="185"/>
+      <c r="E1914" s="185"/>
     </row>
     <row r="1915" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A1915" s="83" t="s">
         <v>137</v>
       </c>
       <c r="B1915" s="87"/>
-      <c r="C1915" s="164"/>
-      <c r="D1915" s="165"/>
-      <c r="E1915" s="165"/>
+      <c r="C1915" s="168"/>
+      <c r="D1915" s="169"/>
+      <c r="E1915" s="169"/>
     </row>
     <row r="1916" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1916" s="84">
@@ -22337,9 +22343,9 @@
         <v>138</v>
       </c>
       <c r="B1932" s="90"/>
-      <c r="C1932" s="166"/>
-      <c r="D1932" s="167"/>
-      <c r="E1932" s="167"/>
+      <c r="C1932" s="170"/>
+      <c r="D1932" s="171"/>
+      <c r="E1932" s="171"/>
     </row>
     <row r="1933" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1933" s="84">
@@ -22490,9 +22496,9 @@
         <v>139</v>
       </c>
       <c r="B1949" s="87"/>
-      <c r="C1949" s="164"/>
-      <c r="D1949" s="165"/>
-      <c r="E1949" s="165"/>
+      <c r="C1949" s="168"/>
+      <c r="D1949" s="169"/>
+      <c r="E1949" s="169"/>
     </row>
     <row r="1950" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1950" s="84">
@@ -22643,9 +22649,9 @@
         <v>140</v>
       </c>
       <c r="B1966" s="87"/>
-      <c r="C1966" s="164"/>
-      <c r="D1966" s="165"/>
-      <c r="E1966" s="165"/>
+      <c r="C1966" s="168"/>
+      <c r="D1966" s="169"/>
+      <c r="E1966" s="169"/>
     </row>
     <row r="1967" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1967" s="84">
@@ -22796,9 +22802,9 @@
         <v>141</v>
       </c>
       <c r="B1983" s="87"/>
-      <c r="C1983" s="164"/>
-      <c r="D1983" s="165"/>
-      <c r="E1983" s="165"/>
+      <c r="C1983" s="168"/>
+      <c r="D1983" s="169"/>
+      <c r="E1983" s="169"/>
     </row>
     <row r="1984" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1984" s="84">
@@ -22949,9 +22955,9 @@
         <v>142</v>
       </c>
       <c r="B2000" s="87"/>
-      <c r="C2000" s="164"/>
-      <c r="D2000" s="165"/>
-      <c r="E2000" s="165"/>
+      <c r="C2000" s="168"/>
+      <c r="D2000" s="169"/>
+      <c r="E2000" s="169"/>
     </row>
     <row r="2001" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2001" s="84">
@@ -23102,9 +23108,9 @@
         <v>143</v>
       </c>
       <c r="B2017" s="87"/>
-      <c r="C2017" s="164"/>
-      <c r="D2017" s="165"/>
-      <c r="E2017" s="165"/>
+      <c r="C2017" s="168"/>
+      <c r="D2017" s="169"/>
+      <c r="E2017" s="169"/>
     </row>
     <row r="2018" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2018" s="84">
@@ -23255,9 +23261,9 @@
         <v>144</v>
       </c>
       <c r="B2034" s="87"/>
-      <c r="C2034" s="164"/>
-      <c r="D2034" s="165"/>
-      <c r="E2034" s="165"/>
+      <c r="C2034" s="168"/>
+      <c r="D2034" s="169"/>
+      <c r="E2034" s="169"/>
     </row>
     <row r="2035" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2035" s="84">
@@ -23408,9 +23414,9 @@
         <v>145</v>
       </c>
       <c r="B2051" s="87"/>
-      <c r="C2051" s="164"/>
-      <c r="D2051" s="165"/>
-      <c r="E2051" s="165"/>
+      <c r="C2051" s="168"/>
+      <c r="D2051" s="169"/>
+      <c r="E2051" s="169"/>
     </row>
     <row r="2052" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2052" s="84">
@@ -23561,9 +23567,9 @@
         <v>146</v>
       </c>
       <c r="B2068" s="87"/>
-      <c r="C2068" s="164"/>
-      <c r="D2068" s="165"/>
-      <c r="E2068" s="165"/>
+      <c r="C2068" s="168"/>
+      <c r="D2068" s="169"/>
+      <c r="E2068" s="169"/>
     </row>
     <row r="2069" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2069" s="84">
@@ -23714,9 +23720,9 @@
         <v>147</v>
       </c>
       <c r="B2085" s="87"/>
-      <c r="C2085" s="164"/>
-      <c r="D2085" s="165"/>
-      <c r="E2085" s="165"/>
+      <c r="C2085" s="168"/>
+      <c r="D2085" s="169"/>
+      <c r="E2085" s="169"/>
     </row>
     <row r="2086" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2086" s="84">
@@ -23867,9 +23873,9 @@
         <v>148</v>
       </c>
       <c r="B2102" s="87"/>
-      <c r="C2102" s="164"/>
-      <c r="D2102" s="165"/>
-      <c r="E2102" s="165"/>
+      <c r="C2102" s="168"/>
+      <c r="D2102" s="169"/>
+      <c r="E2102" s="169"/>
     </row>
     <row r="2103" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2103" s="84">
@@ -24020,9 +24026,9 @@
         <v>97</v>
       </c>
       <c r="B2119" s="87"/>
-      <c r="C2119" s="164"/>
-      <c r="D2119" s="165"/>
-      <c r="E2119" s="165"/>
+      <c r="C2119" s="168"/>
+      <c r="D2119" s="169"/>
+      <c r="E2119" s="169"/>
     </row>
     <row r="2120" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2120" s="84">
@@ -24173,9 +24179,9 @@
         <v>149</v>
       </c>
       <c r="B2136" s="87"/>
-      <c r="C2136" s="164"/>
-      <c r="D2136" s="165"/>
-      <c r="E2136" s="165"/>
+      <c r="C2136" s="168"/>
+      <c r="D2136" s="169"/>
+      <c r="E2136" s="169"/>
     </row>
     <row r="2137" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2137" s="84">
@@ -24326,9 +24332,9 @@
         <v>150</v>
       </c>
       <c r="B2153" s="87"/>
-      <c r="C2153" s="164"/>
-      <c r="D2153" s="165"/>
-      <c r="E2153" s="165"/>
+      <c r="C2153" s="168"/>
+      <c r="D2153" s="169"/>
+      <c r="E2153" s="169"/>
     </row>
     <row r="2154" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2154" s="84">
@@ -24479,9 +24485,9 @@
         <v>151</v>
       </c>
       <c r="B2170" s="87"/>
-      <c r="C2170" s="164"/>
-      <c r="D2170" s="165"/>
-      <c r="E2170" s="165"/>
+      <c r="C2170" s="168"/>
+      <c r="D2170" s="169"/>
+      <c r="E2170" s="169"/>
     </row>
     <row r="2171" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2171" s="84">
@@ -24629,26 +24635,111 @@
     </row>
   </sheetData>
   <mergeCells count="137">
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="C89:E89"/>
-    <mergeCell ref="C21:E21"/>
-    <mergeCell ref="C38:E38"/>
-    <mergeCell ref="C55:E55"/>
-    <mergeCell ref="C72:E72"/>
-    <mergeCell ref="C208:E208"/>
-    <mergeCell ref="C225:E225"/>
-    <mergeCell ref="C242:E242"/>
-    <mergeCell ref="C259:E259"/>
-    <mergeCell ref="C276:E276"/>
-    <mergeCell ref="C277:E277"/>
-    <mergeCell ref="C106:E106"/>
-    <mergeCell ref="C123:E123"/>
-    <mergeCell ref="C140:E140"/>
-    <mergeCell ref="C157:E157"/>
-    <mergeCell ref="C174:E174"/>
-    <mergeCell ref="C191:E191"/>
+    <mergeCell ref="C2034:E2034"/>
+    <mergeCell ref="C2051:E2051"/>
+    <mergeCell ref="C2068:E2068"/>
+    <mergeCell ref="C2085:E2085"/>
+    <mergeCell ref="C2170:E2170"/>
+    <mergeCell ref="C2102:E2102"/>
+    <mergeCell ref="C2119:E2119"/>
+    <mergeCell ref="C2136:E2136"/>
+    <mergeCell ref="C2153:E2153"/>
+    <mergeCell ref="C1932:E1932"/>
+    <mergeCell ref="C1949:E1949"/>
+    <mergeCell ref="C1966:E1966"/>
+    <mergeCell ref="C1983:E1983"/>
+    <mergeCell ref="C2000:E2000"/>
+    <mergeCell ref="C2017:E2017"/>
+    <mergeCell ref="C1846:E1846"/>
+    <mergeCell ref="C1863:E1863"/>
+    <mergeCell ref="C1880:E1880"/>
+    <mergeCell ref="C1897:E1897"/>
+    <mergeCell ref="C1914:E1914"/>
+    <mergeCell ref="C1915:E1915"/>
+    <mergeCell ref="C1744:E1744"/>
+    <mergeCell ref="C1761:E1761"/>
+    <mergeCell ref="C1778:E1778"/>
+    <mergeCell ref="C1795:E1795"/>
+    <mergeCell ref="C1812:E1812"/>
+    <mergeCell ref="C1829:E1829"/>
+    <mergeCell ref="C1642:E1642"/>
+    <mergeCell ref="C1659:E1659"/>
+    <mergeCell ref="C1676:E1676"/>
+    <mergeCell ref="C1693:E1693"/>
+    <mergeCell ref="C1710:E1710"/>
+    <mergeCell ref="C1727:E1727"/>
+    <mergeCell ref="C1556:E1556"/>
+    <mergeCell ref="C1573:E1573"/>
+    <mergeCell ref="C1590:E1590"/>
+    <mergeCell ref="C1607:E1607"/>
+    <mergeCell ref="C1624:E1624"/>
+    <mergeCell ref="C1641:E1641"/>
+    <mergeCell ref="C1454:E1454"/>
+    <mergeCell ref="C1471:E1471"/>
+    <mergeCell ref="C1488:E1488"/>
+    <mergeCell ref="C1505:E1505"/>
+    <mergeCell ref="C1522:E1522"/>
+    <mergeCell ref="C1539:E1539"/>
+    <mergeCell ref="C1368:E1368"/>
+    <mergeCell ref="C1369:E1369"/>
+    <mergeCell ref="C1386:E1386"/>
+    <mergeCell ref="C1403:E1403"/>
+    <mergeCell ref="C1420:E1420"/>
+    <mergeCell ref="C1437:E1437"/>
+    <mergeCell ref="C1266:E1266"/>
+    <mergeCell ref="C1283:E1283"/>
+    <mergeCell ref="C1300:E1300"/>
+    <mergeCell ref="C1317:E1317"/>
+    <mergeCell ref="C1334:E1334"/>
+    <mergeCell ref="C1351:E1351"/>
+    <mergeCell ref="C1164:E1164"/>
+    <mergeCell ref="C1181:E1181"/>
+    <mergeCell ref="C1198:E1198"/>
+    <mergeCell ref="C1215:E1215"/>
+    <mergeCell ref="C1232:E1232"/>
+    <mergeCell ref="C1249:E1249"/>
+    <mergeCell ref="C1078:E1078"/>
+    <mergeCell ref="C1095:E1095"/>
+    <mergeCell ref="C1096:E1096"/>
+    <mergeCell ref="C1113:E1113"/>
+    <mergeCell ref="C1130:E1130"/>
+    <mergeCell ref="C1147:E1147"/>
+    <mergeCell ref="C976:E976"/>
+    <mergeCell ref="C993:E993"/>
+    <mergeCell ref="C1010:E1010"/>
+    <mergeCell ref="C1027:E1027"/>
+    <mergeCell ref="C1044:E1044"/>
+    <mergeCell ref="C1061:E1061"/>
+    <mergeCell ref="C874:E874"/>
+    <mergeCell ref="C891:E891"/>
+    <mergeCell ref="C908:E908"/>
+    <mergeCell ref="C925:E925"/>
+    <mergeCell ref="C942:E942"/>
+    <mergeCell ref="C959:E959"/>
+    <mergeCell ref="C788:E788"/>
+    <mergeCell ref="C805:E805"/>
+    <mergeCell ref="C822:E822"/>
+    <mergeCell ref="C823:E823"/>
+    <mergeCell ref="C840:E840"/>
+    <mergeCell ref="C857:E857"/>
+    <mergeCell ref="C686:E686"/>
+    <mergeCell ref="C703:E703"/>
+    <mergeCell ref="C720:E720"/>
+    <mergeCell ref="C737:E737"/>
+    <mergeCell ref="C754:E754"/>
+    <mergeCell ref="C771:E771"/>
+    <mergeCell ref="C584:E584"/>
+    <mergeCell ref="C601:E601"/>
+    <mergeCell ref="C618:E618"/>
+    <mergeCell ref="C635:E635"/>
+    <mergeCell ref="C652:E652"/>
+    <mergeCell ref="C669:E669"/>
+    <mergeCell ref="C498:E498"/>
+    <mergeCell ref="C515:E515"/>
+    <mergeCell ref="C532:E532"/>
+    <mergeCell ref="C549:E549"/>
+    <mergeCell ref="C550:E550"/>
+    <mergeCell ref="C567:E567"/>
     <mergeCell ref="C396:E396"/>
     <mergeCell ref="C413:E413"/>
     <mergeCell ref="C430:E430"/>
@@ -24661,111 +24752,26 @@
     <mergeCell ref="C345:E345"/>
     <mergeCell ref="C362:E362"/>
     <mergeCell ref="C379:E379"/>
-    <mergeCell ref="C584:E584"/>
-    <mergeCell ref="C601:E601"/>
-    <mergeCell ref="C618:E618"/>
-    <mergeCell ref="C635:E635"/>
-    <mergeCell ref="C652:E652"/>
-    <mergeCell ref="C669:E669"/>
-    <mergeCell ref="C498:E498"/>
-    <mergeCell ref="C515:E515"/>
-    <mergeCell ref="C532:E532"/>
-    <mergeCell ref="C549:E549"/>
-    <mergeCell ref="C550:E550"/>
-    <mergeCell ref="C567:E567"/>
-    <mergeCell ref="C788:E788"/>
-    <mergeCell ref="C805:E805"/>
-    <mergeCell ref="C822:E822"/>
-    <mergeCell ref="C823:E823"/>
-    <mergeCell ref="C840:E840"/>
-    <mergeCell ref="C857:E857"/>
-    <mergeCell ref="C686:E686"/>
-    <mergeCell ref="C703:E703"/>
-    <mergeCell ref="C720:E720"/>
-    <mergeCell ref="C737:E737"/>
-    <mergeCell ref="C754:E754"/>
-    <mergeCell ref="C771:E771"/>
-    <mergeCell ref="C976:E976"/>
-    <mergeCell ref="C993:E993"/>
-    <mergeCell ref="C1010:E1010"/>
-    <mergeCell ref="C1027:E1027"/>
-    <mergeCell ref="C1044:E1044"/>
-    <mergeCell ref="C1061:E1061"/>
-    <mergeCell ref="C874:E874"/>
-    <mergeCell ref="C891:E891"/>
-    <mergeCell ref="C908:E908"/>
-    <mergeCell ref="C925:E925"/>
-    <mergeCell ref="C942:E942"/>
-    <mergeCell ref="C959:E959"/>
-    <mergeCell ref="C1164:E1164"/>
-    <mergeCell ref="C1181:E1181"/>
-    <mergeCell ref="C1198:E1198"/>
-    <mergeCell ref="C1215:E1215"/>
-    <mergeCell ref="C1232:E1232"/>
-    <mergeCell ref="C1249:E1249"/>
-    <mergeCell ref="C1078:E1078"/>
-    <mergeCell ref="C1095:E1095"/>
-    <mergeCell ref="C1096:E1096"/>
-    <mergeCell ref="C1113:E1113"/>
-    <mergeCell ref="C1130:E1130"/>
-    <mergeCell ref="C1147:E1147"/>
-    <mergeCell ref="C1368:E1368"/>
-    <mergeCell ref="C1369:E1369"/>
-    <mergeCell ref="C1386:E1386"/>
-    <mergeCell ref="C1403:E1403"/>
-    <mergeCell ref="C1420:E1420"/>
-    <mergeCell ref="C1437:E1437"/>
-    <mergeCell ref="C1266:E1266"/>
-    <mergeCell ref="C1283:E1283"/>
-    <mergeCell ref="C1300:E1300"/>
-    <mergeCell ref="C1317:E1317"/>
-    <mergeCell ref="C1334:E1334"/>
-    <mergeCell ref="C1351:E1351"/>
-    <mergeCell ref="C1556:E1556"/>
-    <mergeCell ref="C1573:E1573"/>
-    <mergeCell ref="C1590:E1590"/>
-    <mergeCell ref="C1607:E1607"/>
-    <mergeCell ref="C1624:E1624"/>
-    <mergeCell ref="C1641:E1641"/>
-    <mergeCell ref="C1454:E1454"/>
-    <mergeCell ref="C1471:E1471"/>
-    <mergeCell ref="C1488:E1488"/>
-    <mergeCell ref="C1505:E1505"/>
-    <mergeCell ref="C1522:E1522"/>
-    <mergeCell ref="C1539:E1539"/>
-    <mergeCell ref="C1744:E1744"/>
-    <mergeCell ref="C1761:E1761"/>
-    <mergeCell ref="C1778:E1778"/>
-    <mergeCell ref="C1795:E1795"/>
-    <mergeCell ref="C1812:E1812"/>
-    <mergeCell ref="C1829:E1829"/>
-    <mergeCell ref="C1642:E1642"/>
-    <mergeCell ref="C1659:E1659"/>
-    <mergeCell ref="C1676:E1676"/>
-    <mergeCell ref="C1693:E1693"/>
-    <mergeCell ref="C1710:E1710"/>
-    <mergeCell ref="C1727:E1727"/>
-    <mergeCell ref="C1932:E1932"/>
-    <mergeCell ref="C1949:E1949"/>
-    <mergeCell ref="C1966:E1966"/>
-    <mergeCell ref="C1983:E1983"/>
-    <mergeCell ref="C2000:E2000"/>
-    <mergeCell ref="C2017:E2017"/>
-    <mergeCell ref="C1846:E1846"/>
-    <mergeCell ref="C1863:E1863"/>
-    <mergeCell ref="C1880:E1880"/>
-    <mergeCell ref="C1897:E1897"/>
-    <mergeCell ref="C1914:E1914"/>
-    <mergeCell ref="C1915:E1915"/>
-    <mergeCell ref="C2034:E2034"/>
-    <mergeCell ref="C2051:E2051"/>
-    <mergeCell ref="C2068:E2068"/>
-    <mergeCell ref="C2085:E2085"/>
-    <mergeCell ref="C2170:E2170"/>
-    <mergeCell ref="C2102:E2102"/>
-    <mergeCell ref="C2119:E2119"/>
-    <mergeCell ref="C2136:E2136"/>
-    <mergeCell ref="C2153:E2153"/>
+    <mergeCell ref="C225:E225"/>
+    <mergeCell ref="C242:E242"/>
+    <mergeCell ref="C259:E259"/>
+    <mergeCell ref="C276:E276"/>
+    <mergeCell ref="C277:E277"/>
+    <mergeCell ref="C106:E106"/>
+    <mergeCell ref="C123:E123"/>
+    <mergeCell ref="C140:E140"/>
+    <mergeCell ref="C157:E157"/>
+    <mergeCell ref="C174:E174"/>
+    <mergeCell ref="C191:E191"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="C89:E89"/>
+    <mergeCell ref="C21:E21"/>
+    <mergeCell ref="C38:E38"/>
+    <mergeCell ref="C55:E55"/>
+    <mergeCell ref="C72:E72"/>
+    <mergeCell ref="C208:E208"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -24792,51 +24798,51 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="24" thickBot="1">
-      <c r="A1" s="191" t="s">
+      <c r="A1" s="192" t="s">
         <v>156</v>
       </c>
-      <c r="B1" s="191"/>
-      <c r="C1" s="191"/>
-      <c r="D1" s="191"/>
-      <c r="E1" s="191"/>
-      <c r="F1" s="191"/>
-      <c r="G1" s="191"/>
-      <c r="H1" s="191"/>
-      <c r="I1" s="191"/>
-      <c r="J1" s="191"/>
-      <c r="K1" s="191"/>
-      <c r="L1" s="191"/>
+      <c r="B1" s="192"/>
+      <c r="C1" s="192"/>
+      <c r="D1" s="192"/>
+      <c r="E1" s="192"/>
+      <c r="F1" s="192"/>
+      <c r="G1" s="192"/>
+      <c r="H1" s="192"/>
+      <c r="I1" s="192"/>
+      <c r="J1" s="192"/>
+      <c r="K1" s="192"/>
+      <c r="L1" s="192"/>
     </row>
     <row r="2" spans="1:12" ht="18.75" thickBot="1">
-      <c r="A2" s="188" t="s">
+      <c r="A2" s="189" t="s">
         <v>157</v>
       </c>
-      <c r="B2" s="189"/>
-      <c r="C2" s="189"/>
-      <c r="D2" s="189"/>
-      <c r="E2" s="189"/>
-      <c r="F2" s="189"/>
-      <c r="G2" s="189"/>
-      <c r="H2" s="189"/>
-      <c r="I2" s="189"/>
-      <c r="J2" s="189"/>
-      <c r="K2" s="189"/>
-      <c r="L2" s="190"/>
+      <c r="B2" s="190"/>
+      <c r="C2" s="190"/>
+      <c r="D2" s="190"/>
+      <c r="E2" s="190"/>
+      <c r="F2" s="190"/>
+      <c r="G2" s="190"/>
+      <c r="H2" s="190"/>
+      <c r="I2" s="190"/>
+      <c r="J2" s="190"/>
+      <c r="K2" s="190"/>
+      <c r="L2" s="191"/>
     </row>
     <row r="3" spans="1:12" s="31" customFormat="1" ht="16.5" customHeight="1" thickBot="1">
-      <c r="A3" s="185" t="s">
+      <c r="A3" s="186" t="s">
         <v>158</v>
       </c>
-      <c r="B3" s="186"/>
-      <c r="C3" s="186"/>
-      <c r="D3" s="186"/>
-      <c r="E3" s="186"/>
-      <c r="F3" s="186"/>
-      <c r="G3" s="186"/>
-      <c r="H3" s="186"/>
-      <c r="I3" s="186"/>
-      <c r="J3" s="186"/>
-      <c r="K3" s="187"/>
+      <c r="B3" s="187"/>
+      <c r="C3" s="187"/>
+      <c r="D3" s="187"/>
+      <c r="E3" s="187"/>
+      <c r="F3" s="187"/>
+      <c r="G3" s="187"/>
+      <c r="H3" s="187"/>
+      <c r="I3" s="187"/>
+      <c r="J3" s="187"/>
+      <c r="K3" s="188"/>
     </row>
     <row r="4" spans="1:12" s="27" customFormat="1">
       <c r="A4" s="28" t="s">
@@ -25053,19 +25059,19 @@
       <c r="K19" s="2"/>
     </row>
     <row r="20" spans="1:11" ht="18" customHeight="1" thickBot="1">
-      <c r="A20" s="185" t="s">
+      <c r="A20" s="186" t="s">
         <v>166</v>
       </c>
-      <c r="B20" s="186"/>
-      <c r="C20" s="186"/>
-      <c r="D20" s="186"/>
-      <c r="E20" s="186"/>
-      <c r="F20" s="186"/>
-      <c r="G20" s="186"/>
-      <c r="H20" s="186"/>
-      <c r="I20" s="186"/>
-      <c r="J20" s="186"/>
-      <c r="K20" s="187"/>
+      <c r="B20" s="187"/>
+      <c r="C20" s="187"/>
+      <c r="D20" s="187"/>
+      <c r="E20" s="187"/>
+      <c r="F20" s="187"/>
+      <c r="G20" s="187"/>
+      <c r="H20" s="187"/>
+      <c r="I20" s="187"/>
+      <c r="J20" s="187"/>
+      <c r="K20" s="188"/>
     </row>
     <row r="21" spans="1:11">
       <c r="A21" s="28" t="s">
@@ -25282,19 +25288,19 @@
       <c r="K36" s="2"/>
     </row>
     <row r="37" spans="1:11" ht="18" customHeight="1" thickBot="1">
-      <c r="A37" s="185" t="s">
+      <c r="A37" s="186" t="s">
         <v>167</v>
       </c>
-      <c r="B37" s="186"/>
-      <c r="C37" s="186"/>
-      <c r="D37" s="186"/>
-      <c r="E37" s="186"/>
-      <c r="F37" s="186"/>
-      <c r="G37" s="186"/>
-      <c r="H37" s="186"/>
-      <c r="I37" s="186"/>
-      <c r="J37" s="186"/>
-      <c r="K37" s="187"/>
+      <c r="B37" s="187"/>
+      <c r="C37" s="187"/>
+      <c r="D37" s="187"/>
+      <c r="E37" s="187"/>
+      <c r="F37" s="187"/>
+      <c r="G37" s="187"/>
+      <c r="H37" s="187"/>
+      <c r="I37" s="187"/>
+      <c r="J37" s="187"/>
+      <c r="K37" s="188"/>
     </row>
     <row r="38" spans="1:11">
       <c r="A38" s="28" t="s">
@@ -25552,28 +25558,28 @@
       </c>
     </row>
     <row r="3" spans="1:1">
-      <c r="A3" s="192"/>
+      <c r="A3" s="193"/>
     </row>
     <row r="4" spans="1:1">
-      <c r="A4" s="193"/>
+      <c r="A4" s="194"/>
     </row>
     <row r="5" spans="1:1">
-      <c r="A5" s="193"/>
+      <c r="A5" s="194"/>
     </row>
     <row r="6" spans="1:1">
-      <c r="A6" s="193"/>
+      <c r="A6" s="194"/>
     </row>
     <row r="7" spans="1:1">
-      <c r="A7" s="193"/>
+      <c r="A7" s="194"/>
     </row>
     <row r="8" spans="1:1">
-      <c r="A8" s="193"/>
+      <c r="A8" s="194"/>
     </row>
     <row r="9" spans="1:1">
-      <c r="A9" s="193"/>
+      <c r="A9" s="194"/>
     </row>
     <row r="10" spans="1:1" ht="13.5" thickBot="1">
-      <c r="A10" s="194"/>
+      <c r="A10" s="195"/>
     </row>
     <row r="11" spans="1:1" ht="27" customHeight="1">
       <c r="A11" s="22" t="s">
@@ -25756,10 +25762,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="4" customFormat="1" ht="25.5" customHeight="1" thickBot="1">
-      <c r="B1" s="195" t="s">
+      <c r="B1" s="196" t="s">
         <v>162</v>
       </c>
-      <c r="C1" s="196"/>
+      <c r="C1" s="197"/>
       <c r="D1" s="92"/>
       <c r="E1" s="32"/>
     </row>
@@ -25770,7 +25776,7 @@
       <c r="E2" s="119"/>
     </row>
     <row r="3" spans="1:5" ht="12.75" customHeight="1">
-      <c r="A3" s="197" t="s">
+      <c r="A3" s="198" t="s">
         <v>202</v>
       </c>
       <c r="B3" s="131" t="s">
@@ -25784,7 +25790,7 @@
       <c r="E3" s="5"/>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="198"/>
+      <c r="A4" s="199"/>
       <c r="B4" s="128" t="s">
         <v>159</v>
       </c>
@@ -25796,7 +25802,7 @@
       <c r="E4" s="5"/>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="198"/>
+      <c r="A5" s="199"/>
       <c r="B5" s="128" t="s">
         <v>160</v>
       </c>
@@ -25805,7 +25811,7 @@
       <c r="E5" s="5"/>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="198"/>
+      <c r="A6" s="199"/>
       <c r="B6" s="139" t="s">
         <v>204</v>
       </c>
@@ -25817,7 +25823,7 @@
       <c r="E6" s="5"/>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="198"/>
+      <c r="A7" s="199"/>
       <c r="B7" s="128" t="s">
         <v>171</v>
       </c>
@@ -25829,7 +25835,7 @@
       <c r="E7" s="5"/>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="198"/>
+      <c r="A8" s="199"/>
       <c r="B8" s="128" t="s">
         <v>172</v>
       </c>
@@ -25838,7 +25844,7 @@
       <c r="E8" s="5"/>
     </row>
     <row r="9" spans="1:5" ht="13.5" thickBot="1">
-      <c r="A9" s="199"/>
+      <c r="A9" s="200"/>
       <c r="B9" s="136" t="s">
         <v>161</v>
       </c>
@@ -25853,7 +25859,7 @@
       <c r="E10" s="94"/>
     </row>
     <row r="11" spans="1:5" ht="19.5" customHeight="1">
-      <c r="A11" s="197" t="s">
+      <c r="A11" s="198" t="s">
         <v>203</v>
       </c>
       <c r="B11" s="131" t="s">
@@ -25867,7 +25873,7 @@
       <c r="E11" s="5"/>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="198"/>
+      <c r="A12" s="199"/>
       <c r="B12" s="128" t="s">
         <v>159</v>
       </c>
@@ -25879,7 +25885,7 @@
       <c r="E12" s="5"/>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" s="198"/>
+      <c r="A13" s="199"/>
       <c r="B13" s="128" t="s">
         <v>160</v>
       </c>
@@ -25888,7 +25894,7 @@
       <c r="E13" s="5"/>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="198"/>
+      <c r="A14" s="199"/>
       <c r="B14" s="139" t="s">
         <v>204</v>
       </c>
@@ -25900,7 +25906,7 @@
       <c r="E14" s="5"/>
     </row>
     <row r="15" spans="1:5">
-      <c r="A15" s="198"/>
+      <c r="A15" s="199"/>
       <c r="B15" s="128" t="s">
         <v>171</v>
       </c>
@@ -25912,7 +25918,7 @@
       <c r="E15" s="5"/>
     </row>
     <row r="16" spans="1:5">
-      <c r="A16" s="198"/>
+      <c r="A16" s="199"/>
       <c r="B16" s="128" t="s">
         <v>172</v>
       </c>
@@ -25921,7 +25927,7 @@
       <c r="E16" s="5"/>
     </row>
     <row r="17" spans="1:5" ht="13.5" thickBot="1">
-      <c r="A17" s="199"/>
+      <c r="A17" s="200"/>
       <c r="B17" s="136" t="s">
         <v>161</v>
       </c>
@@ -25936,7 +25942,7 @@
       <c r="E18" s="94"/>
     </row>
     <row r="19" spans="1:5" collapsed="1">
-      <c r="A19" s="197" t="s">
+      <c r="A19" s="198" t="s">
         <v>203</v>
       </c>
       <c r="B19" s="131" t="s">
@@ -25945,7 +25951,7 @@
       <c r="C19" s="130"/>
     </row>
     <row r="20" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A20" s="198"/>
+      <c r="A20" s="199"/>
       <c r="B20" s="128" t="s">
         <v>159</v>
       </c>
@@ -25955,14 +25961,14 @@
       </c>
     </row>
     <row r="21" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A21" s="198"/>
+      <c r="A21" s="199"/>
       <c r="B21" s="128" t="s">
         <v>160</v>
       </c>
       <c r="C21" s="133"/>
     </row>
     <row r="22" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A22" s="198"/>
+      <c r="A22" s="199"/>
       <c r="B22" s="139" t="s">
         <v>204</v>
       </c>
@@ -25972,7 +25978,7 @@
       </c>
     </row>
     <row r="23" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A23" s="198"/>
+      <c r="A23" s="199"/>
       <c r="B23" s="128" t="s">
         <v>171</v>
       </c>
@@ -25982,14 +25988,14 @@
       </c>
     </row>
     <row r="24" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A24" s="198"/>
+      <c r="A24" s="199"/>
       <c r="B24" s="128" t="s">
         <v>172</v>
       </c>
       <c r="C24" s="132"/>
     </row>
     <row r="25" spans="1:5" ht="13.5" thickBot="1">
-      <c r="A25" s="199"/>
+      <c r="A25" s="200"/>
       <c r="B25" s="136" t="s">
         <v>161</v>
       </c>
@@ -26024,163 +26030,150 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="33">
-      <c r="A1" s="209" t="s">
+      <c r="A1" s="211" t="s">
         <v>184</v>
       </c>
-      <c r="B1" s="210"/>
+      <c r="B1" s="212"/>
       <c r="C1" s="118"/>
       <c r="D1" s="5"/>
       <c r="E1" s="5"/>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="206" t="s">
+      <c r="A2" s="217" t="s">
         <v>183</v>
       </c>
-      <c r="B2" s="207"/>
+      <c r="B2" s="218"/>
       <c r="C2" s="120"/>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="208" t="s">
+      <c r="A3" s="219" t="s">
         <v>185</v>
       </c>
-      <c r="B3" s="207"/>
+      <c r="B3" s="218"/>
       <c r="C3" s="120"/>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="213"/>
-      <c r="B4" s="214"/>
+      <c r="A4" s="215"/>
+      <c r="B4" s="216"/>
       <c r="C4" s="120"/>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="211" t="s">
+      <c r="A5" s="213" t="s">
         <v>194</v>
       </c>
-      <c r="B5" s="212"/>
+      <c r="B5" s="214"/>
       <c r="C5" s="120"/>
     </row>
     <row r="7" spans="1:5" ht="18.75">
-      <c r="A7" s="217" t="s">
+      <c r="A7" s="205" t="s">
         <v>186</v>
       </c>
-      <c r="B7" s="218"/>
+      <c r="B7" s="206"/>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="120"/>
       <c r="B8" s="9"/>
     </row>
     <row r="9" spans="1:5" ht="39" customHeight="1">
-      <c r="A9" s="215" t="s">
+      <c r="A9" s="207" t="s">
         <v>187</v>
       </c>
-      <c r="B9" s="216"/>
+      <c r="B9" s="208"/>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="202"/>
-      <c r="B10" s="203"/>
+      <c r="A10" s="209"/>
+      <c r="B10" s="210"/>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="204" t="s">
+      <c r="A11" s="201" t="s">
         <v>188</v>
       </c>
-      <c r="B11" s="205"/>
+      <c r="B11" s="202"/>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="204" t="s">
+      <c r="A12" s="201" t="s">
         <v>189</v>
       </c>
-      <c r="B12" s="205"/>
+      <c r="B12" s="202"/>
     </row>
     <row r="13" spans="1:5" ht="43.5" customHeight="1">
-      <c r="A13" s="204" t="s">
+      <c r="A13" s="201" t="s">
         <v>190</v>
       </c>
-      <c r="B13" s="205"/>
+      <c r="B13" s="202"/>
     </row>
     <row r="14" spans="1:5" ht="19.5" customHeight="1">
-      <c r="A14" s="204" t="s">
+      <c r="A14" s="201" t="s">
         <v>191</v>
       </c>
-      <c r="B14" s="205"/>
+      <c r="B14" s="202"/>
     </row>
     <row r="15" spans="1:5" ht="18" customHeight="1">
-      <c r="A15" s="204" t="s">
+      <c r="A15" s="201" t="s">
         <v>192</v>
       </c>
-      <c r="B15" s="205"/>
+      <c r="B15" s="202"/>
     </row>
     <row r="16" spans="1:5" ht="21" customHeight="1">
-      <c r="A16" s="204" t="s">
+      <c r="A16" s="201" t="s">
         <v>193</v>
       </c>
-      <c r="B16" s="205"/>
+      <c r="B16" s="202"/>
     </row>
     <row r="17" spans="1:2" ht="48.75" customHeight="1">
-      <c r="A17" s="200" t="s">
+      <c r="A17" s="203" t="s">
         <v>195</v>
       </c>
-      <c r="B17" s="201"/>
+      <c r="B17" s="204"/>
     </row>
     <row r="19" spans="1:2" ht="18.75">
-      <c r="A19" s="217" t="s">
+      <c r="A19" s="205" t="s">
         <v>197</v>
       </c>
-      <c r="B19" s="218"/>
+      <c r="B19" s="206"/>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="120"/>
       <c r="B20" s="9"/>
     </row>
     <row r="21" spans="1:2">
-      <c r="A21" s="215" t="s">
+      <c r="A21" s="207" t="s">
         <v>198</v>
       </c>
-      <c r="B21" s="216"/>
+      <c r="B21" s="208"/>
     </row>
     <row r="22" spans="1:2">
-      <c r="A22" s="202"/>
-      <c r="B22" s="203"/>
+      <c r="A22" s="209"/>
+      <c r="B22" s="210"/>
     </row>
     <row r="23" spans="1:2">
-      <c r="A23" s="204" t="s">
+      <c r="A23" s="201" t="s">
         <v>199</v>
       </c>
-      <c r="B23" s="205"/>
+      <c r="B23" s="202"/>
     </row>
     <row r="24" spans="1:2">
-      <c r="A24" s="204"/>
-      <c r="B24" s="205"/>
+      <c r="A24" s="201"/>
+      <c r="B24" s="202"/>
     </row>
     <row r="25" spans="1:2">
-      <c r="A25" s="204" t="s">
+      <c r="A25" s="201" t="s">
         <v>200</v>
       </c>
-      <c r="B25" s="205"/>
+      <c r="B25" s="202"/>
     </row>
     <row r="26" spans="1:2">
-      <c r="A26" s="204" t="s">
+      <c r="A26" s="201" t="s">
         <v>201</v>
       </c>
-      <c r="B26" s="205"/>
+      <c r="B26" s="202"/>
     </row>
     <row r="27" spans="1:2">
-      <c r="A27" s="200"/>
-      <c r="B27" s="201"/>
+      <c r="A27" s="203"/>
+      <c r="B27" s="204"/>
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A7:B7"/>
     <mergeCell ref="A17:B17"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
@@ -26191,6 +26184,19 @@
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="A14:B14"/>
     <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A24:B24"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A3" r:id="rId1"/>

</xml_diff>

<commit_message>
Tempo - Stage 1 of HIFI done.
</commit_message>
<xml_diff>
--- a/trunk/Tempo/Tempo.xlsx
+++ b/trunk/Tempo/Tempo.xlsx
@@ -2171,29 +2171,29 @@
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -2229,34 +2229,20 @@
     <xf numFmtId="0" fontId="48" fillId="22" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="46" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="46" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="42" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="4"/>
     </xf>
@@ -2266,6 +2252,20 @@
     <xf numFmtId="0" fontId="43" fillId="0" borderId="33" xfId="3" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" indent="4"/>
     </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="46" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="46" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Accent1" xfId="2" builtinId="29"/>
@@ -2576,8 +2576,8 @@
   <dimension ref="A1:K156"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C38" sqref="C38"/>
+      <pane ySplit="6" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" outlineLevelRow="2"/>
@@ -3356,13 +3356,15 @@
       <c r="B46" s="149" t="s">
         <v>221</v>
       </c>
-      <c r="C46" s="101"/>
+      <c r="C46" s="101">
+        <v>12215</v>
+      </c>
       <c r="D46" s="101">
         <v>13979</v>
       </c>
       <c r="E46" s="123">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1764</v>
       </c>
       <c r="F46" s="105"/>
     </row>
@@ -4900,11 +4902,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="A141:A155"/>
-    <mergeCell ref="A112:A121"/>
-    <mergeCell ref="A82:A96"/>
-    <mergeCell ref="A124:A138"/>
-    <mergeCell ref="A99:A109"/>
     <mergeCell ref="A43:A63"/>
     <mergeCell ref="A66:A79"/>
     <mergeCell ref="C5:D5"/>
@@ -4914,6 +4911,11 @@
     <mergeCell ref="A8:A18"/>
     <mergeCell ref="A21:A40"/>
     <mergeCell ref="C4:E4"/>
+    <mergeCell ref="A141:A155"/>
+    <mergeCell ref="A112:A121"/>
+    <mergeCell ref="A82:A96"/>
+    <mergeCell ref="A124:A138"/>
+    <mergeCell ref="A99:A109"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4945,13 +4947,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="26.25" customHeight="1">
-      <c r="A1" s="165" t="s">
+      <c r="A1" s="183" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="165"/>
-      <c r="C1" s="165"/>
-      <c r="D1" s="165"/>
-      <c r="E1" s="165"/>
+      <c r="B1" s="183"/>
+      <c r="C1" s="183"/>
+      <c r="D1" s="183"/>
+      <c r="E1" s="183"/>
       <c r="F1" s="7"/>
       <c r="G1" s="5"/>
       <c r="H1" s="5"/>
@@ -4981,18 +4983,18 @@
         <v>8</v>
       </c>
       <c r="B3" s="36"/>
-      <c r="C3" s="166"/>
-      <c r="D3" s="167"/>
-      <c r="E3" s="167"/>
+      <c r="C3" s="184"/>
+      <c r="D3" s="185"/>
+      <c r="E3" s="185"/>
     </row>
     <row r="4" spans="1:8" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A4" s="46" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="87"/>
-      <c r="C4" s="168"/>
-      <c r="D4" s="169"/>
-      <c r="E4" s="169"/>
+      <c r="C4" s="165"/>
+      <c r="D4" s="166"/>
+      <c r="E4" s="166"/>
       <c r="F4" s="6"/>
     </row>
     <row r="5" spans="1:8" hidden="1" outlineLevel="2">
@@ -5144,9 +5146,9 @@
         <v>9</v>
       </c>
       <c r="B21" s="90"/>
-      <c r="C21" s="170"/>
-      <c r="D21" s="171"/>
-      <c r="E21" s="171"/>
+      <c r="C21" s="167"/>
+      <c r="D21" s="168"/>
+      <c r="E21" s="168"/>
     </row>
     <row r="22" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A22" s="47">
@@ -5297,9 +5299,9 @@
         <v>10</v>
       </c>
       <c r="B38" s="87"/>
-      <c r="C38" s="168"/>
-      <c r="D38" s="169"/>
-      <c r="E38" s="169"/>
+      <c r="C38" s="165"/>
+      <c r="D38" s="166"/>
+      <c r="E38" s="166"/>
     </row>
     <row r="39" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A39" s="47">
@@ -5450,9 +5452,9 @@
         <v>11</v>
       </c>
       <c r="B55" s="87"/>
-      <c r="C55" s="168"/>
-      <c r="D55" s="169"/>
-      <c r="E55" s="169"/>
+      <c r="C55" s="165"/>
+      <c r="D55" s="166"/>
+      <c r="E55" s="166"/>
     </row>
     <row r="56" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A56" s="47">
@@ -5603,9 +5605,9 @@
         <v>12</v>
       </c>
       <c r="B72" s="87"/>
-      <c r="C72" s="168"/>
-      <c r="D72" s="169"/>
-      <c r="E72" s="169"/>
+      <c r="C72" s="165"/>
+      <c r="D72" s="166"/>
+      <c r="E72" s="166"/>
     </row>
     <row r="73" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A73" s="47">
@@ -5756,9 +5758,9 @@
         <v>13</v>
       </c>
       <c r="B89" s="87"/>
-      <c r="C89" s="168"/>
-      <c r="D89" s="169"/>
-      <c r="E89" s="169"/>
+      <c r="C89" s="165"/>
+      <c r="D89" s="166"/>
+      <c r="E89" s="166"/>
     </row>
     <row r="90" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A90" s="47">
@@ -5909,9 +5911,9 @@
         <v>14</v>
       </c>
       <c r="B106" s="87"/>
-      <c r="C106" s="168"/>
-      <c r="D106" s="169"/>
-      <c r="E106" s="169"/>
+      <c r="C106" s="165"/>
+      <c r="D106" s="166"/>
+      <c r="E106" s="166"/>
     </row>
     <row r="107" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A107" s="47">
@@ -6062,9 +6064,9 @@
         <v>15</v>
       </c>
       <c r="B123" s="87"/>
-      <c r="C123" s="168"/>
-      <c r="D123" s="169"/>
-      <c r="E123" s="169"/>
+      <c r="C123" s="165"/>
+      <c r="D123" s="166"/>
+      <c r="E123" s="166"/>
     </row>
     <row r="124" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A124" s="47">
@@ -6215,9 +6217,9 @@
         <v>16</v>
       </c>
       <c r="B140" s="87"/>
-      <c r="C140" s="168"/>
-      <c r="D140" s="169"/>
-      <c r="E140" s="169"/>
+      <c r="C140" s="165"/>
+      <c r="D140" s="166"/>
+      <c r="E140" s="166"/>
     </row>
     <row r="141" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A141" s="47">
@@ -6368,9 +6370,9 @@
         <v>17</v>
       </c>
       <c r="B157" s="87"/>
-      <c r="C157" s="168"/>
-      <c r="D157" s="169"/>
-      <c r="E157" s="169"/>
+      <c r="C157" s="165"/>
+      <c r="D157" s="166"/>
+      <c r="E157" s="166"/>
     </row>
     <row r="158" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A158" s="47">
@@ -6521,9 +6523,9 @@
         <v>18</v>
       </c>
       <c r="B174" s="87"/>
-      <c r="C174" s="168"/>
-      <c r="D174" s="169"/>
-      <c r="E174" s="169"/>
+      <c r="C174" s="165"/>
+      <c r="D174" s="166"/>
+      <c r="E174" s="166"/>
     </row>
     <row r="175" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A175" s="47">
@@ -6674,9 +6676,9 @@
         <v>19</v>
       </c>
       <c r="B191" s="87"/>
-      <c r="C191" s="168"/>
-      <c r="D191" s="169"/>
-      <c r="E191" s="169"/>
+      <c r="C191" s="165"/>
+      <c r="D191" s="166"/>
+      <c r="E191" s="166"/>
     </row>
     <row r="192" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A192" s="47">
@@ -6827,9 +6829,9 @@
         <v>20</v>
       </c>
       <c r="B208" s="87"/>
-      <c r="C208" s="168"/>
-      <c r="D208" s="169"/>
-      <c r="E208" s="169"/>
+      <c r="C208" s="165"/>
+      <c r="D208" s="166"/>
+      <c r="E208" s="166"/>
     </row>
     <row r="209" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A209" s="47">
@@ -6980,9 +6982,9 @@
         <v>21</v>
       </c>
       <c r="B225" s="87"/>
-      <c r="C225" s="168"/>
-      <c r="D225" s="169"/>
-      <c r="E225" s="169"/>
+      <c r="C225" s="165"/>
+      <c r="D225" s="166"/>
+      <c r="E225" s="166"/>
     </row>
     <row r="226" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A226" s="47">
@@ -7133,9 +7135,9 @@
         <v>22</v>
       </c>
       <c r="B242" s="87"/>
-      <c r="C242" s="168"/>
-      <c r="D242" s="169"/>
-      <c r="E242" s="169"/>
+      <c r="C242" s="165"/>
+      <c r="D242" s="166"/>
+      <c r="E242" s="166"/>
     </row>
     <row r="243" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A243" s="47">
@@ -7286,9 +7288,9 @@
         <v>23</v>
       </c>
       <c r="B259" s="87"/>
-      <c r="C259" s="168"/>
-      <c r="D259" s="169"/>
-      <c r="E259" s="169"/>
+      <c r="C259" s="165"/>
+      <c r="D259" s="166"/>
+      <c r="E259" s="166"/>
     </row>
     <row r="260" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A260" s="47">
@@ -7439,18 +7441,18 @@
         <v>24</v>
       </c>
       <c r="B276" s="37"/>
-      <c r="C276" s="172"/>
-      <c r="D276" s="173"/>
-      <c r="E276" s="173"/>
+      <c r="C276" s="181"/>
+      <c r="D276" s="182"/>
+      <c r="E276" s="182"/>
     </row>
     <row r="277" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A277" s="51" t="s">
         <v>25</v>
       </c>
       <c r="B277" s="87"/>
-      <c r="C277" s="168"/>
-      <c r="D277" s="169"/>
-      <c r="E277" s="169"/>
+      <c r="C277" s="165"/>
+      <c r="D277" s="166"/>
+      <c r="E277" s="166"/>
     </row>
     <row r="278" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A278" s="52">
@@ -7601,9 +7603,9 @@
         <v>26</v>
       </c>
       <c r="B294" s="90"/>
-      <c r="C294" s="170"/>
-      <c r="D294" s="171"/>
-      <c r="E294" s="171"/>
+      <c r="C294" s="167"/>
+      <c r="D294" s="168"/>
+      <c r="E294" s="168"/>
     </row>
     <row r="295" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A295" s="52">
@@ -7754,9 +7756,9 @@
         <v>27</v>
       </c>
       <c r="B311" s="87"/>
-      <c r="C311" s="168"/>
-      <c r="D311" s="169"/>
-      <c r="E311" s="169"/>
+      <c r="C311" s="165"/>
+      <c r="D311" s="166"/>
+      <c r="E311" s="166"/>
     </row>
     <row r="312" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A312" s="52">
@@ -7907,9 +7909,9 @@
         <v>28</v>
       </c>
       <c r="B328" s="87"/>
-      <c r="C328" s="168"/>
-      <c r="D328" s="169"/>
-      <c r="E328" s="169"/>
+      <c r="C328" s="165"/>
+      <c r="D328" s="166"/>
+      <c r="E328" s="166"/>
     </row>
     <row r="329" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A329" s="52">
@@ -8060,9 +8062,9 @@
         <v>29</v>
       </c>
       <c r="B345" s="87"/>
-      <c r="C345" s="168"/>
-      <c r="D345" s="169"/>
-      <c r="E345" s="169"/>
+      <c r="C345" s="165"/>
+      <c r="D345" s="166"/>
+      <c r="E345" s="166"/>
     </row>
     <row r="346" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A346" s="52">
@@ -8213,9 +8215,9 @@
         <v>30</v>
       </c>
       <c r="B362" s="87"/>
-      <c r="C362" s="168"/>
-      <c r="D362" s="169"/>
-      <c r="E362" s="169"/>
+      <c r="C362" s="165"/>
+      <c r="D362" s="166"/>
+      <c r="E362" s="166"/>
     </row>
     <row r="363" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A363" s="52">
@@ -8366,9 +8368,9 @@
         <v>31</v>
       </c>
       <c r="B379" s="87"/>
-      <c r="C379" s="168"/>
-      <c r="D379" s="169"/>
-      <c r="E379" s="169"/>
+      <c r="C379" s="165"/>
+      <c r="D379" s="166"/>
+      <c r="E379" s="166"/>
     </row>
     <row r="380" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A380" s="52">
@@ -8519,9 +8521,9 @@
         <v>32</v>
       </c>
       <c r="B396" s="87"/>
-      <c r="C396" s="168"/>
-      <c r="D396" s="169"/>
-      <c r="E396" s="169"/>
+      <c r="C396" s="165"/>
+      <c r="D396" s="166"/>
+      <c r="E396" s="166"/>
     </row>
     <row r="397" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A397" s="52">
@@ -8672,9 +8674,9 @@
         <v>33</v>
       </c>
       <c r="B413" s="87"/>
-      <c r="C413" s="168"/>
-      <c r="D413" s="169"/>
-      <c r="E413" s="169"/>
+      <c r="C413" s="165"/>
+      <c r="D413" s="166"/>
+      <c r="E413" s="166"/>
     </row>
     <row r="414" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A414" s="52">
@@ -8825,9 +8827,9 @@
         <v>34</v>
       </c>
       <c r="B430" s="87"/>
-      <c r="C430" s="168"/>
-      <c r="D430" s="169"/>
-      <c r="E430" s="169"/>
+      <c r="C430" s="165"/>
+      <c r="D430" s="166"/>
+      <c r="E430" s="166"/>
     </row>
     <row r="431" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A431" s="52">
@@ -8978,9 +8980,9 @@
         <v>35</v>
       </c>
       <c r="B447" s="87"/>
-      <c r="C447" s="168"/>
-      <c r="D447" s="169"/>
-      <c r="E447" s="169"/>
+      <c r="C447" s="165"/>
+      <c r="D447" s="166"/>
+      <c r="E447" s="166"/>
     </row>
     <row r="448" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A448" s="52">
@@ -9131,9 +9133,9 @@
         <v>36</v>
       </c>
       <c r="B464" s="87"/>
-      <c r="C464" s="168"/>
-      <c r="D464" s="169"/>
-      <c r="E464" s="169"/>
+      <c r="C464" s="165"/>
+      <c r="D464" s="166"/>
+      <c r="E464" s="166"/>
     </row>
     <row r="465" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A465" s="52">
@@ -9284,9 +9286,9 @@
         <v>37</v>
       </c>
       <c r="B481" s="87"/>
-      <c r="C481" s="168"/>
-      <c r="D481" s="169"/>
-      <c r="E481" s="169"/>
+      <c r="C481" s="165"/>
+      <c r="D481" s="166"/>
+      <c r="E481" s="166"/>
     </row>
     <row r="482" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A482" s="52">
@@ -9437,9 +9439,9 @@
         <v>38</v>
       </c>
       <c r="B498" s="87"/>
-      <c r="C498" s="168"/>
-      <c r="D498" s="169"/>
-      <c r="E498" s="169"/>
+      <c r="C498" s="165"/>
+      <c r="D498" s="166"/>
+      <c r="E498" s="166"/>
     </row>
     <row r="499" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A499" s="52">
@@ -9590,9 +9592,9 @@
         <v>39</v>
       </c>
       <c r="B515" s="87"/>
-      <c r="C515" s="168"/>
-      <c r="D515" s="169"/>
-      <c r="E515" s="169"/>
+      <c r="C515" s="165"/>
+      <c r="D515" s="166"/>
+      <c r="E515" s="166"/>
     </row>
     <row r="516" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A516" s="52">
@@ -9743,9 +9745,9 @@
         <v>40</v>
       </c>
       <c r="B532" s="87"/>
-      <c r="C532" s="168"/>
-      <c r="D532" s="169"/>
-      <c r="E532" s="169"/>
+      <c r="C532" s="165"/>
+      <c r="D532" s="166"/>
+      <c r="E532" s="166"/>
     </row>
     <row r="533" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A533" s="55">
@@ -9896,18 +9898,18 @@
         <v>50</v>
       </c>
       <c r="B549" s="38"/>
-      <c r="C549" s="174"/>
-      <c r="D549" s="175"/>
-      <c r="E549" s="175"/>
+      <c r="C549" s="179"/>
+      <c r="D549" s="180"/>
+      <c r="E549" s="180"/>
     </row>
     <row r="550" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A550" s="58" t="s">
         <v>51</v>
       </c>
       <c r="B550" s="87"/>
-      <c r="C550" s="168"/>
-      <c r="D550" s="169"/>
-      <c r="E550" s="169"/>
+      <c r="C550" s="165"/>
+      <c r="D550" s="166"/>
+      <c r="E550" s="166"/>
     </row>
     <row r="551" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A551" s="59">
@@ -10058,9 +10060,9 @@
         <v>52</v>
       </c>
       <c r="B567" s="90"/>
-      <c r="C567" s="170"/>
-      <c r="D567" s="171"/>
-      <c r="E567" s="171"/>
+      <c r="C567" s="167"/>
+      <c r="D567" s="168"/>
+      <c r="E567" s="168"/>
     </row>
     <row r="568" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A568" s="59">
@@ -10211,9 +10213,9 @@
         <v>53</v>
       </c>
       <c r="B584" s="87"/>
-      <c r="C584" s="168"/>
-      <c r="D584" s="169"/>
-      <c r="E584" s="169"/>
+      <c r="C584" s="165"/>
+      <c r="D584" s="166"/>
+      <c r="E584" s="166"/>
     </row>
     <row r="585" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A585" s="59">
@@ -10364,9 +10366,9 @@
         <v>54</v>
       </c>
       <c r="B601" s="87"/>
-      <c r="C601" s="168"/>
-      <c r="D601" s="169"/>
-      <c r="E601" s="169"/>
+      <c r="C601" s="165"/>
+      <c r="D601" s="166"/>
+      <c r="E601" s="166"/>
     </row>
     <row r="602" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A602" s="59">
@@ -10517,9 +10519,9 @@
         <v>55</v>
       </c>
       <c r="B618" s="87"/>
-      <c r="C618" s="168"/>
-      <c r="D618" s="169"/>
-      <c r="E618" s="169"/>
+      <c r="C618" s="165"/>
+      <c r="D618" s="166"/>
+      <c r="E618" s="166"/>
     </row>
     <row r="619" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A619" s="59">
@@ -10670,9 +10672,9 @@
         <v>56</v>
       </c>
       <c r="B635" s="87"/>
-      <c r="C635" s="168"/>
-      <c r="D635" s="169"/>
-      <c r="E635" s="169"/>
+      <c r="C635" s="165"/>
+      <c r="D635" s="166"/>
+      <c r="E635" s="166"/>
     </row>
     <row r="636" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A636" s="59">
@@ -10823,9 +10825,9 @@
         <v>57</v>
       </c>
       <c r="B652" s="87"/>
-      <c r="C652" s="168"/>
-      <c r="D652" s="169"/>
-      <c r="E652" s="169"/>
+      <c r="C652" s="165"/>
+      <c r="D652" s="166"/>
+      <c r="E652" s="166"/>
     </row>
     <row r="653" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A653" s="59">
@@ -10976,9 +10978,9 @@
         <v>58</v>
       </c>
       <c r="B669" s="87"/>
-      <c r="C669" s="168"/>
-      <c r="D669" s="169"/>
-      <c r="E669" s="169"/>
+      <c r="C669" s="165"/>
+      <c r="D669" s="166"/>
+      <c r="E669" s="166"/>
     </row>
     <row r="670" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A670" s="59">
@@ -11129,9 +11131,9 @@
         <v>59</v>
       </c>
       <c r="B686" s="87"/>
-      <c r="C686" s="168"/>
-      <c r="D686" s="169"/>
-      <c r="E686" s="169"/>
+      <c r="C686" s="165"/>
+      <c r="D686" s="166"/>
+      <c r="E686" s="166"/>
     </row>
     <row r="687" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A687" s="59">
@@ -11282,9 +11284,9 @@
         <v>60</v>
       </c>
       <c r="B703" s="87"/>
-      <c r="C703" s="168"/>
-      <c r="D703" s="169"/>
-      <c r="E703" s="169"/>
+      <c r="C703" s="165"/>
+      <c r="D703" s="166"/>
+      <c r="E703" s="166"/>
     </row>
     <row r="704" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A704" s="59">
@@ -11435,9 +11437,9 @@
         <v>61</v>
       </c>
       <c r="B720" s="87"/>
-      <c r="C720" s="168"/>
-      <c r="D720" s="169"/>
-      <c r="E720" s="169"/>
+      <c r="C720" s="165"/>
+      <c r="D720" s="166"/>
+      <c r="E720" s="166"/>
     </row>
     <row r="721" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A721" s="59">
@@ -11588,9 +11590,9 @@
         <v>62</v>
       </c>
       <c r="B737" s="87"/>
-      <c r="C737" s="168"/>
-      <c r="D737" s="169"/>
-      <c r="E737" s="169"/>
+      <c r="C737" s="165"/>
+      <c r="D737" s="166"/>
+      <c r="E737" s="166"/>
     </row>
     <row r="738" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A738" s="59">
@@ -11741,9 +11743,9 @@
         <v>63</v>
       </c>
       <c r="B754" s="87"/>
-      <c r="C754" s="168"/>
-      <c r="D754" s="169"/>
-      <c r="E754" s="169"/>
+      <c r="C754" s="165"/>
+      <c r="D754" s="166"/>
+      <c r="E754" s="166"/>
     </row>
     <row r="755" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A755" s="59">
@@ -11894,9 +11896,9 @@
         <v>64</v>
       </c>
       <c r="B771" s="87"/>
-      <c r="C771" s="168"/>
-      <c r="D771" s="169"/>
-      <c r="E771" s="169"/>
+      <c r="C771" s="165"/>
+      <c r="D771" s="166"/>
+      <c r="E771" s="166"/>
     </row>
     <row r="772" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A772" s="59">
@@ -12047,9 +12049,9 @@
         <v>65</v>
       </c>
       <c r="B788" s="87"/>
-      <c r="C788" s="168"/>
-      <c r="D788" s="169"/>
-      <c r="E788" s="169"/>
+      <c r="C788" s="165"/>
+      <c r="D788" s="166"/>
+      <c r="E788" s="166"/>
     </row>
     <row r="789" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A789" s="59">
@@ -12200,9 +12202,9 @@
         <v>66</v>
       </c>
       <c r="B805" s="87"/>
-      <c r="C805" s="168"/>
-      <c r="D805" s="169"/>
-      <c r="E805" s="169"/>
+      <c r="C805" s="165"/>
+      <c r="D805" s="166"/>
+      <c r="E805" s="166"/>
     </row>
     <row r="806" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A806" s="59">
@@ -12353,18 +12355,18 @@
         <v>67</v>
       </c>
       <c r="B822" s="39"/>
-      <c r="C822" s="176"/>
-      <c r="D822" s="177"/>
-      <c r="E822" s="177"/>
+      <c r="C822" s="177"/>
+      <c r="D822" s="178"/>
+      <c r="E822" s="178"/>
     </row>
     <row r="823" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A823" s="63" t="s">
         <v>68</v>
       </c>
       <c r="B823" s="87"/>
-      <c r="C823" s="168"/>
-      <c r="D823" s="169"/>
-      <c r="E823" s="169"/>
+      <c r="C823" s="165"/>
+      <c r="D823" s="166"/>
+      <c r="E823" s="166"/>
     </row>
     <row r="824" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A824" s="64">
@@ -12515,9 +12517,9 @@
         <v>69</v>
       </c>
       <c r="B840" s="90"/>
-      <c r="C840" s="170"/>
-      <c r="D840" s="171"/>
-      <c r="E840" s="171"/>
+      <c r="C840" s="167"/>
+      <c r="D840" s="168"/>
+      <c r="E840" s="168"/>
     </row>
     <row r="841" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A841" s="64">
@@ -12668,9 +12670,9 @@
         <v>70</v>
       </c>
       <c r="B857" s="87"/>
-      <c r="C857" s="168"/>
-      <c r="D857" s="169"/>
-      <c r="E857" s="169"/>
+      <c r="C857" s="165"/>
+      <c r="D857" s="166"/>
+      <c r="E857" s="166"/>
     </row>
     <row r="858" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A858" s="64">
@@ -12821,9 +12823,9 @@
         <v>71</v>
       </c>
       <c r="B874" s="87"/>
-      <c r="C874" s="168"/>
-      <c r="D874" s="169"/>
-      <c r="E874" s="169"/>
+      <c r="C874" s="165"/>
+      <c r="D874" s="166"/>
+      <c r="E874" s="166"/>
     </row>
     <row r="875" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A875" s="64">
@@ -12974,9 +12976,9 @@
         <v>72</v>
       </c>
       <c r="B891" s="87"/>
-      <c r="C891" s="168"/>
-      <c r="D891" s="169"/>
-      <c r="E891" s="169"/>
+      <c r="C891" s="165"/>
+      <c r="D891" s="166"/>
+      <c r="E891" s="166"/>
     </row>
     <row r="892" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A892" s="64">
@@ -13127,9 +13129,9 @@
         <v>73</v>
       </c>
       <c r="B908" s="87"/>
-      <c r="C908" s="168"/>
-      <c r="D908" s="169"/>
-      <c r="E908" s="169"/>
+      <c r="C908" s="165"/>
+      <c r="D908" s="166"/>
+      <c r="E908" s="166"/>
     </row>
     <row r="909" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A909" s="64">
@@ -13280,9 +13282,9 @@
         <v>74</v>
       </c>
       <c r="B925" s="87"/>
-      <c r="C925" s="168"/>
-      <c r="D925" s="169"/>
-      <c r="E925" s="169"/>
+      <c r="C925" s="165"/>
+      <c r="D925" s="166"/>
+      <c r="E925" s="166"/>
     </row>
     <row r="926" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A926" s="64">
@@ -13433,9 +13435,9 @@
         <v>75</v>
       </c>
       <c r="B942" s="87"/>
-      <c r="C942" s="168"/>
-      <c r="D942" s="169"/>
-      <c r="E942" s="169"/>
+      <c r="C942" s="165"/>
+      <c r="D942" s="166"/>
+      <c r="E942" s="166"/>
     </row>
     <row r="943" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A943" s="64">
@@ -13586,9 +13588,9 @@
         <v>76</v>
       </c>
       <c r="B959" s="87"/>
-      <c r="C959" s="168"/>
-      <c r="D959" s="169"/>
-      <c r="E959" s="169"/>
+      <c r="C959" s="165"/>
+      <c r="D959" s="166"/>
+      <c r="E959" s="166"/>
     </row>
     <row r="960" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A960" s="64">
@@ -13739,9 +13741,9 @@
         <v>77</v>
       </c>
       <c r="B976" s="87"/>
-      <c r="C976" s="168"/>
-      <c r="D976" s="169"/>
-      <c r="E976" s="169"/>
+      <c r="C976" s="165"/>
+      <c r="D976" s="166"/>
+      <c r="E976" s="166"/>
     </row>
     <row r="977" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A977" s="64">
@@ -13892,9 +13894,9 @@
         <v>78</v>
       </c>
       <c r="B993" s="87"/>
-      <c r="C993" s="168"/>
-      <c r="D993" s="169"/>
-      <c r="E993" s="169"/>
+      <c r="C993" s="165"/>
+      <c r="D993" s="166"/>
+      <c r="E993" s="166"/>
     </row>
     <row r="994" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A994" s="64">
@@ -14045,9 +14047,9 @@
         <v>79</v>
       </c>
       <c r="B1010" s="87"/>
-      <c r="C1010" s="168"/>
-      <c r="D1010" s="169"/>
-      <c r="E1010" s="169"/>
+      <c r="C1010" s="165"/>
+      <c r="D1010" s="166"/>
+      <c r="E1010" s="166"/>
     </row>
     <row r="1011" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1011" s="64">
@@ -14198,9 +14200,9 @@
         <v>80</v>
       </c>
       <c r="B1027" s="87"/>
-      <c r="C1027" s="168"/>
-      <c r="D1027" s="169"/>
-      <c r="E1027" s="169"/>
+      <c r="C1027" s="165"/>
+      <c r="D1027" s="166"/>
+      <c r="E1027" s="166"/>
     </row>
     <row r="1028" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1028" s="64">
@@ -14351,9 +14353,9 @@
         <v>83</v>
       </c>
       <c r="B1044" s="87"/>
-      <c r="C1044" s="168"/>
-      <c r="D1044" s="169"/>
-      <c r="E1044" s="169"/>
+      <c r="C1044" s="165"/>
+      <c r="D1044" s="166"/>
+      <c r="E1044" s="166"/>
     </row>
     <row r="1045" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1045" s="64">
@@ -14504,9 +14506,9 @@
         <v>82</v>
       </c>
       <c r="B1061" s="87"/>
-      <c r="C1061" s="168"/>
-      <c r="D1061" s="169"/>
-      <c r="E1061" s="169"/>
+      <c r="C1061" s="165"/>
+      <c r="D1061" s="166"/>
+      <c r="E1061" s="166"/>
     </row>
     <row r="1062" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1062" s="64">
@@ -14657,9 +14659,9 @@
         <v>84</v>
       </c>
       <c r="B1078" s="87"/>
-      <c r="C1078" s="168"/>
-      <c r="D1078" s="169"/>
-      <c r="E1078" s="169"/>
+      <c r="C1078" s="165"/>
+      <c r="D1078" s="166"/>
+      <c r="E1078" s="166"/>
     </row>
     <row r="1079" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1079" s="64">
@@ -14810,18 +14812,18 @@
         <v>104</v>
       </c>
       <c r="B1095" s="40"/>
-      <c r="C1095" s="178"/>
-      <c r="D1095" s="179"/>
-      <c r="E1095" s="179"/>
+      <c r="C1095" s="175"/>
+      <c r="D1095" s="176"/>
+      <c r="E1095" s="176"/>
     </row>
     <row r="1096" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A1096" s="68" t="s">
         <v>85</v>
       </c>
       <c r="B1096" s="87"/>
-      <c r="C1096" s="168"/>
-      <c r="D1096" s="169"/>
-      <c r="E1096" s="169"/>
+      <c r="C1096" s="165"/>
+      <c r="D1096" s="166"/>
+      <c r="E1096" s="166"/>
     </row>
     <row r="1097" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1097" s="69">
@@ -14972,9 +14974,9 @@
         <v>86</v>
       </c>
       <c r="B1113" s="90"/>
-      <c r="C1113" s="170"/>
-      <c r="D1113" s="171"/>
-      <c r="E1113" s="171"/>
+      <c r="C1113" s="167"/>
+      <c r="D1113" s="168"/>
+      <c r="E1113" s="168"/>
     </row>
     <row r="1114" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1114" s="69">
@@ -15125,9 +15127,9 @@
         <v>87</v>
       </c>
       <c r="B1130" s="87"/>
-      <c r="C1130" s="168"/>
-      <c r="D1130" s="169"/>
-      <c r="E1130" s="169"/>
+      <c r="C1130" s="165"/>
+      <c r="D1130" s="166"/>
+      <c r="E1130" s="166"/>
     </row>
     <row r="1131" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1131" s="69">
@@ -15278,9 +15280,9 @@
         <v>88</v>
       </c>
       <c r="B1147" s="87"/>
-      <c r="C1147" s="168"/>
-      <c r="D1147" s="169"/>
-      <c r="E1147" s="169"/>
+      <c r="C1147" s="165"/>
+      <c r="D1147" s="166"/>
+      <c r="E1147" s="166"/>
     </row>
     <row r="1148" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1148" s="69">
@@ -15431,9 +15433,9 @@
         <v>89</v>
       </c>
       <c r="B1164" s="87"/>
-      <c r="C1164" s="168"/>
-      <c r="D1164" s="169"/>
-      <c r="E1164" s="169"/>
+      <c r="C1164" s="165"/>
+      <c r="D1164" s="166"/>
+      <c r="E1164" s="166"/>
     </row>
     <row r="1165" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1165" s="69">
@@ -15584,9 +15586,9 @@
         <v>90</v>
       </c>
       <c r="B1181" s="87"/>
-      <c r="C1181" s="168"/>
-      <c r="D1181" s="169"/>
-      <c r="E1181" s="169"/>
+      <c r="C1181" s="165"/>
+      <c r="D1181" s="166"/>
+      <c r="E1181" s="166"/>
     </row>
     <row r="1182" spans="1:5" hidden="1" outlineLevel="3">
       <c r="A1182" s="69">
@@ -15737,9 +15739,9 @@
         <v>91</v>
       </c>
       <c r="B1198" s="87"/>
-      <c r="C1198" s="168"/>
-      <c r="D1198" s="169"/>
-      <c r="E1198" s="169"/>
+      <c r="C1198" s="165"/>
+      <c r="D1198" s="166"/>
+      <c r="E1198" s="166"/>
     </row>
     <row r="1199" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1199" s="69">
@@ -15890,9 +15892,9 @@
         <v>92</v>
       </c>
       <c r="B1215" s="87"/>
-      <c r="C1215" s="168"/>
-      <c r="D1215" s="169"/>
-      <c r="E1215" s="169"/>
+      <c r="C1215" s="165"/>
+      <c r="D1215" s="166"/>
+      <c r="E1215" s="166"/>
     </row>
     <row r="1216" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1216" s="69">
@@ -16043,9 +16045,9 @@
         <v>93</v>
       </c>
       <c r="B1232" s="87"/>
-      <c r="C1232" s="168"/>
-      <c r="D1232" s="169"/>
-      <c r="E1232" s="169"/>
+      <c r="C1232" s="165"/>
+      <c r="D1232" s="166"/>
+      <c r="E1232" s="166"/>
     </row>
     <row r="1233" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1233" s="69">
@@ -16196,9 +16198,9 @@
         <v>94</v>
       </c>
       <c r="B1249" s="87"/>
-      <c r="C1249" s="168"/>
-      <c r="D1249" s="169"/>
-      <c r="E1249" s="169"/>
+      <c r="C1249" s="165"/>
+      <c r="D1249" s="166"/>
+      <c r="E1249" s="166"/>
     </row>
     <row r="1250" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1250" s="69">
@@ -16349,9 +16351,9 @@
         <v>99</v>
       </c>
       <c r="B1266" s="87"/>
-      <c r="C1266" s="168"/>
-      <c r="D1266" s="169"/>
-      <c r="E1266" s="169"/>
+      <c r="C1266" s="165"/>
+      <c r="D1266" s="166"/>
+      <c r="E1266" s="166"/>
     </row>
     <row r="1267" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1267" s="69">
@@ -16502,9 +16504,9 @@
         <v>100</v>
       </c>
       <c r="B1283" s="87"/>
-      <c r="C1283" s="168"/>
-      <c r="D1283" s="169"/>
-      <c r="E1283" s="169"/>
+      <c r="C1283" s="165"/>
+      <c r="D1283" s="166"/>
+      <c r="E1283" s="166"/>
     </row>
     <row r="1284" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1284" s="69">
@@ -16655,9 +16657,9 @@
         <v>101</v>
       </c>
       <c r="B1300" s="87"/>
-      <c r="C1300" s="168"/>
-      <c r="D1300" s="169"/>
-      <c r="E1300" s="169"/>
+      <c r="C1300" s="165"/>
+      <c r="D1300" s="166"/>
+      <c r="E1300" s="166"/>
     </row>
     <row r="1301" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1301" s="69">
@@ -16808,9 +16810,9 @@
         <v>81</v>
       </c>
       <c r="B1317" s="87"/>
-      <c r="C1317" s="168"/>
-      <c r="D1317" s="169"/>
-      <c r="E1317" s="169"/>
+      <c r="C1317" s="165"/>
+      <c r="D1317" s="166"/>
+      <c r="E1317" s="166"/>
     </row>
     <row r="1318" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1318" s="69">
@@ -16961,9 +16963,9 @@
         <v>102</v>
       </c>
       <c r="B1334" s="87"/>
-      <c r="C1334" s="168"/>
-      <c r="D1334" s="169"/>
-      <c r="E1334" s="169"/>
+      <c r="C1334" s="165"/>
+      <c r="D1334" s="166"/>
+      <c r="E1334" s="166"/>
     </row>
     <row r="1335" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1335" s="69">
@@ -17114,9 +17116,9 @@
         <v>98</v>
       </c>
       <c r="B1351" s="87"/>
-      <c r="C1351" s="168"/>
-      <c r="D1351" s="169"/>
-      <c r="E1351" s="169"/>
+      <c r="C1351" s="165"/>
+      <c r="D1351" s="166"/>
+      <c r="E1351" s="166"/>
     </row>
     <row r="1352" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1352" s="69">
@@ -17267,18 +17269,18 @@
         <v>103</v>
       </c>
       <c r="B1368" s="41"/>
-      <c r="C1368" s="180"/>
-      <c r="D1368" s="181"/>
-      <c r="E1368" s="181"/>
+      <c r="C1368" s="173"/>
+      <c r="D1368" s="174"/>
+      <c r="E1368" s="174"/>
     </row>
     <row r="1369" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A1369" s="73" t="s">
         <v>105</v>
       </c>
       <c r="B1369" s="87"/>
-      <c r="C1369" s="168"/>
-      <c r="D1369" s="169"/>
-      <c r="E1369" s="169"/>
+      <c r="C1369" s="165"/>
+      <c r="D1369" s="166"/>
+      <c r="E1369" s="166"/>
     </row>
     <row r="1370" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1370" s="74">
@@ -17429,9 +17431,9 @@
         <v>106</v>
       </c>
       <c r="B1386" s="90"/>
-      <c r="C1386" s="170"/>
-      <c r="D1386" s="171"/>
-      <c r="E1386" s="171"/>
+      <c r="C1386" s="167"/>
+      <c r="D1386" s="168"/>
+      <c r="E1386" s="168"/>
     </row>
     <row r="1387" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1387" s="74">
@@ -17582,9 +17584,9 @@
         <v>107</v>
       </c>
       <c r="B1403" s="87"/>
-      <c r="C1403" s="168"/>
-      <c r="D1403" s="169"/>
-      <c r="E1403" s="169"/>
+      <c r="C1403" s="165"/>
+      <c r="D1403" s="166"/>
+      <c r="E1403" s="166"/>
     </row>
     <row r="1404" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1404" s="74">
@@ -17735,9 +17737,9 @@
         <v>108</v>
       </c>
       <c r="B1420" s="87"/>
-      <c r="C1420" s="168"/>
-      <c r="D1420" s="169"/>
-      <c r="E1420" s="169"/>
+      <c r="C1420" s="165"/>
+      <c r="D1420" s="166"/>
+      <c r="E1420" s="166"/>
     </row>
     <row r="1421" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1421" s="74">
@@ -17888,9 +17890,9 @@
         <v>109</v>
       </c>
       <c r="B1437" s="87"/>
-      <c r="C1437" s="168"/>
-      <c r="D1437" s="169"/>
-      <c r="E1437" s="169"/>
+      <c r="C1437" s="165"/>
+      <c r="D1437" s="166"/>
+      <c r="E1437" s="166"/>
     </row>
     <row r="1438" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1438" s="74">
@@ -18041,9 +18043,9 @@
         <v>110</v>
       </c>
       <c r="B1454" s="87"/>
-      <c r="C1454" s="168"/>
-      <c r="D1454" s="169"/>
-      <c r="E1454" s="169"/>
+      <c r="C1454" s="165"/>
+      <c r="D1454" s="166"/>
+      <c r="E1454" s="166"/>
     </row>
     <row r="1455" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1455" s="74">
@@ -18194,9 +18196,9 @@
         <v>111</v>
       </c>
       <c r="B1471" s="87"/>
-      <c r="C1471" s="168"/>
-      <c r="D1471" s="169"/>
-      <c r="E1471" s="169"/>
+      <c r="C1471" s="165"/>
+      <c r="D1471" s="166"/>
+      <c r="E1471" s="166"/>
     </row>
     <row r="1472" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1472" s="74">
@@ -18347,9 +18349,9 @@
         <v>112</v>
       </c>
       <c r="B1488" s="87"/>
-      <c r="C1488" s="168"/>
-      <c r="D1488" s="169"/>
-      <c r="E1488" s="169"/>
+      <c r="C1488" s="165"/>
+      <c r="D1488" s="166"/>
+      <c r="E1488" s="166"/>
     </row>
     <row r="1489" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1489" s="74">
@@ -18500,9 +18502,9 @@
         <v>113</v>
       </c>
       <c r="B1505" s="87"/>
-      <c r="C1505" s="168"/>
-      <c r="D1505" s="169"/>
-      <c r="E1505" s="169"/>
+      <c r="C1505" s="165"/>
+      <c r="D1505" s="166"/>
+      <c r="E1505" s="166"/>
     </row>
     <row r="1506" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1506" s="74">
@@ -18653,9 +18655,9 @@
         <v>114</v>
       </c>
       <c r="B1522" s="87"/>
-      <c r="C1522" s="168"/>
-      <c r="D1522" s="169"/>
-      <c r="E1522" s="169"/>
+      <c r="C1522" s="165"/>
+      <c r="D1522" s="166"/>
+      <c r="E1522" s="166"/>
     </row>
     <row r="1523" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1523" s="74">
@@ -18806,9 +18808,9 @@
         <v>95</v>
       </c>
       <c r="B1539" s="87"/>
-      <c r="C1539" s="168"/>
-      <c r="D1539" s="169"/>
-      <c r="E1539" s="169"/>
+      <c r="C1539" s="165"/>
+      <c r="D1539" s="166"/>
+      <c r="E1539" s="166"/>
     </row>
     <row r="1540" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1540" s="74">
@@ -18959,9 +18961,9 @@
         <v>115</v>
       </c>
       <c r="B1556" s="87"/>
-      <c r="C1556" s="168"/>
-      <c r="D1556" s="169"/>
-      <c r="E1556" s="169"/>
+      <c r="C1556" s="165"/>
+      <c r="D1556" s="166"/>
+      <c r="E1556" s="166"/>
     </row>
     <row r="1557" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1557" s="74">
@@ -19112,9 +19114,9 @@
         <v>116</v>
       </c>
       <c r="B1573" s="87"/>
-      <c r="C1573" s="168"/>
-      <c r="D1573" s="169"/>
-      <c r="E1573" s="169"/>
+      <c r="C1573" s="165"/>
+      <c r="D1573" s="166"/>
+      <c r="E1573" s="166"/>
     </row>
     <row r="1574" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1574" s="74">
@@ -19265,9 +19267,9 @@
         <v>117</v>
       </c>
       <c r="B1590" s="87"/>
-      <c r="C1590" s="168"/>
-      <c r="D1590" s="169"/>
-      <c r="E1590" s="169"/>
+      <c r="C1590" s="165"/>
+      <c r="D1590" s="166"/>
+      <c r="E1590" s="166"/>
     </row>
     <row r="1591" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1591" s="74">
@@ -19418,9 +19420,9 @@
         <v>118</v>
       </c>
       <c r="B1607" s="87"/>
-      <c r="C1607" s="168"/>
-      <c r="D1607" s="169"/>
-      <c r="E1607" s="169"/>
+      <c r="C1607" s="165"/>
+      <c r="D1607" s="166"/>
+      <c r="E1607" s="166"/>
     </row>
     <row r="1608" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1608" s="74">
@@ -19571,9 +19573,9 @@
         <v>119</v>
       </c>
       <c r="B1624" s="87"/>
-      <c r="C1624" s="168"/>
-      <c r="D1624" s="169"/>
-      <c r="E1624" s="169"/>
+      <c r="C1624" s="165"/>
+      <c r="D1624" s="166"/>
+      <c r="E1624" s="166"/>
     </row>
     <row r="1625" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1625" s="74">
@@ -19724,18 +19726,18 @@
         <v>120</v>
       </c>
       <c r="B1641" s="42"/>
-      <c r="C1641" s="182"/>
-      <c r="D1641" s="183"/>
-      <c r="E1641" s="183"/>
+      <c r="C1641" s="171"/>
+      <c r="D1641" s="172"/>
+      <c r="E1641" s="172"/>
     </row>
     <row r="1642" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A1642" s="78" t="s">
         <v>121</v>
       </c>
       <c r="B1642" s="87"/>
-      <c r="C1642" s="168"/>
-      <c r="D1642" s="169"/>
-      <c r="E1642" s="169"/>
+      <c r="C1642" s="165"/>
+      <c r="D1642" s="166"/>
+      <c r="E1642" s="166"/>
     </row>
     <row r="1643" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1643" s="79">
@@ -19886,9 +19888,9 @@
         <v>122</v>
       </c>
       <c r="B1659" s="90"/>
-      <c r="C1659" s="170"/>
-      <c r="D1659" s="171"/>
-      <c r="E1659" s="171"/>
+      <c r="C1659" s="167"/>
+      <c r="D1659" s="168"/>
+      <c r="E1659" s="168"/>
     </row>
     <row r="1660" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1660" s="79">
@@ -20039,9 +20041,9 @@
         <v>123</v>
       </c>
       <c r="B1676" s="87"/>
-      <c r="C1676" s="168"/>
-      <c r="D1676" s="169"/>
-      <c r="E1676" s="169"/>
+      <c r="C1676" s="165"/>
+      <c r="D1676" s="166"/>
+      <c r="E1676" s="166"/>
     </row>
     <row r="1677" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1677" s="79">
@@ -20192,9 +20194,9 @@
         <v>124</v>
       </c>
       <c r="B1693" s="87"/>
-      <c r="C1693" s="168"/>
-      <c r="D1693" s="169"/>
-      <c r="E1693" s="169"/>
+      <c r="C1693" s="165"/>
+      <c r="D1693" s="166"/>
+      <c r="E1693" s="166"/>
     </row>
     <row r="1694" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1694" s="79">
@@ -20345,9 +20347,9 @@
         <v>125</v>
       </c>
       <c r="B1710" s="87"/>
-      <c r="C1710" s="168"/>
-      <c r="D1710" s="169"/>
-      <c r="E1710" s="169"/>
+      <c r="C1710" s="165"/>
+      <c r="D1710" s="166"/>
+      <c r="E1710" s="166"/>
     </row>
     <row r="1711" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1711" s="79">
@@ -20498,9 +20500,9 @@
         <v>126</v>
       </c>
       <c r="B1727" s="87"/>
-      <c r="C1727" s="168"/>
-      <c r="D1727" s="169"/>
-      <c r="E1727" s="169"/>
+      <c r="C1727" s="165"/>
+      <c r="D1727" s="166"/>
+      <c r="E1727" s="166"/>
     </row>
     <row r="1728" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1728" s="79">
@@ -20651,9 +20653,9 @@
         <v>127</v>
       </c>
       <c r="B1744" s="87"/>
-      <c r="C1744" s="168"/>
-      <c r="D1744" s="169"/>
-      <c r="E1744" s="169"/>
+      <c r="C1744" s="165"/>
+      <c r="D1744" s="166"/>
+      <c r="E1744" s="166"/>
     </row>
     <row r="1745" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1745" s="79">
@@ -20804,9 +20806,9 @@
         <v>128</v>
       </c>
       <c r="B1761" s="87"/>
-      <c r="C1761" s="168"/>
-      <c r="D1761" s="169"/>
-      <c r="E1761" s="169"/>
+      <c r="C1761" s="165"/>
+      <c r="D1761" s="166"/>
+      <c r="E1761" s="166"/>
     </row>
     <row r="1762" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1762" s="79">
@@ -20957,9 +20959,9 @@
         <v>129</v>
       </c>
       <c r="B1778" s="87"/>
-      <c r="C1778" s="168"/>
-      <c r="D1778" s="169"/>
-      <c r="E1778" s="169"/>
+      <c r="C1778" s="165"/>
+      <c r="D1778" s="166"/>
+      <c r="E1778" s="166"/>
     </row>
     <row r="1779" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1779" s="79">
@@ -21110,9 +21112,9 @@
         <v>130</v>
       </c>
       <c r="B1795" s="87"/>
-      <c r="C1795" s="168"/>
-      <c r="D1795" s="169"/>
-      <c r="E1795" s="169"/>
+      <c r="C1795" s="165"/>
+      <c r="D1795" s="166"/>
+      <c r="E1795" s="166"/>
     </row>
     <row r="1796" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1796" s="79">
@@ -21263,9 +21265,9 @@
         <v>131</v>
       </c>
       <c r="B1812" s="87"/>
-      <c r="C1812" s="168"/>
-      <c r="D1812" s="169"/>
-      <c r="E1812" s="169"/>
+      <c r="C1812" s="165"/>
+      <c r="D1812" s="166"/>
+      <c r="E1812" s="166"/>
     </row>
     <row r="1813" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1813" s="79">
@@ -21416,9 +21418,9 @@
         <v>96</v>
       </c>
       <c r="B1829" s="87"/>
-      <c r="C1829" s="168"/>
-      <c r="D1829" s="169"/>
-      <c r="E1829" s="169"/>
+      <c r="C1829" s="165"/>
+      <c r="D1829" s="166"/>
+      <c r="E1829" s="166"/>
     </row>
     <row r="1830" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1830" s="79">
@@ -21569,9 +21571,9 @@
         <v>132</v>
       </c>
       <c r="B1846" s="87"/>
-      <c r="C1846" s="168"/>
-      <c r="D1846" s="169"/>
-      <c r="E1846" s="169"/>
+      <c r="C1846" s="165"/>
+      <c r="D1846" s="166"/>
+      <c r="E1846" s="166"/>
     </row>
     <row r="1847" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1847" s="79">
@@ -21722,9 +21724,9 @@
         <v>133</v>
       </c>
       <c r="B1863" s="87"/>
-      <c r="C1863" s="168"/>
-      <c r="D1863" s="169"/>
-      <c r="E1863" s="169"/>
+      <c r="C1863" s="165"/>
+      <c r="D1863" s="166"/>
+      <c r="E1863" s="166"/>
     </row>
     <row r="1864" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1864" s="79">
@@ -21875,9 +21877,9 @@
         <v>134</v>
       </c>
       <c r="B1880" s="87"/>
-      <c r="C1880" s="168"/>
-      <c r="D1880" s="169"/>
-      <c r="E1880" s="169"/>
+      <c r="C1880" s="165"/>
+      <c r="D1880" s="166"/>
+      <c r="E1880" s="166"/>
     </row>
     <row r="1881" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1881" s="79">
@@ -22028,9 +22030,9 @@
         <v>135</v>
       </c>
       <c r="B1897" s="87"/>
-      <c r="C1897" s="168"/>
-      <c r="D1897" s="169"/>
-      <c r="E1897" s="169"/>
+      <c r="C1897" s="165"/>
+      <c r="D1897" s="166"/>
+      <c r="E1897" s="166"/>
     </row>
     <row r="1898" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1898" s="79">
@@ -22181,18 +22183,18 @@
         <v>136</v>
       </c>
       <c r="B1914" s="43"/>
-      <c r="C1914" s="184"/>
-      <c r="D1914" s="185"/>
-      <c r="E1914" s="185"/>
+      <c r="C1914" s="169"/>
+      <c r="D1914" s="170"/>
+      <c r="E1914" s="170"/>
     </row>
     <row r="1915" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A1915" s="83" t="s">
         <v>137</v>
       </c>
       <c r="B1915" s="87"/>
-      <c r="C1915" s="168"/>
-      <c r="D1915" s="169"/>
-      <c r="E1915" s="169"/>
+      <c r="C1915" s="165"/>
+      <c r="D1915" s="166"/>
+      <c r="E1915" s="166"/>
     </row>
     <row r="1916" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1916" s="84">
@@ -22343,9 +22345,9 @@
         <v>138</v>
       </c>
       <c r="B1932" s="90"/>
-      <c r="C1932" s="170"/>
-      <c r="D1932" s="171"/>
-      <c r="E1932" s="171"/>
+      <c r="C1932" s="167"/>
+      <c r="D1932" s="168"/>
+      <c r="E1932" s="168"/>
     </row>
     <row r="1933" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1933" s="84">
@@ -22496,9 +22498,9 @@
         <v>139</v>
       </c>
       <c r="B1949" s="87"/>
-      <c r="C1949" s="168"/>
-      <c r="D1949" s="169"/>
-      <c r="E1949" s="169"/>
+      <c r="C1949" s="165"/>
+      <c r="D1949" s="166"/>
+      <c r="E1949" s="166"/>
     </row>
     <row r="1950" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1950" s="84">
@@ -22649,9 +22651,9 @@
         <v>140</v>
       </c>
       <c r="B1966" s="87"/>
-      <c r="C1966" s="168"/>
-      <c r="D1966" s="169"/>
-      <c r="E1966" s="169"/>
+      <c r="C1966" s="165"/>
+      <c r="D1966" s="166"/>
+      <c r="E1966" s="166"/>
     </row>
     <row r="1967" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1967" s="84">
@@ -22802,9 +22804,9 @@
         <v>141</v>
       </c>
       <c r="B1983" s="87"/>
-      <c r="C1983" s="168"/>
-      <c r="D1983" s="169"/>
-      <c r="E1983" s="169"/>
+      <c r="C1983" s="165"/>
+      <c r="D1983" s="166"/>
+      <c r="E1983" s="166"/>
     </row>
     <row r="1984" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1984" s="84">
@@ -22955,9 +22957,9 @@
         <v>142</v>
       </c>
       <c r="B2000" s="87"/>
-      <c r="C2000" s="168"/>
-      <c r="D2000" s="169"/>
-      <c r="E2000" s="169"/>
+      <c r="C2000" s="165"/>
+      <c r="D2000" s="166"/>
+      <c r="E2000" s="166"/>
     </row>
     <row r="2001" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2001" s="84">
@@ -23108,9 +23110,9 @@
         <v>143</v>
       </c>
       <c r="B2017" s="87"/>
-      <c r="C2017" s="168"/>
-      <c r="D2017" s="169"/>
-      <c r="E2017" s="169"/>
+      <c r="C2017" s="165"/>
+      <c r="D2017" s="166"/>
+      <c r="E2017" s="166"/>
     </row>
     <row r="2018" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2018" s="84">
@@ -23261,9 +23263,9 @@
         <v>144</v>
       </c>
       <c r="B2034" s="87"/>
-      <c r="C2034" s="168"/>
-      <c r="D2034" s="169"/>
-      <c r="E2034" s="169"/>
+      <c r="C2034" s="165"/>
+      <c r="D2034" s="166"/>
+      <c r="E2034" s="166"/>
     </row>
     <row r="2035" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2035" s="84">
@@ -23414,9 +23416,9 @@
         <v>145</v>
       </c>
       <c r="B2051" s="87"/>
-      <c r="C2051" s="168"/>
-      <c r="D2051" s="169"/>
-      <c r="E2051" s="169"/>
+      <c r="C2051" s="165"/>
+      <c r="D2051" s="166"/>
+      <c r="E2051" s="166"/>
     </row>
     <row r="2052" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2052" s="84">
@@ -23567,9 +23569,9 @@
         <v>146</v>
       </c>
       <c r="B2068" s="87"/>
-      <c r="C2068" s="168"/>
-      <c r="D2068" s="169"/>
-      <c r="E2068" s="169"/>
+      <c r="C2068" s="165"/>
+      <c r="D2068" s="166"/>
+      <c r="E2068" s="166"/>
     </row>
     <row r="2069" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2069" s="84">
@@ -23720,9 +23722,9 @@
         <v>147</v>
       </c>
       <c r="B2085" s="87"/>
-      <c r="C2085" s="168"/>
-      <c r="D2085" s="169"/>
-      <c r="E2085" s="169"/>
+      <c r="C2085" s="165"/>
+      <c r="D2085" s="166"/>
+      <c r="E2085" s="166"/>
     </row>
     <row r="2086" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2086" s="84">
@@ -23873,9 +23875,9 @@
         <v>148</v>
       </c>
       <c r="B2102" s="87"/>
-      <c r="C2102" s="168"/>
-      <c r="D2102" s="169"/>
-      <c r="E2102" s="169"/>
+      <c r="C2102" s="165"/>
+      <c r="D2102" s="166"/>
+      <c r="E2102" s="166"/>
     </row>
     <row r="2103" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2103" s="84">
@@ -24026,9 +24028,9 @@
         <v>97</v>
       </c>
       <c r="B2119" s="87"/>
-      <c r="C2119" s="168"/>
-      <c r="D2119" s="169"/>
-      <c r="E2119" s="169"/>
+      <c r="C2119" s="165"/>
+      <c r="D2119" s="166"/>
+      <c r="E2119" s="166"/>
     </row>
     <row r="2120" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2120" s="84">
@@ -24179,9 +24181,9 @@
         <v>149</v>
       </c>
       <c r="B2136" s="87"/>
-      <c r="C2136" s="168"/>
-      <c r="D2136" s="169"/>
-      <c r="E2136" s="169"/>
+      <c r="C2136" s="165"/>
+      <c r="D2136" s="166"/>
+      <c r="E2136" s="166"/>
     </row>
     <row r="2137" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2137" s="84">
@@ -24332,9 +24334,9 @@
         <v>150</v>
       </c>
       <c r="B2153" s="87"/>
-      <c r="C2153" s="168"/>
-      <c r="D2153" s="169"/>
-      <c r="E2153" s="169"/>
+      <c r="C2153" s="165"/>
+      <c r="D2153" s="166"/>
+      <c r="E2153" s="166"/>
     </row>
     <row r="2154" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2154" s="84">
@@ -24485,9 +24487,9 @@
         <v>151</v>
       </c>
       <c r="B2170" s="87"/>
-      <c r="C2170" s="168"/>
-      <c r="D2170" s="169"/>
-      <c r="E2170" s="169"/>
+      <c r="C2170" s="165"/>
+      <c r="D2170" s="166"/>
+      <c r="E2170" s="166"/>
     </row>
     <row r="2171" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2171" s="84">
@@ -24635,15 +24637,122 @@
     </row>
   </sheetData>
   <mergeCells count="137">
-    <mergeCell ref="C2034:E2034"/>
-    <mergeCell ref="C2051:E2051"/>
-    <mergeCell ref="C2068:E2068"/>
-    <mergeCell ref="C2085:E2085"/>
-    <mergeCell ref="C2170:E2170"/>
-    <mergeCell ref="C2102:E2102"/>
-    <mergeCell ref="C2119:E2119"/>
-    <mergeCell ref="C2136:E2136"/>
-    <mergeCell ref="C2153:E2153"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="C89:E89"/>
+    <mergeCell ref="C21:E21"/>
+    <mergeCell ref="C38:E38"/>
+    <mergeCell ref="C55:E55"/>
+    <mergeCell ref="C72:E72"/>
+    <mergeCell ref="C208:E208"/>
+    <mergeCell ref="C225:E225"/>
+    <mergeCell ref="C242:E242"/>
+    <mergeCell ref="C259:E259"/>
+    <mergeCell ref="C276:E276"/>
+    <mergeCell ref="C277:E277"/>
+    <mergeCell ref="C106:E106"/>
+    <mergeCell ref="C123:E123"/>
+    <mergeCell ref="C140:E140"/>
+    <mergeCell ref="C157:E157"/>
+    <mergeCell ref="C174:E174"/>
+    <mergeCell ref="C191:E191"/>
+    <mergeCell ref="C396:E396"/>
+    <mergeCell ref="C413:E413"/>
+    <mergeCell ref="C430:E430"/>
+    <mergeCell ref="C447:E447"/>
+    <mergeCell ref="C464:E464"/>
+    <mergeCell ref="C481:E481"/>
+    <mergeCell ref="C294:E294"/>
+    <mergeCell ref="C311:E311"/>
+    <mergeCell ref="C328:E328"/>
+    <mergeCell ref="C345:E345"/>
+    <mergeCell ref="C362:E362"/>
+    <mergeCell ref="C379:E379"/>
+    <mergeCell ref="C584:E584"/>
+    <mergeCell ref="C601:E601"/>
+    <mergeCell ref="C618:E618"/>
+    <mergeCell ref="C635:E635"/>
+    <mergeCell ref="C652:E652"/>
+    <mergeCell ref="C669:E669"/>
+    <mergeCell ref="C498:E498"/>
+    <mergeCell ref="C515:E515"/>
+    <mergeCell ref="C532:E532"/>
+    <mergeCell ref="C549:E549"/>
+    <mergeCell ref="C550:E550"/>
+    <mergeCell ref="C567:E567"/>
+    <mergeCell ref="C788:E788"/>
+    <mergeCell ref="C805:E805"/>
+    <mergeCell ref="C822:E822"/>
+    <mergeCell ref="C823:E823"/>
+    <mergeCell ref="C840:E840"/>
+    <mergeCell ref="C857:E857"/>
+    <mergeCell ref="C686:E686"/>
+    <mergeCell ref="C703:E703"/>
+    <mergeCell ref="C720:E720"/>
+    <mergeCell ref="C737:E737"/>
+    <mergeCell ref="C754:E754"/>
+    <mergeCell ref="C771:E771"/>
+    <mergeCell ref="C976:E976"/>
+    <mergeCell ref="C993:E993"/>
+    <mergeCell ref="C1010:E1010"/>
+    <mergeCell ref="C1027:E1027"/>
+    <mergeCell ref="C1044:E1044"/>
+    <mergeCell ref="C1061:E1061"/>
+    <mergeCell ref="C874:E874"/>
+    <mergeCell ref="C891:E891"/>
+    <mergeCell ref="C908:E908"/>
+    <mergeCell ref="C925:E925"/>
+    <mergeCell ref="C942:E942"/>
+    <mergeCell ref="C959:E959"/>
+    <mergeCell ref="C1164:E1164"/>
+    <mergeCell ref="C1181:E1181"/>
+    <mergeCell ref="C1198:E1198"/>
+    <mergeCell ref="C1215:E1215"/>
+    <mergeCell ref="C1232:E1232"/>
+    <mergeCell ref="C1249:E1249"/>
+    <mergeCell ref="C1078:E1078"/>
+    <mergeCell ref="C1095:E1095"/>
+    <mergeCell ref="C1096:E1096"/>
+    <mergeCell ref="C1113:E1113"/>
+    <mergeCell ref="C1130:E1130"/>
+    <mergeCell ref="C1147:E1147"/>
+    <mergeCell ref="C1368:E1368"/>
+    <mergeCell ref="C1369:E1369"/>
+    <mergeCell ref="C1386:E1386"/>
+    <mergeCell ref="C1403:E1403"/>
+    <mergeCell ref="C1420:E1420"/>
+    <mergeCell ref="C1437:E1437"/>
+    <mergeCell ref="C1266:E1266"/>
+    <mergeCell ref="C1283:E1283"/>
+    <mergeCell ref="C1300:E1300"/>
+    <mergeCell ref="C1317:E1317"/>
+    <mergeCell ref="C1334:E1334"/>
+    <mergeCell ref="C1351:E1351"/>
+    <mergeCell ref="C1556:E1556"/>
+    <mergeCell ref="C1573:E1573"/>
+    <mergeCell ref="C1590:E1590"/>
+    <mergeCell ref="C1607:E1607"/>
+    <mergeCell ref="C1624:E1624"/>
+    <mergeCell ref="C1641:E1641"/>
+    <mergeCell ref="C1454:E1454"/>
+    <mergeCell ref="C1471:E1471"/>
+    <mergeCell ref="C1488:E1488"/>
+    <mergeCell ref="C1505:E1505"/>
+    <mergeCell ref="C1522:E1522"/>
+    <mergeCell ref="C1539:E1539"/>
+    <mergeCell ref="C1744:E1744"/>
+    <mergeCell ref="C1761:E1761"/>
+    <mergeCell ref="C1778:E1778"/>
+    <mergeCell ref="C1795:E1795"/>
+    <mergeCell ref="C1812:E1812"/>
+    <mergeCell ref="C1829:E1829"/>
+    <mergeCell ref="C1642:E1642"/>
+    <mergeCell ref="C1659:E1659"/>
+    <mergeCell ref="C1676:E1676"/>
+    <mergeCell ref="C1693:E1693"/>
+    <mergeCell ref="C1710:E1710"/>
+    <mergeCell ref="C1727:E1727"/>
     <mergeCell ref="C1932:E1932"/>
     <mergeCell ref="C1949:E1949"/>
     <mergeCell ref="C1966:E1966"/>
@@ -24656,122 +24765,15 @@
     <mergeCell ref="C1897:E1897"/>
     <mergeCell ref="C1914:E1914"/>
     <mergeCell ref="C1915:E1915"/>
-    <mergeCell ref="C1744:E1744"/>
-    <mergeCell ref="C1761:E1761"/>
-    <mergeCell ref="C1778:E1778"/>
-    <mergeCell ref="C1795:E1795"/>
-    <mergeCell ref="C1812:E1812"/>
-    <mergeCell ref="C1829:E1829"/>
-    <mergeCell ref="C1642:E1642"/>
-    <mergeCell ref="C1659:E1659"/>
-    <mergeCell ref="C1676:E1676"/>
-    <mergeCell ref="C1693:E1693"/>
-    <mergeCell ref="C1710:E1710"/>
-    <mergeCell ref="C1727:E1727"/>
-    <mergeCell ref="C1556:E1556"/>
-    <mergeCell ref="C1573:E1573"/>
-    <mergeCell ref="C1590:E1590"/>
-    <mergeCell ref="C1607:E1607"/>
-    <mergeCell ref="C1624:E1624"/>
-    <mergeCell ref="C1641:E1641"/>
-    <mergeCell ref="C1454:E1454"/>
-    <mergeCell ref="C1471:E1471"/>
-    <mergeCell ref="C1488:E1488"/>
-    <mergeCell ref="C1505:E1505"/>
-    <mergeCell ref="C1522:E1522"/>
-    <mergeCell ref="C1539:E1539"/>
-    <mergeCell ref="C1368:E1368"/>
-    <mergeCell ref="C1369:E1369"/>
-    <mergeCell ref="C1386:E1386"/>
-    <mergeCell ref="C1403:E1403"/>
-    <mergeCell ref="C1420:E1420"/>
-    <mergeCell ref="C1437:E1437"/>
-    <mergeCell ref="C1266:E1266"/>
-    <mergeCell ref="C1283:E1283"/>
-    <mergeCell ref="C1300:E1300"/>
-    <mergeCell ref="C1317:E1317"/>
-    <mergeCell ref="C1334:E1334"/>
-    <mergeCell ref="C1351:E1351"/>
-    <mergeCell ref="C1164:E1164"/>
-    <mergeCell ref="C1181:E1181"/>
-    <mergeCell ref="C1198:E1198"/>
-    <mergeCell ref="C1215:E1215"/>
-    <mergeCell ref="C1232:E1232"/>
-    <mergeCell ref="C1249:E1249"/>
-    <mergeCell ref="C1078:E1078"/>
-    <mergeCell ref="C1095:E1095"/>
-    <mergeCell ref="C1096:E1096"/>
-    <mergeCell ref="C1113:E1113"/>
-    <mergeCell ref="C1130:E1130"/>
-    <mergeCell ref="C1147:E1147"/>
-    <mergeCell ref="C976:E976"/>
-    <mergeCell ref="C993:E993"/>
-    <mergeCell ref="C1010:E1010"/>
-    <mergeCell ref="C1027:E1027"/>
-    <mergeCell ref="C1044:E1044"/>
-    <mergeCell ref="C1061:E1061"/>
-    <mergeCell ref="C874:E874"/>
-    <mergeCell ref="C891:E891"/>
-    <mergeCell ref="C908:E908"/>
-    <mergeCell ref="C925:E925"/>
-    <mergeCell ref="C942:E942"/>
-    <mergeCell ref="C959:E959"/>
-    <mergeCell ref="C788:E788"/>
-    <mergeCell ref="C805:E805"/>
-    <mergeCell ref="C822:E822"/>
-    <mergeCell ref="C823:E823"/>
-    <mergeCell ref="C840:E840"/>
-    <mergeCell ref="C857:E857"/>
-    <mergeCell ref="C686:E686"/>
-    <mergeCell ref="C703:E703"/>
-    <mergeCell ref="C720:E720"/>
-    <mergeCell ref="C737:E737"/>
-    <mergeCell ref="C754:E754"/>
-    <mergeCell ref="C771:E771"/>
-    <mergeCell ref="C584:E584"/>
-    <mergeCell ref="C601:E601"/>
-    <mergeCell ref="C618:E618"/>
-    <mergeCell ref="C635:E635"/>
-    <mergeCell ref="C652:E652"/>
-    <mergeCell ref="C669:E669"/>
-    <mergeCell ref="C498:E498"/>
-    <mergeCell ref="C515:E515"/>
-    <mergeCell ref="C532:E532"/>
-    <mergeCell ref="C549:E549"/>
-    <mergeCell ref="C550:E550"/>
-    <mergeCell ref="C567:E567"/>
-    <mergeCell ref="C396:E396"/>
-    <mergeCell ref="C413:E413"/>
-    <mergeCell ref="C430:E430"/>
-    <mergeCell ref="C447:E447"/>
-    <mergeCell ref="C464:E464"/>
-    <mergeCell ref="C481:E481"/>
-    <mergeCell ref="C294:E294"/>
-    <mergeCell ref="C311:E311"/>
-    <mergeCell ref="C328:E328"/>
-    <mergeCell ref="C345:E345"/>
-    <mergeCell ref="C362:E362"/>
-    <mergeCell ref="C379:E379"/>
-    <mergeCell ref="C225:E225"/>
-    <mergeCell ref="C242:E242"/>
-    <mergeCell ref="C259:E259"/>
-    <mergeCell ref="C276:E276"/>
-    <mergeCell ref="C277:E277"/>
-    <mergeCell ref="C106:E106"/>
-    <mergeCell ref="C123:E123"/>
-    <mergeCell ref="C140:E140"/>
-    <mergeCell ref="C157:E157"/>
-    <mergeCell ref="C174:E174"/>
-    <mergeCell ref="C191:E191"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="C89:E89"/>
-    <mergeCell ref="C21:E21"/>
-    <mergeCell ref="C38:E38"/>
-    <mergeCell ref="C55:E55"/>
-    <mergeCell ref="C72:E72"/>
-    <mergeCell ref="C208:E208"/>
+    <mergeCell ref="C2034:E2034"/>
+    <mergeCell ref="C2051:E2051"/>
+    <mergeCell ref="C2068:E2068"/>
+    <mergeCell ref="C2085:E2085"/>
+    <mergeCell ref="C2170:E2170"/>
+    <mergeCell ref="C2102:E2102"/>
+    <mergeCell ref="C2119:E2119"/>
+    <mergeCell ref="C2136:E2136"/>
+    <mergeCell ref="C2153:E2153"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -26030,150 +26032,163 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="33">
-      <c r="A1" s="211" t="s">
+      <c r="A1" s="210" t="s">
         <v>184</v>
       </c>
-      <c r="B1" s="212"/>
+      <c r="B1" s="211"/>
       <c r="C1" s="118"/>
       <c r="D1" s="5"/>
       <c r="E1" s="5"/>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="217" t="s">
+      <c r="A2" s="207" t="s">
         <v>183</v>
       </c>
-      <c r="B2" s="218"/>
+      <c r="B2" s="208"/>
       <c r="C2" s="120"/>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="219" t="s">
+      <c r="A3" s="209" t="s">
         <v>185</v>
       </c>
-      <c r="B3" s="218"/>
+      <c r="B3" s="208"/>
       <c r="C3" s="120"/>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="215"/>
-      <c r="B4" s="216"/>
+      <c r="A4" s="214"/>
+      <c r="B4" s="215"/>
       <c r="C4" s="120"/>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="213" t="s">
+      <c r="A5" s="212" t="s">
         <v>194</v>
       </c>
-      <c r="B5" s="214"/>
+      <c r="B5" s="213"/>
       <c r="C5" s="120"/>
     </row>
     <row r="7" spans="1:5" ht="18.75">
-      <c r="A7" s="205" t="s">
+      <c r="A7" s="218" t="s">
         <v>186</v>
       </c>
-      <c r="B7" s="206"/>
+      <c r="B7" s="219"/>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="120"/>
       <c r="B8" s="9"/>
     </row>
     <row r="9" spans="1:5" ht="39" customHeight="1">
-      <c r="A9" s="207" t="s">
+      <c r="A9" s="216" t="s">
         <v>187</v>
       </c>
-      <c r="B9" s="208"/>
+      <c r="B9" s="217"/>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="209"/>
-      <c r="B10" s="210"/>
+      <c r="A10" s="203"/>
+      <c r="B10" s="204"/>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="201" t="s">
+      <c r="A11" s="205" t="s">
         <v>188</v>
       </c>
-      <c r="B11" s="202"/>
+      <c r="B11" s="206"/>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="201" t="s">
+      <c r="A12" s="205" t="s">
         <v>189</v>
       </c>
-      <c r="B12" s="202"/>
+      <c r="B12" s="206"/>
     </row>
     <row r="13" spans="1:5" ht="43.5" customHeight="1">
-      <c r="A13" s="201" t="s">
+      <c r="A13" s="205" t="s">
         <v>190</v>
       </c>
-      <c r="B13" s="202"/>
+      <c r="B13" s="206"/>
     </row>
     <row r="14" spans="1:5" ht="19.5" customHeight="1">
-      <c r="A14" s="201" t="s">
+      <c r="A14" s="205" t="s">
         <v>191</v>
       </c>
-      <c r="B14" s="202"/>
+      <c r="B14" s="206"/>
     </row>
     <row r="15" spans="1:5" ht="18" customHeight="1">
-      <c r="A15" s="201" t="s">
+      <c r="A15" s="205" t="s">
         <v>192</v>
       </c>
-      <c r="B15" s="202"/>
+      <c r="B15" s="206"/>
     </row>
     <row r="16" spans="1:5" ht="21" customHeight="1">
-      <c r="A16" s="201" t="s">
+      <c r="A16" s="205" t="s">
         <v>193</v>
       </c>
-      <c r="B16" s="202"/>
+      <c r="B16" s="206"/>
     </row>
     <row r="17" spans="1:2" ht="48.75" customHeight="1">
-      <c r="A17" s="203" t="s">
+      <c r="A17" s="201" t="s">
         <v>195</v>
       </c>
-      <c r="B17" s="204"/>
+      <c r="B17" s="202"/>
     </row>
     <row r="19" spans="1:2" ht="18.75">
-      <c r="A19" s="205" t="s">
+      <c r="A19" s="218" t="s">
         <v>197</v>
       </c>
-      <c r="B19" s="206"/>
+      <c r="B19" s="219"/>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="120"/>
       <c r="B20" s="9"/>
     </row>
     <row r="21" spans="1:2">
-      <c r="A21" s="207" t="s">
+      <c r="A21" s="216" t="s">
         <v>198</v>
       </c>
-      <c r="B21" s="208"/>
+      <c r="B21" s="217"/>
     </row>
     <row r="22" spans="1:2">
-      <c r="A22" s="209"/>
-      <c r="B22" s="210"/>
+      <c r="A22" s="203"/>
+      <c r="B22" s="204"/>
     </row>
     <row r="23" spans="1:2">
-      <c r="A23" s="201" t="s">
+      <c r="A23" s="205" t="s">
         <v>199</v>
       </c>
-      <c r="B23" s="202"/>
+      <c r="B23" s="206"/>
     </row>
     <row r="24" spans="1:2">
-      <c r="A24" s="201"/>
-      <c r="B24" s="202"/>
+      <c r="A24" s="205"/>
+      <c r="B24" s="206"/>
     </row>
     <row r="25" spans="1:2">
-      <c r="A25" s="201" t="s">
+      <c r="A25" s="205" t="s">
         <v>200</v>
       </c>
-      <c r="B25" s="202"/>
+      <c r="B25" s="206"/>
     </row>
     <row r="26" spans="1:2">
-      <c r="A26" s="201" t="s">
+      <c r="A26" s="205" t="s">
         <v>201</v>
       </c>
-      <c r="B26" s="202"/>
+      <c r="B26" s="206"/>
     </row>
     <row r="27" spans="1:2">
-      <c r="A27" s="203"/>
-      <c r="B27" s="204"/>
+      <c r="A27" s="201"/>
+      <c r="B27" s="202"/>
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A7:B7"/>
     <mergeCell ref="A17:B17"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
@@ -26184,19 +26199,6 @@
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="A14:B14"/>
     <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A24:B24"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A3" r:id="rId1"/>

</xml_diff>

<commit_message>
Tempo - some more progress
</commit_message>
<xml_diff>
--- a/trunk/Tempo/Tempo.xlsx
+++ b/trunk/Tempo/Tempo.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1151" uniqueCount="274">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1151" uniqueCount="275">
   <si>
     <t>Notes</t>
   </si>
@@ -882,6 +882,9 @@
   <si>
     <t>8961 = old</t>
   </si>
+  <si>
+    <t>Enter 1st teleport</t>
+  </si>
 </sst>
 </file>
 
@@ -891,10 +894,17 @@
     <numFmt numFmtId="164" formatCode="#,##0;[Red]#,##0"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="49">
+  <fonts count="50">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1850,34 +1860,34 @@
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="27" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="27" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="31" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="220">
+  <cellXfs count="221">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1885,208 +1895,208 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="21" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="25" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="26" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="27" fillId="13" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="28" fillId="13" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="13" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="13" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="13" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="13" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="28" fillId="13" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="30" fillId="16" borderId="23" xfId="2" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="30" fillId="16" borderId="23" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="16" borderId="23" xfId="2" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="31" fillId="16" borderId="23" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="16" borderId="22" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="16" borderId="22" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="27" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="29" fillId="0" borderId="27" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="27" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="30" fillId="0" borderId="27" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="3" fontId="31" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="30" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="29" fillId="0" borderId="30" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="29" fillId="0" borderId="29" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="31" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="29" fillId="17" borderId="31" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="29" fillId="18" borderId="31" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="29" fillId="19" borderId="31" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="30" fillId="20" borderId="23" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="30" fillId="20" borderId="23" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="32" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="30" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="30" fillId="0" borderId="30" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="30" fillId="0" borderId="29" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="32" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="30" fillId="17" borderId="31" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="30" fillId="18" borderId="31" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="30" fillId="19" borderId="31" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="31" fillId="20" borderId="23" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="31" fillId="20" borderId="23" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="20" borderId="22" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="20" borderId="22" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="30" fillId="21" borderId="23" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="30" fillId="21" borderId="23" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="21" borderId="23" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="31" fillId="21" borderId="23" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="21" borderId="22" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="21" borderId="22" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="16" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="41" fillId="16" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="20" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="41" fillId="20" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
-    <xf numFmtId="3" fontId="31" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="29" fillId="0" borderId="42" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="31" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="31" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="31" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="29" fillId="0" borderId="42" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="32" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="30" fillId="0" borderId="42" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="32" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="32" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="32" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="30" fillId="0" borderId="42" xfId="1" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2096,10 +2106,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2120,19 +2130,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="23" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="47" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="48" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="38" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="32" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="48" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="25" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="34" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="37" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="31" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="47" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="24" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="33" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="36" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="36" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="37" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
@@ -2142,130 +2155,130 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="21" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="35" fillId="21" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="20" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="35" fillId="20" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="37" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="23" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="32" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="38" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="33" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="39" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="40" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="16" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="35" fillId="16" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="22" fillId="14" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="20" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="23" fillId="14" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="14" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="14" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="14" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="14" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="48" fillId="22" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="49" fillId="22" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="48" fillId="22" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="49" fillId="22" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="48" fillId="22" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="49" fillId="22" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="46" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="47" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="47" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="4"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="4"/>
     </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="33" xfId="3" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="33" xfId="3" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" indent="4"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="46" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="46" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Accent1" xfId="2" builtinId="29"/>
@@ -2573,11 +2586,11 @@
   <sheetPr>
     <tabColor theme="4" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:K156"/>
+  <dimension ref="A1:K157"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C47" sqref="C47"/>
+      <selection pane="bottomLeft" activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" outlineLevelRow="2"/>
@@ -2605,7 +2618,7 @@
       <c r="F1" s="162"/>
       <c r="G1" s="140"/>
       <c r="H1" s="141">
-        <f>SUM(G1:G65538)</f>
+        <f>SUM(G1:G65539)</f>
         <v>0</v>
       </c>
       <c r="I1" s="141" t="s">
@@ -3332,7 +3345,7 @@
         <v>11282</v>
       </c>
       <c r="E44" s="123">
-        <f t="shared" ref="E44:E63" si="3">IF(AND(C44&gt;0,D44&gt;0), D44-C44, 0)</f>
+        <f t="shared" ref="E44:E64" si="3">IF(AND(C44&gt;0,D44&gt;0), D44-C44, 0)</f>
         <v>0</v>
       </c>
       <c r="F44" s="104"/>
@@ -3370,42 +3383,37 @@
     </row>
     <row r="47" spans="1:9" ht="15" outlineLevel="1">
       <c r="A47" s="156"/>
-      <c r="B47" s="150" t="s">
-        <v>228</v>
-      </c>
-      <c r="C47" s="101"/>
+      <c r="B47" s="220" t="s">
+        <v>274</v>
+      </c>
+      <c r="C47" s="101">
+        <v>13024</v>
+      </c>
       <c r="D47" s="101">
         <v>15531</v>
       </c>
       <c r="E47" s="123">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>2507</v>
       </c>
       <c r="F47" s="105"/>
     </row>
     <row r="48" spans="1:9" ht="15" outlineLevel="1">
       <c r="A48" s="156"/>
-      <c r="B48" s="149" t="s">
+      <c r="B48" s="220"/>
+      <c r="C48" s="101"/>
+      <c r="D48" s="101"/>
+      <c r="E48" s="123"/>
+      <c r="F48" s="105"/>
+    </row>
+    <row r="49" spans="1:6" ht="15" outlineLevel="1">
+      <c r="A49" s="156"/>
+      <c r="B49" s="149" t="s">
         <v>222</v>
-      </c>
-      <c r="C48" s="101"/>
-      <c r="D48" s="101">
-        <v>17009</v>
-      </c>
-      <c r="E48" s="123">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="F48" s="105"/>
-    </row>
-    <row r="49" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A49" s="156"/>
-      <c r="B49" s="150" t="s">
-        <v>229</v>
       </c>
       <c r="C49" s="101"/>
       <c r="D49" s="101">
-        <v>17390</v>
+        <v>17009</v>
       </c>
       <c r="E49" s="123">
         <f t="shared" si="3"/>
@@ -3413,14 +3421,14 @@
       </c>
       <c r="F49" s="105"/>
     </row>
-    <row r="50" spans="1:7" ht="15" outlineLevel="1">
+    <row r="50" spans="1:6" ht="15" outlineLevel="1">
       <c r="A50" s="156"/>
       <c r="B50" s="150" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C50" s="101"/>
       <c r="D50" s="101">
-        <v>17856</v>
+        <v>17390</v>
       </c>
       <c r="E50" s="123">
         <f t="shared" si="3"/>
@@ -3428,14 +3436,14 @@
       </c>
       <c r="F50" s="105"/>
     </row>
-    <row r="51" spans="1:7" ht="15" outlineLevel="1">
+    <row r="51" spans="1:6" ht="15" outlineLevel="1">
       <c r="A51" s="156"/>
       <c r="B51" s="150" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C51" s="101"/>
       <c r="D51" s="101">
-        <v>18332</v>
+        <v>17856</v>
       </c>
       <c r="E51" s="123">
         <f t="shared" si="3"/>
@@ -3443,14 +3451,14 @@
       </c>
       <c r="F51" s="105"/>
     </row>
-    <row r="52" spans="1:7" ht="15" outlineLevel="1">
+    <row r="52" spans="1:6" ht="15" outlineLevel="1">
       <c r="A52" s="156"/>
       <c r="B52" s="150" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C52" s="101"/>
       <c r="D52" s="101">
-        <v>18738</v>
+        <v>18332</v>
       </c>
       <c r="E52" s="123">
         <f t="shared" si="3"/>
@@ -3458,14 +3466,14 @@
       </c>
       <c r="F52" s="105"/>
     </row>
-    <row r="53" spans="1:7" ht="15" outlineLevel="1">
+    <row r="53" spans="1:6" ht="15" outlineLevel="1">
       <c r="A53" s="156"/>
       <c r="B53" s="150" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C53" s="101"/>
       <c r="D53" s="101">
-        <v>19757</v>
+        <v>18738</v>
       </c>
       <c r="E53" s="123">
         <f t="shared" si="3"/>
@@ -3473,14 +3481,14 @@
       </c>
       <c r="F53" s="105"/>
     </row>
-    <row r="54" spans="1:7" ht="15" outlineLevel="1">
+    <row r="54" spans="1:6" ht="15" outlineLevel="1">
       <c r="A54" s="156"/>
       <c r="B54" s="150" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C54" s="101"/>
       <c r="D54" s="101">
-        <v>20174</v>
+        <v>19757</v>
       </c>
       <c r="E54" s="123">
         <f t="shared" si="3"/>
@@ -3488,14 +3496,14 @@
       </c>
       <c r="F54" s="105"/>
     </row>
-    <row r="55" spans="1:7" ht="15" outlineLevel="1">
+    <row r="55" spans="1:6" ht="15" outlineLevel="1">
       <c r="A55" s="156"/>
       <c r="B55" s="150" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C55" s="101"/>
       <c r="D55" s="101">
-        <v>20965</v>
+        <v>20174</v>
       </c>
       <c r="E55" s="123">
         <f t="shared" si="3"/>
@@ -3503,18 +3511,22 @@
       </c>
       <c r="F55" s="105"/>
     </row>
-    <row r="56" spans="1:7" ht="15" outlineLevel="1">
+    <row r="56" spans="1:6" ht="15" outlineLevel="1">
       <c r="A56" s="156"/>
-      <c r="B56" s="100"/>
+      <c r="B56" s="150" t="s">
+        <v>236</v>
+      </c>
       <c r="C56" s="101"/>
-      <c r="D56" s="101"/>
+      <c r="D56" s="101">
+        <v>20965</v>
+      </c>
       <c r="E56" s="123">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="F56" s="105"/>
     </row>
-    <row r="57" spans="1:7" ht="15" outlineLevel="1">
+    <row r="57" spans="1:6" ht="15" outlineLevel="1">
       <c r="A57" s="156"/>
       <c r="B57" s="100"/>
       <c r="C57" s="101"/>
@@ -3525,11 +3537,9 @@
       </c>
       <c r="F57" s="105"/>
     </row>
-    <row r="58" spans="1:7" ht="15" outlineLevel="1">
+    <row r="58" spans="1:6" ht="15" outlineLevel="1">
       <c r="A58" s="156"/>
-      <c r="B58" s="150" t="s">
-        <v>237</v>
-      </c>
+      <c r="B58" s="100"/>
       <c r="C58" s="101"/>
       <c r="D58" s="101"/>
       <c r="E58" s="123">
@@ -3538,29 +3548,27 @@
       </c>
       <c r="F58" s="105"/>
     </row>
-    <row r="59" spans="1:7" ht="15" outlineLevel="1">
+    <row r="59" spans="1:6" ht="15" outlineLevel="1">
       <c r="A59" s="156"/>
       <c r="B59" s="150" t="s">
-        <v>223</v>
+        <v>237</v>
       </c>
       <c r="C59" s="101"/>
-      <c r="D59" s="101">
-        <v>23906</v>
-      </c>
+      <c r="D59" s="101"/>
       <c r="E59" s="123">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="F59" s="105"/>
     </row>
-    <row r="60" spans="1:7" ht="15" outlineLevel="1">
+    <row r="60" spans="1:6" ht="15" outlineLevel="1">
       <c r="A60" s="156"/>
       <c r="B60" s="150" t="s">
-        <v>238</v>
+        <v>223</v>
       </c>
       <c r="C60" s="101"/>
       <c r="D60" s="101">
-        <v>24132</v>
+        <v>23906</v>
       </c>
       <c r="E60" s="123">
         <f t="shared" si="3"/>
@@ -3568,133 +3576,133 @@
       </c>
       <c r="F60" s="105"/>
     </row>
-    <row r="61" spans="1:7" ht="15" outlineLevel="1">
+    <row r="61" spans="1:6" ht="15" outlineLevel="1">
       <c r="A61" s="156"/>
       <c r="B61" s="150" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C61" s="101"/>
       <c r="D61" s="101">
-        <v>24753</v>
-      </c>
-      <c r="E61" s="123"/>
+        <v>24132</v>
+      </c>
+      <c r="E61" s="123">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
       <c r="F61" s="105"/>
     </row>
-    <row r="62" spans="1:7" ht="15" outlineLevel="1">
+    <row r="62" spans="1:6" ht="15" outlineLevel="1">
       <c r="A62" s="156"/>
       <c r="B62" s="150" t="s">
-        <v>217</v>
+        <v>239</v>
       </c>
       <c r="C62" s="101"/>
       <c r="D62" s="101">
+        <v>24753</v>
+      </c>
+      <c r="E62" s="123"/>
+      <c r="F62" s="105"/>
+    </row>
+    <row r="63" spans="1:6" ht="15" outlineLevel="1">
+      <c r="A63" s="156"/>
+      <c r="B63" s="150" t="s">
+        <v>217</v>
+      </c>
+      <c r="C63" s="101"/>
+      <c r="D63" s="101">
         <v>25129</v>
       </c>
-      <c r="E62" s="123">
+      <c r="E63" s="123">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="F62" s="105"/>
-    </row>
-    <row r="63" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="A63" s="156"/>
-      <c r="B63" s="98" t="s">
+      <c r="F63" s="105"/>
+    </row>
+    <row r="64" spans="1:6" ht="15.75" outlineLevel="1" thickBot="1">
+      <c r="A64" s="156"/>
+      <c r="B64" s="98" t="s">
         <v>179</v>
       </c>
-      <c r="C63" s="99"/>
-      <c r="D63" s="99">
+      <c r="C64" s="99"/>
+      <c r="D64" s="99">
         <v>25174</v>
       </c>
-      <c r="E63" s="125">
+      <c r="E64" s="125">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="F63" s="104"/>
-    </row>
-    <row r="64" spans="1:7" ht="17.25" thickTop="1" thickBot="1">
-      <c r="A64" s="116" t="s">
+      <c r="F64" s="104"/>
+    </row>
+    <row r="65" spans="1:8" ht="17.25" thickTop="1" thickBot="1">
+      <c r="A65" s="116" t="s">
         <v>227</v>
       </c>
-      <c r="B64" s="102" t="s">
+      <c r="B65" s="102" t="s">
         <v>173</v>
       </c>
-      <c r="C64" s="103">
-        <f>C63-C44</f>
-        <v>0</v>
-      </c>
-      <c r="D64" s="103">
-        <f>D63-D44</f>
+      <c r="C65" s="103">
+        <f>C64-C44</f>
+        <v>0</v>
+      </c>
+      <c r="D65" s="103">
+        <f>D64-D44</f>
         <v>13892</v>
       </c>
-      <c r="E64" s="126">
-        <f>E63-E44</f>
-        <v>0</v>
-      </c>
-      <c r="F64" s="107"/>
-      <c r="G64" s="112">
-        <f>E64</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65" spans="1:8" ht="13.5" thickBot="1"/>
-    <row r="66" spans="1:8" ht="15" customHeight="1" outlineLevel="1">
-      <c r="A66" s="157" t="s">
+      <c r="E65" s="126">
+        <f>E64-E44</f>
+        <v>0</v>
+      </c>
+      <c r="F65" s="107"/>
+      <c r="G65" s="112">
+        <f>E65</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" ht="13.5" thickBot="1"/>
+    <row r="67" spans="1:8" ht="15" customHeight="1" outlineLevel="1">
+      <c r="A67" s="157" t="s">
         <v>240</v>
       </c>
-      <c r="B66" s="109" t="s">
+      <c r="B67" s="109" t="s">
         <v>175</v>
       </c>
-      <c r="C66" s="110" t="s">
+      <c r="C67" s="110" t="s">
         <v>42</v>
       </c>
-      <c r="D66" s="110" t="s">
+      <c r="D67" s="110" t="s">
         <v>41</v>
       </c>
-      <c r="E66" s="110" t="s">
+      <c r="E67" s="110" t="s">
         <v>43</v>
       </c>
-      <c r="F66" s="111" t="s">
+      <c r="F67" s="111" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="67" spans="1:8" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="A67" s="156"/>
-      <c r="B67" s="98" t="s">
+    <row r="68" spans="1:8" ht="15.75" outlineLevel="1" thickBot="1">
+      <c r="A68" s="156"/>
+      <c r="B68" s="98" t="s">
         <v>177</v>
       </c>
-      <c r="C67" s="99"/>
-      <c r="D67" s="99">
+      <c r="C68" s="99"/>
+      <c r="D68" s="99">
         <v>25174</v>
       </c>
-      <c r="E67" s="123">
-        <f t="shared" ref="E67:E79" si="4">IF(AND(C67&gt;0,D67&gt;0), D67-C67, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="F67" s="104"/>
-      <c r="H67">
+      <c r="E68" s="123">
+        <f t="shared" ref="E68:E80" si="4">IF(AND(C68&gt;0,D68&gt;0), D68-C68, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="F68" s="104"/>
+      <c r="H68">
         <v>49739</v>
       </c>
     </row>
-    <row r="68" spans="1:8" ht="15.75" outlineLevel="1" thickTop="1">
-      <c r="A68" s="156"/>
-      <c r="B68" s="100"/>
-      <c r="C68" s="101"/>
-      <c r="D68" s="101"/>
-      <c r="E68" s="124">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="F68" s="105"/>
-    </row>
-    <row r="69" spans="1:8" ht="15" outlineLevel="1">
+    <row r="69" spans="1:8" ht="15.75" outlineLevel="1" thickTop="1">
       <c r="A69" s="156"/>
-      <c r="B69" s="151" t="s">
-        <v>242</v>
-      </c>
+      <c r="B69" s="100"/>
       <c r="C69" s="101"/>
-      <c r="D69" s="101">
-        <v>26754</v>
-      </c>
-      <c r="E69" s="123">
+      <c r="D69" s="101"/>
+      <c r="E69" s="124">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -3702,9 +3710,13 @@
     </row>
     <row r="70" spans="1:8" ht="15" outlineLevel="1">
       <c r="A70" s="156"/>
-      <c r="B70" s="100"/>
+      <c r="B70" s="151" t="s">
+        <v>242</v>
+      </c>
       <c r="C70" s="101"/>
-      <c r="D70" s="101"/>
+      <c r="D70" s="101">
+        <v>26754</v>
+      </c>
       <c r="E70" s="123">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -3713,13 +3725,9 @@
     </row>
     <row r="71" spans="1:8" ht="15" outlineLevel="1">
       <c r="A71" s="156"/>
-      <c r="B71" s="151" t="s">
-        <v>243</v>
-      </c>
+      <c r="B71" s="100"/>
       <c r="C71" s="101"/>
-      <c r="D71" s="101">
-        <v>27765</v>
-      </c>
+      <c r="D71" s="101"/>
       <c r="E71" s="123">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -3728,9 +3736,13 @@
     </row>
     <row r="72" spans="1:8" ht="15" outlineLevel="1">
       <c r="A72" s="156"/>
-      <c r="B72" s="100"/>
+      <c r="B72" s="151" t="s">
+        <v>243</v>
+      </c>
       <c r="C72" s="101"/>
-      <c r="D72" s="101"/>
+      <c r="D72" s="101">
+        <v>27765</v>
+      </c>
       <c r="E72" s="123">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -3739,13 +3751,9 @@
     </row>
     <row r="73" spans="1:8" ht="15" outlineLevel="1">
       <c r="A73" s="156"/>
-      <c r="B73" s="151" t="s">
-        <v>244</v>
-      </c>
+      <c r="B73" s="100"/>
       <c r="C73" s="101"/>
-      <c r="D73" s="101">
-        <v>30127</v>
-      </c>
+      <c r="D73" s="101"/>
       <c r="E73" s="123">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -3754,9 +3762,13 @@
     </row>
     <row r="74" spans="1:8" ht="15" outlineLevel="1">
       <c r="A74" s="156"/>
-      <c r="B74" s="100"/>
+      <c r="B74" s="151" t="s">
+        <v>244</v>
+      </c>
       <c r="C74" s="101"/>
-      <c r="D74" s="101"/>
+      <c r="D74" s="101">
+        <v>30127</v>
+      </c>
       <c r="E74" s="123">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -3765,13 +3777,9 @@
     </row>
     <row r="75" spans="1:8" ht="15" outlineLevel="1">
       <c r="A75" s="156"/>
-      <c r="B75" s="151" t="s">
-        <v>245</v>
-      </c>
+      <c r="B75" s="100"/>
       <c r="C75" s="101"/>
-      <c r="D75" s="101">
-        <v>33299</v>
-      </c>
+      <c r="D75" s="101"/>
       <c r="E75" s="123">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -3781,11 +3789,11 @@
     <row r="76" spans="1:8" ht="15" outlineLevel="1">
       <c r="A76" s="156"/>
       <c r="B76" s="151" t="s">
-        <v>238</v>
+        <v>245</v>
       </c>
       <c r="C76" s="101"/>
       <c r="D76" s="101">
-        <v>33527</v>
+        <v>33299</v>
       </c>
       <c r="E76" s="123">
         <f t="shared" si="4"/>
@@ -3796,11 +3804,11 @@
     <row r="77" spans="1:8" ht="15" outlineLevel="1">
       <c r="A77" s="156"/>
       <c r="B77" s="151" t="s">
-        <v>246</v>
+        <v>238</v>
       </c>
       <c r="C77" s="101"/>
       <c r="D77" s="101">
-        <v>34309</v>
+        <v>33527</v>
       </c>
       <c r="E77" s="123">
         <f t="shared" si="4"/>
@@ -3811,11 +3819,11 @@
     <row r="78" spans="1:8" ht="15" outlineLevel="1">
       <c r="A78" s="156"/>
       <c r="B78" s="151" t="s">
-        <v>217</v>
+        <v>246</v>
       </c>
       <c r="C78" s="101"/>
       <c r="D78" s="101">
-        <v>34727</v>
+        <v>34309</v>
       </c>
       <c r="E78" s="123">
         <f t="shared" si="4"/>
@@ -3823,110 +3831,110 @@
       </c>
       <c r="F78" s="105"/>
     </row>
-    <row r="79" spans="1:8" ht="15.75" outlineLevel="1" thickBot="1">
+    <row r="79" spans="1:8" ht="15" outlineLevel="1">
       <c r="A79" s="156"/>
-      <c r="B79" s="98" t="s">
+      <c r="B79" s="151" t="s">
+        <v>217</v>
+      </c>
+      <c r="C79" s="101"/>
+      <c r="D79" s="101">
+        <v>34727</v>
+      </c>
+      <c r="E79" s="123">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="F79" s="105"/>
+    </row>
+    <row r="80" spans="1:8" ht="15.75" outlineLevel="1" thickBot="1">
+      <c r="A80" s="156"/>
+      <c r="B80" s="98" t="s">
         <v>179</v>
       </c>
-      <c r="C79" s="99"/>
-      <c r="D79" s="99">
+      <c r="C80" s="99"/>
+      <c r="D80" s="99">
         <v>34795</v>
       </c>
-      <c r="E79" s="125">
+      <c r="E80" s="125">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="F79" s="104"/>
-    </row>
-    <row r="80" spans="1:8" ht="17.25" thickTop="1" thickBot="1">
-      <c r="A80" s="117" t="s">
+      <c r="F80" s="104"/>
+    </row>
+    <row r="81" spans="1:8" ht="17.25" thickTop="1" thickBot="1">
+      <c r="A81" s="117" t="s">
         <v>241</v>
       </c>
-      <c r="B80" s="102" t="s">
+      <c r="B81" s="102" t="s">
         <v>173</v>
       </c>
-      <c r="C80" s="103">
-        <f>C79-C67</f>
-        <v>0</v>
-      </c>
-      <c r="D80" s="103">
-        <f>D79-D67</f>
+      <c r="C81" s="103">
+        <f>C80-C68</f>
+        <v>0</v>
+      </c>
+      <c r="D81" s="103">
+        <f>D80-D68</f>
         <v>9621</v>
       </c>
-      <c r="E80" s="126">
-        <f>E79-E67</f>
-        <v>0</v>
-      </c>
-      <c r="F80" s="108"/>
-      <c r="G80" s="112">
-        <f>E80</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="81" spans="1:8" ht="13.5" thickBot="1"/>
-    <row r="82" spans="1:8" ht="15" customHeight="1" outlineLevel="1">
-      <c r="A82" s="155" t="s">
+      <c r="E81" s="126">
+        <f>E80-E68</f>
+        <v>0</v>
+      </c>
+      <c r="F81" s="108"/>
+      <c r="G81" s="112">
+        <f>E81</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" ht="13.5" thickBot="1"/>
+    <row r="83" spans="1:8" ht="15" customHeight="1" outlineLevel="1">
+      <c r="A83" s="155" t="s">
         <v>247</v>
       </c>
-      <c r="B82" s="113" t="s">
+      <c r="B83" s="113" t="s">
         <v>175</v>
       </c>
-      <c r="C82" s="114" t="s">
+      <c r="C83" s="114" t="s">
         <v>42</v>
       </c>
-      <c r="D82" s="114" t="s">
+      <c r="D83" s="114" t="s">
         <v>41</v>
       </c>
-      <c r="E82" s="114" t="s">
+      <c r="E83" s="114" t="s">
         <v>43</v>
       </c>
-      <c r="F82" s="115" t="s">
+      <c r="F83" s="115" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="83" spans="1:8" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="A83" s="156"/>
-      <c r="B83" s="98" t="s">
+    <row r="84" spans="1:8" ht="15.75" outlineLevel="1" thickBot="1">
+      <c r="A84" s="156"/>
+      <c r="B84" s="98" t="s">
         <v>177</v>
       </c>
-      <c r="C83" s="99"/>
-      <c r="D83" s="99">
+      <c r="C84" s="99"/>
+      <c r="D84" s="99">
         <v>34795</v>
       </c>
-      <c r="E83" s="123">
-        <f t="shared" ref="E83:E96" si="5">IF(AND(C83&gt;0,D83&gt;0), D83-C83, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="F83" s="104"/>
-      <c r="H83">
+      <c r="E84" s="123">
+        <f t="shared" ref="E84:E97" si="5">IF(AND(C84&gt;0,D84&gt;0), D84-C84, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="F84" s="104"/>
+      <c r="H84">
         <v>67476</v>
       </c>
     </row>
-    <row r="84" spans="1:8" ht="15.75" outlineLevel="1" thickTop="1">
-      <c r="A84" s="156"/>
-      <c r="B84" s="151" t="s">
-        <v>228</v>
-      </c>
-      <c r="C84" s="101"/>
-      <c r="D84" s="101">
-        <v>36326</v>
-      </c>
-      <c r="E84" s="124">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="F84" s="105"/>
-    </row>
-    <row r="85" spans="1:8" ht="15" outlineLevel="1">
+    <row r="85" spans="1:8" ht="15.75" outlineLevel="1" thickTop="1">
       <c r="A85" s="156"/>
       <c r="B85" s="151" t="s">
-        <v>221</v>
+        <v>228</v>
       </c>
       <c r="C85" s="101"/>
       <c r="D85" s="101">
-        <v>37764</v>
-      </c>
-      <c r="E85" s="123">
+        <v>36326</v>
+      </c>
+      <c r="E85" s="124">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -3934,9 +3942,13 @@
     </row>
     <row r="86" spans="1:8" ht="15" outlineLevel="1">
       <c r="A86" s="156"/>
-      <c r="B86" s="100"/>
+      <c r="B86" s="151" t="s">
+        <v>221</v>
+      </c>
       <c r="C86" s="101"/>
-      <c r="D86" s="101"/>
+      <c r="D86" s="101">
+        <v>37764</v>
+      </c>
       <c r="E86" s="123">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -3945,13 +3957,9 @@
     </row>
     <row r="87" spans="1:8" ht="15" outlineLevel="1">
       <c r="A87" s="156"/>
-      <c r="B87" s="151" t="s">
-        <v>222</v>
-      </c>
+      <c r="B87" s="100"/>
       <c r="C87" s="101"/>
-      <c r="D87" s="101">
-        <v>43241</v>
-      </c>
+      <c r="D87" s="101"/>
       <c r="E87" s="123">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -3960,9 +3968,13 @@
     </row>
     <row r="88" spans="1:8" ht="15" outlineLevel="1">
       <c r="A88" s="156"/>
-      <c r="B88" s="100"/>
+      <c r="B88" s="151" t="s">
+        <v>222</v>
+      </c>
       <c r="C88" s="101"/>
-      <c r="D88" s="101"/>
+      <c r="D88" s="101">
+        <v>43241</v>
+      </c>
       <c r="E88" s="123">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -3971,13 +3983,9 @@
     </row>
     <row r="89" spans="1:8" ht="15" outlineLevel="1">
       <c r="A89" s="156"/>
-      <c r="B89" s="152" t="s">
-        <v>236</v>
-      </c>
+      <c r="B89" s="100"/>
       <c r="C89" s="101"/>
-      <c r="D89" s="101">
-        <v>45890</v>
-      </c>
+      <c r="D89" s="101"/>
       <c r="E89" s="123">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -3986,9 +3994,13 @@
     </row>
     <row r="90" spans="1:8" ht="15" outlineLevel="1">
       <c r="A90" s="156"/>
-      <c r="B90" s="100"/>
+      <c r="B90" s="152" t="s">
+        <v>236</v>
+      </c>
       <c r="C90" s="101"/>
-      <c r="D90" s="101"/>
+      <c r="D90" s="101">
+        <v>45890</v>
+      </c>
       <c r="E90" s="123">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -4008,13 +4020,9 @@
     </row>
     <row r="92" spans="1:8" ht="15" outlineLevel="1">
       <c r="A92" s="156"/>
-      <c r="B92" s="152" t="s">
-        <v>223</v>
-      </c>
+      <c r="B92" s="100"/>
       <c r="C92" s="101"/>
-      <c r="D92" s="101">
-        <v>49269</v>
-      </c>
+      <c r="D92" s="101"/>
       <c r="E92" s="123">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -4024,11 +4032,11 @@
     <row r="93" spans="1:8" ht="15" outlineLevel="1">
       <c r="A93" s="156"/>
       <c r="B93" s="152" t="s">
-        <v>249</v>
+        <v>223</v>
       </c>
       <c r="C93" s="101"/>
       <c r="D93" s="101">
-        <v>49505</v>
+        <v>49269</v>
       </c>
       <c r="E93" s="123">
         <f t="shared" si="5"/>
@@ -4039,11 +4047,11 @@
     <row r="94" spans="1:8" ht="15" outlineLevel="1">
       <c r="A94" s="156"/>
       <c r="B94" s="152" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C94" s="101"/>
       <c r="D94" s="101">
-        <v>50134</v>
+        <v>49505</v>
       </c>
       <c r="E94" s="123">
         <f t="shared" si="5"/>
@@ -4054,11 +4062,11 @@
     <row r="95" spans="1:8" ht="15" outlineLevel="1">
       <c r="A95" s="156"/>
       <c r="B95" s="152" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C95" s="101"/>
       <c r="D95" s="101">
-        <v>50516</v>
+        <v>50134</v>
       </c>
       <c r="E95" s="123">
         <f t="shared" si="5"/>
@@ -4066,106 +4074,106 @@
       </c>
       <c r="F95" s="105"/>
     </row>
-    <row r="96" spans="1:8" ht="15.75" outlineLevel="1" thickBot="1">
+    <row r="96" spans="1:8" ht="15" outlineLevel="1">
       <c r="A96" s="156"/>
-      <c r="B96" s="98" t="s">
+      <c r="B96" s="152" t="s">
+        <v>251</v>
+      </c>
+      <c r="C96" s="101"/>
+      <c r="D96" s="101">
+        <v>50516</v>
+      </c>
+      <c r="E96" s="123">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="F96" s="105"/>
+    </row>
+    <row r="97" spans="1:8" ht="15.75" outlineLevel="1" thickBot="1">
+      <c r="A97" s="156"/>
+      <c r="B97" s="98" t="s">
         <v>179</v>
       </c>
-      <c r="C96" s="99"/>
-      <c r="D96" s="99">
+      <c r="C97" s="99"/>
+      <c r="D97" s="99">
         <v>50574</v>
       </c>
-      <c r="E96" s="125">
+      <c r="E97" s="125">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="F96" s="104"/>
-    </row>
-    <row r="97" spans="1:8" ht="17.25" thickTop="1" thickBot="1">
-      <c r="A97" s="116" t="s">
+      <c r="F97" s="104"/>
+    </row>
+    <row r="98" spans="1:8" ht="17.25" thickTop="1" thickBot="1">
+      <c r="A98" s="116" t="s">
         <v>248</v>
       </c>
-      <c r="B97" s="102" t="s">
+      <c r="B98" s="102" t="s">
         <v>173</v>
       </c>
-      <c r="C97" s="103">
-        <f>C96-C83</f>
-        <v>0</v>
-      </c>
-      <c r="D97" s="103">
-        <f>D96-D83</f>
+      <c r="C98" s="103">
+        <f>C97-C84</f>
+        <v>0</v>
+      </c>
+      <c r="D98" s="103">
+        <f>D97-D84</f>
         <v>15779</v>
       </c>
-      <c r="E97" s="126">
-        <f>E96-E83</f>
-        <v>0</v>
-      </c>
-      <c r="F97" s="107"/>
-      <c r="G97" s="112">
-        <f>E97</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="98" spans="1:8" ht="13.5" thickBot="1"/>
-    <row r="99" spans="1:8" ht="15" customHeight="1" outlineLevel="1">
-      <c r="A99" s="157" t="s">
+      <c r="E98" s="126">
+        <f>E97-E84</f>
+        <v>0</v>
+      </c>
+      <c r="F98" s="107"/>
+      <c r="G98" s="112">
+        <f>E98</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" ht="13.5" thickBot="1"/>
+    <row r="100" spans="1:8" ht="15" customHeight="1" outlineLevel="1">
+      <c r="A100" s="157" t="s">
         <v>252</v>
       </c>
-      <c r="B99" s="109" t="s">
+      <c r="B100" s="109" t="s">
         <v>175</v>
       </c>
-      <c r="C99" s="110" t="s">
+      <c r="C100" s="110" t="s">
         <v>42</v>
       </c>
-      <c r="D99" s="110" t="s">
+      <c r="D100" s="110" t="s">
         <v>41</v>
       </c>
-      <c r="E99" s="110" t="s">
+      <c r="E100" s="110" t="s">
         <v>43</v>
       </c>
-      <c r="F99" s="111" t="s">
+      <c r="F100" s="111" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="100" spans="1:8" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="A100" s="156"/>
-      <c r="B100" s="98" t="s">
+    <row r="101" spans="1:8" ht="15.75" outlineLevel="1" thickBot="1">
+      <c r="A101" s="156"/>
+      <c r="B101" s="98" t="s">
         <v>177</v>
       </c>
-      <c r="C100" s="99"/>
-      <c r="D100" s="99">
+      <c r="C101" s="99"/>
+      <c r="D101" s="99">
         <v>50574</v>
       </c>
-      <c r="E100" s="123">
-        <f t="shared" ref="E100:E109" si="6">IF(AND(C100&gt;0,D100&gt;0), D100-C100, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="F100" s="104"/>
-      <c r="H100">
+      <c r="E101" s="123">
+        <f t="shared" ref="E101:E110" si="6">IF(AND(C101&gt;0,D101&gt;0), D101-C101, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="F101" s="104"/>
+      <c r="H101">
         <v>105030</v>
       </c>
     </row>
-    <row r="101" spans="1:8" ht="15.75" outlineLevel="1" thickTop="1">
-      <c r="A101" s="156"/>
-      <c r="B101" s="100"/>
-      <c r="C101" s="101"/>
-      <c r="D101" s="101"/>
-      <c r="E101" s="124">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="F101" s="105"/>
-    </row>
-    <row r="102" spans="1:8" ht="15" outlineLevel="1">
+    <row r="102" spans="1:8" ht="15.75" outlineLevel="1" thickTop="1">
       <c r="A102" s="156"/>
-      <c r="B102" s="152" t="s">
-        <v>254</v>
-      </c>
+      <c r="B102" s="100"/>
       <c r="C102" s="101"/>
-      <c r="D102" s="101">
-        <v>52785</v>
-      </c>
-      <c r="E102" s="123">
+      <c r="D102" s="101"/>
+      <c r="E102" s="124">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
@@ -4173,9 +4181,13 @@
     </row>
     <row r="103" spans="1:8" ht="15" outlineLevel="1">
       <c r="A103" s="156"/>
-      <c r="B103" s="100"/>
+      <c r="B103" s="152" t="s">
+        <v>254</v>
+      </c>
       <c r="C103" s="101"/>
-      <c r="D103" s="101"/>
+      <c r="D103" s="101">
+        <v>52785</v>
+      </c>
       <c r="E103" s="123">
         <f t="shared" si="6"/>
         <v>0</v>
@@ -4184,13 +4196,9 @@
     </row>
     <row r="104" spans="1:8" ht="15" outlineLevel="1">
       <c r="A104" s="156"/>
-      <c r="B104" s="152" t="s">
-        <v>255</v>
-      </c>
+      <c r="B104" s="100"/>
       <c r="C104" s="101"/>
-      <c r="D104" s="101">
-        <v>53409</v>
-      </c>
+      <c r="D104" s="101"/>
       <c r="E104" s="123">
         <f t="shared" si="6"/>
         <v>0</v>
@@ -4199,9 +4207,13 @@
     </row>
     <row r="105" spans="1:8" ht="15" outlineLevel="1">
       <c r="A105" s="156"/>
-      <c r="B105" s="100"/>
+      <c r="B105" s="152" t="s">
+        <v>255</v>
+      </c>
       <c r="C105" s="101"/>
-      <c r="D105" s="101"/>
+      <c r="D105" s="101">
+        <v>53409</v>
+      </c>
       <c r="E105" s="123">
         <f t="shared" si="6"/>
         <v>0</v>
@@ -4210,13 +4222,9 @@
     </row>
     <row r="106" spans="1:8" ht="15" outlineLevel="1">
       <c r="A106" s="156"/>
-      <c r="B106" s="152" t="s">
-        <v>223</v>
-      </c>
+      <c r="B106" s="100"/>
       <c r="C106" s="101"/>
-      <c r="D106" s="101">
-        <v>55728</v>
-      </c>
+      <c r="D106" s="101"/>
       <c r="E106" s="123">
         <f t="shared" si="6"/>
         <v>0</v>
@@ -4226,11 +4234,11 @@
     <row r="107" spans="1:8" ht="15" outlineLevel="1">
       <c r="A107" s="156"/>
       <c r="B107" s="152" t="s">
-        <v>249</v>
+        <v>223</v>
       </c>
       <c r="C107" s="101"/>
       <c r="D107" s="101">
-        <v>55956</v>
+        <v>55728</v>
       </c>
       <c r="E107" s="123">
         <f t="shared" si="6"/>
@@ -4241,11 +4249,11 @@
     <row r="108" spans="1:8" ht="15" outlineLevel="1">
       <c r="A108" s="156"/>
       <c r="B108" s="152" t="s">
-        <v>256</v>
+        <v>249</v>
       </c>
       <c r="C108" s="101"/>
       <c r="D108" s="101">
-        <v>56314</v>
+        <v>55956</v>
       </c>
       <c r="E108" s="123">
         <f t="shared" si="6"/>
@@ -4253,110 +4261,110 @@
       </c>
       <c r="F108" s="105"/>
     </row>
-    <row r="109" spans="1:8" ht="15.75" outlineLevel="1" thickBot="1">
+    <row r="109" spans="1:8" ht="15" outlineLevel="1">
       <c r="A109" s="156"/>
-      <c r="B109" s="98" t="s">
+      <c r="B109" s="152" t="s">
+        <v>256</v>
+      </c>
+      <c r="C109" s="101"/>
+      <c r="D109" s="101">
+        <v>56314</v>
+      </c>
+      <c r="E109" s="123">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="F109" s="105"/>
+    </row>
+    <row r="110" spans="1:8" ht="15.75" outlineLevel="1" thickBot="1">
+      <c r="A110" s="156"/>
+      <c r="B110" s="98" t="s">
         <v>179</v>
       </c>
-      <c r="C109" s="99"/>
-      <c r="D109" s="99">
+      <c r="C110" s="99"/>
+      <c r="D110" s="99">
         <v>56373</v>
       </c>
-      <c r="E109" s="125">
+      <c r="E110" s="125">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="F109" s="104"/>
-    </row>
-    <row r="110" spans="1:8" ht="17.25" thickTop="1" thickBot="1">
-      <c r="A110" s="117" t="s">
+      <c r="F110" s="104"/>
+    </row>
+    <row r="111" spans="1:8" ht="17.25" thickTop="1" thickBot="1">
+      <c r="A111" s="117" t="s">
         <v>253</v>
       </c>
-      <c r="B110" s="102" t="s">
+      <c r="B111" s="102" t="s">
         <v>173</v>
       </c>
-      <c r="C110" s="103">
-        <f>C109-C100</f>
-        <v>0</v>
-      </c>
-      <c r="D110" s="103">
-        <f>D109-D100</f>
+      <c r="C111" s="103">
+        <f>C110-C101</f>
+        <v>0</v>
+      </c>
+      <c r="D111" s="103">
+        <f>D110-D101</f>
         <v>5799</v>
       </c>
-      <c r="E110" s="126">
-        <f>E109-E100</f>
-        <v>0</v>
-      </c>
-      <c r="F110" s="108"/>
-      <c r="G110" s="112">
-        <f>E110</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="111" spans="1:8" ht="13.5" thickBot="1"/>
-    <row r="112" spans="1:8" ht="15" customHeight="1" outlineLevel="1">
-      <c r="A112" s="155" t="s">
+      <c r="E111" s="126">
+        <f>E110-E101</f>
+        <v>0</v>
+      </c>
+      <c r="F111" s="108"/>
+      <c r="G111" s="112">
+        <f>E111</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:8" ht="13.5" thickBot="1"/>
+    <row r="113" spans="1:9" ht="15" customHeight="1" outlineLevel="1">
+      <c r="A113" s="155" t="s">
         <v>257</v>
       </c>
-      <c r="B112" s="113" t="s">
+      <c r="B113" s="113" t="s">
         <v>175</v>
       </c>
-      <c r="C112" s="114" t="s">
+      <c r="C113" s="114" t="s">
         <v>42</v>
       </c>
-      <c r="D112" s="114" t="s">
+      <c r="D113" s="114" t="s">
         <v>41</v>
       </c>
-      <c r="E112" s="114" t="s">
+      <c r="E113" s="114" t="s">
         <v>43</v>
       </c>
-      <c r="F112" s="115" t="s">
+      <c r="F113" s="115" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="113" spans="1:9" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="A113" s="156"/>
-      <c r="B113" s="98" t="s">
+    <row r="114" spans="1:9" ht="15.75" outlineLevel="1" thickBot="1">
+      <c r="A114" s="156"/>
+      <c r="B114" s="98" t="s">
         <v>177</v>
       </c>
-      <c r="C113" s="99"/>
-      <c r="D113" s="99">
+      <c r="C114" s="99"/>
+      <c r="D114" s="99">
         <v>56373</v>
       </c>
-      <c r="E113" s="123">
-        <f t="shared" ref="E113:E121" si="7">IF(AND(C113&gt;0,D113&gt;0), D113-C113, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="F113" s="104"/>
-      <c r="H113">
+      <c r="E114" s="123">
+        <f t="shared" ref="E114:E122" si="7">IF(AND(C114&gt;0,D114&gt;0), D114-C114, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="F114" s="104"/>
+      <c r="H114">
         <v>125564</v>
       </c>
-      <c r="I113" s="112">
-        <f>H113-D113</f>
+      <c r="I114" s="112">
+        <f>H114-D114</f>
         <v>69191</v>
       </c>
     </row>
-    <row r="114" spans="1:9" ht="15.75" outlineLevel="1" thickTop="1">
-      <c r="A114" s="156"/>
-      <c r="B114" s="100"/>
-      <c r="C114" s="101"/>
-      <c r="D114" s="101"/>
-      <c r="E114" s="124">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="F114" s="105"/>
-    </row>
-    <row r="115" spans="1:9" ht="15" outlineLevel="1">
+    <row r="115" spans="1:9" ht="15.75" outlineLevel="1" thickTop="1">
       <c r="A115" s="156"/>
-      <c r="B115" s="152" t="s">
-        <v>221</v>
-      </c>
+      <c r="B115" s="100"/>
       <c r="C115" s="101"/>
-      <c r="D115" s="101">
-        <v>58041</v>
-      </c>
-      <c r="E115" s="123">
+      <c r="D115" s="101"/>
+      <c r="E115" s="124">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -4364,9 +4372,13 @@
     </row>
     <row r="116" spans="1:9" ht="15" outlineLevel="1">
       <c r="A116" s="156"/>
-      <c r="B116" s="100"/>
+      <c r="B116" s="152" t="s">
+        <v>221</v>
+      </c>
       <c r="C116" s="101"/>
-      <c r="D116" s="101"/>
+      <c r="D116" s="101">
+        <v>58041</v>
+      </c>
       <c r="E116" s="123">
         <f t="shared" si="7"/>
         <v>0</v>
@@ -4375,13 +4387,9 @@
     </row>
     <row r="117" spans="1:9" ht="15" outlineLevel="1">
       <c r="A117" s="156"/>
-      <c r="B117" s="152" t="s">
-        <v>222</v>
-      </c>
+      <c r="B117" s="100"/>
       <c r="C117" s="101"/>
-      <c r="D117" s="101">
-        <v>60301</v>
-      </c>
+      <c r="D117" s="101"/>
       <c r="E117" s="123">
         <f t="shared" si="7"/>
         <v>0</v>
@@ -4391,11 +4399,11 @@
     <row r="118" spans="1:9" ht="15" outlineLevel="1">
       <c r="A118" s="156"/>
       <c r="B118" s="152" t="s">
-        <v>249</v>
+        <v>222</v>
       </c>
       <c r="C118" s="101"/>
-      <c r="D118" s="153">
-        <v>60529</v>
+      <c r="D118" s="101">
+        <v>60301</v>
       </c>
       <c r="E118" s="123">
         <f t="shared" si="7"/>
@@ -4406,11 +4414,11 @@
     <row r="119" spans="1:9" ht="15" outlineLevel="1">
       <c r="A119" s="156"/>
       <c r="B119" s="152" t="s">
-        <v>259</v>
+        <v>249</v>
       </c>
       <c r="C119" s="101"/>
-      <c r="D119" s="101">
-        <v>61068</v>
+      <c r="D119" s="153">
+        <v>60529</v>
       </c>
       <c r="E119" s="123">
         <f t="shared" si="7"/>
@@ -4421,11 +4429,11 @@
     <row r="120" spans="1:9" ht="15" outlineLevel="1">
       <c r="A120" s="156"/>
       <c r="B120" s="152" t="s">
-        <v>224</v>
+        <v>259</v>
       </c>
       <c r="C120" s="101"/>
       <c r="D120" s="101">
-        <v>61391</v>
+        <v>61068</v>
       </c>
       <c r="E120" s="123">
         <f t="shared" si="7"/>
@@ -4433,106 +4441,110 @@
       </c>
       <c r="F120" s="105"/>
     </row>
-    <row r="121" spans="1:9" ht="15.75" outlineLevel="1" thickBot="1">
+    <row r="121" spans="1:9" ht="15" outlineLevel="1">
       <c r="A121" s="156"/>
-      <c r="B121" s="98" t="s">
+      <c r="B121" s="152" t="s">
+        <v>224</v>
+      </c>
+      <c r="C121" s="101"/>
+      <c r="D121" s="101">
+        <v>61391</v>
+      </c>
+      <c r="E121" s="123">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="F121" s="105"/>
+    </row>
+    <row r="122" spans="1:9" ht="15.75" outlineLevel="1" thickBot="1">
+      <c r="A122" s="156"/>
+      <c r="B122" s="98" t="s">
         <v>179</v>
       </c>
-      <c r="C121" s="99"/>
-      <c r="D121" s="99">
+      <c r="C122" s="99"/>
+      <c r="D122" s="99">
         <v>61438</v>
       </c>
-      <c r="E121" s="125">
+      <c r="E122" s="125">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="F121" s="104"/>
-    </row>
-    <row r="122" spans="1:9" ht="17.25" thickTop="1" thickBot="1">
-      <c r="A122" s="116" t="s">
+      <c r="F122" s="104"/>
+    </row>
+    <row r="123" spans="1:9" ht="17.25" thickTop="1" thickBot="1">
+      <c r="A123" s="116" t="s">
         <v>258</v>
       </c>
-      <c r="B122" s="102" t="s">
+      <c r="B123" s="102" t="s">
         <v>173</v>
       </c>
-      <c r="C122" s="103">
-        <f>C121-C113</f>
-        <v>0</v>
-      </c>
-      <c r="D122" s="103">
-        <f>D121-D113</f>
+      <c r="C123" s="103">
+        <f>C122-C114</f>
+        <v>0</v>
+      </c>
+      <c r="D123" s="103">
+        <f>D122-D114</f>
         <v>5065</v>
       </c>
-      <c r="E122" s="103">
-        <f>E121-E113</f>
-        <v>0</v>
-      </c>
-      <c r="F122" s="107"/>
-      <c r="G122" s="112">
-        <f>E122</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="123" spans="1:9" ht="13.5" thickBot="1"/>
-    <row r="124" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A124" s="157" t="s">
+      <c r="E123" s="103">
+        <f>E122-E114</f>
+        <v>0</v>
+      </c>
+      <c r="F123" s="107"/>
+      <c r="G123" s="112">
+        <f>E123</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="1:9" ht="13.5" thickBot="1"/>
+    <row r="125" spans="1:9" ht="15" outlineLevel="1">
+      <c r="A125" s="157" t="s">
         <v>260</v>
       </c>
-      <c r="B124" s="109" t="s">
+      <c r="B125" s="109" t="s">
         <v>175</v>
       </c>
-      <c r="C124" s="110" t="s">
+      <c r="C125" s="110" t="s">
         <v>42</v>
       </c>
-      <c r="D124" s="110" t="s">
+      <c r="D125" s="110" t="s">
         <v>41</v>
       </c>
-      <c r="E124" s="110" t="s">
+      <c r="E125" s="110" t="s">
         <v>43</v>
       </c>
-      <c r="F124" s="111" t="s">
+      <c r="F125" s="111" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="125" spans="1:9" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="A125" s="156"/>
-      <c r="B125" s="98" t="s">
+    <row r="126" spans="1:9" ht="15.75" outlineLevel="1" thickBot="1">
+      <c r="A126" s="156"/>
+      <c r="B126" s="98" t="s">
         <v>177</v>
       </c>
-      <c r="C125" s="99"/>
-      <c r="D125" s="99">
+      <c r="C126" s="99"/>
+      <c r="D126" s="99">
         <v>61438</v>
       </c>
-      <c r="E125" s="123">
-        <f t="shared" ref="E125:E138" si="8">IF(AND(C125&gt;0,D125&gt;0), D125-C125, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="F125" s="104"/>
-      <c r="H125">
+      <c r="E126" s="123">
+        <f t="shared" ref="E126:E139" si="8">IF(AND(C126&gt;0,D126&gt;0), D126-C126, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="F126" s="104"/>
+      <c r="H126">
         <v>135506</v>
       </c>
-      <c r="I125" s="112">
-        <f>H125-D125</f>
+      <c r="I126" s="112">
+        <f>H126-D126</f>
         <v>74068</v>
       </c>
     </row>
-    <row r="126" spans="1:9" ht="15.75" outlineLevel="1" thickTop="1">
-      <c r="A126" s="156"/>
-      <c r="B126" s="100"/>
-      <c r="C126" s="101"/>
-      <c r="D126" s="101"/>
-      <c r="E126" s="124">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="F126" s="105"/>
-    </row>
-    <row r="127" spans="1:9" ht="15" outlineLevel="1">
+    <row r="127" spans="1:9" ht="15.75" outlineLevel="1" thickTop="1">
       <c r="A127" s="156"/>
       <c r="B127" s="100"/>
       <c r="C127" s="101"/>
       <c r="D127" s="101"/>
-      <c r="E127" s="123">
+      <c r="E127" s="124">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
@@ -4606,36 +4618,36 @@
     </row>
     <row r="134" spans="1:9" ht="15" outlineLevel="1">
       <c r="A134" s="156"/>
-      <c r="B134" s="152" t="s">
-        <v>262</v>
-      </c>
+      <c r="B134" s="100"/>
       <c r="C134" s="101"/>
-      <c r="D134" s="101">
-        <v>66926</v>
-      </c>
+      <c r="D134" s="101"/>
       <c r="E134" s="123">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="F134" s="105"/>
-      <c r="H134">
-        <v>160118</v>
-      </c>
-      <c r="I134" s="112">
-        <f>H134-D134</f>
-        <v>93192</v>
-      </c>
     </row>
     <row r="135" spans="1:9" ht="15" outlineLevel="1">
       <c r="A135" s="156"/>
-      <c r="B135" s="100"/>
+      <c r="B135" s="152" t="s">
+        <v>262</v>
+      </c>
       <c r="C135" s="101"/>
-      <c r="D135" s="101"/>
+      <c r="D135" s="101">
+        <v>66926</v>
+      </c>
       <c r="E135" s="123">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="F135" s="105"/>
+      <c r="H135">
+        <v>160118</v>
+      </c>
+      <c r="I135" s="112">
+        <f>H135-D135</f>
+        <v>93192</v>
+      </c>
     </row>
     <row r="136" spans="1:9" ht="15" outlineLevel="1">
       <c r="A136" s="156"/>
@@ -4659,94 +4671,94 @@
       </c>
       <c r="F137" s="105"/>
     </row>
-    <row r="138" spans="1:9" ht="15.75" outlineLevel="1" thickBot="1">
+    <row r="138" spans="1:9" ht="15" outlineLevel="1">
       <c r="A138" s="156"/>
-      <c r="B138" s="98" t="s">
+      <c r="B138" s="100"/>
+      <c r="C138" s="101"/>
+      <c r="D138" s="101"/>
+      <c r="E138" s="123">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="F138" s="105"/>
+    </row>
+    <row r="139" spans="1:9" ht="15.75" outlineLevel="1" thickBot="1">
+      <c r="A139" s="156"/>
+      <c r="B139" s="98" t="s">
         <v>179</v>
       </c>
-      <c r="C138" s="99"/>
-      <c r="D138" s="99"/>
-      <c r="E138" s="125">
+      <c r="C139" s="99"/>
+      <c r="D139" s="99"/>
+      <c r="E139" s="125">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="F138" s="104"/>
-    </row>
-    <row r="139" spans="1:9" ht="17.25" thickTop="1" thickBot="1">
-      <c r="A139" s="117" t="s">
+      <c r="F139" s="104"/>
+    </row>
+    <row r="140" spans="1:9" ht="17.25" thickTop="1" thickBot="1">
+      <c r="A140" s="117" t="s">
         <v>261</v>
       </c>
-      <c r="B139" s="102" t="s">
+      <c r="B140" s="102" t="s">
         <v>173</v>
       </c>
-      <c r="C139" s="103">
-        <f>C138-C125</f>
-        <v>0</v>
-      </c>
-      <c r="D139" s="103">
-        <f>D138-D125</f>
+      <c r="C140" s="103">
+        <f>C139-C126</f>
+        <v>0</v>
+      </c>
+      <c r="D140" s="103">
+        <f>D139-D126</f>
         <v>-61438</v>
       </c>
-      <c r="E139" s="103">
-        <f>E138-E125</f>
-        <v>0</v>
-      </c>
-      <c r="F139" s="108"/>
-      <c r="G139" s="112">
-        <f>E139</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="141" spans="1:9" ht="15" hidden="1" outlineLevel="2">
-      <c r="A141" s="155" t="s">
+      <c r="E140" s="103">
+        <f>E139-E126</f>
+        <v>0</v>
+      </c>
+      <c r="F140" s="108"/>
+      <c r="G140" s="112">
+        <f>E140</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="142" spans="1:9" ht="15" hidden="1" outlineLevel="2">
+      <c r="A142" s="155" t="s">
         <v>169</v>
       </c>
-      <c r="B141" s="113" t="s">
+      <c r="B142" s="113" t="s">
         <v>175</v>
       </c>
-      <c r="C141" s="114" t="s">
+      <c r="C142" s="114" t="s">
         <v>42</v>
       </c>
-      <c r="D141" s="114" t="s">
+      <c r="D142" s="114" t="s">
         <v>41</v>
       </c>
-      <c r="E141" s="114" t="s">
+      <c r="E142" s="114" t="s">
         <v>43</v>
       </c>
-      <c r="F141" s="115" t="s">
+      <c r="F142" s="115" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="142" spans="1:9" ht="15.75" hidden="1" outlineLevel="2" thickBot="1">
-      <c r="A142" s="156"/>
-      <c r="B142" s="98" t="s">
+    <row r="143" spans="1:9" ht="15.75" hidden="1" outlineLevel="2" thickBot="1">
+      <c r="A143" s="156"/>
+      <c r="B143" s="98" t="s">
         <v>177</v>
       </c>
-      <c r="C142" s="99"/>
-      <c r="D142" s="99"/>
-      <c r="E142" s="123">
-        <f t="shared" ref="E142:E155" si="9">IF(AND(C142&gt;0,D142&gt;0), D142-C142, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="F142" s="104"/>
-    </row>
-    <row r="143" spans="1:9" ht="15.75" hidden="1" outlineLevel="2" thickTop="1">
-      <c r="A143" s="156"/>
-      <c r="B143" s="100"/>
-      <c r="C143" s="101"/>
-      <c r="D143" s="101"/>
-      <c r="E143" s="124">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="F143" s="105"/>
-    </row>
-    <row r="144" spans="1:9" ht="15" hidden="1" outlineLevel="2">
+      <c r="C143" s="99"/>
+      <c r="D143" s="99"/>
+      <c r="E143" s="123">
+        <f t="shared" ref="E143:E156" si="9">IF(AND(C143&gt;0,D143&gt;0), D143-C143, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="F143" s="104"/>
+    </row>
+    <row r="144" spans="1:9" ht="15.75" hidden="1" outlineLevel="2" thickTop="1">
       <c r="A144" s="156"/>
       <c r="B144" s="100"/>
       <c r="C144" s="101"/>
       <c r="D144" s="101"/>
-      <c r="E144" s="123">
+      <c r="E144" s="124">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
@@ -4862,48 +4874,64 @@
       </c>
       <c r="F154" s="105"/>
     </row>
-    <row r="155" spans="1:7" ht="15.75" hidden="1" outlineLevel="2" thickBot="1">
+    <row r="155" spans="1:7" ht="15" hidden="1" outlineLevel="2">
       <c r="A155" s="156"/>
-      <c r="B155" s="98" t="s">
+      <c r="B155" s="100"/>
+      <c r="C155" s="101"/>
+      <c r="D155" s="101"/>
+      <c r="E155" s="123">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="F155" s="105"/>
+    </row>
+    <row r="156" spans="1:7" ht="15.75" hidden="1" outlineLevel="2" thickBot="1">
+      <c r="A156" s="156"/>
+      <c r="B156" s="98" t="s">
         <v>179</v>
       </c>
-      <c r="C155" s="99"/>
-      <c r="D155" s="99"/>
-      <c r="E155" s="125">
+      <c r="C156" s="99"/>
+      <c r="D156" s="99"/>
+      <c r="E156" s="125">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="F155" s="104"/>
-    </row>
-    <row r="156" spans="1:7" ht="16.5" collapsed="1" thickBot="1">
-      <c r="A156" s="116">
+      <c r="F156" s="104"/>
+    </row>
+    <row r="157" spans="1:7" ht="16.5" collapsed="1" thickBot="1">
+      <c r="A157" s="116">
         <v>8</v>
       </c>
-      <c r="B156" s="102" t="s">
+      <c r="B157" s="102" t="s">
         <v>173</v>
       </c>
-      <c r="C156" s="103">
-        <f>C155-C142</f>
-        <v>0</v>
-      </c>
-      <c r="D156" s="103">
-        <f>D155-D142</f>
-        <v>0</v>
-      </c>
-      <c r="E156" s="103">
-        <f>E155-E142</f>
-        <v>0</v>
-      </c>
-      <c r="F156" s="107"/>
-      <c r="G156" s="112">
-        <f>E156</f>
+      <c r="C157" s="103">
+        <f>C156-C143</f>
+        <v>0</v>
+      </c>
+      <c r="D157" s="103">
+        <f>D156-D143</f>
+        <v>0</v>
+      </c>
+      <c r="E157" s="103">
+        <f>E156-E143</f>
+        <v>0</v>
+      </c>
+      <c r="F157" s="107"/>
+      <c r="G157" s="112">
+        <f>E157</f>
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="A43:A63"/>
-    <mergeCell ref="A66:A79"/>
+    <mergeCell ref="A142:A156"/>
+    <mergeCell ref="A113:A122"/>
+    <mergeCell ref="A83:A97"/>
+    <mergeCell ref="A125:A139"/>
+    <mergeCell ref="A100:A110"/>
+    <mergeCell ref="A43:A64"/>
+    <mergeCell ref="A67:A80"/>
     <mergeCell ref="C5:D5"/>
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="A1:B1"/>
@@ -4911,11 +4939,6 @@
     <mergeCell ref="A8:A18"/>
     <mergeCell ref="A21:A40"/>
     <mergeCell ref="C4:E4"/>
-    <mergeCell ref="A141:A155"/>
-    <mergeCell ref="A112:A121"/>
-    <mergeCell ref="A82:A96"/>
-    <mergeCell ref="A124:A138"/>
-    <mergeCell ref="A99:A109"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4947,13 +4970,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="26.25" customHeight="1">
-      <c r="A1" s="183" t="s">
+      <c r="A1" s="165" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="183"/>
-      <c r="C1" s="183"/>
-      <c r="D1" s="183"/>
-      <c r="E1" s="183"/>
+      <c r="B1" s="165"/>
+      <c r="C1" s="165"/>
+      <c r="D1" s="165"/>
+      <c r="E1" s="165"/>
       <c r="F1" s="7"/>
       <c r="G1" s="5"/>
       <c r="H1" s="5"/>
@@ -4983,18 +5006,18 @@
         <v>8</v>
       </c>
       <c r="B3" s="36"/>
-      <c r="C3" s="184"/>
-      <c r="D3" s="185"/>
-      <c r="E3" s="185"/>
+      <c r="C3" s="166"/>
+      <c r="D3" s="167"/>
+      <c r="E3" s="167"/>
     </row>
     <row r="4" spans="1:8" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A4" s="46" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="87"/>
-      <c r="C4" s="165"/>
-      <c r="D4" s="166"/>
-      <c r="E4" s="166"/>
+      <c r="C4" s="168"/>
+      <c r="D4" s="169"/>
+      <c r="E4" s="169"/>
       <c r="F4" s="6"/>
     </row>
     <row r="5" spans="1:8" hidden="1" outlineLevel="2">
@@ -5146,9 +5169,9 @@
         <v>9</v>
       </c>
       <c r="B21" s="90"/>
-      <c r="C21" s="167"/>
-      <c r="D21" s="168"/>
-      <c r="E21" s="168"/>
+      <c r="C21" s="170"/>
+      <c r="D21" s="171"/>
+      <c r="E21" s="171"/>
     </row>
     <row r="22" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A22" s="47">
@@ -5299,9 +5322,9 @@
         <v>10</v>
       </c>
       <c r="B38" s="87"/>
-      <c r="C38" s="165"/>
-      <c r="D38" s="166"/>
-      <c r="E38" s="166"/>
+      <c r="C38" s="168"/>
+      <c r="D38" s="169"/>
+      <c r="E38" s="169"/>
     </row>
     <row r="39" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A39" s="47">
@@ -5452,9 +5475,9 @@
         <v>11</v>
       </c>
       <c r="B55" s="87"/>
-      <c r="C55" s="165"/>
-      <c r="D55" s="166"/>
-      <c r="E55" s="166"/>
+      <c r="C55" s="168"/>
+      <c r="D55" s="169"/>
+      <c r="E55" s="169"/>
     </row>
     <row r="56" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A56" s="47">
@@ -5605,9 +5628,9 @@
         <v>12</v>
       </c>
       <c r="B72" s="87"/>
-      <c r="C72" s="165"/>
-      <c r="D72" s="166"/>
-      <c r="E72" s="166"/>
+      <c r="C72" s="168"/>
+      <c r="D72" s="169"/>
+      <c r="E72" s="169"/>
     </row>
     <row r="73" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A73" s="47">
@@ -5758,9 +5781,9 @@
         <v>13</v>
       </c>
       <c r="B89" s="87"/>
-      <c r="C89" s="165"/>
-      <c r="D89" s="166"/>
-      <c r="E89" s="166"/>
+      <c r="C89" s="168"/>
+      <c r="D89" s="169"/>
+      <c r="E89" s="169"/>
     </row>
     <row r="90" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A90" s="47">
@@ -5911,9 +5934,9 @@
         <v>14</v>
       </c>
       <c r="B106" s="87"/>
-      <c r="C106" s="165"/>
-      <c r="D106" s="166"/>
-      <c r="E106" s="166"/>
+      <c r="C106" s="168"/>
+      <c r="D106" s="169"/>
+      <c r="E106" s="169"/>
     </row>
     <row r="107" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A107" s="47">
@@ -6064,9 +6087,9 @@
         <v>15</v>
       </c>
       <c r="B123" s="87"/>
-      <c r="C123" s="165"/>
-      <c r="D123" s="166"/>
-      <c r="E123" s="166"/>
+      <c r="C123" s="168"/>
+      <c r="D123" s="169"/>
+      <c r="E123" s="169"/>
     </row>
     <row r="124" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A124" s="47">
@@ -6217,9 +6240,9 @@
         <v>16</v>
       </c>
       <c r="B140" s="87"/>
-      <c r="C140" s="165"/>
-      <c r="D140" s="166"/>
-      <c r="E140" s="166"/>
+      <c r="C140" s="168"/>
+      <c r="D140" s="169"/>
+      <c r="E140" s="169"/>
     </row>
     <row r="141" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A141" s="47">
@@ -6370,9 +6393,9 @@
         <v>17</v>
       </c>
       <c r="B157" s="87"/>
-      <c r="C157" s="165"/>
-      <c r="D157" s="166"/>
-      <c r="E157" s="166"/>
+      <c r="C157" s="168"/>
+      <c r="D157" s="169"/>
+      <c r="E157" s="169"/>
     </row>
     <row r="158" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A158" s="47">
@@ -6523,9 +6546,9 @@
         <v>18</v>
       </c>
       <c r="B174" s="87"/>
-      <c r="C174" s="165"/>
-      <c r="D174" s="166"/>
-      <c r="E174" s="166"/>
+      <c r="C174" s="168"/>
+      <c r="D174" s="169"/>
+      <c r="E174" s="169"/>
     </row>
     <row r="175" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A175" s="47">
@@ -6676,9 +6699,9 @@
         <v>19</v>
       </c>
       <c r="B191" s="87"/>
-      <c r="C191" s="165"/>
-      <c r="D191" s="166"/>
-      <c r="E191" s="166"/>
+      <c r="C191" s="168"/>
+      <c r="D191" s="169"/>
+      <c r="E191" s="169"/>
     </row>
     <row r="192" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A192" s="47">
@@ -6829,9 +6852,9 @@
         <v>20</v>
       </c>
       <c r="B208" s="87"/>
-      <c r="C208" s="165"/>
-      <c r="D208" s="166"/>
-      <c r="E208" s="166"/>
+      <c r="C208" s="168"/>
+      <c r="D208" s="169"/>
+      <c r="E208" s="169"/>
     </row>
     <row r="209" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A209" s="47">
@@ -6982,9 +7005,9 @@
         <v>21</v>
       </c>
       <c r="B225" s="87"/>
-      <c r="C225" s="165"/>
-      <c r="D225" s="166"/>
-      <c r="E225" s="166"/>
+      <c r="C225" s="168"/>
+      <c r="D225" s="169"/>
+      <c r="E225" s="169"/>
     </row>
     <row r="226" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A226" s="47">
@@ -7135,9 +7158,9 @@
         <v>22</v>
       </c>
       <c r="B242" s="87"/>
-      <c r="C242" s="165"/>
-      <c r="D242" s="166"/>
-      <c r="E242" s="166"/>
+      <c r="C242" s="168"/>
+      <c r="D242" s="169"/>
+      <c r="E242" s="169"/>
     </row>
     <row r="243" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A243" s="47">
@@ -7288,9 +7311,9 @@
         <v>23</v>
       </c>
       <c r="B259" s="87"/>
-      <c r="C259" s="165"/>
-      <c r="D259" s="166"/>
-      <c r="E259" s="166"/>
+      <c r="C259" s="168"/>
+      <c r="D259" s="169"/>
+      <c r="E259" s="169"/>
     </row>
     <row r="260" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A260" s="47">
@@ -7441,18 +7464,18 @@
         <v>24</v>
       </c>
       <c r="B276" s="37"/>
-      <c r="C276" s="181"/>
-      <c r="D276" s="182"/>
-      <c r="E276" s="182"/>
+      <c r="C276" s="172"/>
+      <c r="D276" s="173"/>
+      <c r="E276" s="173"/>
     </row>
     <row r="277" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A277" s="51" t="s">
         <v>25</v>
       </c>
       <c r="B277" s="87"/>
-      <c r="C277" s="165"/>
-      <c r="D277" s="166"/>
-      <c r="E277" s="166"/>
+      <c r="C277" s="168"/>
+      <c r="D277" s="169"/>
+      <c r="E277" s="169"/>
     </row>
     <row r="278" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A278" s="52">
@@ -7603,9 +7626,9 @@
         <v>26</v>
       </c>
       <c r="B294" s="90"/>
-      <c r="C294" s="167"/>
-      <c r="D294" s="168"/>
-      <c r="E294" s="168"/>
+      <c r="C294" s="170"/>
+      <c r="D294" s="171"/>
+      <c r="E294" s="171"/>
     </row>
     <row r="295" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A295" s="52">
@@ -7756,9 +7779,9 @@
         <v>27</v>
       </c>
       <c r="B311" s="87"/>
-      <c r="C311" s="165"/>
-      <c r="D311" s="166"/>
-      <c r="E311" s="166"/>
+      <c r="C311" s="168"/>
+      <c r="D311" s="169"/>
+      <c r="E311" s="169"/>
     </row>
     <row r="312" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A312" s="52">
@@ -7909,9 +7932,9 @@
         <v>28</v>
       </c>
       <c r="B328" s="87"/>
-      <c r="C328" s="165"/>
-      <c r="D328" s="166"/>
-      <c r="E328" s="166"/>
+      <c r="C328" s="168"/>
+      <c r="D328" s="169"/>
+      <c r="E328" s="169"/>
     </row>
     <row r="329" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A329" s="52">
@@ -8062,9 +8085,9 @@
         <v>29</v>
       </c>
       <c r="B345" s="87"/>
-      <c r="C345" s="165"/>
-      <c r="D345" s="166"/>
-      <c r="E345" s="166"/>
+      <c r="C345" s="168"/>
+      <c r="D345" s="169"/>
+      <c r="E345" s="169"/>
     </row>
     <row r="346" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A346" s="52">
@@ -8215,9 +8238,9 @@
         <v>30</v>
       </c>
       <c r="B362" s="87"/>
-      <c r="C362" s="165"/>
-      <c r="D362" s="166"/>
-      <c r="E362" s="166"/>
+      <c r="C362" s="168"/>
+      <c r="D362" s="169"/>
+      <c r="E362" s="169"/>
     </row>
     <row r="363" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A363" s="52">
@@ -8368,9 +8391,9 @@
         <v>31</v>
       </c>
       <c r="B379" s="87"/>
-      <c r="C379" s="165"/>
-      <c r="D379" s="166"/>
-      <c r="E379" s="166"/>
+      <c r="C379" s="168"/>
+      <c r="D379" s="169"/>
+      <c r="E379" s="169"/>
     </row>
     <row r="380" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A380" s="52">
@@ -8521,9 +8544,9 @@
         <v>32</v>
       </c>
       <c r="B396" s="87"/>
-      <c r="C396" s="165"/>
-      <c r="D396" s="166"/>
-      <c r="E396" s="166"/>
+      <c r="C396" s="168"/>
+      <c r="D396" s="169"/>
+      <c r="E396" s="169"/>
     </row>
     <row r="397" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A397" s="52">
@@ -8674,9 +8697,9 @@
         <v>33</v>
       </c>
       <c r="B413" s="87"/>
-      <c r="C413" s="165"/>
-      <c r="D413" s="166"/>
-      <c r="E413" s="166"/>
+      <c r="C413" s="168"/>
+      <c r="D413" s="169"/>
+      <c r="E413" s="169"/>
     </row>
     <row r="414" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A414" s="52">
@@ -8827,9 +8850,9 @@
         <v>34</v>
       </c>
       <c r="B430" s="87"/>
-      <c r="C430" s="165"/>
-      <c r="D430" s="166"/>
-      <c r="E430" s="166"/>
+      <c r="C430" s="168"/>
+      <c r="D430" s="169"/>
+      <c r="E430" s="169"/>
     </row>
     <row r="431" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A431" s="52">
@@ -8980,9 +9003,9 @@
         <v>35</v>
       </c>
       <c r="B447" s="87"/>
-      <c r="C447" s="165"/>
-      <c r="D447" s="166"/>
-      <c r="E447" s="166"/>
+      <c r="C447" s="168"/>
+      <c r="D447" s="169"/>
+      <c r="E447" s="169"/>
     </row>
     <row r="448" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A448" s="52">
@@ -9133,9 +9156,9 @@
         <v>36</v>
       </c>
       <c r="B464" s="87"/>
-      <c r="C464" s="165"/>
-      <c r="D464" s="166"/>
-      <c r="E464" s="166"/>
+      <c r="C464" s="168"/>
+      <c r="D464" s="169"/>
+      <c r="E464" s="169"/>
     </row>
     <row r="465" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A465" s="52">
@@ -9286,9 +9309,9 @@
         <v>37</v>
       </c>
       <c r="B481" s="87"/>
-      <c r="C481" s="165"/>
-      <c r="D481" s="166"/>
-      <c r="E481" s="166"/>
+      <c r="C481" s="168"/>
+      <c r="D481" s="169"/>
+      <c r="E481" s="169"/>
     </row>
     <row r="482" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A482" s="52">
@@ -9439,9 +9462,9 @@
         <v>38</v>
       </c>
       <c r="B498" s="87"/>
-      <c r="C498" s="165"/>
-      <c r="D498" s="166"/>
-      <c r="E498" s="166"/>
+      <c r="C498" s="168"/>
+      <c r="D498" s="169"/>
+      <c r="E498" s="169"/>
     </row>
     <row r="499" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A499" s="52">
@@ -9592,9 +9615,9 @@
         <v>39</v>
       </c>
       <c r="B515" s="87"/>
-      <c r="C515" s="165"/>
-      <c r="D515" s="166"/>
-      <c r="E515" s="166"/>
+      <c r="C515" s="168"/>
+      <c r="D515" s="169"/>
+      <c r="E515" s="169"/>
     </row>
     <row r="516" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A516" s="52">
@@ -9745,9 +9768,9 @@
         <v>40</v>
       </c>
       <c r="B532" s="87"/>
-      <c r="C532" s="165"/>
-      <c r="D532" s="166"/>
-      <c r="E532" s="166"/>
+      <c r="C532" s="168"/>
+      <c r="D532" s="169"/>
+      <c r="E532" s="169"/>
     </row>
     <row r="533" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A533" s="55">
@@ -9898,18 +9921,18 @@
         <v>50</v>
       </c>
       <c r="B549" s="38"/>
-      <c r="C549" s="179"/>
-      <c r="D549" s="180"/>
-      <c r="E549" s="180"/>
+      <c r="C549" s="174"/>
+      <c r="D549" s="175"/>
+      <c r="E549" s="175"/>
     </row>
     <row r="550" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A550" s="58" t="s">
         <v>51</v>
       </c>
       <c r="B550" s="87"/>
-      <c r="C550" s="165"/>
-      <c r="D550" s="166"/>
-      <c r="E550" s="166"/>
+      <c r="C550" s="168"/>
+      <c r="D550" s="169"/>
+      <c r="E550" s="169"/>
     </row>
     <row r="551" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A551" s="59">
@@ -10060,9 +10083,9 @@
         <v>52</v>
       </c>
       <c r="B567" s="90"/>
-      <c r="C567" s="167"/>
-      <c r="D567" s="168"/>
-      <c r="E567" s="168"/>
+      <c r="C567" s="170"/>
+      <c r="D567" s="171"/>
+      <c r="E567" s="171"/>
     </row>
     <row r="568" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A568" s="59">
@@ -10213,9 +10236,9 @@
         <v>53</v>
       </c>
       <c r="B584" s="87"/>
-      <c r="C584" s="165"/>
-      <c r="D584" s="166"/>
-      <c r="E584" s="166"/>
+      <c r="C584" s="168"/>
+      <c r="D584" s="169"/>
+      <c r="E584" s="169"/>
     </row>
     <row r="585" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A585" s="59">
@@ -10366,9 +10389,9 @@
         <v>54</v>
       </c>
       <c r="B601" s="87"/>
-      <c r="C601" s="165"/>
-      <c r="D601" s="166"/>
-      <c r="E601" s="166"/>
+      <c r="C601" s="168"/>
+      <c r="D601" s="169"/>
+      <c r="E601" s="169"/>
     </row>
     <row r="602" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A602" s="59">
@@ -10519,9 +10542,9 @@
         <v>55</v>
       </c>
       <c r="B618" s="87"/>
-      <c r="C618" s="165"/>
-      <c r="D618" s="166"/>
-      <c r="E618" s="166"/>
+      <c r="C618" s="168"/>
+      <c r="D618" s="169"/>
+      <c r="E618" s="169"/>
     </row>
     <row r="619" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A619" s="59">
@@ -10672,9 +10695,9 @@
         <v>56</v>
       </c>
       <c r="B635" s="87"/>
-      <c r="C635" s="165"/>
-      <c r="D635" s="166"/>
-      <c r="E635" s="166"/>
+      <c r="C635" s="168"/>
+      <c r="D635" s="169"/>
+      <c r="E635" s="169"/>
     </row>
     <row r="636" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A636" s="59">
@@ -10825,9 +10848,9 @@
         <v>57</v>
       </c>
       <c r="B652" s="87"/>
-      <c r="C652" s="165"/>
-      <c r="D652" s="166"/>
-      <c r="E652" s="166"/>
+      <c r="C652" s="168"/>
+      <c r="D652" s="169"/>
+      <c r="E652" s="169"/>
     </row>
     <row r="653" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A653" s="59">
@@ -10978,9 +11001,9 @@
         <v>58</v>
       </c>
       <c r="B669" s="87"/>
-      <c r="C669" s="165"/>
-      <c r="D669" s="166"/>
-      <c r="E669" s="166"/>
+      <c r="C669" s="168"/>
+      <c r="D669" s="169"/>
+      <c r="E669" s="169"/>
     </row>
     <row r="670" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A670" s="59">
@@ -11131,9 +11154,9 @@
         <v>59</v>
       </c>
       <c r="B686" s="87"/>
-      <c r="C686" s="165"/>
-      <c r="D686" s="166"/>
-      <c r="E686" s="166"/>
+      <c r="C686" s="168"/>
+      <c r="D686" s="169"/>
+      <c r="E686" s="169"/>
     </row>
     <row r="687" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A687" s="59">
@@ -11284,9 +11307,9 @@
         <v>60</v>
       </c>
       <c r="B703" s="87"/>
-      <c r="C703" s="165"/>
-      <c r="D703" s="166"/>
-      <c r="E703" s="166"/>
+      <c r="C703" s="168"/>
+      <c r="D703" s="169"/>
+      <c r="E703" s="169"/>
     </row>
     <row r="704" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A704" s="59">
@@ -11437,9 +11460,9 @@
         <v>61</v>
       </c>
       <c r="B720" s="87"/>
-      <c r="C720" s="165"/>
-      <c r="D720" s="166"/>
-      <c r="E720" s="166"/>
+      <c r="C720" s="168"/>
+      <c r="D720" s="169"/>
+      <c r="E720" s="169"/>
     </row>
     <row r="721" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A721" s="59">
@@ -11590,9 +11613,9 @@
         <v>62</v>
       </c>
       <c r="B737" s="87"/>
-      <c r="C737" s="165"/>
-      <c r="D737" s="166"/>
-      <c r="E737" s="166"/>
+      <c r="C737" s="168"/>
+      <c r="D737" s="169"/>
+      <c r="E737" s="169"/>
     </row>
     <row r="738" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A738" s="59">
@@ -11743,9 +11766,9 @@
         <v>63</v>
       </c>
       <c r="B754" s="87"/>
-      <c r="C754" s="165"/>
-      <c r="D754" s="166"/>
-      <c r="E754" s="166"/>
+      <c r="C754" s="168"/>
+      <c r="D754" s="169"/>
+      <c r="E754" s="169"/>
     </row>
     <row r="755" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A755" s="59">
@@ -11896,9 +11919,9 @@
         <v>64</v>
       </c>
       <c r="B771" s="87"/>
-      <c r="C771" s="165"/>
-      <c r="D771" s="166"/>
-      <c r="E771" s="166"/>
+      <c r="C771" s="168"/>
+      <c r="D771" s="169"/>
+      <c r="E771" s="169"/>
     </row>
     <row r="772" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A772" s="59">
@@ -12049,9 +12072,9 @@
         <v>65</v>
       </c>
       <c r="B788" s="87"/>
-      <c r="C788" s="165"/>
-      <c r="D788" s="166"/>
-      <c r="E788" s="166"/>
+      <c r="C788" s="168"/>
+      <c r="D788" s="169"/>
+      <c r="E788" s="169"/>
     </row>
     <row r="789" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A789" s="59">
@@ -12202,9 +12225,9 @@
         <v>66</v>
       </c>
       <c r="B805" s="87"/>
-      <c r="C805" s="165"/>
-      <c r="D805" s="166"/>
-      <c r="E805" s="166"/>
+      <c r="C805" s="168"/>
+      <c r="D805" s="169"/>
+      <c r="E805" s="169"/>
     </row>
     <row r="806" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A806" s="59">
@@ -12355,18 +12378,18 @@
         <v>67</v>
       </c>
       <c r="B822" s="39"/>
-      <c r="C822" s="177"/>
-      <c r="D822" s="178"/>
-      <c r="E822" s="178"/>
+      <c r="C822" s="176"/>
+      <c r="D822" s="177"/>
+      <c r="E822" s="177"/>
     </row>
     <row r="823" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A823" s="63" t="s">
         <v>68</v>
       </c>
       <c r="B823" s="87"/>
-      <c r="C823" s="165"/>
-      <c r="D823" s="166"/>
-      <c r="E823" s="166"/>
+      <c r="C823" s="168"/>
+      <c r="D823" s="169"/>
+      <c r="E823" s="169"/>
     </row>
     <row r="824" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A824" s="64">
@@ -12517,9 +12540,9 @@
         <v>69</v>
       </c>
       <c r="B840" s="90"/>
-      <c r="C840" s="167"/>
-      <c r="D840" s="168"/>
-      <c r="E840" s="168"/>
+      <c r="C840" s="170"/>
+      <c r="D840" s="171"/>
+      <c r="E840" s="171"/>
     </row>
     <row r="841" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A841" s="64">
@@ -12670,9 +12693,9 @@
         <v>70</v>
       </c>
       <c r="B857" s="87"/>
-      <c r="C857" s="165"/>
-      <c r="D857" s="166"/>
-      <c r="E857" s="166"/>
+      <c r="C857" s="168"/>
+      <c r="D857" s="169"/>
+      <c r="E857" s="169"/>
     </row>
     <row r="858" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A858" s="64">
@@ -12823,9 +12846,9 @@
         <v>71</v>
       </c>
       <c r="B874" s="87"/>
-      <c r="C874" s="165"/>
-      <c r="D874" s="166"/>
-      <c r="E874" s="166"/>
+      <c r="C874" s="168"/>
+      <c r="D874" s="169"/>
+      <c r="E874" s="169"/>
     </row>
     <row r="875" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A875" s="64">
@@ -12976,9 +12999,9 @@
         <v>72</v>
       </c>
       <c r="B891" s="87"/>
-      <c r="C891" s="165"/>
-      <c r="D891" s="166"/>
-      <c r="E891" s="166"/>
+      <c r="C891" s="168"/>
+      <c r="D891" s="169"/>
+      <c r="E891" s="169"/>
     </row>
     <row r="892" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A892" s="64">
@@ -13129,9 +13152,9 @@
         <v>73</v>
       </c>
       <c r="B908" s="87"/>
-      <c r="C908" s="165"/>
-      <c r="D908" s="166"/>
-      <c r="E908" s="166"/>
+      <c r="C908" s="168"/>
+      <c r="D908" s="169"/>
+      <c r="E908" s="169"/>
     </row>
     <row r="909" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A909" s="64">
@@ -13282,9 +13305,9 @@
         <v>74</v>
       </c>
       <c r="B925" s="87"/>
-      <c r="C925" s="165"/>
-      <c r="D925" s="166"/>
-      <c r="E925" s="166"/>
+      <c r="C925" s="168"/>
+      <c r="D925" s="169"/>
+      <c r="E925" s="169"/>
     </row>
     <row r="926" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A926" s="64">
@@ -13435,9 +13458,9 @@
         <v>75</v>
       </c>
       <c r="B942" s="87"/>
-      <c r="C942" s="165"/>
-      <c r="D942" s="166"/>
-      <c r="E942" s="166"/>
+      <c r="C942" s="168"/>
+      <c r="D942" s="169"/>
+      <c r="E942" s="169"/>
     </row>
     <row r="943" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A943" s="64">
@@ -13588,9 +13611,9 @@
         <v>76</v>
       </c>
       <c r="B959" s="87"/>
-      <c r="C959" s="165"/>
-      <c r="D959" s="166"/>
-      <c r="E959" s="166"/>
+      <c r="C959" s="168"/>
+      <c r="D959" s="169"/>
+      <c r="E959" s="169"/>
     </row>
     <row r="960" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A960" s="64">
@@ -13741,9 +13764,9 @@
         <v>77</v>
       </c>
       <c r="B976" s="87"/>
-      <c r="C976" s="165"/>
-      <c r="D976" s="166"/>
-      <c r="E976" s="166"/>
+      <c r="C976" s="168"/>
+      <c r="D976" s="169"/>
+      <c r="E976" s="169"/>
     </row>
     <row r="977" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A977" s="64">
@@ -13894,9 +13917,9 @@
         <v>78</v>
       </c>
       <c r="B993" s="87"/>
-      <c r="C993" s="165"/>
-      <c r="D993" s="166"/>
-      <c r="E993" s="166"/>
+      <c r="C993" s="168"/>
+      <c r="D993" s="169"/>
+      <c r="E993" s="169"/>
     </row>
     <row r="994" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A994" s="64">
@@ -14047,9 +14070,9 @@
         <v>79</v>
       </c>
       <c r="B1010" s="87"/>
-      <c r="C1010" s="165"/>
-      <c r="D1010" s="166"/>
-      <c r="E1010" s="166"/>
+      <c r="C1010" s="168"/>
+      <c r="D1010" s="169"/>
+      <c r="E1010" s="169"/>
     </row>
     <row r="1011" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1011" s="64">
@@ -14200,9 +14223,9 @@
         <v>80</v>
       </c>
       <c r="B1027" s="87"/>
-      <c r="C1027" s="165"/>
-      <c r="D1027" s="166"/>
-      <c r="E1027" s="166"/>
+      <c r="C1027" s="168"/>
+      <c r="D1027" s="169"/>
+      <c r="E1027" s="169"/>
     </row>
     <row r="1028" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1028" s="64">
@@ -14353,9 +14376,9 @@
         <v>83</v>
       </c>
       <c r="B1044" s="87"/>
-      <c r="C1044" s="165"/>
-      <c r="D1044" s="166"/>
-      <c r="E1044" s="166"/>
+      <c r="C1044" s="168"/>
+      <c r="D1044" s="169"/>
+      <c r="E1044" s="169"/>
     </row>
     <row r="1045" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1045" s="64">
@@ -14506,9 +14529,9 @@
         <v>82</v>
       </c>
       <c r="B1061" s="87"/>
-      <c r="C1061" s="165"/>
-      <c r="D1061" s="166"/>
-      <c r="E1061" s="166"/>
+      <c r="C1061" s="168"/>
+      <c r="D1061" s="169"/>
+      <c r="E1061" s="169"/>
     </row>
     <row r="1062" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1062" s="64">
@@ -14659,9 +14682,9 @@
         <v>84</v>
       </c>
       <c r="B1078" s="87"/>
-      <c r="C1078" s="165"/>
-      <c r="D1078" s="166"/>
-      <c r="E1078" s="166"/>
+      <c r="C1078" s="168"/>
+      <c r="D1078" s="169"/>
+      <c r="E1078" s="169"/>
     </row>
     <row r="1079" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1079" s="64">
@@ -14812,18 +14835,18 @@
         <v>104</v>
       </c>
       <c r="B1095" s="40"/>
-      <c r="C1095" s="175"/>
-      <c r="D1095" s="176"/>
-      <c r="E1095" s="176"/>
+      <c r="C1095" s="178"/>
+      <c r="D1095" s="179"/>
+      <c r="E1095" s="179"/>
     </row>
     <row r="1096" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A1096" s="68" t="s">
         <v>85</v>
       </c>
       <c r="B1096" s="87"/>
-      <c r="C1096" s="165"/>
-      <c r="D1096" s="166"/>
-      <c r="E1096" s="166"/>
+      <c r="C1096" s="168"/>
+      <c r="D1096" s="169"/>
+      <c r="E1096" s="169"/>
     </row>
     <row r="1097" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1097" s="69">
@@ -14974,9 +14997,9 @@
         <v>86</v>
       </c>
       <c r="B1113" s="90"/>
-      <c r="C1113" s="167"/>
-      <c r="D1113" s="168"/>
-      <c r="E1113" s="168"/>
+      <c r="C1113" s="170"/>
+      <c r="D1113" s="171"/>
+      <c r="E1113" s="171"/>
     </row>
     <row r="1114" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1114" s="69">
@@ -15127,9 +15150,9 @@
         <v>87</v>
       </c>
       <c r="B1130" s="87"/>
-      <c r="C1130" s="165"/>
-      <c r="D1130" s="166"/>
-      <c r="E1130" s="166"/>
+      <c r="C1130" s="168"/>
+      <c r="D1130" s="169"/>
+      <c r="E1130" s="169"/>
     </row>
     <row r="1131" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1131" s="69">
@@ -15280,9 +15303,9 @@
         <v>88</v>
       </c>
       <c r="B1147" s="87"/>
-      <c r="C1147" s="165"/>
-      <c r="D1147" s="166"/>
-      <c r="E1147" s="166"/>
+      <c r="C1147" s="168"/>
+      <c r="D1147" s="169"/>
+      <c r="E1147" s="169"/>
     </row>
     <row r="1148" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1148" s="69">
@@ -15433,9 +15456,9 @@
         <v>89</v>
       </c>
       <c r="B1164" s="87"/>
-      <c r="C1164" s="165"/>
-      <c r="D1164" s="166"/>
-      <c r="E1164" s="166"/>
+      <c r="C1164" s="168"/>
+      <c r="D1164" s="169"/>
+      <c r="E1164" s="169"/>
     </row>
     <row r="1165" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1165" s="69">
@@ -15586,9 +15609,9 @@
         <v>90</v>
       </c>
       <c r="B1181" s="87"/>
-      <c r="C1181" s="165"/>
-      <c r="D1181" s="166"/>
-      <c r="E1181" s="166"/>
+      <c r="C1181" s="168"/>
+      <c r="D1181" s="169"/>
+      <c r="E1181" s="169"/>
     </row>
     <row r="1182" spans="1:5" hidden="1" outlineLevel="3">
       <c r="A1182" s="69">
@@ -15739,9 +15762,9 @@
         <v>91</v>
       </c>
       <c r="B1198" s="87"/>
-      <c r="C1198" s="165"/>
-      <c r="D1198" s="166"/>
-      <c r="E1198" s="166"/>
+      <c r="C1198" s="168"/>
+      <c r="D1198" s="169"/>
+      <c r="E1198" s="169"/>
     </row>
     <row r="1199" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1199" s="69">
@@ -15892,9 +15915,9 @@
         <v>92</v>
       </c>
       <c r="B1215" s="87"/>
-      <c r="C1215" s="165"/>
-      <c r="D1215" s="166"/>
-      <c r="E1215" s="166"/>
+      <c r="C1215" s="168"/>
+      <c r="D1215" s="169"/>
+      <c r="E1215" s="169"/>
     </row>
     <row r="1216" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1216" s="69">
@@ -16045,9 +16068,9 @@
         <v>93</v>
       </c>
       <c r="B1232" s="87"/>
-      <c r="C1232" s="165"/>
-      <c r="D1232" s="166"/>
-      <c r="E1232" s="166"/>
+      <c r="C1232" s="168"/>
+      <c r="D1232" s="169"/>
+      <c r="E1232" s="169"/>
     </row>
     <row r="1233" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1233" s="69">
@@ -16198,9 +16221,9 @@
         <v>94</v>
       </c>
       <c r="B1249" s="87"/>
-      <c r="C1249" s="165"/>
-      <c r="D1249" s="166"/>
-      <c r="E1249" s="166"/>
+      <c r="C1249" s="168"/>
+      <c r="D1249" s="169"/>
+      <c r="E1249" s="169"/>
     </row>
     <row r="1250" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1250" s="69">
@@ -16351,9 +16374,9 @@
         <v>99</v>
       </c>
       <c r="B1266" s="87"/>
-      <c r="C1266" s="165"/>
-      <c r="D1266" s="166"/>
-      <c r="E1266" s="166"/>
+      <c r="C1266" s="168"/>
+      <c r="D1266" s="169"/>
+      <c r="E1266" s="169"/>
     </row>
     <row r="1267" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1267" s="69">
@@ -16504,9 +16527,9 @@
         <v>100</v>
       </c>
       <c r="B1283" s="87"/>
-      <c r="C1283" s="165"/>
-      <c r="D1283" s="166"/>
-      <c r="E1283" s="166"/>
+      <c r="C1283" s="168"/>
+      <c r="D1283" s="169"/>
+      <c r="E1283" s="169"/>
     </row>
     <row r="1284" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1284" s="69">
@@ -16657,9 +16680,9 @@
         <v>101</v>
       </c>
       <c r="B1300" s="87"/>
-      <c r="C1300" s="165"/>
-      <c r="D1300" s="166"/>
-      <c r="E1300" s="166"/>
+      <c r="C1300" s="168"/>
+      <c r="D1300" s="169"/>
+      <c r="E1300" s="169"/>
     </row>
     <row r="1301" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1301" s="69">
@@ -16810,9 +16833,9 @@
         <v>81</v>
       </c>
       <c r="B1317" s="87"/>
-      <c r="C1317" s="165"/>
-      <c r="D1317" s="166"/>
-      <c r="E1317" s="166"/>
+      <c r="C1317" s="168"/>
+      <c r="D1317" s="169"/>
+      <c r="E1317" s="169"/>
     </row>
     <row r="1318" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1318" s="69">
@@ -16963,9 +16986,9 @@
         <v>102</v>
       </c>
       <c r="B1334" s="87"/>
-      <c r="C1334" s="165"/>
-      <c r="D1334" s="166"/>
-      <c r="E1334" s="166"/>
+      <c r="C1334" s="168"/>
+      <c r="D1334" s="169"/>
+      <c r="E1334" s="169"/>
     </row>
     <row r="1335" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1335" s="69">
@@ -17116,9 +17139,9 @@
         <v>98</v>
       </c>
       <c r="B1351" s="87"/>
-      <c r="C1351" s="165"/>
-      <c r="D1351" s="166"/>
-      <c r="E1351" s="166"/>
+      <c r="C1351" s="168"/>
+      <c r="D1351" s="169"/>
+      <c r="E1351" s="169"/>
     </row>
     <row r="1352" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1352" s="69">
@@ -17269,18 +17292,18 @@
         <v>103</v>
       </c>
       <c r="B1368" s="41"/>
-      <c r="C1368" s="173"/>
-      <c r="D1368" s="174"/>
-      <c r="E1368" s="174"/>
+      <c r="C1368" s="180"/>
+      <c r="D1368" s="181"/>
+      <c r="E1368" s="181"/>
     </row>
     <row r="1369" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A1369" s="73" t="s">
         <v>105</v>
       </c>
       <c r="B1369" s="87"/>
-      <c r="C1369" s="165"/>
-      <c r="D1369" s="166"/>
-      <c r="E1369" s="166"/>
+      <c r="C1369" s="168"/>
+      <c r="D1369" s="169"/>
+      <c r="E1369" s="169"/>
     </row>
     <row r="1370" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1370" s="74">
@@ -17431,9 +17454,9 @@
         <v>106</v>
       </c>
       <c r="B1386" s="90"/>
-      <c r="C1386" s="167"/>
-      <c r="D1386" s="168"/>
-      <c r="E1386" s="168"/>
+      <c r="C1386" s="170"/>
+      <c r="D1386" s="171"/>
+      <c r="E1386" s="171"/>
     </row>
     <row r="1387" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1387" s="74">
@@ -17584,9 +17607,9 @@
         <v>107</v>
       </c>
       <c r="B1403" s="87"/>
-      <c r="C1403" s="165"/>
-      <c r="D1403" s="166"/>
-      <c r="E1403" s="166"/>
+      <c r="C1403" s="168"/>
+      <c r="D1403" s="169"/>
+      <c r="E1403" s="169"/>
     </row>
     <row r="1404" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1404" s="74">
@@ -17737,9 +17760,9 @@
         <v>108</v>
       </c>
       <c r="B1420" s="87"/>
-      <c r="C1420" s="165"/>
-      <c r="D1420" s="166"/>
-      <c r="E1420" s="166"/>
+      <c r="C1420" s="168"/>
+      <c r="D1420" s="169"/>
+      <c r="E1420" s="169"/>
     </row>
     <row r="1421" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1421" s="74">
@@ -17890,9 +17913,9 @@
         <v>109</v>
       </c>
       <c r="B1437" s="87"/>
-      <c r="C1437" s="165"/>
-      <c r="D1437" s="166"/>
-      <c r="E1437" s="166"/>
+      <c r="C1437" s="168"/>
+      <c r="D1437" s="169"/>
+      <c r="E1437" s="169"/>
     </row>
     <row r="1438" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1438" s="74">
@@ -18043,9 +18066,9 @@
         <v>110</v>
       </c>
       <c r="B1454" s="87"/>
-      <c r="C1454" s="165"/>
-      <c r="D1454" s="166"/>
-      <c r="E1454" s="166"/>
+      <c r="C1454" s="168"/>
+      <c r="D1454" s="169"/>
+      <c r="E1454" s="169"/>
     </row>
     <row r="1455" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1455" s="74">
@@ -18196,9 +18219,9 @@
         <v>111</v>
       </c>
       <c r="B1471" s="87"/>
-      <c r="C1471" s="165"/>
-      <c r="D1471" s="166"/>
-      <c r="E1471" s="166"/>
+      <c r="C1471" s="168"/>
+      <c r="D1471" s="169"/>
+      <c r="E1471" s="169"/>
     </row>
     <row r="1472" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1472" s="74">
@@ -18349,9 +18372,9 @@
         <v>112</v>
       </c>
       <c r="B1488" s="87"/>
-      <c r="C1488" s="165"/>
-      <c r="D1488" s="166"/>
-      <c r="E1488" s="166"/>
+      <c r="C1488" s="168"/>
+      <c r="D1488" s="169"/>
+      <c r="E1488" s="169"/>
     </row>
     <row r="1489" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1489" s="74">
@@ -18502,9 +18525,9 @@
         <v>113</v>
       </c>
       <c r="B1505" s="87"/>
-      <c r="C1505" s="165"/>
-      <c r="D1505" s="166"/>
-      <c r="E1505" s="166"/>
+      <c r="C1505" s="168"/>
+      <c r="D1505" s="169"/>
+      <c r="E1505" s="169"/>
     </row>
     <row r="1506" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1506" s="74">
@@ -18655,9 +18678,9 @@
         <v>114</v>
       </c>
       <c r="B1522" s="87"/>
-      <c r="C1522" s="165"/>
-      <c r="D1522" s="166"/>
-      <c r="E1522" s="166"/>
+      <c r="C1522" s="168"/>
+      <c r="D1522" s="169"/>
+      <c r="E1522" s="169"/>
     </row>
     <row r="1523" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1523" s="74">
@@ -18808,9 +18831,9 @@
         <v>95</v>
       </c>
       <c r="B1539" s="87"/>
-      <c r="C1539" s="165"/>
-      <c r="D1539" s="166"/>
-      <c r="E1539" s="166"/>
+      <c r="C1539" s="168"/>
+      <c r="D1539" s="169"/>
+      <c r="E1539" s="169"/>
     </row>
     <row r="1540" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1540" s="74">
@@ -18961,9 +18984,9 @@
         <v>115</v>
       </c>
       <c r="B1556" s="87"/>
-      <c r="C1556" s="165"/>
-      <c r="D1556" s="166"/>
-      <c r="E1556" s="166"/>
+      <c r="C1556" s="168"/>
+      <c r="D1556" s="169"/>
+      <c r="E1556" s="169"/>
     </row>
     <row r="1557" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1557" s="74">
@@ -19114,9 +19137,9 @@
         <v>116</v>
       </c>
       <c r="B1573" s="87"/>
-      <c r="C1573" s="165"/>
-      <c r="D1573" s="166"/>
-      <c r="E1573" s="166"/>
+      <c r="C1573" s="168"/>
+      <c r="D1573" s="169"/>
+      <c r="E1573" s="169"/>
     </row>
     <row r="1574" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1574" s="74">
@@ -19267,9 +19290,9 @@
         <v>117</v>
       </c>
       <c r="B1590" s="87"/>
-      <c r="C1590" s="165"/>
-      <c r="D1590" s="166"/>
-      <c r="E1590" s="166"/>
+      <c r="C1590" s="168"/>
+      <c r="D1590" s="169"/>
+      <c r="E1590" s="169"/>
     </row>
     <row r="1591" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1591" s="74">
@@ -19420,9 +19443,9 @@
         <v>118</v>
       </c>
       <c r="B1607" s="87"/>
-      <c r="C1607" s="165"/>
-      <c r="D1607" s="166"/>
-      <c r="E1607" s="166"/>
+      <c r="C1607" s="168"/>
+      <c r="D1607" s="169"/>
+      <c r="E1607" s="169"/>
     </row>
     <row r="1608" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1608" s="74">
@@ -19573,9 +19596,9 @@
         <v>119</v>
       </c>
       <c r="B1624" s="87"/>
-      <c r="C1624" s="165"/>
-      <c r="D1624" s="166"/>
-      <c r="E1624" s="166"/>
+      <c r="C1624" s="168"/>
+      <c r="D1624" s="169"/>
+      <c r="E1624" s="169"/>
     </row>
     <row r="1625" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1625" s="74">
@@ -19726,18 +19749,18 @@
         <v>120</v>
       </c>
       <c r="B1641" s="42"/>
-      <c r="C1641" s="171"/>
-      <c r="D1641" s="172"/>
-      <c r="E1641" s="172"/>
+      <c r="C1641" s="182"/>
+      <c r="D1641" s="183"/>
+      <c r="E1641" s="183"/>
     </row>
     <row r="1642" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A1642" s="78" t="s">
         <v>121</v>
       </c>
       <c r="B1642" s="87"/>
-      <c r="C1642" s="165"/>
-      <c r="D1642" s="166"/>
-      <c r="E1642" s="166"/>
+      <c r="C1642" s="168"/>
+      <c r="D1642" s="169"/>
+      <c r="E1642" s="169"/>
     </row>
     <row r="1643" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1643" s="79">
@@ -19888,9 +19911,9 @@
         <v>122</v>
       </c>
       <c r="B1659" s="90"/>
-      <c r="C1659" s="167"/>
-      <c r="D1659" s="168"/>
-      <c r="E1659" s="168"/>
+      <c r="C1659" s="170"/>
+      <c r="D1659" s="171"/>
+      <c r="E1659" s="171"/>
     </row>
     <row r="1660" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1660" s="79">
@@ -20041,9 +20064,9 @@
         <v>123</v>
       </c>
       <c r="B1676" s="87"/>
-      <c r="C1676" s="165"/>
-      <c r="D1676" s="166"/>
-      <c r="E1676" s="166"/>
+      <c r="C1676" s="168"/>
+      <c r="D1676" s="169"/>
+      <c r="E1676" s="169"/>
     </row>
     <row r="1677" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1677" s="79">
@@ -20194,9 +20217,9 @@
         <v>124</v>
       </c>
       <c r="B1693" s="87"/>
-      <c r="C1693" s="165"/>
-      <c r="D1693" s="166"/>
-      <c r="E1693" s="166"/>
+      <c r="C1693" s="168"/>
+      <c r="D1693" s="169"/>
+      <c r="E1693" s="169"/>
     </row>
     <row r="1694" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1694" s="79">
@@ -20347,9 +20370,9 @@
         <v>125</v>
       </c>
       <c r="B1710" s="87"/>
-      <c r="C1710" s="165"/>
-      <c r="D1710" s="166"/>
-      <c r="E1710" s="166"/>
+      <c r="C1710" s="168"/>
+      <c r="D1710" s="169"/>
+      <c r="E1710" s="169"/>
     </row>
     <row r="1711" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1711" s="79">
@@ -20500,9 +20523,9 @@
         <v>126</v>
       </c>
       <c r="B1727" s="87"/>
-      <c r="C1727" s="165"/>
-      <c r="D1727" s="166"/>
-      <c r="E1727" s="166"/>
+      <c r="C1727" s="168"/>
+      <c r="D1727" s="169"/>
+      <c r="E1727" s="169"/>
     </row>
     <row r="1728" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1728" s="79">
@@ -20653,9 +20676,9 @@
         <v>127</v>
       </c>
       <c r="B1744" s="87"/>
-      <c r="C1744" s="165"/>
-      <c r="D1744" s="166"/>
-      <c r="E1744" s="166"/>
+      <c r="C1744" s="168"/>
+      <c r="D1744" s="169"/>
+      <c r="E1744" s="169"/>
     </row>
     <row r="1745" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1745" s="79">
@@ -20806,9 +20829,9 @@
         <v>128</v>
       </c>
       <c r="B1761" s="87"/>
-      <c r="C1761" s="165"/>
-      <c r="D1761" s="166"/>
-      <c r="E1761" s="166"/>
+      <c r="C1761" s="168"/>
+      <c r="D1761" s="169"/>
+      <c r="E1761" s="169"/>
     </row>
     <row r="1762" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1762" s="79">
@@ -20959,9 +20982,9 @@
         <v>129</v>
       </c>
       <c r="B1778" s="87"/>
-      <c r="C1778" s="165"/>
-      <c r="D1778" s="166"/>
-      <c r="E1778" s="166"/>
+      <c r="C1778" s="168"/>
+      <c r="D1778" s="169"/>
+      <c r="E1778" s="169"/>
     </row>
     <row r="1779" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1779" s="79">
@@ -21112,9 +21135,9 @@
         <v>130</v>
       </c>
       <c r="B1795" s="87"/>
-      <c r="C1795" s="165"/>
-      <c r="D1795" s="166"/>
-      <c r="E1795" s="166"/>
+      <c r="C1795" s="168"/>
+      <c r="D1795" s="169"/>
+      <c r="E1795" s="169"/>
     </row>
     <row r="1796" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1796" s="79">
@@ -21265,9 +21288,9 @@
         <v>131</v>
       </c>
       <c r="B1812" s="87"/>
-      <c r="C1812" s="165"/>
-      <c r="D1812" s="166"/>
-      <c r="E1812" s="166"/>
+      <c r="C1812" s="168"/>
+      <c r="D1812" s="169"/>
+      <c r="E1812" s="169"/>
     </row>
     <row r="1813" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1813" s="79">
@@ -21418,9 +21441,9 @@
         <v>96</v>
       </c>
       <c r="B1829" s="87"/>
-      <c r="C1829" s="165"/>
-      <c r="D1829" s="166"/>
-      <c r="E1829" s="166"/>
+      <c r="C1829" s="168"/>
+      <c r="D1829" s="169"/>
+      <c r="E1829" s="169"/>
     </row>
     <row r="1830" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1830" s="79">
@@ -21571,9 +21594,9 @@
         <v>132</v>
       </c>
       <c r="B1846" s="87"/>
-      <c r="C1846" s="165"/>
-      <c r="D1846" s="166"/>
-      <c r="E1846" s="166"/>
+      <c r="C1846" s="168"/>
+      <c r="D1846" s="169"/>
+      <c r="E1846" s="169"/>
     </row>
     <row r="1847" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1847" s="79">
@@ -21724,9 +21747,9 @@
         <v>133</v>
       </c>
       <c r="B1863" s="87"/>
-      <c r="C1863" s="165"/>
-      <c r="D1863" s="166"/>
-      <c r="E1863" s="166"/>
+      <c r="C1863" s="168"/>
+      <c r="D1863" s="169"/>
+      <c r="E1863" s="169"/>
     </row>
     <row r="1864" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1864" s="79">
@@ -21877,9 +21900,9 @@
         <v>134</v>
       </c>
       <c r="B1880" s="87"/>
-      <c r="C1880" s="165"/>
-      <c r="D1880" s="166"/>
-      <c r="E1880" s="166"/>
+      <c r="C1880" s="168"/>
+      <c r="D1880" s="169"/>
+      <c r="E1880" s="169"/>
     </row>
     <row r="1881" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1881" s="79">
@@ -22030,9 +22053,9 @@
         <v>135</v>
       </c>
       <c r="B1897" s="87"/>
-      <c r="C1897" s="165"/>
-      <c r="D1897" s="166"/>
-      <c r="E1897" s="166"/>
+      <c r="C1897" s="168"/>
+      <c r="D1897" s="169"/>
+      <c r="E1897" s="169"/>
     </row>
     <row r="1898" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1898" s="79">
@@ -22183,18 +22206,18 @@
         <v>136</v>
       </c>
       <c r="B1914" s="43"/>
-      <c r="C1914" s="169"/>
-      <c r="D1914" s="170"/>
-      <c r="E1914" s="170"/>
+      <c r="C1914" s="184"/>
+      <c r="D1914" s="185"/>
+      <c r="E1914" s="185"/>
     </row>
     <row r="1915" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A1915" s="83" t="s">
         <v>137</v>
       </c>
       <c r="B1915" s="87"/>
-      <c r="C1915" s="165"/>
-      <c r="D1915" s="166"/>
-      <c r="E1915" s="166"/>
+      <c r="C1915" s="168"/>
+      <c r="D1915" s="169"/>
+      <c r="E1915" s="169"/>
     </row>
     <row r="1916" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1916" s="84">
@@ -22345,9 +22368,9 @@
         <v>138</v>
       </c>
       <c r="B1932" s="90"/>
-      <c r="C1932" s="167"/>
-      <c r="D1932" s="168"/>
-      <c r="E1932" s="168"/>
+      <c r="C1932" s="170"/>
+      <c r="D1932" s="171"/>
+      <c r="E1932" s="171"/>
     </row>
     <row r="1933" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1933" s="84">
@@ -22498,9 +22521,9 @@
         <v>139</v>
       </c>
       <c r="B1949" s="87"/>
-      <c r="C1949" s="165"/>
-      <c r="D1949" s="166"/>
-      <c r="E1949" s="166"/>
+      <c r="C1949" s="168"/>
+      <c r="D1949" s="169"/>
+      <c r="E1949" s="169"/>
     </row>
     <row r="1950" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1950" s="84">
@@ -22651,9 +22674,9 @@
         <v>140</v>
       </c>
       <c r="B1966" s="87"/>
-      <c r="C1966" s="165"/>
-      <c r="D1966" s="166"/>
-      <c r="E1966" s="166"/>
+      <c r="C1966" s="168"/>
+      <c r="D1966" s="169"/>
+      <c r="E1966" s="169"/>
     </row>
     <row r="1967" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1967" s="84">
@@ -22804,9 +22827,9 @@
         <v>141</v>
       </c>
       <c r="B1983" s="87"/>
-      <c r="C1983" s="165"/>
-      <c r="D1983" s="166"/>
-      <c r="E1983" s="166"/>
+      <c r="C1983" s="168"/>
+      <c r="D1983" s="169"/>
+      <c r="E1983" s="169"/>
     </row>
     <row r="1984" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1984" s="84">
@@ -22957,9 +22980,9 @@
         <v>142</v>
       </c>
       <c r="B2000" s="87"/>
-      <c r="C2000" s="165"/>
-      <c r="D2000" s="166"/>
-      <c r="E2000" s="166"/>
+      <c r="C2000" s="168"/>
+      <c r="D2000" s="169"/>
+      <c r="E2000" s="169"/>
     </row>
     <row r="2001" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2001" s="84">
@@ -23110,9 +23133,9 @@
         <v>143</v>
       </c>
       <c r="B2017" s="87"/>
-      <c r="C2017" s="165"/>
-      <c r="D2017" s="166"/>
-      <c r="E2017" s="166"/>
+      <c r="C2017" s="168"/>
+      <c r="D2017" s="169"/>
+      <c r="E2017" s="169"/>
     </row>
     <row r="2018" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2018" s="84">
@@ -23263,9 +23286,9 @@
         <v>144</v>
       </c>
       <c r="B2034" s="87"/>
-      <c r="C2034" s="165"/>
-      <c r="D2034" s="166"/>
-      <c r="E2034" s="166"/>
+      <c r="C2034" s="168"/>
+      <c r="D2034" s="169"/>
+      <c r="E2034" s="169"/>
     </row>
     <row r="2035" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2035" s="84">
@@ -23416,9 +23439,9 @@
         <v>145</v>
       </c>
       <c r="B2051" s="87"/>
-      <c r="C2051" s="165"/>
-      <c r="D2051" s="166"/>
-      <c r="E2051" s="166"/>
+      <c r="C2051" s="168"/>
+      <c r="D2051" s="169"/>
+      <c r="E2051" s="169"/>
     </row>
     <row r="2052" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2052" s="84">
@@ -23569,9 +23592,9 @@
         <v>146</v>
       </c>
       <c r="B2068" s="87"/>
-      <c r="C2068" s="165"/>
-      <c r="D2068" s="166"/>
-      <c r="E2068" s="166"/>
+      <c r="C2068" s="168"/>
+      <c r="D2068" s="169"/>
+      <c r="E2068" s="169"/>
     </row>
     <row r="2069" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2069" s="84">
@@ -23722,9 +23745,9 @@
         <v>147</v>
       </c>
       <c r="B2085" s="87"/>
-      <c r="C2085" s="165"/>
-      <c r="D2085" s="166"/>
-      <c r="E2085" s="166"/>
+      <c r="C2085" s="168"/>
+      <c r="D2085" s="169"/>
+      <c r="E2085" s="169"/>
     </row>
     <row r="2086" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2086" s="84">
@@ -23875,9 +23898,9 @@
         <v>148</v>
       </c>
       <c r="B2102" s="87"/>
-      <c r="C2102" s="165"/>
-      <c r="D2102" s="166"/>
-      <c r="E2102" s="166"/>
+      <c r="C2102" s="168"/>
+      <c r="D2102" s="169"/>
+      <c r="E2102" s="169"/>
     </row>
     <row r="2103" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2103" s="84">
@@ -24028,9 +24051,9 @@
         <v>97</v>
       </c>
       <c r="B2119" s="87"/>
-      <c r="C2119" s="165"/>
-      <c r="D2119" s="166"/>
-      <c r="E2119" s="166"/>
+      <c r="C2119" s="168"/>
+      <c r="D2119" s="169"/>
+      <c r="E2119" s="169"/>
     </row>
     <row r="2120" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2120" s="84">
@@ -24181,9 +24204,9 @@
         <v>149</v>
       </c>
       <c r="B2136" s="87"/>
-      <c r="C2136" s="165"/>
-      <c r="D2136" s="166"/>
-      <c r="E2136" s="166"/>
+      <c r="C2136" s="168"/>
+      <c r="D2136" s="169"/>
+      <c r="E2136" s="169"/>
     </row>
     <row r="2137" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2137" s="84">
@@ -24334,9 +24357,9 @@
         <v>150</v>
       </c>
       <c r="B2153" s="87"/>
-      <c r="C2153" s="165"/>
-      <c r="D2153" s="166"/>
-      <c r="E2153" s="166"/>
+      <c r="C2153" s="168"/>
+      <c r="D2153" s="169"/>
+      <c r="E2153" s="169"/>
     </row>
     <row r="2154" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2154" s="84">
@@ -24487,9 +24510,9 @@
         <v>151</v>
       </c>
       <c r="B2170" s="87"/>
-      <c r="C2170" s="165"/>
-      <c r="D2170" s="166"/>
-      <c r="E2170" s="166"/>
+      <c r="C2170" s="168"/>
+      <c r="D2170" s="169"/>
+      <c r="E2170" s="169"/>
     </row>
     <row r="2171" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2171" s="84">
@@ -24637,26 +24660,111 @@
     </row>
   </sheetData>
   <mergeCells count="137">
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="C89:E89"/>
-    <mergeCell ref="C21:E21"/>
-    <mergeCell ref="C38:E38"/>
-    <mergeCell ref="C55:E55"/>
-    <mergeCell ref="C72:E72"/>
-    <mergeCell ref="C208:E208"/>
-    <mergeCell ref="C225:E225"/>
-    <mergeCell ref="C242:E242"/>
-    <mergeCell ref="C259:E259"/>
-    <mergeCell ref="C276:E276"/>
-    <mergeCell ref="C277:E277"/>
-    <mergeCell ref="C106:E106"/>
-    <mergeCell ref="C123:E123"/>
-    <mergeCell ref="C140:E140"/>
-    <mergeCell ref="C157:E157"/>
-    <mergeCell ref="C174:E174"/>
-    <mergeCell ref="C191:E191"/>
+    <mergeCell ref="C2034:E2034"/>
+    <mergeCell ref="C2051:E2051"/>
+    <mergeCell ref="C2068:E2068"/>
+    <mergeCell ref="C2085:E2085"/>
+    <mergeCell ref="C2170:E2170"/>
+    <mergeCell ref="C2102:E2102"/>
+    <mergeCell ref="C2119:E2119"/>
+    <mergeCell ref="C2136:E2136"/>
+    <mergeCell ref="C2153:E2153"/>
+    <mergeCell ref="C1932:E1932"/>
+    <mergeCell ref="C1949:E1949"/>
+    <mergeCell ref="C1966:E1966"/>
+    <mergeCell ref="C1983:E1983"/>
+    <mergeCell ref="C2000:E2000"/>
+    <mergeCell ref="C2017:E2017"/>
+    <mergeCell ref="C1846:E1846"/>
+    <mergeCell ref="C1863:E1863"/>
+    <mergeCell ref="C1880:E1880"/>
+    <mergeCell ref="C1897:E1897"/>
+    <mergeCell ref="C1914:E1914"/>
+    <mergeCell ref="C1915:E1915"/>
+    <mergeCell ref="C1744:E1744"/>
+    <mergeCell ref="C1761:E1761"/>
+    <mergeCell ref="C1778:E1778"/>
+    <mergeCell ref="C1795:E1795"/>
+    <mergeCell ref="C1812:E1812"/>
+    <mergeCell ref="C1829:E1829"/>
+    <mergeCell ref="C1642:E1642"/>
+    <mergeCell ref="C1659:E1659"/>
+    <mergeCell ref="C1676:E1676"/>
+    <mergeCell ref="C1693:E1693"/>
+    <mergeCell ref="C1710:E1710"/>
+    <mergeCell ref="C1727:E1727"/>
+    <mergeCell ref="C1556:E1556"/>
+    <mergeCell ref="C1573:E1573"/>
+    <mergeCell ref="C1590:E1590"/>
+    <mergeCell ref="C1607:E1607"/>
+    <mergeCell ref="C1624:E1624"/>
+    <mergeCell ref="C1641:E1641"/>
+    <mergeCell ref="C1454:E1454"/>
+    <mergeCell ref="C1471:E1471"/>
+    <mergeCell ref="C1488:E1488"/>
+    <mergeCell ref="C1505:E1505"/>
+    <mergeCell ref="C1522:E1522"/>
+    <mergeCell ref="C1539:E1539"/>
+    <mergeCell ref="C1368:E1368"/>
+    <mergeCell ref="C1369:E1369"/>
+    <mergeCell ref="C1386:E1386"/>
+    <mergeCell ref="C1403:E1403"/>
+    <mergeCell ref="C1420:E1420"/>
+    <mergeCell ref="C1437:E1437"/>
+    <mergeCell ref="C1266:E1266"/>
+    <mergeCell ref="C1283:E1283"/>
+    <mergeCell ref="C1300:E1300"/>
+    <mergeCell ref="C1317:E1317"/>
+    <mergeCell ref="C1334:E1334"/>
+    <mergeCell ref="C1351:E1351"/>
+    <mergeCell ref="C1164:E1164"/>
+    <mergeCell ref="C1181:E1181"/>
+    <mergeCell ref="C1198:E1198"/>
+    <mergeCell ref="C1215:E1215"/>
+    <mergeCell ref="C1232:E1232"/>
+    <mergeCell ref="C1249:E1249"/>
+    <mergeCell ref="C1078:E1078"/>
+    <mergeCell ref="C1095:E1095"/>
+    <mergeCell ref="C1096:E1096"/>
+    <mergeCell ref="C1113:E1113"/>
+    <mergeCell ref="C1130:E1130"/>
+    <mergeCell ref="C1147:E1147"/>
+    <mergeCell ref="C976:E976"/>
+    <mergeCell ref="C993:E993"/>
+    <mergeCell ref="C1010:E1010"/>
+    <mergeCell ref="C1027:E1027"/>
+    <mergeCell ref="C1044:E1044"/>
+    <mergeCell ref="C1061:E1061"/>
+    <mergeCell ref="C874:E874"/>
+    <mergeCell ref="C891:E891"/>
+    <mergeCell ref="C908:E908"/>
+    <mergeCell ref="C925:E925"/>
+    <mergeCell ref="C942:E942"/>
+    <mergeCell ref="C959:E959"/>
+    <mergeCell ref="C788:E788"/>
+    <mergeCell ref="C805:E805"/>
+    <mergeCell ref="C822:E822"/>
+    <mergeCell ref="C823:E823"/>
+    <mergeCell ref="C840:E840"/>
+    <mergeCell ref="C857:E857"/>
+    <mergeCell ref="C686:E686"/>
+    <mergeCell ref="C703:E703"/>
+    <mergeCell ref="C720:E720"/>
+    <mergeCell ref="C737:E737"/>
+    <mergeCell ref="C754:E754"/>
+    <mergeCell ref="C771:E771"/>
+    <mergeCell ref="C584:E584"/>
+    <mergeCell ref="C601:E601"/>
+    <mergeCell ref="C618:E618"/>
+    <mergeCell ref="C635:E635"/>
+    <mergeCell ref="C652:E652"/>
+    <mergeCell ref="C669:E669"/>
+    <mergeCell ref="C498:E498"/>
+    <mergeCell ref="C515:E515"/>
+    <mergeCell ref="C532:E532"/>
+    <mergeCell ref="C549:E549"/>
+    <mergeCell ref="C550:E550"/>
+    <mergeCell ref="C567:E567"/>
     <mergeCell ref="C396:E396"/>
     <mergeCell ref="C413:E413"/>
     <mergeCell ref="C430:E430"/>
@@ -24669,113 +24777,28 @@
     <mergeCell ref="C345:E345"/>
     <mergeCell ref="C362:E362"/>
     <mergeCell ref="C379:E379"/>
-    <mergeCell ref="C584:E584"/>
-    <mergeCell ref="C601:E601"/>
-    <mergeCell ref="C618:E618"/>
-    <mergeCell ref="C635:E635"/>
-    <mergeCell ref="C652:E652"/>
-    <mergeCell ref="C669:E669"/>
-    <mergeCell ref="C498:E498"/>
-    <mergeCell ref="C515:E515"/>
-    <mergeCell ref="C532:E532"/>
-    <mergeCell ref="C549:E549"/>
-    <mergeCell ref="C550:E550"/>
-    <mergeCell ref="C567:E567"/>
-    <mergeCell ref="C788:E788"/>
-    <mergeCell ref="C805:E805"/>
-    <mergeCell ref="C822:E822"/>
-    <mergeCell ref="C823:E823"/>
-    <mergeCell ref="C840:E840"/>
-    <mergeCell ref="C857:E857"/>
-    <mergeCell ref="C686:E686"/>
-    <mergeCell ref="C703:E703"/>
-    <mergeCell ref="C720:E720"/>
-    <mergeCell ref="C737:E737"/>
-    <mergeCell ref="C754:E754"/>
-    <mergeCell ref="C771:E771"/>
-    <mergeCell ref="C976:E976"/>
-    <mergeCell ref="C993:E993"/>
-    <mergeCell ref="C1010:E1010"/>
-    <mergeCell ref="C1027:E1027"/>
-    <mergeCell ref="C1044:E1044"/>
-    <mergeCell ref="C1061:E1061"/>
-    <mergeCell ref="C874:E874"/>
-    <mergeCell ref="C891:E891"/>
-    <mergeCell ref="C908:E908"/>
-    <mergeCell ref="C925:E925"/>
-    <mergeCell ref="C942:E942"/>
-    <mergeCell ref="C959:E959"/>
-    <mergeCell ref="C1164:E1164"/>
-    <mergeCell ref="C1181:E1181"/>
-    <mergeCell ref="C1198:E1198"/>
-    <mergeCell ref="C1215:E1215"/>
-    <mergeCell ref="C1232:E1232"/>
-    <mergeCell ref="C1249:E1249"/>
-    <mergeCell ref="C1078:E1078"/>
-    <mergeCell ref="C1095:E1095"/>
-    <mergeCell ref="C1096:E1096"/>
-    <mergeCell ref="C1113:E1113"/>
-    <mergeCell ref="C1130:E1130"/>
-    <mergeCell ref="C1147:E1147"/>
-    <mergeCell ref="C1368:E1368"/>
-    <mergeCell ref="C1369:E1369"/>
-    <mergeCell ref="C1386:E1386"/>
-    <mergeCell ref="C1403:E1403"/>
-    <mergeCell ref="C1420:E1420"/>
-    <mergeCell ref="C1437:E1437"/>
-    <mergeCell ref="C1266:E1266"/>
-    <mergeCell ref="C1283:E1283"/>
-    <mergeCell ref="C1300:E1300"/>
-    <mergeCell ref="C1317:E1317"/>
-    <mergeCell ref="C1334:E1334"/>
-    <mergeCell ref="C1351:E1351"/>
-    <mergeCell ref="C1556:E1556"/>
-    <mergeCell ref="C1573:E1573"/>
-    <mergeCell ref="C1590:E1590"/>
-    <mergeCell ref="C1607:E1607"/>
-    <mergeCell ref="C1624:E1624"/>
-    <mergeCell ref="C1641:E1641"/>
-    <mergeCell ref="C1454:E1454"/>
-    <mergeCell ref="C1471:E1471"/>
-    <mergeCell ref="C1488:E1488"/>
-    <mergeCell ref="C1505:E1505"/>
-    <mergeCell ref="C1522:E1522"/>
-    <mergeCell ref="C1539:E1539"/>
-    <mergeCell ref="C1744:E1744"/>
-    <mergeCell ref="C1761:E1761"/>
-    <mergeCell ref="C1778:E1778"/>
-    <mergeCell ref="C1795:E1795"/>
-    <mergeCell ref="C1812:E1812"/>
-    <mergeCell ref="C1829:E1829"/>
-    <mergeCell ref="C1642:E1642"/>
-    <mergeCell ref="C1659:E1659"/>
-    <mergeCell ref="C1676:E1676"/>
-    <mergeCell ref="C1693:E1693"/>
-    <mergeCell ref="C1710:E1710"/>
-    <mergeCell ref="C1727:E1727"/>
-    <mergeCell ref="C1932:E1932"/>
-    <mergeCell ref="C1949:E1949"/>
-    <mergeCell ref="C1966:E1966"/>
-    <mergeCell ref="C1983:E1983"/>
-    <mergeCell ref="C2000:E2000"/>
-    <mergeCell ref="C2017:E2017"/>
-    <mergeCell ref="C1846:E1846"/>
-    <mergeCell ref="C1863:E1863"/>
-    <mergeCell ref="C1880:E1880"/>
-    <mergeCell ref="C1897:E1897"/>
-    <mergeCell ref="C1914:E1914"/>
-    <mergeCell ref="C1915:E1915"/>
-    <mergeCell ref="C2034:E2034"/>
-    <mergeCell ref="C2051:E2051"/>
-    <mergeCell ref="C2068:E2068"/>
-    <mergeCell ref="C2085:E2085"/>
-    <mergeCell ref="C2170:E2170"/>
-    <mergeCell ref="C2102:E2102"/>
-    <mergeCell ref="C2119:E2119"/>
-    <mergeCell ref="C2136:E2136"/>
-    <mergeCell ref="C2153:E2153"/>
+    <mergeCell ref="C225:E225"/>
+    <mergeCell ref="C242:E242"/>
+    <mergeCell ref="C259:E259"/>
+    <mergeCell ref="C276:E276"/>
+    <mergeCell ref="C277:E277"/>
+    <mergeCell ref="C106:E106"/>
+    <mergeCell ref="C123:E123"/>
+    <mergeCell ref="C140:E140"/>
+    <mergeCell ref="C157:E157"/>
+    <mergeCell ref="C174:E174"/>
+    <mergeCell ref="C191:E191"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="C89:E89"/>
+    <mergeCell ref="C21:E21"/>
+    <mergeCell ref="C38:E38"/>
+    <mergeCell ref="C55:E55"/>
+    <mergeCell ref="C72:E72"/>
+    <mergeCell ref="C208:E208"/>
   </mergeCells>
-  <phoneticPr fontId="6" type="noConversion"/>
+  <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967294" verticalDpi="0" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
@@ -25526,7 +25549,7 @@
     <mergeCell ref="A3:K3"/>
     <mergeCell ref="A20:K20"/>
   </mergeCells>
-  <phoneticPr fontId="6" type="noConversion"/>
+  <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
@@ -25737,7 +25760,7 @@
   <mergeCells count="1">
     <mergeCell ref="A3:A10"/>
   </mergeCells>
-  <phoneticPr fontId="6" type="noConversion"/>
+  <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
@@ -26010,7 +26033,7 @@
     <mergeCell ref="A11:A17"/>
     <mergeCell ref="A19:A25"/>
   </mergeCells>
-  <phoneticPr fontId="6" type="noConversion"/>
+  <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
@@ -26032,163 +26055,150 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="33">
-      <c r="A1" s="210" t="s">
+      <c r="A1" s="211" t="s">
         <v>184</v>
       </c>
-      <c r="B1" s="211"/>
+      <c r="B1" s="212"/>
       <c r="C1" s="118"/>
       <c r="D1" s="5"/>
       <c r="E1" s="5"/>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="207" t="s">
+      <c r="A2" s="217" t="s">
         <v>183</v>
       </c>
-      <c r="B2" s="208"/>
+      <c r="B2" s="218"/>
       <c r="C2" s="120"/>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="209" t="s">
+      <c r="A3" s="219" t="s">
         <v>185</v>
       </c>
-      <c r="B3" s="208"/>
+      <c r="B3" s="218"/>
       <c r="C3" s="120"/>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="214"/>
-      <c r="B4" s="215"/>
+      <c r="A4" s="215"/>
+      <c r="B4" s="216"/>
       <c r="C4" s="120"/>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="212" t="s">
+      <c r="A5" s="213" t="s">
         <v>194</v>
       </c>
-      <c r="B5" s="213"/>
+      <c r="B5" s="214"/>
       <c r="C5" s="120"/>
     </row>
     <row r="7" spans="1:5" ht="18.75">
-      <c r="A7" s="218" t="s">
+      <c r="A7" s="205" t="s">
         <v>186</v>
       </c>
-      <c r="B7" s="219"/>
+      <c r="B7" s="206"/>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="120"/>
       <c r="B8" s="9"/>
     </row>
     <row r="9" spans="1:5" ht="39" customHeight="1">
-      <c r="A9" s="216" t="s">
+      <c r="A9" s="207" t="s">
         <v>187</v>
       </c>
-      <c r="B9" s="217"/>
+      <c r="B9" s="208"/>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="203"/>
-      <c r="B10" s="204"/>
+      <c r="A10" s="209"/>
+      <c r="B10" s="210"/>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="205" t="s">
+      <c r="A11" s="201" t="s">
         <v>188</v>
       </c>
-      <c r="B11" s="206"/>
+      <c r="B11" s="202"/>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="205" t="s">
+      <c r="A12" s="201" t="s">
         <v>189</v>
       </c>
-      <c r="B12" s="206"/>
+      <c r="B12" s="202"/>
     </row>
     <row r="13" spans="1:5" ht="43.5" customHeight="1">
-      <c r="A13" s="205" t="s">
+      <c r="A13" s="201" t="s">
         <v>190</v>
       </c>
-      <c r="B13" s="206"/>
+      <c r="B13" s="202"/>
     </row>
     <row r="14" spans="1:5" ht="19.5" customHeight="1">
-      <c r="A14" s="205" t="s">
+      <c r="A14" s="201" t="s">
         <v>191</v>
       </c>
-      <c r="B14" s="206"/>
+      <c r="B14" s="202"/>
     </row>
     <row r="15" spans="1:5" ht="18" customHeight="1">
-      <c r="A15" s="205" t="s">
+      <c r="A15" s="201" t="s">
         <v>192</v>
       </c>
-      <c r="B15" s="206"/>
+      <c r="B15" s="202"/>
     </row>
     <row r="16" spans="1:5" ht="21" customHeight="1">
-      <c r="A16" s="205" t="s">
+      <c r="A16" s="201" t="s">
         <v>193</v>
       </c>
-      <c r="B16" s="206"/>
+      <c r="B16" s="202"/>
     </row>
     <row r="17" spans="1:2" ht="48.75" customHeight="1">
-      <c r="A17" s="201" t="s">
+      <c r="A17" s="203" t="s">
         <v>195</v>
       </c>
-      <c r="B17" s="202"/>
+      <c r="B17" s="204"/>
     </row>
     <row r="19" spans="1:2" ht="18.75">
-      <c r="A19" s="218" t="s">
+      <c r="A19" s="205" t="s">
         <v>197</v>
       </c>
-      <c r="B19" s="219"/>
+      <c r="B19" s="206"/>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="120"/>
       <c r="B20" s="9"/>
     </row>
     <row r="21" spans="1:2">
-      <c r="A21" s="216" t="s">
+      <c r="A21" s="207" t="s">
         <v>198</v>
       </c>
-      <c r="B21" s="217"/>
+      <c r="B21" s="208"/>
     </row>
     <row r="22" spans="1:2">
-      <c r="A22" s="203"/>
-      <c r="B22" s="204"/>
+      <c r="A22" s="209"/>
+      <c r="B22" s="210"/>
     </row>
     <row r="23" spans="1:2">
-      <c r="A23" s="205" t="s">
+      <c r="A23" s="201" t="s">
         <v>199</v>
       </c>
-      <c r="B23" s="206"/>
+      <c r="B23" s="202"/>
     </row>
     <row r="24" spans="1:2">
-      <c r="A24" s="205"/>
-      <c r="B24" s="206"/>
+      <c r="A24" s="201"/>
+      <c r="B24" s="202"/>
     </row>
     <row r="25" spans="1:2">
-      <c r="A25" s="205" t="s">
+      <c r="A25" s="201" t="s">
         <v>200</v>
       </c>
-      <c r="B25" s="206"/>
+      <c r="B25" s="202"/>
     </row>
     <row r="26" spans="1:2">
-      <c r="A26" s="205" t="s">
+      <c r="A26" s="201" t="s">
         <v>201</v>
       </c>
-      <c r="B26" s="206"/>
+      <c r="B26" s="202"/>
     </row>
     <row r="27" spans="1:2">
-      <c r="A27" s="201"/>
-      <c r="B27" s="202"/>
+      <c r="A27" s="203"/>
+      <c r="B27" s="204"/>
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A7:B7"/>
     <mergeCell ref="A17:B17"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
@@ -26199,6 +26209,19 @@
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="A14:B14"/>
     <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A24:B24"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A3" r:id="rId1"/>

</xml_diff>

<commit_message>
Tempo - HiFi Stage 2 complete.
</commit_message>
<xml_diff>
--- a/trunk/Tempo/Tempo.xlsx
+++ b/trunk/Tempo/Tempo.xlsx
@@ -2159,6 +2159,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="35" fillId="21" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -2181,29 +2184,29 @@
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="20" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="18" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="20" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="19" fillId="13" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -2239,34 +2242,20 @@
     <xf numFmtId="0" fontId="49" fillId="22" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="46" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="47" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="47" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="43" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="4"/>
     </xf>
@@ -2276,9 +2265,20 @@
     <xf numFmtId="0" fontId="44" fillId="0" borderId="33" xfId="3" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" indent="4"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="47" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="47" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="46" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Accent1" xfId="2" builtinId="29"/>
@@ -2589,8 +2589,8 @@
   <dimension ref="A1:K157"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B50" sqref="B50"/>
+      <pane ySplit="6" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C50" sqref="C50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" outlineLevelRow="2"/>
@@ -2606,16 +2606,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="33">
-      <c r="A1" s="160" t="s">
+      <c r="A1" s="161" t="s">
         <v>205</v>
       </c>
-      <c r="B1" s="159"/>
-      <c r="C1" s="161" t="s">
+      <c r="B1" s="160"/>
+      <c r="C1" s="162" t="s">
         <v>170</v>
       </c>
-      <c r="D1" s="161"/>
-      <c r="E1" s="161"/>
-      <c r="F1" s="162"/>
+      <c r="D1" s="162"/>
+      <c r="E1" s="162"/>
+      <c r="F1" s="163"/>
       <c r="G1" s="140"/>
       <c r="H1" s="141">
         <f>SUM(G1:G65539)</f>
@@ -2680,11 +2680,11 @@
       <c r="B4" s="146" t="s">
         <v>228</v>
       </c>
-      <c r="C4" s="158" t="s">
+      <c r="C4" s="159" t="s">
         <v>232</v>
       </c>
-      <c r="D4" s="158"/>
-      <c r="E4" s="164"/>
+      <c r="D4" s="159"/>
+      <c r="E4" s="165"/>
       <c r="F4" s="143"/>
       <c r="G4" s="140"/>
       <c r="H4" s="140"/>
@@ -2699,10 +2699,10 @@
       <c r="B5" s="147" t="s">
         <v>177</v>
       </c>
-      <c r="C5" s="158" t="s">
+      <c r="C5" s="159" t="s">
         <v>218</v>
       </c>
-      <c r="D5" s="158"/>
+      <c r="D5" s="159"/>
       <c r="E5" s="147"/>
       <c r="F5" s="147"/>
       <c r="G5" s="148" t="s">
@@ -2726,10 +2726,10 @@
       <c r="B6" s="147" t="s">
         <v>179</v>
       </c>
-      <c r="C6" s="158" t="s">
+      <c r="C6" s="159" t="s">
         <v>168</v>
       </c>
-      <c r="D6" s="159"/>
+      <c r="D6" s="160"/>
       <c r="E6" s="147"/>
       <c r="F6" s="143"/>
       <c r="G6" s="140"/>
@@ -2753,7 +2753,7 @@
       <c r="F7" s="93"/>
     </row>
     <row r="8" spans="1:11" ht="15" customHeight="1" outlineLevel="1">
-      <c r="A8" s="163" t="s">
+      <c r="A8" s="164" t="s">
         <v>180</v>
       </c>
       <c r="B8" s="95" t="s">
@@ -2773,7 +2773,7 @@
       </c>
     </row>
     <row r="9" spans="1:11" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="A9" s="156"/>
+      <c r="A9" s="157"/>
       <c r="B9" s="98" t="s">
         <v>177</v>
       </c>
@@ -2787,7 +2787,7 @@
       <c r="F9" s="104"/>
     </row>
     <row r="10" spans="1:11" ht="15.75" outlineLevel="1" thickTop="1">
-      <c r="A10" s="156"/>
+      <c r="A10" s="157"/>
       <c r="B10" s="149" t="s">
         <v>208</v>
       </c>
@@ -2804,7 +2804,7 @@
       <c r="F10" s="105"/>
     </row>
     <row r="11" spans="1:11" ht="15" outlineLevel="1">
-      <c r="A11" s="156"/>
+      <c r="A11" s="157"/>
       <c r="B11" s="149" t="s">
         <v>214</v>
       </c>
@@ -2821,7 +2821,7 @@
       <c r="F11" s="105"/>
     </row>
     <row r="12" spans="1:11" ht="15" outlineLevel="1">
-      <c r="A12" s="156"/>
+      <c r="A12" s="157"/>
       <c r="B12" s="149" t="s">
         <v>209</v>
       </c>
@@ -2838,7 +2838,7 @@
       <c r="F12" s="105"/>
     </row>
     <row r="13" spans="1:11" ht="15" outlineLevel="1">
-      <c r="A13" s="156"/>
+      <c r="A13" s="157"/>
       <c r="B13" s="149" t="s">
         <v>213</v>
       </c>
@@ -2855,7 +2855,7 @@
       <c r="F13" s="105"/>
     </row>
     <row r="14" spans="1:11" ht="15" outlineLevel="1">
-      <c r="A14" s="156"/>
+      <c r="A14" s="157"/>
       <c r="B14" s="149" t="s">
         <v>214</v>
       </c>
@@ -2872,7 +2872,7 @@
       <c r="F14" s="105"/>
     </row>
     <row r="15" spans="1:11" ht="15" outlineLevel="1">
-      <c r="A15" s="156"/>
+      <c r="A15" s="157"/>
       <c r="B15" s="149" t="s">
         <v>215</v>
       </c>
@@ -2889,7 +2889,7 @@
       <c r="F15" s="105"/>
     </row>
     <row r="16" spans="1:11" ht="15" outlineLevel="1">
-      <c r="A16" s="156"/>
+      <c r="A16" s="157"/>
       <c r="B16" s="149" t="s">
         <v>216</v>
       </c>
@@ -2906,7 +2906,7 @@
       <c r="F16" s="105"/>
     </row>
     <row r="17" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A17" s="156"/>
+      <c r="A17" s="157"/>
       <c r="B17" s="149" t="s">
         <v>217</v>
       </c>
@@ -2923,7 +2923,7 @@
       <c r="F17" s="105"/>
     </row>
     <row r="18" spans="1:8" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="A18" s="156"/>
+      <c r="A18" s="157"/>
       <c r="B18" s="98" t="s">
         <v>179</v>
       </c>
@@ -2966,7 +2966,7 @@
     </row>
     <row r="20" spans="1:8" ht="13.5" thickBot="1"/>
     <row r="21" spans="1:8" ht="15" customHeight="1" outlineLevel="1">
-      <c r="A21" s="157" t="s">
+      <c r="A21" s="158" t="s">
         <v>219</v>
       </c>
       <c r="B21" s="109" t="s">
@@ -2986,7 +2986,7 @@
       </c>
     </row>
     <row r="22" spans="1:8" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="A22" s="156"/>
+      <c r="A22" s="157"/>
       <c r="B22" s="98" t="s">
         <v>177</v>
       </c>
@@ -3003,7 +3003,7 @@
       <c r="F22" s="104"/>
     </row>
     <row r="23" spans="1:8" ht="15.75" outlineLevel="1" thickTop="1">
-      <c r="A23" s="156"/>
+      <c r="A23" s="157"/>
       <c r="B23" s="149" t="s">
         <v>175</v>
       </c>
@@ -3016,7 +3016,7 @@
       <c r="F23" s="105"/>
     </row>
     <row r="24" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A24" s="156"/>
+      <c r="A24" s="157"/>
       <c r="B24" s="149" t="s">
         <v>221</v>
       </c>
@@ -3036,7 +3036,7 @@
       </c>
     </row>
     <row r="25" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A25" s="156"/>
+      <c r="A25" s="157"/>
       <c r="B25" s="149"/>
       <c r="C25" s="101"/>
       <c r="D25" s="101"/>
@@ -3047,7 +3047,7 @@
       <c r="F25" s="105"/>
     </row>
     <row r="26" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A26" s="156"/>
+      <c r="A26" s="157"/>
       <c r="B26" s="100"/>
       <c r="C26" s="101"/>
       <c r="D26" s="101"/>
@@ -3058,7 +3058,7 @@
       <c r="F26" s="105"/>
     </row>
     <row r="27" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A27" s="156"/>
+      <c r="A27" s="157"/>
       <c r="B27" s="100"/>
       <c r="C27" s="101"/>
       <c r="D27" s="101"/>
@@ -3069,7 +3069,7 @@
       <c r="F27" s="105"/>
     </row>
     <row r="28" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A28" s="156"/>
+      <c r="A28" s="157"/>
       <c r="B28" s="149" t="s">
         <v>222</v>
       </c>
@@ -3089,7 +3089,7 @@
       </c>
     </row>
     <row r="29" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A29" s="156"/>
+      <c r="A29" s="157"/>
       <c r="B29" s="154" t="s">
         <v>264</v>
       </c>
@@ -3107,7 +3107,7 @@
       </c>
     </row>
     <row r="30" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A30" s="156"/>
+      <c r="A30" s="157"/>
       <c r="B30" s="154" t="s">
         <v>265</v>
       </c>
@@ -3123,7 +3123,7 @@
       </c>
     </row>
     <row r="31" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A31" s="156"/>
+      <c r="A31" s="157"/>
       <c r="B31" s="154" t="s">
         <v>266</v>
       </c>
@@ -3139,7 +3139,7 @@
       </c>
     </row>
     <row r="32" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A32" s="156"/>
+      <c r="A32" s="157"/>
       <c r="B32" s="154" t="s">
         <v>267</v>
       </c>
@@ -3155,7 +3155,7 @@
       </c>
     </row>
     <row r="33" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A33" s="156"/>
+      <c r="A33" s="157"/>
       <c r="B33" s="154" t="s">
         <v>269</v>
       </c>
@@ -3171,7 +3171,7 @@
       </c>
     </row>
     <row r="34" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A34" s="156"/>
+      <c r="A34" s="157"/>
       <c r="B34" s="154" t="s">
         <v>270</v>
       </c>
@@ -3187,7 +3187,7 @@
       </c>
     </row>
     <row r="35" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A35" s="156"/>
+      <c r="A35" s="157"/>
       <c r="B35" s="154" t="s">
         <v>271</v>
       </c>
@@ -3206,7 +3206,7 @@
       </c>
     </row>
     <row r="36" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A36" s="156"/>
+      <c r="A36" s="157"/>
       <c r="B36" s="149" t="s">
         <v>223</v>
       </c>
@@ -3226,7 +3226,7 @@
       </c>
     </row>
     <row r="37" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A37" s="156"/>
+      <c r="A37" s="157"/>
       <c r="B37" s="149" t="s">
         <v>224</v>
       </c>
@@ -3243,7 +3243,7 @@
       <c r="F37" s="105"/>
     </row>
     <row r="38" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A38" s="156"/>
+      <c r="A38" s="157"/>
       <c r="B38" s="149" t="s">
         <v>225</v>
       </c>
@@ -3260,7 +3260,7 @@
       <c r="F38" s="105"/>
     </row>
     <row r="39" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A39" s="156"/>
+      <c r="A39" s="157"/>
       <c r="B39" s="149" t="s">
         <v>217</v>
       </c>
@@ -3277,7 +3277,7 @@
       <c r="F39" s="105"/>
     </row>
     <row r="40" spans="1:9" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="A40" s="156"/>
+      <c r="A40" s="157"/>
       <c r="B40" s="98" t="s">
         <v>179</v>
       </c>
@@ -3316,7 +3316,7 @@
     </row>
     <row r="42" spans="1:9" ht="13.5" thickBot="1"/>
     <row r="43" spans="1:9" ht="15" customHeight="1" outlineLevel="1">
-      <c r="A43" s="155" t="s">
+      <c r="A43" s="156" t="s">
         <v>226</v>
       </c>
       <c r="B43" s="113" t="s">
@@ -3336,7 +3336,7 @@
       </c>
     </row>
     <row r="44" spans="1:9" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="A44" s="156"/>
+      <c r="A44" s="157"/>
       <c r="B44" s="98" t="s">
         <v>177</v>
       </c>
@@ -3354,7 +3354,7 @@
       </c>
     </row>
     <row r="45" spans="1:9" ht="15.75" outlineLevel="1" thickTop="1">
-      <c r="A45" s="156"/>
+      <c r="A45" s="157"/>
       <c r="B45" s="100"/>
       <c r="C45" s="101"/>
       <c r="D45" s="101"/>
@@ -3365,7 +3365,7 @@
       <c r="F45" s="105"/>
     </row>
     <row r="46" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A46" s="156"/>
+      <c r="A46" s="157"/>
       <c r="B46" s="149" t="s">
         <v>221</v>
       </c>
@@ -3382,8 +3382,8 @@
       <c r="F46" s="105"/>
     </row>
     <row r="47" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A47" s="156"/>
-      <c r="B47" s="220" t="s">
+      <c r="A47" s="157"/>
+      <c r="B47" s="155" t="s">
         <v>274</v>
       </c>
       <c r="C47" s="101">
@@ -3399,30 +3399,32 @@
       <c r="F47" s="105"/>
     </row>
     <row r="48" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A48" s="156"/>
-      <c r="B48" s="220"/>
+      <c r="A48" s="157"/>
+      <c r="B48" s="155"/>
       <c r="C48" s="101"/>
       <c r="D48" s="101"/>
       <c r="E48" s="123"/>
       <c r="F48" s="105"/>
     </row>
     <row r="49" spans="1:6" ht="15" outlineLevel="1">
-      <c r="A49" s="156"/>
+      <c r="A49" s="157"/>
       <c r="B49" s="149" t="s">
         <v>222</v>
       </c>
-      <c r="C49" s="101"/>
+      <c r="C49" s="101">
+        <v>14149</v>
+      </c>
       <c r="D49" s="101">
         <v>17009</v>
       </c>
       <c r="E49" s="123">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>2860</v>
       </c>
       <c r="F49" s="105"/>
     </row>
     <row r="50" spans="1:6" ht="15" outlineLevel="1">
-      <c r="A50" s="156"/>
+      <c r="A50" s="157"/>
       <c r="B50" s="150" t="s">
         <v>229</v>
       </c>
@@ -3437,7 +3439,7 @@
       <c r="F50" s="105"/>
     </row>
     <row r="51" spans="1:6" ht="15" outlineLevel="1">
-      <c r="A51" s="156"/>
+      <c r="A51" s="157"/>
       <c r="B51" s="150" t="s">
         <v>230</v>
       </c>
@@ -3452,7 +3454,7 @@
       <c r="F51" s="105"/>
     </row>
     <row r="52" spans="1:6" ht="15" outlineLevel="1">
-      <c r="A52" s="156"/>
+      <c r="A52" s="157"/>
       <c r="B52" s="150" t="s">
         <v>231</v>
       </c>
@@ -3467,7 +3469,7 @@
       <c r="F52" s="105"/>
     </row>
     <row r="53" spans="1:6" ht="15" outlineLevel="1">
-      <c r="A53" s="156"/>
+      <c r="A53" s="157"/>
       <c r="B53" s="150" t="s">
         <v>233</v>
       </c>
@@ -3482,7 +3484,7 @@
       <c r="F53" s="105"/>
     </row>
     <row r="54" spans="1:6" ht="15" outlineLevel="1">
-      <c r="A54" s="156"/>
+      <c r="A54" s="157"/>
       <c r="B54" s="150" t="s">
         <v>234</v>
       </c>
@@ -3497,7 +3499,7 @@
       <c r="F54" s="105"/>
     </row>
     <row r="55" spans="1:6" ht="15" outlineLevel="1">
-      <c r="A55" s="156"/>
+      <c r="A55" s="157"/>
       <c r="B55" s="150" t="s">
         <v>235</v>
       </c>
@@ -3512,7 +3514,7 @@
       <c r="F55" s="105"/>
     </row>
     <row r="56" spans="1:6" ht="15" outlineLevel="1">
-      <c r="A56" s="156"/>
+      <c r="A56" s="157"/>
       <c r="B56" s="150" t="s">
         <v>236</v>
       </c>
@@ -3527,7 +3529,7 @@
       <c r="F56" s="105"/>
     </row>
     <row r="57" spans="1:6" ht="15" outlineLevel="1">
-      <c r="A57" s="156"/>
+      <c r="A57" s="157"/>
       <c r="B57" s="100"/>
       <c r="C57" s="101"/>
       <c r="D57" s="101"/>
@@ -3538,7 +3540,7 @@
       <c r="F57" s="105"/>
     </row>
     <row r="58" spans="1:6" ht="15" outlineLevel="1">
-      <c r="A58" s="156"/>
+      <c r="A58" s="157"/>
       <c r="B58" s="100"/>
       <c r="C58" s="101"/>
       <c r="D58" s="101"/>
@@ -3549,7 +3551,7 @@
       <c r="F58" s="105"/>
     </row>
     <row r="59" spans="1:6" ht="15" outlineLevel="1">
-      <c r="A59" s="156"/>
+      <c r="A59" s="157"/>
       <c r="B59" s="150" t="s">
         <v>237</v>
       </c>
@@ -3562,7 +3564,7 @@
       <c r="F59" s="105"/>
     </row>
     <row r="60" spans="1:6" ht="15" outlineLevel="1">
-      <c r="A60" s="156"/>
+      <c r="A60" s="157"/>
       <c r="B60" s="150" t="s">
         <v>223</v>
       </c>
@@ -3577,7 +3579,7 @@
       <c r="F60" s="105"/>
     </row>
     <row r="61" spans="1:6" ht="15" outlineLevel="1">
-      <c r="A61" s="156"/>
+      <c r="A61" s="157"/>
       <c r="B61" s="150" t="s">
         <v>238</v>
       </c>
@@ -3592,7 +3594,7 @@
       <c r="F61" s="105"/>
     </row>
     <row r="62" spans="1:6" ht="15" outlineLevel="1">
-      <c r="A62" s="156"/>
+      <c r="A62" s="157"/>
       <c r="B62" s="150" t="s">
         <v>239</v>
       </c>
@@ -3604,7 +3606,7 @@
       <c r="F62" s="105"/>
     </row>
     <row r="63" spans="1:6" ht="15" outlineLevel="1">
-      <c r="A63" s="156"/>
+      <c r="A63" s="157"/>
       <c r="B63" s="150" t="s">
         <v>217</v>
       </c>
@@ -3619,7 +3621,7 @@
       <c r="F63" s="105"/>
     </row>
     <row r="64" spans="1:6" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="A64" s="156"/>
+      <c r="A64" s="157"/>
       <c r="B64" s="98" t="s">
         <v>179</v>
       </c>
@@ -3660,7 +3662,7 @@
     </row>
     <row r="66" spans="1:8" ht="13.5" thickBot="1"/>
     <row r="67" spans="1:8" ht="15" customHeight="1" outlineLevel="1">
-      <c r="A67" s="157" t="s">
+      <c r="A67" s="158" t="s">
         <v>240</v>
       </c>
       <c r="B67" s="109" t="s">
@@ -3680,7 +3682,7 @@
       </c>
     </row>
     <row r="68" spans="1:8" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="A68" s="156"/>
+      <c r="A68" s="157"/>
       <c r="B68" s="98" t="s">
         <v>177</v>
       </c>
@@ -3698,7 +3700,7 @@
       </c>
     </row>
     <row r="69" spans="1:8" ht="15.75" outlineLevel="1" thickTop="1">
-      <c r="A69" s="156"/>
+      <c r="A69" s="157"/>
       <c r="B69" s="100"/>
       <c r="C69" s="101"/>
       <c r="D69" s="101"/>
@@ -3709,7 +3711,7 @@
       <c r="F69" s="105"/>
     </row>
     <row r="70" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A70" s="156"/>
+      <c r="A70" s="157"/>
       <c r="B70" s="151" t="s">
         <v>242</v>
       </c>
@@ -3724,7 +3726,7 @@
       <c r="F70" s="105"/>
     </row>
     <row r="71" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A71" s="156"/>
+      <c r="A71" s="157"/>
       <c r="B71" s="100"/>
       <c r="C71" s="101"/>
       <c r="D71" s="101"/>
@@ -3735,7 +3737,7 @@
       <c r="F71" s="105"/>
     </row>
     <row r="72" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A72" s="156"/>
+      <c r="A72" s="157"/>
       <c r="B72" s="151" t="s">
         <v>243</v>
       </c>
@@ -3750,7 +3752,7 @@
       <c r="F72" s="105"/>
     </row>
     <row r="73" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A73" s="156"/>
+      <c r="A73" s="157"/>
       <c r="B73" s="100"/>
       <c r="C73" s="101"/>
       <c r="D73" s="101"/>
@@ -3761,7 +3763,7 @@
       <c r="F73" s="105"/>
     </row>
     <row r="74" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A74" s="156"/>
+      <c r="A74" s="157"/>
       <c r="B74" s="151" t="s">
         <v>244</v>
       </c>
@@ -3776,7 +3778,7 @@
       <c r="F74" s="105"/>
     </row>
     <row r="75" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A75" s="156"/>
+      <c r="A75" s="157"/>
       <c r="B75" s="100"/>
       <c r="C75" s="101"/>
       <c r="D75" s="101"/>
@@ -3787,7 +3789,7 @@
       <c r="F75" s="105"/>
     </row>
     <row r="76" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A76" s="156"/>
+      <c r="A76" s="157"/>
       <c r="B76" s="151" t="s">
         <v>245</v>
       </c>
@@ -3802,7 +3804,7 @@
       <c r="F76" s="105"/>
     </row>
     <row r="77" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A77" s="156"/>
+      <c r="A77" s="157"/>
       <c r="B77" s="151" t="s">
         <v>238</v>
       </c>
@@ -3817,7 +3819,7 @@
       <c r="F77" s="105"/>
     </row>
     <row r="78" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A78" s="156"/>
+      <c r="A78" s="157"/>
       <c r="B78" s="151" t="s">
         <v>246</v>
       </c>
@@ -3832,7 +3834,7 @@
       <c r="F78" s="105"/>
     </row>
     <row r="79" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A79" s="156"/>
+      <c r="A79" s="157"/>
       <c r="B79" s="151" t="s">
         <v>217</v>
       </c>
@@ -3847,7 +3849,7 @@
       <c r="F79" s="105"/>
     </row>
     <row r="80" spans="1:8" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="A80" s="156"/>
+      <c r="A80" s="157"/>
       <c r="B80" s="98" t="s">
         <v>179</v>
       </c>
@@ -3888,7 +3890,7 @@
     </row>
     <row r="82" spans="1:8" ht="13.5" thickBot="1"/>
     <row r="83" spans="1:8" ht="15" customHeight="1" outlineLevel="1">
-      <c r="A83" s="155" t="s">
+      <c r="A83" s="156" t="s">
         <v>247</v>
       </c>
       <c r="B83" s="113" t="s">
@@ -3908,7 +3910,7 @@
       </c>
     </row>
     <row r="84" spans="1:8" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="A84" s="156"/>
+      <c r="A84" s="157"/>
       <c r="B84" s="98" t="s">
         <v>177</v>
       </c>
@@ -3926,7 +3928,7 @@
       </c>
     </row>
     <row r="85" spans="1:8" ht="15.75" outlineLevel="1" thickTop="1">
-      <c r="A85" s="156"/>
+      <c r="A85" s="157"/>
       <c r="B85" s="151" t="s">
         <v>228</v>
       </c>
@@ -3941,7 +3943,7 @@
       <c r="F85" s="105"/>
     </row>
     <row r="86" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A86" s="156"/>
+      <c r="A86" s="157"/>
       <c r="B86" s="151" t="s">
         <v>221</v>
       </c>
@@ -3956,7 +3958,7 @@
       <c r="F86" s="105"/>
     </row>
     <row r="87" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A87" s="156"/>
+      <c r="A87" s="157"/>
       <c r="B87" s="100"/>
       <c r="C87" s="101"/>
       <c r="D87" s="101"/>
@@ -3967,7 +3969,7 @@
       <c r="F87" s="105"/>
     </row>
     <row r="88" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A88" s="156"/>
+      <c r="A88" s="157"/>
       <c r="B88" s="151" t="s">
         <v>222</v>
       </c>
@@ -3982,7 +3984,7 @@
       <c r="F88" s="105"/>
     </row>
     <row r="89" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A89" s="156"/>
+      <c r="A89" s="157"/>
       <c r="B89" s="100"/>
       <c r="C89" s="101"/>
       <c r="D89" s="101"/>
@@ -3993,7 +3995,7 @@
       <c r="F89" s="105"/>
     </row>
     <row r="90" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A90" s="156"/>
+      <c r="A90" s="157"/>
       <c r="B90" s="152" t="s">
         <v>236</v>
       </c>
@@ -4008,7 +4010,7 @@
       <c r="F90" s="105"/>
     </row>
     <row r="91" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A91" s="156"/>
+      <c r="A91" s="157"/>
       <c r="B91" s="100"/>
       <c r="C91" s="101"/>
       <c r="D91" s="101"/>
@@ -4019,7 +4021,7 @@
       <c r="F91" s="105"/>
     </row>
     <row r="92" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A92" s="156"/>
+      <c r="A92" s="157"/>
       <c r="B92" s="100"/>
       <c r="C92" s="101"/>
       <c r="D92" s="101"/>
@@ -4030,7 +4032,7 @@
       <c r="F92" s="105"/>
     </row>
     <row r="93" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A93" s="156"/>
+      <c r="A93" s="157"/>
       <c r="B93" s="152" t="s">
         <v>223</v>
       </c>
@@ -4045,7 +4047,7 @@
       <c r="F93" s="105"/>
     </row>
     <row r="94" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A94" s="156"/>
+      <c r="A94" s="157"/>
       <c r="B94" s="152" t="s">
         <v>249</v>
       </c>
@@ -4060,7 +4062,7 @@
       <c r="F94" s="105"/>
     </row>
     <row r="95" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A95" s="156"/>
+      <c r="A95" s="157"/>
       <c r="B95" s="152" t="s">
         <v>250</v>
       </c>
@@ -4075,7 +4077,7 @@
       <c r="F95" s="105"/>
     </row>
     <row r="96" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A96" s="156"/>
+      <c r="A96" s="157"/>
       <c r="B96" s="152" t="s">
         <v>251</v>
       </c>
@@ -4090,7 +4092,7 @@
       <c r="F96" s="105"/>
     </row>
     <row r="97" spans="1:8" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="A97" s="156"/>
+      <c r="A97" s="157"/>
       <c r="B97" s="98" t="s">
         <v>179</v>
       </c>
@@ -4131,7 +4133,7 @@
     </row>
     <row r="99" spans="1:8" ht="13.5" thickBot="1"/>
     <row r="100" spans="1:8" ht="15" customHeight="1" outlineLevel="1">
-      <c r="A100" s="157" t="s">
+      <c r="A100" s="158" t="s">
         <v>252</v>
       </c>
       <c r="B100" s="109" t="s">
@@ -4151,7 +4153,7 @@
       </c>
     </row>
     <row r="101" spans="1:8" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="A101" s="156"/>
+      <c r="A101" s="157"/>
       <c r="B101" s="98" t="s">
         <v>177</v>
       </c>
@@ -4169,7 +4171,7 @@
       </c>
     </row>
     <row r="102" spans="1:8" ht="15.75" outlineLevel="1" thickTop="1">
-      <c r="A102" s="156"/>
+      <c r="A102" s="157"/>
       <c r="B102" s="100"/>
       <c r="C102" s="101"/>
       <c r="D102" s="101"/>
@@ -4180,7 +4182,7 @@
       <c r="F102" s="105"/>
     </row>
     <row r="103" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A103" s="156"/>
+      <c r="A103" s="157"/>
       <c r="B103" s="152" t="s">
         <v>254</v>
       </c>
@@ -4195,7 +4197,7 @@
       <c r="F103" s="105"/>
     </row>
     <row r="104" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A104" s="156"/>
+      <c r="A104" s="157"/>
       <c r="B104" s="100"/>
       <c r="C104" s="101"/>
       <c r="D104" s="101"/>
@@ -4206,7 +4208,7 @@
       <c r="F104" s="105"/>
     </row>
     <row r="105" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A105" s="156"/>
+      <c r="A105" s="157"/>
       <c r="B105" s="152" t="s">
         <v>255</v>
       </c>
@@ -4221,7 +4223,7 @@
       <c r="F105" s="105"/>
     </row>
     <row r="106" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A106" s="156"/>
+      <c r="A106" s="157"/>
       <c r="B106" s="100"/>
       <c r="C106" s="101"/>
       <c r="D106" s="101"/>
@@ -4232,7 +4234,7 @@
       <c r="F106" s="105"/>
     </row>
     <row r="107" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A107" s="156"/>
+      <c r="A107" s="157"/>
       <c r="B107" s="152" t="s">
         <v>223</v>
       </c>
@@ -4247,7 +4249,7 @@
       <c r="F107" s="105"/>
     </row>
     <row r="108" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A108" s="156"/>
+      <c r="A108" s="157"/>
       <c r="B108" s="152" t="s">
         <v>249</v>
       </c>
@@ -4262,7 +4264,7 @@
       <c r="F108" s="105"/>
     </row>
     <row r="109" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A109" s="156"/>
+      <c r="A109" s="157"/>
       <c r="B109" s="152" t="s">
         <v>256</v>
       </c>
@@ -4277,7 +4279,7 @@
       <c r="F109" s="105"/>
     </row>
     <row r="110" spans="1:8" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="A110" s="156"/>
+      <c r="A110" s="157"/>
       <c r="B110" s="98" t="s">
         <v>179</v>
       </c>
@@ -4318,7 +4320,7 @@
     </row>
     <row r="112" spans="1:8" ht="13.5" thickBot="1"/>
     <row r="113" spans="1:9" ht="15" customHeight="1" outlineLevel="1">
-      <c r="A113" s="155" t="s">
+      <c r="A113" s="156" t="s">
         <v>257</v>
       </c>
       <c r="B113" s="113" t="s">
@@ -4338,7 +4340,7 @@
       </c>
     </row>
     <row r="114" spans="1:9" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="A114" s="156"/>
+      <c r="A114" s="157"/>
       <c r="B114" s="98" t="s">
         <v>177</v>
       </c>
@@ -4360,7 +4362,7 @@
       </c>
     </row>
     <row r="115" spans="1:9" ht="15.75" outlineLevel="1" thickTop="1">
-      <c r="A115" s="156"/>
+      <c r="A115" s="157"/>
       <c r="B115" s="100"/>
       <c r="C115" s="101"/>
       <c r="D115" s="101"/>
@@ -4371,7 +4373,7 @@
       <c r="F115" s="105"/>
     </row>
     <row r="116" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A116" s="156"/>
+      <c r="A116" s="157"/>
       <c r="B116" s="152" t="s">
         <v>221</v>
       </c>
@@ -4386,7 +4388,7 @@
       <c r="F116" s="105"/>
     </row>
     <row r="117" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A117" s="156"/>
+      <c r="A117" s="157"/>
       <c r="B117" s="100"/>
       <c r="C117" s="101"/>
       <c r="D117" s="101"/>
@@ -4397,7 +4399,7 @@
       <c r="F117" s="105"/>
     </row>
     <row r="118" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A118" s="156"/>
+      <c r="A118" s="157"/>
       <c r="B118" s="152" t="s">
         <v>222</v>
       </c>
@@ -4412,7 +4414,7 @@
       <c r="F118" s="105"/>
     </row>
     <row r="119" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A119" s="156"/>
+      <c r="A119" s="157"/>
       <c r="B119" s="152" t="s">
         <v>249</v>
       </c>
@@ -4427,7 +4429,7 @@
       <c r="F119" s="105"/>
     </row>
     <row r="120" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A120" s="156"/>
+      <c r="A120" s="157"/>
       <c r="B120" s="152" t="s">
         <v>259</v>
       </c>
@@ -4442,7 +4444,7 @@
       <c r="F120" s="105"/>
     </row>
     <row r="121" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A121" s="156"/>
+      <c r="A121" s="157"/>
       <c r="B121" s="152" t="s">
         <v>224</v>
       </c>
@@ -4457,7 +4459,7 @@
       <c r="F121" s="105"/>
     </row>
     <row r="122" spans="1:9" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="A122" s="156"/>
+      <c r="A122" s="157"/>
       <c r="B122" s="98" t="s">
         <v>179</v>
       </c>
@@ -4498,7 +4500,7 @@
     </row>
     <row r="124" spans="1:9" ht="13.5" thickBot="1"/>
     <row r="125" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A125" s="157" t="s">
+      <c r="A125" s="158" t="s">
         <v>260</v>
       </c>
       <c r="B125" s="109" t="s">
@@ -4518,7 +4520,7 @@
       </c>
     </row>
     <row r="126" spans="1:9" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="A126" s="156"/>
+      <c r="A126" s="157"/>
       <c r="B126" s="98" t="s">
         <v>177</v>
       </c>
@@ -4540,7 +4542,7 @@
       </c>
     </row>
     <row r="127" spans="1:9" ht="15.75" outlineLevel="1" thickTop="1">
-      <c r="A127" s="156"/>
+      <c r="A127" s="157"/>
       <c r="B127" s="100"/>
       <c r="C127" s="101"/>
       <c r="D127" s="101"/>
@@ -4551,7 +4553,7 @@
       <c r="F127" s="105"/>
     </row>
     <row r="128" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A128" s="156"/>
+      <c r="A128" s="157"/>
       <c r="B128" s="100"/>
       <c r="C128" s="101"/>
       <c r="D128" s="101"/>
@@ -4562,7 +4564,7 @@
       <c r="F128" s="105"/>
     </row>
     <row r="129" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A129" s="156"/>
+      <c r="A129" s="157"/>
       <c r="B129" s="100"/>
       <c r="C129" s="101"/>
       <c r="D129" s="101"/>
@@ -4573,7 +4575,7 @@
       <c r="F129" s="105"/>
     </row>
     <row r="130" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A130" s="156"/>
+      <c r="A130" s="157"/>
       <c r="B130" s="100"/>
       <c r="C130" s="101"/>
       <c r="D130" s="101"/>
@@ -4584,7 +4586,7 @@
       <c r="F130" s="105"/>
     </row>
     <row r="131" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A131" s="156"/>
+      <c r="A131" s="157"/>
       <c r="B131" s="100"/>
       <c r="C131" s="101"/>
       <c r="D131" s="101"/>
@@ -4595,7 +4597,7 @@
       <c r="F131" s="105"/>
     </row>
     <row r="132" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A132" s="156"/>
+      <c r="A132" s="157"/>
       <c r="B132" s="100"/>
       <c r="C132" s="101"/>
       <c r="D132" s="101"/>
@@ -4606,7 +4608,7 @@
       <c r="F132" s="105"/>
     </row>
     <row r="133" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A133" s="156"/>
+      <c r="A133" s="157"/>
       <c r="B133" s="100"/>
       <c r="C133" s="101"/>
       <c r="D133" s="101"/>
@@ -4617,7 +4619,7 @@
       <c r="F133" s="105"/>
     </row>
     <row r="134" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A134" s="156"/>
+      <c r="A134" s="157"/>
       <c r="B134" s="100"/>
       <c r="C134" s="101"/>
       <c r="D134" s="101"/>
@@ -4628,7 +4630,7 @@
       <c r="F134" s="105"/>
     </row>
     <row r="135" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A135" s="156"/>
+      <c r="A135" s="157"/>
       <c r="B135" s="152" t="s">
         <v>262</v>
       </c>
@@ -4650,7 +4652,7 @@
       </c>
     </row>
     <row r="136" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A136" s="156"/>
+      <c r="A136" s="157"/>
       <c r="B136" s="100"/>
       <c r="C136" s="101"/>
       <c r="D136" s="101"/>
@@ -4661,7 +4663,7 @@
       <c r="F136" s="105"/>
     </row>
     <row r="137" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A137" s="156"/>
+      <c r="A137" s="157"/>
       <c r="B137" s="100"/>
       <c r="C137" s="101"/>
       <c r="D137" s="101"/>
@@ -4672,7 +4674,7 @@
       <c r="F137" s="105"/>
     </row>
     <row r="138" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A138" s="156"/>
+      <c r="A138" s="157"/>
       <c r="B138" s="100"/>
       <c r="C138" s="101"/>
       <c r="D138" s="101"/>
@@ -4683,7 +4685,7 @@
       <c r="F138" s="105"/>
     </row>
     <row r="139" spans="1:9" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="A139" s="156"/>
+      <c r="A139" s="157"/>
       <c r="B139" s="98" t="s">
         <v>179</v>
       </c>
@@ -4721,7 +4723,7 @@
       </c>
     </row>
     <row r="142" spans="1:9" ht="15" hidden="1" outlineLevel="2">
-      <c r="A142" s="155" t="s">
+      <c r="A142" s="156" t="s">
         <v>169</v>
       </c>
       <c r="B142" s="113" t="s">
@@ -4741,7 +4743,7 @@
       </c>
     </row>
     <row r="143" spans="1:9" ht="15.75" hidden="1" outlineLevel="2" thickBot="1">
-      <c r="A143" s="156"/>
+      <c r="A143" s="157"/>
       <c r="B143" s="98" t="s">
         <v>177</v>
       </c>
@@ -4754,7 +4756,7 @@
       <c r="F143" s="104"/>
     </row>
     <row r="144" spans="1:9" ht="15.75" hidden="1" outlineLevel="2" thickTop="1">
-      <c r="A144" s="156"/>
+      <c r="A144" s="157"/>
       <c r="B144" s="100"/>
       <c r="C144" s="101"/>
       <c r="D144" s="101"/>
@@ -4765,7 +4767,7 @@
       <c r="F144" s="105"/>
     </row>
     <row r="145" spans="1:7" ht="15" hidden="1" outlineLevel="2">
-      <c r="A145" s="156"/>
+      <c r="A145" s="157"/>
       <c r="B145" s="100"/>
       <c r="C145" s="101"/>
       <c r="D145" s="101"/>
@@ -4776,7 +4778,7 @@
       <c r="F145" s="105"/>
     </row>
     <row r="146" spans="1:7" ht="15" hidden="1" outlineLevel="2">
-      <c r="A146" s="156"/>
+      <c r="A146" s="157"/>
       <c r="B146" s="100"/>
       <c r="C146" s="101"/>
       <c r="D146" s="101"/>
@@ -4787,7 +4789,7 @@
       <c r="F146" s="105"/>
     </row>
     <row r="147" spans="1:7" ht="15" hidden="1" outlineLevel="2">
-      <c r="A147" s="156"/>
+      <c r="A147" s="157"/>
       <c r="B147" s="100"/>
       <c r="C147" s="101"/>
       <c r="D147" s="101"/>
@@ -4798,7 +4800,7 @@
       <c r="F147" s="105"/>
     </row>
     <row r="148" spans="1:7" ht="15" hidden="1" outlineLevel="2">
-      <c r="A148" s="156"/>
+      <c r="A148" s="157"/>
       <c r="B148" s="100"/>
       <c r="C148" s="101"/>
       <c r="D148" s="101"/>
@@ -4809,7 +4811,7 @@
       <c r="F148" s="105"/>
     </row>
     <row r="149" spans="1:7" ht="15" hidden="1" outlineLevel="2">
-      <c r="A149" s="156"/>
+      <c r="A149" s="157"/>
       <c r="B149" s="100"/>
       <c r="C149" s="101"/>
       <c r="D149" s="101"/>
@@ -4820,7 +4822,7 @@
       <c r="F149" s="105"/>
     </row>
     <row r="150" spans="1:7" ht="15" hidden="1" outlineLevel="2">
-      <c r="A150" s="156"/>
+      <c r="A150" s="157"/>
       <c r="B150" s="100"/>
       <c r="C150" s="101"/>
       <c r="D150" s="101"/>
@@ -4831,7 +4833,7 @@
       <c r="F150" s="105"/>
     </row>
     <row r="151" spans="1:7" ht="15" hidden="1" outlineLevel="2">
-      <c r="A151" s="156"/>
+      <c r="A151" s="157"/>
       <c r="B151" s="100"/>
       <c r="C151" s="101"/>
       <c r="D151" s="101"/>
@@ -4842,7 +4844,7 @@
       <c r="F151" s="105"/>
     </row>
     <row r="152" spans="1:7" ht="15" hidden="1" outlineLevel="2">
-      <c r="A152" s="156"/>
+      <c r="A152" s="157"/>
       <c r="B152" s="100"/>
       <c r="C152" s="101"/>
       <c r="D152" s="101"/>
@@ -4853,7 +4855,7 @@
       <c r="F152" s="105"/>
     </row>
     <row r="153" spans="1:7" ht="15" hidden="1" outlineLevel="2">
-      <c r="A153" s="156"/>
+      <c r="A153" s="157"/>
       <c r="B153" s="100"/>
       <c r="C153" s="101"/>
       <c r="D153" s="101"/>
@@ -4864,7 +4866,7 @@
       <c r="F153" s="105"/>
     </row>
     <row r="154" spans="1:7" ht="15" hidden="1" outlineLevel="2">
-      <c r="A154" s="156"/>
+      <c r="A154" s="157"/>
       <c r="B154" s="100"/>
       <c r="C154" s="101"/>
       <c r="D154" s="101"/>
@@ -4875,7 +4877,7 @@
       <c r="F154" s="105"/>
     </row>
     <row r="155" spans="1:7" ht="15" hidden="1" outlineLevel="2">
-      <c r="A155" s="156"/>
+      <c r="A155" s="157"/>
       <c r="B155" s="100"/>
       <c r="C155" s="101"/>
       <c r="D155" s="101"/>
@@ -4886,7 +4888,7 @@
       <c r="F155" s="105"/>
     </row>
     <row r="156" spans="1:7" ht="15.75" hidden="1" outlineLevel="2" thickBot="1">
-      <c r="A156" s="156"/>
+      <c r="A156" s="157"/>
       <c r="B156" s="98" t="s">
         <v>179</v>
       </c>
@@ -4925,11 +4927,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="A142:A156"/>
-    <mergeCell ref="A113:A122"/>
-    <mergeCell ref="A83:A97"/>
-    <mergeCell ref="A125:A139"/>
-    <mergeCell ref="A100:A110"/>
     <mergeCell ref="A43:A64"/>
     <mergeCell ref="A67:A80"/>
     <mergeCell ref="C5:D5"/>
@@ -4939,6 +4936,11 @@
     <mergeCell ref="A8:A18"/>
     <mergeCell ref="A21:A40"/>
     <mergeCell ref="C4:E4"/>
+    <mergeCell ref="A142:A156"/>
+    <mergeCell ref="A113:A122"/>
+    <mergeCell ref="A83:A97"/>
+    <mergeCell ref="A125:A139"/>
+    <mergeCell ref="A100:A110"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4970,13 +4972,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="26.25" customHeight="1">
-      <c r="A1" s="165" t="s">
+      <c r="A1" s="184" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="165"/>
-      <c r="C1" s="165"/>
-      <c r="D1" s="165"/>
-      <c r="E1" s="165"/>
+      <c r="B1" s="184"/>
+      <c r="C1" s="184"/>
+      <c r="D1" s="184"/>
+      <c r="E1" s="184"/>
       <c r="F1" s="7"/>
       <c r="G1" s="5"/>
       <c r="H1" s="5"/>
@@ -5006,18 +5008,18 @@
         <v>8</v>
       </c>
       <c r="B3" s="36"/>
-      <c r="C3" s="166"/>
-      <c r="D3" s="167"/>
-      <c r="E3" s="167"/>
+      <c r="C3" s="185"/>
+      <c r="D3" s="186"/>
+      <c r="E3" s="186"/>
     </row>
     <row r="4" spans="1:8" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A4" s="46" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="87"/>
-      <c r="C4" s="168"/>
-      <c r="D4" s="169"/>
-      <c r="E4" s="169"/>
+      <c r="C4" s="166"/>
+      <c r="D4" s="167"/>
+      <c r="E4" s="167"/>
       <c r="F4" s="6"/>
     </row>
     <row r="5" spans="1:8" hidden="1" outlineLevel="2">
@@ -5169,9 +5171,9 @@
         <v>9</v>
       </c>
       <c r="B21" s="90"/>
-      <c r="C21" s="170"/>
-      <c r="D21" s="171"/>
-      <c r="E21" s="171"/>
+      <c r="C21" s="168"/>
+      <c r="D21" s="169"/>
+      <c r="E21" s="169"/>
     </row>
     <row r="22" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A22" s="47">
@@ -5322,9 +5324,9 @@
         <v>10</v>
       </c>
       <c r="B38" s="87"/>
-      <c r="C38" s="168"/>
-      <c r="D38" s="169"/>
-      <c r="E38" s="169"/>
+      <c r="C38" s="166"/>
+      <c r="D38" s="167"/>
+      <c r="E38" s="167"/>
     </row>
     <row r="39" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A39" s="47">
@@ -5475,9 +5477,9 @@
         <v>11</v>
       </c>
       <c r="B55" s="87"/>
-      <c r="C55" s="168"/>
-      <c r="D55" s="169"/>
-      <c r="E55" s="169"/>
+      <c r="C55" s="166"/>
+      <c r="D55" s="167"/>
+      <c r="E55" s="167"/>
     </row>
     <row r="56" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A56" s="47">
@@ -5628,9 +5630,9 @@
         <v>12</v>
       </c>
       <c r="B72" s="87"/>
-      <c r="C72" s="168"/>
-      <c r="D72" s="169"/>
-      <c r="E72" s="169"/>
+      <c r="C72" s="166"/>
+      <c r="D72" s="167"/>
+      <c r="E72" s="167"/>
     </row>
     <row r="73" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A73" s="47">
@@ -5781,9 +5783,9 @@
         <v>13</v>
       </c>
       <c r="B89" s="87"/>
-      <c r="C89" s="168"/>
-      <c r="D89" s="169"/>
-      <c r="E89" s="169"/>
+      <c r="C89" s="166"/>
+      <c r="D89" s="167"/>
+      <c r="E89" s="167"/>
     </row>
     <row r="90" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A90" s="47">
@@ -5934,9 +5936,9 @@
         <v>14</v>
       </c>
       <c r="B106" s="87"/>
-      <c r="C106" s="168"/>
-      <c r="D106" s="169"/>
-      <c r="E106" s="169"/>
+      <c r="C106" s="166"/>
+      <c r="D106" s="167"/>
+      <c r="E106" s="167"/>
     </row>
     <row r="107" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A107" s="47">
@@ -6087,9 +6089,9 @@
         <v>15</v>
       </c>
       <c r="B123" s="87"/>
-      <c r="C123" s="168"/>
-      <c r="D123" s="169"/>
-      <c r="E123" s="169"/>
+      <c r="C123" s="166"/>
+      <c r="D123" s="167"/>
+      <c r="E123" s="167"/>
     </row>
     <row r="124" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A124" s="47">
@@ -6240,9 +6242,9 @@
         <v>16</v>
       </c>
       <c r="B140" s="87"/>
-      <c r="C140" s="168"/>
-      <c r="D140" s="169"/>
-      <c r="E140" s="169"/>
+      <c r="C140" s="166"/>
+      <c r="D140" s="167"/>
+      <c r="E140" s="167"/>
     </row>
     <row r="141" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A141" s="47">
@@ -6393,9 +6395,9 @@
         <v>17</v>
       </c>
       <c r="B157" s="87"/>
-      <c r="C157" s="168"/>
-      <c r="D157" s="169"/>
-      <c r="E157" s="169"/>
+      <c r="C157" s="166"/>
+      <c r="D157" s="167"/>
+      <c r="E157" s="167"/>
     </row>
     <row r="158" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A158" s="47">
@@ -6546,9 +6548,9 @@
         <v>18</v>
       </c>
       <c r="B174" s="87"/>
-      <c r="C174" s="168"/>
-      <c r="D174" s="169"/>
-      <c r="E174" s="169"/>
+      <c r="C174" s="166"/>
+      <c r="D174" s="167"/>
+      <c r="E174" s="167"/>
     </row>
     <row r="175" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A175" s="47">
@@ -6699,9 +6701,9 @@
         <v>19</v>
       </c>
       <c r="B191" s="87"/>
-      <c r="C191" s="168"/>
-      <c r="D191" s="169"/>
-      <c r="E191" s="169"/>
+      <c r="C191" s="166"/>
+      <c r="D191" s="167"/>
+      <c r="E191" s="167"/>
     </row>
     <row r="192" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A192" s="47">
@@ -6852,9 +6854,9 @@
         <v>20</v>
       </c>
       <c r="B208" s="87"/>
-      <c r="C208" s="168"/>
-      <c r="D208" s="169"/>
-      <c r="E208" s="169"/>
+      <c r="C208" s="166"/>
+      <c r="D208" s="167"/>
+      <c r="E208" s="167"/>
     </row>
     <row r="209" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A209" s="47">
@@ -7005,9 +7007,9 @@
         <v>21</v>
       </c>
       <c r="B225" s="87"/>
-      <c r="C225" s="168"/>
-      <c r="D225" s="169"/>
-      <c r="E225" s="169"/>
+      <c r="C225" s="166"/>
+      <c r="D225" s="167"/>
+      <c r="E225" s="167"/>
     </row>
     <row r="226" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A226" s="47">
@@ -7158,9 +7160,9 @@
         <v>22</v>
       </c>
       <c r="B242" s="87"/>
-      <c r="C242" s="168"/>
-      <c r="D242" s="169"/>
-      <c r="E242" s="169"/>
+      <c r="C242" s="166"/>
+      <c r="D242" s="167"/>
+      <c r="E242" s="167"/>
     </row>
     <row r="243" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A243" s="47">
@@ -7311,9 +7313,9 @@
         <v>23</v>
       </c>
       <c r="B259" s="87"/>
-      <c r="C259" s="168"/>
-      <c r="D259" s="169"/>
-      <c r="E259" s="169"/>
+      <c r="C259" s="166"/>
+      <c r="D259" s="167"/>
+      <c r="E259" s="167"/>
     </row>
     <row r="260" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A260" s="47">
@@ -7464,18 +7466,18 @@
         <v>24</v>
       </c>
       <c r="B276" s="37"/>
-      <c r="C276" s="172"/>
-      <c r="D276" s="173"/>
-      <c r="E276" s="173"/>
+      <c r="C276" s="182"/>
+      <c r="D276" s="183"/>
+      <c r="E276" s="183"/>
     </row>
     <row r="277" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A277" s="51" t="s">
         <v>25</v>
       </c>
       <c r="B277" s="87"/>
-      <c r="C277" s="168"/>
-      <c r="D277" s="169"/>
-      <c r="E277" s="169"/>
+      <c r="C277" s="166"/>
+      <c r="D277" s="167"/>
+      <c r="E277" s="167"/>
     </row>
     <row r="278" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A278" s="52">
@@ -7626,9 +7628,9 @@
         <v>26</v>
       </c>
       <c r="B294" s="90"/>
-      <c r="C294" s="170"/>
-      <c r="D294" s="171"/>
-      <c r="E294" s="171"/>
+      <c r="C294" s="168"/>
+      <c r="D294" s="169"/>
+      <c r="E294" s="169"/>
     </row>
     <row r="295" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A295" s="52">
@@ -7779,9 +7781,9 @@
         <v>27</v>
       </c>
       <c r="B311" s="87"/>
-      <c r="C311" s="168"/>
-      <c r="D311" s="169"/>
-      <c r="E311" s="169"/>
+      <c r="C311" s="166"/>
+      <c r="D311" s="167"/>
+      <c r="E311" s="167"/>
     </row>
     <row r="312" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A312" s="52">
@@ -7932,9 +7934,9 @@
         <v>28</v>
       </c>
       <c r="B328" s="87"/>
-      <c r="C328" s="168"/>
-      <c r="D328" s="169"/>
-      <c r="E328" s="169"/>
+      <c r="C328" s="166"/>
+      <c r="D328" s="167"/>
+      <c r="E328" s="167"/>
     </row>
     <row r="329" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A329" s="52">
@@ -8085,9 +8087,9 @@
         <v>29</v>
       </c>
       <c r="B345" s="87"/>
-      <c r="C345" s="168"/>
-      <c r="D345" s="169"/>
-      <c r="E345" s="169"/>
+      <c r="C345" s="166"/>
+      <c r="D345" s="167"/>
+      <c r="E345" s="167"/>
     </row>
     <row r="346" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A346" s="52">
@@ -8238,9 +8240,9 @@
         <v>30</v>
       </c>
       <c r="B362" s="87"/>
-      <c r="C362" s="168"/>
-      <c r="D362" s="169"/>
-      <c r="E362" s="169"/>
+      <c r="C362" s="166"/>
+      <c r="D362" s="167"/>
+      <c r="E362" s="167"/>
     </row>
     <row r="363" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A363" s="52">
@@ -8391,9 +8393,9 @@
         <v>31</v>
       </c>
       <c r="B379" s="87"/>
-      <c r="C379" s="168"/>
-      <c r="D379" s="169"/>
-      <c r="E379" s="169"/>
+      <c r="C379" s="166"/>
+      <c r="D379" s="167"/>
+      <c r="E379" s="167"/>
     </row>
     <row r="380" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A380" s="52">
@@ -8544,9 +8546,9 @@
         <v>32</v>
       </c>
       <c r="B396" s="87"/>
-      <c r="C396" s="168"/>
-      <c r="D396" s="169"/>
-      <c r="E396" s="169"/>
+      <c r="C396" s="166"/>
+      <c r="D396" s="167"/>
+      <c r="E396" s="167"/>
     </row>
     <row r="397" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A397" s="52">
@@ -8697,9 +8699,9 @@
         <v>33</v>
       </c>
       <c r="B413" s="87"/>
-      <c r="C413" s="168"/>
-      <c r="D413" s="169"/>
-      <c r="E413" s="169"/>
+      <c r="C413" s="166"/>
+      <c r="D413" s="167"/>
+      <c r="E413" s="167"/>
     </row>
     <row r="414" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A414" s="52">
@@ -8850,9 +8852,9 @@
         <v>34</v>
       </c>
       <c r="B430" s="87"/>
-      <c r="C430" s="168"/>
-      <c r="D430" s="169"/>
-      <c r="E430" s="169"/>
+      <c r="C430" s="166"/>
+      <c r="D430" s="167"/>
+      <c r="E430" s="167"/>
     </row>
     <row r="431" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A431" s="52">
@@ -9003,9 +9005,9 @@
         <v>35</v>
       </c>
       <c r="B447" s="87"/>
-      <c r="C447" s="168"/>
-      <c r="D447" s="169"/>
-      <c r="E447" s="169"/>
+      <c r="C447" s="166"/>
+      <c r="D447" s="167"/>
+      <c r="E447" s="167"/>
     </row>
     <row r="448" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A448" s="52">
@@ -9156,9 +9158,9 @@
         <v>36</v>
       </c>
       <c r="B464" s="87"/>
-      <c r="C464" s="168"/>
-      <c r="D464" s="169"/>
-      <c r="E464" s="169"/>
+      <c r="C464" s="166"/>
+      <c r="D464" s="167"/>
+      <c r="E464" s="167"/>
     </row>
     <row r="465" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A465" s="52">
@@ -9309,9 +9311,9 @@
         <v>37</v>
       </c>
       <c r="B481" s="87"/>
-      <c r="C481" s="168"/>
-      <c r="D481" s="169"/>
-      <c r="E481" s="169"/>
+      <c r="C481" s="166"/>
+      <c r="D481" s="167"/>
+      <c r="E481" s="167"/>
     </row>
     <row r="482" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A482" s="52">
@@ -9462,9 +9464,9 @@
         <v>38</v>
       </c>
       <c r="B498" s="87"/>
-      <c r="C498" s="168"/>
-      <c r="D498" s="169"/>
-      <c r="E498" s="169"/>
+      <c r="C498" s="166"/>
+      <c r="D498" s="167"/>
+      <c r="E498" s="167"/>
     </row>
     <row r="499" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A499" s="52">
@@ -9615,9 +9617,9 @@
         <v>39</v>
       </c>
       <c r="B515" s="87"/>
-      <c r="C515" s="168"/>
-      <c r="D515" s="169"/>
-      <c r="E515" s="169"/>
+      <c r="C515" s="166"/>
+      <c r="D515" s="167"/>
+      <c r="E515" s="167"/>
     </row>
     <row r="516" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A516" s="52">
@@ -9768,9 +9770,9 @@
         <v>40</v>
       </c>
       <c r="B532" s="87"/>
-      <c r="C532" s="168"/>
-      <c r="D532" s="169"/>
-      <c r="E532" s="169"/>
+      <c r="C532" s="166"/>
+      <c r="D532" s="167"/>
+      <c r="E532" s="167"/>
     </row>
     <row r="533" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A533" s="55">
@@ -9921,18 +9923,18 @@
         <v>50</v>
       </c>
       <c r="B549" s="38"/>
-      <c r="C549" s="174"/>
-      <c r="D549" s="175"/>
-      <c r="E549" s="175"/>
+      <c r="C549" s="180"/>
+      <c r="D549" s="181"/>
+      <c r="E549" s="181"/>
     </row>
     <row r="550" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A550" s="58" t="s">
         <v>51</v>
       </c>
       <c r="B550" s="87"/>
-      <c r="C550" s="168"/>
-      <c r="D550" s="169"/>
-      <c r="E550" s="169"/>
+      <c r="C550" s="166"/>
+      <c r="D550" s="167"/>
+      <c r="E550" s="167"/>
     </row>
     <row r="551" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A551" s="59">
@@ -10083,9 +10085,9 @@
         <v>52</v>
       </c>
       <c r="B567" s="90"/>
-      <c r="C567" s="170"/>
-      <c r="D567" s="171"/>
-      <c r="E567" s="171"/>
+      <c r="C567" s="168"/>
+      <c r="D567" s="169"/>
+      <c r="E567" s="169"/>
     </row>
     <row r="568" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A568" s="59">
@@ -10236,9 +10238,9 @@
         <v>53</v>
       </c>
       <c r="B584" s="87"/>
-      <c r="C584" s="168"/>
-      <c r="D584" s="169"/>
-      <c r="E584" s="169"/>
+      <c r="C584" s="166"/>
+      <c r="D584" s="167"/>
+      <c r="E584" s="167"/>
     </row>
     <row r="585" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A585" s="59">
@@ -10389,9 +10391,9 @@
         <v>54</v>
       </c>
       <c r="B601" s="87"/>
-      <c r="C601" s="168"/>
-      <c r="D601" s="169"/>
-      <c r="E601" s="169"/>
+      <c r="C601" s="166"/>
+      <c r="D601" s="167"/>
+      <c r="E601" s="167"/>
     </row>
     <row r="602" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A602" s="59">
@@ -10542,9 +10544,9 @@
         <v>55</v>
       </c>
       <c r="B618" s="87"/>
-      <c r="C618" s="168"/>
-      <c r="D618" s="169"/>
-      <c r="E618" s="169"/>
+      <c r="C618" s="166"/>
+      <c r="D618" s="167"/>
+      <c r="E618" s="167"/>
     </row>
     <row r="619" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A619" s="59">
@@ -10695,9 +10697,9 @@
         <v>56</v>
       </c>
       <c r="B635" s="87"/>
-      <c r="C635" s="168"/>
-      <c r="D635" s="169"/>
-      <c r="E635" s="169"/>
+      <c r="C635" s="166"/>
+      <c r="D635" s="167"/>
+      <c r="E635" s="167"/>
     </row>
     <row r="636" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A636" s="59">
@@ -10848,9 +10850,9 @@
         <v>57</v>
       </c>
       <c r="B652" s="87"/>
-      <c r="C652" s="168"/>
-      <c r="D652" s="169"/>
-      <c r="E652" s="169"/>
+      <c r="C652" s="166"/>
+      <c r="D652" s="167"/>
+      <c r="E652" s="167"/>
     </row>
     <row r="653" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A653" s="59">
@@ -11001,9 +11003,9 @@
         <v>58</v>
       </c>
       <c r="B669" s="87"/>
-      <c r="C669" s="168"/>
-      <c r="D669" s="169"/>
-      <c r="E669" s="169"/>
+      <c r="C669" s="166"/>
+      <c r="D669" s="167"/>
+      <c r="E669" s="167"/>
     </row>
     <row r="670" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A670" s="59">
@@ -11154,9 +11156,9 @@
         <v>59</v>
       </c>
       <c r="B686" s="87"/>
-      <c r="C686" s="168"/>
-      <c r="D686" s="169"/>
-      <c r="E686" s="169"/>
+      <c r="C686" s="166"/>
+      <c r="D686" s="167"/>
+      <c r="E686" s="167"/>
     </row>
     <row r="687" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A687" s="59">
@@ -11307,9 +11309,9 @@
         <v>60</v>
       </c>
       <c r="B703" s="87"/>
-      <c r="C703" s="168"/>
-      <c r="D703" s="169"/>
-      <c r="E703" s="169"/>
+      <c r="C703" s="166"/>
+      <c r="D703" s="167"/>
+      <c r="E703" s="167"/>
     </row>
     <row r="704" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A704" s="59">
@@ -11460,9 +11462,9 @@
         <v>61</v>
       </c>
       <c r="B720" s="87"/>
-      <c r="C720" s="168"/>
-      <c r="D720" s="169"/>
-      <c r="E720" s="169"/>
+      <c r="C720" s="166"/>
+      <c r="D720" s="167"/>
+      <c r="E720" s="167"/>
     </row>
     <row r="721" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A721" s="59">
@@ -11613,9 +11615,9 @@
         <v>62</v>
       </c>
       <c r="B737" s="87"/>
-      <c r="C737" s="168"/>
-      <c r="D737" s="169"/>
-      <c r="E737" s="169"/>
+      <c r="C737" s="166"/>
+      <c r="D737" s="167"/>
+      <c r="E737" s="167"/>
     </row>
     <row r="738" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A738" s="59">
@@ -11766,9 +11768,9 @@
         <v>63</v>
       </c>
       <c r="B754" s="87"/>
-      <c r="C754" s="168"/>
-      <c r="D754" s="169"/>
-      <c r="E754" s="169"/>
+      <c r="C754" s="166"/>
+      <c r="D754" s="167"/>
+      <c r="E754" s="167"/>
     </row>
     <row r="755" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A755" s="59">
@@ -11919,9 +11921,9 @@
         <v>64</v>
       </c>
       <c r="B771" s="87"/>
-      <c r="C771" s="168"/>
-      <c r="D771" s="169"/>
-      <c r="E771" s="169"/>
+      <c r="C771" s="166"/>
+      <c r="D771" s="167"/>
+      <c r="E771" s="167"/>
     </row>
     <row r="772" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A772" s="59">
@@ -12072,9 +12074,9 @@
         <v>65</v>
       </c>
       <c r="B788" s="87"/>
-      <c r="C788" s="168"/>
-      <c r="D788" s="169"/>
-      <c r="E788" s="169"/>
+      <c r="C788" s="166"/>
+      <c r="D788" s="167"/>
+      <c r="E788" s="167"/>
     </row>
     <row r="789" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A789" s="59">
@@ -12225,9 +12227,9 @@
         <v>66</v>
       </c>
       <c r="B805" s="87"/>
-      <c r="C805" s="168"/>
-      <c r="D805" s="169"/>
-      <c r="E805" s="169"/>
+      <c r="C805" s="166"/>
+      <c r="D805" s="167"/>
+      <c r="E805" s="167"/>
     </row>
     <row r="806" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A806" s="59">
@@ -12378,18 +12380,18 @@
         <v>67</v>
       </c>
       <c r="B822" s="39"/>
-      <c r="C822" s="176"/>
-      <c r="D822" s="177"/>
-      <c r="E822" s="177"/>
+      <c r="C822" s="178"/>
+      <c r="D822" s="179"/>
+      <c r="E822" s="179"/>
     </row>
     <row r="823" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A823" s="63" t="s">
         <v>68</v>
       </c>
       <c r="B823" s="87"/>
-      <c r="C823" s="168"/>
-      <c r="D823" s="169"/>
-      <c r="E823" s="169"/>
+      <c r="C823" s="166"/>
+      <c r="D823" s="167"/>
+      <c r="E823" s="167"/>
     </row>
     <row r="824" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A824" s="64">
@@ -12540,9 +12542,9 @@
         <v>69</v>
       </c>
       <c r="B840" s="90"/>
-      <c r="C840" s="170"/>
-      <c r="D840" s="171"/>
-      <c r="E840" s="171"/>
+      <c r="C840" s="168"/>
+      <c r="D840" s="169"/>
+      <c r="E840" s="169"/>
     </row>
     <row r="841" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A841" s="64">
@@ -12693,9 +12695,9 @@
         <v>70</v>
       </c>
       <c r="B857" s="87"/>
-      <c r="C857" s="168"/>
-      <c r="D857" s="169"/>
-      <c r="E857" s="169"/>
+      <c r="C857" s="166"/>
+      <c r="D857" s="167"/>
+      <c r="E857" s="167"/>
     </row>
     <row r="858" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A858" s="64">
@@ -12846,9 +12848,9 @@
         <v>71</v>
       </c>
       <c r="B874" s="87"/>
-      <c r="C874" s="168"/>
-      <c r="D874" s="169"/>
-      <c r="E874" s="169"/>
+      <c r="C874" s="166"/>
+      <c r="D874" s="167"/>
+      <c r="E874" s="167"/>
     </row>
     <row r="875" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A875" s="64">
@@ -12999,9 +13001,9 @@
         <v>72</v>
       </c>
       <c r="B891" s="87"/>
-      <c r="C891" s="168"/>
-      <c r="D891" s="169"/>
-      <c r="E891" s="169"/>
+      <c r="C891" s="166"/>
+      <c r="D891" s="167"/>
+      <c r="E891" s="167"/>
     </row>
     <row r="892" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A892" s="64">
@@ -13152,9 +13154,9 @@
         <v>73</v>
       </c>
       <c r="B908" s="87"/>
-      <c r="C908" s="168"/>
-      <c r="D908" s="169"/>
-      <c r="E908" s="169"/>
+      <c r="C908" s="166"/>
+      <c r="D908" s="167"/>
+      <c r="E908" s="167"/>
     </row>
     <row r="909" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A909" s="64">
@@ -13305,9 +13307,9 @@
         <v>74</v>
       </c>
       <c r="B925" s="87"/>
-      <c r="C925" s="168"/>
-      <c r="D925" s="169"/>
-      <c r="E925" s="169"/>
+      <c r="C925" s="166"/>
+      <c r="D925" s="167"/>
+      <c r="E925" s="167"/>
     </row>
     <row r="926" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A926" s="64">
@@ -13458,9 +13460,9 @@
         <v>75</v>
       </c>
       <c r="B942" s="87"/>
-      <c r="C942" s="168"/>
-      <c r="D942" s="169"/>
-      <c r="E942" s="169"/>
+      <c r="C942" s="166"/>
+      <c r="D942" s="167"/>
+      <c r="E942" s="167"/>
     </row>
     <row r="943" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A943" s="64">
@@ -13611,9 +13613,9 @@
         <v>76</v>
       </c>
       <c r="B959" s="87"/>
-      <c r="C959" s="168"/>
-      <c r="D959" s="169"/>
-      <c r="E959" s="169"/>
+      <c r="C959" s="166"/>
+      <c r="D959" s="167"/>
+      <c r="E959" s="167"/>
     </row>
     <row r="960" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A960" s="64">
@@ -13764,9 +13766,9 @@
         <v>77</v>
       </c>
       <c r="B976" s="87"/>
-      <c r="C976" s="168"/>
-      <c r="D976" s="169"/>
-      <c r="E976" s="169"/>
+      <c r="C976" s="166"/>
+      <c r="D976" s="167"/>
+      <c r="E976" s="167"/>
     </row>
     <row r="977" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A977" s="64">
@@ -13917,9 +13919,9 @@
         <v>78</v>
       </c>
       <c r="B993" s="87"/>
-      <c r="C993" s="168"/>
-      <c r="D993" s="169"/>
-      <c r="E993" s="169"/>
+      <c r="C993" s="166"/>
+      <c r="D993" s="167"/>
+      <c r="E993" s="167"/>
     </row>
     <row r="994" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A994" s="64">
@@ -14070,9 +14072,9 @@
         <v>79</v>
       </c>
       <c r="B1010" s="87"/>
-      <c r="C1010" s="168"/>
-      <c r="D1010" s="169"/>
-      <c r="E1010" s="169"/>
+      <c r="C1010" s="166"/>
+      <c r="D1010" s="167"/>
+      <c r="E1010" s="167"/>
     </row>
     <row r="1011" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1011" s="64">
@@ -14223,9 +14225,9 @@
         <v>80</v>
       </c>
       <c r="B1027" s="87"/>
-      <c r="C1027" s="168"/>
-      <c r="D1027" s="169"/>
-      <c r="E1027" s="169"/>
+      <c r="C1027" s="166"/>
+      <c r="D1027" s="167"/>
+      <c r="E1027" s="167"/>
     </row>
     <row r="1028" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1028" s="64">
@@ -14376,9 +14378,9 @@
         <v>83</v>
       </c>
       <c r="B1044" s="87"/>
-      <c r="C1044" s="168"/>
-      <c r="D1044" s="169"/>
-      <c r="E1044" s="169"/>
+      <c r="C1044" s="166"/>
+      <c r="D1044" s="167"/>
+      <c r="E1044" s="167"/>
     </row>
     <row r="1045" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1045" s="64">
@@ -14529,9 +14531,9 @@
         <v>82</v>
       </c>
       <c r="B1061" s="87"/>
-      <c r="C1061" s="168"/>
-      <c r="D1061" s="169"/>
-      <c r="E1061" s="169"/>
+      <c r="C1061" s="166"/>
+      <c r="D1061" s="167"/>
+      <c r="E1061" s="167"/>
     </row>
     <row r="1062" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1062" s="64">
@@ -14682,9 +14684,9 @@
         <v>84</v>
       </c>
       <c r="B1078" s="87"/>
-      <c r="C1078" s="168"/>
-      <c r="D1078" s="169"/>
-      <c r="E1078" s="169"/>
+      <c r="C1078" s="166"/>
+      <c r="D1078" s="167"/>
+      <c r="E1078" s="167"/>
     </row>
     <row r="1079" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1079" s="64">
@@ -14835,18 +14837,18 @@
         <v>104</v>
       </c>
       <c r="B1095" s="40"/>
-      <c r="C1095" s="178"/>
-      <c r="D1095" s="179"/>
-      <c r="E1095" s="179"/>
+      <c r="C1095" s="176"/>
+      <c r="D1095" s="177"/>
+      <c r="E1095" s="177"/>
     </row>
     <row r="1096" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A1096" s="68" t="s">
         <v>85</v>
       </c>
       <c r="B1096" s="87"/>
-      <c r="C1096" s="168"/>
-      <c r="D1096" s="169"/>
-      <c r="E1096" s="169"/>
+      <c r="C1096" s="166"/>
+      <c r="D1096" s="167"/>
+      <c r="E1096" s="167"/>
     </row>
     <row r="1097" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1097" s="69">
@@ -14997,9 +14999,9 @@
         <v>86</v>
       </c>
       <c r="B1113" s="90"/>
-      <c r="C1113" s="170"/>
-      <c r="D1113" s="171"/>
-      <c r="E1113" s="171"/>
+      <c r="C1113" s="168"/>
+      <c r="D1113" s="169"/>
+      <c r="E1113" s="169"/>
     </row>
     <row r="1114" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1114" s="69">
@@ -15150,9 +15152,9 @@
         <v>87</v>
       </c>
       <c r="B1130" s="87"/>
-      <c r="C1130" s="168"/>
-      <c r="D1130" s="169"/>
-      <c r="E1130" s="169"/>
+      <c r="C1130" s="166"/>
+      <c r="D1130" s="167"/>
+      <c r="E1130" s="167"/>
     </row>
     <row r="1131" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1131" s="69">
@@ -15303,9 +15305,9 @@
         <v>88</v>
       </c>
       <c r="B1147" s="87"/>
-      <c r="C1147" s="168"/>
-      <c r="D1147" s="169"/>
-      <c r="E1147" s="169"/>
+      <c r="C1147" s="166"/>
+      <c r="D1147" s="167"/>
+      <c r="E1147" s="167"/>
     </row>
     <row r="1148" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1148" s="69">
@@ -15456,9 +15458,9 @@
         <v>89</v>
       </c>
       <c r="B1164" s="87"/>
-      <c r="C1164" s="168"/>
-      <c r="D1164" s="169"/>
-      <c r="E1164" s="169"/>
+      <c r="C1164" s="166"/>
+      <c r="D1164" s="167"/>
+      <c r="E1164" s="167"/>
     </row>
     <row r="1165" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1165" s="69">
@@ -15609,9 +15611,9 @@
         <v>90</v>
       </c>
       <c r="B1181" s="87"/>
-      <c r="C1181" s="168"/>
-      <c r="D1181" s="169"/>
-      <c r="E1181" s="169"/>
+      <c r="C1181" s="166"/>
+      <c r="D1181" s="167"/>
+      <c r="E1181" s="167"/>
     </row>
     <row r="1182" spans="1:5" hidden="1" outlineLevel="3">
       <c r="A1182" s="69">
@@ -15762,9 +15764,9 @@
         <v>91</v>
       </c>
       <c r="B1198" s="87"/>
-      <c r="C1198" s="168"/>
-      <c r="D1198" s="169"/>
-      <c r="E1198" s="169"/>
+      <c r="C1198" s="166"/>
+      <c r="D1198" s="167"/>
+      <c r="E1198" s="167"/>
     </row>
     <row r="1199" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1199" s="69">
@@ -15915,9 +15917,9 @@
         <v>92</v>
       </c>
       <c r="B1215" s="87"/>
-      <c r="C1215" s="168"/>
-      <c r="D1215" s="169"/>
-      <c r="E1215" s="169"/>
+      <c r="C1215" s="166"/>
+      <c r="D1215" s="167"/>
+      <c r="E1215" s="167"/>
     </row>
     <row r="1216" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1216" s="69">
@@ -16068,9 +16070,9 @@
         <v>93</v>
       </c>
       <c r="B1232" s="87"/>
-      <c r="C1232" s="168"/>
-      <c r="D1232" s="169"/>
-      <c r="E1232" s="169"/>
+      <c r="C1232" s="166"/>
+      <c r="D1232" s="167"/>
+      <c r="E1232" s="167"/>
     </row>
     <row r="1233" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1233" s="69">
@@ -16221,9 +16223,9 @@
         <v>94</v>
       </c>
       <c r="B1249" s="87"/>
-      <c r="C1249" s="168"/>
-      <c r="D1249" s="169"/>
-      <c r="E1249" s="169"/>
+      <c r="C1249" s="166"/>
+      <c r="D1249" s="167"/>
+      <c r="E1249" s="167"/>
     </row>
     <row r="1250" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1250" s="69">
@@ -16374,9 +16376,9 @@
         <v>99</v>
       </c>
       <c r="B1266" s="87"/>
-      <c r="C1266" s="168"/>
-      <c r="D1266" s="169"/>
-      <c r="E1266" s="169"/>
+      <c r="C1266" s="166"/>
+      <c r="D1266" s="167"/>
+      <c r="E1266" s="167"/>
     </row>
     <row r="1267" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1267" s="69">
@@ -16527,9 +16529,9 @@
         <v>100</v>
       </c>
       <c r="B1283" s="87"/>
-      <c r="C1283" s="168"/>
-      <c r="D1283" s="169"/>
-      <c r="E1283" s="169"/>
+      <c r="C1283" s="166"/>
+      <c r="D1283" s="167"/>
+      <c r="E1283" s="167"/>
     </row>
     <row r="1284" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1284" s="69">
@@ -16680,9 +16682,9 @@
         <v>101</v>
       </c>
       <c r="B1300" s="87"/>
-      <c r="C1300" s="168"/>
-      <c r="D1300" s="169"/>
-      <c r="E1300" s="169"/>
+      <c r="C1300" s="166"/>
+      <c r="D1300" s="167"/>
+      <c r="E1300" s="167"/>
     </row>
     <row r="1301" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1301" s="69">
@@ -16833,9 +16835,9 @@
         <v>81</v>
       </c>
       <c r="B1317" s="87"/>
-      <c r="C1317" s="168"/>
-      <c r="D1317" s="169"/>
-      <c r="E1317" s="169"/>
+      <c r="C1317" s="166"/>
+      <c r="D1317" s="167"/>
+      <c r="E1317" s="167"/>
     </row>
     <row r="1318" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1318" s="69">
@@ -16986,9 +16988,9 @@
         <v>102</v>
       </c>
       <c r="B1334" s="87"/>
-      <c r="C1334" s="168"/>
-      <c r="D1334" s="169"/>
-      <c r="E1334" s="169"/>
+      <c r="C1334" s="166"/>
+      <c r="D1334" s="167"/>
+      <c r="E1334" s="167"/>
     </row>
     <row r="1335" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1335" s="69">
@@ -17139,9 +17141,9 @@
         <v>98</v>
       </c>
       <c r="B1351" s="87"/>
-      <c r="C1351" s="168"/>
-      <c r="D1351" s="169"/>
-      <c r="E1351" s="169"/>
+      <c r="C1351" s="166"/>
+      <c r="D1351" s="167"/>
+      <c r="E1351" s="167"/>
     </row>
     <row r="1352" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1352" s="69">
@@ -17292,18 +17294,18 @@
         <v>103</v>
       </c>
       <c r="B1368" s="41"/>
-      <c r="C1368" s="180"/>
-      <c r="D1368" s="181"/>
-      <c r="E1368" s="181"/>
+      <c r="C1368" s="174"/>
+      <c r="D1368" s="175"/>
+      <c r="E1368" s="175"/>
     </row>
     <row r="1369" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A1369" s="73" t="s">
         <v>105</v>
       </c>
       <c r="B1369" s="87"/>
-      <c r="C1369" s="168"/>
-      <c r="D1369" s="169"/>
-      <c r="E1369" s="169"/>
+      <c r="C1369" s="166"/>
+      <c r="D1369" s="167"/>
+      <c r="E1369" s="167"/>
     </row>
     <row r="1370" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1370" s="74">
@@ -17454,9 +17456,9 @@
         <v>106</v>
       </c>
       <c r="B1386" s="90"/>
-      <c r="C1386" s="170"/>
-      <c r="D1386" s="171"/>
-      <c r="E1386" s="171"/>
+      <c r="C1386" s="168"/>
+      <c r="D1386" s="169"/>
+      <c r="E1386" s="169"/>
     </row>
     <row r="1387" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1387" s="74">
@@ -17607,9 +17609,9 @@
         <v>107</v>
       </c>
       <c r="B1403" s="87"/>
-      <c r="C1403" s="168"/>
-      <c r="D1403" s="169"/>
-      <c r="E1403" s="169"/>
+      <c r="C1403" s="166"/>
+      <c r="D1403" s="167"/>
+      <c r="E1403" s="167"/>
     </row>
     <row r="1404" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1404" s="74">
@@ -17760,9 +17762,9 @@
         <v>108</v>
       </c>
       <c r="B1420" s="87"/>
-      <c r="C1420" s="168"/>
-      <c r="D1420" s="169"/>
-      <c r="E1420" s="169"/>
+      <c r="C1420" s="166"/>
+      <c r="D1420" s="167"/>
+      <c r="E1420" s="167"/>
     </row>
     <row r="1421" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1421" s="74">
@@ -17913,9 +17915,9 @@
         <v>109</v>
       </c>
       <c r="B1437" s="87"/>
-      <c r="C1437" s="168"/>
-      <c r="D1437" s="169"/>
-      <c r="E1437" s="169"/>
+      <c r="C1437" s="166"/>
+      <c r="D1437" s="167"/>
+      <c r="E1437" s="167"/>
     </row>
     <row r="1438" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1438" s="74">
@@ -18066,9 +18068,9 @@
         <v>110</v>
       </c>
       <c r="B1454" s="87"/>
-      <c r="C1454" s="168"/>
-      <c r="D1454" s="169"/>
-      <c r="E1454" s="169"/>
+      <c r="C1454" s="166"/>
+      <c r="D1454" s="167"/>
+      <c r="E1454" s="167"/>
     </row>
     <row r="1455" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1455" s="74">
@@ -18219,9 +18221,9 @@
         <v>111</v>
       </c>
       <c r="B1471" s="87"/>
-      <c r="C1471" s="168"/>
-      <c r="D1471" s="169"/>
-      <c r="E1471" s="169"/>
+      <c r="C1471" s="166"/>
+      <c r="D1471" s="167"/>
+      <c r="E1471" s="167"/>
     </row>
     <row r="1472" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1472" s="74">
@@ -18372,9 +18374,9 @@
         <v>112</v>
       </c>
       <c r="B1488" s="87"/>
-      <c r="C1488" s="168"/>
-      <c r="D1488" s="169"/>
-      <c r="E1488" s="169"/>
+      <c r="C1488" s="166"/>
+      <c r="D1488" s="167"/>
+      <c r="E1488" s="167"/>
     </row>
     <row r="1489" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1489" s="74">
@@ -18525,9 +18527,9 @@
         <v>113</v>
       </c>
       <c r="B1505" s="87"/>
-      <c r="C1505" s="168"/>
-      <c r="D1505" s="169"/>
-      <c r="E1505" s="169"/>
+      <c r="C1505" s="166"/>
+      <c r="D1505" s="167"/>
+      <c r="E1505" s="167"/>
     </row>
     <row r="1506" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1506" s="74">
@@ -18678,9 +18680,9 @@
         <v>114</v>
       </c>
       <c r="B1522" s="87"/>
-      <c r="C1522" s="168"/>
-      <c r="D1522" s="169"/>
-      <c r="E1522" s="169"/>
+      <c r="C1522" s="166"/>
+      <c r="D1522" s="167"/>
+      <c r="E1522" s="167"/>
     </row>
     <row r="1523" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1523" s="74">
@@ -18831,9 +18833,9 @@
         <v>95</v>
       </c>
       <c r="B1539" s="87"/>
-      <c r="C1539" s="168"/>
-      <c r="D1539" s="169"/>
-      <c r="E1539" s="169"/>
+      <c r="C1539" s="166"/>
+      <c r="D1539" s="167"/>
+      <c r="E1539" s="167"/>
     </row>
     <row r="1540" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1540" s="74">
@@ -18984,9 +18986,9 @@
         <v>115</v>
       </c>
       <c r="B1556" s="87"/>
-      <c r="C1556" s="168"/>
-      <c r="D1556" s="169"/>
-      <c r="E1556" s="169"/>
+      <c r="C1556" s="166"/>
+      <c r="D1556" s="167"/>
+      <c r="E1556" s="167"/>
     </row>
     <row r="1557" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1557" s="74">
@@ -19137,9 +19139,9 @@
         <v>116</v>
       </c>
       <c r="B1573" s="87"/>
-      <c r="C1573" s="168"/>
-      <c r="D1573" s="169"/>
-      <c r="E1573" s="169"/>
+      <c r="C1573" s="166"/>
+      <c r="D1573" s="167"/>
+      <c r="E1573" s="167"/>
     </row>
     <row r="1574" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1574" s="74">
@@ -19290,9 +19292,9 @@
         <v>117</v>
       </c>
       <c r="B1590" s="87"/>
-      <c r="C1590" s="168"/>
-      <c r="D1590" s="169"/>
-      <c r="E1590" s="169"/>
+      <c r="C1590" s="166"/>
+      <c r="D1590" s="167"/>
+      <c r="E1590" s="167"/>
     </row>
     <row r="1591" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1591" s="74">
@@ -19443,9 +19445,9 @@
         <v>118</v>
       </c>
       <c r="B1607" s="87"/>
-      <c r="C1607" s="168"/>
-      <c r="D1607" s="169"/>
-      <c r="E1607" s="169"/>
+      <c r="C1607" s="166"/>
+      <c r="D1607" s="167"/>
+      <c r="E1607" s="167"/>
     </row>
     <row r="1608" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1608" s="74">
@@ -19596,9 +19598,9 @@
         <v>119</v>
       </c>
       <c r="B1624" s="87"/>
-      <c r="C1624" s="168"/>
-      <c r="D1624" s="169"/>
-      <c r="E1624" s="169"/>
+      <c r="C1624" s="166"/>
+      <c r="D1624" s="167"/>
+      <c r="E1624" s="167"/>
     </row>
     <row r="1625" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1625" s="74">
@@ -19749,18 +19751,18 @@
         <v>120</v>
       </c>
       <c r="B1641" s="42"/>
-      <c r="C1641" s="182"/>
-      <c r="D1641" s="183"/>
-      <c r="E1641" s="183"/>
+      <c r="C1641" s="172"/>
+      <c r="D1641" s="173"/>
+      <c r="E1641" s="173"/>
     </row>
     <row r="1642" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A1642" s="78" t="s">
         <v>121</v>
       </c>
       <c r="B1642" s="87"/>
-      <c r="C1642" s="168"/>
-      <c r="D1642" s="169"/>
-      <c r="E1642" s="169"/>
+      <c r="C1642" s="166"/>
+      <c r="D1642" s="167"/>
+      <c r="E1642" s="167"/>
     </row>
     <row r="1643" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1643" s="79">
@@ -19911,9 +19913,9 @@
         <v>122</v>
       </c>
       <c r="B1659" s="90"/>
-      <c r="C1659" s="170"/>
-      <c r="D1659" s="171"/>
-      <c r="E1659" s="171"/>
+      <c r="C1659" s="168"/>
+      <c r="D1659" s="169"/>
+      <c r="E1659" s="169"/>
     </row>
     <row r="1660" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1660" s="79">
@@ -20064,9 +20066,9 @@
         <v>123</v>
       </c>
       <c r="B1676" s="87"/>
-      <c r="C1676" s="168"/>
-      <c r="D1676" s="169"/>
-      <c r="E1676" s="169"/>
+      <c r="C1676" s="166"/>
+      <c r="D1676" s="167"/>
+      <c r="E1676" s="167"/>
     </row>
     <row r="1677" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1677" s="79">
@@ -20217,9 +20219,9 @@
         <v>124</v>
       </c>
       <c r="B1693" s="87"/>
-      <c r="C1693" s="168"/>
-      <c r="D1693" s="169"/>
-      <c r="E1693" s="169"/>
+      <c r="C1693" s="166"/>
+      <c r="D1693" s="167"/>
+      <c r="E1693" s="167"/>
     </row>
     <row r="1694" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1694" s="79">
@@ -20370,9 +20372,9 @@
         <v>125</v>
       </c>
       <c r="B1710" s="87"/>
-      <c r="C1710" s="168"/>
-      <c r="D1710" s="169"/>
-      <c r="E1710" s="169"/>
+      <c r="C1710" s="166"/>
+      <c r="D1710" s="167"/>
+      <c r="E1710" s="167"/>
     </row>
     <row r="1711" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1711" s="79">
@@ -20523,9 +20525,9 @@
         <v>126</v>
       </c>
       <c r="B1727" s="87"/>
-      <c r="C1727" s="168"/>
-      <c r="D1727" s="169"/>
-      <c r="E1727" s="169"/>
+      <c r="C1727" s="166"/>
+      <c r="D1727" s="167"/>
+      <c r="E1727" s="167"/>
     </row>
     <row r="1728" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1728" s="79">
@@ -20676,9 +20678,9 @@
         <v>127</v>
       </c>
       <c r="B1744" s="87"/>
-      <c r="C1744" s="168"/>
-      <c r="D1744" s="169"/>
-      <c r="E1744" s="169"/>
+      <c r="C1744" s="166"/>
+      <c r="D1744" s="167"/>
+      <c r="E1744" s="167"/>
     </row>
     <row r="1745" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1745" s="79">
@@ -20829,9 +20831,9 @@
         <v>128</v>
       </c>
       <c r="B1761" s="87"/>
-      <c r="C1761" s="168"/>
-      <c r="D1761" s="169"/>
-      <c r="E1761" s="169"/>
+      <c r="C1761" s="166"/>
+      <c r="D1761" s="167"/>
+      <c r="E1761" s="167"/>
     </row>
     <row r="1762" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1762" s="79">
@@ -20982,9 +20984,9 @@
         <v>129</v>
       </c>
       <c r="B1778" s="87"/>
-      <c r="C1778" s="168"/>
-      <c r="D1778" s="169"/>
-      <c r="E1778" s="169"/>
+      <c r="C1778" s="166"/>
+      <c r="D1778" s="167"/>
+      <c r="E1778" s="167"/>
     </row>
     <row r="1779" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1779" s="79">
@@ -21135,9 +21137,9 @@
         <v>130</v>
       </c>
       <c r="B1795" s="87"/>
-      <c r="C1795" s="168"/>
-      <c r="D1795" s="169"/>
-      <c r="E1795" s="169"/>
+      <c r="C1795" s="166"/>
+      <c r="D1795" s="167"/>
+      <c r="E1795" s="167"/>
     </row>
     <row r="1796" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1796" s="79">
@@ -21288,9 +21290,9 @@
         <v>131</v>
       </c>
       <c r="B1812" s="87"/>
-      <c r="C1812" s="168"/>
-      <c r="D1812" s="169"/>
-      <c r="E1812" s="169"/>
+      <c r="C1812" s="166"/>
+      <c r="D1812" s="167"/>
+      <c r="E1812" s="167"/>
     </row>
     <row r="1813" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1813" s="79">
@@ -21441,9 +21443,9 @@
         <v>96</v>
       </c>
       <c r="B1829" s="87"/>
-      <c r="C1829" s="168"/>
-      <c r="D1829" s="169"/>
-      <c r="E1829" s="169"/>
+      <c r="C1829" s="166"/>
+      <c r="D1829" s="167"/>
+      <c r="E1829" s="167"/>
     </row>
     <row r="1830" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1830" s="79">
@@ -21594,9 +21596,9 @@
         <v>132</v>
       </c>
       <c r="B1846" s="87"/>
-      <c r="C1846" s="168"/>
-      <c r="D1846" s="169"/>
-      <c r="E1846" s="169"/>
+      <c r="C1846" s="166"/>
+      <c r="D1846" s="167"/>
+      <c r="E1846" s="167"/>
     </row>
     <row r="1847" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1847" s="79">
@@ -21747,9 +21749,9 @@
         <v>133</v>
       </c>
       <c r="B1863" s="87"/>
-      <c r="C1863" s="168"/>
-      <c r="D1863" s="169"/>
-      <c r="E1863" s="169"/>
+      <c r="C1863" s="166"/>
+      <c r="D1863" s="167"/>
+      <c r="E1863" s="167"/>
     </row>
     <row r="1864" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1864" s="79">
@@ -21900,9 +21902,9 @@
         <v>134</v>
       </c>
       <c r="B1880" s="87"/>
-      <c r="C1880" s="168"/>
-      <c r="D1880" s="169"/>
-      <c r="E1880" s="169"/>
+      <c r="C1880" s="166"/>
+      <c r="D1880" s="167"/>
+      <c r="E1880" s="167"/>
     </row>
     <row r="1881" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1881" s="79">
@@ -22053,9 +22055,9 @@
         <v>135</v>
       </c>
       <c r="B1897" s="87"/>
-      <c r="C1897" s="168"/>
-      <c r="D1897" s="169"/>
-      <c r="E1897" s="169"/>
+      <c r="C1897" s="166"/>
+      <c r="D1897" s="167"/>
+      <c r="E1897" s="167"/>
     </row>
     <row r="1898" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1898" s="79">
@@ -22206,18 +22208,18 @@
         <v>136</v>
       </c>
       <c r="B1914" s="43"/>
-      <c r="C1914" s="184"/>
-      <c r="D1914" s="185"/>
-      <c r="E1914" s="185"/>
+      <c r="C1914" s="170"/>
+      <c r="D1914" s="171"/>
+      <c r="E1914" s="171"/>
     </row>
     <row r="1915" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A1915" s="83" t="s">
         <v>137</v>
       </c>
       <c r="B1915" s="87"/>
-      <c r="C1915" s="168"/>
-      <c r="D1915" s="169"/>
-      <c r="E1915" s="169"/>
+      <c r="C1915" s="166"/>
+      <c r="D1915" s="167"/>
+      <c r="E1915" s="167"/>
     </row>
     <row r="1916" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1916" s="84">
@@ -22368,9 +22370,9 @@
         <v>138</v>
       </c>
       <c r="B1932" s="90"/>
-      <c r="C1932" s="170"/>
-      <c r="D1932" s="171"/>
-      <c r="E1932" s="171"/>
+      <c r="C1932" s="168"/>
+      <c r="D1932" s="169"/>
+      <c r="E1932" s="169"/>
     </row>
     <row r="1933" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1933" s="84">
@@ -22521,9 +22523,9 @@
         <v>139</v>
       </c>
       <c r="B1949" s="87"/>
-      <c r="C1949" s="168"/>
-      <c r="D1949" s="169"/>
-      <c r="E1949" s="169"/>
+      <c r="C1949" s="166"/>
+      <c r="D1949" s="167"/>
+      <c r="E1949" s="167"/>
     </row>
     <row r="1950" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1950" s="84">
@@ -22674,9 +22676,9 @@
         <v>140</v>
       </c>
       <c r="B1966" s="87"/>
-      <c r="C1966" s="168"/>
-      <c r="D1966" s="169"/>
-      <c r="E1966" s="169"/>
+      <c r="C1966" s="166"/>
+      <c r="D1966" s="167"/>
+      <c r="E1966" s="167"/>
     </row>
     <row r="1967" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1967" s="84">
@@ -22827,9 +22829,9 @@
         <v>141</v>
       </c>
       <c r="B1983" s="87"/>
-      <c r="C1983" s="168"/>
-      <c r="D1983" s="169"/>
-      <c r="E1983" s="169"/>
+      <c r="C1983" s="166"/>
+      <c r="D1983" s="167"/>
+      <c r="E1983" s="167"/>
     </row>
     <row r="1984" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1984" s="84">
@@ -22980,9 +22982,9 @@
         <v>142</v>
       </c>
       <c r="B2000" s="87"/>
-      <c r="C2000" s="168"/>
-      <c r="D2000" s="169"/>
-      <c r="E2000" s="169"/>
+      <c r="C2000" s="166"/>
+      <c r="D2000" s="167"/>
+      <c r="E2000" s="167"/>
     </row>
     <row r="2001" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2001" s="84">
@@ -23133,9 +23135,9 @@
         <v>143</v>
       </c>
       <c r="B2017" s="87"/>
-      <c r="C2017" s="168"/>
-      <c r="D2017" s="169"/>
-      <c r="E2017" s="169"/>
+      <c r="C2017" s="166"/>
+      <c r="D2017" s="167"/>
+      <c r="E2017" s="167"/>
     </row>
     <row r="2018" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2018" s="84">
@@ -23286,9 +23288,9 @@
         <v>144</v>
       </c>
       <c r="B2034" s="87"/>
-      <c r="C2034" s="168"/>
-      <c r="D2034" s="169"/>
-      <c r="E2034" s="169"/>
+      <c r="C2034" s="166"/>
+      <c r="D2034" s="167"/>
+      <c r="E2034" s="167"/>
     </row>
     <row r="2035" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2035" s="84">
@@ -23439,9 +23441,9 @@
         <v>145</v>
       </c>
       <c r="B2051" s="87"/>
-      <c r="C2051" s="168"/>
-      <c r="D2051" s="169"/>
-      <c r="E2051" s="169"/>
+      <c r="C2051" s="166"/>
+      <c r="D2051" s="167"/>
+      <c r="E2051" s="167"/>
     </row>
     <row r="2052" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2052" s="84">
@@ -23592,9 +23594,9 @@
         <v>146</v>
       </c>
       <c r="B2068" s="87"/>
-      <c r="C2068" s="168"/>
-      <c r="D2068" s="169"/>
-      <c r="E2068" s="169"/>
+      <c r="C2068" s="166"/>
+      <c r="D2068" s="167"/>
+      <c r="E2068" s="167"/>
     </row>
     <row r="2069" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2069" s="84">
@@ -23745,9 +23747,9 @@
         <v>147</v>
       </c>
       <c r="B2085" s="87"/>
-      <c r="C2085" s="168"/>
-      <c r="D2085" s="169"/>
-      <c r="E2085" s="169"/>
+      <c r="C2085" s="166"/>
+      <c r="D2085" s="167"/>
+      <c r="E2085" s="167"/>
     </row>
     <row r="2086" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2086" s="84">
@@ -23898,9 +23900,9 @@
         <v>148</v>
       </c>
       <c r="B2102" s="87"/>
-      <c r="C2102" s="168"/>
-      <c r="D2102" s="169"/>
-      <c r="E2102" s="169"/>
+      <c r="C2102" s="166"/>
+      <c r="D2102" s="167"/>
+      <c r="E2102" s="167"/>
     </row>
     <row r="2103" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2103" s="84">
@@ -24051,9 +24053,9 @@
         <v>97</v>
       </c>
       <c r="B2119" s="87"/>
-      <c r="C2119" s="168"/>
-      <c r="D2119" s="169"/>
-      <c r="E2119" s="169"/>
+      <c r="C2119" s="166"/>
+      <c r="D2119" s="167"/>
+      <c r="E2119" s="167"/>
     </row>
     <row r="2120" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2120" s="84">
@@ -24204,9 +24206,9 @@
         <v>149</v>
       </c>
       <c r="B2136" s="87"/>
-      <c r="C2136" s="168"/>
-      <c r="D2136" s="169"/>
-      <c r="E2136" s="169"/>
+      <c r="C2136" s="166"/>
+      <c r="D2136" s="167"/>
+      <c r="E2136" s="167"/>
     </row>
     <row r="2137" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2137" s="84">
@@ -24357,9 +24359,9 @@
         <v>150</v>
       </c>
       <c r="B2153" s="87"/>
-      <c r="C2153" s="168"/>
-      <c r="D2153" s="169"/>
-      <c r="E2153" s="169"/>
+      <c r="C2153" s="166"/>
+      <c r="D2153" s="167"/>
+      <c r="E2153" s="167"/>
     </row>
     <row r="2154" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2154" s="84">
@@ -24510,9 +24512,9 @@
         <v>151</v>
       </c>
       <c r="B2170" s="87"/>
-      <c r="C2170" s="168"/>
-      <c r="D2170" s="169"/>
-      <c r="E2170" s="169"/>
+      <c r="C2170" s="166"/>
+      <c r="D2170" s="167"/>
+      <c r="E2170" s="167"/>
     </row>
     <row r="2171" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2171" s="84">
@@ -24660,15 +24662,122 @@
     </row>
   </sheetData>
   <mergeCells count="137">
-    <mergeCell ref="C2034:E2034"/>
-    <mergeCell ref="C2051:E2051"/>
-    <mergeCell ref="C2068:E2068"/>
-    <mergeCell ref="C2085:E2085"/>
-    <mergeCell ref="C2170:E2170"/>
-    <mergeCell ref="C2102:E2102"/>
-    <mergeCell ref="C2119:E2119"/>
-    <mergeCell ref="C2136:E2136"/>
-    <mergeCell ref="C2153:E2153"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="C89:E89"/>
+    <mergeCell ref="C21:E21"/>
+    <mergeCell ref="C38:E38"/>
+    <mergeCell ref="C55:E55"/>
+    <mergeCell ref="C72:E72"/>
+    <mergeCell ref="C208:E208"/>
+    <mergeCell ref="C225:E225"/>
+    <mergeCell ref="C242:E242"/>
+    <mergeCell ref="C259:E259"/>
+    <mergeCell ref="C276:E276"/>
+    <mergeCell ref="C277:E277"/>
+    <mergeCell ref="C106:E106"/>
+    <mergeCell ref="C123:E123"/>
+    <mergeCell ref="C140:E140"/>
+    <mergeCell ref="C157:E157"/>
+    <mergeCell ref="C174:E174"/>
+    <mergeCell ref="C191:E191"/>
+    <mergeCell ref="C396:E396"/>
+    <mergeCell ref="C413:E413"/>
+    <mergeCell ref="C430:E430"/>
+    <mergeCell ref="C447:E447"/>
+    <mergeCell ref="C464:E464"/>
+    <mergeCell ref="C481:E481"/>
+    <mergeCell ref="C294:E294"/>
+    <mergeCell ref="C311:E311"/>
+    <mergeCell ref="C328:E328"/>
+    <mergeCell ref="C345:E345"/>
+    <mergeCell ref="C362:E362"/>
+    <mergeCell ref="C379:E379"/>
+    <mergeCell ref="C584:E584"/>
+    <mergeCell ref="C601:E601"/>
+    <mergeCell ref="C618:E618"/>
+    <mergeCell ref="C635:E635"/>
+    <mergeCell ref="C652:E652"/>
+    <mergeCell ref="C669:E669"/>
+    <mergeCell ref="C498:E498"/>
+    <mergeCell ref="C515:E515"/>
+    <mergeCell ref="C532:E532"/>
+    <mergeCell ref="C549:E549"/>
+    <mergeCell ref="C550:E550"/>
+    <mergeCell ref="C567:E567"/>
+    <mergeCell ref="C788:E788"/>
+    <mergeCell ref="C805:E805"/>
+    <mergeCell ref="C822:E822"/>
+    <mergeCell ref="C823:E823"/>
+    <mergeCell ref="C840:E840"/>
+    <mergeCell ref="C857:E857"/>
+    <mergeCell ref="C686:E686"/>
+    <mergeCell ref="C703:E703"/>
+    <mergeCell ref="C720:E720"/>
+    <mergeCell ref="C737:E737"/>
+    <mergeCell ref="C754:E754"/>
+    <mergeCell ref="C771:E771"/>
+    <mergeCell ref="C976:E976"/>
+    <mergeCell ref="C993:E993"/>
+    <mergeCell ref="C1010:E1010"/>
+    <mergeCell ref="C1027:E1027"/>
+    <mergeCell ref="C1044:E1044"/>
+    <mergeCell ref="C1061:E1061"/>
+    <mergeCell ref="C874:E874"/>
+    <mergeCell ref="C891:E891"/>
+    <mergeCell ref="C908:E908"/>
+    <mergeCell ref="C925:E925"/>
+    <mergeCell ref="C942:E942"/>
+    <mergeCell ref="C959:E959"/>
+    <mergeCell ref="C1164:E1164"/>
+    <mergeCell ref="C1181:E1181"/>
+    <mergeCell ref="C1198:E1198"/>
+    <mergeCell ref="C1215:E1215"/>
+    <mergeCell ref="C1232:E1232"/>
+    <mergeCell ref="C1249:E1249"/>
+    <mergeCell ref="C1078:E1078"/>
+    <mergeCell ref="C1095:E1095"/>
+    <mergeCell ref="C1096:E1096"/>
+    <mergeCell ref="C1113:E1113"/>
+    <mergeCell ref="C1130:E1130"/>
+    <mergeCell ref="C1147:E1147"/>
+    <mergeCell ref="C1368:E1368"/>
+    <mergeCell ref="C1369:E1369"/>
+    <mergeCell ref="C1386:E1386"/>
+    <mergeCell ref="C1403:E1403"/>
+    <mergeCell ref="C1420:E1420"/>
+    <mergeCell ref="C1437:E1437"/>
+    <mergeCell ref="C1266:E1266"/>
+    <mergeCell ref="C1283:E1283"/>
+    <mergeCell ref="C1300:E1300"/>
+    <mergeCell ref="C1317:E1317"/>
+    <mergeCell ref="C1334:E1334"/>
+    <mergeCell ref="C1351:E1351"/>
+    <mergeCell ref="C1556:E1556"/>
+    <mergeCell ref="C1573:E1573"/>
+    <mergeCell ref="C1590:E1590"/>
+    <mergeCell ref="C1607:E1607"/>
+    <mergeCell ref="C1624:E1624"/>
+    <mergeCell ref="C1641:E1641"/>
+    <mergeCell ref="C1454:E1454"/>
+    <mergeCell ref="C1471:E1471"/>
+    <mergeCell ref="C1488:E1488"/>
+    <mergeCell ref="C1505:E1505"/>
+    <mergeCell ref="C1522:E1522"/>
+    <mergeCell ref="C1539:E1539"/>
+    <mergeCell ref="C1744:E1744"/>
+    <mergeCell ref="C1761:E1761"/>
+    <mergeCell ref="C1778:E1778"/>
+    <mergeCell ref="C1795:E1795"/>
+    <mergeCell ref="C1812:E1812"/>
+    <mergeCell ref="C1829:E1829"/>
+    <mergeCell ref="C1642:E1642"/>
+    <mergeCell ref="C1659:E1659"/>
+    <mergeCell ref="C1676:E1676"/>
+    <mergeCell ref="C1693:E1693"/>
+    <mergeCell ref="C1710:E1710"/>
+    <mergeCell ref="C1727:E1727"/>
     <mergeCell ref="C1932:E1932"/>
     <mergeCell ref="C1949:E1949"/>
     <mergeCell ref="C1966:E1966"/>
@@ -24681,122 +24790,15 @@
     <mergeCell ref="C1897:E1897"/>
     <mergeCell ref="C1914:E1914"/>
     <mergeCell ref="C1915:E1915"/>
-    <mergeCell ref="C1744:E1744"/>
-    <mergeCell ref="C1761:E1761"/>
-    <mergeCell ref="C1778:E1778"/>
-    <mergeCell ref="C1795:E1795"/>
-    <mergeCell ref="C1812:E1812"/>
-    <mergeCell ref="C1829:E1829"/>
-    <mergeCell ref="C1642:E1642"/>
-    <mergeCell ref="C1659:E1659"/>
-    <mergeCell ref="C1676:E1676"/>
-    <mergeCell ref="C1693:E1693"/>
-    <mergeCell ref="C1710:E1710"/>
-    <mergeCell ref="C1727:E1727"/>
-    <mergeCell ref="C1556:E1556"/>
-    <mergeCell ref="C1573:E1573"/>
-    <mergeCell ref="C1590:E1590"/>
-    <mergeCell ref="C1607:E1607"/>
-    <mergeCell ref="C1624:E1624"/>
-    <mergeCell ref="C1641:E1641"/>
-    <mergeCell ref="C1454:E1454"/>
-    <mergeCell ref="C1471:E1471"/>
-    <mergeCell ref="C1488:E1488"/>
-    <mergeCell ref="C1505:E1505"/>
-    <mergeCell ref="C1522:E1522"/>
-    <mergeCell ref="C1539:E1539"/>
-    <mergeCell ref="C1368:E1368"/>
-    <mergeCell ref="C1369:E1369"/>
-    <mergeCell ref="C1386:E1386"/>
-    <mergeCell ref="C1403:E1403"/>
-    <mergeCell ref="C1420:E1420"/>
-    <mergeCell ref="C1437:E1437"/>
-    <mergeCell ref="C1266:E1266"/>
-    <mergeCell ref="C1283:E1283"/>
-    <mergeCell ref="C1300:E1300"/>
-    <mergeCell ref="C1317:E1317"/>
-    <mergeCell ref="C1334:E1334"/>
-    <mergeCell ref="C1351:E1351"/>
-    <mergeCell ref="C1164:E1164"/>
-    <mergeCell ref="C1181:E1181"/>
-    <mergeCell ref="C1198:E1198"/>
-    <mergeCell ref="C1215:E1215"/>
-    <mergeCell ref="C1232:E1232"/>
-    <mergeCell ref="C1249:E1249"/>
-    <mergeCell ref="C1078:E1078"/>
-    <mergeCell ref="C1095:E1095"/>
-    <mergeCell ref="C1096:E1096"/>
-    <mergeCell ref="C1113:E1113"/>
-    <mergeCell ref="C1130:E1130"/>
-    <mergeCell ref="C1147:E1147"/>
-    <mergeCell ref="C976:E976"/>
-    <mergeCell ref="C993:E993"/>
-    <mergeCell ref="C1010:E1010"/>
-    <mergeCell ref="C1027:E1027"/>
-    <mergeCell ref="C1044:E1044"/>
-    <mergeCell ref="C1061:E1061"/>
-    <mergeCell ref="C874:E874"/>
-    <mergeCell ref="C891:E891"/>
-    <mergeCell ref="C908:E908"/>
-    <mergeCell ref="C925:E925"/>
-    <mergeCell ref="C942:E942"/>
-    <mergeCell ref="C959:E959"/>
-    <mergeCell ref="C788:E788"/>
-    <mergeCell ref="C805:E805"/>
-    <mergeCell ref="C822:E822"/>
-    <mergeCell ref="C823:E823"/>
-    <mergeCell ref="C840:E840"/>
-    <mergeCell ref="C857:E857"/>
-    <mergeCell ref="C686:E686"/>
-    <mergeCell ref="C703:E703"/>
-    <mergeCell ref="C720:E720"/>
-    <mergeCell ref="C737:E737"/>
-    <mergeCell ref="C754:E754"/>
-    <mergeCell ref="C771:E771"/>
-    <mergeCell ref="C584:E584"/>
-    <mergeCell ref="C601:E601"/>
-    <mergeCell ref="C618:E618"/>
-    <mergeCell ref="C635:E635"/>
-    <mergeCell ref="C652:E652"/>
-    <mergeCell ref="C669:E669"/>
-    <mergeCell ref="C498:E498"/>
-    <mergeCell ref="C515:E515"/>
-    <mergeCell ref="C532:E532"/>
-    <mergeCell ref="C549:E549"/>
-    <mergeCell ref="C550:E550"/>
-    <mergeCell ref="C567:E567"/>
-    <mergeCell ref="C396:E396"/>
-    <mergeCell ref="C413:E413"/>
-    <mergeCell ref="C430:E430"/>
-    <mergeCell ref="C447:E447"/>
-    <mergeCell ref="C464:E464"/>
-    <mergeCell ref="C481:E481"/>
-    <mergeCell ref="C294:E294"/>
-    <mergeCell ref="C311:E311"/>
-    <mergeCell ref="C328:E328"/>
-    <mergeCell ref="C345:E345"/>
-    <mergeCell ref="C362:E362"/>
-    <mergeCell ref="C379:E379"/>
-    <mergeCell ref="C225:E225"/>
-    <mergeCell ref="C242:E242"/>
-    <mergeCell ref="C259:E259"/>
-    <mergeCell ref="C276:E276"/>
-    <mergeCell ref="C277:E277"/>
-    <mergeCell ref="C106:E106"/>
-    <mergeCell ref="C123:E123"/>
-    <mergeCell ref="C140:E140"/>
-    <mergeCell ref="C157:E157"/>
-    <mergeCell ref="C174:E174"/>
-    <mergeCell ref="C191:E191"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="C89:E89"/>
-    <mergeCell ref="C21:E21"/>
-    <mergeCell ref="C38:E38"/>
-    <mergeCell ref="C55:E55"/>
-    <mergeCell ref="C72:E72"/>
-    <mergeCell ref="C208:E208"/>
+    <mergeCell ref="C2034:E2034"/>
+    <mergeCell ref="C2051:E2051"/>
+    <mergeCell ref="C2068:E2068"/>
+    <mergeCell ref="C2085:E2085"/>
+    <mergeCell ref="C2170:E2170"/>
+    <mergeCell ref="C2102:E2102"/>
+    <mergeCell ref="C2119:E2119"/>
+    <mergeCell ref="C2136:E2136"/>
+    <mergeCell ref="C2153:E2153"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -24823,51 +24825,51 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="24" thickBot="1">
-      <c r="A1" s="192" t="s">
+      <c r="A1" s="193" t="s">
         <v>156</v>
       </c>
-      <c r="B1" s="192"/>
-      <c r="C1" s="192"/>
-      <c r="D1" s="192"/>
-      <c r="E1" s="192"/>
-      <c r="F1" s="192"/>
-      <c r="G1" s="192"/>
-      <c r="H1" s="192"/>
-      <c r="I1" s="192"/>
-      <c r="J1" s="192"/>
-      <c r="K1" s="192"/>
-      <c r="L1" s="192"/>
+      <c r="B1" s="193"/>
+      <c r="C1" s="193"/>
+      <c r="D1" s="193"/>
+      <c r="E1" s="193"/>
+      <c r="F1" s="193"/>
+      <c r="G1" s="193"/>
+      <c r="H1" s="193"/>
+      <c r="I1" s="193"/>
+      <c r="J1" s="193"/>
+      <c r="K1" s="193"/>
+      <c r="L1" s="193"/>
     </row>
     <row r="2" spans="1:12" ht="18.75" thickBot="1">
-      <c r="A2" s="189" t="s">
+      <c r="A2" s="190" t="s">
         <v>157</v>
       </c>
-      <c r="B2" s="190"/>
-      <c r="C2" s="190"/>
-      <c r="D2" s="190"/>
-      <c r="E2" s="190"/>
-      <c r="F2" s="190"/>
-      <c r="G2" s="190"/>
-      <c r="H2" s="190"/>
-      <c r="I2" s="190"/>
-      <c r="J2" s="190"/>
-      <c r="K2" s="190"/>
-      <c r="L2" s="191"/>
+      <c r="B2" s="191"/>
+      <c r="C2" s="191"/>
+      <c r="D2" s="191"/>
+      <c r="E2" s="191"/>
+      <c r="F2" s="191"/>
+      <c r="G2" s="191"/>
+      <c r="H2" s="191"/>
+      <c r="I2" s="191"/>
+      <c r="J2" s="191"/>
+      <c r="K2" s="191"/>
+      <c r="L2" s="192"/>
     </row>
     <row r="3" spans="1:12" s="31" customFormat="1" ht="16.5" customHeight="1" thickBot="1">
-      <c r="A3" s="186" t="s">
+      <c r="A3" s="187" t="s">
         <v>158</v>
       </c>
-      <c r="B3" s="187"/>
-      <c r="C3" s="187"/>
-      <c r="D3" s="187"/>
-      <c r="E3" s="187"/>
-      <c r="F3" s="187"/>
-      <c r="G3" s="187"/>
-      <c r="H3" s="187"/>
-      <c r="I3" s="187"/>
-      <c r="J3" s="187"/>
-      <c r="K3" s="188"/>
+      <c r="B3" s="188"/>
+      <c r="C3" s="188"/>
+      <c r="D3" s="188"/>
+      <c r="E3" s="188"/>
+      <c r="F3" s="188"/>
+      <c r="G3" s="188"/>
+      <c r="H3" s="188"/>
+      <c r="I3" s="188"/>
+      <c r="J3" s="188"/>
+      <c r="K3" s="189"/>
     </row>
     <row r="4" spans="1:12" s="27" customFormat="1">
       <c r="A4" s="28" t="s">
@@ -25084,19 +25086,19 @@
       <c r="K19" s="2"/>
     </row>
     <row r="20" spans="1:11" ht="18" customHeight="1" thickBot="1">
-      <c r="A20" s="186" t="s">
+      <c r="A20" s="187" t="s">
         <v>166</v>
       </c>
-      <c r="B20" s="187"/>
-      <c r="C20" s="187"/>
-      <c r="D20" s="187"/>
-      <c r="E20" s="187"/>
-      <c r="F20" s="187"/>
-      <c r="G20" s="187"/>
-      <c r="H20" s="187"/>
-      <c r="I20" s="187"/>
-      <c r="J20" s="187"/>
-      <c r="K20" s="188"/>
+      <c r="B20" s="188"/>
+      <c r="C20" s="188"/>
+      <c r="D20" s="188"/>
+      <c r="E20" s="188"/>
+      <c r="F20" s="188"/>
+      <c r="G20" s="188"/>
+      <c r="H20" s="188"/>
+      <c r="I20" s="188"/>
+      <c r="J20" s="188"/>
+      <c r="K20" s="189"/>
     </row>
     <row r="21" spans="1:11">
       <c r="A21" s="28" t="s">
@@ -25313,19 +25315,19 @@
       <c r="K36" s="2"/>
     </row>
     <row r="37" spans="1:11" ht="18" customHeight="1" thickBot="1">
-      <c r="A37" s="186" t="s">
+      <c r="A37" s="187" t="s">
         <v>167</v>
       </c>
-      <c r="B37" s="187"/>
-      <c r="C37" s="187"/>
-      <c r="D37" s="187"/>
-      <c r="E37" s="187"/>
-      <c r="F37" s="187"/>
-      <c r="G37" s="187"/>
-      <c r="H37" s="187"/>
-      <c r="I37" s="187"/>
-      <c r="J37" s="187"/>
-      <c r="K37" s="188"/>
+      <c r="B37" s="188"/>
+      <c r="C37" s="188"/>
+      <c r="D37" s="188"/>
+      <c r="E37" s="188"/>
+      <c r="F37" s="188"/>
+      <c r="G37" s="188"/>
+      <c r="H37" s="188"/>
+      <c r="I37" s="188"/>
+      <c r="J37" s="188"/>
+      <c r="K37" s="189"/>
     </row>
     <row r="38" spans="1:11">
       <c r="A38" s="28" t="s">
@@ -25583,28 +25585,28 @@
       </c>
     </row>
     <row r="3" spans="1:1">
-      <c r="A3" s="193"/>
+      <c r="A3" s="194"/>
     </row>
     <row r="4" spans="1:1">
-      <c r="A4" s="194"/>
+      <c r="A4" s="195"/>
     </row>
     <row r="5" spans="1:1">
-      <c r="A5" s="194"/>
+      <c r="A5" s="195"/>
     </row>
     <row r="6" spans="1:1">
-      <c r="A6" s="194"/>
+      <c r="A6" s="195"/>
     </row>
     <row r="7" spans="1:1">
-      <c r="A7" s="194"/>
+      <c r="A7" s="195"/>
     </row>
     <row r="8" spans="1:1">
-      <c r="A8" s="194"/>
+      <c r="A8" s="195"/>
     </row>
     <row r="9" spans="1:1">
-      <c r="A9" s="194"/>
+      <c r="A9" s="195"/>
     </row>
     <row r="10" spans="1:1" ht="13.5" thickBot="1">
-      <c r="A10" s="195"/>
+      <c r="A10" s="196"/>
     </row>
     <row r="11" spans="1:1" ht="27" customHeight="1">
       <c r="A11" s="22" t="s">
@@ -25787,10 +25789,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="4" customFormat="1" ht="25.5" customHeight="1" thickBot="1">
-      <c r="B1" s="196" t="s">
+      <c r="B1" s="197" t="s">
         <v>162</v>
       </c>
-      <c r="C1" s="197"/>
+      <c r="C1" s="198"/>
       <c r="D1" s="92"/>
       <c r="E1" s="32"/>
     </row>
@@ -25801,7 +25803,7 @@
       <c r="E2" s="119"/>
     </row>
     <row r="3" spans="1:5" ht="12.75" customHeight="1">
-      <c r="A3" s="198" t="s">
+      <c r="A3" s="199" t="s">
         <v>202</v>
       </c>
       <c r="B3" s="131" t="s">
@@ -25815,7 +25817,7 @@
       <c r="E3" s="5"/>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="199"/>
+      <c r="A4" s="200"/>
       <c r="B4" s="128" t="s">
         <v>159</v>
       </c>
@@ -25827,7 +25829,7 @@
       <c r="E4" s="5"/>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="199"/>
+      <c r="A5" s="200"/>
       <c r="B5" s="128" t="s">
         <v>160</v>
       </c>
@@ -25836,7 +25838,7 @@
       <c r="E5" s="5"/>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="199"/>
+      <c r="A6" s="200"/>
       <c r="B6" s="139" t="s">
         <v>204</v>
       </c>
@@ -25848,7 +25850,7 @@
       <c r="E6" s="5"/>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="199"/>
+      <c r="A7" s="200"/>
       <c r="B7" s="128" t="s">
         <v>171</v>
       </c>
@@ -25860,7 +25862,7 @@
       <c r="E7" s="5"/>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="199"/>
+      <c r="A8" s="200"/>
       <c r="B8" s="128" t="s">
         <v>172</v>
       </c>
@@ -25869,7 +25871,7 @@
       <c r="E8" s="5"/>
     </row>
     <row r="9" spans="1:5" ht="13.5" thickBot="1">
-      <c r="A9" s="200"/>
+      <c r="A9" s="201"/>
       <c r="B9" s="136" t="s">
         <v>161</v>
       </c>
@@ -25884,7 +25886,7 @@
       <c r="E10" s="94"/>
     </row>
     <row r="11" spans="1:5" ht="19.5" customHeight="1">
-      <c r="A11" s="198" t="s">
+      <c r="A11" s="199" t="s">
         <v>203</v>
       </c>
       <c r="B11" s="131" t="s">
@@ -25898,7 +25900,7 @@
       <c r="E11" s="5"/>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="199"/>
+      <c r="A12" s="200"/>
       <c r="B12" s="128" t="s">
         <v>159</v>
       </c>
@@ -25910,7 +25912,7 @@
       <c r="E12" s="5"/>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" s="199"/>
+      <c r="A13" s="200"/>
       <c r="B13" s="128" t="s">
         <v>160</v>
       </c>
@@ -25919,7 +25921,7 @@
       <c r="E13" s="5"/>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="199"/>
+      <c r="A14" s="200"/>
       <c r="B14" s="139" t="s">
         <v>204</v>
       </c>
@@ -25931,7 +25933,7 @@
       <c r="E14" s="5"/>
     </row>
     <row r="15" spans="1:5">
-      <c r="A15" s="199"/>
+      <c r="A15" s="200"/>
       <c r="B15" s="128" t="s">
         <v>171</v>
       </c>
@@ -25943,7 +25945,7 @@
       <c r="E15" s="5"/>
     </row>
     <row r="16" spans="1:5">
-      <c r="A16" s="199"/>
+      <c r="A16" s="200"/>
       <c r="B16" s="128" t="s">
         <v>172</v>
       </c>
@@ -25952,7 +25954,7 @@
       <c r="E16" s="5"/>
     </row>
     <row r="17" spans="1:5" ht="13.5" thickBot="1">
-      <c r="A17" s="200"/>
+      <c r="A17" s="201"/>
       <c r="B17" s="136" t="s">
         <v>161</v>
       </c>
@@ -25967,7 +25969,7 @@
       <c r="E18" s="94"/>
     </row>
     <row r="19" spans="1:5" collapsed="1">
-      <c r="A19" s="198" t="s">
+      <c r="A19" s="199" t="s">
         <v>203</v>
       </c>
       <c r="B19" s="131" t="s">
@@ -25976,7 +25978,7 @@
       <c r="C19" s="130"/>
     </row>
     <row r="20" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A20" s="199"/>
+      <c r="A20" s="200"/>
       <c r="B20" s="128" t="s">
         <v>159</v>
       </c>
@@ -25986,14 +25988,14 @@
       </c>
     </row>
     <row r="21" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A21" s="199"/>
+      <c r="A21" s="200"/>
       <c r="B21" s="128" t="s">
         <v>160</v>
       </c>
       <c r="C21" s="133"/>
     </row>
     <row r="22" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A22" s="199"/>
+      <c r="A22" s="200"/>
       <c r="B22" s="139" t="s">
         <v>204</v>
       </c>
@@ -26003,7 +26005,7 @@
       </c>
     </row>
     <row r="23" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A23" s="199"/>
+      <c r="A23" s="200"/>
       <c r="B23" s="128" t="s">
         <v>171</v>
       </c>
@@ -26013,14 +26015,14 @@
       </c>
     </row>
     <row r="24" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A24" s="199"/>
+      <c r="A24" s="200"/>
       <c r="B24" s="128" t="s">
         <v>172</v>
       </c>
       <c r="C24" s="132"/>
     </row>
     <row r="25" spans="1:5" ht="13.5" thickBot="1">
-      <c r="A25" s="200"/>
+      <c r="A25" s="201"/>
       <c r="B25" s="136" t="s">
         <v>161</v>
       </c>
@@ -26064,17 +26066,17 @@
       <c r="E1" s="5"/>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="217" t="s">
+      <c r="A2" s="208" t="s">
         <v>183</v>
       </c>
-      <c r="B2" s="218"/>
+      <c r="B2" s="209"/>
       <c r="C2" s="120"/>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="219" t="s">
+      <c r="A3" s="210" t="s">
         <v>185</v>
       </c>
-      <c r="B3" s="218"/>
+      <c r="B3" s="209"/>
       <c r="C3" s="120"/>
     </row>
     <row r="4" spans="1:5">
@@ -26090,115 +26092,128 @@
       <c r="C5" s="120"/>
     </row>
     <row r="7" spans="1:5" ht="18.75">
-      <c r="A7" s="205" t="s">
+      <c r="A7" s="219" t="s">
         <v>186</v>
       </c>
-      <c r="B7" s="206"/>
+      <c r="B7" s="220"/>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="120"/>
       <c r="B8" s="9"/>
     </row>
     <row r="9" spans="1:5" ht="39" customHeight="1">
-      <c r="A9" s="207" t="s">
+      <c r="A9" s="217" t="s">
         <v>187</v>
       </c>
-      <c r="B9" s="208"/>
+      <c r="B9" s="218"/>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="209"/>
-      <c r="B10" s="210"/>
+      <c r="A10" s="204"/>
+      <c r="B10" s="205"/>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="201" t="s">
+      <c r="A11" s="206" t="s">
         <v>188</v>
       </c>
-      <c r="B11" s="202"/>
+      <c r="B11" s="207"/>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="201" t="s">
+      <c r="A12" s="206" t="s">
         <v>189</v>
       </c>
-      <c r="B12" s="202"/>
+      <c r="B12" s="207"/>
     </row>
     <row r="13" spans="1:5" ht="43.5" customHeight="1">
-      <c r="A13" s="201" t="s">
+      <c r="A13" s="206" t="s">
         <v>190</v>
       </c>
-      <c r="B13" s="202"/>
+      <c r="B13" s="207"/>
     </row>
     <row r="14" spans="1:5" ht="19.5" customHeight="1">
-      <c r="A14" s="201" t="s">
+      <c r="A14" s="206" t="s">
         <v>191</v>
       </c>
-      <c r="B14" s="202"/>
+      <c r="B14" s="207"/>
     </row>
     <row r="15" spans="1:5" ht="18" customHeight="1">
-      <c r="A15" s="201" t="s">
+      <c r="A15" s="206" t="s">
         <v>192</v>
       </c>
-      <c r="B15" s="202"/>
+      <c r="B15" s="207"/>
     </row>
     <row r="16" spans="1:5" ht="21" customHeight="1">
-      <c r="A16" s="201" t="s">
+      <c r="A16" s="206" t="s">
         <v>193</v>
       </c>
-      <c r="B16" s="202"/>
+      <c r="B16" s="207"/>
     </row>
     <row r="17" spans="1:2" ht="48.75" customHeight="1">
-      <c r="A17" s="203" t="s">
+      <c r="A17" s="202" t="s">
         <v>195</v>
       </c>
-      <c r="B17" s="204"/>
+      <c r="B17" s="203"/>
     </row>
     <row r="19" spans="1:2" ht="18.75">
-      <c r="A19" s="205" t="s">
+      <c r="A19" s="219" t="s">
         <v>197</v>
       </c>
-      <c r="B19" s="206"/>
+      <c r="B19" s="220"/>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="120"/>
       <c r="B20" s="9"/>
     </row>
     <row r="21" spans="1:2">
-      <c r="A21" s="207" t="s">
+      <c r="A21" s="217" t="s">
         <v>198</v>
       </c>
-      <c r="B21" s="208"/>
+      <c r="B21" s="218"/>
     </row>
     <row r="22" spans="1:2">
-      <c r="A22" s="209"/>
-      <c r="B22" s="210"/>
+      <c r="A22" s="204"/>
+      <c r="B22" s="205"/>
     </row>
     <row r="23" spans="1:2">
-      <c r="A23" s="201" t="s">
+      <c r="A23" s="206" t="s">
         <v>199</v>
       </c>
-      <c r="B23" s="202"/>
+      <c r="B23" s="207"/>
     </row>
     <row r="24" spans="1:2">
-      <c r="A24" s="201"/>
-      <c r="B24" s="202"/>
+      <c r="A24" s="206"/>
+      <c r="B24" s="207"/>
     </row>
     <row r="25" spans="1:2">
-      <c r="A25" s="201" t="s">
+      <c r="A25" s="206" t="s">
         <v>200</v>
       </c>
-      <c r="B25" s="202"/>
+      <c r="B25" s="207"/>
     </row>
     <row r="26" spans="1:2">
-      <c r="A26" s="201" t="s">
+      <c r="A26" s="206" t="s">
         <v>201</v>
       </c>
-      <c r="B26" s="202"/>
+      <c r="B26" s="207"/>
     </row>
     <row r="27" spans="1:2">
-      <c r="A27" s="203"/>
-      <c r="B27" s="204"/>
+      <c r="A27" s="202"/>
+      <c r="B27" s="203"/>
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A7:B7"/>
     <mergeCell ref="A17:B17"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
@@ -26209,19 +26224,6 @@
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="A14:B14"/>
     <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A24:B24"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A3" r:id="rId1"/>

</xml_diff>

<commit_message>
Tempo - HiFi Stage 3 done.
</commit_message>
<xml_diff>
--- a/trunk/Tempo/Tempo.xlsx
+++ b/trunk/Tempo/Tempo.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1151" uniqueCount="275">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1152" uniqueCount="276">
   <si>
     <t>Notes</t>
   </si>
@@ -885,6 +885,9 @@
   <si>
     <t>Enter 1st teleport</t>
   </si>
+  <si>
+    <t>1st Move</t>
+  </si>
 </sst>
 </file>
 
@@ -894,10 +897,17 @@
     <numFmt numFmtId="164" formatCode="#,##0;[Red]#,##0"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="50">
+  <fonts count="51">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1860,34 +1870,34 @@
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="27" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="31" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="27" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="221">
+  <cellXfs count="222">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1895,208 +1905,208 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="22" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="19" fillId="13" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="20" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="26" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
+    <xf numFmtId="0" fontId="20" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="27" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="28" fillId="13" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="29" fillId="13" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="13" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="13" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="13" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="13" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="29" fillId="13" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="31" fillId="16" borderId="23" xfId="2" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="31" fillId="16" borderId="23" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="32" fillId="16" borderId="23" xfId="2" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="32" fillId="16" borderId="23" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="16" borderId="22" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="32" fillId="16" borderId="22" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="27" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="30" fillId="0" borderId="27" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="27" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="31" fillId="0" borderId="27" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="3" fontId="32" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="30" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="30" fillId="0" borderId="30" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="30" fillId="0" borderId="29" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="32" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="30" fillId="17" borderId="31" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="30" fillId="18" borderId="31" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="30" fillId="19" borderId="31" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="31" fillId="20" borderId="23" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="31" fillId="20" borderId="23" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="33" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="30" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="31" fillId="0" borderId="30" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="31" fillId="0" borderId="29" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="33" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="31" fillId="17" borderId="31" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="31" fillId="18" borderId="31" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="31" fillId="19" borderId="31" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="32" fillId="20" borderId="23" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="32" fillId="20" borderId="23" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="20" borderId="22" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="32" fillId="20" borderId="22" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="31" fillId="21" borderId="23" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="31" fillId="21" borderId="23" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="32" fillId="21" borderId="23" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="32" fillId="21" borderId="23" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="21" borderId="22" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="32" fillId="21" borderId="22" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="41" fillId="16" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="42" fillId="16" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="41" fillId="20" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="42" fillId="20" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
-    <xf numFmtId="3" fontId="32" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="30" fillId="0" borderId="42" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="32" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="32" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="32" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="30" fillId="0" borderId="42" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="33" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="31" fillId="0" borderId="42" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="33" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="33" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="33" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="31" fillId="0" borderId="42" xfId="1" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2106,10 +2116,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2130,19 +2140,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="23" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="48" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="49" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="39" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="33" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="49" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="26" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="35" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="38" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="32" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="48" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="25" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="34" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="37" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="37" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="38" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
@@ -2152,133 +2165,133 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="21" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="36" fillId="21" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="20" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="36" fillId="20" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="38" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="23" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="33" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="39" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="34" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="40" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="41" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="16" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="36" fillId="16" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="19" fillId="13" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="20" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="18" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="23" fillId="14" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="20" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="21" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="21" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="24" fillId="14" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="14" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="14" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="14" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="14" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="24" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="49" fillId="22" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="50" fillId="22" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="49" fillId="22" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="50" fillId="22" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="49" fillId="22" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="50" fillId="22" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="47" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="48" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="48" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="46" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="46" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="4"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="4"/>
     </xf>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="33" xfId="3" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="33" xfId="3" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" indent="4"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="47" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="47" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="46" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Accent1" xfId="2" builtinId="29"/>
@@ -2586,11 +2599,11 @@
   <sheetPr>
     <tabColor theme="4" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:K157"/>
+  <dimension ref="A1:K158"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C50" sqref="C50"/>
+      <selection pane="bottomLeft" activeCell="C58" sqref="C58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" outlineLevelRow="2"/>
@@ -2618,7 +2631,7 @@
       <c r="F1" s="163"/>
       <c r="G1" s="140"/>
       <c r="H1" s="141">
-        <f>SUM(G1:G65539)</f>
+        <f>SUM(G1:G65540)</f>
         <v>0</v>
       </c>
       <c r="I1" s="141" t="s">
@@ -3345,7 +3358,7 @@
         <v>11282</v>
       </c>
       <c r="E44" s="123">
-        <f t="shared" ref="E44:E64" si="3">IF(AND(C44&gt;0,D44&gt;0), D44-C44, 0)</f>
+        <f t="shared" ref="E44:E65" si="3">IF(AND(C44&gt;0,D44&gt;0), D44-C44, 0)</f>
         <v>0</v>
       </c>
       <c r="F44" s="104"/>
@@ -3389,12 +3402,10 @@
       <c r="C47" s="101">
         <v>13024</v>
       </c>
-      <c r="D47" s="101">
-        <v>15531</v>
-      </c>
+      <c r="D47" s="101"/>
       <c r="E47" s="123">
         <f t="shared" si="3"/>
-        <v>2507</v>
+        <v>0</v>
       </c>
       <c r="F47" s="105"/>
     </row>
@@ -3425,117 +3436,132 @@
     </row>
     <row r="50" spans="1:6" ht="15" outlineLevel="1">
       <c r="A50" s="157"/>
-      <c r="B50" s="150" t="s">
-        <v>229</v>
-      </c>
-      <c r="C50" s="101"/>
-      <c r="D50" s="101">
-        <v>17390</v>
-      </c>
-      <c r="E50" s="123">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
+      <c r="B50" s="221" t="s">
+        <v>275</v>
+      </c>
+      <c r="C50" s="101">
+        <v>14433</v>
+      </c>
+      <c r="D50" s="101"/>
+      <c r="E50" s="123"/>
       <c r="F50" s="105"/>
     </row>
     <row r="51" spans="1:6" ht="15" outlineLevel="1">
       <c r="A51" s="157"/>
       <c r="B51" s="150" t="s">
-        <v>230</v>
-      </c>
-      <c r="C51" s="101"/>
+        <v>229</v>
+      </c>
+      <c r="C51" s="101">
+        <v>14517</v>
+      </c>
       <c r="D51" s="101">
-        <v>17856</v>
+        <v>17390</v>
       </c>
       <c r="E51" s="123">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>2873</v>
       </c>
       <c r="F51" s="105"/>
     </row>
     <row r="52" spans="1:6" ht="15" outlineLevel="1">
       <c r="A52" s="157"/>
       <c r="B52" s="150" t="s">
-        <v>231</v>
-      </c>
-      <c r="C52" s="101"/>
+        <v>230</v>
+      </c>
+      <c r="C52" s="101">
+        <v>14945</v>
+      </c>
       <c r="D52" s="101">
-        <v>18332</v>
+        <v>17856</v>
       </c>
       <c r="E52" s="123">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>2911</v>
       </c>
       <c r="F52" s="105"/>
     </row>
     <row r="53" spans="1:6" ht="15" outlineLevel="1">
       <c r="A53" s="157"/>
       <c r="B53" s="150" t="s">
-        <v>233</v>
-      </c>
-      <c r="C53" s="101"/>
+        <v>231</v>
+      </c>
+      <c r="C53" s="101">
+        <v>15393</v>
+      </c>
       <c r="D53" s="101">
-        <v>18738</v>
+        <v>18332</v>
       </c>
       <c r="E53" s="123">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>2939</v>
       </c>
       <c r="F53" s="105"/>
     </row>
     <row r="54" spans="1:6" ht="15" outlineLevel="1">
       <c r="A54" s="157"/>
       <c r="B54" s="150" t="s">
-        <v>234</v>
-      </c>
-      <c r="C54" s="101"/>
+        <v>233</v>
+      </c>
+      <c r="C54" s="101">
+        <v>15797</v>
+      </c>
       <c r="D54" s="101">
-        <v>19757</v>
+        <v>18738</v>
       </c>
       <c r="E54" s="123">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>2941</v>
       </c>
       <c r="F54" s="105"/>
     </row>
     <row r="55" spans="1:6" ht="15" outlineLevel="1">
       <c r="A55" s="157"/>
       <c r="B55" s="150" t="s">
-        <v>235</v>
-      </c>
-      <c r="C55" s="101"/>
+        <v>234</v>
+      </c>
+      <c r="C55" s="101">
+        <v>16590</v>
+      </c>
       <c r="D55" s="101">
-        <v>20174</v>
+        <v>19757</v>
       </c>
       <c r="E55" s="123">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>3167</v>
       </c>
       <c r="F55" s="105"/>
     </row>
     <row r="56" spans="1:6" ht="15" outlineLevel="1">
       <c r="A56" s="157"/>
       <c r="B56" s="150" t="s">
-        <v>236</v>
-      </c>
-      <c r="C56" s="101"/>
+        <v>235</v>
+      </c>
+      <c r="C56" s="101">
+        <v>17005</v>
+      </c>
       <c r="D56" s="101">
-        <v>20965</v>
+        <v>20174</v>
       </c>
       <c r="E56" s="123">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>3169</v>
       </c>
       <c r="F56" s="105"/>
     </row>
     <row r="57" spans="1:6" ht="15" outlineLevel="1">
       <c r="A57" s="157"/>
-      <c r="B57" s="100"/>
-      <c r="C57" s="101"/>
-      <c r="D57" s="101"/>
+      <c r="B57" s="150" t="s">
+        <v>236</v>
+      </c>
+      <c r="C57" s="101">
+        <v>17761</v>
+      </c>
+      <c r="D57" s="101">
+        <v>20965</v>
+      </c>
       <c r="E57" s="123">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>3204</v>
       </c>
       <c r="F57" s="105"/>
     </row>
@@ -3552,9 +3578,7 @@
     </row>
     <row r="59" spans="1:6" ht="15" outlineLevel="1">
       <c r="A59" s="157"/>
-      <c r="B59" s="150" t="s">
-        <v>237</v>
-      </c>
+      <c r="B59" s="100"/>
       <c r="C59" s="101"/>
       <c r="D59" s="101"/>
       <c r="E59" s="123">
@@ -3566,12 +3590,10 @@
     <row r="60" spans="1:6" ht="15" outlineLevel="1">
       <c r="A60" s="157"/>
       <c r="B60" s="150" t="s">
-        <v>223</v>
+        <v>237</v>
       </c>
       <c r="C60" s="101"/>
-      <c r="D60" s="101">
-        <v>23906</v>
-      </c>
+      <c r="D60" s="101"/>
       <c r="E60" s="123">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -3581,11 +3603,11 @@
     <row r="61" spans="1:6" ht="15" outlineLevel="1">
       <c r="A61" s="157"/>
       <c r="B61" s="150" t="s">
-        <v>238</v>
+        <v>223</v>
       </c>
       <c r="C61" s="101"/>
       <c r="D61" s="101">
-        <v>24132</v>
+        <v>23906</v>
       </c>
       <c r="E61" s="123">
         <f t="shared" si="3"/>
@@ -3596,130 +3618,130 @@
     <row r="62" spans="1:6" ht="15" outlineLevel="1">
       <c r="A62" s="157"/>
       <c r="B62" s="150" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C62" s="101"/>
       <c r="D62" s="101">
-        <v>24753</v>
-      </c>
-      <c r="E62" s="123"/>
+        <v>24132</v>
+      </c>
+      <c r="E62" s="123">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
       <c r="F62" s="105"/>
     </row>
     <row r="63" spans="1:6" ht="15" outlineLevel="1">
       <c r="A63" s="157"/>
       <c r="B63" s="150" t="s">
-        <v>217</v>
+        <v>239</v>
       </c>
       <c r="C63" s="101"/>
       <c r="D63" s="101">
+        <v>24753</v>
+      </c>
+      <c r="E63" s="123"/>
+      <c r="F63" s="105"/>
+    </row>
+    <row r="64" spans="1:6" ht="15" outlineLevel="1">
+      <c r="A64" s="157"/>
+      <c r="B64" s="150" t="s">
+        <v>217</v>
+      </c>
+      <c r="C64" s="101"/>
+      <c r="D64" s="101">
         <v>25129</v>
       </c>
-      <c r="E63" s="123">
+      <c r="E64" s="123">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="F63" s="105"/>
-    </row>
-    <row r="64" spans="1:6" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="A64" s="157"/>
-      <c r="B64" s="98" t="s">
+      <c r="F64" s="105"/>
+    </row>
+    <row r="65" spans="1:8" ht="15.75" outlineLevel="1" thickBot="1">
+      <c r="A65" s="157"/>
+      <c r="B65" s="98" t="s">
         <v>179</v>
       </c>
-      <c r="C64" s="99"/>
-      <c r="D64" s="99">
+      <c r="C65" s="99"/>
+      <c r="D65" s="99">
         <v>25174</v>
       </c>
-      <c r="E64" s="125">
+      <c r="E65" s="125">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="F64" s="104"/>
-    </row>
-    <row r="65" spans="1:8" ht="17.25" thickTop="1" thickBot="1">
-      <c r="A65" s="116" t="s">
+      <c r="F65" s="104"/>
+    </row>
+    <row r="66" spans="1:8" ht="17.25" thickTop="1" thickBot="1">
+      <c r="A66" s="116" t="s">
         <v>227</v>
       </c>
-      <c r="B65" s="102" t="s">
+      <c r="B66" s="102" t="s">
         <v>173</v>
       </c>
-      <c r="C65" s="103">
-        <f>C64-C44</f>
-        <v>0</v>
-      </c>
-      <c r="D65" s="103">
-        <f>D64-D44</f>
+      <c r="C66" s="103">
+        <f>C65-C44</f>
+        <v>0</v>
+      </c>
+      <c r="D66" s="103">
+        <f>D65-D44</f>
         <v>13892</v>
       </c>
-      <c r="E65" s="126">
-        <f>E64-E44</f>
-        <v>0</v>
-      </c>
-      <c r="F65" s="107"/>
-      <c r="G65" s="112">
-        <f>E65</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="66" spans="1:8" ht="13.5" thickBot="1"/>
-    <row r="67" spans="1:8" ht="15" customHeight="1" outlineLevel="1">
-      <c r="A67" s="158" t="s">
+      <c r="E66" s="126">
+        <f>E65-E44</f>
+        <v>0</v>
+      </c>
+      <c r="F66" s="107"/>
+      <c r="G66" s="112">
+        <f>E66</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" ht="13.5" thickBot="1"/>
+    <row r="68" spans="1:8" ht="15" customHeight="1" outlineLevel="1">
+      <c r="A68" s="158" t="s">
         <v>240</v>
       </c>
-      <c r="B67" s="109" t="s">
+      <c r="B68" s="109" t="s">
         <v>175</v>
       </c>
-      <c r="C67" s="110" t="s">
+      <c r="C68" s="110" t="s">
         <v>42</v>
       </c>
-      <c r="D67" s="110" t="s">
+      <c r="D68" s="110" t="s">
         <v>41</v>
       </c>
-      <c r="E67" s="110" t="s">
+      <c r="E68" s="110" t="s">
         <v>43</v>
       </c>
-      <c r="F67" s="111" t="s">
+      <c r="F68" s="111" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="68" spans="1:8" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="A68" s="157"/>
-      <c r="B68" s="98" t="s">
+    <row r="69" spans="1:8" ht="15.75" outlineLevel="1" thickBot="1">
+      <c r="A69" s="157"/>
+      <c r="B69" s="98" t="s">
         <v>177</v>
       </c>
-      <c r="C68" s="99"/>
-      <c r="D68" s="99">
+      <c r="C69" s="99"/>
+      <c r="D69" s="99">
         <v>25174</v>
       </c>
-      <c r="E68" s="123">
-        <f t="shared" ref="E68:E80" si="4">IF(AND(C68&gt;0,D68&gt;0), D68-C68, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="F68" s="104"/>
-      <c r="H68">
+      <c r="E69" s="123">
+        <f t="shared" ref="E69:E81" si="4">IF(AND(C69&gt;0,D69&gt;0), D69-C69, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="F69" s="104"/>
+      <c r="H69">
         <v>49739</v>
       </c>
     </row>
-    <row r="69" spans="1:8" ht="15.75" outlineLevel="1" thickTop="1">
-      <c r="A69" s="157"/>
-      <c r="B69" s="100"/>
-      <c r="C69" s="101"/>
-      <c r="D69" s="101"/>
-      <c r="E69" s="124">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="F69" s="105"/>
-    </row>
-    <row r="70" spans="1:8" ht="15" outlineLevel="1">
+    <row r="70" spans="1:8" ht="15.75" outlineLevel="1" thickTop="1">
       <c r="A70" s="157"/>
-      <c r="B70" s="151" t="s">
-        <v>242</v>
-      </c>
+      <c r="B70" s="100"/>
       <c r="C70" s="101"/>
-      <c r="D70" s="101">
-        <v>26754</v>
-      </c>
-      <c r="E70" s="123">
+      <c r="D70" s="101"/>
+      <c r="E70" s="124">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -3727,9 +3749,13 @@
     </row>
     <row r="71" spans="1:8" ht="15" outlineLevel="1">
       <c r="A71" s="157"/>
-      <c r="B71" s="100"/>
+      <c r="B71" s="151" t="s">
+        <v>242</v>
+      </c>
       <c r="C71" s="101"/>
-      <c r="D71" s="101"/>
+      <c r="D71" s="101">
+        <v>26754</v>
+      </c>
       <c r="E71" s="123">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -3738,13 +3764,9 @@
     </row>
     <row r="72" spans="1:8" ht="15" outlineLevel="1">
       <c r="A72" s="157"/>
-      <c r="B72" s="151" t="s">
-        <v>243</v>
-      </c>
+      <c r="B72" s="100"/>
       <c r="C72" s="101"/>
-      <c r="D72" s="101">
-        <v>27765</v>
-      </c>
+      <c r="D72" s="101"/>
       <c r="E72" s="123">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -3753,9 +3775,13 @@
     </row>
     <row r="73" spans="1:8" ht="15" outlineLevel="1">
       <c r="A73" s="157"/>
-      <c r="B73" s="100"/>
+      <c r="B73" s="151" t="s">
+        <v>243</v>
+      </c>
       <c r="C73" s="101"/>
-      <c r="D73" s="101"/>
+      <c r="D73" s="101">
+        <v>27765</v>
+      </c>
       <c r="E73" s="123">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -3764,13 +3790,9 @@
     </row>
     <row r="74" spans="1:8" ht="15" outlineLevel="1">
       <c r="A74" s="157"/>
-      <c r="B74" s="151" t="s">
-        <v>244</v>
-      </c>
+      <c r="B74" s="100"/>
       <c r="C74" s="101"/>
-      <c r="D74" s="101">
-        <v>30127</v>
-      </c>
+      <c r="D74" s="101"/>
       <c r="E74" s="123">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -3779,9 +3801,13 @@
     </row>
     <row r="75" spans="1:8" ht="15" outlineLevel="1">
       <c r="A75" s="157"/>
-      <c r="B75" s="100"/>
+      <c r="B75" s="151" t="s">
+        <v>244</v>
+      </c>
       <c r="C75" s="101"/>
-      <c r="D75" s="101"/>
+      <c r="D75" s="101">
+        <v>30127</v>
+      </c>
       <c r="E75" s="123">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -3790,13 +3816,9 @@
     </row>
     <row r="76" spans="1:8" ht="15" outlineLevel="1">
       <c r="A76" s="157"/>
-      <c r="B76" s="151" t="s">
-        <v>245</v>
-      </c>
+      <c r="B76" s="100"/>
       <c r="C76" s="101"/>
-      <c r="D76" s="101">
-        <v>33299</v>
-      </c>
+      <c r="D76" s="101"/>
       <c r="E76" s="123">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -3806,11 +3828,11 @@
     <row r="77" spans="1:8" ht="15" outlineLevel="1">
       <c r="A77" s="157"/>
       <c r="B77" s="151" t="s">
-        <v>238</v>
+        <v>245</v>
       </c>
       <c r="C77" s="101"/>
       <c r="D77" s="101">
-        <v>33527</v>
+        <v>33299</v>
       </c>
       <c r="E77" s="123">
         <f t="shared" si="4"/>
@@ -3821,11 +3843,11 @@
     <row r="78" spans="1:8" ht="15" outlineLevel="1">
       <c r="A78" s="157"/>
       <c r="B78" s="151" t="s">
-        <v>246</v>
+        <v>238</v>
       </c>
       <c r="C78" s="101"/>
       <c r="D78" s="101">
-        <v>34309</v>
+        <v>33527</v>
       </c>
       <c r="E78" s="123">
         <f t="shared" si="4"/>
@@ -3836,11 +3858,11 @@
     <row r="79" spans="1:8" ht="15" outlineLevel="1">
       <c r="A79" s="157"/>
       <c r="B79" s="151" t="s">
-        <v>217</v>
+        <v>246</v>
       </c>
       <c r="C79" s="101"/>
       <c r="D79" s="101">
-        <v>34727</v>
+        <v>34309</v>
       </c>
       <c r="E79" s="123">
         <f t="shared" si="4"/>
@@ -3848,110 +3870,110 @@
       </c>
       <c r="F79" s="105"/>
     </row>
-    <row r="80" spans="1:8" ht="15.75" outlineLevel="1" thickBot="1">
+    <row r="80" spans="1:8" ht="15" outlineLevel="1">
       <c r="A80" s="157"/>
-      <c r="B80" s="98" t="s">
+      <c r="B80" s="151" t="s">
+        <v>217</v>
+      </c>
+      <c r="C80" s="101"/>
+      <c r="D80" s="101">
+        <v>34727</v>
+      </c>
+      <c r="E80" s="123">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="F80" s="105"/>
+    </row>
+    <row r="81" spans="1:8" ht="15.75" outlineLevel="1" thickBot="1">
+      <c r="A81" s="157"/>
+      <c r="B81" s="98" t="s">
         <v>179</v>
       </c>
-      <c r="C80" s="99"/>
-      <c r="D80" s="99">
+      <c r="C81" s="99"/>
+      <c r="D81" s="99">
         <v>34795</v>
       </c>
-      <c r="E80" s="125">
+      <c r="E81" s="125">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="F80" s="104"/>
-    </row>
-    <row r="81" spans="1:8" ht="17.25" thickTop="1" thickBot="1">
-      <c r="A81" s="117" t="s">
+      <c r="F81" s="104"/>
+    </row>
+    <row r="82" spans="1:8" ht="17.25" thickTop="1" thickBot="1">
+      <c r="A82" s="117" t="s">
         <v>241</v>
       </c>
-      <c r="B81" s="102" t="s">
+      <c r="B82" s="102" t="s">
         <v>173</v>
       </c>
-      <c r="C81" s="103">
-        <f>C80-C68</f>
-        <v>0</v>
-      </c>
-      <c r="D81" s="103">
-        <f>D80-D68</f>
+      <c r="C82" s="103">
+        <f>C81-C69</f>
+        <v>0</v>
+      </c>
+      <c r="D82" s="103">
+        <f>D81-D69</f>
         <v>9621</v>
       </c>
-      <c r="E81" s="126">
-        <f>E80-E68</f>
-        <v>0</v>
-      </c>
-      <c r="F81" s="108"/>
-      <c r="G81" s="112">
-        <f>E81</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="82" spans="1:8" ht="13.5" thickBot="1"/>
-    <row r="83" spans="1:8" ht="15" customHeight="1" outlineLevel="1">
-      <c r="A83" s="156" t="s">
+      <c r="E82" s="126">
+        <f>E81-E69</f>
+        <v>0</v>
+      </c>
+      <c r="F82" s="108"/>
+      <c r="G82" s="112">
+        <f>E82</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" ht="13.5" thickBot="1"/>
+    <row r="84" spans="1:8" ht="15" customHeight="1" outlineLevel="1">
+      <c r="A84" s="156" t="s">
         <v>247</v>
       </c>
-      <c r="B83" s="113" t="s">
+      <c r="B84" s="113" t="s">
         <v>175</v>
       </c>
-      <c r="C83" s="114" t="s">
+      <c r="C84" s="114" t="s">
         <v>42</v>
       </c>
-      <c r="D83" s="114" t="s">
+      <c r="D84" s="114" t="s">
         <v>41</v>
       </c>
-      <c r="E83" s="114" t="s">
+      <c r="E84" s="114" t="s">
         <v>43</v>
       </c>
-      <c r="F83" s="115" t="s">
+      <c r="F84" s="115" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="84" spans="1:8" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="A84" s="157"/>
-      <c r="B84" s="98" t="s">
+    <row r="85" spans="1:8" ht="15.75" outlineLevel="1" thickBot="1">
+      <c r="A85" s="157"/>
+      <c r="B85" s="98" t="s">
         <v>177</v>
       </c>
-      <c r="C84" s="99"/>
-      <c r="D84" s="99">
+      <c r="C85" s="99"/>
+      <c r="D85" s="99">
         <v>34795</v>
       </c>
-      <c r="E84" s="123">
-        <f t="shared" ref="E84:E97" si="5">IF(AND(C84&gt;0,D84&gt;0), D84-C84, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="F84" s="104"/>
-      <c r="H84">
+      <c r="E85" s="123">
+        <f t="shared" ref="E85:E98" si="5">IF(AND(C85&gt;0,D85&gt;0), D85-C85, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="F85" s="104"/>
+      <c r="H85">
         <v>67476</v>
       </c>
     </row>
-    <row r="85" spans="1:8" ht="15.75" outlineLevel="1" thickTop="1">
-      <c r="A85" s="157"/>
-      <c r="B85" s="151" t="s">
-        <v>228</v>
-      </c>
-      <c r="C85" s="101"/>
-      <c r="D85" s="101">
-        <v>36326</v>
-      </c>
-      <c r="E85" s="124">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="F85" s="105"/>
-    </row>
-    <row r="86" spans="1:8" ht="15" outlineLevel="1">
+    <row r="86" spans="1:8" ht="15.75" outlineLevel="1" thickTop="1">
       <c r="A86" s="157"/>
       <c r="B86" s="151" t="s">
-        <v>221</v>
+        <v>228</v>
       </c>
       <c r="C86" s="101"/>
       <c r="D86" s="101">
-        <v>37764</v>
-      </c>
-      <c r="E86" s="123">
+        <v>36326</v>
+      </c>
+      <c r="E86" s="124">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -3959,9 +3981,13 @@
     </row>
     <row r="87" spans="1:8" ht="15" outlineLevel="1">
       <c r="A87" s="157"/>
-      <c r="B87" s="100"/>
+      <c r="B87" s="151" t="s">
+        <v>221</v>
+      </c>
       <c r="C87" s="101"/>
-      <c r="D87" s="101"/>
+      <c r="D87" s="101">
+        <v>37764</v>
+      </c>
       <c r="E87" s="123">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -3970,13 +3996,9 @@
     </row>
     <row r="88" spans="1:8" ht="15" outlineLevel="1">
       <c r="A88" s="157"/>
-      <c r="B88" s="151" t="s">
-        <v>222</v>
-      </c>
+      <c r="B88" s="100"/>
       <c r="C88" s="101"/>
-      <c r="D88" s="101">
-        <v>43241</v>
-      </c>
+      <c r="D88" s="101"/>
       <c r="E88" s="123">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -3985,9 +4007,13 @@
     </row>
     <row r="89" spans="1:8" ht="15" outlineLevel="1">
       <c r="A89" s="157"/>
-      <c r="B89" s="100"/>
+      <c r="B89" s="151" t="s">
+        <v>222</v>
+      </c>
       <c r="C89" s="101"/>
-      <c r="D89" s="101"/>
+      <c r="D89" s="101">
+        <v>43241</v>
+      </c>
       <c r="E89" s="123">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -3996,13 +4022,9 @@
     </row>
     <row r="90" spans="1:8" ht="15" outlineLevel="1">
       <c r="A90" s="157"/>
-      <c r="B90" s="152" t="s">
-        <v>236</v>
-      </c>
+      <c r="B90" s="100"/>
       <c r="C90" s="101"/>
-      <c r="D90" s="101">
-        <v>45890</v>
-      </c>
+      <c r="D90" s="101"/>
       <c r="E90" s="123">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -4011,9 +4033,13 @@
     </row>
     <row r="91" spans="1:8" ht="15" outlineLevel="1">
       <c r="A91" s="157"/>
-      <c r="B91" s="100"/>
+      <c r="B91" s="152" t="s">
+        <v>236</v>
+      </c>
       <c r="C91" s="101"/>
-      <c r="D91" s="101"/>
+      <c r="D91" s="101">
+        <v>45890</v>
+      </c>
       <c r="E91" s="123">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -4033,13 +4059,9 @@
     </row>
     <row r="93" spans="1:8" ht="15" outlineLevel="1">
       <c r="A93" s="157"/>
-      <c r="B93" s="152" t="s">
-        <v>223</v>
-      </c>
+      <c r="B93" s="100"/>
       <c r="C93" s="101"/>
-      <c r="D93" s="101">
-        <v>49269</v>
-      </c>
+      <c r="D93" s="101"/>
       <c r="E93" s="123">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -4049,11 +4071,11 @@
     <row r="94" spans="1:8" ht="15" outlineLevel="1">
       <c r="A94" s="157"/>
       <c r="B94" s="152" t="s">
-        <v>249</v>
+        <v>223</v>
       </c>
       <c r="C94" s="101"/>
       <c r="D94" s="101">
-        <v>49505</v>
+        <v>49269</v>
       </c>
       <c r="E94" s="123">
         <f t="shared" si="5"/>
@@ -4064,11 +4086,11 @@
     <row r="95" spans="1:8" ht="15" outlineLevel="1">
       <c r="A95" s="157"/>
       <c r="B95" s="152" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C95" s="101"/>
       <c r="D95" s="101">
-        <v>50134</v>
+        <v>49505</v>
       </c>
       <c r="E95" s="123">
         <f t="shared" si="5"/>
@@ -4079,11 +4101,11 @@
     <row r="96" spans="1:8" ht="15" outlineLevel="1">
       <c r="A96" s="157"/>
       <c r="B96" s="152" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C96" s="101"/>
       <c r="D96" s="101">
-        <v>50516</v>
+        <v>50134</v>
       </c>
       <c r="E96" s="123">
         <f t="shared" si="5"/>
@@ -4091,106 +4113,106 @@
       </c>
       <c r="F96" s="105"/>
     </row>
-    <row r="97" spans="1:8" ht="15.75" outlineLevel="1" thickBot="1">
+    <row r="97" spans="1:8" ht="15" outlineLevel="1">
       <c r="A97" s="157"/>
-      <c r="B97" s="98" t="s">
+      <c r="B97" s="152" t="s">
+        <v>251</v>
+      </c>
+      <c r="C97" s="101"/>
+      <c r="D97" s="101">
+        <v>50516</v>
+      </c>
+      <c r="E97" s="123">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="F97" s="105"/>
+    </row>
+    <row r="98" spans="1:8" ht="15.75" outlineLevel="1" thickBot="1">
+      <c r="A98" s="157"/>
+      <c r="B98" s="98" t="s">
         <v>179</v>
       </c>
-      <c r="C97" s="99"/>
-      <c r="D97" s="99">
+      <c r="C98" s="99"/>
+      <c r="D98" s="99">
         <v>50574</v>
       </c>
-      <c r="E97" s="125">
+      <c r="E98" s="125">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="F97" s="104"/>
-    </row>
-    <row r="98" spans="1:8" ht="17.25" thickTop="1" thickBot="1">
-      <c r="A98" s="116" t="s">
+      <c r="F98" s="104"/>
+    </row>
+    <row r="99" spans="1:8" ht="17.25" thickTop="1" thickBot="1">
+      <c r="A99" s="116" t="s">
         <v>248</v>
       </c>
-      <c r="B98" s="102" t="s">
+      <c r="B99" s="102" t="s">
         <v>173</v>
       </c>
-      <c r="C98" s="103">
-        <f>C97-C84</f>
-        <v>0</v>
-      </c>
-      <c r="D98" s="103">
-        <f>D97-D84</f>
+      <c r="C99" s="103">
+        <f>C98-C85</f>
+        <v>0</v>
+      </c>
+      <c r="D99" s="103">
+        <f>D98-D85</f>
         <v>15779</v>
       </c>
-      <c r="E98" s="126">
-        <f>E97-E84</f>
-        <v>0</v>
-      </c>
-      <c r="F98" s="107"/>
-      <c r="G98" s="112">
-        <f>E98</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="99" spans="1:8" ht="13.5" thickBot="1"/>
-    <row r="100" spans="1:8" ht="15" customHeight="1" outlineLevel="1">
-      <c r="A100" s="158" t="s">
+      <c r="E99" s="126">
+        <f>E98-E85</f>
+        <v>0</v>
+      </c>
+      <c r="F99" s="107"/>
+      <c r="G99" s="112">
+        <f>E99</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" ht="13.5" thickBot="1"/>
+    <row r="101" spans="1:8" ht="15" customHeight="1" outlineLevel="1">
+      <c r="A101" s="158" t="s">
         <v>252</v>
       </c>
-      <c r="B100" s="109" t="s">
+      <c r="B101" s="109" t="s">
         <v>175</v>
       </c>
-      <c r="C100" s="110" t="s">
+      <c r="C101" s="110" t="s">
         <v>42</v>
       </c>
-      <c r="D100" s="110" t="s">
+      <c r="D101" s="110" t="s">
         <v>41</v>
       </c>
-      <c r="E100" s="110" t="s">
+      <c r="E101" s="110" t="s">
         <v>43</v>
       </c>
-      <c r="F100" s="111" t="s">
+      <c r="F101" s="111" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="101" spans="1:8" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="A101" s="157"/>
-      <c r="B101" s="98" t="s">
+    <row r="102" spans="1:8" ht="15.75" outlineLevel="1" thickBot="1">
+      <c r="A102" s="157"/>
+      <c r="B102" s="98" t="s">
         <v>177</v>
       </c>
-      <c r="C101" s="99"/>
-      <c r="D101" s="99">
+      <c r="C102" s="99"/>
+      <c r="D102" s="99">
         <v>50574</v>
       </c>
-      <c r="E101" s="123">
-        <f t="shared" ref="E101:E110" si="6">IF(AND(C101&gt;0,D101&gt;0), D101-C101, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="F101" s="104"/>
-      <c r="H101">
+      <c r="E102" s="123">
+        <f t="shared" ref="E102:E111" si="6">IF(AND(C102&gt;0,D102&gt;0), D102-C102, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="F102" s="104"/>
+      <c r="H102">
         <v>105030</v>
       </c>
     </row>
-    <row r="102" spans="1:8" ht="15.75" outlineLevel="1" thickTop="1">
-      <c r="A102" s="157"/>
-      <c r="B102" s="100"/>
-      <c r="C102" s="101"/>
-      <c r="D102" s="101"/>
-      <c r="E102" s="124">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="F102" s="105"/>
-    </row>
-    <row r="103" spans="1:8" ht="15" outlineLevel="1">
+    <row r="103" spans="1:8" ht="15.75" outlineLevel="1" thickTop="1">
       <c r="A103" s="157"/>
-      <c r="B103" s="152" t="s">
-        <v>254</v>
-      </c>
+      <c r="B103" s="100"/>
       <c r="C103" s="101"/>
-      <c r="D103" s="101">
-        <v>52785</v>
-      </c>
-      <c r="E103" s="123">
+      <c r="D103" s="101"/>
+      <c r="E103" s="124">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
@@ -4198,9 +4220,13 @@
     </row>
     <row r="104" spans="1:8" ht="15" outlineLevel="1">
       <c r="A104" s="157"/>
-      <c r="B104" s="100"/>
+      <c r="B104" s="152" t="s">
+        <v>254</v>
+      </c>
       <c r="C104" s="101"/>
-      <c r="D104" s="101"/>
+      <c r="D104" s="101">
+        <v>52785</v>
+      </c>
       <c r="E104" s="123">
         <f t="shared" si="6"/>
         <v>0</v>
@@ -4209,13 +4235,9 @@
     </row>
     <row r="105" spans="1:8" ht="15" outlineLevel="1">
       <c r="A105" s="157"/>
-      <c r="B105" s="152" t="s">
-        <v>255</v>
-      </c>
+      <c r="B105" s="100"/>
       <c r="C105" s="101"/>
-      <c r="D105" s="101">
-        <v>53409</v>
-      </c>
+      <c r="D105" s="101"/>
       <c r="E105" s="123">
         <f t="shared" si="6"/>
         <v>0</v>
@@ -4224,9 +4246,13 @@
     </row>
     <row r="106" spans="1:8" ht="15" outlineLevel="1">
       <c r="A106" s="157"/>
-      <c r="B106" s="100"/>
+      <c r="B106" s="152" t="s">
+        <v>255</v>
+      </c>
       <c r="C106" s="101"/>
-      <c r="D106" s="101"/>
+      <c r="D106" s="101">
+        <v>53409</v>
+      </c>
       <c r="E106" s="123">
         <f t="shared" si="6"/>
         <v>0</v>
@@ -4235,13 +4261,9 @@
     </row>
     <row r="107" spans="1:8" ht="15" outlineLevel="1">
       <c r="A107" s="157"/>
-      <c r="B107" s="152" t="s">
-        <v>223</v>
-      </c>
+      <c r="B107" s="100"/>
       <c r="C107" s="101"/>
-      <c r="D107" s="101">
-        <v>55728</v>
-      </c>
+      <c r="D107" s="101"/>
       <c r="E107" s="123">
         <f t="shared" si="6"/>
         <v>0</v>
@@ -4251,11 +4273,11 @@
     <row r="108" spans="1:8" ht="15" outlineLevel="1">
       <c r="A108" s="157"/>
       <c r="B108" s="152" t="s">
-        <v>249</v>
+        <v>223</v>
       </c>
       <c r="C108" s="101"/>
       <c r="D108" s="101">
-        <v>55956</v>
+        <v>55728</v>
       </c>
       <c r="E108" s="123">
         <f t="shared" si="6"/>
@@ -4266,11 +4288,11 @@
     <row r="109" spans="1:8" ht="15" outlineLevel="1">
       <c r="A109" s="157"/>
       <c r="B109" s="152" t="s">
-        <v>256</v>
+        <v>249</v>
       </c>
       <c r="C109" s="101"/>
       <c r="D109" s="101">
-        <v>56314</v>
+        <v>55956</v>
       </c>
       <c r="E109" s="123">
         <f t="shared" si="6"/>
@@ -4278,110 +4300,110 @@
       </c>
       <c r="F109" s="105"/>
     </row>
-    <row r="110" spans="1:8" ht="15.75" outlineLevel="1" thickBot="1">
+    <row r="110" spans="1:8" ht="15" outlineLevel="1">
       <c r="A110" s="157"/>
-      <c r="B110" s="98" t="s">
+      <c r="B110" s="152" t="s">
+        <v>256</v>
+      </c>
+      <c r="C110" s="101"/>
+      <c r="D110" s="101">
+        <v>56314</v>
+      </c>
+      <c r="E110" s="123">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="F110" s="105"/>
+    </row>
+    <row r="111" spans="1:8" ht="15.75" outlineLevel="1" thickBot="1">
+      <c r="A111" s="157"/>
+      <c r="B111" s="98" t="s">
         <v>179</v>
       </c>
-      <c r="C110" s="99"/>
-      <c r="D110" s="99">
+      <c r="C111" s="99"/>
+      <c r="D111" s="99">
         <v>56373</v>
       </c>
-      <c r="E110" s="125">
+      <c r="E111" s="125">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="F110" s="104"/>
-    </row>
-    <row r="111" spans="1:8" ht="17.25" thickTop="1" thickBot="1">
-      <c r="A111" s="117" t="s">
+      <c r="F111" s="104"/>
+    </row>
+    <row r="112" spans="1:8" ht="17.25" thickTop="1" thickBot="1">
+      <c r="A112" s="117" t="s">
         <v>253</v>
       </c>
-      <c r="B111" s="102" t="s">
+      <c r="B112" s="102" t="s">
         <v>173</v>
       </c>
-      <c r="C111" s="103">
-        <f>C110-C101</f>
-        <v>0</v>
-      </c>
-      <c r="D111" s="103">
-        <f>D110-D101</f>
+      <c r="C112" s="103">
+        <f>C111-C102</f>
+        <v>0</v>
+      </c>
+      <c r="D112" s="103">
+        <f>D111-D102</f>
         <v>5799</v>
       </c>
-      <c r="E111" s="126">
-        <f>E110-E101</f>
-        <v>0</v>
-      </c>
-      <c r="F111" s="108"/>
-      <c r="G111" s="112">
-        <f>E111</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="112" spans="1:8" ht="13.5" thickBot="1"/>
-    <row r="113" spans="1:9" ht="15" customHeight="1" outlineLevel="1">
-      <c r="A113" s="156" t="s">
+      <c r="E112" s="126">
+        <f>E111-E102</f>
+        <v>0</v>
+      </c>
+      <c r="F112" s="108"/>
+      <c r="G112" s="112">
+        <f>E112</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="1:9" ht="13.5" thickBot="1"/>
+    <row r="114" spans="1:9" ht="15" customHeight="1" outlineLevel="1">
+      <c r="A114" s="156" t="s">
         <v>257</v>
       </c>
-      <c r="B113" s="113" t="s">
+      <c r="B114" s="113" t="s">
         <v>175</v>
       </c>
-      <c r="C113" s="114" t="s">
+      <c r="C114" s="114" t="s">
         <v>42</v>
       </c>
-      <c r="D113" s="114" t="s">
+      <c r="D114" s="114" t="s">
         <v>41</v>
       </c>
-      <c r="E113" s="114" t="s">
+      <c r="E114" s="114" t="s">
         <v>43</v>
       </c>
-      <c r="F113" s="115" t="s">
+      <c r="F114" s="115" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="114" spans="1:9" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="A114" s="157"/>
-      <c r="B114" s="98" t="s">
+    <row r="115" spans="1:9" ht="15.75" outlineLevel="1" thickBot="1">
+      <c r="A115" s="157"/>
+      <c r="B115" s="98" t="s">
         <v>177</v>
       </c>
-      <c r="C114" s="99"/>
-      <c r="D114" s="99">
+      <c r="C115" s="99"/>
+      <c r="D115" s="99">
         <v>56373</v>
       </c>
-      <c r="E114" s="123">
-        <f t="shared" ref="E114:E122" si="7">IF(AND(C114&gt;0,D114&gt;0), D114-C114, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="F114" s="104"/>
-      <c r="H114">
+      <c r="E115" s="123">
+        <f t="shared" ref="E115:E123" si="7">IF(AND(C115&gt;0,D115&gt;0), D115-C115, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="F115" s="104"/>
+      <c r="H115">
         <v>125564</v>
       </c>
-      <c r="I114" s="112">
-        <f>H114-D114</f>
+      <c r="I115" s="112">
+        <f>H115-D115</f>
         <v>69191</v>
       </c>
     </row>
-    <row r="115" spans="1:9" ht="15.75" outlineLevel="1" thickTop="1">
-      <c r="A115" s="157"/>
-      <c r="B115" s="100"/>
-      <c r="C115" s="101"/>
-      <c r="D115" s="101"/>
-      <c r="E115" s="124">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="F115" s="105"/>
-    </row>
-    <row r="116" spans="1:9" ht="15" outlineLevel="1">
+    <row r="116" spans="1:9" ht="15.75" outlineLevel="1" thickTop="1">
       <c r="A116" s="157"/>
-      <c r="B116" s="152" t="s">
-        <v>221</v>
-      </c>
+      <c r="B116" s="100"/>
       <c r="C116" s="101"/>
-      <c r="D116" s="101">
-        <v>58041</v>
-      </c>
-      <c r="E116" s="123">
+      <c r="D116" s="101"/>
+      <c r="E116" s="124">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -4389,9 +4411,13 @@
     </row>
     <row r="117" spans="1:9" ht="15" outlineLevel="1">
       <c r="A117" s="157"/>
-      <c r="B117" s="100"/>
+      <c r="B117" s="152" t="s">
+        <v>221</v>
+      </c>
       <c r="C117" s="101"/>
-      <c r="D117" s="101"/>
+      <c r="D117" s="101">
+        <v>58041</v>
+      </c>
       <c r="E117" s="123">
         <f t="shared" si="7"/>
         <v>0</v>
@@ -4400,13 +4426,9 @@
     </row>
     <row r="118" spans="1:9" ht="15" outlineLevel="1">
       <c r="A118" s="157"/>
-      <c r="B118" s="152" t="s">
-        <v>222</v>
-      </c>
+      <c r="B118" s="100"/>
       <c r="C118" s="101"/>
-      <c r="D118" s="101">
-        <v>60301</v>
-      </c>
+      <c r="D118" s="101"/>
       <c r="E118" s="123">
         <f t="shared" si="7"/>
         <v>0</v>
@@ -4416,11 +4438,11 @@
     <row r="119" spans="1:9" ht="15" outlineLevel="1">
       <c r="A119" s="157"/>
       <c r="B119" s="152" t="s">
-        <v>249</v>
+        <v>222</v>
       </c>
       <c r="C119" s="101"/>
-      <c r="D119" s="153">
-        <v>60529</v>
+      <c r="D119" s="101">
+        <v>60301</v>
       </c>
       <c r="E119" s="123">
         <f t="shared" si="7"/>
@@ -4431,11 +4453,11 @@
     <row r="120" spans="1:9" ht="15" outlineLevel="1">
       <c r="A120" s="157"/>
       <c r="B120" s="152" t="s">
-        <v>259</v>
+        <v>249</v>
       </c>
       <c r="C120" s="101"/>
-      <c r="D120" s="101">
-        <v>61068</v>
+      <c r="D120" s="153">
+        <v>60529</v>
       </c>
       <c r="E120" s="123">
         <f t="shared" si="7"/>
@@ -4446,11 +4468,11 @@
     <row r="121" spans="1:9" ht="15" outlineLevel="1">
       <c r="A121" s="157"/>
       <c r="B121" s="152" t="s">
-        <v>224</v>
+        <v>259</v>
       </c>
       <c r="C121" s="101"/>
       <c r="D121" s="101">
-        <v>61391</v>
+        <v>61068</v>
       </c>
       <c r="E121" s="123">
         <f t="shared" si="7"/>
@@ -4458,106 +4480,110 @@
       </c>
       <c r="F121" s="105"/>
     </row>
-    <row r="122" spans="1:9" ht="15.75" outlineLevel="1" thickBot="1">
+    <row r="122" spans="1:9" ht="15" outlineLevel="1">
       <c r="A122" s="157"/>
-      <c r="B122" s="98" t="s">
+      <c r="B122" s="152" t="s">
+        <v>224</v>
+      </c>
+      <c r="C122" s="101"/>
+      <c r="D122" s="101">
+        <v>61391</v>
+      </c>
+      <c r="E122" s="123">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="F122" s="105"/>
+    </row>
+    <row r="123" spans="1:9" ht="15.75" outlineLevel="1" thickBot="1">
+      <c r="A123" s="157"/>
+      <c r="B123" s="98" t="s">
         <v>179</v>
       </c>
-      <c r="C122" s="99"/>
-      <c r="D122" s="99">
+      <c r="C123" s="99"/>
+      <c r="D123" s="99">
         <v>61438</v>
       </c>
-      <c r="E122" s="125">
+      <c r="E123" s="125">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="F122" s="104"/>
-    </row>
-    <row r="123" spans="1:9" ht="17.25" thickTop="1" thickBot="1">
-      <c r="A123" s="116" t="s">
+      <c r="F123" s="104"/>
+    </row>
+    <row r="124" spans="1:9" ht="17.25" thickTop="1" thickBot="1">
+      <c r="A124" s="116" t="s">
         <v>258</v>
       </c>
-      <c r="B123" s="102" t="s">
+      <c r="B124" s="102" t="s">
         <v>173</v>
       </c>
-      <c r="C123" s="103">
-        <f>C122-C114</f>
-        <v>0</v>
-      </c>
-      <c r="D123" s="103">
-        <f>D122-D114</f>
+      <c r="C124" s="103">
+        <f>C123-C115</f>
+        <v>0</v>
+      </c>
+      <c r="D124" s="103">
+        <f>D123-D115</f>
         <v>5065</v>
       </c>
-      <c r="E123" s="103">
-        <f>E122-E114</f>
-        <v>0</v>
-      </c>
-      <c r="F123" s="107"/>
-      <c r="G123" s="112">
-        <f>E123</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="124" spans="1:9" ht="13.5" thickBot="1"/>
-    <row r="125" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A125" s="158" t="s">
+      <c r="E124" s="103">
+        <f>E123-E115</f>
+        <v>0</v>
+      </c>
+      <c r="F124" s="107"/>
+      <c r="G124" s="112">
+        <f>E124</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125" spans="1:9" ht="13.5" thickBot="1"/>
+    <row r="126" spans="1:9" ht="15" outlineLevel="1">
+      <c r="A126" s="158" t="s">
         <v>260</v>
       </c>
-      <c r="B125" s="109" t="s">
+      <c r="B126" s="109" t="s">
         <v>175</v>
       </c>
-      <c r="C125" s="110" t="s">
+      <c r="C126" s="110" t="s">
         <v>42</v>
       </c>
-      <c r="D125" s="110" t="s">
+      <c r="D126" s="110" t="s">
         <v>41</v>
       </c>
-      <c r="E125" s="110" t="s">
+      <c r="E126" s="110" t="s">
         <v>43</v>
       </c>
-      <c r="F125" s="111" t="s">
+      <c r="F126" s="111" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="126" spans="1:9" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="A126" s="157"/>
-      <c r="B126" s="98" t="s">
+    <row r="127" spans="1:9" ht="15.75" outlineLevel="1" thickBot="1">
+      <c r="A127" s="157"/>
+      <c r="B127" s="98" t="s">
         <v>177</v>
       </c>
-      <c r="C126" s="99"/>
-      <c r="D126" s="99">
+      <c r="C127" s="99"/>
+      <c r="D127" s="99">
         <v>61438</v>
       </c>
-      <c r="E126" s="123">
-        <f t="shared" ref="E126:E139" si="8">IF(AND(C126&gt;0,D126&gt;0), D126-C126, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="F126" s="104"/>
-      <c r="H126">
+      <c r="E127" s="123">
+        <f t="shared" ref="E127:E140" si="8">IF(AND(C127&gt;0,D127&gt;0), D127-C127, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="F127" s="104"/>
+      <c r="H127">
         <v>135506</v>
       </c>
-      <c r="I126" s="112">
-        <f>H126-D126</f>
+      <c r="I127" s="112">
+        <f>H127-D127</f>
         <v>74068</v>
       </c>
     </row>
-    <row r="127" spans="1:9" ht="15.75" outlineLevel="1" thickTop="1">
-      <c r="A127" s="157"/>
-      <c r="B127" s="100"/>
-      <c r="C127" s="101"/>
-      <c r="D127" s="101"/>
-      <c r="E127" s="124">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="F127" s="105"/>
-    </row>
-    <row r="128" spans="1:9" ht="15" outlineLevel="1">
+    <row r="128" spans="1:9" ht="15.75" outlineLevel="1" thickTop="1">
       <c r="A128" s="157"/>
       <c r="B128" s="100"/>
       <c r="C128" s="101"/>
       <c r="D128" s="101"/>
-      <c r="E128" s="123">
+      <c r="E128" s="124">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
@@ -4631,36 +4657,36 @@
     </row>
     <row r="135" spans="1:9" ht="15" outlineLevel="1">
       <c r="A135" s="157"/>
-      <c r="B135" s="152" t="s">
-        <v>262</v>
-      </c>
+      <c r="B135" s="100"/>
       <c r="C135" s="101"/>
-      <c r="D135" s="101">
-        <v>66926</v>
-      </c>
+      <c r="D135" s="101"/>
       <c r="E135" s="123">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="F135" s="105"/>
-      <c r="H135">
-        <v>160118</v>
-      </c>
-      <c r="I135" s="112">
-        <f>H135-D135</f>
-        <v>93192</v>
-      </c>
     </row>
     <row r="136" spans="1:9" ht="15" outlineLevel="1">
       <c r="A136" s="157"/>
-      <c r="B136" s="100"/>
+      <c r="B136" s="152" t="s">
+        <v>262</v>
+      </c>
       <c r="C136" s="101"/>
-      <c r="D136" s="101"/>
+      <c r="D136" s="101">
+        <v>66926</v>
+      </c>
       <c r="E136" s="123">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="F136" s="105"/>
+      <c r="H136">
+        <v>160118</v>
+      </c>
+      <c r="I136" s="112">
+        <f>H136-D136</f>
+        <v>93192</v>
+      </c>
     </row>
     <row r="137" spans="1:9" ht="15" outlineLevel="1">
       <c r="A137" s="157"/>
@@ -4684,94 +4710,94 @@
       </c>
       <c r="F138" s="105"/>
     </row>
-    <row r="139" spans="1:9" ht="15.75" outlineLevel="1" thickBot="1">
+    <row r="139" spans="1:9" ht="15" outlineLevel="1">
       <c r="A139" s="157"/>
-      <c r="B139" s="98" t="s">
+      <c r="B139" s="100"/>
+      <c r="C139" s="101"/>
+      <c r="D139" s="101"/>
+      <c r="E139" s="123">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="F139" s="105"/>
+    </row>
+    <row r="140" spans="1:9" ht="15.75" outlineLevel="1" thickBot="1">
+      <c r="A140" s="157"/>
+      <c r="B140" s="98" t="s">
         <v>179</v>
       </c>
-      <c r="C139" s="99"/>
-      <c r="D139" s="99"/>
-      <c r="E139" s="125">
+      <c r="C140" s="99"/>
+      <c r="D140" s="99"/>
+      <c r="E140" s="125">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="F139" s="104"/>
-    </row>
-    <row r="140" spans="1:9" ht="17.25" thickTop="1" thickBot="1">
-      <c r="A140" s="117" t="s">
+      <c r="F140" s="104"/>
+    </row>
+    <row r="141" spans="1:9" ht="17.25" thickTop="1" thickBot="1">
+      <c r="A141" s="117" t="s">
         <v>261</v>
       </c>
-      <c r="B140" s="102" t="s">
+      <c r="B141" s="102" t="s">
         <v>173</v>
       </c>
-      <c r="C140" s="103">
-        <f>C139-C126</f>
-        <v>0</v>
-      </c>
-      <c r="D140" s="103">
-        <f>D139-D126</f>
+      <c r="C141" s="103">
+        <f>C140-C127</f>
+        <v>0</v>
+      </c>
+      <c r="D141" s="103">
+        <f>D140-D127</f>
         <v>-61438</v>
       </c>
-      <c r="E140" s="103">
-        <f>E139-E126</f>
-        <v>0</v>
-      </c>
-      <c r="F140" s="108"/>
-      <c r="G140" s="112">
-        <f>E140</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="142" spans="1:9" ht="15" hidden="1" outlineLevel="2">
-      <c r="A142" s="156" t="s">
+      <c r="E141" s="103">
+        <f>E140-E127</f>
+        <v>0</v>
+      </c>
+      <c r="F141" s="108"/>
+      <c r="G141" s="112">
+        <f>E141</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="143" spans="1:9" ht="15" hidden="1" outlineLevel="2">
+      <c r="A143" s="156" t="s">
         <v>169</v>
       </c>
-      <c r="B142" s="113" t="s">
+      <c r="B143" s="113" t="s">
         <v>175</v>
       </c>
-      <c r="C142" s="114" t="s">
+      <c r="C143" s="114" t="s">
         <v>42</v>
       </c>
-      <c r="D142" s="114" t="s">
+      <c r="D143" s="114" t="s">
         <v>41</v>
       </c>
-      <c r="E142" s="114" t="s">
+      <c r="E143" s="114" t="s">
         <v>43</v>
       </c>
-      <c r="F142" s="115" t="s">
+      <c r="F143" s="115" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="143" spans="1:9" ht="15.75" hidden="1" outlineLevel="2" thickBot="1">
-      <c r="A143" s="157"/>
-      <c r="B143" s="98" t="s">
+    <row r="144" spans="1:9" ht="15.75" hidden="1" outlineLevel="2" thickBot="1">
+      <c r="A144" s="157"/>
+      <c r="B144" s="98" t="s">
         <v>177</v>
       </c>
-      <c r="C143" s="99"/>
-      <c r="D143" s="99"/>
-      <c r="E143" s="123">
-        <f t="shared" ref="E143:E156" si="9">IF(AND(C143&gt;0,D143&gt;0), D143-C143, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="F143" s="104"/>
-    </row>
-    <row r="144" spans="1:9" ht="15.75" hidden="1" outlineLevel="2" thickTop="1">
-      <c r="A144" s="157"/>
-      <c r="B144" s="100"/>
-      <c r="C144" s="101"/>
-      <c r="D144" s="101"/>
-      <c r="E144" s="124">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="F144" s="105"/>
-    </row>
-    <row r="145" spans="1:7" ht="15" hidden="1" outlineLevel="2">
+      <c r="C144" s="99"/>
+      <c r="D144" s="99"/>
+      <c r="E144" s="123">
+        <f t="shared" ref="E144:E157" si="9">IF(AND(C144&gt;0,D144&gt;0), D144-C144, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="F144" s="104"/>
+    </row>
+    <row r="145" spans="1:7" ht="15.75" hidden="1" outlineLevel="2" thickTop="1">
       <c r="A145" s="157"/>
       <c r="B145" s="100"/>
       <c r="C145" s="101"/>
       <c r="D145" s="101"/>
-      <c r="E145" s="123">
+      <c r="E145" s="124">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
@@ -4887,48 +4913,64 @@
       </c>
       <c r="F155" s="105"/>
     </row>
-    <row r="156" spans="1:7" ht="15.75" hidden="1" outlineLevel="2" thickBot="1">
+    <row r="156" spans="1:7" ht="15" hidden="1" outlineLevel="2">
       <c r="A156" s="157"/>
-      <c r="B156" s="98" t="s">
+      <c r="B156" s="100"/>
+      <c r="C156" s="101"/>
+      <c r="D156" s="101"/>
+      <c r="E156" s="123">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="F156" s="105"/>
+    </row>
+    <row r="157" spans="1:7" ht="15.75" hidden="1" outlineLevel="2" thickBot="1">
+      <c r="A157" s="157"/>
+      <c r="B157" s="98" t="s">
         <v>179</v>
       </c>
-      <c r="C156" s="99"/>
-      <c r="D156" s="99"/>
-      <c r="E156" s="125">
+      <c r="C157" s="99"/>
+      <c r="D157" s="99"/>
+      <c r="E157" s="125">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="F156" s="104"/>
-    </row>
-    <row r="157" spans="1:7" ht="16.5" collapsed="1" thickBot="1">
-      <c r="A157" s="116">
+      <c r="F157" s="104"/>
+    </row>
+    <row r="158" spans="1:7" ht="16.5" collapsed="1" thickBot="1">
+      <c r="A158" s="116">
         <v>8</v>
       </c>
-      <c r="B157" s="102" t="s">
+      <c r="B158" s="102" t="s">
         <v>173</v>
       </c>
-      <c r="C157" s="103">
-        <f>C156-C143</f>
-        <v>0</v>
-      </c>
-      <c r="D157" s="103">
-        <f>D156-D143</f>
-        <v>0</v>
-      </c>
-      <c r="E157" s="103">
-        <f>E156-E143</f>
-        <v>0</v>
-      </c>
-      <c r="F157" s="107"/>
-      <c r="G157" s="112">
-        <f>E157</f>
+      <c r="C158" s="103">
+        <f>C157-C144</f>
+        <v>0</v>
+      </c>
+      <c r="D158" s="103">
+        <f>D157-D144</f>
+        <v>0</v>
+      </c>
+      <c r="E158" s="103">
+        <f>E157-E144</f>
+        <v>0</v>
+      </c>
+      <c r="F158" s="107"/>
+      <c r="G158" s="112">
+        <f>E158</f>
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="A43:A64"/>
-    <mergeCell ref="A67:A80"/>
+    <mergeCell ref="A143:A157"/>
+    <mergeCell ref="A114:A123"/>
+    <mergeCell ref="A84:A98"/>
+    <mergeCell ref="A126:A140"/>
+    <mergeCell ref="A101:A111"/>
+    <mergeCell ref="A43:A65"/>
+    <mergeCell ref="A68:A81"/>
     <mergeCell ref="C5:D5"/>
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="A1:B1"/>
@@ -4936,11 +4978,6 @@
     <mergeCell ref="A8:A18"/>
     <mergeCell ref="A21:A40"/>
     <mergeCell ref="C4:E4"/>
-    <mergeCell ref="A142:A156"/>
-    <mergeCell ref="A113:A122"/>
-    <mergeCell ref="A83:A97"/>
-    <mergeCell ref="A125:A139"/>
-    <mergeCell ref="A100:A110"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4972,13 +5009,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="26.25" customHeight="1">
-      <c r="A1" s="184" t="s">
+      <c r="A1" s="166" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="184"/>
-      <c r="C1" s="184"/>
-      <c r="D1" s="184"/>
-      <c r="E1" s="184"/>
+      <c r="B1" s="166"/>
+      <c r="C1" s="166"/>
+      <c r="D1" s="166"/>
+      <c r="E1" s="166"/>
       <c r="F1" s="7"/>
       <c r="G1" s="5"/>
       <c r="H1" s="5"/>
@@ -5008,18 +5045,18 @@
         <v>8</v>
       </c>
       <c r="B3" s="36"/>
-      <c r="C3" s="185"/>
-      <c r="D3" s="186"/>
-      <c r="E3" s="186"/>
+      <c r="C3" s="167"/>
+      <c r="D3" s="168"/>
+      <c r="E3" s="168"/>
     </row>
     <row r="4" spans="1:8" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A4" s="46" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="87"/>
-      <c r="C4" s="166"/>
-      <c r="D4" s="167"/>
-      <c r="E4" s="167"/>
+      <c r="C4" s="169"/>
+      <c r="D4" s="170"/>
+      <c r="E4" s="170"/>
       <c r="F4" s="6"/>
     </row>
     <row r="5" spans="1:8" hidden="1" outlineLevel="2">
@@ -5171,9 +5208,9 @@
         <v>9</v>
       </c>
       <c r="B21" s="90"/>
-      <c r="C21" s="168"/>
-      <c r="D21" s="169"/>
-      <c r="E21" s="169"/>
+      <c r="C21" s="171"/>
+      <c r="D21" s="172"/>
+      <c r="E21" s="172"/>
     </row>
     <row r="22" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A22" s="47">
@@ -5324,9 +5361,9 @@
         <v>10</v>
       </c>
       <c r="B38" s="87"/>
-      <c r="C38" s="166"/>
-      <c r="D38" s="167"/>
-      <c r="E38" s="167"/>
+      <c r="C38" s="169"/>
+      <c r="D38" s="170"/>
+      <c r="E38" s="170"/>
     </row>
     <row r="39" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A39" s="47">
@@ -5477,9 +5514,9 @@
         <v>11</v>
       </c>
       <c r="B55" s="87"/>
-      <c r="C55" s="166"/>
-      <c r="D55" s="167"/>
-      <c r="E55" s="167"/>
+      <c r="C55" s="169"/>
+      <c r="D55" s="170"/>
+      <c r="E55" s="170"/>
     </row>
     <row r="56" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A56" s="47">
@@ -5630,9 +5667,9 @@
         <v>12</v>
       </c>
       <c r="B72" s="87"/>
-      <c r="C72" s="166"/>
-      <c r="D72" s="167"/>
-      <c r="E72" s="167"/>
+      <c r="C72" s="169"/>
+      <c r="D72" s="170"/>
+      <c r="E72" s="170"/>
     </row>
     <row r="73" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A73" s="47">
@@ -5783,9 +5820,9 @@
         <v>13</v>
       </c>
       <c r="B89" s="87"/>
-      <c r="C89" s="166"/>
-      <c r="D89" s="167"/>
-      <c r="E89" s="167"/>
+      <c r="C89" s="169"/>
+      <c r="D89" s="170"/>
+      <c r="E89" s="170"/>
     </row>
     <row r="90" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A90" s="47">
@@ -5936,9 +5973,9 @@
         <v>14</v>
       </c>
       <c r="B106" s="87"/>
-      <c r="C106" s="166"/>
-      <c r="D106" s="167"/>
-      <c r="E106" s="167"/>
+      <c r="C106" s="169"/>
+      <c r="D106" s="170"/>
+      <c r="E106" s="170"/>
     </row>
     <row r="107" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A107" s="47">
@@ -6089,9 +6126,9 @@
         <v>15</v>
       </c>
       <c r="B123" s="87"/>
-      <c r="C123" s="166"/>
-      <c r="D123" s="167"/>
-      <c r="E123" s="167"/>
+      <c r="C123" s="169"/>
+      <c r="D123" s="170"/>
+      <c r="E123" s="170"/>
     </row>
     <row r="124" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A124" s="47">
@@ -6242,9 +6279,9 @@
         <v>16</v>
       </c>
       <c r="B140" s="87"/>
-      <c r="C140" s="166"/>
-      <c r="D140" s="167"/>
-      <c r="E140" s="167"/>
+      <c r="C140" s="169"/>
+      <c r="D140" s="170"/>
+      <c r="E140" s="170"/>
     </row>
     <row r="141" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A141" s="47">
@@ -6395,9 +6432,9 @@
         <v>17</v>
       </c>
       <c r="B157" s="87"/>
-      <c r="C157" s="166"/>
-      <c r="D157" s="167"/>
-      <c r="E157" s="167"/>
+      <c r="C157" s="169"/>
+      <c r="D157" s="170"/>
+      <c r="E157" s="170"/>
     </row>
     <row r="158" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A158" s="47">
@@ -6548,9 +6585,9 @@
         <v>18</v>
       </c>
       <c r="B174" s="87"/>
-      <c r="C174" s="166"/>
-      <c r="D174" s="167"/>
-      <c r="E174" s="167"/>
+      <c r="C174" s="169"/>
+      <c r="D174" s="170"/>
+      <c r="E174" s="170"/>
     </row>
     <row r="175" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A175" s="47">
@@ -6701,9 +6738,9 @@
         <v>19</v>
       </c>
       <c r="B191" s="87"/>
-      <c r="C191" s="166"/>
-      <c r="D191" s="167"/>
-      <c r="E191" s="167"/>
+      <c r="C191" s="169"/>
+      <c r="D191" s="170"/>
+      <c r="E191" s="170"/>
     </row>
     <row r="192" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A192" s="47">
@@ -6854,9 +6891,9 @@
         <v>20</v>
       </c>
       <c r="B208" s="87"/>
-      <c r="C208" s="166"/>
-      <c r="D208" s="167"/>
-      <c r="E208" s="167"/>
+      <c r="C208" s="169"/>
+      <c r="D208" s="170"/>
+      <c r="E208" s="170"/>
     </row>
     <row r="209" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A209" s="47">
@@ -7007,9 +7044,9 @@
         <v>21</v>
       </c>
       <c r="B225" s="87"/>
-      <c r="C225" s="166"/>
-      <c r="D225" s="167"/>
-      <c r="E225" s="167"/>
+      <c r="C225" s="169"/>
+      <c r="D225" s="170"/>
+      <c r="E225" s="170"/>
     </row>
     <row r="226" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A226" s="47">
@@ -7160,9 +7197,9 @@
         <v>22</v>
       </c>
       <c r="B242" s="87"/>
-      <c r="C242" s="166"/>
-      <c r="D242" s="167"/>
-      <c r="E242" s="167"/>
+      <c r="C242" s="169"/>
+      <c r="D242" s="170"/>
+      <c r="E242" s="170"/>
     </row>
     <row r="243" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A243" s="47">
@@ -7313,9 +7350,9 @@
         <v>23</v>
       </c>
       <c r="B259" s="87"/>
-      <c r="C259" s="166"/>
-      <c r="D259" s="167"/>
-      <c r="E259" s="167"/>
+      <c r="C259" s="169"/>
+      <c r="D259" s="170"/>
+      <c r="E259" s="170"/>
     </row>
     <row r="260" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A260" s="47">
@@ -7466,18 +7503,18 @@
         <v>24</v>
       </c>
       <c r="B276" s="37"/>
-      <c r="C276" s="182"/>
-      <c r="D276" s="183"/>
-      <c r="E276" s="183"/>
+      <c r="C276" s="173"/>
+      <c r="D276" s="174"/>
+      <c r="E276" s="174"/>
     </row>
     <row r="277" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A277" s="51" t="s">
         <v>25</v>
       </c>
       <c r="B277" s="87"/>
-      <c r="C277" s="166"/>
-      <c r="D277" s="167"/>
-      <c r="E277" s="167"/>
+      <c r="C277" s="169"/>
+      <c r="D277" s="170"/>
+      <c r="E277" s="170"/>
     </row>
     <row r="278" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A278" s="52">
@@ -7628,9 +7665,9 @@
         <v>26</v>
       </c>
       <c r="B294" s="90"/>
-      <c r="C294" s="168"/>
-      <c r="D294" s="169"/>
-      <c r="E294" s="169"/>
+      <c r="C294" s="171"/>
+      <c r="D294" s="172"/>
+      <c r="E294" s="172"/>
     </row>
     <row r="295" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A295" s="52">
@@ -7781,9 +7818,9 @@
         <v>27</v>
       </c>
       <c r="B311" s="87"/>
-      <c r="C311" s="166"/>
-      <c r="D311" s="167"/>
-      <c r="E311" s="167"/>
+      <c r="C311" s="169"/>
+      <c r="D311" s="170"/>
+      <c r="E311" s="170"/>
     </row>
     <row r="312" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A312" s="52">
@@ -7934,9 +7971,9 @@
         <v>28</v>
       </c>
       <c r="B328" s="87"/>
-      <c r="C328" s="166"/>
-      <c r="D328" s="167"/>
-      <c r="E328" s="167"/>
+      <c r="C328" s="169"/>
+      <c r="D328" s="170"/>
+      <c r="E328" s="170"/>
     </row>
     <row r="329" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A329" s="52">
@@ -8087,9 +8124,9 @@
         <v>29</v>
       </c>
       <c r="B345" s="87"/>
-      <c r="C345" s="166"/>
-      <c r="D345" s="167"/>
-      <c r="E345" s="167"/>
+      <c r="C345" s="169"/>
+      <c r="D345" s="170"/>
+      <c r="E345" s="170"/>
     </row>
     <row r="346" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A346" s="52">
@@ -8240,9 +8277,9 @@
         <v>30</v>
       </c>
       <c r="B362" s="87"/>
-      <c r="C362" s="166"/>
-      <c r="D362" s="167"/>
-      <c r="E362" s="167"/>
+      <c r="C362" s="169"/>
+      <c r="D362" s="170"/>
+      <c r="E362" s="170"/>
     </row>
     <row r="363" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A363" s="52">
@@ -8393,9 +8430,9 @@
         <v>31</v>
       </c>
       <c r="B379" s="87"/>
-      <c r="C379" s="166"/>
-      <c r="D379" s="167"/>
-      <c r="E379" s="167"/>
+      <c r="C379" s="169"/>
+      <c r="D379" s="170"/>
+      <c r="E379" s="170"/>
     </row>
     <row r="380" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A380" s="52">
@@ -8546,9 +8583,9 @@
         <v>32</v>
       </c>
       <c r="B396" s="87"/>
-      <c r="C396" s="166"/>
-      <c r="D396" s="167"/>
-      <c r="E396" s="167"/>
+      <c r="C396" s="169"/>
+      <c r="D396" s="170"/>
+      <c r="E396" s="170"/>
     </row>
     <row r="397" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A397" s="52">
@@ -8699,9 +8736,9 @@
         <v>33</v>
       </c>
       <c r="B413" s="87"/>
-      <c r="C413" s="166"/>
-      <c r="D413" s="167"/>
-      <c r="E413" s="167"/>
+      <c r="C413" s="169"/>
+      <c r="D413" s="170"/>
+      <c r="E413" s="170"/>
     </row>
     <row r="414" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A414" s="52">
@@ -8852,9 +8889,9 @@
         <v>34</v>
       </c>
       <c r="B430" s="87"/>
-      <c r="C430" s="166"/>
-      <c r="D430" s="167"/>
-      <c r="E430" s="167"/>
+      <c r="C430" s="169"/>
+      <c r="D430" s="170"/>
+      <c r="E430" s="170"/>
     </row>
     <row r="431" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A431" s="52">
@@ -9005,9 +9042,9 @@
         <v>35</v>
       </c>
       <c r="B447" s="87"/>
-      <c r="C447" s="166"/>
-      <c r="D447" s="167"/>
-      <c r="E447" s="167"/>
+      <c r="C447" s="169"/>
+      <c r="D447" s="170"/>
+      <c r="E447" s="170"/>
     </row>
     <row r="448" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A448" s="52">
@@ -9158,9 +9195,9 @@
         <v>36</v>
       </c>
       <c r="B464" s="87"/>
-      <c r="C464" s="166"/>
-      <c r="D464" s="167"/>
-      <c r="E464" s="167"/>
+      <c r="C464" s="169"/>
+      <c r="D464" s="170"/>
+      <c r="E464" s="170"/>
     </row>
     <row r="465" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A465" s="52">
@@ -9311,9 +9348,9 @@
         <v>37</v>
       </c>
       <c r="B481" s="87"/>
-      <c r="C481" s="166"/>
-      <c r="D481" s="167"/>
-      <c r="E481" s="167"/>
+      <c r="C481" s="169"/>
+      <c r="D481" s="170"/>
+      <c r="E481" s="170"/>
     </row>
     <row r="482" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A482" s="52">
@@ -9464,9 +9501,9 @@
         <v>38</v>
       </c>
       <c r="B498" s="87"/>
-      <c r="C498" s="166"/>
-      <c r="D498" s="167"/>
-      <c r="E498" s="167"/>
+      <c r="C498" s="169"/>
+      <c r="D498" s="170"/>
+      <c r="E498" s="170"/>
     </row>
     <row r="499" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A499" s="52">
@@ -9617,9 +9654,9 @@
         <v>39</v>
       </c>
       <c r="B515" s="87"/>
-      <c r="C515" s="166"/>
-      <c r="D515" s="167"/>
-      <c r="E515" s="167"/>
+      <c r="C515" s="169"/>
+      <c r="D515" s="170"/>
+      <c r="E515" s="170"/>
     </row>
     <row r="516" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A516" s="52">
@@ -9770,9 +9807,9 @@
         <v>40</v>
       </c>
       <c r="B532" s="87"/>
-      <c r="C532" s="166"/>
-      <c r="D532" s="167"/>
-      <c r="E532" s="167"/>
+      <c r="C532" s="169"/>
+      <c r="D532" s="170"/>
+      <c r="E532" s="170"/>
     </row>
     <row r="533" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A533" s="55">
@@ -9923,18 +9960,18 @@
         <v>50</v>
       </c>
       <c r="B549" s="38"/>
-      <c r="C549" s="180"/>
-      <c r="D549" s="181"/>
-      <c r="E549" s="181"/>
+      <c r="C549" s="175"/>
+      <c r="D549" s="176"/>
+      <c r="E549" s="176"/>
     </row>
     <row r="550" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A550" s="58" t="s">
         <v>51</v>
       </c>
       <c r="B550" s="87"/>
-      <c r="C550" s="166"/>
-      <c r="D550" s="167"/>
-      <c r="E550" s="167"/>
+      <c r="C550" s="169"/>
+      <c r="D550" s="170"/>
+      <c r="E550" s="170"/>
     </row>
     <row r="551" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A551" s="59">
@@ -10085,9 +10122,9 @@
         <v>52</v>
       </c>
       <c r="B567" s="90"/>
-      <c r="C567" s="168"/>
-      <c r="D567" s="169"/>
-      <c r="E567" s="169"/>
+      <c r="C567" s="171"/>
+      <c r="D567" s="172"/>
+      <c r="E567" s="172"/>
     </row>
     <row r="568" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A568" s="59">
@@ -10238,9 +10275,9 @@
         <v>53</v>
       </c>
       <c r="B584" s="87"/>
-      <c r="C584" s="166"/>
-      <c r="D584" s="167"/>
-      <c r="E584" s="167"/>
+      <c r="C584" s="169"/>
+      <c r="D584" s="170"/>
+      <c r="E584" s="170"/>
     </row>
     <row r="585" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A585" s="59">
@@ -10391,9 +10428,9 @@
         <v>54</v>
       </c>
       <c r="B601" s="87"/>
-      <c r="C601" s="166"/>
-      <c r="D601" s="167"/>
-      <c r="E601" s="167"/>
+      <c r="C601" s="169"/>
+      <c r="D601" s="170"/>
+      <c r="E601" s="170"/>
     </row>
     <row r="602" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A602" s="59">
@@ -10544,9 +10581,9 @@
         <v>55</v>
       </c>
       <c r="B618" s="87"/>
-      <c r="C618" s="166"/>
-      <c r="D618" s="167"/>
-      <c r="E618" s="167"/>
+      <c r="C618" s="169"/>
+      <c r="D618" s="170"/>
+      <c r="E618" s="170"/>
     </row>
     <row r="619" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A619" s="59">
@@ -10697,9 +10734,9 @@
         <v>56</v>
       </c>
       <c r="B635" s="87"/>
-      <c r="C635" s="166"/>
-      <c r="D635" s="167"/>
-      <c r="E635" s="167"/>
+      <c r="C635" s="169"/>
+      <c r="D635" s="170"/>
+      <c r="E635" s="170"/>
     </row>
     <row r="636" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A636" s="59">
@@ -10850,9 +10887,9 @@
         <v>57</v>
       </c>
       <c r="B652" s="87"/>
-      <c r="C652" s="166"/>
-      <c r="D652" s="167"/>
-      <c r="E652" s="167"/>
+      <c r="C652" s="169"/>
+      <c r="D652" s="170"/>
+      <c r="E652" s="170"/>
     </row>
     <row r="653" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A653" s="59">
@@ -11003,9 +11040,9 @@
         <v>58</v>
       </c>
       <c r="B669" s="87"/>
-      <c r="C669" s="166"/>
-      <c r="D669" s="167"/>
-      <c r="E669" s="167"/>
+      <c r="C669" s="169"/>
+      <c r="D669" s="170"/>
+      <c r="E669" s="170"/>
     </row>
     <row r="670" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A670" s="59">
@@ -11156,9 +11193,9 @@
         <v>59</v>
       </c>
       <c r="B686" s="87"/>
-      <c r="C686" s="166"/>
-      <c r="D686" s="167"/>
-      <c r="E686" s="167"/>
+      <c r="C686" s="169"/>
+      <c r="D686" s="170"/>
+      <c r="E686" s="170"/>
     </row>
     <row r="687" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A687" s="59">
@@ -11309,9 +11346,9 @@
         <v>60</v>
       </c>
       <c r="B703" s="87"/>
-      <c r="C703" s="166"/>
-      <c r="D703" s="167"/>
-      <c r="E703" s="167"/>
+      <c r="C703" s="169"/>
+      <c r="D703" s="170"/>
+      <c r="E703" s="170"/>
     </row>
     <row r="704" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A704" s="59">
@@ -11462,9 +11499,9 @@
         <v>61</v>
       </c>
       <c r="B720" s="87"/>
-      <c r="C720" s="166"/>
-      <c r="D720" s="167"/>
-      <c r="E720" s="167"/>
+      <c r="C720" s="169"/>
+      <c r="D720" s="170"/>
+      <c r="E720" s="170"/>
     </row>
     <row r="721" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A721" s="59">
@@ -11615,9 +11652,9 @@
         <v>62</v>
       </c>
       <c r="B737" s="87"/>
-      <c r="C737" s="166"/>
-      <c r="D737" s="167"/>
-      <c r="E737" s="167"/>
+      <c r="C737" s="169"/>
+      <c r="D737" s="170"/>
+      <c r="E737" s="170"/>
     </row>
     <row r="738" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A738" s="59">
@@ -11768,9 +11805,9 @@
         <v>63</v>
       </c>
       <c r="B754" s="87"/>
-      <c r="C754" s="166"/>
-      <c r="D754" s="167"/>
-      <c r="E754" s="167"/>
+      <c r="C754" s="169"/>
+      <c r="D754" s="170"/>
+      <c r="E754" s="170"/>
     </row>
     <row r="755" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A755" s="59">
@@ -11921,9 +11958,9 @@
         <v>64</v>
       </c>
       <c r="B771" s="87"/>
-      <c r="C771" s="166"/>
-      <c r="D771" s="167"/>
-      <c r="E771" s="167"/>
+      <c r="C771" s="169"/>
+      <c r="D771" s="170"/>
+      <c r="E771" s="170"/>
     </row>
     <row r="772" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A772" s="59">
@@ -12074,9 +12111,9 @@
         <v>65</v>
       </c>
       <c r="B788" s="87"/>
-      <c r="C788" s="166"/>
-      <c r="D788" s="167"/>
-      <c r="E788" s="167"/>
+      <c r="C788" s="169"/>
+      <c r="D788" s="170"/>
+      <c r="E788" s="170"/>
     </row>
     <row r="789" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A789" s="59">
@@ -12227,9 +12264,9 @@
         <v>66</v>
       </c>
       <c r="B805" s="87"/>
-      <c r="C805" s="166"/>
-      <c r="D805" s="167"/>
-      <c r="E805" s="167"/>
+      <c r="C805" s="169"/>
+      <c r="D805" s="170"/>
+      <c r="E805" s="170"/>
     </row>
     <row r="806" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A806" s="59">
@@ -12380,18 +12417,18 @@
         <v>67</v>
       </c>
       <c r="B822" s="39"/>
-      <c r="C822" s="178"/>
-      <c r="D822" s="179"/>
-      <c r="E822" s="179"/>
+      <c r="C822" s="177"/>
+      <c r="D822" s="178"/>
+      <c r="E822" s="178"/>
     </row>
     <row r="823" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A823" s="63" t="s">
         <v>68</v>
       </c>
       <c r="B823" s="87"/>
-      <c r="C823" s="166"/>
-      <c r="D823" s="167"/>
-      <c r="E823" s="167"/>
+      <c r="C823" s="169"/>
+      <c r="D823" s="170"/>
+      <c r="E823" s="170"/>
     </row>
     <row r="824" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A824" s="64">
@@ -12542,9 +12579,9 @@
         <v>69</v>
       </c>
       <c r="B840" s="90"/>
-      <c r="C840" s="168"/>
-      <c r="D840" s="169"/>
-      <c r="E840" s="169"/>
+      <c r="C840" s="171"/>
+      <c r="D840" s="172"/>
+      <c r="E840" s="172"/>
     </row>
     <row r="841" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A841" s="64">
@@ -12695,9 +12732,9 @@
         <v>70</v>
       </c>
       <c r="B857" s="87"/>
-      <c r="C857" s="166"/>
-      <c r="D857" s="167"/>
-      <c r="E857" s="167"/>
+      <c r="C857" s="169"/>
+      <c r="D857" s="170"/>
+      <c r="E857" s="170"/>
     </row>
     <row r="858" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A858" s="64">
@@ -12848,9 +12885,9 @@
         <v>71</v>
       </c>
       <c r="B874" s="87"/>
-      <c r="C874" s="166"/>
-      <c r="D874" s="167"/>
-      <c r="E874" s="167"/>
+      <c r="C874" s="169"/>
+      <c r="D874" s="170"/>
+      <c r="E874" s="170"/>
     </row>
     <row r="875" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A875" s="64">
@@ -13001,9 +13038,9 @@
         <v>72</v>
       </c>
       <c r="B891" s="87"/>
-      <c r="C891" s="166"/>
-      <c r="D891" s="167"/>
-      <c r="E891" s="167"/>
+      <c r="C891" s="169"/>
+      <c r="D891" s="170"/>
+      <c r="E891" s="170"/>
     </row>
     <row r="892" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A892" s="64">
@@ -13154,9 +13191,9 @@
         <v>73</v>
       </c>
       <c r="B908" s="87"/>
-      <c r="C908" s="166"/>
-      <c r="D908" s="167"/>
-      <c r="E908" s="167"/>
+      <c r="C908" s="169"/>
+      <c r="D908" s="170"/>
+      <c r="E908" s="170"/>
     </row>
     <row r="909" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A909" s="64">
@@ -13307,9 +13344,9 @@
         <v>74</v>
       </c>
       <c r="B925" s="87"/>
-      <c r="C925" s="166"/>
-      <c r="D925" s="167"/>
-      <c r="E925" s="167"/>
+      <c r="C925" s="169"/>
+      <c r="D925" s="170"/>
+      <c r="E925" s="170"/>
     </row>
     <row r="926" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A926" s="64">
@@ -13460,9 +13497,9 @@
         <v>75</v>
       </c>
       <c r="B942" s="87"/>
-      <c r="C942" s="166"/>
-      <c r="D942" s="167"/>
-      <c r="E942" s="167"/>
+      <c r="C942" s="169"/>
+      <c r="D942" s="170"/>
+      <c r="E942" s="170"/>
     </row>
     <row r="943" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A943" s="64">
@@ -13613,9 +13650,9 @@
         <v>76</v>
       </c>
       <c r="B959" s="87"/>
-      <c r="C959" s="166"/>
-      <c r="D959" s="167"/>
-      <c r="E959" s="167"/>
+      <c r="C959" s="169"/>
+      <c r="D959" s="170"/>
+      <c r="E959" s="170"/>
     </row>
     <row r="960" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A960" s="64">
@@ -13766,9 +13803,9 @@
         <v>77</v>
       </c>
       <c r="B976" s="87"/>
-      <c r="C976" s="166"/>
-      <c r="D976" s="167"/>
-      <c r="E976" s="167"/>
+      <c r="C976" s="169"/>
+      <c r="D976" s="170"/>
+      <c r="E976" s="170"/>
     </row>
     <row r="977" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A977" s="64">
@@ -13919,9 +13956,9 @@
         <v>78</v>
       </c>
       <c r="B993" s="87"/>
-      <c r="C993" s="166"/>
-      <c r="D993" s="167"/>
-      <c r="E993" s="167"/>
+      <c r="C993" s="169"/>
+      <c r="D993" s="170"/>
+      <c r="E993" s="170"/>
     </row>
     <row r="994" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A994" s="64">
@@ -14072,9 +14109,9 @@
         <v>79</v>
       </c>
       <c r="B1010" s="87"/>
-      <c r="C1010" s="166"/>
-      <c r="D1010" s="167"/>
-      <c r="E1010" s="167"/>
+      <c r="C1010" s="169"/>
+      <c r="D1010" s="170"/>
+      <c r="E1010" s="170"/>
     </row>
     <row r="1011" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1011" s="64">
@@ -14225,9 +14262,9 @@
         <v>80</v>
       </c>
       <c r="B1027" s="87"/>
-      <c r="C1027" s="166"/>
-      <c r="D1027" s="167"/>
-      <c r="E1027" s="167"/>
+      <c r="C1027" s="169"/>
+      <c r="D1027" s="170"/>
+      <c r="E1027" s="170"/>
     </row>
     <row r="1028" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1028" s="64">
@@ -14378,9 +14415,9 @@
         <v>83</v>
       </c>
       <c r="B1044" s="87"/>
-      <c r="C1044" s="166"/>
-      <c r="D1044" s="167"/>
-      <c r="E1044" s="167"/>
+      <c r="C1044" s="169"/>
+      <c r="D1044" s="170"/>
+      <c r="E1044" s="170"/>
     </row>
     <row r="1045" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1045" s="64">
@@ -14531,9 +14568,9 @@
         <v>82</v>
       </c>
       <c r="B1061" s="87"/>
-      <c r="C1061" s="166"/>
-      <c r="D1061" s="167"/>
-      <c r="E1061" s="167"/>
+      <c r="C1061" s="169"/>
+      <c r="D1061" s="170"/>
+      <c r="E1061" s="170"/>
     </row>
     <row r="1062" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1062" s="64">
@@ -14684,9 +14721,9 @@
         <v>84</v>
       </c>
       <c r="B1078" s="87"/>
-      <c r="C1078" s="166"/>
-      <c r="D1078" s="167"/>
-      <c r="E1078" s="167"/>
+      <c r="C1078" s="169"/>
+      <c r="D1078" s="170"/>
+      <c r="E1078" s="170"/>
     </row>
     <row r="1079" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1079" s="64">
@@ -14837,18 +14874,18 @@
         <v>104</v>
       </c>
       <c r="B1095" s="40"/>
-      <c r="C1095" s="176"/>
-      <c r="D1095" s="177"/>
-      <c r="E1095" s="177"/>
+      <c r="C1095" s="179"/>
+      <c r="D1095" s="180"/>
+      <c r="E1095" s="180"/>
     </row>
     <row r="1096" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A1096" s="68" t="s">
         <v>85</v>
       </c>
       <c r="B1096" s="87"/>
-      <c r="C1096" s="166"/>
-      <c r="D1096" s="167"/>
-      <c r="E1096" s="167"/>
+      <c r="C1096" s="169"/>
+      <c r="D1096" s="170"/>
+      <c r="E1096" s="170"/>
     </row>
     <row r="1097" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1097" s="69">
@@ -14999,9 +15036,9 @@
         <v>86</v>
       </c>
       <c r="B1113" s="90"/>
-      <c r="C1113" s="168"/>
-      <c r="D1113" s="169"/>
-      <c r="E1113" s="169"/>
+      <c r="C1113" s="171"/>
+      <c r="D1113" s="172"/>
+      <c r="E1113" s="172"/>
     </row>
     <row r="1114" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1114" s="69">
@@ -15152,9 +15189,9 @@
         <v>87</v>
       </c>
       <c r="B1130" s="87"/>
-      <c r="C1130" s="166"/>
-      <c r="D1130" s="167"/>
-      <c r="E1130" s="167"/>
+      <c r="C1130" s="169"/>
+      <c r="D1130" s="170"/>
+      <c r="E1130" s="170"/>
     </row>
     <row r="1131" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1131" s="69">
@@ -15305,9 +15342,9 @@
         <v>88</v>
       </c>
       <c r="B1147" s="87"/>
-      <c r="C1147" s="166"/>
-      <c r="D1147" s="167"/>
-      <c r="E1147" s="167"/>
+      <c r="C1147" s="169"/>
+      <c r="D1147" s="170"/>
+      <c r="E1147" s="170"/>
     </row>
     <row r="1148" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1148" s="69">
@@ -15458,9 +15495,9 @@
         <v>89</v>
       </c>
       <c r="B1164" s="87"/>
-      <c r="C1164" s="166"/>
-      <c r="D1164" s="167"/>
-      <c r="E1164" s="167"/>
+      <c r="C1164" s="169"/>
+      <c r="D1164" s="170"/>
+      <c r="E1164" s="170"/>
     </row>
     <row r="1165" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1165" s="69">
@@ -15611,9 +15648,9 @@
         <v>90</v>
       </c>
       <c r="B1181" s="87"/>
-      <c r="C1181" s="166"/>
-      <c r="D1181" s="167"/>
-      <c r="E1181" s="167"/>
+      <c r="C1181" s="169"/>
+      <c r="D1181" s="170"/>
+      <c r="E1181" s="170"/>
     </row>
     <row r="1182" spans="1:5" hidden="1" outlineLevel="3">
       <c r="A1182" s="69">
@@ -15764,9 +15801,9 @@
         <v>91</v>
       </c>
       <c r="B1198" s="87"/>
-      <c r="C1198" s="166"/>
-      <c r="D1198" s="167"/>
-      <c r="E1198" s="167"/>
+      <c r="C1198" s="169"/>
+      <c r="D1198" s="170"/>
+      <c r="E1198" s="170"/>
     </row>
     <row r="1199" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1199" s="69">
@@ -15917,9 +15954,9 @@
         <v>92</v>
       </c>
       <c r="B1215" s="87"/>
-      <c r="C1215" s="166"/>
-      <c r="D1215" s="167"/>
-      <c r="E1215" s="167"/>
+      <c r="C1215" s="169"/>
+      <c r="D1215" s="170"/>
+      <c r="E1215" s="170"/>
     </row>
     <row r="1216" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1216" s="69">
@@ -16070,9 +16107,9 @@
         <v>93</v>
       </c>
       <c r="B1232" s="87"/>
-      <c r="C1232" s="166"/>
-      <c r="D1232" s="167"/>
-      <c r="E1232" s="167"/>
+      <c r="C1232" s="169"/>
+      <c r="D1232" s="170"/>
+      <c r="E1232" s="170"/>
     </row>
     <row r="1233" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1233" s="69">
@@ -16223,9 +16260,9 @@
         <v>94</v>
       </c>
       <c r="B1249" s="87"/>
-      <c r="C1249" s="166"/>
-      <c r="D1249" s="167"/>
-      <c r="E1249" s="167"/>
+      <c r="C1249" s="169"/>
+      <c r="D1249" s="170"/>
+      <c r="E1249" s="170"/>
     </row>
     <row r="1250" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1250" s="69">
@@ -16376,9 +16413,9 @@
         <v>99</v>
       </c>
       <c r="B1266" s="87"/>
-      <c r="C1266" s="166"/>
-      <c r="D1266" s="167"/>
-      <c r="E1266" s="167"/>
+      <c r="C1266" s="169"/>
+      <c r="D1266" s="170"/>
+      <c r="E1266" s="170"/>
     </row>
     <row r="1267" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1267" s="69">
@@ -16529,9 +16566,9 @@
         <v>100</v>
       </c>
       <c r="B1283" s="87"/>
-      <c r="C1283" s="166"/>
-      <c r="D1283" s="167"/>
-      <c r="E1283" s="167"/>
+      <c r="C1283" s="169"/>
+      <c r="D1283" s="170"/>
+      <c r="E1283" s="170"/>
     </row>
     <row r="1284" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1284" s="69">
@@ -16682,9 +16719,9 @@
         <v>101</v>
       </c>
       <c r="B1300" s="87"/>
-      <c r="C1300" s="166"/>
-      <c r="D1300" s="167"/>
-      <c r="E1300" s="167"/>
+      <c r="C1300" s="169"/>
+      <c r="D1300" s="170"/>
+      <c r="E1300" s="170"/>
     </row>
     <row r="1301" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1301" s="69">
@@ -16835,9 +16872,9 @@
         <v>81</v>
       </c>
       <c r="B1317" s="87"/>
-      <c r="C1317" s="166"/>
-      <c r="D1317" s="167"/>
-      <c r="E1317" s="167"/>
+      <c r="C1317" s="169"/>
+      <c r="D1317" s="170"/>
+      <c r="E1317" s="170"/>
     </row>
     <row r="1318" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1318" s="69">
@@ -16988,9 +17025,9 @@
         <v>102</v>
       </c>
       <c r="B1334" s="87"/>
-      <c r="C1334" s="166"/>
-      <c r="D1334" s="167"/>
-      <c r="E1334" s="167"/>
+      <c r="C1334" s="169"/>
+      <c r="D1334" s="170"/>
+      <c r="E1334" s="170"/>
     </row>
     <row r="1335" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1335" s="69">
@@ -17141,9 +17178,9 @@
         <v>98</v>
       </c>
       <c r="B1351" s="87"/>
-      <c r="C1351" s="166"/>
-      <c r="D1351" s="167"/>
-      <c r="E1351" s="167"/>
+      <c r="C1351" s="169"/>
+      <c r="D1351" s="170"/>
+      <c r="E1351" s="170"/>
     </row>
     <row r="1352" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1352" s="69">
@@ -17294,18 +17331,18 @@
         <v>103</v>
       </c>
       <c r="B1368" s="41"/>
-      <c r="C1368" s="174"/>
-      <c r="D1368" s="175"/>
-      <c r="E1368" s="175"/>
+      <c r="C1368" s="181"/>
+      <c r="D1368" s="182"/>
+      <c r="E1368" s="182"/>
     </row>
     <row r="1369" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A1369" s="73" t="s">
         <v>105</v>
       </c>
       <c r="B1369" s="87"/>
-      <c r="C1369" s="166"/>
-      <c r="D1369" s="167"/>
-      <c r="E1369" s="167"/>
+      <c r="C1369" s="169"/>
+      <c r="D1369" s="170"/>
+      <c r="E1369" s="170"/>
     </row>
     <row r="1370" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1370" s="74">
@@ -17456,9 +17493,9 @@
         <v>106</v>
       </c>
       <c r="B1386" s="90"/>
-      <c r="C1386" s="168"/>
-      <c r="D1386" s="169"/>
-      <c r="E1386" s="169"/>
+      <c r="C1386" s="171"/>
+      <c r="D1386" s="172"/>
+      <c r="E1386" s="172"/>
     </row>
     <row r="1387" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1387" s="74">
@@ -17609,9 +17646,9 @@
         <v>107</v>
       </c>
       <c r="B1403" s="87"/>
-      <c r="C1403" s="166"/>
-      <c r="D1403" s="167"/>
-      <c r="E1403" s="167"/>
+      <c r="C1403" s="169"/>
+      <c r="D1403" s="170"/>
+      <c r="E1403" s="170"/>
     </row>
     <row r="1404" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1404" s="74">
@@ -17762,9 +17799,9 @@
         <v>108</v>
       </c>
       <c r="B1420" s="87"/>
-      <c r="C1420" s="166"/>
-      <c r="D1420" s="167"/>
-      <c r="E1420" s="167"/>
+      <c r="C1420" s="169"/>
+      <c r="D1420" s="170"/>
+      <c r="E1420" s="170"/>
     </row>
     <row r="1421" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1421" s="74">
@@ -17915,9 +17952,9 @@
         <v>109</v>
       </c>
       <c r="B1437" s="87"/>
-      <c r="C1437" s="166"/>
-      <c r="D1437" s="167"/>
-      <c r="E1437" s="167"/>
+      <c r="C1437" s="169"/>
+      <c r="D1437" s="170"/>
+      <c r="E1437" s="170"/>
     </row>
     <row r="1438" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1438" s="74">
@@ -18068,9 +18105,9 @@
         <v>110</v>
       </c>
       <c r="B1454" s="87"/>
-      <c r="C1454" s="166"/>
-      <c r="D1454" s="167"/>
-      <c r="E1454" s="167"/>
+      <c r="C1454" s="169"/>
+      <c r="D1454" s="170"/>
+      <c r="E1454" s="170"/>
     </row>
     <row r="1455" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1455" s="74">
@@ -18221,9 +18258,9 @@
         <v>111</v>
       </c>
       <c r="B1471" s="87"/>
-      <c r="C1471" s="166"/>
-      <c r="D1471" s="167"/>
-      <c r="E1471" s="167"/>
+      <c r="C1471" s="169"/>
+      <c r="D1471" s="170"/>
+      <c r="E1471" s="170"/>
     </row>
     <row r="1472" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1472" s="74">
@@ -18374,9 +18411,9 @@
         <v>112</v>
       </c>
       <c r="B1488" s="87"/>
-      <c r="C1488" s="166"/>
-      <c r="D1488" s="167"/>
-      <c r="E1488" s="167"/>
+      <c r="C1488" s="169"/>
+      <c r="D1488" s="170"/>
+      <c r="E1488" s="170"/>
     </row>
     <row r="1489" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1489" s="74">
@@ -18527,9 +18564,9 @@
         <v>113</v>
       </c>
       <c r="B1505" s="87"/>
-      <c r="C1505" s="166"/>
-      <c r="D1505" s="167"/>
-      <c r="E1505" s="167"/>
+      <c r="C1505" s="169"/>
+      <c r="D1505" s="170"/>
+      <c r="E1505" s="170"/>
     </row>
     <row r="1506" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1506" s="74">
@@ -18680,9 +18717,9 @@
         <v>114</v>
       </c>
       <c r="B1522" s="87"/>
-      <c r="C1522" s="166"/>
-      <c r="D1522" s="167"/>
-      <c r="E1522" s="167"/>
+      <c r="C1522" s="169"/>
+      <c r="D1522" s="170"/>
+      <c r="E1522" s="170"/>
     </row>
     <row r="1523" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1523" s="74">
@@ -18833,9 +18870,9 @@
         <v>95</v>
       </c>
       <c r="B1539" s="87"/>
-      <c r="C1539" s="166"/>
-      <c r="D1539" s="167"/>
-      <c r="E1539" s="167"/>
+      <c r="C1539" s="169"/>
+      <c r="D1539" s="170"/>
+      <c r="E1539" s="170"/>
     </row>
     <row r="1540" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1540" s="74">
@@ -18986,9 +19023,9 @@
         <v>115</v>
       </c>
       <c r="B1556" s="87"/>
-      <c r="C1556" s="166"/>
-      <c r="D1556" s="167"/>
-      <c r="E1556" s="167"/>
+      <c r="C1556" s="169"/>
+      <c r="D1556" s="170"/>
+      <c r="E1556" s="170"/>
     </row>
     <row r="1557" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1557" s="74">
@@ -19139,9 +19176,9 @@
         <v>116</v>
       </c>
       <c r="B1573" s="87"/>
-      <c r="C1573" s="166"/>
-      <c r="D1573" s="167"/>
-      <c r="E1573" s="167"/>
+      <c r="C1573" s="169"/>
+      <c r="D1573" s="170"/>
+      <c r="E1573" s="170"/>
     </row>
     <row r="1574" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1574" s="74">
@@ -19292,9 +19329,9 @@
         <v>117</v>
       </c>
       <c r="B1590" s="87"/>
-      <c r="C1590" s="166"/>
-      <c r="D1590" s="167"/>
-      <c r="E1590" s="167"/>
+      <c r="C1590" s="169"/>
+      <c r="D1590" s="170"/>
+      <c r="E1590" s="170"/>
     </row>
     <row r="1591" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1591" s="74">
@@ -19445,9 +19482,9 @@
         <v>118</v>
       </c>
       <c r="B1607" s="87"/>
-      <c r="C1607" s="166"/>
-      <c r="D1607" s="167"/>
-      <c r="E1607" s="167"/>
+      <c r="C1607" s="169"/>
+      <c r="D1607" s="170"/>
+      <c r="E1607" s="170"/>
     </row>
     <row r="1608" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1608" s="74">
@@ -19598,9 +19635,9 @@
         <v>119</v>
       </c>
       <c r="B1624" s="87"/>
-      <c r="C1624" s="166"/>
-      <c r="D1624" s="167"/>
-      <c r="E1624" s="167"/>
+      <c r="C1624" s="169"/>
+      <c r="D1624" s="170"/>
+      <c r="E1624" s="170"/>
     </row>
     <row r="1625" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1625" s="74">
@@ -19751,18 +19788,18 @@
         <v>120</v>
       </c>
       <c r="B1641" s="42"/>
-      <c r="C1641" s="172"/>
-      <c r="D1641" s="173"/>
-      <c r="E1641" s="173"/>
+      <c r="C1641" s="183"/>
+      <c r="D1641" s="184"/>
+      <c r="E1641" s="184"/>
     </row>
     <row r="1642" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A1642" s="78" t="s">
         <v>121</v>
       </c>
       <c r="B1642" s="87"/>
-      <c r="C1642" s="166"/>
-      <c r="D1642" s="167"/>
-      <c r="E1642" s="167"/>
+      <c r="C1642" s="169"/>
+      <c r="D1642" s="170"/>
+      <c r="E1642" s="170"/>
     </row>
     <row r="1643" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1643" s="79">
@@ -19913,9 +19950,9 @@
         <v>122</v>
       </c>
       <c r="B1659" s="90"/>
-      <c r="C1659" s="168"/>
-      <c r="D1659" s="169"/>
-      <c r="E1659" s="169"/>
+      <c r="C1659" s="171"/>
+      <c r="D1659" s="172"/>
+      <c r="E1659" s="172"/>
     </row>
     <row r="1660" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1660" s="79">
@@ -20066,9 +20103,9 @@
         <v>123</v>
       </c>
       <c r="B1676" s="87"/>
-      <c r="C1676" s="166"/>
-      <c r="D1676" s="167"/>
-      <c r="E1676" s="167"/>
+      <c r="C1676" s="169"/>
+      <c r="D1676" s="170"/>
+      <c r="E1676" s="170"/>
     </row>
     <row r="1677" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1677" s="79">
@@ -20219,9 +20256,9 @@
         <v>124</v>
       </c>
       <c r="B1693" s="87"/>
-      <c r="C1693" s="166"/>
-      <c r="D1693" s="167"/>
-      <c r="E1693" s="167"/>
+      <c r="C1693" s="169"/>
+      <c r="D1693" s="170"/>
+      <c r="E1693" s="170"/>
     </row>
     <row r="1694" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1694" s="79">
@@ -20372,9 +20409,9 @@
         <v>125</v>
       </c>
       <c r="B1710" s="87"/>
-      <c r="C1710" s="166"/>
-      <c r="D1710" s="167"/>
-      <c r="E1710" s="167"/>
+      <c r="C1710" s="169"/>
+      <c r="D1710" s="170"/>
+      <c r="E1710" s="170"/>
     </row>
     <row r="1711" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1711" s="79">
@@ -20525,9 +20562,9 @@
         <v>126</v>
       </c>
       <c r="B1727" s="87"/>
-      <c r="C1727" s="166"/>
-      <c r="D1727" s="167"/>
-      <c r="E1727" s="167"/>
+      <c r="C1727" s="169"/>
+      <c r="D1727" s="170"/>
+      <c r="E1727" s="170"/>
     </row>
     <row r="1728" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1728" s="79">
@@ -20678,9 +20715,9 @@
         <v>127</v>
       </c>
       <c r="B1744" s="87"/>
-      <c r="C1744" s="166"/>
-      <c r="D1744" s="167"/>
-      <c r="E1744" s="167"/>
+      <c r="C1744" s="169"/>
+      <c r="D1744" s="170"/>
+      <c r="E1744" s="170"/>
     </row>
     <row r="1745" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1745" s="79">
@@ -20831,9 +20868,9 @@
         <v>128</v>
       </c>
       <c r="B1761" s="87"/>
-      <c r="C1761" s="166"/>
-      <c r="D1761" s="167"/>
-      <c r="E1761" s="167"/>
+      <c r="C1761" s="169"/>
+      <c r="D1761" s="170"/>
+      <c r="E1761" s="170"/>
     </row>
     <row r="1762" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1762" s="79">
@@ -20984,9 +21021,9 @@
         <v>129</v>
       </c>
       <c r="B1778" s="87"/>
-      <c r="C1778" s="166"/>
-      <c r="D1778" s="167"/>
-      <c r="E1778" s="167"/>
+      <c r="C1778" s="169"/>
+      <c r="D1778" s="170"/>
+      <c r="E1778" s="170"/>
     </row>
     <row r="1779" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1779" s="79">
@@ -21137,9 +21174,9 @@
         <v>130</v>
       </c>
       <c r="B1795" s="87"/>
-      <c r="C1795" s="166"/>
-      <c r="D1795" s="167"/>
-      <c r="E1795" s="167"/>
+      <c r="C1795" s="169"/>
+      <c r="D1795" s="170"/>
+      <c r="E1795" s="170"/>
     </row>
     <row r="1796" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1796" s="79">
@@ -21290,9 +21327,9 @@
         <v>131</v>
       </c>
       <c r="B1812" s="87"/>
-      <c r="C1812" s="166"/>
-      <c r="D1812" s="167"/>
-      <c r="E1812" s="167"/>
+      <c r="C1812" s="169"/>
+      <c r="D1812" s="170"/>
+      <c r="E1812" s="170"/>
     </row>
     <row r="1813" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1813" s="79">
@@ -21443,9 +21480,9 @@
         <v>96</v>
       </c>
       <c r="B1829" s="87"/>
-      <c r="C1829" s="166"/>
-      <c r="D1829" s="167"/>
-      <c r="E1829" s="167"/>
+      <c r="C1829" s="169"/>
+      <c r="D1829" s="170"/>
+      <c r="E1829" s="170"/>
     </row>
     <row r="1830" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1830" s="79">
@@ -21596,9 +21633,9 @@
         <v>132</v>
       </c>
       <c r="B1846" s="87"/>
-      <c r="C1846" s="166"/>
-      <c r="D1846" s="167"/>
-      <c r="E1846" s="167"/>
+      <c r="C1846" s="169"/>
+      <c r="D1846" s="170"/>
+      <c r="E1846" s="170"/>
     </row>
     <row r="1847" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1847" s="79">
@@ -21749,9 +21786,9 @@
         <v>133</v>
       </c>
       <c r="B1863" s="87"/>
-      <c r="C1863" s="166"/>
-      <c r="D1863" s="167"/>
-      <c r="E1863" s="167"/>
+      <c r="C1863" s="169"/>
+      <c r="D1863" s="170"/>
+      <c r="E1863" s="170"/>
     </row>
     <row r="1864" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1864" s="79">
@@ -21902,9 +21939,9 @@
         <v>134</v>
       </c>
       <c r="B1880" s="87"/>
-      <c r="C1880" s="166"/>
-      <c r="D1880" s="167"/>
-      <c r="E1880" s="167"/>
+      <c r="C1880" s="169"/>
+      <c r="D1880" s="170"/>
+      <c r="E1880" s="170"/>
     </row>
     <row r="1881" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1881" s="79">
@@ -22055,9 +22092,9 @@
         <v>135</v>
       </c>
       <c r="B1897" s="87"/>
-      <c r="C1897" s="166"/>
-      <c r="D1897" s="167"/>
-      <c r="E1897" s="167"/>
+      <c r="C1897" s="169"/>
+      <c r="D1897" s="170"/>
+      <c r="E1897" s="170"/>
     </row>
     <row r="1898" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1898" s="79">
@@ -22208,18 +22245,18 @@
         <v>136</v>
       </c>
       <c r="B1914" s="43"/>
-      <c r="C1914" s="170"/>
-      <c r="D1914" s="171"/>
-      <c r="E1914" s="171"/>
+      <c r="C1914" s="185"/>
+      <c r="D1914" s="186"/>
+      <c r="E1914" s="186"/>
     </row>
     <row r="1915" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A1915" s="83" t="s">
         <v>137</v>
       </c>
       <c r="B1915" s="87"/>
-      <c r="C1915" s="166"/>
-      <c r="D1915" s="167"/>
-      <c r="E1915" s="167"/>
+      <c r="C1915" s="169"/>
+      <c r="D1915" s="170"/>
+      <c r="E1915" s="170"/>
     </row>
     <row r="1916" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1916" s="84">
@@ -22370,9 +22407,9 @@
         <v>138</v>
       </c>
       <c r="B1932" s="90"/>
-      <c r="C1932" s="168"/>
-      <c r="D1932" s="169"/>
-      <c r="E1932" s="169"/>
+      <c r="C1932" s="171"/>
+      <c r="D1932" s="172"/>
+      <c r="E1932" s="172"/>
     </row>
     <row r="1933" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1933" s="84">
@@ -22523,9 +22560,9 @@
         <v>139</v>
       </c>
       <c r="B1949" s="87"/>
-      <c r="C1949" s="166"/>
-      <c r="D1949" s="167"/>
-      <c r="E1949" s="167"/>
+      <c r="C1949" s="169"/>
+      <c r="D1949" s="170"/>
+      <c r="E1949" s="170"/>
     </row>
     <row r="1950" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1950" s="84">
@@ -22676,9 +22713,9 @@
         <v>140</v>
       </c>
       <c r="B1966" s="87"/>
-      <c r="C1966" s="166"/>
-      <c r="D1966" s="167"/>
-      <c r="E1966" s="167"/>
+      <c r="C1966" s="169"/>
+      <c r="D1966" s="170"/>
+      <c r="E1966" s="170"/>
     </row>
     <row r="1967" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1967" s="84">
@@ -22829,9 +22866,9 @@
         <v>141</v>
       </c>
       <c r="B1983" s="87"/>
-      <c r="C1983" s="166"/>
-      <c r="D1983" s="167"/>
-      <c r="E1983" s="167"/>
+      <c r="C1983" s="169"/>
+      <c r="D1983" s="170"/>
+      <c r="E1983" s="170"/>
     </row>
     <row r="1984" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1984" s="84">
@@ -22982,9 +23019,9 @@
         <v>142</v>
       </c>
       <c r="B2000" s="87"/>
-      <c r="C2000" s="166"/>
-      <c r="D2000" s="167"/>
-      <c r="E2000" s="167"/>
+      <c r="C2000" s="169"/>
+      <c r="D2000" s="170"/>
+      <c r="E2000" s="170"/>
     </row>
     <row r="2001" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2001" s="84">
@@ -23135,9 +23172,9 @@
         <v>143</v>
       </c>
       <c r="B2017" s="87"/>
-      <c r="C2017" s="166"/>
-      <c r="D2017" s="167"/>
-      <c r="E2017" s="167"/>
+      <c r="C2017" s="169"/>
+      <c r="D2017" s="170"/>
+      <c r="E2017" s="170"/>
     </row>
     <row r="2018" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2018" s="84">
@@ -23288,9 +23325,9 @@
         <v>144</v>
       </c>
       <c r="B2034" s="87"/>
-      <c r="C2034" s="166"/>
-      <c r="D2034" s="167"/>
-      <c r="E2034" s="167"/>
+      <c r="C2034" s="169"/>
+      <c r="D2034" s="170"/>
+      <c r="E2034" s="170"/>
     </row>
     <row r="2035" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2035" s="84">
@@ -23441,9 +23478,9 @@
         <v>145</v>
       </c>
       <c r="B2051" s="87"/>
-      <c r="C2051" s="166"/>
-      <c r="D2051" s="167"/>
-      <c r="E2051" s="167"/>
+      <c r="C2051" s="169"/>
+      <c r="D2051" s="170"/>
+      <c r="E2051" s="170"/>
     </row>
     <row r="2052" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2052" s="84">
@@ -23594,9 +23631,9 @@
         <v>146</v>
       </c>
       <c r="B2068" s="87"/>
-      <c r="C2068" s="166"/>
-      <c r="D2068" s="167"/>
-      <c r="E2068" s="167"/>
+      <c r="C2068" s="169"/>
+      <c r="D2068" s="170"/>
+      <c r="E2068" s="170"/>
     </row>
     <row r="2069" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2069" s="84">
@@ -23747,9 +23784,9 @@
         <v>147</v>
       </c>
       <c r="B2085" s="87"/>
-      <c r="C2085" s="166"/>
-      <c r="D2085" s="167"/>
-      <c r="E2085" s="167"/>
+      <c r="C2085" s="169"/>
+      <c r="D2085" s="170"/>
+      <c r="E2085" s="170"/>
     </row>
     <row r="2086" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2086" s="84">
@@ -23900,9 +23937,9 @@
         <v>148</v>
       </c>
       <c r="B2102" s="87"/>
-      <c r="C2102" s="166"/>
-      <c r="D2102" s="167"/>
-      <c r="E2102" s="167"/>
+      <c r="C2102" s="169"/>
+      <c r="D2102" s="170"/>
+      <c r="E2102" s="170"/>
     </row>
     <row r="2103" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2103" s="84">
@@ -24053,9 +24090,9 @@
         <v>97</v>
       </c>
       <c r="B2119" s="87"/>
-      <c r="C2119" s="166"/>
-      <c r="D2119" s="167"/>
-      <c r="E2119" s="167"/>
+      <c r="C2119" s="169"/>
+      <c r="D2119" s="170"/>
+      <c r="E2119" s="170"/>
     </row>
     <row r="2120" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2120" s="84">
@@ -24206,9 +24243,9 @@
         <v>149</v>
       </c>
       <c r="B2136" s="87"/>
-      <c r="C2136" s="166"/>
-      <c r="D2136" s="167"/>
-      <c r="E2136" s="167"/>
+      <c r="C2136" s="169"/>
+      <c r="D2136" s="170"/>
+      <c r="E2136" s="170"/>
     </row>
     <row r="2137" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2137" s="84">
@@ -24359,9 +24396,9 @@
         <v>150</v>
       </c>
       <c r="B2153" s="87"/>
-      <c r="C2153" s="166"/>
-      <c r="D2153" s="167"/>
-      <c r="E2153" s="167"/>
+      <c r="C2153" s="169"/>
+      <c r="D2153" s="170"/>
+      <c r="E2153" s="170"/>
     </row>
     <row r="2154" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2154" s="84">
@@ -24512,9 +24549,9 @@
         <v>151</v>
       </c>
       <c r="B2170" s="87"/>
-      <c r="C2170" s="166"/>
-      <c r="D2170" s="167"/>
-      <c r="E2170" s="167"/>
+      <c r="C2170" s="169"/>
+      <c r="D2170" s="170"/>
+      <c r="E2170" s="170"/>
     </row>
     <row r="2171" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2171" s="84">
@@ -24662,26 +24699,111 @@
     </row>
   </sheetData>
   <mergeCells count="137">
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="C89:E89"/>
-    <mergeCell ref="C21:E21"/>
-    <mergeCell ref="C38:E38"/>
-    <mergeCell ref="C55:E55"/>
-    <mergeCell ref="C72:E72"/>
-    <mergeCell ref="C208:E208"/>
-    <mergeCell ref="C225:E225"/>
-    <mergeCell ref="C242:E242"/>
-    <mergeCell ref="C259:E259"/>
-    <mergeCell ref="C276:E276"/>
-    <mergeCell ref="C277:E277"/>
-    <mergeCell ref="C106:E106"/>
-    <mergeCell ref="C123:E123"/>
-    <mergeCell ref="C140:E140"/>
-    <mergeCell ref="C157:E157"/>
-    <mergeCell ref="C174:E174"/>
-    <mergeCell ref="C191:E191"/>
+    <mergeCell ref="C2034:E2034"/>
+    <mergeCell ref="C2051:E2051"/>
+    <mergeCell ref="C2068:E2068"/>
+    <mergeCell ref="C2085:E2085"/>
+    <mergeCell ref="C2170:E2170"/>
+    <mergeCell ref="C2102:E2102"/>
+    <mergeCell ref="C2119:E2119"/>
+    <mergeCell ref="C2136:E2136"/>
+    <mergeCell ref="C2153:E2153"/>
+    <mergeCell ref="C1932:E1932"/>
+    <mergeCell ref="C1949:E1949"/>
+    <mergeCell ref="C1966:E1966"/>
+    <mergeCell ref="C1983:E1983"/>
+    <mergeCell ref="C2000:E2000"/>
+    <mergeCell ref="C2017:E2017"/>
+    <mergeCell ref="C1846:E1846"/>
+    <mergeCell ref="C1863:E1863"/>
+    <mergeCell ref="C1880:E1880"/>
+    <mergeCell ref="C1897:E1897"/>
+    <mergeCell ref="C1914:E1914"/>
+    <mergeCell ref="C1915:E1915"/>
+    <mergeCell ref="C1744:E1744"/>
+    <mergeCell ref="C1761:E1761"/>
+    <mergeCell ref="C1778:E1778"/>
+    <mergeCell ref="C1795:E1795"/>
+    <mergeCell ref="C1812:E1812"/>
+    <mergeCell ref="C1829:E1829"/>
+    <mergeCell ref="C1642:E1642"/>
+    <mergeCell ref="C1659:E1659"/>
+    <mergeCell ref="C1676:E1676"/>
+    <mergeCell ref="C1693:E1693"/>
+    <mergeCell ref="C1710:E1710"/>
+    <mergeCell ref="C1727:E1727"/>
+    <mergeCell ref="C1556:E1556"/>
+    <mergeCell ref="C1573:E1573"/>
+    <mergeCell ref="C1590:E1590"/>
+    <mergeCell ref="C1607:E1607"/>
+    <mergeCell ref="C1624:E1624"/>
+    <mergeCell ref="C1641:E1641"/>
+    <mergeCell ref="C1454:E1454"/>
+    <mergeCell ref="C1471:E1471"/>
+    <mergeCell ref="C1488:E1488"/>
+    <mergeCell ref="C1505:E1505"/>
+    <mergeCell ref="C1522:E1522"/>
+    <mergeCell ref="C1539:E1539"/>
+    <mergeCell ref="C1368:E1368"/>
+    <mergeCell ref="C1369:E1369"/>
+    <mergeCell ref="C1386:E1386"/>
+    <mergeCell ref="C1403:E1403"/>
+    <mergeCell ref="C1420:E1420"/>
+    <mergeCell ref="C1437:E1437"/>
+    <mergeCell ref="C1266:E1266"/>
+    <mergeCell ref="C1283:E1283"/>
+    <mergeCell ref="C1300:E1300"/>
+    <mergeCell ref="C1317:E1317"/>
+    <mergeCell ref="C1334:E1334"/>
+    <mergeCell ref="C1351:E1351"/>
+    <mergeCell ref="C1164:E1164"/>
+    <mergeCell ref="C1181:E1181"/>
+    <mergeCell ref="C1198:E1198"/>
+    <mergeCell ref="C1215:E1215"/>
+    <mergeCell ref="C1232:E1232"/>
+    <mergeCell ref="C1249:E1249"/>
+    <mergeCell ref="C1078:E1078"/>
+    <mergeCell ref="C1095:E1095"/>
+    <mergeCell ref="C1096:E1096"/>
+    <mergeCell ref="C1113:E1113"/>
+    <mergeCell ref="C1130:E1130"/>
+    <mergeCell ref="C1147:E1147"/>
+    <mergeCell ref="C976:E976"/>
+    <mergeCell ref="C993:E993"/>
+    <mergeCell ref="C1010:E1010"/>
+    <mergeCell ref="C1027:E1027"/>
+    <mergeCell ref="C1044:E1044"/>
+    <mergeCell ref="C1061:E1061"/>
+    <mergeCell ref="C874:E874"/>
+    <mergeCell ref="C891:E891"/>
+    <mergeCell ref="C908:E908"/>
+    <mergeCell ref="C925:E925"/>
+    <mergeCell ref="C942:E942"/>
+    <mergeCell ref="C959:E959"/>
+    <mergeCell ref="C788:E788"/>
+    <mergeCell ref="C805:E805"/>
+    <mergeCell ref="C822:E822"/>
+    <mergeCell ref="C823:E823"/>
+    <mergeCell ref="C840:E840"/>
+    <mergeCell ref="C857:E857"/>
+    <mergeCell ref="C686:E686"/>
+    <mergeCell ref="C703:E703"/>
+    <mergeCell ref="C720:E720"/>
+    <mergeCell ref="C737:E737"/>
+    <mergeCell ref="C754:E754"/>
+    <mergeCell ref="C771:E771"/>
+    <mergeCell ref="C584:E584"/>
+    <mergeCell ref="C601:E601"/>
+    <mergeCell ref="C618:E618"/>
+    <mergeCell ref="C635:E635"/>
+    <mergeCell ref="C652:E652"/>
+    <mergeCell ref="C669:E669"/>
+    <mergeCell ref="C498:E498"/>
+    <mergeCell ref="C515:E515"/>
+    <mergeCell ref="C532:E532"/>
+    <mergeCell ref="C549:E549"/>
+    <mergeCell ref="C550:E550"/>
+    <mergeCell ref="C567:E567"/>
     <mergeCell ref="C396:E396"/>
     <mergeCell ref="C413:E413"/>
     <mergeCell ref="C430:E430"/>
@@ -24694,113 +24816,28 @@
     <mergeCell ref="C345:E345"/>
     <mergeCell ref="C362:E362"/>
     <mergeCell ref="C379:E379"/>
-    <mergeCell ref="C584:E584"/>
-    <mergeCell ref="C601:E601"/>
-    <mergeCell ref="C618:E618"/>
-    <mergeCell ref="C635:E635"/>
-    <mergeCell ref="C652:E652"/>
-    <mergeCell ref="C669:E669"/>
-    <mergeCell ref="C498:E498"/>
-    <mergeCell ref="C515:E515"/>
-    <mergeCell ref="C532:E532"/>
-    <mergeCell ref="C549:E549"/>
-    <mergeCell ref="C550:E550"/>
-    <mergeCell ref="C567:E567"/>
-    <mergeCell ref="C788:E788"/>
-    <mergeCell ref="C805:E805"/>
-    <mergeCell ref="C822:E822"/>
-    <mergeCell ref="C823:E823"/>
-    <mergeCell ref="C840:E840"/>
-    <mergeCell ref="C857:E857"/>
-    <mergeCell ref="C686:E686"/>
-    <mergeCell ref="C703:E703"/>
-    <mergeCell ref="C720:E720"/>
-    <mergeCell ref="C737:E737"/>
-    <mergeCell ref="C754:E754"/>
-    <mergeCell ref="C771:E771"/>
-    <mergeCell ref="C976:E976"/>
-    <mergeCell ref="C993:E993"/>
-    <mergeCell ref="C1010:E1010"/>
-    <mergeCell ref="C1027:E1027"/>
-    <mergeCell ref="C1044:E1044"/>
-    <mergeCell ref="C1061:E1061"/>
-    <mergeCell ref="C874:E874"/>
-    <mergeCell ref="C891:E891"/>
-    <mergeCell ref="C908:E908"/>
-    <mergeCell ref="C925:E925"/>
-    <mergeCell ref="C942:E942"/>
-    <mergeCell ref="C959:E959"/>
-    <mergeCell ref="C1164:E1164"/>
-    <mergeCell ref="C1181:E1181"/>
-    <mergeCell ref="C1198:E1198"/>
-    <mergeCell ref="C1215:E1215"/>
-    <mergeCell ref="C1232:E1232"/>
-    <mergeCell ref="C1249:E1249"/>
-    <mergeCell ref="C1078:E1078"/>
-    <mergeCell ref="C1095:E1095"/>
-    <mergeCell ref="C1096:E1096"/>
-    <mergeCell ref="C1113:E1113"/>
-    <mergeCell ref="C1130:E1130"/>
-    <mergeCell ref="C1147:E1147"/>
-    <mergeCell ref="C1368:E1368"/>
-    <mergeCell ref="C1369:E1369"/>
-    <mergeCell ref="C1386:E1386"/>
-    <mergeCell ref="C1403:E1403"/>
-    <mergeCell ref="C1420:E1420"/>
-    <mergeCell ref="C1437:E1437"/>
-    <mergeCell ref="C1266:E1266"/>
-    <mergeCell ref="C1283:E1283"/>
-    <mergeCell ref="C1300:E1300"/>
-    <mergeCell ref="C1317:E1317"/>
-    <mergeCell ref="C1334:E1334"/>
-    <mergeCell ref="C1351:E1351"/>
-    <mergeCell ref="C1556:E1556"/>
-    <mergeCell ref="C1573:E1573"/>
-    <mergeCell ref="C1590:E1590"/>
-    <mergeCell ref="C1607:E1607"/>
-    <mergeCell ref="C1624:E1624"/>
-    <mergeCell ref="C1641:E1641"/>
-    <mergeCell ref="C1454:E1454"/>
-    <mergeCell ref="C1471:E1471"/>
-    <mergeCell ref="C1488:E1488"/>
-    <mergeCell ref="C1505:E1505"/>
-    <mergeCell ref="C1522:E1522"/>
-    <mergeCell ref="C1539:E1539"/>
-    <mergeCell ref="C1744:E1744"/>
-    <mergeCell ref="C1761:E1761"/>
-    <mergeCell ref="C1778:E1778"/>
-    <mergeCell ref="C1795:E1795"/>
-    <mergeCell ref="C1812:E1812"/>
-    <mergeCell ref="C1829:E1829"/>
-    <mergeCell ref="C1642:E1642"/>
-    <mergeCell ref="C1659:E1659"/>
-    <mergeCell ref="C1676:E1676"/>
-    <mergeCell ref="C1693:E1693"/>
-    <mergeCell ref="C1710:E1710"/>
-    <mergeCell ref="C1727:E1727"/>
-    <mergeCell ref="C1932:E1932"/>
-    <mergeCell ref="C1949:E1949"/>
-    <mergeCell ref="C1966:E1966"/>
-    <mergeCell ref="C1983:E1983"/>
-    <mergeCell ref="C2000:E2000"/>
-    <mergeCell ref="C2017:E2017"/>
-    <mergeCell ref="C1846:E1846"/>
-    <mergeCell ref="C1863:E1863"/>
-    <mergeCell ref="C1880:E1880"/>
-    <mergeCell ref="C1897:E1897"/>
-    <mergeCell ref="C1914:E1914"/>
-    <mergeCell ref="C1915:E1915"/>
-    <mergeCell ref="C2034:E2034"/>
-    <mergeCell ref="C2051:E2051"/>
-    <mergeCell ref="C2068:E2068"/>
-    <mergeCell ref="C2085:E2085"/>
-    <mergeCell ref="C2170:E2170"/>
-    <mergeCell ref="C2102:E2102"/>
-    <mergeCell ref="C2119:E2119"/>
-    <mergeCell ref="C2136:E2136"/>
-    <mergeCell ref="C2153:E2153"/>
+    <mergeCell ref="C225:E225"/>
+    <mergeCell ref="C242:E242"/>
+    <mergeCell ref="C259:E259"/>
+    <mergeCell ref="C276:E276"/>
+    <mergeCell ref="C277:E277"/>
+    <mergeCell ref="C106:E106"/>
+    <mergeCell ref="C123:E123"/>
+    <mergeCell ref="C140:E140"/>
+    <mergeCell ref="C157:E157"/>
+    <mergeCell ref="C174:E174"/>
+    <mergeCell ref="C191:E191"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="C89:E89"/>
+    <mergeCell ref="C21:E21"/>
+    <mergeCell ref="C38:E38"/>
+    <mergeCell ref="C55:E55"/>
+    <mergeCell ref="C72:E72"/>
+    <mergeCell ref="C208:E208"/>
   </mergeCells>
-  <phoneticPr fontId="7" type="noConversion"/>
+  <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967294" verticalDpi="0" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
@@ -25551,7 +25588,7 @@
     <mergeCell ref="A3:K3"/>
     <mergeCell ref="A20:K20"/>
   </mergeCells>
-  <phoneticPr fontId="7" type="noConversion"/>
+  <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
@@ -25762,7 +25799,7 @@
   <mergeCells count="1">
     <mergeCell ref="A3:A10"/>
   </mergeCells>
-  <phoneticPr fontId="7" type="noConversion"/>
+  <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
@@ -26035,7 +26072,7 @@
     <mergeCell ref="A11:A17"/>
     <mergeCell ref="A19:A25"/>
   </mergeCells>
-  <phoneticPr fontId="7" type="noConversion"/>
+  <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
@@ -26057,163 +26094,150 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="33">
-      <c r="A1" s="211" t="s">
+      <c r="A1" s="212" t="s">
         <v>184</v>
       </c>
-      <c r="B1" s="212"/>
+      <c r="B1" s="213"/>
       <c r="C1" s="118"/>
       <c r="D1" s="5"/>
       <c r="E1" s="5"/>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="208" t="s">
+      <c r="A2" s="218" t="s">
         <v>183</v>
       </c>
-      <c r="B2" s="209"/>
+      <c r="B2" s="219"/>
       <c r="C2" s="120"/>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="210" t="s">
+      <c r="A3" s="220" t="s">
         <v>185</v>
       </c>
-      <c r="B3" s="209"/>
+      <c r="B3" s="219"/>
       <c r="C3" s="120"/>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="215"/>
-      <c r="B4" s="216"/>
+      <c r="A4" s="216"/>
+      <c r="B4" s="217"/>
       <c r="C4" s="120"/>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="213" t="s">
+      <c r="A5" s="214" t="s">
         <v>194</v>
       </c>
-      <c r="B5" s="214"/>
+      <c r="B5" s="215"/>
       <c r="C5" s="120"/>
     </row>
     <row r="7" spans="1:5" ht="18.75">
-      <c r="A7" s="219" t="s">
+      <c r="A7" s="206" t="s">
         <v>186</v>
       </c>
-      <c r="B7" s="220"/>
+      <c r="B7" s="207"/>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="120"/>
       <c r="B8" s="9"/>
     </row>
     <row r="9" spans="1:5" ht="39" customHeight="1">
-      <c r="A9" s="217" t="s">
+      <c r="A9" s="208" t="s">
         <v>187</v>
       </c>
-      <c r="B9" s="218"/>
+      <c r="B9" s="209"/>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="204"/>
-      <c r="B10" s="205"/>
+      <c r="A10" s="210"/>
+      <c r="B10" s="211"/>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="206" t="s">
+      <c r="A11" s="202" t="s">
         <v>188</v>
       </c>
-      <c r="B11" s="207"/>
+      <c r="B11" s="203"/>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="206" t="s">
+      <c r="A12" s="202" t="s">
         <v>189</v>
       </c>
-      <c r="B12" s="207"/>
+      <c r="B12" s="203"/>
     </row>
     <row r="13" spans="1:5" ht="43.5" customHeight="1">
-      <c r="A13" s="206" t="s">
+      <c r="A13" s="202" t="s">
         <v>190</v>
       </c>
-      <c r="B13" s="207"/>
+      <c r="B13" s="203"/>
     </row>
     <row r="14" spans="1:5" ht="19.5" customHeight="1">
-      <c r="A14" s="206" t="s">
+      <c r="A14" s="202" t="s">
         <v>191</v>
       </c>
-      <c r="B14" s="207"/>
+      <c r="B14" s="203"/>
     </row>
     <row r="15" spans="1:5" ht="18" customHeight="1">
-      <c r="A15" s="206" t="s">
+      <c r="A15" s="202" t="s">
         <v>192</v>
       </c>
-      <c r="B15" s="207"/>
+      <c r="B15" s="203"/>
     </row>
     <row r="16" spans="1:5" ht="21" customHeight="1">
-      <c r="A16" s="206" t="s">
+      <c r="A16" s="202" t="s">
         <v>193</v>
       </c>
-      <c r="B16" s="207"/>
+      <c r="B16" s="203"/>
     </row>
     <row r="17" spans="1:2" ht="48.75" customHeight="1">
-      <c r="A17" s="202" t="s">
+      <c r="A17" s="204" t="s">
         <v>195</v>
       </c>
-      <c r="B17" s="203"/>
+      <c r="B17" s="205"/>
     </row>
     <row r="19" spans="1:2" ht="18.75">
-      <c r="A19" s="219" t="s">
+      <c r="A19" s="206" t="s">
         <v>197</v>
       </c>
-      <c r="B19" s="220"/>
+      <c r="B19" s="207"/>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="120"/>
       <c r="B20" s="9"/>
     </row>
     <row r="21" spans="1:2">
-      <c r="A21" s="217" t="s">
+      <c r="A21" s="208" t="s">
         <v>198</v>
       </c>
-      <c r="B21" s="218"/>
+      <c r="B21" s="209"/>
     </row>
     <row r="22" spans="1:2">
-      <c r="A22" s="204"/>
-      <c r="B22" s="205"/>
+      <c r="A22" s="210"/>
+      <c r="B22" s="211"/>
     </row>
     <row r="23" spans="1:2">
-      <c r="A23" s="206" t="s">
+      <c r="A23" s="202" t="s">
         <v>199</v>
       </c>
-      <c r="B23" s="207"/>
+      <c r="B23" s="203"/>
     </row>
     <row r="24" spans="1:2">
-      <c r="A24" s="206"/>
-      <c r="B24" s="207"/>
+      <c r="A24" s="202"/>
+      <c r="B24" s="203"/>
     </row>
     <row r="25" spans="1:2">
-      <c r="A25" s="206" t="s">
+      <c r="A25" s="202" t="s">
         <v>200</v>
       </c>
-      <c r="B25" s="207"/>
+      <c r="B25" s="203"/>
     </row>
     <row r="26" spans="1:2">
-      <c r="A26" s="206" t="s">
+      <c r="A26" s="202" t="s">
         <v>201</v>
       </c>
-      <c r="B26" s="207"/>
+      <c r="B26" s="203"/>
     </row>
     <row r="27" spans="1:2">
-      <c r="A27" s="202"/>
-      <c r="B27" s="203"/>
+      <c r="A27" s="204"/>
+      <c r="B27" s="205"/>
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A7:B7"/>
     <mergeCell ref="A17:B17"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
@@ -26224,6 +26248,19 @@
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="A14:B14"/>
     <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A24:B24"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A3" r:id="rId1"/>

</xml_diff>

<commit_message>
Tempo - the small improvement in stage 2 resulted in beating the delay frame rule of stage 3.  50 faster measured from the first teleport of stage 3.
</commit_message>
<xml_diff>
--- a/trunk/Tempo/Tempo.xlsx
+++ b/trunk/Tempo/Tempo.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1152" uniqueCount="276">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1153" uniqueCount="277">
   <si>
     <t>Notes</t>
   </si>
@@ -888,6 +888,9 @@
   <si>
     <t>1st Move</t>
   </si>
+  <si>
+    <t>Enter 2nd teleport</t>
+  </si>
 </sst>
 </file>
 
@@ -897,10 +900,17 @@
     <numFmt numFmtId="164" formatCode="#,##0;[Red]#,##0"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="51">
+  <fonts count="52">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1870,34 +1880,34 @@
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="27" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="32" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="27" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="33" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="46" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="222">
+  <cellXfs count="223">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1905,208 +1915,208 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="23" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="18" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="20" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="21" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="21" fillId="13" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="27" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
+    <xf numFmtId="0" fontId="21" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="28" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="29" fillId="13" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="30" fillId="13" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="13" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="13" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="13" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="13" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="30" fillId="13" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="32" fillId="16" borderId="23" xfId="2" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="32" fillId="16" borderId="23" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="33" fillId="16" borderId="23" xfId="2" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="33" fillId="16" borderId="23" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="16" borderId="22" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="33" fillId="16" borderId="22" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="27" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="31" fillId="0" borderId="27" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="27" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="32" fillId="0" borderId="27" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="3" fontId="33" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="30" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="31" fillId="0" borderId="30" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="31" fillId="0" borderId="29" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="33" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="31" fillId="17" borderId="31" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="31" fillId="18" borderId="31" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="31" fillId="19" borderId="31" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="32" fillId="20" borderId="23" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="32" fillId="20" borderId="23" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="34" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="30" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="32" fillId="0" borderId="30" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="32" fillId="0" borderId="29" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="34" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="32" fillId="17" borderId="31" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="32" fillId="18" borderId="31" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="32" fillId="19" borderId="31" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="33" fillId="20" borderId="23" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="33" fillId="20" borderId="23" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="20" borderId="22" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="33" fillId="20" borderId="22" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="32" fillId="21" borderId="23" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="32" fillId="21" borderId="23" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="33" fillId="21" borderId="23" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="33" fillId="21" borderId="23" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="21" borderId="22" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="33" fillId="21" borderId="22" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="42" fillId="16" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="43" fillId="16" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="42" fillId="20" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="43" fillId="20" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
-    <xf numFmtId="3" fontId="33" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="31" fillId="0" borderId="42" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="33" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="33" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="33" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="31" fillId="0" borderId="42" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="34" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="32" fillId="0" borderId="42" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="34" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="34" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="34" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="32" fillId="0" borderId="42" xfId="1" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2116,10 +2126,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2140,19 +2150,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="23" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="49" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="50" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="40" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="34" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="50" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="27" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="36" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="39" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="33" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="49" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="26" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="35" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="38" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="38" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="39" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
@@ -2162,135 +2175,135 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
+    <xf numFmtId="3" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="3" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="21" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="21" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="20" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="20" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="39" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="23" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="34" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="40" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="35" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="41" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="41" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="42" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="16" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="16" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="18" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="20" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="21" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="21" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="24" fillId="14" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="21" fillId="13" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="22" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="25" fillId="14" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="14" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="14" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="14" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="14" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="25" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="50" fillId="22" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="51" fillId="22" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="50" fillId="22" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="51" fillId="22" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="50" fillId="22" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="51" fillId="22" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="47" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="48" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="48" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="49" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="48" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="49" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="46" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="46" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="47" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="47" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="4"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="4"/>
     </xf>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="33" xfId="3" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="46" fillId="0" borderId="33" xfId="3" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" indent="4"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -2603,7 +2616,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C58" sqref="C58"/>
+      <selection pane="bottomLeft" activeCell="C52" sqref="C52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" outlineLevelRow="2"/>
@@ -2619,16 +2632,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="33">
-      <c r="A1" s="161" t="s">
+      <c r="A1" s="163" t="s">
         <v>205</v>
       </c>
-      <c r="B1" s="160"/>
-      <c r="C1" s="162" t="s">
+      <c r="B1" s="162"/>
+      <c r="C1" s="164" t="s">
         <v>170</v>
       </c>
-      <c r="D1" s="162"/>
-      <c r="E1" s="162"/>
-      <c r="F1" s="163"/>
+      <c r="D1" s="164"/>
+      <c r="E1" s="164"/>
+      <c r="F1" s="165"/>
       <c r="G1" s="140"/>
       <c r="H1" s="141">
         <f>SUM(G1:G65540)</f>
@@ -2693,11 +2706,11 @@
       <c r="B4" s="146" t="s">
         <v>228</v>
       </c>
-      <c r="C4" s="159" t="s">
+      <c r="C4" s="161" t="s">
         <v>232</v>
       </c>
-      <c r="D4" s="159"/>
-      <c r="E4" s="165"/>
+      <c r="D4" s="161"/>
+      <c r="E4" s="167"/>
       <c r="F4" s="143"/>
       <c r="G4" s="140"/>
       <c r="H4" s="140"/>
@@ -2712,10 +2725,10 @@
       <c r="B5" s="147" t="s">
         <v>177</v>
       </c>
-      <c r="C5" s="159" t="s">
+      <c r="C5" s="161" t="s">
         <v>218</v>
       </c>
-      <c r="D5" s="159"/>
+      <c r="D5" s="161"/>
       <c r="E5" s="147"/>
       <c r="F5" s="147"/>
       <c r="G5" s="148" t="s">
@@ -2739,10 +2752,10 @@
       <c r="B6" s="147" t="s">
         <v>179</v>
       </c>
-      <c r="C6" s="159" t="s">
+      <c r="C6" s="161" t="s">
         <v>168</v>
       </c>
-      <c r="D6" s="160"/>
+      <c r="D6" s="162"/>
       <c r="E6" s="147"/>
       <c r="F6" s="143"/>
       <c r="G6" s="140"/>
@@ -2766,7 +2779,7 @@
       <c r="F7" s="93"/>
     </row>
     <row r="8" spans="1:11" ht="15" customHeight="1" outlineLevel="1">
-      <c r="A8" s="164" t="s">
+      <c r="A8" s="166" t="s">
         <v>180</v>
       </c>
       <c r="B8" s="95" t="s">
@@ -2786,7 +2799,7 @@
       </c>
     </row>
     <row r="9" spans="1:11" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="A9" s="157"/>
+      <c r="A9" s="159"/>
       <c r="B9" s="98" t="s">
         <v>177</v>
       </c>
@@ -2800,7 +2813,7 @@
       <c r="F9" s="104"/>
     </row>
     <row r="10" spans="1:11" ht="15.75" outlineLevel="1" thickTop="1">
-      <c r="A10" s="157"/>
+      <c r="A10" s="159"/>
       <c r="B10" s="149" t="s">
         <v>208</v>
       </c>
@@ -2817,7 +2830,7 @@
       <c r="F10" s="105"/>
     </row>
     <row r="11" spans="1:11" ht="15" outlineLevel="1">
-      <c r="A11" s="157"/>
+      <c r="A11" s="159"/>
       <c r="B11" s="149" t="s">
         <v>214</v>
       </c>
@@ -2834,7 +2847,7 @@
       <c r="F11" s="105"/>
     </row>
     <row r="12" spans="1:11" ht="15" outlineLevel="1">
-      <c r="A12" s="157"/>
+      <c r="A12" s="159"/>
       <c r="B12" s="149" t="s">
         <v>209</v>
       </c>
@@ -2851,7 +2864,7 @@
       <c r="F12" s="105"/>
     </row>
     <row r="13" spans="1:11" ht="15" outlineLevel="1">
-      <c r="A13" s="157"/>
+      <c r="A13" s="159"/>
       <c r="B13" s="149" t="s">
         <v>213</v>
       </c>
@@ -2868,7 +2881,7 @@
       <c r="F13" s="105"/>
     </row>
     <row r="14" spans="1:11" ht="15" outlineLevel="1">
-      <c r="A14" s="157"/>
+      <c r="A14" s="159"/>
       <c r="B14" s="149" t="s">
         <v>214</v>
       </c>
@@ -2885,7 +2898,7 @@
       <c r="F14" s="105"/>
     </row>
     <row r="15" spans="1:11" ht="15" outlineLevel="1">
-      <c r="A15" s="157"/>
+      <c r="A15" s="159"/>
       <c r="B15" s="149" t="s">
         <v>215</v>
       </c>
@@ -2902,7 +2915,7 @@
       <c r="F15" s="105"/>
     </row>
     <row r="16" spans="1:11" ht="15" outlineLevel="1">
-      <c r="A16" s="157"/>
+      <c r="A16" s="159"/>
       <c r="B16" s="149" t="s">
         <v>216</v>
       </c>
@@ -2919,7 +2932,7 @@
       <c r="F16" s="105"/>
     </row>
     <row r="17" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A17" s="157"/>
+      <c r="A17" s="159"/>
       <c r="B17" s="149" t="s">
         <v>217</v>
       </c>
@@ -2936,7 +2949,7 @@
       <c r="F17" s="105"/>
     </row>
     <row r="18" spans="1:8" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="A18" s="157"/>
+      <c r="A18" s="159"/>
       <c r="B18" s="98" t="s">
         <v>179</v>
       </c>
@@ -2979,7 +2992,7 @@
     </row>
     <row r="20" spans="1:8" ht="13.5" thickBot="1"/>
     <row r="21" spans="1:8" ht="15" customHeight="1" outlineLevel="1">
-      <c r="A21" s="158" t="s">
+      <c r="A21" s="160" t="s">
         <v>219</v>
       </c>
       <c r="B21" s="109" t="s">
@@ -2999,7 +3012,7 @@
       </c>
     </row>
     <row r="22" spans="1:8" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="A22" s="157"/>
+      <c r="A22" s="159"/>
       <c r="B22" s="98" t="s">
         <v>177</v>
       </c>
@@ -3016,7 +3029,7 @@
       <c r="F22" s="104"/>
     </row>
     <row r="23" spans="1:8" ht="15.75" outlineLevel="1" thickTop="1">
-      <c r="A23" s="157"/>
+      <c r="A23" s="159"/>
       <c r="B23" s="149" t="s">
         <v>175</v>
       </c>
@@ -3029,7 +3042,7 @@
       <c r="F23" s="105"/>
     </row>
     <row r="24" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A24" s="157"/>
+      <c r="A24" s="159"/>
       <c r="B24" s="149" t="s">
         <v>221</v>
       </c>
@@ -3049,7 +3062,7 @@
       </c>
     </row>
     <row r="25" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A25" s="157"/>
+      <c r="A25" s="159"/>
       <c r="B25" s="149"/>
       <c r="C25" s="101"/>
       <c r="D25" s="101"/>
@@ -3060,7 +3073,7 @@
       <c r="F25" s="105"/>
     </row>
     <row r="26" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A26" s="157"/>
+      <c r="A26" s="159"/>
       <c r="B26" s="100"/>
       <c r="C26" s="101"/>
       <c r="D26" s="101"/>
@@ -3071,7 +3084,7 @@
       <c r="F26" s="105"/>
     </row>
     <row r="27" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A27" s="157"/>
+      <c r="A27" s="159"/>
       <c r="B27" s="100"/>
       <c r="C27" s="101"/>
       <c r="D27" s="101"/>
@@ -3082,7 +3095,7 @@
       <c r="F27" s="105"/>
     </row>
     <row r="28" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A28" s="157"/>
+      <c r="A28" s="159"/>
       <c r="B28" s="149" t="s">
         <v>222</v>
       </c>
@@ -3102,7 +3115,7 @@
       </c>
     </row>
     <row r="29" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A29" s="157"/>
+      <c r="A29" s="159"/>
       <c r="B29" s="154" t="s">
         <v>264</v>
       </c>
@@ -3120,7 +3133,7 @@
       </c>
     </row>
     <row r="30" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A30" s="157"/>
+      <c r="A30" s="159"/>
       <c r="B30" s="154" t="s">
         <v>265</v>
       </c>
@@ -3136,7 +3149,7 @@
       </c>
     </row>
     <row r="31" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A31" s="157"/>
+      <c r="A31" s="159"/>
       <c r="B31" s="154" t="s">
         <v>266</v>
       </c>
@@ -3152,7 +3165,7 @@
       </c>
     </row>
     <row r="32" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A32" s="157"/>
+      <c r="A32" s="159"/>
       <c r="B32" s="154" t="s">
         <v>267</v>
       </c>
@@ -3168,7 +3181,7 @@
       </c>
     </row>
     <row r="33" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A33" s="157"/>
+      <c r="A33" s="159"/>
       <c r="B33" s="154" t="s">
         <v>269</v>
       </c>
@@ -3184,7 +3197,7 @@
       </c>
     </row>
     <row r="34" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A34" s="157"/>
+      <c r="A34" s="159"/>
       <c r="B34" s="154" t="s">
         <v>270</v>
       </c>
@@ -3200,7 +3213,7 @@
       </c>
     </row>
     <row r="35" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A35" s="157"/>
+      <c r="A35" s="159"/>
       <c r="B35" s="154" t="s">
         <v>271</v>
       </c>
@@ -3219,7 +3232,7 @@
       </c>
     </row>
     <row r="36" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A36" s="157"/>
+      <c r="A36" s="159"/>
       <c r="B36" s="149" t="s">
         <v>223</v>
       </c>
@@ -3239,7 +3252,7 @@
       </c>
     </row>
     <row r="37" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A37" s="157"/>
+      <c r="A37" s="159"/>
       <c r="B37" s="149" t="s">
         <v>224</v>
       </c>
@@ -3256,7 +3269,7 @@
       <c r="F37" s="105"/>
     </row>
     <row r="38" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A38" s="157"/>
+      <c r="A38" s="159"/>
       <c r="B38" s="149" t="s">
         <v>225</v>
       </c>
@@ -3273,7 +3286,7 @@
       <c r="F38" s="105"/>
     </row>
     <row r="39" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A39" s="157"/>
+      <c r="A39" s="159"/>
       <c r="B39" s="149" t="s">
         <v>217</v>
       </c>
@@ -3290,7 +3303,7 @@
       <c r="F39" s="105"/>
     </row>
     <row r="40" spans="1:9" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="A40" s="157"/>
+      <c r="A40" s="159"/>
       <c r="B40" s="98" t="s">
         <v>179</v>
       </c>
@@ -3329,7 +3342,7 @@
     </row>
     <row r="42" spans="1:9" ht="13.5" thickBot="1"/>
     <row r="43" spans="1:9" ht="15" customHeight="1" outlineLevel="1">
-      <c r="A43" s="156" t="s">
+      <c r="A43" s="158" t="s">
         <v>226</v>
       </c>
       <c r="B43" s="113" t="s">
@@ -3349,7 +3362,7 @@
       </c>
     </row>
     <row r="44" spans="1:9" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="A44" s="157"/>
+      <c r="A44" s="159"/>
       <c r="B44" s="98" t="s">
         <v>177</v>
       </c>
@@ -3367,7 +3380,7 @@
       </c>
     </row>
     <row r="45" spans="1:9" ht="15.75" outlineLevel="1" thickTop="1">
-      <c r="A45" s="157"/>
+      <c r="A45" s="159"/>
       <c r="B45" s="100"/>
       <c r="C45" s="101"/>
       <c r="D45" s="101"/>
@@ -3378,7 +3391,7 @@
       <c r="F45" s="105"/>
     </row>
     <row r="46" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A46" s="157"/>
+      <c r="A46" s="159"/>
       <c r="B46" s="149" t="s">
         <v>221</v>
       </c>
@@ -3395,7 +3408,7 @@
       <c r="F46" s="105"/>
     </row>
     <row r="47" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A47" s="157"/>
+      <c r="A47" s="159"/>
       <c r="B47" s="155" t="s">
         <v>274</v>
       </c>
@@ -3410,33 +3423,43 @@
       <c r="F47" s="105"/>
     </row>
     <row r="48" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A48" s="157"/>
-      <c r="B48" s="155"/>
-      <c r="C48" s="101"/>
+      <c r="A48" s="159"/>
+      <c r="B48" s="157" t="s">
+        <v>276</v>
+      </c>
+      <c r="C48" s="101">
+        <v>13549</v>
+      </c>
       <c r="D48" s="101"/>
       <c r="E48" s="123"/>
       <c r="F48" s="105"/>
-    </row>
-    <row r="49" spans="1:6" ht="15" outlineLevel="1">
-      <c r="A49" s="157"/>
+      <c r="H48">
+        <v>13556</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" ht="15" outlineLevel="1">
+      <c r="A49" s="159"/>
       <c r="B49" s="149" t="s">
         <v>222</v>
       </c>
       <c r="C49" s="101">
-        <v>14149</v>
+        <v>14140</v>
       </c>
       <c r="D49" s="101">
         <v>17009</v>
       </c>
       <c r="E49" s="123">
         <f t="shared" si="3"/>
-        <v>2860</v>
+        <v>2869</v>
       </c>
       <c r="F49" s="105"/>
-    </row>
-    <row r="50" spans="1:6" ht="15" outlineLevel="1">
-      <c r="A50" s="157"/>
-      <c r="B50" s="221" t="s">
+      <c r="H49">
+        <v>14149</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" ht="15" outlineLevel="1">
+      <c r="A50" s="159"/>
+      <c r="B50" s="156" t="s">
         <v>275</v>
       </c>
       <c r="C50" s="101">
@@ -3446,25 +3469,28 @@
       <c r="E50" s="123"/>
       <c r="F50" s="105"/>
     </row>
-    <row r="51" spans="1:6" ht="15" outlineLevel="1">
-      <c r="A51" s="157"/>
+    <row r="51" spans="1:8" ht="15" outlineLevel="1">
+      <c r="A51" s="159"/>
       <c r="B51" s="150" t="s">
         <v>229</v>
       </c>
       <c r="C51" s="101">
-        <v>14517</v>
+        <v>14467</v>
       </c>
       <c r="D51" s="101">
         <v>17390</v>
       </c>
       <c r="E51" s="123">
         <f t="shared" si="3"/>
-        <v>2873</v>
+        <v>2923</v>
       </c>
       <c r="F51" s="105"/>
-    </row>
-    <row r="52" spans="1:6" ht="15" outlineLevel="1">
-      <c r="A52" s="157"/>
+      <c r="H51">
+        <v>14517</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" ht="15" outlineLevel="1">
+      <c r="A52" s="159"/>
       <c r="B52" s="150" t="s">
         <v>230</v>
       </c>
@@ -3480,8 +3506,8 @@
       </c>
       <c r="F52" s="105"/>
     </row>
-    <row r="53" spans="1:6" ht="15" outlineLevel="1">
-      <c r="A53" s="157"/>
+    <row r="53" spans="1:8" ht="15" outlineLevel="1">
+      <c r="A53" s="159"/>
       <c r="B53" s="150" t="s">
         <v>231</v>
       </c>
@@ -3497,8 +3523,8 @@
       </c>
       <c r="F53" s="105"/>
     </row>
-    <row r="54" spans="1:6" ht="15" outlineLevel="1">
-      <c r="A54" s="157"/>
+    <row r="54" spans="1:8" ht="15" outlineLevel="1">
+      <c r="A54" s="159"/>
       <c r="B54" s="150" t="s">
         <v>233</v>
       </c>
@@ -3514,8 +3540,8 @@
       </c>
       <c r="F54" s="105"/>
     </row>
-    <row r="55" spans="1:6" ht="15" outlineLevel="1">
-      <c r="A55" s="157"/>
+    <row r="55" spans="1:8" ht="15" outlineLevel="1">
+      <c r="A55" s="159"/>
       <c r="B55" s="150" t="s">
         <v>234</v>
       </c>
@@ -3531,8 +3557,8 @@
       </c>
       <c r="F55" s="105"/>
     </row>
-    <row r="56" spans="1:6" ht="15" outlineLevel="1">
-      <c r="A56" s="157"/>
+    <row r="56" spans="1:8" ht="15" outlineLevel="1">
+      <c r="A56" s="159"/>
       <c r="B56" s="150" t="s">
         <v>235</v>
       </c>
@@ -3548,8 +3574,8 @@
       </c>
       <c r="F56" s="105"/>
     </row>
-    <row r="57" spans="1:6" ht="15" outlineLevel="1">
-      <c r="A57" s="157"/>
+    <row r="57" spans="1:8" ht="15" outlineLevel="1">
+      <c r="A57" s="159"/>
       <c r="B57" s="150" t="s">
         <v>236</v>
       </c>
@@ -3565,8 +3591,8 @@
       </c>
       <c r="F57" s="105"/>
     </row>
-    <row r="58" spans="1:6" ht="15" outlineLevel="1">
-      <c r="A58" s="157"/>
+    <row r="58" spans="1:8" ht="15" outlineLevel="1">
+      <c r="A58" s="159"/>
       <c r="B58" s="100"/>
       <c r="C58" s="101"/>
       <c r="D58" s="101"/>
@@ -3576,8 +3602,8 @@
       </c>
       <c r="F58" s="105"/>
     </row>
-    <row r="59" spans="1:6" ht="15" outlineLevel="1">
-      <c r="A59" s="157"/>
+    <row r="59" spans="1:8" ht="15" outlineLevel="1">
+      <c r="A59" s="159"/>
       <c r="B59" s="100"/>
       <c r="C59" s="101"/>
       <c r="D59" s="101"/>
@@ -3587,8 +3613,8 @@
       </c>
       <c r="F59" s="105"/>
     </row>
-    <row r="60" spans="1:6" ht="15" outlineLevel="1">
-      <c r="A60" s="157"/>
+    <row r="60" spans="1:8" ht="15" outlineLevel="1">
+      <c r="A60" s="159"/>
       <c r="B60" s="150" t="s">
         <v>237</v>
       </c>
@@ -3600,8 +3626,8 @@
       </c>
       <c r="F60" s="105"/>
     </row>
-    <row r="61" spans="1:6" ht="15" outlineLevel="1">
-      <c r="A61" s="157"/>
+    <row r="61" spans="1:8" ht="15" outlineLevel="1">
+      <c r="A61" s="159"/>
       <c r="B61" s="150" t="s">
         <v>223</v>
       </c>
@@ -3615,8 +3641,8 @@
       </c>
       <c r="F61" s="105"/>
     </row>
-    <row r="62" spans="1:6" ht="15" outlineLevel="1">
-      <c r="A62" s="157"/>
+    <row r="62" spans="1:8" ht="15" outlineLevel="1">
+      <c r="A62" s="159"/>
       <c r="B62" s="150" t="s">
         <v>238</v>
       </c>
@@ -3630,8 +3656,8 @@
       </c>
       <c r="F62" s="105"/>
     </row>
-    <row r="63" spans="1:6" ht="15" outlineLevel="1">
-      <c r="A63" s="157"/>
+    <row r="63" spans="1:8" ht="15" outlineLevel="1">
+      <c r="A63" s="159"/>
       <c r="B63" s="150" t="s">
         <v>239</v>
       </c>
@@ -3642,8 +3668,8 @@
       <c r="E63" s="123"/>
       <c r="F63" s="105"/>
     </row>
-    <row r="64" spans="1:6" ht="15" outlineLevel="1">
-      <c r="A64" s="157"/>
+    <row r="64" spans="1:8" ht="15" outlineLevel="1">
+      <c r="A64" s="159"/>
       <c r="B64" s="150" t="s">
         <v>217</v>
       </c>
@@ -3658,7 +3684,7 @@
       <c r="F64" s="105"/>
     </row>
     <row r="65" spans="1:8" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="A65" s="157"/>
+      <c r="A65" s="159"/>
       <c r="B65" s="98" t="s">
         <v>179</v>
       </c>
@@ -3699,7 +3725,7 @@
     </row>
     <row r="67" spans="1:8" ht="13.5" thickBot="1"/>
     <row r="68" spans="1:8" ht="15" customHeight="1" outlineLevel="1">
-      <c r="A68" s="158" t="s">
+      <c r="A68" s="160" t="s">
         <v>240</v>
       </c>
       <c r="B68" s="109" t="s">
@@ -3719,7 +3745,7 @@
       </c>
     </row>
     <row r="69" spans="1:8" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="A69" s="157"/>
+      <c r="A69" s="159"/>
       <c r="B69" s="98" t="s">
         <v>177</v>
       </c>
@@ -3737,7 +3763,7 @@
       </c>
     </row>
     <row r="70" spans="1:8" ht="15.75" outlineLevel="1" thickTop="1">
-      <c r="A70" s="157"/>
+      <c r="A70" s="159"/>
       <c r="B70" s="100"/>
       <c r="C70" s="101"/>
       <c r="D70" s="101"/>
@@ -3748,7 +3774,7 @@
       <c r="F70" s="105"/>
     </row>
     <row r="71" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A71" s="157"/>
+      <c r="A71" s="159"/>
       <c r="B71" s="151" t="s">
         <v>242</v>
       </c>
@@ -3763,7 +3789,7 @@
       <c r="F71" s="105"/>
     </row>
     <row r="72" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A72" s="157"/>
+      <c r="A72" s="159"/>
       <c r="B72" s="100"/>
       <c r="C72" s="101"/>
       <c r="D72" s="101"/>
@@ -3774,7 +3800,7 @@
       <c r="F72" s="105"/>
     </row>
     <row r="73" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A73" s="157"/>
+      <c r="A73" s="159"/>
       <c r="B73" s="151" t="s">
         <v>243</v>
       </c>
@@ -3789,7 +3815,7 @@
       <c r="F73" s="105"/>
     </row>
     <row r="74" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A74" s="157"/>
+      <c r="A74" s="159"/>
       <c r="B74" s="100"/>
       <c r="C74" s="101"/>
       <c r="D74" s="101"/>
@@ -3800,7 +3826,7 @@
       <c r="F74" s="105"/>
     </row>
     <row r="75" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A75" s="157"/>
+      <c r="A75" s="159"/>
       <c r="B75" s="151" t="s">
         <v>244</v>
       </c>
@@ -3815,7 +3841,7 @@
       <c r="F75" s="105"/>
     </row>
     <row r="76" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A76" s="157"/>
+      <c r="A76" s="159"/>
       <c r="B76" s="100"/>
       <c r="C76" s="101"/>
       <c r="D76" s="101"/>
@@ -3826,7 +3852,7 @@
       <c r="F76" s="105"/>
     </row>
     <row r="77" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A77" s="157"/>
+      <c r="A77" s="159"/>
       <c r="B77" s="151" t="s">
         <v>245</v>
       </c>
@@ -3841,7 +3867,7 @@
       <c r="F77" s="105"/>
     </row>
     <row r="78" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A78" s="157"/>
+      <c r="A78" s="159"/>
       <c r="B78" s="151" t="s">
         <v>238</v>
       </c>
@@ -3856,7 +3882,7 @@
       <c r="F78" s="105"/>
     </row>
     <row r="79" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A79" s="157"/>
+      <c r="A79" s="159"/>
       <c r="B79" s="151" t="s">
         <v>246</v>
       </c>
@@ -3871,7 +3897,7 @@
       <c r="F79" s="105"/>
     </row>
     <row r="80" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A80" s="157"/>
+      <c r="A80" s="159"/>
       <c r="B80" s="151" t="s">
         <v>217</v>
       </c>
@@ -3886,7 +3912,7 @@
       <c r="F80" s="105"/>
     </row>
     <row r="81" spans="1:8" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="A81" s="157"/>
+      <c r="A81" s="159"/>
       <c r="B81" s="98" t="s">
         <v>179</v>
       </c>
@@ -3927,7 +3953,7 @@
     </row>
     <row r="83" spans="1:8" ht="13.5" thickBot="1"/>
     <row r="84" spans="1:8" ht="15" customHeight="1" outlineLevel="1">
-      <c r="A84" s="156" t="s">
+      <c r="A84" s="158" t="s">
         <v>247</v>
       </c>
       <c r="B84" s="113" t="s">
@@ -3947,7 +3973,7 @@
       </c>
     </row>
     <row r="85" spans="1:8" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="A85" s="157"/>
+      <c r="A85" s="159"/>
       <c r="B85" s="98" t="s">
         <v>177</v>
       </c>
@@ -3965,7 +3991,7 @@
       </c>
     </row>
     <row r="86" spans="1:8" ht="15.75" outlineLevel="1" thickTop="1">
-      <c r="A86" s="157"/>
+      <c r="A86" s="159"/>
       <c r="B86" s="151" t="s">
         <v>228</v>
       </c>
@@ -3980,7 +4006,7 @@
       <c r="F86" s="105"/>
     </row>
     <row r="87" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A87" s="157"/>
+      <c r="A87" s="159"/>
       <c r="B87" s="151" t="s">
         <v>221</v>
       </c>
@@ -3995,7 +4021,7 @@
       <c r="F87" s="105"/>
     </row>
     <row r="88" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A88" s="157"/>
+      <c r="A88" s="159"/>
       <c r="B88" s="100"/>
       <c r="C88" s="101"/>
       <c r="D88" s="101"/>
@@ -4006,7 +4032,7 @@
       <c r="F88" s="105"/>
     </row>
     <row r="89" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A89" s="157"/>
+      <c r="A89" s="159"/>
       <c r="B89" s="151" t="s">
         <v>222</v>
       </c>
@@ -4021,7 +4047,7 @@
       <c r="F89" s="105"/>
     </row>
     <row r="90" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A90" s="157"/>
+      <c r="A90" s="159"/>
       <c r="B90" s="100"/>
       <c r="C90" s="101"/>
       <c r="D90" s="101"/>
@@ -4032,7 +4058,7 @@
       <c r="F90" s="105"/>
     </row>
     <row r="91" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A91" s="157"/>
+      <c r="A91" s="159"/>
       <c r="B91" s="152" t="s">
         <v>236</v>
       </c>
@@ -4047,7 +4073,7 @@
       <c r="F91" s="105"/>
     </row>
     <row r="92" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A92" s="157"/>
+      <c r="A92" s="159"/>
       <c r="B92" s="100"/>
       <c r="C92" s="101"/>
       <c r="D92" s="101"/>
@@ -4058,7 +4084,7 @@
       <c r="F92" s="105"/>
     </row>
     <row r="93" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A93" s="157"/>
+      <c r="A93" s="159"/>
       <c r="B93" s="100"/>
       <c r="C93" s="101"/>
       <c r="D93" s="101"/>
@@ -4069,7 +4095,7 @@
       <c r="F93" s="105"/>
     </row>
     <row r="94" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A94" s="157"/>
+      <c r="A94" s="159"/>
       <c r="B94" s="152" t="s">
         <v>223</v>
       </c>
@@ -4084,7 +4110,7 @@
       <c r="F94" s="105"/>
     </row>
     <row r="95" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A95" s="157"/>
+      <c r="A95" s="159"/>
       <c r="B95" s="152" t="s">
         <v>249</v>
       </c>
@@ -4099,7 +4125,7 @@
       <c r="F95" s="105"/>
     </row>
     <row r="96" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A96" s="157"/>
+      <c r="A96" s="159"/>
       <c r="B96" s="152" t="s">
         <v>250</v>
       </c>
@@ -4114,7 +4140,7 @@
       <c r="F96" s="105"/>
     </row>
     <row r="97" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A97" s="157"/>
+      <c r="A97" s="159"/>
       <c r="B97" s="152" t="s">
         <v>251</v>
       </c>
@@ -4129,7 +4155,7 @@
       <c r="F97" s="105"/>
     </row>
     <row r="98" spans="1:8" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="A98" s="157"/>
+      <c r="A98" s="159"/>
       <c r="B98" s="98" t="s">
         <v>179</v>
       </c>
@@ -4170,7 +4196,7 @@
     </row>
     <row r="100" spans="1:8" ht="13.5" thickBot="1"/>
     <row r="101" spans="1:8" ht="15" customHeight="1" outlineLevel="1">
-      <c r="A101" s="158" t="s">
+      <c r="A101" s="160" t="s">
         <v>252</v>
       </c>
       <c r="B101" s="109" t="s">
@@ -4190,7 +4216,7 @@
       </c>
     </row>
     <row r="102" spans="1:8" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="A102" s="157"/>
+      <c r="A102" s="159"/>
       <c r="B102" s="98" t="s">
         <v>177</v>
       </c>
@@ -4208,7 +4234,7 @@
       </c>
     </row>
     <row r="103" spans="1:8" ht="15.75" outlineLevel="1" thickTop="1">
-      <c r="A103" s="157"/>
+      <c r="A103" s="159"/>
       <c r="B103" s="100"/>
       <c r="C103" s="101"/>
       <c r="D103" s="101"/>
@@ -4219,7 +4245,7 @@
       <c r="F103" s="105"/>
     </row>
     <row r="104" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A104" s="157"/>
+      <c r="A104" s="159"/>
       <c r="B104" s="152" t="s">
         <v>254</v>
       </c>
@@ -4234,7 +4260,7 @@
       <c r="F104" s="105"/>
     </row>
     <row r="105" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A105" s="157"/>
+      <c r="A105" s="159"/>
       <c r="B105" s="100"/>
       <c r="C105" s="101"/>
       <c r="D105" s="101"/>
@@ -4245,7 +4271,7 @@
       <c r="F105" s="105"/>
     </row>
     <row r="106" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A106" s="157"/>
+      <c r="A106" s="159"/>
       <c r="B106" s="152" t="s">
         <v>255</v>
       </c>
@@ -4260,7 +4286,7 @@
       <c r="F106" s="105"/>
     </row>
     <row r="107" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A107" s="157"/>
+      <c r="A107" s="159"/>
       <c r="B107" s="100"/>
       <c r="C107" s="101"/>
       <c r="D107" s="101"/>
@@ -4271,7 +4297,7 @@
       <c r="F107" s="105"/>
     </row>
     <row r="108" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A108" s="157"/>
+      <c r="A108" s="159"/>
       <c r="B108" s="152" t="s">
         <v>223</v>
       </c>
@@ -4286,7 +4312,7 @@
       <c r="F108" s="105"/>
     </row>
     <row r="109" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A109" s="157"/>
+      <c r="A109" s="159"/>
       <c r="B109" s="152" t="s">
         <v>249</v>
       </c>
@@ -4301,7 +4327,7 @@
       <c r="F109" s="105"/>
     </row>
     <row r="110" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A110" s="157"/>
+      <c r="A110" s="159"/>
       <c r="B110" s="152" t="s">
         <v>256</v>
       </c>
@@ -4316,7 +4342,7 @@
       <c r="F110" s="105"/>
     </row>
     <row r="111" spans="1:8" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="A111" s="157"/>
+      <c r="A111" s="159"/>
       <c r="B111" s="98" t="s">
         <v>179</v>
       </c>
@@ -4357,7 +4383,7 @@
     </row>
     <row r="113" spans="1:9" ht="13.5" thickBot="1"/>
     <row r="114" spans="1:9" ht="15" customHeight="1" outlineLevel="1">
-      <c r="A114" s="156" t="s">
+      <c r="A114" s="158" t="s">
         <v>257</v>
       </c>
       <c r="B114" s="113" t="s">
@@ -4377,7 +4403,7 @@
       </c>
     </row>
     <row r="115" spans="1:9" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="A115" s="157"/>
+      <c r="A115" s="159"/>
       <c r="B115" s="98" t="s">
         <v>177</v>
       </c>
@@ -4399,7 +4425,7 @@
       </c>
     </row>
     <row r="116" spans="1:9" ht="15.75" outlineLevel="1" thickTop="1">
-      <c r="A116" s="157"/>
+      <c r="A116" s="159"/>
       <c r="B116" s="100"/>
       <c r="C116" s="101"/>
       <c r="D116" s="101"/>
@@ -4410,7 +4436,7 @@
       <c r="F116" s="105"/>
     </row>
     <row r="117" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A117" s="157"/>
+      <c r="A117" s="159"/>
       <c r="B117" s="152" t="s">
         <v>221</v>
       </c>
@@ -4425,7 +4451,7 @@
       <c r="F117" s="105"/>
     </row>
     <row r="118" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A118" s="157"/>
+      <c r="A118" s="159"/>
       <c r="B118" s="100"/>
       <c r="C118" s="101"/>
       <c r="D118" s="101"/>
@@ -4436,7 +4462,7 @@
       <c r="F118" s="105"/>
     </row>
     <row r="119" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A119" s="157"/>
+      <c r="A119" s="159"/>
       <c r="B119" s="152" t="s">
         <v>222</v>
       </c>
@@ -4451,7 +4477,7 @@
       <c r="F119" s="105"/>
     </row>
     <row r="120" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A120" s="157"/>
+      <c r="A120" s="159"/>
       <c r="B120" s="152" t="s">
         <v>249</v>
       </c>
@@ -4466,7 +4492,7 @@
       <c r="F120" s="105"/>
     </row>
     <row r="121" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A121" s="157"/>
+      <c r="A121" s="159"/>
       <c r="B121" s="152" t="s">
         <v>259</v>
       </c>
@@ -4481,7 +4507,7 @@
       <c r="F121" s="105"/>
     </row>
     <row r="122" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A122" s="157"/>
+      <c r="A122" s="159"/>
       <c r="B122" s="152" t="s">
         <v>224</v>
       </c>
@@ -4496,7 +4522,7 @@
       <c r="F122" s="105"/>
     </row>
     <row r="123" spans="1:9" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="A123" s="157"/>
+      <c r="A123" s="159"/>
       <c r="B123" s="98" t="s">
         <v>179</v>
       </c>
@@ -4537,7 +4563,7 @@
     </row>
     <row r="125" spans="1:9" ht="13.5" thickBot="1"/>
     <row r="126" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A126" s="158" t="s">
+      <c r="A126" s="160" t="s">
         <v>260</v>
       </c>
       <c r="B126" s="109" t="s">
@@ -4557,7 +4583,7 @@
       </c>
     </row>
     <row r="127" spans="1:9" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="A127" s="157"/>
+      <c r="A127" s="159"/>
       <c r="B127" s="98" t="s">
         <v>177</v>
       </c>
@@ -4579,7 +4605,7 @@
       </c>
     </row>
     <row r="128" spans="1:9" ht="15.75" outlineLevel="1" thickTop="1">
-      <c r="A128" s="157"/>
+      <c r="A128" s="159"/>
       <c r="B128" s="100"/>
       <c r="C128" s="101"/>
       <c r="D128" s="101"/>
@@ -4590,7 +4616,7 @@
       <c r="F128" s="105"/>
     </row>
     <row r="129" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A129" s="157"/>
+      <c r="A129" s="159"/>
       <c r="B129" s="100"/>
       <c r="C129" s="101"/>
       <c r="D129" s="101"/>
@@ -4601,7 +4627,7 @@
       <c r="F129" s="105"/>
     </row>
     <row r="130" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A130" s="157"/>
+      <c r="A130" s="159"/>
       <c r="B130" s="100"/>
       <c r="C130" s="101"/>
       <c r="D130" s="101"/>
@@ -4612,7 +4638,7 @@
       <c r="F130" s="105"/>
     </row>
     <row r="131" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A131" s="157"/>
+      <c r="A131" s="159"/>
       <c r="B131" s="100"/>
       <c r="C131" s="101"/>
       <c r="D131" s="101"/>
@@ -4623,7 +4649,7 @@
       <c r="F131" s="105"/>
     </row>
     <row r="132" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A132" s="157"/>
+      <c r="A132" s="159"/>
       <c r="B132" s="100"/>
       <c r="C132" s="101"/>
       <c r="D132" s="101"/>
@@ -4634,7 +4660,7 @@
       <c r="F132" s="105"/>
     </row>
     <row r="133" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A133" s="157"/>
+      <c r="A133" s="159"/>
       <c r="B133" s="100"/>
       <c r="C133" s="101"/>
       <c r="D133" s="101"/>
@@ -4645,7 +4671,7 @@
       <c r="F133" s="105"/>
     </row>
     <row r="134" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A134" s="157"/>
+      <c r="A134" s="159"/>
       <c r="B134" s="100"/>
       <c r="C134" s="101"/>
       <c r="D134" s="101"/>
@@ -4656,7 +4682,7 @@
       <c r="F134" s="105"/>
     </row>
     <row r="135" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A135" s="157"/>
+      <c r="A135" s="159"/>
       <c r="B135" s="100"/>
       <c r="C135" s="101"/>
       <c r="D135" s="101"/>
@@ -4667,7 +4693,7 @@
       <c r="F135" s="105"/>
     </row>
     <row r="136" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A136" s="157"/>
+      <c r="A136" s="159"/>
       <c r="B136" s="152" t="s">
         <v>262</v>
       </c>
@@ -4689,7 +4715,7 @@
       </c>
     </row>
     <row r="137" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A137" s="157"/>
+      <c r="A137" s="159"/>
       <c r="B137" s="100"/>
       <c r="C137" s="101"/>
       <c r="D137" s="101"/>
@@ -4700,7 +4726,7 @@
       <c r="F137" s="105"/>
     </row>
     <row r="138" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A138" s="157"/>
+      <c r="A138" s="159"/>
       <c r="B138" s="100"/>
       <c r="C138" s="101"/>
       <c r="D138" s="101"/>
@@ -4711,7 +4737,7 @@
       <c r="F138" s="105"/>
     </row>
     <row r="139" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A139" s="157"/>
+      <c r="A139" s="159"/>
       <c r="B139" s="100"/>
       <c r="C139" s="101"/>
       <c r="D139" s="101"/>
@@ -4722,7 +4748,7 @@
       <c r="F139" s="105"/>
     </row>
     <row r="140" spans="1:9" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="A140" s="157"/>
+      <c r="A140" s="159"/>
       <c r="B140" s="98" t="s">
         <v>179</v>
       </c>
@@ -4760,7 +4786,7 @@
       </c>
     </row>
     <row r="143" spans="1:9" ht="15" hidden="1" outlineLevel="2">
-      <c r="A143" s="156" t="s">
+      <c r="A143" s="158" t="s">
         <v>169</v>
       </c>
       <c r="B143" s="113" t="s">
@@ -4780,7 +4806,7 @@
       </c>
     </row>
     <row r="144" spans="1:9" ht="15.75" hidden="1" outlineLevel="2" thickBot="1">
-      <c r="A144" s="157"/>
+      <c r="A144" s="159"/>
       <c r="B144" s="98" t="s">
         <v>177</v>
       </c>
@@ -4793,7 +4819,7 @@
       <c r="F144" s="104"/>
     </row>
     <row r="145" spans="1:7" ht="15.75" hidden="1" outlineLevel="2" thickTop="1">
-      <c r="A145" s="157"/>
+      <c r="A145" s="159"/>
       <c r="B145" s="100"/>
       <c r="C145" s="101"/>
       <c r="D145" s="101"/>
@@ -4804,7 +4830,7 @@
       <c r="F145" s="105"/>
     </row>
     <row r="146" spans="1:7" ht="15" hidden="1" outlineLevel="2">
-      <c r="A146" s="157"/>
+      <c r="A146" s="159"/>
       <c r="B146" s="100"/>
       <c r="C146" s="101"/>
       <c r="D146" s="101"/>
@@ -4815,7 +4841,7 @@
       <c r="F146" s="105"/>
     </row>
     <row r="147" spans="1:7" ht="15" hidden="1" outlineLevel="2">
-      <c r="A147" s="157"/>
+      <c r="A147" s="159"/>
       <c r="B147" s="100"/>
       <c r="C147" s="101"/>
       <c r="D147" s="101"/>
@@ -4826,7 +4852,7 @@
       <c r="F147" s="105"/>
     </row>
     <row r="148" spans="1:7" ht="15" hidden="1" outlineLevel="2">
-      <c r="A148" s="157"/>
+      <c r="A148" s="159"/>
       <c r="B148" s="100"/>
       <c r="C148" s="101"/>
       <c r="D148" s="101"/>
@@ -4837,7 +4863,7 @@
       <c r="F148" s="105"/>
     </row>
     <row r="149" spans="1:7" ht="15" hidden="1" outlineLevel="2">
-      <c r="A149" s="157"/>
+      <c r="A149" s="159"/>
       <c r="B149" s="100"/>
       <c r="C149" s="101"/>
       <c r="D149" s="101"/>
@@ -4848,7 +4874,7 @@
       <c r="F149" s="105"/>
     </row>
     <row r="150" spans="1:7" ht="15" hidden="1" outlineLevel="2">
-      <c r="A150" s="157"/>
+      <c r="A150" s="159"/>
       <c r="B150" s="100"/>
       <c r="C150" s="101"/>
       <c r="D150" s="101"/>
@@ -4859,7 +4885,7 @@
       <c r="F150" s="105"/>
     </row>
     <row r="151" spans="1:7" ht="15" hidden="1" outlineLevel="2">
-      <c r="A151" s="157"/>
+      <c r="A151" s="159"/>
       <c r="B151" s="100"/>
       <c r="C151" s="101"/>
       <c r="D151" s="101"/>
@@ -4870,7 +4896,7 @@
       <c r="F151" s="105"/>
     </row>
     <row r="152" spans="1:7" ht="15" hidden="1" outlineLevel="2">
-      <c r="A152" s="157"/>
+      <c r="A152" s="159"/>
       <c r="B152" s="100"/>
       <c r="C152" s="101"/>
       <c r="D152" s="101"/>
@@ -4881,7 +4907,7 @@
       <c r="F152" s="105"/>
     </row>
     <row r="153" spans="1:7" ht="15" hidden="1" outlineLevel="2">
-      <c r="A153" s="157"/>
+      <c r="A153" s="159"/>
       <c r="B153" s="100"/>
       <c r="C153" s="101"/>
       <c r="D153" s="101"/>
@@ -4892,7 +4918,7 @@
       <c r="F153" s="105"/>
     </row>
     <row r="154" spans="1:7" ht="15" hidden="1" outlineLevel="2">
-      <c r="A154" s="157"/>
+      <c r="A154" s="159"/>
       <c r="B154" s="100"/>
       <c r="C154" s="101"/>
       <c r="D154" s="101"/>
@@ -4903,7 +4929,7 @@
       <c r="F154" s="105"/>
     </row>
     <row r="155" spans="1:7" ht="15" hidden="1" outlineLevel="2">
-      <c r="A155" s="157"/>
+      <c r="A155" s="159"/>
       <c r="B155" s="100"/>
       <c r="C155" s="101"/>
       <c r="D155" s="101"/>
@@ -4914,7 +4940,7 @@
       <c r="F155" s="105"/>
     </row>
     <row r="156" spans="1:7" ht="15" hidden="1" outlineLevel="2">
-      <c r="A156" s="157"/>
+      <c r="A156" s="159"/>
       <c r="B156" s="100"/>
       <c r="C156" s="101"/>
       <c r="D156" s="101"/>
@@ -4925,7 +4951,7 @@
       <c r="F156" s="105"/>
     </row>
     <row r="157" spans="1:7" ht="15.75" hidden="1" outlineLevel="2" thickBot="1">
-      <c r="A157" s="157"/>
+      <c r="A157" s="159"/>
       <c r="B157" s="98" t="s">
         <v>179</v>
       </c>
@@ -5009,13 +5035,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="26.25" customHeight="1">
-      <c r="A1" s="166" t="s">
+      <c r="A1" s="168" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="166"/>
-      <c r="C1" s="166"/>
-      <c r="D1" s="166"/>
-      <c r="E1" s="166"/>
+      <c r="B1" s="168"/>
+      <c r="C1" s="168"/>
+      <c r="D1" s="168"/>
+      <c r="E1" s="168"/>
       <c r="F1" s="7"/>
       <c r="G1" s="5"/>
       <c r="H1" s="5"/>
@@ -5045,18 +5071,18 @@
         <v>8</v>
       </c>
       <c r="B3" s="36"/>
-      <c r="C3" s="167"/>
-      <c r="D3" s="168"/>
-      <c r="E3" s="168"/>
+      <c r="C3" s="169"/>
+      <c r="D3" s="170"/>
+      <c r="E3" s="170"/>
     </row>
     <row r="4" spans="1:8" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A4" s="46" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="87"/>
-      <c r="C4" s="169"/>
-      <c r="D4" s="170"/>
-      <c r="E4" s="170"/>
+      <c r="C4" s="171"/>
+      <c r="D4" s="172"/>
+      <c r="E4" s="172"/>
       <c r="F4" s="6"/>
     </row>
     <row r="5" spans="1:8" hidden="1" outlineLevel="2">
@@ -5208,9 +5234,9 @@
         <v>9</v>
       </c>
       <c r="B21" s="90"/>
-      <c r="C21" s="171"/>
-      <c r="D21" s="172"/>
-      <c r="E21" s="172"/>
+      <c r="C21" s="173"/>
+      <c r="D21" s="174"/>
+      <c r="E21" s="174"/>
     </row>
     <row r="22" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A22" s="47">
@@ -5361,9 +5387,9 @@
         <v>10</v>
       </c>
       <c r="B38" s="87"/>
-      <c r="C38" s="169"/>
-      <c r="D38" s="170"/>
-      <c r="E38" s="170"/>
+      <c r="C38" s="171"/>
+      <c r="D38" s="172"/>
+      <c r="E38" s="172"/>
     </row>
     <row r="39" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A39" s="47">
@@ -5514,9 +5540,9 @@
         <v>11</v>
       </c>
       <c r="B55" s="87"/>
-      <c r="C55" s="169"/>
-      <c r="D55" s="170"/>
-      <c r="E55" s="170"/>
+      <c r="C55" s="171"/>
+      <c r="D55" s="172"/>
+      <c r="E55" s="172"/>
     </row>
     <row r="56" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A56" s="47">
@@ -5667,9 +5693,9 @@
         <v>12</v>
       </c>
       <c r="B72" s="87"/>
-      <c r="C72" s="169"/>
-      <c r="D72" s="170"/>
-      <c r="E72" s="170"/>
+      <c r="C72" s="171"/>
+      <c r="D72" s="172"/>
+      <c r="E72" s="172"/>
     </row>
     <row r="73" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A73" s="47">
@@ -5820,9 +5846,9 @@
         <v>13</v>
       </c>
       <c r="B89" s="87"/>
-      <c r="C89" s="169"/>
-      <c r="D89" s="170"/>
-      <c r="E89" s="170"/>
+      <c r="C89" s="171"/>
+      <c r="D89" s="172"/>
+      <c r="E89" s="172"/>
     </row>
     <row r="90" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A90" s="47">
@@ -5973,9 +5999,9 @@
         <v>14</v>
       </c>
       <c r="B106" s="87"/>
-      <c r="C106" s="169"/>
-      <c r="D106" s="170"/>
-      <c r="E106" s="170"/>
+      <c r="C106" s="171"/>
+      <c r="D106" s="172"/>
+      <c r="E106" s="172"/>
     </row>
     <row r="107" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A107" s="47">
@@ -6126,9 +6152,9 @@
         <v>15</v>
       </c>
       <c r="B123" s="87"/>
-      <c r="C123" s="169"/>
-      <c r="D123" s="170"/>
-      <c r="E123" s="170"/>
+      <c r="C123" s="171"/>
+      <c r="D123" s="172"/>
+      <c r="E123" s="172"/>
     </row>
     <row r="124" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A124" s="47">
@@ -6279,9 +6305,9 @@
         <v>16</v>
       </c>
       <c r="B140" s="87"/>
-      <c r="C140" s="169"/>
-      <c r="D140" s="170"/>
-      <c r="E140" s="170"/>
+      <c r="C140" s="171"/>
+      <c r="D140" s="172"/>
+      <c r="E140" s="172"/>
     </row>
     <row r="141" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A141" s="47">
@@ -6432,9 +6458,9 @@
         <v>17</v>
       </c>
       <c r="B157" s="87"/>
-      <c r="C157" s="169"/>
-      <c r="D157" s="170"/>
-      <c r="E157" s="170"/>
+      <c r="C157" s="171"/>
+      <c r="D157" s="172"/>
+      <c r="E157" s="172"/>
     </row>
     <row r="158" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A158" s="47">
@@ -6585,9 +6611,9 @@
         <v>18</v>
       </c>
       <c r="B174" s="87"/>
-      <c r="C174" s="169"/>
-      <c r="D174" s="170"/>
-      <c r="E174" s="170"/>
+      <c r="C174" s="171"/>
+      <c r="D174" s="172"/>
+      <c r="E174" s="172"/>
     </row>
     <row r="175" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A175" s="47">
@@ -6738,9 +6764,9 @@
         <v>19</v>
       </c>
       <c r="B191" s="87"/>
-      <c r="C191" s="169"/>
-      <c r="D191" s="170"/>
-      <c r="E191" s="170"/>
+      <c r="C191" s="171"/>
+      <c r="D191" s="172"/>
+      <c r="E191" s="172"/>
     </row>
     <row r="192" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A192" s="47">
@@ -6891,9 +6917,9 @@
         <v>20</v>
       </c>
       <c r="B208" s="87"/>
-      <c r="C208" s="169"/>
-      <c r="D208" s="170"/>
-      <c r="E208" s="170"/>
+      <c r="C208" s="171"/>
+      <c r="D208" s="172"/>
+      <c r="E208" s="172"/>
     </row>
     <row r="209" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A209" s="47">
@@ -7044,9 +7070,9 @@
         <v>21</v>
       </c>
       <c r="B225" s="87"/>
-      <c r="C225" s="169"/>
-      <c r="D225" s="170"/>
-      <c r="E225" s="170"/>
+      <c r="C225" s="171"/>
+      <c r="D225" s="172"/>
+      <c r="E225" s="172"/>
     </row>
     <row r="226" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A226" s="47">
@@ -7197,9 +7223,9 @@
         <v>22</v>
       </c>
       <c r="B242" s="87"/>
-      <c r="C242" s="169"/>
-      <c r="D242" s="170"/>
-      <c r="E242" s="170"/>
+      <c r="C242" s="171"/>
+      <c r="D242" s="172"/>
+      <c r="E242" s="172"/>
     </row>
     <row r="243" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A243" s="47">
@@ -7350,9 +7376,9 @@
         <v>23</v>
       </c>
       <c r="B259" s="87"/>
-      <c r="C259" s="169"/>
-      <c r="D259" s="170"/>
-      <c r="E259" s="170"/>
+      <c r="C259" s="171"/>
+      <c r="D259" s="172"/>
+      <c r="E259" s="172"/>
     </row>
     <row r="260" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A260" s="47">
@@ -7503,18 +7529,18 @@
         <v>24</v>
       </c>
       <c r="B276" s="37"/>
-      <c r="C276" s="173"/>
-      <c r="D276" s="174"/>
-      <c r="E276" s="174"/>
+      <c r="C276" s="175"/>
+      <c r="D276" s="176"/>
+      <c r="E276" s="176"/>
     </row>
     <row r="277" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A277" s="51" t="s">
         <v>25</v>
       </c>
       <c r="B277" s="87"/>
-      <c r="C277" s="169"/>
-      <c r="D277" s="170"/>
-      <c r="E277" s="170"/>
+      <c r="C277" s="171"/>
+      <c r="D277" s="172"/>
+      <c r="E277" s="172"/>
     </row>
     <row r="278" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A278" s="52">
@@ -7665,9 +7691,9 @@
         <v>26</v>
       </c>
       <c r="B294" s="90"/>
-      <c r="C294" s="171"/>
-      <c r="D294" s="172"/>
-      <c r="E294" s="172"/>
+      <c r="C294" s="173"/>
+      <c r="D294" s="174"/>
+      <c r="E294" s="174"/>
     </row>
     <row r="295" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A295" s="52">
@@ -7818,9 +7844,9 @@
         <v>27</v>
       </c>
       <c r="B311" s="87"/>
-      <c r="C311" s="169"/>
-      <c r="D311" s="170"/>
-      <c r="E311" s="170"/>
+      <c r="C311" s="171"/>
+      <c r="D311" s="172"/>
+      <c r="E311" s="172"/>
     </row>
     <row r="312" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A312" s="52">
@@ -7971,9 +7997,9 @@
         <v>28</v>
       </c>
       <c r="B328" s="87"/>
-      <c r="C328" s="169"/>
-      <c r="D328" s="170"/>
-      <c r="E328" s="170"/>
+      <c r="C328" s="171"/>
+      <c r="D328" s="172"/>
+      <c r="E328" s="172"/>
     </row>
     <row r="329" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A329" s="52">
@@ -8124,9 +8150,9 @@
         <v>29</v>
       </c>
       <c r="B345" s="87"/>
-      <c r="C345" s="169"/>
-      <c r="D345" s="170"/>
-      <c r="E345" s="170"/>
+      <c r="C345" s="171"/>
+      <c r="D345" s="172"/>
+      <c r="E345" s="172"/>
     </row>
     <row r="346" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A346" s="52">
@@ -8277,9 +8303,9 @@
         <v>30</v>
       </c>
       <c r="B362" s="87"/>
-      <c r="C362" s="169"/>
-      <c r="D362" s="170"/>
-      <c r="E362" s="170"/>
+      <c r="C362" s="171"/>
+      <c r="D362" s="172"/>
+      <c r="E362" s="172"/>
     </row>
     <row r="363" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A363" s="52">
@@ -8430,9 +8456,9 @@
         <v>31</v>
       </c>
       <c r="B379" s="87"/>
-      <c r="C379" s="169"/>
-      <c r="D379" s="170"/>
-      <c r="E379" s="170"/>
+      <c r="C379" s="171"/>
+      <c r="D379" s="172"/>
+      <c r="E379" s="172"/>
     </row>
     <row r="380" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A380" s="52">
@@ -8583,9 +8609,9 @@
         <v>32</v>
       </c>
       <c r="B396" s="87"/>
-      <c r="C396" s="169"/>
-      <c r="D396" s="170"/>
-      <c r="E396" s="170"/>
+      <c r="C396" s="171"/>
+      <c r="D396" s="172"/>
+      <c r="E396" s="172"/>
     </row>
     <row r="397" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A397" s="52">
@@ -8736,9 +8762,9 @@
         <v>33</v>
       </c>
       <c r="B413" s="87"/>
-      <c r="C413" s="169"/>
-      <c r="D413" s="170"/>
-      <c r="E413" s="170"/>
+      <c r="C413" s="171"/>
+      <c r="D413" s="172"/>
+      <c r="E413" s="172"/>
     </row>
     <row r="414" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A414" s="52">
@@ -8889,9 +8915,9 @@
         <v>34</v>
       </c>
       <c r="B430" s="87"/>
-      <c r="C430" s="169"/>
-      <c r="D430" s="170"/>
-      <c r="E430" s="170"/>
+      <c r="C430" s="171"/>
+      <c r="D430" s="172"/>
+      <c r="E430" s="172"/>
     </row>
     <row r="431" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A431" s="52">
@@ -9042,9 +9068,9 @@
         <v>35</v>
       </c>
       <c r="B447" s="87"/>
-      <c r="C447" s="169"/>
-      <c r="D447" s="170"/>
-      <c r="E447" s="170"/>
+      <c r="C447" s="171"/>
+      <c r="D447" s="172"/>
+      <c r="E447" s="172"/>
     </row>
     <row r="448" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A448" s="52">
@@ -9195,9 +9221,9 @@
         <v>36</v>
       </c>
       <c r="B464" s="87"/>
-      <c r="C464" s="169"/>
-      <c r="D464" s="170"/>
-      <c r="E464" s="170"/>
+      <c r="C464" s="171"/>
+      <c r="D464" s="172"/>
+      <c r="E464" s="172"/>
     </row>
     <row r="465" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A465" s="52">
@@ -9348,9 +9374,9 @@
         <v>37</v>
       </c>
       <c r="B481" s="87"/>
-      <c r="C481" s="169"/>
-      <c r="D481" s="170"/>
-      <c r="E481" s="170"/>
+      <c r="C481" s="171"/>
+      <c r="D481" s="172"/>
+      <c r="E481" s="172"/>
     </row>
     <row r="482" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A482" s="52">
@@ -9501,9 +9527,9 @@
         <v>38</v>
       </c>
       <c r="B498" s="87"/>
-      <c r="C498" s="169"/>
-      <c r="D498" s="170"/>
-      <c r="E498" s="170"/>
+      <c r="C498" s="171"/>
+      <c r="D498" s="172"/>
+      <c r="E498" s="172"/>
     </row>
     <row r="499" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A499" s="52">
@@ -9654,9 +9680,9 @@
         <v>39</v>
       </c>
       <c r="B515" s="87"/>
-      <c r="C515" s="169"/>
-      <c r="D515" s="170"/>
-      <c r="E515" s="170"/>
+      <c r="C515" s="171"/>
+      <c r="D515" s="172"/>
+      <c r="E515" s="172"/>
     </row>
     <row r="516" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A516" s="52">
@@ -9807,9 +9833,9 @@
         <v>40</v>
       </c>
       <c r="B532" s="87"/>
-      <c r="C532" s="169"/>
-      <c r="D532" s="170"/>
-      <c r="E532" s="170"/>
+      <c r="C532" s="171"/>
+      <c r="D532" s="172"/>
+      <c r="E532" s="172"/>
     </row>
     <row r="533" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A533" s="55">
@@ -9960,18 +9986,18 @@
         <v>50</v>
       </c>
       <c r="B549" s="38"/>
-      <c r="C549" s="175"/>
-      <c r="D549" s="176"/>
-      <c r="E549" s="176"/>
+      <c r="C549" s="177"/>
+      <c r="D549" s="178"/>
+      <c r="E549" s="178"/>
     </row>
     <row r="550" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A550" s="58" t="s">
         <v>51</v>
       </c>
       <c r="B550" s="87"/>
-      <c r="C550" s="169"/>
-      <c r="D550" s="170"/>
-      <c r="E550" s="170"/>
+      <c r="C550" s="171"/>
+      <c r="D550" s="172"/>
+      <c r="E550" s="172"/>
     </row>
     <row r="551" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A551" s="59">
@@ -10122,9 +10148,9 @@
         <v>52</v>
       </c>
       <c r="B567" s="90"/>
-      <c r="C567" s="171"/>
-      <c r="D567" s="172"/>
-      <c r="E567" s="172"/>
+      <c r="C567" s="173"/>
+      <c r="D567" s="174"/>
+      <c r="E567" s="174"/>
     </row>
     <row r="568" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A568" s="59">
@@ -10275,9 +10301,9 @@
         <v>53</v>
       </c>
       <c r="B584" s="87"/>
-      <c r="C584" s="169"/>
-      <c r="D584" s="170"/>
-      <c r="E584" s="170"/>
+      <c r="C584" s="171"/>
+      <c r="D584" s="172"/>
+      <c r="E584" s="172"/>
     </row>
     <row r="585" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A585" s="59">
@@ -10428,9 +10454,9 @@
         <v>54</v>
       </c>
       <c r="B601" s="87"/>
-      <c r="C601" s="169"/>
-      <c r="D601" s="170"/>
-      <c r="E601" s="170"/>
+      <c r="C601" s="171"/>
+      <c r="D601" s="172"/>
+      <c r="E601" s="172"/>
     </row>
     <row r="602" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A602" s="59">
@@ -10581,9 +10607,9 @@
         <v>55</v>
       </c>
       <c r="B618" s="87"/>
-      <c r="C618" s="169"/>
-      <c r="D618" s="170"/>
-      <c r="E618" s="170"/>
+      <c r="C618" s="171"/>
+      <c r="D618" s="172"/>
+      <c r="E618" s="172"/>
     </row>
     <row r="619" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A619" s="59">
@@ -10734,9 +10760,9 @@
         <v>56</v>
       </c>
       <c r="B635" s="87"/>
-      <c r="C635" s="169"/>
-      <c r="D635" s="170"/>
-      <c r="E635" s="170"/>
+      <c r="C635" s="171"/>
+      <c r="D635" s="172"/>
+      <c r="E635" s="172"/>
     </row>
     <row r="636" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A636" s="59">
@@ -10887,9 +10913,9 @@
         <v>57</v>
       </c>
       <c r="B652" s="87"/>
-      <c r="C652" s="169"/>
-      <c r="D652" s="170"/>
-      <c r="E652" s="170"/>
+      <c r="C652" s="171"/>
+      <c r="D652" s="172"/>
+      <c r="E652" s="172"/>
     </row>
     <row r="653" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A653" s="59">
@@ -11040,9 +11066,9 @@
         <v>58</v>
       </c>
       <c r="B669" s="87"/>
-      <c r="C669" s="169"/>
-      <c r="D669" s="170"/>
-      <c r="E669" s="170"/>
+      <c r="C669" s="171"/>
+      <c r="D669" s="172"/>
+      <c r="E669" s="172"/>
     </row>
     <row r="670" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A670" s="59">
@@ -11193,9 +11219,9 @@
         <v>59</v>
       </c>
       <c r="B686" s="87"/>
-      <c r="C686" s="169"/>
-      <c r="D686" s="170"/>
-      <c r="E686" s="170"/>
+      <c r="C686" s="171"/>
+      <c r="D686" s="172"/>
+      <c r="E686" s="172"/>
     </row>
     <row r="687" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A687" s="59">
@@ -11346,9 +11372,9 @@
         <v>60</v>
       </c>
       <c r="B703" s="87"/>
-      <c r="C703" s="169"/>
-      <c r="D703" s="170"/>
-      <c r="E703" s="170"/>
+      <c r="C703" s="171"/>
+      <c r="D703" s="172"/>
+      <c r="E703" s="172"/>
     </row>
     <row r="704" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A704" s="59">
@@ -11499,9 +11525,9 @@
         <v>61</v>
       </c>
       <c r="B720" s="87"/>
-      <c r="C720" s="169"/>
-      <c r="D720" s="170"/>
-      <c r="E720" s="170"/>
+      <c r="C720" s="171"/>
+      <c r="D720" s="172"/>
+      <c r="E720" s="172"/>
     </row>
     <row r="721" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A721" s="59">
@@ -11652,9 +11678,9 @@
         <v>62</v>
       </c>
       <c r="B737" s="87"/>
-      <c r="C737" s="169"/>
-      <c r="D737" s="170"/>
-      <c r="E737" s="170"/>
+      <c r="C737" s="171"/>
+      <c r="D737" s="172"/>
+      <c r="E737" s="172"/>
     </row>
     <row r="738" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A738" s="59">
@@ -11805,9 +11831,9 @@
         <v>63</v>
       </c>
       <c r="B754" s="87"/>
-      <c r="C754" s="169"/>
-      <c r="D754" s="170"/>
-      <c r="E754" s="170"/>
+      <c r="C754" s="171"/>
+      <c r="D754" s="172"/>
+      <c r="E754" s="172"/>
     </row>
     <row r="755" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A755" s="59">
@@ -11958,9 +11984,9 @@
         <v>64</v>
       </c>
       <c r="B771" s="87"/>
-      <c r="C771" s="169"/>
-      <c r="D771" s="170"/>
-      <c r="E771" s="170"/>
+      <c r="C771" s="171"/>
+      <c r="D771" s="172"/>
+      <c r="E771" s="172"/>
     </row>
     <row r="772" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A772" s="59">
@@ -12111,9 +12137,9 @@
         <v>65</v>
       </c>
       <c r="B788" s="87"/>
-      <c r="C788" s="169"/>
-      <c r="D788" s="170"/>
-      <c r="E788" s="170"/>
+      <c r="C788" s="171"/>
+      <c r="D788" s="172"/>
+      <c r="E788" s="172"/>
     </row>
     <row r="789" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A789" s="59">
@@ -12264,9 +12290,9 @@
         <v>66</v>
       </c>
       <c r="B805" s="87"/>
-      <c r="C805" s="169"/>
-      <c r="D805" s="170"/>
-      <c r="E805" s="170"/>
+      <c r="C805" s="171"/>
+      <c r="D805" s="172"/>
+      <c r="E805" s="172"/>
     </row>
     <row r="806" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A806" s="59">
@@ -12417,18 +12443,18 @@
         <v>67</v>
       </c>
       <c r="B822" s="39"/>
-      <c r="C822" s="177"/>
-      <c r="D822" s="178"/>
-      <c r="E822" s="178"/>
+      <c r="C822" s="179"/>
+      <c r="D822" s="180"/>
+      <c r="E822" s="180"/>
     </row>
     <row r="823" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A823" s="63" t="s">
         <v>68</v>
       </c>
       <c r="B823" s="87"/>
-      <c r="C823" s="169"/>
-      <c r="D823" s="170"/>
-      <c r="E823" s="170"/>
+      <c r="C823" s="171"/>
+      <c r="D823" s="172"/>
+      <c r="E823" s="172"/>
     </row>
     <row r="824" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A824" s="64">
@@ -12579,9 +12605,9 @@
         <v>69</v>
       </c>
       <c r="B840" s="90"/>
-      <c r="C840" s="171"/>
-      <c r="D840" s="172"/>
-      <c r="E840" s="172"/>
+      <c r="C840" s="173"/>
+      <c r="D840" s="174"/>
+      <c r="E840" s="174"/>
     </row>
     <row r="841" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A841" s="64">
@@ -12732,9 +12758,9 @@
         <v>70</v>
       </c>
       <c r="B857" s="87"/>
-      <c r="C857" s="169"/>
-      <c r="D857" s="170"/>
-      <c r="E857" s="170"/>
+      <c r="C857" s="171"/>
+      <c r="D857" s="172"/>
+      <c r="E857" s="172"/>
     </row>
     <row r="858" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A858" s="64">
@@ -12885,9 +12911,9 @@
         <v>71</v>
       </c>
       <c r="B874" s="87"/>
-      <c r="C874" s="169"/>
-      <c r="D874" s="170"/>
-      <c r="E874" s="170"/>
+      <c r="C874" s="171"/>
+      <c r="D874" s="172"/>
+      <c r="E874" s="172"/>
     </row>
     <row r="875" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A875" s="64">
@@ -13038,9 +13064,9 @@
         <v>72</v>
       </c>
       <c r="B891" s="87"/>
-      <c r="C891" s="169"/>
-      <c r="D891" s="170"/>
-      <c r="E891" s="170"/>
+      <c r="C891" s="171"/>
+      <c r="D891" s="172"/>
+      <c r="E891" s="172"/>
     </row>
     <row r="892" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A892" s="64">
@@ -13191,9 +13217,9 @@
         <v>73</v>
       </c>
       <c r="B908" s="87"/>
-      <c r="C908" s="169"/>
-      <c r="D908" s="170"/>
-      <c r="E908" s="170"/>
+      <c r="C908" s="171"/>
+      <c r="D908" s="172"/>
+      <c r="E908" s="172"/>
     </row>
     <row r="909" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A909" s="64">
@@ -13344,9 +13370,9 @@
         <v>74</v>
       </c>
       <c r="B925" s="87"/>
-      <c r="C925" s="169"/>
-      <c r="D925" s="170"/>
-      <c r="E925" s="170"/>
+      <c r="C925" s="171"/>
+      <c r="D925" s="172"/>
+      <c r="E925" s="172"/>
     </row>
     <row r="926" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A926" s="64">
@@ -13497,9 +13523,9 @@
         <v>75</v>
       </c>
       <c r="B942" s="87"/>
-      <c r="C942" s="169"/>
-      <c r="D942" s="170"/>
-      <c r="E942" s="170"/>
+      <c r="C942" s="171"/>
+      <c r="D942" s="172"/>
+      <c r="E942" s="172"/>
     </row>
     <row r="943" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A943" s="64">
@@ -13650,9 +13676,9 @@
         <v>76</v>
       </c>
       <c r="B959" s="87"/>
-      <c r="C959" s="169"/>
-      <c r="D959" s="170"/>
-      <c r="E959" s="170"/>
+      <c r="C959" s="171"/>
+      <c r="D959" s="172"/>
+      <c r="E959" s="172"/>
     </row>
     <row r="960" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A960" s="64">
@@ -13803,9 +13829,9 @@
         <v>77</v>
       </c>
       <c r="B976" s="87"/>
-      <c r="C976" s="169"/>
-      <c r="D976" s="170"/>
-      <c r="E976" s="170"/>
+      <c r="C976" s="171"/>
+      <c r="D976" s="172"/>
+      <c r="E976" s="172"/>
     </row>
     <row r="977" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A977" s="64">
@@ -13956,9 +13982,9 @@
         <v>78</v>
       </c>
       <c r="B993" s="87"/>
-      <c r="C993" s="169"/>
-      <c r="D993" s="170"/>
-      <c r="E993" s="170"/>
+      <c r="C993" s="171"/>
+      <c r="D993" s="172"/>
+      <c r="E993" s="172"/>
     </row>
     <row r="994" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A994" s="64">
@@ -14109,9 +14135,9 @@
         <v>79</v>
       </c>
       <c r="B1010" s="87"/>
-      <c r="C1010" s="169"/>
-      <c r="D1010" s="170"/>
-      <c r="E1010" s="170"/>
+      <c r="C1010" s="171"/>
+      <c r="D1010" s="172"/>
+      <c r="E1010" s="172"/>
     </row>
     <row r="1011" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1011" s="64">
@@ -14262,9 +14288,9 @@
         <v>80</v>
       </c>
       <c r="B1027" s="87"/>
-      <c r="C1027" s="169"/>
-      <c r="D1027" s="170"/>
-      <c r="E1027" s="170"/>
+      <c r="C1027" s="171"/>
+      <c r="D1027" s="172"/>
+      <c r="E1027" s="172"/>
     </row>
     <row r="1028" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1028" s="64">
@@ -14415,9 +14441,9 @@
         <v>83</v>
       </c>
       <c r="B1044" s="87"/>
-      <c r="C1044" s="169"/>
-      <c r="D1044" s="170"/>
-      <c r="E1044" s="170"/>
+      <c r="C1044" s="171"/>
+      <c r="D1044" s="172"/>
+      <c r="E1044" s="172"/>
     </row>
     <row r="1045" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1045" s="64">
@@ -14568,9 +14594,9 @@
         <v>82</v>
       </c>
       <c r="B1061" s="87"/>
-      <c r="C1061" s="169"/>
-      <c r="D1061" s="170"/>
-      <c r="E1061" s="170"/>
+      <c r="C1061" s="171"/>
+      <c r="D1061" s="172"/>
+      <c r="E1061" s="172"/>
     </row>
     <row r="1062" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1062" s="64">
@@ -14721,9 +14747,9 @@
         <v>84</v>
       </c>
       <c r="B1078" s="87"/>
-      <c r="C1078" s="169"/>
-      <c r="D1078" s="170"/>
-      <c r="E1078" s="170"/>
+      <c r="C1078" s="171"/>
+      <c r="D1078" s="172"/>
+      <c r="E1078" s="172"/>
     </row>
     <row r="1079" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1079" s="64">
@@ -14874,18 +14900,18 @@
         <v>104</v>
       </c>
       <c r="B1095" s="40"/>
-      <c r="C1095" s="179"/>
-      <c r="D1095" s="180"/>
-      <c r="E1095" s="180"/>
+      <c r="C1095" s="181"/>
+      <c r="D1095" s="182"/>
+      <c r="E1095" s="182"/>
     </row>
     <row r="1096" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A1096" s="68" t="s">
         <v>85</v>
       </c>
       <c r="B1096" s="87"/>
-      <c r="C1096" s="169"/>
-      <c r="D1096" s="170"/>
-      <c r="E1096" s="170"/>
+      <c r="C1096" s="171"/>
+      <c r="D1096" s="172"/>
+      <c r="E1096" s="172"/>
     </row>
     <row r="1097" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1097" s="69">
@@ -15036,9 +15062,9 @@
         <v>86</v>
       </c>
       <c r="B1113" s="90"/>
-      <c r="C1113" s="171"/>
-      <c r="D1113" s="172"/>
-      <c r="E1113" s="172"/>
+      <c r="C1113" s="173"/>
+      <c r="D1113" s="174"/>
+      <c r="E1113" s="174"/>
     </row>
     <row r="1114" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1114" s="69">
@@ -15189,9 +15215,9 @@
         <v>87</v>
       </c>
       <c r="B1130" s="87"/>
-      <c r="C1130" s="169"/>
-      <c r="D1130" s="170"/>
-      <c r="E1130" s="170"/>
+      <c r="C1130" s="171"/>
+      <c r="D1130" s="172"/>
+      <c r="E1130" s="172"/>
     </row>
     <row r="1131" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1131" s="69">
@@ -15342,9 +15368,9 @@
         <v>88</v>
       </c>
       <c r="B1147" s="87"/>
-      <c r="C1147" s="169"/>
-      <c r="D1147" s="170"/>
-      <c r="E1147" s="170"/>
+      <c r="C1147" s="171"/>
+      <c r="D1147" s="172"/>
+      <c r="E1147" s="172"/>
     </row>
     <row r="1148" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1148" s="69">
@@ -15495,9 +15521,9 @@
         <v>89</v>
       </c>
       <c r="B1164" s="87"/>
-      <c r="C1164" s="169"/>
-      <c r="D1164" s="170"/>
-      <c r="E1164" s="170"/>
+      <c r="C1164" s="171"/>
+      <c r="D1164" s="172"/>
+      <c r="E1164" s="172"/>
     </row>
     <row r="1165" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1165" s="69">
@@ -15648,9 +15674,9 @@
         <v>90</v>
       </c>
       <c r="B1181" s="87"/>
-      <c r="C1181" s="169"/>
-      <c r="D1181" s="170"/>
-      <c r="E1181" s="170"/>
+      <c r="C1181" s="171"/>
+      <c r="D1181" s="172"/>
+      <c r="E1181" s="172"/>
     </row>
     <row r="1182" spans="1:5" hidden="1" outlineLevel="3">
       <c r="A1182" s="69">
@@ -15801,9 +15827,9 @@
         <v>91</v>
       </c>
       <c r="B1198" s="87"/>
-      <c r="C1198" s="169"/>
-      <c r="D1198" s="170"/>
-      <c r="E1198" s="170"/>
+      <c r="C1198" s="171"/>
+      <c r="D1198" s="172"/>
+      <c r="E1198" s="172"/>
     </row>
     <row r="1199" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1199" s="69">
@@ -15954,9 +15980,9 @@
         <v>92</v>
       </c>
       <c r="B1215" s="87"/>
-      <c r="C1215" s="169"/>
-      <c r="D1215" s="170"/>
-      <c r="E1215" s="170"/>
+      <c r="C1215" s="171"/>
+      <c r="D1215" s="172"/>
+      <c r="E1215" s="172"/>
     </row>
     <row r="1216" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1216" s="69">
@@ -16107,9 +16133,9 @@
         <v>93</v>
       </c>
       <c r="B1232" s="87"/>
-      <c r="C1232" s="169"/>
-      <c r="D1232" s="170"/>
-      <c r="E1232" s="170"/>
+      <c r="C1232" s="171"/>
+      <c r="D1232" s="172"/>
+      <c r="E1232" s="172"/>
     </row>
     <row r="1233" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1233" s="69">
@@ -16260,9 +16286,9 @@
         <v>94</v>
       </c>
       <c r="B1249" s="87"/>
-      <c r="C1249" s="169"/>
-      <c r="D1249" s="170"/>
-      <c r="E1249" s="170"/>
+      <c r="C1249" s="171"/>
+      <c r="D1249" s="172"/>
+      <c r="E1249" s="172"/>
     </row>
     <row r="1250" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1250" s="69">
@@ -16413,9 +16439,9 @@
         <v>99</v>
       </c>
       <c r="B1266" s="87"/>
-      <c r="C1266" s="169"/>
-      <c r="D1266" s="170"/>
-      <c r="E1266" s="170"/>
+      <c r="C1266" s="171"/>
+      <c r="D1266" s="172"/>
+      <c r="E1266" s="172"/>
     </row>
     <row r="1267" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1267" s="69">
@@ -16566,9 +16592,9 @@
         <v>100</v>
       </c>
       <c r="B1283" s="87"/>
-      <c r="C1283" s="169"/>
-      <c r="D1283" s="170"/>
-      <c r="E1283" s="170"/>
+      <c r="C1283" s="171"/>
+      <c r="D1283" s="172"/>
+      <c r="E1283" s="172"/>
     </row>
     <row r="1284" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1284" s="69">
@@ -16719,9 +16745,9 @@
         <v>101</v>
       </c>
       <c r="B1300" s="87"/>
-      <c r="C1300" s="169"/>
-      <c r="D1300" s="170"/>
-      <c r="E1300" s="170"/>
+      <c r="C1300" s="171"/>
+      <c r="D1300" s="172"/>
+      <c r="E1300" s="172"/>
     </row>
     <row r="1301" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1301" s="69">
@@ -16872,9 +16898,9 @@
         <v>81</v>
       </c>
       <c r="B1317" s="87"/>
-      <c r="C1317" s="169"/>
-      <c r="D1317" s="170"/>
-      <c r="E1317" s="170"/>
+      <c r="C1317" s="171"/>
+      <c r="D1317" s="172"/>
+      <c r="E1317" s="172"/>
     </row>
     <row r="1318" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1318" s="69">
@@ -17025,9 +17051,9 @@
         <v>102</v>
       </c>
       <c r="B1334" s="87"/>
-      <c r="C1334" s="169"/>
-      <c r="D1334" s="170"/>
-      <c r="E1334" s="170"/>
+      <c r="C1334" s="171"/>
+      <c r="D1334" s="172"/>
+      <c r="E1334" s="172"/>
     </row>
     <row r="1335" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1335" s="69">
@@ -17178,9 +17204,9 @@
         <v>98</v>
       </c>
       <c r="B1351" s="87"/>
-      <c r="C1351" s="169"/>
-      <c r="D1351" s="170"/>
-      <c r="E1351" s="170"/>
+      <c r="C1351" s="171"/>
+      <c r="D1351" s="172"/>
+      <c r="E1351" s="172"/>
     </row>
     <row r="1352" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1352" s="69">
@@ -17331,18 +17357,18 @@
         <v>103</v>
       </c>
       <c r="B1368" s="41"/>
-      <c r="C1368" s="181"/>
-      <c r="D1368" s="182"/>
-      <c r="E1368" s="182"/>
+      <c r="C1368" s="183"/>
+      <c r="D1368" s="184"/>
+      <c r="E1368" s="184"/>
     </row>
     <row r="1369" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A1369" s="73" t="s">
         <v>105</v>
       </c>
       <c r="B1369" s="87"/>
-      <c r="C1369" s="169"/>
-      <c r="D1369" s="170"/>
-      <c r="E1369" s="170"/>
+      <c r="C1369" s="171"/>
+      <c r="D1369" s="172"/>
+      <c r="E1369" s="172"/>
     </row>
     <row r="1370" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1370" s="74">
@@ -17493,9 +17519,9 @@
         <v>106</v>
       </c>
       <c r="B1386" s="90"/>
-      <c r="C1386" s="171"/>
-      <c r="D1386" s="172"/>
-      <c r="E1386" s="172"/>
+      <c r="C1386" s="173"/>
+      <c r="D1386" s="174"/>
+      <c r="E1386" s="174"/>
     </row>
     <row r="1387" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1387" s="74">
@@ -17646,9 +17672,9 @@
         <v>107</v>
       </c>
       <c r="B1403" s="87"/>
-      <c r="C1403" s="169"/>
-      <c r="D1403" s="170"/>
-      <c r="E1403" s="170"/>
+      <c r="C1403" s="171"/>
+      <c r="D1403" s="172"/>
+      <c r="E1403" s="172"/>
     </row>
     <row r="1404" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1404" s="74">
@@ -17799,9 +17825,9 @@
         <v>108</v>
       </c>
       <c r="B1420" s="87"/>
-      <c r="C1420" s="169"/>
-      <c r="D1420" s="170"/>
-      <c r="E1420" s="170"/>
+      <c r="C1420" s="171"/>
+      <c r="D1420" s="172"/>
+      <c r="E1420" s="172"/>
     </row>
     <row r="1421" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1421" s="74">
@@ -17952,9 +17978,9 @@
         <v>109</v>
       </c>
       <c r="B1437" s="87"/>
-      <c r="C1437" s="169"/>
-      <c r="D1437" s="170"/>
-      <c r="E1437" s="170"/>
+      <c r="C1437" s="171"/>
+      <c r="D1437" s="172"/>
+      <c r="E1437" s="172"/>
     </row>
     <row r="1438" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1438" s="74">
@@ -18105,9 +18131,9 @@
         <v>110</v>
       </c>
       <c r="B1454" s="87"/>
-      <c r="C1454" s="169"/>
-      <c r="D1454" s="170"/>
-      <c r="E1454" s="170"/>
+      <c r="C1454" s="171"/>
+      <c r="D1454" s="172"/>
+      <c r="E1454" s="172"/>
     </row>
     <row r="1455" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1455" s="74">
@@ -18258,9 +18284,9 @@
         <v>111</v>
       </c>
       <c r="B1471" s="87"/>
-      <c r="C1471" s="169"/>
-      <c r="D1471" s="170"/>
-      <c r="E1471" s="170"/>
+      <c r="C1471" s="171"/>
+      <c r="D1471" s="172"/>
+      <c r="E1471" s="172"/>
     </row>
     <row r="1472" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1472" s="74">
@@ -18411,9 +18437,9 @@
         <v>112</v>
       </c>
       <c r="B1488" s="87"/>
-      <c r="C1488" s="169"/>
-      <c r="D1488" s="170"/>
-      <c r="E1488" s="170"/>
+      <c r="C1488" s="171"/>
+      <c r="D1488" s="172"/>
+      <c r="E1488" s="172"/>
     </row>
     <row r="1489" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1489" s="74">
@@ -18564,9 +18590,9 @@
         <v>113</v>
       </c>
       <c r="B1505" s="87"/>
-      <c r="C1505" s="169"/>
-      <c r="D1505" s="170"/>
-      <c r="E1505" s="170"/>
+      <c r="C1505" s="171"/>
+      <c r="D1505" s="172"/>
+      <c r="E1505" s="172"/>
     </row>
     <row r="1506" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1506" s="74">
@@ -18717,9 +18743,9 @@
         <v>114</v>
       </c>
       <c r="B1522" s="87"/>
-      <c r="C1522" s="169"/>
-      <c r="D1522" s="170"/>
-      <c r="E1522" s="170"/>
+      <c r="C1522" s="171"/>
+      <c r="D1522" s="172"/>
+      <c r="E1522" s="172"/>
     </row>
     <row r="1523" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1523" s="74">
@@ -18870,9 +18896,9 @@
         <v>95</v>
       </c>
       <c r="B1539" s="87"/>
-      <c r="C1539" s="169"/>
-      <c r="D1539" s="170"/>
-      <c r="E1539" s="170"/>
+      <c r="C1539" s="171"/>
+      <c r="D1539" s="172"/>
+      <c r="E1539" s="172"/>
     </row>
     <row r="1540" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1540" s="74">
@@ -19023,9 +19049,9 @@
         <v>115</v>
       </c>
       <c r="B1556" s="87"/>
-      <c r="C1556" s="169"/>
-      <c r="D1556" s="170"/>
-      <c r="E1556" s="170"/>
+      <c r="C1556" s="171"/>
+      <c r="D1556" s="172"/>
+      <c r="E1556" s="172"/>
     </row>
     <row r="1557" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1557" s="74">
@@ -19176,9 +19202,9 @@
         <v>116</v>
       </c>
       <c r="B1573" s="87"/>
-      <c r="C1573" s="169"/>
-      <c r="D1573" s="170"/>
-      <c r="E1573" s="170"/>
+      <c r="C1573" s="171"/>
+      <c r="D1573" s="172"/>
+      <c r="E1573" s="172"/>
     </row>
     <row r="1574" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1574" s="74">
@@ -19329,9 +19355,9 @@
         <v>117</v>
       </c>
       <c r="B1590" s="87"/>
-      <c r="C1590" s="169"/>
-      <c r="D1590" s="170"/>
-      <c r="E1590" s="170"/>
+      <c r="C1590" s="171"/>
+      <c r="D1590" s="172"/>
+      <c r="E1590" s="172"/>
     </row>
     <row r="1591" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1591" s="74">
@@ -19482,9 +19508,9 @@
         <v>118</v>
       </c>
       <c r="B1607" s="87"/>
-      <c r="C1607" s="169"/>
-      <c r="D1607" s="170"/>
-      <c r="E1607" s="170"/>
+      <c r="C1607" s="171"/>
+      <c r="D1607" s="172"/>
+      <c r="E1607" s="172"/>
     </row>
     <row r="1608" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1608" s="74">
@@ -19635,9 +19661,9 @@
         <v>119</v>
       </c>
       <c r="B1624" s="87"/>
-      <c r="C1624" s="169"/>
-      <c r="D1624" s="170"/>
-      <c r="E1624" s="170"/>
+      <c r="C1624" s="171"/>
+      <c r="D1624" s="172"/>
+      <c r="E1624" s="172"/>
     </row>
     <row r="1625" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1625" s="74">
@@ -19788,18 +19814,18 @@
         <v>120</v>
       </c>
       <c r="B1641" s="42"/>
-      <c r="C1641" s="183"/>
-      <c r="D1641" s="184"/>
-      <c r="E1641" s="184"/>
+      <c r="C1641" s="185"/>
+      <c r="D1641" s="186"/>
+      <c r="E1641" s="186"/>
     </row>
     <row r="1642" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A1642" s="78" t="s">
         <v>121</v>
       </c>
       <c r="B1642" s="87"/>
-      <c r="C1642" s="169"/>
-      <c r="D1642" s="170"/>
-      <c r="E1642" s="170"/>
+      <c r="C1642" s="171"/>
+      <c r="D1642" s="172"/>
+      <c r="E1642" s="172"/>
     </row>
     <row r="1643" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1643" s="79">
@@ -19950,9 +19976,9 @@
         <v>122</v>
       </c>
       <c r="B1659" s="90"/>
-      <c r="C1659" s="171"/>
-      <c r="D1659" s="172"/>
-      <c r="E1659" s="172"/>
+      <c r="C1659" s="173"/>
+      <c r="D1659" s="174"/>
+      <c r="E1659" s="174"/>
     </row>
     <row r="1660" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1660" s="79">
@@ -20103,9 +20129,9 @@
         <v>123</v>
       </c>
       <c r="B1676" s="87"/>
-      <c r="C1676" s="169"/>
-      <c r="D1676" s="170"/>
-      <c r="E1676" s="170"/>
+      <c r="C1676" s="171"/>
+      <c r="D1676" s="172"/>
+      <c r="E1676" s="172"/>
     </row>
     <row r="1677" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1677" s="79">
@@ -20256,9 +20282,9 @@
         <v>124</v>
       </c>
       <c r="B1693" s="87"/>
-      <c r="C1693" s="169"/>
-      <c r="D1693" s="170"/>
-      <c r="E1693" s="170"/>
+      <c r="C1693" s="171"/>
+      <c r="D1693" s="172"/>
+      <c r="E1693" s="172"/>
     </row>
     <row r="1694" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1694" s="79">
@@ -20409,9 +20435,9 @@
         <v>125</v>
       </c>
       <c r="B1710" s="87"/>
-      <c r="C1710" s="169"/>
-      <c r="D1710" s="170"/>
-      <c r="E1710" s="170"/>
+      <c r="C1710" s="171"/>
+      <c r="D1710" s="172"/>
+      <c r="E1710" s="172"/>
     </row>
     <row r="1711" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1711" s="79">
@@ -20562,9 +20588,9 @@
         <v>126</v>
       </c>
       <c r="B1727" s="87"/>
-      <c r="C1727" s="169"/>
-      <c r="D1727" s="170"/>
-      <c r="E1727" s="170"/>
+      <c r="C1727" s="171"/>
+      <c r="D1727" s="172"/>
+      <c r="E1727" s="172"/>
     </row>
     <row r="1728" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1728" s="79">
@@ -20715,9 +20741,9 @@
         <v>127</v>
       </c>
       <c r="B1744" s="87"/>
-      <c r="C1744" s="169"/>
-      <c r="D1744" s="170"/>
-      <c r="E1744" s="170"/>
+      <c r="C1744" s="171"/>
+      <c r="D1744" s="172"/>
+      <c r="E1744" s="172"/>
     </row>
     <row r="1745" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1745" s="79">
@@ -20868,9 +20894,9 @@
         <v>128</v>
       </c>
       <c r="B1761" s="87"/>
-      <c r="C1761" s="169"/>
-      <c r="D1761" s="170"/>
-      <c r="E1761" s="170"/>
+      <c r="C1761" s="171"/>
+      <c r="D1761" s="172"/>
+      <c r="E1761" s="172"/>
     </row>
     <row r="1762" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1762" s="79">
@@ -21021,9 +21047,9 @@
         <v>129</v>
       </c>
       <c r="B1778" s="87"/>
-      <c r="C1778" s="169"/>
-      <c r="D1778" s="170"/>
-      <c r="E1778" s="170"/>
+      <c r="C1778" s="171"/>
+      <c r="D1778" s="172"/>
+      <c r="E1778" s="172"/>
     </row>
     <row r="1779" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1779" s="79">
@@ -21174,9 +21200,9 @@
         <v>130</v>
       </c>
       <c r="B1795" s="87"/>
-      <c r="C1795" s="169"/>
-      <c r="D1795" s="170"/>
-      <c r="E1795" s="170"/>
+      <c r="C1795" s="171"/>
+      <c r="D1795" s="172"/>
+      <c r="E1795" s="172"/>
     </row>
     <row r="1796" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1796" s="79">
@@ -21327,9 +21353,9 @@
         <v>131</v>
       </c>
       <c r="B1812" s="87"/>
-      <c r="C1812" s="169"/>
-      <c r="D1812" s="170"/>
-      <c r="E1812" s="170"/>
+      <c r="C1812" s="171"/>
+      <c r="D1812" s="172"/>
+      <c r="E1812" s="172"/>
     </row>
     <row r="1813" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1813" s="79">
@@ -21480,9 +21506,9 @@
         <v>96</v>
       </c>
       <c r="B1829" s="87"/>
-      <c r="C1829" s="169"/>
-      <c r="D1829" s="170"/>
-      <c r="E1829" s="170"/>
+      <c r="C1829" s="171"/>
+      <c r="D1829" s="172"/>
+      <c r="E1829" s="172"/>
     </row>
     <row r="1830" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1830" s="79">
@@ -21633,9 +21659,9 @@
         <v>132</v>
       </c>
       <c r="B1846" s="87"/>
-      <c r="C1846" s="169"/>
-      <c r="D1846" s="170"/>
-      <c r="E1846" s="170"/>
+      <c r="C1846" s="171"/>
+      <c r="D1846" s="172"/>
+      <c r="E1846" s="172"/>
     </row>
     <row r="1847" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1847" s="79">
@@ -21786,9 +21812,9 @@
         <v>133</v>
       </c>
       <c r="B1863" s="87"/>
-      <c r="C1863" s="169"/>
-      <c r="D1863" s="170"/>
-      <c r="E1863" s="170"/>
+      <c r="C1863" s="171"/>
+      <c r="D1863" s="172"/>
+      <c r="E1863" s="172"/>
     </row>
     <row r="1864" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1864" s="79">
@@ -21939,9 +21965,9 @@
         <v>134</v>
       </c>
       <c r="B1880" s="87"/>
-      <c r="C1880" s="169"/>
-      <c r="D1880" s="170"/>
-      <c r="E1880" s="170"/>
+      <c r="C1880" s="171"/>
+      <c r="D1880" s="172"/>
+      <c r="E1880" s="172"/>
     </row>
     <row r="1881" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1881" s="79">
@@ -22092,9 +22118,9 @@
         <v>135</v>
       </c>
       <c r="B1897" s="87"/>
-      <c r="C1897" s="169"/>
-      <c r="D1897" s="170"/>
-      <c r="E1897" s="170"/>
+      <c r="C1897" s="171"/>
+      <c r="D1897" s="172"/>
+      <c r="E1897" s="172"/>
     </row>
     <row r="1898" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1898" s="79">
@@ -22245,18 +22271,18 @@
         <v>136</v>
       </c>
       <c r="B1914" s="43"/>
-      <c r="C1914" s="185"/>
-      <c r="D1914" s="186"/>
-      <c r="E1914" s="186"/>
+      <c r="C1914" s="187"/>
+      <c r="D1914" s="188"/>
+      <c r="E1914" s="188"/>
     </row>
     <row r="1915" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A1915" s="83" t="s">
         <v>137</v>
       </c>
       <c r="B1915" s="87"/>
-      <c r="C1915" s="169"/>
-      <c r="D1915" s="170"/>
-      <c r="E1915" s="170"/>
+      <c r="C1915" s="171"/>
+      <c r="D1915" s="172"/>
+      <c r="E1915" s="172"/>
     </row>
     <row r="1916" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1916" s="84">
@@ -22407,9 +22433,9 @@
         <v>138</v>
       </c>
       <c r="B1932" s="90"/>
-      <c r="C1932" s="171"/>
-      <c r="D1932" s="172"/>
-      <c r="E1932" s="172"/>
+      <c r="C1932" s="173"/>
+      <c r="D1932" s="174"/>
+      <c r="E1932" s="174"/>
     </row>
     <row r="1933" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1933" s="84">
@@ -22560,9 +22586,9 @@
         <v>139</v>
       </c>
       <c r="B1949" s="87"/>
-      <c r="C1949" s="169"/>
-      <c r="D1949" s="170"/>
-      <c r="E1949" s="170"/>
+      <c r="C1949" s="171"/>
+      <c r="D1949" s="172"/>
+      <c r="E1949" s="172"/>
     </row>
     <row r="1950" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1950" s="84">
@@ -22713,9 +22739,9 @@
         <v>140</v>
       </c>
       <c r="B1966" s="87"/>
-      <c r="C1966" s="169"/>
-      <c r="D1966" s="170"/>
-      <c r="E1966" s="170"/>
+      <c r="C1966" s="171"/>
+      <c r="D1966" s="172"/>
+      <c r="E1966" s="172"/>
     </row>
     <row r="1967" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1967" s="84">
@@ -22866,9 +22892,9 @@
         <v>141</v>
       </c>
       <c r="B1983" s="87"/>
-      <c r="C1983" s="169"/>
-      <c r="D1983" s="170"/>
-      <c r="E1983" s="170"/>
+      <c r="C1983" s="171"/>
+      <c r="D1983" s="172"/>
+      <c r="E1983" s="172"/>
     </row>
     <row r="1984" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1984" s="84">
@@ -23019,9 +23045,9 @@
         <v>142</v>
       </c>
       <c r="B2000" s="87"/>
-      <c r="C2000" s="169"/>
-      <c r="D2000" s="170"/>
-      <c r="E2000" s="170"/>
+      <c r="C2000" s="171"/>
+      <c r="D2000" s="172"/>
+      <c r="E2000" s="172"/>
     </row>
     <row r="2001" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2001" s="84">
@@ -23172,9 +23198,9 @@
         <v>143</v>
       </c>
       <c r="B2017" s="87"/>
-      <c r="C2017" s="169"/>
-      <c r="D2017" s="170"/>
-      <c r="E2017" s="170"/>
+      <c r="C2017" s="171"/>
+      <c r="D2017" s="172"/>
+      <c r="E2017" s="172"/>
     </row>
     <row r="2018" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2018" s="84">
@@ -23325,9 +23351,9 @@
         <v>144</v>
       </c>
       <c r="B2034" s="87"/>
-      <c r="C2034" s="169"/>
-      <c r="D2034" s="170"/>
-      <c r="E2034" s="170"/>
+      <c r="C2034" s="171"/>
+      <c r="D2034" s="172"/>
+      <c r="E2034" s="172"/>
     </row>
     <row r="2035" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2035" s="84">
@@ -23478,9 +23504,9 @@
         <v>145</v>
       </c>
       <c r="B2051" s="87"/>
-      <c r="C2051" s="169"/>
-      <c r="D2051" s="170"/>
-      <c r="E2051" s="170"/>
+      <c r="C2051" s="171"/>
+      <c r="D2051" s="172"/>
+      <c r="E2051" s="172"/>
     </row>
     <row r="2052" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2052" s="84">
@@ -23631,9 +23657,9 @@
         <v>146</v>
       </c>
       <c r="B2068" s="87"/>
-      <c r="C2068" s="169"/>
-      <c r="D2068" s="170"/>
-      <c r="E2068" s="170"/>
+      <c r="C2068" s="171"/>
+      <c r="D2068" s="172"/>
+      <c r="E2068" s="172"/>
     </row>
     <row r="2069" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2069" s="84">
@@ -23784,9 +23810,9 @@
         <v>147</v>
       </c>
       <c r="B2085" s="87"/>
-      <c r="C2085" s="169"/>
-      <c r="D2085" s="170"/>
-      <c r="E2085" s="170"/>
+      <c r="C2085" s="171"/>
+      <c r="D2085" s="172"/>
+      <c r="E2085" s="172"/>
     </row>
     <row r="2086" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2086" s="84">
@@ -23937,9 +23963,9 @@
         <v>148</v>
       </c>
       <c r="B2102" s="87"/>
-      <c r="C2102" s="169"/>
-      <c r="D2102" s="170"/>
-      <c r="E2102" s="170"/>
+      <c r="C2102" s="171"/>
+      <c r="D2102" s="172"/>
+      <c r="E2102" s="172"/>
     </row>
     <row r="2103" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2103" s="84">
@@ -24090,9 +24116,9 @@
         <v>97</v>
       </c>
       <c r="B2119" s="87"/>
-      <c r="C2119" s="169"/>
-      <c r="D2119" s="170"/>
-      <c r="E2119" s="170"/>
+      <c r="C2119" s="171"/>
+      <c r="D2119" s="172"/>
+      <c r="E2119" s="172"/>
     </row>
     <row r="2120" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2120" s="84">
@@ -24243,9 +24269,9 @@
         <v>149</v>
       </c>
       <c r="B2136" s="87"/>
-      <c r="C2136" s="169"/>
-      <c r="D2136" s="170"/>
-      <c r="E2136" s="170"/>
+      <c r="C2136" s="171"/>
+      <c r="D2136" s="172"/>
+      <c r="E2136" s="172"/>
     </row>
     <row r="2137" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2137" s="84">
@@ -24396,9 +24422,9 @@
         <v>150</v>
       </c>
       <c r="B2153" s="87"/>
-      <c r="C2153" s="169"/>
-      <c r="D2153" s="170"/>
-      <c r="E2153" s="170"/>
+      <c r="C2153" s="171"/>
+      <c r="D2153" s="172"/>
+      <c r="E2153" s="172"/>
     </row>
     <row r="2154" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2154" s="84">
@@ -24549,9 +24575,9 @@
         <v>151</v>
       </c>
       <c r="B2170" s="87"/>
-      <c r="C2170" s="169"/>
-      <c r="D2170" s="170"/>
-      <c r="E2170" s="170"/>
+      <c r="C2170" s="171"/>
+      <c r="D2170" s="172"/>
+      <c r="E2170" s="172"/>
     </row>
     <row r="2171" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2171" s="84">
@@ -24837,7 +24863,7 @@
     <mergeCell ref="C72:E72"/>
     <mergeCell ref="C208:E208"/>
   </mergeCells>
-  <phoneticPr fontId="8" type="noConversion"/>
+  <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967294" verticalDpi="0" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
@@ -24862,51 +24888,51 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="24" thickBot="1">
-      <c r="A1" s="193" t="s">
+      <c r="A1" s="195" t="s">
         <v>156</v>
       </c>
-      <c r="B1" s="193"/>
-      <c r="C1" s="193"/>
-      <c r="D1" s="193"/>
-      <c r="E1" s="193"/>
-      <c r="F1" s="193"/>
-      <c r="G1" s="193"/>
-      <c r="H1" s="193"/>
-      <c r="I1" s="193"/>
-      <c r="J1" s="193"/>
-      <c r="K1" s="193"/>
-      <c r="L1" s="193"/>
+      <c r="B1" s="195"/>
+      <c r="C1" s="195"/>
+      <c r="D1" s="195"/>
+      <c r="E1" s="195"/>
+      <c r="F1" s="195"/>
+      <c r="G1" s="195"/>
+      <c r="H1" s="195"/>
+      <c r="I1" s="195"/>
+      <c r="J1" s="195"/>
+      <c r="K1" s="195"/>
+      <c r="L1" s="195"/>
     </row>
     <row r="2" spans="1:12" ht="18.75" thickBot="1">
-      <c r="A2" s="190" t="s">
+      <c r="A2" s="192" t="s">
         <v>157</v>
       </c>
-      <c r="B2" s="191"/>
-      <c r="C2" s="191"/>
-      <c r="D2" s="191"/>
-      <c r="E2" s="191"/>
-      <c r="F2" s="191"/>
-      <c r="G2" s="191"/>
-      <c r="H2" s="191"/>
-      <c r="I2" s="191"/>
-      <c r="J2" s="191"/>
-      <c r="K2" s="191"/>
-      <c r="L2" s="192"/>
+      <c r="B2" s="193"/>
+      <c r="C2" s="193"/>
+      <c r="D2" s="193"/>
+      <c r="E2" s="193"/>
+      <c r="F2" s="193"/>
+      <c r="G2" s="193"/>
+      <c r="H2" s="193"/>
+      <c r="I2" s="193"/>
+      <c r="J2" s="193"/>
+      <c r="K2" s="193"/>
+      <c r="L2" s="194"/>
     </row>
     <row r="3" spans="1:12" s="31" customFormat="1" ht="16.5" customHeight="1" thickBot="1">
-      <c r="A3" s="187" t="s">
+      <c r="A3" s="189" t="s">
         <v>158</v>
       </c>
-      <c r="B3" s="188"/>
-      <c r="C3" s="188"/>
-      <c r="D3" s="188"/>
-      <c r="E3" s="188"/>
-      <c r="F3" s="188"/>
-      <c r="G3" s="188"/>
-      <c r="H3" s="188"/>
-      <c r="I3" s="188"/>
-      <c r="J3" s="188"/>
-      <c r="K3" s="189"/>
+      <c r="B3" s="190"/>
+      <c r="C3" s="190"/>
+      <c r="D3" s="190"/>
+      <c r="E3" s="190"/>
+      <c r="F3" s="190"/>
+      <c r="G3" s="190"/>
+      <c r="H3" s="190"/>
+      <c r="I3" s="190"/>
+      <c r="J3" s="190"/>
+      <c r="K3" s="191"/>
     </row>
     <row r="4" spans="1:12" s="27" customFormat="1">
       <c r="A4" s="28" t="s">
@@ -25123,19 +25149,19 @@
       <c r="K19" s="2"/>
     </row>
     <row r="20" spans="1:11" ht="18" customHeight="1" thickBot="1">
-      <c r="A20" s="187" t="s">
+      <c r="A20" s="189" t="s">
         <v>166</v>
       </c>
-      <c r="B20" s="188"/>
-      <c r="C20" s="188"/>
-      <c r="D20" s="188"/>
-      <c r="E20" s="188"/>
-      <c r="F20" s="188"/>
-      <c r="G20" s="188"/>
-      <c r="H20" s="188"/>
-      <c r="I20" s="188"/>
-      <c r="J20" s="188"/>
-      <c r="K20" s="189"/>
+      <c r="B20" s="190"/>
+      <c r="C20" s="190"/>
+      <c r="D20" s="190"/>
+      <c r="E20" s="190"/>
+      <c r="F20" s="190"/>
+      <c r="G20" s="190"/>
+      <c r="H20" s="190"/>
+      <c r="I20" s="190"/>
+      <c r="J20" s="190"/>
+      <c r="K20" s="191"/>
     </row>
     <row r="21" spans="1:11">
       <c r="A21" s="28" t="s">
@@ -25352,19 +25378,19 @@
       <c r="K36" s="2"/>
     </row>
     <row r="37" spans="1:11" ht="18" customHeight="1" thickBot="1">
-      <c r="A37" s="187" t="s">
+      <c r="A37" s="189" t="s">
         <v>167</v>
       </c>
-      <c r="B37" s="188"/>
-      <c r="C37" s="188"/>
-      <c r="D37" s="188"/>
-      <c r="E37" s="188"/>
-      <c r="F37" s="188"/>
-      <c r="G37" s="188"/>
-      <c r="H37" s="188"/>
-      <c r="I37" s="188"/>
-      <c r="J37" s="188"/>
-      <c r="K37" s="189"/>
+      <c r="B37" s="190"/>
+      <c r="C37" s="190"/>
+      <c r="D37" s="190"/>
+      <c r="E37" s="190"/>
+      <c r="F37" s="190"/>
+      <c r="G37" s="190"/>
+      <c r="H37" s="190"/>
+      <c r="I37" s="190"/>
+      <c r="J37" s="190"/>
+      <c r="K37" s="191"/>
     </row>
     <row r="38" spans="1:11">
       <c r="A38" s="28" t="s">
@@ -25588,7 +25614,7 @@
     <mergeCell ref="A3:K3"/>
     <mergeCell ref="A20:K20"/>
   </mergeCells>
-  <phoneticPr fontId="8" type="noConversion"/>
+  <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
@@ -25622,28 +25648,28 @@
       </c>
     </row>
     <row r="3" spans="1:1">
-      <c r="A3" s="194"/>
+      <c r="A3" s="196"/>
     </row>
     <row r="4" spans="1:1">
-      <c r="A4" s="195"/>
+      <c r="A4" s="197"/>
     </row>
     <row r="5" spans="1:1">
-      <c r="A5" s="195"/>
+      <c r="A5" s="197"/>
     </row>
     <row r="6" spans="1:1">
-      <c r="A6" s="195"/>
+      <c r="A6" s="197"/>
     </row>
     <row r="7" spans="1:1">
-      <c r="A7" s="195"/>
+      <c r="A7" s="197"/>
     </row>
     <row r="8" spans="1:1">
-      <c r="A8" s="195"/>
+      <c r="A8" s="197"/>
     </row>
     <row r="9" spans="1:1">
-      <c r="A9" s="195"/>
+      <c r="A9" s="197"/>
     </row>
     <row r="10" spans="1:1" ht="13.5" thickBot="1">
-      <c r="A10" s="196"/>
+      <c r="A10" s="198"/>
     </row>
     <row r="11" spans="1:1" ht="27" customHeight="1">
       <c r="A11" s="22" t="s">
@@ -25799,7 +25825,7 @@
   <mergeCells count="1">
     <mergeCell ref="A3:A10"/>
   </mergeCells>
-  <phoneticPr fontId="8" type="noConversion"/>
+  <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
@@ -25826,10 +25852,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="4" customFormat="1" ht="25.5" customHeight="1" thickBot="1">
-      <c r="B1" s="197" t="s">
+      <c r="B1" s="199" t="s">
         <v>162</v>
       </c>
-      <c r="C1" s="198"/>
+      <c r="C1" s="200"/>
       <c r="D1" s="92"/>
       <c r="E1" s="32"/>
     </row>
@@ -25840,7 +25866,7 @@
       <c r="E2" s="119"/>
     </row>
     <row r="3" spans="1:5" ht="12.75" customHeight="1">
-      <c r="A3" s="199" t="s">
+      <c r="A3" s="201" t="s">
         <v>202</v>
       </c>
       <c r="B3" s="131" t="s">
@@ -25854,7 +25880,7 @@
       <c r="E3" s="5"/>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="200"/>
+      <c r="A4" s="202"/>
       <c r="B4" s="128" t="s">
         <v>159</v>
       </c>
@@ -25866,7 +25892,7 @@
       <c r="E4" s="5"/>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="200"/>
+      <c r="A5" s="202"/>
       <c r="B5" s="128" t="s">
         <v>160</v>
       </c>
@@ -25875,7 +25901,7 @@
       <c r="E5" s="5"/>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="200"/>
+      <c r="A6" s="202"/>
       <c r="B6" s="139" t="s">
         <v>204</v>
       </c>
@@ -25887,7 +25913,7 @@
       <c r="E6" s="5"/>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="200"/>
+      <c r="A7" s="202"/>
       <c r="B7" s="128" t="s">
         <v>171</v>
       </c>
@@ -25899,7 +25925,7 @@
       <c r="E7" s="5"/>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="200"/>
+      <c r="A8" s="202"/>
       <c r="B8" s="128" t="s">
         <v>172</v>
       </c>
@@ -25908,7 +25934,7 @@
       <c r="E8" s="5"/>
     </row>
     <row r="9" spans="1:5" ht="13.5" thickBot="1">
-      <c r="A9" s="201"/>
+      <c r="A9" s="203"/>
       <c r="B9" s="136" t="s">
         <v>161</v>
       </c>
@@ -25923,7 +25949,7 @@
       <c r="E10" s="94"/>
     </row>
     <row r="11" spans="1:5" ht="19.5" customHeight="1">
-      <c r="A11" s="199" t="s">
+      <c r="A11" s="201" t="s">
         <v>203</v>
       </c>
       <c r="B11" s="131" t="s">
@@ -25937,7 +25963,7 @@
       <c r="E11" s="5"/>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="200"/>
+      <c r="A12" s="202"/>
       <c r="B12" s="128" t="s">
         <v>159</v>
       </c>
@@ -25949,7 +25975,7 @@
       <c r="E12" s="5"/>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" s="200"/>
+      <c r="A13" s="202"/>
       <c r="B13" s="128" t="s">
         <v>160</v>
       </c>
@@ -25958,7 +25984,7 @@
       <c r="E13" s="5"/>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="200"/>
+      <c r="A14" s="202"/>
       <c r="B14" s="139" t="s">
         <v>204</v>
       </c>
@@ -25970,7 +25996,7 @@
       <c r="E14" s="5"/>
     </row>
     <row r="15" spans="1:5">
-      <c r="A15" s="200"/>
+      <c r="A15" s="202"/>
       <c r="B15" s="128" t="s">
         <v>171</v>
       </c>
@@ -25982,7 +26008,7 @@
       <c r="E15" s="5"/>
     </row>
     <row r="16" spans="1:5">
-      <c r="A16" s="200"/>
+      <c r="A16" s="202"/>
       <c r="B16" s="128" t="s">
         <v>172</v>
       </c>
@@ -25991,7 +26017,7 @@
       <c r="E16" s="5"/>
     </row>
     <row r="17" spans="1:5" ht="13.5" thickBot="1">
-      <c r="A17" s="201"/>
+      <c r="A17" s="203"/>
       <c r="B17" s="136" t="s">
         <v>161</v>
       </c>
@@ -26006,7 +26032,7 @@
       <c r="E18" s="94"/>
     </row>
     <row r="19" spans="1:5" collapsed="1">
-      <c r="A19" s="199" t="s">
+      <c r="A19" s="201" t="s">
         <v>203</v>
       </c>
       <c r="B19" s="131" t="s">
@@ -26015,7 +26041,7 @@
       <c r="C19" s="130"/>
     </row>
     <row r="20" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A20" s="200"/>
+      <c r="A20" s="202"/>
       <c r="B20" s="128" t="s">
         <v>159</v>
       </c>
@@ -26025,14 +26051,14 @@
       </c>
     </row>
     <row r="21" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A21" s="200"/>
+      <c r="A21" s="202"/>
       <c r="B21" s="128" t="s">
         <v>160</v>
       </c>
       <c r="C21" s="133"/>
     </row>
     <row r="22" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A22" s="200"/>
+      <c r="A22" s="202"/>
       <c r="B22" s="139" t="s">
         <v>204</v>
       </c>
@@ -26042,7 +26068,7 @@
       </c>
     </row>
     <row r="23" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A23" s="200"/>
+      <c r="A23" s="202"/>
       <c r="B23" s="128" t="s">
         <v>171</v>
       </c>
@@ -26052,14 +26078,14 @@
       </c>
     </row>
     <row r="24" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A24" s="200"/>
+      <c r="A24" s="202"/>
       <c r="B24" s="128" t="s">
         <v>172</v>
       </c>
       <c r="C24" s="132"/>
     </row>
     <row r="25" spans="1:5" ht="13.5" thickBot="1">
-      <c r="A25" s="201"/>
+      <c r="A25" s="203"/>
       <c r="B25" s="136" t="s">
         <v>161</v>
       </c>
@@ -26072,7 +26098,7 @@
     <mergeCell ref="A11:A17"/>
     <mergeCell ref="A19:A25"/>
   </mergeCells>
-  <phoneticPr fontId="8" type="noConversion"/>
+  <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
@@ -26094,147 +26120,147 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="33">
-      <c r="A1" s="212" t="s">
+      <c r="A1" s="214" t="s">
         <v>184</v>
       </c>
-      <c r="B1" s="213"/>
+      <c r="B1" s="215"/>
       <c r="C1" s="118"/>
       <c r="D1" s="5"/>
       <c r="E1" s="5"/>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="218" t="s">
+      <c r="A2" s="220" t="s">
         <v>183</v>
       </c>
-      <c r="B2" s="219"/>
+      <c r="B2" s="221"/>
       <c r="C2" s="120"/>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="220" t="s">
+      <c r="A3" s="222" t="s">
         <v>185</v>
       </c>
-      <c r="B3" s="219"/>
+      <c r="B3" s="221"/>
       <c r="C3" s="120"/>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="216"/>
-      <c r="B4" s="217"/>
+      <c r="A4" s="218"/>
+      <c r="B4" s="219"/>
       <c r="C4" s="120"/>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="214" t="s">
+      <c r="A5" s="216" t="s">
         <v>194</v>
       </c>
-      <c r="B5" s="215"/>
+      <c r="B5" s="217"/>
       <c r="C5" s="120"/>
     </row>
     <row r="7" spans="1:5" ht="18.75">
-      <c r="A7" s="206" t="s">
+      <c r="A7" s="208" t="s">
         <v>186</v>
       </c>
-      <c r="B7" s="207"/>
+      <c r="B7" s="209"/>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="120"/>
       <c r="B8" s="9"/>
     </row>
     <row r="9" spans="1:5" ht="39" customHeight="1">
-      <c r="A9" s="208" t="s">
+      <c r="A9" s="210" t="s">
         <v>187</v>
       </c>
-      <c r="B9" s="209"/>
+      <c r="B9" s="211"/>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="210"/>
-      <c r="B10" s="211"/>
+      <c r="A10" s="212"/>
+      <c r="B10" s="213"/>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="202" t="s">
+      <c r="A11" s="204" t="s">
         <v>188</v>
       </c>
-      <c r="B11" s="203"/>
+      <c r="B11" s="205"/>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="202" t="s">
+      <c r="A12" s="204" t="s">
         <v>189</v>
       </c>
-      <c r="B12" s="203"/>
+      <c r="B12" s="205"/>
     </row>
     <row r="13" spans="1:5" ht="43.5" customHeight="1">
-      <c r="A13" s="202" t="s">
+      <c r="A13" s="204" t="s">
         <v>190</v>
       </c>
-      <c r="B13" s="203"/>
+      <c r="B13" s="205"/>
     </row>
     <row r="14" spans="1:5" ht="19.5" customHeight="1">
-      <c r="A14" s="202" t="s">
+      <c r="A14" s="204" t="s">
         <v>191</v>
       </c>
-      <c r="B14" s="203"/>
+      <c r="B14" s="205"/>
     </row>
     <row r="15" spans="1:5" ht="18" customHeight="1">
-      <c r="A15" s="202" t="s">
+      <c r="A15" s="204" t="s">
         <v>192</v>
       </c>
-      <c r="B15" s="203"/>
+      <c r="B15" s="205"/>
     </row>
     <row r="16" spans="1:5" ht="21" customHeight="1">
-      <c r="A16" s="202" t="s">
+      <c r="A16" s="204" t="s">
         <v>193</v>
       </c>
-      <c r="B16" s="203"/>
+      <c r="B16" s="205"/>
     </row>
     <row r="17" spans="1:2" ht="48.75" customHeight="1">
-      <c r="A17" s="204" t="s">
+      <c r="A17" s="206" t="s">
         <v>195</v>
       </c>
-      <c r="B17" s="205"/>
+      <c r="B17" s="207"/>
     </row>
     <row r="19" spans="1:2" ht="18.75">
-      <c r="A19" s="206" t="s">
+      <c r="A19" s="208" t="s">
         <v>197</v>
       </c>
-      <c r="B19" s="207"/>
+      <c r="B19" s="209"/>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="120"/>
       <c r="B20" s="9"/>
     </row>
     <row r="21" spans="1:2">
-      <c r="A21" s="208" t="s">
+      <c r="A21" s="210" t="s">
         <v>198</v>
       </c>
-      <c r="B21" s="209"/>
+      <c r="B21" s="211"/>
     </row>
     <row r="22" spans="1:2">
-      <c r="A22" s="210"/>
-      <c r="B22" s="211"/>
+      <c r="A22" s="212"/>
+      <c r="B22" s="213"/>
     </row>
     <row r="23" spans="1:2">
-      <c r="A23" s="202" t="s">
+      <c r="A23" s="204" t="s">
         <v>199</v>
       </c>
-      <c r="B23" s="203"/>
+      <c r="B23" s="205"/>
     </row>
     <row r="24" spans="1:2">
-      <c r="A24" s="202"/>
-      <c r="B24" s="203"/>
+      <c r="A24" s="204"/>
+      <c r="B24" s="205"/>
     </row>
     <row r="25" spans="1:2">
-      <c r="A25" s="202" t="s">
+      <c r="A25" s="204" t="s">
         <v>200</v>
       </c>
-      <c r="B25" s="203"/>
+      <c r="B25" s="205"/>
     </row>
     <row r="26" spans="1:2">
-      <c r="A26" s="202" t="s">
+      <c r="A26" s="204" t="s">
         <v>201</v>
       </c>
-      <c r="B26" s="203"/>
+      <c r="B26" s="205"/>
     </row>
     <row r="27" spans="1:2">
-      <c r="A27" s="204"/>
-      <c r="B27" s="205"/>
+      <c r="A27" s="206"/>
+      <c r="B27" s="207"/>
     </row>
   </sheetData>
   <mergeCells count="23">

</xml_diff>

<commit_message>
Tempo - redo of stage 3 complete - 58 frames ahead compared to the previous stage 3 end.
</commit_message>
<xml_diff>
--- a/trunk/Tempo/Tempo.xlsx
+++ b/trunk/Tempo/Tempo.xlsx
@@ -2210,29 +2210,29 @@
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="21" fillId="13" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="22" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="21" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="10" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="21" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="21" fillId="13" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="22" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="12" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="12" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="12" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -2268,34 +2268,20 @@
     <xf numFmtId="0" fontId="51" fillId="22" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="48" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="49" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="49" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="47" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="47" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="45" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="4"/>
     </xf>
@@ -2305,6 +2291,20 @@
     <xf numFmtId="0" fontId="46" fillId="0" borderId="33" xfId="3" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" indent="4"/>
     </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="47" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="47" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="49" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="49" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="48" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Accent1" xfId="2" builtinId="29"/>
@@ -2616,7 +2616,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C52" sqref="C52"/>
+      <selection pane="bottomLeft" activeCell="C58" sqref="C58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" outlineLevelRow="2"/>
@@ -3437,7 +3437,7 @@
         <v>13556</v>
       </c>
     </row>
-    <row r="49" spans="1:8" ht="15" outlineLevel="1">
+    <row r="49" spans="1:9" ht="15" outlineLevel="1">
       <c r="A49" s="159"/>
       <c r="B49" s="149" t="s">
         <v>222</v>
@@ -3457,7 +3457,7 @@
         <v>14149</v>
       </c>
     </row>
-    <row r="50" spans="1:8" ht="15" outlineLevel="1">
+    <row r="50" spans="1:9" ht="15" outlineLevel="1">
       <c r="A50" s="159"/>
       <c r="B50" s="156" t="s">
         <v>275</v>
@@ -3469,7 +3469,7 @@
       <c r="E50" s="123"/>
       <c r="F50" s="105"/>
     </row>
-    <row r="51" spans="1:8" ht="15" outlineLevel="1">
+    <row r="51" spans="1:9" ht="15" outlineLevel="1">
       <c r="A51" s="159"/>
       <c r="B51" s="150" t="s">
         <v>229</v>
@@ -3488,110 +3488,156 @@
       <c r="H51">
         <v>14517</v>
       </c>
-    </row>
-    <row r="52" spans="1:8" ht="15" outlineLevel="1">
+      <c r="I51" s="112">
+        <f>H51-C51</f>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" ht="15" outlineLevel="1">
       <c r="A52" s="159"/>
       <c r="B52" s="150" t="s">
         <v>230</v>
       </c>
       <c r="C52" s="101">
-        <v>14945</v>
+        <v>14896</v>
       </c>
       <c r="D52" s="101">
         <v>17856</v>
       </c>
       <c r="E52" s="123">
         <f t="shared" si="3"/>
-        <v>2911</v>
+        <v>2960</v>
       </c>
       <c r="F52" s="105"/>
-    </row>
-    <row r="53" spans="1:8" ht="15" outlineLevel="1">
+      <c r="H52" s="101">
+        <v>14945</v>
+      </c>
+      <c r="I52" s="112">
+        <f t="shared" ref="I52:I57" si="4">H52-C52</f>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" ht="15" outlineLevel="1">
       <c r="A53" s="159"/>
       <c r="B53" s="150" t="s">
         <v>231</v>
       </c>
       <c r="C53" s="101">
-        <v>15393</v>
+        <v>15340</v>
       </c>
       <c r="D53" s="101">
         <v>18332</v>
       </c>
       <c r="E53" s="123">
         <f t="shared" si="3"/>
-        <v>2939</v>
+        <v>2992</v>
       </c>
       <c r="F53" s="105"/>
-    </row>
-    <row r="54" spans="1:8" ht="15" outlineLevel="1">
+      <c r="H53" s="101">
+        <v>15393</v>
+      </c>
+      <c r="I53" s="112">
+        <f t="shared" si="4"/>
+        <v>53</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" ht="15" outlineLevel="1">
       <c r="A54" s="159"/>
       <c r="B54" s="150" t="s">
         <v>233</v>
       </c>
       <c r="C54" s="101">
-        <v>15797</v>
+        <v>15744</v>
       </c>
       <c r="D54" s="101">
         <v>18738</v>
       </c>
       <c r="E54" s="123">
         <f t="shared" si="3"/>
-        <v>2941</v>
+        <v>2994</v>
       </c>
       <c r="F54" s="105"/>
-    </row>
-    <row r="55" spans="1:8" ht="15" outlineLevel="1">
+      <c r="H54" s="101">
+        <v>15797</v>
+      </c>
+      <c r="I54" s="112">
+        <f t="shared" si="4"/>
+        <v>53</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" ht="15" outlineLevel="1">
       <c r="A55" s="159"/>
       <c r="B55" s="150" t="s">
         <v>234</v>
       </c>
       <c r="C55" s="101">
-        <v>16590</v>
+        <v>16532</v>
       </c>
       <c r="D55" s="101">
         <v>19757</v>
       </c>
       <c r="E55" s="123">
         <f t="shared" si="3"/>
-        <v>3167</v>
+        <v>3225</v>
       </c>
       <c r="F55" s="105"/>
-    </row>
-    <row r="56" spans="1:8" ht="15" outlineLevel="1">
+      <c r="H55" s="101">
+        <v>16590</v>
+      </c>
+      <c r="I55" s="112">
+        <f t="shared" si="4"/>
+        <v>58</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" ht="15" outlineLevel="1">
       <c r="A56" s="159"/>
       <c r="B56" s="150" t="s">
         <v>235</v>
       </c>
       <c r="C56" s="101">
-        <v>17005</v>
+        <v>16947</v>
       </c>
       <c r="D56" s="101">
         <v>20174</v>
       </c>
       <c r="E56" s="123">
         <f t="shared" si="3"/>
-        <v>3169</v>
+        <v>3227</v>
       </c>
       <c r="F56" s="105"/>
-    </row>
-    <row r="57" spans="1:8" ht="15" outlineLevel="1">
+      <c r="H56" s="101">
+        <v>17005</v>
+      </c>
+      <c r="I56" s="112">
+        <f t="shared" si="4"/>
+        <v>58</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" ht="15" outlineLevel="1">
       <c r="A57" s="159"/>
       <c r="B57" s="150" t="s">
         <v>236</v>
       </c>
       <c r="C57" s="101">
-        <v>17761</v>
+        <v>17703</v>
       </c>
       <c r="D57" s="101">
         <v>20965</v>
       </c>
       <c r="E57" s="123">
         <f t="shared" si="3"/>
-        <v>3204</v>
+        <v>3262</v>
       </c>
       <c r="F57" s="105"/>
-    </row>
-    <row r="58" spans="1:8" ht="15" outlineLevel="1">
+      <c r="H57" s="101">
+        <v>17761</v>
+      </c>
+      <c r="I57" s="112">
+        <f t="shared" si="4"/>
+        <v>58</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" ht="15" outlineLevel="1">
       <c r="A58" s="159"/>
       <c r="B58" s="100"/>
       <c r="C58" s="101"/>
@@ -3602,7 +3648,7 @@
       </c>
       <c r="F58" s="105"/>
     </row>
-    <row r="59" spans="1:8" ht="15" outlineLevel="1">
+    <row r="59" spans="1:9" ht="15" outlineLevel="1">
       <c r="A59" s="159"/>
       <c r="B59" s="100"/>
       <c r="C59" s="101"/>
@@ -3613,7 +3659,7 @@
       </c>
       <c r="F59" s="105"/>
     </row>
-    <row r="60" spans="1:8" ht="15" outlineLevel="1">
+    <row r="60" spans="1:9" ht="15" outlineLevel="1">
       <c r="A60" s="159"/>
       <c r="B60" s="150" t="s">
         <v>237</v>
@@ -3626,7 +3672,7 @@
       </c>
       <c r="F60" s="105"/>
     </row>
-    <row r="61" spans="1:8" ht="15" outlineLevel="1">
+    <row r="61" spans="1:9" ht="15" outlineLevel="1">
       <c r="A61" s="159"/>
       <c r="B61" s="150" t="s">
         <v>223</v>
@@ -3641,7 +3687,7 @@
       </c>
       <c r="F61" s="105"/>
     </row>
-    <row r="62" spans="1:8" ht="15" outlineLevel="1">
+    <row r="62" spans="1:9" ht="15" outlineLevel="1">
       <c r="A62" s="159"/>
       <c r="B62" s="150" t="s">
         <v>238</v>
@@ -3656,7 +3702,7 @@
       </c>
       <c r="F62" s="105"/>
     </row>
-    <row r="63" spans="1:8" ht="15" outlineLevel="1">
+    <row r="63" spans="1:9" ht="15" outlineLevel="1">
       <c r="A63" s="159"/>
       <c r="B63" s="150" t="s">
         <v>239</v>
@@ -3668,7 +3714,7 @@
       <c r="E63" s="123"/>
       <c r="F63" s="105"/>
     </row>
-    <row r="64" spans="1:8" ht="15" outlineLevel="1">
+    <row r="64" spans="1:9" ht="15" outlineLevel="1">
       <c r="A64" s="159"/>
       <c r="B64" s="150" t="s">
         <v>217</v>
@@ -3754,7 +3800,7 @@
         <v>25174</v>
       </c>
       <c r="E69" s="123">
-        <f t="shared" ref="E69:E81" si="4">IF(AND(C69&gt;0,D69&gt;0), D69-C69, 0)</f>
+        <f t="shared" ref="E69:E81" si="5">IF(AND(C69&gt;0,D69&gt;0), D69-C69, 0)</f>
         <v>0</v>
       </c>
       <c r="F69" s="104"/>
@@ -3768,7 +3814,7 @@
       <c r="C70" s="101"/>
       <c r="D70" s="101"/>
       <c r="E70" s="124">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F70" s="105"/>
@@ -3783,7 +3829,7 @@
         <v>26754</v>
       </c>
       <c r="E71" s="123">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F71" s="105"/>
@@ -3794,7 +3840,7 @@
       <c r="C72" s="101"/>
       <c r="D72" s="101"/>
       <c r="E72" s="123">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F72" s="105"/>
@@ -3809,7 +3855,7 @@
         <v>27765</v>
       </c>
       <c r="E73" s="123">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F73" s="105"/>
@@ -3820,7 +3866,7 @@
       <c r="C74" s="101"/>
       <c r="D74" s="101"/>
       <c r="E74" s="123">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F74" s="105"/>
@@ -3835,7 +3881,7 @@
         <v>30127</v>
       </c>
       <c r="E75" s="123">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F75" s="105"/>
@@ -3846,7 +3892,7 @@
       <c r="C76" s="101"/>
       <c r="D76" s="101"/>
       <c r="E76" s="123">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F76" s="105"/>
@@ -3861,7 +3907,7 @@
         <v>33299</v>
       </c>
       <c r="E77" s="123">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F77" s="105"/>
@@ -3876,7 +3922,7 @@
         <v>33527</v>
       </c>
       <c r="E78" s="123">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F78" s="105"/>
@@ -3891,7 +3937,7 @@
         <v>34309</v>
       </c>
       <c r="E79" s="123">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F79" s="105"/>
@@ -3906,7 +3952,7 @@
         <v>34727</v>
       </c>
       <c r="E80" s="123">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F80" s="105"/>
@@ -3921,7 +3967,7 @@
         <v>34795</v>
       </c>
       <c r="E81" s="125">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F81" s="104"/>
@@ -3982,7 +4028,7 @@
         <v>34795</v>
       </c>
       <c r="E85" s="123">
-        <f t="shared" ref="E85:E98" si="5">IF(AND(C85&gt;0,D85&gt;0), D85-C85, 0)</f>
+        <f t="shared" ref="E85:E98" si="6">IF(AND(C85&gt;0,D85&gt;0), D85-C85, 0)</f>
         <v>0</v>
       </c>
       <c r="F85" s="104"/>
@@ -4000,7 +4046,7 @@
         <v>36326</v>
       </c>
       <c r="E86" s="124">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="F86" s="105"/>
@@ -4015,7 +4061,7 @@
         <v>37764</v>
       </c>
       <c r="E87" s="123">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="F87" s="105"/>
@@ -4026,7 +4072,7 @@
       <c r="C88" s="101"/>
       <c r="D88" s="101"/>
       <c r="E88" s="123">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="F88" s="105"/>
@@ -4041,7 +4087,7 @@
         <v>43241</v>
       </c>
       <c r="E89" s="123">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="F89" s="105"/>
@@ -4052,7 +4098,7 @@
       <c r="C90" s="101"/>
       <c r="D90" s="101"/>
       <c r="E90" s="123">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="F90" s="105"/>
@@ -4067,7 +4113,7 @@
         <v>45890</v>
       </c>
       <c r="E91" s="123">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="F91" s="105"/>
@@ -4078,7 +4124,7 @@
       <c r="C92" s="101"/>
       <c r="D92" s="101"/>
       <c r="E92" s="123">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="F92" s="105"/>
@@ -4089,7 +4135,7 @@
       <c r="C93" s="101"/>
       <c r="D93" s="101"/>
       <c r="E93" s="123">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="F93" s="105"/>
@@ -4104,7 +4150,7 @@
         <v>49269</v>
       </c>
       <c r="E94" s="123">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="F94" s="105"/>
@@ -4119,7 +4165,7 @@
         <v>49505</v>
       </c>
       <c r="E95" s="123">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="F95" s="105"/>
@@ -4134,7 +4180,7 @@
         <v>50134</v>
       </c>
       <c r="E96" s="123">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="F96" s="105"/>
@@ -4149,7 +4195,7 @@
         <v>50516</v>
       </c>
       <c r="E97" s="123">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="F97" s="105"/>
@@ -4164,7 +4210,7 @@
         <v>50574</v>
       </c>
       <c r="E98" s="125">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="F98" s="104"/>
@@ -4225,7 +4271,7 @@
         <v>50574</v>
       </c>
       <c r="E102" s="123">
-        <f t="shared" ref="E102:E111" si="6">IF(AND(C102&gt;0,D102&gt;0), D102-C102, 0)</f>
+        <f t="shared" ref="E102:E111" si="7">IF(AND(C102&gt;0,D102&gt;0), D102-C102, 0)</f>
         <v>0</v>
       </c>
       <c r="F102" s="104"/>
@@ -4239,7 +4285,7 @@
       <c r="C103" s="101"/>
       <c r="D103" s="101"/>
       <c r="E103" s="124">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="F103" s="105"/>
@@ -4254,7 +4300,7 @@
         <v>52785</v>
       </c>
       <c r="E104" s="123">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="F104" s="105"/>
@@ -4265,7 +4311,7 @@
       <c r="C105" s="101"/>
       <c r="D105" s="101"/>
       <c r="E105" s="123">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="F105" s="105"/>
@@ -4280,7 +4326,7 @@
         <v>53409</v>
       </c>
       <c r="E106" s="123">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="F106" s="105"/>
@@ -4291,7 +4337,7 @@
       <c r="C107" s="101"/>
       <c r="D107" s="101"/>
       <c r="E107" s="123">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="F107" s="105"/>
@@ -4306,7 +4352,7 @@
         <v>55728</v>
       </c>
       <c r="E108" s="123">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="F108" s="105"/>
@@ -4321,7 +4367,7 @@
         <v>55956</v>
       </c>
       <c r="E109" s="123">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="F109" s="105"/>
@@ -4336,7 +4382,7 @@
         <v>56314</v>
       </c>
       <c r="E110" s="123">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="F110" s="105"/>
@@ -4351,7 +4397,7 @@
         <v>56373</v>
       </c>
       <c r="E111" s="125">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="F111" s="104"/>
@@ -4412,7 +4458,7 @@
         <v>56373</v>
       </c>
       <c r="E115" s="123">
-        <f t="shared" ref="E115:E123" si="7">IF(AND(C115&gt;0,D115&gt;0), D115-C115, 0)</f>
+        <f t="shared" ref="E115:E123" si="8">IF(AND(C115&gt;0,D115&gt;0), D115-C115, 0)</f>
         <v>0</v>
       </c>
       <c r="F115" s="104"/>
@@ -4430,7 +4476,7 @@
       <c r="C116" s="101"/>
       <c r="D116" s="101"/>
       <c r="E116" s="124">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="F116" s="105"/>
@@ -4445,7 +4491,7 @@
         <v>58041</v>
       </c>
       <c r="E117" s="123">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="F117" s="105"/>
@@ -4456,7 +4502,7 @@
       <c r="C118" s="101"/>
       <c r="D118" s="101"/>
       <c r="E118" s="123">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="F118" s="105"/>
@@ -4471,7 +4517,7 @@
         <v>60301</v>
       </c>
       <c r="E119" s="123">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="F119" s="105"/>
@@ -4486,7 +4532,7 @@
         <v>60529</v>
       </c>
       <c r="E120" s="123">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="F120" s="105"/>
@@ -4501,7 +4547,7 @@
         <v>61068</v>
       </c>
       <c r="E121" s="123">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="F121" s="105"/>
@@ -4516,7 +4562,7 @@
         <v>61391</v>
       </c>
       <c r="E122" s="123">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="F122" s="105"/>
@@ -4531,7 +4577,7 @@
         <v>61438</v>
       </c>
       <c r="E123" s="125">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="F123" s="104"/>
@@ -4592,7 +4638,7 @@
         <v>61438</v>
       </c>
       <c r="E127" s="123">
-        <f t="shared" ref="E127:E140" si="8">IF(AND(C127&gt;0,D127&gt;0), D127-C127, 0)</f>
+        <f t="shared" ref="E127:E140" si="9">IF(AND(C127&gt;0,D127&gt;0), D127-C127, 0)</f>
         <v>0</v>
       </c>
       <c r="F127" s="104"/>
@@ -4610,7 +4656,7 @@
       <c r="C128" s="101"/>
       <c r="D128" s="101"/>
       <c r="E128" s="124">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="F128" s="105"/>
@@ -4621,7 +4667,7 @@
       <c r="C129" s="101"/>
       <c r="D129" s="101"/>
       <c r="E129" s="123">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="F129" s="105"/>
@@ -4632,7 +4678,7 @@
       <c r="C130" s="101"/>
       <c r="D130" s="101"/>
       <c r="E130" s="123">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="F130" s="105"/>
@@ -4643,7 +4689,7 @@
       <c r="C131" s="101"/>
       <c r="D131" s="101"/>
       <c r="E131" s="123">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="F131" s="105"/>
@@ -4654,7 +4700,7 @@
       <c r="C132" s="101"/>
       <c r="D132" s="101"/>
       <c r="E132" s="123">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="F132" s="105"/>
@@ -4665,7 +4711,7 @@
       <c r="C133" s="101"/>
       <c r="D133" s="101"/>
       <c r="E133" s="123">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="F133" s="105"/>
@@ -4676,7 +4722,7 @@
       <c r="C134" s="101"/>
       <c r="D134" s="101"/>
       <c r="E134" s="123">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="F134" s="105"/>
@@ -4687,7 +4733,7 @@
       <c r="C135" s="101"/>
       <c r="D135" s="101"/>
       <c r="E135" s="123">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="F135" s="105"/>
@@ -4702,7 +4748,7 @@
         <v>66926</v>
       </c>
       <c r="E136" s="123">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="F136" s="105"/>
@@ -4720,7 +4766,7 @@
       <c r="C137" s="101"/>
       <c r="D137" s="101"/>
       <c r="E137" s="123">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="F137" s="105"/>
@@ -4731,7 +4777,7 @@
       <c r="C138" s="101"/>
       <c r="D138" s="101"/>
       <c r="E138" s="123">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="F138" s="105"/>
@@ -4742,7 +4788,7 @@
       <c r="C139" s="101"/>
       <c r="D139" s="101"/>
       <c r="E139" s="123">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="F139" s="105"/>
@@ -4755,7 +4801,7 @@
       <c r="C140" s="99"/>
       <c r="D140" s="99"/>
       <c r="E140" s="125">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="F140" s="104"/>
@@ -4813,7 +4859,7 @@
       <c r="C144" s="99"/>
       <c r="D144" s="99"/>
       <c r="E144" s="123">
-        <f t="shared" ref="E144:E157" si="9">IF(AND(C144&gt;0,D144&gt;0), D144-C144, 0)</f>
+        <f t="shared" ref="E144:E157" si="10">IF(AND(C144&gt;0,D144&gt;0), D144-C144, 0)</f>
         <v>0</v>
       </c>
       <c r="F144" s="104"/>
@@ -4824,7 +4870,7 @@
       <c r="C145" s="101"/>
       <c r="D145" s="101"/>
       <c r="E145" s="124">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="F145" s="105"/>
@@ -4835,7 +4881,7 @@
       <c r="C146" s="101"/>
       <c r="D146" s="101"/>
       <c r="E146" s="123">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="F146" s="105"/>
@@ -4846,7 +4892,7 @@
       <c r="C147" s="101"/>
       <c r="D147" s="101"/>
       <c r="E147" s="123">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="F147" s="105"/>
@@ -4857,7 +4903,7 @@
       <c r="C148" s="101"/>
       <c r="D148" s="101"/>
       <c r="E148" s="123">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="F148" s="105"/>
@@ -4868,7 +4914,7 @@
       <c r="C149" s="101"/>
       <c r="D149" s="101"/>
       <c r="E149" s="123">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="F149" s="105"/>
@@ -4879,7 +4925,7 @@
       <c r="C150" s="101"/>
       <c r="D150" s="101"/>
       <c r="E150" s="123">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="F150" s="105"/>
@@ -4890,7 +4936,7 @@
       <c r="C151" s="101"/>
       <c r="D151" s="101"/>
       <c r="E151" s="123">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="F151" s="105"/>
@@ -4901,7 +4947,7 @@
       <c r="C152" s="101"/>
       <c r="D152" s="101"/>
       <c r="E152" s="123">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="F152" s="105"/>
@@ -4912,7 +4958,7 @@
       <c r="C153" s="101"/>
       <c r="D153" s="101"/>
       <c r="E153" s="123">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="F153" s="105"/>
@@ -4923,7 +4969,7 @@
       <c r="C154" s="101"/>
       <c r="D154" s="101"/>
       <c r="E154" s="123">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="F154" s="105"/>
@@ -4934,7 +4980,7 @@
       <c r="C155" s="101"/>
       <c r="D155" s="101"/>
       <c r="E155" s="123">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="F155" s="105"/>
@@ -4945,7 +4991,7 @@
       <c r="C156" s="101"/>
       <c r="D156" s="101"/>
       <c r="E156" s="123">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="F156" s="105"/>
@@ -4958,7 +5004,7 @@
       <c r="C157" s="99"/>
       <c r="D157" s="99"/>
       <c r="E157" s="125">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="F157" s="104"/>
@@ -4990,11 +5036,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="A143:A157"/>
-    <mergeCell ref="A114:A123"/>
-    <mergeCell ref="A84:A98"/>
-    <mergeCell ref="A126:A140"/>
-    <mergeCell ref="A101:A111"/>
     <mergeCell ref="A43:A65"/>
     <mergeCell ref="A68:A81"/>
     <mergeCell ref="C5:D5"/>
@@ -5004,6 +5045,11 @@
     <mergeCell ref="A8:A18"/>
     <mergeCell ref="A21:A40"/>
     <mergeCell ref="C4:E4"/>
+    <mergeCell ref="A143:A157"/>
+    <mergeCell ref="A114:A123"/>
+    <mergeCell ref="A84:A98"/>
+    <mergeCell ref="A126:A140"/>
+    <mergeCell ref="A101:A111"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -5035,13 +5081,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="26.25" customHeight="1">
-      <c r="A1" s="168" t="s">
+      <c r="A1" s="186" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="168"/>
-      <c r="C1" s="168"/>
-      <c r="D1" s="168"/>
-      <c r="E1" s="168"/>
+      <c r="B1" s="186"/>
+      <c r="C1" s="186"/>
+      <c r="D1" s="186"/>
+      <c r="E1" s="186"/>
       <c r="F1" s="7"/>
       <c r="G1" s="5"/>
       <c r="H1" s="5"/>
@@ -5071,18 +5117,18 @@
         <v>8</v>
       </c>
       <c r="B3" s="36"/>
-      <c r="C3" s="169"/>
-      <c r="D3" s="170"/>
-      <c r="E3" s="170"/>
+      <c r="C3" s="187"/>
+      <c r="D3" s="188"/>
+      <c r="E3" s="188"/>
     </row>
     <row r="4" spans="1:8" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A4" s="46" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="87"/>
-      <c r="C4" s="171"/>
-      <c r="D4" s="172"/>
-      <c r="E4" s="172"/>
+      <c r="C4" s="168"/>
+      <c r="D4" s="169"/>
+      <c r="E4" s="169"/>
       <c r="F4" s="6"/>
     </row>
     <row r="5" spans="1:8" hidden="1" outlineLevel="2">
@@ -5234,9 +5280,9 @@
         <v>9</v>
       </c>
       <c r="B21" s="90"/>
-      <c r="C21" s="173"/>
-      <c r="D21" s="174"/>
-      <c r="E21" s="174"/>
+      <c r="C21" s="170"/>
+      <c r="D21" s="171"/>
+      <c r="E21" s="171"/>
     </row>
     <row r="22" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A22" s="47">
@@ -5387,9 +5433,9 @@
         <v>10</v>
       </c>
       <c r="B38" s="87"/>
-      <c r="C38" s="171"/>
-      <c r="D38" s="172"/>
-      <c r="E38" s="172"/>
+      <c r="C38" s="168"/>
+      <c r="D38" s="169"/>
+      <c r="E38" s="169"/>
     </row>
     <row r="39" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A39" s="47">
@@ -5540,9 +5586,9 @@
         <v>11</v>
       </c>
       <c r="B55" s="87"/>
-      <c r="C55" s="171"/>
-      <c r="D55" s="172"/>
-      <c r="E55" s="172"/>
+      <c r="C55" s="168"/>
+      <c r="D55" s="169"/>
+      <c r="E55" s="169"/>
     </row>
     <row r="56" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A56" s="47">
@@ -5693,9 +5739,9 @@
         <v>12</v>
       </c>
       <c r="B72" s="87"/>
-      <c r="C72" s="171"/>
-      <c r="D72" s="172"/>
-      <c r="E72" s="172"/>
+      <c r="C72" s="168"/>
+      <c r="D72" s="169"/>
+      <c r="E72" s="169"/>
     </row>
     <row r="73" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A73" s="47">
@@ -5846,9 +5892,9 @@
         <v>13</v>
       </c>
       <c r="B89" s="87"/>
-      <c r="C89" s="171"/>
-      <c r="D89" s="172"/>
-      <c r="E89" s="172"/>
+      <c r="C89" s="168"/>
+      <c r="D89" s="169"/>
+      <c r="E89" s="169"/>
     </row>
     <row r="90" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A90" s="47">
@@ -5999,9 +6045,9 @@
         <v>14</v>
       </c>
       <c r="B106" s="87"/>
-      <c r="C106" s="171"/>
-      <c r="D106" s="172"/>
-      <c r="E106" s="172"/>
+      <c r="C106" s="168"/>
+      <c r="D106" s="169"/>
+      <c r="E106" s="169"/>
     </row>
     <row r="107" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A107" s="47">
@@ -6152,9 +6198,9 @@
         <v>15</v>
       </c>
       <c r="B123" s="87"/>
-      <c r="C123" s="171"/>
-      <c r="D123" s="172"/>
-      <c r="E123" s="172"/>
+      <c r="C123" s="168"/>
+      <c r="D123" s="169"/>
+      <c r="E123" s="169"/>
     </row>
     <row r="124" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A124" s="47">
@@ -6305,9 +6351,9 @@
         <v>16</v>
       </c>
       <c r="B140" s="87"/>
-      <c r="C140" s="171"/>
-      <c r="D140" s="172"/>
-      <c r="E140" s="172"/>
+      <c r="C140" s="168"/>
+      <c r="D140" s="169"/>
+      <c r="E140" s="169"/>
     </row>
     <row r="141" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A141" s="47">
@@ -6458,9 +6504,9 @@
         <v>17</v>
       </c>
       <c r="B157" s="87"/>
-      <c r="C157" s="171"/>
-      <c r="D157" s="172"/>
-      <c r="E157" s="172"/>
+      <c r="C157" s="168"/>
+      <c r="D157" s="169"/>
+      <c r="E157" s="169"/>
     </row>
     <row r="158" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A158" s="47">
@@ -6611,9 +6657,9 @@
         <v>18</v>
       </c>
       <c r="B174" s="87"/>
-      <c r="C174" s="171"/>
-      <c r="D174" s="172"/>
-      <c r="E174" s="172"/>
+      <c r="C174" s="168"/>
+      <c r="D174" s="169"/>
+      <c r="E174" s="169"/>
     </row>
     <row r="175" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A175" s="47">
@@ -6764,9 +6810,9 @@
         <v>19</v>
       </c>
       <c r="B191" s="87"/>
-      <c r="C191" s="171"/>
-      <c r="D191" s="172"/>
-      <c r="E191" s="172"/>
+      <c r="C191" s="168"/>
+      <c r="D191" s="169"/>
+      <c r="E191" s="169"/>
     </row>
     <row r="192" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A192" s="47">
@@ -6917,9 +6963,9 @@
         <v>20</v>
       </c>
       <c r="B208" s="87"/>
-      <c r="C208" s="171"/>
-      <c r="D208" s="172"/>
-      <c r="E208" s="172"/>
+      <c r="C208" s="168"/>
+      <c r="D208" s="169"/>
+      <c r="E208" s="169"/>
     </row>
     <row r="209" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A209" s="47">
@@ -7070,9 +7116,9 @@
         <v>21</v>
       </c>
       <c r="B225" s="87"/>
-      <c r="C225" s="171"/>
-      <c r="D225" s="172"/>
-      <c r="E225" s="172"/>
+      <c r="C225" s="168"/>
+      <c r="D225" s="169"/>
+      <c r="E225" s="169"/>
     </row>
     <row r="226" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A226" s="47">
@@ -7223,9 +7269,9 @@
         <v>22</v>
       </c>
       <c r="B242" s="87"/>
-      <c r="C242" s="171"/>
-      <c r="D242" s="172"/>
-      <c r="E242" s="172"/>
+      <c r="C242" s="168"/>
+      <c r="D242" s="169"/>
+      <c r="E242" s="169"/>
     </row>
     <row r="243" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A243" s="47">
@@ -7376,9 +7422,9 @@
         <v>23</v>
       </c>
       <c r="B259" s="87"/>
-      <c r="C259" s="171"/>
-      <c r="D259" s="172"/>
-      <c r="E259" s="172"/>
+      <c r="C259" s="168"/>
+      <c r="D259" s="169"/>
+      <c r="E259" s="169"/>
     </row>
     <row r="260" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A260" s="47">
@@ -7529,18 +7575,18 @@
         <v>24</v>
       </c>
       <c r="B276" s="37"/>
-      <c r="C276" s="175"/>
-      <c r="D276" s="176"/>
-      <c r="E276" s="176"/>
+      <c r="C276" s="184"/>
+      <c r="D276" s="185"/>
+      <c r="E276" s="185"/>
     </row>
     <row r="277" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A277" s="51" t="s">
         <v>25</v>
       </c>
       <c r="B277" s="87"/>
-      <c r="C277" s="171"/>
-      <c r="D277" s="172"/>
-      <c r="E277" s="172"/>
+      <c r="C277" s="168"/>
+      <c r="D277" s="169"/>
+      <c r="E277" s="169"/>
     </row>
     <row r="278" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A278" s="52">
@@ -7691,9 +7737,9 @@
         <v>26</v>
       </c>
       <c r="B294" s="90"/>
-      <c r="C294" s="173"/>
-      <c r="D294" s="174"/>
-      <c r="E294" s="174"/>
+      <c r="C294" s="170"/>
+      <c r="D294" s="171"/>
+      <c r="E294" s="171"/>
     </row>
     <row r="295" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A295" s="52">
@@ -7844,9 +7890,9 @@
         <v>27</v>
       </c>
       <c r="B311" s="87"/>
-      <c r="C311" s="171"/>
-      <c r="D311" s="172"/>
-      <c r="E311" s="172"/>
+      <c r="C311" s="168"/>
+      <c r="D311" s="169"/>
+      <c r="E311" s="169"/>
     </row>
     <row r="312" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A312" s="52">
@@ -7997,9 +8043,9 @@
         <v>28</v>
       </c>
       <c r="B328" s="87"/>
-      <c r="C328" s="171"/>
-      <c r="D328" s="172"/>
-      <c r="E328" s="172"/>
+      <c r="C328" s="168"/>
+      <c r="D328" s="169"/>
+      <c r="E328" s="169"/>
     </row>
     <row r="329" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A329" s="52">
@@ -8150,9 +8196,9 @@
         <v>29</v>
       </c>
       <c r="B345" s="87"/>
-      <c r="C345" s="171"/>
-      <c r="D345" s="172"/>
-      <c r="E345" s="172"/>
+      <c r="C345" s="168"/>
+      <c r="D345" s="169"/>
+      <c r="E345" s="169"/>
     </row>
     <row r="346" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A346" s="52">
@@ -8303,9 +8349,9 @@
         <v>30</v>
       </c>
       <c r="B362" s="87"/>
-      <c r="C362" s="171"/>
-      <c r="D362" s="172"/>
-      <c r="E362" s="172"/>
+      <c r="C362" s="168"/>
+      <c r="D362" s="169"/>
+      <c r="E362" s="169"/>
     </row>
     <row r="363" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A363" s="52">
@@ -8456,9 +8502,9 @@
         <v>31</v>
       </c>
       <c r="B379" s="87"/>
-      <c r="C379" s="171"/>
-      <c r="D379" s="172"/>
-      <c r="E379" s="172"/>
+      <c r="C379" s="168"/>
+      <c r="D379" s="169"/>
+      <c r="E379" s="169"/>
     </row>
     <row r="380" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A380" s="52">
@@ -8609,9 +8655,9 @@
         <v>32</v>
       </c>
       <c r="B396" s="87"/>
-      <c r="C396" s="171"/>
-      <c r="D396" s="172"/>
-      <c r="E396" s="172"/>
+      <c r="C396" s="168"/>
+      <c r="D396" s="169"/>
+      <c r="E396" s="169"/>
     </row>
     <row r="397" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A397" s="52">
@@ -8762,9 +8808,9 @@
         <v>33</v>
       </c>
       <c r="B413" s="87"/>
-      <c r="C413" s="171"/>
-      <c r="D413" s="172"/>
-      <c r="E413" s="172"/>
+      <c r="C413" s="168"/>
+      <c r="D413" s="169"/>
+      <c r="E413" s="169"/>
     </row>
     <row r="414" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A414" s="52">
@@ -8915,9 +8961,9 @@
         <v>34</v>
       </c>
       <c r="B430" s="87"/>
-      <c r="C430" s="171"/>
-      <c r="D430" s="172"/>
-      <c r="E430" s="172"/>
+      <c r="C430" s="168"/>
+      <c r="D430" s="169"/>
+      <c r="E430" s="169"/>
     </row>
     <row r="431" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A431" s="52">
@@ -9068,9 +9114,9 @@
         <v>35</v>
       </c>
       <c r="B447" s="87"/>
-      <c r="C447" s="171"/>
-      <c r="D447" s="172"/>
-      <c r="E447" s="172"/>
+      <c r="C447" s="168"/>
+      <c r="D447" s="169"/>
+      <c r="E447" s="169"/>
     </row>
     <row r="448" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A448" s="52">
@@ -9221,9 +9267,9 @@
         <v>36</v>
       </c>
       <c r="B464" s="87"/>
-      <c r="C464" s="171"/>
-      <c r="D464" s="172"/>
-      <c r="E464" s="172"/>
+      <c r="C464" s="168"/>
+      <c r="D464" s="169"/>
+      <c r="E464" s="169"/>
     </row>
     <row r="465" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A465" s="52">
@@ -9374,9 +9420,9 @@
         <v>37</v>
       </c>
       <c r="B481" s="87"/>
-      <c r="C481" s="171"/>
-      <c r="D481" s="172"/>
-      <c r="E481" s="172"/>
+      <c r="C481" s="168"/>
+      <c r="D481" s="169"/>
+      <c r="E481" s="169"/>
     </row>
     <row r="482" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A482" s="52">
@@ -9527,9 +9573,9 @@
         <v>38</v>
       </c>
       <c r="B498" s="87"/>
-      <c r="C498" s="171"/>
-      <c r="D498" s="172"/>
-      <c r="E498" s="172"/>
+      <c r="C498" s="168"/>
+      <c r="D498" s="169"/>
+      <c r="E498" s="169"/>
     </row>
     <row r="499" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A499" s="52">
@@ -9680,9 +9726,9 @@
         <v>39</v>
       </c>
       <c r="B515" s="87"/>
-      <c r="C515" s="171"/>
-      <c r="D515" s="172"/>
-      <c r="E515" s="172"/>
+      <c r="C515" s="168"/>
+      <c r="D515" s="169"/>
+      <c r="E515" s="169"/>
     </row>
     <row r="516" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A516" s="52">
@@ -9833,9 +9879,9 @@
         <v>40</v>
       </c>
       <c r="B532" s="87"/>
-      <c r="C532" s="171"/>
-      <c r="D532" s="172"/>
-      <c r="E532" s="172"/>
+      <c r="C532" s="168"/>
+      <c r="D532" s="169"/>
+      <c r="E532" s="169"/>
     </row>
     <row r="533" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A533" s="55">
@@ -9986,18 +10032,18 @@
         <v>50</v>
       </c>
       <c r="B549" s="38"/>
-      <c r="C549" s="177"/>
-      <c r="D549" s="178"/>
-      <c r="E549" s="178"/>
+      <c r="C549" s="182"/>
+      <c r="D549" s="183"/>
+      <c r="E549" s="183"/>
     </row>
     <row r="550" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A550" s="58" t="s">
         <v>51</v>
       </c>
       <c r="B550" s="87"/>
-      <c r="C550" s="171"/>
-      <c r="D550" s="172"/>
-      <c r="E550" s="172"/>
+      <c r="C550" s="168"/>
+      <c r="D550" s="169"/>
+      <c r="E550" s="169"/>
     </row>
     <row r="551" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A551" s="59">
@@ -10148,9 +10194,9 @@
         <v>52</v>
       </c>
       <c r="B567" s="90"/>
-      <c r="C567" s="173"/>
-      <c r="D567" s="174"/>
-      <c r="E567" s="174"/>
+      <c r="C567" s="170"/>
+      <c r="D567" s="171"/>
+      <c r="E567" s="171"/>
     </row>
     <row r="568" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A568" s="59">
@@ -10301,9 +10347,9 @@
         <v>53</v>
       </c>
       <c r="B584" s="87"/>
-      <c r="C584" s="171"/>
-      <c r="D584" s="172"/>
-      <c r="E584" s="172"/>
+      <c r="C584" s="168"/>
+      <c r="D584" s="169"/>
+      <c r="E584" s="169"/>
     </row>
     <row r="585" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A585" s="59">
@@ -10454,9 +10500,9 @@
         <v>54</v>
       </c>
       <c r="B601" s="87"/>
-      <c r="C601" s="171"/>
-      <c r="D601" s="172"/>
-      <c r="E601" s="172"/>
+      <c r="C601" s="168"/>
+      <c r="D601" s="169"/>
+      <c r="E601" s="169"/>
     </row>
     <row r="602" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A602" s="59">
@@ -10607,9 +10653,9 @@
         <v>55</v>
       </c>
       <c r="B618" s="87"/>
-      <c r="C618" s="171"/>
-      <c r="D618" s="172"/>
-      <c r="E618" s="172"/>
+      <c r="C618" s="168"/>
+      <c r="D618" s="169"/>
+      <c r="E618" s="169"/>
     </row>
     <row r="619" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A619" s="59">
@@ -10760,9 +10806,9 @@
         <v>56</v>
       </c>
       <c r="B635" s="87"/>
-      <c r="C635" s="171"/>
-      <c r="D635" s="172"/>
-      <c r="E635" s="172"/>
+      <c r="C635" s="168"/>
+      <c r="D635" s="169"/>
+      <c r="E635" s="169"/>
     </row>
     <row r="636" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A636" s="59">
@@ -10913,9 +10959,9 @@
         <v>57</v>
       </c>
       <c r="B652" s="87"/>
-      <c r="C652" s="171"/>
-      <c r="D652" s="172"/>
-      <c r="E652" s="172"/>
+      <c r="C652" s="168"/>
+      <c r="D652" s="169"/>
+      <c r="E652" s="169"/>
     </row>
     <row r="653" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A653" s="59">
@@ -11066,9 +11112,9 @@
         <v>58</v>
       </c>
       <c r="B669" s="87"/>
-      <c r="C669" s="171"/>
-      <c r="D669" s="172"/>
-      <c r="E669" s="172"/>
+      <c r="C669" s="168"/>
+      <c r="D669" s="169"/>
+      <c r="E669" s="169"/>
     </row>
     <row r="670" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A670" s="59">
@@ -11219,9 +11265,9 @@
         <v>59</v>
       </c>
       <c r="B686" s="87"/>
-      <c r="C686" s="171"/>
-      <c r="D686" s="172"/>
-      <c r="E686" s="172"/>
+      <c r="C686" s="168"/>
+      <c r="D686" s="169"/>
+      <c r="E686" s="169"/>
     </row>
     <row r="687" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A687" s="59">
@@ -11372,9 +11418,9 @@
         <v>60</v>
       </c>
       <c r="B703" s="87"/>
-      <c r="C703" s="171"/>
-      <c r="D703" s="172"/>
-      <c r="E703" s="172"/>
+      <c r="C703" s="168"/>
+      <c r="D703" s="169"/>
+      <c r="E703" s="169"/>
     </row>
     <row r="704" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A704" s="59">
@@ -11525,9 +11571,9 @@
         <v>61</v>
       </c>
       <c r="B720" s="87"/>
-      <c r="C720" s="171"/>
-      <c r="D720" s="172"/>
-      <c r="E720" s="172"/>
+      <c r="C720" s="168"/>
+      <c r="D720" s="169"/>
+      <c r="E720" s="169"/>
     </row>
     <row r="721" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A721" s="59">
@@ -11678,9 +11724,9 @@
         <v>62</v>
       </c>
       <c r="B737" s="87"/>
-      <c r="C737" s="171"/>
-      <c r="D737" s="172"/>
-      <c r="E737" s="172"/>
+      <c r="C737" s="168"/>
+      <c r="D737" s="169"/>
+      <c r="E737" s="169"/>
     </row>
     <row r="738" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A738" s="59">
@@ -11831,9 +11877,9 @@
         <v>63</v>
       </c>
       <c r="B754" s="87"/>
-      <c r="C754" s="171"/>
-      <c r="D754" s="172"/>
-      <c r="E754" s="172"/>
+      <c r="C754" s="168"/>
+      <c r="D754" s="169"/>
+      <c r="E754" s="169"/>
     </row>
     <row r="755" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A755" s="59">
@@ -11984,9 +12030,9 @@
         <v>64</v>
       </c>
       <c r="B771" s="87"/>
-      <c r="C771" s="171"/>
-      <c r="D771" s="172"/>
-      <c r="E771" s="172"/>
+      <c r="C771" s="168"/>
+      <c r="D771" s="169"/>
+      <c r="E771" s="169"/>
     </row>
     <row r="772" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A772" s="59">
@@ -12137,9 +12183,9 @@
         <v>65</v>
       </c>
       <c r="B788" s="87"/>
-      <c r="C788" s="171"/>
-      <c r="D788" s="172"/>
-      <c r="E788" s="172"/>
+      <c r="C788" s="168"/>
+      <c r="D788" s="169"/>
+      <c r="E788" s="169"/>
     </row>
     <row r="789" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A789" s="59">
@@ -12290,9 +12336,9 @@
         <v>66</v>
       </c>
       <c r="B805" s="87"/>
-      <c r="C805" s="171"/>
-      <c r="D805" s="172"/>
-      <c r="E805" s="172"/>
+      <c r="C805" s="168"/>
+      <c r="D805" s="169"/>
+      <c r="E805" s="169"/>
     </row>
     <row r="806" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A806" s="59">
@@ -12443,18 +12489,18 @@
         <v>67</v>
       </c>
       <c r="B822" s="39"/>
-      <c r="C822" s="179"/>
-      <c r="D822" s="180"/>
-      <c r="E822" s="180"/>
+      <c r="C822" s="180"/>
+      <c r="D822" s="181"/>
+      <c r="E822" s="181"/>
     </row>
     <row r="823" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A823" s="63" t="s">
         <v>68</v>
       </c>
       <c r="B823" s="87"/>
-      <c r="C823" s="171"/>
-      <c r="D823" s="172"/>
-      <c r="E823" s="172"/>
+      <c r="C823" s="168"/>
+      <c r="D823" s="169"/>
+      <c r="E823" s="169"/>
     </row>
     <row r="824" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A824" s="64">
@@ -12605,9 +12651,9 @@
         <v>69</v>
       </c>
       <c r="B840" s="90"/>
-      <c r="C840" s="173"/>
-      <c r="D840" s="174"/>
-      <c r="E840" s="174"/>
+      <c r="C840" s="170"/>
+      <c r="D840" s="171"/>
+      <c r="E840" s="171"/>
     </row>
     <row r="841" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A841" s="64">
@@ -12758,9 +12804,9 @@
         <v>70</v>
       </c>
       <c r="B857" s="87"/>
-      <c r="C857" s="171"/>
-      <c r="D857" s="172"/>
-      <c r="E857" s="172"/>
+      <c r="C857" s="168"/>
+      <c r="D857" s="169"/>
+      <c r="E857" s="169"/>
     </row>
     <row r="858" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A858" s="64">
@@ -12911,9 +12957,9 @@
         <v>71</v>
       </c>
       <c r="B874" s="87"/>
-      <c r="C874" s="171"/>
-      <c r="D874" s="172"/>
-      <c r="E874" s="172"/>
+      <c r="C874" s="168"/>
+      <c r="D874" s="169"/>
+      <c r="E874" s="169"/>
     </row>
     <row r="875" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A875" s="64">
@@ -13064,9 +13110,9 @@
         <v>72</v>
       </c>
       <c r="B891" s="87"/>
-      <c r="C891" s="171"/>
-      <c r="D891" s="172"/>
-      <c r="E891" s="172"/>
+      <c r="C891" s="168"/>
+      <c r="D891" s="169"/>
+      <c r="E891" s="169"/>
     </row>
     <row r="892" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A892" s="64">
@@ -13217,9 +13263,9 @@
         <v>73</v>
       </c>
       <c r="B908" s="87"/>
-      <c r="C908" s="171"/>
-      <c r="D908" s="172"/>
-      <c r="E908" s="172"/>
+      <c r="C908" s="168"/>
+      <c r="D908" s="169"/>
+      <c r="E908" s="169"/>
     </row>
     <row r="909" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A909" s="64">
@@ -13370,9 +13416,9 @@
         <v>74</v>
       </c>
       <c r="B925" s="87"/>
-      <c r="C925" s="171"/>
-      <c r="D925" s="172"/>
-      <c r="E925" s="172"/>
+      <c r="C925" s="168"/>
+      <c r="D925" s="169"/>
+      <c r="E925" s="169"/>
     </row>
     <row r="926" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A926" s="64">
@@ -13523,9 +13569,9 @@
         <v>75</v>
       </c>
       <c r="B942" s="87"/>
-      <c r="C942" s="171"/>
-      <c r="D942" s="172"/>
-      <c r="E942" s="172"/>
+      <c r="C942" s="168"/>
+      <c r="D942" s="169"/>
+      <c r="E942" s="169"/>
     </row>
     <row r="943" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A943" s="64">
@@ -13676,9 +13722,9 @@
         <v>76</v>
       </c>
       <c r="B959" s="87"/>
-      <c r="C959" s="171"/>
-      <c r="D959" s="172"/>
-      <c r="E959" s="172"/>
+      <c r="C959" s="168"/>
+      <c r="D959" s="169"/>
+      <c r="E959" s="169"/>
     </row>
     <row r="960" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A960" s="64">
@@ -13829,9 +13875,9 @@
         <v>77</v>
       </c>
       <c r="B976" s="87"/>
-      <c r="C976" s="171"/>
-      <c r="D976" s="172"/>
-      <c r="E976" s="172"/>
+      <c r="C976" s="168"/>
+      <c r="D976" s="169"/>
+      <c r="E976" s="169"/>
     </row>
     <row r="977" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A977" s="64">
@@ -13982,9 +14028,9 @@
         <v>78</v>
       </c>
       <c r="B993" s="87"/>
-      <c r="C993" s="171"/>
-      <c r="D993" s="172"/>
-      <c r="E993" s="172"/>
+      <c r="C993" s="168"/>
+      <c r="D993" s="169"/>
+      <c r="E993" s="169"/>
     </row>
     <row r="994" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A994" s="64">
@@ -14135,9 +14181,9 @@
         <v>79</v>
       </c>
       <c r="B1010" s="87"/>
-      <c r="C1010" s="171"/>
-      <c r="D1010" s="172"/>
-      <c r="E1010" s="172"/>
+      <c r="C1010" s="168"/>
+      <c r="D1010" s="169"/>
+      <c r="E1010" s="169"/>
     </row>
     <row r="1011" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1011" s="64">
@@ -14288,9 +14334,9 @@
         <v>80</v>
       </c>
       <c r="B1027" s="87"/>
-      <c r="C1027" s="171"/>
-      <c r="D1027" s="172"/>
-      <c r="E1027" s="172"/>
+      <c r="C1027" s="168"/>
+      <c r="D1027" s="169"/>
+      <c r="E1027" s="169"/>
     </row>
     <row r="1028" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1028" s="64">
@@ -14441,9 +14487,9 @@
         <v>83</v>
       </c>
       <c r="B1044" s="87"/>
-      <c r="C1044" s="171"/>
-      <c r="D1044" s="172"/>
-      <c r="E1044" s="172"/>
+      <c r="C1044" s="168"/>
+      <c r="D1044" s="169"/>
+      <c r="E1044" s="169"/>
     </row>
     <row r="1045" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1045" s="64">
@@ -14594,9 +14640,9 @@
         <v>82</v>
       </c>
       <c r="B1061" s="87"/>
-      <c r="C1061" s="171"/>
-      <c r="D1061" s="172"/>
-      <c r="E1061" s="172"/>
+      <c r="C1061" s="168"/>
+      <c r="D1061" s="169"/>
+      <c r="E1061" s="169"/>
     </row>
     <row r="1062" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1062" s="64">
@@ -14747,9 +14793,9 @@
         <v>84</v>
       </c>
       <c r="B1078" s="87"/>
-      <c r="C1078" s="171"/>
-      <c r="D1078" s="172"/>
-      <c r="E1078" s="172"/>
+      <c r="C1078" s="168"/>
+      <c r="D1078" s="169"/>
+      <c r="E1078" s="169"/>
     </row>
     <row r="1079" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1079" s="64">
@@ -14900,18 +14946,18 @@
         <v>104</v>
       </c>
       <c r="B1095" s="40"/>
-      <c r="C1095" s="181"/>
-      <c r="D1095" s="182"/>
-      <c r="E1095" s="182"/>
+      <c r="C1095" s="178"/>
+      <c r="D1095" s="179"/>
+      <c r="E1095" s="179"/>
     </row>
     <row r="1096" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A1096" s="68" t="s">
         <v>85</v>
       </c>
       <c r="B1096" s="87"/>
-      <c r="C1096" s="171"/>
-      <c r="D1096" s="172"/>
-      <c r="E1096" s="172"/>
+      <c r="C1096" s="168"/>
+      <c r="D1096" s="169"/>
+      <c r="E1096" s="169"/>
     </row>
     <row r="1097" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1097" s="69">
@@ -15062,9 +15108,9 @@
         <v>86</v>
       </c>
       <c r="B1113" s="90"/>
-      <c r="C1113" s="173"/>
-      <c r="D1113" s="174"/>
-      <c r="E1113" s="174"/>
+      <c r="C1113" s="170"/>
+      <c r="D1113" s="171"/>
+      <c r="E1113" s="171"/>
     </row>
     <row r="1114" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1114" s="69">
@@ -15215,9 +15261,9 @@
         <v>87</v>
       </c>
       <c r="B1130" s="87"/>
-      <c r="C1130" s="171"/>
-      <c r="D1130" s="172"/>
-      <c r="E1130" s="172"/>
+      <c r="C1130" s="168"/>
+      <c r="D1130" s="169"/>
+      <c r="E1130" s="169"/>
     </row>
     <row r="1131" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1131" s="69">
@@ -15368,9 +15414,9 @@
         <v>88</v>
       </c>
       <c r="B1147" s="87"/>
-      <c r="C1147" s="171"/>
-      <c r="D1147" s="172"/>
-      <c r="E1147" s="172"/>
+      <c r="C1147" s="168"/>
+      <c r="D1147" s="169"/>
+      <c r="E1147" s="169"/>
     </row>
     <row r="1148" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1148" s="69">
@@ -15521,9 +15567,9 @@
         <v>89</v>
       </c>
       <c r="B1164" s="87"/>
-      <c r="C1164" s="171"/>
-      <c r="D1164" s="172"/>
-      <c r="E1164" s="172"/>
+      <c r="C1164" s="168"/>
+      <c r="D1164" s="169"/>
+      <c r="E1164" s="169"/>
     </row>
     <row r="1165" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1165" s="69">
@@ -15674,9 +15720,9 @@
         <v>90</v>
       </c>
       <c r="B1181" s="87"/>
-      <c r="C1181" s="171"/>
-      <c r="D1181" s="172"/>
-      <c r="E1181" s="172"/>
+      <c r="C1181" s="168"/>
+      <c r="D1181" s="169"/>
+      <c r="E1181" s="169"/>
     </row>
     <row r="1182" spans="1:5" hidden="1" outlineLevel="3">
       <c r="A1182" s="69">
@@ -15827,9 +15873,9 @@
         <v>91</v>
       </c>
       <c r="B1198" s="87"/>
-      <c r="C1198" s="171"/>
-      <c r="D1198" s="172"/>
-      <c r="E1198" s="172"/>
+      <c r="C1198" s="168"/>
+      <c r="D1198" s="169"/>
+      <c r="E1198" s="169"/>
     </row>
     <row r="1199" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1199" s="69">
@@ -15980,9 +16026,9 @@
         <v>92</v>
       </c>
       <c r="B1215" s="87"/>
-      <c r="C1215" s="171"/>
-      <c r="D1215" s="172"/>
-      <c r="E1215" s="172"/>
+      <c r="C1215" s="168"/>
+      <c r="D1215" s="169"/>
+      <c r="E1215" s="169"/>
     </row>
     <row r="1216" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1216" s="69">
@@ -16133,9 +16179,9 @@
         <v>93</v>
       </c>
       <c r="B1232" s="87"/>
-      <c r="C1232" s="171"/>
-      <c r="D1232" s="172"/>
-      <c r="E1232" s="172"/>
+      <c r="C1232" s="168"/>
+      <c r="D1232" s="169"/>
+      <c r="E1232" s="169"/>
     </row>
     <row r="1233" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1233" s="69">
@@ -16286,9 +16332,9 @@
         <v>94</v>
       </c>
       <c r="B1249" s="87"/>
-      <c r="C1249" s="171"/>
-      <c r="D1249" s="172"/>
-      <c r="E1249" s="172"/>
+      <c r="C1249" s="168"/>
+      <c r="D1249" s="169"/>
+      <c r="E1249" s="169"/>
     </row>
     <row r="1250" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1250" s="69">
@@ -16439,9 +16485,9 @@
         <v>99</v>
       </c>
       <c r="B1266" s="87"/>
-      <c r="C1266" s="171"/>
-      <c r="D1266" s="172"/>
-      <c r="E1266" s="172"/>
+      <c r="C1266" s="168"/>
+      <c r="D1266" s="169"/>
+      <c r="E1266" s="169"/>
     </row>
     <row r="1267" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1267" s="69">
@@ -16592,9 +16638,9 @@
         <v>100</v>
       </c>
       <c r="B1283" s="87"/>
-      <c r="C1283" s="171"/>
-      <c r="D1283" s="172"/>
-      <c r="E1283" s="172"/>
+      <c r="C1283" s="168"/>
+      <c r="D1283" s="169"/>
+      <c r="E1283" s="169"/>
     </row>
     <row r="1284" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1284" s="69">
@@ -16745,9 +16791,9 @@
         <v>101</v>
       </c>
       <c r="B1300" s="87"/>
-      <c r="C1300" s="171"/>
-      <c r="D1300" s="172"/>
-      <c r="E1300" s="172"/>
+      <c r="C1300" s="168"/>
+      <c r="D1300" s="169"/>
+      <c r="E1300" s="169"/>
     </row>
     <row r="1301" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1301" s="69">
@@ -16898,9 +16944,9 @@
         <v>81</v>
       </c>
       <c r="B1317" s="87"/>
-      <c r="C1317" s="171"/>
-      <c r="D1317" s="172"/>
-      <c r="E1317" s="172"/>
+      <c r="C1317" s="168"/>
+      <c r="D1317" s="169"/>
+      <c r="E1317" s="169"/>
     </row>
     <row r="1318" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1318" s="69">
@@ -17051,9 +17097,9 @@
         <v>102</v>
       </c>
       <c r="B1334" s="87"/>
-      <c r="C1334" s="171"/>
-      <c r="D1334" s="172"/>
-      <c r="E1334" s="172"/>
+      <c r="C1334" s="168"/>
+      <c r="D1334" s="169"/>
+      <c r="E1334" s="169"/>
     </row>
     <row r="1335" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1335" s="69">
@@ -17204,9 +17250,9 @@
         <v>98</v>
       </c>
       <c r="B1351" s="87"/>
-      <c r="C1351" s="171"/>
-      <c r="D1351" s="172"/>
-      <c r="E1351" s="172"/>
+      <c r="C1351" s="168"/>
+      <c r="D1351" s="169"/>
+      <c r="E1351" s="169"/>
     </row>
     <row r="1352" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1352" s="69">
@@ -17357,18 +17403,18 @@
         <v>103</v>
       </c>
       <c r="B1368" s="41"/>
-      <c r="C1368" s="183"/>
-      <c r="D1368" s="184"/>
-      <c r="E1368" s="184"/>
+      <c r="C1368" s="176"/>
+      <c r="D1368" s="177"/>
+      <c r="E1368" s="177"/>
     </row>
     <row r="1369" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A1369" s="73" t="s">
         <v>105</v>
       </c>
       <c r="B1369" s="87"/>
-      <c r="C1369" s="171"/>
-      <c r="D1369" s="172"/>
-      <c r="E1369" s="172"/>
+      <c r="C1369" s="168"/>
+      <c r="D1369" s="169"/>
+      <c r="E1369" s="169"/>
     </row>
     <row r="1370" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1370" s="74">
@@ -17519,9 +17565,9 @@
         <v>106</v>
       </c>
       <c r="B1386" s="90"/>
-      <c r="C1386" s="173"/>
-      <c r="D1386" s="174"/>
-      <c r="E1386" s="174"/>
+      <c r="C1386" s="170"/>
+      <c r="D1386" s="171"/>
+      <c r="E1386" s="171"/>
     </row>
     <row r="1387" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1387" s="74">
@@ -17672,9 +17718,9 @@
         <v>107</v>
       </c>
       <c r="B1403" s="87"/>
-      <c r="C1403" s="171"/>
-      <c r="D1403" s="172"/>
-      <c r="E1403" s="172"/>
+      <c r="C1403" s="168"/>
+      <c r="D1403" s="169"/>
+      <c r="E1403" s="169"/>
     </row>
     <row r="1404" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1404" s="74">
@@ -17825,9 +17871,9 @@
         <v>108</v>
       </c>
       <c r="B1420" s="87"/>
-      <c r="C1420" s="171"/>
-      <c r="D1420" s="172"/>
-      <c r="E1420" s="172"/>
+      <c r="C1420" s="168"/>
+      <c r="D1420" s="169"/>
+      <c r="E1420" s="169"/>
     </row>
     <row r="1421" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1421" s="74">
@@ -17978,9 +18024,9 @@
         <v>109</v>
       </c>
       <c r="B1437" s="87"/>
-      <c r="C1437" s="171"/>
-      <c r="D1437" s="172"/>
-      <c r="E1437" s="172"/>
+      <c r="C1437" s="168"/>
+      <c r="D1437" s="169"/>
+      <c r="E1437" s="169"/>
     </row>
     <row r="1438" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1438" s="74">
@@ -18131,9 +18177,9 @@
         <v>110</v>
       </c>
       <c r="B1454" s="87"/>
-      <c r="C1454" s="171"/>
-      <c r="D1454" s="172"/>
-      <c r="E1454" s="172"/>
+      <c r="C1454" s="168"/>
+      <c r="D1454" s="169"/>
+      <c r="E1454" s="169"/>
     </row>
     <row r="1455" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1455" s="74">
@@ -18284,9 +18330,9 @@
         <v>111</v>
       </c>
       <c r="B1471" s="87"/>
-      <c r="C1471" s="171"/>
-      <c r="D1471" s="172"/>
-      <c r="E1471" s="172"/>
+      <c r="C1471" s="168"/>
+      <c r="D1471" s="169"/>
+      <c r="E1471" s="169"/>
     </row>
     <row r="1472" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1472" s="74">
@@ -18437,9 +18483,9 @@
         <v>112</v>
       </c>
       <c r="B1488" s="87"/>
-      <c r="C1488" s="171"/>
-      <c r="D1488" s="172"/>
-      <c r="E1488" s="172"/>
+      <c r="C1488" s="168"/>
+      <c r="D1488" s="169"/>
+      <c r="E1488" s="169"/>
     </row>
     <row r="1489" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1489" s="74">
@@ -18590,9 +18636,9 @@
         <v>113</v>
       </c>
       <c r="B1505" s="87"/>
-      <c r="C1505" s="171"/>
-      <c r="D1505" s="172"/>
-      <c r="E1505" s="172"/>
+      <c r="C1505" s="168"/>
+      <c r="D1505" s="169"/>
+      <c r="E1505" s="169"/>
     </row>
     <row r="1506" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1506" s="74">
@@ -18743,9 +18789,9 @@
         <v>114</v>
       </c>
       <c r="B1522" s="87"/>
-      <c r="C1522" s="171"/>
-      <c r="D1522" s="172"/>
-      <c r="E1522" s="172"/>
+      <c r="C1522" s="168"/>
+      <c r="D1522" s="169"/>
+      <c r="E1522" s="169"/>
     </row>
     <row r="1523" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1523" s="74">
@@ -18896,9 +18942,9 @@
         <v>95</v>
       </c>
       <c r="B1539" s="87"/>
-      <c r="C1539" s="171"/>
-      <c r="D1539" s="172"/>
-      <c r="E1539" s="172"/>
+      <c r="C1539" s="168"/>
+      <c r="D1539" s="169"/>
+      <c r="E1539" s="169"/>
     </row>
     <row r="1540" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1540" s="74">
@@ -19049,9 +19095,9 @@
         <v>115</v>
       </c>
       <c r="B1556" s="87"/>
-      <c r="C1556" s="171"/>
-      <c r="D1556" s="172"/>
-      <c r="E1556" s="172"/>
+      <c r="C1556" s="168"/>
+      <c r="D1556" s="169"/>
+      <c r="E1556" s="169"/>
     </row>
     <row r="1557" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1557" s="74">
@@ -19202,9 +19248,9 @@
         <v>116</v>
       </c>
       <c r="B1573" s="87"/>
-      <c r="C1573" s="171"/>
-      <c r="D1573" s="172"/>
-      <c r="E1573" s="172"/>
+      <c r="C1573" s="168"/>
+      <c r="D1573" s="169"/>
+      <c r="E1573" s="169"/>
     </row>
     <row r="1574" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1574" s="74">
@@ -19355,9 +19401,9 @@
         <v>117</v>
       </c>
       <c r="B1590" s="87"/>
-      <c r="C1590" s="171"/>
-      <c r="D1590" s="172"/>
-      <c r="E1590" s="172"/>
+      <c r="C1590" s="168"/>
+      <c r="D1590" s="169"/>
+      <c r="E1590" s="169"/>
     </row>
     <row r="1591" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1591" s="74">
@@ -19508,9 +19554,9 @@
         <v>118</v>
       </c>
       <c r="B1607" s="87"/>
-      <c r="C1607" s="171"/>
-      <c r="D1607" s="172"/>
-      <c r="E1607" s="172"/>
+      <c r="C1607" s="168"/>
+      <c r="D1607" s="169"/>
+      <c r="E1607" s="169"/>
     </row>
     <row r="1608" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1608" s="74">
@@ -19661,9 +19707,9 @@
         <v>119</v>
       </c>
       <c r="B1624" s="87"/>
-      <c r="C1624" s="171"/>
-      <c r="D1624" s="172"/>
-      <c r="E1624" s="172"/>
+      <c r="C1624" s="168"/>
+      <c r="D1624" s="169"/>
+      <c r="E1624" s="169"/>
     </row>
     <row r="1625" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1625" s="74">
@@ -19814,18 +19860,18 @@
         <v>120</v>
       </c>
       <c r="B1641" s="42"/>
-      <c r="C1641" s="185"/>
-      <c r="D1641" s="186"/>
-      <c r="E1641" s="186"/>
+      <c r="C1641" s="174"/>
+      <c r="D1641" s="175"/>
+      <c r="E1641" s="175"/>
     </row>
     <row r="1642" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A1642" s="78" t="s">
         <v>121</v>
       </c>
       <c r="B1642" s="87"/>
-      <c r="C1642" s="171"/>
-      <c r="D1642" s="172"/>
-      <c r="E1642" s="172"/>
+      <c r="C1642" s="168"/>
+      <c r="D1642" s="169"/>
+      <c r="E1642" s="169"/>
     </row>
     <row r="1643" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1643" s="79">
@@ -19976,9 +20022,9 @@
         <v>122</v>
       </c>
       <c r="B1659" s="90"/>
-      <c r="C1659" s="173"/>
-      <c r="D1659" s="174"/>
-      <c r="E1659" s="174"/>
+      <c r="C1659" s="170"/>
+      <c r="D1659" s="171"/>
+      <c r="E1659" s="171"/>
     </row>
     <row r="1660" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1660" s="79">
@@ -20129,9 +20175,9 @@
         <v>123</v>
       </c>
       <c r="B1676" s="87"/>
-      <c r="C1676" s="171"/>
-      <c r="D1676" s="172"/>
-      <c r="E1676" s="172"/>
+      <c r="C1676" s="168"/>
+      <c r="D1676" s="169"/>
+      <c r="E1676" s="169"/>
     </row>
     <row r="1677" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1677" s="79">
@@ -20282,9 +20328,9 @@
         <v>124</v>
       </c>
       <c r="B1693" s="87"/>
-      <c r="C1693" s="171"/>
-      <c r="D1693" s="172"/>
-      <c r="E1693" s="172"/>
+      <c r="C1693" s="168"/>
+      <c r="D1693" s="169"/>
+      <c r="E1693" s="169"/>
     </row>
     <row r="1694" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1694" s="79">
@@ -20435,9 +20481,9 @@
         <v>125</v>
       </c>
       <c r="B1710" s="87"/>
-      <c r="C1710" s="171"/>
-      <c r="D1710" s="172"/>
-      <c r="E1710" s="172"/>
+      <c r="C1710" s="168"/>
+      <c r="D1710" s="169"/>
+      <c r="E1710" s="169"/>
     </row>
     <row r="1711" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1711" s="79">
@@ -20588,9 +20634,9 @@
         <v>126</v>
       </c>
       <c r="B1727" s="87"/>
-      <c r="C1727" s="171"/>
-      <c r="D1727" s="172"/>
-      <c r="E1727" s="172"/>
+      <c r="C1727" s="168"/>
+      <c r="D1727" s="169"/>
+      <c r="E1727" s="169"/>
     </row>
     <row r="1728" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1728" s="79">
@@ -20741,9 +20787,9 @@
         <v>127</v>
       </c>
       <c r="B1744" s="87"/>
-      <c r="C1744" s="171"/>
-      <c r="D1744" s="172"/>
-      <c r="E1744" s="172"/>
+      <c r="C1744" s="168"/>
+      <c r="D1744" s="169"/>
+      <c r="E1744" s="169"/>
     </row>
     <row r="1745" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1745" s="79">
@@ -20894,9 +20940,9 @@
         <v>128</v>
       </c>
       <c r="B1761" s="87"/>
-      <c r="C1761" s="171"/>
-      <c r="D1761" s="172"/>
-      <c r="E1761" s="172"/>
+      <c r="C1761" s="168"/>
+      <c r="D1761" s="169"/>
+      <c r="E1761" s="169"/>
     </row>
     <row r="1762" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1762" s="79">
@@ -21047,9 +21093,9 @@
         <v>129</v>
       </c>
       <c r="B1778" s="87"/>
-      <c r="C1778" s="171"/>
-      <c r="D1778" s="172"/>
-      <c r="E1778" s="172"/>
+      <c r="C1778" s="168"/>
+      <c r="D1778" s="169"/>
+      <c r="E1778" s="169"/>
     </row>
     <row r="1779" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1779" s="79">
@@ -21200,9 +21246,9 @@
         <v>130</v>
       </c>
       <c r="B1795" s="87"/>
-      <c r="C1795" s="171"/>
-      <c r="D1795" s="172"/>
-      <c r="E1795" s="172"/>
+      <c r="C1795" s="168"/>
+      <c r="D1795" s="169"/>
+      <c r="E1795" s="169"/>
     </row>
     <row r="1796" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1796" s="79">
@@ -21353,9 +21399,9 @@
         <v>131</v>
       </c>
       <c r="B1812" s="87"/>
-      <c r="C1812" s="171"/>
-      <c r="D1812" s="172"/>
-      <c r="E1812" s="172"/>
+      <c r="C1812" s="168"/>
+      <c r="D1812" s="169"/>
+      <c r="E1812" s="169"/>
     </row>
     <row r="1813" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1813" s="79">
@@ -21506,9 +21552,9 @@
         <v>96</v>
       </c>
       <c r="B1829" s="87"/>
-      <c r="C1829" s="171"/>
-      <c r="D1829" s="172"/>
-      <c r="E1829" s="172"/>
+      <c r="C1829" s="168"/>
+      <c r="D1829" s="169"/>
+      <c r="E1829" s="169"/>
     </row>
     <row r="1830" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1830" s="79">
@@ -21659,9 +21705,9 @@
         <v>132</v>
       </c>
       <c r="B1846" s="87"/>
-      <c r="C1846" s="171"/>
-      <c r="D1846" s="172"/>
-      <c r="E1846" s="172"/>
+      <c r="C1846" s="168"/>
+      <c r="D1846" s="169"/>
+      <c r="E1846" s="169"/>
     </row>
     <row r="1847" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1847" s="79">
@@ -21812,9 +21858,9 @@
         <v>133</v>
       </c>
       <c r="B1863" s="87"/>
-      <c r="C1863" s="171"/>
-      <c r="D1863" s="172"/>
-      <c r="E1863" s="172"/>
+      <c r="C1863" s="168"/>
+      <c r="D1863" s="169"/>
+      <c r="E1863" s="169"/>
     </row>
     <row r="1864" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1864" s="79">
@@ -21965,9 +22011,9 @@
         <v>134</v>
       </c>
       <c r="B1880" s="87"/>
-      <c r="C1880" s="171"/>
-      <c r="D1880" s="172"/>
-      <c r="E1880" s="172"/>
+      <c r="C1880" s="168"/>
+      <c r="D1880" s="169"/>
+      <c r="E1880" s="169"/>
     </row>
     <row r="1881" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1881" s="79">
@@ -22118,9 +22164,9 @@
         <v>135</v>
       </c>
       <c r="B1897" s="87"/>
-      <c r="C1897" s="171"/>
-      <c r="D1897" s="172"/>
-      <c r="E1897" s="172"/>
+      <c r="C1897" s="168"/>
+      <c r="D1897" s="169"/>
+      <c r="E1897" s="169"/>
     </row>
     <row r="1898" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1898" s="79">
@@ -22271,18 +22317,18 @@
         <v>136</v>
       </c>
       <c r="B1914" s="43"/>
-      <c r="C1914" s="187"/>
-      <c r="D1914" s="188"/>
-      <c r="E1914" s="188"/>
+      <c r="C1914" s="172"/>
+      <c r="D1914" s="173"/>
+      <c r="E1914" s="173"/>
     </row>
     <row r="1915" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A1915" s="83" t="s">
         <v>137</v>
       </c>
       <c r="B1915" s="87"/>
-      <c r="C1915" s="171"/>
-      <c r="D1915" s="172"/>
-      <c r="E1915" s="172"/>
+      <c r="C1915" s="168"/>
+      <c r="D1915" s="169"/>
+      <c r="E1915" s="169"/>
     </row>
     <row r="1916" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1916" s="84">
@@ -22433,9 +22479,9 @@
         <v>138</v>
       </c>
       <c r="B1932" s="90"/>
-      <c r="C1932" s="173"/>
-      <c r="D1932" s="174"/>
-      <c r="E1932" s="174"/>
+      <c r="C1932" s="170"/>
+      <c r="D1932" s="171"/>
+      <c r="E1932" s="171"/>
     </row>
     <row r="1933" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1933" s="84">
@@ -22586,9 +22632,9 @@
         <v>139</v>
       </c>
       <c r="B1949" s="87"/>
-      <c r="C1949" s="171"/>
-      <c r="D1949" s="172"/>
-      <c r="E1949" s="172"/>
+      <c r="C1949" s="168"/>
+      <c r="D1949" s="169"/>
+      <c r="E1949" s="169"/>
     </row>
     <row r="1950" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1950" s="84">
@@ -22739,9 +22785,9 @@
         <v>140</v>
       </c>
       <c r="B1966" s="87"/>
-      <c r="C1966" s="171"/>
-      <c r="D1966" s="172"/>
-      <c r="E1966" s="172"/>
+      <c r="C1966" s="168"/>
+      <c r="D1966" s="169"/>
+      <c r="E1966" s="169"/>
     </row>
     <row r="1967" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1967" s="84">
@@ -22892,9 +22938,9 @@
         <v>141</v>
       </c>
       <c r="B1983" s="87"/>
-      <c r="C1983" s="171"/>
-      <c r="D1983" s="172"/>
-      <c r="E1983" s="172"/>
+      <c r="C1983" s="168"/>
+      <c r="D1983" s="169"/>
+      <c r="E1983" s="169"/>
     </row>
     <row r="1984" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1984" s="84">
@@ -23045,9 +23091,9 @@
         <v>142</v>
       </c>
       <c r="B2000" s="87"/>
-      <c r="C2000" s="171"/>
-      <c r="D2000" s="172"/>
-      <c r="E2000" s="172"/>
+      <c r="C2000" s="168"/>
+      <c r="D2000" s="169"/>
+      <c r="E2000" s="169"/>
     </row>
     <row r="2001" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2001" s="84">
@@ -23198,9 +23244,9 @@
         <v>143</v>
       </c>
       <c r="B2017" s="87"/>
-      <c r="C2017" s="171"/>
-      <c r="D2017" s="172"/>
-      <c r="E2017" s="172"/>
+      <c r="C2017" s="168"/>
+      <c r="D2017" s="169"/>
+      <c r="E2017" s="169"/>
     </row>
     <row r="2018" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2018" s="84">
@@ -23351,9 +23397,9 @@
         <v>144</v>
       </c>
       <c r="B2034" s="87"/>
-      <c r="C2034" s="171"/>
-      <c r="D2034" s="172"/>
-      <c r="E2034" s="172"/>
+      <c r="C2034" s="168"/>
+      <c r="D2034" s="169"/>
+      <c r="E2034" s="169"/>
     </row>
     <row r="2035" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2035" s="84">
@@ -23504,9 +23550,9 @@
         <v>145</v>
       </c>
       <c r="B2051" s="87"/>
-      <c r="C2051" s="171"/>
-      <c r="D2051" s="172"/>
-      <c r="E2051" s="172"/>
+      <c r="C2051" s="168"/>
+      <c r="D2051" s="169"/>
+      <c r="E2051" s="169"/>
     </row>
     <row r="2052" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2052" s="84">
@@ -23657,9 +23703,9 @@
         <v>146</v>
       </c>
       <c r="B2068" s="87"/>
-      <c r="C2068" s="171"/>
-      <c r="D2068" s="172"/>
-      <c r="E2068" s="172"/>
+      <c r="C2068" s="168"/>
+      <c r="D2068" s="169"/>
+      <c r="E2068" s="169"/>
     </row>
     <row r="2069" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2069" s="84">
@@ -23810,9 +23856,9 @@
         <v>147</v>
       </c>
       <c r="B2085" s="87"/>
-      <c r="C2085" s="171"/>
-      <c r="D2085" s="172"/>
-      <c r="E2085" s="172"/>
+      <c r="C2085" s="168"/>
+      <c r="D2085" s="169"/>
+      <c r="E2085" s="169"/>
     </row>
     <row r="2086" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2086" s="84">
@@ -23963,9 +24009,9 @@
         <v>148</v>
       </c>
       <c r="B2102" s="87"/>
-      <c r="C2102" s="171"/>
-      <c r="D2102" s="172"/>
-      <c r="E2102" s="172"/>
+      <c r="C2102" s="168"/>
+      <c r="D2102" s="169"/>
+      <c r="E2102" s="169"/>
     </row>
     <row r="2103" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2103" s="84">
@@ -24116,9 +24162,9 @@
         <v>97</v>
       </c>
       <c r="B2119" s="87"/>
-      <c r="C2119" s="171"/>
-      <c r="D2119" s="172"/>
-      <c r="E2119" s="172"/>
+      <c r="C2119" s="168"/>
+      <c r="D2119" s="169"/>
+      <c r="E2119" s="169"/>
     </row>
     <row r="2120" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2120" s="84">
@@ -24269,9 +24315,9 @@
         <v>149</v>
       </c>
       <c r="B2136" s="87"/>
-      <c r="C2136" s="171"/>
-      <c r="D2136" s="172"/>
-      <c r="E2136" s="172"/>
+      <c r="C2136" s="168"/>
+      <c r="D2136" s="169"/>
+      <c r="E2136" s="169"/>
     </row>
     <row r="2137" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2137" s="84">
@@ -24422,9 +24468,9 @@
         <v>150</v>
       </c>
       <c r="B2153" s="87"/>
-      <c r="C2153" s="171"/>
-      <c r="D2153" s="172"/>
-      <c r="E2153" s="172"/>
+      <c r="C2153" s="168"/>
+      <c r="D2153" s="169"/>
+      <c r="E2153" s="169"/>
     </row>
     <row r="2154" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2154" s="84">
@@ -24575,9 +24621,9 @@
         <v>151</v>
       </c>
       <c r="B2170" s="87"/>
-      <c r="C2170" s="171"/>
-      <c r="D2170" s="172"/>
-      <c r="E2170" s="172"/>
+      <c r="C2170" s="168"/>
+      <c r="D2170" s="169"/>
+      <c r="E2170" s="169"/>
     </row>
     <row r="2171" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2171" s="84">
@@ -24725,15 +24771,122 @@
     </row>
   </sheetData>
   <mergeCells count="137">
-    <mergeCell ref="C2034:E2034"/>
-    <mergeCell ref="C2051:E2051"/>
-    <mergeCell ref="C2068:E2068"/>
-    <mergeCell ref="C2085:E2085"/>
-    <mergeCell ref="C2170:E2170"/>
-    <mergeCell ref="C2102:E2102"/>
-    <mergeCell ref="C2119:E2119"/>
-    <mergeCell ref="C2136:E2136"/>
-    <mergeCell ref="C2153:E2153"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="C89:E89"/>
+    <mergeCell ref="C21:E21"/>
+    <mergeCell ref="C38:E38"/>
+    <mergeCell ref="C55:E55"/>
+    <mergeCell ref="C72:E72"/>
+    <mergeCell ref="C208:E208"/>
+    <mergeCell ref="C225:E225"/>
+    <mergeCell ref="C242:E242"/>
+    <mergeCell ref="C259:E259"/>
+    <mergeCell ref="C276:E276"/>
+    <mergeCell ref="C277:E277"/>
+    <mergeCell ref="C106:E106"/>
+    <mergeCell ref="C123:E123"/>
+    <mergeCell ref="C140:E140"/>
+    <mergeCell ref="C157:E157"/>
+    <mergeCell ref="C174:E174"/>
+    <mergeCell ref="C191:E191"/>
+    <mergeCell ref="C396:E396"/>
+    <mergeCell ref="C413:E413"/>
+    <mergeCell ref="C430:E430"/>
+    <mergeCell ref="C447:E447"/>
+    <mergeCell ref="C464:E464"/>
+    <mergeCell ref="C481:E481"/>
+    <mergeCell ref="C294:E294"/>
+    <mergeCell ref="C311:E311"/>
+    <mergeCell ref="C328:E328"/>
+    <mergeCell ref="C345:E345"/>
+    <mergeCell ref="C362:E362"/>
+    <mergeCell ref="C379:E379"/>
+    <mergeCell ref="C584:E584"/>
+    <mergeCell ref="C601:E601"/>
+    <mergeCell ref="C618:E618"/>
+    <mergeCell ref="C635:E635"/>
+    <mergeCell ref="C652:E652"/>
+    <mergeCell ref="C669:E669"/>
+    <mergeCell ref="C498:E498"/>
+    <mergeCell ref="C515:E515"/>
+    <mergeCell ref="C532:E532"/>
+    <mergeCell ref="C549:E549"/>
+    <mergeCell ref="C550:E550"/>
+    <mergeCell ref="C567:E567"/>
+    <mergeCell ref="C788:E788"/>
+    <mergeCell ref="C805:E805"/>
+    <mergeCell ref="C822:E822"/>
+    <mergeCell ref="C823:E823"/>
+    <mergeCell ref="C840:E840"/>
+    <mergeCell ref="C857:E857"/>
+    <mergeCell ref="C686:E686"/>
+    <mergeCell ref="C703:E703"/>
+    <mergeCell ref="C720:E720"/>
+    <mergeCell ref="C737:E737"/>
+    <mergeCell ref="C754:E754"/>
+    <mergeCell ref="C771:E771"/>
+    <mergeCell ref="C976:E976"/>
+    <mergeCell ref="C993:E993"/>
+    <mergeCell ref="C1010:E1010"/>
+    <mergeCell ref="C1027:E1027"/>
+    <mergeCell ref="C1044:E1044"/>
+    <mergeCell ref="C1061:E1061"/>
+    <mergeCell ref="C874:E874"/>
+    <mergeCell ref="C891:E891"/>
+    <mergeCell ref="C908:E908"/>
+    <mergeCell ref="C925:E925"/>
+    <mergeCell ref="C942:E942"/>
+    <mergeCell ref="C959:E959"/>
+    <mergeCell ref="C1164:E1164"/>
+    <mergeCell ref="C1181:E1181"/>
+    <mergeCell ref="C1198:E1198"/>
+    <mergeCell ref="C1215:E1215"/>
+    <mergeCell ref="C1232:E1232"/>
+    <mergeCell ref="C1249:E1249"/>
+    <mergeCell ref="C1078:E1078"/>
+    <mergeCell ref="C1095:E1095"/>
+    <mergeCell ref="C1096:E1096"/>
+    <mergeCell ref="C1113:E1113"/>
+    <mergeCell ref="C1130:E1130"/>
+    <mergeCell ref="C1147:E1147"/>
+    <mergeCell ref="C1368:E1368"/>
+    <mergeCell ref="C1369:E1369"/>
+    <mergeCell ref="C1386:E1386"/>
+    <mergeCell ref="C1403:E1403"/>
+    <mergeCell ref="C1420:E1420"/>
+    <mergeCell ref="C1437:E1437"/>
+    <mergeCell ref="C1266:E1266"/>
+    <mergeCell ref="C1283:E1283"/>
+    <mergeCell ref="C1300:E1300"/>
+    <mergeCell ref="C1317:E1317"/>
+    <mergeCell ref="C1334:E1334"/>
+    <mergeCell ref="C1351:E1351"/>
+    <mergeCell ref="C1556:E1556"/>
+    <mergeCell ref="C1573:E1573"/>
+    <mergeCell ref="C1590:E1590"/>
+    <mergeCell ref="C1607:E1607"/>
+    <mergeCell ref="C1624:E1624"/>
+    <mergeCell ref="C1641:E1641"/>
+    <mergeCell ref="C1454:E1454"/>
+    <mergeCell ref="C1471:E1471"/>
+    <mergeCell ref="C1488:E1488"/>
+    <mergeCell ref="C1505:E1505"/>
+    <mergeCell ref="C1522:E1522"/>
+    <mergeCell ref="C1539:E1539"/>
+    <mergeCell ref="C1744:E1744"/>
+    <mergeCell ref="C1761:E1761"/>
+    <mergeCell ref="C1778:E1778"/>
+    <mergeCell ref="C1795:E1795"/>
+    <mergeCell ref="C1812:E1812"/>
+    <mergeCell ref="C1829:E1829"/>
+    <mergeCell ref="C1642:E1642"/>
+    <mergeCell ref="C1659:E1659"/>
+    <mergeCell ref="C1676:E1676"/>
+    <mergeCell ref="C1693:E1693"/>
+    <mergeCell ref="C1710:E1710"/>
+    <mergeCell ref="C1727:E1727"/>
     <mergeCell ref="C1932:E1932"/>
     <mergeCell ref="C1949:E1949"/>
     <mergeCell ref="C1966:E1966"/>
@@ -24746,122 +24899,15 @@
     <mergeCell ref="C1897:E1897"/>
     <mergeCell ref="C1914:E1914"/>
     <mergeCell ref="C1915:E1915"/>
-    <mergeCell ref="C1744:E1744"/>
-    <mergeCell ref="C1761:E1761"/>
-    <mergeCell ref="C1778:E1778"/>
-    <mergeCell ref="C1795:E1795"/>
-    <mergeCell ref="C1812:E1812"/>
-    <mergeCell ref="C1829:E1829"/>
-    <mergeCell ref="C1642:E1642"/>
-    <mergeCell ref="C1659:E1659"/>
-    <mergeCell ref="C1676:E1676"/>
-    <mergeCell ref="C1693:E1693"/>
-    <mergeCell ref="C1710:E1710"/>
-    <mergeCell ref="C1727:E1727"/>
-    <mergeCell ref="C1556:E1556"/>
-    <mergeCell ref="C1573:E1573"/>
-    <mergeCell ref="C1590:E1590"/>
-    <mergeCell ref="C1607:E1607"/>
-    <mergeCell ref="C1624:E1624"/>
-    <mergeCell ref="C1641:E1641"/>
-    <mergeCell ref="C1454:E1454"/>
-    <mergeCell ref="C1471:E1471"/>
-    <mergeCell ref="C1488:E1488"/>
-    <mergeCell ref="C1505:E1505"/>
-    <mergeCell ref="C1522:E1522"/>
-    <mergeCell ref="C1539:E1539"/>
-    <mergeCell ref="C1368:E1368"/>
-    <mergeCell ref="C1369:E1369"/>
-    <mergeCell ref="C1386:E1386"/>
-    <mergeCell ref="C1403:E1403"/>
-    <mergeCell ref="C1420:E1420"/>
-    <mergeCell ref="C1437:E1437"/>
-    <mergeCell ref="C1266:E1266"/>
-    <mergeCell ref="C1283:E1283"/>
-    <mergeCell ref="C1300:E1300"/>
-    <mergeCell ref="C1317:E1317"/>
-    <mergeCell ref="C1334:E1334"/>
-    <mergeCell ref="C1351:E1351"/>
-    <mergeCell ref="C1164:E1164"/>
-    <mergeCell ref="C1181:E1181"/>
-    <mergeCell ref="C1198:E1198"/>
-    <mergeCell ref="C1215:E1215"/>
-    <mergeCell ref="C1232:E1232"/>
-    <mergeCell ref="C1249:E1249"/>
-    <mergeCell ref="C1078:E1078"/>
-    <mergeCell ref="C1095:E1095"/>
-    <mergeCell ref="C1096:E1096"/>
-    <mergeCell ref="C1113:E1113"/>
-    <mergeCell ref="C1130:E1130"/>
-    <mergeCell ref="C1147:E1147"/>
-    <mergeCell ref="C976:E976"/>
-    <mergeCell ref="C993:E993"/>
-    <mergeCell ref="C1010:E1010"/>
-    <mergeCell ref="C1027:E1027"/>
-    <mergeCell ref="C1044:E1044"/>
-    <mergeCell ref="C1061:E1061"/>
-    <mergeCell ref="C874:E874"/>
-    <mergeCell ref="C891:E891"/>
-    <mergeCell ref="C908:E908"/>
-    <mergeCell ref="C925:E925"/>
-    <mergeCell ref="C942:E942"/>
-    <mergeCell ref="C959:E959"/>
-    <mergeCell ref="C788:E788"/>
-    <mergeCell ref="C805:E805"/>
-    <mergeCell ref="C822:E822"/>
-    <mergeCell ref="C823:E823"/>
-    <mergeCell ref="C840:E840"/>
-    <mergeCell ref="C857:E857"/>
-    <mergeCell ref="C686:E686"/>
-    <mergeCell ref="C703:E703"/>
-    <mergeCell ref="C720:E720"/>
-    <mergeCell ref="C737:E737"/>
-    <mergeCell ref="C754:E754"/>
-    <mergeCell ref="C771:E771"/>
-    <mergeCell ref="C584:E584"/>
-    <mergeCell ref="C601:E601"/>
-    <mergeCell ref="C618:E618"/>
-    <mergeCell ref="C635:E635"/>
-    <mergeCell ref="C652:E652"/>
-    <mergeCell ref="C669:E669"/>
-    <mergeCell ref="C498:E498"/>
-    <mergeCell ref="C515:E515"/>
-    <mergeCell ref="C532:E532"/>
-    <mergeCell ref="C549:E549"/>
-    <mergeCell ref="C550:E550"/>
-    <mergeCell ref="C567:E567"/>
-    <mergeCell ref="C396:E396"/>
-    <mergeCell ref="C413:E413"/>
-    <mergeCell ref="C430:E430"/>
-    <mergeCell ref="C447:E447"/>
-    <mergeCell ref="C464:E464"/>
-    <mergeCell ref="C481:E481"/>
-    <mergeCell ref="C294:E294"/>
-    <mergeCell ref="C311:E311"/>
-    <mergeCell ref="C328:E328"/>
-    <mergeCell ref="C345:E345"/>
-    <mergeCell ref="C362:E362"/>
-    <mergeCell ref="C379:E379"/>
-    <mergeCell ref="C225:E225"/>
-    <mergeCell ref="C242:E242"/>
-    <mergeCell ref="C259:E259"/>
-    <mergeCell ref="C276:E276"/>
-    <mergeCell ref="C277:E277"/>
-    <mergeCell ref="C106:E106"/>
-    <mergeCell ref="C123:E123"/>
-    <mergeCell ref="C140:E140"/>
-    <mergeCell ref="C157:E157"/>
-    <mergeCell ref="C174:E174"/>
-    <mergeCell ref="C191:E191"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="C89:E89"/>
-    <mergeCell ref="C21:E21"/>
-    <mergeCell ref="C38:E38"/>
-    <mergeCell ref="C55:E55"/>
-    <mergeCell ref="C72:E72"/>
-    <mergeCell ref="C208:E208"/>
+    <mergeCell ref="C2034:E2034"/>
+    <mergeCell ref="C2051:E2051"/>
+    <mergeCell ref="C2068:E2068"/>
+    <mergeCell ref="C2085:E2085"/>
+    <mergeCell ref="C2170:E2170"/>
+    <mergeCell ref="C2102:E2102"/>
+    <mergeCell ref="C2119:E2119"/>
+    <mergeCell ref="C2136:E2136"/>
+    <mergeCell ref="C2153:E2153"/>
   </mergeCells>
   <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -26120,150 +26166,163 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="33">
-      <c r="A1" s="214" t="s">
+      <c r="A1" s="213" t="s">
         <v>184</v>
       </c>
-      <c r="B1" s="215"/>
+      <c r="B1" s="214"/>
       <c r="C1" s="118"/>
       <c r="D1" s="5"/>
       <c r="E1" s="5"/>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="220" t="s">
+      <c r="A2" s="210" t="s">
         <v>183</v>
       </c>
-      <c r="B2" s="221"/>
+      <c r="B2" s="211"/>
       <c r="C2" s="120"/>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="222" t="s">
+      <c r="A3" s="212" t="s">
         <v>185</v>
       </c>
-      <c r="B3" s="221"/>
+      <c r="B3" s="211"/>
       <c r="C3" s="120"/>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="218"/>
-      <c r="B4" s="219"/>
+      <c r="A4" s="217"/>
+      <c r="B4" s="218"/>
       <c r="C4" s="120"/>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="216" t="s">
+      <c r="A5" s="215" t="s">
         <v>194</v>
       </c>
-      <c r="B5" s="217"/>
+      <c r="B5" s="216"/>
       <c r="C5" s="120"/>
     </row>
     <row r="7" spans="1:5" ht="18.75">
-      <c r="A7" s="208" t="s">
+      <c r="A7" s="221" t="s">
         <v>186</v>
       </c>
-      <c r="B7" s="209"/>
+      <c r="B7" s="222"/>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="120"/>
       <c r="B8" s="9"/>
     </row>
     <row r="9" spans="1:5" ht="39" customHeight="1">
-      <c r="A9" s="210" t="s">
+      <c r="A9" s="219" t="s">
         <v>187</v>
       </c>
-      <c r="B9" s="211"/>
+      <c r="B9" s="220"/>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="212"/>
-      <c r="B10" s="213"/>
+      <c r="A10" s="206"/>
+      <c r="B10" s="207"/>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="204" t="s">
+      <c r="A11" s="208" t="s">
         <v>188</v>
       </c>
-      <c r="B11" s="205"/>
+      <c r="B11" s="209"/>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="204" t="s">
+      <c r="A12" s="208" t="s">
         <v>189</v>
       </c>
-      <c r="B12" s="205"/>
+      <c r="B12" s="209"/>
     </row>
     <row r="13" spans="1:5" ht="43.5" customHeight="1">
-      <c r="A13" s="204" t="s">
+      <c r="A13" s="208" t="s">
         <v>190</v>
       </c>
-      <c r="B13" s="205"/>
+      <c r="B13" s="209"/>
     </row>
     <row r="14" spans="1:5" ht="19.5" customHeight="1">
-      <c r="A14" s="204" t="s">
+      <c r="A14" s="208" t="s">
         <v>191</v>
       </c>
-      <c r="B14" s="205"/>
+      <c r="B14" s="209"/>
     </row>
     <row r="15" spans="1:5" ht="18" customHeight="1">
-      <c r="A15" s="204" t="s">
+      <c r="A15" s="208" t="s">
         <v>192</v>
       </c>
-      <c r="B15" s="205"/>
+      <c r="B15" s="209"/>
     </row>
     <row r="16" spans="1:5" ht="21" customHeight="1">
-      <c r="A16" s="204" t="s">
+      <c r="A16" s="208" t="s">
         <v>193</v>
       </c>
-      <c r="B16" s="205"/>
+      <c r="B16" s="209"/>
     </row>
     <row r="17" spans="1:2" ht="48.75" customHeight="1">
-      <c r="A17" s="206" t="s">
+      <c r="A17" s="204" t="s">
         <v>195</v>
       </c>
-      <c r="B17" s="207"/>
+      <c r="B17" s="205"/>
     </row>
     <row r="19" spans="1:2" ht="18.75">
-      <c r="A19" s="208" t="s">
+      <c r="A19" s="221" t="s">
         <v>197</v>
       </c>
-      <c r="B19" s="209"/>
+      <c r="B19" s="222"/>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="120"/>
       <c r="B20" s="9"/>
     </row>
     <row r="21" spans="1:2">
-      <c r="A21" s="210" t="s">
+      <c r="A21" s="219" t="s">
         <v>198</v>
       </c>
-      <c r="B21" s="211"/>
+      <c r="B21" s="220"/>
     </row>
     <row r="22" spans="1:2">
-      <c r="A22" s="212"/>
-      <c r="B22" s="213"/>
+      <c r="A22" s="206"/>
+      <c r="B22" s="207"/>
     </row>
     <row r="23" spans="1:2">
-      <c r="A23" s="204" t="s">
+      <c r="A23" s="208" t="s">
         <v>199</v>
       </c>
-      <c r="B23" s="205"/>
+      <c r="B23" s="209"/>
     </row>
     <row r="24" spans="1:2">
-      <c r="A24" s="204"/>
-      <c r="B24" s="205"/>
+      <c r="A24" s="208"/>
+      <c r="B24" s="209"/>
     </row>
     <row r="25" spans="1:2">
-      <c r="A25" s="204" t="s">
+      <c r="A25" s="208" t="s">
         <v>200</v>
       </c>
-      <c r="B25" s="205"/>
+      <c r="B25" s="209"/>
     </row>
     <row r="26" spans="1:2">
-      <c r="A26" s="204" t="s">
+      <c r="A26" s="208" t="s">
         <v>201</v>
       </c>
-      <c r="B26" s="205"/>
+      <c r="B26" s="209"/>
     </row>
     <row r="27" spans="1:2">
-      <c r="A27" s="206"/>
-      <c r="B27" s="207"/>
+      <c r="A27" s="204"/>
+      <c r="B27" s="205"/>
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A7:B7"/>
     <mergeCell ref="A17:B17"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
@@ -26274,19 +26333,6 @@
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="A14:B14"/>
     <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A24:B24"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A3" r:id="rId1"/>

</xml_diff>

<commit_message>
Tempo - some boss fight action.
</commit_message>
<xml_diff>
--- a/trunk/Tempo/Tempo.xlsx
+++ b/trunk/Tempo/Tempo.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1153" uniqueCount="277">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1156" uniqueCount="277">
   <si>
     <t>Notes</t>
   </si>
@@ -900,10 +900,17 @@
     <numFmt numFmtId="164" formatCode="#,##0;[Red]#,##0"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="52">
+  <fonts count="53">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1880,34 +1887,34 @@
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="27" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="33" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="46" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="27" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="34" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="47" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="223">
+  <cellXfs count="224">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1915,208 +1922,208 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="24" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="21" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="21" fillId="13" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="22" fillId="13" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="28" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="29" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="30" fillId="13" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="22" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="31" fillId="13" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="13" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="32" fillId="13" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="13" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="32" fillId="13" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="31" fillId="13" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="33" fillId="16" borderId="23" xfId="2" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="33" fillId="16" borderId="23" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="34" fillId="16" borderId="23" xfId="2" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="34" fillId="16" borderId="23" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="16" borderId="22" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="34" fillId="16" borderId="22" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="27" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="32" fillId="0" borderId="27" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="27" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="33" fillId="0" borderId="27" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="3" fontId="34" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="30" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="32" fillId="0" borderId="30" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="32" fillId="0" borderId="29" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="34" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="32" fillId="17" borderId="31" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="32" fillId="18" borderId="31" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="32" fillId="19" borderId="31" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="33" fillId="20" borderId="23" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="33" fillId="20" borderId="23" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="35" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="30" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="33" fillId="0" borderId="30" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="33" fillId="0" borderId="29" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="35" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="33" fillId="17" borderId="31" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="33" fillId="18" borderId="31" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="33" fillId="19" borderId="31" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="34" fillId="20" borderId="23" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="34" fillId="20" borderId="23" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="20" borderId="22" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="34" fillId="20" borderId="22" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="33" fillId="21" borderId="23" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="33" fillId="21" borderId="23" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="34" fillId="21" borderId="23" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="34" fillId="21" borderId="23" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="21" borderId="22" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="34" fillId="21" borderId="22" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="43" fillId="16" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="44" fillId="16" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="43" fillId="20" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="44" fillId="20" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
-    <xf numFmtId="3" fontId="34" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="32" fillId="0" borderId="42" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="34" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="34" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="34" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="32" fillId="0" borderId="42" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="35" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="33" fillId="0" borderId="42" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="35" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="35" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="35" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="33" fillId="0" borderId="42" xfId="1" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2126,10 +2133,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2150,19 +2157,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="23" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="50" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="51" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="41" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="35" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="51" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="28" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="37" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="40" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="34" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="50" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="27" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="36" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="39" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="39" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="40" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
@@ -2172,10 +2182,10 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
+    <xf numFmtId="3" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="3" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
@@ -2185,126 +2195,126 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="21" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="38" fillId="21" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="20" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="38" fillId="20" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="40" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="23" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="35" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="41" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="36" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="42" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="42" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="43" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="16" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="38" fillId="16" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="21" fillId="13" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="22" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="21" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="25" fillId="14" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="23" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="22" fillId="13" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="23" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="26" fillId="14" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="14" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="14" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="14" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="14" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="26" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="51" fillId="22" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="52" fillId="22" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="51" fillId="22" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="52" fillId="22" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="51" fillId="22" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="52" fillId="22" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="49" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="50" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="50" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="48" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="48" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="46" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="4"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="4"/>
     </xf>
-    <xf numFmtId="0" fontId="46" fillId="0" borderId="33" xfId="3" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="47" fillId="0" borderId="33" xfId="3" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" indent="4"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="47" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="47" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="49" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="49" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="48" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Accent1" xfId="2" builtinId="29"/>
@@ -2612,11 +2622,11 @@
   <sheetPr>
     <tabColor theme="4" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:K158"/>
+  <dimension ref="A1:K161"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C58" sqref="C58"/>
+      <pane ySplit="6" topLeftCell="A48" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C61" sqref="C61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" outlineLevelRow="2"/>
@@ -2644,7 +2654,7 @@
       <c r="F1" s="165"/>
       <c r="G1" s="140"/>
       <c r="H1" s="141">
-        <f>SUM(G1:G65540)</f>
+        <f>SUM(G1:G65543)</f>
         <v>0</v>
       </c>
       <c r="I1" s="141" t="s">
@@ -3371,7 +3381,7 @@
         <v>11282</v>
       </c>
       <c r="E44" s="123">
-        <f t="shared" ref="E44:E65" si="3">IF(AND(C44&gt;0,D44&gt;0), D44-C44, 0)</f>
+        <f t="shared" ref="E44:E68" si="3">IF(AND(C44&gt;0,D44&gt;0), D44-C44, 0)</f>
         <v>0</v>
       </c>
       <c r="F44" s="104"/>
@@ -3639,8 +3649,12 @@
     </row>
     <row r="58" spans="1:9" ht="15" outlineLevel="1">
       <c r="A58" s="159"/>
-      <c r="B58" s="100"/>
-      <c r="C58" s="101"/>
+      <c r="B58" s="223" t="s">
+        <v>264</v>
+      </c>
+      <c r="C58" s="101">
+        <v>18087</v>
+      </c>
       <c r="D58" s="101"/>
       <c r="E58" s="123">
         <f t="shared" si="3"/>
@@ -3650,52 +3664,55 @@
     </row>
     <row r="59" spans="1:9" ht="15" outlineLevel="1">
       <c r="A59" s="159"/>
-      <c r="B59" s="100"/>
-      <c r="C59" s="101"/>
+      <c r="B59" s="223" t="s">
+        <v>265</v>
+      </c>
+      <c r="C59" s="101">
+        <v>18213</v>
+      </c>
       <c r="D59" s="101"/>
       <c r="E59" s="123">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="F59" s="105"/>
+      <c r="I59" s="112">
+        <f>C59-C58</f>
+        <v>126</v>
+      </c>
     </row>
     <row r="60" spans="1:9" ht="15" outlineLevel="1">
       <c r="A60" s="159"/>
-      <c r="B60" s="150" t="s">
-        <v>237</v>
-      </c>
-      <c r="C60" s="101"/>
+      <c r="B60" s="223" t="s">
+        <v>266</v>
+      </c>
+      <c r="C60" s="101">
+        <v>18306</v>
+      </c>
       <c r="D60" s="101"/>
       <c r="E60" s="123">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="F60" s="105"/>
+      <c r="I60" s="112">
+        <f>C60-C59</f>
+        <v>93</v>
+      </c>
     </row>
     <row r="61" spans="1:9" ht="15" outlineLevel="1">
       <c r="A61" s="159"/>
-      <c r="B61" s="150" t="s">
-        <v>223</v>
-      </c>
+      <c r="B61" s="223"/>
       <c r="C61" s="101"/>
-      <c r="D61" s="101">
-        <v>23906</v>
-      </c>
-      <c r="E61" s="123">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
+      <c r="D61" s="101"/>
+      <c r="E61" s="123"/>
       <c r="F61" s="105"/>
     </row>
     <row r="62" spans="1:9" ht="15" outlineLevel="1">
       <c r="A62" s="159"/>
-      <c r="B62" s="150" t="s">
-        <v>238</v>
-      </c>
+      <c r="B62" s="100"/>
       <c r="C62" s="101"/>
-      <c r="D62" s="101">
-        <v>24132</v>
-      </c>
+      <c r="D62" s="101"/>
       <c r="E62" s="123">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -3705,23 +3722,24 @@
     <row r="63" spans="1:9" ht="15" outlineLevel="1">
       <c r="A63" s="159"/>
       <c r="B63" s="150" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C63" s="101"/>
-      <c r="D63" s="101">
-        <v>24753</v>
-      </c>
-      <c r="E63" s="123"/>
+      <c r="D63" s="101"/>
+      <c r="E63" s="123">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
       <c r="F63" s="105"/>
     </row>
     <row r="64" spans="1:9" ht="15" outlineLevel="1">
       <c r="A64" s="159"/>
       <c r="B64" s="150" t="s">
-        <v>217</v>
+        <v>223</v>
       </c>
       <c r="C64" s="101"/>
       <c r="D64" s="101">
-        <v>25129</v>
+        <v>23906</v>
       </c>
       <c r="E64" s="123">
         <f t="shared" si="3"/>
@@ -3729,132 +3747,133 @@
       </c>
       <c r="F64" s="105"/>
     </row>
-    <row r="65" spans="1:8" ht="15.75" outlineLevel="1" thickBot="1">
+    <row r="65" spans="1:8" ht="15" outlineLevel="1">
       <c r="A65" s="159"/>
-      <c r="B65" s="98" t="s">
+      <c r="B65" s="150" t="s">
+        <v>238</v>
+      </c>
+      <c r="C65" s="101"/>
+      <c r="D65" s="101">
+        <v>24132</v>
+      </c>
+      <c r="E65" s="123">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F65" s="105"/>
+    </row>
+    <row r="66" spans="1:8" ht="15" outlineLevel="1">
+      <c r="A66" s="159"/>
+      <c r="B66" s="150" t="s">
+        <v>239</v>
+      </c>
+      <c r="C66" s="101"/>
+      <c r="D66" s="101">
+        <v>24753</v>
+      </c>
+      <c r="E66" s="123"/>
+      <c r="F66" s="105"/>
+    </row>
+    <row r="67" spans="1:8" ht="15" outlineLevel="1">
+      <c r="A67" s="159"/>
+      <c r="B67" s="150" t="s">
+        <v>217</v>
+      </c>
+      <c r="C67" s="101"/>
+      <c r="D67" s="101">
+        <v>25129</v>
+      </c>
+      <c r="E67" s="123">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F67" s="105"/>
+    </row>
+    <row r="68" spans="1:8" ht="15.75" outlineLevel="1" thickBot="1">
+      <c r="A68" s="159"/>
+      <c r="B68" s="98" t="s">
         <v>179</v>
       </c>
-      <c r="C65" s="99"/>
-      <c r="D65" s="99">
+      <c r="C68" s="99"/>
+      <c r="D68" s="99">
         <v>25174</v>
       </c>
-      <c r="E65" s="125">
+      <c r="E68" s="125">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="F65" s="104"/>
-    </row>
-    <row r="66" spans="1:8" ht="17.25" thickTop="1" thickBot="1">
-      <c r="A66" s="116" t="s">
+      <c r="F68" s="104"/>
+    </row>
+    <row r="69" spans="1:8" ht="17.25" thickTop="1" thickBot="1">
+      <c r="A69" s="116" t="s">
         <v>227</v>
       </c>
-      <c r="B66" s="102" t="s">
+      <c r="B69" s="102" t="s">
         <v>173</v>
       </c>
-      <c r="C66" s="103">
-        <f>C65-C44</f>
-        <v>0</v>
-      </c>
-      <c r="D66" s="103">
-        <f>D65-D44</f>
+      <c r="C69" s="103">
+        <f>C68-C44</f>
+        <v>0</v>
+      </c>
+      <c r="D69" s="103">
+        <f>D68-D44</f>
         <v>13892</v>
       </c>
-      <c r="E66" s="126">
-        <f>E65-E44</f>
-        <v>0</v>
-      </c>
-      <c r="F66" s="107"/>
-      <c r="G66" s="112">
-        <f>E66</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="67" spans="1:8" ht="13.5" thickBot="1"/>
-    <row r="68" spans="1:8" ht="15" customHeight="1" outlineLevel="1">
-      <c r="A68" s="160" t="s">
+      <c r="E69" s="126">
+        <f>E68-E44</f>
+        <v>0</v>
+      </c>
+      <c r="F69" s="107"/>
+      <c r="G69" s="112">
+        <f>E69</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" ht="13.5" thickBot="1"/>
+    <row r="71" spans="1:8" ht="15" customHeight="1" outlineLevel="1">
+      <c r="A71" s="160" t="s">
         <v>240</v>
       </c>
-      <c r="B68" s="109" t="s">
+      <c r="B71" s="109" t="s">
         <v>175</v>
       </c>
-      <c r="C68" s="110" t="s">
+      <c r="C71" s="110" t="s">
         <v>42</v>
       </c>
-      <c r="D68" s="110" t="s">
+      <c r="D71" s="110" t="s">
         <v>41</v>
       </c>
-      <c r="E68" s="110" t="s">
+      <c r="E71" s="110" t="s">
         <v>43</v>
       </c>
-      <c r="F68" s="111" t="s">
+      <c r="F71" s="111" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="69" spans="1:8" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="A69" s="159"/>
-      <c r="B69" s="98" t="s">
+    <row r="72" spans="1:8" ht="15.75" outlineLevel="1" thickBot="1">
+      <c r="A72" s="159"/>
+      <c r="B72" s="98" t="s">
         <v>177</v>
       </c>
-      <c r="C69" s="99"/>
-      <c r="D69" s="99">
+      <c r="C72" s="99"/>
+      <c r="D72" s="99">
         <v>25174</v>
       </c>
-      <c r="E69" s="123">
-        <f t="shared" ref="E69:E81" si="5">IF(AND(C69&gt;0,D69&gt;0), D69-C69, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="F69" s="104"/>
-      <c r="H69">
+      <c r="E72" s="123">
+        <f t="shared" ref="E72:E84" si="5">IF(AND(C72&gt;0,D72&gt;0), D72-C72, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="F72" s="104"/>
+      <c r="H72">
         <v>49739</v>
       </c>
     </row>
-    <row r="70" spans="1:8" ht="15.75" outlineLevel="1" thickTop="1">
-      <c r="A70" s="159"/>
-      <c r="B70" s="100"/>
-      <c r="C70" s="101"/>
-      <c r="D70" s="101"/>
-      <c r="E70" s="124">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="F70" s="105"/>
-    </row>
-    <row r="71" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A71" s="159"/>
-      <c r="B71" s="151" t="s">
-        <v>242</v>
-      </c>
-      <c r="C71" s="101"/>
-      <c r="D71" s="101">
-        <v>26754</v>
-      </c>
-      <c r="E71" s="123">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="F71" s="105"/>
-    </row>
-    <row r="72" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A72" s="159"/>
-      <c r="B72" s="100"/>
-      <c r="C72" s="101"/>
-      <c r="D72" s="101"/>
-      <c r="E72" s="123">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="F72" s="105"/>
-    </row>
-    <row r="73" spans="1:8" ht="15" outlineLevel="1">
+    <row r="73" spans="1:8" ht="15.75" outlineLevel="1" thickTop="1">
       <c r="A73" s="159"/>
-      <c r="B73" s="151" t="s">
-        <v>243</v>
-      </c>
+      <c r="B73" s="100"/>
       <c r="C73" s="101"/>
-      <c r="D73" s="101">
-        <v>27765</v>
-      </c>
-      <c r="E73" s="123">
+      <c r="D73" s="101"/>
+      <c r="E73" s="124">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -3862,9 +3881,13 @@
     </row>
     <row r="74" spans="1:8" ht="15" outlineLevel="1">
       <c r="A74" s="159"/>
-      <c r="B74" s="100"/>
+      <c r="B74" s="151" t="s">
+        <v>242</v>
+      </c>
       <c r="C74" s="101"/>
-      <c r="D74" s="101"/>
+      <c r="D74" s="101">
+        <v>26754</v>
+      </c>
       <c r="E74" s="123">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -3873,13 +3896,9 @@
     </row>
     <row r="75" spans="1:8" ht="15" outlineLevel="1">
       <c r="A75" s="159"/>
-      <c r="B75" s="151" t="s">
-        <v>244</v>
-      </c>
+      <c r="B75" s="100"/>
       <c r="C75" s="101"/>
-      <c r="D75" s="101">
-        <v>30127</v>
-      </c>
+      <c r="D75" s="101"/>
       <c r="E75" s="123">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -3888,9 +3907,13 @@
     </row>
     <row r="76" spans="1:8" ht="15" outlineLevel="1">
       <c r="A76" s="159"/>
-      <c r="B76" s="100"/>
+      <c r="B76" s="151" t="s">
+        <v>243</v>
+      </c>
       <c r="C76" s="101"/>
-      <c r="D76" s="101"/>
+      <c r="D76" s="101">
+        <v>27765</v>
+      </c>
       <c r="E76" s="123">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -3899,13 +3922,9 @@
     </row>
     <row r="77" spans="1:8" ht="15" outlineLevel="1">
       <c r="A77" s="159"/>
-      <c r="B77" s="151" t="s">
-        <v>245</v>
-      </c>
+      <c r="B77" s="100"/>
       <c r="C77" s="101"/>
-      <c r="D77" s="101">
-        <v>33299</v>
-      </c>
+      <c r="D77" s="101"/>
       <c r="E77" s="123">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -3915,11 +3934,11 @@
     <row r="78" spans="1:8" ht="15" outlineLevel="1">
       <c r="A78" s="159"/>
       <c r="B78" s="151" t="s">
-        <v>238</v>
+        <v>244</v>
       </c>
       <c r="C78" s="101"/>
       <c r="D78" s="101">
-        <v>33527</v>
+        <v>30127</v>
       </c>
       <c r="E78" s="123">
         <f t="shared" si="5"/>
@@ -3929,13 +3948,9 @@
     </row>
     <row r="79" spans="1:8" ht="15" outlineLevel="1">
       <c r="A79" s="159"/>
-      <c r="B79" s="151" t="s">
-        <v>246</v>
-      </c>
+      <c r="B79" s="100"/>
       <c r="C79" s="101"/>
-      <c r="D79" s="101">
-        <v>34309</v>
-      </c>
+      <c r="D79" s="101"/>
       <c r="E79" s="123">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -3945,11 +3960,11 @@
     <row r="80" spans="1:8" ht="15" outlineLevel="1">
       <c r="A80" s="159"/>
       <c r="B80" s="151" t="s">
-        <v>217</v>
+        <v>245</v>
       </c>
       <c r="C80" s="101"/>
       <c r="D80" s="101">
-        <v>34727</v>
+        <v>33299</v>
       </c>
       <c r="E80" s="123">
         <f t="shared" si="5"/>
@@ -3957,136 +3972,140 @@
       </c>
       <c r="F80" s="105"/>
     </row>
-    <row r="81" spans="1:8" ht="15.75" outlineLevel="1" thickBot="1">
+    <row r="81" spans="1:8" ht="15" outlineLevel="1">
       <c r="A81" s="159"/>
-      <c r="B81" s="98" t="s">
+      <c r="B81" s="151" t="s">
+        <v>238</v>
+      </c>
+      <c r="C81" s="101"/>
+      <c r="D81" s="101">
+        <v>33527</v>
+      </c>
+      <c r="E81" s="123">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="F81" s="105"/>
+    </row>
+    <row r="82" spans="1:8" ht="15" outlineLevel="1">
+      <c r="A82" s="159"/>
+      <c r="B82" s="151" t="s">
+        <v>246</v>
+      </c>
+      <c r="C82" s="101"/>
+      <c r="D82" s="101">
+        <v>34309</v>
+      </c>
+      <c r="E82" s="123">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="F82" s="105"/>
+    </row>
+    <row r="83" spans="1:8" ht="15" outlineLevel="1">
+      <c r="A83" s="159"/>
+      <c r="B83" s="151" t="s">
+        <v>217</v>
+      </c>
+      <c r="C83" s="101"/>
+      <c r="D83" s="101">
+        <v>34727</v>
+      </c>
+      <c r="E83" s="123">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="F83" s="105"/>
+    </row>
+    <row r="84" spans="1:8" ht="15.75" outlineLevel="1" thickBot="1">
+      <c r="A84" s="159"/>
+      <c r="B84" s="98" t="s">
         <v>179</v>
       </c>
-      <c r="C81" s="99"/>
-      <c r="D81" s="99">
+      <c r="C84" s="99"/>
+      <c r="D84" s="99">
         <v>34795</v>
       </c>
-      <c r="E81" s="125">
+      <c r="E84" s="125">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="F81" s="104"/>
-    </row>
-    <row r="82" spans="1:8" ht="17.25" thickTop="1" thickBot="1">
-      <c r="A82" s="117" t="s">
+      <c r="F84" s="104"/>
+    </row>
+    <row r="85" spans="1:8" ht="17.25" thickTop="1" thickBot="1">
+      <c r="A85" s="117" t="s">
         <v>241</v>
       </c>
-      <c r="B82" s="102" t="s">
+      <c r="B85" s="102" t="s">
         <v>173</v>
       </c>
-      <c r="C82" s="103">
-        <f>C81-C69</f>
-        <v>0</v>
-      </c>
-      <c r="D82" s="103">
-        <f>D81-D69</f>
+      <c r="C85" s="103">
+        <f>C84-C72</f>
+        <v>0</v>
+      </c>
+      <c r="D85" s="103">
+        <f>D84-D72</f>
         <v>9621</v>
       </c>
-      <c r="E82" s="126">
-        <f>E81-E69</f>
-        <v>0</v>
-      </c>
-      <c r="F82" s="108"/>
-      <c r="G82" s="112">
-        <f>E82</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="83" spans="1:8" ht="13.5" thickBot="1"/>
-    <row r="84" spans="1:8" ht="15" customHeight="1" outlineLevel="1">
-      <c r="A84" s="158" t="s">
+      <c r="E85" s="126">
+        <f>E84-E72</f>
+        <v>0</v>
+      </c>
+      <c r="F85" s="108"/>
+      <c r="G85" s="112">
+        <f>E85</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" ht="13.5" thickBot="1"/>
+    <row r="87" spans="1:8" ht="15" customHeight="1" outlineLevel="1">
+      <c r="A87" s="158" t="s">
         <v>247</v>
       </c>
-      <c r="B84" s="113" t="s">
+      <c r="B87" s="113" t="s">
         <v>175</v>
       </c>
-      <c r="C84" s="114" t="s">
+      <c r="C87" s="114" t="s">
         <v>42</v>
       </c>
-      <c r="D84" s="114" t="s">
+      <c r="D87" s="114" t="s">
         <v>41</v>
       </c>
-      <c r="E84" s="114" t="s">
+      <c r="E87" s="114" t="s">
         <v>43</v>
       </c>
-      <c r="F84" s="115" t="s">
+      <c r="F87" s="115" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="85" spans="1:8" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="A85" s="159"/>
-      <c r="B85" s="98" t="s">
+    <row r="88" spans="1:8" ht="15.75" outlineLevel="1" thickBot="1">
+      <c r="A88" s="159"/>
+      <c r="B88" s="98" t="s">
         <v>177</v>
       </c>
-      <c r="C85" s="99"/>
-      <c r="D85" s="99">
+      <c r="C88" s="99"/>
+      <c r="D88" s="99">
         <v>34795</v>
       </c>
-      <c r="E85" s="123">
-        <f t="shared" ref="E85:E98" si="6">IF(AND(C85&gt;0,D85&gt;0), D85-C85, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="F85" s="104"/>
-      <c r="H85">
+      <c r="E88" s="123">
+        <f t="shared" ref="E88:E101" si="6">IF(AND(C88&gt;0,D88&gt;0), D88-C88, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="F88" s="104"/>
+      <c r="H88">
         <v>67476</v>
       </c>
     </row>
-    <row r="86" spans="1:8" ht="15.75" outlineLevel="1" thickTop="1">
-      <c r="A86" s="159"/>
-      <c r="B86" s="151" t="s">
-        <v>228</v>
-      </c>
-      <c r="C86" s="101"/>
-      <c r="D86" s="101">
-        <v>36326</v>
-      </c>
-      <c r="E86" s="124">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="F86" s="105"/>
-    </row>
-    <row r="87" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A87" s="159"/>
-      <c r="B87" s="151" t="s">
-        <v>221</v>
-      </c>
-      <c r="C87" s="101"/>
-      <c r="D87" s="101">
-        <v>37764</v>
-      </c>
-      <c r="E87" s="123">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="F87" s="105"/>
-    </row>
-    <row r="88" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A88" s="159"/>
-      <c r="B88" s="100"/>
-      <c r="C88" s="101"/>
-      <c r="D88" s="101"/>
-      <c r="E88" s="123">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="F88" s="105"/>
-    </row>
-    <row r="89" spans="1:8" ht="15" outlineLevel="1">
+    <row r="89" spans="1:8" ht="15.75" outlineLevel="1" thickTop="1">
       <c r="A89" s="159"/>
       <c r="B89" s="151" t="s">
-        <v>222</v>
+        <v>228</v>
       </c>
       <c r="C89" s="101"/>
       <c r="D89" s="101">
-        <v>43241</v>
-      </c>
-      <c r="E89" s="123">
+        <v>36326</v>
+      </c>
+      <c r="E89" s="124">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
@@ -4094,9 +4113,13 @@
     </row>
     <row r="90" spans="1:8" ht="15" outlineLevel="1">
       <c r="A90" s="159"/>
-      <c r="B90" s="100"/>
+      <c r="B90" s="151" t="s">
+        <v>221</v>
+      </c>
       <c r="C90" s="101"/>
-      <c r="D90" s="101"/>
+      <c r="D90" s="101">
+        <v>37764</v>
+      </c>
       <c r="E90" s="123">
         <f t="shared" si="6"/>
         <v>0</v>
@@ -4105,13 +4128,9 @@
     </row>
     <row r="91" spans="1:8" ht="15" outlineLevel="1">
       <c r="A91" s="159"/>
-      <c r="B91" s="152" t="s">
-        <v>236</v>
-      </c>
+      <c r="B91" s="100"/>
       <c r="C91" s="101"/>
-      <c r="D91" s="101">
-        <v>45890</v>
-      </c>
+      <c r="D91" s="101"/>
       <c r="E91" s="123">
         <f t="shared" si="6"/>
         <v>0</v>
@@ -4120,9 +4139,13 @@
     </row>
     <row r="92" spans="1:8" ht="15" outlineLevel="1">
       <c r="A92" s="159"/>
-      <c r="B92" s="100"/>
+      <c r="B92" s="151" t="s">
+        <v>222</v>
+      </c>
       <c r="C92" s="101"/>
-      <c r="D92" s="101"/>
+      <c r="D92" s="101">
+        <v>43241</v>
+      </c>
       <c r="E92" s="123">
         <f t="shared" si="6"/>
         <v>0</v>
@@ -4143,11 +4166,11 @@
     <row r="94" spans="1:8" ht="15" outlineLevel="1">
       <c r="A94" s="159"/>
       <c r="B94" s="152" t="s">
-        <v>223</v>
+        <v>236</v>
       </c>
       <c r="C94" s="101"/>
       <c r="D94" s="101">
-        <v>49269</v>
+        <v>45890</v>
       </c>
       <c r="E94" s="123">
         <f t="shared" si="6"/>
@@ -4157,13 +4180,9 @@
     </row>
     <row r="95" spans="1:8" ht="15" outlineLevel="1">
       <c r="A95" s="159"/>
-      <c r="B95" s="152" t="s">
-        <v>249</v>
-      </c>
+      <c r="B95" s="100"/>
       <c r="C95" s="101"/>
-      <c r="D95" s="101">
-        <v>49505</v>
-      </c>
+      <c r="D95" s="101"/>
       <c r="E95" s="123">
         <f t="shared" si="6"/>
         <v>0</v>
@@ -4172,13 +4191,9 @@
     </row>
     <row r="96" spans="1:8" ht="15" outlineLevel="1">
       <c r="A96" s="159"/>
-      <c r="B96" s="152" t="s">
-        <v>250</v>
-      </c>
+      <c r="B96" s="100"/>
       <c r="C96" s="101"/>
-      <c r="D96" s="101">
-        <v>50134</v>
-      </c>
+      <c r="D96" s="101"/>
       <c r="E96" s="123">
         <f t="shared" si="6"/>
         <v>0</v>
@@ -4188,11 +4203,11 @@
     <row r="97" spans="1:8" ht="15" outlineLevel="1">
       <c r="A97" s="159"/>
       <c r="B97" s="152" t="s">
-        <v>251</v>
+        <v>223</v>
       </c>
       <c r="C97" s="101"/>
       <c r="D97" s="101">
-        <v>50516</v>
+        <v>49269</v>
       </c>
       <c r="E97" s="123">
         <f t="shared" si="6"/>
@@ -4200,132 +4215,136 @@
       </c>
       <c r="F97" s="105"/>
     </row>
-    <row r="98" spans="1:8" ht="15.75" outlineLevel="1" thickBot="1">
+    <row r="98" spans="1:8" ht="15" outlineLevel="1">
       <c r="A98" s="159"/>
-      <c r="B98" s="98" t="s">
+      <c r="B98" s="152" t="s">
+        <v>249</v>
+      </c>
+      <c r="C98" s="101"/>
+      <c r="D98" s="101">
+        <v>49505</v>
+      </c>
+      <c r="E98" s="123">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="F98" s="105"/>
+    </row>
+    <row r="99" spans="1:8" ht="15" outlineLevel="1">
+      <c r="A99" s="159"/>
+      <c r="B99" s="152" t="s">
+        <v>250</v>
+      </c>
+      <c r="C99" s="101"/>
+      <c r="D99" s="101">
+        <v>50134</v>
+      </c>
+      <c r="E99" s="123">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="F99" s="105"/>
+    </row>
+    <row r="100" spans="1:8" ht="15" outlineLevel="1">
+      <c r="A100" s="159"/>
+      <c r="B100" s="152" t="s">
+        <v>251</v>
+      </c>
+      <c r="C100" s="101"/>
+      <c r="D100" s="101">
+        <v>50516</v>
+      </c>
+      <c r="E100" s="123">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="F100" s="105"/>
+    </row>
+    <row r="101" spans="1:8" ht="15.75" outlineLevel="1" thickBot="1">
+      <c r="A101" s="159"/>
+      <c r="B101" s="98" t="s">
         <v>179</v>
       </c>
-      <c r="C98" s="99"/>
-      <c r="D98" s="99">
+      <c r="C101" s="99"/>
+      <c r="D101" s="99">
         <v>50574</v>
       </c>
-      <c r="E98" s="125">
+      <c r="E101" s="125">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="F98" s="104"/>
-    </row>
-    <row r="99" spans="1:8" ht="17.25" thickTop="1" thickBot="1">
-      <c r="A99" s="116" t="s">
+      <c r="F101" s="104"/>
+    </row>
+    <row r="102" spans="1:8" ht="17.25" thickTop="1" thickBot="1">
+      <c r="A102" s="116" t="s">
         <v>248</v>
       </c>
-      <c r="B99" s="102" t="s">
+      <c r="B102" s="102" t="s">
         <v>173</v>
       </c>
-      <c r="C99" s="103">
-        <f>C98-C85</f>
-        <v>0</v>
-      </c>
-      <c r="D99" s="103">
-        <f>D98-D85</f>
+      <c r="C102" s="103">
+        <f>C101-C88</f>
+        <v>0</v>
+      </c>
+      <c r="D102" s="103">
+        <f>D101-D88</f>
         <v>15779</v>
       </c>
-      <c r="E99" s="126">
-        <f>E98-E85</f>
-        <v>0</v>
-      </c>
-      <c r="F99" s="107"/>
-      <c r="G99" s="112">
-        <f>E99</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="100" spans="1:8" ht="13.5" thickBot="1"/>
-    <row r="101" spans="1:8" ht="15" customHeight="1" outlineLevel="1">
-      <c r="A101" s="160" t="s">
+      <c r="E102" s="126">
+        <f>E101-E88</f>
+        <v>0</v>
+      </c>
+      <c r="F102" s="107"/>
+      <c r="G102" s="112">
+        <f>E102</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8" ht="13.5" thickBot="1"/>
+    <row r="104" spans="1:8" ht="15" customHeight="1" outlineLevel="1">
+      <c r="A104" s="160" t="s">
         <v>252</v>
       </c>
-      <c r="B101" s="109" t="s">
+      <c r="B104" s="109" t="s">
         <v>175</v>
       </c>
-      <c r="C101" s="110" t="s">
+      <c r="C104" s="110" t="s">
         <v>42</v>
       </c>
-      <c r="D101" s="110" t="s">
+      <c r="D104" s="110" t="s">
         <v>41</v>
       </c>
-      <c r="E101" s="110" t="s">
+      <c r="E104" s="110" t="s">
         <v>43</v>
       </c>
-      <c r="F101" s="111" t="s">
+      <c r="F104" s="111" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="102" spans="1:8" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="A102" s="159"/>
-      <c r="B102" s="98" t="s">
+    <row r="105" spans="1:8" ht="15.75" outlineLevel="1" thickBot="1">
+      <c r="A105" s="159"/>
+      <c r="B105" s="98" t="s">
         <v>177</v>
       </c>
-      <c r="C102" s="99"/>
-      <c r="D102" s="99">
+      <c r="C105" s="99"/>
+      <c r="D105" s="99">
         <v>50574</v>
       </c>
-      <c r="E102" s="123">
-        <f t="shared" ref="E102:E111" si="7">IF(AND(C102&gt;0,D102&gt;0), D102-C102, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="F102" s="104"/>
-      <c r="H102">
+      <c r="E105" s="123">
+        <f t="shared" ref="E105:E114" si="7">IF(AND(C105&gt;0,D105&gt;0), D105-C105, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="F105" s="104"/>
+      <c r="H105">
         <v>105030</v>
       </c>
     </row>
-    <row r="103" spans="1:8" ht="15.75" outlineLevel="1" thickTop="1">
-      <c r="A103" s="159"/>
-      <c r="B103" s="100"/>
-      <c r="C103" s="101"/>
-      <c r="D103" s="101"/>
-      <c r="E103" s="124">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="F103" s="105"/>
-    </row>
-    <row r="104" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A104" s="159"/>
-      <c r="B104" s="152" t="s">
-        <v>254</v>
-      </c>
-      <c r="C104" s="101"/>
-      <c r="D104" s="101">
-        <v>52785</v>
-      </c>
-      <c r="E104" s="123">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="F104" s="105"/>
-    </row>
-    <row r="105" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A105" s="159"/>
-      <c r="B105" s="100"/>
-      <c r="C105" s="101"/>
-      <c r="D105" s="101"/>
-      <c r="E105" s="123">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="F105" s="105"/>
-    </row>
-    <row r="106" spans="1:8" ht="15" outlineLevel="1">
+    <row r="106" spans="1:8" ht="15.75" outlineLevel="1" thickTop="1">
       <c r="A106" s="159"/>
-      <c r="B106" s="152" t="s">
-        <v>255</v>
-      </c>
+      <c r="B106" s="100"/>
       <c r="C106" s="101"/>
-      <c r="D106" s="101">
-        <v>53409</v>
-      </c>
-      <c r="E106" s="123">
+      <c r="D106" s="101"/>
+      <c r="E106" s="124">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -4333,9 +4352,13 @@
     </row>
     <row r="107" spans="1:8" ht="15" outlineLevel="1">
       <c r="A107" s="159"/>
-      <c r="B107" s="100"/>
+      <c r="B107" s="152" t="s">
+        <v>254</v>
+      </c>
       <c r="C107" s="101"/>
-      <c r="D107" s="101"/>
+      <c r="D107" s="101">
+        <v>52785</v>
+      </c>
       <c r="E107" s="123">
         <f t="shared" si="7"/>
         <v>0</v>
@@ -4344,13 +4367,9 @@
     </row>
     <row r="108" spans="1:8" ht="15" outlineLevel="1">
       <c r="A108" s="159"/>
-      <c r="B108" s="152" t="s">
-        <v>223</v>
-      </c>
+      <c r="B108" s="100"/>
       <c r="C108" s="101"/>
-      <c r="D108" s="101">
-        <v>55728</v>
-      </c>
+      <c r="D108" s="101"/>
       <c r="E108" s="123">
         <f t="shared" si="7"/>
         <v>0</v>
@@ -4360,11 +4379,11 @@
     <row r="109" spans="1:8" ht="15" outlineLevel="1">
       <c r="A109" s="159"/>
       <c r="B109" s="152" t="s">
-        <v>249</v>
+        <v>255</v>
       </c>
       <c r="C109" s="101"/>
       <c r="D109" s="101">
-        <v>55956</v>
+        <v>53409</v>
       </c>
       <c r="E109" s="123">
         <f t="shared" si="7"/>
@@ -4374,149 +4393,149 @@
     </row>
     <row r="110" spans="1:8" ht="15" outlineLevel="1">
       <c r="A110" s="159"/>
-      <c r="B110" s="152" t="s">
-        <v>256</v>
-      </c>
+      <c r="B110" s="100"/>
       <c r="C110" s="101"/>
-      <c r="D110" s="101">
-        <v>56314</v>
-      </c>
+      <c r="D110" s="101"/>
       <c r="E110" s="123">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="F110" s="105"/>
     </row>
-    <row r="111" spans="1:8" ht="15.75" outlineLevel="1" thickBot="1">
+    <row r="111" spans="1:8" ht="15" outlineLevel="1">
       <c r="A111" s="159"/>
-      <c r="B111" s="98" t="s">
+      <c r="B111" s="152" t="s">
+        <v>223</v>
+      </c>
+      <c r="C111" s="101"/>
+      <c r="D111" s="101">
+        <v>55728</v>
+      </c>
+      <c r="E111" s="123">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="F111" s="105"/>
+    </row>
+    <row r="112" spans="1:8" ht="15" outlineLevel="1">
+      <c r="A112" s="159"/>
+      <c r="B112" s="152" t="s">
+        <v>249</v>
+      </c>
+      <c r="C112" s="101"/>
+      <c r="D112" s="101">
+        <v>55956</v>
+      </c>
+      <c r="E112" s="123">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="F112" s="105"/>
+    </row>
+    <row r="113" spans="1:9" ht="15" outlineLevel="1">
+      <c r="A113" s="159"/>
+      <c r="B113" s="152" t="s">
+        <v>256</v>
+      </c>
+      <c r="C113" s="101"/>
+      <c r="D113" s="101">
+        <v>56314</v>
+      </c>
+      <c r="E113" s="123">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="F113" s="105"/>
+    </row>
+    <row r="114" spans="1:9" ht="15.75" outlineLevel="1" thickBot="1">
+      <c r="A114" s="159"/>
+      <c r="B114" s="98" t="s">
         <v>179</v>
       </c>
-      <c r="C111" s="99"/>
-      <c r="D111" s="99">
+      <c r="C114" s="99"/>
+      <c r="D114" s="99">
         <v>56373</v>
       </c>
-      <c r="E111" s="125">
+      <c r="E114" s="125">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="F111" s="104"/>
-    </row>
-    <row r="112" spans="1:8" ht="17.25" thickTop="1" thickBot="1">
-      <c r="A112" s="117" t="s">
+      <c r="F114" s="104"/>
+    </row>
+    <row r="115" spans="1:9" ht="17.25" thickTop="1" thickBot="1">
+      <c r="A115" s="117" t="s">
         <v>253</v>
       </c>
-      <c r="B112" s="102" t="s">
+      <c r="B115" s="102" t="s">
         <v>173</v>
       </c>
-      <c r="C112" s="103">
-        <f>C111-C102</f>
-        <v>0</v>
-      </c>
-      <c r="D112" s="103">
-        <f>D111-D102</f>
+      <c r="C115" s="103">
+        <f>C114-C105</f>
+        <v>0</v>
+      </c>
+      <c r="D115" s="103">
+        <f>D114-D105</f>
         <v>5799</v>
       </c>
-      <c r="E112" s="126">
-        <f>E111-E102</f>
-        <v>0</v>
-      </c>
-      <c r="F112" s="108"/>
-      <c r="G112" s="112">
-        <f>E112</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="113" spans="1:9" ht="13.5" thickBot="1"/>
-    <row r="114" spans="1:9" ht="15" customHeight="1" outlineLevel="1">
-      <c r="A114" s="158" t="s">
+      <c r="E115" s="126">
+        <f>E114-E105</f>
+        <v>0</v>
+      </c>
+      <c r="F115" s="108"/>
+      <c r="G115" s="112">
+        <f>E115</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="1:9" ht="13.5" thickBot="1"/>
+    <row r="117" spans="1:9" ht="15" customHeight="1" outlineLevel="1">
+      <c r="A117" s="158" t="s">
         <v>257</v>
       </c>
-      <c r="B114" s="113" t="s">
+      <c r="B117" s="113" t="s">
         <v>175</v>
       </c>
-      <c r="C114" s="114" t="s">
+      <c r="C117" s="114" t="s">
         <v>42</v>
       </c>
-      <c r="D114" s="114" t="s">
+      <c r="D117" s="114" t="s">
         <v>41</v>
       </c>
-      <c r="E114" s="114" t="s">
+      <c r="E117" s="114" t="s">
         <v>43</v>
       </c>
-      <c r="F114" s="115" t="s">
+      <c r="F117" s="115" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="115" spans="1:9" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="A115" s="159"/>
-      <c r="B115" s="98" t="s">
+    <row r="118" spans="1:9" ht="15.75" outlineLevel="1" thickBot="1">
+      <c r="A118" s="159"/>
+      <c r="B118" s="98" t="s">
         <v>177</v>
       </c>
-      <c r="C115" s="99"/>
-      <c r="D115" s="99">
+      <c r="C118" s="99"/>
+      <c r="D118" s="99">
         <v>56373</v>
       </c>
-      <c r="E115" s="123">
-        <f t="shared" ref="E115:E123" si="8">IF(AND(C115&gt;0,D115&gt;0), D115-C115, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="F115" s="104"/>
-      <c r="H115">
+      <c r="E118" s="123">
+        <f t="shared" ref="E118:E126" si="8">IF(AND(C118&gt;0,D118&gt;0), D118-C118, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="F118" s="104"/>
+      <c r="H118">
         <v>125564</v>
       </c>
-      <c r="I115" s="112">
-        <f>H115-D115</f>
+      <c r="I118" s="112">
+        <f>H118-D118</f>
         <v>69191</v>
       </c>
     </row>
-    <row r="116" spans="1:9" ht="15.75" outlineLevel="1" thickTop="1">
-      <c r="A116" s="159"/>
-      <c r="B116" s="100"/>
-      <c r="C116" s="101"/>
-      <c r="D116" s="101"/>
-      <c r="E116" s="124">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="F116" s="105"/>
-    </row>
-    <row r="117" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A117" s="159"/>
-      <c r="B117" s="152" t="s">
-        <v>221</v>
-      </c>
-      <c r="C117" s="101"/>
-      <c r="D117" s="101">
-        <v>58041</v>
-      </c>
-      <c r="E117" s="123">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="F117" s="105"/>
-    </row>
-    <row r="118" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A118" s="159"/>
-      <c r="B118" s="100"/>
-      <c r="C118" s="101"/>
-      <c r="D118" s="101"/>
-      <c r="E118" s="123">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="F118" s="105"/>
-    </row>
-    <row r="119" spans="1:9" ht="15" outlineLevel="1">
+    <row r="119" spans="1:9" ht="15.75" outlineLevel="1" thickTop="1">
       <c r="A119" s="159"/>
-      <c r="B119" s="152" t="s">
-        <v>222</v>
-      </c>
+      <c r="B119" s="100"/>
       <c r="C119" s="101"/>
-      <c r="D119" s="101">
-        <v>60301</v>
-      </c>
-      <c r="E119" s="123">
+      <c r="D119" s="101"/>
+      <c r="E119" s="124">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
@@ -4525,11 +4544,11 @@
     <row r="120" spans="1:9" ht="15" outlineLevel="1">
       <c r="A120" s="159"/>
       <c r="B120" s="152" t="s">
-        <v>249</v>
+        <v>221</v>
       </c>
       <c r="C120" s="101"/>
-      <c r="D120" s="153">
-        <v>60529</v>
+      <c r="D120" s="101">
+        <v>58041</v>
       </c>
       <c r="E120" s="123">
         <f t="shared" si="8"/>
@@ -4539,13 +4558,9 @@
     </row>
     <row r="121" spans="1:9" ht="15" outlineLevel="1">
       <c r="A121" s="159"/>
-      <c r="B121" s="152" t="s">
-        <v>259</v>
-      </c>
+      <c r="B121" s="100"/>
       <c r="C121" s="101"/>
-      <c r="D121" s="101">
-        <v>61068</v>
-      </c>
+      <c r="D121" s="101"/>
       <c r="E121" s="123">
         <f t="shared" si="8"/>
         <v>0</v>
@@ -4555,11 +4570,11 @@
     <row r="122" spans="1:9" ht="15" outlineLevel="1">
       <c r="A122" s="159"/>
       <c r="B122" s="152" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C122" s="101"/>
       <c r="D122" s="101">
-        <v>61391</v>
+        <v>60301</v>
       </c>
       <c r="E122" s="123">
         <f t="shared" si="8"/>
@@ -4567,128 +4582,140 @@
       </c>
       <c r="F122" s="105"/>
     </row>
-    <row r="123" spans="1:9" ht="15.75" outlineLevel="1" thickBot="1">
+    <row r="123" spans="1:9" ht="15" outlineLevel="1">
       <c r="A123" s="159"/>
-      <c r="B123" s="98" t="s">
+      <c r="B123" s="152" t="s">
+        <v>249</v>
+      </c>
+      <c r="C123" s="101"/>
+      <c r="D123" s="153">
+        <v>60529</v>
+      </c>
+      <c r="E123" s="123">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="F123" s="105"/>
+    </row>
+    <row r="124" spans="1:9" ht="15" outlineLevel="1">
+      <c r="A124" s="159"/>
+      <c r="B124" s="152" t="s">
+        <v>259</v>
+      </c>
+      <c r="C124" s="101"/>
+      <c r="D124" s="101">
+        <v>61068</v>
+      </c>
+      <c r="E124" s="123">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="F124" s="105"/>
+    </row>
+    <row r="125" spans="1:9" ht="15" outlineLevel="1">
+      <c r="A125" s="159"/>
+      <c r="B125" s="152" t="s">
+        <v>224</v>
+      </c>
+      <c r="C125" s="101"/>
+      <c r="D125" s="101">
+        <v>61391</v>
+      </c>
+      <c r="E125" s="123">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="F125" s="105"/>
+    </row>
+    <row r="126" spans="1:9" ht="15.75" outlineLevel="1" thickBot="1">
+      <c r="A126" s="159"/>
+      <c r="B126" s="98" t="s">
         <v>179</v>
       </c>
-      <c r="C123" s="99"/>
-      <c r="D123" s="99">
+      <c r="C126" s="99"/>
+      <c r="D126" s="99">
         <v>61438</v>
       </c>
-      <c r="E123" s="125">
+      <c r="E126" s="125">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="F123" s="104"/>
-    </row>
-    <row r="124" spans="1:9" ht="17.25" thickTop="1" thickBot="1">
-      <c r="A124" s="116" t="s">
+      <c r="F126" s="104"/>
+    </row>
+    <row r="127" spans="1:9" ht="17.25" thickTop="1" thickBot="1">
+      <c r="A127" s="116" t="s">
         <v>258</v>
       </c>
-      <c r="B124" s="102" t="s">
+      <c r="B127" s="102" t="s">
         <v>173</v>
       </c>
-      <c r="C124" s="103">
-        <f>C123-C115</f>
-        <v>0</v>
-      </c>
-      <c r="D124" s="103">
-        <f>D123-D115</f>
+      <c r="C127" s="103">
+        <f>C126-C118</f>
+        <v>0</v>
+      </c>
+      <c r="D127" s="103">
+        <f>D126-D118</f>
         <v>5065</v>
       </c>
-      <c r="E124" s="103">
-        <f>E123-E115</f>
-        <v>0</v>
-      </c>
-      <c r="F124" s="107"/>
-      <c r="G124" s="112">
-        <f>E124</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="125" spans="1:9" ht="13.5" thickBot="1"/>
-    <row r="126" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A126" s="160" t="s">
+      <c r="E127" s="103">
+        <f>E126-E118</f>
+        <v>0</v>
+      </c>
+      <c r="F127" s="107"/>
+      <c r="G127" s="112">
+        <f>E127</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128" spans="1:9" ht="13.5" thickBot="1"/>
+    <row r="129" spans="1:9" ht="15" outlineLevel="1">
+      <c r="A129" s="160" t="s">
         <v>260</v>
       </c>
-      <c r="B126" s="109" t="s">
+      <c r="B129" s="109" t="s">
         <v>175</v>
       </c>
-      <c r="C126" s="110" t="s">
+      <c r="C129" s="110" t="s">
         <v>42</v>
       </c>
-      <c r="D126" s="110" t="s">
+      <c r="D129" s="110" t="s">
         <v>41</v>
       </c>
-      <c r="E126" s="110" t="s">
+      <c r="E129" s="110" t="s">
         <v>43</v>
       </c>
-      <c r="F126" s="111" t="s">
+      <c r="F129" s="111" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="127" spans="1:9" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="A127" s="159"/>
-      <c r="B127" s="98" t="s">
+    <row r="130" spans="1:9" ht="15.75" outlineLevel="1" thickBot="1">
+      <c r="A130" s="159"/>
+      <c r="B130" s="98" t="s">
         <v>177</v>
       </c>
-      <c r="C127" s="99"/>
-      <c r="D127" s="99">
+      <c r="C130" s="99"/>
+      <c r="D130" s="99">
         <v>61438</v>
       </c>
-      <c r="E127" s="123">
-        <f t="shared" ref="E127:E140" si="9">IF(AND(C127&gt;0,D127&gt;0), D127-C127, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="F127" s="104"/>
-      <c r="H127">
+      <c r="E130" s="123">
+        <f t="shared" ref="E130:E143" si="9">IF(AND(C130&gt;0,D130&gt;0), D130-C130, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="F130" s="104"/>
+      <c r="H130">
         <v>135506</v>
       </c>
-      <c r="I127" s="112">
-        <f>H127-D127</f>
+      <c r="I130" s="112">
+        <f>H130-D130</f>
         <v>74068</v>
       </c>
     </row>
-    <row r="128" spans="1:9" ht="15.75" outlineLevel="1" thickTop="1">
-      <c r="A128" s="159"/>
-      <c r="B128" s="100"/>
-      <c r="C128" s="101"/>
-      <c r="D128" s="101"/>
-      <c r="E128" s="124">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="F128" s="105"/>
-    </row>
-    <row r="129" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A129" s="159"/>
-      <c r="B129" s="100"/>
-      <c r="C129" s="101"/>
-      <c r="D129" s="101"/>
-      <c r="E129" s="123">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="F129" s="105"/>
-    </row>
-    <row r="130" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A130" s="159"/>
-      <c r="B130" s="100"/>
-      <c r="C130" s="101"/>
-      <c r="D130" s="101"/>
-      <c r="E130" s="123">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="F130" s="105"/>
-    </row>
-    <row r="131" spans="1:9" ht="15" outlineLevel="1">
+    <row r="131" spans="1:9" ht="15.75" outlineLevel="1" thickTop="1">
       <c r="A131" s="159"/>
       <c r="B131" s="100"/>
       <c r="C131" s="101"/>
       <c r="D131" s="101"/>
-      <c r="E131" s="123">
+      <c r="E131" s="124">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
@@ -4740,25 +4767,14 @@
     </row>
     <row r="136" spans="1:9" ht="15" outlineLevel="1">
       <c r="A136" s="159"/>
-      <c r="B136" s="152" t="s">
-        <v>262</v>
-      </c>
+      <c r="B136" s="100"/>
       <c r="C136" s="101"/>
-      <c r="D136" s="101">
-        <v>66926</v>
-      </c>
+      <c r="D136" s="101"/>
       <c r="E136" s="123">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="F136" s="105"/>
-      <c r="H136">
-        <v>160118</v>
-      </c>
-      <c r="I136" s="112">
-        <f>H136-D136</f>
-        <v>93192</v>
-      </c>
     </row>
     <row r="137" spans="1:9" ht="15" outlineLevel="1">
       <c r="A137" s="159"/>
@@ -4784,131 +4800,142 @@
     </row>
     <row r="139" spans="1:9" ht="15" outlineLevel="1">
       <c r="A139" s="159"/>
-      <c r="B139" s="100"/>
+      <c r="B139" s="152" t="s">
+        <v>262</v>
+      </c>
       <c r="C139" s="101"/>
-      <c r="D139" s="101"/>
+      <c r="D139" s="101">
+        <v>66926</v>
+      </c>
       <c r="E139" s="123">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="F139" s="105"/>
-    </row>
-    <row r="140" spans="1:9" ht="15.75" outlineLevel="1" thickBot="1">
+      <c r="H139">
+        <v>160118</v>
+      </c>
+      <c r="I139" s="112">
+        <f>H139-D139</f>
+        <v>93192</v>
+      </c>
+    </row>
+    <row r="140" spans="1:9" ht="15" outlineLevel="1">
       <c r="A140" s="159"/>
-      <c r="B140" s="98" t="s">
+      <c r="B140" s="100"/>
+      <c r="C140" s="101"/>
+      <c r="D140" s="101"/>
+      <c r="E140" s="123">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="F140" s="105"/>
+    </row>
+    <row r="141" spans="1:9" ht="15" outlineLevel="1">
+      <c r="A141" s="159"/>
+      <c r="B141" s="100"/>
+      <c r="C141" s="101"/>
+      <c r="D141" s="101"/>
+      <c r="E141" s="123">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="F141" s="105"/>
+    </row>
+    <row r="142" spans="1:9" ht="15" outlineLevel="1">
+      <c r="A142" s="159"/>
+      <c r="B142" s="100"/>
+      <c r="C142" s="101"/>
+      <c r="D142" s="101"/>
+      <c r="E142" s="123">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="F142" s="105"/>
+    </row>
+    <row r="143" spans="1:9" ht="15.75" outlineLevel="1" thickBot="1">
+      <c r="A143" s="159"/>
+      <c r="B143" s="98" t="s">
         <v>179</v>
       </c>
-      <c r="C140" s="99"/>
-      <c r="D140" s="99"/>
-      <c r="E140" s="125">
+      <c r="C143" s="99"/>
+      <c r="D143" s="99"/>
+      <c r="E143" s="125">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="F140" s="104"/>
-    </row>
-    <row r="141" spans="1:9" ht="17.25" thickTop="1" thickBot="1">
-      <c r="A141" s="117" t="s">
+      <c r="F143" s="104"/>
+    </row>
+    <row r="144" spans="1:9" ht="17.25" thickTop="1" thickBot="1">
+      <c r="A144" s="117" t="s">
         <v>261</v>
       </c>
-      <c r="B141" s="102" t="s">
+      <c r="B144" s="102" t="s">
         <v>173</v>
       </c>
-      <c r="C141" s="103">
-        <f>C140-C127</f>
-        <v>0</v>
-      </c>
-      <c r="D141" s="103">
-        <f>D140-D127</f>
+      <c r="C144" s="103">
+        <f>C143-C130</f>
+        <v>0</v>
+      </c>
+      <c r="D144" s="103">
+        <f>D143-D130</f>
         <v>-61438</v>
       </c>
-      <c r="E141" s="103">
-        <f>E140-E127</f>
-        <v>0</v>
-      </c>
-      <c r="F141" s="108"/>
-      <c r="G141" s="112">
-        <f>E141</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="143" spans="1:9" ht="15" hidden="1" outlineLevel="2">
-      <c r="A143" s="158" t="s">
+      <c r="E144" s="103">
+        <f>E143-E130</f>
+        <v>0</v>
+      </c>
+      <c r="F144" s="108"/>
+      <c r="G144" s="112">
+        <f>E144</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="146" spans="1:6" ht="15" hidden="1" outlineLevel="2">
+      <c r="A146" s="158" t="s">
         <v>169</v>
       </c>
-      <c r="B143" s="113" t="s">
+      <c r="B146" s="113" t="s">
         <v>175</v>
       </c>
-      <c r="C143" s="114" t="s">
+      <c r="C146" s="114" t="s">
         <v>42</v>
       </c>
-      <c r="D143" s="114" t="s">
+      <c r="D146" s="114" t="s">
         <v>41</v>
       </c>
-      <c r="E143" s="114" t="s">
+      <c r="E146" s="114" t="s">
         <v>43</v>
       </c>
-      <c r="F143" s="115" t="s">
+      <c r="F146" s="115" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="144" spans="1:9" ht="15.75" hidden="1" outlineLevel="2" thickBot="1">
-      <c r="A144" s="159"/>
-      <c r="B144" s="98" t="s">
+    <row r="147" spans="1:6" ht="15.75" hidden="1" outlineLevel="2" thickBot="1">
+      <c r="A147" s="159"/>
+      <c r="B147" s="98" t="s">
         <v>177</v>
       </c>
-      <c r="C144" s="99"/>
-      <c r="D144" s="99"/>
-      <c r="E144" s="123">
-        <f t="shared" ref="E144:E157" si="10">IF(AND(C144&gt;0,D144&gt;0), D144-C144, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="F144" s="104"/>
-    </row>
-    <row r="145" spans="1:7" ht="15.75" hidden="1" outlineLevel="2" thickTop="1">
-      <c r="A145" s="159"/>
-      <c r="B145" s="100"/>
-      <c r="C145" s="101"/>
-      <c r="D145" s="101"/>
-      <c r="E145" s="124">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="F145" s="105"/>
-    </row>
-    <row r="146" spans="1:7" ht="15" hidden="1" outlineLevel="2">
-      <c r="A146" s="159"/>
-      <c r="B146" s="100"/>
-      <c r="C146" s="101"/>
-      <c r="D146" s="101"/>
-      <c r="E146" s="123">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="F146" s="105"/>
-    </row>
-    <row r="147" spans="1:7" ht="15" hidden="1" outlineLevel="2">
-      <c r="A147" s="159"/>
-      <c r="B147" s="100"/>
-      <c r="C147" s="101"/>
-      <c r="D147" s="101"/>
+      <c r="C147" s="99"/>
+      <c r="D147" s="99"/>
       <c r="E147" s="123">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="F147" s="105"/>
-    </row>
-    <row r="148" spans="1:7" ht="15" hidden="1" outlineLevel="2">
+        <f t="shared" ref="E147:E160" si="10">IF(AND(C147&gt;0,D147&gt;0), D147-C147, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="F147" s="104"/>
+    </row>
+    <row r="148" spans="1:6" ht="15.75" hidden="1" outlineLevel="2" thickTop="1">
       <c r="A148" s="159"/>
       <c r="B148" s="100"/>
       <c r="C148" s="101"/>
       <c r="D148" s="101"/>
-      <c r="E148" s="123">
+      <c r="E148" s="124">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="F148" s="105"/>
     </row>
-    <row r="149" spans="1:7" ht="15" hidden="1" outlineLevel="2">
+    <row r="149" spans="1:6" ht="15" hidden="1" outlineLevel="2">
       <c r="A149" s="159"/>
       <c r="B149" s="100"/>
       <c r="C149" s="101"/>
@@ -4919,7 +4946,7 @@
       </c>
       <c r="F149" s="105"/>
     </row>
-    <row r="150" spans="1:7" ht="15" hidden="1" outlineLevel="2">
+    <row r="150" spans="1:6" ht="15" hidden="1" outlineLevel="2">
       <c r="A150" s="159"/>
       <c r="B150" s="100"/>
       <c r="C150" s="101"/>
@@ -4930,7 +4957,7 @@
       </c>
       <c r="F150" s="105"/>
     </row>
-    <row r="151" spans="1:7" ht="15" hidden="1" outlineLevel="2">
+    <row r="151" spans="1:6" ht="15" hidden="1" outlineLevel="2">
       <c r="A151" s="159"/>
       <c r="B151" s="100"/>
       <c r="C151" s="101"/>
@@ -4941,7 +4968,7 @@
       </c>
       <c r="F151" s="105"/>
     </row>
-    <row r="152" spans="1:7" ht="15" hidden="1" outlineLevel="2">
+    <row r="152" spans="1:6" ht="15" hidden="1" outlineLevel="2">
       <c r="A152" s="159"/>
       <c r="B152" s="100"/>
       <c r="C152" s="101"/>
@@ -4952,7 +4979,7 @@
       </c>
       <c r="F152" s="105"/>
     </row>
-    <row r="153" spans="1:7" ht="15" hidden="1" outlineLevel="2">
+    <row r="153" spans="1:6" ht="15" hidden="1" outlineLevel="2">
       <c r="A153" s="159"/>
       <c r="B153" s="100"/>
       <c r="C153" s="101"/>
@@ -4963,7 +4990,7 @@
       </c>
       <c r="F153" s="105"/>
     </row>
-    <row r="154" spans="1:7" ht="15" hidden="1" outlineLevel="2">
+    <row r="154" spans="1:6" ht="15" hidden="1" outlineLevel="2">
       <c r="A154" s="159"/>
       <c r="B154" s="100"/>
       <c r="C154" s="101"/>
@@ -4974,7 +5001,7 @@
       </c>
       <c r="F154" s="105"/>
     </row>
-    <row r="155" spans="1:7" ht="15" hidden="1" outlineLevel="2">
+    <row r="155" spans="1:6" ht="15" hidden="1" outlineLevel="2">
       <c r="A155" s="159"/>
       <c r="B155" s="100"/>
       <c r="C155" s="101"/>
@@ -4985,7 +5012,7 @@
       </c>
       <c r="F155" s="105"/>
     </row>
-    <row r="156" spans="1:7" ht="15" hidden="1" outlineLevel="2">
+    <row r="156" spans="1:6" ht="15" hidden="1" outlineLevel="2">
       <c r="A156" s="159"/>
       <c r="B156" s="100"/>
       <c r="C156" s="101"/>
@@ -4996,48 +5023,86 @@
       </c>
       <c r="F156" s="105"/>
     </row>
-    <row r="157" spans="1:7" ht="15.75" hidden="1" outlineLevel="2" thickBot="1">
+    <row r="157" spans="1:6" ht="15" hidden="1" outlineLevel="2">
       <c r="A157" s="159"/>
-      <c r="B157" s="98" t="s">
+      <c r="B157" s="100"/>
+      <c r="C157" s="101"/>
+      <c r="D157" s="101"/>
+      <c r="E157" s="123">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="F157" s="105"/>
+    </row>
+    <row r="158" spans="1:6" ht="15" hidden="1" outlineLevel="2">
+      <c r="A158" s="159"/>
+      <c r="B158" s="100"/>
+      <c r="C158" s="101"/>
+      <c r="D158" s="101"/>
+      <c r="E158" s="123">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="F158" s="105"/>
+    </row>
+    <row r="159" spans="1:6" ht="15" hidden="1" outlineLevel="2">
+      <c r="A159" s="159"/>
+      <c r="B159" s="100"/>
+      <c r="C159" s="101"/>
+      <c r="D159" s="101"/>
+      <c r="E159" s="123">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="F159" s="105"/>
+    </row>
+    <row r="160" spans="1:6" ht="15.75" hidden="1" outlineLevel="2" thickBot="1">
+      <c r="A160" s="159"/>
+      <c r="B160" s="98" t="s">
         <v>179</v>
       </c>
-      <c r="C157" s="99"/>
-      <c r="D157" s="99"/>
-      <c r="E157" s="125">
+      <c r="C160" s="99"/>
+      <c r="D160" s="99"/>
+      <c r="E160" s="125">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="F157" s="104"/>
-    </row>
-    <row r="158" spans="1:7" ht="16.5" collapsed="1" thickBot="1">
-      <c r="A158" s="116">
+      <c r="F160" s="104"/>
+    </row>
+    <row r="161" spans="1:7" ht="16.5" collapsed="1" thickBot="1">
+      <c r="A161" s="116">
         <v>8</v>
       </c>
-      <c r="B158" s="102" t="s">
+      <c r="B161" s="102" t="s">
         <v>173</v>
       </c>
-      <c r="C158" s="103">
-        <f>C157-C144</f>
-        <v>0</v>
-      </c>
-      <c r="D158" s="103">
-        <f>D157-D144</f>
-        <v>0</v>
-      </c>
-      <c r="E158" s="103">
-        <f>E157-E144</f>
-        <v>0</v>
-      </c>
-      <c r="F158" s="107"/>
-      <c r="G158" s="112">
-        <f>E158</f>
+      <c r="C161" s="103">
+        <f>C160-C147</f>
+        <v>0</v>
+      </c>
+      <c r="D161" s="103">
+        <f>D160-D147</f>
+        <v>0</v>
+      </c>
+      <c r="E161" s="103">
+        <f>E160-E147</f>
+        <v>0</v>
+      </c>
+      <c r="F161" s="107"/>
+      <c r="G161" s="112">
+        <f>E161</f>
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="A43:A65"/>
-    <mergeCell ref="A68:A81"/>
+    <mergeCell ref="A146:A160"/>
+    <mergeCell ref="A117:A126"/>
+    <mergeCell ref="A87:A101"/>
+    <mergeCell ref="A129:A143"/>
+    <mergeCell ref="A104:A114"/>
+    <mergeCell ref="A43:A68"/>
+    <mergeCell ref="A71:A84"/>
     <mergeCell ref="C5:D5"/>
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="A1:B1"/>
@@ -5045,11 +5110,6 @@
     <mergeCell ref="A8:A18"/>
     <mergeCell ref="A21:A40"/>
     <mergeCell ref="C4:E4"/>
-    <mergeCell ref="A143:A157"/>
-    <mergeCell ref="A114:A123"/>
-    <mergeCell ref="A84:A98"/>
-    <mergeCell ref="A126:A140"/>
-    <mergeCell ref="A101:A111"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -5081,13 +5141,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="26.25" customHeight="1">
-      <c r="A1" s="186" t="s">
+      <c r="A1" s="168" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="186"/>
-      <c r="C1" s="186"/>
-      <c r="D1" s="186"/>
-      <c r="E1" s="186"/>
+      <c r="B1" s="168"/>
+      <c r="C1" s="168"/>
+      <c r="D1" s="168"/>
+      <c r="E1" s="168"/>
       <c r="F1" s="7"/>
       <c r="G1" s="5"/>
       <c r="H1" s="5"/>
@@ -5117,18 +5177,18 @@
         <v>8</v>
       </c>
       <c r="B3" s="36"/>
-      <c r="C3" s="187"/>
-      <c r="D3" s="188"/>
-      <c r="E3" s="188"/>
+      <c r="C3" s="169"/>
+      <c r="D3" s="170"/>
+      <c r="E3" s="170"/>
     </row>
     <row r="4" spans="1:8" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A4" s="46" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="87"/>
-      <c r="C4" s="168"/>
-      <c r="D4" s="169"/>
-      <c r="E4" s="169"/>
+      <c r="C4" s="171"/>
+      <c r="D4" s="172"/>
+      <c r="E4" s="172"/>
       <c r="F4" s="6"/>
     </row>
     <row r="5" spans="1:8" hidden="1" outlineLevel="2">
@@ -5280,9 +5340,9 @@
         <v>9</v>
       </c>
       <c r="B21" s="90"/>
-      <c r="C21" s="170"/>
-      <c r="D21" s="171"/>
-      <c r="E21" s="171"/>
+      <c r="C21" s="173"/>
+      <c r="D21" s="174"/>
+      <c r="E21" s="174"/>
     </row>
     <row r="22" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A22" s="47">
@@ -5433,9 +5493,9 @@
         <v>10</v>
       </c>
       <c r="B38" s="87"/>
-      <c r="C38" s="168"/>
-      <c r="D38" s="169"/>
-      <c r="E38" s="169"/>
+      <c r="C38" s="171"/>
+      <c r="D38" s="172"/>
+      <c r="E38" s="172"/>
     </row>
     <row r="39" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A39" s="47">
@@ -5586,9 +5646,9 @@
         <v>11</v>
       </c>
       <c r="B55" s="87"/>
-      <c r="C55" s="168"/>
-      <c r="D55" s="169"/>
-      <c r="E55" s="169"/>
+      <c r="C55" s="171"/>
+      <c r="D55" s="172"/>
+      <c r="E55" s="172"/>
     </row>
     <row r="56" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A56" s="47">
@@ -5739,9 +5799,9 @@
         <v>12</v>
       </c>
       <c r="B72" s="87"/>
-      <c r="C72" s="168"/>
-      <c r="D72" s="169"/>
-      <c r="E72" s="169"/>
+      <c r="C72" s="171"/>
+      <c r="D72" s="172"/>
+      <c r="E72" s="172"/>
     </row>
     <row r="73" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A73" s="47">
@@ -5892,9 +5952,9 @@
         <v>13</v>
       </c>
       <c r="B89" s="87"/>
-      <c r="C89" s="168"/>
-      <c r="D89" s="169"/>
-      <c r="E89" s="169"/>
+      <c r="C89" s="171"/>
+      <c r="D89" s="172"/>
+      <c r="E89" s="172"/>
     </row>
     <row r="90" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A90" s="47">
@@ -6045,9 +6105,9 @@
         <v>14</v>
       </c>
       <c r="B106" s="87"/>
-      <c r="C106" s="168"/>
-      <c r="D106" s="169"/>
-      <c r="E106" s="169"/>
+      <c r="C106" s="171"/>
+      <c r="D106" s="172"/>
+      <c r="E106" s="172"/>
     </row>
     <row r="107" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A107" s="47">
@@ -6198,9 +6258,9 @@
         <v>15</v>
       </c>
       <c r="B123" s="87"/>
-      <c r="C123" s="168"/>
-      <c r="D123" s="169"/>
-      <c r="E123" s="169"/>
+      <c r="C123" s="171"/>
+      <c r="D123" s="172"/>
+      <c r="E123" s="172"/>
     </row>
     <row r="124" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A124" s="47">
@@ -6351,9 +6411,9 @@
         <v>16</v>
       </c>
       <c r="B140" s="87"/>
-      <c r="C140" s="168"/>
-      <c r="D140" s="169"/>
-      <c r="E140" s="169"/>
+      <c r="C140" s="171"/>
+      <c r="D140" s="172"/>
+      <c r="E140" s="172"/>
     </row>
     <row r="141" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A141" s="47">
@@ -6504,9 +6564,9 @@
         <v>17</v>
       </c>
       <c r="B157" s="87"/>
-      <c r="C157" s="168"/>
-      <c r="D157" s="169"/>
-      <c r="E157" s="169"/>
+      <c r="C157" s="171"/>
+      <c r="D157" s="172"/>
+      <c r="E157" s="172"/>
     </row>
     <row r="158" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A158" s="47">
@@ -6657,9 +6717,9 @@
         <v>18</v>
       </c>
       <c r="B174" s="87"/>
-      <c r="C174" s="168"/>
-      <c r="D174" s="169"/>
-      <c r="E174" s="169"/>
+      <c r="C174" s="171"/>
+      <c r="D174" s="172"/>
+      <c r="E174" s="172"/>
     </row>
     <row r="175" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A175" s="47">
@@ -6810,9 +6870,9 @@
         <v>19</v>
       </c>
       <c r="B191" s="87"/>
-      <c r="C191" s="168"/>
-      <c r="D191" s="169"/>
-      <c r="E191" s="169"/>
+      <c r="C191" s="171"/>
+      <c r="D191" s="172"/>
+      <c r="E191" s="172"/>
     </row>
     <row r="192" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A192" s="47">
@@ -6963,9 +7023,9 @@
         <v>20</v>
       </c>
       <c r="B208" s="87"/>
-      <c r="C208" s="168"/>
-      <c r="D208" s="169"/>
-      <c r="E208" s="169"/>
+      <c r="C208" s="171"/>
+      <c r="D208" s="172"/>
+      <c r="E208" s="172"/>
     </row>
     <row r="209" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A209" s="47">
@@ -7116,9 +7176,9 @@
         <v>21</v>
       </c>
       <c r="B225" s="87"/>
-      <c r="C225" s="168"/>
-      <c r="D225" s="169"/>
-      <c r="E225" s="169"/>
+      <c r="C225" s="171"/>
+      <c r="D225" s="172"/>
+      <c r="E225" s="172"/>
     </row>
     <row r="226" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A226" s="47">
@@ -7269,9 +7329,9 @@
         <v>22</v>
       </c>
       <c r="B242" s="87"/>
-      <c r="C242" s="168"/>
-      <c r="D242" s="169"/>
-      <c r="E242" s="169"/>
+      <c r="C242" s="171"/>
+      <c r="D242" s="172"/>
+      <c r="E242" s="172"/>
     </row>
     <row r="243" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A243" s="47">
@@ -7422,9 +7482,9 @@
         <v>23</v>
       </c>
       <c r="B259" s="87"/>
-      <c r="C259" s="168"/>
-      <c r="D259" s="169"/>
-      <c r="E259" s="169"/>
+      <c r="C259" s="171"/>
+      <c r="D259" s="172"/>
+      <c r="E259" s="172"/>
     </row>
     <row r="260" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A260" s="47">
@@ -7575,18 +7635,18 @@
         <v>24</v>
       </c>
       <c r="B276" s="37"/>
-      <c r="C276" s="184"/>
-      <c r="D276" s="185"/>
-      <c r="E276" s="185"/>
+      <c r="C276" s="175"/>
+      <c r="D276" s="176"/>
+      <c r="E276" s="176"/>
     </row>
     <row r="277" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A277" s="51" t="s">
         <v>25</v>
       </c>
       <c r="B277" s="87"/>
-      <c r="C277" s="168"/>
-      <c r="D277" s="169"/>
-      <c r="E277" s="169"/>
+      <c r="C277" s="171"/>
+      <c r="D277" s="172"/>
+      <c r="E277" s="172"/>
     </row>
     <row r="278" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A278" s="52">
@@ -7737,9 +7797,9 @@
         <v>26</v>
       </c>
       <c r="B294" s="90"/>
-      <c r="C294" s="170"/>
-      <c r="D294" s="171"/>
-      <c r="E294" s="171"/>
+      <c r="C294" s="173"/>
+      <c r="D294" s="174"/>
+      <c r="E294" s="174"/>
     </row>
     <row r="295" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A295" s="52">
@@ -7890,9 +7950,9 @@
         <v>27</v>
       </c>
       <c r="B311" s="87"/>
-      <c r="C311" s="168"/>
-      <c r="D311" s="169"/>
-      <c r="E311" s="169"/>
+      <c r="C311" s="171"/>
+      <c r="D311" s="172"/>
+      <c r="E311" s="172"/>
     </row>
     <row r="312" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A312" s="52">
@@ -8043,9 +8103,9 @@
         <v>28</v>
       </c>
       <c r="B328" s="87"/>
-      <c r="C328" s="168"/>
-      <c r="D328" s="169"/>
-      <c r="E328" s="169"/>
+      <c r="C328" s="171"/>
+      <c r="D328" s="172"/>
+      <c r="E328" s="172"/>
     </row>
     <row r="329" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A329" s="52">
@@ -8196,9 +8256,9 @@
         <v>29</v>
       </c>
       <c r="B345" s="87"/>
-      <c r="C345" s="168"/>
-      <c r="D345" s="169"/>
-      <c r="E345" s="169"/>
+      <c r="C345" s="171"/>
+      <c r="D345" s="172"/>
+      <c r="E345" s="172"/>
     </row>
     <row r="346" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A346" s="52">
@@ -8349,9 +8409,9 @@
         <v>30</v>
       </c>
       <c r="B362" s="87"/>
-      <c r="C362" s="168"/>
-      <c r="D362" s="169"/>
-      <c r="E362" s="169"/>
+      <c r="C362" s="171"/>
+      <c r="D362" s="172"/>
+      <c r="E362" s="172"/>
     </row>
     <row r="363" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A363" s="52">
@@ -8502,9 +8562,9 @@
         <v>31</v>
       </c>
       <c r="B379" s="87"/>
-      <c r="C379" s="168"/>
-      <c r="D379" s="169"/>
-      <c r="E379" s="169"/>
+      <c r="C379" s="171"/>
+      <c r="D379" s="172"/>
+      <c r="E379" s="172"/>
     </row>
     <row r="380" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A380" s="52">
@@ -8655,9 +8715,9 @@
         <v>32</v>
       </c>
       <c r="B396" s="87"/>
-      <c r="C396" s="168"/>
-      <c r="D396" s="169"/>
-      <c r="E396" s="169"/>
+      <c r="C396" s="171"/>
+      <c r="D396" s="172"/>
+      <c r="E396" s="172"/>
     </row>
     <row r="397" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A397" s="52">
@@ -8808,9 +8868,9 @@
         <v>33</v>
       </c>
       <c r="B413" s="87"/>
-      <c r="C413" s="168"/>
-      <c r="D413" s="169"/>
-      <c r="E413" s="169"/>
+      <c r="C413" s="171"/>
+      <c r="D413" s="172"/>
+      <c r="E413" s="172"/>
     </row>
     <row r="414" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A414" s="52">
@@ -8961,9 +9021,9 @@
         <v>34</v>
       </c>
       <c r="B430" s="87"/>
-      <c r="C430" s="168"/>
-      <c r="D430" s="169"/>
-      <c r="E430" s="169"/>
+      <c r="C430" s="171"/>
+      <c r="D430" s="172"/>
+      <c r="E430" s="172"/>
     </row>
     <row r="431" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A431" s="52">
@@ -9114,9 +9174,9 @@
         <v>35</v>
       </c>
       <c r="B447" s="87"/>
-      <c r="C447" s="168"/>
-      <c r="D447" s="169"/>
-      <c r="E447" s="169"/>
+      <c r="C447" s="171"/>
+      <c r="D447" s="172"/>
+      <c r="E447" s="172"/>
     </row>
     <row r="448" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A448" s="52">
@@ -9267,9 +9327,9 @@
         <v>36</v>
       </c>
       <c r="B464" s="87"/>
-      <c r="C464" s="168"/>
-      <c r="D464" s="169"/>
-      <c r="E464" s="169"/>
+      <c r="C464" s="171"/>
+      <c r="D464" s="172"/>
+      <c r="E464" s="172"/>
     </row>
     <row r="465" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A465" s="52">
@@ -9420,9 +9480,9 @@
         <v>37</v>
       </c>
       <c r="B481" s="87"/>
-      <c r="C481" s="168"/>
-      <c r="D481" s="169"/>
-      <c r="E481" s="169"/>
+      <c r="C481" s="171"/>
+      <c r="D481" s="172"/>
+      <c r="E481" s="172"/>
     </row>
     <row r="482" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A482" s="52">
@@ -9573,9 +9633,9 @@
         <v>38</v>
       </c>
       <c r="B498" s="87"/>
-      <c r="C498" s="168"/>
-      <c r="D498" s="169"/>
-      <c r="E498" s="169"/>
+      <c r="C498" s="171"/>
+      <c r="D498" s="172"/>
+      <c r="E498" s="172"/>
     </row>
     <row r="499" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A499" s="52">
@@ -9726,9 +9786,9 @@
         <v>39</v>
       </c>
       <c r="B515" s="87"/>
-      <c r="C515" s="168"/>
-      <c r="D515" s="169"/>
-      <c r="E515" s="169"/>
+      <c r="C515" s="171"/>
+      <c r="D515" s="172"/>
+      <c r="E515" s="172"/>
     </row>
     <row r="516" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A516" s="52">
@@ -9879,9 +9939,9 @@
         <v>40</v>
       </c>
       <c r="B532" s="87"/>
-      <c r="C532" s="168"/>
-      <c r="D532" s="169"/>
-      <c r="E532" s="169"/>
+      <c r="C532" s="171"/>
+      <c r="D532" s="172"/>
+      <c r="E532" s="172"/>
     </row>
     <row r="533" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A533" s="55">
@@ -10032,18 +10092,18 @@
         <v>50</v>
       </c>
       <c r="B549" s="38"/>
-      <c r="C549" s="182"/>
-      <c r="D549" s="183"/>
-      <c r="E549" s="183"/>
+      <c r="C549" s="177"/>
+      <c r="D549" s="178"/>
+      <c r="E549" s="178"/>
     </row>
     <row r="550" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A550" s="58" t="s">
         <v>51</v>
       </c>
       <c r="B550" s="87"/>
-      <c r="C550" s="168"/>
-      <c r="D550" s="169"/>
-      <c r="E550" s="169"/>
+      <c r="C550" s="171"/>
+      <c r="D550" s="172"/>
+      <c r="E550" s="172"/>
     </row>
     <row r="551" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A551" s="59">
@@ -10194,9 +10254,9 @@
         <v>52</v>
       </c>
       <c r="B567" s="90"/>
-      <c r="C567" s="170"/>
-      <c r="D567" s="171"/>
-      <c r="E567" s="171"/>
+      <c r="C567" s="173"/>
+      <c r="D567" s="174"/>
+      <c r="E567" s="174"/>
     </row>
     <row r="568" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A568" s="59">
@@ -10347,9 +10407,9 @@
         <v>53</v>
       </c>
       <c r="B584" s="87"/>
-      <c r="C584" s="168"/>
-      <c r="D584" s="169"/>
-      <c r="E584" s="169"/>
+      <c r="C584" s="171"/>
+      <c r="D584" s="172"/>
+      <c r="E584" s="172"/>
     </row>
     <row r="585" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A585" s="59">
@@ -10500,9 +10560,9 @@
         <v>54</v>
       </c>
       <c r="B601" s="87"/>
-      <c r="C601" s="168"/>
-      <c r="D601" s="169"/>
-      <c r="E601" s="169"/>
+      <c r="C601" s="171"/>
+      <c r="D601" s="172"/>
+      <c r="E601" s="172"/>
     </row>
     <row r="602" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A602" s="59">
@@ -10653,9 +10713,9 @@
         <v>55</v>
       </c>
       <c r="B618" s="87"/>
-      <c r="C618" s="168"/>
-      <c r="D618" s="169"/>
-      <c r="E618" s="169"/>
+      <c r="C618" s="171"/>
+      <c r="D618" s="172"/>
+      <c r="E618" s="172"/>
     </row>
     <row r="619" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A619" s="59">
@@ -10806,9 +10866,9 @@
         <v>56</v>
       </c>
       <c r="B635" s="87"/>
-      <c r="C635" s="168"/>
-      <c r="D635" s="169"/>
-      <c r="E635" s="169"/>
+      <c r="C635" s="171"/>
+      <c r="D635" s="172"/>
+      <c r="E635" s="172"/>
     </row>
     <row r="636" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A636" s="59">
@@ -10959,9 +11019,9 @@
         <v>57</v>
       </c>
       <c r="B652" s="87"/>
-      <c r="C652" s="168"/>
-      <c r="D652" s="169"/>
-      <c r="E652" s="169"/>
+      <c r="C652" s="171"/>
+      <c r="D652" s="172"/>
+      <c r="E652" s="172"/>
     </row>
     <row r="653" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A653" s="59">
@@ -11112,9 +11172,9 @@
         <v>58</v>
       </c>
       <c r="B669" s="87"/>
-      <c r="C669" s="168"/>
-      <c r="D669" s="169"/>
-      <c r="E669" s="169"/>
+      <c r="C669" s="171"/>
+      <c r="D669" s="172"/>
+      <c r="E669" s="172"/>
     </row>
     <row r="670" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A670" s="59">
@@ -11265,9 +11325,9 @@
         <v>59</v>
       </c>
       <c r="B686" s="87"/>
-      <c r="C686" s="168"/>
-      <c r="D686" s="169"/>
-      <c r="E686" s="169"/>
+      <c r="C686" s="171"/>
+      <c r="D686" s="172"/>
+      <c r="E686" s="172"/>
     </row>
     <row r="687" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A687" s="59">
@@ -11418,9 +11478,9 @@
         <v>60</v>
       </c>
       <c r="B703" s="87"/>
-      <c r="C703" s="168"/>
-      <c r="D703" s="169"/>
-      <c r="E703" s="169"/>
+      <c r="C703" s="171"/>
+      <c r="D703" s="172"/>
+      <c r="E703" s="172"/>
     </row>
     <row r="704" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A704" s="59">
@@ -11571,9 +11631,9 @@
         <v>61</v>
       </c>
       <c r="B720" s="87"/>
-      <c r="C720" s="168"/>
-      <c r="D720" s="169"/>
-      <c r="E720" s="169"/>
+      <c r="C720" s="171"/>
+      <c r="D720" s="172"/>
+      <c r="E720" s="172"/>
     </row>
     <row r="721" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A721" s="59">
@@ -11724,9 +11784,9 @@
         <v>62</v>
       </c>
       <c r="B737" s="87"/>
-      <c r="C737" s="168"/>
-      <c r="D737" s="169"/>
-      <c r="E737" s="169"/>
+      <c r="C737" s="171"/>
+      <c r="D737" s="172"/>
+      <c r="E737" s="172"/>
     </row>
     <row r="738" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A738" s="59">
@@ -11877,9 +11937,9 @@
         <v>63</v>
       </c>
       <c r="B754" s="87"/>
-      <c r="C754" s="168"/>
-      <c r="D754" s="169"/>
-      <c r="E754" s="169"/>
+      <c r="C754" s="171"/>
+      <c r="D754" s="172"/>
+      <c r="E754" s="172"/>
     </row>
     <row r="755" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A755" s="59">
@@ -12030,9 +12090,9 @@
         <v>64</v>
       </c>
       <c r="B771" s="87"/>
-      <c r="C771" s="168"/>
-      <c r="D771" s="169"/>
-      <c r="E771" s="169"/>
+      <c r="C771" s="171"/>
+      <c r="D771" s="172"/>
+      <c r="E771" s="172"/>
     </row>
     <row r="772" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A772" s="59">
@@ -12183,9 +12243,9 @@
         <v>65</v>
       </c>
       <c r="B788" s="87"/>
-      <c r="C788" s="168"/>
-      <c r="D788" s="169"/>
-      <c r="E788" s="169"/>
+      <c r="C788" s="171"/>
+      <c r="D788" s="172"/>
+      <c r="E788" s="172"/>
     </row>
     <row r="789" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A789" s="59">
@@ -12336,9 +12396,9 @@
         <v>66</v>
       </c>
       <c r="B805" s="87"/>
-      <c r="C805" s="168"/>
-      <c r="D805" s="169"/>
-      <c r="E805" s="169"/>
+      <c r="C805" s="171"/>
+      <c r="D805" s="172"/>
+      <c r="E805" s="172"/>
     </row>
     <row r="806" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A806" s="59">
@@ -12489,18 +12549,18 @@
         <v>67</v>
       </c>
       <c r="B822" s="39"/>
-      <c r="C822" s="180"/>
-      <c r="D822" s="181"/>
-      <c r="E822" s="181"/>
+      <c r="C822" s="179"/>
+      <c r="D822" s="180"/>
+      <c r="E822" s="180"/>
     </row>
     <row r="823" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A823" s="63" t="s">
         <v>68</v>
       </c>
       <c r="B823" s="87"/>
-      <c r="C823" s="168"/>
-      <c r="D823" s="169"/>
-      <c r="E823" s="169"/>
+      <c r="C823" s="171"/>
+      <c r="D823" s="172"/>
+      <c r="E823" s="172"/>
     </row>
     <row r="824" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A824" s="64">
@@ -12651,9 +12711,9 @@
         <v>69</v>
       </c>
       <c r="B840" s="90"/>
-      <c r="C840" s="170"/>
-      <c r="D840" s="171"/>
-      <c r="E840" s="171"/>
+      <c r="C840" s="173"/>
+      <c r="D840" s="174"/>
+      <c r="E840" s="174"/>
     </row>
     <row r="841" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A841" s="64">
@@ -12804,9 +12864,9 @@
         <v>70</v>
       </c>
       <c r="B857" s="87"/>
-      <c r="C857" s="168"/>
-      <c r="D857" s="169"/>
-      <c r="E857" s="169"/>
+      <c r="C857" s="171"/>
+      <c r="D857" s="172"/>
+      <c r="E857" s="172"/>
     </row>
     <row r="858" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A858" s="64">
@@ -12957,9 +13017,9 @@
         <v>71</v>
       </c>
       <c r="B874" s="87"/>
-      <c r="C874" s="168"/>
-      <c r="D874" s="169"/>
-      <c r="E874" s="169"/>
+      <c r="C874" s="171"/>
+      <c r="D874" s="172"/>
+      <c r="E874" s="172"/>
     </row>
     <row r="875" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A875" s="64">
@@ -13110,9 +13170,9 @@
         <v>72</v>
       </c>
       <c r="B891" s="87"/>
-      <c r="C891" s="168"/>
-      <c r="D891" s="169"/>
-      <c r="E891" s="169"/>
+      <c r="C891" s="171"/>
+      <c r="D891" s="172"/>
+      <c r="E891" s="172"/>
     </row>
     <row r="892" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A892" s="64">
@@ -13263,9 +13323,9 @@
         <v>73</v>
       </c>
       <c r="B908" s="87"/>
-      <c r="C908" s="168"/>
-      <c r="D908" s="169"/>
-      <c r="E908" s="169"/>
+      <c r="C908" s="171"/>
+      <c r="D908" s="172"/>
+      <c r="E908" s="172"/>
     </row>
     <row r="909" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A909" s="64">
@@ -13416,9 +13476,9 @@
         <v>74</v>
       </c>
       <c r="B925" s="87"/>
-      <c r="C925" s="168"/>
-      <c r="D925" s="169"/>
-      <c r="E925" s="169"/>
+      <c r="C925" s="171"/>
+      <c r="D925" s="172"/>
+      <c r="E925" s="172"/>
     </row>
     <row r="926" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A926" s="64">
@@ -13569,9 +13629,9 @@
         <v>75</v>
       </c>
       <c r="B942" s="87"/>
-      <c r="C942" s="168"/>
-      <c r="D942" s="169"/>
-      <c r="E942" s="169"/>
+      <c r="C942" s="171"/>
+      <c r="D942" s="172"/>
+      <c r="E942" s="172"/>
     </row>
     <row r="943" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A943" s="64">
@@ -13722,9 +13782,9 @@
         <v>76</v>
       </c>
       <c r="B959" s="87"/>
-      <c r="C959" s="168"/>
-      <c r="D959" s="169"/>
-      <c r="E959" s="169"/>
+      <c r="C959" s="171"/>
+      <c r="D959" s="172"/>
+      <c r="E959" s="172"/>
     </row>
     <row r="960" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A960" s="64">
@@ -13875,9 +13935,9 @@
         <v>77</v>
       </c>
       <c r="B976" s="87"/>
-      <c r="C976" s="168"/>
-      <c r="D976" s="169"/>
-      <c r="E976" s="169"/>
+      <c r="C976" s="171"/>
+      <c r="D976" s="172"/>
+      <c r="E976" s="172"/>
     </row>
     <row r="977" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A977" s="64">
@@ -14028,9 +14088,9 @@
         <v>78</v>
       </c>
       <c r="B993" s="87"/>
-      <c r="C993" s="168"/>
-      <c r="D993" s="169"/>
-      <c r="E993" s="169"/>
+      <c r="C993" s="171"/>
+      <c r="D993" s="172"/>
+      <c r="E993" s="172"/>
     </row>
     <row r="994" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A994" s="64">
@@ -14181,9 +14241,9 @@
         <v>79</v>
       </c>
       <c r="B1010" s="87"/>
-      <c r="C1010" s="168"/>
-      <c r="D1010" s="169"/>
-      <c r="E1010" s="169"/>
+      <c r="C1010" s="171"/>
+      <c r="D1010" s="172"/>
+      <c r="E1010" s="172"/>
     </row>
     <row r="1011" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1011" s="64">
@@ -14334,9 +14394,9 @@
         <v>80</v>
       </c>
       <c r="B1027" s="87"/>
-      <c r="C1027" s="168"/>
-      <c r="D1027" s="169"/>
-      <c r="E1027" s="169"/>
+      <c r="C1027" s="171"/>
+      <c r="D1027" s="172"/>
+      <c r="E1027" s="172"/>
     </row>
     <row r="1028" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1028" s="64">
@@ -14487,9 +14547,9 @@
         <v>83</v>
       </c>
       <c r="B1044" s="87"/>
-      <c r="C1044" s="168"/>
-      <c r="D1044" s="169"/>
-      <c r="E1044" s="169"/>
+      <c r="C1044" s="171"/>
+      <c r="D1044" s="172"/>
+      <c r="E1044" s="172"/>
     </row>
     <row r="1045" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1045" s="64">
@@ -14640,9 +14700,9 @@
         <v>82</v>
       </c>
       <c r="B1061" s="87"/>
-      <c r="C1061" s="168"/>
-      <c r="D1061" s="169"/>
-      <c r="E1061" s="169"/>
+      <c r="C1061" s="171"/>
+      <c r="D1061" s="172"/>
+      <c r="E1061" s="172"/>
     </row>
     <row r="1062" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1062" s="64">
@@ -14793,9 +14853,9 @@
         <v>84</v>
       </c>
       <c r="B1078" s="87"/>
-      <c r="C1078" s="168"/>
-      <c r="D1078" s="169"/>
-      <c r="E1078" s="169"/>
+      <c r="C1078" s="171"/>
+      <c r="D1078" s="172"/>
+      <c r="E1078" s="172"/>
     </row>
     <row r="1079" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1079" s="64">
@@ -14946,18 +15006,18 @@
         <v>104</v>
       </c>
       <c r="B1095" s="40"/>
-      <c r="C1095" s="178"/>
-      <c r="D1095" s="179"/>
-      <c r="E1095" s="179"/>
+      <c r="C1095" s="181"/>
+      <c r="D1095" s="182"/>
+      <c r="E1095" s="182"/>
     </row>
     <row r="1096" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A1096" s="68" t="s">
         <v>85</v>
       </c>
       <c r="B1096" s="87"/>
-      <c r="C1096" s="168"/>
-      <c r="D1096" s="169"/>
-      <c r="E1096" s="169"/>
+      <c r="C1096" s="171"/>
+      <c r="D1096" s="172"/>
+      <c r="E1096" s="172"/>
     </row>
     <row r="1097" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1097" s="69">
@@ -15108,9 +15168,9 @@
         <v>86</v>
       </c>
       <c r="B1113" s="90"/>
-      <c r="C1113" s="170"/>
-      <c r="D1113" s="171"/>
-      <c r="E1113" s="171"/>
+      <c r="C1113" s="173"/>
+      <c r="D1113" s="174"/>
+      <c r="E1113" s="174"/>
     </row>
     <row r="1114" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1114" s="69">
@@ -15261,9 +15321,9 @@
         <v>87</v>
       </c>
       <c r="B1130" s="87"/>
-      <c r="C1130" s="168"/>
-      <c r="D1130" s="169"/>
-      <c r="E1130" s="169"/>
+      <c r="C1130" s="171"/>
+      <c r="D1130" s="172"/>
+      <c r="E1130" s="172"/>
     </row>
     <row r="1131" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1131" s="69">
@@ -15414,9 +15474,9 @@
         <v>88</v>
       </c>
       <c r="B1147" s="87"/>
-      <c r="C1147" s="168"/>
-      <c r="D1147" s="169"/>
-      <c r="E1147" s="169"/>
+      <c r="C1147" s="171"/>
+      <c r="D1147" s="172"/>
+      <c r="E1147" s="172"/>
     </row>
     <row r="1148" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1148" s="69">
@@ -15567,9 +15627,9 @@
         <v>89</v>
       </c>
       <c r="B1164" s="87"/>
-      <c r="C1164" s="168"/>
-      <c r="D1164" s="169"/>
-      <c r="E1164" s="169"/>
+      <c r="C1164" s="171"/>
+      <c r="D1164" s="172"/>
+      <c r="E1164" s="172"/>
     </row>
     <row r="1165" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1165" s="69">
@@ -15720,9 +15780,9 @@
         <v>90</v>
       </c>
       <c r="B1181" s="87"/>
-      <c r="C1181" s="168"/>
-      <c r="D1181" s="169"/>
-      <c r="E1181" s="169"/>
+      <c r="C1181" s="171"/>
+      <c r="D1181" s="172"/>
+      <c r="E1181" s="172"/>
     </row>
     <row r="1182" spans="1:5" hidden="1" outlineLevel="3">
       <c r="A1182" s="69">
@@ -15873,9 +15933,9 @@
         <v>91</v>
       </c>
       <c r="B1198" s="87"/>
-      <c r="C1198" s="168"/>
-      <c r="D1198" s="169"/>
-      <c r="E1198" s="169"/>
+      <c r="C1198" s="171"/>
+      <c r="D1198" s="172"/>
+      <c r="E1198" s="172"/>
     </row>
     <row r="1199" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1199" s="69">
@@ -16026,9 +16086,9 @@
         <v>92</v>
       </c>
       <c r="B1215" s="87"/>
-      <c r="C1215" s="168"/>
-      <c r="D1215" s="169"/>
-      <c r="E1215" s="169"/>
+      <c r="C1215" s="171"/>
+      <c r="D1215" s="172"/>
+      <c r="E1215" s="172"/>
     </row>
     <row r="1216" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1216" s="69">
@@ -16179,9 +16239,9 @@
         <v>93</v>
       </c>
       <c r="B1232" s="87"/>
-      <c r="C1232" s="168"/>
-      <c r="D1232" s="169"/>
-      <c r="E1232" s="169"/>
+      <c r="C1232" s="171"/>
+      <c r="D1232" s="172"/>
+      <c r="E1232" s="172"/>
     </row>
     <row r="1233" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1233" s="69">
@@ -16332,9 +16392,9 @@
         <v>94</v>
       </c>
       <c r="B1249" s="87"/>
-      <c r="C1249" s="168"/>
-      <c r="D1249" s="169"/>
-      <c r="E1249" s="169"/>
+      <c r="C1249" s="171"/>
+      <c r="D1249" s="172"/>
+      <c r="E1249" s="172"/>
     </row>
     <row r="1250" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1250" s="69">
@@ -16485,9 +16545,9 @@
         <v>99</v>
       </c>
       <c r="B1266" s="87"/>
-      <c r="C1266" s="168"/>
-      <c r="D1266" s="169"/>
-      <c r="E1266" s="169"/>
+      <c r="C1266" s="171"/>
+      <c r="D1266" s="172"/>
+      <c r="E1266" s="172"/>
     </row>
     <row r="1267" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1267" s="69">
@@ -16638,9 +16698,9 @@
         <v>100</v>
       </c>
       <c r="B1283" s="87"/>
-      <c r="C1283" s="168"/>
-      <c r="D1283" s="169"/>
-      <c r="E1283" s="169"/>
+      <c r="C1283" s="171"/>
+      <c r="D1283" s="172"/>
+      <c r="E1283" s="172"/>
     </row>
     <row r="1284" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1284" s="69">
@@ -16791,9 +16851,9 @@
         <v>101</v>
       </c>
       <c r="B1300" s="87"/>
-      <c r="C1300" s="168"/>
-      <c r="D1300" s="169"/>
-      <c r="E1300" s="169"/>
+      <c r="C1300" s="171"/>
+      <c r="D1300" s="172"/>
+      <c r="E1300" s="172"/>
     </row>
     <row r="1301" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1301" s="69">
@@ -16944,9 +17004,9 @@
         <v>81</v>
       </c>
       <c r="B1317" s="87"/>
-      <c r="C1317" s="168"/>
-      <c r="D1317" s="169"/>
-      <c r="E1317" s="169"/>
+      <c r="C1317" s="171"/>
+      <c r="D1317" s="172"/>
+      <c r="E1317" s="172"/>
     </row>
     <row r="1318" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1318" s="69">
@@ -17097,9 +17157,9 @@
         <v>102</v>
       </c>
       <c r="B1334" s="87"/>
-      <c r="C1334" s="168"/>
-      <c r="D1334" s="169"/>
-      <c r="E1334" s="169"/>
+      <c r="C1334" s="171"/>
+      <c r="D1334" s="172"/>
+      <c r="E1334" s="172"/>
     </row>
     <row r="1335" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1335" s="69">
@@ -17250,9 +17310,9 @@
         <v>98</v>
       </c>
       <c r="B1351" s="87"/>
-      <c r="C1351" s="168"/>
-      <c r="D1351" s="169"/>
-      <c r="E1351" s="169"/>
+      <c r="C1351" s="171"/>
+      <c r="D1351" s="172"/>
+      <c r="E1351" s="172"/>
     </row>
     <row r="1352" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1352" s="69">
@@ -17403,18 +17463,18 @@
         <v>103</v>
       </c>
       <c r="B1368" s="41"/>
-      <c r="C1368" s="176"/>
-      <c r="D1368" s="177"/>
-      <c r="E1368" s="177"/>
+      <c r="C1368" s="183"/>
+      <c r="D1368" s="184"/>
+      <c r="E1368" s="184"/>
     </row>
     <row r="1369" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A1369" s="73" t="s">
         <v>105</v>
       </c>
       <c r="B1369" s="87"/>
-      <c r="C1369" s="168"/>
-      <c r="D1369" s="169"/>
-      <c r="E1369" s="169"/>
+      <c r="C1369" s="171"/>
+      <c r="D1369" s="172"/>
+      <c r="E1369" s="172"/>
     </row>
     <row r="1370" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1370" s="74">
@@ -17565,9 +17625,9 @@
         <v>106</v>
       </c>
       <c r="B1386" s="90"/>
-      <c r="C1386" s="170"/>
-      <c r="D1386" s="171"/>
-      <c r="E1386" s="171"/>
+      <c r="C1386" s="173"/>
+      <c r="D1386" s="174"/>
+      <c r="E1386" s="174"/>
     </row>
     <row r="1387" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1387" s="74">
@@ -17718,9 +17778,9 @@
         <v>107</v>
       </c>
       <c r="B1403" s="87"/>
-      <c r="C1403" s="168"/>
-      <c r="D1403" s="169"/>
-      <c r="E1403" s="169"/>
+      <c r="C1403" s="171"/>
+      <c r="D1403" s="172"/>
+      <c r="E1403" s="172"/>
     </row>
     <row r="1404" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1404" s="74">
@@ -17871,9 +17931,9 @@
         <v>108</v>
       </c>
       <c r="B1420" s="87"/>
-      <c r="C1420" s="168"/>
-      <c r="D1420" s="169"/>
-      <c r="E1420" s="169"/>
+      <c r="C1420" s="171"/>
+      <c r="D1420" s="172"/>
+      <c r="E1420" s="172"/>
     </row>
     <row r="1421" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1421" s="74">
@@ -18024,9 +18084,9 @@
         <v>109</v>
       </c>
       <c r="B1437" s="87"/>
-      <c r="C1437" s="168"/>
-      <c r="D1437" s="169"/>
-      <c r="E1437" s="169"/>
+      <c r="C1437" s="171"/>
+      <c r="D1437" s="172"/>
+      <c r="E1437" s="172"/>
     </row>
     <row r="1438" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1438" s="74">
@@ -18177,9 +18237,9 @@
         <v>110</v>
       </c>
       <c r="B1454" s="87"/>
-      <c r="C1454" s="168"/>
-      <c r="D1454" s="169"/>
-      <c r="E1454" s="169"/>
+      <c r="C1454" s="171"/>
+      <c r="D1454" s="172"/>
+      <c r="E1454" s="172"/>
     </row>
     <row r="1455" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1455" s="74">
@@ -18330,9 +18390,9 @@
         <v>111</v>
       </c>
       <c r="B1471" s="87"/>
-      <c r="C1471" s="168"/>
-      <c r="D1471" s="169"/>
-      <c r="E1471" s="169"/>
+      <c r="C1471" s="171"/>
+      <c r="D1471" s="172"/>
+      <c r="E1471" s="172"/>
     </row>
     <row r="1472" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1472" s="74">
@@ -18483,9 +18543,9 @@
         <v>112</v>
       </c>
       <c r="B1488" s="87"/>
-      <c r="C1488" s="168"/>
-      <c r="D1488" s="169"/>
-      <c r="E1488" s="169"/>
+      <c r="C1488" s="171"/>
+      <c r="D1488" s="172"/>
+      <c r="E1488" s="172"/>
     </row>
     <row r="1489" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1489" s="74">
@@ -18636,9 +18696,9 @@
         <v>113</v>
       </c>
       <c r="B1505" s="87"/>
-      <c r="C1505" s="168"/>
-      <c r="D1505" s="169"/>
-      <c r="E1505" s="169"/>
+      <c r="C1505" s="171"/>
+      <c r="D1505" s="172"/>
+      <c r="E1505" s="172"/>
     </row>
     <row r="1506" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1506" s="74">
@@ -18789,9 +18849,9 @@
         <v>114</v>
       </c>
       <c r="B1522" s="87"/>
-      <c r="C1522" s="168"/>
-      <c r="D1522" s="169"/>
-      <c r="E1522" s="169"/>
+      <c r="C1522" s="171"/>
+      <c r="D1522" s="172"/>
+      <c r="E1522" s="172"/>
     </row>
     <row r="1523" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1523" s="74">
@@ -18942,9 +19002,9 @@
         <v>95</v>
       </c>
       <c r="B1539" s="87"/>
-      <c r="C1539" s="168"/>
-      <c r="D1539" s="169"/>
-      <c r="E1539" s="169"/>
+      <c r="C1539" s="171"/>
+      <c r="D1539" s="172"/>
+      <c r="E1539" s="172"/>
     </row>
     <row r="1540" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1540" s="74">
@@ -19095,9 +19155,9 @@
         <v>115</v>
       </c>
       <c r="B1556" s="87"/>
-      <c r="C1556" s="168"/>
-      <c r="D1556" s="169"/>
-      <c r="E1556" s="169"/>
+      <c r="C1556" s="171"/>
+      <c r="D1556" s="172"/>
+      <c r="E1556" s="172"/>
     </row>
     <row r="1557" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1557" s="74">
@@ -19248,9 +19308,9 @@
         <v>116</v>
       </c>
       <c r="B1573" s="87"/>
-      <c r="C1573" s="168"/>
-      <c r="D1573" s="169"/>
-      <c r="E1573" s="169"/>
+      <c r="C1573" s="171"/>
+      <c r="D1573" s="172"/>
+      <c r="E1573" s="172"/>
     </row>
     <row r="1574" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1574" s="74">
@@ -19401,9 +19461,9 @@
         <v>117</v>
       </c>
       <c r="B1590" s="87"/>
-      <c r="C1590" s="168"/>
-      <c r="D1590" s="169"/>
-      <c r="E1590" s="169"/>
+      <c r="C1590" s="171"/>
+      <c r="D1590" s="172"/>
+      <c r="E1590" s="172"/>
     </row>
     <row r="1591" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1591" s="74">
@@ -19554,9 +19614,9 @@
         <v>118</v>
       </c>
       <c r="B1607" s="87"/>
-      <c r="C1607" s="168"/>
-      <c r="D1607" s="169"/>
-      <c r="E1607" s="169"/>
+      <c r="C1607" s="171"/>
+      <c r="D1607" s="172"/>
+      <c r="E1607" s="172"/>
     </row>
     <row r="1608" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1608" s="74">
@@ -19707,9 +19767,9 @@
         <v>119</v>
       </c>
       <c r="B1624" s="87"/>
-      <c r="C1624" s="168"/>
-      <c r="D1624" s="169"/>
-      <c r="E1624" s="169"/>
+      <c r="C1624" s="171"/>
+      <c r="D1624" s="172"/>
+      <c r="E1624" s="172"/>
     </row>
     <row r="1625" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1625" s="74">
@@ -19860,18 +19920,18 @@
         <v>120</v>
       </c>
       <c r="B1641" s="42"/>
-      <c r="C1641" s="174"/>
-      <c r="D1641" s="175"/>
-      <c r="E1641" s="175"/>
+      <c r="C1641" s="185"/>
+      <c r="D1641" s="186"/>
+      <c r="E1641" s="186"/>
     </row>
     <row r="1642" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A1642" s="78" t="s">
         <v>121</v>
       </c>
       <c r="B1642" s="87"/>
-      <c r="C1642" s="168"/>
-      <c r="D1642" s="169"/>
-      <c r="E1642" s="169"/>
+      <c r="C1642" s="171"/>
+      <c r="D1642" s="172"/>
+      <c r="E1642" s="172"/>
     </row>
     <row r="1643" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1643" s="79">
@@ -20022,9 +20082,9 @@
         <v>122</v>
       </c>
       <c r="B1659" s="90"/>
-      <c r="C1659" s="170"/>
-      <c r="D1659" s="171"/>
-      <c r="E1659" s="171"/>
+      <c r="C1659" s="173"/>
+      <c r="D1659" s="174"/>
+      <c r="E1659" s="174"/>
     </row>
     <row r="1660" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1660" s="79">
@@ -20175,9 +20235,9 @@
         <v>123</v>
       </c>
       <c r="B1676" s="87"/>
-      <c r="C1676" s="168"/>
-      <c r="D1676" s="169"/>
-      <c r="E1676" s="169"/>
+      <c r="C1676" s="171"/>
+      <c r="D1676" s="172"/>
+      <c r="E1676" s="172"/>
     </row>
     <row r="1677" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1677" s="79">
@@ -20328,9 +20388,9 @@
         <v>124</v>
       </c>
       <c r="B1693" s="87"/>
-      <c r="C1693" s="168"/>
-      <c r="D1693" s="169"/>
-      <c r="E1693" s="169"/>
+      <c r="C1693" s="171"/>
+      <c r="D1693" s="172"/>
+      <c r="E1693" s="172"/>
     </row>
     <row r="1694" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1694" s="79">
@@ -20481,9 +20541,9 @@
         <v>125</v>
       </c>
       <c r="B1710" s="87"/>
-      <c r="C1710" s="168"/>
-      <c r="D1710" s="169"/>
-      <c r="E1710" s="169"/>
+      <c r="C1710" s="171"/>
+      <c r="D1710" s="172"/>
+      <c r="E1710" s="172"/>
     </row>
     <row r="1711" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1711" s="79">
@@ -20634,9 +20694,9 @@
         <v>126</v>
       </c>
       <c r="B1727" s="87"/>
-      <c r="C1727" s="168"/>
-      <c r="D1727" s="169"/>
-      <c r="E1727" s="169"/>
+      <c r="C1727" s="171"/>
+      <c r="D1727" s="172"/>
+      <c r="E1727" s="172"/>
     </row>
     <row r="1728" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1728" s="79">
@@ -20787,9 +20847,9 @@
         <v>127</v>
       </c>
       <c r="B1744" s="87"/>
-      <c r="C1744" s="168"/>
-      <c r="D1744" s="169"/>
-      <c r="E1744" s="169"/>
+      <c r="C1744" s="171"/>
+      <c r="D1744" s="172"/>
+      <c r="E1744" s="172"/>
     </row>
     <row r="1745" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1745" s="79">
@@ -20940,9 +21000,9 @@
         <v>128</v>
       </c>
       <c r="B1761" s="87"/>
-      <c r="C1761" s="168"/>
-      <c r="D1761" s="169"/>
-      <c r="E1761" s="169"/>
+      <c r="C1761" s="171"/>
+      <c r="D1761" s="172"/>
+      <c r="E1761" s="172"/>
     </row>
     <row r="1762" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1762" s="79">
@@ -21093,9 +21153,9 @@
         <v>129</v>
       </c>
       <c r="B1778" s="87"/>
-      <c r="C1778" s="168"/>
-      <c r="D1778" s="169"/>
-      <c r="E1778" s="169"/>
+      <c r="C1778" s="171"/>
+      <c r="D1778" s="172"/>
+      <c r="E1778" s="172"/>
     </row>
     <row r="1779" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1779" s="79">
@@ -21246,9 +21306,9 @@
         <v>130</v>
       </c>
       <c r="B1795" s="87"/>
-      <c r="C1795" s="168"/>
-      <c r="D1795" s="169"/>
-      <c r="E1795" s="169"/>
+      <c r="C1795" s="171"/>
+      <c r="D1795" s="172"/>
+      <c r="E1795" s="172"/>
     </row>
     <row r="1796" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1796" s="79">
@@ -21399,9 +21459,9 @@
         <v>131</v>
       </c>
       <c r="B1812" s="87"/>
-      <c r="C1812" s="168"/>
-      <c r="D1812" s="169"/>
-      <c r="E1812" s="169"/>
+      <c r="C1812" s="171"/>
+      <c r="D1812" s="172"/>
+      <c r="E1812" s="172"/>
     </row>
     <row r="1813" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1813" s="79">
@@ -21552,9 +21612,9 @@
         <v>96</v>
       </c>
       <c r="B1829" s="87"/>
-      <c r="C1829" s="168"/>
-      <c r="D1829" s="169"/>
-      <c r="E1829" s="169"/>
+      <c r="C1829" s="171"/>
+      <c r="D1829" s="172"/>
+      <c r="E1829" s="172"/>
     </row>
     <row r="1830" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1830" s="79">
@@ -21705,9 +21765,9 @@
         <v>132</v>
       </c>
       <c r="B1846" s="87"/>
-      <c r="C1846" s="168"/>
-      <c r="D1846" s="169"/>
-      <c r="E1846" s="169"/>
+      <c r="C1846" s="171"/>
+      <c r="D1846" s="172"/>
+      <c r="E1846" s="172"/>
     </row>
     <row r="1847" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1847" s="79">
@@ -21858,9 +21918,9 @@
         <v>133</v>
       </c>
       <c r="B1863" s="87"/>
-      <c r="C1863" s="168"/>
-      <c r="D1863" s="169"/>
-      <c r="E1863" s="169"/>
+      <c r="C1863" s="171"/>
+      <c r="D1863" s="172"/>
+      <c r="E1863" s="172"/>
     </row>
     <row r="1864" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1864" s="79">
@@ -22011,9 +22071,9 @@
         <v>134</v>
       </c>
       <c r="B1880" s="87"/>
-      <c r="C1880" s="168"/>
-      <c r="D1880" s="169"/>
-      <c r="E1880" s="169"/>
+      <c r="C1880" s="171"/>
+      <c r="D1880" s="172"/>
+      <c r="E1880" s="172"/>
     </row>
     <row r="1881" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1881" s="79">
@@ -22164,9 +22224,9 @@
         <v>135</v>
       </c>
       <c r="B1897" s="87"/>
-      <c r="C1897" s="168"/>
-      <c r="D1897" s="169"/>
-      <c r="E1897" s="169"/>
+      <c r="C1897" s="171"/>
+      <c r="D1897" s="172"/>
+      <c r="E1897" s="172"/>
     </row>
     <row r="1898" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1898" s="79">
@@ -22317,18 +22377,18 @@
         <v>136</v>
       </c>
       <c r="B1914" s="43"/>
-      <c r="C1914" s="172"/>
-      <c r="D1914" s="173"/>
-      <c r="E1914" s="173"/>
+      <c r="C1914" s="187"/>
+      <c r="D1914" s="188"/>
+      <c r="E1914" s="188"/>
     </row>
     <row r="1915" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A1915" s="83" t="s">
         <v>137</v>
       </c>
       <c r="B1915" s="87"/>
-      <c r="C1915" s="168"/>
-      <c r="D1915" s="169"/>
-      <c r="E1915" s="169"/>
+      <c r="C1915" s="171"/>
+      <c r="D1915" s="172"/>
+      <c r="E1915" s="172"/>
     </row>
     <row r="1916" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1916" s="84">
@@ -22479,9 +22539,9 @@
         <v>138</v>
       </c>
       <c r="B1932" s="90"/>
-      <c r="C1932" s="170"/>
-      <c r="D1932" s="171"/>
-      <c r="E1932" s="171"/>
+      <c r="C1932" s="173"/>
+      <c r="D1932" s="174"/>
+      <c r="E1932" s="174"/>
     </row>
     <row r="1933" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1933" s="84">
@@ -22632,9 +22692,9 @@
         <v>139</v>
       </c>
       <c r="B1949" s="87"/>
-      <c r="C1949" s="168"/>
-      <c r="D1949" s="169"/>
-      <c r="E1949" s="169"/>
+      <c r="C1949" s="171"/>
+      <c r="D1949" s="172"/>
+      <c r="E1949" s="172"/>
     </row>
     <row r="1950" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1950" s="84">
@@ -22785,9 +22845,9 @@
         <v>140</v>
       </c>
       <c r="B1966" s="87"/>
-      <c r="C1966" s="168"/>
-      <c r="D1966" s="169"/>
-      <c r="E1966" s="169"/>
+      <c r="C1966" s="171"/>
+      <c r="D1966" s="172"/>
+      <c r="E1966" s="172"/>
     </row>
     <row r="1967" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1967" s="84">
@@ -22938,9 +22998,9 @@
         <v>141</v>
       </c>
       <c r="B1983" s="87"/>
-      <c r="C1983" s="168"/>
-      <c r="D1983" s="169"/>
-      <c r="E1983" s="169"/>
+      <c r="C1983" s="171"/>
+      <c r="D1983" s="172"/>
+      <c r="E1983" s="172"/>
     </row>
     <row r="1984" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1984" s="84">
@@ -23091,9 +23151,9 @@
         <v>142</v>
       </c>
       <c r="B2000" s="87"/>
-      <c r="C2000" s="168"/>
-      <c r="D2000" s="169"/>
-      <c r="E2000" s="169"/>
+      <c r="C2000" s="171"/>
+      <c r="D2000" s="172"/>
+      <c r="E2000" s="172"/>
     </row>
     <row r="2001" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2001" s="84">
@@ -23244,9 +23304,9 @@
         <v>143</v>
       </c>
       <c r="B2017" s="87"/>
-      <c r="C2017" s="168"/>
-      <c r="D2017" s="169"/>
-      <c r="E2017" s="169"/>
+      <c r="C2017" s="171"/>
+      <c r="D2017" s="172"/>
+      <c r="E2017" s="172"/>
     </row>
     <row r="2018" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2018" s="84">
@@ -23397,9 +23457,9 @@
         <v>144</v>
       </c>
       <c r="B2034" s="87"/>
-      <c r="C2034" s="168"/>
-      <c r="D2034" s="169"/>
-      <c r="E2034" s="169"/>
+      <c r="C2034" s="171"/>
+      <c r="D2034" s="172"/>
+      <c r="E2034" s="172"/>
     </row>
     <row r="2035" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2035" s="84">
@@ -23550,9 +23610,9 @@
         <v>145</v>
       </c>
       <c r="B2051" s="87"/>
-      <c r="C2051" s="168"/>
-      <c r="D2051" s="169"/>
-      <c r="E2051" s="169"/>
+      <c r="C2051" s="171"/>
+      <c r="D2051" s="172"/>
+      <c r="E2051" s="172"/>
     </row>
     <row r="2052" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2052" s="84">
@@ -23703,9 +23763,9 @@
         <v>146</v>
       </c>
       <c r="B2068" s="87"/>
-      <c r="C2068" s="168"/>
-      <c r="D2068" s="169"/>
-      <c r="E2068" s="169"/>
+      <c r="C2068" s="171"/>
+      <c r="D2068" s="172"/>
+      <c r="E2068" s="172"/>
     </row>
     <row r="2069" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2069" s="84">
@@ -23856,9 +23916,9 @@
         <v>147</v>
       </c>
       <c r="B2085" s="87"/>
-      <c r="C2085" s="168"/>
-      <c r="D2085" s="169"/>
-      <c r="E2085" s="169"/>
+      <c r="C2085" s="171"/>
+      <c r="D2085" s="172"/>
+      <c r="E2085" s="172"/>
     </row>
     <row r="2086" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2086" s="84">
@@ -24009,9 +24069,9 @@
         <v>148</v>
       </c>
       <c r="B2102" s="87"/>
-      <c r="C2102" s="168"/>
-      <c r="D2102" s="169"/>
-      <c r="E2102" s="169"/>
+      <c r="C2102" s="171"/>
+      <c r="D2102" s="172"/>
+      <c r="E2102" s="172"/>
     </row>
     <row r="2103" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2103" s="84">
@@ -24162,9 +24222,9 @@
         <v>97</v>
       </c>
       <c r="B2119" s="87"/>
-      <c r="C2119" s="168"/>
-      <c r="D2119" s="169"/>
-      <c r="E2119" s="169"/>
+      <c r="C2119" s="171"/>
+      <c r="D2119" s="172"/>
+      <c r="E2119" s="172"/>
     </row>
     <row r="2120" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2120" s="84">
@@ -24315,9 +24375,9 @@
         <v>149</v>
       </c>
       <c r="B2136" s="87"/>
-      <c r="C2136" s="168"/>
-      <c r="D2136" s="169"/>
-      <c r="E2136" s="169"/>
+      <c r="C2136" s="171"/>
+      <c r="D2136" s="172"/>
+      <c r="E2136" s="172"/>
     </row>
     <row r="2137" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2137" s="84">
@@ -24468,9 +24528,9 @@
         <v>150</v>
       </c>
       <c r="B2153" s="87"/>
-      <c r="C2153" s="168"/>
-      <c r="D2153" s="169"/>
-      <c r="E2153" s="169"/>
+      <c r="C2153" s="171"/>
+      <c r="D2153" s="172"/>
+      <c r="E2153" s="172"/>
     </row>
     <row r="2154" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2154" s="84">
@@ -24621,9 +24681,9 @@
         <v>151</v>
       </c>
       <c r="B2170" s="87"/>
-      <c r="C2170" s="168"/>
-      <c r="D2170" s="169"/>
-      <c r="E2170" s="169"/>
+      <c r="C2170" s="171"/>
+      <c r="D2170" s="172"/>
+      <c r="E2170" s="172"/>
     </row>
     <row r="2171" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2171" s="84">
@@ -24771,26 +24831,111 @@
     </row>
   </sheetData>
   <mergeCells count="137">
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="C89:E89"/>
-    <mergeCell ref="C21:E21"/>
-    <mergeCell ref="C38:E38"/>
-    <mergeCell ref="C55:E55"/>
-    <mergeCell ref="C72:E72"/>
-    <mergeCell ref="C208:E208"/>
-    <mergeCell ref="C225:E225"/>
-    <mergeCell ref="C242:E242"/>
-    <mergeCell ref="C259:E259"/>
-    <mergeCell ref="C276:E276"/>
-    <mergeCell ref="C277:E277"/>
-    <mergeCell ref="C106:E106"/>
-    <mergeCell ref="C123:E123"/>
-    <mergeCell ref="C140:E140"/>
-    <mergeCell ref="C157:E157"/>
-    <mergeCell ref="C174:E174"/>
-    <mergeCell ref="C191:E191"/>
+    <mergeCell ref="C2034:E2034"/>
+    <mergeCell ref="C2051:E2051"/>
+    <mergeCell ref="C2068:E2068"/>
+    <mergeCell ref="C2085:E2085"/>
+    <mergeCell ref="C2170:E2170"/>
+    <mergeCell ref="C2102:E2102"/>
+    <mergeCell ref="C2119:E2119"/>
+    <mergeCell ref="C2136:E2136"/>
+    <mergeCell ref="C2153:E2153"/>
+    <mergeCell ref="C1932:E1932"/>
+    <mergeCell ref="C1949:E1949"/>
+    <mergeCell ref="C1966:E1966"/>
+    <mergeCell ref="C1983:E1983"/>
+    <mergeCell ref="C2000:E2000"/>
+    <mergeCell ref="C2017:E2017"/>
+    <mergeCell ref="C1846:E1846"/>
+    <mergeCell ref="C1863:E1863"/>
+    <mergeCell ref="C1880:E1880"/>
+    <mergeCell ref="C1897:E1897"/>
+    <mergeCell ref="C1914:E1914"/>
+    <mergeCell ref="C1915:E1915"/>
+    <mergeCell ref="C1744:E1744"/>
+    <mergeCell ref="C1761:E1761"/>
+    <mergeCell ref="C1778:E1778"/>
+    <mergeCell ref="C1795:E1795"/>
+    <mergeCell ref="C1812:E1812"/>
+    <mergeCell ref="C1829:E1829"/>
+    <mergeCell ref="C1642:E1642"/>
+    <mergeCell ref="C1659:E1659"/>
+    <mergeCell ref="C1676:E1676"/>
+    <mergeCell ref="C1693:E1693"/>
+    <mergeCell ref="C1710:E1710"/>
+    <mergeCell ref="C1727:E1727"/>
+    <mergeCell ref="C1556:E1556"/>
+    <mergeCell ref="C1573:E1573"/>
+    <mergeCell ref="C1590:E1590"/>
+    <mergeCell ref="C1607:E1607"/>
+    <mergeCell ref="C1624:E1624"/>
+    <mergeCell ref="C1641:E1641"/>
+    <mergeCell ref="C1454:E1454"/>
+    <mergeCell ref="C1471:E1471"/>
+    <mergeCell ref="C1488:E1488"/>
+    <mergeCell ref="C1505:E1505"/>
+    <mergeCell ref="C1522:E1522"/>
+    <mergeCell ref="C1539:E1539"/>
+    <mergeCell ref="C1368:E1368"/>
+    <mergeCell ref="C1369:E1369"/>
+    <mergeCell ref="C1386:E1386"/>
+    <mergeCell ref="C1403:E1403"/>
+    <mergeCell ref="C1420:E1420"/>
+    <mergeCell ref="C1437:E1437"/>
+    <mergeCell ref="C1266:E1266"/>
+    <mergeCell ref="C1283:E1283"/>
+    <mergeCell ref="C1300:E1300"/>
+    <mergeCell ref="C1317:E1317"/>
+    <mergeCell ref="C1334:E1334"/>
+    <mergeCell ref="C1351:E1351"/>
+    <mergeCell ref="C1164:E1164"/>
+    <mergeCell ref="C1181:E1181"/>
+    <mergeCell ref="C1198:E1198"/>
+    <mergeCell ref="C1215:E1215"/>
+    <mergeCell ref="C1232:E1232"/>
+    <mergeCell ref="C1249:E1249"/>
+    <mergeCell ref="C1078:E1078"/>
+    <mergeCell ref="C1095:E1095"/>
+    <mergeCell ref="C1096:E1096"/>
+    <mergeCell ref="C1113:E1113"/>
+    <mergeCell ref="C1130:E1130"/>
+    <mergeCell ref="C1147:E1147"/>
+    <mergeCell ref="C976:E976"/>
+    <mergeCell ref="C993:E993"/>
+    <mergeCell ref="C1010:E1010"/>
+    <mergeCell ref="C1027:E1027"/>
+    <mergeCell ref="C1044:E1044"/>
+    <mergeCell ref="C1061:E1061"/>
+    <mergeCell ref="C874:E874"/>
+    <mergeCell ref="C891:E891"/>
+    <mergeCell ref="C908:E908"/>
+    <mergeCell ref="C925:E925"/>
+    <mergeCell ref="C942:E942"/>
+    <mergeCell ref="C959:E959"/>
+    <mergeCell ref="C788:E788"/>
+    <mergeCell ref="C805:E805"/>
+    <mergeCell ref="C822:E822"/>
+    <mergeCell ref="C823:E823"/>
+    <mergeCell ref="C840:E840"/>
+    <mergeCell ref="C857:E857"/>
+    <mergeCell ref="C686:E686"/>
+    <mergeCell ref="C703:E703"/>
+    <mergeCell ref="C720:E720"/>
+    <mergeCell ref="C737:E737"/>
+    <mergeCell ref="C754:E754"/>
+    <mergeCell ref="C771:E771"/>
+    <mergeCell ref="C584:E584"/>
+    <mergeCell ref="C601:E601"/>
+    <mergeCell ref="C618:E618"/>
+    <mergeCell ref="C635:E635"/>
+    <mergeCell ref="C652:E652"/>
+    <mergeCell ref="C669:E669"/>
+    <mergeCell ref="C498:E498"/>
+    <mergeCell ref="C515:E515"/>
+    <mergeCell ref="C532:E532"/>
+    <mergeCell ref="C549:E549"/>
+    <mergeCell ref="C550:E550"/>
+    <mergeCell ref="C567:E567"/>
     <mergeCell ref="C396:E396"/>
     <mergeCell ref="C413:E413"/>
     <mergeCell ref="C430:E430"/>
@@ -24803,113 +24948,28 @@
     <mergeCell ref="C345:E345"/>
     <mergeCell ref="C362:E362"/>
     <mergeCell ref="C379:E379"/>
-    <mergeCell ref="C584:E584"/>
-    <mergeCell ref="C601:E601"/>
-    <mergeCell ref="C618:E618"/>
-    <mergeCell ref="C635:E635"/>
-    <mergeCell ref="C652:E652"/>
-    <mergeCell ref="C669:E669"/>
-    <mergeCell ref="C498:E498"/>
-    <mergeCell ref="C515:E515"/>
-    <mergeCell ref="C532:E532"/>
-    <mergeCell ref="C549:E549"/>
-    <mergeCell ref="C550:E550"/>
-    <mergeCell ref="C567:E567"/>
-    <mergeCell ref="C788:E788"/>
-    <mergeCell ref="C805:E805"/>
-    <mergeCell ref="C822:E822"/>
-    <mergeCell ref="C823:E823"/>
-    <mergeCell ref="C840:E840"/>
-    <mergeCell ref="C857:E857"/>
-    <mergeCell ref="C686:E686"/>
-    <mergeCell ref="C703:E703"/>
-    <mergeCell ref="C720:E720"/>
-    <mergeCell ref="C737:E737"/>
-    <mergeCell ref="C754:E754"/>
-    <mergeCell ref="C771:E771"/>
-    <mergeCell ref="C976:E976"/>
-    <mergeCell ref="C993:E993"/>
-    <mergeCell ref="C1010:E1010"/>
-    <mergeCell ref="C1027:E1027"/>
-    <mergeCell ref="C1044:E1044"/>
-    <mergeCell ref="C1061:E1061"/>
-    <mergeCell ref="C874:E874"/>
-    <mergeCell ref="C891:E891"/>
-    <mergeCell ref="C908:E908"/>
-    <mergeCell ref="C925:E925"/>
-    <mergeCell ref="C942:E942"/>
-    <mergeCell ref="C959:E959"/>
-    <mergeCell ref="C1164:E1164"/>
-    <mergeCell ref="C1181:E1181"/>
-    <mergeCell ref="C1198:E1198"/>
-    <mergeCell ref="C1215:E1215"/>
-    <mergeCell ref="C1232:E1232"/>
-    <mergeCell ref="C1249:E1249"/>
-    <mergeCell ref="C1078:E1078"/>
-    <mergeCell ref="C1095:E1095"/>
-    <mergeCell ref="C1096:E1096"/>
-    <mergeCell ref="C1113:E1113"/>
-    <mergeCell ref="C1130:E1130"/>
-    <mergeCell ref="C1147:E1147"/>
-    <mergeCell ref="C1368:E1368"/>
-    <mergeCell ref="C1369:E1369"/>
-    <mergeCell ref="C1386:E1386"/>
-    <mergeCell ref="C1403:E1403"/>
-    <mergeCell ref="C1420:E1420"/>
-    <mergeCell ref="C1437:E1437"/>
-    <mergeCell ref="C1266:E1266"/>
-    <mergeCell ref="C1283:E1283"/>
-    <mergeCell ref="C1300:E1300"/>
-    <mergeCell ref="C1317:E1317"/>
-    <mergeCell ref="C1334:E1334"/>
-    <mergeCell ref="C1351:E1351"/>
-    <mergeCell ref="C1556:E1556"/>
-    <mergeCell ref="C1573:E1573"/>
-    <mergeCell ref="C1590:E1590"/>
-    <mergeCell ref="C1607:E1607"/>
-    <mergeCell ref="C1624:E1624"/>
-    <mergeCell ref="C1641:E1641"/>
-    <mergeCell ref="C1454:E1454"/>
-    <mergeCell ref="C1471:E1471"/>
-    <mergeCell ref="C1488:E1488"/>
-    <mergeCell ref="C1505:E1505"/>
-    <mergeCell ref="C1522:E1522"/>
-    <mergeCell ref="C1539:E1539"/>
-    <mergeCell ref="C1744:E1744"/>
-    <mergeCell ref="C1761:E1761"/>
-    <mergeCell ref="C1778:E1778"/>
-    <mergeCell ref="C1795:E1795"/>
-    <mergeCell ref="C1812:E1812"/>
-    <mergeCell ref="C1829:E1829"/>
-    <mergeCell ref="C1642:E1642"/>
-    <mergeCell ref="C1659:E1659"/>
-    <mergeCell ref="C1676:E1676"/>
-    <mergeCell ref="C1693:E1693"/>
-    <mergeCell ref="C1710:E1710"/>
-    <mergeCell ref="C1727:E1727"/>
-    <mergeCell ref="C1932:E1932"/>
-    <mergeCell ref="C1949:E1949"/>
-    <mergeCell ref="C1966:E1966"/>
-    <mergeCell ref="C1983:E1983"/>
-    <mergeCell ref="C2000:E2000"/>
-    <mergeCell ref="C2017:E2017"/>
-    <mergeCell ref="C1846:E1846"/>
-    <mergeCell ref="C1863:E1863"/>
-    <mergeCell ref="C1880:E1880"/>
-    <mergeCell ref="C1897:E1897"/>
-    <mergeCell ref="C1914:E1914"/>
-    <mergeCell ref="C1915:E1915"/>
-    <mergeCell ref="C2034:E2034"/>
-    <mergeCell ref="C2051:E2051"/>
-    <mergeCell ref="C2068:E2068"/>
-    <mergeCell ref="C2085:E2085"/>
-    <mergeCell ref="C2170:E2170"/>
-    <mergeCell ref="C2102:E2102"/>
-    <mergeCell ref="C2119:E2119"/>
-    <mergeCell ref="C2136:E2136"/>
-    <mergeCell ref="C2153:E2153"/>
+    <mergeCell ref="C225:E225"/>
+    <mergeCell ref="C242:E242"/>
+    <mergeCell ref="C259:E259"/>
+    <mergeCell ref="C276:E276"/>
+    <mergeCell ref="C277:E277"/>
+    <mergeCell ref="C106:E106"/>
+    <mergeCell ref="C123:E123"/>
+    <mergeCell ref="C140:E140"/>
+    <mergeCell ref="C157:E157"/>
+    <mergeCell ref="C174:E174"/>
+    <mergeCell ref="C191:E191"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="C89:E89"/>
+    <mergeCell ref="C21:E21"/>
+    <mergeCell ref="C38:E38"/>
+    <mergeCell ref="C55:E55"/>
+    <mergeCell ref="C72:E72"/>
+    <mergeCell ref="C208:E208"/>
   </mergeCells>
-  <phoneticPr fontId="9" type="noConversion"/>
+  <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967294" verticalDpi="0" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
@@ -25660,7 +25720,7 @@
     <mergeCell ref="A3:K3"/>
     <mergeCell ref="A20:K20"/>
   </mergeCells>
-  <phoneticPr fontId="9" type="noConversion"/>
+  <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
@@ -25871,7 +25931,7 @@
   <mergeCells count="1">
     <mergeCell ref="A3:A10"/>
   </mergeCells>
-  <phoneticPr fontId="9" type="noConversion"/>
+  <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
@@ -26144,7 +26204,7 @@
     <mergeCell ref="A11:A17"/>
     <mergeCell ref="A19:A25"/>
   </mergeCells>
-  <phoneticPr fontId="9" type="noConversion"/>
+  <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
@@ -26166,163 +26226,150 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="33">
-      <c r="A1" s="213" t="s">
+      <c r="A1" s="214" t="s">
         <v>184</v>
       </c>
-      <c r="B1" s="214"/>
+      <c r="B1" s="215"/>
       <c r="C1" s="118"/>
       <c r="D1" s="5"/>
       <c r="E1" s="5"/>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="210" t="s">
+      <c r="A2" s="220" t="s">
         <v>183</v>
       </c>
-      <c r="B2" s="211"/>
+      <c r="B2" s="221"/>
       <c r="C2" s="120"/>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="212" t="s">
+      <c r="A3" s="222" t="s">
         <v>185</v>
       </c>
-      <c r="B3" s="211"/>
+      <c r="B3" s="221"/>
       <c r="C3" s="120"/>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="217"/>
-      <c r="B4" s="218"/>
+      <c r="A4" s="218"/>
+      <c r="B4" s="219"/>
       <c r="C4" s="120"/>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="215" t="s">
+      <c r="A5" s="216" t="s">
         <v>194</v>
       </c>
-      <c r="B5" s="216"/>
+      <c r="B5" s="217"/>
       <c r="C5" s="120"/>
     </row>
     <row r="7" spans="1:5" ht="18.75">
-      <c r="A7" s="221" t="s">
+      <c r="A7" s="208" t="s">
         <v>186</v>
       </c>
-      <c r="B7" s="222"/>
+      <c r="B7" s="209"/>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="120"/>
       <c r="B8" s="9"/>
     </row>
     <row r="9" spans="1:5" ht="39" customHeight="1">
-      <c r="A9" s="219" t="s">
+      <c r="A9" s="210" t="s">
         <v>187</v>
       </c>
-      <c r="B9" s="220"/>
+      <c r="B9" s="211"/>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="206"/>
-      <c r="B10" s="207"/>
+      <c r="A10" s="212"/>
+      <c r="B10" s="213"/>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="208" t="s">
+      <c r="A11" s="204" t="s">
         <v>188</v>
       </c>
-      <c r="B11" s="209"/>
+      <c r="B11" s="205"/>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="208" t="s">
+      <c r="A12" s="204" t="s">
         <v>189</v>
       </c>
-      <c r="B12" s="209"/>
+      <c r="B12" s="205"/>
     </row>
     <row r="13" spans="1:5" ht="43.5" customHeight="1">
-      <c r="A13" s="208" t="s">
+      <c r="A13" s="204" t="s">
         <v>190</v>
       </c>
-      <c r="B13" s="209"/>
+      <c r="B13" s="205"/>
     </row>
     <row r="14" spans="1:5" ht="19.5" customHeight="1">
-      <c r="A14" s="208" t="s">
+      <c r="A14" s="204" t="s">
         <v>191</v>
       </c>
-      <c r="B14" s="209"/>
+      <c r="B14" s="205"/>
     </row>
     <row r="15" spans="1:5" ht="18" customHeight="1">
-      <c r="A15" s="208" t="s">
+      <c r="A15" s="204" t="s">
         <v>192</v>
       </c>
-      <c r="B15" s="209"/>
+      <c r="B15" s="205"/>
     </row>
     <row r="16" spans="1:5" ht="21" customHeight="1">
-      <c r="A16" s="208" t="s">
+      <c r="A16" s="204" t="s">
         <v>193</v>
       </c>
-      <c r="B16" s="209"/>
+      <c r="B16" s="205"/>
     </row>
     <row r="17" spans="1:2" ht="48.75" customHeight="1">
-      <c r="A17" s="204" t="s">
+      <c r="A17" s="206" t="s">
         <v>195</v>
       </c>
-      <c r="B17" s="205"/>
+      <c r="B17" s="207"/>
     </row>
     <row r="19" spans="1:2" ht="18.75">
-      <c r="A19" s="221" t="s">
+      <c r="A19" s="208" t="s">
         <v>197</v>
       </c>
-      <c r="B19" s="222"/>
+      <c r="B19" s="209"/>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="120"/>
       <c r="B20" s="9"/>
     </row>
     <row r="21" spans="1:2">
-      <c r="A21" s="219" t="s">
+      <c r="A21" s="210" t="s">
         <v>198</v>
       </c>
-      <c r="B21" s="220"/>
+      <c r="B21" s="211"/>
     </row>
     <row r="22" spans="1:2">
-      <c r="A22" s="206"/>
-      <c r="B22" s="207"/>
+      <c r="A22" s="212"/>
+      <c r="B22" s="213"/>
     </row>
     <row r="23" spans="1:2">
-      <c r="A23" s="208" t="s">
+      <c r="A23" s="204" t="s">
         <v>199</v>
       </c>
-      <c r="B23" s="209"/>
+      <c r="B23" s="205"/>
     </row>
     <row r="24" spans="1:2">
-      <c r="A24" s="208"/>
-      <c r="B24" s="209"/>
+      <c r="A24" s="204"/>
+      <c r="B24" s="205"/>
     </row>
     <row r="25" spans="1:2">
-      <c r="A25" s="208" t="s">
+      <c r="A25" s="204" t="s">
         <v>200</v>
       </c>
-      <c r="B25" s="209"/>
+      <c r="B25" s="205"/>
     </row>
     <row r="26" spans="1:2">
-      <c r="A26" s="208" t="s">
+      <c r="A26" s="204" t="s">
         <v>201</v>
       </c>
-      <c r="B26" s="209"/>
+      <c r="B26" s="205"/>
     </row>
     <row r="27" spans="1:2">
-      <c r="A27" s="204"/>
-      <c r="B27" s="205"/>
+      <c r="A27" s="206"/>
+      <c r="B27" s="207"/>
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A7:B7"/>
     <mergeCell ref="A17:B17"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
@@ -26333,6 +26380,19 @@
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="A14:B14"/>
     <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A24:B24"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A3" r:id="rId1"/>

</xml_diff>

<commit_message>
Tempo - Indigestion stage 2 done.
</commit_message>
<xml_diff>
--- a/trunk/Tempo/Tempo.xlsx
+++ b/trunk/Tempo/Tempo.xlsx
@@ -2215,6 +2215,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="40" fillId="21" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -2237,29 +2238,29 @@
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="24" fillId="13" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="25" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="24" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="25" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="22" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="23" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="21" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="13" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="21" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="22" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="23" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="24" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="25" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="24" fillId="13" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="25" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="15" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="15" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="15" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -2295,34 +2296,20 @@
     <xf numFmtId="0" fontId="54" fillId="22" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="51" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="52" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="52" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="50" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="50" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="48" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="4"/>
     </xf>
@@ -2332,7 +2319,20 @@
     <xf numFmtId="0" fontId="49" fillId="0" borderId="33" xfId="3" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" indent="4"/>
     </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="50" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="50" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="51" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Accent1" xfId="2" builtinId="29"/>
@@ -2660,16 +2660,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="33">
-      <c r="A1" s="165" t="s">
+      <c r="A1" s="166" t="s">
         <v>205</v>
       </c>
-      <c r="B1" s="164"/>
-      <c r="C1" s="166" t="s">
+      <c r="B1" s="165"/>
+      <c r="C1" s="167" t="s">
         <v>170</v>
       </c>
-      <c r="D1" s="166"/>
-      <c r="E1" s="166"/>
-      <c r="F1" s="167"/>
+      <c r="D1" s="167"/>
+      <c r="E1" s="167"/>
+      <c r="F1" s="168"/>
       <c r="G1" s="140"/>
       <c r="H1" s="141">
         <f>SUM(G1:G65545)</f>
@@ -2734,11 +2734,11 @@
       <c r="B4" s="146" t="s">
         <v>228</v>
       </c>
-      <c r="C4" s="163" t="s">
+      <c r="C4" s="164" t="s">
         <v>232</v>
       </c>
-      <c r="D4" s="163"/>
-      <c r="E4" s="169"/>
+      <c r="D4" s="164"/>
+      <c r="E4" s="170"/>
       <c r="F4" s="143"/>
       <c r="G4" s="140"/>
       <c r="H4" s="140"/>
@@ -2753,10 +2753,10 @@
       <c r="B5" s="147" t="s">
         <v>177</v>
       </c>
-      <c r="C5" s="163" t="s">
+      <c r="C5" s="164" t="s">
         <v>218</v>
       </c>
-      <c r="D5" s="163"/>
+      <c r="D5" s="164"/>
       <c r="E5" s="147"/>
       <c r="F5" s="147"/>
       <c r="G5" s="148" t="s">
@@ -2780,10 +2780,10 @@
       <c r="B6" s="147" t="s">
         <v>179</v>
       </c>
-      <c r="C6" s="163" t="s">
+      <c r="C6" s="164" t="s">
         <v>168</v>
       </c>
-      <c r="D6" s="164"/>
+      <c r="D6" s="165"/>
       <c r="E6" s="147"/>
       <c r="F6" s="143"/>
       <c r="G6" s="140"/>
@@ -2807,7 +2807,7 @@
       <c r="F7" s="93"/>
     </row>
     <row r="8" spans="1:11" ht="15" customHeight="1" outlineLevel="1">
-      <c r="A8" s="168" t="s">
+      <c r="A8" s="169" t="s">
         <v>180</v>
       </c>
       <c r="B8" s="95" t="s">
@@ -2827,7 +2827,7 @@
       </c>
     </row>
     <row r="9" spans="1:11" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="A9" s="161"/>
+      <c r="A9" s="162"/>
       <c r="B9" s="98" t="s">
         <v>177</v>
       </c>
@@ -2841,7 +2841,7 @@
       <c r="F9" s="104"/>
     </row>
     <row r="10" spans="1:11" ht="15.75" outlineLevel="1" thickTop="1">
-      <c r="A10" s="161"/>
+      <c r="A10" s="162"/>
       <c r="B10" s="149" t="s">
         <v>208</v>
       </c>
@@ -2858,7 +2858,7 @@
       <c r="F10" s="105"/>
     </row>
     <row r="11" spans="1:11" ht="15" outlineLevel="1">
-      <c r="A11" s="161"/>
+      <c r="A11" s="162"/>
       <c r="B11" s="149" t="s">
         <v>214</v>
       </c>
@@ -2875,7 +2875,7 @@
       <c r="F11" s="105"/>
     </row>
     <row r="12" spans="1:11" ht="15" outlineLevel="1">
-      <c r="A12" s="161"/>
+      <c r="A12" s="162"/>
       <c r="B12" s="149" t="s">
         <v>209</v>
       </c>
@@ -2892,7 +2892,7 @@
       <c r="F12" s="105"/>
     </row>
     <row r="13" spans="1:11" ht="15" outlineLevel="1">
-      <c r="A13" s="161"/>
+      <c r="A13" s="162"/>
       <c r="B13" s="149" t="s">
         <v>213</v>
       </c>
@@ -2909,7 +2909,7 @@
       <c r="F13" s="105"/>
     </row>
     <row r="14" spans="1:11" ht="15" outlineLevel="1">
-      <c r="A14" s="161"/>
+      <c r="A14" s="162"/>
       <c r="B14" s="149" t="s">
         <v>214</v>
       </c>
@@ -2926,7 +2926,7 @@
       <c r="F14" s="105"/>
     </row>
     <row r="15" spans="1:11" ht="15" outlineLevel="1">
-      <c r="A15" s="161"/>
+      <c r="A15" s="162"/>
       <c r="B15" s="149" t="s">
         <v>215</v>
       </c>
@@ -2943,7 +2943,7 @@
       <c r="F15" s="105"/>
     </row>
     <row r="16" spans="1:11" ht="15" outlineLevel="1">
-      <c r="A16" s="161"/>
+      <c r="A16" s="162"/>
       <c r="B16" s="149" t="s">
         <v>216</v>
       </c>
@@ -2960,7 +2960,7 @@
       <c r="F16" s="105"/>
     </row>
     <row r="17" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A17" s="161"/>
+      <c r="A17" s="162"/>
       <c r="B17" s="149" t="s">
         <v>217</v>
       </c>
@@ -2977,7 +2977,7 @@
       <c r="F17" s="105"/>
     </row>
     <row r="18" spans="1:8" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="A18" s="161"/>
+      <c r="A18" s="162"/>
       <c r="B18" s="98" t="s">
         <v>179</v>
       </c>
@@ -3020,7 +3020,7 @@
     </row>
     <row r="20" spans="1:8" ht="13.5" thickBot="1"/>
     <row r="21" spans="1:8" ht="15" customHeight="1" outlineLevel="1">
-      <c r="A21" s="162" t="s">
+      <c r="A21" s="163" t="s">
         <v>219</v>
       </c>
       <c r="B21" s="109" t="s">
@@ -3040,7 +3040,7 @@
       </c>
     </row>
     <row r="22" spans="1:8" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="A22" s="161"/>
+      <c r="A22" s="162"/>
       <c r="B22" s="98" t="s">
         <v>177</v>
       </c>
@@ -3057,7 +3057,7 @@
       <c r="F22" s="104"/>
     </row>
     <row r="23" spans="1:8" ht="15.75" outlineLevel="1" thickTop="1">
-      <c r="A23" s="161"/>
+      <c r="A23" s="162"/>
       <c r="B23" s="149" t="s">
         <v>175</v>
       </c>
@@ -3070,7 +3070,7 @@
       <c r="F23" s="105"/>
     </row>
     <row r="24" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A24" s="161"/>
+      <c r="A24" s="162"/>
       <c r="B24" s="149" t="s">
         <v>221</v>
       </c>
@@ -3090,7 +3090,7 @@
       </c>
     </row>
     <row r="25" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A25" s="161"/>
+      <c r="A25" s="162"/>
       <c r="B25" s="149"/>
       <c r="C25" s="101"/>
       <c r="D25" s="101"/>
@@ -3101,7 +3101,7 @@
       <c r="F25" s="105"/>
     </row>
     <row r="26" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A26" s="161"/>
+      <c r="A26" s="162"/>
       <c r="B26" s="100"/>
       <c r="C26" s="101"/>
       <c r="D26" s="101"/>
@@ -3112,7 +3112,7 @@
       <c r="F26" s="105"/>
     </row>
     <row r="27" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A27" s="161"/>
+      <c r="A27" s="162"/>
       <c r="B27" s="100"/>
       <c r="C27" s="101"/>
       <c r="D27" s="101"/>
@@ -3123,7 +3123,7 @@
       <c r="F27" s="105"/>
     </row>
     <row r="28" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A28" s="161"/>
+      <c r="A28" s="162"/>
       <c r="B28" s="149" t="s">
         <v>222</v>
       </c>
@@ -3143,7 +3143,7 @@
       </c>
     </row>
     <row r="29" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A29" s="161"/>
+      <c r="A29" s="162"/>
       <c r="B29" s="154" t="s">
         <v>263</v>
       </c>
@@ -3161,7 +3161,7 @@
       </c>
     </row>
     <row r="30" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A30" s="161"/>
+      <c r="A30" s="162"/>
       <c r="B30" s="154" t="s">
         <v>264</v>
       </c>
@@ -3177,7 +3177,7 @@
       </c>
     </row>
     <row r="31" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A31" s="161"/>
+      <c r="A31" s="162"/>
       <c r="B31" s="154" t="s">
         <v>265</v>
       </c>
@@ -3193,7 +3193,7 @@
       </c>
     </row>
     <row r="32" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A32" s="161"/>
+      <c r="A32" s="162"/>
       <c r="B32" s="154" t="s">
         <v>266</v>
       </c>
@@ -3209,7 +3209,7 @@
       </c>
     </row>
     <row r="33" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A33" s="161"/>
+      <c r="A33" s="162"/>
       <c r="B33" s="154" t="s">
         <v>268</v>
       </c>
@@ -3225,7 +3225,7 @@
       </c>
     </row>
     <row r="34" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A34" s="161"/>
+      <c r="A34" s="162"/>
       <c r="B34" s="154" t="s">
         <v>269</v>
       </c>
@@ -3241,7 +3241,7 @@
       </c>
     </row>
     <row r="35" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A35" s="161"/>
+      <c r="A35" s="162"/>
       <c r="B35" s="154" t="s">
         <v>270</v>
       </c>
@@ -3260,7 +3260,7 @@
       </c>
     </row>
     <row r="36" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A36" s="161"/>
+      <c r="A36" s="162"/>
       <c r="B36" s="149" t="s">
         <v>223</v>
       </c>
@@ -3280,7 +3280,7 @@
       </c>
     </row>
     <row r="37" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A37" s="161"/>
+      <c r="A37" s="162"/>
       <c r="B37" s="149" t="s">
         <v>224</v>
       </c>
@@ -3297,7 +3297,7 @@
       <c r="F37" s="105"/>
     </row>
     <row r="38" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A38" s="161"/>
+      <c r="A38" s="162"/>
       <c r="B38" s="149" t="s">
         <v>225</v>
       </c>
@@ -3314,7 +3314,7 @@
       <c r="F38" s="105"/>
     </row>
     <row r="39" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A39" s="161"/>
+      <c r="A39" s="162"/>
       <c r="B39" s="149" t="s">
         <v>217</v>
       </c>
@@ -3331,7 +3331,7 @@
       <c r="F39" s="105"/>
     </row>
     <row r="40" spans="1:9" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="A40" s="161"/>
+      <c r="A40" s="162"/>
       <c r="B40" s="98" t="s">
         <v>179</v>
       </c>
@@ -3370,7 +3370,7 @@
     </row>
     <row r="42" spans="1:9" ht="13.5" thickBot="1"/>
     <row r="43" spans="1:9" ht="15" customHeight="1" outlineLevel="1">
-      <c r="A43" s="160" t="s">
+      <c r="A43" s="161" t="s">
         <v>226</v>
       </c>
       <c r="B43" s="113" t="s">
@@ -3390,7 +3390,7 @@
       </c>
     </row>
     <row r="44" spans="1:9" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="A44" s="161"/>
+      <c r="A44" s="162"/>
       <c r="B44" s="98" t="s">
         <v>177</v>
       </c>
@@ -3408,7 +3408,7 @@
       </c>
     </row>
     <row r="45" spans="1:9" ht="15.75" outlineLevel="1" thickTop="1">
-      <c r="A45" s="161"/>
+      <c r="A45" s="162"/>
       <c r="B45" s="100"/>
       <c r="C45" s="101"/>
       <c r="D45" s="101"/>
@@ -3419,7 +3419,7 @@
       <c r="F45" s="105"/>
     </row>
     <row r="46" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A46" s="161"/>
+      <c r="A46" s="162"/>
       <c r="B46" s="149" t="s">
         <v>221</v>
       </c>
@@ -3436,7 +3436,7 @@
       <c r="F46" s="105"/>
     </row>
     <row r="47" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A47" s="161"/>
+      <c r="A47" s="162"/>
       <c r="B47" s="155" t="s">
         <v>273</v>
       </c>
@@ -3451,7 +3451,7 @@
       <c r="F47" s="105"/>
     </row>
     <row r="48" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A48" s="161"/>
+      <c r="A48" s="162"/>
       <c r="B48" s="157" t="s">
         <v>275</v>
       </c>
@@ -3466,7 +3466,7 @@
       </c>
     </row>
     <row r="49" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A49" s="161"/>
+      <c r="A49" s="162"/>
       <c r="B49" s="149" t="s">
         <v>222</v>
       </c>
@@ -3486,7 +3486,7 @@
       </c>
     </row>
     <row r="50" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A50" s="161"/>
+      <c r="A50" s="162"/>
       <c r="B50" s="156" t="s">
         <v>274</v>
       </c>
@@ -3498,7 +3498,7 @@
       <c r="F50" s="105"/>
     </row>
     <row r="51" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A51" s="161"/>
+      <c r="A51" s="162"/>
       <c r="B51" s="150" t="s">
         <v>229</v>
       </c>
@@ -3522,7 +3522,7 @@
       </c>
     </row>
     <row r="52" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A52" s="161"/>
+      <c r="A52" s="162"/>
       <c r="B52" s="150" t="s">
         <v>230</v>
       </c>
@@ -3546,7 +3546,7 @@
       </c>
     </row>
     <row r="53" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A53" s="161"/>
+      <c r="A53" s="162"/>
       <c r="B53" s="150" t="s">
         <v>231</v>
       </c>
@@ -3570,7 +3570,7 @@
       </c>
     </row>
     <row r="54" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A54" s="161"/>
+      <c r="A54" s="162"/>
       <c r="B54" s="150" t="s">
         <v>233</v>
       </c>
@@ -3594,7 +3594,7 @@
       </c>
     </row>
     <row r="55" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A55" s="161"/>
+      <c r="A55" s="162"/>
       <c r="B55" s="150" t="s">
         <v>234</v>
       </c>
@@ -3618,7 +3618,7 @@
       </c>
     </row>
     <row r="56" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A56" s="161"/>
+      <c r="A56" s="162"/>
       <c r="B56" s="150" t="s">
         <v>235</v>
       </c>
@@ -3642,7 +3642,7 @@
       </c>
     </row>
     <row r="57" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A57" s="161"/>
+      <c r="A57" s="162"/>
       <c r="B57" s="150" t="s">
         <v>236</v>
       </c>
@@ -3666,7 +3666,7 @@
       </c>
     </row>
     <row r="58" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A58" s="161"/>
+      <c r="A58" s="162"/>
       <c r="B58" s="158" t="s">
         <v>263</v>
       </c>
@@ -3681,7 +3681,7 @@
       <c r="F58" s="105"/>
     </row>
     <row r="59" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A59" s="161"/>
+      <c r="A59" s="162"/>
       <c r="B59" s="158" t="s">
         <v>264</v>
       </c>
@@ -3700,7 +3700,7 @@
       </c>
     </row>
     <row r="60" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A60" s="161"/>
+      <c r="A60" s="162"/>
       <c r="B60" s="158" t="s">
         <v>265</v>
       </c>
@@ -3719,7 +3719,7 @@
       </c>
     </row>
     <row r="61" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A61" s="161"/>
+      <c r="A61" s="162"/>
       <c r="B61" s="159" t="s">
         <v>266</v>
       </c>
@@ -3738,7 +3738,7 @@
       </c>
     </row>
     <row r="62" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A62" s="161"/>
+      <c r="A62" s="162"/>
       <c r="B62" s="159" t="s">
         <v>268</v>
       </c>
@@ -3757,7 +3757,7 @@
       </c>
     </row>
     <row r="63" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A63" s="161"/>
+      <c r="A63" s="162"/>
       <c r="B63" s="159" t="s">
         <v>269</v>
       </c>
@@ -3776,7 +3776,7 @@
       </c>
     </row>
     <row r="64" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A64" s="161"/>
+      <c r="A64" s="162"/>
       <c r="B64" s="159" t="s">
         <v>276</v>
       </c>
@@ -3795,7 +3795,7 @@
       </c>
     </row>
     <row r="65" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A65" s="161"/>
+      <c r="A65" s="162"/>
       <c r="B65" s="159" t="s">
         <v>276</v>
       </c>
@@ -3814,7 +3814,7 @@
       </c>
     </row>
     <row r="66" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A66" s="161"/>
+      <c r="A66" s="162"/>
       <c r="B66" s="150" t="s">
         <v>223</v>
       </c>
@@ -3831,7 +3831,7 @@
       <c r="F66" s="105"/>
     </row>
     <row r="67" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A67" s="161"/>
+      <c r="A67" s="162"/>
       <c r="B67" s="150" t="s">
         <v>237</v>
       </c>
@@ -3848,7 +3848,7 @@
       <c r="F67" s="105"/>
     </row>
     <row r="68" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A68" s="161"/>
+      <c r="A68" s="162"/>
       <c r="B68" s="150" t="s">
         <v>238</v>
       </c>
@@ -3865,7 +3865,7 @@
       <c r="F68" s="105"/>
     </row>
     <row r="69" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A69" s="161"/>
+      <c r="A69" s="162"/>
       <c r="B69" s="150" t="s">
         <v>217</v>
       </c>
@@ -3882,7 +3882,7 @@
       <c r="F69" s="105"/>
     </row>
     <row r="70" spans="1:9" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="A70" s="161"/>
+      <c r="A70" s="162"/>
       <c r="B70" s="98" t="s">
         <v>179</v>
       </c>
@@ -3925,7 +3925,7 @@
     </row>
     <row r="72" spans="1:9" ht="13.5" thickBot="1"/>
     <row r="73" spans="1:9" ht="15" customHeight="1" outlineLevel="1">
-      <c r="A73" s="162" t="s">
+      <c r="A73" s="163" t="s">
         <v>239</v>
       </c>
       <c r="B73" s="109" t="s">
@@ -3945,7 +3945,7 @@
       </c>
     </row>
     <row r="74" spans="1:9" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="A74" s="161"/>
+      <c r="A74" s="162"/>
       <c r="B74" s="98" t="s">
         <v>177</v>
       </c>
@@ -3965,7 +3965,7 @@
       </c>
     </row>
     <row r="75" spans="1:9" ht="15.75" outlineLevel="1" thickTop="1">
-      <c r="A75" s="161"/>
+      <c r="A75" s="162"/>
       <c r="B75" s="100"/>
       <c r="C75" s="101"/>
       <c r="D75" s="101"/>
@@ -3976,7 +3976,7 @@
       <c r="F75" s="105"/>
     </row>
     <row r="76" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A76" s="161"/>
+      <c r="A76" s="162"/>
       <c r="B76" s="151" t="s">
         <v>241</v>
       </c>
@@ -3993,9 +3993,9 @@
       <c r="F76" s="105"/>
     </row>
     <row r="77" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A77" s="161"/>
+      <c r="A77" s="162"/>
       <c r="B77" s="100"/>
-      <c r="C77" s="225"/>
+      <c r="C77" s="160"/>
       <c r="D77" s="101"/>
       <c r="E77" s="123">
         <f t="shared" si="6"/>
@@ -4004,24 +4004,24 @@
       <c r="F77" s="105"/>
     </row>
     <row r="78" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A78" s="161"/>
+      <c r="A78" s="162"/>
       <c r="B78" s="151" t="s">
         <v>242</v>
       </c>
       <c r="C78" s="101">
-        <v>26007</v>
+        <v>23856</v>
       </c>
       <c r="D78" s="101">
         <v>27765</v>
       </c>
       <c r="E78" s="123">
         <f t="shared" si="6"/>
-        <v>1758</v>
+        <v>3909</v>
       </c>
       <c r="F78" s="105"/>
     </row>
     <row r="79" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A79" s="161"/>
+      <c r="A79" s="162"/>
       <c r="B79" s="100"/>
       <c r="C79" s="101"/>
       <c r="D79" s="101"/>
@@ -4032,7 +4032,7 @@
       <c r="F79" s="105"/>
     </row>
     <row r="80" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A80" s="161"/>
+      <c r="A80" s="162"/>
       <c r="B80" s="151" t="s">
         <v>243</v>
       </c>
@@ -4047,7 +4047,7 @@
       <c r="F80" s="105"/>
     </row>
     <row r="81" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A81" s="161"/>
+      <c r="A81" s="162"/>
       <c r="B81" s="100"/>
       <c r="C81" s="101"/>
       <c r="D81" s="101"/>
@@ -4058,7 +4058,7 @@
       <c r="F81" s="105"/>
     </row>
     <row r="82" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A82" s="161"/>
+      <c r="A82" s="162"/>
       <c r="B82" s="151" t="s">
         <v>244</v>
       </c>
@@ -4073,7 +4073,7 @@
       <c r="F82" s="105"/>
     </row>
     <row r="83" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A83" s="161"/>
+      <c r="A83" s="162"/>
       <c r="B83" s="151" t="s">
         <v>237</v>
       </c>
@@ -4088,7 +4088,7 @@
       <c r="F83" s="105"/>
     </row>
     <row r="84" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A84" s="161"/>
+      <c r="A84" s="162"/>
       <c r="B84" s="151" t="s">
         <v>245</v>
       </c>
@@ -4103,7 +4103,7 @@
       <c r="F84" s="105"/>
     </row>
     <row r="85" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A85" s="161"/>
+      <c r="A85" s="162"/>
       <c r="B85" s="151" t="s">
         <v>217</v>
       </c>
@@ -4118,7 +4118,7 @@
       <c r="F85" s="105"/>
     </row>
     <row r="86" spans="1:8" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="A86" s="161"/>
+      <c r="A86" s="162"/>
       <c r="B86" s="98" t="s">
         <v>179</v>
       </c>
@@ -4159,7 +4159,7 @@
     </row>
     <row r="88" spans="1:8" ht="13.5" thickBot="1"/>
     <row r="89" spans="1:8" ht="15" customHeight="1" outlineLevel="1">
-      <c r="A89" s="160" t="s">
+      <c r="A89" s="161" t="s">
         <v>246</v>
       </c>
       <c r="B89" s="113" t="s">
@@ -4179,7 +4179,7 @@
       </c>
     </row>
     <row r="90" spans="1:8" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="A90" s="161"/>
+      <c r="A90" s="162"/>
       <c r="B90" s="98" t="s">
         <v>177</v>
       </c>
@@ -4197,7 +4197,7 @@
       </c>
     </row>
     <row r="91" spans="1:8" ht="15.75" outlineLevel="1" thickTop="1">
-      <c r="A91" s="161"/>
+      <c r="A91" s="162"/>
       <c r="B91" s="151" t="s">
         <v>228</v>
       </c>
@@ -4212,7 +4212,7 @@
       <c r="F91" s="105"/>
     </row>
     <row r="92" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A92" s="161"/>
+      <c r="A92" s="162"/>
       <c r="B92" s="151" t="s">
         <v>221</v>
       </c>
@@ -4227,7 +4227,7 @@
       <c r="F92" s="105"/>
     </row>
     <row r="93" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A93" s="161"/>
+      <c r="A93" s="162"/>
       <c r="B93" s="100"/>
       <c r="C93" s="101"/>
       <c r="D93" s="101"/>
@@ -4238,7 +4238,7 @@
       <c r="F93" s="105"/>
     </row>
     <row r="94" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A94" s="161"/>
+      <c r="A94" s="162"/>
       <c r="B94" s="151" t="s">
         <v>222</v>
       </c>
@@ -4253,7 +4253,7 @@
       <c r="F94" s="105"/>
     </row>
     <row r="95" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A95" s="161"/>
+      <c r="A95" s="162"/>
       <c r="B95" s="100"/>
       <c r="C95" s="101"/>
       <c r="D95" s="101"/>
@@ -4264,7 +4264,7 @@
       <c r="F95" s="105"/>
     </row>
     <row r="96" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A96" s="161"/>
+      <c r="A96" s="162"/>
       <c r="B96" s="152" t="s">
         <v>236</v>
       </c>
@@ -4279,7 +4279,7 @@
       <c r="F96" s="105"/>
     </row>
     <row r="97" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A97" s="161"/>
+      <c r="A97" s="162"/>
       <c r="B97" s="100"/>
       <c r="C97" s="101"/>
       <c r="D97" s="101"/>
@@ -4290,7 +4290,7 @@
       <c r="F97" s="105"/>
     </row>
     <row r="98" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A98" s="161"/>
+      <c r="A98" s="162"/>
       <c r="B98" s="100"/>
       <c r="C98" s="101"/>
       <c r="D98" s="101"/>
@@ -4301,7 +4301,7 @@
       <c r="F98" s="105"/>
     </row>
     <row r="99" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A99" s="161"/>
+      <c r="A99" s="162"/>
       <c r="B99" s="152" t="s">
         <v>223</v>
       </c>
@@ -4316,7 +4316,7 @@
       <c r="F99" s="105"/>
     </row>
     <row r="100" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A100" s="161"/>
+      <c r="A100" s="162"/>
       <c r="B100" s="152" t="s">
         <v>248</v>
       </c>
@@ -4331,7 +4331,7 @@
       <c r="F100" s="105"/>
     </row>
     <row r="101" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A101" s="161"/>
+      <c r="A101" s="162"/>
       <c r="B101" s="152" t="s">
         <v>249</v>
       </c>
@@ -4346,7 +4346,7 @@
       <c r="F101" s="105"/>
     </row>
     <row r="102" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A102" s="161"/>
+      <c r="A102" s="162"/>
       <c r="B102" s="152" t="s">
         <v>250</v>
       </c>
@@ -4361,7 +4361,7 @@
       <c r="F102" s="105"/>
     </row>
     <row r="103" spans="1:8" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="A103" s="161"/>
+      <c r="A103" s="162"/>
       <c r="B103" s="98" t="s">
         <v>179</v>
       </c>
@@ -4402,7 +4402,7 @@
     </row>
     <row r="105" spans="1:8" ht="13.5" thickBot="1"/>
     <row r="106" spans="1:8" ht="15" customHeight="1" outlineLevel="1">
-      <c r="A106" s="162" t="s">
+      <c r="A106" s="163" t="s">
         <v>251</v>
       </c>
       <c r="B106" s="109" t="s">
@@ -4422,7 +4422,7 @@
       </c>
     </row>
     <row r="107" spans="1:8" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="A107" s="161"/>
+      <c r="A107" s="162"/>
       <c r="B107" s="98" t="s">
         <v>177</v>
       </c>
@@ -4440,7 +4440,7 @@
       </c>
     </row>
     <row r="108" spans="1:8" ht="15.75" outlineLevel="1" thickTop="1">
-      <c r="A108" s="161"/>
+      <c r="A108" s="162"/>
       <c r="B108" s="100"/>
       <c r="C108" s="101"/>
       <c r="D108" s="101"/>
@@ -4451,7 +4451,7 @@
       <c r="F108" s="105"/>
     </row>
     <row r="109" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A109" s="161"/>
+      <c r="A109" s="162"/>
       <c r="B109" s="152" t="s">
         <v>253</v>
       </c>
@@ -4466,7 +4466,7 @@
       <c r="F109" s="105"/>
     </row>
     <row r="110" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A110" s="161"/>
+      <c r="A110" s="162"/>
       <c r="B110" s="100"/>
       <c r="C110" s="101"/>
       <c r="D110" s="101"/>
@@ -4477,7 +4477,7 @@
       <c r="F110" s="105"/>
     </row>
     <row r="111" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A111" s="161"/>
+      <c r="A111" s="162"/>
       <c r="B111" s="152" t="s">
         <v>254</v>
       </c>
@@ -4492,7 +4492,7 @@
       <c r="F111" s="105"/>
     </row>
     <row r="112" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A112" s="161"/>
+      <c r="A112" s="162"/>
       <c r="B112" s="100"/>
       <c r="C112" s="101"/>
       <c r="D112" s="101"/>
@@ -4503,7 +4503,7 @@
       <c r="F112" s="105"/>
     </row>
     <row r="113" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A113" s="161"/>
+      <c r="A113" s="162"/>
       <c r="B113" s="152" t="s">
         <v>223</v>
       </c>
@@ -4518,7 +4518,7 @@
       <c r="F113" s="105"/>
     </row>
     <row r="114" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A114" s="161"/>
+      <c r="A114" s="162"/>
       <c r="B114" s="152" t="s">
         <v>248</v>
       </c>
@@ -4533,7 +4533,7 @@
       <c r="F114" s="105"/>
     </row>
     <row r="115" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A115" s="161"/>
+      <c r="A115" s="162"/>
       <c r="B115" s="152" t="s">
         <v>255</v>
       </c>
@@ -4548,7 +4548,7 @@
       <c r="F115" s="105"/>
     </row>
     <row r="116" spans="1:9" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="A116" s="161"/>
+      <c r="A116" s="162"/>
       <c r="B116" s="98" t="s">
         <v>179</v>
       </c>
@@ -4589,7 +4589,7 @@
     </row>
     <row r="118" spans="1:9" ht="13.5" thickBot="1"/>
     <row r="119" spans="1:9" ht="15" customHeight="1" outlineLevel="1">
-      <c r="A119" s="160" t="s">
+      <c r="A119" s="161" t="s">
         <v>256</v>
       </c>
       <c r="B119" s="113" t="s">
@@ -4609,7 +4609,7 @@
       </c>
     </row>
     <row r="120" spans="1:9" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="A120" s="161"/>
+      <c r="A120" s="162"/>
       <c r="B120" s="98" t="s">
         <v>177</v>
       </c>
@@ -4631,7 +4631,7 @@
       </c>
     </row>
     <row r="121" spans="1:9" ht="15.75" outlineLevel="1" thickTop="1">
-      <c r="A121" s="161"/>
+      <c r="A121" s="162"/>
       <c r="B121" s="100"/>
       <c r="C121" s="101"/>
       <c r="D121" s="101"/>
@@ -4642,7 +4642,7 @@
       <c r="F121" s="105"/>
     </row>
     <row r="122" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A122" s="161"/>
+      <c r="A122" s="162"/>
       <c r="B122" s="152" t="s">
         <v>221</v>
       </c>
@@ -4657,7 +4657,7 @@
       <c r="F122" s="105"/>
     </row>
     <row r="123" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A123" s="161"/>
+      <c r="A123" s="162"/>
       <c r="B123" s="100"/>
       <c r="C123" s="101"/>
       <c r="D123" s="101"/>
@@ -4668,7 +4668,7 @@
       <c r="F123" s="105"/>
     </row>
     <row r="124" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A124" s="161"/>
+      <c r="A124" s="162"/>
       <c r="B124" s="152" t="s">
         <v>222</v>
       </c>
@@ -4683,7 +4683,7 @@
       <c r="F124" s="105"/>
     </row>
     <row r="125" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A125" s="161"/>
+      <c r="A125" s="162"/>
       <c r="B125" s="152" t="s">
         <v>248</v>
       </c>
@@ -4698,7 +4698,7 @@
       <c r="F125" s="105"/>
     </row>
     <row r="126" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A126" s="161"/>
+      <c r="A126" s="162"/>
       <c r="B126" s="152" t="s">
         <v>258</v>
       </c>
@@ -4713,7 +4713,7 @@
       <c r="F126" s="105"/>
     </row>
     <row r="127" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A127" s="161"/>
+      <c r="A127" s="162"/>
       <c r="B127" s="152" t="s">
         <v>224</v>
       </c>
@@ -4728,7 +4728,7 @@
       <c r="F127" s="105"/>
     </row>
     <row r="128" spans="1:9" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="A128" s="161"/>
+      <c r="A128" s="162"/>
       <c r="B128" s="98" t="s">
         <v>179</v>
       </c>
@@ -4769,7 +4769,7 @@
     </row>
     <row r="130" spans="1:9" ht="13.5" thickBot="1"/>
     <row r="131" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A131" s="162" t="s">
+      <c r="A131" s="163" t="s">
         <v>259</v>
       </c>
       <c r="B131" s="109" t="s">
@@ -4789,7 +4789,7 @@
       </c>
     </row>
     <row r="132" spans="1:9" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="A132" s="161"/>
+      <c r="A132" s="162"/>
       <c r="B132" s="98" t="s">
         <v>177</v>
       </c>
@@ -4811,7 +4811,7 @@
       </c>
     </row>
     <row r="133" spans="1:9" ht="15.75" outlineLevel="1" thickTop="1">
-      <c r="A133" s="161"/>
+      <c r="A133" s="162"/>
       <c r="B133" s="100"/>
       <c r="C133" s="101"/>
       <c r="D133" s="101"/>
@@ -4822,7 +4822,7 @@
       <c r="F133" s="105"/>
     </row>
     <row r="134" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A134" s="161"/>
+      <c r="A134" s="162"/>
       <c r="B134" s="100"/>
       <c r="C134" s="101"/>
       <c r="D134" s="101"/>
@@ -4833,7 +4833,7 @@
       <c r="F134" s="105"/>
     </row>
     <row r="135" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A135" s="161"/>
+      <c r="A135" s="162"/>
       <c r="B135" s="100"/>
       <c r="C135" s="101"/>
       <c r="D135" s="101"/>
@@ -4844,7 +4844,7 @@
       <c r="F135" s="105"/>
     </row>
     <row r="136" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A136" s="161"/>
+      <c r="A136" s="162"/>
       <c r="B136" s="100"/>
       <c r="C136" s="101"/>
       <c r="D136" s="101"/>
@@ -4855,7 +4855,7 @@
       <c r="F136" s="105"/>
     </row>
     <row r="137" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A137" s="161"/>
+      <c r="A137" s="162"/>
       <c r="B137" s="100"/>
       <c r="C137" s="101"/>
       <c r="D137" s="101"/>
@@ -4866,7 +4866,7 @@
       <c r="F137" s="105"/>
     </row>
     <row r="138" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A138" s="161"/>
+      <c r="A138" s="162"/>
       <c r="B138" s="100"/>
       <c r="C138" s="101"/>
       <c r="D138" s="101"/>
@@ -4877,7 +4877,7 @@
       <c r="F138" s="105"/>
     </row>
     <row r="139" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A139" s="161"/>
+      <c r="A139" s="162"/>
       <c r="B139" s="100"/>
       <c r="C139" s="101"/>
       <c r="D139" s="101"/>
@@ -4888,7 +4888,7 @@
       <c r="F139" s="105"/>
     </row>
     <row r="140" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A140" s="161"/>
+      <c r="A140" s="162"/>
       <c r="B140" s="100"/>
       <c r="C140" s="101"/>
       <c r="D140" s="101"/>
@@ -4899,7 +4899,7 @@
       <c r="F140" s="105"/>
     </row>
     <row r="141" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A141" s="161"/>
+      <c r="A141" s="162"/>
       <c r="B141" s="152" t="s">
         <v>261</v>
       </c>
@@ -4921,7 +4921,7 @@
       </c>
     </row>
     <row r="142" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A142" s="161"/>
+      <c r="A142" s="162"/>
       <c r="B142" s="100"/>
       <c r="C142" s="101"/>
       <c r="D142" s="101"/>
@@ -4932,7 +4932,7 @@
       <c r="F142" s="105"/>
     </row>
     <row r="143" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A143" s="161"/>
+      <c r="A143" s="162"/>
       <c r="B143" s="100"/>
       <c r="C143" s="101"/>
       <c r="D143" s="101"/>
@@ -4943,7 +4943,7 @@
       <c r="F143" s="105"/>
     </row>
     <row r="144" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A144" s="161"/>
+      <c r="A144" s="162"/>
       <c r="B144" s="100"/>
       <c r="C144" s="101"/>
       <c r="D144" s="101"/>
@@ -4954,7 +4954,7 @@
       <c r="F144" s="105"/>
     </row>
     <row r="145" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="A145" s="161"/>
+      <c r="A145" s="162"/>
       <c r="B145" s="98" t="s">
         <v>179</v>
       </c>
@@ -4992,7 +4992,7 @@
       </c>
     </row>
     <row r="148" spans="1:7" ht="15" hidden="1" outlineLevel="2">
-      <c r="A148" s="160" t="s">
+      <c r="A148" s="161" t="s">
         <v>169</v>
       </c>
       <c r="B148" s="113" t="s">
@@ -5012,7 +5012,7 @@
       </c>
     </row>
     <row r="149" spans="1:7" ht="15.75" hidden="1" outlineLevel="2" thickBot="1">
-      <c r="A149" s="161"/>
+      <c r="A149" s="162"/>
       <c r="B149" s="98" t="s">
         <v>177</v>
       </c>
@@ -5025,7 +5025,7 @@
       <c r="F149" s="104"/>
     </row>
     <row r="150" spans="1:7" ht="15.75" hidden="1" outlineLevel="2" thickTop="1">
-      <c r="A150" s="161"/>
+      <c r="A150" s="162"/>
       <c r="B150" s="100"/>
       <c r="C150" s="101"/>
       <c r="D150" s="101"/>
@@ -5036,7 +5036,7 @@
       <c r="F150" s="105"/>
     </row>
     <row r="151" spans="1:7" ht="15" hidden="1" outlineLevel="2">
-      <c r="A151" s="161"/>
+      <c r="A151" s="162"/>
       <c r="B151" s="100"/>
       <c r="C151" s="101"/>
       <c r="D151" s="101"/>
@@ -5047,7 +5047,7 @@
       <c r="F151" s="105"/>
     </row>
     <row r="152" spans="1:7" ht="15" hidden="1" outlineLevel="2">
-      <c r="A152" s="161"/>
+      <c r="A152" s="162"/>
       <c r="B152" s="100"/>
       <c r="C152" s="101"/>
       <c r="D152" s="101"/>
@@ -5058,7 +5058,7 @@
       <c r="F152" s="105"/>
     </row>
     <row r="153" spans="1:7" ht="15" hidden="1" outlineLevel="2">
-      <c r="A153" s="161"/>
+      <c r="A153" s="162"/>
       <c r="B153" s="100"/>
       <c r="C153" s="101"/>
       <c r="D153" s="101"/>
@@ -5069,7 +5069,7 @@
       <c r="F153" s="105"/>
     </row>
     <row r="154" spans="1:7" ht="15" hidden="1" outlineLevel="2">
-      <c r="A154" s="161"/>
+      <c r="A154" s="162"/>
       <c r="B154" s="100"/>
       <c r="C154" s="101"/>
       <c r="D154" s="101"/>
@@ -5080,7 +5080,7 @@
       <c r="F154" s="105"/>
     </row>
     <row r="155" spans="1:7" ht="15" hidden="1" outlineLevel="2">
-      <c r="A155" s="161"/>
+      <c r="A155" s="162"/>
       <c r="B155" s="100"/>
       <c r="C155" s="101"/>
       <c r="D155" s="101"/>
@@ -5091,7 +5091,7 @@
       <c r="F155" s="105"/>
     </row>
     <row r="156" spans="1:7" ht="15" hidden="1" outlineLevel="2">
-      <c r="A156" s="161"/>
+      <c r="A156" s="162"/>
       <c r="B156" s="100"/>
       <c r="C156" s="101"/>
       <c r="D156" s="101"/>
@@ -5102,7 +5102,7 @@
       <c r="F156" s="105"/>
     </row>
     <row r="157" spans="1:7" ht="15" hidden="1" outlineLevel="2">
-      <c r="A157" s="161"/>
+      <c r="A157" s="162"/>
       <c r="B157" s="100"/>
       <c r="C157" s="101"/>
       <c r="D157" s="101"/>
@@ -5113,7 +5113,7 @@
       <c r="F157" s="105"/>
     </row>
     <row r="158" spans="1:7" ht="15" hidden="1" outlineLevel="2">
-      <c r="A158" s="161"/>
+      <c r="A158" s="162"/>
       <c r="B158" s="100"/>
       <c r="C158" s="101"/>
       <c r="D158" s="101"/>
@@ -5124,7 +5124,7 @@
       <c r="F158" s="105"/>
     </row>
     <row r="159" spans="1:7" ht="15" hidden="1" outlineLevel="2">
-      <c r="A159" s="161"/>
+      <c r="A159" s="162"/>
       <c r="B159" s="100"/>
       <c r="C159" s="101"/>
       <c r="D159" s="101"/>
@@ -5135,7 +5135,7 @@
       <c r="F159" s="105"/>
     </row>
     <row r="160" spans="1:7" ht="15" hidden="1" outlineLevel="2">
-      <c r="A160" s="161"/>
+      <c r="A160" s="162"/>
       <c r="B160" s="100"/>
       <c r="C160" s="101"/>
       <c r="D160" s="101"/>
@@ -5146,7 +5146,7 @@
       <c r="F160" s="105"/>
     </row>
     <row r="161" spans="1:7" ht="15" hidden="1" outlineLevel="2">
-      <c r="A161" s="161"/>
+      <c r="A161" s="162"/>
       <c r="B161" s="100"/>
       <c r="C161" s="101"/>
       <c r="D161" s="101"/>
@@ -5157,7 +5157,7 @@
       <c r="F161" s="105"/>
     </row>
     <row r="162" spans="1:7" ht="15.75" hidden="1" outlineLevel="2" thickBot="1">
-      <c r="A162" s="161"/>
+      <c r="A162" s="162"/>
       <c r="B162" s="98" t="s">
         <v>179</v>
       </c>
@@ -5196,11 +5196,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="A148:A162"/>
-    <mergeCell ref="A119:A128"/>
-    <mergeCell ref="A89:A103"/>
-    <mergeCell ref="A131:A145"/>
-    <mergeCell ref="A106:A116"/>
     <mergeCell ref="A43:A70"/>
     <mergeCell ref="A73:A86"/>
     <mergeCell ref="C5:D5"/>
@@ -5210,6 +5205,11 @@
     <mergeCell ref="A8:A18"/>
     <mergeCell ref="A21:A40"/>
     <mergeCell ref="C4:E4"/>
+    <mergeCell ref="A148:A162"/>
+    <mergeCell ref="A119:A128"/>
+    <mergeCell ref="A89:A103"/>
+    <mergeCell ref="A131:A145"/>
+    <mergeCell ref="A106:A116"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -5241,13 +5241,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="26.25" customHeight="1">
-      <c r="A1" s="170" t="s">
+      <c r="A1" s="189" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="170"/>
-      <c r="C1" s="170"/>
-      <c r="D1" s="170"/>
-      <c r="E1" s="170"/>
+      <c r="B1" s="189"/>
+      <c r="C1" s="189"/>
+      <c r="D1" s="189"/>
+      <c r="E1" s="189"/>
       <c r="F1" s="7"/>
       <c r="G1" s="5"/>
       <c r="H1" s="5"/>
@@ -5277,18 +5277,18 @@
         <v>8</v>
       </c>
       <c r="B3" s="36"/>
-      <c r="C3" s="171"/>
-      <c r="D3" s="172"/>
-      <c r="E3" s="172"/>
+      <c r="C3" s="190"/>
+      <c r="D3" s="191"/>
+      <c r="E3" s="191"/>
     </row>
     <row r="4" spans="1:8" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A4" s="46" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="87"/>
-      <c r="C4" s="173"/>
-      <c r="D4" s="174"/>
-      <c r="E4" s="174"/>
+      <c r="C4" s="171"/>
+      <c r="D4" s="172"/>
+      <c r="E4" s="172"/>
       <c r="F4" s="6"/>
     </row>
     <row r="5" spans="1:8" hidden="1" outlineLevel="2">
@@ -5440,9 +5440,9 @@
         <v>9</v>
       </c>
       <c r="B21" s="90"/>
-      <c r="C21" s="175"/>
-      <c r="D21" s="176"/>
-      <c r="E21" s="176"/>
+      <c r="C21" s="173"/>
+      <c r="D21" s="174"/>
+      <c r="E21" s="174"/>
     </row>
     <row r="22" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A22" s="47">
@@ -5593,9 +5593,9 @@
         <v>10</v>
       </c>
       <c r="B38" s="87"/>
-      <c r="C38" s="173"/>
-      <c r="D38" s="174"/>
-      <c r="E38" s="174"/>
+      <c r="C38" s="171"/>
+      <c r="D38" s="172"/>
+      <c r="E38" s="172"/>
     </row>
     <row r="39" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A39" s="47">
@@ -5746,9 +5746,9 @@
         <v>11</v>
       </c>
       <c r="B55" s="87"/>
-      <c r="C55" s="173"/>
-      <c r="D55" s="174"/>
-      <c r="E55" s="174"/>
+      <c r="C55" s="171"/>
+      <c r="D55" s="172"/>
+      <c r="E55" s="172"/>
     </row>
     <row r="56" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A56" s="47">
@@ -5899,9 +5899,9 @@
         <v>12</v>
       </c>
       <c r="B72" s="87"/>
-      <c r="C72" s="173"/>
-      <c r="D72" s="174"/>
-      <c r="E72" s="174"/>
+      <c r="C72" s="171"/>
+      <c r="D72" s="172"/>
+      <c r="E72" s="172"/>
     </row>
     <row r="73" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A73" s="47">
@@ -6052,9 +6052,9 @@
         <v>13</v>
       </c>
       <c r="B89" s="87"/>
-      <c r="C89" s="173"/>
-      <c r="D89" s="174"/>
-      <c r="E89" s="174"/>
+      <c r="C89" s="171"/>
+      <c r="D89" s="172"/>
+      <c r="E89" s="172"/>
     </row>
     <row r="90" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A90" s="47">
@@ -6205,9 +6205,9 @@
         <v>14</v>
       </c>
       <c r="B106" s="87"/>
-      <c r="C106" s="173"/>
-      <c r="D106" s="174"/>
-      <c r="E106" s="174"/>
+      <c r="C106" s="171"/>
+      <c r="D106" s="172"/>
+      <c r="E106" s="172"/>
     </row>
     <row r="107" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A107" s="47">
@@ -6358,9 +6358,9 @@
         <v>15</v>
       </c>
       <c r="B123" s="87"/>
-      <c r="C123" s="173"/>
-      <c r="D123" s="174"/>
-      <c r="E123" s="174"/>
+      <c r="C123" s="171"/>
+      <c r="D123" s="172"/>
+      <c r="E123" s="172"/>
     </row>
     <row r="124" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A124" s="47">
@@ -6511,9 +6511,9 @@
         <v>16</v>
       </c>
       <c r="B140" s="87"/>
-      <c r="C140" s="173"/>
-      <c r="D140" s="174"/>
-      <c r="E140" s="174"/>
+      <c r="C140" s="171"/>
+      <c r="D140" s="172"/>
+      <c r="E140" s="172"/>
     </row>
     <row r="141" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A141" s="47">
@@ -6664,9 +6664,9 @@
         <v>17</v>
       </c>
       <c r="B157" s="87"/>
-      <c r="C157" s="173"/>
-      <c r="D157" s="174"/>
-      <c r="E157" s="174"/>
+      <c r="C157" s="171"/>
+      <c r="D157" s="172"/>
+      <c r="E157" s="172"/>
     </row>
     <row r="158" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A158" s="47">
@@ -6817,9 +6817,9 @@
         <v>18</v>
       </c>
       <c r="B174" s="87"/>
-      <c r="C174" s="173"/>
-      <c r="D174" s="174"/>
-      <c r="E174" s="174"/>
+      <c r="C174" s="171"/>
+      <c r="D174" s="172"/>
+      <c r="E174" s="172"/>
     </row>
     <row r="175" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A175" s="47">
@@ -6970,9 +6970,9 @@
         <v>19</v>
       </c>
       <c r="B191" s="87"/>
-      <c r="C191" s="173"/>
-      <c r="D191" s="174"/>
-      <c r="E191" s="174"/>
+      <c r="C191" s="171"/>
+      <c r="D191" s="172"/>
+      <c r="E191" s="172"/>
     </row>
     <row r="192" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A192" s="47">
@@ -7123,9 +7123,9 @@
         <v>20</v>
       </c>
       <c r="B208" s="87"/>
-      <c r="C208" s="173"/>
-      <c r="D208" s="174"/>
-      <c r="E208" s="174"/>
+      <c r="C208" s="171"/>
+      <c r="D208" s="172"/>
+      <c r="E208" s="172"/>
     </row>
     <row r="209" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A209" s="47">
@@ -7276,9 +7276,9 @@
         <v>21</v>
       </c>
       <c r="B225" s="87"/>
-      <c r="C225" s="173"/>
-      <c r="D225" s="174"/>
-      <c r="E225" s="174"/>
+      <c r="C225" s="171"/>
+      <c r="D225" s="172"/>
+      <c r="E225" s="172"/>
     </row>
     <row r="226" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A226" s="47">
@@ -7429,9 +7429,9 @@
         <v>22</v>
       </c>
       <c r="B242" s="87"/>
-      <c r="C242" s="173"/>
-      <c r="D242" s="174"/>
-      <c r="E242" s="174"/>
+      <c r="C242" s="171"/>
+      <c r="D242" s="172"/>
+      <c r="E242" s="172"/>
     </row>
     <row r="243" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A243" s="47">
@@ -7582,9 +7582,9 @@
         <v>23</v>
       </c>
       <c r="B259" s="87"/>
-      <c r="C259" s="173"/>
-      <c r="D259" s="174"/>
-      <c r="E259" s="174"/>
+      <c r="C259" s="171"/>
+      <c r="D259" s="172"/>
+      <c r="E259" s="172"/>
     </row>
     <row r="260" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A260" s="47">
@@ -7735,18 +7735,18 @@
         <v>24</v>
       </c>
       <c r="B276" s="37"/>
-      <c r="C276" s="177"/>
-      <c r="D276" s="178"/>
-      <c r="E276" s="178"/>
+      <c r="C276" s="187"/>
+      <c r="D276" s="188"/>
+      <c r="E276" s="188"/>
     </row>
     <row r="277" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A277" s="51" t="s">
         <v>25</v>
       </c>
       <c r="B277" s="87"/>
-      <c r="C277" s="173"/>
-      <c r="D277" s="174"/>
-      <c r="E277" s="174"/>
+      <c r="C277" s="171"/>
+      <c r="D277" s="172"/>
+      <c r="E277" s="172"/>
     </row>
     <row r="278" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A278" s="52">
@@ -7897,9 +7897,9 @@
         <v>26</v>
       </c>
       <c r="B294" s="90"/>
-      <c r="C294" s="175"/>
-      <c r="D294" s="176"/>
-      <c r="E294" s="176"/>
+      <c r="C294" s="173"/>
+      <c r="D294" s="174"/>
+      <c r="E294" s="174"/>
     </row>
     <row r="295" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A295" s="52">
@@ -8050,9 +8050,9 @@
         <v>27</v>
       </c>
       <c r="B311" s="87"/>
-      <c r="C311" s="173"/>
-      <c r="D311" s="174"/>
-      <c r="E311" s="174"/>
+      <c r="C311" s="171"/>
+      <c r="D311" s="172"/>
+      <c r="E311" s="172"/>
     </row>
     <row r="312" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A312" s="52">
@@ -8203,9 +8203,9 @@
         <v>28</v>
       </c>
       <c r="B328" s="87"/>
-      <c r="C328" s="173"/>
-      <c r="D328" s="174"/>
-      <c r="E328" s="174"/>
+      <c r="C328" s="171"/>
+      <c r="D328" s="172"/>
+      <c r="E328" s="172"/>
     </row>
     <row r="329" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A329" s="52">
@@ -8356,9 +8356,9 @@
         <v>29</v>
       </c>
       <c r="B345" s="87"/>
-      <c r="C345" s="173"/>
-      <c r="D345" s="174"/>
-      <c r="E345" s="174"/>
+      <c r="C345" s="171"/>
+      <c r="D345" s="172"/>
+      <c r="E345" s="172"/>
     </row>
     <row r="346" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A346" s="52">
@@ -8509,9 +8509,9 @@
         <v>30</v>
       </c>
       <c r="B362" s="87"/>
-      <c r="C362" s="173"/>
-      <c r="D362" s="174"/>
-      <c r="E362" s="174"/>
+      <c r="C362" s="171"/>
+      <c r="D362" s="172"/>
+      <c r="E362" s="172"/>
     </row>
     <row r="363" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A363" s="52">
@@ -8662,9 +8662,9 @@
         <v>31</v>
       </c>
       <c r="B379" s="87"/>
-      <c r="C379" s="173"/>
-      <c r="D379" s="174"/>
-      <c r="E379" s="174"/>
+      <c r="C379" s="171"/>
+      <c r="D379" s="172"/>
+      <c r="E379" s="172"/>
     </row>
     <row r="380" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A380" s="52">
@@ -8815,9 +8815,9 @@
         <v>32</v>
       </c>
       <c r="B396" s="87"/>
-      <c r="C396" s="173"/>
-      <c r="D396" s="174"/>
-      <c r="E396" s="174"/>
+      <c r="C396" s="171"/>
+      <c r="D396" s="172"/>
+      <c r="E396" s="172"/>
     </row>
     <row r="397" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A397" s="52">
@@ -8968,9 +8968,9 @@
         <v>33</v>
       </c>
       <c r="B413" s="87"/>
-      <c r="C413" s="173"/>
-      <c r="D413" s="174"/>
-      <c r="E413" s="174"/>
+      <c r="C413" s="171"/>
+      <c r="D413" s="172"/>
+      <c r="E413" s="172"/>
     </row>
     <row r="414" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A414" s="52">
@@ -9121,9 +9121,9 @@
         <v>34</v>
       </c>
       <c r="B430" s="87"/>
-      <c r="C430" s="173"/>
-      <c r="D430" s="174"/>
-      <c r="E430" s="174"/>
+      <c r="C430" s="171"/>
+      <c r="D430" s="172"/>
+      <c r="E430" s="172"/>
     </row>
     <row r="431" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A431" s="52">
@@ -9274,9 +9274,9 @@
         <v>35</v>
       </c>
       <c r="B447" s="87"/>
-      <c r="C447" s="173"/>
-      <c r="D447" s="174"/>
-      <c r="E447" s="174"/>
+      <c r="C447" s="171"/>
+      <c r="D447" s="172"/>
+      <c r="E447" s="172"/>
     </row>
     <row r="448" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A448" s="52">
@@ -9427,9 +9427,9 @@
         <v>36</v>
       </c>
       <c r="B464" s="87"/>
-      <c r="C464" s="173"/>
-      <c r="D464" s="174"/>
-      <c r="E464" s="174"/>
+      <c r="C464" s="171"/>
+      <c r="D464" s="172"/>
+      <c r="E464" s="172"/>
     </row>
     <row r="465" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A465" s="52">
@@ -9580,9 +9580,9 @@
         <v>37</v>
       </c>
       <c r="B481" s="87"/>
-      <c r="C481" s="173"/>
-      <c r="D481" s="174"/>
-      <c r="E481" s="174"/>
+      <c r="C481" s="171"/>
+      <c r="D481" s="172"/>
+      <c r="E481" s="172"/>
     </row>
     <row r="482" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A482" s="52">
@@ -9733,9 +9733,9 @@
         <v>38</v>
       </c>
       <c r="B498" s="87"/>
-      <c r="C498" s="173"/>
-      <c r="D498" s="174"/>
-      <c r="E498" s="174"/>
+      <c r="C498" s="171"/>
+      <c r="D498" s="172"/>
+      <c r="E498" s="172"/>
     </row>
     <row r="499" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A499" s="52">
@@ -9886,9 +9886,9 @@
         <v>39</v>
       </c>
       <c r="B515" s="87"/>
-      <c r="C515" s="173"/>
-      <c r="D515" s="174"/>
-      <c r="E515" s="174"/>
+      <c r="C515" s="171"/>
+      <c r="D515" s="172"/>
+      <c r="E515" s="172"/>
     </row>
     <row r="516" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A516" s="52">
@@ -10039,9 +10039,9 @@
         <v>40</v>
       </c>
       <c r="B532" s="87"/>
-      <c r="C532" s="173"/>
-      <c r="D532" s="174"/>
-      <c r="E532" s="174"/>
+      <c r="C532" s="171"/>
+      <c r="D532" s="172"/>
+      <c r="E532" s="172"/>
     </row>
     <row r="533" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A533" s="55">
@@ -10192,18 +10192,18 @@
         <v>50</v>
       </c>
       <c r="B549" s="38"/>
-      <c r="C549" s="179"/>
-      <c r="D549" s="180"/>
-      <c r="E549" s="180"/>
+      <c r="C549" s="185"/>
+      <c r="D549" s="186"/>
+      <c r="E549" s="186"/>
     </row>
     <row r="550" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A550" s="58" t="s">
         <v>51</v>
       </c>
       <c r="B550" s="87"/>
-      <c r="C550" s="173"/>
-      <c r="D550" s="174"/>
-      <c r="E550" s="174"/>
+      <c r="C550" s="171"/>
+      <c r="D550" s="172"/>
+      <c r="E550" s="172"/>
     </row>
     <row r="551" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A551" s="59">
@@ -10354,9 +10354,9 @@
         <v>52</v>
       </c>
       <c r="B567" s="90"/>
-      <c r="C567" s="175"/>
-      <c r="D567" s="176"/>
-      <c r="E567" s="176"/>
+      <c r="C567" s="173"/>
+      <c r="D567" s="174"/>
+      <c r="E567" s="174"/>
     </row>
     <row r="568" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A568" s="59">
@@ -10507,9 +10507,9 @@
         <v>53</v>
       </c>
       <c r="B584" s="87"/>
-      <c r="C584" s="173"/>
-      <c r="D584" s="174"/>
-      <c r="E584" s="174"/>
+      <c r="C584" s="171"/>
+      <c r="D584" s="172"/>
+      <c r="E584" s="172"/>
     </row>
     <row r="585" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A585" s="59">
@@ -10660,9 +10660,9 @@
         <v>54</v>
       </c>
       <c r="B601" s="87"/>
-      <c r="C601" s="173"/>
-      <c r="D601" s="174"/>
-      <c r="E601" s="174"/>
+      <c r="C601" s="171"/>
+      <c r="D601" s="172"/>
+      <c r="E601" s="172"/>
     </row>
     <row r="602" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A602" s="59">
@@ -10813,9 +10813,9 @@
         <v>55</v>
       </c>
       <c r="B618" s="87"/>
-      <c r="C618" s="173"/>
-      <c r="D618" s="174"/>
-      <c r="E618" s="174"/>
+      <c r="C618" s="171"/>
+      <c r="D618" s="172"/>
+      <c r="E618" s="172"/>
     </row>
     <row r="619" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A619" s="59">
@@ -10966,9 +10966,9 @@
         <v>56</v>
       </c>
       <c r="B635" s="87"/>
-      <c r="C635" s="173"/>
-      <c r="D635" s="174"/>
-      <c r="E635" s="174"/>
+      <c r="C635" s="171"/>
+      <c r="D635" s="172"/>
+      <c r="E635" s="172"/>
     </row>
     <row r="636" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A636" s="59">
@@ -11119,9 +11119,9 @@
         <v>57</v>
       </c>
       <c r="B652" s="87"/>
-      <c r="C652" s="173"/>
-      <c r="D652" s="174"/>
-      <c r="E652" s="174"/>
+      <c r="C652" s="171"/>
+      <c r="D652" s="172"/>
+      <c r="E652" s="172"/>
     </row>
     <row r="653" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A653" s="59">
@@ -11272,9 +11272,9 @@
         <v>58</v>
       </c>
       <c r="B669" s="87"/>
-      <c r="C669" s="173"/>
-      <c r="D669" s="174"/>
-      <c r="E669" s="174"/>
+      <c r="C669" s="171"/>
+      <c r="D669" s="172"/>
+      <c r="E669" s="172"/>
     </row>
     <row r="670" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A670" s="59">
@@ -11425,9 +11425,9 @@
         <v>59</v>
       </c>
       <c r="B686" s="87"/>
-      <c r="C686" s="173"/>
-      <c r="D686" s="174"/>
-      <c r="E686" s="174"/>
+      <c r="C686" s="171"/>
+      <c r="D686" s="172"/>
+      <c r="E686" s="172"/>
     </row>
     <row r="687" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A687" s="59">
@@ -11578,9 +11578,9 @@
         <v>60</v>
       </c>
       <c r="B703" s="87"/>
-      <c r="C703" s="173"/>
-      <c r="D703" s="174"/>
-      <c r="E703" s="174"/>
+      <c r="C703" s="171"/>
+      <c r="D703" s="172"/>
+      <c r="E703" s="172"/>
     </row>
     <row r="704" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A704" s="59">
@@ -11731,9 +11731,9 @@
         <v>61</v>
       </c>
       <c r="B720" s="87"/>
-      <c r="C720" s="173"/>
-      <c r="D720" s="174"/>
-      <c r="E720" s="174"/>
+      <c r="C720" s="171"/>
+      <c r="D720" s="172"/>
+      <c r="E720" s="172"/>
     </row>
     <row r="721" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A721" s="59">
@@ -11884,9 +11884,9 @@
         <v>62</v>
       </c>
       <c r="B737" s="87"/>
-      <c r="C737" s="173"/>
-      <c r="D737" s="174"/>
-      <c r="E737" s="174"/>
+      <c r="C737" s="171"/>
+      <c r="D737" s="172"/>
+      <c r="E737" s="172"/>
     </row>
     <row r="738" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A738" s="59">
@@ -12037,9 +12037,9 @@
         <v>63</v>
       </c>
       <c r="B754" s="87"/>
-      <c r="C754" s="173"/>
-      <c r="D754" s="174"/>
-      <c r="E754" s="174"/>
+      <c r="C754" s="171"/>
+      <c r="D754" s="172"/>
+      <c r="E754" s="172"/>
     </row>
     <row r="755" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A755" s="59">
@@ -12190,9 +12190,9 @@
         <v>64</v>
       </c>
       <c r="B771" s="87"/>
-      <c r="C771" s="173"/>
-      <c r="D771" s="174"/>
-      <c r="E771" s="174"/>
+      <c r="C771" s="171"/>
+      <c r="D771" s="172"/>
+      <c r="E771" s="172"/>
     </row>
     <row r="772" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A772" s="59">
@@ -12343,9 +12343,9 @@
         <v>65</v>
       </c>
       <c r="B788" s="87"/>
-      <c r="C788" s="173"/>
-      <c r="D788" s="174"/>
-      <c r="E788" s="174"/>
+      <c r="C788" s="171"/>
+      <c r="D788" s="172"/>
+      <c r="E788" s="172"/>
     </row>
     <row r="789" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A789" s="59">
@@ -12496,9 +12496,9 @@
         <v>66</v>
       </c>
       <c r="B805" s="87"/>
-      <c r="C805" s="173"/>
-      <c r="D805" s="174"/>
-      <c r="E805" s="174"/>
+      <c r="C805" s="171"/>
+      <c r="D805" s="172"/>
+      <c r="E805" s="172"/>
     </row>
     <row r="806" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A806" s="59">
@@ -12649,18 +12649,18 @@
         <v>67</v>
       </c>
       <c r="B822" s="39"/>
-      <c r="C822" s="181"/>
-      <c r="D822" s="182"/>
-      <c r="E822" s="182"/>
+      <c r="C822" s="183"/>
+      <c r="D822" s="184"/>
+      <c r="E822" s="184"/>
     </row>
     <row r="823" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A823" s="63" t="s">
         <v>68</v>
       </c>
       <c r="B823" s="87"/>
-      <c r="C823" s="173"/>
-      <c r="D823" s="174"/>
-      <c r="E823" s="174"/>
+      <c r="C823" s="171"/>
+      <c r="D823" s="172"/>
+      <c r="E823" s="172"/>
     </row>
     <row r="824" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A824" s="64">
@@ -12811,9 +12811,9 @@
         <v>69</v>
       </c>
       <c r="B840" s="90"/>
-      <c r="C840" s="175"/>
-      <c r="D840" s="176"/>
-      <c r="E840" s="176"/>
+      <c r="C840" s="173"/>
+      <c r="D840" s="174"/>
+      <c r="E840" s="174"/>
     </row>
     <row r="841" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A841" s="64">
@@ -12964,9 +12964,9 @@
         <v>70</v>
       </c>
       <c r="B857" s="87"/>
-      <c r="C857" s="173"/>
-      <c r="D857" s="174"/>
-      <c r="E857" s="174"/>
+      <c r="C857" s="171"/>
+      <c r="D857" s="172"/>
+      <c r="E857" s="172"/>
     </row>
     <row r="858" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A858" s="64">
@@ -13117,9 +13117,9 @@
         <v>71</v>
       </c>
       <c r="B874" s="87"/>
-      <c r="C874" s="173"/>
-      <c r="D874" s="174"/>
-      <c r="E874" s="174"/>
+      <c r="C874" s="171"/>
+      <c r="D874" s="172"/>
+      <c r="E874" s="172"/>
     </row>
     <row r="875" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A875" s="64">
@@ -13270,9 +13270,9 @@
         <v>72</v>
       </c>
       <c r="B891" s="87"/>
-      <c r="C891" s="173"/>
-      <c r="D891" s="174"/>
-      <c r="E891" s="174"/>
+      <c r="C891" s="171"/>
+      <c r="D891" s="172"/>
+      <c r="E891" s="172"/>
     </row>
     <row r="892" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A892" s="64">
@@ -13423,9 +13423,9 @@
         <v>73</v>
       </c>
       <c r="B908" s="87"/>
-      <c r="C908" s="173"/>
-      <c r="D908" s="174"/>
-      <c r="E908" s="174"/>
+      <c r="C908" s="171"/>
+      <c r="D908" s="172"/>
+      <c r="E908" s="172"/>
     </row>
     <row r="909" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A909" s="64">
@@ -13576,9 +13576,9 @@
         <v>74</v>
       </c>
       <c r="B925" s="87"/>
-      <c r="C925" s="173"/>
-      <c r="D925" s="174"/>
-      <c r="E925" s="174"/>
+      <c r="C925" s="171"/>
+      <c r="D925" s="172"/>
+      <c r="E925" s="172"/>
     </row>
     <row r="926" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A926" s="64">
@@ -13729,9 +13729,9 @@
         <v>75</v>
       </c>
       <c r="B942" s="87"/>
-      <c r="C942" s="173"/>
-      <c r="D942" s="174"/>
-      <c r="E942" s="174"/>
+      <c r="C942" s="171"/>
+      <c r="D942" s="172"/>
+      <c r="E942" s="172"/>
     </row>
     <row r="943" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A943" s="64">
@@ -13882,9 +13882,9 @@
         <v>76</v>
       </c>
       <c r="B959" s="87"/>
-      <c r="C959" s="173"/>
-      <c r="D959" s="174"/>
-      <c r="E959" s="174"/>
+      <c r="C959" s="171"/>
+      <c r="D959" s="172"/>
+      <c r="E959" s="172"/>
     </row>
     <row r="960" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A960" s="64">
@@ -14035,9 +14035,9 @@
         <v>77</v>
       </c>
       <c r="B976" s="87"/>
-      <c r="C976" s="173"/>
-      <c r="D976" s="174"/>
-      <c r="E976" s="174"/>
+      <c r="C976" s="171"/>
+      <c r="D976" s="172"/>
+      <c r="E976" s="172"/>
     </row>
     <row r="977" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A977" s="64">
@@ -14188,9 +14188,9 @@
         <v>78</v>
       </c>
       <c r="B993" s="87"/>
-      <c r="C993" s="173"/>
-      <c r="D993" s="174"/>
-      <c r="E993" s="174"/>
+      <c r="C993" s="171"/>
+      <c r="D993" s="172"/>
+      <c r="E993" s="172"/>
     </row>
     <row r="994" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A994" s="64">
@@ -14341,9 +14341,9 @@
         <v>79</v>
       </c>
       <c r="B1010" s="87"/>
-      <c r="C1010" s="173"/>
-      <c r="D1010" s="174"/>
-      <c r="E1010" s="174"/>
+      <c r="C1010" s="171"/>
+      <c r="D1010" s="172"/>
+      <c r="E1010" s="172"/>
     </row>
     <row r="1011" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1011" s="64">
@@ -14494,9 +14494,9 @@
         <v>80</v>
       </c>
       <c r="B1027" s="87"/>
-      <c r="C1027" s="173"/>
-      <c r="D1027" s="174"/>
-      <c r="E1027" s="174"/>
+      <c r="C1027" s="171"/>
+      <c r="D1027" s="172"/>
+      <c r="E1027" s="172"/>
     </row>
     <row r="1028" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1028" s="64">
@@ -14647,9 +14647,9 @@
         <v>83</v>
       </c>
       <c r="B1044" s="87"/>
-      <c r="C1044" s="173"/>
-      <c r="D1044" s="174"/>
-      <c r="E1044" s="174"/>
+      <c r="C1044" s="171"/>
+      <c r="D1044" s="172"/>
+      <c r="E1044" s="172"/>
     </row>
     <row r="1045" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1045" s="64">
@@ -14800,9 +14800,9 @@
         <v>82</v>
       </c>
       <c r="B1061" s="87"/>
-      <c r="C1061" s="173"/>
-      <c r="D1061" s="174"/>
-      <c r="E1061" s="174"/>
+      <c r="C1061" s="171"/>
+      <c r="D1061" s="172"/>
+      <c r="E1061" s="172"/>
     </row>
     <row r="1062" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1062" s="64">
@@ -14953,9 +14953,9 @@
         <v>84</v>
       </c>
       <c r="B1078" s="87"/>
-      <c r="C1078" s="173"/>
-      <c r="D1078" s="174"/>
-      <c r="E1078" s="174"/>
+      <c r="C1078" s="171"/>
+      <c r="D1078" s="172"/>
+      <c r="E1078" s="172"/>
     </row>
     <row r="1079" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1079" s="64">
@@ -15106,18 +15106,18 @@
         <v>104</v>
       </c>
       <c r="B1095" s="40"/>
-      <c r="C1095" s="183"/>
-      <c r="D1095" s="184"/>
-      <c r="E1095" s="184"/>
+      <c r="C1095" s="181"/>
+      <c r="D1095" s="182"/>
+      <c r="E1095" s="182"/>
     </row>
     <row r="1096" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A1096" s="68" t="s">
         <v>85</v>
       </c>
       <c r="B1096" s="87"/>
-      <c r="C1096" s="173"/>
-      <c r="D1096" s="174"/>
-      <c r="E1096" s="174"/>
+      <c r="C1096" s="171"/>
+      <c r="D1096" s="172"/>
+      <c r="E1096" s="172"/>
     </row>
     <row r="1097" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1097" s="69">
@@ -15268,9 +15268,9 @@
         <v>86</v>
       </c>
       <c r="B1113" s="90"/>
-      <c r="C1113" s="175"/>
-      <c r="D1113" s="176"/>
-      <c r="E1113" s="176"/>
+      <c r="C1113" s="173"/>
+      <c r="D1113" s="174"/>
+      <c r="E1113" s="174"/>
     </row>
     <row r="1114" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1114" s="69">
@@ -15421,9 +15421,9 @@
         <v>87</v>
       </c>
       <c r="B1130" s="87"/>
-      <c r="C1130" s="173"/>
-      <c r="D1130" s="174"/>
-      <c r="E1130" s="174"/>
+      <c r="C1130" s="171"/>
+      <c r="D1130" s="172"/>
+      <c r="E1130" s="172"/>
     </row>
     <row r="1131" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1131" s="69">
@@ -15574,9 +15574,9 @@
         <v>88</v>
       </c>
       <c r="B1147" s="87"/>
-      <c r="C1147" s="173"/>
-      <c r="D1147" s="174"/>
-      <c r="E1147" s="174"/>
+      <c r="C1147" s="171"/>
+      <c r="D1147" s="172"/>
+      <c r="E1147" s="172"/>
     </row>
     <row r="1148" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1148" s="69">
@@ -15727,9 +15727,9 @@
         <v>89</v>
       </c>
       <c r="B1164" s="87"/>
-      <c r="C1164" s="173"/>
-      <c r="D1164" s="174"/>
-      <c r="E1164" s="174"/>
+      <c r="C1164" s="171"/>
+      <c r="D1164" s="172"/>
+      <c r="E1164" s="172"/>
     </row>
     <row r="1165" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1165" s="69">
@@ -15880,9 +15880,9 @@
         <v>90</v>
       </c>
       <c r="B1181" s="87"/>
-      <c r="C1181" s="173"/>
-      <c r="D1181" s="174"/>
-      <c r="E1181" s="174"/>
+      <c r="C1181" s="171"/>
+      <c r="D1181" s="172"/>
+      <c r="E1181" s="172"/>
     </row>
     <row r="1182" spans="1:5" hidden="1" outlineLevel="3">
       <c r="A1182" s="69">
@@ -16033,9 +16033,9 @@
         <v>91</v>
       </c>
       <c r="B1198" s="87"/>
-      <c r="C1198" s="173"/>
-      <c r="D1198" s="174"/>
-      <c r="E1198" s="174"/>
+      <c r="C1198" s="171"/>
+      <c r="D1198" s="172"/>
+      <c r="E1198" s="172"/>
     </row>
     <row r="1199" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1199" s="69">
@@ -16186,9 +16186,9 @@
         <v>92</v>
       </c>
       <c r="B1215" s="87"/>
-      <c r="C1215" s="173"/>
-      <c r="D1215" s="174"/>
-      <c r="E1215" s="174"/>
+      <c r="C1215" s="171"/>
+      <c r="D1215" s="172"/>
+      <c r="E1215" s="172"/>
     </row>
     <row r="1216" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1216" s="69">
@@ -16339,9 +16339,9 @@
         <v>93</v>
       </c>
       <c r="B1232" s="87"/>
-      <c r="C1232" s="173"/>
-      <c r="D1232" s="174"/>
-      <c r="E1232" s="174"/>
+      <c r="C1232" s="171"/>
+      <c r="D1232" s="172"/>
+      <c r="E1232" s="172"/>
     </row>
     <row r="1233" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1233" s="69">
@@ -16492,9 +16492,9 @@
         <v>94</v>
       </c>
       <c r="B1249" s="87"/>
-      <c r="C1249" s="173"/>
-      <c r="D1249" s="174"/>
-      <c r="E1249" s="174"/>
+      <c r="C1249" s="171"/>
+      <c r="D1249" s="172"/>
+      <c r="E1249" s="172"/>
     </row>
     <row r="1250" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1250" s="69">
@@ -16645,9 +16645,9 @@
         <v>99</v>
       </c>
       <c r="B1266" s="87"/>
-      <c r="C1266" s="173"/>
-      <c r="D1266" s="174"/>
-      <c r="E1266" s="174"/>
+      <c r="C1266" s="171"/>
+      <c r="D1266" s="172"/>
+      <c r="E1266" s="172"/>
     </row>
     <row r="1267" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1267" s="69">
@@ -16798,9 +16798,9 @@
         <v>100</v>
       </c>
       <c r="B1283" s="87"/>
-      <c r="C1283" s="173"/>
-      <c r="D1283" s="174"/>
-      <c r="E1283" s="174"/>
+      <c r="C1283" s="171"/>
+      <c r="D1283" s="172"/>
+      <c r="E1283" s="172"/>
     </row>
     <row r="1284" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1284" s="69">
@@ -16951,9 +16951,9 @@
         <v>101</v>
       </c>
       <c r="B1300" s="87"/>
-      <c r="C1300" s="173"/>
-      <c r="D1300" s="174"/>
-      <c r="E1300" s="174"/>
+      <c r="C1300" s="171"/>
+      <c r="D1300" s="172"/>
+      <c r="E1300" s="172"/>
     </row>
     <row r="1301" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1301" s="69">
@@ -17104,9 +17104,9 @@
         <v>81</v>
       </c>
       <c r="B1317" s="87"/>
-      <c r="C1317" s="173"/>
-      <c r="D1317" s="174"/>
-      <c r="E1317" s="174"/>
+      <c r="C1317" s="171"/>
+      <c r="D1317" s="172"/>
+      <c r="E1317" s="172"/>
     </row>
     <row r="1318" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1318" s="69">
@@ -17257,9 +17257,9 @@
         <v>102</v>
       </c>
       <c r="B1334" s="87"/>
-      <c r="C1334" s="173"/>
-      <c r="D1334" s="174"/>
-      <c r="E1334" s="174"/>
+      <c r="C1334" s="171"/>
+      <c r="D1334" s="172"/>
+      <c r="E1334" s="172"/>
     </row>
     <row r="1335" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1335" s="69">
@@ -17410,9 +17410,9 @@
         <v>98</v>
       </c>
       <c r="B1351" s="87"/>
-      <c r="C1351" s="173"/>
-      <c r="D1351" s="174"/>
-      <c r="E1351" s="174"/>
+      <c r="C1351" s="171"/>
+      <c r="D1351" s="172"/>
+      <c r="E1351" s="172"/>
     </row>
     <row r="1352" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1352" s="69">
@@ -17563,18 +17563,18 @@
         <v>103</v>
       </c>
       <c r="B1368" s="41"/>
-      <c r="C1368" s="185"/>
-      <c r="D1368" s="186"/>
-      <c r="E1368" s="186"/>
+      <c r="C1368" s="179"/>
+      <c r="D1368" s="180"/>
+      <c r="E1368" s="180"/>
     </row>
     <row r="1369" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A1369" s="73" t="s">
         <v>105</v>
       </c>
       <c r="B1369" s="87"/>
-      <c r="C1369" s="173"/>
-      <c r="D1369" s="174"/>
-      <c r="E1369" s="174"/>
+      <c r="C1369" s="171"/>
+      <c r="D1369" s="172"/>
+      <c r="E1369" s="172"/>
     </row>
     <row r="1370" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1370" s="74">
@@ -17725,9 +17725,9 @@
         <v>106</v>
       </c>
       <c r="B1386" s="90"/>
-      <c r="C1386" s="175"/>
-      <c r="D1386" s="176"/>
-      <c r="E1386" s="176"/>
+      <c r="C1386" s="173"/>
+      <c r="D1386" s="174"/>
+      <c r="E1386" s="174"/>
     </row>
     <row r="1387" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1387" s="74">
@@ -17878,9 +17878,9 @@
         <v>107</v>
       </c>
       <c r="B1403" s="87"/>
-      <c r="C1403" s="173"/>
-      <c r="D1403" s="174"/>
-      <c r="E1403" s="174"/>
+      <c r="C1403" s="171"/>
+      <c r="D1403" s="172"/>
+      <c r="E1403" s="172"/>
     </row>
     <row r="1404" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1404" s="74">
@@ -18031,9 +18031,9 @@
         <v>108</v>
       </c>
       <c r="B1420" s="87"/>
-      <c r="C1420" s="173"/>
-      <c r="D1420" s="174"/>
-      <c r="E1420" s="174"/>
+      <c r="C1420" s="171"/>
+      <c r="D1420" s="172"/>
+      <c r="E1420" s="172"/>
     </row>
     <row r="1421" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1421" s="74">
@@ -18184,9 +18184,9 @@
         <v>109</v>
       </c>
       <c r="B1437" s="87"/>
-      <c r="C1437" s="173"/>
-      <c r="D1437" s="174"/>
-      <c r="E1437" s="174"/>
+      <c r="C1437" s="171"/>
+      <c r="D1437" s="172"/>
+      <c r="E1437" s="172"/>
     </row>
     <row r="1438" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1438" s="74">
@@ -18337,9 +18337,9 @@
         <v>110</v>
       </c>
       <c r="B1454" s="87"/>
-      <c r="C1454" s="173"/>
-      <c r="D1454" s="174"/>
-      <c r="E1454" s="174"/>
+      <c r="C1454" s="171"/>
+      <c r="D1454" s="172"/>
+      <c r="E1454" s="172"/>
     </row>
     <row r="1455" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1455" s="74">
@@ -18490,9 +18490,9 @@
         <v>111</v>
       </c>
       <c r="B1471" s="87"/>
-      <c r="C1471" s="173"/>
-      <c r="D1471" s="174"/>
-      <c r="E1471" s="174"/>
+      <c r="C1471" s="171"/>
+      <c r="D1471" s="172"/>
+      <c r="E1471" s="172"/>
     </row>
     <row r="1472" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1472" s="74">
@@ -18643,9 +18643,9 @@
         <v>112</v>
       </c>
       <c r="B1488" s="87"/>
-      <c r="C1488" s="173"/>
-      <c r="D1488" s="174"/>
-      <c r="E1488" s="174"/>
+      <c r="C1488" s="171"/>
+      <c r="D1488" s="172"/>
+      <c r="E1488" s="172"/>
     </row>
     <row r="1489" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1489" s="74">
@@ -18796,9 +18796,9 @@
         <v>113</v>
       </c>
       <c r="B1505" s="87"/>
-      <c r="C1505" s="173"/>
-      <c r="D1505" s="174"/>
-      <c r="E1505" s="174"/>
+      <c r="C1505" s="171"/>
+      <c r="D1505" s="172"/>
+      <c r="E1505" s="172"/>
     </row>
     <row r="1506" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1506" s="74">
@@ -18949,9 +18949,9 @@
         <v>114</v>
       </c>
       <c r="B1522" s="87"/>
-      <c r="C1522" s="173"/>
-      <c r="D1522" s="174"/>
-      <c r="E1522" s="174"/>
+      <c r="C1522" s="171"/>
+      <c r="D1522" s="172"/>
+      <c r="E1522" s="172"/>
     </row>
     <row r="1523" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1523" s="74">
@@ -19102,9 +19102,9 @@
         <v>95</v>
       </c>
       <c r="B1539" s="87"/>
-      <c r="C1539" s="173"/>
-      <c r="D1539" s="174"/>
-      <c r="E1539" s="174"/>
+      <c r="C1539" s="171"/>
+      <c r="D1539" s="172"/>
+      <c r="E1539" s="172"/>
     </row>
     <row r="1540" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1540" s="74">
@@ -19255,9 +19255,9 @@
         <v>115</v>
       </c>
       <c r="B1556" s="87"/>
-      <c r="C1556" s="173"/>
-      <c r="D1556" s="174"/>
-      <c r="E1556" s="174"/>
+      <c r="C1556" s="171"/>
+      <c r="D1556" s="172"/>
+      <c r="E1556" s="172"/>
     </row>
     <row r="1557" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1557" s="74">
@@ -19408,9 +19408,9 @@
         <v>116</v>
       </c>
       <c r="B1573" s="87"/>
-      <c r="C1573" s="173"/>
-      <c r="D1573" s="174"/>
-      <c r="E1573" s="174"/>
+      <c r="C1573" s="171"/>
+      <c r="D1573" s="172"/>
+      <c r="E1573" s="172"/>
     </row>
     <row r="1574" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1574" s="74">
@@ -19561,9 +19561,9 @@
         <v>117</v>
       </c>
       <c r="B1590" s="87"/>
-      <c r="C1590" s="173"/>
-      <c r="D1590" s="174"/>
-      <c r="E1590" s="174"/>
+      <c r="C1590" s="171"/>
+      <c r="D1590" s="172"/>
+      <c r="E1590" s="172"/>
     </row>
     <row r="1591" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1591" s="74">
@@ -19714,9 +19714,9 @@
         <v>118</v>
       </c>
       <c r="B1607" s="87"/>
-      <c r="C1607" s="173"/>
-      <c r="D1607" s="174"/>
-      <c r="E1607" s="174"/>
+      <c r="C1607" s="171"/>
+      <c r="D1607" s="172"/>
+      <c r="E1607" s="172"/>
     </row>
     <row r="1608" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1608" s="74">
@@ -19867,9 +19867,9 @@
         <v>119</v>
       </c>
       <c r="B1624" s="87"/>
-      <c r="C1624" s="173"/>
-      <c r="D1624" s="174"/>
-      <c r="E1624" s="174"/>
+      <c r="C1624" s="171"/>
+      <c r="D1624" s="172"/>
+      <c r="E1624" s="172"/>
     </row>
     <row r="1625" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1625" s="74">
@@ -20020,18 +20020,18 @@
         <v>120</v>
       </c>
       <c r="B1641" s="42"/>
-      <c r="C1641" s="187"/>
-      <c r="D1641" s="188"/>
-      <c r="E1641" s="188"/>
+      <c r="C1641" s="177"/>
+      <c r="D1641" s="178"/>
+      <c r="E1641" s="178"/>
     </row>
     <row r="1642" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A1642" s="78" t="s">
         <v>121</v>
       </c>
       <c r="B1642" s="87"/>
-      <c r="C1642" s="173"/>
-      <c r="D1642" s="174"/>
-      <c r="E1642" s="174"/>
+      <c r="C1642" s="171"/>
+      <c r="D1642" s="172"/>
+      <c r="E1642" s="172"/>
     </row>
     <row r="1643" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1643" s="79">
@@ -20182,9 +20182,9 @@
         <v>122</v>
       </c>
       <c r="B1659" s="90"/>
-      <c r="C1659" s="175"/>
-      <c r="D1659" s="176"/>
-      <c r="E1659" s="176"/>
+      <c r="C1659" s="173"/>
+      <c r="D1659" s="174"/>
+      <c r="E1659" s="174"/>
     </row>
     <row r="1660" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1660" s="79">
@@ -20335,9 +20335,9 @@
         <v>123</v>
       </c>
       <c r="B1676" s="87"/>
-      <c r="C1676" s="173"/>
-      <c r="D1676" s="174"/>
-      <c r="E1676" s="174"/>
+      <c r="C1676" s="171"/>
+      <c r="D1676" s="172"/>
+      <c r="E1676" s="172"/>
     </row>
     <row r="1677" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1677" s="79">
@@ -20488,9 +20488,9 @@
         <v>124</v>
       </c>
       <c r="B1693" s="87"/>
-      <c r="C1693" s="173"/>
-      <c r="D1693" s="174"/>
-      <c r="E1693" s="174"/>
+      <c r="C1693" s="171"/>
+      <c r="D1693" s="172"/>
+      <c r="E1693" s="172"/>
     </row>
     <row r="1694" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1694" s="79">
@@ -20641,9 +20641,9 @@
         <v>125</v>
       </c>
       <c r="B1710" s="87"/>
-      <c r="C1710" s="173"/>
-      <c r="D1710" s="174"/>
-      <c r="E1710" s="174"/>
+      <c r="C1710" s="171"/>
+      <c r="D1710" s="172"/>
+      <c r="E1710" s="172"/>
     </row>
     <row r="1711" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1711" s="79">
@@ -20794,9 +20794,9 @@
         <v>126</v>
       </c>
       <c r="B1727" s="87"/>
-      <c r="C1727" s="173"/>
-      <c r="D1727" s="174"/>
-      <c r="E1727" s="174"/>
+      <c r="C1727" s="171"/>
+      <c r="D1727" s="172"/>
+      <c r="E1727" s="172"/>
     </row>
     <row r="1728" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1728" s="79">
@@ -20947,9 +20947,9 @@
         <v>127</v>
       </c>
       <c r="B1744" s="87"/>
-      <c r="C1744" s="173"/>
-      <c r="D1744" s="174"/>
-      <c r="E1744" s="174"/>
+      <c r="C1744" s="171"/>
+      <c r="D1744" s="172"/>
+      <c r="E1744" s="172"/>
     </row>
     <row r="1745" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1745" s="79">
@@ -21100,9 +21100,9 @@
         <v>128</v>
       </c>
       <c r="B1761" s="87"/>
-      <c r="C1761" s="173"/>
-      <c r="D1761" s="174"/>
-      <c r="E1761" s="174"/>
+      <c r="C1761" s="171"/>
+      <c r="D1761" s="172"/>
+      <c r="E1761" s="172"/>
     </row>
     <row r="1762" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1762" s="79">
@@ -21253,9 +21253,9 @@
         <v>129</v>
       </c>
       <c r="B1778" s="87"/>
-      <c r="C1778" s="173"/>
-      <c r="D1778" s="174"/>
-      <c r="E1778" s="174"/>
+      <c r="C1778" s="171"/>
+      <c r="D1778" s="172"/>
+      <c r="E1778" s="172"/>
     </row>
     <row r="1779" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1779" s="79">
@@ -21406,9 +21406,9 @@
         <v>130</v>
       </c>
       <c r="B1795" s="87"/>
-      <c r="C1795" s="173"/>
-      <c r="D1795" s="174"/>
-      <c r="E1795" s="174"/>
+      <c r="C1795" s="171"/>
+      <c r="D1795" s="172"/>
+      <c r="E1795" s="172"/>
     </row>
     <row r="1796" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1796" s="79">
@@ -21559,9 +21559,9 @@
         <v>131</v>
       </c>
       <c r="B1812" s="87"/>
-      <c r="C1812" s="173"/>
-      <c r="D1812" s="174"/>
-      <c r="E1812" s="174"/>
+      <c r="C1812" s="171"/>
+      <c r="D1812" s="172"/>
+      <c r="E1812" s="172"/>
     </row>
     <row r="1813" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1813" s="79">
@@ -21712,9 +21712,9 @@
         <v>96</v>
       </c>
       <c r="B1829" s="87"/>
-      <c r="C1829" s="173"/>
-      <c r="D1829" s="174"/>
-      <c r="E1829" s="174"/>
+      <c r="C1829" s="171"/>
+      <c r="D1829" s="172"/>
+      <c r="E1829" s="172"/>
     </row>
     <row r="1830" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1830" s="79">
@@ -21865,9 +21865,9 @@
         <v>132</v>
       </c>
       <c r="B1846" s="87"/>
-      <c r="C1846" s="173"/>
-      <c r="D1846" s="174"/>
-      <c r="E1846" s="174"/>
+      <c r="C1846" s="171"/>
+      <c r="D1846" s="172"/>
+      <c r="E1846" s="172"/>
     </row>
     <row r="1847" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1847" s="79">
@@ -22018,9 +22018,9 @@
         <v>133</v>
       </c>
       <c r="B1863" s="87"/>
-      <c r="C1863" s="173"/>
-      <c r="D1863" s="174"/>
-      <c r="E1863" s="174"/>
+      <c r="C1863" s="171"/>
+      <c r="D1863" s="172"/>
+      <c r="E1863" s="172"/>
     </row>
     <row r="1864" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1864" s="79">
@@ -22171,9 +22171,9 @@
         <v>134</v>
       </c>
       <c r="B1880" s="87"/>
-      <c r="C1880" s="173"/>
-      <c r="D1880" s="174"/>
-      <c r="E1880" s="174"/>
+      <c r="C1880" s="171"/>
+      <c r="D1880" s="172"/>
+      <c r="E1880" s="172"/>
     </row>
     <row r="1881" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1881" s="79">
@@ -22324,9 +22324,9 @@
         <v>135</v>
       </c>
       <c r="B1897" s="87"/>
-      <c r="C1897" s="173"/>
-      <c r="D1897" s="174"/>
-      <c r="E1897" s="174"/>
+      <c r="C1897" s="171"/>
+      <c r="D1897" s="172"/>
+      <c r="E1897" s="172"/>
     </row>
     <row r="1898" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1898" s="79">
@@ -22477,18 +22477,18 @@
         <v>136</v>
       </c>
       <c r="B1914" s="43"/>
-      <c r="C1914" s="189"/>
-      <c r="D1914" s="190"/>
-      <c r="E1914" s="190"/>
+      <c r="C1914" s="175"/>
+      <c r="D1914" s="176"/>
+      <c r="E1914" s="176"/>
     </row>
     <row r="1915" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A1915" s="83" t="s">
         <v>137</v>
       </c>
       <c r="B1915" s="87"/>
-      <c r="C1915" s="173"/>
-      <c r="D1915" s="174"/>
-      <c r="E1915" s="174"/>
+      <c r="C1915" s="171"/>
+      <c r="D1915" s="172"/>
+      <c r="E1915" s="172"/>
     </row>
     <row r="1916" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1916" s="84">
@@ -22639,9 +22639,9 @@
         <v>138</v>
       </c>
       <c r="B1932" s="90"/>
-      <c r="C1932" s="175"/>
-      <c r="D1932" s="176"/>
-      <c r="E1932" s="176"/>
+      <c r="C1932" s="173"/>
+      <c r="D1932" s="174"/>
+      <c r="E1932" s="174"/>
     </row>
     <row r="1933" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1933" s="84">
@@ -22792,9 +22792,9 @@
         <v>139</v>
       </c>
       <c r="B1949" s="87"/>
-      <c r="C1949" s="173"/>
-      <c r="D1949" s="174"/>
-      <c r="E1949" s="174"/>
+      <c r="C1949" s="171"/>
+      <c r="D1949" s="172"/>
+      <c r="E1949" s="172"/>
     </row>
     <row r="1950" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1950" s="84">
@@ -22945,9 +22945,9 @@
         <v>140</v>
       </c>
       <c r="B1966" s="87"/>
-      <c r="C1966" s="173"/>
-      <c r="D1966" s="174"/>
-      <c r="E1966" s="174"/>
+      <c r="C1966" s="171"/>
+      <c r="D1966" s="172"/>
+      <c r="E1966" s="172"/>
     </row>
     <row r="1967" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1967" s="84">
@@ -23098,9 +23098,9 @@
         <v>141</v>
       </c>
       <c r="B1983" s="87"/>
-      <c r="C1983" s="173"/>
-      <c r="D1983" s="174"/>
-      <c r="E1983" s="174"/>
+      <c r="C1983" s="171"/>
+      <c r="D1983" s="172"/>
+      <c r="E1983" s="172"/>
     </row>
     <row r="1984" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1984" s="84">
@@ -23251,9 +23251,9 @@
         <v>142</v>
       </c>
       <c r="B2000" s="87"/>
-      <c r="C2000" s="173"/>
-      <c r="D2000" s="174"/>
-      <c r="E2000" s="174"/>
+      <c r="C2000" s="171"/>
+      <c r="D2000" s="172"/>
+      <c r="E2000" s="172"/>
     </row>
     <row r="2001" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2001" s="84">
@@ -23404,9 +23404,9 @@
         <v>143</v>
       </c>
       <c r="B2017" s="87"/>
-      <c r="C2017" s="173"/>
-      <c r="D2017" s="174"/>
-      <c r="E2017" s="174"/>
+      <c r="C2017" s="171"/>
+      <c r="D2017" s="172"/>
+      <c r="E2017" s="172"/>
     </row>
     <row r="2018" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2018" s="84">
@@ -23557,9 +23557,9 @@
         <v>144</v>
       </c>
       <c r="B2034" s="87"/>
-      <c r="C2034" s="173"/>
-      <c r="D2034" s="174"/>
-      <c r="E2034" s="174"/>
+      <c r="C2034" s="171"/>
+      <c r="D2034" s="172"/>
+      <c r="E2034" s="172"/>
     </row>
     <row r="2035" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2035" s="84">
@@ -23710,9 +23710,9 @@
         <v>145</v>
       </c>
       <c r="B2051" s="87"/>
-      <c r="C2051" s="173"/>
-      <c r="D2051" s="174"/>
-      <c r="E2051" s="174"/>
+      <c r="C2051" s="171"/>
+      <c r="D2051" s="172"/>
+      <c r="E2051" s="172"/>
     </row>
     <row r="2052" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2052" s="84">
@@ -23863,9 +23863,9 @@
         <v>146</v>
       </c>
       <c r="B2068" s="87"/>
-      <c r="C2068" s="173"/>
-      <c r="D2068" s="174"/>
-      <c r="E2068" s="174"/>
+      <c r="C2068" s="171"/>
+      <c r="D2068" s="172"/>
+      <c r="E2068" s="172"/>
     </row>
     <row r="2069" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2069" s="84">
@@ -24016,9 +24016,9 @@
         <v>147</v>
       </c>
       <c r="B2085" s="87"/>
-      <c r="C2085" s="173"/>
-      <c r="D2085" s="174"/>
-      <c r="E2085" s="174"/>
+      <c r="C2085" s="171"/>
+      <c r="D2085" s="172"/>
+      <c r="E2085" s="172"/>
     </row>
     <row r="2086" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2086" s="84">
@@ -24169,9 +24169,9 @@
         <v>148</v>
       </c>
       <c r="B2102" s="87"/>
-      <c r="C2102" s="173"/>
-      <c r="D2102" s="174"/>
-      <c r="E2102" s="174"/>
+      <c r="C2102" s="171"/>
+      <c r="D2102" s="172"/>
+      <c r="E2102" s="172"/>
     </row>
     <row r="2103" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2103" s="84">
@@ -24322,9 +24322,9 @@
         <v>97</v>
       </c>
       <c r="B2119" s="87"/>
-      <c r="C2119" s="173"/>
-      <c r="D2119" s="174"/>
-      <c r="E2119" s="174"/>
+      <c r="C2119" s="171"/>
+      <c r="D2119" s="172"/>
+      <c r="E2119" s="172"/>
     </row>
     <row r="2120" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2120" s="84">
@@ -24475,9 +24475,9 @@
         <v>149</v>
       </c>
       <c r="B2136" s="87"/>
-      <c r="C2136" s="173"/>
-      <c r="D2136" s="174"/>
-      <c r="E2136" s="174"/>
+      <c r="C2136" s="171"/>
+      <c r="D2136" s="172"/>
+      <c r="E2136" s="172"/>
     </row>
     <row r="2137" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2137" s="84">
@@ -24628,9 +24628,9 @@
         <v>150</v>
       </c>
       <c r="B2153" s="87"/>
-      <c r="C2153" s="173"/>
-      <c r="D2153" s="174"/>
-      <c r="E2153" s="174"/>
+      <c r="C2153" s="171"/>
+      <c r="D2153" s="172"/>
+      <c r="E2153" s="172"/>
     </row>
     <row r="2154" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2154" s="84">
@@ -24781,9 +24781,9 @@
         <v>151</v>
       </c>
       <c r="B2170" s="87"/>
-      <c r="C2170" s="173"/>
-      <c r="D2170" s="174"/>
-      <c r="E2170" s="174"/>
+      <c r="C2170" s="171"/>
+      <c r="D2170" s="172"/>
+      <c r="E2170" s="172"/>
     </row>
     <row r="2171" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2171" s="84">
@@ -24931,15 +24931,122 @@
     </row>
   </sheetData>
   <mergeCells count="137">
-    <mergeCell ref="C2034:E2034"/>
-    <mergeCell ref="C2051:E2051"/>
-    <mergeCell ref="C2068:E2068"/>
-    <mergeCell ref="C2085:E2085"/>
-    <mergeCell ref="C2170:E2170"/>
-    <mergeCell ref="C2102:E2102"/>
-    <mergeCell ref="C2119:E2119"/>
-    <mergeCell ref="C2136:E2136"/>
-    <mergeCell ref="C2153:E2153"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="C89:E89"/>
+    <mergeCell ref="C21:E21"/>
+    <mergeCell ref="C38:E38"/>
+    <mergeCell ref="C55:E55"/>
+    <mergeCell ref="C72:E72"/>
+    <mergeCell ref="C208:E208"/>
+    <mergeCell ref="C225:E225"/>
+    <mergeCell ref="C242:E242"/>
+    <mergeCell ref="C259:E259"/>
+    <mergeCell ref="C276:E276"/>
+    <mergeCell ref="C277:E277"/>
+    <mergeCell ref="C106:E106"/>
+    <mergeCell ref="C123:E123"/>
+    <mergeCell ref="C140:E140"/>
+    <mergeCell ref="C157:E157"/>
+    <mergeCell ref="C174:E174"/>
+    <mergeCell ref="C191:E191"/>
+    <mergeCell ref="C396:E396"/>
+    <mergeCell ref="C413:E413"/>
+    <mergeCell ref="C430:E430"/>
+    <mergeCell ref="C447:E447"/>
+    <mergeCell ref="C464:E464"/>
+    <mergeCell ref="C481:E481"/>
+    <mergeCell ref="C294:E294"/>
+    <mergeCell ref="C311:E311"/>
+    <mergeCell ref="C328:E328"/>
+    <mergeCell ref="C345:E345"/>
+    <mergeCell ref="C362:E362"/>
+    <mergeCell ref="C379:E379"/>
+    <mergeCell ref="C584:E584"/>
+    <mergeCell ref="C601:E601"/>
+    <mergeCell ref="C618:E618"/>
+    <mergeCell ref="C635:E635"/>
+    <mergeCell ref="C652:E652"/>
+    <mergeCell ref="C669:E669"/>
+    <mergeCell ref="C498:E498"/>
+    <mergeCell ref="C515:E515"/>
+    <mergeCell ref="C532:E532"/>
+    <mergeCell ref="C549:E549"/>
+    <mergeCell ref="C550:E550"/>
+    <mergeCell ref="C567:E567"/>
+    <mergeCell ref="C788:E788"/>
+    <mergeCell ref="C805:E805"/>
+    <mergeCell ref="C822:E822"/>
+    <mergeCell ref="C823:E823"/>
+    <mergeCell ref="C840:E840"/>
+    <mergeCell ref="C857:E857"/>
+    <mergeCell ref="C686:E686"/>
+    <mergeCell ref="C703:E703"/>
+    <mergeCell ref="C720:E720"/>
+    <mergeCell ref="C737:E737"/>
+    <mergeCell ref="C754:E754"/>
+    <mergeCell ref="C771:E771"/>
+    <mergeCell ref="C976:E976"/>
+    <mergeCell ref="C993:E993"/>
+    <mergeCell ref="C1010:E1010"/>
+    <mergeCell ref="C1027:E1027"/>
+    <mergeCell ref="C1044:E1044"/>
+    <mergeCell ref="C1061:E1061"/>
+    <mergeCell ref="C874:E874"/>
+    <mergeCell ref="C891:E891"/>
+    <mergeCell ref="C908:E908"/>
+    <mergeCell ref="C925:E925"/>
+    <mergeCell ref="C942:E942"/>
+    <mergeCell ref="C959:E959"/>
+    <mergeCell ref="C1164:E1164"/>
+    <mergeCell ref="C1181:E1181"/>
+    <mergeCell ref="C1198:E1198"/>
+    <mergeCell ref="C1215:E1215"/>
+    <mergeCell ref="C1232:E1232"/>
+    <mergeCell ref="C1249:E1249"/>
+    <mergeCell ref="C1078:E1078"/>
+    <mergeCell ref="C1095:E1095"/>
+    <mergeCell ref="C1096:E1096"/>
+    <mergeCell ref="C1113:E1113"/>
+    <mergeCell ref="C1130:E1130"/>
+    <mergeCell ref="C1147:E1147"/>
+    <mergeCell ref="C1368:E1368"/>
+    <mergeCell ref="C1369:E1369"/>
+    <mergeCell ref="C1386:E1386"/>
+    <mergeCell ref="C1403:E1403"/>
+    <mergeCell ref="C1420:E1420"/>
+    <mergeCell ref="C1437:E1437"/>
+    <mergeCell ref="C1266:E1266"/>
+    <mergeCell ref="C1283:E1283"/>
+    <mergeCell ref="C1300:E1300"/>
+    <mergeCell ref="C1317:E1317"/>
+    <mergeCell ref="C1334:E1334"/>
+    <mergeCell ref="C1351:E1351"/>
+    <mergeCell ref="C1556:E1556"/>
+    <mergeCell ref="C1573:E1573"/>
+    <mergeCell ref="C1590:E1590"/>
+    <mergeCell ref="C1607:E1607"/>
+    <mergeCell ref="C1624:E1624"/>
+    <mergeCell ref="C1641:E1641"/>
+    <mergeCell ref="C1454:E1454"/>
+    <mergeCell ref="C1471:E1471"/>
+    <mergeCell ref="C1488:E1488"/>
+    <mergeCell ref="C1505:E1505"/>
+    <mergeCell ref="C1522:E1522"/>
+    <mergeCell ref="C1539:E1539"/>
+    <mergeCell ref="C1744:E1744"/>
+    <mergeCell ref="C1761:E1761"/>
+    <mergeCell ref="C1778:E1778"/>
+    <mergeCell ref="C1795:E1795"/>
+    <mergeCell ref="C1812:E1812"/>
+    <mergeCell ref="C1829:E1829"/>
+    <mergeCell ref="C1642:E1642"/>
+    <mergeCell ref="C1659:E1659"/>
+    <mergeCell ref="C1676:E1676"/>
+    <mergeCell ref="C1693:E1693"/>
+    <mergeCell ref="C1710:E1710"/>
+    <mergeCell ref="C1727:E1727"/>
     <mergeCell ref="C1932:E1932"/>
     <mergeCell ref="C1949:E1949"/>
     <mergeCell ref="C1966:E1966"/>
@@ -24952,122 +25059,15 @@
     <mergeCell ref="C1897:E1897"/>
     <mergeCell ref="C1914:E1914"/>
     <mergeCell ref="C1915:E1915"/>
-    <mergeCell ref="C1744:E1744"/>
-    <mergeCell ref="C1761:E1761"/>
-    <mergeCell ref="C1778:E1778"/>
-    <mergeCell ref="C1795:E1795"/>
-    <mergeCell ref="C1812:E1812"/>
-    <mergeCell ref="C1829:E1829"/>
-    <mergeCell ref="C1642:E1642"/>
-    <mergeCell ref="C1659:E1659"/>
-    <mergeCell ref="C1676:E1676"/>
-    <mergeCell ref="C1693:E1693"/>
-    <mergeCell ref="C1710:E1710"/>
-    <mergeCell ref="C1727:E1727"/>
-    <mergeCell ref="C1556:E1556"/>
-    <mergeCell ref="C1573:E1573"/>
-    <mergeCell ref="C1590:E1590"/>
-    <mergeCell ref="C1607:E1607"/>
-    <mergeCell ref="C1624:E1624"/>
-    <mergeCell ref="C1641:E1641"/>
-    <mergeCell ref="C1454:E1454"/>
-    <mergeCell ref="C1471:E1471"/>
-    <mergeCell ref="C1488:E1488"/>
-    <mergeCell ref="C1505:E1505"/>
-    <mergeCell ref="C1522:E1522"/>
-    <mergeCell ref="C1539:E1539"/>
-    <mergeCell ref="C1368:E1368"/>
-    <mergeCell ref="C1369:E1369"/>
-    <mergeCell ref="C1386:E1386"/>
-    <mergeCell ref="C1403:E1403"/>
-    <mergeCell ref="C1420:E1420"/>
-    <mergeCell ref="C1437:E1437"/>
-    <mergeCell ref="C1266:E1266"/>
-    <mergeCell ref="C1283:E1283"/>
-    <mergeCell ref="C1300:E1300"/>
-    <mergeCell ref="C1317:E1317"/>
-    <mergeCell ref="C1334:E1334"/>
-    <mergeCell ref="C1351:E1351"/>
-    <mergeCell ref="C1164:E1164"/>
-    <mergeCell ref="C1181:E1181"/>
-    <mergeCell ref="C1198:E1198"/>
-    <mergeCell ref="C1215:E1215"/>
-    <mergeCell ref="C1232:E1232"/>
-    <mergeCell ref="C1249:E1249"/>
-    <mergeCell ref="C1078:E1078"/>
-    <mergeCell ref="C1095:E1095"/>
-    <mergeCell ref="C1096:E1096"/>
-    <mergeCell ref="C1113:E1113"/>
-    <mergeCell ref="C1130:E1130"/>
-    <mergeCell ref="C1147:E1147"/>
-    <mergeCell ref="C976:E976"/>
-    <mergeCell ref="C993:E993"/>
-    <mergeCell ref="C1010:E1010"/>
-    <mergeCell ref="C1027:E1027"/>
-    <mergeCell ref="C1044:E1044"/>
-    <mergeCell ref="C1061:E1061"/>
-    <mergeCell ref="C874:E874"/>
-    <mergeCell ref="C891:E891"/>
-    <mergeCell ref="C908:E908"/>
-    <mergeCell ref="C925:E925"/>
-    <mergeCell ref="C942:E942"/>
-    <mergeCell ref="C959:E959"/>
-    <mergeCell ref="C788:E788"/>
-    <mergeCell ref="C805:E805"/>
-    <mergeCell ref="C822:E822"/>
-    <mergeCell ref="C823:E823"/>
-    <mergeCell ref="C840:E840"/>
-    <mergeCell ref="C857:E857"/>
-    <mergeCell ref="C686:E686"/>
-    <mergeCell ref="C703:E703"/>
-    <mergeCell ref="C720:E720"/>
-    <mergeCell ref="C737:E737"/>
-    <mergeCell ref="C754:E754"/>
-    <mergeCell ref="C771:E771"/>
-    <mergeCell ref="C584:E584"/>
-    <mergeCell ref="C601:E601"/>
-    <mergeCell ref="C618:E618"/>
-    <mergeCell ref="C635:E635"/>
-    <mergeCell ref="C652:E652"/>
-    <mergeCell ref="C669:E669"/>
-    <mergeCell ref="C498:E498"/>
-    <mergeCell ref="C515:E515"/>
-    <mergeCell ref="C532:E532"/>
-    <mergeCell ref="C549:E549"/>
-    <mergeCell ref="C550:E550"/>
-    <mergeCell ref="C567:E567"/>
-    <mergeCell ref="C396:E396"/>
-    <mergeCell ref="C413:E413"/>
-    <mergeCell ref="C430:E430"/>
-    <mergeCell ref="C447:E447"/>
-    <mergeCell ref="C464:E464"/>
-    <mergeCell ref="C481:E481"/>
-    <mergeCell ref="C294:E294"/>
-    <mergeCell ref="C311:E311"/>
-    <mergeCell ref="C328:E328"/>
-    <mergeCell ref="C345:E345"/>
-    <mergeCell ref="C362:E362"/>
-    <mergeCell ref="C379:E379"/>
-    <mergeCell ref="C225:E225"/>
-    <mergeCell ref="C242:E242"/>
-    <mergeCell ref="C259:E259"/>
-    <mergeCell ref="C276:E276"/>
-    <mergeCell ref="C277:E277"/>
-    <mergeCell ref="C106:E106"/>
-    <mergeCell ref="C123:E123"/>
-    <mergeCell ref="C140:E140"/>
-    <mergeCell ref="C157:E157"/>
-    <mergeCell ref="C174:E174"/>
-    <mergeCell ref="C191:E191"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="C89:E89"/>
-    <mergeCell ref="C21:E21"/>
-    <mergeCell ref="C38:E38"/>
-    <mergeCell ref="C55:E55"/>
-    <mergeCell ref="C72:E72"/>
-    <mergeCell ref="C208:E208"/>
+    <mergeCell ref="C2034:E2034"/>
+    <mergeCell ref="C2051:E2051"/>
+    <mergeCell ref="C2068:E2068"/>
+    <mergeCell ref="C2085:E2085"/>
+    <mergeCell ref="C2170:E2170"/>
+    <mergeCell ref="C2102:E2102"/>
+    <mergeCell ref="C2119:E2119"/>
+    <mergeCell ref="C2136:E2136"/>
+    <mergeCell ref="C2153:E2153"/>
   </mergeCells>
   <phoneticPr fontId="12" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -25094,51 +25094,51 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="24" thickBot="1">
-      <c r="A1" s="197" t="s">
+      <c r="A1" s="198" t="s">
         <v>156</v>
       </c>
-      <c r="B1" s="197"/>
-      <c r="C1" s="197"/>
-      <c r="D1" s="197"/>
-      <c r="E1" s="197"/>
-      <c r="F1" s="197"/>
-      <c r="G1" s="197"/>
-      <c r="H1" s="197"/>
-      <c r="I1" s="197"/>
-      <c r="J1" s="197"/>
-      <c r="K1" s="197"/>
-      <c r="L1" s="197"/>
+      <c r="B1" s="198"/>
+      <c r="C1" s="198"/>
+      <c r="D1" s="198"/>
+      <c r="E1" s="198"/>
+      <c r="F1" s="198"/>
+      <c r="G1" s="198"/>
+      <c r="H1" s="198"/>
+      <c r="I1" s="198"/>
+      <c r="J1" s="198"/>
+      <c r="K1" s="198"/>
+      <c r="L1" s="198"/>
     </row>
     <row r="2" spans="1:12" ht="18.75" thickBot="1">
-      <c r="A2" s="194" t="s">
+      <c r="A2" s="195" t="s">
         <v>157</v>
       </c>
-      <c r="B2" s="195"/>
-      <c r="C2" s="195"/>
-      <c r="D2" s="195"/>
-      <c r="E2" s="195"/>
-      <c r="F2" s="195"/>
-      <c r="G2" s="195"/>
-      <c r="H2" s="195"/>
-      <c r="I2" s="195"/>
-      <c r="J2" s="195"/>
-      <c r="K2" s="195"/>
-      <c r="L2" s="196"/>
+      <c r="B2" s="196"/>
+      <c r="C2" s="196"/>
+      <c r="D2" s="196"/>
+      <c r="E2" s="196"/>
+      <c r="F2" s="196"/>
+      <c r="G2" s="196"/>
+      <c r="H2" s="196"/>
+      <c r="I2" s="196"/>
+      <c r="J2" s="196"/>
+      <c r="K2" s="196"/>
+      <c r="L2" s="197"/>
     </row>
     <row r="3" spans="1:12" s="31" customFormat="1" ht="16.5" customHeight="1" thickBot="1">
-      <c r="A3" s="191" t="s">
+      <c r="A3" s="192" t="s">
         <v>158</v>
       </c>
-      <c r="B3" s="192"/>
-      <c r="C3" s="192"/>
-      <c r="D3" s="192"/>
-      <c r="E3" s="192"/>
-      <c r="F3" s="192"/>
-      <c r="G3" s="192"/>
-      <c r="H3" s="192"/>
-      <c r="I3" s="192"/>
-      <c r="J3" s="192"/>
-      <c r="K3" s="193"/>
+      <c r="B3" s="193"/>
+      <c r="C3" s="193"/>
+      <c r="D3" s="193"/>
+      <c r="E3" s="193"/>
+      <c r="F3" s="193"/>
+      <c r="G3" s="193"/>
+      <c r="H3" s="193"/>
+      <c r="I3" s="193"/>
+      <c r="J3" s="193"/>
+      <c r="K3" s="194"/>
     </row>
     <row r="4" spans="1:12" s="27" customFormat="1">
       <c r="A4" s="28" t="s">
@@ -25355,19 +25355,19 @@
       <c r="K19" s="2"/>
     </row>
     <row r="20" spans="1:11" ht="18" customHeight="1" thickBot="1">
-      <c r="A20" s="191" t="s">
+      <c r="A20" s="192" t="s">
         <v>166</v>
       </c>
-      <c r="B20" s="192"/>
-      <c r="C20" s="192"/>
-      <c r="D20" s="192"/>
-      <c r="E20" s="192"/>
-      <c r="F20" s="192"/>
-      <c r="G20" s="192"/>
-      <c r="H20" s="192"/>
-      <c r="I20" s="192"/>
-      <c r="J20" s="192"/>
-      <c r="K20" s="193"/>
+      <c r="B20" s="193"/>
+      <c r="C20" s="193"/>
+      <c r="D20" s="193"/>
+      <c r="E20" s="193"/>
+      <c r="F20" s="193"/>
+      <c r="G20" s="193"/>
+      <c r="H20" s="193"/>
+      <c r="I20" s="193"/>
+      <c r="J20" s="193"/>
+      <c r="K20" s="194"/>
     </row>
     <row r="21" spans="1:11">
       <c r="A21" s="28" t="s">
@@ -25584,19 +25584,19 @@
       <c r="K36" s="2"/>
     </row>
     <row r="37" spans="1:11" ht="18" customHeight="1" thickBot="1">
-      <c r="A37" s="191" t="s">
+      <c r="A37" s="192" t="s">
         <v>167</v>
       </c>
-      <c r="B37" s="192"/>
-      <c r="C37" s="192"/>
-      <c r="D37" s="192"/>
-      <c r="E37" s="192"/>
-      <c r="F37" s="192"/>
-      <c r="G37" s="192"/>
-      <c r="H37" s="192"/>
-      <c r="I37" s="192"/>
-      <c r="J37" s="192"/>
-      <c r="K37" s="193"/>
+      <c r="B37" s="193"/>
+      <c r="C37" s="193"/>
+      <c r="D37" s="193"/>
+      <c r="E37" s="193"/>
+      <c r="F37" s="193"/>
+      <c r="G37" s="193"/>
+      <c r="H37" s="193"/>
+      <c r="I37" s="193"/>
+      <c r="J37" s="193"/>
+      <c r="K37" s="194"/>
     </row>
     <row r="38" spans="1:11">
       <c r="A38" s="28" t="s">
@@ -25854,28 +25854,28 @@
       </c>
     </row>
     <row r="3" spans="1:1">
-      <c r="A3" s="198"/>
+      <c r="A3" s="199"/>
     </row>
     <row r="4" spans="1:1">
-      <c r="A4" s="199"/>
+      <c r="A4" s="200"/>
     </row>
     <row r="5" spans="1:1">
-      <c r="A5" s="199"/>
+      <c r="A5" s="200"/>
     </row>
     <row r="6" spans="1:1">
-      <c r="A6" s="199"/>
+      <c r="A6" s="200"/>
     </row>
     <row r="7" spans="1:1">
-      <c r="A7" s="199"/>
+      <c r="A7" s="200"/>
     </row>
     <row r="8" spans="1:1">
-      <c r="A8" s="199"/>
+      <c r="A8" s="200"/>
     </row>
     <row r="9" spans="1:1">
-      <c r="A9" s="199"/>
+      <c r="A9" s="200"/>
     </row>
     <row r="10" spans="1:1" ht="13.5" thickBot="1">
-      <c r="A10" s="200"/>
+      <c r="A10" s="201"/>
     </row>
     <row r="11" spans="1:1" ht="27" customHeight="1">
       <c r="A11" s="22" t="s">
@@ -26058,10 +26058,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="4" customFormat="1" ht="25.5" customHeight="1" thickBot="1">
-      <c r="B1" s="201" t="s">
+      <c r="B1" s="202" t="s">
         <v>162</v>
       </c>
-      <c r="C1" s="202"/>
+      <c r="C1" s="203"/>
       <c r="D1" s="92"/>
       <c r="E1" s="32"/>
     </row>
@@ -26072,7 +26072,7 @@
       <c r="E2" s="119"/>
     </row>
     <row r="3" spans="1:5" ht="12.75" customHeight="1">
-      <c r="A3" s="203" t="s">
+      <c r="A3" s="204" t="s">
         <v>202</v>
       </c>
       <c r="B3" s="131" t="s">
@@ -26086,7 +26086,7 @@
       <c r="E3" s="5"/>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="204"/>
+      <c r="A4" s="205"/>
       <c r="B4" s="128" t="s">
         <v>159</v>
       </c>
@@ -26098,7 +26098,7 @@
       <c r="E4" s="5"/>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="204"/>
+      <c r="A5" s="205"/>
       <c r="B5" s="128" t="s">
         <v>160</v>
       </c>
@@ -26107,7 +26107,7 @@
       <c r="E5" s="5"/>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="204"/>
+      <c r="A6" s="205"/>
       <c r="B6" s="139" t="s">
         <v>204</v>
       </c>
@@ -26119,7 +26119,7 @@
       <c r="E6" s="5"/>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="204"/>
+      <c r="A7" s="205"/>
       <c r="B7" s="128" t="s">
         <v>171</v>
       </c>
@@ -26131,7 +26131,7 @@
       <c r="E7" s="5"/>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="204"/>
+      <c r="A8" s="205"/>
       <c r="B8" s="128" t="s">
         <v>172</v>
       </c>
@@ -26140,7 +26140,7 @@
       <c r="E8" s="5"/>
     </row>
     <row r="9" spans="1:5" ht="13.5" thickBot="1">
-      <c r="A9" s="205"/>
+      <c r="A9" s="206"/>
       <c r="B9" s="136" t="s">
         <v>161</v>
       </c>
@@ -26155,7 +26155,7 @@
       <c r="E10" s="94"/>
     </row>
     <row r="11" spans="1:5" ht="19.5" customHeight="1">
-      <c r="A11" s="203" t="s">
+      <c r="A11" s="204" t="s">
         <v>203</v>
       </c>
       <c r="B11" s="131" t="s">
@@ -26169,7 +26169,7 @@
       <c r="E11" s="5"/>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="204"/>
+      <c r="A12" s="205"/>
       <c r="B12" s="128" t="s">
         <v>159</v>
       </c>
@@ -26181,7 +26181,7 @@
       <c r="E12" s="5"/>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" s="204"/>
+      <c r="A13" s="205"/>
       <c r="B13" s="128" t="s">
         <v>160</v>
       </c>
@@ -26190,7 +26190,7 @@
       <c r="E13" s="5"/>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="204"/>
+      <c r="A14" s="205"/>
       <c r="B14" s="139" t="s">
         <v>204</v>
       </c>
@@ -26202,7 +26202,7 @@
       <c r="E14" s="5"/>
     </row>
     <row r="15" spans="1:5">
-      <c r="A15" s="204"/>
+      <c r="A15" s="205"/>
       <c r="B15" s="128" t="s">
         <v>171</v>
       </c>
@@ -26214,7 +26214,7 @@
       <c r="E15" s="5"/>
     </row>
     <row r="16" spans="1:5">
-      <c r="A16" s="204"/>
+      <c r="A16" s="205"/>
       <c r="B16" s="128" t="s">
         <v>172</v>
       </c>
@@ -26223,7 +26223,7 @@
       <c r="E16" s="5"/>
     </row>
     <row r="17" spans="1:5" ht="13.5" thickBot="1">
-      <c r="A17" s="205"/>
+      <c r="A17" s="206"/>
       <c r="B17" s="136" t="s">
         <v>161</v>
       </c>
@@ -26238,7 +26238,7 @@
       <c r="E18" s="94"/>
     </row>
     <row r="19" spans="1:5" collapsed="1">
-      <c r="A19" s="203" t="s">
+      <c r="A19" s="204" t="s">
         <v>203</v>
       </c>
       <c r="B19" s="131" t="s">
@@ -26247,7 +26247,7 @@
       <c r="C19" s="130"/>
     </row>
     <row r="20" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A20" s="204"/>
+      <c r="A20" s="205"/>
       <c r="B20" s="128" t="s">
         <v>159</v>
       </c>
@@ -26257,14 +26257,14 @@
       </c>
     </row>
     <row r="21" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A21" s="204"/>
+      <c r="A21" s="205"/>
       <c r="B21" s="128" t="s">
         <v>160</v>
       </c>
       <c r="C21" s="133"/>
     </row>
     <row r="22" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A22" s="204"/>
+      <c r="A22" s="205"/>
       <c r="B22" s="139" t="s">
         <v>204</v>
       </c>
@@ -26274,7 +26274,7 @@
       </c>
     </row>
     <row r="23" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A23" s="204"/>
+      <c r="A23" s="205"/>
       <c r="B23" s="128" t="s">
         <v>171</v>
       </c>
@@ -26284,14 +26284,14 @@
       </c>
     </row>
     <row r="24" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A24" s="204"/>
+      <c r="A24" s="205"/>
       <c r="B24" s="128" t="s">
         <v>172</v>
       </c>
       <c r="C24" s="132"/>
     </row>
     <row r="25" spans="1:5" ht="13.5" thickBot="1">
-      <c r="A25" s="205"/>
+      <c r="A25" s="206"/>
       <c r="B25" s="136" t="s">
         <v>161</v>
       </c>
@@ -26335,17 +26335,17 @@
       <c r="E1" s="5"/>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="222" t="s">
+      <c r="A2" s="213" t="s">
         <v>183</v>
       </c>
-      <c r="B2" s="223"/>
+      <c r="B2" s="214"/>
       <c r="C2" s="120"/>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="224" t="s">
+      <c r="A3" s="215" t="s">
         <v>185</v>
       </c>
-      <c r="B3" s="223"/>
+      <c r="B3" s="214"/>
       <c r="C3" s="120"/>
     </row>
     <row r="4" spans="1:5">
@@ -26361,115 +26361,128 @@
       <c r="C5" s="120"/>
     </row>
     <row r="7" spans="1:5" ht="18.75">
-      <c r="A7" s="210" t="s">
+      <c r="A7" s="224" t="s">
         <v>186</v>
       </c>
-      <c r="B7" s="211"/>
+      <c r="B7" s="225"/>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="120"/>
       <c r="B8" s="9"/>
     </row>
     <row r="9" spans="1:5" ht="39" customHeight="1">
-      <c r="A9" s="212" t="s">
+      <c r="A9" s="222" t="s">
         <v>187</v>
       </c>
-      <c r="B9" s="213"/>
+      <c r="B9" s="223"/>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="214"/>
-      <c r="B10" s="215"/>
+      <c r="A10" s="209"/>
+      <c r="B10" s="210"/>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="206" t="s">
+      <c r="A11" s="211" t="s">
         <v>188</v>
       </c>
-      <c r="B11" s="207"/>
+      <c r="B11" s="212"/>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="206" t="s">
+      <c r="A12" s="211" t="s">
         <v>189</v>
       </c>
-      <c r="B12" s="207"/>
+      <c r="B12" s="212"/>
     </row>
     <row r="13" spans="1:5" ht="43.5" customHeight="1">
-      <c r="A13" s="206" t="s">
+      <c r="A13" s="211" t="s">
         <v>190</v>
       </c>
-      <c r="B13" s="207"/>
+      <c r="B13" s="212"/>
     </row>
     <row r="14" spans="1:5" ht="19.5" customHeight="1">
-      <c r="A14" s="206" t="s">
+      <c r="A14" s="211" t="s">
         <v>191</v>
       </c>
-      <c r="B14" s="207"/>
+      <c r="B14" s="212"/>
     </row>
     <row r="15" spans="1:5" ht="18" customHeight="1">
-      <c r="A15" s="206" t="s">
+      <c r="A15" s="211" t="s">
         <v>192</v>
       </c>
-      <c r="B15" s="207"/>
+      <c r="B15" s="212"/>
     </row>
     <row r="16" spans="1:5" ht="21" customHeight="1">
-      <c r="A16" s="206" t="s">
+      <c r="A16" s="211" t="s">
         <v>193</v>
       </c>
-      <c r="B16" s="207"/>
+      <c r="B16" s="212"/>
     </row>
     <row r="17" spans="1:2" ht="48.75" customHeight="1">
-      <c r="A17" s="208" t="s">
+      <c r="A17" s="207" t="s">
         <v>195</v>
       </c>
-      <c r="B17" s="209"/>
+      <c r="B17" s="208"/>
     </row>
     <row r="19" spans="1:2" ht="18.75">
-      <c r="A19" s="210" t="s">
+      <c r="A19" s="224" t="s">
         <v>197</v>
       </c>
-      <c r="B19" s="211"/>
+      <c r="B19" s="225"/>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="120"/>
       <c r="B20" s="9"/>
     </row>
     <row r="21" spans="1:2">
-      <c r="A21" s="212" t="s">
+      <c r="A21" s="222" t="s">
         <v>198</v>
       </c>
-      <c r="B21" s="213"/>
+      <c r="B21" s="223"/>
     </row>
     <row r="22" spans="1:2">
-      <c r="A22" s="214"/>
-      <c r="B22" s="215"/>
+      <c r="A22" s="209"/>
+      <c r="B22" s="210"/>
     </row>
     <row r="23" spans="1:2">
-      <c r="A23" s="206" t="s">
+      <c r="A23" s="211" t="s">
         <v>199</v>
       </c>
-      <c r="B23" s="207"/>
+      <c r="B23" s="212"/>
     </row>
     <row r="24" spans="1:2">
-      <c r="A24" s="206"/>
-      <c r="B24" s="207"/>
+      <c r="A24" s="211"/>
+      <c r="B24" s="212"/>
     </row>
     <row r="25" spans="1:2">
-      <c r="A25" s="206" t="s">
+      <c r="A25" s="211" t="s">
         <v>200</v>
       </c>
-      <c r="B25" s="207"/>
+      <c r="B25" s="212"/>
     </row>
     <row r="26" spans="1:2">
-      <c r="A26" s="206" t="s">
+      <c r="A26" s="211" t="s">
         <v>201</v>
       </c>
-      <c r="B26" s="207"/>
+      <c r="B26" s="212"/>
     </row>
     <row r="27" spans="1:2">
-      <c r="A27" s="208"/>
-      <c r="B27" s="209"/>
+      <c r="A27" s="207"/>
+      <c r="B27" s="208"/>
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A7:B7"/>
     <mergeCell ref="A17:B17"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
@@ -26480,19 +26493,6 @@
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="A14:B14"/>
     <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A24:B24"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A3" r:id="rId1"/>

</xml_diff>

<commit_message>
Tempo - Circus Stage 1 done.
</commit_message>
<xml_diff>
--- a/trunk/Tempo/Tempo.xlsx
+++ b/trunk/Tempo/Tempo.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1169" uniqueCount="278">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1168" uniqueCount="277">
   <si>
     <t>Notes</t>
   </si>
@@ -890,9 +890,6 @@
   </si>
   <si>
     <t>7th Hit</t>
-  </si>
-  <si>
-    <t>p</t>
   </si>
 </sst>
 </file>
@@ -2228,6 +2225,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="41" fillId="21" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -2250,29 +2251,29 @@
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="25" fillId="13" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="26" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="25" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="26" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="23" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="24" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="21" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="22" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="14" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="21" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="22" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="23" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="24" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="25" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="26" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="25" fillId="13" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="26" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="16" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="16" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="16" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -2308,20 +2309,34 @@
     <xf numFmtId="0" fontId="55" fillId="22" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="53" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="53" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="51" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="51" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="49" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="4"/>
     </xf>
@@ -2331,24 +2346,6 @@
     <xf numFmtId="0" fontId="50" fillId="0" borderId="33" xfId="3" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" indent="4"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="51" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="51" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="53" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="53" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="52" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Accent1" xfId="2" builtinId="29"/>
@@ -2660,7 +2657,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A87" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C95" sqref="C95"/>
+      <selection pane="bottomLeft" activeCell="C97" sqref="C97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" outlineLevelRow="2"/>
@@ -2676,16 +2673,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="33">
-      <c r="A1" s="166" t="s">
+      <c r="A1" s="168" t="s">
         <v>205</v>
       </c>
-      <c r="B1" s="165"/>
-      <c r="C1" s="167" t="s">
+      <c r="B1" s="167"/>
+      <c r="C1" s="169" t="s">
         <v>170</v>
       </c>
-      <c r="D1" s="167"/>
-      <c r="E1" s="167"/>
-      <c r="F1" s="168"/>
+      <c r="D1" s="169"/>
+      <c r="E1" s="169"/>
+      <c r="F1" s="170"/>
       <c r="G1" s="140"/>
       <c r="H1" s="141">
         <f>SUM(G1:G65549)</f>
@@ -2750,11 +2747,11 @@
       <c r="B4" s="146" t="s">
         <v>228</v>
       </c>
-      <c r="C4" s="164" t="s">
+      <c r="C4" s="166" t="s">
         <v>232</v>
       </c>
-      <c r="D4" s="164"/>
-      <c r="E4" s="170"/>
+      <c r="D4" s="166"/>
+      <c r="E4" s="172"/>
       <c r="F4" s="143"/>
       <c r="G4" s="140"/>
       <c r="H4" s="140"/>
@@ -2769,10 +2766,10 @@
       <c r="B5" s="147" t="s">
         <v>177</v>
       </c>
-      <c r="C5" s="164" t="s">
+      <c r="C5" s="166" t="s">
         <v>218</v>
       </c>
-      <c r="D5" s="164"/>
+      <c r="D5" s="166"/>
       <c r="E5" s="147"/>
       <c r="F5" s="147"/>
       <c r="G5" s="148" t="s">
@@ -2796,10 +2793,10 @@
       <c r="B6" s="147" t="s">
         <v>179</v>
       </c>
-      <c r="C6" s="164" t="s">
+      <c r="C6" s="166" t="s">
         <v>168</v>
       </c>
-      <c r="D6" s="165"/>
+      <c r="D6" s="167"/>
       <c r="E6" s="147"/>
       <c r="F6" s="143"/>
       <c r="G6" s="140"/>
@@ -2823,7 +2820,7 @@
       <c r="F7" s="93"/>
     </row>
     <row r="8" spans="1:11" ht="15" customHeight="1" outlineLevel="1">
-      <c r="A8" s="169" t="s">
+      <c r="A8" s="171" t="s">
         <v>180</v>
       </c>
       <c r="B8" s="95" t="s">
@@ -2843,7 +2840,7 @@
       </c>
     </row>
     <row r="9" spans="1:11" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="A9" s="162"/>
+      <c r="A9" s="164"/>
       <c r="B9" s="98" t="s">
         <v>177</v>
       </c>
@@ -2857,7 +2854,7 @@
       <c r="F9" s="104"/>
     </row>
     <row r="10" spans="1:11" ht="15.75" outlineLevel="1" thickTop="1">
-      <c r="A10" s="162"/>
+      <c r="A10" s="164"/>
       <c r="B10" s="149" t="s">
         <v>208</v>
       </c>
@@ -2874,7 +2871,7 @@
       <c r="F10" s="105"/>
     </row>
     <row r="11" spans="1:11" ht="15" outlineLevel="1">
-      <c r="A11" s="162"/>
+      <c r="A11" s="164"/>
       <c r="B11" s="149" t="s">
         <v>214</v>
       </c>
@@ -2891,7 +2888,7 @@
       <c r="F11" s="105"/>
     </row>
     <row r="12" spans="1:11" ht="15" outlineLevel="1">
-      <c r="A12" s="162"/>
+      <c r="A12" s="164"/>
       <c r="B12" s="149" t="s">
         <v>209</v>
       </c>
@@ -2908,7 +2905,7 @@
       <c r="F12" s="105"/>
     </row>
     <row r="13" spans="1:11" ht="15" outlineLevel="1">
-      <c r="A13" s="162"/>
+      <c r="A13" s="164"/>
       <c r="B13" s="149" t="s">
         <v>213</v>
       </c>
@@ -2925,7 +2922,7 @@
       <c r="F13" s="105"/>
     </row>
     <row r="14" spans="1:11" ht="15" outlineLevel="1">
-      <c r="A14" s="162"/>
+      <c r="A14" s="164"/>
       <c r="B14" s="149" t="s">
         <v>214</v>
       </c>
@@ -2942,7 +2939,7 @@
       <c r="F14" s="105"/>
     </row>
     <row r="15" spans="1:11" ht="15" outlineLevel="1">
-      <c r="A15" s="162"/>
+      <c r="A15" s="164"/>
       <c r="B15" s="149" t="s">
         <v>215</v>
       </c>
@@ -2959,7 +2956,7 @@
       <c r="F15" s="105"/>
     </row>
     <row r="16" spans="1:11" ht="15" outlineLevel="1">
-      <c r="A16" s="162"/>
+      <c r="A16" s="164"/>
       <c r="B16" s="149" t="s">
         <v>216</v>
       </c>
@@ -2976,7 +2973,7 @@
       <c r="F16" s="105"/>
     </row>
     <row r="17" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A17" s="162"/>
+      <c r="A17" s="164"/>
       <c r="B17" s="149" t="s">
         <v>217</v>
       </c>
@@ -2993,7 +2990,7 @@
       <c r="F17" s="105"/>
     </row>
     <row r="18" spans="1:8" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="A18" s="162"/>
+      <c r="A18" s="164"/>
       <c r="B18" s="98" t="s">
         <v>179</v>
       </c>
@@ -3036,7 +3033,7 @@
     </row>
     <row r="20" spans="1:8" ht="13.5" thickBot="1"/>
     <row r="21" spans="1:8" ht="15" customHeight="1" outlineLevel="1">
-      <c r="A21" s="163" t="s">
+      <c r="A21" s="165" t="s">
         <v>219</v>
       </c>
       <c r="B21" s="109" t="s">
@@ -3056,7 +3053,7 @@
       </c>
     </row>
     <row r="22" spans="1:8" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="A22" s="162"/>
+      <c r="A22" s="164"/>
       <c r="B22" s="98" t="s">
         <v>177</v>
       </c>
@@ -3073,7 +3070,7 @@
       <c r="F22" s="104"/>
     </row>
     <row r="23" spans="1:8" ht="15.75" outlineLevel="1" thickTop="1">
-      <c r="A23" s="162"/>
+      <c r="A23" s="164"/>
       <c r="B23" s="149" t="s">
         <v>175</v>
       </c>
@@ -3086,7 +3083,7 @@
       <c r="F23" s="105"/>
     </row>
     <row r="24" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A24" s="162"/>
+      <c r="A24" s="164"/>
       <c r="B24" s="149" t="s">
         <v>221</v>
       </c>
@@ -3106,7 +3103,7 @@
       </c>
     </row>
     <row r="25" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A25" s="162"/>
+      <c r="A25" s="164"/>
       <c r="B25" s="149"/>
       <c r="C25" s="101"/>
       <c r="D25" s="101"/>
@@ -3117,7 +3114,7 @@
       <c r="F25" s="105"/>
     </row>
     <row r="26" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A26" s="162"/>
+      <c r="A26" s="164"/>
       <c r="B26" s="100"/>
       <c r="C26" s="101"/>
       <c r="D26" s="101"/>
@@ -3128,7 +3125,7 @@
       <c r="F26" s="105"/>
     </row>
     <row r="27" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A27" s="162"/>
+      <c r="A27" s="164"/>
       <c r="B27" s="100"/>
       <c r="C27" s="101"/>
       <c r="D27" s="101"/>
@@ -3139,7 +3136,7 @@
       <c r="F27" s="105"/>
     </row>
     <row r="28" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A28" s="162"/>
+      <c r="A28" s="164"/>
       <c r="B28" s="149" t="s">
         <v>222</v>
       </c>
@@ -3159,7 +3156,7 @@
       </c>
     </row>
     <row r="29" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A29" s="162"/>
+      <c r="A29" s="164"/>
       <c r="B29" s="154" t="s">
         <v>263</v>
       </c>
@@ -3177,7 +3174,7 @@
       </c>
     </row>
     <row r="30" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A30" s="162"/>
+      <c r="A30" s="164"/>
       <c r="B30" s="154" t="s">
         <v>264</v>
       </c>
@@ -3193,7 +3190,7 @@
       </c>
     </row>
     <row r="31" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A31" s="162"/>
+      <c r="A31" s="164"/>
       <c r="B31" s="154" t="s">
         <v>265</v>
       </c>
@@ -3209,7 +3206,7 @@
       </c>
     </row>
     <row r="32" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A32" s="162"/>
+      <c r="A32" s="164"/>
       <c r="B32" s="154" t="s">
         <v>266</v>
       </c>
@@ -3225,7 +3222,7 @@
       </c>
     </row>
     <row r="33" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A33" s="162"/>
+      <c r="A33" s="164"/>
       <c r="B33" s="154" t="s">
         <v>268</v>
       </c>
@@ -3241,7 +3238,7 @@
       </c>
     </row>
     <row r="34" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A34" s="162"/>
+      <c r="A34" s="164"/>
       <c r="B34" s="154" t="s">
         <v>269</v>
       </c>
@@ -3257,7 +3254,7 @@
       </c>
     </row>
     <row r="35" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A35" s="162"/>
+      <c r="A35" s="164"/>
       <c r="B35" s="154" t="s">
         <v>270</v>
       </c>
@@ -3276,7 +3273,7 @@
       </c>
     </row>
     <row r="36" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A36" s="162"/>
+      <c r="A36" s="164"/>
       <c r="B36" s="149" t="s">
         <v>223</v>
       </c>
@@ -3296,7 +3293,7 @@
       </c>
     </row>
     <row r="37" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A37" s="162"/>
+      <c r="A37" s="164"/>
       <c r="B37" s="149" t="s">
         <v>224</v>
       </c>
@@ -3313,7 +3310,7 @@
       <c r="F37" s="105"/>
     </row>
     <row r="38" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A38" s="162"/>
+      <c r="A38" s="164"/>
       <c r="B38" s="149" t="s">
         <v>225</v>
       </c>
@@ -3330,7 +3327,7 @@
       <c r="F38" s="105"/>
     </row>
     <row r="39" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A39" s="162"/>
+      <c r="A39" s="164"/>
       <c r="B39" s="149" t="s">
         <v>217</v>
       </c>
@@ -3347,7 +3344,7 @@
       <c r="F39" s="105"/>
     </row>
     <row r="40" spans="1:9" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="A40" s="162"/>
+      <c r="A40" s="164"/>
       <c r="B40" s="98" t="s">
         <v>179</v>
       </c>
@@ -3386,7 +3383,7 @@
     </row>
     <row r="42" spans="1:9" ht="13.5" thickBot="1"/>
     <row r="43" spans="1:9" ht="15" customHeight="1" outlineLevel="1">
-      <c r="A43" s="161" t="s">
+      <c r="A43" s="163" t="s">
         <v>226</v>
       </c>
       <c r="B43" s="113" t="s">
@@ -3406,7 +3403,7 @@
       </c>
     </row>
     <row r="44" spans="1:9" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="A44" s="162"/>
+      <c r="A44" s="164"/>
       <c r="B44" s="98" t="s">
         <v>177</v>
       </c>
@@ -3424,7 +3421,7 @@
       </c>
     </row>
     <row r="45" spans="1:9" ht="15.75" outlineLevel="1" thickTop="1">
-      <c r="A45" s="162"/>
+      <c r="A45" s="164"/>
       <c r="B45" s="100"/>
       <c r="C45" s="101"/>
       <c r="D45" s="101"/>
@@ -3435,7 +3432,7 @@
       <c r="F45" s="105"/>
     </row>
     <row r="46" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A46" s="162"/>
+      <c r="A46" s="164"/>
       <c r="B46" s="149" t="s">
         <v>221</v>
       </c>
@@ -3452,7 +3449,7 @@
       <c r="F46" s="105"/>
     </row>
     <row r="47" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A47" s="162"/>
+      <c r="A47" s="164"/>
       <c r="B47" s="155" t="s">
         <v>273</v>
       </c>
@@ -3467,7 +3464,7 @@
       <c r="F47" s="105"/>
     </row>
     <row r="48" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A48" s="162"/>
+      <c r="A48" s="164"/>
       <c r="B48" s="157" t="s">
         <v>275</v>
       </c>
@@ -3482,7 +3479,7 @@
       </c>
     </row>
     <row r="49" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A49" s="162"/>
+      <c r="A49" s="164"/>
       <c r="B49" s="149" t="s">
         <v>222</v>
       </c>
@@ -3502,7 +3499,7 @@
       </c>
     </row>
     <row r="50" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A50" s="162"/>
+      <c r="A50" s="164"/>
       <c r="B50" s="156" t="s">
         <v>274</v>
       </c>
@@ -3514,7 +3511,7 @@
       <c r="F50" s="105"/>
     </row>
     <row r="51" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A51" s="162"/>
+      <c r="A51" s="164"/>
       <c r="B51" s="150" t="s">
         <v>229</v>
       </c>
@@ -3538,7 +3535,7 @@
       </c>
     </row>
     <row r="52" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A52" s="162"/>
+      <c r="A52" s="164"/>
       <c r="B52" s="150" t="s">
         <v>230</v>
       </c>
@@ -3562,7 +3559,7 @@
       </c>
     </row>
     <row r="53" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A53" s="162"/>
+      <c r="A53" s="164"/>
       <c r="B53" s="150" t="s">
         <v>231</v>
       </c>
@@ -3586,7 +3583,7 @@
       </c>
     </row>
     <row r="54" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A54" s="162"/>
+      <c r="A54" s="164"/>
       <c r="B54" s="150" t="s">
         <v>233</v>
       </c>
@@ -3610,7 +3607,7 @@
       </c>
     </row>
     <row r="55" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A55" s="162"/>
+      <c r="A55" s="164"/>
       <c r="B55" s="150" t="s">
         <v>234</v>
       </c>
@@ -3634,7 +3631,7 @@
       </c>
     </row>
     <row r="56" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A56" s="162"/>
+      <c r="A56" s="164"/>
       <c r="B56" s="150" t="s">
         <v>235</v>
       </c>
@@ -3658,7 +3655,7 @@
       </c>
     </row>
     <row r="57" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A57" s="162"/>
+      <c r="A57" s="164"/>
       <c r="B57" s="150" t="s">
         <v>236</v>
       </c>
@@ -3682,7 +3679,7 @@
       </c>
     </row>
     <row r="58" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A58" s="162"/>
+      <c r="A58" s="164"/>
       <c r="B58" s="158" t="s">
         <v>263</v>
       </c>
@@ -3697,7 +3694,7 @@
       <c r="F58" s="105"/>
     </row>
     <row r="59" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A59" s="162"/>
+      <c r="A59" s="164"/>
       <c r="B59" s="158" t="s">
         <v>264</v>
       </c>
@@ -3716,7 +3713,7 @@
       </c>
     </row>
     <row r="60" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A60" s="162"/>
+      <c r="A60" s="164"/>
       <c r="B60" s="158" t="s">
         <v>265</v>
       </c>
@@ -3735,7 +3732,7 @@
       </c>
     </row>
     <row r="61" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A61" s="162"/>
+      <c r="A61" s="164"/>
       <c r="B61" s="159" t="s">
         <v>266</v>
       </c>
@@ -3754,7 +3751,7 @@
       </c>
     </row>
     <row r="62" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A62" s="162"/>
+      <c r="A62" s="164"/>
       <c r="B62" s="159" t="s">
         <v>268</v>
       </c>
@@ -3773,7 +3770,7 @@
       </c>
     </row>
     <row r="63" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A63" s="162"/>
+      <c r="A63" s="164"/>
       <c r="B63" s="159" t="s">
         <v>269</v>
       </c>
@@ -3792,7 +3789,7 @@
       </c>
     </row>
     <row r="64" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A64" s="162"/>
+      <c r="A64" s="164"/>
       <c r="B64" s="159" t="s">
         <v>276</v>
       </c>
@@ -3811,7 +3808,7 @@
       </c>
     </row>
     <row r="65" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A65" s="162"/>
+      <c r="A65" s="164"/>
       <c r="B65" s="159" t="s">
         <v>276</v>
       </c>
@@ -3830,7 +3827,7 @@
       </c>
     </row>
     <row r="66" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A66" s="162"/>
+      <c r="A66" s="164"/>
       <c r="B66" s="150" t="s">
         <v>223</v>
       </c>
@@ -3847,7 +3844,7 @@
       <c r="F66" s="105"/>
     </row>
     <row r="67" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A67" s="162"/>
+      <c r="A67" s="164"/>
       <c r="B67" s="150" t="s">
         <v>237</v>
       </c>
@@ -3864,7 +3861,7 @@
       <c r="F67" s="105"/>
     </row>
     <row r="68" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A68" s="162"/>
+      <c r="A68" s="164"/>
       <c r="B68" s="150" t="s">
         <v>238</v>
       </c>
@@ -3881,7 +3878,7 @@
       <c r="F68" s="105"/>
     </row>
     <row r="69" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A69" s="162"/>
+      <c r="A69" s="164"/>
       <c r="B69" s="150" t="s">
         <v>217</v>
       </c>
@@ -3898,7 +3895,7 @@
       <c r="F69" s="105"/>
     </row>
     <row r="70" spans="1:9" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="A70" s="162"/>
+      <c r="A70" s="164"/>
       <c r="B70" s="98" t="s">
         <v>179</v>
       </c>
@@ -3941,7 +3938,7 @@
     </row>
     <row r="72" spans="1:9" ht="13.5" thickBot="1"/>
     <row r="73" spans="1:9" ht="15" customHeight="1" outlineLevel="1">
-      <c r="A73" s="163" t="s">
+      <c r="A73" s="165" t="s">
         <v>239</v>
       </c>
       <c r="B73" s="109" t="s">
@@ -3961,7 +3958,7 @@
       </c>
     </row>
     <row r="74" spans="1:9" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="A74" s="162"/>
+      <c r="A74" s="164"/>
       <c r="B74" s="98" t="s">
         <v>177</v>
       </c>
@@ -3981,7 +3978,7 @@
       </c>
     </row>
     <row r="75" spans="1:9" ht="15.75" outlineLevel="1" thickTop="1">
-      <c r="A75" s="162"/>
+      <c r="A75" s="164"/>
       <c r="B75" s="151" t="s">
         <v>241</v>
       </c>
@@ -3998,7 +3995,7 @@
       <c r="F75" s="105"/>
     </row>
     <row r="76" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A76" s="162"/>
+      <c r="A76" s="164"/>
       <c r="B76" s="151" t="s">
         <v>242</v>
       </c>
@@ -4015,7 +4012,7 @@
       <c r="F76" s="105"/>
     </row>
     <row r="77" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A77" s="162"/>
+      <c r="A77" s="164"/>
       <c r="B77" s="151" t="s">
         <v>243</v>
       </c>
@@ -4032,7 +4029,7 @@
       <c r="F77" s="105"/>
     </row>
     <row r="78" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A78" s="162"/>
+      <c r="A78" s="164"/>
       <c r="B78" s="160" t="s">
         <v>263</v>
       </c>
@@ -4047,7 +4044,7 @@
       <c r="F78" s="105"/>
     </row>
     <row r="79" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A79" s="162"/>
+      <c r="A79" s="164"/>
       <c r="B79" s="160" t="s">
         <v>264</v>
       </c>
@@ -4066,7 +4063,7 @@
       </c>
     </row>
     <row r="80" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A80" s="162"/>
+      <c r="A80" s="164"/>
       <c r="B80" s="160" t="s">
         <v>265</v>
       </c>
@@ -4085,7 +4082,7 @@
       </c>
     </row>
     <row r="81" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A81" s="162"/>
+      <c r="A81" s="164"/>
       <c r="B81" s="160" t="s">
         <v>266</v>
       </c>
@@ -4104,7 +4101,7 @@
       </c>
     </row>
     <row r="82" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A82" s="162"/>
+      <c r="A82" s="164"/>
       <c r="B82" s="160" t="s">
         <v>268</v>
       </c>
@@ -4123,7 +4120,7 @@
       </c>
     </row>
     <row r="83" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A83" s="162"/>
+      <c r="A83" s="164"/>
       <c r="B83" s="160" t="s">
         <v>269</v>
       </c>
@@ -4142,8 +4139,8 @@
       </c>
     </row>
     <row r="84" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A84" s="162"/>
-      <c r="B84" s="226" t="s">
+      <c r="A84" s="164"/>
+      <c r="B84" s="161" t="s">
         <v>276</v>
       </c>
       <c r="C84" s="101">
@@ -4158,8 +4155,8 @@
       <c r="H84" s="112"/>
     </row>
     <row r="85" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A85" s="162"/>
-      <c r="B85" s="226" t="s">
+      <c r="A85" s="164"/>
+      <c r="B85" s="161" t="s">
         <v>270</v>
       </c>
       <c r="C85" s="101">
@@ -4173,7 +4170,7 @@
       <c r="F85" s="105"/>
     </row>
     <row r="86" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A86" s="162"/>
+      <c r="A86" s="164"/>
       <c r="B86" s="151" t="s">
         <v>244</v>
       </c>
@@ -4190,7 +4187,7 @@
       <c r="F86" s="105"/>
     </row>
     <row r="87" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A87" s="162"/>
+      <c r="A87" s="164"/>
       <c r="B87" s="151" t="s">
         <v>237</v>
       </c>
@@ -4207,7 +4204,7 @@
       <c r="F87" s="105"/>
     </row>
     <row r="88" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A88" s="162"/>
+      <c r="A88" s="164"/>
       <c r="B88" s="151" t="s">
         <v>245</v>
       </c>
@@ -4224,7 +4221,7 @@
       <c r="F88" s="105"/>
     </row>
     <row r="89" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A89" s="162"/>
+      <c r="A89" s="164"/>
       <c r="B89" s="151" t="s">
         <v>217</v>
       </c>
@@ -4241,7 +4238,7 @@
       <c r="F89" s="105"/>
     </row>
     <row r="90" spans="1:8" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="A90" s="162"/>
+      <c r="A90" s="164"/>
       <c r="B90" s="98" t="s">
         <v>179</v>
       </c>
@@ -4284,7 +4281,7 @@
     </row>
     <row r="92" spans="1:8" ht="13.5" thickBot="1"/>
     <row r="93" spans="1:8" ht="15" customHeight="1" outlineLevel="1">
-      <c r="A93" s="161" t="s">
+      <c r="A93" s="163" t="s">
         <v>246</v>
       </c>
       <c r="B93" s="113" t="s">
@@ -4304,7 +4301,7 @@
       </c>
     </row>
     <row r="94" spans="1:8" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="A94" s="162"/>
+      <c r="A94" s="164"/>
       <c r="B94" s="98" t="s">
         <v>177</v>
       </c>
@@ -4324,39 +4321,41 @@
       </c>
     </row>
     <row r="95" spans="1:8" ht="15.75" outlineLevel="1" thickTop="1">
-      <c r="A95" s="162"/>
+      <c r="A95" s="164"/>
       <c r="B95" s="151" t="s">
         <v>228</v>
       </c>
-      <c r="C95" s="227" t="s">
-        <v>277</v>
+      <c r="C95" s="162">
+        <v>29952</v>
       </c>
       <c r="D95" s="101">
         <v>36326</v>
       </c>
-      <c r="E95" s="124" t="e">
+      <c r="E95" s="124">
         <f t="shared" si="7"/>
-        <v>#VALUE!</v>
+        <v>6374</v>
       </c>
       <c r="F95" s="105"/>
     </row>
     <row r="96" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A96" s="162"/>
+      <c r="A96" s="164"/>
       <c r="B96" s="151" t="s">
         <v>221</v>
       </c>
-      <c r="C96" s="101"/>
+      <c r="C96" s="101">
+        <v>31107</v>
+      </c>
       <c r="D96" s="101">
         <v>37764</v>
       </c>
       <c r="E96" s="123">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>6657</v>
       </c>
       <c r="F96" s="105"/>
     </row>
     <row r="97" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A97" s="162"/>
+      <c r="A97" s="164"/>
       <c r="B97" s="100"/>
       <c r="C97" s="101"/>
       <c r="D97" s="101"/>
@@ -4367,7 +4366,7 @@
       <c r="F97" s="105"/>
     </row>
     <row r="98" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A98" s="162"/>
+      <c r="A98" s="164"/>
       <c r="B98" s="151" t="s">
         <v>222</v>
       </c>
@@ -4382,7 +4381,7 @@
       <c r="F98" s="105"/>
     </row>
     <row r="99" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A99" s="162"/>
+      <c r="A99" s="164"/>
       <c r="B99" s="100"/>
       <c r="C99" s="101"/>
       <c r="D99" s="101"/>
@@ -4393,7 +4392,7 @@
       <c r="F99" s="105"/>
     </row>
     <row r="100" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A100" s="162"/>
+      <c r="A100" s="164"/>
       <c r="B100" s="152" t="s">
         <v>236</v>
       </c>
@@ -4408,7 +4407,7 @@
       <c r="F100" s="105"/>
     </row>
     <row r="101" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A101" s="162"/>
+      <c r="A101" s="164"/>
       <c r="B101" s="100"/>
       <c r="C101" s="101"/>
       <c r="D101" s="101"/>
@@ -4419,7 +4418,7 @@
       <c r="F101" s="105"/>
     </row>
     <row r="102" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A102" s="162"/>
+      <c r="A102" s="164"/>
       <c r="B102" s="100"/>
       <c r="C102" s="101"/>
       <c r="D102" s="101"/>
@@ -4430,7 +4429,7 @@
       <c r="F102" s="105"/>
     </row>
     <row r="103" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A103" s="162"/>
+      <c r="A103" s="164"/>
       <c r="B103" s="152" t="s">
         <v>223</v>
       </c>
@@ -4445,7 +4444,7 @@
       <c r="F103" s="105"/>
     </row>
     <row r="104" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A104" s="162"/>
+      <c r="A104" s="164"/>
       <c r="B104" s="152" t="s">
         <v>248</v>
       </c>
@@ -4460,7 +4459,7 @@
       <c r="F104" s="105"/>
     </row>
     <row r="105" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A105" s="162"/>
+      <c r="A105" s="164"/>
       <c r="B105" s="152" t="s">
         <v>249</v>
       </c>
@@ -4475,7 +4474,7 @@
       <c r="F105" s="105"/>
     </row>
     <row r="106" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A106" s="162"/>
+      <c r="A106" s="164"/>
       <c r="B106" s="152" t="s">
         <v>250</v>
       </c>
@@ -4490,7 +4489,7 @@
       <c r="F106" s="105"/>
     </row>
     <row r="107" spans="1:8" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="A107" s="162"/>
+      <c r="A107" s="164"/>
       <c r="B107" s="98" t="s">
         <v>179</v>
       </c>
@@ -4531,7 +4530,7 @@
     </row>
     <row r="109" spans="1:8" ht="13.5" thickBot="1"/>
     <row r="110" spans="1:8" ht="15" customHeight="1" outlineLevel="1">
-      <c r="A110" s="163" t="s">
+      <c r="A110" s="165" t="s">
         <v>251</v>
       </c>
       <c r="B110" s="109" t="s">
@@ -4551,7 +4550,7 @@
       </c>
     </row>
     <row r="111" spans="1:8" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="A111" s="162"/>
+      <c r="A111" s="164"/>
       <c r="B111" s="98" t="s">
         <v>177</v>
       </c>
@@ -4569,7 +4568,7 @@
       </c>
     </row>
     <row r="112" spans="1:8" ht="15.75" outlineLevel="1" thickTop="1">
-      <c r="A112" s="162"/>
+      <c r="A112" s="164"/>
       <c r="B112" s="100"/>
       <c r="C112" s="101"/>
       <c r="D112" s="101"/>
@@ -4580,7 +4579,7 @@
       <c r="F112" s="105"/>
     </row>
     <row r="113" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A113" s="162"/>
+      <c r="A113" s="164"/>
       <c r="B113" s="152" t="s">
         <v>253</v>
       </c>
@@ -4595,7 +4594,7 @@
       <c r="F113" s="105"/>
     </row>
     <row r="114" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A114" s="162"/>
+      <c r="A114" s="164"/>
       <c r="B114" s="100"/>
       <c r="C114" s="101"/>
       <c r="D114" s="101"/>
@@ -4606,7 +4605,7 @@
       <c r="F114" s="105"/>
     </row>
     <row r="115" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A115" s="162"/>
+      <c r="A115" s="164"/>
       <c r="B115" s="152" t="s">
         <v>254</v>
       </c>
@@ -4621,7 +4620,7 @@
       <c r="F115" s="105"/>
     </row>
     <row r="116" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A116" s="162"/>
+      <c r="A116" s="164"/>
       <c r="B116" s="100"/>
       <c r="C116" s="101"/>
       <c r="D116" s="101"/>
@@ -4632,7 +4631,7 @@
       <c r="F116" s="105"/>
     </row>
     <row r="117" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A117" s="162"/>
+      <c r="A117" s="164"/>
       <c r="B117" s="152" t="s">
         <v>223</v>
       </c>
@@ -4647,7 +4646,7 @@
       <c r="F117" s="105"/>
     </row>
     <row r="118" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A118" s="162"/>
+      <c r="A118" s="164"/>
       <c r="B118" s="152" t="s">
         <v>248</v>
       </c>
@@ -4662,7 +4661,7 @@
       <c r="F118" s="105"/>
     </row>
     <row r="119" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A119" s="162"/>
+      <c r="A119" s="164"/>
       <c r="B119" s="152" t="s">
         <v>255</v>
       </c>
@@ -4677,7 +4676,7 @@
       <c r="F119" s="105"/>
     </row>
     <row r="120" spans="1:9" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="A120" s="162"/>
+      <c r="A120" s="164"/>
       <c r="B120" s="98" t="s">
         <v>179</v>
       </c>
@@ -4718,7 +4717,7 @@
     </row>
     <row r="122" spans="1:9" ht="13.5" thickBot="1"/>
     <row r="123" spans="1:9" ht="15" customHeight="1" outlineLevel="1">
-      <c r="A123" s="161" t="s">
+      <c r="A123" s="163" t="s">
         <v>256</v>
       </c>
       <c r="B123" s="113" t="s">
@@ -4738,7 +4737,7 @@
       </c>
     </row>
     <row r="124" spans="1:9" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="A124" s="162"/>
+      <c r="A124" s="164"/>
       <c r="B124" s="98" t="s">
         <v>177</v>
       </c>
@@ -4760,7 +4759,7 @@
       </c>
     </row>
     <row r="125" spans="1:9" ht="15.75" outlineLevel="1" thickTop="1">
-      <c r="A125" s="162"/>
+      <c r="A125" s="164"/>
       <c r="B125" s="100"/>
       <c r="C125" s="101"/>
       <c r="D125" s="101"/>
@@ -4771,7 +4770,7 @@
       <c r="F125" s="105"/>
     </row>
     <row r="126" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A126" s="162"/>
+      <c r="A126" s="164"/>
       <c r="B126" s="152" t="s">
         <v>221</v>
       </c>
@@ -4786,7 +4785,7 @@
       <c r="F126" s="105"/>
     </row>
     <row r="127" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A127" s="162"/>
+      <c r="A127" s="164"/>
       <c r="B127" s="100"/>
       <c r="C127" s="101"/>
       <c r="D127" s="101"/>
@@ -4797,7 +4796,7 @@
       <c r="F127" s="105"/>
     </row>
     <row r="128" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A128" s="162"/>
+      <c r="A128" s="164"/>
       <c r="B128" s="152" t="s">
         <v>222</v>
       </c>
@@ -4812,7 +4811,7 @@
       <c r="F128" s="105"/>
     </row>
     <row r="129" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A129" s="162"/>
+      <c r="A129" s="164"/>
       <c r="B129" s="152" t="s">
         <v>248</v>
       </c>
@@ -4827,7 +4826,7 @@
       <c r="F129" s="105"/>
     </row>
     <row r="130" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A130" s="162"/>
+      <c r="A130" s="164"/>
       <c r="B130" s="152" t="s">
         <v>258</v>
       </c>
@@ -4842,7 +4841,7 @@
       <c r="F130" s="105"/>
     </row>
     <row r="131" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A131" s="162"/>
+      <c r="A131" s="164"/>
       <c r="B131" s="152" t="s">
         <v>224</v>
       </c>
@@ -4857,7 +4856,7 @@
       <c r="F131" s="105"/>
     </row>
     <row r="132" spans="1:9" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="A132" s="162"/>
+      <c r="A132" s="164"/>
       <c r="B132" s="98" t="s">
         <v>179</v>
       </c>
@@ -4898,7 +4897,7 @@
     </row>
     <row r="134" spans="1:9" ht="13.5" thickBot="1"/>
     <row r="135" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A135" s="163" t="s">
+      <c r="A135" s="165" t="s">
         <v>259</v>
       </c>
       <c r="B135" s="109" t="s">
@@ -4918,7 +4917,7 @@
       </c>
     </row>
     <row r="136" spans="1:9" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="A136" s="162"/>
+      <c r="A136" s="164"/>
       <c r="B136" s="98" t="s">
         <v>177</v>
       </c>
@@ -4940,7 +4939,7 @@
       </c>
     </row>
     <row r="137" spans="1:9" ht="15.75" outlineLevel="1" thickTop="1">
-      <c r="A137" s="162"/>
+      <c r="A137" s="164"/>
       <c r="B137" s="100"/>
       <c r="C137" s="101"/>
       <c r="D137" s="101"/>
@@ -4951,7 +4950,7 @@
       <c r="F137" s="105"/>
     </row>
     <row r="138" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A138" s="162"/>
+      <c r="A138" s="164"/>
       <c r="B138" s="100"/>
       <c r="C138" s="101"/>
       <c r="D138" s="101"/>
@@ -4962,7 +4961,7 @@
       <c r="F138" s="105"/>
     </row>
     <row r="139" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A139" s="162"/>
+      <c r="A139" s="164"/>
       <c r="B139" s="100"/>
       <c r="C139" s="101"/>
       <c r="D139" s="101"/>
@@ -4973,7 +4972,7 @@
       <c r="F139" s="105"/>
     </row>
     <row r="140" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A140" s="162"/>
+      <c r="A140" s="164"/>
       <c r="B140" s="100"/>
       <c r="C140" s="101"/>
       <c r="D140" s="101"/>
@@ -4984,7 +4983,7 @@
       <c r="F140" s="105"/>
     </row>
     <row r="141" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A141" s="162"/>
+      <c r="A141" s="164"/>
       <c r="B141" s="100"/>
       <c r="C141" s="101"/>
       <c r="D141" s="101"/>
@@ -4995,7 +4994,7 @@
       <c r="F141" s="105"/>
     </row>
     <row r="142" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A142" s="162"/>
+      <c r="A142" s="164"/>
       <c r="B142" s="100"/>
       <c r="C142" s="101"/>
       <c r="D142" s="101"/>
@@ -5006,7 +5005,7 @@
       <c r="F142" s="105"/>
     </row>
     <row r="143" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A143" s="162"/>
+      <c r="A143" s="164"/>
       <c r="B143" s="100"/>
       <c r="C143" s="101"/>
       <c r="D143" s="101"/>
@@ -5017,7 +5016,7 @@
       <c r="F143" s="105"/>
     </row>
     <row r="144" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A144" s="162"/>
+      <c r="A144" s="164"/>
       <c r="B144" s="100"/>
       <c r="C144" s="101"/>
       <c r="D144" s="101"/>
@@ -5028,7 +5027,7 @@
       <c r="F144" s="105"/>
     </row>
     <row r="145" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A145" s="162"/>
+      <c r="A145" s="164"/>
       <c r="B145" s="152" t="s">
         <v>261</v>
       </c>
@@ -5050,7 +5049,7 @@
       </c>
     </row>
     <row r="146" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A146" s="162"/>
+      <c r="A146" s="164"/>
       <c r="B146" s="100"/>
       <c r="C146" s="101"/>
       <c r="D146" s="101"/>
@@ -5061,7 +5060,7 @@
       <c r="F146" s="105"/>
     </row>
     <row r="147" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A147" s="162"/>
+      <c r="A147" s="164"/>
       <c r="B147" s="100"/>
       <c r="C147" s="101"/>
       <c r="D147" s="101"/>
@@ -5072,7 +5071,7 @@
       <c r="F147" s="105"/>
     </row>
     <row r="148" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A148" s="162"/>
+      <c r="A148" s="164"/>
       <c r="B148" s="100"/>
       <c r="C148" s="101"/>
       <c r="D148" s="101"/>
@@ -5083,7 +5082,7 @@
       <c r="F148" s="105"/>
     </row>
     <row r="149" spans="1:9" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="A149" s="162"/>
+      <c r="A149" s="164"/>
       <c r="B149" s="98" t="s">
         <v>179</v>
       </c>
@@ -5121,7 +5120,7 @@
       </c>
     </row>
     <row r="152" spans="1:9" ht="15" hidden="1" outlineLevel="2">
-      <c r="A152" s="161" t="s">
+      <c r="A152" s="163" t="s">
         <v>169</v>
       </c>
       <c r="B152" s="113" t="s">
@@ -5141,7 +5140,7 @@
       </c>
     </row>
     <row r="153" spans="1:9" ht="15.75" hidden="1" outlineLevel="2" thickBot="1">
-      <c r="A153" s="162"/>
+      <c r="A153" s="164"/>
       <c r="B153" s="98" t="s">
         <v>177</v>
       </c>
@@ -5154,7 +5153,7 @@
       <c r="F153" s="104"/>
     </row>
     <row r="154" spans="1:9" ht="15.75" hidden="1" outlineLevel="2" thickTop="1">
-      <c r="A154" s="162"/>
+      <c r="A154" s="164"/>
       <c r="B154" s="100"/>
       <c r="C154" s="101"/>
       <c r="D154" s="101"/>
@@ -5165,7 +5164,7 @@
       <c r="F154" s="105"/>
     </row>
     <row r="155" spans="1:9" ht="15" hidden="1" outlineLevel="2">
-      <c r="A155" s="162"/>
+      <c r="A155" s="164"/>
       <c r="B155" s="100"/>
       <c r="C155" s="101"/>
       <c r="D155" s="101"/>
@@ -5176,7 +5175,7 @@
       <c r="F155" s="105"/>
     </row>
     <row r="156" spans="1:9" ht="15" hidden="1" outlineLevel="2">
-      <c r="A156" s="162"/>
+      <c r="A156" s="164"/>
       <c r="B156" s="100"/>
       <c r="C156" s="101"/>
       <c r="D156" s="101"/>
@@ -5187,7 +5186,7 @@
       <c r="F156" s="105"/>
     </row>
     <row r="157" spans="1:9" ht="15" hidden="1" outlineLevel="2">
-      <c r="A157" s="162"/>
+      <c r="A157" s="164"/>
       <c r="B157" s="100"/>
       <c r="C157" s="101"/>
       <c r="D157" s="101"/>
@@ -5198,7 +5197,7 @@
       <c r="F157" s="105"/>
     </row>
     <row r="158" spans="1:9" ht="15" hidden="1" outlineLevel="2">
-      <c r="A158" s="162"/>
+      <c r="A158" s="164"/>
       <c r="B158" s="100"/>
       <c r="C158" s="101"/>
       <c r="D158" s="101"/>
@@ -5209,7 +5208,7 @@
       <c r="F158" s="105"/>
     </row>
     <row r="159" spans="1:9" ht="15" hidden="1" outlineLevel="2">
-      <c r="A159" s="162"/>
+      <c r="A159" s="164"/>
       <c r="B159" s="100"/>
       <c r="C159" s="101"/>
       <c r="D159" s="101"/>
@@ -5220,7 +5219,7 @@
       <c r="F159" s="105"/>
     </row>
     <row r="160" spans="1:9" ht="15" hidden="1" outlineLevel="2">
-      <c r="A160" s="162"/>
+      <c r="A160" s="164"/>
       <c r="B160" s="100"/>
       <c r="C160" s="101"/>
       <c r="D160" s="101"/>
@@ -5231,7 +5230,7 @@
       <c r="F160" s="105"/>
     </row>
     <row r="161" spans="1:7" ht="15" hidden="1" outlineLevel="2">
-      <c r="A161" s="162"/>
+      <c r="A161" s="164"/>
       <c r="B161" s="100"/>
       <c r="C161" s="101"/>
       <c r="D161" s="101"/>
@@ -5242,7 +5241,7 @@
       <c r="F161" s="105"/>
     </row>
     <row r="162" spans="1:7" ht="15" hidden="1" outlineLevel="2">
-      <c r="A162" s="162"/>
+      <c r="A162" s="164"/>
       <c r="B162" s="100"/>
       <c r="C162" s="101"/>
       <c r="D162" s="101"/>
@@ -5253,7 +5252,7 @@
       <c r="F162" s="105"/>
     </row>
     <row r="163" spans="1:7" ht="15" hidden="1" outlineLevel="2">
-      <c r="A163" s="162"/>
+      <c r="A163" s="164"/>
       <c r="B163" s="100"/>
       <c r="C163" s="101"/>
       <c r="D163" s="101"/>
@@ -5264,7 +5263,7 @@
       <c r="F163" s="105"/>
     </row>
     <row r="164" spans="1:7" ht="15" hidden="1" outlineLevel="2">
-      <c r="A164" s="162"/>
+      <c r="A164" s="164"/>
       <c r="B164" s="100"/>
       <c r="C164" s="101"/>
       <c r="D164" s="101"/>
@@ -5275,7 +5274,7 @@
       <c r="F164" s="105"/>
     </row>
     <row r="165" spans="1:7" ht="15" hidden="1" outlineLevel="2">
-      <c r="A165" s="162"/>
+      <c r="A165" s="164"/>
       <c r="B165" s="100"/>
       <c r="C165" s="101"/>
       <c r="D165" s="101"/>
@@ -5286,7 +5285,7 @@
       <c r="F165" s="105"/>
     </row>
     <row r="166" spans="1:7" ht="15.75" hidden="1" outlineLevel="2" thickBot="1">
-      <c r="A166" s="162"/>
+      <c r="A166" s="164"/>
       <c r="B166" s="98" t="s">
         <v>179</v>
       </c>
@@ -5325,6 +5324,11 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="A152:A166"/>
+    <mergeCell ref="A123:A132"/>
+    <mergeCell ref="A93:A107"/>
+    <mergeCell ref="A135:A149"/>
+    <mergeCell ref="A110:A120"/>
     <mergeCell ref="A43:A70"/>
     <mergeCell ref="A73:A90"/>
     <mergeCell ref="C5:D5"/>
@@ -5334,11 +5338,6 @@
     <mergeCell ref="A8:A18"/>
     <mergeCell ref="A21:A40"/>
     <mergeCell ref="C4:E4"/>
-    <mergeCell ref="A152:A166"/>
-    <mergeCell ref="A123:A132"/>
-    <mergeCell ref="A93:A107"/>
-    <mergeCell ref="A135:A149"/>
-    <mergeCell ref="A110:A120"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -5370,13 +5369,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="26.25" customHeight="1">
-      <c r="A1" s="189" t="s">
+      <c r="A1" s="173" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="189"/>
-      <c r="C1" s="189"/>
-      <c r="D1" s="189"/>
-      <c r="E1" s="189"/>
+      <c r="B1" s="173"/>
+      <c r="C1" s="173"/>
+      <c r="D1" s="173"/>
+      <c r="E1" s="173"/>
       <c r="F1" s="7"/>
       <c r="G1" s="5"/>
       <c r="H1" s="5"/>
@@ -5406,18 +5405,18 @@
         <v>8</v>
       </c>
       <c r="B3" s="36"/>
-      <c r="C3" s="190"/>
-      <c r="D3" s="191"/>
-      <c r="E3" s="191"/>
+      <c r="C3" s="174"/>
+      <c r="D3" s="175"/>
+      <c r="E3" s="175"/>
     </row>
     <row r="4" spans="1:8" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A4" s="46" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="87"/>
-      <c r="C4" s="171"/>
-      <c r="D4" s="172"/>
-      <c r="E4" s="172"/>
+      <c r="C4" s="176"/>
+      <c r="D4" s="177"/>
+      <c r="E4" s="177"/>
       <c r="F4" s="6"/>
     </row>
     <row r="5" spans="1:8" hidden="1" outlineLevel="2">
@@ -5569,9 +5568,9 @@
         <v>9</v>
       </c>
       <c r="B21" s="90"/>
-      <c r="C21" s="173"/>
-      <c r="D21" s="174"/>
-      <c r="E21" s="174"/>
+      <c r="C21" s="178"/>
+      <c r="D21" s="179"/>
+      <c r="E21" s="179"/>
     </row>
     <row r="22" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A22" s="47">
@@ -5722,9 +5721,9 @@
         <v>10</v>
       </c>
       <c r="B38" s="87"/>
-      <c r="C38" s="171"/>
-      <c r="D38" s="172"/>
-      <c r="E38" s="172"/>
+      <c r="C38" s="176"/>
+      <c r="D38" s="177"/>
+      <c r="E38" s="177"/>
     </row>
     <row r="39" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A39" s="47">
@@ -5875,9 +5874,9 @@
         <v>11</v>
       </c>
       <c r="B55" s="87"/>
-      <c r="C55" s="171"/>
-      <c r="D55" s="172"/>
-      <c r="E55" s="172"/>
+      <c r="C55" s="176"/>
+      <c r="D55" s="177"/>
+      <c r="E55" s="177"/>
     </row>
     <row r="56" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A56" s="47">
@@ -6028,9 +6027,9 @@
         <v>12</v>
       </c>
       <c r="B72" s="87"/>
-      <c r="C72" s="171"/>
-      <c r="D72" s="172"/>
-      <c r="E72" s="172"/>
+      <c r="C72" s="176"/>
+      <c r="D72" s="177"/>
+      <c r="E72" s="177"/>
     </row>
     <row r="73" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A73" s="47">
@@ -6181,9 +6180,9 @@
         <v>13</v>
       </c>
       <c r="B89" s="87"/>
-      <c r="C89" s="171"/>
-      <c r="D89" s="172"/>
-      <c r="E89" s="172"/>
+      <c r="C89" s="176"/>
+      <c r="D89" s="177"/>
+      <c r="E89" s="177"/>
     </row>
     <row r="90" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A90" s="47">
@@ -6334,9 +6333,9 @@
         <v>14</v>
       </c>
       <c r="B106" s="87"/>
-      <c r="C106" s="171"/>
-      <c r="D106" s="172"/>
-      <c r="E106" s="172"/>
+      <c r="C106" s="176"/>
+      <c r="D106" s="177"/>
+      <c r="E106" s="177"/>
     </row>
     <row r="107" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A107" s="47">
@@ -6487,9 +6486,9 @@
         <v>15</v>
       </c>
       <c r="B123" s="87"/>
-      <c r="C123" s="171"/>
-      <c r="D123" s="172"/>
-      <c r="E123" s="172"/>
+      <c r="C123" s="176"/>
+      <c r="D123" s="177"/>
+      <c r="E123" s="177"/>
     </row>
     <row r="124" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A124" s="47">
@@ -6640,9 +6639,9 @@
         <v>16</v>
       </c>
       <c r="B140" s="87"/>
-      <c r="C140" s="171"/>
-      <c r="D140" s="172"/>
-      <c r="E140" s="172"/>
+      <c r="C140" s="176"/>
+      <c r="D140" s="177"/>
+      <c r="E140" s="177"/>
     </row>
     <row r="141" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A141" s="47">
@@ -6793,9 +6792,9 @@
         <v>17</v>
       </c>
       <c r="B157" s="87"/>
-      <c r="C157" s="171"/>
-      <c r="D157" s="172"/>
-      <c r="E157" s="172"/>
+      <c r="C157" s="176"/>
+      <c r="D157" s="177"/>
+      <c r="E157" s="177"/>
     </row>
     <row r="158" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A158" s="47">
@@ -6946,9 +6945,9 @@
         <v>18</v>
       </c>
       <c r="B174" s="87"/>
-      <c r="C174" s="171"/>
-      <c r="D174" s="172"/>
-      <c r="E174" s="172"/>
+      <c r="C174" s="176"/>
+      <c r="D174" s="177"/>
+      <c r="E174" s="177"/>
     </row>
     <row r="175" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A175" s="47">
@@ -7099,9 +7098,9 @@
         <v>19</v>
       </c>
       <c r="B191" s="87"/>
-      <c r="C191" s="171"/>
-      <c r="D191" s="172"/>
-      <c r="E191" s="172"/>
+      <c r="C191" s="176"/>
+      <c r="D191" s="177"/>
+      <c r="E191" s="177"/>
     </row>
     <row r="192" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A192" s="47">
@@ -7252,9 +7251,9 @@
         <v>20</v>
       </c>
       <c r="B208" s="87"/>
-      <c r="C208" s="171"/>
-      <c r="D208" s="172"/>
-      <c r="E208" s="172"/>
+      <c r="C208" s="176"/>
+      <c r="D208" s="177"/>
+      <c r="E208" s="177"/>
     </row>
     <row r="209" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A209" s="47">
@@ -7405,9 +7404,9 @@
         <v>21</v>
       </c>
       <c r="B225" s="87"/>
-      <c r="C225" s="171"/>
-      <c r="D225" s="172"/>
-      <c r="E225" s="172"/>
+      <c r="C225" s="176"/>
+      <c r="D225" s="177"/>
+      <c r="E225" s="177"/>
     </row>
     <row r="226" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A226" s="47">
@@ -7558,9 +7557,9 @@
         <v>22</v>
       </c>
       <c r="B242" s="87"/>
-      <c r="C242" s="171"/>
-      <c r="D242" s="172"/>
-      <c r="E242" s="172"/>
+      <c r="C242" s="176"/>
+      <c r="D242" s="177"/>
+      <c r="E242" s="177"/>
     </row>
     <row r="243" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A243" s="47">
@@ -7711,9 +7710,9 @@
         <v>23</v>
       </c>
       <c r="B259" s="87"/>
-      <c r="C259" s="171"/>
-      <c r="D259" s="172"/>
-      <c r="E259" s="172"/>
+      <c r="C259" s="176"/>
+      <c r="D259" s="177"/>
+      <c r="E259" s="177"/>
     </row>
     <row r="260" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A260" s="47">
@@ -7864,18 +7863,18 @@
         <v>24</v>
       </c>
       <c r="B276" s="37"/>
-      <c r="C276" s="187"/>
-      <c r="D276" s="188"/>
-      <c r="E276" s="188"/>
+      <c r="C276" s="180"/>
+      <c r="D276" s="181"/>
+      <c r="E276" s="181"/>
     </row>
     <row r="277" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A277" s="51" t="s">
         <v>25</v>
       </c>
       <c r="B277" s="87"/>
-      <c r="C277" s="171"/>
-      <c r="D277" s="172"/>
-      <c r="E277" s="172"/>
+      <c r="C277" s="176"/>
+      <c r="D277" s="177"/>
+      <c r="E277" s="177"/>
     </row>
     <row r="278" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A278" s="52">
@@ -8026,9 +8025,9 @@
         <v>26</v>
       </c>
       <c r="B294" s="90"/>
-      <c r="C294" s="173"/>
-      <c r="D294" s="174"/>
-      <c r="E294" s="174"/>
+      <c r="C294" s="178"/>
+      <c r="D294" s="179"/>
+      <c r="E294" s="179"/>
     </row>
     <row r="295" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A295" s="52">
@@ -8179,9 +8178,9 @@
         <v>27</v>
       </c>
       <c r="B311" s="87"/>
-      <c r="C311" s="171"/>
-      <c r="D311" s="172"/>
-      <c r="E311" s="172"/>
+      <c r="C311" s="176"/>
+      <c r="D311" s="177"/>
+      <c r="E311" s="177"/>
     </row>
     <row r="312" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A312" s="52">
@@ -8332,9 +8331,9 @@
         <v>28</v>
       </c>
       <c r="B328" s="87"/>
-      <c r="C328" s="171"/>
-      <c r="D328" s="172"/>
-      <c r="E328" s="172"/>
+      <c r="C328" s="176"/>
+      <c r="D328" s="177"/>
+      <c r="E328" s="177"/>
     </row>
     <row r="329" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A329" s="52">
@@ -8485,9 +8484,9 @@
         <v>29</v>
       </c>
       <c r="B345" s="87"/>
-      <c r="C345" s="171"/>
-      <c r="D345" s="172"/>
-      <c r="E345" s="172"/>
+      <c r="C345" s="176"/>
+      <c r="D345" s="177"/>
+      <c r="E345" s="177"/>
     </row>
     <row r="346" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A346" s="52">
@@ -8638,9 +8637,9 @@
         <v>30</v>
       </c>
       <c r="B362" s="87"/>
-      <c r="C362" s="171"/>
-      <c r="D362" s="172"/>
-      <c r="E362" s="172"/>
+      <c r="C362" s="176"/>
+      <c r="D362" s="177"/>
+      <c r="E362" s="177"/>
     </row>
     <row r="363" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A363" s="52">
@@ -8791,9 +8790,9 @@
         <v>31</v>
       </c>
       <c r="B379" s="87"/>
-      <c r="C379" s="171"/>
-      <c r="D379" s="172"/>
-      <c r="E379" s="172"/>
+      <c r="C379" s="176"/>
+      <c r="D379" s="177"/>
+      <c r="E379" s="177"/>
     </row>
     <row r="380" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A380" s="52">
@@ -8944,9 +8943,9 @@
         <v>32</v>
       </c>
       <c r="B396" s="87"/>
-      <c r="C396" s="171"/>
-      <c r="D396" s="172"/>
-      <c r="E396" s="172"/>
+      <c r="C396" s="176"/>
+      <c r="D396" s="177"/>
+      <c r="E396" s="177"/>
     </row>
     <row r="397" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A397" s="52">
@@ -9097,9 +9096,9 @@
         <v>33</v>
       </c>
       <c r="B413" s="87"/>
-      <c r="C413" s="171"/>
-      <c r="D413" s="172"/>
-      <c r="E413" s="172"/>
+      <c r="C413" s="176"/>
+      <c r="D413" s="177"/>
+      <c r="E413" s="177"/>
     </row>
     <row r="414" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A414" s="52">
@@ -9250,9 +9249,9 @@
         <v>34</v>
       </c>
       <c r="B430" s="87"/>
-      <c r="C430" s="171"/>
-      <c r="D430" s="172"/>
-      <c r="E430" s="172"/>
+      <c r="C430" s="176"/>
+      <c r="D430" s="177"/>
+      <c r="E430" s="177"/>
     </row>
     <row r="431" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A431" s="52">
@@ -9403,9 +9402,9 @@
         <v>35</v>
       </c>
       <c r="B447" s="87"/>
-      <c r="C447" s="171"/>
-      <c r="D447" s="172"/>
-      <c r="E447" s="172"/>
+      <c r="C447" s="176"/>
+      <c r="D447" s="177"/>
+      <c r="E447" s="177"/>
     </row>
     <row r="448" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A448" s="52">
@@ -9556,9 +9555,9 @@
         <v>36</v>
       </c>
       <c r="B464" s="87"/>
-      <c r="C464" s="171"/>
-      <c r="D464" s="172"/>
-      <c r="E464" s="172"/>
+      <c r="C464" s="176"/>
+      <c r="D464" s="177"/>
+      <c r="E464" s="177"/>
     </row>
     <row r="465" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A465" s="52">
@@ -9709,9 +9708,9 @@
         <v>37</v>
       </c>
       <c r="B481" s="87"/>
-      <c r="C481" s="171"/>
-      <c r="D481" s="172"/>
-      <c r="E481" s="172"/>
+      <c r="C481" s="176"/>
+      <c r="D481" s="177"/>
+      <c r="E481" s="177"/>
     </row>
     <row r="482" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A482" s="52">
@@ -9862,9 +9861,9 @@
         <v>38</v>
       </c>
       <c r="B498" s="87"/>
-      <c r="C498" s="171"/>
-      <c r="D498" s="172"/>
-      <c r="E498" s="172"/>
+      <c r="C498" s="176"/>
+      <c r="D498" s="177"/>
+      <c r="E498" s="177"/>
     </row>
     <row r="499" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A499" s="52">
@@ -10015,9 +10014,9 @@
         <v>39</v>
       </c>
       <c r="B515" s="87"/>
-      <c r="C515" s="171"/>
-      <c r="D515" s="172"/>
-      <c r="E515" s="172"/>
+      <c r="C515" s="176"/>
+      <c r="D515" s="177"/>
+      <c r="E515" s="177"/>
     </row>
     <row r="516" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A516" s="52">
@@ -10168,9 +10167,9 @@
         <v>40</v>
       </c>
       <c r="B532" s="87"/>
-      <c r="C532" s="171"/>
-      <c r="D532" s="172"/>
-      <c r="E532" s="172"/>
+      <c r="C532" s="176"/>
+      <c r="D532" s="177"/>
+      <c r="E532" s="177"/>
     </row>
     <row r="533" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A533" s="55">
@@ -10321,18 +10320,18 @@
         <v>50</v>
       </c>
       <c r="B549" s="38"/>
-      <c r="C549" s="185"/>
-      <c r="D549" s="186"/>
-      <c r="E549" s="186"/>
+      <c r="C549" s="182"/>
+      <c r="D549" s="183"/>
+      <c r="E549" s="183"/>
     </row>
     <row r="550" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A550" s="58" t="s">
         <v>51</v>
       </c>
       <c r="B550" s="87"/>
-      <c r="C550" s="171"/>
-      <c r="D550" s="172"/>
-      <c r="E550" s="172"/>
+      <c r="C550" s="176"/>
+      <c r="D550" s="177"/>
+      <c r="E550" s="177"/>
     </row>
     <row r="551" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A551" s="59">
@@ -10483,9 +10482,9 @@
         <v>52</v>
       </c>
       <c r="B567" s="90"/>
-      <c r="C567" s="173"/>
-      <c r="D567" s="174"/>
-      <c r="E567" s="174"/>
+      <c r="C567" s="178"/>
+      <c r="D567" s="179"/>
+      <c r="E567" s="179"/>
     </row>
     <row r="568" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A568" s="59">
@@ -10636,9 +10635,9 @@
         <v>53</v>
       </c>
       <c r="B584" s="87"/>
-      <c r="C584" s="171"/>
-      <c r="D584" s="172"/>
-      <c r="E584" s="172"/>
+      <c r="C584" s="176"/>
+      <c r="D584" s="177"/>
+      <c r="E584" s="177"/>
     </row>
     <row r="585" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A585" s="59">
@@ -10789,9 +10788,9 @@
         <v>54</v>
       </c>
       <c r="B601" s="87"/>
-      <c r="C601" s="171"/>
-      <c r="D601" s="172"/>
-      <c r="E601" s="172"/>
+      <c r="C601" s="176"/>
+      <c r="D601" s="177"/>
+      <c r="E601" s="177"/>
     </row>
     <row r="602" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A602" s="59">
@@ -10942,9 +10941,9 @@
         <v>55</v>
       </c>
       <c r="B618" s="87"/>
-      <c r="C618" s="171"/>
-      <c r="D618" s="172"/>
-      <c r="E618" s="172"/>
+      <c r="C618" s="176"/>
+      <c r="D618" s="177"/>
+      <c r="E618" s="177"/>
     </row>
     <row r="619" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A619" s="59">
@@ -11095,9 +11094,9 @@
         <v>56</v>
       </c>
       <c r="B635" s="87"/>
-      <c r="C635" s="171"/>
-      <c r="D635" s="172"/>
-      <c r="E635" s="172"/>
+      <c r="C635" s="176"/>
+      <c r="D635" s="177"/>
+      <c r="E635" s="177"/>
     </row>
     <row r="636" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A636" s="59">
@@ -11248,9 +11247,9 @@
         <v>57</v>
       </c>
       <c r="B652" s="87"/>
-      <c r="C652" s="171"/>
-      <c r="D652" s="172"/>
-      <c r="E652" s="172"/>
+      <c r="C652" s="176"/>
+      <c r="D652" s="177"/>
+      <c r="E652" s="177"/>
     </row>
     <row r="653" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A653" s="59">
@@ -11401,9 +11400,9 @@
         <v>58</v>
       </c>
       <c r="B669" s="87"/>
-      <c r="C669" s="171"/>
-      <c r="D669" s="172"/>
-      <c r="E669" s="172"/>
+      <c r="C669" s="176"/>
+      <c r="D669" s="177"/>
+      <c r="E669" s="177"/>
     </row>
     <row r="670" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A670" s="59">
@@ -11554,9 +11553,9 @@
         <v>59</v>
       </c>
       <c r="B686" s="87"/>
-      <c r="C686" s="171"/>
-      <c r="D686" s="172"/>
-      <c r="E686" s="172"/>
+      <c r="C686" s="176"/>
+      <c r="D686" s="177"/>
+      <c r="E686" s="177"/>
     </row>
     <row r="687" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A687" s="59">
@@ -11707,9 +11706,9 @@
         <v>60</v>
       </c>
       <c r="B703" s="87"/>
-      <c r="C703" s="171"/>
-      <c r="D703" s="172"/>
-      <c r="E703" s="172"/>
+      <c r="C703" s="176"/>
+      <c r="D703" s="177"/>
+      <c r="E703" s="177"/>
     </row>
     <row r="704" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A704" s="59">
@@ -11860,9 +11859,9 @@
         <v>61</v>
       </c>
       <c r="B720" s="87"/>
-      <c r="C720" s="171"/>
-      <c r="D720" s="172"/>
-      <c r="E720" s="172"/>
+      <c r="C720" s="176"/>
+      <c r="D720" s="177"/>
+      <c r="E720" s="177"/>
     </row>
     <row r="721" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A721" s="59">
@@ -12013,9 +12012,9 @@
         <v>62</v>
       </c>
       <c r="B737" s="87"/>
-      <c r="C737" s="171"/>
-      <c r="D737" s="172"/>
-      <c r="E737" s="172"/>
+      <c r="C737" s="176"/>
+      <c r="D737" s="177"/>
+      <c r="E737" s="177"/>
     </row>
     <row r="738" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A738" s="59">
@@ -12166,9 +12165,9 @@
         <v>63</v>
       </c>
       <c r="B754" s="87"/>
-      <c r="C754" s="171"/>
-      <c r="D754" s="172"/>
-      <c r="E754" s="172"/>
+      <c r="C754" s="176"/>
+      <c r="D754" s="177"/>
+      <c r="E754" s="177"/>
     </row>
     <row r="755" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A755" s="59">
@@ -12319,9 +12318,9 @@
         <v>64</v>
       </c>
       <c r="B771" s="87"/>
-      <c r="C771" s="171"/>
-      <c r="D771" s="172"/>
-      <c r="E771" s="172"/>
+      <c r="C771" s="176"/>
+      <c r="D771" s="177"/>
+      <c r="E771" s="177"/>
     </row>
     <row r="772" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A772" s="59">
@@ -12472,9 +12471,9 @@
         <v>65</v>
       </c>
       <c r="B788" s="87"/>
-      <c r="C788" s="171"/>
-      <c r="D788" s="172"/>
-      <c r="E788" s="172"/>
+      <c r="C788" s="176"/>
+      <c r="D788" s="177"/>
+      <c r="E788" s="177"/>
     </row>
     <row r="789" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A789" s="59">
@@ -12625,9 +12624,9 @@
         <v>66</v>
       </c>
       <c r="B805" s="87"/>
-      <c r="C805" s="171"/>
-      <c r="D805" s="172"/>
-      <c r="E805" s="172"/>
+      <c r="C805" s="176"/>
+      <c r="D805" s="177"/>
+      <c r="E805" s="177"/>
     </row>
     <row r="806" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A806" s="59">
@@ -12778,18 +12777,18 @@
         <v>67</v>
       </c>
       <c r="B822" s="39"/>
-      <c r="C822" s="183"/>
-      <c r="D822" s="184"/>
-      <c r="E822" s="184"/>
+      <c r="C822" s="184"/>
+      <c r="D822" s="185"/>
+      <c r="E822" s="185"/>
     </row>
     <row r="823" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A823" s="63" t="s">
         <v>68</v>
       </c>
       <c r="B823" s="87"/>
-      <c r="C823" s="171"/>
-      <c r="D823" s="172"/>
-      <c r="E823" s="172"/>
+      <c r="C823" s="176"/>
+      <c r="D823" s="177"/>
+      <c r="E823" s="177"/>
     </row>
     <row r="824" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A824" s="64">
@@ -12940,9 +12939,9 @@
         <v>69</v>
       </c>
       <c r="B840" s="90"/>
-      <c r="C840" s="173"/>
-      <c r="D840" s="174"/>
-      <c r="E840" s="174"/>
+      <c r="C840" s="178"/>
+      <c r="D840" s="179"/>
+      <c r="E840" s="179"/>
     </row>
     <row r="841" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A841" s="64">
@@ -13093,9 +13092,9 @@
         <v>70</v>
       </c>
       <c r="B857" s="87"/>
-      <c r="C857" s="171"/>
-      <c r="D857" s="172"/>
-      <c r="E857" s="172"/>
+      <c r="C857" s="176"/>
+      <c r="D857" s="177"/>
+      <c r="E857" s="177"/>
     </row>
     <row r="858" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A858" s="64">
@@ -13246,9 +13245,9 @@
         <v>71</v>
       </c>
       <c r="B874" s="87"/>
-      <c r="C874" s="171"/>
-      <c r="D874" s="172"/>
-      <c r="E874" s="172"/>
+      <c r="C874" s="176"/>
+      <c r="D874" s="177"/>
+      <c r="E874" s="177"/>
     </row>
     <row r="875" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A875" s="64">
@@ -13399,9 +13398,9 @@
         <v>72</v>
       </c>
       <c r="B891" s="87"/>
-      <c r="C891" s="171"/>
-      <c r="D891" s="172"/>
-      <c r="E891" s="172"/>
+      <c r="C891" s="176"/>
+      <c r="D891" s="177"/>
+      <c r="E891" s="177"/>
     </row>
     <row r="892" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A892" s="64">
@@ -13552,9 +13551,9 @@
         <v>73</v>
       </c>
       <c r="B908" s="87"/>
-      <c r="C908" s="171"/>
-      <c r="D908" s="172"/>
-      <c r="E908" s="172"/>
+      <c r="C908" s="176"/>
+      <c r="D908" s="177"/>
+      <c r="E908" s="177"/>
     </row>
     <row r="909" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A909" s="64">
@@ -13705,9 +13704,9 @@
         <v>74</v>
       </c>
       <c r="B925" s="87"/>
-      <c r="C925" s="171"/>
-      <c r="D925" s="172"/>
-      <c r="E925" s="172"/>
+      <c r="C925" s="176"/>
+      <c r="D925" s="177"/>
+      <c r="E925" s="177"/>
     </row>
     <row r="926" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A926" s="64">
@@ -13858,9 +13857,9 @@
         <v>75</v>
       </c>
       <c r="B942" s="87"/>
-      <c r="C942" s="171"/>
-      <c r="D942" s="172"/>
-      <c r="E942" s="172"/>
+      <c r="C942" s="176"/>
+      <c r="D942" s="177"/>
+      <c r="E942" s="177"/>
     </row>
     <row r="943" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A943" s="64">
@@ -14011,9 +14010,9 @@
         <v>76</v>
       </c>
       <c r="B959" s="87"/>
-      <c r="C959" s="171"/>
-      <c r="D959" s="172"/>
-      <c r="E959" s="172"/>
+      <c r="C959" s="176"/>
+      <c r="D959" s="177"/>
+      <c r="E959" s="177"/>
     </row>
     <row r="960" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A960" s="64">
@@ -14164,9 +14163,9 @@
         <v>77</v>
       </c>
       <c r="B976" s="87"/>
-      <c r="C976" s="171"/>
-      <c r="D976" s="172"/>
-      <c r="E976" s="172"/>
+      <c r="C976" s="176"/>
+      <c r="D976" s="177"/>
+      <c r="E976" s="177"/>
     </row>
     <row r="977" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A977" s="64">
@@ -14317,9 +14316,9 @@
         <v>78</v>
       </c>
       <c r="B993" s="87"/>
-      <c r="C993" s="171"/>
-      <c r="D993" s="172"/>
-      <c r="E993" s="172"/>
+      <c r="C993" s="176"/>
+      <c r="D993" s="177"/>
+      <c r="E993" s="177"/>
     </row>
     <row r="994" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A994" s="64">
@@ -14470,9 +14469,9 @@
         <v>79</v>
       </c>
       <c r="B1010" s="87"/>
-      <c r="C1010" s="171"/>
-      <c r="D1010" s="172"/>
-      <c r="E1010" s="172"/>
+      <c r="C1010" s="176"/>
+      <c r="D1010" s="177"/>
+      <c r="E1010" s="177"/>
     </row>
     <row r="1011" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1011" s="64">
@@ -14623,9 +14622,9 @@
         <v>80</v>
       </c>
       <c r="B1027" s="87"/>
-      <c r="C1027" s="171"/>
-      <c r="D1027" s="172"/>
-      <c r="E1027" s="172"/>
+      <c r="C1027" s="176"/>
+      <c r="D1027" s="177"/>
+      <c r="E1027" s="177"/>
     </row>
     <row r="1028" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1028" s="64">
@@ -14776,9 +14775,9 @@
         <v>83</v>
       </c>
       <c r="B1044" s="87"/>
-      <c r="C1044" s="171"/>
-      <c r="D1044" s="172"/>
-      <c r="E1044" s="172"/>
+      <c r="C1044" s="176"/>
+      <c r="D1044" s="177"/>
+      <c r="E1044" s="177"/>
     </row>
     <row r="1045" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1045" s="64">
@@ -14929,9 +14928,9 @@
         <v>82</v>
       </c>
       <c r="B1061" s="87"/>
-      <c r="C1061" s="171"/>
-      <c r="D1061" s="172"/>
-      <c r="E1061" s="172"/>
+      <c r="C1061" s="176"/>
+      <c r="D1061" s="177"/>
+      <c r="E1061" s="177"/>
     </row>
     <row r="1062" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1062" s="64">
@@ -15082,9 +15081,9 @@
         <v>84</v>
       </c>
       <c r="B1078" s="87"/>
-      <c r="C1078" s="171"/>
-      <c r="D1078" s="172"/>
-      <c r="E1078" s="172"/>
+      <c r="C1078" s="176"/>
+      <c r="D1078" s="177"/>
+      <c r="E1078" s="177"/>
     </row>
     <row r="1079" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1079" s="64">
@@ -15235,18 +15234,18 @@
         <v>104</v>
       </c>
       <c r="B1095" s="40"/>
-      <c r="C1095" s="181"/>
-      <c r="D1095" s="182"/>
-      <c r="E1095" s="182"/>
+      <c r="C1095" s="186"/>
+      <c r="D1095" s="187"/>
+      <c r="E1095" s="187"/>
     </row>
     <row r="1096" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A1096" s="68" t="s">
         <v>85</v>
       </c>
       <c r="B1096" s="87"/>
-      <c r="C1096" s="171"/>
-      <c r="D1096" s="172"/>
-      <c r="E1096" s="172"/>
+      <c r="C1096" s="176"/>
+      <c r="D1096" s="177"/>
+      <c r="E1096" s="177"/>
     </row>
     <row r="1097" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1097" s="69">
@@ -15397,9 +15396,9 @@
         <v>86</v>
       </c>
       <c r="B1113" s="90"/>
-      <c r="C1113" s="173"/>
-      <c r="D1113" s="174"/>
-      <c r="E1113" s="174"/>
+      <c r="C1113" s="178"/>
+      <c r="D1113" s="179"/>
+      <c r="E1113" s="179"/>
     </row>
     <row r="1114" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1114" s="69">
@@ -15550,9 +15549,9 @@
         <v>87</v>
       </c>
       <c r="B1130" s="87"/>
-      <c r="C1130" s="171"/>
-      <c r="D1130" s="172"/>
-      <c r="E1130" s="172"/>
+      <c r="C1130" s="176"/>
+      <c r="D1130" s="177"/>
+      <c r="E1130" s="177"/>
     </row>
     <row r="1131" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1131" s="69">
@@ -15703,9 +15702,9 @@
         <v>88</v>
       </c>
       <c r="B1147" s="87"/>
-      <c r="C1147" s="171"/>
-      <c r="D1147" s="172"/>
-      <c r="E1147" s="172"/>
+      <c r="C1147" s="176"/>
+      <c r="D1147" s="177"/>
+      <c r="E1147" s="177"/>
     </row>
     <row r="1148" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1148" s="69">
@@ -15856,9 +15855,9 @@
         <v>89</v>
       </c>
       <c r="B1164" s="87"/>
-      <c r="C1164" s="171"/>
-      <c r="D1164" s="172"/>
-      <c r="E1164" s="172"/>
+      <c r="C1164" s="176"/>
+      <c r="D1164" s="177"/>
+      <c r="E1164" s="177"/>
     </row>
     <row r="1165" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1165" s="69">
@@ -16009,9 +16008,9 @@
         <v>90</v>
       </c>
       <c r="B1181" s="87"/>
-      <c r="C1181" s="171"/>
-      <c r="D1181" s="172"/>
-      <c r="E1181" s="172"/>
+      <c r="C1181" s="176"/>
+      <c r="D1181" s="177"/>
+      <c r="E1181" s="177"/>
     </row>
     <row r="1182" spans="1:5" hidden="1" outlineLevel="3">
       <c r="A1182" s="69">
@@ -16162,9 +16161,9 @@
         <v>91</v>
       </c>
       <c r="B1198" s="87"/>
-      <c r="C1198" s="171"/>
-      <c r="D1198" s="172"/>
-      <c r="E1198" s="172"/>
+      <c r="C1198" s="176"/>
+      <c r="D1198" s="177"/>
+      <c r="E1198" s="177"/>
     </row>
     <row r="1199" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1199" s="69">
@@ -16315,9 +16314,9 @@
         <v>92</v>
       </c>
       <c r="B1215" s="87"/>
-      <c r="C1215" s="171"/>
-      <c r="D1215" s="172"/>
-      <c r="E1215" s="172"/>
+      <c r="C1215" s="176"/>
+      <c r="D1215" s="177"/>
+      <c r="E1215" s="177"/>
     </row>
     <row r="1216" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1216" s="69">
@@ -16468,9 +16467,9 @@
         <v>93</v>
       </c>
       <c r="B1232" s="87"/>
-      <c r="C1232" s="171"/>
-      <c r="D1232" s="172"/>
-      <c r="E1232" s="172"/>
+      <c r="C1232" s="176"/>
+      <c r="D1232" s="177"/>
+      <c r="E1232" s="177"/>
     </row>
     <row r="1233" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1233" s="69">
@@ -16621,9 +16620,9 @@
         <v>94</v>
       </c>
       <c r="B1249" s="87"/>
-      <c r="C1249" s="171"/>
-      <c r="D1249" s="172"/>
-      <c r="E1249" s="172"/>
+      <c r="C1249" s="176"/>
+      <c r="D1249" s="177"/>
+      <c r="E1249" s="177"/>
     </row>
     <row r="1250" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1250" s="69">
@@ -16774,9 +16773,9 @@
         <v>99</v>
       </c>
       <c r="B1266" s="87"/>
-      <c r="C1266" s="171"/>
-      <c r="D1266" s="172"/>
-      <c r="E1266" s="172"/>
+      <c r="C1266" s="176"/>
+      <c r="D1266" s="177"/>
+      <c r="E1266" s="177"/>
     </row>
     <row r="1267" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1267" s="69">
@@ -16927,9 +16926,9 @@
         <v>100</v>
       </c>
       <c r="B1283" s="87"/>
-      <c r="C1283" s="171"/>
-      <c r="D1283" s="172"/>
-      <c r="E1283" s="172"/>
+      <c r="C1283" s="176"/>
+      <c r="D1283" s="177"/>
+      <c r="E1283" s="177"/>
     </row>
     <row r="1284" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1284" s="69">
@@ -17080,9 +17079,9 @@
         <v>101</v>
       </c>
       <c r="B1300" s="87"/>
-      <c r="C1300" s="171"/>
-      <c r="D1300" s="172"/>
-      <c r="E1300" s="172"/>
+      <c r="C1300" s="176"/>
+      <c r="D1300" s="177"/>
+      <c r="E1300" s="177"/>
     </row>
     <row r="1301" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1301" s="69">
@@ -17233,9 +17232,9 @@
         <v>81</v>
       </c>
       <c r="B1317" s="87"/>
-      <c r="C1317" s="171"/>
-      <c r="D1317" s="172"/>
-      <c r="E1317" s="172"/>
+      <c r="C1317" s="176"/>
+      <c r="D1317" s="177"/>
+      <c r="E1317" s="177"/>
     </row>
     <row r="1318" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1318" s="69">
@@ -17386,9 +17385,9 @@
         <v>102</v>
       </c>
       <c r="B1334" s="87"/>
-      <c r="C1334" s="171"/>
-      <c r="D1334" s="172"/>
-      <c r="E1334" s="172"/>
+      <c r="C1334" s="176"/>
+      <c r="D1334" s="177"/>
+      <c r="E1334" s="177"/>
     </row>
     <row r="1335" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1335" s="69">
@@ -17539,9 +17538,9 @@
         <v>98</v>
       </c>
       <c r="B1351" s="87"/>
-      <c r="C1351" s="171"/>
-      <c r="D1351" s="172"/>
-      <c r="E1351" s="172"/>
+      <c r="C1351" s="176"/>
+      <c r="D1351" s="177"/>
+      <c r="E1351" s="177"/>
     </row>
     <row r="1352" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1352" s="69">
@@ -17692,18 +17691,18 @@
         <v>103</v>
       </c>
       <c r="B1368" s="41"/>
-      <c r="C1368" s="179"/>
-      <c r="D1368" s="180"/>
-      <c r="E1368" s="180"/>
+      <c r="C1368" s="188"/>
+      <c r="D1368" s="189"/>
+      <c r="E1368" s="189"/>
     </row>
     <row r="1369" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A1369" s="73" t="s">
         <v>105</v>
       </c>
       <c r="B1369" s="87"/>
-      <c r="C1369" s="171"/>
-      <c r="D1369" s="172"/>
-      <c r="E1369" s="172"/>
+      <c r="C1369" s="176"/>
+      <c r="D1369" s="177"/>
+      <c r="E1369" s="177"/>
     </row>
     <row r="1370" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1370" s="74">
@@ -17854,9 +17853,9 @@
         <v>106</v>
       </c>
       <c r="B1386" s="90"/>
-      <c r="C1386" s="173"/>
-      <c r="D1386" s="174"/>
-      <c r="E1386" s="174"/>
+      <c r="C1386" s="178"/>
+      <c r="D1386" s="179"/>
+      <c r="E1386" s="179"/>
     </row>
     <row r="1387" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1387" s="74">
@@ -18007,9 +18006,9 @@
         <v>107</v>
       </c>
       <c r="B1403" s="87"/>
-      <c r="C1403" s="171"/>
-      <c r="D1403" s="172"/>
-      <c r="E1403" s="172"/>
+      <c r="C1403" s="176"/>
+      <c r="D1403" s="177"/>
+      <c r="E1403" s="177"/>
     </row>
     <row r="1404" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1404" s="74">
@@ -18160,9 +18159,9 @@
         <v>108</v>
       </c>
       <c r="B1420" s="87"/>
-      <c r="C1420" s="171"/>
-      <c r="D1420" s="172"/>
-      <c r="E1420" s="172"/>
+      <c r="C1420" s="176"/>
+      <c r="D1420" s="177"/>
+      <c r="E1420" s="177"/>
     </row>
     <row r="1421" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1421" s="74">
@@ -18313,9 +18312,9 @@
         <v>109</v>
       </c>
       <c r="B1437" s="87"/>
-      <c r="C1437" s="171"/>
-      <c r="D1437" s="172"/>
-      <c r="E1437" s="172"/>
+      <c r="C1437" s="176"/>
+      <c r="D1437" s="177"/>
+      <c r="E1437" s="177"/>
     </row>
     <row r="1438" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1438" s="74">
@@ -18466,9 +18465,9 @@
         <v>110</v>
       </c>
       <c r="B1454" s="87"/>
-      <c r="C1454" s="171"/>
-      <c r="D1454" s="172"/>
-      <c r="E1454" s="172"/>
+      <c r="C1454" s="176"/>
+      <c r="D1454" s="177"/>
+      <c r="E1454" s="177"/>
     </row>
     <row r="1455" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1455" s="74">
@@ -18619,9 +18618,9 @@
         <v>111</v>
       </c>
       <c r="B1471" s="87"/>
-      <c r="C1471" s="171"/>
-      <c r="D1471" s="172"/>
-      <c r="E1471" s="172"/>
+      <c r="C1471" s="176"/>
+      <c r="D1471" s="177"/>
+      <c r="E1471" s="177"/>
     </row>
     <row r="1472" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1472" s="74">
@@ -18772,9 +18771,9 @@
         <v>112</v>
       </c>
       <c r="B1488" s="87"/>
-      <c r="C1488" s="171"/>
-      <c r="D1488" s="172"/>
-      <c r="E1488" s="172"/>
+      <c r="C1488" s="176"/>
+      <c r="D1488" s="177"/>
+      <c r="E1488" s="177"/>
     </row>
     <row r="1489" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1489" s="74">
@@ -18925,9 +18924,9 @@
         <v>113</v>
       </c>
       <c r="B1505" s="87"/>
-      <c r="C1505" s="171"/>
-      <c r="D1505" s="172"/>
-      <c r="E1505" s="172"/>
+      <c r="C1505" s="176"/>
+      <c r="D1505" s="177"/>
+      <c r="E1505" s="177"/>
     </row>
     <row r="1506" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1506" s="74">
@@ -19078,9 +19077,9 @@
         <v>114</v>
       </c>
       <c r="B1522" s="87"/>
-      <c r="C1522" s="171"/>
-      <c r="D1522" s="172"/>
-      <c r="E1522" s="172"/>
+      <c r="C1522" s="176"/>
+      <c r="D1522" s="177"/>
+      <c r="E1522" s="177"/>
     </row>
     <row r="1523" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1523" s="74">
@@ -19231,9 +19230,9 @@
         <v>95</v>
       </c>
       <c r="B1539" s="87"/>
-      <c r="C1539" s="171"/>
-      <c r="D1539" s="172"/>
-      <c r="E1539" s="172"/>
+      <c r="C1539" s="176"/>
+      <c r="D1539" s="177"/>
+      <c r="E1539" s="177"/>
     </row>
     <row r="1540" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1540" s="74">
@@ -19384,9 +19383,9 @@
         <v>115</v>
       </c>
       <c r="B1556" s="87"/>
-      <c r="C1556" s="171"/>
-      <c r="D1556" s="172"/>
-      <c r="E1556" s="172"/>
+      <c r="C1556" s="176"/>
+      <c r="D1556" s="177"/>
+      <c r="E1556" s="177"/>
     </row>
     <row r="1557" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1557" s="74">
@@ -19537,9 +19536,9 @@
         <v>116</v>
       </c>
       <c r="B1573" s="87"/>
-      <c r="C1573" s="171"/>
-      <c r="D1573" s="172"/>
-      <c r="E1573" s="172"/>
+      <c r="C1573" s="176"/>
+      <c r="D1573" s="177"/>
+      <c r="E1573" s="177"/>
     </row>
     <row r="1574" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1574" s="74">
@@ -19690,9 +19689,9 @@
         <v>117</v>
       </c>
       <c r="B1590" s="87"/>
-      <c r="C1590" s="171"/>
-      <c r="D1590" s="172"/>
-      <c r="E1590" s="172"/>
+      <c r="C1590" s="176"/>
+      <c r="D1590" s="177"/>
+      <c r="E1590" s="177"/>
     </row>
     <row r="1591" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1591" s="74">
@@ -19843,9 +19842,9 @@
         <v>118</v>
       </c>
       <c r="B1607" s="87"/>
-      <c r="C1607" s="171"/>
-      <c r="D1607" s="172"/>
-      <c r="E1607" s="172"/>
+      <c r="C1607" s="176"/>
+      <c r="D1607" s="177"/>
+      <c r="E1607" s="177"/>
     </row>
     <row r="1608" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1608" s="74">
@@ -19996,9 +19995,9 @@
         <v>119</v>
       </c>
       <c r="B1624" s="87"/>
-      <c r="C1624" s="171"/>
-      <c r="D1624" s="172"/>
-      <c r="E1624" s="172"/>
+      <c r="C1624" s="176"/>
+      <c r="D1624" s="177"/>
+      <c r="E1624" s="177"/>
     </row>
     <row r="1625" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1625" s="74">
@@ -20149,18 +20148,18 @@
         <v>120</v>
       </c>
       <c r="B1641" s="42"/>
-      <c r="C1641" s="177"/>
-      <c r="D1641" s="178"/>
-      <c r="E1641" s="178"/>
+      <c r="C1641" s="190"/>
+      <c r="D1641" s="191"/>
+      <c r="E1641" s="191"/>
     </row>
     <row r="1642" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A1642" s="78" t="s">
         <v>121</v>
       </c>
       <c r="B1642" s="87"/>
-      <c r="C1642" s="171"/>
-      <c r="D1642" s="172"/>
-      <c r="E1642" s="172"/>
+      <c r="C1642" s="176"/>
+      <c r="D1642" s="177"/>
+      <c r="E1642" s="177"/>
     </row>
     <row r="1643" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1643" s="79">
@@ -20311,9 +20310,9 @@
         <v>122</v>
       </c>
       <c r="B1659" s="90"/>
-      <c r="C1659" s="173"/>
-      <c r="D1659" s="174"/>
-      <c r="E1659" s="174"/>
+      <c r="C1659" s="178"/>
+      <c r="D1659" s="179"/>
+      <c r="E1659" s="179"/>
     </row>
     <row r="1660" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1660" s="79">
@@ -20464,9 +20463,9 @@
         <v>123</v>
       </c>
       <c r="B1676" s="87"/>
-      <c r="C1676" s="171"/>
-      <c r="D1676" s="172"/>
-      <c r="E1676" s="172"/>
+      <c r="C1676" s="176"/>
+      <c r="D1676" s="177"/>
+      <c r="E1676" s="177"/>
     </row>
     <row r="1677" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1677" s="79">
@@ -20617,9 +20616,9 @@
         <v>124</v>
       </c>
       <c r="B1693" s="87"/>
-      <c r="C1693" s="171"/>
-      <c r="D1693" s="172"/>
-      <c r="E1693" s="172"/>
+      <c r="C1693" s="176"/>
+      <c r="D1693" s="177"/>
+      <c r="E1693" s="177"/>
     </row>
     <row r="1694" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1694" s="79">
@@ -20770,9 +20769,9 @@
         <v>125</v>
       </c>
       <c r="B1710" s="87"/>
-      <c r="C1710" s="171"/>
-      <c r="D1710" s="172"/>
-      <c r="E1710" s="172"/>
+      <c r="C1710" s="176"/>
+      <c r="D1710" s="177"/>
+      <c r="E1710" s="177"/>
     </row>
     <row r="1711" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1711" s="79">
@@ -20923,9 +20922,9 @@
         <v>126</v>
       </c>
       <c r="B1727" s="87"/>
-      <c r="C1727" s="171"/>
-      <c r="D1727" s="172"/>
-      <c r="E1727" s="172"/>
+      <c r="C1727" s="176"/>
+      <c r="D1727" s="177"/>
+      <c r="E1727" s="177"/>
     </row>
     <row r="1728" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1728" s="79">
@@ -21076,9 +21075,9 @@
         <v>127</v>
       </c>
       <c r="B1744" s="87"/>
-      <c r="C1744" s="171"/>
-      <c r="D1744" s="172"/>
-      <c r="E1744" s="172"/>
+      <c r="C1744" s="176"/>
+      <c r="D1744" s="177"/>
+      <c r="E1744" s="177"/>
     </row>
     <row r="1745" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1745" s="79">
@@ -21229,9 +21228,9 @@
         <v>128</v>
       </c>
       <c r="B1761" s="87"/>
-      <c r="C1761" s="171"/>
-      <c r="D1761" s="172"/>
-      <c r="E1761" s="172"/>
+      <c r="C1761" s="176"/>
+      <c r="D1761" s="177"/>
+      <c r="E1761" s="177"/>
     </row>
     <row r="1762" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1762" s="79">
@@ -21382,9 +21381,9 @@
         <v>129</v>
       </c>
       <c r="B1778" s="87"/>
-      <c r="C1778" s="171"/>
-      <c r="D1778" s="172"/>
-      <c r="E1778" s="172"/>
+      <c r="C1778" s="176"/>
+      <c r="D1778" s="177"/>
+      <c r="E1778" s="177"/>
     </row>
     <row r="1779" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1779" s="79">
@@ -21535,9 +21534,9 @@
         <v>130</v>
       </c>
       <c r="B1795" s="87"/>
-      <c r="C1795" s="171"/>
-      <c r="D1795" s="172"/>
-      <c r="E1795" s="172"/>
+      <c r="C1795" s="176"/>
+      <c r="D1795" s="177"/>
+      <c r="E1795" s="177"/>
     </row>
     <row r="1796" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1796" s="79">
@@ -21688,9 +21687,9 @@
         <v>131</v>
       </c>
       <c r="B1812" s="87"/>
-      <c r="C1812" s="171"/>
-      <c r="D1812" s="172"/>
-      <c r="E1812" s="172"/>
+      <c r="C1812" s="176"/>
+      <c r="D1812" s="177"/>
+      <c r="E1812" s="177"/>
     </row>
     <row r="1813" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1813" s="79">
@@ -21841,9 +21840,9 @@
         <v>96</v>
       </c>
       <c r="B1829" s="87"/>
-      <c r="C1829" s="171"/>
-      <c r="D1829" s="172"/>
-      <c r="E1829" s="172"/>
+      <c r="C1829" s="176"/>
+      <c r="D1829" s="177"/>
+      <c r="E1829" s="177"/>
     </row>
     <row r="1830" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1830" s="79">
@@ -21994,9 +21993,9 @@
         <v>132</v>
       </c>
       <c r="B1846" s="87"/>
-      <c r="C1846" s="171"/>
-      <c r="D1846" s="172"/>
-      <c r="E1846" s="172"/>
+      <c r="C1846" s="176"/>
+      <c r="D1846" s="177"/>
+      <c r="E1846" s="177"/>
     </row>
     <row r="1847" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1847" s="79">
@@ -22147,9 +22146,9 @@
         <v>133</v>
       </c>
       <c r="B1863" s="87"/>
-      <c r="C1863" s="171"/>
-      <c r="D1863" s="172"/>
-      <c r="E1863" s="172"/>
+      <c r="C1863" s="176"/>
+      <c r="D1863" s="177"/>
+      <c r="E1863" s="177"/>
     </row>
     <row r="1864" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1864" s="79">
@@ -22300,9 +22299,9 @@
         <v>134</v>
       </c>
       <c r="B1880" s="87"/>
-      <c r="C1880" s="171"/>
-      <c r="D1880" s="172"/>
-      <c r="E1880" s="172"/>
+      <c r="C1880" s="176"/>
+      <c r="D1880" s="177"/>
+      <c r="E1880" s="177"/>
     </row>
     <row r="1881" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1881" s="79">
@@ -22453,9 +22452,9 @@
         <v>135</v>
       </c>
       <c r="B1897" s="87"/>
-      <c r="C1897" s="171"/>
-      <c r="D1897" s="172"/>
-      <c r="E1897" s="172"/>
+      <c r="C1897" s="176"/>
+      <c r="D1897" s="177"/>
+      <c r="E1897" s="177"/>
     </row>
     <row r="1898" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1898" s="79">
@@ -22606,18 +22605,18 @@
         <v>136</v>
       </c>
       <c r="B1914" s="43"/>
-      <c r="C1914" s="175"/>
-      <c r="D1914" s="176"/>
-      <c r="E1914" s="176"/>
+      <c r="C1914" s="192"/>
+      <c r="D1914" s="193"/>
+      <c r="E1914" s="193"/>
     </row>
     <row r="1915" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A1915" s="83" t="s">
         <v>137</v>
       </c>
       <c r="B1915" s="87"/>
-      <c r="C1915" s="171"/>
-      <c r="D1915" s="172"/>
-      <c r="E1915" s="172"/>
+      <c r="C1915" s="176"/>
+      <c r="D1915" s="177"/>
+      <c r="E1915" s="177"/>
     </row>
     <row r="1916" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1916" s="84">
@@ -22768,9 +22767,9 @@
         <v>138</v>
       </c>
       <c r="B1932" s="90"/>
-      <c r="C1932" s="173"/>
-      <c r="D1932" s="174"/>
-      <c r="E1932" s="174"/>
+      <c r="C1932" s="178"/>
+      <c r="D1932" s="179"/>
+      <c r="E1932" s="179"/>
     </row>
     <row r="1933" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1933" s="84">
@@ -22921,9 +22920,9 @@
         <v>139</v>
       </c>
       <c r="B1949" s="87"/>
-      <c r="C1949" s="171"/>
-      <c r="D1949" s="172"/>
-      <c r="E1949" s="172"/>
+      <c r="C1949" s="176"/>
+      <c r="D1949" s="177"/>
+      <c r="E1949" s="177"/>
     </row>
     <row r="1950" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1950" s="84">
@@ -23074,9 +23073,9 @@
         <v>140</v>
       </c>
       <c r="B1966" s="87"/>
-      <c r="C1966" s="171"/>
-      <c r="D1966" s="172"/>
-      <c r="E1966" s="172"/>
+      <c r="C1966" s="176"/>
+      <c r="D1966" s="177"/>
+      <c r="E1966" s="177"/>
     </row>
     <row r="1967" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1967" s="84">
@@ -23227,9 +23226,9 @@
         <v>141</v>
       </c>
       <c r="B1983" s="87"/>
-      <c r="C1983" s="171"/>
-      <c r="D1983" s="172"/>
-      <c r="E1983" s="172"/>
+      <c r="C1983" s="176"/>
+      <c r="D1983" s="177"/>
+      <c r="E1983" s="177"/>
     </row>
     <row r="1984" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1984" s="84">
@@ -23380,9 +23379,9 @@
         <v>142</v>
       </c>
       <c r="B2000" s="87"/>
-      <c r="C2000" s="171"/>
-      <c r="D2000" s="172"/>
-      <c r="E2000" s="172"/>
+      <c r="C2000" s="176"/>
+      <c r="D2000" s="177"/>
+      <c r="E2000" s="177"/>
     </row>
     <row r="2001" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2001" s="84">
@@ -23533,9 +23532,9 @@
         <v>143</v>
       </c>
       <c r="B2017" s="87"/>
-      <c r="C2017" s="171"/>
-      <c r="D2017" s="172"/>
-      <c r="E2017" s="172"/>
+      <c r="C2017" s="176"/>
+      <c r="D2017" s="177"/>
+      <c r="E2017" s="177"/>
     </row>
     <row r="2018" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2018" s="84">
@@ -23686,9 +23685,9 @@
         <v>144</v>
       </c>
       <c r="B2034" s="87"/>
-      <c r="C2034" s="171"/>
-      <c r="D2034" s="172"/>
-      <c r="E2034" s="172"/>
+      <c r="C2034" s="176"/>
+      <c r="D2034" s="177"/>
+      <c r="E2034" s="177"/>
     </row>
     <row r="2035" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2035" s="84">
@@ -23839,9 +23838,9 @@
         <v>145</v>
       </c>
       <c r="B2051" s="87"/>
-      <c r="C2051" s="171"/>
-      <c r="D2051" s="172"/>
-      <c r="E2051" s="172"/>
+      <c r="C2051" s="176"/>
+      <c r="D2051" s="177"/>
+      <c r="E2051" s="177"/>
     </row>
     <row r="2052" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2052" s="84">
@@ -23992,9 +23991,9 @@
         <v>146</v>
       </c>
       <c r="B2068" s="87"/>
-      <c r="C2068" s="171"/>
-      <c r="D2068" s="172"/>
-      <c r="E2068" s="172"/>
+      <c r="C2068" s="176"/>
+      <c r="D2068" s="177"/>
+      <c r="E2068" s="177"/>
     </row>
     <row r="2069" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2069" s="84">
@@ -24145,9 +24144,9 @@
         <v>147</v>
       </c>
       <c r="B2085" s="87"/>
-      <c r="C2085" s="171"/>
-      <c r="D2085" s="172"/>
-      <c r="E2085" s="172"/>
+      <c r="C2085" s="176"/>
+      <c r="D2085" s="177"/>
+      <c r="E2085" s="177"/>
     </row>
     <row r="2086" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2086" s="84">
@@ -24298,9 +24297,9 @@
         <v>148</v>
       </c>
       <c r="B2102" s="87"/>
-      <c r="C2102" s="171"/>
-      <c r="D2102" s="172"/>
-      <c r="E2102" s="172"/>
+      <c r="C2102" s="176"/>
+      <c r="D2102" s="177"/>
+      <c r="E2102" s="177"/>
     </row>
     <row r="2103" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2103" s="84">
@@ -24451,9 +24450,9 @@
         <v>97</v>
       </c>
       <c r="B2119" s="87"/>
-      <c r="C2119" s="171"/>
-      <c r="D2119" s="172"/>
-      <c r="E2119" s="172"/>
+      <c r="C2119" s="176"/>
+      <c r="D2119" s="177"/>
+      <c r="E2119" s="177"/>
     </row>
     <row r="2120" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2120" s="84">
@@ -24604,9 +24603,9 @@
         <v>149</v>
       </c>
       <c r="B2136" s="87"/>
-      <c r="C2136" s="171"/>
-      <c r="D2136" s="172"/>
-      <c r="E2136" s="172"/>
+      <c r="C2136" s="176"/>
+      <c r="D2136" s="177"/>
+      <c r="E2136" s="177"/>
     </row>
     <row r="2137" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2137" s="84">
@@ -24757,9 +24756,9 @@
         <v>150</v>
       </c>
       <c r="B2153" s="87"/>
-      <c r="C2153" s="171"/>
-      <c r="D2153" s="172"/>
-      <c r="E2153" s="172"/>
+      <c r="C2153" s="176"/>
+      <c r="D2153" s="177"/>
+      <c r="E2153" s="177"/>
     </row>
     <row r="2154" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2154" s="84">
@@ -24910,9 +24909,9 @@
         <v>151</v>
       </c>
       <c r="B2170" s="87"/>
-      <c r="C2170" s="171"/>
-      <c r="D2170" s="172"/>
-      <c r="E2170" s="172"/>
+      <c r="C2170" s="176"/>
+      <c r="D2170" s="177"/>
+      <c r="E2170" s="177"/>
     </row>
     <row r="2171" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2171" s="84">
@@ -25060,26 +25059,111 @@
     </row>
   </sheetData>
   <mergeCells count="137">
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="C89:E89"/>
-    <mergeCell ref="C21:E21"/>
-    <mergeCell ref="C38:E38"/>
-    <mergeCell ref="C55:E55"/>
-    <mergeCell ref="C72:E72"/>
-    <mergeCell ref="C208:E208"/>
-    <mergeCell ref="C225:E225"/>
-    <mergeCell ref="C242:E242"/>
-    <mergeCell ref="C259:E259"/>
-    <mergeCell ref="C276:E276"/>
-    <mergeCell ref="C277:E277"/>
-    <mergeCell ref="C106:E106"/>
-    <mergeCell ref="C123:E123"/>
-    <mergeCell ref="C140:E140"/>
-    <mergeCell ref="C157:E157"/>
-    <mergeCell ref="C174:E174"/>
-    <mergeCell ref="C191:E191"/>
+    <mergeCell ref="C2034:E2034"/>
+    <mergeCell ref="C2051:E2051"/>
+    <mergeCell ref="C2068:E2068"/>
+    <mergeCell ref="C2085:E2085"/>
+    <mergeCell ref="C2170:E2170"/>
+    <mergeCell ref="C2102:E2102"/>
+    <mergeCell ref="C2119:E2119"/>
+    <mergeCell ref="C2136:E2136"/>
+    <mergeCell ref="C2153:E2153"/>
+    <mergeCell ref="C1932:E1932"/>
+    <mergeCell ref="C1949:E1949"/>
+    <mergeCell ref="C1966:E1966"/>
+    <mergeCell ref="C1983:E1983"/>
+    <mergeCell ref="C2000:E2000"/>
+    <mergeCell ref="C2017:E2017"/>
+    <mergeCell ref="C1846:E1846"/>
+    <mergeCell ref="C1863:E1863"/>
+    <mergeCell ref="C1880:E1880"/>
+    <mergeCell ref="C1897:E1897"/>
+    <mergeCell ref="C1914:E1914"/>
+    <mergeCell ref="C1915:E1915"/>
+    <mergeCell ref="C1744:E1744"/>
+    <mergeCell ref="C1761:E1761"/>
+    <mergeCell ref="C1778:E1778"/>
+    <mergeCell ref="C1795:E1795"/>
+    <mergeCell ref="C1812:E1812"/>
+    <mergeCell ref="C1829:E1829"/>
+    <mergeCell ref="C1642:E1642"/>
+    <mergeCell ref="C1659:E1659"/>
+    <mergeCell ref="C1676:E1676"/>
+    <mergeCell ref="C1693:E1693"/>
+    <mergeCell ref="C1710:E1710"/>
+    <mergeCell ref="C1727:E1727"/>
+    <mergeCell ref="C1556:E1556"/>
+    <mergeCell ref="C1573:E1573"/>
+    <mergeCell ref="C1590:E1590"/>
+    <mergeCell ref="C1607:E1607"/>
+    <mergeCell ref="C1624:E1624"/>
+    <mergeCell ref="C1641:E1641"/>
+    <mergeCell ref="C1454:E1454"/>
+    <mergeCell ref="C1471:E1471"/>
+    <mergeCell ref="C1488:E1488"/>
+    <mergeCell ref="C1505:E1505"/>
+    <mergeCell ref="C1522:E1522"/>
+    <mergeCell ref="C1539:E1539"/>
+    <mergeCell ref="C1368:E1368"/>
+    <mergeCell ref="C1369:E1369"/>
+    <mergeCell ref="C1386:E1386"/>
+    <mergeCell ref="C1403:E1403"/>
+    <mergeCell ref="C1420:E1420"/>
+    <mergeCell ref="C1437:E1437"/>
+    <mergeCell ref="C1266:E1266"/>
+    <mergeCell ref="C1283:E1283"/>
+    <mergeCell ref="C1300:E1300"/>
+    <mergeCell ref="C1317:E1317"/>
+    <mergeCell ref="C1334:E1334"/>
+    <mergeCell ref="C1351:E1351"/>
+    <mergeCell ref="C1164:E1164"/>
+    <mergeCell ref="C1181:E1181"/>
+    <mergeCell ref="C1198:E1198"/>
+    <mergeCell ref="C1215:E1215"/>
+    <mergeCell ref="C1232:E1232"/>
+    <mergeCell ref="C1249:E1249"/>
+    <mergeCell ref="C1078:E1078"/>
+    <mergeCell ref="C1095:E1095"/>
+    <mergeCell ref="C1096:E1096"/>
+    <mergeCell ref="C1113:E1113"/>
+    <mergeCell ref="C1130:E1130"/>
+    <mergeCell ref="C1147:E1147"/>
+    <mergeCell ref="C976:E976"/>
+    <mergeCell ref="C993:E993"/>
+    <mergeCell ref="C1010:E1010"/>
+    <mergeCell ref="C1027:E1027"/>
+    <mergeCell ref="C1044:E1044"/>
+    <mergeCell ref="C1061:E1061"/>
+    <mergeCell ref="C874:E874"/>
+    <mergeCell ref="C891:E891"/>
+    <mergeCell ref="C908:E908"/>
+    <mergeCell ref="C925:E925"/>
+    <mergeCell ref="C942:E942"/>
+    <mergeCell ref="C959:E959"/>
+    <mergeCell ref="C788:E788"/>
+    <mergeCell ref="C805:E805"/>
+    <mergeCell ref="C822:E822"/>
+    <mergeCell ref="C823:E823"/>
+    <mergeCell ref="C840:E840"/>
+    <mergeCell ref="C857:E857"/>
+    <mergeCell ref="C686:E686"/>
+    <mergeCell ref="C703:E703"/>
+    <mergeCell ref="C720:E720"/>
+    <mergeCell ref="C737:E737"/>
+    <mergeCell ref="C754:E754"/>
+    <mergeCell ref="C771:E771"/>
+    <mergeCell ref="C584:E584"/>
+    <mergeCell ref="C601:E601"/>
+    <mergeCell ref="C618:E618"/>
+    <mergeCell ref="C635:E635"/>
+    <mergeCell ref="C652:E652"/>
+    <mergeCell ref="C669:E669"/>
+    <mergeCell ref="C498:E498"/>
+    <mergeCell ref="C515:E515"/>
+    <mergeCell ref="C532:E532"/>
+    <mergeCell ref="C549:E549"/>
+    <mergeCell ref="C550:E550"/>
+    <mergeCell ref="C567:E567"/>
     <mergeCell ref="C396:E396"/>
     <mergeCell ref="C413:E413"/>
     <mergeCell ref="C430:E430"/>
@@ -25092,111 +25176,26 @@
     <mergeCell ref="C345:E345"/>
     <mergeCell ref="C362:E362"/>
     <mergeCell ref="C379:E379"/>
-    <mergeCell ref="C584:E584"/>
-    <mergeCell ref="C601:E601"/>
-    <mergeCell ref="C618:E618"/>
-    <mergeCell ref="C635:E635"/>
-    <mergeCell ref="C652:E652"/>
-    <mergeCell ref="C669:E669"/>
-    <mergeCell ref="C498:E498"/>
-    <mergeCell ref="C515:E515"/>
-    <mergeCell ref="C532:E532"/>
-    <mergeCell ref="C549:E549"/>
-    <mergeCell ref="C550:E550"/>
-    <mergeCell ref="C567:E567"/>
-    <mergeCell ref="C788:E788"/>
-    <mergeCell ref="C805:E805"/>
-    <mergeCell ref="C822:E822"/>
-    <mergeCell ref="C823:E823"/>
-    <mergeCell ref="C840:E840"/>
-    <mergeCell ref="C857:E857"/>
-    <mergeCell ref="C686:E686"/>
-    <mergeCell ref="C703:E703"/>
-    <mergeCell ref="C720:E720"/>
-    <mergeCell ref="C737:E737"/>
-    <mergeCell ref="C754:E754"/>
-    <mergeCell ref="C771:E771"/>
-    <mergeCell ref="C976:E976"/>
-    <mergeCell ref="C993:E993"/>
-    <mergeCell ref="C1010:E1010"/>
-    <mergeCell ref="C1027:E1027"/>
-    <mergeCell ref="C1044:E1044"/>
-    <mergeCell ref="C1061:E1061"/>
-    <mergeCell ref="C874:E874"/>
-    <mergeCell ref="C891:E891"/>
-    <mergeCell ref="C908:E908"/>
-    <mergeCell ref="C925:E925"/>
-    <mergeCell ref="C942:E942"/>
-    <mergeCell ref="C959:E959"/>
-    <mergeCell ref="C1164:E1164"/>
-    <mergeCell ref="C1181:E1181"/>
-    <mergeCell ref="C1198:E1198"/>
-    <mergeCell ref="C1215:E1215"/>
-    <mergeCell ref="C1232:E1232"/>
-    <mergeCell ref="C1249:E1249"/>
-    <mergeCell ref="C1078:E1078"/>
-    <mergeCell ref="C1095:E1095"/>
-    <mergeCell ref="C1096:E1096"/>
-    <mergeCell ref="C1113:E1113"/>
-    <mergeCell ref="C1130:E1130"/>
-    <mergeCell ref="C1147:E1147"/>
-    <mergeCell ref="C1368:E1368"/>
-    <mergeCell ref="C1369:E1369"/>
-    <mergeCell ref="C1386:E1386"/>
-    <mergeCell ref="C1403:E1403"/>
-    <mergeCell ref="C1420:E1420"/>
-    <mergeCell ref="C1437:E1437"/>
-    <mergeCell ref="C1266:E1266"/>
-    <mergeCell ref="C1283:E1283"/>
-    <mergeCell ref="C1300:E1300"/>
-    <mergeCell ref="C1317:E1317"/>
-    <mergeCell ref="C1334:E1334"/>
-    <mergeCell ref="C1351:E1351"/>
-    <mergeCell ref="C1556:E1556"/>
-    <mergeCell ref="C1573:E1573"/>
-    <mergeCell ref="C1590:E1590"/>
-    <mergeCell ref="C1607:E1607"/>
-    <mergeCell ref="C1624:E1624"/>
-    <mergeCell ref="C1641:E1641"/>
-    <mergeCell ref="C1454:E1454"/>
-    <mergeCell ref="C1471:E1471"/>
-    <mergeCell ref="C1488:E1488"/>
-    <mergeCell ref="C1505:E1505"/>
-    <mergeCell ref="C1522:E1522"/>
-    <mergeCell ref="C1539:E1539"/>
-    <mergeCell ref="C1744:E1744"/>
-    <mergeCell ref="C1761:E1761"/>
-    <mergeCell ref="C1778:E1778"/>
-    <mergeCell ref="C1795:E1795"/>
-    <mergeCell ref="C1812:E1812"/>
-    <mergeCell ref="C1829:E1829"/>
-    <mergeCell ref="C1642:E1642"/>
-    <mergeCell ref="C1659:E1659"/>
-    <mergeCell ref="C1676:E1676"/>
-    <mergeCell ref="C1693:E1693"/>
-    <mergeCell ref="C1710:E1710"/>
-    <mergeCell ref="C1727:E1727"/>
-    <mergeCell ref="C1932:E1932"/>
-    <mergeCell ref="C1949:E1949"/>
-    <mergeCell ref="C1966:E1966"/>
-    <mergeCell ref="C1983:E1983"/>
-    <mergeCell ref="C2000:E2000"/>
-    <mergeCell ref="C2017:E2017"/>
-    <mergeCell ref="C1846:E1846"/>
-    <mergeCell ref="C1863:E1863"/>
-    <mergeCell ref="C1880:E1880"/>
-    <mergeCell ref="C1897:E1897"/>
-    <mergeCell ref="C1914:E1914"/>
-    <mergeCell ref="C1915:E1915"/>
-    <mergeCell ref="C2034:E2034"/>
-    <mergeCell ref="C2051:E2051"/>
-    <mergeCell ref="C2068:E2068"/>
-    <mergeCell ref="C2085:E2085"/>
-    <mergeCell ref="C2170:E2170"/>
-    <mergeCell ref="C2102:E2102"/>
-    <mergeCell ref="C2119:E2119"/>
-    <mergeCell ref="C2136:E2136"/>
-    <mergeCell ref="C2153:E2153"/>
+    <mergeCell ref="C225:E225"/>
+    <mergeCell ref="C242:E242"/>
+    <mergeCell ref="C259:E259"/>
+    <mergeCell ref="C276:E276"/>
+    <mergeCell ref="C277:E277"/>
+    <mergeCell ref="C106:E106"/>
+    <mergeCell ref="C123:E123"/>
+    <mergeCell ref="C140:E140"/>
+    <mergeCell ref="C157:E157"/>
+    <mergeCell ref="C174:E174"/>
+    <mergeCell ref="C191:E191"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="C89:E89"/>
+    <mergeCell ref="C21:E21"/>
+    <mergeCell ref="C38:E38"/>
+    <mergeCell ref="C55:E55"/>
+    <mergeCell ref="C72:E72"/>
+    <mergeCell ref="C208:E208"/>
   </mergeCells>
   <phoneticPr fontId="13" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -25223,51 +25222,51 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="24" thickBot="1">
-      <c r="A1" s="198" t="s">
+      <c r="A1" s="200" t="s">
         <v>156</v>
       </c>
-      <c r="B1" s="198"/>
-      <c r="C1" s="198"/>
-      <c r="D1" s="198"/>
-      <c r="E1" s="198"/>
-      <c r="F1" s="198"/>
-      <c r="G1" s="198"/>
-      <c r="H1" s="198"/>
-      <c r="I1" s="198"/>
-      <c r="J1" s="198"/>
-      <c r="K1" s="198"/>
-      <c r="L1" s="198"/>
+      <c r="B1" s="200"/>
+      <c r="C1" s="200"/>
+      <c r="D1" s="200"/>
+      <c r="E1" s="200"/>
+      <c r="F1" s="200"/>
+      <c r="G1" s="200"/>
+      <c r="H1" s="200"/>
+      <c r="I1" s="200"/>
+      <c r="J1" s="200"/>
+      <c r="K1" s="200"/>
+      <c r="L1" s="200"/>
     </row>
     <row r="2" spans="1:12" ht="18.75" thickBot="1">
-      <c r="A2" s="195" t="s">
+      <c r="A2" s="197" t="s">
         <v>157</v>
       </c>
-      <c r="B2" s="196"/>
-      <c r="C2" s="196"/>
-      <c r="D2" s="196"/>
-      <c r="E2" s="196"/>
-      <c r="F2" s="196"/>
-      <c r="G2" s="196"/>
-      <c r="H2" s="196"/>
-      <c r="I2" s="196"/>
-      <c r="J2" s="196"/>
-      <c r="K2" s="196"/>
-      <c r="L2" s="197"/>
+      <c r="B2" s="198"/>
+      <c r="C2" s="198"/>
+      <c r="D2" s="198"/>
+      <c r="E2" s="198"/>
+      <c r="F2" s="198"/>
+      <c r="G2" s="198"/>
+      <c r="H2" s="198"/>
+      <c r="I2" s="198"/>
+      <c r="J2" s="198"/>
+      <c r="K2" s="198"/>
+      <c r="L2" s="199"/>
     </row>
     <row r="3" spans="1:12" s="31" customFormat="1" ht="16.5" customHeight="1" thickBot="1">
-      <c r="A3" s="192" t="s">
+      <c r="A3" s="194" t="s">
         <v>158</v>
       </c>
-      <c r="B3" s="193"/>
-      <c r="C3" s="193"/>
-      <c r="D3" s="193"/>
-      <c r="E3" s="193"/>
-      <c r="F3" s="193"/>
-      <c r="G3" s="193"/>
-      <c r="H3" s="193"/>
-      <c r="I3" s="193"/>
-      <c r="J3" s="193"/>
-      <c r="K3" s="194"/>
+      <c r="B3" s="195"/>
+      <c r="C3" s="195"/>
+      <c r="D3" s="195"/>
+      <c r="E3" s="195"/>
+      <c r="F3" s="195"/>
+      <c r="G3" s="195"/>
+      <c r="H3" s="195"/>
+      <c r="I3" s="195"/>
+      <c r="J3" s="195"/>
+      <c r="K3" s="196"/>
     </row>
     <row r="4" spans="1:12" s="27" customFormat="1">
       <c r="A4" s="28" t="s">
@@ -25484,19 +25483,19 @@
       <c r="K19" s="2"/>
     </row>
     <row r="20" spans="1:11" ht="18" customHeight="1" thickBot="1">
-      <c r="A20" s="192" t="s">
+      <c r="A20" s="194" t="s">
         <v>166</v>
       </c>
-      <c r="B20" s="193"/>
-      <c r="C20" s="193"/>
-      <c r="D20" s="193"/>
-      <c r="E20" s="193"/>
-      <c r="F20" s="193"/>
-      <c r="G20" s="193"/>
-      <c r="H20" s="193"/>
-      <c r="I20" s="193"/>
-      <c r="J20" s="193"/>
-      <c r="K20" s="194"/>
+      <c r="B20" s="195"/>
+      <c r="C20" s="195"/>
+      <c r="D20" s="195"/>
+      <c r="E20" s="195"/>
+      <c r="F20" s="195"/>
+      <c r="G20" s="195"/>
+      <c r="H20" s="195"/>
+      <c r="I20" s="195"/>
+      <c r="J20" s="195"/>
+      <c r="K20" s="196"/>
     </row>
     <row r="21" spans="1:11">
       <c r="A21" s="28" t="s">
@@ -25713,19 +25712,19 @@
       <c r="K36" s="2"/>
     </row>
     <row r="37" spans="1:11" ht="18" customHeight="1" thickBot="1">
-      <c r="A37" s="192" t="s">
+      <c r="A37" s="194" t="s">
         <v>167</v>
       </c>
-      <c r="B37" s="193"/>
-      <c r="C37" s="193"/>
-      <c r="D37" s="193"/>
-      <c r="E37" s="193"/>
-      <c r="F37" s="193"/>
-      <c r="G37" s="193"/>
-      <c r="H37" s="193"/>
-      <c r="I37" s="193"/>
-      <c r="J37" s="193"/>
-      <c r="K37" s="194"/>
+      <c r="B37" s="195"/>
+      <c r="C37" s="195"/>
+      <c r="D37" s="195"/>
+      <c r="E37" s="195"/>
+      <c r="F37" s="195"/>
+      <c r="G37" s="195"/>
+      <c r="H37" s="195"/>
+      <c r="I37" s="195"/>
+      <c r="J37" s="195"/>
+      <c r="K37" s="196"/>
     </row>
     <row r="38" spans="1:11">
       <c r="A38" s="28" t="s">
@@ -25983,28 +25982,28 @@
       </c>
     </row>
     <row r="3" spans="1:1">
-      <c r="A3" s="199"/>
+      <c r="A3" s="201"/>
     </row>
     <row r="4" spans="1:1">
-      <c r="A4" s="200"/>
+      <c r="A4" s="202"/>
     </row>
     <row r="5" spans="1:1">
-      <c r="A5" s="200"/>
+      <c r="A5" s="202"/>
     </row>
     <row r="6" spans="1:1">
-      <c r="A6" s="200"/>
+      <c r="A6" s="202"/>
     </row>
     <row r="7" spans="1:1">
-      <c r="A7" s="200"/>
+      <c r="A7" s="202"/>
     </row>
     <row r="8" spans="1:1">
-      <c r="A8" s="200"/>
+      <c r="A8" s="202"/>
     </row>
     <row r="9" spans="1:1">
-      <c r="A9" s="200"/>
+      <c r="A9" s="202"/>
     </row>
     <row r="10" spans="1:1" ht="13.5" thickBot="1">
-      <c r="A10" s="201"/>
+      <c r="A10" s="203"/>
     </row>
     <row r="11" spans="1:1" ht="27" customHeight="1">
       <c r="A11" s="22" t="s">
@@ -26187,10 +26186,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="4" customFormat="1" ht="25.5" customHeight="1" thickBot="1">
-      <c r="B1" s="202" t="s">
+      <c r="B1" s="204" t="s">
         <v>162</v>
       </c>
-      <c r="C1" s="203"/>
+      <c r="C1" s="205"/>
       <c r="D1" s="92"/>
       <c r="E1" s="32"/>
     </row>
@@ -26201,7 +26200,7 @@
       <c r="E2" s="119"/>
     </row>
     <row r="3" spans="1:5" ht="12.75" customHeight="1">
-      <c r="A3" s="204" t="s">
+      <c r="A3" s="206" t="s">
         <v>202</v>
       </c>
       <c r="B3" s="131" t="s">
@@ -26215,7 +26214,7 @@
       <c r="E3" s="5"/>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="205"/>
+      <c r="A4" s="207"/>
       <c r="B4" s="128" t="s">
         <v>159</v>
       </c>
@@ -26227,7 +26226,7 @@
       <c r="E4" s="5"/>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="205"/>
+      <c r="A5" s="207"/>
       <c r="B5" s="128" t="s">
         <v>160</v>
       </c>
@@ -26236,7 +26235,7 @@
       <c r="E5" s="5"/>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="205"/>
+      <c r="A6" s="207"/>
       <c r="B6" s="139" t="s">
         <v>204</v>
       </c>
@@ -26248,7 +26247,7 @@
       <c r="E6" s="5"/>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="205"/>
+      <c r="A7" s="207"/>
       <c r="B7" s="128" t="s">
         <v>171</v>
       </c>
@@ -26260,7 +26259,7 @@
       <c r="E7" s="5"/>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="205"/>
+      <c r="A8" s="207"/>
       <c r="B8" s="128" t="s">
         <v>172</v>
       </c>
@@ -26269,7 +26268,7 @@
       <c r="E8" s="5"/>
     </row>
     <row r="9" spans="1:5" ht="13.5" thickBot="1">
-      <c r="A9" s="206"/>
+      <c r="A9" s="208"/>
       <c r="B9" s="136" t="s">
         <v>161</v>
       </c>
@@ -26284,7 +26283,7 @@
       <c r="E10" s="94"/>
     </row>
     <row r="11" spans="1:5" ht="19.5" customHeight="1">
-      <c r="A11" s="204" t="s">
+      <c r="A11" s="206" t="s">
         <v>203</v>
       </c>
       <c r="B11" s="131" t="s">
@@ -26298,7 +26297,7 @@
       <c r="E11" s="5"/>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="205"/>
+      <c r="A12" s="207"/>
       <c r="B12" s="128" t="s">
         <v>159</v>
       </c>
@@ -26310,7 +26309,7 @@
       <c r="E12" s="5"/>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" s="205"/>
+      <c r="A13" s="207"/>
       <c r="B13" s="128" t="s">
         <v>160</v>
       </c>
@@ -26319,7 +26318,7 @@
       <c r="E13" s="5"/>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="205"/>
+      <c r="A14" s="207"/>
       <c r="B14" s="139" t="s">
         <v>204</v>
       </c>
@@ -26331,7 +26330,7 @@
       <c r="E14" s="5"/>
     </row>
     <row r="15" spans="1:5">
-      <c r="A15" s="205"/>
+      <c r="A15" s="207"/>
       <c r="B15" s="128" t="s">
         <v>171</v>
       </c>
@@ -26343,7 +26342,7 @@
       <c r="E15" s="5"/>
     </row>
     <row r="16" spans="1:5">
-      <c r="A16" s="205"/>
+      <c r="A16" s="207"/>
       <c r="B16" s="128" t="s">
         <v>172</v>
       </c>
@@ -26352,7 +26351,7 @@
       <c r="E16" s="5"/>
     </row>
     <row r="17" spans="1:5" ht="13.5" thickBot="1">
-      <c r="A17" s="206"/>
+      <c r="A17" s="208"/>
       <c r="B17" s="136" t="s">
         <v>161</v>
       </c>
@@ -26367,7 +26366,7 @@
       <c r="E18" s="94"/>
     </row>
     <row r="19" spans="1:5" collapsed="1">
-      <c r="A19" s="204" t="s">
+      <c r="A19" s="206" t="s">
         <v>203</v>
       </c>
       <c r="B19" s="131" t="s">
@@ -26376,7 +26375,7 @@
       <c r="C19" s="130"/>
     </row>
     <row r="20" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A20" s="205"/>
+      <c r="A20" s="207"/>
       <c r="B20" s="128" t="s">
         <v>159</v>
       </c>
@@ -26386,14 +26385,14 @@
       </c>
     </row>
     <row r="21" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A21" s="205"/>
+      <c r="A21" s="207"/>
       <c r="B21" s="128" t="s">
         <v>160</v>
       </c>
       <c r="C21" s="133"/>
     </row>
     <row r="22" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A22" s="205"/>
+      <c r="A22" s="207"/>
       <c r="B22" s="139" t="s">
         <v>204</v>
       </c>
@@ -26403,7 +26402,7 @@
       </c>
     </row>
     <row r="23" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A23" s="205"/>
+      <c r="A23" s="207"/>
       <c r="B23" s="128" t="s">
         <v>171</v>
       </c>
@@ -26413,14 +26412,14 @@
       </c>
     </row>
     <row r="24" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A24" s="205"/>
+      <c r="A24" s="207"/>
       <c r="B24" s="128" t="s">
         <v>172</v>
       </c>
       <c r="C24" s="132"/>
     </row>
     <row r="25" spans="1:5" ht="13.5" thickBot="1">
-      <c r="A25" s="206"/>
+      <c r="A25" s="208"/>
       <c r="B25" s="136" t="s">
         <v>161</v>
       </c>
@@ -26455,163 +26454,150 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="33">
-      <c r="A1" s="216" t="s">
+      <c r="A1" s="219" t="s">
         <v>184</v>
       </c>
-      <c r="B1" s="217"/>
+      <c r="B1" s="220"/>
       <c r="C1" s="118"/>
       <c r="D1" s="5"/>
       <c r="E1" s="5"/>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="213" t="s">
+      <c r="A2" s="225" t="s">
         <v>183</v>
       </c>
-      <c r="B2" s="214"/>
+      <c r="B2" s="226"/>
       <c r="C2" s="120"/>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="215" t="s">
+      <c r="A3" s="227" t="s">
         <v>185</v>
       </c>
-      <c r="B3" s="214"/>
+      <c r="B3" s="226"/>
       <c r="C3" s="120"/>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="220"/>
-      <c r="B4" s="221"/>
+      <c r="A4" s="223"/>
+      <c r="B4" s="224"/>
       <c r="C4" s="120"/>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="218" t="s">
+      <c r="A5" s="221" t="s">
         <v>194</v>
       </c>
-      <c r="B5" s="219"/>
+      <c r="B5" s="222"/>
       <c r="C5" s="120"/>
     </row>
     <row r="7" spans="1:5" ht="18.75">
-      <c r="A7" s="224" t="s">
+      <c r="A7" s="213" t="s">
         <v>186</v>
       </c>
-      <c r="B7" s="225"/>
+      <c r="B7" s="214"/>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="120"/>
       <c r="B8" s="9"/>
     </row>
     <row r="9" spans="1:5" ht="39" customHeight="1">
-      <c r="A9" s="222" t="s">
+      <c r="A9" s="215" t="s">
         <v>187</v>
       </c>
-      <c r="B9" s="223"/>
+      <c r="B9" s="216"/>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="209"/>
-      <c r="B10" s="210"/>
+      <c r="A10" s="217"/>
+      <c r="B10" s="218"/>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="211" t="s">
+      <c r="A11" s="209" t="s">
         <v>188</v>
       </c>
-      <c r="B11" s="212"/>
+      <c r="B11" s="210"/>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="211" t="s">
+      <c r="A12" s="209" t="s">
         <v>189</v>
       </c>
-      <c r="B12" s="212"/>
+      <c r="B12" s="210"/>
     </row>
     <row r="13" spans="1:5" ht="43.5" customHeight="1">
-      <c r="A13" s="211" t="s">
+      <c r="A13" s="209" t="s">
         <v>190</v>
       </c>
-      <c r="B13" s="212"/>
+      <c r="B13" s="210"/>
     </row>
     <row r="14" spans="1:5" ht="19.5" customHeight="1">
-      <c r="A14" s="211" t="s">
+      <c r="A14" s="209" t="s">
         <v>191</v>
       </c>
-      <c r="B14" s="212"/>
+      <c r="B14" s="210"/>
     </row>
     <row r="15" spans="1:5" ht="18" customHeight="1">
-      <c r="A15" s="211" t="s">
+      <c r="A15" s="209" t="s">
         <v>192</v>
       </c>
-      <c r="B15" s="212"/>
+      <c r="B15" s="210"/>
     </row>
     <row r="16" spans="1:5" ht="21" customHeight="1">
-      <c r="A16" s="211" t="s">
+      <c r="A16" s="209" t="s">
         <v>193</v>
       </c>
-      <c r="B16" s="212"/>
+      <c r="B16" s="210"/>
     </row>
     <row r="17" spans="1:2" ht="48.75" customHeight="1">
-      <c r="A17" s="207" t="s">
+      <c r="A17" s="211" t="s">
         <v>195</v>
       </c>
-      <c r="B17" s="208"/>
+      <c r="B17" s="212"/>
     </row>
     <row r="19" spans="1:2" ht="18.75">
-      <c r="A19" s="224" t="s">
+      <c r="A19" s="213" t="s">
         <v>197</v>
       </c>
-      <c r="B19" s="225"/>
+      <c r="B19" s="214"/>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="120"/>
       <c r="B20" s="9"/>
     </row>
     <row r="21" spans="1:2">
-      <c r="A21" s="222" t="s">
+      <c r="A21" s="215" t="s">
         <v>198</v>
       </c>
-      <c r="B21" s="223"/>
+      <c r="B21" s="216"/>
     </row>
     <row r="22" spans="1:2">
-      <c r="A22" s="209"/>
-      <c r="B22" s="210"/>
+      <c r="A22" s="217"/>
+      <c r="B22" s="218"/>
     </row>
     <row r="23" spans="1:2">
-      <c r="A23" s="211" t="s">
+      <c r="A23" s="209" t="s">
         <v>199</v>
       </c>
-      <c r="B23" s="212"/>
+      <c r="B23" s="210"/>
     </row>
     <row r="24" spans="1:2">
-      <c r="A24" s="211"/>
-      <c r="B24" s="212"/>
+      <c r="A24" s="209"/>
+      <c r="B24" s="210"/>
     </row>
     <row r="25" spans="1:2">
-      <c r="A25" s="211" t="s">
+      <c r="A25" s="209" t="s">
         <v>200</v>
       </c>
-      <c r="B25" s="212"/>
+      <c r="B25" s="210"/>
     </row>
     <row r="26" spans="1:2">
-      <c r="A26" s="211" t="s">
+      <c r="A26" s="209" t="s">
         <v>201</v>
       </c>
-      <c r="B26" s="212"/>
+      <c r="B26" s="210"/>
     </row>
     <row r="27" spans="1:2">
-      <c r="A27" s="207"/>
-      <c r="B27" s="208"/>
+      <c r="A27" s="211"/>
+      <c r="B27" s="212"/>
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A7:B7"/>
     <mergeCell ref="A17:B17"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
@@ -26622,6 +26608,19 @@
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="A14:B14"/>
     <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A24:B24"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A3" r:id="rId1"/>

</xml_diff>

<commit_message>
Tempo - Cicus Stage 3 done.
</commit_message>
<xml_diff>
--- a/trunk/Tempo/Tempo.xlsx
+++ b/trunk/Tempo/Tempo.xlsx
@@ -2251,29 +2251,29 @@
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="25" fillId="13" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="26" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="25" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="26" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="23" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="24" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="21" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="22" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="14" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="21" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="22" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="23" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="24" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="25" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="26" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="25" fillId="13" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="26" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="16" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="16" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="16" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -2309,34 +2309,20 @@
     <xf numFmtId="0" fontId="55" fillId="22" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="52" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="53" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="53" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="51" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="51" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="49" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="4"/>
     </xf>
@@ -2346,6 +2332,20 @@
     <xf numFmtId="0" fontId="50" fillId="0" borderId="33" xfId="3" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" indent="4"/>
     </xf>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="51" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="51" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="53" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="53" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Accent1" xfId="2" builtinId="29"/>
@@ -2657,7 +2657,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A87" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C97" sqref="C97"/>
+      <selection pane="bottomLeft" activeCell="C101" sqref="C101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" outlineLevelRow="2"/>
@@ -4370,13 +4370,15 @@
       <c r="B98" s="151" t="s">
         <v>222</v>
       </c>
-      <c r="C98" s="101"/>
+      <c r="C98" s="101">
+        <v>34305</v>
+      </c>
       <c r="D98" s="101">
         <v>43241</v>
       </c>
       <c r="E98" s="123">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>8936</v>
       </c>
       <c r="F98" s="105"/>
     </row>
@@ -4396,13 +4398,15 @@
       <c r="B100" s="152" t="s">
         <v>236</v>
       </c>
-      <c r="C100" s="101"/>
+      <c r="C100" s="101">
+        <v>36049</v>
+      </c>
       <c r="D100" s="101">
         <v>45890</v>
       </c>
       <c r="E100" s="123">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>9841</v>
       </c>
       <c r="F100" s="105"/>
     </row>
@@ -5324,11 +5328,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="A152:A166"/>
-    <mergeCell ref="A123:A132"/>
-    <mergeCell ref="A93:A107"/>
-    <mergeCell ref="A135:A149"/>
-    <mergeCell ref="A110:A120"/>
     <mergeCell ref="A43:A70"/>
     <mergeCell ref="A73:A90"/>
     <mergeCell ref="C5:D5"/>
@@ -5338,6 +5337,11 @@
     <mergeCell ref="A8:A18"/>
     <mergeCell ref="A21:A40"/>
     <mergeCell ref="C4:E4"/>
+    <mergeCell ref="A152:A166"/>
+    <mergeCell ref="A123:A132"/>
+    <mergeCell ref="A93:A107"/>
+    <mergeCell ref="A135:A149"/>
+    <mergeCell ref="A110:A120"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -5369,13 +5373,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="26.25" customHeight="1">
-      <c r="A1" s="173" t="s">
+      <c r="A1" s="191" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="173"/>
-      <c r="C1" s="173"/>
-      <c r="D1" s="173"/>
-      <c r="E1" s="173"/>
+      <c r="B1" s="191"/>
+      <c r="C1" s="191"/>
+      <c r="D1" s="191"/>
+      <c r="E1" s="191"/>
       <c r="F1" s="7"/>
       <c r="G1" s="5"/>
       <c r="H1" s="5"/>
@@ -5405,18 +5409,18 @@
         <v>8</v>
       </c>
       <c r="B3" s="36"/>
-      <c r="C3" s="174"/>
-      <c r="D3" s="175"/>
-      <c r="E3" s="175"/>
+      <c r="C3" s="192"/>
+      <c r="D3" s="193"/>
+      <c r="E3" s="193"/>
     </row>
     <row r="4" spans="1:8" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A4" s="46" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="87"/>
-      <c r="C4" s="176"/>
-      <c r="D4" s="177"/>
-      <c r="E4" s="177"/>
+      <c r="C4" s="173"/>
+      <c r="D4" s="174"/>
+      <c r="E4" s="174"/>
       <c r="F4" s="6"/>
     </row>
     <row r="5" spans="1:8" hidden="1" outlineLevel="2">
@@ -5568,9 +5572,9 @@
         <v>9</v>
       </c>
       <c r="B21" s="90"/>
-      <c r="C21" s="178"/>
-      <c r="D21" s="179"/>
-      <c r="E21" s="179"/>
+      <c r="C21" s="175"/>
+      <c r="D21" s="176"/>
+      <c r="E21" s="176"/>
     </row>
     <row r="22" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A22" s="47">
@@ -5721,9 +5725,9 @@
         <v>10</v>
       </c>
       <c r="B38" s="87"/>
-      <c r="C38" s="176"/>
-      <c r="D38" s="177"/>
-      <c r="E38" s="177"/>
+      <c r="C38" s="173"/>
+      <c r="D38" s="174"/>
+      <c r="E38" s="174"/>
     </row>
     <row r="39" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A39" s="47">
@@ -5874,9 +5878,9 @@
         <v>11</v>
       </c>
       <c r="B55" s="87"/>
-      <c r="C55" s="176"/>
-      <c r="D55" s="177"/>
-      <c r="E55" s="177"/>
+      <c r="C55" s="173"/>
+      <c r="D55" s="174"/>
+      <c r="E55" s="174"/>
     </row>
     <row r="56" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A56" s="47">
@@ -6027,9 +6031,9 @@
         <v>12</v>
       </c>
       <c r="B72" s="87"/>
-      <c r="C72" s="176"/>
-      <c r="D72" s="177"/>
-      <c r="E72" s="177"/>
+      <c r="C72" s="173"/>
+      <c r="D72" s="174"/>
+      <c r="E72" s="174"/>
     </row>
     <row r="73" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A73" s="47">
@@ -6180,9 +6184,9 @@
         <v>13</v>
       </c>
       <c r="B89" s="87"/>
-      <c r="C89" s="176"/>
-      <c r="D89" s="177"/>
-      <c r="E89" s="177"/>
+      <c r="C89" s="173"/>
+      <c r="D89" s="174"/>
+      <c r="E89" s="174"/>
     </row>
     <row r="90" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A90" s="47">
@@ -6333,9 +6337,9 @@
         <v>14</v>
       </c>
       <c r="B106" s="87"/>
-      <c r="C106" s="176"/>
-      <c r="D106" s="177"/>
-      <c r="E106" s="177"/>
+      <c r="C106" s="173"/>
+      <c r="D106" s="174"/>
+      <c r="E106" s="174"/>
     </row>
     <row r="107" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A107" s="47">
@@ -6486,9 +6490,9 @@
         <v>15</v>
       </c>
       <c r="B123" s="87"/>
-      <c r="C123" s="176"/>
-      <c r="D123" s="177"/>
-      <c r="E123" s="177"/>
+      <c r="C123" s="173"/>
+      <c r="D123" s="174"/>
+      <c r="E123" s="174"/>
     </row>
     <row r="124" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A124" s="47">
@@ -6639,9 +6643,9 @@
         <v>16</v>
       </c>
       <c r="B140" s="87"/>
-      <c r="C140" s="176"/>
-      <c r="D140" s="177"/>
-      <c r="E140" s="177"/>
+      <c r="C140" s="173"/>
+      <c r="D140" s="174"/>
+      <c r="E140" s="174"/>
     </row>
     <row r="141" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A141" s="47">
@@ -6792,9 +6796,9 @@
         <v>17</v>
       </c>
       <c r="B157" s="87"/>
-      <c r="C157" s="176"/>
-      <c r="D157" s="177"/>
-      <c r="E157" s="177"/>
+      <c r="C157" s="173"/>
+      <c r="D157" s="174"/>
+      <c r="E157" s="174"/>
     </row>
     <row r="158" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A158" s="47">
@@ -6945,9 +6949,9 @@
         <v>18</v>
       </c>
       <c r="B174" s="87"/>
-      <c r="C174" s="176"/>
-      <c r="D174" s="177"/>
-      <c r="E174" s="177"/>
+      <c r="C174" s="173"/>
+      <c r="D174" s="174"/>
+      <c r="E174" s="174"/>
     </row>
     <row r="175" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A175" s="47">
@@ -7098,9 +7102,9 @@
         <v>19</v>
       </c>
       <c r="B191" s="87"/>
-      <c r="C191" s="176"/>
-      <c r="D191" s="177"/>
-      <c r="E191" s="177"/>
+      <c r="C191" s="173"/>
+      <c r="D191" s="174"/>
+      <c r="E191" s="174"/>
     </row>
     <row r="192" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A192" s="47">
@@ -7251,9 +7255,9 @@
         <v>20</v>
       </c>
       <c r="B208" s="87"/>
-      <c r="C208" s="176"/>
-      <c r="D208" s="177"/>
-      <c r="E208" s="177"/>
+      <c r="C208" s="173"/>
+      <c r="D208" s="174"/>
+      <c r="E208" s="174"/>
     </row>
     <row r="209" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A209" s="47">
@@ -7404,9 +7408,9 @@
         <v>21</v>
       </c>
       <c r="B225" s="87"/>
-      <c r="C225" s="176"/>
-      <c r="D225" s="177"/>
-      <c r="E225" s="177"/>
+      <c r="C225" s="173"/>
+      <c r="D225" s="174"/>
+      <c r="E225" s="174"/>
     </row>
     <row r="226" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A226" s="47">
@@ -7557,9 +7561,9 @@
         <v>22</v>
       </c>
       <c r="B242" s="87"/>
-      <c r="C242" s="176"/>
-      <c r="D242" s="177"/>
-      <c r="E242" s="177"/>
+      <c r="C242" s="173"/>
+      <c r="D242" s="174"/>
+      <c r="E242" s="174"/>
     </row>
     <row r="243" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A243" s="47">
@@ -7710,9 +7714,9 @@
         <v>23</v>
       </c>
       <c r="B259" s="87"/>
-      <c r="C259" s="176"/>
-      <c r="D259" s="177"/>
-      <c r="E259" s="177"/>
+      <c r="C259" s="173"/>
+      <c r="D259" s="174"/>
+      <c r="E259" s="174"/>
     </row>
     <row r="260" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A260" s="47">
@@ -7863,18 +7867,18 @@
         <v>24</v>
       </c>
       <c r="B276" s="37"/>
-      <c r="C276" s="180"/>
-      <c r="D276" s="181"/>
-      <c r="E276" s="181"/>
+      <c r="C276" s="189"/>
+      <c r="D276" s="190"/>
+      <c r="E276" s="190"/>
     </row>
     <row r="277" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A277" s="51" t="s">
         <v>25</v>
       </c>
       <c r="B277" s="87"/>
-      <c r="C277" s="176"/>
-      <c r="D277" s="177"/>
-      <c r="E277" s="177"/>
+      <c r="C277" s="173"/>
+      <c r="D277" s="174"/>
+      <c r="E277" s="174"/>
     </row>
     <row r="278" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A278" s="52">
@@ -8025,9 +8029,9 @@
         <v>26</v>
       </c>
       <c r="B294" s="90"/>
-      <c r="C294" s="178"/>
-      <c r="D294" s="179"/>
-      <c r="E294" s="179"/>
+      <c r="C294" s="175"/>
+      <c r="D294" s="176"/>
+      <c r="E294" s="176"/>
     </row>
     <row r="295" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A295" s="52">
@@ -8178,9 +8182,9 @@
         <v>27</v>
       </c>
       <c r="B311" s="87"/>
-      <c r="C311" s="176"/>
-      <c r="D311" s="177"/>
-      <c r="E311" s="177"/>
+      <c r="C311" s="173"/>
+      <c r="D311" s="174"/>
+      <c r="E311" s="174"/>
     </row>
     <row r="312" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A312" s="52">
@@ -8331,9 +8335,9 @@
         <v>28</v>
       </c>
       <c r="B328" s="87"/>
-      <c r="C328" s="176"/>
-      <c r="D328" s="177"/>
-      <c r="E328" s="177"/>
+      <c r="C328" s="173"/>
+      <c r="D328" s="174"/>
+      <c r="E328" s="174"/>
     </row>
     <row r="329" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A329" s="52">
@@ -8484,9 +8488,9 @@
         <v>29</v>
       </c>
       <c r="B345" s="87"/>
-      <c r="C345" s="176"/>
-      <c r="D345" s="177"/>
-      <c r="E345" s="177"/>
+      <c r="C345" s="173"/>
+      <c r="D345" s="174"/>
+      <c r="E345" s="174"/>
     </row>
     <row r="346" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A346" s="52">
@@ -8637,9 +8641,9 @@
         <v>30</v>
       </c>
       <c r="B362" s="87"/>
-      <c r="C362" s="176"/>
-      <c r="D362" s="177"/>
-      <c r="E362" s="177"/>
+      <c r="C362" s="173"/>
+      <c r="D362" s="174"/>
+      <c r="E362" s="174"/>
     </row>
     <row r="363" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A363" s="52">
@@ -8790,9 +8794,9 @@
         <v>31</v>
       </c>
       <c r="B379" s="87"/>
-      <c r="C379" s="176"/>
-      <c r="D379" s="177"/>
-      <c r="E379" s="177"/>
+      <c r="C379" s="173"/>
+      <c r="D379" s="174"/>
+      <c r="E379" s="174"/>
     </row>
     <row r="380" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A380" s="52">
@@ -8943,9 +8947,9 @@
         <v>32</v>
       </c>
       <c r="B396" s="87"/>
-      <c r="C396" s="176"/>
-      <c r="D396" s="177"/>
-      <c r="E396" s="177"/>
+      <c r="C396" s="173"/>
+      <c r="D396" s="174"/>
+      <c r="E396" s="174"/>
     </row>
     <row r="397" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A397" s="52">
@@ -9096,9 +9100,9 @@
         <v>33</v>
       </c>
       <c r="B413" s="87"/>
-      <c r="C413" s="176"/>
-      <c r="D413" s="177"/>
-      <c r="E413" s="177"/>
+      <c r="C413" s="173"/>
+      <c r="D413" s="174"/>
+      <c r="E413" s="174"/>
     </row>
     <row r="414" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A414" s="52">
@@ -9249,9 +9253,9 @@
         <v>34</v>
       </c>
       <c r="B430" s="87"/>
-      <c r="C430" s="176"/>
-      <c r="D430" s="177"/>
-      <c r="E430" s="177"/>
+      <c r="C430" s="173"/>
+      <c r="D430" s="174"/>
+      <c r="E430" s="174"/>
     </row>
     <row r="431" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A431" s="52">
@@ -9402,9 +9406,9 @@
         <v>35</v>
       </c>
       <c r="B447" s="87"/>
-      <c r="C447" s="176"/>
-      <c r="D447" s="177"/>
-      <c r="E447" s="177"/>
+      <c r="C447" s="173"/>
+      <c r="D447" s="174"/>
+      <c r="E447" s="174"/>
     </row>
     <row r="448" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A448" s="52">
@@ -9555,9 +9559,9 @@
         <v>36</v>
       </c>
       <c r="B464" s="87"/>
-      <c r="C464" s="176"/>
-      <c r="D464" s="177"/>
-      <c r="E464" s="177"/>
+      <c r="C464" s="173"/>
+      <c r="D464" s="174"/>
+      <c r="E464" s="174"/>
     </row>
     <row r="465" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A465" s="52">
@@ -9708,9 +9712,9 @@
         <v>37</v>
       </c>
       <c r="B481" s="87"/>
-      <c r="C481" s="176"/>
-      <c r="D481" s="177"/>
-      <c r="E481" s="177"/>
+      <c r="C481" s="173"/>
+      <c r="D481" s="174"/>
+      <c r="E481" s="174"/>
     </row>
     <row r="482" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A482" s="52">
@@ -9861,9 +9865,9 @@
         <v>38</v>
       </c>
       <c r="B498" s="87"/>
-      <c r="C498" s="176"/>
-      <c r="D498" s="177"/>
-      <c r="E498" s="177"/>
+      <c r="C498" s="173"/>
+      <c r="D498" s="174"/>
+      <c r="E498" s="174"/>
     </row>
     <row r="499" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A499" s="52">
@@ -10014,9 +10018,9 @@
         <v>39</v>
       </c>
       <c r="B515" s="87"/>
-      <c r="C515" s="176"/>
-      <c r="D515" s="177"/>
-      <c r="E515" s="177"/>
+      <c r="C515" s="173"/>
+      <c r="D515" s="174"/>
+      <c r="E515" s="174"/>
     </row>
     <row r="516" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A516" s="52">
@@ -10167,9 +10171,9 @@
         <v>40</v>
       </c>
       <c r="B532" s="87"/>
-      <c r="C532" s="176"/>
-      <c r="D532" s="177"/>
-      <c r="E532" s="177"/>
+      <c r="C532" s="173"/>
+      <c r="D532" s="174"/>
+      <c r="E532" s="174"/>
     </row>
     <row r="533" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A533" s="55">
@@ -10320,18 +10324,18 @@
         <v>50</v>
       </c>
       <c r="B549" s="38"/>
-      <c r="C549" s="182"/>
-      <c r="D549" s="183"/>
-      <c r="E549" s="183"/>
+      <c r="C549" s="187"/>
+      <c r="D549" s="188"/>
+      <c r="E549" s="188"/>
     </row>
     <row r="550" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A550" s="58" t="s">
         <v>51</v>
       </c>
       <c r="B550" s="87"/>
-      <c r="C550" s="176"/>
-      <c r="D550" s="177"/>
-      <c r="E550" s="177"/>
+      <c r="C550" s="173"/>
+      <c r="D550" s="174"/>
+      <c r="E550" s="174"/>
     </row>
     <row r="551" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A551" s="59">
@@ -10482,9 +10486,9 @@
         <v>52</v>
       </c>
       <c r="B567" s="90"/>
-      <c r="C567" s="178"/>
-      <c r="D567" s="179"/>
-      <c r="E567" s="179"/>
+      <c r="C567" s="175"/>
+      <c r="D567" s="176"/>
+      <c r="E567" s="176"/>
     </row>
     <row r="568" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A568" s="59">
@@ -10635,9 +10639,9 @@
         <v>53</v>
       </c>
       <c r="B584" s="87"/>
-      <c r="C584" s="176"/>
-      <c r="D584" s="177"/>
-      <c r="E584" s="177"/>
+      <c r="C584" s="173"/>
+      <c r="D584" s="174"/>
+      <c r="E584" s="174"/>
     </row>
     <row r="585" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A585" s="59">
@@ -10788,9 +10792,9 @@
         <v>54</v>
       </c>
       <c r="B601" s="87"/>
-      <c r="C601" s="176"/>
-      <c r="D601" s="177"/>
-      <c r="E601" s="177"/>
+      <c r="C601" s="173"/>
+      <c r="D601" s="174"/>
+      <c r="E601" s="174"/>
     </row>
     <row r="602" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A602" s="59">
@@ -10941,9 +10945,9 @@
         <v>55</v>
       </c>
       <c r="B618" s="87"/>
-      <c r="C618" s="176"/>
-      <c r="D618" s="177"/>
-      <c r="E618" s="177"/>
+      <c r="C618" s="173"/>
+      <c r="D618" s="174"/>
+      <c r="E618" s="174"/>
     </row>
     <row r="619" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A619" s="59">
@@ -11094,9 +11098,9 @@
         <v>56</v>
       </c>
       <c r="B635" s="87"/>
-      <c r="C635" s="176"/>
-      <c r="D635" s="177"/>
-      <c r="E635" s="177"/>
+      <c r="C635" s="173"/>
+      <c r="D635" s="174"/>
+      <c r="E635" s="174"/>
     </row>
     <row r="636" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A636" s="59">
@@ -11247,9 +11251,9 @@
         <v>57</v>
       </c>
       <c r="B652" s="87"/>
-      <c r="C652" s="176"/>
-      <c r="D652" s="177"/>
-      <c r="E652" s="177"/>
+      <c r="C652" s="173"/>
+      <c r="D652" s="174"/>
+      <c r="E652" s="174"/>
     </row>
     <row r="653" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A653" s="59">
@@ -11400,9 +11404,9 @@
         <v>58</v>
       </c>
       <c r="B669" s="87"/>
-      <c r="C669" s="176"/>
-      <c r="D669" s="177"/>
-      <c r="E669" s="177"/>
+      <c r="C669" s="173"/>
+      <c r="D669" s="174"/>
+      <c r="E669" s="174"/>
     </row>
     <row r="670" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A670" s="59">
@@ -11553,9 +11557,9 @@
         <v>59</v>
       </c>
       <c r="B686" s="87"/>
-      <c r="C686" s="176"/>
-      <c r="D686" s="177"/>
-      <c r="E686" s="177"/>
+      <c r="C686" s="173"/>
+      <c r="D686" s="174"/>
+      <c r="E686" s="174"/>
     </row>
     <row r="687" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A687" s="59">
@@ -11706,9 +11710,9 @@
         <v>60</v>
       </c>
       <c r="B703" s="87"/>
-      <c r="C703" s="176"/>
-      <c r="D703" s="177"/>
-      <c r="E703" s="177"/>
+      <c r="C703" s="173"/>
+      <c r="D703" s="174"/>
+      <c r="E703" s="174"/>
     </row>
     <row r="704" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A704" s="59">
@@ -11859,9 +11863,9 @@
         <v>61</v>
       </c>
       <c r="B720" s="87"/>
-      <c r="C720" s="176"/>
-      <c r="D720" s="177"/>
-      <c r="E720" s="177"/>
+      <c r="C720" s="173"/>
+      <c r="D720" s="174"/>
+      <c r="E720" s="174"/>
     </row>
     <row r="721" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A721" s="59">
@@ -12012,9 +12016,9 @@
         <v>62</v>
       </c>
       <c r="B737" s="87"/>
-      <c r="C737" s="176"/>
-      <c r="D737" s="177"/>
-      <c r="E737" s="177"/>
+      <c r="C737" s="173"/>
+      <c r="D737" s="174"/>
+      <c r="E737" s="174"/>
     </row>
     <row r="738" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A738" s="59">
@@ -12165,9 +12169,9 @@
         <v>63</v>
       </c>
       <c r="B754" s="87"/>
-      <c r="C754" s="176"/>
-      <c r="D754" s="177"/>
-      <c r="E754" s="177"/>
+      <c r="C754" s="173"/>
+      <c r="D754" s="174"/>
+      <c r="E754" s="174"/>
     </row>
     <row r="755" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A755" s="59">
@@ -12318,9 +12322,9 @@
         <v>64</v>
       </c>
       <c r="B771" s="87"/>
-      <c r="C771" s="176"/>
-      <c r="D771" s="177"/>
-      <c r="E771" s="177"/>
+      <c r="C771" s="173"/>
+      <c r="D771" s="174"/>
+      <c r="E771" s="174"/>
     </row>
     <row r="772" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A772" s="59">
@@ -12471,9 +12475,9 @@
         <v>65</v>
       </c>
       <c r="B788" s="87"/>
-      <c r="C788" s="176"/>
-      <c r="D788" s="177"/>
-      <c r="E788" s="177"/>
+      <c r="C788" s="173"/>
+      <c r="D788" s="174"/>
+      <c r="E788" s="174"/>
     </row>
     <row r="789" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A789" s="59">
@@ -12624,9 +12628,9 @@
         <v>66</v>
       </c>
       <c r="B805" s="87"/>
-      <c r="C805" s="176"/>
-      <c r="D805" s="177"/>
-      <c r="E805" s="177"/>
+      <c r="C805" s="173"/>
+      <c r="D805" s="174"/>
+      <c r="E805" s="174"/>
     </row>
     <row r="806" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A806" s="59">
@@ -12777,18 +12781,18 @@
         <v>67</v>
       </c>
       <c r="B822" s="39"/>
-      <c r="C822" s="184"/>
-      <c r="D822" s="185"/>
-      <c r="E822" s="185"/>
+      <c r="C822" s="185"/>
+      <c r="D822" s="186"/>
+      <c r="E822" s="186"/>
     </row>
     <row r="823" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A823" s="63" t="s">
         <v>68</v>
       </c>
       <c r="B823" s="87"/>
-      <c r="C823" s="176"/>
-      <c r="D823" s="177"/>
-      <c r="E823" s="177"/>
+      <c r="C823" s="173"/>
+      <c r="D823" s="174"/>
+      <c r="E823" s="174"/>
     </row>
     <row r="824" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A824" s="64">
@@ -12939,9 +12943,9 @@
         <v>69</v>
       </c>
       <c r="B840" s="90"/>
-      <c r="C840" s="178"/>
-      <c r="D840" s="179"/>
-      <c r="E840" s="179"/>
+      <c r="C840" s="175"/>
+      <c r="D840" s="176"/>
+      <c r="E840" s="176"/>
     </row>
     <row r="841" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A841" s="64">
@@ -13092,9 +13096,9 @@
         <v>70</v>
       </c>
       <c r="B857" s="87"/>
-      <c r="C857" s="176"/>
-      <c r="D857" s="177"/>
-      <c r="E857" s="177"/>
+      <c r="C857" s="173"/>
+      <c r="D857" s="174"/>
+      <c r="E857" s="174"/>
     </row>
     <row r="858" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A858" s="64">
@@ -13245,9 +13249,9 @@
         <v>71</v>
       </c>
       <c r="B874" s="87"/>
-      <c r="C874" s="176"/>
-      <c r="D874" s="177"/>
-      <c r="E874" s="177"/>
+      <c r="C874" s="173"/>
+      <c r="D874" s="174"/>
+      <c r="E874" s="174"/>
     </row>
     <row r="875" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A875" s="64">
@@ -13398,9 +13402,9 @@
         <v>72</v>
       </c>
       <c r="B891" s="87"/>
-      <c r="C891" s="176"/>
-      <c r="D891" s="177"/>
-      <c r="E891" s="177"/>
+      <c r="C891" s="173"/>
+      <c r="D891" s="174"/>
+      <c r="E891" s="174"/>
     </row>
     <row r="892" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A892" s="64">
@@ -13551,9 +13555,9 @@
         <v>73</v>
       </c>
       <c r="B908" s="87"/>
-      <c r="C908" s="176"/>
-      <c r="D908" s="177"/>
-      <c r="E908" s="177"/>
+      <c r="C908" s="173"/>
+      <c r="D908" s="174"/>
+      <c r="E908" s="174"/>
     </row>
     <row r="909" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A909" s="64">
@@ -13704,9 +13708,9 @@
         <v>74</v>
       </c>
       <c r="B925" s="87"/>
-      <c r="C925" s="176"/>
-      <c r="D925" s="177"/>
-      <c r="E925" s="177"/>
+      <c r="C925" s="173"/>
+      <c r="D925" s="174"/>
+      <c r="E925" s="174"/>
     </row>
     <row r="926" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A926" s="64">
@@ -13857,9 +13861,9 @@
         <v>75</v>
       </c>
       <c r="B942" s="87"/>
-      <c r="C942" s="176"/>
-      <c r="D942" s="177"/>
-      <c r="E942" s="177"/>
+      <c r="C942" s="173"/>
+      <c r="D942" s="174"/>
+      <c r="E942" s="174"/>
     </row>
     <row r="943" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A943" s="64">
@@ -14010,9 +14014,9 @@
         <v>76</v>
       </c>
       <c r="B959" s="87"/>
-      <c r="C959" s="176"/>
-      <c r="D959" s="177"/>
-      <c r="E959" s="177"/>
+      <c r="C959" s="173"/>
+      <c r="D959" s="174"/>
+      <c r="E959" s="174"/>
     </row>
     <row r="960" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A960" s="64">
@@ -14163,9 +14167,9 @@
         <v>77</v>
       </c>
       <c r="B976" s="87"/>
-      <c r="C976" s="176"/>
-      <c r="D976" s="177"/>
-      <c r="E976" s="177"/>
+      <c r="C976" s="173"/>
+      <c r="D976" s="174"/>
+      <c r="E976" s="174"/>
     </row>
     <row r="977" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A977" s="64">
@@ -14316,9 +14320,9 @@
         <v>78</v>
       </c>
       <c r="B993" s="87"/>
-      <c r="C993" s="176"/>
-      <c r="D993" s="177"/>
-      <c r="E993" s="177"/>
+      <c r="C993" s="173"/>
+      <c r="D993" s="174"/>
+      <c r="E993" s="174"/>
     </row>
     <row r="994" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A994" s="64">
@@ -14469,9 +14473,9 @@
         <v>79</v>
       </c>
       <c r="B1010" s="87"/>
-      <c r="C1010" s="176"/>
-      <c r="D1010" s="177"/>
-      <c r="E1010" s="177"/>
+      <c r="C1010" s="173"/>
+      <c r="D1010" s="174"/>
+      <c r="E1010" s="174"/>
     </row>
     <row r="1011" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1011" s="64">
@@ -14622,9 +14626,9 @@
         <v>80</v>
       </c>
       <c r="B1027" s="87"/>
-      <c r="C1027" s="176"/>
-      <c r="D1027" s="177"/>
-      <c r="E1027" s="177"/>
+      <c r="C1027" s="173"/>
+      <c r="D1027" s="174"/>
+      <c r="E1027" s="174"/>
     </row>
     <row r="1028" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1028" s="64">
@@ -14775,9 +14779,9 @@
         <v>83</v>
       </c>
       <c r="B1044" s="87"/>
-      <c r="C1044" s="176"/>
-      <c r="D1044" s="177"/>
-      <c r="E1044" s="177"/>
+      <c r="C1044" s="173"/>
+      <c r="D1044" s="174"/>
+      <c r="E1044" s="174"/>
     </row>
     <row r="1045" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1045" s="64">
@@ -14928,9 +14932,9 @@
         <v>82</v>
       </c>
       <c r="B1061" s="87"/>
-      <c r="C1061" s="176"/>
-      <c r="D1061" s="177"/>
-      <c r="E1061" s="177"/>
+      <c r="C1061" s="173"/>
+      <c r="D1061" s="174"/>
+      <c r="E1061" s="174"/>
     </row>
     <row r="1062" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1062" s="64">
@@ -15081,9 +15085,9 @@
         <v>84</v>
       </c>
       <c r="B1078" s="87"/>
-      <c r="C1078" s="176"/>
-      <c r="D1078" s="177"/>
-      <c r="E1078" s="177"/>
+      <c r="C1078" s="173"/>
+      <c r="D1078" s="174"/>
+      <c r="E1078" s="174"/>
     </row>
     <row r="1079" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1079" s="64">
@@ -15234,18 +15238,18 @@
         <v>104</v>
       </c>
       <c r="B1095" s="40"/>
-      <c r="C1095" s="186"/>
-      <c r="D1095" s="187"/>
-      <c r="E1095" s="187"/>
+      <c r="C1095" s="183"/>
+      <c r="D1095" s="184"/>
+      <c r="E1095" s="184"/>
     </row>
     <row r="1096" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A1096" s="68" t="s">
         <v>85</v>
       </c>
       <c r="B1096" s="87"/>
-      <c r="C1096" s="176"/>
-      <c r="D1096" s="177"/>
-      <c r="E1096" s="177"/>
+      <c r="C1096" s="173"/>
+      <c r="D1096" s="174"/>
+      <c r="E1096" s="174"/>
     </row>
     <row r="1097" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1097" s="69">
@@ -15396,9 +15400,9 @@
         <v>86</v>
       </c>
       <c r="B1113" s="90"/>
-      <c r="C1113" s="178"/>
-      <c r="D1113" s="179"/>
-      <c r="E1113" s="179"/>
+      <c r="C1113" s="175"/>
+      <c r="D1113" s="176"/>
+      <c r="E1113" s="176"/>
     </row>
     <row r="1114" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1114" s="69">
@@ -15549,9 +15553,9 @@
         <v>87</v>
       </c>
       <c r="B1130" s="87"/>
-      <c r="C1130" s="176"/>
-      <c r="D1130" s="177"/>
-      <c r="E1130" s="177"/>
+      <c r="C1130" s="173"/>
+      <c r="D1130" s="174"/>
+      <c r="E1130" s="174"/>
     </row>
     <row r="1131" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1131" s="69">
@@ -15702,9 +15706,9 @@
         <v>88</v>
       </c>
       <c r="B1147" s="87"/>
-      <c r="C1147" s="176"/>
-      <c r="D1147" s="177"/>
-      <c r="E1147" s="177"/>
+      <c r="C1147" s="173"/>
+      <c r="D1147" s="174"/>
+      <c r="E1147" s="174"/>
     </row>
     <row r="1148" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1148" s="69">
@@ -15855,9 +15859,9 @@
         <v>89</v>
       </c>
       <c r="B1164" s="87"/>
-      <c r="C1164" s="176"/>
-      <c r="D1164" s="177"/>
-      <c r="E1164" s="177"/>
+      <c r="C1164" s="173"/>
+      <c r="D1164" s="174"/>
+      <c r="E1164" s="174"/>
     </row>
     <row r="1165" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1165" s="69">
@@ -16008,9 +16012,9 @@
         <v>90</v>
       </c>
       <c r="B1181" s="87"/>
-      <c r="C1181" s="176"/>
-      <c r="D1181" s="177"/>
-      <c r="E1181" s="177"/>
+      <c r="C1181" s="173"/>
+      <c r="D1181" s="174"/>
+      <c r="E1181" s="174"/>
     </row>
     <row r="1182" spans="1:5" hidden="1" outlineLevel="3">
       <c r="A1182" s="69">
@@ -16161,9 +16165,9 @@
         <v>91</v>
       </c>
       <c r="B1198" s="87"/>
-      <c r="C1198" s="176"/>
-      <c r="D1198" s="177"/>
-      <c r="E1198" s="177"/>
+      <c r="C1198" s="173"/>
+      <c r="D1198" s="174"/>
+      <c r="E1198" s="174"/>
     </row>
     <row r="1199" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1199" s="69">
@@ -16314,9 +16318,9 @@
         <v>92</v>
       </c>
       <c r="B1215" s="87"/>
-      <c r="C1215" s="176"/>
-      <c r="D1215" s="177"/>
-      <c r="E1215" s="177"/>
+      <c r="C1215" s="173"/>
+      <c r="D1215" s="174"/>
+      <c r="E1215" s="174"/>
     </row>
     <row r="1216" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1216" s="69">
@@ -16467,9 +16471,9 @@
         <v>93</v>
       </c>
       <c r="B1232" s="87"/>
-      <c r="C1232" s="176"/>
-      <c r="D1232" s="177"/>
-      <c r="E1232" s="177"/>
+      <c r="C1232" s="173"/>
+      <c r="D1232" s="174"/>
+      <c r="E1232" s="174"/>
     </row>
     <row r="1233" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1233" s="69">
@@ -16620,9 +16624,9 @@
         <v>94</v>
       </c>
       <c r="B1249" s="87"/>
-      <c r="C1249" s="176"/>
-      <c r="D1249" s="177"/>
-      <c r="E1249" s="177"/>
+      <c r="C1249" s="173"/>
+      <c r="D1249" s="174"/>
+      <c r="E1249" s="174"/>
     </row>
     <row r="1250" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1250" s="69">
@@ -16773,9 +16777,9 @@
         <v>99</v>
       </c>
       <c r="B1266" s="87"/>
-      <c r="C1266" s="176"/>
-      <c r="D1266" s="177"/>
-      <c r="E1266" s="177"/>
+      <c r="C1266" s="173"/>
+      <c r="D1266" s="174"/>
+      <c r="E1266" s="174"/>
     </row>
     <row r="1267" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1267" s="69">
@@ -16926,9 +16930,9 @@
         <v>100</v>
       </c>
       <c r="B1283" s="87"/>
-      <c r="C1283" s="176"/>
-      <c r="D1283" s="177"/>
-      <c r="E1283" s="177"/>
+      <c r="C1283" s="173"/>
+      <c r="D1283" s="174"/>
+      <c r="E1283" s="174"/>
     </row>
     <row r="1284" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1284" s="69">
@@ -17079,9 +17083,9 @@
         <v>101</v>
       </c>
       <c r="B1300" s="87"/>
-      <c r="C1300" s="176"/>
-      <c r="D1300" s="177"/>
-      <c r="E1300" s="177"/>
+      <c r="C1300" s="173"/>
+      <c r="D1300" s="174"/>
+      <c r="E1300" s="174"/>
     </row>
     <row r="1301" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1301" s="69">
@@ -17232,9 +17236,9 @@
         <v>81</v>
       </c>
       <c r="B1317" s="87"/>
-      <c r="C1317" s="176"/>
-      <c r="D1317" s="177"/>
-      <c r="E1317" s="177"/>
+      <c r="C1317" s="173"/>
+      <c r="D1317" s="174"/>
+      <c r="E1317" s="174"/>
     </row>
     <row r="1318" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1318" s="69">
@@ -17385,9 +17389,9 @@
         <v>102</v>
       </c>
       <c r="B1334" s="87"/>
-      <c r="C1334" s="176"/>
-      <c r="D1334" s="177"/>
-      <c r="E1334" s="177"/>
+      <c r="C1334" s="173"/>
+      <c r="D1334" s="174"/>
+      <c r="E1334" s="174"/>
     </row>
     <row r="1335" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1335" s="69">
@@ -17538,9 +17542,9 @@
         <v>98</v>
       </c>
       <c r="B1351" s="87"/>
-      <c r="C1351" s="176"/>
-      <c r="D1351" s="177"/>
-      <c r="E1351" s="177"/>
+      <c r="C1351" s="173"/>
+      <c r="D1351" s="174"/>
+      <c r="E1351" s="174"/>
     </row>
     <row r="1352" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1352" s="69">
@@ -17691,18 +17695,18 @@
         <v>103</v>
       </c>
       <c r="B1368" s="41"/>
-      <c r="C1368" s="188"/>
-      <c r="D1368" s="189"/>
-      <c r="E1368" s="189"/>
+      <c r="C1368" s="181"/>
+      <c r="D1368" s="182"/>
+      <c r="E1368" s="182"/>
     </row>
     <row r="1369" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A1369" s="73" t="s">
         <v>105</v>
       </c>
       <c r="B1369" s="87"/>
-      <c r="C1369" s="176"/>
-      <c r="D1369" s="177"/>
-      <c r="E1369" s="177"/>
+      <c r="C1369" s="173"/>
+      <c r="D1369" s="174"/>
+      <c r="E1369" s="174"/>
     </row>
     <row r="1370" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1370" s="74">
@@ -17853,9 +17857,9 @@
         <v>106</v>
       </c>
       <c r="B1386" s="90"/>
-      <c r="C1386" s="178"/>
-      <c r="D1386" s="179"/>
-      <c r="E1386" s="179"/>
+      <c r="C1386" s="175"/>
+      <c r="D1386" s="176"/>
+      <c r="E1386" s="176"/>
     </row>
     <row r="1387" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1387" s="74">
@@ -18006,9 +18010,9 @@
         <v>107</v>
       </c>
       <c r="B1403" s="87"/>
-      <c r="C1403" s="176"/>
-      <c r="D1403" s="177"/>
-      <c r="E1403" s="177"/>
+      <c r="C1403" s="173"/>
+      <c r="D1403" s="174"/>
+      <c r="E1403" s="174"/>
     </row>
     <row r="1404" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1404" s="74">
@@ -18159,9 +18163,9 @@
         <v>108</v>
       </c>
       <c r="B1420" s="87"/>
-      <c r="C1420" s="176"/>
-      <c r="D1420" s="177"/>
-      <c r="E1420" s="177"/>
+      <c r="C1420" s="173"/>
+      <c r="D1420" s="174"/>
+      <c r="E1420" s="174"/>
     </row>
     <row r="1421" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1421" s="74">
@@ -18312,9 +18316,9 @@
         <v>109</v>
       </c>
       <c r="B1437" s="87"/>
-      <c r="C1437" s="176"/>
-      <c r="D1437" s="177"/>
-      <c r="E1437" s="177"/>
+      <c r="C1437" s="173"/>
+      <c r="D1437" s="174"/>
+      <c r="E1437" s="174"/>
     </row>
     <row r="1438" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1438" s="74">
@@ -18465,9 +18469,9 @@
         <v>110</v>
       </c>
       <c r="B1454" s="87"/>
-      <c r="C1454" s="176"/>
-      <c r="D1454" s="177"/>
-      <c r="E1454" s="177"/>
+      <c r="C1454" s="173"/>
+      <c r="D1454" s="174"/>
+      <c r="E1454" s="174"/>
     </row>
     <row r="1455" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1455" s="74">
@@ -18618,9 +18622,9 @@
         <v>111</v>
       </c>
       <c r="B1471" s="87"/>
-      <c r="C1471" s="176"/>
-      <c r="D1471" s="177"/>
-      <c r="E1471" s="177"/>
+      <c r="C1471" s="173"/>
+      <c r="D1471" s="174"/>
+      <c r="E1471" s="174"/>
     </row>
     <row r="1472" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1472" s="74">
@@ -18771,9 +18775,9 @@
         <v>112</v>
       </c>
       <c r="B1488" s="87"/>
-      <c r="C1488" s="176"/>
-      <c r="D1488" s="177"/>
-      <c r="E1488" s="177"/>
+      <c r="C1488" s="173"/>
+      <c r="D1488" s="174"/>
+      <c r="E1488" s="174"/>
     </row>
     <row r="1489" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1489" s="74">
@@ -18924,9 +18928,9 @@
         <v>113</v>
       </c>
       <c r="B1505" s="87"/>
-      <c r="C1505" s="176"/>
-      <c r="D1505" s="177"/>
-      <c r="E1505" s="177"/>
+      <c r="C1505" s="173"/>
+      <c r="D1505" s="174"/>
+      <c r="E1505" s="174"/>
     </row>
     <row r="1506" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1506" s="74">
@@ -19077,9 +19081,9 @@
         <v>114</v>
       </c>
       <c r="B1522" s="87"/>
-      <c r="C1522" s="176"/>
-      <c r="D1522" s="177"/>
-      <c r="E1522" s="177"/>
+      <c r="C1522" s="173"/>
+      <c r="D1522" s="174"/>
+      <c r="E1522" s="174"/>
     </row>
     <row r="1523" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1523" s="74">
@@ -19230,9 +19234,9 @@
         <v>95</v>
       </c>
       <c r="B1539" s="87"/>
-      <c r="C1539" s="176"/>
-      <c r="D1539" s="177"/>
-      <c r="E1539" s="177"/>
+      <c r="C1539" s="173"/>
+      <c r="D1539" s="174"/>
+      <c r="E1539" s="174"/>
     </row>
     <row r="1540" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1540" s="74">
@@ -19383,9 +19387,9 @@
         <v>115</v>
       </c>
       <c r="B1556" s="87"/>
-      <c r="C1556" s="176"/>
-      <c r="D1556" s="177"/>
-      <c r="E1556" s="177"/>
+      <c r="C1556" s="173"/>
+      <c r="D1556" s="174"/>
+      <c r="E1556" s="174"/>
     </row>
     <row r="1557" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1557" s="74">
@@ -19536,9 +19540,9 @@
         <v>116</v>
       </c>
       <c r="B1573" s="87"/>
-      <c r="C1573" s="176"/>
-      <c r="D1573" s="177"/>
-      <c r="E1573" s="177"/>
+      <c r="C1573" s="173"/>
+      <c r="D1573" s="174"/>
+      <c r="E1573" s="174"/>
     </row>
     <row r="1574" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1574" s="74">
@@ -19689,9 +19693,9 @@
         <v>117</v>
       </c>
       <c r="B1590" s="87"/>
-      <c r="C1590" s="176"/>
-      <c r="D1590" s="177"/>
-      <c r="E1590" s="177"/>
+      <c r="C1590" s="173"/>
+      <c r="D1590" s="174"/>
+      <c r="E1590" s="174"/>
     </row>
     <row r="1591" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1591" s="74">
@@ -19842,9 +19846,9 @@
         <v>118</v>
       </c>
       <c r="B1607" s="87"/>
-      <c r="C1607" s="176"/>
-      <c r="D1607" s="177"/>
-      <c r="E1607" s="177"/>
+      <c r="C1607" s="173"/>
+      <c r="D1607" s="174"/>
+      <c r="E1607" s="174"/>
     </row>
     <row r="1608" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1608" s="74">
@@ -19995,9 +19999,9 @@
         <v>119</v>
       </c>
       <c r="B1624" s="87"/>
-      <c r="C1624" s="176"/>
-      <c r="D1624" s="177"/>
-      <c r="E1624" s="177"/>
+      <c r="C1624" s="173"/>
+      <c r="D1624" s="174"/>
+      <c r="E1624" s="174"/>
     </row>
     <row r="1625" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1625" s="74">
@@ -20148,18 +20152,18 @@
         <v>120</v>
       </c>
       <c r="B1641" s="42"/>
-      <c r="C1641" s="190"/>
-      <c r="D1641" s="191"/>
-      <c r="E1641" s="191"/>
+      <c r="C1641" s="179"/>
+      <c r="D1641" s="180"/>
+      <c r="E1641" s="180"/>
     </row>
     <row r="1642" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A1642" s="78" t="s">
         <v>121</v>
       </c>
       <c r="B1642" s="87"/>
-      <c r="C1642" s="176"/>
-      <c r="D1642" s="177"/>
-      <c r="E1642" s="177"/>
+      <c r="C1642" s="173"/>
+      <c r="D1642" s="174"/>
+      <c r="E1642" s="174"/>
     </row>
     <row r="1643" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1643" s="79">
@@ -20310,9 +20314,9 @@
         <v>122</v>
       </c>
       <c r="B1659" s="90"/>
-      <c r="C1659" s="178"/>
-      <c r="D1659" s="179"/>
-      <c r="E1659" s="179"/>
+      <c r="C1659" s="175"/>
+      <c r="D1659" s="176"/>
+      <c r="E1659" s="176"/>
     </row>
     <row r="1660" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1660" s="79">
@@ -20463,9 +20467,9 @@
         <v>123</v>
       </c>
       <c r="B1676" s="87"/>
-      <c r="C1676" s="176"/>
-      <c r="D1676" s="177"/>
-      <c r="E1676" s="177"/>
+      <c r="C1676" s="173"/>
+      <c r="D1676" s="174"/>
+      <c r="E1676" s="174"/>
     </row>
     <row r="1677" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1677" s="79">
@@ -20616,9 +20620,9 @@
         <v>124</v>
       </c>
       <c r="B1693" s="87"/>
-      <c r="C1693" s="176"/>
-      <c r="D1693" s="177"/>
-      <c r="E1693" s="177"/>
+      <c r="C1693" s="173"/>
+      <c r="D1693" s="174"/>
+      <c r="E1693" s="174"/>
     </row>
     <row r="1694" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1694" s="79">
@@ -20769,9 +20773,9 @@
         <v>125</v>
       </c>
       <c r="B1710" s="87"/>
-      <c r="C1710" s="176"/>
-      <c r="D1710" s="177"/>
-      <c r="E1710" s="177"/>
+      <c r="C1710" s="173"/>
+      <c r="D1710" s="174"/>
+      <c r="E1710" s="174"/>
     </row>
     <row r="1711" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1711" s="79">
@@ -20922,9 +20926,9 @@
         <v>126</v>
       </c>
       <c r="B1727" s="87"/>
-      <c r="C1727" s="176"/>
-      <c r="D1727" s="177"/>
-      <c r="E1727" s="177"/>
+      <c r="C1727" s="173"/>
+      <c r="D1727" s="174"/>
+      <c r="E1727" s="174"/>
     </row>
     <row r="1728" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1728" s="79">
@@ -21075,9 +21079,9 @@
         <v>127</v>
       </c>
       <c r="B1744" s="87"/>
-      <c r="C1744" s="176"/>
-      <c r="D1744" s="177"/>
-      <c r="E1744" s="177"/>
+      <c r="C1744" s="173"/>
+      <c r="D1744" s="174"/>
+      <c r="E1744" s="174"/>
     </row>
     <row r="1745" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1745" s="79">
@@ -21228,9 +21232,9 @@
         <v>128</v>
       </c>
       <c r="B1761" s="87"/>
-      <c r="C1761" s="176"/>
-      <c r="D1761" s="177"/>
-      <c r="E1761" s="177"/>
+      <c r="C1761" s="173"/>
+      <c r="D1761" s="174"/>
+      <c r="E1761" s="174"/>
     </row>
     <row r="1762" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1762" s="79">
@@ -21381,9 +21385,9 @@
         <v>129</v>
       </c>
       <c r="B1778" s="87"/>
-      <c r="C1778" s="176"/>
-      <c r="D1778" s="177"/>
-      <c r="E1778" s="177"/>
+      <c r="C1778" s="173"/>
+      <c r="D1778" s="174"/>
+      <c r="E1778" s="174"/>
     </row>
     <row r="1779" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1779" s="79">
@@ -21534,9 +21538,9 @@
         <v>130</v>
       </c>
       <c r="B1795" s="87"/>
-      <c r="C1795" s="176"/>
-      <c r="D1795" s="177"/>
-      <c r="E1795" s="177"/>
+      <c r="C1795" s="173"/>
+      <c r="D1795" s="174"/>
+      <c r="E1795" s="174"/>
     </row>
     <row r="1796" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1796" s="79">
@@ -21687,9 +21691,9 @@
         <v>131</v>
       </c>
       <c r="B1812" s="87"/>
-      <c r="C1812" s="176"/>
-      <c r="D1812" s="177"/>
-      <c r="E1812" s="177"/>
+      <c r="C1812" s="173"/>
+      <c r="D1812" s="174"/>
+      <c r="E1812" s="174"/>
     </row>
     <row r="1813" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1813" s="79">
@@ -21840,9 +21844,9 @@
         <v>96</v>
       </c>
       <c r="B1829" s="87"/>
-      <c r="C1829" s="176"/>
-      <c r="D1829" s="177"/>
-      <c r="E1829" s="177"/>
+      <c r="C1829" s="173"/>
+      <c r="D1829" s="174"/>
+      <c r="E1829" s="174"/>
     </row>
     <row r="1830" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1830" s="79">
@@ -21993,9 +21997,9 @@
         <v>132</v>
       </c>
       <c r="B1846" s="87"/>
-      <c r="C1846" s="176"/>
-      <c r="D1846" s="177"/>
-      <c r="E1846" s="177"/>
+      <c r="C1846" s="173"/>
+      <c r="D1846" s="174"/>
+      <c r="E1846" s="174"/>
     </row>
     <row r="1847" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1847" s="79">
@@ -22146,9 +22150,9 @@
         <v>133</v>
       </c>
       <c r="B1863" s="87"/>
-      <c r="C1863" s="176"/>
-      <c r="D1863" s="177"/>
-      <c r="E1863" s="177"/>
+      <c r="C1863" s="173"/>
+      <c r="D1863" s="174"/>
+      <c r="E1863" s="174"/>
     </row>
     <row r="1864" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1864" s="79">
@@ -22299,9 +22303,9 @@
         <v>134</v>
       </c>
       <c r="B1880" s="87"/>
-      <c r="C1880" s="176"/>
-      <c r="D1880" s="177"/>
-      <c r="E1880" s="177"/>
+      <c r="C1880" s="173"/>
+      <c r="D1880" s="174"/>
+      <c r="E1880" s="174"/>
     </row>
     <row r="1881" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1881" s="79">
@@ -22452,9 +22456,9 @@
         <v>135</v>
       </c>
       <c r="B1897" s="87"/>
-      <c r="C1897" s="176"/>
-      <c r="D1897" s="177"/>
-      <c r="E1897" s="177"/>
+      <c r="C1897" s="173"/>
+      <c r="D1897" s="174"/>
+      <c r="E1897" s="174"/>
     </row>
     <row r="1898" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1898" s="79">
@@ -22605,18 +22609,18 @@
         <v>136</v>
       </c>
       <c r="B1914" s="43"/>
-      <c r="C1914" s="192"/>
-      <c r="D1914" s="193"/>
-      <c r="E1914" s="193"/>
+      <c r="C1914" s="177"/>
+      <c r="D1914" s="178"/>
+      <c r="E1914" s="178"/>
     </row>
     <row r="1915" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A1915" s="83" t="s">
         <v>137</v>
       </c>
       <c r="B1915" s="87"/>
-      <c r="C1915" s="176"/>
-      <c r="D1915" s="177"/>
-      <c r="E1915" s="177"/>
+      <c r="C1915" s="173"/>
+      <c r="D1915" s="174"/>
+      <c r="E1915" s="174"/>
     </row>
     <row r="1916" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1916" s="84">
@@ -22767,9 +22771,9 @@
         <v>138</v>
       </c>
       <c r="B1932" s="90"/>
-      <c r="C1932" s="178"/>
-      <c r="D1932" s="179"/>
-      <c r="E1932" s="179"/>
+      <c r="C1932" s="175"/>
+      <c r="D1932" s="176"/>
+      <c r="E1932" s="176"/>
     </row>
     <row r="1933" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1933" s="84">
@@ -22920,9 +22924,9 @@
         <v>139</v>
       </c>
       <c r="B1949" s="87"/>
-      <c r="C1949" s="176"/>
-      <c r="D1949" s="177"/>
-      <c r="E1949" s="177"/>
+      <c r="C1949" s="173"/>
+      <c r="D1949" s="174"/>
+      <c r="E1949" s="174"/>
     </row>
     <row r="1950" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1950" s="84">
@@ -23073,9 +23077,9 @@
         <v>140</v>
       </c>
       <c r="B1966" s="87"/>
-      <c r="C1966" s="176"/>
-      <c r="D1966" s="177"/>
-      <c r="E1966" s="177"/>
+      <c r="C1966" s="173"/>
+      <c r="D1966" s="174"/>
+      <c r="E1966" s="174"/>
     </row>
     <row r="1967" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1967" s="84">
@@ -23226,9 +23230,9 @@
         <v>141</v>
       </c>
       <c r="B1983" s="87"/>
-      <c r="C1983" s="176"/>
-      <c r="D1983" s="177"/>
-      <c r="E1983" s="177"/>
+      <c r="C1983" s="173"/>
+      <c r="D1983" s="174"/>
+      <c r="E1983" s="174"/>
     </row>
     <row r="1984" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1984" s="84">
@@ -23379,9 +23383,9 @@
         <v>142</v>
       </c>
       <c r="B2000" s="87"/>
-      <c r="C2000" s="176"/>
-      <c r="D2000" s="177"/>
-      <c r="E2000" s="177"/>
+      <c r="C2000" s="173"/>
+      <c r="D2000" s="174"/>
+      <c r="E2000" s="174"/>
     </row>
     <row r="2001" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2001" s="84">
@@ -23532,9 +23536,9 @@
         <v>143</v>
       </c>
       <c r="B2017" s="87"/>
-      <c r="C2017" s="176"/>
-      <c r="D2017" s="177"/>
-      <c r="E2017" s="177"/>
+      <c r="C2017" s="173"/>
+      <c r="D2017" s="174"/>
+      <c r="E2017" s="174"/>
     </row>
     <row r="2018" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2018" s="84">
@@ -23685,9 +23689,9 @@
         <v>144</v>
       </c>
       <c r="B2034" s="87"/>
-      <c r="C2034" s="176"/>
-      <c r="D2034" s="177"/>
-      <c r="E2034" s="177"/>
+      <c r="C2034" s="173"/>
+      <c r="D2034" s="174"/>
+      <c r="E2034" s="174"/>
     </row>
     <row r="2035" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2035" s="84">
@@ -23838,9 +23842,9 @@
         <v>145</v>
       </c>
       <c r="B2051" s="87"/>
-      <c r="C2051" s="176"/>
-      <c r="D2051" s="177"/>
-      <c r="E2051" s="177"/>
+      <c r="C2051" s="173"/>
+      <c r="D2051" s="174"/>
+      <c r="E2051" s="174"/>
     </row>
     <row r="2052" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2052" s="84">
@@ -23991,9 +23995,9 @@
         <v>146</v>
       </c>
       <c r="B2068" s="87"/>
-      <c r="C2068" s="176"/>
-      <c r="D2068" s="177"/>
-      <c r="E2068" s="177"/>
+      <c r="C2068" s="173"/>
+      <c r="D2068" s="174"/>
+      <c r="E2068" s="174"/>
     </row>
     <row r="2069" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2069" s="84">
@@ -24144,9 +24148,9 @@
         <v>147</v>
       </c>
       <c r="B2085" s="87"/>
-      <c r="C2085" s="176"/>
-      <c r="D2085" s="177"/>
-      <c r="E2085" s="177"/>
+      <c r="C2085" s="173"/>
+      <c r="D2085" s="174"/>
+      <c r="E2085" s="174"/>
     </row>
     <row r="2086" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2086" s="84">
@@ -24297,9 +24301,9 @@
         <v>148</v>
       </c>
       <c r="B2102" s="87"/>
-      <c r="C2102" s="176"/>
-      <c r="D2102" s="177"/>
-      <c r="E2102" s="177"/>
+      <c r="C2102" s="173"/>
+      <c r="D2102" s="174"/>
+      <c r="E2102" s="174"/>
     </row>
     <row r="2103" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2103" s="84">
@@ -24450,9 +24454,9 @@
         <v>97</v>
       </c>
       <c r="B2119" s="87"/>
-      <c r="C2119" s="176"/>
-      <c r="D2119" s="177"/>
-      <c r="E2119" s="177"/>
+      <c r="C2119" s="173"/>
+      <c r="D2119" s="174"/>
+      <c r="E2119" s="174"/>
     </row>
     <row r="2120" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2120" s="84">
@@ -24603,9 +24607,9 @@
         <v>149</v>
       </c>
       <c r="B2136" s="87"/>
-      <c r="C2136" s="176"/>
-      <c r="D2136" s="177"/>
-      <c r="E2136" s="177"/>
+      <c r="C2136" s="173"/>
+      <c r="D2136" s="174"/>
+      <c r="E2136" s="174"/>
     </row>
     <row r="2137" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2137" s="84">
@@ -24756,9 +24760,9 @@
         <v>150</v>
       </c>
       <c r="B2153" s="87"/>
-      <c r="C2153" s="176"/>
-      <c r="D2153" s="177"/>
-      <c r="E2153" s="177"/>
+      <c r="C2153" s="173"/>
+      <c r="D2153" s="174"/>
+      <c r="E2153" s="174"/>
     </row>
     <row r="2154" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2154" s="84">
@@ -24909,9 +24913,9 @@
         <v>151</v>
       </c>
       <c r="B2170" s="87"/>
-      <c r="C2170" s="176"/>
-      <c r="D2170" s="177"/>
-      <c r="E2170" s="177"/>
+      <c r="C2170" s="173"/>
+      <c r="D2170" s="174"/>
+      <c r="E2170" s="174"/>
     </row>
     <row r="2171" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2171" s="84">
@@ -25059,15 +25063,122 @@
     </row>
   </sheetData>
   <mergeCells count="137">
-    <mergeCell ref="C2034:E2034"/>
-    <mergeCell ref="C2051:E2051"/>
-    <mergeCell ref="C2068:E2068"/>
-    <mergeCell ref="C2085:E2085"/>
-    <mergeCell ref="C2170:E2170"/>
-    <mergeCell ref="C2102:E2102"/>
-    <mergeCell ref="C2119:E2119"/>
-    <mergeCell ref="C2136:E2136"/>
-    <mergeCell ref="C2153:E2153"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="C89:E89"/>
+    <mergeCell ref="C21:E21"/>
+    <mergeCell ref="C38:E38"/>
+    <mergeCell ref="C55:E55"/>
+    <mergeCell ref="C72:E72"/>
+    <mergeCell ref="C208:E208"/>
+    <mergeCell ref="C225:E225"/>
+    <mergeCell ref="C242:E242"/>
+    <mergeCell ref="C259:E259"/>
+    <mergeCell ref="C276:E276"/>
+    <mergeCell ref="C277:E277"/>
+    <mergeCell ref="C106:E106"/>
+    <mergeCell ref="C123:E123"/>
+    <mergeCell ref="C140:E140"/>
+    <mergeCell ref="C157:E157"/>
+    <mergeCell ref="C174:E174"/>
+    <mergeCell ref="C191:E191"/>
+    <mergeCell ref="C396:E396"/>
+    <mergeCell ref="C413:E413"/>
+    <mergeCell ref="C430:E430"/>
+    <mergeCell ref="C447:E447"/>
+    <mergeCell ref="C464:E464"/>
+    <mergeCell ref="C481:E481"/>
+    <mergeCell ref="C294:E294"/>
+    <mergeCell ref="C311:E311"/>
+    <mergeCell ref="C328:E328"/>
+    <mergeCell ref="C345:E345"/>
+    <mergeCell ref="C362:E362"/>
+    <mergeCell ref="C379:E379"/>
+    <mergeCell ref="C584:E584"/>
+    <mergeCell ref="C601:E601"/>
+    <mergeCell ref="C618:E618"/>
+    <mergeCell ref="C635:E635"/>
+    <mergeCell ref="C652:E652"/>
+    <mergeCell ref="C669:E669"/>
+    <mergeCell ref="C498:E498"/>
+    <mergeCell ref="C515:E515"/>
+    <mergeCell ref="C532:E532"/>
+    <mergeCell ref="C549:E549"/>
+    <mergeCell ref="C550:E550"/>
+    <mergeCell ref="C567:E567"/>
+    <mergeCell ref="C788:E788"/>
+    <mergeCell ref="C805:E805"/>
+    <mergeCell ref="C822:E822"/>
+    <mergeCell ref="C823:E823"/>
+    <mergeCell ref="C840:E840"/>
+    <mergeCell ref="C857:E857"/>
+    <mergeCell ref="C686:E686"/>
+    <mergeCell ref="C703:E703"/>
+    <mergeCell ref="C720:E720"/>
+    <mergeCell ref="C737:E737"/>
+    <mergeCell ref="C754:E754"/>
+    <mergeCell ref="C771:E771"/>
+    <mergeCell ref="C976:E976"/>
+    <mergeCell ref="C993:E993"/>
+    <mergeCell ref="C1010:E1010"/>
+    <mergeCell ref="C1027:E1027"/>
+    <mergeCell ref="C1044:E1044"/>
+    <mergeCell ref="C1061:E1061"/>
+    <mergeCell ref="C874:E874"/>
+    <mergeCell ref="C891:E891"/>
+    <mergeCell ref="C908:E908"/>
+    <mergeCell ref="C925:E925"/>
+    <mergeCell ref="C942:E942"/>
+    <mergeCell ref="C959:E959"/>
+    <mergeCell ref="C1164:E1164"/>
+    <mergeCell ref="C1181:E1181"/>
+    <mergeCell ref="C1198:E1198"/>
+    <mergeCell ref="C1215:E1215"/>
+    <mergeCell ref="C1232:E1232"/>
+    <mergeCell ref="C1249:E1249"/>
+    <mergeCell ref="C1078:E1078"/>
+    <mergeCell ref="C1095:E1095"/>
+    <mergeCell ref="C1096:E1096"/>
+    <mergeCell ref="C1113:E1113"/>
+    <mergeCell ref="C1130:E1130"/>
+    <mergeCell ref="C1147:E1147"/>
+    <mergeCell ref="C1368:E1368"/>
+    <mergeCell ref="C1369:E1369"/>
+    <mergeCell ref="C1386:E1386"/>
+    <mergeCell ref="C1403:E1403"/>
+    <mergeCell ref="C1420:E1420"/>
+    <mergeCell ref="C1437:E1437"/>
+    <mergeCell ref="C1266:E1266"/>
+    <mergeCell ref="C1283:E1283"/>
+    <mergeCell ref="C1300:E1300"/>
+    <mergeCell ref="C1317:E1317"/>
+    <mergeCell ref="C1334:E1334"/>
+    <mergeCell ref="C1351:E1351"/>
+    <mergeCell ref="C1556:E1556"/>
+    <mergeCell ref="C1573:E1573"/>
+    <mergeCell ref="C1590:E1590"/>
+    <mergeCell ref="C1607:E1607"/>
+    <mergeCell ref="C1624:E1624"/>
+    <mergeCell ref="C1641:E1641"/>
+    <mergeCell ref="C1454:E1454"/>
+    <mergeCell ref="C1471:E1471"/>
+    <mergeCell ref="C1488:E1488"/>
+    <mergeCell ref="C1505:E1505"/>
+    <mergeCell ref="C1522:E1522"/>
+    <mergeCell ref="C1539:E1539"/>
+    <mergeCell ref="C1744:E1744"/>
+    <mergeCell ref="C1761:E1761"/>
+    <mergeCell ref="C1778:E1778"/>
+    <mergeCell ref="C1795:E1795"/>
+    <mergeCell ref="C1812:E1812"/>
+    <mergeCell ref="C1829:E1829"/>
+    <mergeCell ref="C1642:E1642"/>
+    <mergeCell ref="C1659:E1659"/>
+    <mergeCell ref="C1676:E1676"/>
+    <mergeCell ref="C1693:E1693"/>
+    <mergeCell ref="C1710:E1710"/>
+    <mergeCell ref="C1727:E1727"/>
     <mergeCell ref="C1932:E1932"/>
     <mergeCell ref="C1949:E1949"/>
     <mergeCell ref="C1966:E1966"/>
@@ -25080,122 +25191,15 @@
     <mergeCell ref="C1897:E1897"/>
     <mergeCell ref="C1914:E1914"/>
     <mergeCell ref="C1915:E1915"/>
-    <mergeCell ref="C1744:E1744"/>
-    <mergeCell ref="C1761:E1761"/>
-    <mergeCell ref="C1778:E1778"/>
-    <mergeCell ref="C1795:E1795"/>
-    <mergeCell ref="C1812:E1812"/>
-    <mergeCell ref="C1829:E1829"/>
-    <mergeCell ref="C1642:E1642"/>
-    <mergeCell ref="C1659:E1659"/>
-    <mergeCell ref="C1676:E1676"/>
-    <mergeCell ref="C1693:E1693"/>
-    <mergeCell ref="C1710:E1710"/>
-    <mergeCell ref="C1727:E1727"/>
-    <mergeCell ref="C1556:E1556"/>
-    <mergeCell ref="C1573:E1573"/>
-    <mergeCell ref="C1590:E1590"/>
-    <mergeCell ref="C1607:E1607"/>
-    <mergeCell ref="C1624:E1624"/>
-    <mergeCell ref="C1641:E1641"/>
-    <mergeCell ref="C1454:E1454"/>
-    <mergeCell ref="C1471:E1471"/>
-    <mergeCell ref="C1488:E1488"/>
-    <mergeCell ref="C1505:E1505"/>
-    <mergeCell ref="C1522:E1522"/>
-    <mergeCell ref="C1539:E1539"/>
-    <mergeCell ref="C1368:E1368"/>
-    <mergeCell ref="C1369:E1369"/>
-    <mergeCell ref="C1386:E1386"/>
-    <mergeCell ref="C1403:E1403"/>
-    <mergeCell ref="C1420:E1420"/>
-    <mergeCell ref="C1437:E1437"/>
-    <mergeCell ref="C1266:E1266"/>
-    <mergeCell ref="C1283:E1283"/>
-    <mergeCell ref="C1300:E1300"/>
-    <mergeCell ref="C1317:E1317"/>
-    <mergeCell ref="C1334:E1334"/>
-    <mergeCell ref="C1351:E1351"/>
-    <mergeCell ref="C1164:E1164"/>
-    <mergeCell ref="C1181:E1181"/>
-    <mergeCell ref="C1198:E1198"/>
-    <mergeCell ref="C1215:E1215"/>
-    <mergeCell ref="C1232:E1232"/>
-    <mergeCell ref="C1249:E1249"/>
-    <mergeCell ref="C1078:E1078"/>
-    <mergeCell ref="C1095:E1095"/>
-    <mergeCell ref="C1096:E1096"/>
-    <mergeCell ref="C1113:E1113"/>
-    <mergeCell ref="C1130:E1130"/>
-    <mergeCell ref="C1147:E1147"/>
-    <mergeCell ref="C976:E976"/>
-    <mergeCell ref="C993:E993"/>
-    <mergeCell ref="C1010:E1010"/>
-    <mergeCell ref="C1027:E1027"/>
-    <mergeCell ref="C1044:E1044"/>
-    <mergeCell ref="C1061:E1061"/>
-    <mergeCell ref="C874:E874"/>
-    <mergeCell ref="C891:E891"/>
-    <mergeCell ref="C908:E908"/>
-    <mergeCell ref="C925:E925"/>
-    <mergeCell ref="C942:E942"/>
-    <mergeCell ref="C959:E959"/>
-    <mergeCell ref="C788:E788"/>
-    <mergeCell ref="C805:E805"/>
-    <mergeCell ref="C822:E822"/>
-    <mergeCell ref="C823:E823"/>
-    <mergeCell ref="C840:E840"/>
-    <mergeCell ref="C857:E857"/>
-    <mergeCell ref="C686:E686"/>
-    <mergeCell ref="C703:E703"/>
-    <mergeCell ref="C720:E720"/>
-    <mergeCell ref="C737:E737"/>
-    <mergeCell ref="C754:E754"/>
-    <mergeCell ref="C771:E771"/>
-    <mergeCell ref="C584:E584"/>
-    <mergeCell ref="C601:E601"/>
-    <mergeCell ref="C618:E618"/>
-    <mergeCell ref="C635:E635"/>
-    <mergeCell ref="C652:E652"/>
-    <mergeCell ref="C669:E669"/>
-    <mergeCell ref="C498:E498"/>
-    <mergeCell ref="C515:E515"/>
-    <mergeCell ref="C532:E532"/>
-    <mergeCell ref="C549:E549"/>
-    <mergeCell ref="C550:E550"/>
-    <mergeCell ref="C567:E567"/>
-    <mergeCell ref="C396:E396"/>
-    <mergeCell ref="C413:E413"/>
-    <mergeCell ref="C430:E430"/>
-    <mergeCell ref="C447:E447"/>
-    <mergeCell ref="C464:E464"/>
-    <mergeCell ref="C481:E481"/>
-    <mergeCell ref="C294:E294"/>
-    <mergeCell ref="C311:E311"/>
-    <mergeCell ref="C328:E328"/>
-    <mergeCell ref="C345:E345"/>
-    <mergeCell ref="C362:E362"/>
-    <mergeCell ref="C379:E379"/>
-    <mergeCell ref="C225:E225"/>
-    <mergeCell ref="C242:E242"/>
-    <mergeCell ref="C259:E259"/>
-    <mergeCell ref="C276:E276"/>
-    <mergeCell ref="C277:E277"/>
-    <mergeCell ref="C106:E106"/>
-    <mergeCell ref="C123:E123"/>
-    <mergeCell ref="C140:E140"/>
-    <mergeCell ref="C157:E157"/>
-    <mergeCell ref="C174:E174"/>
-    <mergeCell ref="C191:E191"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="C89:E89"/>
-    <mergeCell ref="C21:E21"/>
-    <mergeCell ref="C38:E38"/>
-    <mergeCell ref="C55:E55"/>
-    <mergeCell ref="C72:E72"/>
-    <mergeCell ref="C208:E208"/>
+    <mergeCell ref="C2034:E2034"/>
+    <mergeCell ref="C2051:E2051"/>
+    <mergeCell ref="C2068:E2068"/>
+    <mergeCell ref="C2085:E2085"/>
+    <mergeCell ref="C2170:E2170"/>
+    <mergeCell ref="C2102:E2102"/>
+    <mergeCell ref="C2119:E2119"/>
+    <mergeCell ref="C2136:E2136"/>
+    <mergeCell ref="C2153:E2153"/>
   </mergeCells>
   <phoneticPr fontId="13" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -26454,150 +26458,163 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="33">
-      <c r="A1" s="219" t="s">
+      <c r="A1" s="218" t="s">
         <v>184</v>
       </c>
-      <c r="B1" s="220"/>
+      <c r="B1" s="219"/>
       <c r="C1" s="118"/>
       <c r="D1" s="5"/>
       <c r="E1" s="5"/>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="225" t="s">
+      <c r="A2" s="215" t="s">
         <v>183</v>
       </c>
-      <c r="B2" s="226"/>
+      <c r="B2" s="216"/>
       <c r="C2" s="120"/>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="227" t="s">
+      <c r="A3" s="217" t="s">
         <v>185</v>
       </c>
-      <c r="B3" s="226"/>
+      <c r="B3" s="216"/>
       <c r="C3" s="120"/>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="223"/>
-      <c r="B4" s="224"/>
+      <c r="A4" s="222"/>
+      <c r="B4" s="223"/>
       <c r="C4" s="120"/>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="221" t="s">
+      <c r="A5" s="220" t="s">
         <v>194</v>
       </c>
-      <c r="B5" s="222"/>
+      <c r="B5" s="221"/>
       <c r="C5" s="120"/>
     </row>
     <row r="7" spans="1:5" ht="18.75">
-      <c r="A7" s="213" t="s">
+      <c r="A7" s="226" t="s">
         <v>186</v>
       </c>
-      <c r="B7" s="214"/>
+      <c r="B7" s="227"/>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="120"/>
       <c r="B8" s="9"/>
     </row>
     <row r="9" spans="1:5" ht="39" customHeight="1">
-      <c r="A9" s="215" t="s">
+      <c r="A9" s="224" t="s">
         <v>187</v>
       </c>
-      <c r="B9" s="216"/>
+      <c r="B9" s="225"/>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="217"/>
-      <c r="B10" s="218"/>
+      <c r="A10" s="211"/>
+      <c r="B10" s="212"/>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="209" t="s">
+      <c r="A11" s="213" t="s">
         <v>188</v>
       </c>
-      <c r="B11" s="210"/>
+      <c r="B11" s="214"/>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="209" t="s">
+      <c r="A12" s="213" t="s">
         <v>189</v>
       </c>
-      <c r="B12" s="210"/>
+      <c r="B12" s="214"/>
     </row>
     <row r="13" spans="1:5" ht="43.5" customHeight="1">
-      <c r="A13" s="209" t="s">
+      <c r="A13" s="213" t="s">
         <v>190</v>
       </c>
-      <c r="B13" s="210"/>
+      <c r="B13" s="214"/>
     </row>
     <row r="14" spans="1:5" ht="19.5" customHeight="1">
-      <c r="A14" s="209" t="s">
+      <c r="A14" s="213" t="s">
         <v>191</v>
       </c>
-      <c r="B14" s="210"/>
+      <c r="B14" s="214"/>
     </row>
     <row r="15" spans="1:5" ht="18" customHeight="1">
-      <c r="A15" s="209" t="s">
+      <c r="A15" s="213" t="s">
         <v>192</v>
       </c>
-      <c r="B15" s="210"/>
+      <c r="B15" s="214"/>
     </row>
     <row r="16" spans="1:5" ht="21" customHeight="1">
-      <c r="A16" s="209" t="s">
+      <c r="A16" s="213" t="s">
         <v>193</v>
       </c>
-      <c r="B16" s="210"/>
+      <c r="B16" s="214"/>
     </row>
     <row r="17" spans="1:2" ht="48.75" customHeight="1">
-      <c r="A17" s="211" t="s">
+      <c r="A17" s="209" t="s">
         <v>195</v>
       </c>
-      <c r="B17" s="212"/>
+      <c r="B17" s="210"/>
     </row>
     <row r="19" spans="1:2" ht="18.75">
-      <c r="A19" s="213" t="s">
+      <c r="A19" s="226" t="s">
         <v>197</v>
       </c>
-      <c r="B19" s="214"/>
+      <c r="B19" s="227"/>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="120"/>
       <c r="B20" s="9"/>
     </row>
     <row r="21" spans="1:2">
-      <c r="A21" s="215" t="s">
+      <c r="A21" s="224" t="s">
         <v>198</v>
       </c>
-      <c r="B21" s="216"/>
+      <c r="B21" s="225"/>
     </row>
     <row r="22" spans="1:2">
-      <c r="A22" s="217"/>
-      <c r="B22" s="218"/>
+      <c r="A22" s="211"/>
+      <c r="B22" s="212"/>
     </row>
     <row r="23" spans="1:2">
-      <c r="A23" s="209" t="s">
+      <c r="A23" s="213" t="s">
         <v>199</v>
       </c>
-      <c r="B23" s="210"/>
+      <c r="B23" s="214"/>
     </row>
     <row r="24" spans="1:2">
-      <c r="A24" s="209"/>
-      <c r="B24" s="210"/>
+      <c r="A24" s="213"/>
+      <c r="B24" s="214"/>
     </row>
     <row r="25" spans="1:2">
-      <c r="A25" s="209" t="s">
+      <c r="A25" s="213" t="s">
         <v>200</v>
       </c>
-      <c r="B25" s="210"/>
+      <c r="B25" s="214"/>
     </row>
     <row r="26" spans="1:2">
-      <c r="A26" s="209" t="s">
+      <c r="A26" s="213" t="s">
         <v>201</v>
       </c>
-      <c r="B26" s="210"/>
+      <c r="B26" s="214"/>
     </row>
     <row r="27" spans="1:2">
-      <c r="A27" s="211"/>
-      <c r="B27" s="212"/>
+      <c r="A27" s="209"/>
+      <c r="B27" s="210"/>
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A7:B7"/>
     <mergeCell ref="A17:B17"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
@@ -26608,19 +26625,6 @@
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="A14:B14"/>
     <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A24:B24"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A3" r:id="rId1"/>

</xml_diff>

<commit_message>
Tempo - boss 4 done - with glitch!
</commit_message>
<xml_diff>
--- a/trunk/Tempo/Tempo.xlsx
+++ b/trunk/Tempo/Tempo.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1168" uniqueCount="277">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1169" uniqueCount="278">
   <si>
     <t>Notes</t>
   </si>
@@ -891,6 +891,9 @@
   <si>
     <t>7th Hit</t>
   </si>
+  <si>
+    <t>Boss defeated (HP = 0)</t>
+  </si>
 </sst>
 </file>
 
@@ -900,10 +903,17 @@
     <numFmt numFmtId="164" formatCode="#,##0;[Red]#,##0"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="56">
+  <fonts count="57">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1908,34 +1918,34 @@
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="27" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="37" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="50" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="27" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="38" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="51" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="228">
+  <cellXfs count="229">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="27" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="28" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1943,208 +1953,208 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="28" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="21" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="23" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="25" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="25" fillId="13" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="20" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="22" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="24" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="26" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="26" fillId="13" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="21" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="20" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="21" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="32" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="32" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="21" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="20" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="21" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="10" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="21" fillId="12" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="32" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
+    <xf numFmtId="0" fontId="26" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="33" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="34" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="34" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="34" fillId="13" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="33" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="26" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="35" fillId="13" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="13" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="36" fillId="13" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="13" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="36" fillId="13" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="35" fillId="13" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="37" fillId="16" borderId="23" xfId="2" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="37" fillId="16" borderId="23" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="38" fillId="16" borderId="23" xfId="2" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="38" fillId="16" borderId="23" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="16" borderId="22" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="38" fillId="16" borderId="22" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="27" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="36" fillId="0" borderId="27" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="27" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="37" fillId="0" borderId="27" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="3" fontId="38" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="30" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="36" fillId="0" borderId="30" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="36" fillId="0" borderId="29" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="38" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="36" fillId="17" borderId="31" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="36" fillId="18" borderId="31" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="36" fillId="19" borderId="31" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="37" fillId="20" borderId="23" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="37" fillId="20" borderId="23" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="39" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="30" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="37" fillId="0" borderId="30" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="37" fillId="0" borderId="29" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="39" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="37" fillId="17" borderId="31" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="37" fillId="18" borderId="31" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="37" fillId="19" borderId="31" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="38" fillId="20" borderId="23" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="38" fillId="20" borderId="23" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="20" borderId="22" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="38" fillId="20" borderId="22" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="37" fillId="21" borderId="23" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="37" fillId="21" borderId="23" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="38" fillId="21" borderId="23" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="38" fillId="21" borderId="23" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="21" borderId="22" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="38" fillId="21" borderId="22" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="47" fillId="16" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="48" fillId="16" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="47" fillId="20" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="48" fillId="20" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
-    <xf numFmtId="3" fontId="38" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="36" fillId="0" borderId="42" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="38" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="38" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="38" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="36" fillId="0" borderId="42" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="39" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="37" fillId="0" borderId="42" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="39" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="39" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="39" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="37" fillId="0" borderId="42" xfId="1" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2154,10 +2164,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2178,19 +2188,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="23" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="54" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="55" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="45" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="39" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="55" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="32" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="41" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="44" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="38" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="54" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="31" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="40" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="43" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="43" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="44" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
@@ -2200,10 +2213,10 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
+    <xf numFmtId="3" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="3" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
@@ -2225,127 +2238,127 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="41" fillId="21" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="42" fillId="21" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="41" fillId="20" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="42" fillId="20" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="43" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="44" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="23" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="39" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="45" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="40" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="46" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="46" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="47" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="41" fillId="16" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="42" fillId="16" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="25" fillId="13" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="26" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="25" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="26" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="23" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="24" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="21" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="22" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="29" fillId="14" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="22" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="23" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="24" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="25" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="26" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="27" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="26" fillId="13" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="27" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="30" fillId="14" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="14" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="14" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="14" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="14" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="30" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="55" fillId="22" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="56" fillId="22" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="55" fillId="22" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="56" fillId="22" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="55" fillId="22" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="56" fillId="22" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="53" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="54" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="54" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="49" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="50" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="4"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="4"/>
     </xf>
-    <xf numFmtId="0" fontId="50" fillId="0" borderId="33" xfId="3" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="51" fillId="0" borderId="33" xfId="3" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" indent="4"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="51" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="51" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="53" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="53" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="52" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Accent1" xfId="2" builtinId="29"/>
@@ -2657,7 +2670,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A87" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C101" sqref="C101"/>
+      <selection pane="bottomLeft" activeCell="C104" sqref="C104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" outlineLevelRow="2"/>
@@ -4423,8 +4436,12 @@
     </row>
     <row r="102" spans="1:8" ht="15" outlineLevel="1">
       <c r="A102" s="164"/>
-      <c r="B102" s="100"/>
-      <c r="C102" s="101"/>
+      <c r="B102" s="228" t="s">
+        <v>277</v>
+      </c>
+      <c r="C102" s="101">
+        <v>38010</v>
+      </c>
       <c r="D102" s="101"/>
       <c r="E102" s="123">
         <f t="shared" si="7"/>
@@ -4437,13 +4454,15 @@
       <c r="B103" s="152" t="s">
         <v>223</v>
       </c>
-      <c r="C103" s="101"/>
+      <c r="C103" s="101">
+        <v>37902</v>
+      </c>
       <c r="D103" s="101">
         <v>49269</v>
       </c>
       <c r="E103" s="123">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>11367</v>
       </c>
       <c r="F103" s="105"/>
     </row>
@@ -5328,6 +5347,11 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="A152:A166"/>
+    <mergeCell ref="A123:A132"/>
+    <mergeCell ref="A93:A107"/>
+    <mergeCell ref="A135:A149"/>
+    <mergeCell ref="A110:A120"/>
     <mergeCell ref="A43:A70"/>
     <mergeCell ref="A73:A90"/>
     <mergeCell ref="C5:D5"/>
@@ -5337,11 +5361,6 @@
     <mergeCell ref="A8:A18"/>
     <mergeCell ref="A21:A40"/>
     <mergeCell ref="C4:E4"/>
-    <mergeCell ref="A152:A166"/>
-    <mergeCell ref="A123:A132"/>
-    <mergeCell ref="A93:A107"/>
-    <mergeCell ref="A135:A149"/>
-    <mergeCell ref="A110:A120"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -5373,13 +5392,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="26.25" customHeight="1">
-      <c r="A1" s="191" t="s">
+      <c r="A1" s="173" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="191"/>
-      <c r="C1" s="191"/>
-      <c r="D1" s="191"/>
-      <c r="E1" s="191"/>
+      <c r="B1" s="173"/>
+      <c r="C1" s="173"/>
+      <c r="D1" s="173"/>
+      <c r="E1" s="173"/>
       <c r="F1" s="7"/>
       <c r="G1" s="5"/>
       <c r="H1" s="5"/>
@@ -5409,18 +5428,18 @@
         <v>8</v>
       </c>
       <c r="B3" s="36"/>
-      <c r="C3" s="192"/>
-      <c r="D3" s="193"/>
-      <c r="E3" s="193"/>
+      <c r="C3" s="174"/>
+      <c r="D3" s="175"/>
+      <c r="E3" s="175"/>
     </row>
     <row r="4" spans="1:8" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A4" s="46" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="87"/>
-      <c r="C4" s="173"/>
-      <c r="D4" s="174"/>
-      <c r="E4" s="174"/>
+      <c r="C4" s="176"/>
+      <c r="D4" s="177"/>
+      <c r="E4" s="177"/>
       <c r="F4" s="6"/>
     </row>
     <row r="5" spans="1:8" hidden="1" outlineLevel="2">
@@ -5572,9 +5591,9 @@
         <v>9</v>
       </c>
       <c r="B21" s="90"/>
-      <c r="C21" s="175"/>
-      <c r="D21" s="176"/>
-      <c r="E21" s="176"/>
+      <c r="C21" s="178"/>
+      <c r="D21" s="179"/>
+      <c r="E21" s="179"/>
     </row>
     <row r="22" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A22" s="47">
@@ -5725,9 +5744,9 @@
         <v>10</v>
       </c>
       <c r="B38" s="87"/>
-      <c r="C38" s="173"/>
-      <c r="D38" s="174"/>
-      <c r="E38" s="174"/>
+      <c r="C38" s="176"/>
+      <c r="D38" s="177"/>
+      <c r="E38" s="177"/>
     </row>
     <row r="39" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A39" s="47">
@@ -5878,9 +5897,9 @@
         <v>11</v>
       </c>
       <c r="B55" s="87"/>
-      <c r="C55" s="173"/>
-      <c r="D55" s="174"/>
-      <c r="E55" s="174"/>
+      <c r="C55" s="176"/>
+      <c r="D55" s="177"/>
+      <c r="E55" s="177"/>
     </row>
     <row r="56" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A56" s="47">
@@ -6031,9 +6050,9 @@
         <v>12</v>
       </c>
       <c r="B72" s="87"/>
-      <c r="C72" s="173"/>
-      <c r="D72" s="174"/>
-      <c r="E72" s="174"/>
+      <c r="C72" s="176"/>
+      <c r="D72" s="177"/>
+      <c r="E72" s="177"/>
     </row>
     <row r="73" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A73" s="47">
@@ -6184,9 +6203,9 @@
         <v>13</v>
       </c>
       <c r="B89" s="87"/>
-      <c r="C89" s="173"/>
-      <c r="D89" s="174"/>
-      <c r="E89" s="174"/>
+      <c r="C89" s="176"/>
+      <c r="D89" s="177"/>
+      <c r="E89" s="177"/>
     </row>
     <row r="90" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A90" s="47">
@@ -6337,9 +6356,9 @@
         <v>14</v>
       </c>
       <c r="B106" s="87"/>
-      <c r="C106" s="173"/>
-      <c r="D106" s="174"/>
-      <c r="E106" s="174"/>
+      <c r="C106" s="176"/>
+      <c r="D106" s="177"/>
+      <c r="E106" s="177"/>
     </row>
     <row r="107" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A107" s="47">
@@ -6490,9 +6509,9 @@
         <v>15</v>
       </c>
       <c r="B123" s="87"/>
-      <c r="C123" s="173"/>
-      <c r="D123" s="174"/>
-      <c r="E123" s="174"/>
+      <c r="C123" s="176"/>
+      <c r="D123" s="177"/>
+      <c r="E123" s="177"/>
     </row>
     <row r="124" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A124" s="47">
@@ -6643,9 +6662,9 @@
         <v>16</v>
       </c>
       <c r="B140" s="87"/>
-      <c r="C140" s="173"/>
-      <c r="D140" s="174"/>
-      <c r="E140" s="174"/>
+      <c r="C140" s="176"/>
+      <c r="D140" s="177"/>
+      <c r="E140" s="177"/>
     </row>
     <row r="141" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A141" s="47">
@@ -6796,9 +6815,9 @@
         <v>17</v>
       </c>
       <c r="B157" s="87"/>
-      <c r="C157" s="173"/>
-      <c r="D157" s="174"/>
-      <c r="E157" s="174"/>
+      <c r="C157" s="176"/>
+      <c r="D157" s="177"/>
+      <c r="E157" s="177"/>
     </row>
     <row r="158" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A158" s="47">
@@ -6949,9 +6968,9 @@
         <v>18</v>
       </c>
       <c r="B174" s="87"/>
-      <c r="C174" s="173"/>
-      <c r="D174" s="174"/>
-      <c r="E174" s="174"/>
+      <c r="C174" s="176"/>
+      <c r="D174" s="177"/>
+      <c r="E174" s="177"/>
     </row>
     <row r="175" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A175" s="47">
@@ -7102,9 +7121,9 @@
         <v>19</v>
       </c>
       <c r="B191" s="87"/>
-      <c r="C191" s="173"/>
-      <c r="D191" s="174"/>
-      <c r="E191" s="174"/>
+      <c r="C191" s="176"/>
+      <c r="D191" s="177"/>
+      <c r="E191" s="177"/>
     </row>
     <row r="192" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A192" s="47">
@@ -7255,9 +7274,9 @@
         <v>20</v>
       </c>
       <c r="B208" s="87"/>
-      <c r="C208" s="173"/>
-      <c r="D208" s="174"/>
-      <c r="E208" s="174"/>
+      <c r="C208" s="176"/>
+      <c r="D208" s="177"/>
+      <c r="E208" s="177"/>
     </row>
     <row r="209" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A209" s="47">
@@ -7408,9 +7427,9 @@
         <v>21</v>
       </c>
       <c r="B225" s="87"/>
-      <c r="C225" s="173"/>
-      <c r="D225" s="174"/>
-      <c r="E225" s="174"/>
+      <c r="C225" s="176"/>
+      <c r="D225" s="177"/>
+      <c r="E225" s="177"/>
     </row>
     <row r="226" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A226" s="47">
@@ -7561,9 +7580,9 @@
         <v>22</v>
       </c>
       <c r="B242" s="87"/>
-      <c r="C242" s="173"/>
-      <c r="D242" s="174"/>
-      <c r="E242" s="174"/>
+      <c r="C242" s="176"/>
+      <c r="D242" s="177"/>
+      <c r="E242" s="177"/>
     </row>
     <row r="243" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A243" s="47">
@@ -7714,9 +7733,9 @@
         <v>23</v>
       </c>
       <c r="B259" s="87"/>
-      <c r="C259" s="173"/>
-      <c r="D259" s="174"/>
-      <c r="E259" s="174"/>
+      <c r="C259" s="176"/>
+      <c r="D259" s="177"/>
+      <c r="E259" s="177"/>
     </row>
     <row r="260" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A260" s="47">
@@ -7867,18 +7886,18 @@
         <v>24</v>
       </c>
       <c r="B276" s="37"/>
-      <c r="C276" s="189"/>
-      <c r="D276" s="190"/>
-      <c r="E276" s="190"/>
+      <c r="C276" s="180"/>
+      <c r="D276" s="181"/>
+      <c r="E276" s="181"/>
     </row>
     <row r="277" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A277" s="51" t="s">
         <v>25</v>
       </c>
       <c r="B277" s="87"/>
-      <c r="C277" s="173"/>
-      <c r="D277" s="174"/>
-      <c r="E277" s="174"/>
+      <c r="C277" s="176"/>
+      <c r="D277" s="177"/>
+      <c r="E277" s="177"/>
     </row>
     <row r="278" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A278" s="52">
@@ -8029,9 +8048,9 @@
         <v>26</v>
       </c>
       <c r="B294" s="90"/>
-      <c r="C294" s="175"/>
-      <c r="D294" s="176"/>
-      <c r="E294" s="176"/>
+      <c r="C294" s="178"/>
+      <c r="D294" s="179"/>
+      <c r="E294" s="179"/>
     </row>
     <row r="295" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A295" s="52">
@@ -8182,9 +8201,9 @@
         <v>27</v>
       </c>
       <c r="B311" s="87"/>
-      <c r="C311" s="173"/>
-      <c r="D311" s="174"/>
-      <c r="E311" s="174"/>
+      <c r="C311" s="176"/>
+      <c r="D311" s="177"/>
+      <c r="E311" s="177"/>
     </row>
     <row r="312" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A312" s="52">
@@ -8335,9 +8354,9 @@
         <v>28</v>
       </c>
       <c r="B328" s="87"/>
-      <c r="C328" s="173"/>
-      <c r="D328" s="174"/>
-      <c r="E328" s="174"/>
+      <c r="C328" s="176"/>
+      <c r="D328" s="177"/>
+      <c r="E328" s="177"/>
     </row>
     <row r="329" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A329" s="52">
@@ -8488,9 +8507,9 @@
         <v>29</v>
       </c>
       <c r="B345" s="87"/>
-      <c r="C345" s="173"/>
-      <c r="D345" s="174"/>
-      <c r="E345" s="174"/>
+      <c r="C345" s="176"/>
+      <c r="D345" s="177"/>
+      <c r="E345" s="177"/>
     </row>
     <row r="346" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A346" s="52">
@@ -8641,9 +8660,9 @@
         <v>30</v>
       </c>
       <c r="B362" s="87"/>
-      <c r="C362" s="173"/>
-      <c r="D362" s="174"/>
-      <c r="E362" s="174"/>
+      <c r="C362" s="176"/>
+      <c r="D362" s="177"/>
+      <c r="E362" s="177"/>
     </row>
     <row r="363" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A363" s="52">
@@ -8794,9 +8813,9 @@
         <v>31</v>
       </c>
       <c r="B379" s="87"/>
-      <c r="C379" s="173"/>
-      <c r="D379" s="174"/>
-      <c r="E379" s="174"/>
+      <c r="C379" s="176"/>
+      <c r="D379" s="177"/>
+      <c r="E379" s="177"/>
     </row>
     <row r="380" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A380" s="52">
@@ -8947,9 +8966,9 @@
         <v>32</v>
       </c>
       <c r="B396" s="87"/>
-      <c r="C396" s="173"/>
-      <c r="D396" s="174"/>
-      <c r="E396" s="174"/>
+      <c r="C396" s="176"/>
+      <c r="D396" s="177"/>
+      <c r="E396" s="177"/>
     </row>
     <row r="397" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A397" s="52">
@@ -9100,9 +9119,9 @@
         <v>33</v>
       </c>
       <c r="B413" s="87"/>
-      <c r="C413" s="173"/>
-      <c r="D413" s="174"/>
-      <c r="E413" s="174"/>
+      <c r="C413" s="176"/>
+      <c r="D413" s="177"/>
+      <c r="E413" s="177"/>
     </row>
     <row r="414" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A414" s="52">
@@ -9253,9 +9272,9 @@
         <v>34</v>
       </c>
       <c r="B430" s="87"/>
-      <c r="C430" s="173"/>
-      <c r="D430" s="174"/>
-      <c r="E430" s="174"/>
+      <c r="C430" s="176"/>
+      <c r="D430" s="177"/>
+      <c r="E430" s="177"/>
     </row>
     <row r="431" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A431" s="52">
@@ -9406,9 +9425,9 @@
         <v>35</v>
       </c>
       <c r="B447" s="87"/>
-      <c r="C447" s="173"/>
-      <c r="D447" s="174"/>
-      <c r="E447" s="174"/>
+      <c r="C447" s="176"/>
+      <c r="D447" s="177"/>
+      <c r="E447" s="177"/>
     </row>
     <row r="448" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A448" s="52">
@@ -9559,9 +9578,9 @@
         <v>36</v>
       </c>
       <c r="B464" s="87"/>
-      <c r="C464" s="173"/>
-      <c r="D464" s="174"/>
-      <c r="E464" s="174"/>
+      <c r="C464" s="176"/>
+      <c r="D464" s="177"/>
+      <c r="E464" s="177"/>
     </row>
     <row r="465" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A465" s="52">
@@ -9712,9 +9731,9 @@
         <v>37</v>
       </c>
       <c r="B481" s="87"/>
-      <c r="C481" s="173"/>
-      <c r="D481" s="174"/>
-      <c r="E481" s="174"/>
+      <c r="C481" s="176"/>
+      <c r="D481" s="177"/>
+      <c r="E481" s="177"/>
     </row>
     <row r="482" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A482" s="52">
@@ -9865,9 +9884,9 @@
         <v>38</v>
       </c>
       <c r="B498" s="87"/>
-      <c r="C498" s="173"/>
-      <c r="D498" s="174"/>
-      <c r="E498" s="174"/>
+      <c r="C498" s="176"/>
+      <c r="D498" s="177"/>
+      <c r="E498" s="177"/>
     </row>
     <row r="499" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A499" s="52">
@@ -10018,9 +10037,9 @@
         <v>39</v>
       </c>
       <c r="B515" s="87"/>
-      <c r="C515" s="173"/>
-      <c r="D515" s="174"/>
-      <c r="E515" s="174"/>
+      <c r="C515" s="176"/>
+      <c r="D515" s="177"/>
+      <c r="E515" s="177"/>
     </row>
     <row r="516" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A516" s="52">
@@ -10171,9 +10190,9 @@
         <v>40</v>
       </c>
       <c r="B532" s="87"/>
-      <c r="C532" s="173"/>
-      <c r="D532" s="174"/>
-      <c r="E532" s="174"/>
+      <c r="C532" s="176"/>
+      <c r="D532" s="177"/>
+      <c r="E532" s="177"/>
     </row>
     <row r="533" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A533" s="55">
@@ -10324,18 +10343,18 @@
         <v>50</v>
       </c>
       <c r="B549" s="38"/>
-      <c r="C549" s="187"/>
-      <c r="D549" s="188"/>
-      <c r="E549" s="188"/>
+      <c r="C549" s="182"/>
+      <c r="D549" s="183"/>
+      <c r="E549" s="183"/>
     </row>
     <row r="550" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A550" s="58" t="s">
         <v>51</v>
       </c>
       <c r="B550" s="87"/>
-      <c r="C550" s="173"/>
-      <c r="D550" s="174"/>
-      <c r="E550" s="174"/>
+      <c r="C550" s="176"/>
+      <c r="D550" s="177"/>
+      <c r="E550" s="177"/>
     </row>
     <row r="551" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A551" s="59">
@@ -10486,9 +10505,9 @@
         <v>52</v>
       </c>
       <c r="B567" s="90"/>
-      <c r="C567" s="175"/>
-      <c r="D567" s="176"/>
-      <c r="E567" s="176"/>
+      <c r="C567" s="178"/>
+      <c r="D567" s="179"/>
+      <c r="E567" s="179"/>
     </row>
     <row r="568" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A568" s="59">
@@ -10639,9 +10658,9 @@
         <v>53</v>
       </c>
       <c r="B584" s="87"/>
-      <c r="C584" s="173"/>
-      <c r="D584" s="174"/>
-      <c r="E584" s="174"/>
+      <c r="C584" s="176"/>
+      <c r="D584" s="177"/>
+      <c r="E584" s="177"/>
     </row>
     <row r="585" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A585" s="59">
@@ -10792,9 +10811,9 @@
         <v>54</v>
       </c>
       <c r="B601" s="87"/>
-      <c r="C601" s="173"/>
-      <c r="D601" s="174"/>
-      <c r="E601" s="174"/>
+      <c r="C601" s="176"/>
+      <c r="D601" s="177"/>
+      <c r="E601" s="177"/>
     </row>
     <row r="602" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A602" s="59">
@@ -10945,9 +10964,9 @@
         <v>55</v>
       </c>
       <c r="B618" s="87"/>
-      <c r="C618" s="173"/>
-      <c r="D618" s="174"/>
-      <c r="E618" s="174"/>
+      <c r="C618" s="176"/>
+      <c r="D618" s="177"/>
+      <c r="E618" s="177"/>
     </row>
     <row r="619" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A619" s="59">
@@ -11098,9 +11117,9 @@
         <v>56</v>
       </c>
       <c r="B635" s="87"/>
-      <c r="C635" s="173"/>
-      <c r="D635" s="174"/>
-      <c r="E635" s="174"/>
+      <c r="C635" s="176"/>
+      <c r="D635" s="177"/>
+      <c r="E635" s="177"/>
     </row>
     <row r="636" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A636" s="59">
@@ -11251,9 +11270,9 @@
         <v>57</v>
       </c>
       <c r="B652" s="87"/>
-      <c r="C652" s="173"/>
-      <c r="D652" s="174"/>
-      <c r="E652" s="174"/>
+      <c r="C652" s="176"/>
+      <c r="D652" s="177"/>
+      <c r="E652" s="177"/>
     </row>
     <row r="653" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A653" s="59">
@@ -11404,9 +11423,9 @@
         <v>58</v>
       </c>
       <c r="B669" s="87"/>
-      <c r="C669" s="173"/>
-      <c r="D669" s="174"/>
-      <c r="E669" s="174"/>
+      <c r="C669" s="176"/>
+      <c r="D669" s="177"/>
+      <c r="E669" s="177"/>
     </row>
     <row r="670" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A670" s="59">
@@ -11557,9 +11576,9 @@
         <v>59</v>
       </c>
       <c r="B686" s="87"/>
-      <c r="C686" s="173"/>
-      <c r="D686" s="174"/>
-      <c r="E686" s="174"/>
+      <c r="C686" s="176"/>
+      <c r="D686" s="177"/>
+      <c r="E686" s="177"/>
     </row>
     <row r="687" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A687" s="59">
@@ -11710,9 +11729,9 @@
         <v>60</v>
       </c>
       <c r="B703" s="87"/>
-      <c r="C703" s="173"/>
-      <c r="D703" s="174"/>
-      <c r="E703" s="174"/>
+      <c r="C703" s="176"/>
+      <c r="D703" s="177"/>
+      <c r="E703" s="177"/>
     </row>
     <row r="704" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A704" s="59">
@@ -11863,9 +11882,9 @@
         <v>61</v>
       </c>
       <c r="B720" s="87"/>
-      <c r="C720" s="173"/>
-      <c r="D720" s="174"/>
-      <c r="E720" s="174"/>
+      <c r="C720" s="176"/>
+      <c r="D720" s="177"/>
+      <c r="E720" s="177"/>
     </row>
     <row r="721" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A721" s="59">
@@ -12016,9 +12035,9 @@
         <v>62</v>
       </c>
       <c r="B737" s="87"/>
-      <c r="C737" s="173"/>
-      <c r="D737" s="174"/>
-      <c r="E737" s="174"/>
+      <c r="C737" s="176"/>
+      <c r="D737" s="177"/>
+      <c r="E737" s="177"/>
     </row>
     <row r="738" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A738" s="59">
@@ -12169,9 +12188,9 @@
         <v>63</v>
       </c>
       <c r="B754" s="87"/>
-      <c r="C754" s="173"/>
-      <c r="D754" s="174"/>
-      <c r="E754" s="174"/>
+      <c r="C754" s="176"/>
+      <c r="D754" s="177"/>
+      <c r="E754" s="177"/>
     </row>
     <row r="755" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A755" s="59">
@@ -12322,9 +12341,9 @@
         <v>64</v>
       </c>
       <c r="B771" s="87"/>
-      <c r="C771" s="173"/>
-      <c r="D771" s="174"/>
-      <c r="E771" s="174"/>
+      <c r="C771" s="176"/>
+      <c r="D771" s="177"/>
+      <c r="E771" s="177"/>
     </row>
     <row r="772" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A772" s="59">
@@ -12475,9 +12494,9 @@
         <v>65</v>
       </c>
       <c r="B788" s="87"/>
-      <c r="C788" s="173"/>
-      <c r="D788" s="174"/>
-      <c r="E788" s="174"/>
+      <c r="C788" s="176"/>
+      <c r="D788" s="177"/>
+      <c r="E788" s="177"/>
     </row>
     <row r="789" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A789" s="59">
@@ -12628,9 +12647,9 @@
         <v>66</v>
       </c>
       <c r="B805" s="87"/>
-      <c r="C805" s="173"/>
-      <c r="D805" s="174"/>
-      <c r="E805" s="174"/>
+      <c r="C805" s="176"/>
+      <c r="D805" s="177"/>
+      <c r="E805" s="177"/>
     </row>
     <row r="806" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A806" s="59">
@@ -12781,18 +12800,18 @@
         <v>67</v>
       </c>
       <c r="B822" s="39"/>
-      <c r="C822" s="185"/>
-      <c r="D822" s="186"/>
-      <c r="E822" s="186"/>
+      <c r="C822" s="184"/>
+      <c r="D822" s="185"/>
+      <c r="E822" s="185"/>
     </row>
     <row r="823" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A823" s="63" t="s">
         <v>68</v>
       </c>
       <c r="B823" s="87"/>
-      <c r="C823" s="173"/>
-      <c r="D823" s="174"/>
-      <c r="E823" s="174"/>
+      <c r="C823" s="176"/>
+      <c r="D823" s="177"/>
+      <c r="E823" s="177"/>
     </row>
     <row r="824" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A824" s="64">
@@ -12943,9 +12962,9 @@
         <v>69</v>
       </c>
       <c r="B840" s="90"/>
-      <c r="C840" s="175"/>
-      <c r="D840" s="176"/>
-      <c r="E840" s="176"/>
+      <c r="C840" s="178"/>
+      <c r="D840" s="179"/>
+      <c r="E840" s="179"/>
     </row>
     <row r="841" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A841" s="64">
@@ -13096,9 +13115,9 @@
         <v>70</v>
       </c>
       <c r="B857" s="87"/>
-      <c r="C857" s="173"/>
-      <c r="D857" s="174"/>
-      <c r="E857" s="174"/>
+      <c r="C857" s="176"/>
+      <c r="D857" s="177"/>
+      <c r="E857" s="177"/>
     </row>
     <row r="858" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A858" s="64">
@@ -13249,9 +13268,9 @@
         <v>71</v>
       </c>
       <c r="B874" s="87"/>
-      <c r="C874" s="173"/>
-      <c r="D874" s="174"/>
-      <c r="E874" s="174"/>
+      <c r="C874" s="176"/>
+      <c r="D874" s="177"/>
+      <c r="E874" s="177"/>
     </row>
     <row r="875" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A875" s="64">
@@ -13402,9 +13421,9 @@
         <v>72</v>
       </c>
       <c r="B891" s="87"/>
-      <c r="C891" s="173"/>
-      <c r="D891" s="174"/>
-      <c r="E891" s="174"/>
+      <c r="C891" s="176"/>
+      <c r="D891" s="177"/>
+      <c r="E891" s="177"/>
     </row>
     <row r="892" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A892" s="64">
@@ -13555,9 +13574,9 @@
         <v>73</v>
       </c>
       <c r="B908" s="87"/>
-      <c r="C908" s="173"/>
-      <c r="D908" s="174"/>
-      <c r="E908" s="174"/>
+      <c r="C908" s="176"/>
+      <c r="D908" s="177"/>
+      <c r="E908" s="177"/>
     </row>
     <row r="909" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A909" s="64">
@@ -13708,9 +13727,9 @@
         <v>74</v>
       </c>
       <c r="B925" s="87"/>
-      <c r="C925" s="173"/>
-      <c r="D925" s="174"/>
-      <c r="E925" s="174"/>
+      <c r="C925" s="176"/>
+      <c r="D925" s="177"/>
+      <c r="E925" s="177"/>
     </row>
     <row r="926" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A926" s="64">
@@ -13861,9 +13880,9 @@
         <v>75</v>
       </c>
       <c r="B942" s="87"/>
-      <c r="C942" s="173"/>
-      <c r="D942" s="174"/>
-      <c r="E942" s="174"/>
+      <c r="C942" s="176"/>
+      <c r="D942" s="177"/>
+      <c r="E942" s="177"/>
     </row>
     <row r="943" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A943" s="64">
@@ -14014,9 +14033,9 @@
         <v>76</v>
       </c>
       <c r="B959" s="87"/>
-      <c r="C959" s="173"/>
-      <c r="D959" s="174"/>
-      <c r="E959" s="174"/>
+      <c r="C959" s="176"/>
+      <c r="D959" s="177"/>
+      <c r="E959" s="177"/>
     </row>
     <row r="960" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A960" s="64">
@@ -14167,9 +14186,9 @@
         <v>77</v>
       </c>
       <c r="B976" s="87"/>
-      <c r="C976" s="173"/>
-      <c r="D976" s="174"/>
-      <c r="E976" s="174"/>
+      <c r="C976" s="176"/>
+      <c r="D976" s="177"/>
+      <c r="E976" s="177"/>
     </row>
     <row r="977" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A977" s="64">
@@ -14320,9 +14339,9 @@
         <v>78</v>
       </c>
       <c r="B993" s="87"/>
-      <c r="C993" s="173"/>
-      <c r="D993" s="174"/>
-      <c r="E993" s="174"/>
+      <c r="C993" s="176"/>
+      <c r="D993" s="177"/>
+      <c r="E993" s="177"/>
     </row>
     <row r="994" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A994" s="64">
@@ -14473,9 +14492,9 @@
         <v>79</v>
       </c>
       <c r="B1010" s="87"/>
-      <c r="C1010" s="173"/>
-      <c r="D1010" s="174"/>
-      <c r="E1010" s="174"/>
+      <c r="C1010" s="176"/>
+      <c r="D1010" s="177"/>
+      <c r="E1010" s="177"/>
     </row>
     <row r="1011" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1011" s="64">
@@ -14626,9 +14645,9 @@
         <v>80</v>
       </c>
       <c r="B1027" s="87"/>
-      <c r="C1027" s="173"/>
-      <c r="D1027" s="174"/>
-      <c r="E1027" s="174"/>
+      <c r="C1027" s="176"/>
+      <c r="D1027" s="177"/>
+      <c r="E1027" s="177"/>
     </row>
     <row r="1028" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1028" s="64">
@@ -14779,9 +14798,9 @@
         <v>83</v>
       </c>
       <c r="B1044" s="87"/>
-      <c r="C1044" s="173"/>
-      <c r="D1044" s="174"/>
-      <c r="E1044" s="174"/>
+      <c r="C1044" s="176"/>
+      <c r="D1044" s="177"/>
+      <c r="E1044" s="177"/>
     </row>
     <row r="1045" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1045" s="64">
@@ -14932,9 +14951,9 @@
         <v>82</v>
       </c>
       <c r="B1061" s="87"/>
-      <c r="C1061" s="173"/>
-      <c r="D1061" s="174"/>
-      <c r="E1061" s="174"/>
+      <c r="C1061" s="176"/>
+      <c r="D1061" s="177"/>
+      <c r="E1061" s="177"/>
     </row>
     <row r="1062" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1062" s="64">
@@ -15085,9 +15104,9 @@
         <v>84</v>
       </c>
       <c r="B1078" s="87"/>
-      <c r="C1078" s="173"/>
-      <c r="D1078" s="174"/>
-      <c r="E1078" s="174"/>
+      <c r="C1078" s="176"/>
+      <c r="D1078" s="177"/>
+      <c r="E1078" s="177"/>
     </row>
     <row r="1079" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1079" s="64">
@@ -15238,18 +15257,18 @@
         <v>104</v>
       </c>
       <c r="B1095" s="40"/>
-      <c r="C1095" s="183"/>
-      <c r="D1095" s="184"/>
-      <c r="E1095" s="184"/>
+      <c r="C1095" s="186"/>
+      <c r="D1095" s="187"/>
+      <c r="E1095" s="187"/>
     </row>
     <row r="1096" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A1096" s="68" t="s">
         <v>85</v>
       </c>
       <c r="B1096" s="87"/>
-      <c r="C1096" s="173"/>
-      <c r="D1096" s="174"/>
-      <c r="E1096" s="174"/>
+      <c r="C1096" s="176"/>
+      <c r="D1096" s="177"/>
+      <c r="E1096" s="177"/>
     </row>
     <row r="1097" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1097" s="69">
@@ -15400,9 +15419,9 @@
         <v>86</v>
       </c>
       <c r="B1113" s="90"/>
-      <c r="C1113" s="175"/>
-      <c r="D1113" s="176"/>
-      <c r="E1113" s="176"/>
+      <c r="C1113" s="178"/>
+      <c r="D1113" s="179"/>
+      <c r="E1113" s="179"/>
     </row>
     <row r="1114" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1114" s="69">
@@ -15553,9 +15572,9 @@
         <v>87</v>
       </c>
       <c r="B1130" s="87"/>
-      <c r="C1130" s="173"/>
-      <c r="D1130" s="174"/>
-      <c r="E1130" s="174"/>
+      <c r="C1130" s="176"/>
+      <c r="D1130" s="177"/>
+      <c r="E1130" s="177"/>
     </row>
     <row r="1131" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1131" s="69">
@@ -15706,9 +15725,9 @@
         <v>88</v>
       </c>
       <c r="B1147" s="87"/>
-      <c r="C1147" s="173"/>
-      <c r="D1147" s="174"/>
-      <c r="E1147" s="174"/>
+      <c r="C1147" s="176"/>
+      <c r="D1147" s="177"/>
+      <c r="E1147" s="177"/>
     </row>
     <row r="1148" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1148" s="69">
@@ -15859,9 +15878,9 @@
         <v>89</v>
       </c>
       <c r="B1164" s="87"/>
-      <c r="C1164" s="173"/>
-      <c r="D1164" s="174"/>
-      <c r="E1164" s="174"/>
+      <c r="C1164" s="176"/>
+      <c r="D1164" s="177"/>
+      <c r="E1164" s="177"/>
     </row>
     <row r="1165" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1165" s="69">
@@ -16012,9 +16031,9 @@
         <v>90</v>
       </c>
       <c r="B1181" s="87"/>
-      <c r="C1181" s="173"/>
-      <c r="D1181" s="174"/>
-      <c r="E1181" s="174"/>
+      <c r="C1181" s="176"/>
+      <c r="D1181" s="177"/>
+      <c r="E1181" s="177"/>
     </row>
     <row r="1182" spans="1:5" hidden="1" outlineLevel="3">
       <c r="A1182" s="69">
@@ -16165,9 +16184,9 @@
         <v>91</v>
       </c>
       <c r="B1198" s="87"/>
-      <c r="C1198" s="173"/>
-      <c r="D1198" s="174"/>
-      <c r="E1198" s="174"/>
+      <c r="C1198" s="176"/>
+      <c r="D1198" s="177"/>
+      <c r="E1198" s="177"/>
     </row>
     <row r="1199" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1199" s="69">
@@ -16318,9 +16337,9 @@
         <v>92</v>
       </c>
       <c r="B1215" s="87"/>
-      <c r="C1215" s="173"/>
-      <c r="D1215" s="174"/>
-      <c r="E1215" s="174"/>
+      <c r="C1215" s="176"/>
+      <c r="D1215" s="177"/>
+      <c r="E1215" s="177"/>
     </row>
     <row r="1216" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1216" s="69">
@@ -16471,9 +16490,9 @@
         <v>93</v>
       </c>
       <c r="B1232" s="87"/>
-      <c r="C1232" s="173"/>
-      <c r="D1232" s="174"/>
-      <c r="E1232" s="174"/>
+      <c r="C1232" s="176"/>
+      <c r="D1232" s="177"/>
+      <c r="E1232" s="177"/>
     </row>
     <row r="1233" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1233" s="69">
@@ -16624,9 +16643,9 @@
         <v>94</v>
       </c>
       <c r="B1249" s="87"/>
-      <c r="C1249" s="173"/>
-      <c r="D1249" s="174"/>
-      <c r="E1249" s="174"/>
+      <c r="C1249" s="176"/>
+      <c r="D1249" s="177"/>
+      <c r="E1249" s="177"/>
     </row>
     <row r="1250" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1250" s="69">
@@ -16777,9 +16796,9 @@
         <v>99</v>
       </c>
       <c r="B1266" s="87"/>
-      <c r="C1266" s="173"/>
-      <c r="D1266" s="174"/>
-      <c r="E1266" s="174"/>
+      <c r="C1266" s="176"/>
+      <c r="D1266" s="177"/>
+      <c r="E1266" s="177"/>
     </row>
     <row r="1267" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1267" s="69">
@@ -16930,9 +16949,9 @@
         <v>100</v>
       </c>
       <c r="B1283" s="87"/>
-      <c r="C1283" s="173"/>
-      <c r="D1283" s="174"/>
-      <c r="E1283" s="174"/>
+      <c r="C1283" s="176"/>
+      <c r="D1283" s="177"/>
+      <c r="E1283" s="177"/>
     </row>
     <row r="1284" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1284" s="69">
@@ -17083,9 +17102,9 @@
         <v>101</v>
       </c>
       <c r="B1300" s="87"/>
-      <c r="C1300" s="173"/>
-      <c r="D1300" s="174"/>
-      <c r="E1300" s="174"/>
+      <c r="C1300" s="176"/>
+      <c r="D1300" s="177"/>
+      <c r="E1300" s="177"/>
     </row>
     <row r="1301" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1301" s="69">
@@ -17236,9 +17255,9 @@
         <v>81</v>
       </c>
       <c r="B1317" s="87"/>
-      <c r="C1317" s="173"/>
-      <c r="D1317" s="174"/>
-      <c r="E1317" s="174"/>
+      <c r="C1317" s="176"/>
+      <c r="D1317" s="177"/>
+      <c r="E1317" s="177"/>
     </row>
     <row r="1318" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1318" s="69">
@@ -17389,9 +17408,9 @@
         <v>102</v>
       </c>
       <c r="B1334" s="87"/>
-      <c r="C1334" s="173"/>
-      <c r="D1334" s="174"/>
-      <c r="E1334" s="174"/>
+      <c r="C1334" s="176"/>
+      <c r="D1334" s="177"/>
+      <c r="E1334" s="177"/>
     </row>
     <row r="1335" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1335" s="69">
@@ -17542,9 +17561,9 @@
         <v>98</v>
       </c>
       <c r="B1351" s="87"/>
-      <c r="C1351" s="173"/>
-      <c r="D1351" s="174"/>
-      <c r="E1351" s="174"/>
+      <c r="C1351" s="176"/>
+      <c r="D1351" s="177"/>
+      <c r="E1351" s="177"/>
     </row>
     <row r="1352" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1352" s="69">
@@ -17695,18 +17714,18 @@
         <v>103</v>
       </c>
       <c r="B1368" s="41"/>
-      <c r="C1368" s="181"/>
-      <c r="D1368" s="182"/>
-      <c r="E1368" s="182"/>
+      <c r="C1368" s="188"/>
+      <c r="D1368" s="189"/>
+      <c r="E1368" s="189"/>
     </row>
     <row r="1369" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A1369" s="73" t="s">
         <v>105</v>
       </c>
       <c r="B1369" s="87"/>
-      <c r="C1369" s="173"/>
-      <c r="D1369" s="174"/>
-      <c r="E1369" s="174"/>
+      <c r="C1369" s="176"/>
+      <c r="D1369" s="177"/>
+      <c r="E1369" s="177"/>
     </row>
     <row r="1370" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1370" s="74">
@@ -17857,9 +17876,9 @@
         <v>106</v>
       </c>
       <c r="B1386" s="90"/>
-      <c r="C1386" s="175"/>
-      <c r="D1386" s="176"/>
-      <c r="E1386" s="176"/>
+      <c r="C1386" s="178"/>
+      <c r="D1386" s="179"/>
+      <c r="E1386" s="179"/>
     </row>
     <row r="1387" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1387" s="74">
@@ -18010,9 +18029,9 @@
         <v>107</v>
       </c>
       <c r="B1403" s="87"/>
-      <c r="C1403" s="173"/>
-      <c r="D1403" s="174"/>
-      <c r="E1403" s="174"/>
+      <c r="C1403" s="176"/>
+      <c r="D1403" s="177"/>
+      <c r="E1403" s="177"/>
     </row>
     <row r="1404" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1404" s="74">
@@ -18163,9 +18182,9 @@
         <v>108</v>
       </c>
       <c r="B1420" s="87"/>
-      <c r="C1420" s="173"/>
-      <c r="D1420" s="174"/>
-      <c r="E1420" s="174"/>
+      <c r="C1420" s="176"/>
+      <c r="D1420" s="177"/>
+      <c r="E1420" s="177"/>
     </row>
     <row r="1421" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1421" s="74">
@@ -18316,9 +18335,9 @@
         <v>109</v>
       </c>
       <c r="B1437" s="87"/>
-      <c r="C1437" s="173"/>
-      <c r="D1437" s="174"/>
-      <c r="E1437" s="174"/>
+      <c r="C1437" s="176"/>
+      <c r="D1437" s="177"/>
+      <c r="E1437" s="177"/>
     </row>
     <row r="1438" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1438" s="74">
@@ -18469,9 +18488,9 @@
         <v>110</v>
       </c>
       <c r="B1454" s="87"/>
-      <c r="C1454" s="173"/>
-      <c r="D1454" s="174"/>
-      <c r="E1454" s="174"/>
+      <c r="C1454" s="176"/>
+      <c r="D1454" s="177"/>
+      <c r="E1454" s="177"/>
     </row>
     <row r="1455" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1455" s="74">
@@ -18622,9 +18641,9 @@
         <v>111</v>
       </c>
       <c r="B1471" s="87"/>
-      <c r="C1471" s="173"/>
-      <c r="D1471" s="174"/>
-      <c r="E1471" s="174"/>
+      <c r="C1471" s="176"/>
+      <c r="D1471" s="177"/>
+      <c r="E1471" s="177"/>
     </row>
     <row r="1472" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1472" s="74">
@@ -18775,9 +18794,9 @@
         <v>112</v>
       </c>
       <c r="B1488" s="87"/>
-      <c r="C1488" s="173"/>
-      <c r="D1488" s="174"/>
-      <c r="E1488" s="174"/>
+      <c r="C1488" s="176"/>
+      <c r="D1488" s="177"/>
+      <c r="E1488" s="177"/>
     </row>
     <row r="1489" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1489" s="74">
@@ -18928,9 +18947,9 @@
         <v>113</v>
       </c>
       <c r="B1505" s="87"/>
-      <c r="C1505" s="173"/>
-      <c r="D1505" s="174"/>
-      <c r="E1505" s="174"/>
+      <c r="C1505" s="176"/>
+      <c r="D1505" s="177"/>
+      <c r="E1505" s="177"/>
     </row>
     <row r="1506" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1506" s="74">
@@ -19081,9 +19100,9 @@
         <v>114</v>
       </c>
       <c r="B1522" s="87"/>
-      <c r="C1522" s="173"/>
-      <c r="D1522" s="174"/>
-      <c r="E1522" s="174"/>
+      <c r="C1522" s="176"/>
+      <c r="D1522" s="177"/>
+      <c r="E1522" s="177"/>
     </row>
     <row r="1523" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1523" s="74">
@@ -19234,9 +19253,9 @@
         <v>95</v>
       </c>
       <c r="B1539" s="87"/>
-      <c r="C1539" s="173"/>
-      <c r="D1539" s="174"/>
-      <c r="E1539" s="174"/>
+      <c r="C1539" s="176"/>
+      <c r="D1539" s="177"/>
+      <c r="E1539" s="177"/>
     </row>
     <row r="1540" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1540" s="74">
@@ -19387,9 +19406,9 @@
         <v>115</v>
       </c>
       <c r="B1556" s="87"/>
-      <c r="C1556" s="173"/>
-      <c r="D1556" s="174"/>
-      <c r="E1556" s="174"/>
+      <c r="C1556" s="176"/>
+      <c r="D1556" s="177"/>
+      <c r="E1556" s="177"/>
     </row>
     <row r="1557" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1557" s="74">
@@ -19540,9 +19559,9 @@
         <v>116</v>
       </c>
       <c r="B1573" s="87"/>
-      <c r="C1573" s="173"/>
-      <c r="D1573" s="174"/>
-      <c r="E1573" s="174"/>
+      <c r="C1573" s="176"/>
+      <c r="D1573" s="177"/>
+      <c r="E1573" s="177"/>
     </row>
     <row r="1574" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1574" s="74">
@@ -19693,9 +19712,9 @@
         <v>117</v>
       </c>
       <c r="B1590" s="87"/>
-      <c r="C1590" s="173"/>
-      <c r="D1590" s="174"/>
-      <c r="E1590" s="174"/>
+      <c r="C1590" s="176"/>
+      <c r="D1590" s="177"/>
+      <c r="E1590" s="177"/>
     </row>
     <row r="1591" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1591" s="74">
@@ -19846,9 +19865,9 @@
         <v>118</v>
       </c>
       <c r="B1607" s="87"/>
-      <c r="C1607" s="173"/>
-      <c r="D1607" s="174"/>
-      <c r="E1607" s="174"/>
+      <c r="C1607" s="176"/>
+      <c r="D1607" s="177"/>
+      <c r="E1607" s="177"/>
     </row>
     <row r="1608" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1608" s="74">
@@ -19999,9 +20018,9 @@
         <v>119</v>
       </c>
       <c r="B1624" s="87"/>
-      <c r="C1624" s="173"/>
-      <c r="D1624" s="174"/>
-      <c r="E1624" s="174"/>
+      <c r="C1624" s="176"/>
+      <c r="D1624" s="177"/>
+      <c r="E1624" s="177"/>
     </row>
     <row r="1625" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1625" s="74">
@@ -20152,18 +20171,18 @@
         <v>120</v>
       </c>
       <c r="B1641" s="42"/>
-      <c r="C1641" s="179"/>
-      <c r="D1641" s="180"/>
-      <c r="E1641" s="180"/>
+      <c r="C1641" s="190"/>
+      <c r="D1641" s="191"/>
+      <c r="E1641" s="191"/>
     </row>
     <row r="1642" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A1642" s="78" t="s">
         <v>121</v>
       </c>
       <c r="B1642" s="87"/>
-      <c r="C1642" s="173"/>
-      <c r="D1642" s="174"/>
-      <c r="E1642" s="174"/>
+      <c r="C1642" s="176"/>
+      <c r="D1642" s="177"/>
+      <c r="E1642" s="177"/>
     </row>
     <row r="1643" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1643" s="79">
@@ -20314,9 +20333,9 @@
         <v>122</v>
       </c>
       <c r="B1659" s="90"/>
-      <c r="C1659" s="175"/>
-      <c r="D1659" s="176"/>
-      <c r="E1659" s="176"/>
+      <c r="C1659" s="178"/>
+      <c r="D1659" s="179"/>
+      <c r="E1659" s="179"/>
     </row>
     <row r="1660" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1660" s="79">
@@ -20467,9 +20486,9 @@
         <v>123</v>
       </c>
       <c r="B1676" s="87"/>
-      <c r="C1676" s="173"/>
-      <c r="D1676" s="174"/>
-      <c r="E1676" s="174"/>
+      <c r="C1676" s="176"/>
+      <c r="D1676" s="177"/>
+      <c r="E1676" s="177"/>
     </row>
     <row r="1677" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1677" s="79">
@@ -20620,9 +20639,9 @@
         <v>124</v>
       </c>
       <c r="B1693" s="87"/>
-      <c r="C1693" s="173"/>
-      <c r="D1693" s="174"/>
-      <c r="E1693" s="174"/>
+      <c r="C1693" s="176"/>
+      <c r="D1693" s="177"/>
+      <c r="E1693" s="177"/>
     </row>
     <row r="1694" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1694" s="79">
@@ -20773,9 +20792,9 @@
         <v>125</v>
       </c>
       <c r="B1710" s="87"/>
-      <c r="C1710" s="173"/>
-      <c r="D1710" s="174"/>
-      <c r="E1710" s="174"/>
+      <c r="C1710" s="176"/>
+      <c r="D1710" s="177"/>
+      <c r="E1710" s="177"/>
     </row>
     <row r="1711" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1711" s="79">
@@ -20926,9 +20945,9 @@
         <v>126</v>
       </c>
       <c r="B1727" s="87"/>
-      <c r="C1727" s="173"/>
-      <c r="D1727" s="174"/>
-      <c r="E1727" s="174"/>
+      <c r="C1727" s="176"/>
+      <c r="D1727" s="177"/>
+      <c r="E1727" s="177"/>
     </row>
     <row r="1728" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1728" s="79">
@@ -21079,9 +21098,9 @@
         <v>127</v>
       </c>
       <c r="B1744" s="87"/>
-      <c r="C1744" s="173"/>
-      <c r="D1744" s="174"/>
-      <c r="E1744" s="174"/>
+      <c r="C1744" s="176"/>
+      <c r="D1744" s="177"/>
+      <c r="E1744" s="177"/>
     </row>
     <row r="1745" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1745" s="79">
@@ -21232,9 +21251,9 @@
         <v>128</v>
       </c>
       <c r="B1761" s="87"/>
-      <c r="C1761" s="173"/>
-      <c r="D1761" s="174"/>
-      <c r="E1761" s="174"/>
+      <c r="C1761" s="176"/>
+      <c r="D1761" s="177"/>
+      <c r="E1761" s="177"/>
     </row>
     <row r="1762" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1762" s="79">
@@ -21385,9 +21404,9 @@
         <v>129</v>
       </c>
       <c r="B1778" s="87"/>
-      <c r="C1778" s="173"/>
-      <c r="D1778" s="174"/>
-      <c r="E1778" s="174"/>
+      <c r="C1778" s="176"/>
+      <c r="D1778" s="177"/>
+      <c r="E1778" s="177"/>
     </row>
     <row r="1779" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1779" s="79">
@@ -21538,9 +21557,9 @@
         <v>130</v>
       </c>
       <c r="B1795" s="87"/>
-      <c r="C1795" s="173"/>
-      <c r="D1795" s="174"/>
-      <c r="E1795" s="174"/>
+      <c r="C1795" s="176"/>
+      <c r="D1795" s="177"/>
+      <c r="E1795" s="177"/>
     </row>
     <row r="1796" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1796" s="79">
@@ -21691,9 +21710,9 @@
         <v>131</v>
       </c>
       <c r="B1812" s="87"/>
-      <c r="C1812" s="173"/>
-      <c r="D1812" s="174"/>
-      <c r="E1812" s="174"/>
+      <c r="C1812" s="176"/>
+      <c r="D1812" s="177"/>
+      <c r="E1812" s="177"/>
     </row>
     <row r="1813" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1813" s="79">
@@ -21844,9 +21863,9 @@
         <v>96</v>
       </c>
       <c r="B1829" s="87"/>
-      <c r="C1829" s="173"/>
-      <c r="D1829" s="174"/>
-      <c r="E1829" s="174"/>
+      <c r="C1829" s="176"/>
+      <c r="D1829" s="177"/>
+      <c r="E1829" s="177"/>
     </row>
     <row r="1830" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1830" s="79">
@@ -21997,9 +22016,9 @@
         <v>132</v>
       </c>
       <c r="B1846" s="87"/>
-      <c r="C1846" s="173"/>
-      <c r="D1846" s="174"/>
-      <c r="E1846" s="174"/>
+      <c r="C1846" s="176"/>
+      <c r="D1846" s="177"/>
+      <c r="E1846" s="177"/>
     </row>
     <row r="1847" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1847" s="79">
@@ -22150,9 +22169,9 @@
         <v>133</v>
       </c>
       <c r="B1863" s="87"/>
-      <c r="C1863" s="173"/>
-      <c r="D1863" s="174"/>
-      <c r="E1863" s="174"/>
+      <c r="C1863" s="176"/>
+      <c r="D1863" s="177"/>
+      <c r="E1863" s="177"/>
     </row>
     <row r="1864" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1864" s="79">
@@ -22303,9 +22322,9 @@
         <v>134</v>
       </c>
       <c r="B1880" s="87"/>
-      <c r="C1880" s="173"/>
-      <c r="D1880" s="174"/>
-      <c r="E1880" s="174"/>
+      <c r="C1880" s="176"/>
+      <c r="D1880" s="177"/>
+      <c r="E1880" s="177"/>
     </row>
     <row r="1881" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1881" s="79">
@@ -22456,9 +22475,9 @@
         <v>135</v>
       </c>
       <c r="B1897" s="87"/>
-      <c r="C1897" s="173"/>
-      <c r="D1897" s="174"/>
-      <c r="E1897" s="174"/>
+      <c r="C1897" s="176"/>
+      <c r="D1897" s="177"/>
+      <c r="E1897" s="177"/>
     </row>
     <row r="1898" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1898" s="79">
@@ -22609,18 +22628,18 @@
         <v>136</v>
       </c>
       <c r="B1914" s="43"/>
-      <c r="C1914" s="177"/>
-      <c r="D1914" s="178"/>
-      <c r="E1914" s="178"/>
+      <c r="C1914" s="192"/>
+      <c r="D1914" s="193"/>
+      <c r="E1914" s="193"/>
     </row>
     <row r="1915" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A1915" s="83" t="s">
         <v>137</v>
       </c>
       <c r="B1915" s="87"/>
-      <c r="C1915" s="173"/>
-      <c r="D1915" s="174"/>
-      <c r="E1915" s="174"/>
+      <c r="C1915" s="176"/>
+      <c r="D1915" s="177"/>
+      <c r="E1915" s="177"/>
     </row>
     <row r="1916" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1916" s="84">
@@ -22771,9 +22790,9 @@
         <v>138</v>
       </c>
       <c r="B1932" s="90"/>
-      <c r="C1932" s="175"/>
-      <c r="D1932" s="176"/>
-      <c r="E1932" s="176"/>
+      <c r="C1932" s="178"/>
+      <c r="D1932" s="179"/>
+      <c r="E1932" s="179"/>
     </row>
     <row r="1933" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1933" s="84">
@@ -22924,9 +22943,9 @@
         <v>139</v>
       </c>
       <c r="B1949" s="87"/>
-      <c r="C1949" s="173"/>
-      <c r="D1949" s="174"/>
-      <c r="E1949" s="174"/>
+      <c r="C1949" s="176"/>
+      <c r="D1949" s="177"/>
+      <c r="E1949" s="177"/>
     </row>
     <row r="1950" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1950" s="84">
@@ -23077,9 +23096,9 @@
         <v>140</v>
       </c>
       <c r="B1966" s="87"/>
-      <c r="C1966" s="173"/>
-      <c r="D1966" s="174"/>
-      <c r="E1966" s="174"/>
+      <c r="C1966" s="176"/>
+      <c r="D1966" s="177"/>
+      <c r="E1966" s="177"/>
     </row>
     <row r="1967" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1967" s="84">
@@ -23230,9 +23249,9 @@
         <v>141</v>
       </c>
       <c r="B1983" s="87"/>
-      <c r="C1983" s="173"/>
-      <c r="D1983" s="174"/>
-      <c r="E1983" s="174"/>
+      <c r="C1983" s="176"/>
+      <c r="D1983" s="177"/>
+      <c r="E1983" s="177"/>
     </row>
     <row r="1984" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1984" s="84">
@@ -23383,9 +23402,9 @@
         <v>142</v>
       </c>
       <c r="B2000" s="87"/>
-      <c r="C2000" s="173"/>
-      <c r="D2000" s="174"/>
-      <c r="E2000" s="174"/>
+      <c r="C2000" s="176"/>
+      <c r="D2000" s="177"/>
+      <c r="E2000" s="177"/>
     </row>
     <row r="2001" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2001" s="84">
@@ -23536,9 +23555,9 @@
         <v>143</v>
       </c>
       <c r="B2017" s="87"/>
-      <c r="C2017" s="173"/>
-      <c r="D2017" s="174"/>
-      <c r="E2017" s="174"/>
+      <c r="C2017" s="176"/>
+      <c r="D2017" s="177"/>
+      <c r="E2017" s="177"/>
     </row>
     <row r="2018" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2018" s="84">
@@ -23689,9 +23708,9 @@
         <v>144</v>
       </c>
       <c r="B2034" s="87"/>
-      <c r="C2034" s="173"/>
-      <c r="D2034" s="174"/>
-      <c r="E2034" s="174"/>
+      <c r="C2034" s="176"/>
+      <c r="D2034" s="177"/>
+      <c r="E2034" s="177"/>
     </row>
     <row r="2035" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2035" s="84">
@@ -23842,9 +23861,9 @@
         <v>145</v>
       </c>
       <c r="B2051" s="87"/>
-      <c r="C2051" s="173"/>
-      <c r="D2051" s="174"/>
-      <c r="E2051" s="174"/>
+      <c r="C2051" s="176"/>
+      <c r="D2051" s="177"/>
+      <c r="E2051" s="177"/>
     </row>
     <row r="2052" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2052" s="84">
@@ -23995,9 +24014,9 @@
         <v>146</v>
       </c>
       <c r="B2068" s="87"/>
-      <c r="C2068" s="173"/>
-      <c r="D2068" s="174"/>
-      <c r="E2068" s="174"/>
+      <c r="C2068" s="176"/>
+      <c r="D2068" s="177"/>
+      <c r="E2068" s="177"/>
     </row>
     <row r="2069" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2069" s="84">
@@ -24148,9 +24167,9 @@
         <v>147</v>
       </c>
       <c r="B2085" s="87"/>
-      <c r="C2085" s="173"/>
-      <c r="D2085" s="174"/>
-      <c r="E2085" s="174"/>
+      <c r="C2085" s="176"/>
+      <c r="D2085" s="177"/>
+      <c r="E2085" s="177"/>
     </row>
     <row r="2086" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2086" s="84">
@@ -24301,9 +24320,9 @@
         <v>148</v>
       </c>
       <c r="B2102" s="87"/>
-      <c r="C2102" s="173"/>
-      <c r="D2102" s="174"/>
-      <c r="E2102" s="174"/>
+      <c r="C2102" s="176"/>
+      <c r="D2102" s="177"/>
+      <c r="E2102" s="177"/>
     </row>
     <row r="2103" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2103" s="84">
@@ -24454,9 +24473,9 @@
         <v>97</v>
       </c>
       <c r="B2119" s="87"/>
-      <c r="C2119" s="173"/>
-      <c r="D2119" s="174"/>
-      <c r="E2119" s="174"/>
+      <c r="C2119" s="176"/>
+      <c r="D2119" s="177"/>
+      <c r="E2119" s="177"/>
     </row>
     <row r="2120" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2120" s="84">
@@ -24607,9 +24626,9 @@
         <v>149</v>
       </c>
       <c r="B2136" s="87"/>
-      <c r="C2136" s="173"/>
-      <c r="D2136" s="174"/>
-      <c r="E2136" s="174"/>
+      <c r="C2136" s="176"/>
+      <c r="D2136" s="177"/>
+      <c r="E2136" s="177"/>
     </row>
     <row r="2137" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2137" s="84">
@@ -24760,9 +24779,9 @@
         <v>150</v>
       </c>
       <c r="B2153" s="87"/>
-      <c r="C2153" s="173"/>
-      <c r="D2153" s="174"/>
-      <c r="E2153" s="174"/>
+      <c r="C2153" s="176"/>
+      <c r="D2153" s="177"/>
+      <c r="E2153" s="177"/>
     </row>
     <row r="2154" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2154" s="84">
@@ -24913,9 +24932,9 @@
         <v>151</v>
       </c>
       <c r="B2170" s="87"/>
-      <c r="C2170" s="173"/>
-      <c r="D2170" s="174"/>
-      <c r="E2170" s="174"/>
+      <c r="C2170" s="176"/>
+      <c r="D2170" s="177"/>
+      <c r="E2170" s="177"/>
     </row>
     <row r="2171" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2171" s="84">
@@ -25063,26 +25082,111 @@
     </row>
   </sheetData>
   <mergeCells count="137">
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="C89:E89"/>
-    <mergeCell ref="C21:E21"/>
-    <mergeCell ref="C38:E38"/>
-    <mergeCell ref="C55:E55"/>
-    <mergeCell ref="C72:E72"/>
-    <mergeCell ref="C208:E208"/>
-    <mergeCell ref="C225:E225"/>
-    <mergeCell ref="C242:E242"/>
-    <mergeCell ref="C259:E259"/>
-    <mergeCell ref="C276:E276"/>
-    <mergeCell ref="C277:E277"/>
-    <mergeCell ref="C106:E106"/>
-    <mergeCell ref="C123:E123"/>
-    <mergeCell ref="C140:E140"/>
-    <mergeCell ref="C157:E157"/>
-    <mergeCell ref="C174:E174"/>
-    <mergeCell ref="C191:E191"/>
+    <mergeCell ref="C2034:E2034"/>
+    <mergeCell ref="C2051:E2051"/>
+    <mergeCell ref="C2068:E2068"/>
+    <mergeCell ref="C2085:E2085"/>
+    <mergeCell ref="C2170:E2170"/>
+    <mergeCell ref="C2102:E2102"/>
+    <mergeCell ref="C2119:E2119"/>
+    <mergeCell ref="C2136:E2136"/>
+    <mergeCell ref="C2153:E2153"/>
+    <mergeCell ref="C1932:E1932"/>
+    <mergeCell ref="C1949:E1949"/>
+    <mergeCell ref="C1966:E1966"/>
+    <mergeCell ref="C1983:E1983"/>
+    <mergeCell ref="C2000:E2000"/>
+    <mergeCell ref="C2017:E2017"/>
+    <mergeCell ref="C1846:E1846"/>
+    <mergeCell ref="C1863:E1863"/>
+    <mergeCell ref="C1880:E1880"/>
+    <mergeCell ref="C1897:E1897"/>
+    <mergeCell ref="C1914:E1914"/>
+    <mergeCell ref="C1915:E1915"/>
+    <mergeCell ref="C1744:E1744"/>
+    <mergeCell ref="C1761:E1761"/>
+    <mergeCell ref="C1778:E1778"/>
+    <mergeCell ref="C1795:E1795"/>
+    <mergeCell ref="C1812:E1812"/>
+    <mergeCell ref="C1829:E1829"/>
+    <mergeCell ref="C1642:E1642"/>
+    <mergeCell ref="C1659:E1659"/>
+    <mergeCell ref="C1676:E1676"/>
+    <mergeCell ref="C1693:E1693"/>
+    <mergeCell ref="C1710:E1710"/>
+    <mergeCell ref="C1727:E1727"/>
+    <mergeCell ref="C1556:E1556"/>
+    <mergeCell ref="C1573:E1573"/>
+    <mergeCell ref="C1590:E1590"/>
+    <mergeCell ref="C1607:E1607"/>
+    <mergeCell ref="C1624:E1624"/>
+    <mergeCell ref="C1641:E1641"/>
+    <mergeCell ref="C1454:E1454"/>
+    <mergeCell ref="C1471:E1471"/>
+    <mergeCell ref="C1488:E1488"/>
+    <mergeCell ref="C1505:E1505"/>
+    <mergeCell ref="C1522:E1522"/>
+    <mergeCell ref="C1539:E1539"/>
+    <mergeCell ref="C1368:E1368"/>
+    <mergeCell ref="C1369:E1369"/>
+    <mergeCell ref="C1386:E1386"/>
+    <mergeCell ref="C1403:E1403"/>
+    <mergeCell ref="C1420:E1420"/>
+    <mergeCell ref="C1437:E1437"/>
+    <mergeCell ref="C1266:E1266"/>
+    <mergeCell ref="C1283:E1283"/>
+    <mergeCell ref="C1300:E1300"/>
+    <mergeCell ref="C1317:E1317"/>
+    <mergeCell ref="C1334:E1334"/>
+    <mergeCell ref="C1351:E1351"/>
+    <mergeCell ref="C1164:E1164"/>
+    <mergeCell ref="C1181:E1181"/>
+    <mergeCell ref="C1198:E1198"/>
+    <mergeCell ref="C1215:E1215"/>
+    <mergeCell ref="C1232:E1232"/>
+    <mergeCell ref="C1249:E1249"/>
+    <mergeCell ref="C1078:E1078"/>
+    <mergeCell ref="C1095:E1095"/>
+    <mergeCell ref="C1096:E1096"/>
+    <mergeCell ref="C1113:E1113"/>
+    <mergeCell ref="C1130:E1130"/>
+    <mergeCell ref="C1147:E1147"/>
+    <mergeCell ref="C976:E976"/>
+    <mergeCell ref="C993:E993"/>
+    <mergeCell ref="C1010:E1010"/>
+    <mergeCell ref="C1027:E1027"/>
+    <mergeCell ref="C1044:E1044"/>
+    <mergeCell ref="C1061:E1061"/>
+    <mergeCell ref="C874:E874"/>
+    <mergeCell ref="C891:E891"/>
+    <mergeCell ref="C908:E908"/>
+    <mergeCell ref="C925:E925"/>
+    <mergeCell ref="C942:E942"/>
+    <mergeCell ref="C959:E959"/>
+    <mergeCell ref="C788:E788"/>
+    <mergeCell ref="C805:E805"/>
+    <mergeCell ref="C822:E822"/>
+    <mergeCell ref="C823:E823"/>
+    <mergeCell ref="C840:E840"/>
+    <mergeCell ref="C857:E857"/>
+    <mergeCell ref="C686:E686"/>
+    <mergeCell ref="C703:E703"/>
+    <mergeCell ref="C720:E720"/>
+    <mergeCell ref="C737:E737"/>
+    <mergeCell ref="C754:E754"/>
+    <mergeCell ref="C771:E771"/>
+    <mergeCell ref="C584:E584"/>
+    <mergeCell ref="C601:E601"/>
+    <mergeCell ref="C618:E618"/>
+    <mergeCell ref="C635:E635"/>
+    <mergeCell ref="C652:E652"/>
+    <mergeCell ref="C669:E669"/>
+    <mergeCell ref="C498:E498"/>
+    <mergeCell ref="C515:E515"/>
+    <mergeCell ref="C532:E532"/>
+    <mergeCell ref="C549:E549"/>
+    <mergeCell ref="C550:E550"/>
+    <mergeCell ref="C567:E567"/>
     <mergeCell ref="C396:E396"/>
     <mergeCell ref="C413:E413"/>
     <mergeCell ref="C430:E430"/>
@@ -25095,113 +25199,28 @@
     <mergeCell ref="C345:E345"/>
     <mergeCell ref="C362:E362"/>
     <mergeCell ref="C379:E379"/>
-    <mergeCell ref="C584:E584"/>
-    <mergeCell ref="C601:E601"/>
-    <mergeCell ref="C618:E618"/>
-    <mergeCell ref="C635:E635"/>
-    <mergeCell ref="C652:E652"/>
-    <mergeCell ref="C669:E669"/>
-    <mergeCell ref="C498:E498"/>
-    <mergeCell ref="C515:E515"/>
-    <mergeCell ref="C532:E532"/>
-    <mergeCell ref="C549:E549"/>
-    <mergeCell ref="C550:E550"/>
-    <mergeCell ref="C567:E567"/>
-    <mergeCell ref="C788:E788"/>
-    <mergeCell ref="C805:E805"/>
-    <mergeCell ref="C822:E822"/>
-    <mergeCell ref="C823:E823"/>
-    <mergeCell ref="C840:E840"/>
-    <mergeCell ref="C857:E857"/>
-    <mergeCell ref="C686:E686"/>
-    <mergeCell ref="C703:E703"/>
-    <mergeCell ref="C720:E720"/>
-    <mergeCell ref="C737:E737"/>
-    <mergeCell ref="C754:E754"/>
-    <mergeCell ref="C771:E771"/>
-    <mergeCell ref="C976:E976"/>
-    <mergeCell ref="C993:E993"/>
-    <mergeCell ref="C1010:E1010"/>
-    <mergeCell ref="C1027:E1027"/>
-    <mergeCell ref="C1044:E1044"/>
-    <mergeCell ref="C1061:E1061"/>
-    <mergeCell ref="C874:E874"/>
-    <mergeCell ref="C891:E891"/>
-    <mergeCell ref="C908:E908"/>
-    <mergeCell ref="C925:E925"/>
-    <mergeCell ref="C942:E942"/>
-    <mergeCell ref="C959:E959"/>
-    <mergeCell ref="C1164:E1164"/>
-    <mergeCell ref="C1181:E1181"/>
-    <mergeCell ref="C1198:E1198"/>
-    <mergeCell ref="C1215:E1215"/>
-    <mergeCell ref="C1232:E1232"/>
-    <mergeCell ref="C1249:E1249"/>
-    <mergeCell ref="C1078:E1078"/>
-    <mergeCell ref="C1095:E1095"/>
-    <mergeCell ref="C1096:E1096"/>
-    <mergeCell ref="C1113:E1113"/>
-    <mergeCell ref="C1130:E1130"/>
-    <mergeCell ref="C1147:E1147"/>
-    <mergeCell ref="C1368:E1368"/>
-    <mergeCell ref="C1369:E1369"/>
-    <mergeCell ref="C1386:E1386"/>
-    <mergeCell ref="C1403:E1403"/>
-    <mergeCell ref="C1420:E1420"/>
-    <mergeCell ref="C1437:E1437"/>
-    <mergeCell ref="C1266:E1266"/>
-    <mergeCell ref="C1283:E1283"/>
-    <mergeCell ref="C1300:E1300"/>
-    <mergeCell ref="C1317:E1317"/>
-    <mergeCell ref="C1334:E1334"/>
-    <mergeCell ref="C1351:E1351"/>
-    <mergeCell ref="C1556:E1556"/>
-    <mergeCell ref="C1573:E1573"/>
-    <mergeCell ref="C1590:E1590"/>
-    <mergeCell ref="C1607:E1607"/>
-    <mergeCell ref="C1624:E1624"/>
-    <mergeCell ref="C1641:E1641"/>
-    <mergeCell ref="C1454:E1454"/>
-    <mergeCell ref="C1471:E1471"/>
-    <mergeCell ref="C1488:E1488"/>
-    <mergeCell ref="C1505:E1505"/>
-    <mergeCell ref="C1522:E1522"/>
-    <mergeCell ref="C1539:E1539"/>
-    <mergeCell ref="C1744:E1744"/>
-    <mergeCell ref="C1761:E1761"/>
-    <mergeCell ref="C1778:E1778"/>
-    <mergeCell ref="C1795:E1795"/>
-    <mergeCell ref="C1812:E1812"/>
-    <mergeCell ref="C1829:E1829"/>
-    <mergeCell ref="C1642:E1642"/>
-    <mergeCell ref="C1659:E1659"/>
-    <mergeCell ref="C1676:E1676"/>
-    <mergeCell ref="C1693:E1693"/>
-    <mergeCell ref="C1710:E1710"/>
-    <mergeCell ref="C1727:E1727"/>
-    <mergeCell ref="C1932:E1932"/>
-    <mergeCell ref="C1949:E1949"/>
-    <mergeCell ref="C1966:E1966"/>
-    <mergeCell ref="C1983:E1983"/>
-    <mergeCell ref="C2000:E2000"/>
-    <mergeCell ref="C2017:E2017"/>
-    <mergeCell ref="C1846:E1846"/>
-    <mergeCell ref="C1863:E1863"/>
-    <mergeCell ref="C1880:E1880"/>
-    <mergeCell ref="C1897:E1897"/>
-    <mergeCell ref="C1914:E1914"/>
-    <mergeCell ref="C1915:E1915"/>
-    <mergeCell ref="C2034:E2034"/>
-    <mergeCell ref="C2051:E2051"/>
-    <mergeCell ref="C2068:E2068"/>
-    <mergeCell ref="C2085:E2085"/>
-    <mergeCell ref="C2170:E2170"/>
-    <mergeCell ref="C2102:E2102"/>
-    <mergeCell ref="C2119:E2119"/>
-    <mergeCell ref="C2136:E2136"/>
-    <mergeCell ref="C2153:E2153"/>
+    <mergeCell ref="C225:E225"/>
+    <mergeCell ref="C242:E242"/>
+    <mergeCell ref="C259:E259"/>
+    <mergeCell ref="C276:E276"/>
+    <mergeCell ref="C277:E277"/>
+    <mergeCell ref="C106:E106"/>
+    <mergeCell ref="C123:E123"/>
+    <mergeCell ref="C140:E140"/>
+    <mergeCell ref="C157:E157"/>
+    <mergeCell ref="C174:E174"/>
+    <mergeCell ref="C191:E191"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="C89:E89"/>
+    <mergeCell ref="C21:E21"/>
+    <mergeCell ref="C38:E38"/>
+    <mergeCell ref="C55:E55"/>
+    <mergeCell ref="C72:E72"/>
+    <mergeCell ref="C208:E208"/>
   </mergeCells>
-  <phoneticPr fontId="13" type="noConversion"/>
+  <phoneticPr fontId="14" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967294" verticalDpi="0" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
@@ -25952,7 +25971,7 @@
     <mergeCell ref="A3:K3"/>
     <mergeCell ref="A20:K20"/>
   </mergeCells>
-  <phoneticPr fontId="13" type="noConversion"/>
+  <phoneticPr fontId="14" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
@@ -26163,7 +26182,7 @@
   <mergeCells count="1">
     <mergeCell ref="A3:A10"/>
   </mergeCells>
-  <phoneticPr fontId="13" type="noConversion"/>
+  <phoneticPr fontId="14" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
@@ -26436,7 +26455,7 @@
     <mergeCell ref="A11:A17"/>
     <mergeCell ref="A19:A25"/>
   </mergeCells>
-  <phoneticPr fontId="13" type="noConversion"/>
+  <phoneticPr fontId="14" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
@@ -26458,163 +26477,150 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="33">
-      <c r="A1" s="218" t="s">
+      <c r="A1" s="219" t="s">
         <v>184</v>
       </c>
-      <c r="B1" s="219"/>
+      <c r="B1" s="220"/>
       <c r="C1" s="118"/>
       <c r="D1" s="5"/>
       <c r="E1" s="5"/>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="215" t="s">
+      <c r="A2" s="225" t="s">
         <v>183</v>
       </c>
-      <c r="B2" s="216"/>
+      <c r="B2" s="226"/>
       <c r="C2" s="120"/>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="217" t="s">
+      <c r="A3" s="227" t="s">
         <v>185</v>
       </c>
-      <c r="B3" s="216"/>
+      <c r="B3" s="226"/>
       <c r="C3" s="120"/>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="222"/>
-      <c r="B4" s="223"/>
+      <c r="A4" s="223"/>
+      <c r="B4" s="224"/>
       <c r="C4" s="120"/>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="220" t="s">
+      <c r="A5" s="221" t="s">
         <v>194</v>
       </c>
-      <c r="B5" s="221"/>
+      <c r="B5" s="222"/>
       <c r="C5" s="120"/>
     </row>
     <row r="7" spans="1:5" ht="18.75">
-      <c r="A7" s="226" t="s">
+      <c r="A7" s="213" t="s">
         <v>186</v>
       </c>
-      <c r="B7" s="227"/>
+      <c r="B7" s="214"/>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="120"/>
       <c r="B8" s="9"/>
     </row>
     <row r="9" spans="1:5" ht="39" customHeight="1">
-      <c r="A9" s="224" t="s">
+      <c r="A9" s="215" t="s">
         <v>187</v>
       </c>
-      <c r="B9" s="225"/>
+      <c r="B9" s="216"/>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="211"/>
-      <c r="B10" s="212"/>
+      <c r="A10" s="217"/>
+      <c r="B10" s="218"/>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="213" t="s">
+      <c r="A11" s="209" t="s">
         <v>188</v>
       </c>
-      <c r="B11" s="214"/>
+      <c r="B11" s="210"/>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="213" t="s">
+      <c r="A12" s="209" t="s">
         <v>189</v>
       </c>
-      <c r="B12" s="214"/>
+      <c r="B12" s="210"/>
     </row>
     <row r="13" spans="1:5" ht="43.5" customHeight="1">
-      <c r="A13" s="213" t="s">
+      <c r="A13" s="209" t="s">
         <v>190</v>
       </c>
-      <c r="B13" s="214"/>
+      <c r="B13" s="210"/>
     </row>
     <row r="14" spans="1:5" ht="19.5" customHeight="1">
-      <c r="A14" s="213" t="s">
+      <c r="A14" s="209" t="s">
         <v>191</v>
       </c>
-      <c r="B14" s="214"/>
+      <c r="B14" s="210"/>
     </row>
     <row r="15" spans="1:5" ht="18" customHeight="1">
-      <c r="A15" s="213" t="s">
+      <c r="A15" s="209" t="s">
         <v>192</v>
       </c>
-      <c r="B15" s="214"/>
+      <c r="B15" s="210"/>
     </row>
     <row r="16" spans="1:5" ht="21" customHeight="1">
-      <c r="A16" s="213" t="s">
+      <c r="A16" s="209" t="s">
         <v>193</v>
       </c>
-      <c r="B16" s="214"/>
+      <c r="B16" s="210"/>
     </row>
     <row r="17" spans="1:2" ht="48.75" customHeight="1">
-      <c r="A17" s="209" t="s">
+      <c r="A17" s="211" t="s">
         <v>195</v>
       </c>
-      <c r="B17" s="210"/>
+      <c r="B17" s="212"/>
     </row>
     <row r="19" spans="1:2" ht="18.75">
-      <c r="A19" s="226" t="s">
+      <c r="A19" s="213" t="s">
         <v>197</v>
       </c>
-      <c r="B19" s="227"/>
+      <c r="B19" s="214"/>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="120"/>
       <c r="B20" s="9"/>
     </row>
     <row r="21" spans="1:2">
-      <c r="A21" s="224" t="s">
+      <c r="A21" s="215" t="s">
         <v>198</v>
       </c>
-      <c r="B21" s="225"/>
+      <c r="B21" s="216"/>
     </row>
     <row r="22" spans="1:2">
-      <c r="A22" s="211"/>
-      <c r="B22" s="212"/>
+      <c r="A22" s="217"/>
+      <c r="B22" s="218"/>
     </row>
     <row r="23" spans="1:2">
-      <c r="A23" s="213" t="s">
+      <c r="A23" s="209" t="s">
         <v>199</v>
       </c>
-      <c r="B23" s="214"/>
+      <c r="B23" s="210"/>
     </row>
     <row r="24" spans="1:2">
-      <c r="A24" s="213"/>
-      <c r="B24" s="214"/>
+      <c r="A24" s="209"/>
+      <c r="B24" s="210"/>
     </row>
     <row r="25" spans="1:2">
-      <c r="A25" s="213" t="s">
+      <c r="A25" s="209" t="s">
         <v>200</v>
       </c>
-      <c r="B25" s="214"/>
+      <c r="B25" s="210"/>
     </row>
     <row r="26" spans="1:2">
-      <c r="A26" s="213" t="s">
+      <c r="A26" s="209" t="s">
         <v>201</v>
       </c>
-      <c r="B26" s="214"/>
+      <c r="B26" s="210"/>
     </row>
     <row r="27" spans="1:2">
-      <c r="A27" s="209"/>
-      <c r="B27" s="210"/>
+      <c r="A27" s="211"/>
+      <c r="B27" s="212"/>
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A7:B7"/>
     <mergeCell ref="A17:B17"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
@@ -26625,6 +26631,19 @@
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="A14:B14"/>
     <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A24:B24"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A3" r:id="rId1"/>

</xml_diff>

<commit_message>
Tempo - Boss redone, saved 30 frames, recorded up to Jungle performance, level savestate for jungle performance.
</commit_message>
<xml_diff>
--- a/trunk/Tempo/Tempo.xlsx
+++ b/trunk/Tempo/Tempo.xlsx
@@ -2239,6 +2239,9 @@
       <alignment horizontal="left" indent="1"/>
     </xf>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="42" fillId="21" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -2261,29 +2264,29 @@
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="26" fillId="13" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="27" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="26" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="27" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="24" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="25" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="22" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="23" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="15" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="22" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="23" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="24" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="25" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="26" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="27" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="26" fillId="13" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="27" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="17" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="17" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="17" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -2319,34 +2322,20 @@
     <xf numFmtId="0" fontId="56" fillId="22" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="53" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="54" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="54" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="52" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="52" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="50" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="4"/>
     </xf>
@@ -2356,9 +2345,20 @@
     <xf numFmtId="0" fontId="51" fillId="0" borderId="33" xfId="3" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" indent="4"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="54" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="54" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="53" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Accent1" xfId="2" builtinId="29"/>
@@ -2669,8 +2669,8 @@
   <dimension ref="A1:K167"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A87" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C104" sqref="C104"/>
+      <pane ySplit="6" topLeftCell="A96" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C112" sqref="C112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" outlineLevelRow="2"/>
@@ -2686,16 +2686,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="33">
-      <c r="A1" s="168" t="s">
+      <c r="A1" s="169" t="s">
         <v>205</v>
       </c>
-      <c r="B1" s="167"/>
-      <c r="C1" s="169" t="s">
+      <c r="B1" s="168"/>
+      <c r="C1" s="170" t="s">
         <v>170</v>
       </c>
-      <c r="D1" s="169"/>
-      <c r="E1" s="169"/>
-      <c r="F1" s="170"/>
+      <c r="D1" s="170"/>
+      <c r="E1" s="170"/>
+      <c r="F1" s="171"/>
       <c r="G1" s="140"/>
       <c r="H1" s="141">
         <f>SUM(G1:G65549)</f>
@@ -2760,11 +2760,11 @@
       <c r="B4" s="146" t="s">
         <v>228</v>
       </c>
-      <c r="C4" s="166" t="s">
+      <c r="C4" s="167" t="s">
         <v>232</v>
       </c>
-      <c r="D4" s="166"/>
-      <c r="E4" s="172"/>
+      <c r="D4" s="167"/>
+      <c r="E4" s="173"/>
       <c r="F4" s="143"/>
       <c r="G4" s="140"/>
       <c r="H4" s="140"/>
@@ -2779,10 +2779,10 @@
       <c r="B5" s="147" t="s">
         <v>177</v>
       </c>
-      <c r="C5" s="166" t="s">
+      <c r="C5" s="167" t="s">
         <v>218</v>
       </c>
-      <c r="D5" s="166"/>
+      <c r="D5" s="167"/>
       <c r="E5" s="147"/>
       <c r="F5" s="147"/>
       <c r="G5" s="148" t="s">
@@ -2806,10 +2806,10 @@
       <c r="B6" s="147" t="s">
         <v>179</v>
       </c>
-      <c r="C6" s="166" t="s">
+      <c r="C6" s="167" t="s">
         <v>168</v>
       </c>
-      <c r="D6" s="167"/>
+      <c r="D6" s="168"/>
       <c r="E6" s="147"/>
       <c r="F6" s="143"/>
       <c r="G6" s="140"/>
@@ -2833,7 +2833,7 @@
       <c r="F7" s="93"/>
     </row>
     <row r="8" spans="1:11" ht="15" customHeight="1" outlineLevel="1">
-      <c r="A8" s="171" t="s">
+      <c r="A8" s="172" t="s">
         <v>180</v>
       </c>
       <c r="B8" s="95" t="s">
@@ -2853,7 +2853,7 @@
       </c>
     </row>
     <row r="9" spans="1:11" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="A9" s="164"/>
+      <c r="A9" s="165"/>
       <c r="B9" s="98" t="s">
         <v>177</v>
       </c>
@@ -2867,7 +2867,7 @@
       <c r="F9" s="104"/>
     </row>
     <row r="10" spans="1:11" ht="15.75" outlineLevel="1" thickTop="1">
-      <c r="A10" s="164"/>
+      <c r="A10" s="165"/>
       <c r="B10" s="149" t="s">
         <v>208</v>
       </c>
@@ -2884,7 +2884,7 @@
       <c r="F10" s="105"/>
     </row>
     <row r="11" spans="1:11" ht="15" outlineLevel="1">
-      <c r="A11" s="164"/>
+      <c r="A11" s="165"/>
       <c r="B11" s="149" t="s">
         <v>214</v>
       </c>
@@ -2901,7 +2901,7 @@
       <c r="F11" s="105"/>
     </row>
     <row r="12" spans="1:11" ht="15" outlineLevel="1">
-      <c r="A12" s="164"/>
+      <c r="A12" s="165"/>
       <c r="B12" s="149" t="s">
         <v>209</v>
       </c>
@@ -2918,7 +2918,7 @@
       <c r="F12" s="105"/>
     </row>
     <row r="13" spans="1:11" ht="15" outlineLevel="1">
-      <c r="A13" s="164"/>
+      <c r="A13" s="165"/>
       <c r="B13" s="149" t="s">
         <v>213</v>
       </c>
@@ -2935,7 +2935,7 @@
       <c r="F13" s="105"/>
     </row>
     <row r="14" spans="1:11" ht="15" outlineLevel="1">
-      <c r="A14" s="164"/>
+      <c r="A14" s="165"/>
       <c r="B14" s="149" t="s">
         <v>214</v>
       </c>
@@ -2952,7 +2952,7 @@
       <c r="F14" s="105"/>
     </row>
     <row r="15" spans="1:11" ht="15" outlineLevel="1">
-      <c r="A15" s="164"/>
+      <c r="A15" s="165"/>
       <c r="B15" s="149" t="s">
         <v>215</v>
       </c>
@@ -2969,7 +2969,7 @@
       <c r="F15" s="105"/>
     </row>
     <row r="16" spans="1:11" ht="15" outlineLevel="1">
-      <c r="A16" s="164"/>
+      <c r="A16" s="165"/>
       <c r="B16" s="149" t="s">
         <v>216</v>
       </c>
@@ -2986,7 +2986,7 @@
       <c r="F16" s="105"/>
     </row>
     <row r="17" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A17" s="164"/>
+      <c r="A17" s="165"/>
       <c r="B17" s="149" t="s">
         <v>217</v>
       </c>
@@ -3003,7 +3003,7 @@
       <c r="F17" s="105"/>
     </row>
     <row r="18" spans="1:8" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="A18" s="164"/>
+      <c r="A18" s="165"/>
       <c r="B18" s="98" t="s">
         <v>179</v>
       </c>
@@ -3046,7 +3046,7 @@
     </row>
     <row r="20" spans="1:8" ht="13.5" thickBot="1"/>
     <row r="21" spans="1:8" ht="15" customHeight="1" outlineLevel="1">
-      <c r="A21" s="165" t="s">
+      <c r="A21" s="166" t="s">
         <v>219</v>
       </c>
       <c r="B21" s="109" t="s">
@@ -3066,7 +3066,7 @@
       </c>
     </row>
     <row r="22" spans="1:8" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="A22" s="164"/>
+      <c r="A22" s="165"/>
       <c r="B22" s="98" t="s">
         <v>177</v>
       </c>
@@ -3083,7 +3083,7 @@
       <c r="F22" s="104"/>
     </row>
     <row r="23" spans="1:8" ht="15.75" outlineLevel="1" thickTop="1">
-      <c r="A23" s="164"/>
+      <c r="A23" s="165"/>
       <c r="B23" s="149" t="s">
         <v>175</v>
       </c>
@@ -3096,7 +3096,7 @@
       <c r="F23" s="105"/>
     </row>
     <row r="24" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A24" s="164"/>
+      <c r="A24" s="165"/>
       <c r="B24" s="149" t="s">
         <v>221</v>
       </c>
@@ -3116,7 +3116,7 @@
       </c>
     </row>
     <row r="25" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A25" s="164"/>
+      <c r="A25" s="165"/>
       <c r="B25" s="149"/>
       <c r="C25" s="101"/>
       <c r="D25" s="101"/>
@@ -3127,7 +3127,7 @@
       <c r="F25" s="105"/>
     </row>
     <row r="26" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A26" s="164"/>
+      <c r="A26" s="165"/>
       <c r="B26" s="100"/>
       <c r="C26" s="101"/>
       <c r="D26" s="101"/>
@@ -3138,7 +3138,7 @@
       <c r="F26" s="105"/>
     </row>
     <row r="27" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A27" s="164"/>
+      <c r="A27" s="165"/>
       <c r="B27" s="100"/>
       <c r="C27" s="101"/>
       <c r="D27" s="101"/>
@@ -3149,7 +3149,7 @@
       <c r="F27" s="105"/>
     </row>
     <row r="28" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A28" s="164"/>
+      <c r="A28" s="165"/>
       <c r="B28" s="149" t="s">
         <v>222</v>
       </c>
@@ -3169,7 +3169,7 @@
       </c>
     </row>
     <row r="29" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A29" s="164"/>
+      <c r="A29" s="165"/>
       <c r="B29" s="154" t="s">
         <v>263</v>
       </c>
@@ -3187,7 +3187,7 @@
       </c>
     </row>
     <row r="30" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A30" s="164"/>
+      <c r="A30" s="165"/>
       <c r="B30" s="154" t="s">
         <v>264</v>
       </c>
@@ -3203,7 +3203,7 @@
       </c>
     </row>
     <row r="31" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A31" s="164"/>
+      <c r="A31" s="165"/>
       <c r="B31" s="154" t="s">
         <v>265</v>
       </c>
@@ -3219,7 +3219,7 @@
       </c>
     </row>
     <row r="32" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A32" s="164"/>
+      <c r="A32" s="165"/>
       <c r="B32" s="154" t="s">
         <v>266</v>
       </c>
@@ -3235,7 +3235,7 @@
       </c>
     </row>
     <row r="33" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A33" s="164"/>
+      <c r="A33" s="165"/>
       <c r="B33" s="154" t="s">
         <v>268</v>
       </c>
@@ -3251,7 +3251,7 @@
       </c>
     </row>
     <row r="34" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A34" s="164"/>
+      <c r="A34" s="165"/>
       <c r="B34" s="154" t="s">
         <v>269</v>
       </c>
@@ -3267,7 +3267,7 @@
       </c>
     </row>
     <row r="35" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A35" s="164"/>
+      <c r="A35" s="165"/>
       <c r="B35" s="154" t="s">
         <v>270</v>
       </c>
@@ -3286,7 +3286,7 @@
       </c>
     </row>
     <row r="36" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A36" s="164"/>
+      <c r="A36" s="165"/>
       <c r="B36" s="149" t="s">
         <v>223</v>
       </c>
@@ -3306,7 +3306,7 @@
       </c>
     </row>
     <row r="37" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A37" s="164"/>
+      <c r="A37" s="165"/>
       <c r="B37" s="149" t="s">
         <v>224</v>
       </c>
@@ -3323,7 +3323,7 @@
       <c r="F37" s="105"/>
     </row>
     <row r="38" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A38" s="164"/>
+      <c r="A38" s="165"/>
       <c r="B38" s="149" t="s">
         <v>225</v>
       </c>
@@ -3340,7 +3340,7 @@
       <c r="F38" s="105"/>
     </row>
     <row r="39" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A39" s="164"/>
+      <c r="A39" s="165"/>
       <c r="B39" s="149" t="s">
         <v>217</v>
       </c>
@@ -3357,7 +3357,7 @@
       <c r="F39" s="105"/>
     </row>
     <row r="40" spans="1:9" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="A40" s="164"/>
+      <c r="A40" s="165"/>
       <c r="B40" s="98" t="s">
         <v>179</v>
       </c>
@@ -3396,7 +3396,7 @@
     </row>
     <row r="42" spans="1:9" ht="13.5" thickBot="1"/>
     <row r="43" spans="1:9" ht="15" customHeight="1" outlineLevel="1">
-      <c r="A43" s="163" t="s">
+      <c r="A43" s="164" t="s">
         <v>226</v>
       </c>
       <c r="B43" s="113" t="s">
@@ -3416,7 +3416,7 @@
       </c>
     </row>
     <row r="44" spans="1:9" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="A44" s="164"/>
+      <c r="A44" s="165"/>
       <c r="B44" s="98" t="s">
         <v>177</v>
       </c>
@@ -3434,7 +3434,7 @@
       </c>
     </row>
     <row r="45" spans="1:9" ht="15.75" outlineLevel="1" thickTop="1">
-      <c r="A45" s="164"/>
+      <c r="A45" s="165"/>
       <c r="B45" s="100"/>
       <c r="C45" s="101"/>
       <c r="D45" s="101"/>
@@ -3445,7 +3445,7 @@
       <c r="F45" s="105"/>
     </row>
     <row r="46" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A46" s="164"/>
+      <c r="A46" s="165"/>
       <c r="B46" s="149" t="s">
         <v>221</v>
       </c>
@@ -3462,7 +3462,7 @@
       <c r="F46" s="105"/>
     </row>
     <row r="47" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A47" s="164"/>
+      <c r="A47" s="165"/>
       <c r="B47" s="155" t="s">
         <v>273</v>
       </c>
@@ -3477,7 +3477,7 @@
       <c r="F47" s="105"/>
     </row>
     <row r="48" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A48" s="164"/>
+      <c r="A48" s="165"/>
       <c r="B48" s="157" t="s">
         <v>275</v>
       </c>
@@ -3492,7 +3492,7 @@
       </c>
     </row>
     <row r="49" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A49" s="164"/>
+      <c r="A49" s="165"/>
       <c r="B49" s="149" t="s">
         <v>222</v>
       </c>
@@ -3512,7 +3512,7 @@
       </c>
     </row>
     <row r="50" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A50" s="164"/>
+      <c r="A50" s="165"/>
       <c r="B50" s="156" t="s">
         <v>274</v>
       </c>
@@ -3524,7 +3524,7 @@
       <c r="F50" s="105"/>
     </row>
     <row r="51" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A51" s="164"/>
+      <c r="A51" s="165"/>
       <c r="B51" s="150" t="s">
         <v>229</v>
       </c>
@@ -3548,7 +3548,7 @@
       </c>
     </row>
     <row r="52" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A52" s="164"/>
+      <c r="A52" s="165"/>
       <c r="B52" s="150" t="s">
         <v>230</v>
       </c>
@@ -3572,7 +3572,7 @@
       </c>
     </row>
     <row r="53" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A53" s="164"/>
+      <c r="A53" s="165"/>
       <c r="B53" s="150" t="s">
         <v>231</v>
       </c>
@@ -3596,7 +3596,7 @@
       </c>
     </row>
     <row r="54" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A54" s="164"/>
+      <c r="A54" s="165"/>
       <c r="B54" s="150" t="s">
         <v>233</v>
       </c>
@@ -3620,7 +3620,7 @@
       </c>
     </row>
     <row r="55" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A55" s="164"/>
+      <c r="A55" s="165"/>
       <c r="B55" s="150" t="s">
         <v>234</v>
       </c>
@@ -3644,7 +3644,7 @@
       </c>
     </row>
     <row r="56" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A56" s="164"/>
+      <c r="A56" s="165"/>
       <c r="B56" s="150" t="s">
         <v>235</v>
       </c>
@@ -3668,7 +3668,7 @@
       </c>
     </row>
     <row r="57" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A57" s="164"/>
+      <c r="A57" s="165"/>
       <c r="B57" s="150" t="s">
         <v>236</v>
       </c>
@@ -3692,7 +3692,7 @@
       </c>
     </row>
     <row r="58" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A58" s="164"/>
+      <c r="A58" s="165"/>
       <c r="B58" s="158" t="s">
         <v>263</v>
       </c>
@@ -3707,7 +3707,7 @@
       <c r="F58" s="105"/>
     </row>
     <row r="59" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A59" s="164"/>
+      <c r="A59" s="165"/>
       <c r="B59" s="158" t="s">
         <v>264</v>
       </c>
@@ -3726,7 +3726,7 @@
       </c>
     </row>
     <row r="60" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A60" s="164"/>
+      <c r="A60" s="165"/>
       <c r="B60" s="158" t="s">
         <v>265</v>
       </c>
@@ -3745,7 +3745,7 @@
       </c>
     </row>
     <row r="61" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A61" s="164"/>
+      <c r="A61" s="165"/>
       <c r="B61" s="159" t="s">
         <v>266</v>
       </c>
@@ -3764,7 +3764,7 @@
       </c>
     </row>
     <row r="62" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A62" s="164"/>
+      <c r="A62" s="165"/>
       <c r="B62" s="159" t="s">
         <v>268</v>
       </c>
@@ -3783,7 +3783,7 @@
       </c>
     </row>
     <row r="63" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A63" s="164"/>
+      <c r="A63" s="165"/>
       <c r="B63" s="159" t="s">
         <v>269</v>
       </c>
@@ -3802,7 +3802,7 @@
       </c>
     </row>
     <row r="64" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A64" s="164"/>
+      <c r="A64" s="165"/>
       <c r="B64" s="159" t="s">
         <v>276</v>
       </c>
@@ -3821,7 +3821,7 @@
       </c>
     </row>
     <row r="65" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A65" s="164"/>
+      <c r="A65" s="165"/>
       <c r="B65" s="159" t="s">
         <v>276</v>
       </c>
@@ -3840,7 +3840,7 @@
       </c>
     </row>
     <row r="66" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A66" s="164"/>
+      <c r="A66" s="165"/>
       <c r="B66" s="150" t="s">
         <v>223</v>
       </c>
@@ -3857,7 +3857,7 @@
       <c r="F66" s="105"/>
     </row>
     <row r="67" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A67" s="164"/>
+      <c r="A67" s="165"/>
       <c r="B67" s="150" t="s">
         <v>237</v>
       </c>
@@ -3874,7 +3874,7 @@
       <c r="F67" s="105"/>
     </row>
     <row r="68" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A68" s="164"/>
+      <c r="A68" s="165"/>
       <c r="B68" s="150" t="s">
         <v>238</v>
       </c>
@@ -3891,7 +3891,7 @@
       <c r="F68" s="105"/>
     </row>
     <row r="69" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A69" s="164"/>
+      <c r="A69" s="165"/>
       <c r="B69" s="150" t="s">
         <v>217</v>
       </c>
@@ -3908,7 +3908,7 @@
       <c r="F69" s="105"/>
     </row>
     <row r="70" spans="1:9" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="A70" s="164"/>
+      <c r="A70" s="165"/>
       <c r="B70" s="98" t="s">
         <v>179</v>
       </c>
@@ -3951,7 +3951,7 @@
     </row>
     <row r="72" spans="1:9" ht="13.5" thickBot="1"/>
     <row r="73" spans="1:9" ht="15" customHeight="1" outlineLevel="1">
-      <c r="A73" s="165" t="s">
+      <c r="A73" s="166" t="s">
         <v>239</v>
       </c>
       <c r="B73" s="109" t="s">
@@ -3971,7 +3971,7 @@
       </c>
     </row>
     <row r="74" spans="1:9" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="A74" s="164"/>
+      <c r="A74" s="165"/>
       <c r="B74" s="98" t="s">
         <v>177</v>
       </c>
@@ -3991,7 +3991,7 @@
       </c>
     </row>
     <row r="75" spans="1:9" ht="15.75" outlineLevel="1" thickTop="1">
-      <c r="A75" s="164"/>
+      <c r="A75" s="165"/>
       <c r="B75" s="151" t="s">
         <v>241</v>
       </c>
@@ -4008,7 +4008,7 @@
       <c r="F75" s="105"/>
     </row>
     <row r="76" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A76" s="164"/>
+      <c r="A76" s="165"/>
       <c r="B76" s="151" t="s">
         <v>242</v>
       </c>
@@ -4025,7 +4025,7 @@
       <c r="F76" s="105"/>
     </row>
     <row r="77" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A77" s="164"/>
+      <c r="A77" s="165"/>
       <c r="B77" s="151" t="s">
         <v>243</v>
       </c>
@@ -4042,7 +4042,7 @@
       <c r="F77" s="105"/>
     </row>
     <row r="78" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A78" s="164"/>
+      <c r="A78" s="165"/>
       <c r="B78" s="160" t="s">
         <v>263</v>
       </c>
@@ -4057,7 +4057,7 @@
       <c r="F78" s="105"/>
     </row>
     <row r="79" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A79" s="164"/>
+      <c r="A79" s="165"/>
       <c r="B79" s="160" t="s">
         <v>264</v>
       </c>
@@ -4076,7 +4076,7 @@
       </c>
     </row>
     <row r="80" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A80" s="164"/>
+      <c r="A80" s="165"/>
       <c r="B80" s="160" t="s">
         <v>265</v>
       </c>
@@ -4095,7 +4095,7 @@
       </c>
     </row>
     <row r="81" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A81" s="164"/>
+      <c r="A81" s="165"/>
       <c r="B81" s="160" t="s">
         <v>266</v>
       </c>
@@ -4114,7 +4114,7 @@
       </c>
     </row>
     <row r="82" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A82" s="164"/>
+      <c r="A82" s="165"/>
       <c r="B82" s="160" t="s">
         <v>268</v>
       </c>
@@ -4133,7 +4133,7 @@
       </c>
     </row>
     <row r="83" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A83" s="164"/>
+      <c r="A83" s="165"/>
       <c r="B83" s="160" t="s">
         <v>269</v>
       </c>
@@ -4152,7 +4152,7 @@
       </c>
     </row>
     <row r="84" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A84" s="164"/>
+      <c r="A84" s="165"/>
       <c r="B84" s="161" t="s">
         <v>276</v>
       </c>
@@ -4168,7 +4168,7 @@
       <c r="H84" s="112"/>
     </row>
     <row r="85" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A85" s="164"/>
+      <c r="A85" s="165"/>
       <c r="B85" s="161" t="s">
         <v>270</v>
       </c>
@@ -4183,7 +4183,7 @@
       <c r="F85" s="105"/>
     </row>
     <row r="86" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A86" s="164"/>
+      <c r="A86" s="165"/>
       <c r="B86" s="151" t="s">
         <v>244</v>
       </c>
@@ -4200,7 +4200,7 @@
       <c r="F86" s="105"/>
     </row>
     <row r="87" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A87" s="164"/>
+      <c r="A87" s="165"/>
       <c r="B87" s="151" t="s">
         <v>237</v>
       </c>
@@ -4217,7 +4217,7 @@
       <c r="F87" s="105"/>
     </row>
     <row r="88" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A88" s="164"/>
+      <c r="A88" s="165"/>
       <c r="B88" s="151" t="s">
         <v>245</v>
       </c>
@@ -4234,7 +4234,7 @@
       <c r="F88" s="105"/>
     </row>
     <row r="89" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A89" s="164"/>
+      <c r="A89" s="165"/>
       <c r="B89" s="151" t="s">
         <v>217</v>
       </c>
@@ -4251,7 +4251,7 @@
       <c r="F89" s="105"/>
     </row>
     <row r="90" spans="1:8" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="A90" s="164"/>
+      <c r="A90" s="165"/>
       <c r="B90" s="98" t="s">
         <v>179</v>
       </c>
@@ -4294,7 +4294,7 @@
     </row>
     <row r="92" spans="1:8" ht="13.5" thickBot="1"/>
     <row r="93" spans="1:8" ht="15" customHeight="1" outlineLevel="1">
-      <c r="A93" s="163" t="s">
+      <c r="A93" s="164" t="s">
         <v>246</v>
       </c>
       <c r="B93" s="113" t="s">
@@ -4314,7 +4314,7 @@
       </c>
     </row>
     <row r="94" spans="1:8" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="A94" s="164"/>
+      <c r="A94" s="165"/>
       <c r="B94" s="98" t="s">
         <v>177</v>
       </c>
@@ -4334,7 +4334,7 @@
       </c>
     </row>
     <row r="95" spans="1:8" ht="15.75" outlineLevel="1" thickTop="1">
-      <c r="A95" s="164"/>
+      <c r="A95" s="165"/>
       <c r="B95" s="151" t="s">
         <v>228</v>
       </c>
@@ -4351,7 +4351,7 @@
       <c r="F95" s="105"/>
     </row>
     <row r="96" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A96" s="164"/>
+      <c r="A96" s="165"/>
       <c r="B96" s="151" t="s">
         <v>221</v>
       </c>
@@ -4368,7 +4368,7 @@
       <c r="F96" s="105"/>
     </row>
     <row r="97" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A97" s="164"/>
+      <c r="A97" s="165"/>
       <c r="B97" s="100"/>
       <c r="C97" s="101"/>
       <c r="D97" s="101"/>
@@ -4379,7 +4379,7 @@
       <c r="F97" s="105"/>
     </row>
     <row r="98" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A98" s="164"/>
+      <c r="A98" s="165"/>
       <c r="B98" s="151" t="s">
         <v>222</v>
       </c>
@@ -4396,7 +4396,7 @@
       <c r="F98" s="105"/>
     </row>
     <row r="99" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A99" s="164"/>
+      <c r="A99" s="165"/>
       <c r="B99" s="100"/>
       <c r="C99" s="101"/>
       <c r="D99" s="101"/>
@@ -4407,7 +4407,7 @@
       <c r="F99" s="105"/>
     </row>
     <row r="100" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A100" s="164"/>
+      <c r="A100" s="165"/>
       <c r="B100" s="152" t="s">
         <v>236</v>
       </c>
@@ -4424,7 +4424,7 @@
       <c r="F100" s="105"/>
     </row>
     <row r="101" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A101" s="164"/>
+      <c r="A101" s="165"/>
       <c r="B101" s="100"/>
       <c r="C101" s="101"/>
       <c r="D101" s="101"/>
@@ -4435,8 +4435,8 @@
       <c r="F101" s="105"/>
     </row>
     <row r="102" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A102" s="164"/>
-      <c r="B102" s="228" t="s">
+      <c r="A102" s="165"/>
+      <c r="B102" s="163" t="s">
         <v>277</v>
       </c>
       <c r="C102" s="101">
@@ -4450,79 +4450,87 @@
       <c r="F102" s="105"/>
     </row>
     <row r="103" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A103" s="164"/>
+      <c r="A103" s="165"/>
       <c r="B103" s="152" t="s">
         <v>223</v>
       </c>
       <c r="C103" s="101">
-        <v>37902</v>
+        <v>37872</v>
       </c>
       <c r="D103" s="101">
         <v>49269</v>
       </c>
       <c r="E103" s="123">
         <f t="shared" si="7"/>
-        <v>11367</v>
+        <v>11397</v>
       </c>
       <c r="F103" s="105"/>
     </row>
     <row r="104" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A104" s="164"/>
+      <c r="A104" s="165"/>
       <c r="B104" s="152" t="s">
         <v>248</v>
       </c>
-      <c r="C104" s="101"/>
+      <c r="C104" s="101">
+        <v>38102</v>
+      </c>
       <c r="D104" s="101">
         <v>49505</v>
       </c>
       <c r="E104" s="123">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>11403</v>
       </c>
       <c r="F104" s="105"/>
     </row>
     <row r="105" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A105" s="164"/>
+      <c r="A105" s="165"/>
       <c r="B105" s="152" t="s">
         <v>249</v>
       </c>
-      <c r="C105" s="101"/>
+      <c r="C105" s="101">
+        <v>38724</v>
+      </c>
       <c r="D105" s="101">
         <v>50134</v>
       </c>
       <c r="E105" s="123">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>11410</v>
       </c>
       <c r="F105" s="105"/>
     </row>
     <row r="106" spans="1:8" ht="15" outlineLevel="1">
-      <c r="A106" s="164"/>
+      <c r="A106" s="165"/>
       <c r="B106" s="152" t="s">
         <v>250</v>
       </c>
-      <c r="C106" s="101"/>
+      <c r="C106" s="101">
+        <v>39106</v>
+      </c>
       <c r="D106" s="101">
         <v>50516</v>
       </c>
       <c r="E106" s="123">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>11410</v>
       </c>
       <c r="F106" s="105"/>
     </row>
     <row r="107" spans="1:8" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="A107" s="164"/>
+      <c r="A107" s="165"/>
       <c r="B107" s="98" t="s">
         <v>179</v>
       </c>
-      <c r="C107" s="99"/>
+      <c r="C107" s="99">
+        <v>39166</v>
+      </c>
       <c r="D107" s="99">
         <v>50574</v>
       </c>
       <c r="E107" s="125">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>11408</v>
       </c>
       <c r="F107" s="104"/>
     </row>
@@ -4535,7 +4543,7 @@
       </c>
       <c r="C108" s="103">
         <f>C107-C94</f>
-        <v>-29446</v>
+        <v>9720</v>
       </c>
       <c r="D108" s="103">
         <f>D107-D94</f>
@@ -4543,17 +4551,17 @@
       </c>
       <c r="E108" s="126">
         <f>E107-E94</f>
-        <v>-5349</v>
+        <v>6059</v>
       </c>
       <c r="F108" s="107"/>
       <c r="G108" s="112">
         <f>E108</f>
-        <v>-5349</v>
+        <v>6059</v>
       </c>
     </row>
     <row r="109" spans="1:8" ht="13.5" thickBot="1"/>
     <row r="110" spans="1:8" ht="15" customHeight="1" outlineLevel="1">
-      <c r="A110" s="165" t="s">
+      <c r="A110" s="166" t="s">
         <v>251</v>
       </c>
       <c r="B110" s="109" t="s">
@@ -4573,17 +4581,19 @@
       </c>
     </row>
     <row r="111" spans="1:8" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="A111" s="164"/>
+      <c r="A111" s="165"/>
       <c r="B111" s="98" t="s">
         <v>177</v>
       </c>
-      <c r="C111" s="99"/>
+      <c r="C111" s="99">
+        <v>39166</v>
+      </c>
       <c r="D111" s="99">
         <v>50574</v>
       </c>
       <c r="E111" s="123">
         <f t="shared" ref="E111:E120" si="8">IF(AND(C111&gt;0,D111&gt;0), D111-C111, 0)</f>
-        <v>0</v>
+        <v>11408</v>
       </c>
       <c r="F111" s="104"/>
       <c r="H111">
@@ -4591,7 +4601,7 @@
       </c>
     </row>
     <row r="112" spans="1:8" ht="15.75" outlineLevel="1" thickTop="1">
-      <c r="A112" s="164"/>
+      <c r="A112" s="165"/>
       <c r="B112" s="100"/>
       <c r="C112" s="101"/>
       <c r="D112" s="101"/>
@@ -4602,7 +4612,7 @@
       <c r="F112" s="105"/>
     </row>
     <row r="113" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A113" s="164"/>
+      <c r="A113" s="165"/>
       <c r="B113" s="152" t="s">
         <v>253</v>
       </c>
@@ -4617,7 +4627,7 @@
       <c r="F113" s="105"/>
     </row>
     <row r="114" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A114" s="164"/>
+      <c r="A114" s="165"/>
       <c r="B114" s="100"/>
       <c r="C114" s="101"/>
       <c r="D114" s="101"/>
@@ -4628,7 +4638,7 @@
       <c r="F114" s="105"/>
     </row>
     <row r="115" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A115" s="164"/>
+      <c r="A115" s="165"/>
       <c r="B115" s="152" t="s">
         <v>254</v>
       </c>
@@ -4643,7 +4653,7 @@
       <c r="F115" s="105"/>
     </row>
     <row r="116" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A116" s="164"/>
+      <c r="A116" s="165"/>
       <c r="B116" s="100"/>
       <c r="C116" s="101"/>
       <c r="D116" s="101"/>
@@ -4654,7 +4664,7 @@
       <c r="F116" s="105"/>
     </row>
     <row r="117" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A117" s="164"/>
+      <c r="A117" s="165"/>
       <c r="B117" s="152" t="s">
         <v>223</v>
       </c>
@@ -4669,7 +4679,7 @@
       <c r="F117" s="105"/>
     </row>
     <row r="118" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A118" s="164"/>
+      <c r="A118" s="165"/>
       <c r="B118" s="152" t="s">
         <v>248</v>
       </c>
@@ -4684,7 +4694,7 @@
       <c r="F118" s="105"/>
     </row>
     <row r="119" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A119" s="164"/>
+      <c r="A119" s="165"/>
       <c r="B119" s="152" t="s">
         <v>255</v>
       </c>
@@ -4699,7 +4709,7 @@
       <c r="F119" s="105"/>
     </row>
     <row r="120" spans="1:9" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="A120" s="164"/>
+      <c r="A120" s="165"/>
       <c r="B120" s="98" t="s">
         <v>179</v>
       </c>
@@ -4722,7 +4732,7 @@
       </c>
       <c r="C121" s="103">
         <f>C120-C111</f>
-        <v>0</v>
+        <v>-39166</v>
       </c>
       <c r="D121" s="103">
         <f>D120-D111</f>
@@ -4730,17 +4740,17 @@
       </c>
       <c r="E121" s="126">
         <f>E120-E111</f>
-        <v>0</v>
+        <v>-11408</v>
       </c>
       <c r="F121" s="108"/>
       <c r="G121" s="112">
         <f>E121</f>
-        <v>0</v>
+        <v>-11408</v>
       </c>
     </row>
     <row r="122" spans="1:9" ht="13.5" thickBot="1"/>
     <row r="123" spans="1:9" ht="15" customHeight="1" outlineLevel="1">
-      <c r="A123" s="163" t="s">
+      <c r="A123" s="164" t="s">
         <v>256</v>
       </c>
       <c r="B123" s="113" t="s">
@@ -4760,7 +4770,7 @@
       </c>
     </row>
     <row r="124" spans="1:9" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="A124" s="164"/>
+      <c r="A124" s="165"/>
       <c r="B124" s="98" t="s">
         <v>177</v>
       </c>
@@ -4782,7 +4792,7 @@
       </c>
     </row>
     <row r="125" spans="1:9" ht="15.75" outlineLevel="1" thickTop="1">
-      <c r="A125" s="164"/>
+      <c r="A125" s="165"/>
       <c r="B125" s="100"/>
       <c r="C125" s="101"/>
       <c r="D125" s="101"/>
@@ -4793,7 +4803,7 @@
       <c r="F125" s="105"/>
     </row>
     <row r="126" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A126" s="164"/>
+      <c r="A126" s="165"/>
       <c r="B126" s="152" t="s">
         <v>221</v>
       </c>
@@ -4808,7 +4818,7 @@
       <c r="F126" s="105"/>
     </row>
     <row r="127" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A127" s="164"/>
+      <c r="A127" s="165"/>
       <c r="B127" s="100"/>
       <c r="C127" s="101"/>
       <c r="D127" s="101"/>
@@ -4819,7 +4829,7 @@
       <c r="F127" s="105"/>
     </row>
     <row r="128" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A128" s="164"/>
+      <c r="A128" s="165"/>
       <c r="B128" s="152" t="s">
         <v>222</v>
       </c>
@@ -4834,7 +4844,7 @@
       <c r="F128" s="105"/>
     </row>
     <row r="129" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A129" s="164"/>
+      <c r="A129" s="165"/>
       <c r="B129" s="152" t="s">
         <v>248</v>
       </c>
@@ -4849,7 +4859,7 @@
       <c r="F129" s="105"/>
     </row>
     <row r="130" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A130" s="164"/>
+      <c r="A130" s="165"/>
       <c r="B130" s="152" t="s">
         <v>258</v>
       </c>
@@ -4864,7 +4874,7 @@
       <c r="F130" s="105"/>
     </row>
     <row r="131" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A131" s="164"/>
+      <c r="A131" s="165"/>
       <c r="B131" s="152" t="s">
         <v>224</v>
       </c>
@@ -4879,7 +4889,7 @@
       <c r="F131" s="105"/>
     </row>
     <row r="132" spans="1:9" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="A132" s="164"/>
+      <c r="A132" s="165"/>
       <c r="B132" s="98" t="s">
         <v>179</v>
       </c>
@@ -4920,7 +4930,7 @@
     </row>
     <row r="134" spans="1:9" ht="13.5" thickBot="1"/>
     <row r="135" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A135" s="165" t="s">
+      <c r="A135" s="166" t="s">
         <v>259</v>
       </c>
       <c r="B135" s="109" t="s">
@@ -4940,7 +4950,7 @@
       </c>
     </row>
     <row r="136" spans="1:9" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="A136" s="164"/>
+      <c r="A136" s="165"/>
       <c r="B136" s="98" t="s">
         <v>177</v>
       </c>
@@ -4962,7 +4972,7 @@
       </c>
     </row>
     <row r="137" spans="1:9" ht="15.75" outlineLevel="1" thickTop="1">
-      <c r="A137" s="164"/>
+      <c r="A137" s="165"/>
       <c r="B137" s="100"/>
       <c r="C137" s="101"/>
       <c r="D137" s="101"/>
@@ -4973,7 +4983,7 @@
       <c r="F137" s="105"/>
     </row>
     <row r="138" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A138" s="164"/>
+      <c r="A138" s="165"/>
       <c r="B138" s="100"/>
       <c r="C138" s="101"/>
       <c r="D138" s="101"/>
@@ -4984,7 +4994,7 @@
       <c r="F138" s="105"/>
     </row>
     <row r="139" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A139" s="164"/>
+      <c r="A139" s="165"/>
       <c r="B139" s="100"/>
       <c r="C139" s="101"/>
       <c r="D139" s="101"/>
@@ -4995,7 +5005,7 @@
       <c r="F139" s="105"/>
     </row>
     <row r="140" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A140" s="164"/>
+      <c r="A140" s="165"/>
       <c r="B140" s="100"/>
       <c r="C140" s="101"/>
       <c r="D140" s="101"/>
@@ -5006,7 +5016,7 @@
       <c r="F140" s="105"/>
     </row>
     <row r="141" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A141" s="164"/>
+      <c r="A141" s="165"/>
       <c r="B141" s="100"/>
       <c r="C141" s="101"/>
       <c r="D141" s="101"/>
@@ -5017,7 +5027,7 @@
       <c r="F141" s="105"/>
     </row>
     <row r="142" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A142" s="164"/>
+      <c r="A142" s="165"/>
       <c r="B142" s="100"/>
       <c r="C142" s="101"/>
       <c r="D142" s="101"/>
@@ -5028,7 +5038,7 @@
       <c r="F142" s="105"/>
     </row>
     <row r="143" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A143" s="164"/>
+      <c r="A143" s="165"/>
       <c r="B143" s="100"/>
       <c r="C143" s="101"/>
       <c r="D143" s="101"/>
@@ -5039,7 +5049,7 @@
       <c r="F143" s="105"/>
     </row>
     <row r="144" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A144" s="164"/>
+      <c r="A144" s="165"/>
       <c r="B144" s="100"/>
       <c r="C144" s="101"/>
       <c r="D144" s="101"/>
@@ -5050,7 +5060,7 @@
       <c r="F144" s="105"/>
     </row>
     <row r="145" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A145" s="164"/>
+      <c r="A145" s="165"/>
       <c r="B145" s="152" t="s">
         <v>261</v>
       </c>
@@ -5072,7 +5082,7 @@
       </c>
     </row>
     <row r="146" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A146" s="164"/>
+      <c r="A146" s="165"/>
       <c r="B146" s="100"/>
       <c r="C146" s="101"/>
       <c r="D146" s="101"/>
@@ -5083,7 +5093,7 @@
       <c r="F146" s="105"/>
     </row>
     <row r="147" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A147" s="164"/>
+      <c r="A147" s="165"/>
       <c r="B147" s="100"/>
       <c r="C147" s="101"/>
       <c r="D147" s="101"/>
@@ -5094,7 +5104,7 @@
       <c r="F147" s="105"/>
     </row>
     <row r="148" spans="1:9" ht="15" outlineLevel="1">
-      <c r="A148" s="164"/>
+      <c r="A148" s="165"/>
       <c r="B148" s="100"/>
       <c r="C148" s="101"/>
       <c r="D148" s="101"/>
@@ -5105,7 +5115,7 @@
       <c r="F148" s="105"/>
     </row>
     <row r="149" spans="1:9" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="A149" s="164"/>
+      <c r="A149" s="165"/>
       <c r="B149" s="98" t="s">
         <v>179</v>
       </c>
@@ -5143,7 +5153,7 @@
       </c>
     </row>
     <row r="152" spans="1:9" ht="15" hidden="1" outlineLevel="2">
-      <c r="A152" s="163" t="s">
+      <c r="A152" s="164" t="s">
         <v>169</v>
       </c>
       <c r="B152" s="113" t="s">
@@ -5163,7 +5173,7 @@
       </c>
     </row>
     <row r="153" spans="1:9" ht="15.75" hidden="1" outlineLevel="2" thickBot="1">
-      <c r="A153" s="164"/>
+      <c r="A153" s="165"/>
       <c r="B153" s="98" t="s">
         <v>177</v>
       </c>
@@ -5176,7 +5186,7 @@
       <c r="F153" s="104"/>
     </row>
     <row r="154" spans="1:9" ht="15.75" hidden="1" outlineLevel="2" thickTop="1">
-      <c r="A154" s="164"/>
+      <c r="A154" s="165"/>
       <c r="B154" s="100"/>
       <c r="C154" s="101"/>
       <c r="D154" s="101"/>
@@ -5187,7 +5197,7 @@
       <c r="F154" s="105"/>
     </row>
     <row r="155" spans="1:9" ht="15" hidden="1" outlineLevel="2">
-      <c r="A155" s="164"/>
+      <c r="A155" s="165"/>
       <c r="B155" s="100"/>
       <c r="C155" s="101"/>
       <c r="D155" s="101"/>
@@ -5198,7 +5208,7 @@
       <c r="F155" s="105"/>
     </row>
     <row r="156" spans="1:9" ht="15" hidden="1" outlineLevel="2">
-      <c r="A156" s="164"/>
+      <c r="A156" s="165"/>
       <c r="B156" s="100"/>
       <c r="C156" s="101"/>
       <c r="D156" s="101"/>
@@ -5209,7 +5219,7 @@
       <c r="F156" s="105"/>
     </row>
     <row r="157" spans="1:9" ht="15" hidden="1" outlineLevel="2">
-      <c r="A157" s="164"/>
+      <c r="A157" s="165"/>
       <c r="B157" s="100"/>
       <c r="C157" s="101"/>
       <c r="D157" s="101"/>
@@ -5220,7 +5230,7 @@
       <c r="F157" s="105"/>
     </row>
     <row r="158" spans="1:9" ht="15" hidden="1" outlineLevel="2">
-      <c r="A158" s="164"/>
+      <c r="A158" s="165"/>
       <c r="B158" s="100"/>
       <c r="C158" s="101"/>
       <c r="D158" s="101"/>
@@ -5231,7 +5241,7 @@
       <c r="F158" s="105"/>
     </row>
     <row r="159" spans="1:9" ht="15" hidden="1" outlineLevel="2">
-      <c r="A159" s="164"/>
+      <c r="A159" s="165"/>
       <c r="B159" s="100"/>
       <c r="C159" s="101"/>
       <c r="D159" s="101"/>
@@ -5242,7 +5252,7 @@
       <c r="F159" s="105"/>
     </row>
     <row r="160" spans="1:9" ht="15" hidden="1" outlineLevel="2">
-      <c r="A160" s="164"/>
+      <c r="A160" s="165"/>
       <c r="B160" s="100"/>
       <c r="C160" s="101"/>
       <c r="D160" s="101"/>
@@ -5253,7 +5263,7 @@
       <c r="F160" s="105"/>
     </row>
     <row r="161" spans="1:7" ht="15" hidden="1" outlineLevel="2">
-      <c r="A161" s="164"/>
+      <c r="A161" s="165"/>
       <c r="B161" s="100"/>
       <c r="C161" s="101"/>
       <c r="D161" s="101"/>
@@ -5264,7 +5274,7 @@
       <c r="F161" s="105"/>
     </row>
     <row r="162" spans="1:7" ht="15" hidden="1" outlineLevel="2">
-      <c r="A162" s="164"/>
+      <c r="A162" s="165"/>
       <c r="B162" s="100"/>
       <c r="C162" s="101"/>
       <c r="D162" s="101"/>
@@ -5275,7 +5285,7 @@
       <c r="F162" s="105"/>
     </row>
     <row r="163" spans="1:7" ht="15" hidden="1" outlineLevel="2">
-      <c r="A163" s="164"/>
+      <c r="A163" s="165"/>
       <c r="B163" s="100"/>
       <c r="C163" s="101"/>
       <c r="D163" s="101"/>
@@ -5286,7 +5296,7 @@
       <c r="F163" s="105"/>
     </row>
     <row r="164" spans="1:7" ht="15" hidden="1" outlineLevel="2">
-      <c r="A164" s="164"/>
+      <c r="A164" s="165"/>
       <c r="B164" s="100"/>
       <c r="C164" s="101"/>
       <c r="D164" s="101"/>
@@ -5297,7 +5307,7 @@
       <c r="F164" s="105"/>
     </row>
     <row r="165" spans="1:7" ht="15" hidden="1" outlineLevel="2">
-      <c r="A165" s="164"/>
+      <c r="A165" s="165"/>
       <c r="B165" s="100"/>
       <c r="C165" s="101"/>
       <c r="D165" s="101"/>
@@ -5308,7 +5318,7 @@
       <c r="F165" s="105"/>
     </row>
     <row r="166" spans="1:7" ht="15.75" hidden="1" outlineLevel="2" thickBot="1">
-      <c r="A166" s="164"/>
+      <c r="A166" s="165"/>
       <c r="B166" s="98" t="s">
         <v>179</v>
       </c>
@@ -5347,11 +5357,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="A152:A166"/>
-    <mergeCell ref="A123:A132"/>
-    <mergeCell ref="A93:A107"/>
-    <mergeCell ref="A135:A149"/>
-    <mergeCell ref="A110:A120"/>
     <mergeCell ref="A43:A70"/>
     <mergeCell ref="A73:A90"/>
     <mergeCell ref="C5:D5"/>
@@ -5361,6 +5366,11 @@
     <mergeCell ref="A8:A18"/>
     <mergeCell ref="A21:A40"/>
     <mergeCell ref="C4:E4"/>
+    <mergeCell ref="A152:A166"/>
+    <mergeCell ref="A123:A132"/>
+    <mergeCell ref="A93:A107"/>
+    <mergeCell ref="A135:A149"/>
+    <mergeCell ref="A110:A120"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -5392,13 +5402,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="26.25" customHeight="1">
-      <c r="A1" s="173" t="s">
+      <c r="A1" s="192" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="173"/>
-      <c r="C1" s="173"/>
-      <c r="D1" s="173"/>
-      <c r="E1" s="173"/>
+      <c r="B1" s="192"/>
+      <c r="C1" s="192"/>
+      <c r="D1" s="192"/>
+      <c r="E1" s="192"/>
       <c r="F1" s="7"/>
       <c r="G1" s="5"/>
       <c r="H1" s="5"/>
@@ -5428,18 +5438,18 @@
         <v>8</v>
       </c>
       <c r="B3" s="36"/>
-      <c r="C3" s="174"/>
-      <c r="D3" s="175"/>
-      <c r="E3" s="175"/>
+      <c r="C3" s="193"/>
+      <c r="D3" s="194"/>
+      <c r="E3" s="194"/>
     </row>
     <row r="4" spans="1:8" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A4" s="46" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="87"/>
-      <c r="C4" s="176"/>
-      <c r="D4" s="177"/>
-      <c r="E4" s="177"/>
+      <c r="C4" s="174"/>
+      <c r="D4" s="175"/>
+      <c r="E4" s="175"/>
       <c r="F4" s="6"/>
     </row>
     <row r="5" spans="1:8" hidden="1" outlineLevel="2">
@@ -5591,9 +5601,9 @@
         <v>9</v>
       </c>
       <c r="B21" s="90"/>
-      <c r="C21" s="178"/>
-      <c r="D21" s="179"/>
-      <c r="E21" s="179"/>
+      <c r="C21" s="176"/>
+      <c r="D21" s="177"/>
+      <c r="E21" s="177"/>
     </row>
     <row r="22" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A22" s="47">
@@ -5744,9 +5754,9 @@
         <v>10</v>
       </c>
       <c r="B38" s="87"/>
-      <c r="C38" s="176"/>
-      <c r="D38" s="177"/>
-      <c r="E38" s="177"/>
+      <c r="C38" s="174"/>
+      <c r="D38" s="175"/>
+      <c r="E38" s="175"/>
     </row>
     <row r="39" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A39" s="47">
@@ -5897,9 +5907,9 @@
         <v>11</v>
       </c>
       <c r="B55" s="87"/>
-      <c r="C55" s="176"/>
-      <c r="D55" s="177"/>
-      <c r="E55" s="177"/>
+      <c r="C55" s="174"/>
+      <c r="D55" s="175"/>
+      <c r="E55" s="175"/>
     </row>
     <row r="56" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A56" s="47">
@@ -6050,9 +6060,9 @@
         <v>12</v>
       </c>
       <c r="B72" s="87"/>
-      <c r="C72" s="176"/>
-      <c r="D72" s="177"/>
-      <c r="E72" s="177"/>
+      <c r="C72" s="174"/>
+      <c r="D72" s="175"/>
+      <c r="E72" s="175"/>
     </row>
     <row r="73" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A73" s="47">
@@ -6203,9 +6213,9 @@
         <v>13</v>
       </c>
       <c r="B89" s="87"/>
-      <c r="C89" s="176"/>
-      <c r="D89" s="177"/>
-      <c r="E89" s="177"/>
+      <c r="C89" s="174"/>
+      <c r="D89" s="175"/>
+      <c r="E89" s="175"/>
     </row>
     <row r="90" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A90" s="47">
@@ -6356,9 +6366,9 @@
         <v>14</v>
       </c>
       <c r="B106" s="87"/>
-      <c r="C106" s="176"/>
-      <c r="D106" s="177"/>
-      <c r="E106" s="177"/>
+      <c r="C106" s="174"/>
+      <c r="D106" s="175"/>
+      <c r="E106" s="175"/>
     </row>
     <row r="107" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A107" s="47">
@@ -6509,9 +6519,9 @@
         <v>15</v>
       </c>
       <c r="B123" s="87"/>
-      <c r="C123" s="176"/>
-      <c r="D123" s="177"/>
-      <c r="E123" s="177"/>
+      <c r="C123" s="174"/>
+      <c r="D123" s="175"/>
+      <c r="E123" s="175"/>
     </row>
     <row r="124" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A124" s="47">
@@ -6662,9 +6672,9 @@
         <v>16</v>
       </c>
       <c r="B140" s="87"/>
-      <c r="C140" s="176"/>
-      <c r="D140" s="177"/>
-      <c r="E140" s="177"/>
+      <c r="C140" s="174"/>
+      <c r="D140" s="175"/>
+      <c r="E140" s="175"/>
     </row>
     <row r="141" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A141" s="47">
@@ -6815,9 +6825,9 @@
         <v>17</v>
       </c>
       <c r="B157" s="87"/>
-      <c r="C157" s="176"/>
-      <c r="D157" s="177"/>
-      <c r="E157" s="177"/>
+      <c r="C157" s="174"/>
+      <c r="D157" s="175"/>
+      <c r="E157" s="175"/>
     </row>
     <row r="158" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A158" s="47">
@@ -6968,9 +6978,9 @@
         <v>18</v>
       </c>
       <c r="B174" s="87"/>
-      <c r="C174" s="176"/>
-      <c r="D174" s="177"/>
-      <c r="E174" s="177"/>
+      <c r="C174" s="174"/>
+      <c r="D174" s="175"/>
+      <c r="E174" s="175"/>
     </row>
     <row r="175" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A175" s="47">
@@ -7121,9 +7131,9 @@
         <v>19</v>
       </c>
       <c r="B191" s="87"/>
-      <c r="C191" s="176"/>
-      <c r="D191" s="177"/>
-      <c r="E191" s="177"/>
+      <c r="C191" s="174"/>
+      <c r="D191" s="175"/>
+      <c r="E191" s="175"/>
     </row>
     <row r="192" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A192" s="47">
@@ -7274,9 +7284,9 @@
         <v>20</v>
       </c>
       <c r="B208" s="87"/>
-      <c r="C208" s="176"/>
-      <c r="D208" s="177"/>
-      <c r="E208" s="177"/>
+      <c r="C208" s="174"/>
+      <c r="D208" s="175"/>
+      <c r="E208" s="175"/>
     </row>
     <row r="209" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A209" s="47">
@@ -7427,9 +7437,9 @@
         <v>21</v>
       </c>
       <c r="B225" s="87"/>
-      <c r="C225" s="176"/>
-      <c r="D225" s="177"/>
-      <c r="E225" s="177"/>
+      <c r="C225" s="174"/>
+      <c r="D225" s="175"/>
+      <c r="E225" s="175"/>
     </row>
     <row r="226" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A226" s="47">
@@ -7580,9 +7590,9 @@
         <v>22</v>
       </c>
       <c r="B242" s="87"/>
-      <c r="C242" s="176"/>
-      <c r="D242" s="177"/>
-      <c r="E242" s="177"/>
+      <c r="C242" s="174"/>
+      <c r="D242" s="175"/>
+      <c r="E242" s="175"/>
     </row>
     <row r="243" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A243" s="47">
@@ -7733,9 +7743,9 @@
         <v>23</v>
       </c>
       <c r="B259" s="87"/>
-      <c r="C259" s="176"/>
-      <c r="D259" s="177"/>
-      <c r="E259" s="177"/>
+      <c r="C259" s="174"/>
+      <c r="D259" s="175"/>
+      <c r="E259" s="175"/>
     </row>
     <row r="260" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A260" s="47">
@@ -7886,18 +7896,18 @@
         <v>24</v>
       </c>
       <c r="B276" s="37"/>
-      <c r="C276" s="180"/>
-      <c r="D276" s="181"/>
-      <c r="E276" s="181"/>
+      <c r="C276" s="190"/>
+      <c r="D276" s="191"/>
+      <c r="E276" s="191"/>
     </row>
     <row r="277" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A277" s="51" t="s">
         <v>25</v>
       </c>
       <c r="B277" s="87"/>
-      <c r="C277" s="176"/>
-      <c r="D277" s="177"/>
-      <c r="E277" s="177"/>
+      <c r="C277" s="174"/>
+      <c r="D277" s="175"/>
+      <c r="E277" s="175"/>
     </row>
     <row r="278" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A278" s="52">
@@ -8048,9 +8058,9 @@
         <v>26</v>
       </c>
       <c r="B294" s="90"/>
-      <c r="C294" s="178"/>
-      <c r="D294" s="179"/>
-      <c r="E294" s="179"/>
+      <c r="C294" s="176"/>
+      <c r="D294" s="177"/>
+      <c r="E294" s="177"/>
     </row>
     <row r="295" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A295" s="52">
@@ -8201,9 +8211,9 @@
         <v>27</v>
       </c>
       <c r="B311" s="87"/>
-      <c r="C311" s="176"/>
-      <c r="D311" s="177"/>
-      <c r="E311" s="177"/>
+      <c r="C311" s="174"/>
+      <c r="D311" s="175"/>
+      <c r="E311" s="175"/>
     </row>
     <row r="312" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A312" s="52">
@@ -8354,9 +8364,9 @@
         <v>28</v>
       </c>
       <c r="B328" s="87"/>
-      <c r="C328" s="176"/>
-      <c r="D328" s="177"/>
-      <c r="E328" s="177"/>
+      <c r="C328" s="174"/>
+      <c r="D328" s="175"/>
+      <c r="E328" s="175"/>
     </row>
     <row r="329" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A329" s="52">
@@ -8507,9 +8517,9 @@
         <v>29</v>
       </c>
       <c r="B345" s="87"/>
-      <c r="C345" s="176"/>
-      <c r="D345" s="177"/>
-      <c r="E345" s="177"/>
+      <c r="C345" s="174"/>
+      <c r="D345" s="175"/>
+      <c r="E345" s="175"/>
     </row>
     <row r="346" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A346" s="52">
@@ -8660,9 +8670,9 @@
         <v>30</v>
       </c>
       <c r="B362" s="87"/>
-      <c r="C362" s="176"/>
-      <c r="D362" s="177"/>
-      <c r="E362" s="177"/>
+      <c r="C362" s="174"/>
+      <c r="D362" s="175"/>
+      <c r="E362" s="175"/>
     </row>
     <row r="363" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A363" s="52">
@@ -8813,9 +8823,9 @@
         <v>31</v>
       </c>
       <c r="B379" s="87"/>
-      <c r="C379" s="176"/>
-      <c r="D379" s="177"/>
-      <c r="E379" s="177"/>
+      <c r="C379" s="174"/>
+      <c r="D379" s="175"/>
+      <c r="E379" s="175"/>
     </row>
     <row r="380" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A380" s="52">
@@ -8966,9 +8976,9 @@
         <v>32</v>
       </c>
       <c r="B396" s="87"/>
-      <c r="C396" s="176"/>
-      <c r="D396" s="177"/>
-      <c r="E396" s="177"/>
+      <c r="C396" s="174"/>
+      <c r="D396" s="175"/>
+      <c r="E396" s="175"/>
     </row>
     <row r="397" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A397" s="52">
@@ -9119,9 +9129,9 @@
         <v>33</v>
       </c>
       <c r="B413" s="87"/>
-      <c r="C413" s="176"/>
-      <c r="D413" s="177"/>
-      <c r="E413" s="177"/>
+      <c r="C413" s="174"/>
+      <c r="D413" s="175"/>
+      <c r="E413" s="175"/>
     </row>
     <row r="414" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A414" s="52">
@@ -9272,9 +9282,9 @@
         <v>34</v>
       </c>
       <c r="B430" s="87"/>
-      <c r="C430" s="176"/>
-      <c r="D430" s="177"/>
-      <c r="E430" s="177"/>
+      <c r="C430" s="174"/>
+      <c r="D430" s="175"/>
+      <c r="E430" s="175"/>
     </row>
     <row r="431" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A431" s="52">
@@ -9425,9 +9435,9 @@
         <v>35</v>
       </c>
       <c r="B447" s="87"/>
-      <c r="C447" s="176"/>
-      <c r="D447" s="177"/>
-      <c r="E447" s="177"/>
+      <c r="C447" s="174"/>
+      <c r="D447" s="175"/>
+      <c r="E447" s="175"/>
     </row>
     <row r="448" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A448" s="52">
@@ -9578,9 +9588,9 @@
         <v>36</v>
       </c>
       <c r="B464" s="87"/>
-      <c r="C464" s="176"/>
-      <c r="D464" s="177"/>
-      <c r="E464" s="177"/>
+      <c r="C464" s="174"/>
+      <c r="D464" s="175"/>
+      <c r="E464" s="175"/>
     </row>
     <row r="465" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A465" s="52">
@@ -9731,9 +9741,9 @@
         <v>37</v>
       </c>
       <c r="B481" s="87"/>
-      <c r="C481" s="176"/>
-      <c r="D481" s="177"/>
-      <c r="E481" s="177"/>
+      <c r="C481" s="174"/>
+      <c r="D481" s="175"/>
+      <c r="E481" s="175"/>
     </row>
     <row r="482" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A482" s="52">
@@ -9884,9 +9894,9 @@
         <v>38</v>
       </c>
       <c r="B498" s="87"/>
-      <c r="C498" s="176"/>
-      <c r="D498" s="177"/>
-      <c r="E498" s="177"/>
+      <c r="C498" s="174"/>
+      <c r="D498" s="175"/>
+      <c r="E498" s="175"/>
     </row>
     <row r="499" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A499" s="52">
@@ -10037,9 +10047,9 @@
         <v>39</v>
       </c>
       <c r="B515" s="87"/>
-      <c r="C515" s="176"/>
-      <c r="D515" s="177"/>
-      <c r="E515" s="177"/>
+      <c r="C515" s="174"/>
+      <c r="D515" s="175"/>
+      <c r="E515" s="175"/>
     </row>
     <row r="516" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A516" s="52">
@@ -10190,9 +10200,9 @@
         <v>40</v>
       </c>
       <c r="B532" s="87"/>
-      <c r="C532" s="176"/>
-      <c r="D532" s="177"/>
-      <c r="E532" s="177"/>
+      <c r="C532" s="174"/>
+      <c r="D532" s="175"/>
+      <c r="E532" s="175"/>
     </row>
     <row r="533" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A533" s="55">
@@ -10343,18 +10353,18 @@
         <v>50</v>
       </c>
       <c r="B549" s="38"/>
-      <c r="C549" s="182"/>
-      <c r="D549" s="183"/>
-      <c r="E549" s="183"/>
+      <c r="C549" s="188"/>
+      <c r="D549" s="189"/>
+      <c r="E549" s="189"/>
     </row>
     <row r="550" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A550" s="58" t="s">
         <v>51</v>
       </c>
       <c r="B550" s="87"/>
-      <c r="C550" s="176"/>
-      <c r="D550" s="177"/>
-      <c r="E550" s="177"/>
+      <c r="C550" s="174"/>
+      <c r="D550" s="175"/>
+      <c r="E550" s="175"/>
     </row>
     <row r="551" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A551" s="59">
@@ -10505,9 +10515,9 @@
         <v>52</v>
       </c>
       <c r="B567" s="90"/>
-      <c r="C567" s="178"/>
-      <c r="D567" s="179"/>
-      <c r="E567" s="179"/>
+      <c r="C567" s="176"/>
+      <c r="D567" s="177"/>
+      <c r="E567" s="177"/>
     </row>
     <row r="568" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A568" s="59">
@@ -10658,9 +10668,9 @@
         <v>53</v>
       </c>
       <c r="B584" s="87"/>
-      <c r="C584" s="176"/>
-      <c r="D584" s="177"/>
-      <c r="E584" s="177"/>
+      <c r="C584" s="174"/>
+      <c r="D584" s="175"/>
+      <c r="E584" s="175"/>
     </row>
     <row r="585" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A585" s="59">
@@ -10811,9 +10821,9 @@
         <v>54</v>
       </c>
       <c r="B601" s="87"/>
-      <c r="C601" s="176"/>
-      <c r="D601" s="177"/>
-      <c r="E601" s="177"/>
+      <c r="C601" s="174"/>
+      <c r="D601" s="175"/>
+      <c r="E601" s="175"/>
     </row>
     <row r="602" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A602" s="59">
@@ -10964,9 +10974,9 @@
         <v>55</v>
       </c>
       <c r="B618" s="87"/>
-      <c r="C618" s="176"/>
-      <c r="D618" s="177"/>
-      <c r="E618" s="177"/>
+      <c r="C618" s="174"/>
+      <c r="D618" s="175"/>
+      <c r="E618" s="175"/>
     </row>
     <row r="619" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A619" s="59">
@@ -11117,9 +11127,9 @@
         <v>56</v>
       </c>
       <c r="B635" s="87"/>
-      <c r="C635" s="176"/>
-      <c r="D635" s="177"/>
-      <c r="E635" s="177"/>
+      <c r="C635" s="174"/>
+      <c r="D635" s="175"/>
+      <c r="E635" s="175"/>
     </row>
     <row r="636" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A636" s="59">
@@ -11270,9 +11280,9 @@
         <v>57</v>
       </c>
       <c r="B652" s="87"/>
-      <c r="C652" s="176"/>
-      <c r="D652" s="177"/>
-      <c r="E652" s="177"/>
+      <c r="C652" s="174"/>
+      <c r="D652" s="175"/>
+      <c r="E652" s="175"/>
     </row>
     <row r="653" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A653" s="59">
@@ -11423,9 +11433,9 @@
         <v>58</v>
       </c>
       <c r="B669" s="87"/>
-      <c r="C669" s="176"/>
-      <c r="D669" s="177"/>
-      <c r="E669" s="177"/>
+      <c r="C669" s="174"/>
+      <c r="D669" s="175"/>
+      <c r="E669" s="175"/>
     </row>
     <row r="670" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A670" s="59">
@@ -11576,9 +11586,9 @@
         <v>59</v>
       </c>
       <c r="B686" s="87"/>
-      <c r="C686" s="176"/>
-      <c r="D686" s="177"/>
-      <c r="E686" s="177"/>
+      <c r="C686" s="174"/>
+      <c r="D686" s="175"/>
+      <c r="E686" s="175"/>
     </row>
     <row r="687" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A687" s="59">
@@ -11729,9 +11739,9 @@
         <v>60</v>
       </c>
       <c r="B703" s="87"/>
-      <c r="C703" s="176"/>
-      <c r="D703" s="177"/>
-      <c r="E703" s="177"/>
+      <c r="C703" s="174"/>
+      <c r="D703" s="175"/>
+      <c r="E703" s="175"/>
     </row>
     <row r="704" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A704" s="59">
@@ -11882,9 +11892,9 @@
         <v>61</v>
       </c>
       <c r="B720" s="87"/>
-      <c r="C720" s="176"/>
-      <c r="D720" s="177"/>
-      <c r="E720" s="177"/>
+      <c r="C720" s="174"/>
+      <c r="D720" s="175"/>
+      <c r="E720" s="175"/>
     </row>
     <row r="721" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A721" s="59">
@@ -12035,9 +12045,9 @@
         <v>62</v>
       </c>
       <c r="B737" s="87"/>
-      <c r="C737" s="176"/>
-      <c r="D737" s="177"/>
-      <c r="E737" s="177"/>
+      <c r="C737" s="174"/>
+      <c r="D737" s="175"/>
+      <c r="E737" s="175"/>
     </row>
     <row r="738" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A738" s="59">
@@ -12188,9 +12198,9 @@
         <v>63</v>
       </c>
       <c r="B754" s="87"/>
-      <c r="C754" s="176"/>
-      <c r="D754" s="177"/>
-      <c r="E754" s="177"/>
+      <c r="C754" s="174"/>
+      <c r="D754" s="175"/>
+      <c r="E754" s="175"/>
     </row>
     <row r="755" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A755" s="59">
@@ -12341,9 +12351,9 @@
         <v>64</v>
       </c>
       <c r="B771" s="87"/>
-      <c r="C771" s="176"/>
-      <c r="D771" s="177"/>
-      <c r="E771" s="177"/>
+      <c r="C771" s="174"/>
+      <c r="D771" s="175"/>
+      <c r="E771" s="175"/>
     </row>
     <row r="772" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A772" s="59">
@@ -12494,9 +12504,9 @@
         <v>65</v>
       </c>
       <c r="B788" s="87"/>
-      <c r="C788" s="176"/>
-      <c r="D788" s="177"/>
-      <c r="E788" s="177"/>
+      <c r="C788" s="174"/>
+      <c r="D788" s="175"/>
+      <c r="E788" s="175"/>
     </row>
     <row r="789" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A789" s="59">
@@ -12647,9 +12657,9 @@
         <v>66</v>
       </c>
       <c r="B805" s="87"/>
-      <c r="C805" s="176"/>
-      <c r="D805" s="177"/>
-      <c r="E805" s="177"/>
+      <c r="C805" s="174"/>
+      <c r="D805" s="175"/>
+      <c r="E805" s="175"/>
     </row>
     <row r="806" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A806" s="59">
@@ -12800,18 +12810,18 @@
         <v>67</v>
       </c>
       <c r="B822" s="39"/>
-      <c r="C822" s="184"/>
-      <c r="D822" s="185"/>
-      <c r="E822" s="185"/>
+      <c r="C822" s="186"/>
+      <c r="D822" s="187"/>
+      <c r="E822" s="187"/>
     </row>
     <row r="823" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A823" s="63" t="s">
         <v>68</v>
       </c>
       <c r="B823" s="87"/>
-      <c r="C823" s="176"/>
-      <c r="D823" s="177"/>
-      <c r="E823" s="177"/>
+      <c r="C823" s="174"/>
+      <c r="D823" s="175"/>
+      <c r="E823" s="175"/>
     </row>
     <row r="824" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A824" s="64">
@@ -12962,9 +12972,9 @@
         <v>69</v>
       </c>
       <c r="B840" s="90"/>
-      <c r="C840" s="178"/>
-      <c r="D840" s="179"/>
-      <c r="E840" s="179"/>
+      <c r="C840" s="176"/>
+      <c r="D840" s="177"/>
+      <c r="E840" s="177"/>
     </row>
     <row r="841" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A841" s="64">
@@ -13115,9 +13125,9 @@
         <v>70</v>
       </c>
       <c r="B857" s="87"/>
-      <c r="C857" s="176"/>
-      <c r="D857" s="177"/>
-      <c r="E857" s="177"/>
+      <c r="C857" s="174"/>
+      <c r="D857" s="175"/>
+      <c r="E857" s="175"/>
     </row>
     <row r="858" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A858" s="64">
@@ -13268,9 +13278,9 @@
         <v>71</v>
       </c>
       <c r="B874" s="87"/>
-      <c r="C874" s="176"/>
-      <c r="D874" s="177"/>
-      <c r="E874" s="177"/>
+      <c r="C874" s="174"/>
+      <c r="D874" s="175"/>
+      <c r="E874" s="175"/>
     </row>
     <row r="875" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A875" s="64">
@@ -13421,9 +13431,9 @@
         <v>72</v>
       </c>
       <c r="B891" s="87"/>
-      <c r="C891" s="176"/>
-      <c r="D891" s="177"/>
-      <c r="E891" s="177"/>
+      <c r="C891" s="174"/>
+      <c r="D891" s="175"/>
+      <c r="E891" s="175"/>
     </row>
     <row r="892" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A892" s="64">
@@ -13574,9 +13584,9 @@
         <v>73</v>
       </c>
       <c r="B908" s="87"/>
-      <c r="C908" s="176"/>
-      <c r="D908" s="177"/>
-      <c r="E908" s="177"/>
+      <c r="C908" s="174"/>
+      <c r="D908" s="175"/>
+      <c r="E908" s="175"/>
     </row>
     <row r="909" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A909" s="64">
@@ -13727,9 +13737,9 @@
         <v>74</v>
       </c>
       <c r="B925" s="87"/>
-      <c r="C925" s="176"/>
-      <c r="D925" s="177"/>
-      <c r="E925" s="177"/>
+      <c r="C925" s="174"/>
+      <c r="D925" s="175"/>
+      <c r="E925" s="175"/>
     </row>
     <row r="926" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A926" s="64">
@@ -13880,9 +13890,9 @@
         <v>75</v>
       </c>
       <c r="B942" s="87"/>
-      <c r="C942" s="176"/>
-      <c r="D942" s="177"/>
-      <c r="E942" s="177"/>
+      <c r="C942" s="174"/>
+      <c r="D942" s="175"/>
+      <c r="E942" s="175"/>
     </row>
     <row r="943" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A943" s="64">
@@ -14033,9 +14043,9 @@
         <v>76</v>
       </c>
       <c r="B959" s="87"/>
-      <c r="C959" s="176"/>
-      <c r="D959" s="177"/>
-      <c r="E959" s="177"/>
+      <c r="C959" s="174"/>
+      <c r="D959" s="175"/>
+      <c r="E959" s="175"/>
     </row>
     <row r="960" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A960" s="64">
@@ -14186,9 +14196,9 @@
         <v>77</v>
       </c>
       <c r="B976" s="87"/>
-      <c r="C976" s="176"/>
-      <c r="D976" s="177"/>
-      <c r="E976" s="177"/>
+      <c r="C976" s="174"/>
+      <c r="D976" s="175"/>
+      <c r="E976" s="175"/>
     </row>
     <row r="977" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A977" s="64">
@@ -14339,9 +14349,9 @@
         <v>78</v>
       </c>
       <c r="B993" s="87"/>
-      <c r="C993" s="176"/>
-      <c r="D993" s="177"/>
-      <c r="E993" s="177"/>
+      <c r="C993" s="174"/>
+      <c r="D993" s="175"/>
+      <c r="E993" s="175"/>
     </row>
     <row r="994" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A994" s="64">
@@ -14492,9 +14502,9 @@
         <v>79</v>
       </c>
       <c r="B1010" s="87"/>
-      <c r="C1010" s="176"/>
-      <c r="D1010" s="177"/>
-      <c r="E1010" s="177"/>
+      <c r="C1010" s="174"/>
+      <c r="D1010" s="175"/>
+      <c r="E1010" s="175"/>
     </row>
     <row r="1011" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1011" s="64">
@@ -14645,9 +14655,9 @@
         <v>80</v>
       </c>
       <c r="B1027" s="87"/>
-      <c r="C1027" s="176"/>
-      <c r="D1027" s="177"/>
-      <c r="E1027" s="177"/>
+      <c r="C1027" s="174"/>
+      <c r="D1027" s="175"/>
+      <c r="E1027" s="175"/>
     </row>
     <row r="1028" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1028" s="64">
@@ -14798,9 +14808,9 @@
         <v>83</v>
       </c>
       <c r="B1044" s="87"/>
-      <c r="C1044" s="176"/>
-      <c r="D1044" s="177"/>
-      <c r="E1044" s="177"/>
+      <c r="C1044" s="174"/>
+      <c r="D1044" s="175"/>
+      <c r="E1044" s="175"/>
     </row>
     <row r="1045" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1045" s="64">
@@ -14951,9 +14961,9 @@
         <v>82</v>
       </c>
       <c r="B1061" s="87"/>
-      <c r="C1061" s="176"/>
-      <c r="D1061" s="177"/>
-      <c r="E1061" s="177"/>
+      <c r="C1061" s="174"/>
+      <c r="D1061" s="175"/>
+      <c r="E1061" s="175"/>
     </row>
     <row r="1062" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1062" s="64">
@@ -15104,9 +15114,9 @@
         <v>84</v>
       </c>
       <c r="B1078" s="87"/>
-      <c r="C1078" s="176"/>
-      <c r="D1078" s="177"/>
-      <c r="E1078" s="177"/>
+      <c r="C1078" s="174"/>
+      <c r="D1078" s="175"/>
+      <c r="E1078" s="175"/>
     </row>
     <row r="1079" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1079" s="64">
@@ -15257,18 +15267,18 @@
         <v>104</v>
       </c>
       <c r="B1095" s="40"/>
-      <c r="C1095" s="186"/>
-      <c r="D1095" s="187"/>
-      <c r="E1095" s="187"/>
+      <c r="C1095" s="184"/>
+      <c r="D1095" s="185"/>
+      <c r="E1095" s="185"/>
     </row>
     <row r="1096" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A1096" s="68" t="s">
         <v>85</v>
       </c>
       <c r="B1096" s="87"/>
-      <c r="C1096" s="176"/>
-      <c r="D1096" s="177"/>
-      <c r="E1096" s="177"/>
+      <c r="C1096" s="174"/>
+      <c r="D1096" s="175"/>
+      <c r="E1096" s="175"/>
     </row>
     <row r="1097" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1097" s="69">
@@ -15419,9 +15429,9 @@
         <v>86</v>
       </c>
       <c r="B1113" s="90"/>
-      <c r="C1113" s="178"/>
-      <c r="D1113" s="179"/>
-      <c r="E1113" s="179"/>
+      <c r="C1113" s="176"/>
+      <c r="D1113" s="177"/>
+      <c r="E1113" s="177"/>
     </row>
     <row r="1114" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1114" s="69">
@@ -15572,9 +15582,9 @@
         <v>87</v>
       </c>
       <c r="B1130" s="87"/>
-      <c r="C1130" s="176"/>
-      <c r="D1130" s="177"/>
-      <c r="E1130" s="177"/>
+      <c r="C1130" s="174"/>
+      <c r="D1130" s="175"/>
+      <c r="E1130" s="175"/>
     </row>
     <row r="1131" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1131" s="69">
@@ -15725,9 +15735,9 @@
         <v>88</v>
       </c>
       <c r="B1147" s="87"/>
-      <c r="C1147" s="176"/>
-      <c r="D1147" s="177"/>
-      <c r="E1147" s="177"/>
+      <c r="C1147" s="174"/>
+      <c r="D1147" s="175"/>
+      <c r="E1147" s="175"/>
     </row>
     <row r="1148" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1148" s="69">
@@ -15878,9 +15888,9 @@
         <v>89</v>
       </c>
       <c r="B1164" s="87"/>
-      <c r="C1164" s="176"/>
-      <c r="D1164" s="177"/>
-      <c r="E1164" s="177"/>
+      <c r="C1164" s="174"/>
+      <c r="D1164" s="175"/>
+      <c r="E1164" s="175"/>
     </row>
     <row r="1165" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1165" s="69">
@@ -16031,9 +16041,9 @@
         <v>90</v>
       </c>
       <c r="B1181" s="87"/>
-      <c r="C1181" s="176"/>
-      <c r="D1181" s="177"/>
-      <c r="E1181" s="177"/>
+      <c r="C1181" s="174"/>
+      <c r="D1181" s="175"/>
+      <c r="E1181" s="175"/>
     </row>
     <row r="1182" spans="1:5" hidden="1" outlineLevel="3">
       <c r="A1182" s="69">
@@ -16184,9 +16194,9 @@
         <v>91</v>
       </c>
       <c r="B1198" s="87"/>
-      <c r="C1198" s="176"/>
-      <c r="D1198" s="177"/>
-      <c r="E1198" s="177"/>
+      <c r="C1198" s="174"/>
+      <c r="D1198" s="175"/>
+      <c r="E1198" s="175"/>
     </row>
     <row r="1199" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1199" s="69">
@@ -16337,9 +16347,9 @@
         <v>92</v>
       </c>
       <c r="B1215" s="87"/>
-      <c r="C1215" s="176"/>
-      <c r="D1215" s="177"/>
-      <c r="E1215" s="177"/>
+      <c r="C1215" s="174"/>
+      <c r="D1215" s="175"/>
+      <c r="E1215" s="175"/>
     </row>
     <row r="1216" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1216" s="69">
@@ -16490,9 +16500,9 @@
         <v>93</v>
       </c>
       <c r="B1232" s="87"/>
-      <c r="C1232" s="176"/>
-      <c r="D1232" s="177"/>
-      <c r="E1232" s="177"/>
+      <c r="C1232" s="174"/>
+      <c r="D1232" s="175"/>
+      <c r="E1232" s="175"/>
     </row>
     <row r="1233" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1233" s="69">
@@ -16643,9 +16653,9 @@
         <v>94</v>
       </c>
       <c r="B1249" s="87"/>
-      <c r="C1249" s="176"/>
-      <c r="D1249" s="177"/>
-      <c r="E1249" s="177"/>
+      <c r="C1249" s="174"/>
+      <c r="D1249" s="175"/>
+      <c r="E1249" s="175"/>
     </row>
     <row r="1250" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1250" s="69">
@@ -16796,9 +16806,9 @@
         <v>99</v>
       </c>
       <c r="B1266" s="87"/>
-      <c r="C1266" s="176"/>
-      <c r="D1266" s="177"/>
-      <c r="E1266" s="177"/>
+      <c r="C1266" s="174"/>
+      <c r="D1266" s="175"/>
+      <c r="E1266" s="175"/>
     </row>
     <row r="1267" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1267" s="69">
@@ -16949,9 +16959,9 @@
         <v>100</v>
       </c>
       <c r="B1283" s="87"/>
-      <c r="C1283" s="176"/>
-      <c r="D1283" s="177"/>
-      <c r="E1283" s="177"/>
+      <c r="C1283" s="174"/>
+      <c r="D1283" s="175"/>
+      <c r="E1283" s="175"/>
     </row>
     <row r="1284" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1284" s="69">
@@ -17102,9 +17112,9 @@
         <v>101</v>
       </c>
       <c r="B1300" s="87"/>
-      <c r="C1300" s="176"/>
-      <c r="D1300" s="177"/>
-      <c r="E1300" s="177"/>
+      <c r="C1300" s="174"/>
+      <c r="D1300" s="175"/>
+      <c r="E1300" s="175"/>
     </row>
     <row r="1301" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1301" s="69">
@@ -17255,9 +17265,9 @@
         <v>81</v>
       </c>
       <c r="B1317" s="87"/>
-      <c r="C1317" s="176"/>
-      <c r="D1317" s="177"/>
-      <c r="E1317" s="177"/>
+      <c r="C1317" s="174"/>
+      <c r="D1317" s="175"/>
+      <c r="E1317" s="175"/>
     </row>
     <row r="1318" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1318" s="69">
@@ -17408,9 +17418,9 @@
         <v>102</v>
       </c>
       <c r="B1334" s="87"/>
-      <c r="C1334" s="176"/>
-      <c r="D1334" s="177"/>
-      <c r="E1334" s="177"/>
+      <c r="C1334" s="174"/>
+      <c r="D1334" s="175"/>
+      <c r="E1334" s="175"/>
     </row>
     <row r="1335" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1335" s="69">
@@ -17561,9 +17571,9 @@
         <v>98</v>
       </c>
       <c r="B1351" s="87"/>
-      <c r="C1351" s="176"/>
-      <c r="D1351" s="177"/>
-      <c r="E1351" s="177"/>
+      <c r="C1351" s="174"/>
+      <c r="D1351" s="175"/>
+      <c r="E1351" s="175"/>
     </row>
     <row r="1352" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1352" s="69">
@@ -17714,18 +17724,18 @@
         <v>103</v>
       </c>
       <c r="B1368" s="41"/>
-      <c r="C1368" s="188"/>
-      <c r="D1368" s="189"/>
-      <c r="E1368" s="189"/>
+      <c r="C1368" s="182"/>
+      <c r="D1368" s="183"/>
+      <c r="E1368" s="183"/>
     </row>
     <row r="1369" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A1369" s="73" t="s">
         <v>105</v>
       </c>
       <c r="B1369" s="87"/>
-      <c r="C1369" s="176"/>
-      <c r="D1369" s="177"/>
-      <c r="E1369" s="177"/>
+      <c r="C1369" s="174"/>
+      <c r="D1369" s="175"/>
+      <c r="E1369" s="175"/>
     </row>
     <row r="1370" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1370" s="74">
@@ -17876,9 +17886,9 @@
         <v>106</v>
       </c>
       <c r="B1386" s="90"/>
-      <c r="C1386" s="178"/>
-      <c r="D1386" s="179"/>
-      <c r="E1386" s="179"/>
+      <c r="C1386" s="176"/>
+      <c r="D1386" s="177"/>
+      <c r="E1386" s="177"/>
     </row>
     <row r="1387" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1387" s="74">
@@ -18029,9 +18039,9 @@
         <v>107</v>
       </c>
       <c r="B1403" s="87"/>
-      <c r="C1403" s="176"/>
-      <c r="D1403" s="177"/>
-      <c r="E1403" s="177"/>
+      <c r="C1403" s="174"/>
+      <c r="D1403" s="175"/>
+      <c r="E1403" s="175"/>
     </row>
     <row r="1404" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1404" s="74">
@@ -18182,9 +18192,9 @@
         <v>108</v>
       </c>
       <c r="B1420" s="87"/>
-      <c r="C1420" s="176"/>
-      <c r="D1420" s="177"/>
-      <c r="E1420" s="177"/>
+      <c r="C1420" s="174"/>
+      <c r="D1420" s="175"/>
+      <c r="E1420" s="175"/>
     </row>
     <row r="1421" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1421" s="74">
@@ -18335,9 +18345,9 @@
         <v>109</v>
       </c>
       <c r="B1437" s="87"/>
-      <c r="C1437" s="176"/>
-      <c r="D1437" s="177"/>
-      <c r="E1437" s="177"/>
+      <c r="C1437" s="174"/>
+      <c r="D1437" s="175"/>
+      <c r="E1437" s="175"/>
     </row>
     <row r="1438" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1438" s="74">
@@ -18488,9 +18498,9 @@
         <v>110</v>
       </c>
       <c r="B1454" s="87"/>
-      <c r="C1454" s="176"/>
-      <c r="D1454" s="177"/>
-      <c r="E1454" s="177"/>
+      <c r="C1454" s="174"/>
+      <c r="D1454" s="175"/>
+      <c r="E1454" s="175"/>
     </row>
     <row r="1455" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1455" s="74">
@@ -18641,9 +18651,9 @@
         <v>111</v>
       </c>
       <c r="B1471" s="87"/>
-      <c r="C1471" s="176"/>
-      <c r="D1471" s="177"/>
-      <c r="E1471" s="177"/>
+      <c r="C1471" s="174"/>
+      <c r="D1471" s="175"/>
+      <c r="E1471" s="175"/>
     </row>
     <row r="1472" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1472" s="74">
@@ -18794,9 +18804,9 @@
         <v>112</v>
       </c>
       <c r="B1488" s="87"/>
-      <c r="C1488" s="176"/>
-      <c r="D1488" s="177"/>
-      <c r="E1488" s="177"/>
+      <c r="C1488" s="174"/>
+      <c r="D1488" s="175"/>
+      <c r="E1488" s="175"/>
     </row>
     <row r="1489" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1489" s="74">
@@ -18947,9 +18957,9 @@
         <v>113</v>
       </c>
       <c r="B1505" s="87"/>
-      <c r="C1505" s="176"/>
-      <c r="D1505" s="177"/>
-      <c r="E1505" s="177"/>
+      <c r="C1505" s="174"/>
+      <c r="D1505" s="175"/>
+      <c r="E1505" s="175"/>
     </row>
     <row r="1506" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1506" s="74">
@@ -19100,9 +19110,9 @@
         <v>114</v>
       </c>
       <c r="B1522" s="87"/>
-      <c r="C1522" s="176"/>
-      <c r="D1522" s="177"/>
-      <c r="E1522" s="177"/>
+      <c r="C1522" s="174"/>
+      <c r="D1522" s="175"/>
+      <c r="E1522" s="175"/>
     </row>
     <row r="1523" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1523" s="74">
@@ -19253,9 +19263,9 @@
         <v>95</v>
       </c>
       <c r="B1539" s="87"/>
-      <c r="C1539" s="176"/>
-      <c r="D1539" s="177"/>
-      <c r="E1539" s="177"/>
+      <c r="C1539" s="174"/>
+      <c r="D1539" s="175"/>
+      <c r="E1539" s="175"/>
     </row>
     <row r="1540" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1540" s="74">
@@ -19406,9 +19416,9 @@
         <v>115</v>
       </c>
       <c r="B1556" s="87"/>
-      <c r="C1556" s="176"/>
-      <c r="D1556" s="177"/>
-      <c r="E1556" s="177"/>
+      <c r="C1556" s="174"/>
+      <c r="D1556" s="175"/>
+      <c r="E1556" s="175"/>
     </row>
     <row r="1557" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1557" s="74">
@@ -19559,9 +19569,9 @@
         <v>116</v>
       </c>
       <c r="B1573" s="87"/>
-      <c r="C1573" s="176"/>
-      <c r="D1573" s="177"/>
-      <c r="E1573" s="177"/>
+      <c r="C1573" s="174"/>
+      <c r="D1573" s="175"/>
+      <c r="E1573" s="175"/>
     </row>
     <row r="1574" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1574" s="74">
@@ -19712,9 +19722,9 @@
         <v>117</v>
       </c>
       <c r="B1590" s="87"/>
-      <c r="C1590" s="176"/>
-      <c r="D1590" s="177"/>
-      <c r="E1590" s="177"/>
+      <c r="C1590" s="174"/>
+      <c r="D1590" s="175"/>
+      <c r="E1590" s="175"/>
     </row>
     <row r="1591" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1591" s="74">
@@ -19865,9 +19875,9 @@
         <v>118</v>
       </c>
       <c r="B1607" s="87"/>
-      <c r="C1607" s="176"/>
-      <c r="D1607" s="177"/>
-      <c r="E1607" s="177"/>
+      <c r="C1607" s="174"/>
+      <c r="D1607" s="175"/>
+      <c r="E1607" s="175"/>
     </row>
     <row r="1608" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1608" s="74">
@@ -20018,9 +20028,9 @@
         <v>119</v>
       </c>
       <c r="B1624" s="87"/>
-      <c r="C1624" s="176"/>
-      <c r="D1624" s="177"/>
-      <c r="E1624" s="177"/>
+      <c r="C1624" s="174"/>
+      <c r="D1624" s="175"/>
+      <c r="E1624" s="175"/>
     </row>
     <row r="1625" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1625" s="74">
@@ -20171,18 +20181,18 @@
         <v>120</v>
       </c>
       <c r="B1641" s="42"/>
-      <c r="C1641" s="190"/>
-      <c r="D1641" s="191"/>
-      <c r="E1641" s="191"/>
+      <c r="C1641" s="180"/>
+      <c r="D1641" s="181"/>
+      <c r="E1641" s="181"/>
     </row>
     <row r="1642" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A1642" s="78" t="s">
         <v>121</v>
       </c>
       <c r="B1642" s="87"/>
-      <c r="C1642" s="176"/>
-      <c r="D1642" s="177"/>
-      <c r="E1642" s="177"/>
+      <c r="C1642" s="174"/>
+      <c r="D1642" s="175"/>
+      <c r="E1642" s="175"/>
     </row>
     <row r="1643" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1643" s="79">
@@ -20333,9 +20343,9 @@
         <v>122</v>
       </c>
       <c r="B1659" s="90"/>
-      <c r="C1659" s="178"/>
-      <c r="D1659" s="179"/>
-      <c r="E1659" s="179"/>
+      <c r="C1659" s="176"/>
+      <c r="D1659" s="177"/>
+      <c r="E1659" s="177"/>
     </row>
     <row r="1660" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1660" s="79">
@@ -20486,9 +20496,9 @@
         <v>123</v>
       </c>
       <c r="B1676" s="87"/>
-      <c r="C1676" s="176"/>
-      <c r="D1676" s="177"/>
-      <c r="E1676" s="177"/>
+      <c r="C1676" s="174"/>
+      <c r="D1676" s="175"/>
+      <c r="E1676" s="175"/>
     </row>
     <row r="1677" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1677" s="79">
@@ -20639,9 +20649,9 @@
         <v>124</v>
       </c>
       <c r="B1693" s="87"/>
-      <c r="C1693" s="176"/>
-      <c r="D1693" s="177"/>
-      <c r="E1693" s="177"/>
+      <c r="C1693" s="174"/>
+      <c r="D1693" s="175"/>
+      <c r="E1693" s="175"/>
     </row>
     <row r="1694" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1694" s="79">
@@ -20792,9 +20802,9 @@
         <v>125</v>
       </c>
       <c r="B1710" s="87"/>
-      <c r="C1710" s="176"/>
-      <c r="D1710" s="177"/>
-      <c r="E1710" s="177"/>
+      <c r="C1710" s="174"/>
+      <c r="D1710" s="175"/>
+      <c r="E1710" s="175"/>
     </row>
     <row r="1711" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1711" s="79">
@@ -20945,9 +20955,9 @@
         <v>126</v>
       </c>
       <c r="B1727" s="87"/>
-      <c r="C1727" s="176"/>
-      <c r="D1727" s="177"/>
-      <c r="E1727" s="177"/>
+      <c r="C1727" s="174"/>
+      <c r="D1727" s="175"/>
+      <c r="E1727" s="175"/>
     </row>
     <row r="1728" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1728" s="79">
@@ -21098,9 +21108,9 @@
         <v>127</v>
       </c>
       <c r="B1744" s="87"/>
-      <c r="C1744" s="176"/>
-      <c r="D1744" s="177"/>
-      <c r="E1744" s="177"/>
+      <c r="C1744" s="174"/>
+      <c r="D1744" s="175"/>
+      <c r="E1744" s="175"/>
     </row>
     <row r="1745" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1745" s="79">
@@ -21251,9 +21261,9 @@
         <v>128</v>
       </c>
       <c r="B1761" s="87"/>
-      <c r="C1761" s="176"/>
-      <c r="D1761" s="177"/>
-      <c r="E1761" s="177"/>
+      <c r="C1761" s="174"/>
+      <c r="D1761" s="175"/>
+      <c r="E1761" s="175"/>
     </row>
     <row r="1762" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1762" s="79">
@@ -21404,9 +21414,9 @@
         <v>129</v>
       </c>
       <c r="B1778" s="87"/>
-      <c r="C1778" s="176"/>
-      <c r="D1778" s="177"/>
-      <c r="E1778" s="177"/>
+      <c r="C1778" s="174"/>
+      <c r="D1778" s="175"/>
+      <c r="E1778" s="175"/>
     </row>
     <row r="1779" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1779" s="79">
@@ -21557,9 +21567,9 @@
         <v>130</v>
       </c>
       <c r="B1795" s="87"/>
-      <c r="C1795" s="176"/>
-      <c r="D1795" s="177"/>
-      <c r="E1795" s="177"/>
+      <c r="C1795" s="174"/>
+      <c r="D1795" s="175"/>
+      <c r="E1795" s="175"/>
     </row>
     <row r="1796" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1796" s="79">
@@ -21710,9 +21720,9 @@
         <v>131</v>
       </c>
       <c r="B1812" s="87"/>
-      <c r="C1812" s="176"/>
-      <c r="D1812" s="177"/>
-      <c r="E1812" s="177"/>
+      <c r="C1812" s="174"/>
+      <c r="D1812" s="175"/>
+      <c r="E1812" s="175"/>
     </row>
     <row r="1813" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1813" s="79">
@@ -21863,9 +21873,9 @@
         <v>96</v>
       </c>
       <c r="B1829" s="87"/>
-      <c r="C1829" s="176"/>
-      <c r="D1829" s="177"/>
-      <c r="E1829" s="177"/>
+      <c r="C1829" s="174"/>
+      <c r="D1829" s="175"/>
+      <c r="E1829" s="175"/>
     </row>
     <row r="1830" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1830" s="79">
@@ -22016,9 +22026,9 @@
         <v>132</v>
       </c>
       <c r="B1846" s="87"/>
-      <c r="C1846" s="176"/>
-      <c r="D1846" s="177"/>
-      <c r="E1846" s="177"/>
+      <c r="C1846" s="174"/>
+      <c r="D1846" s="175"/>
+      <c r="E1846" s="175"/>
     </row>
     <row r="1847" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1847" s="79">
@@ -22169,9 +22179,9 @@
         <v>133</v>
       </c>
       <c r="B1863" s="87"/>
-      <c r="C1863" s="176"/>
-      <c r="D1863" s="177"/>
-      <c r="E1863" s="177"/>
+      <c r="C1863" s="174"/>
+      <c r="D1863" s="175"/>
+      <c r="E1863" s="175"/>
     </row>
     <row r="1864" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1864" s="79">
@@ -22322,9 +22332,9 @@
         <v>134</v>
       </c>
       <c r="B1880" s="87"/>
-      <c r="C1880" s="176"/>
-      <c r="D1880" s="177"/>
-      <c r="E1880" s="177"/>
+      <c r="C1880" s="174"/>
+      <c r="D1880" s="175"/>
+      <c r="E1880" s="175"/>
     </row>
     <row r="1881" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1881" s="79">
@@ -22475,9 +22485,9 @@
         <v>135</v>
       </c>
       <c r="B1897" s="87"/>
-      <c r="C1897" s="176"/>
-      <c r="D1897" s="177"/>
-      <c r="E1897" s="177"/>
+      <c r="C1897" s="174"/>
+      <c r="D1897" s="175"/>
+      <c r="E1897" s="175"/>
     </row>
     <row r="1898" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1898" s="79">
@@ -22628,18 +22638,18 @@
         <v>136</v>
       </c>
       <c r="B1914" s="43"/>
-      <c r="C1914" s="192"/>
-      <c r="D1914" s="193"/>
-      <c r="E1914" s="193"/>
+      <c r="C1914" s="178"/>
+      <c r="D1914" s="179"/>
+      <c r="E1914" s="179"/>
     </row>
     <row r="1915" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A1915" s="83" t="s">
         <v>137</v>
       </c>
       <c r="B1915" s="87"/>
-      <c r="C1915" s="176"/>
-      <c r="D1915" s="177"/>
-      <c r="E1915" s="177"/>
+      <c r="C1915" s="174"/>
+      <c r="D1915" s="175"/>
+      <c r="E1915" s="175"/>
     </row>
     <row r="1916" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1916" s="84">
@@ -22790,9 +22800,9 @@
         <v>138</v>
       </c>
       <c r="B1932" s="90"/>
-      <c r="C1932" s="178"/>
-      <c r="D1932" s="179"/>
-      <c r="E1932" s="179"/>
+      <c r="C1932" s="176"/>
+      <c r="D1932" s="177"/>
+      <c r="E1932" s="177"/>
     </row>
     <row r="1933" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1933" s="84">
@@ -22943,9 +22953,9 @@
         <v>139</v>
       </c>
       <c r="B1949" s="87"/>
-      <c r="C1949" s="176"/>
-      <c r="D1949" s="177"/>
-      <c r="E1949" s="177"/>
+      <c r="C1949" s="174"/>
+      <c r="D1949" s="175"/>
+      <c r="E1949" s="175"/>
     </row>
     <row r="1950" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1950" s="84">
@@ -23096,9 +23106,9 @@
         <v>140</v>
       </c>
       <c r="B1966" s="87"/>
-      <c r="C1966" s="176"/>
-      <c r="D1966" s="177"/>
-      <c r="E1966" s="177"/>
+      <c r="C1966" s="174"/>
+      <c r="D1966" s="175"/>
+      <c r="E1966" s="175"/>
     </row>
     <row r="1967" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1967" s="84">
@@ -23249,9 +23259,9 @@
         <v>141</v>
       </c>
       <c r="B1983" s="87"/>
-      <c r="C1983" s="176"/>
-      <c r="D1983" s="177"/>
-      <c r="E1983" s="177"/>
+      <c r="C1983" s="174"/>
+      <c r="D1983" s="175"/>
+      <c r="E1983" s="175"/>
     </row>
     <row r="1984" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1984" s="84">
@@ -23402,9 +23412,9 @@
         <v>142</v>
       </c>
       <c r="B2000" s="87"/>
-      <c r="C2000" s="176"/>
-      <c r="D2000" s="177"/>
-      <c r="E2000" s="177"/>
+      <c r="C2000" s="174"/>
+      <c r="D2000" s="175"/>
+      <c r="E2000" s="175"/>
     </row>
     <row r="2001" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2001" s="84">
@@ -23555,9 +23565,9 @@
         <v>143</v>
       </c>
       <c r="B2017" s="87"/>
-      <c r="C2017" s="176"/>
-      <c r="D2017" s="177"/>
-      <c r="E2017" s="177"/>
+      <c r="C2017" s="174"/>
+      <c r="D2017" s="175"/>
+      <c r="E2017" s="175"/>
     </row>
     <row r="2018" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2018" s="84">
@@ -23708,9 +23718,9 @@
         <v>144</v>
       </c>
       <c r="B2034" s="87"/>
-      <c r="C2034" s="176"/>
-      <c r="D2034" s="177"/>
-      <c r="E2034" s="177"/>
+      <c r="C2034" s="174"/>
+      <c r="D2034" s="175"/>
+      <c r="E2034" s="175"/>
     </row>
     <row r="2035" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2035" s="84">
@@ -23861,9 +23871,9 @@
         <v>145</v>
       </c>
       <c r="B2051" s="87"/>
-      <c r="C2051" s="176"/>
-      <c r="D2051" s="177"/>
-      <c r="E2051" s="177"/>
+      <c r="C2051" s="174"/>
+      <c r="D2051" s="175"/>
+      <c r="E2051" s="175"/>
     </row>
     <row r="2052" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2052" s="84">
@@ -24014,9 +24024,9 @@
         <v>146</v>
       </c>
       <c r="B2068" s="87"/>
-      <c r="C2068" s="176"/>
-      <c r="D2068" s="177"/>
-      <c r="E2068" s="177"/>
+      <c r="C2068" s="174"/>
+      <c r="D2068" s="175"/>
+      <c r="E2068" s="175"/>
     </row>
     <row r="2069" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2069" s="84">
@@ -24167,9 +24177,9 @@
         <v>147</v>
       </c>
       <c r="B2085" s="87"/>
-      <c r="C2085" s="176"/>
-      <c r="D2085" s="177"/>
-      <c r="E2085" s="177"/>
+      <c r="C2085" s="174"/>
+      <c r="D2085" s="175"/>
+      <c r="E2085" s="175"/>
     </row>
     <row r="2086" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2086" s="84">
@@ -24320,9 +24330,9 @@
         <v>148</v>
       </c>
       <c r="B2102" s="87"/>
-      <c r="C2102" s="176"/>
-      <c r="D2102" s="177"/>
-      <c r="E2102" s="177"/>
+      <c r="C2102" s="174"/>
+      <c r="D2102" s="175"/>
+      <c r="E2102" s="175"/>
     </row>
     <row r="2103" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2103" s="84">
@@ -24473,9 +24483,9 @@
         <v>97</v>
       </c>
       <c r="B2119" s="87"/>
-      <c r="C2119" s="176"/>
-      <c r="D2119" s="177"/>
-      <c r="E2119" s="177"/>
+      <c r="C2119" s="174"/>
+      <c r="D2119" s="175"/>
+      <c r="E2119" s="175"/>
     </row>
     <row r="2120" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2120" s="84">
@@ -24626,9 +24636,9 @@
         <v>149</v>
       </c>
       <c r="B2136" s="87"/>
-      <c r="C2136" s="176"/>
-      <c r="D2136" s="177"/>
-      <c r="E2136" s="177"/>
+      <c r="C2136" s="174"/>
+      <c r="D2136" s="175"/>
+      <c r="E2136" s="175"/>
     </row>
     <row r="2137" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2137" s="84">
@@ -24779,9 +24789,9 @@
         <v>150</v>
       </c>
       <c r="B2153" s="87"/>
-      <c r="C2153" s="176"/>
-      <c r="D2153" s="177"/>
-      <c r="E2153" s="177"/>
+      <c r="C2153" s="174"/>
+      <c r="D2153" s="175"/>
+      <c r="E2153" s="175"/>
     </row>
     <row r="2154" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2154" s="84">
@@ -24932,9 +24942,9 @@
         <v>151</v>
       </c>
       <c r="B2170" s="87"/>
-      <c r="C2170" s="176"/>
-      <c r="D2170" s="177"/>
-      <c r="E2170" s="177"/>
+      <c r="C2170" s="174"/>
+      <c r="D2170" s="175"/>
+      <c r="E2170" s="175"/>
     </row>
     <row r="2171" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2171" s="84">
@@ -25082,15 +25092,122 @@
     </row>
   </sheetData>
   <mergeCells count="137">
-    <mergeCell ref="C2034:E2034"/>
-    <mergeCell ref="C2051:E2051"/>
-    <mergeCell ref="C2068:E2068"/>
-    <mergeCell ref="C2085:E2085"/>
-    <mergeCell ref="C2170:E2170"/>
-    <mergeCell ref="C2102:E2102"/>
-    <mergeCell ref="C2119:E2119"/>
-    <mergeCell ref="C2136:E2136"/>
-    <mergeCell ref="C2153:E2153"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="C89:E89"/>
+    <mergeCell ref="C21:E21"/>
+    <mergeCell ref="C38:E38"/>
+    <mergeCell ref="C55:E55"/>
+    <mergeCell ref="C72:E72"/>
+    <mergeCell ref="C208:E208"/>
+    <mergeCell ref="C225:E225"/>
+    <mergeCell ref="C242:E242"/>
+    <mergeCell ref="C259:E259"/>
+    <mergeCell ref="C276:E276"/>
+    <mergeCell ref="C277:E277"/>
+    <mergeCell ref="C106:E106"/>
+    <mergeCell ref="C123:E123"/>
+    <mergeCell ref="C140:E140"/>
+    <mergeCell ref="C157:E157"/>
+    <mergeCell ref="C174:E174"/>
+    <mergeCell ref="C191:E191"/>
+    <mergeCell ref="C396:E396"/>
+    <mergeCell ref="C413:E413"/>
+    <mergeCell ref="C430:E430"/>
+    <mergeCell ref="C447:E447"/>
+    <mergeCell ref="C464:E464"/>
+    <mergeCell ref="C481:E481"/>
+    <mergeCell ref="C294:E294"/>
+    <mergeCell ref="C311:E311"/>
+    <mergeCell ref="C328:E328"/>
+    <mergeCell ref="C345:E345"/>
+    <mergeCell ref="C362:E362"/>
+    <mergeCell ref="C379:E379"/>
+    <mergeCell ref="C584:E584"/>
+    <mergeCell ref="C601:E601"/>
+    <mergeCell ref="C618:E618"/>
+    <mergeCell ref="C635:E635"/>
+    <mergeCell ref="C652:E652"/>
+    <mergeCell ref="C669:E669"/>
+    <mergeCell ref="C498:E498"/>
+    <mergeCell ref="C515:E515"/>
+    <mergeCell ref="C532:E532"/>
+    <mergeCell ref="C549:E549"/>
+    <mergeCell ref="C550:E550"/>
+    <mergeCell ref="C567:E567"/>
+    <mergeCell ref="C788:E788"/>
+    <mergeCell ref="C805:E805"/>
+    <mergeCell ref="C822:E822"/>
+    <mergeCell ref="C823:E823"/>
+    <mergeCell ref="C840:E840"/>
+    <mergeCell ref="C857:E857"/>
+    <mergeCell ref="C686:E686"/>
+    <mergeCell ref="C703:E703"/>
+    <mergeCell ref="C720:E720"/>
+    <mergeCell ref="C737:E737"/>
+    <mergeCell ref="C754:E754"/>
+    <mergeCell ref="C771:E771"/>
+    <mergeCell ref="C976:E976"/>
+    <mergeCell ref="C993:E993"/>
+    <mergeCell ref="C1010:E1010"/>
+    <mergeCell ref="C1027:E1027"/>
+    <mergeCell ref="C1044:E1044"/>
+    <mergeCell ref="C1061:E1061"/>
+    <mergeCell ref="C874:E874"/>
+    <mergeCell ref="C891:E891"/>
+    <mergeCell ref="C908:E908"/>
+    <mergeCell ref="C925:E925"/>
+    <mergeCell ref="C942:E942"/>
+    <mergeCell ref="C959:E959"/>
+    <mergeCell ref="C1164:E1164"/>
+    <mergeCell ref="C1181:E1181"/>
+    <mergeCell ref="C1198:E1198"/>
+    <mergeCell ref="C1215:E1215"/>
+    <mergeCell ref="C1232:E1232"/>
+    <mergeCell ref="C1249:E1249"/>
+    <mergeCell ref="C1078:E1078"/>
+    <mergeCell ref="C1095:E1095"/>
+    <mergeCell ref="C1096:E1096"/>
+    <mergeCell ref="C1113:E1113"/>
+    <mergeCell ref="C1130:E1130"/>
+    <mergeCell ref="C1147:E1147"/>
+    <mergeCell ref="C1368:E1368"/>
+    <mergeCell ref="C1369:E1369"/>
+    <mergeCell ref="C1386:E1386"/>
+    <mergeCell ref="C1403:E1403"/>
+    <mergeCell ref="C1420:E1420"/>
+    <mergeCell ref="C1437:E1437"/>
+    <mergeCell ref="C1266:E1266"/>
+    <mergeCell ref="C1283:E1283"/>
+    <mergeCell ref="C1300:E1300"/>
+    <mergeCell ref="C1317:E1317"/>
+    <mergeCell ref="C1334:E1334"/>
+    <mergeCell ref="C1351:E1351"/>
+    <mergeCell ref="C1556:E1556"/>
+    <mergeCell ref="C1573:E1573"/>
+    <mergeCell ref="C1590:E1590"/>
+    <mergeCell ref="C1607:E1607"/>
+    <mergeCell ref="C1624:E1624"/>
+    <mergeCell ref="C1641:E1641"/>
+    <mergeCell ref="C1454:E1454"/>
+    <mergeCell ref="C1471:E1471"/>
+    <mergeCell ref="C1488:E1488"/>
+    <mergeCell ref="C1505:E1505"/>
+    <mergeCell ref="C1522:E1522"/>
+    <mergeCell ref="C1539:E1539"/>
+    <mergeCell ref="C1744:E1744"/>
+    <mergeCell ref="C1761:E1761"/>
+    <mergeCell ref="C1778:E1778"/>
+    <mergeCell ref="C1795:E1795"/>
+    <mergeCell ref="C1812:E1812"/>
+    <mergeCell ref="C1829:E1829"/>
+    <mergeCell ref="C1642:E1642"/>
+    <mergeCell ref="C1659:E1659"/>
+    <mergeCell ref="C1676:E1676"/>
+    <mergeCell ref="C1693:E1693"/>
+    <mergeCell ref="C1710:E1710"/>
+    <mergeCell ref="C1727:E1727"/>
     <mergeCell ref="C1932:E1932"/>
     <mergeCell ref="C1949:E1949"/>
     <mergeCell ref="C1966:E1966"/>
@@ -25103,122 +25220,15 @@
     <mergeCell ref="C1897:E1897"/>
     <mergeCell ref="C1914:E1914"/>
     <mergeCell ref="C1915:E1915"/>
-    <mergeCell ref="C1744:E1744"/>
-    <mergeCell ref="C1761:E1761"/>
-    <mergeCell ref="C1778:E1778"/>
-    <mergeCell ref="C1795:E1795"/>
-    <mergeCell ref="C1812:E1812"/>
-    <mergeCell ref="C1829:E1829"/>
-    <mergeCell ref="C1642:E1642"/>
-    <mergeCell ref="C1659:E1659"/>
-    <mergeCell ref="C1676:E1676"/>
-    <mergeCell ref="C1693:E1693"/>
-    <mergeCell ref="C1710:E1710"/>
-    <mergeCell ref="C1727:E1727"/>
-    <mergeCell ref="C1556:E1556"/>
-    <mergeCell ref="C1573:E1573"/>
-    <mergeCell ref="C1590:E1590"/>
-    <mergeCell ref="C1607:E1607"/>
-    <mergeCell ref="C1624:E1624"/>
-    <mergeCell ref="C1641:E1641"/>
-    <mergeCell ref="C1454:E1454"/>
-    <mergeCell ref="C1471:E1471"/>
-    <mergeCell ref="C1488:E1488"/>
-    <mergeCell ref="C1505:E1505"/>
-    <mergeCell ref="C1522:E1522"/>
-    <mergeCell ref="C1539:E1539"/>
-    <mergeCell ref="C1368:E1368"/>
-    <mergeCell ref="C1369:E1369"/>
-    <mergeCell ref="C1386:E1386"/>
-    <mergeCell ref="C1403:E1403"/>
-    <mergeCell ref="C1420:E1420"/>
-    <mergeCell ref="C1437:E1437"/>
-    <mergeCell ref="C1266:E1266"/>
-    <mergeCell ref="C1283:E1283"/>
-    <mergeCell ref="C1300:E1300"/>
-    <mergeCell ref="C1317:E1317"/>
-    <mergeCell ref="C1334:E1334"/>
-    <mergeCell ref="C1351:E1351"/>
-    <mergeCell ref="C1164:E1164"/>
-    <mergeCell ref="C1181:E1181"/>
-    <mergeCell ref="C1198:E1198"/>
-    <mergeCell ref="C1215:E1215"/>
-    <mergeCell ref="C1232:E1232"/>
-    <mergeCell ref="C1249:E1249"/>
-    <mergeCell ref="C1078:E1078"/>
-    <mergeCell ref="C1095:E1095"/>
-    <mergeCell ref="C1096:E1096"/>
-    <mergeCell ref="C1113:E1113"/>
-    <mergeCell ref="C1130:E1130"/>
-    <mergeCell ref="C1147:E1147"/>
-    <mergeCell ref="C976:E976"/>
-    <mergeCell ref="C993:E993"/>
-    <mergeCell ref="C1010:E1010"/>
-    <mergeCell ref="C1027:E1027"/>
-    <mergeCell ref="C1044:E1044"/>
-    <mergeCell ref="C1061:E1061"/>
-    <mergeCell ref="C874:E874"/>
-    <mergeCell ref="C891:E891"/>
-    <mergeCell ref="C908:E908"/>
-    <mergeCell ref="C925:E925"/>
-    <mergeCell ref="C942:E942"/>
-    <mergeCell ref="C959:E959"/>
-    <mergeCell ref="C788:E788"/>
-    <mergeCell ref="C805:E805"/>
-    <mergeCell ref="C822:E822"/>
-    <mergeCell ref="C823:E823"/>
-    <mergeCell ref="C840:E840"/>
-    <mergeCell ref="C857:E857"/>
-    <mergeCell ref="C686:E686"/>
-    <mergeCell ref="C703:E703"/>
-    <mergeCell ref="C720:E720"/>
-    <mergeCell ref="C737:E737"/>
-    <mergeCell ref="C754:E754"/>
-    <mergeCell ref="C771:E771"/>
-    <mergeCell ref="C584:E584"/>
-    <mergeCell ref="C601:E601"/>
-    <mergeCell ref="C618:E618"/>
-    <mergeCell ref="C635:E635"/>
-    <mergeCell ref="C652:E652"/>
-    <mergeCell ref="C669:E669"/>
-    <mergeCell ref="C498:E498"/>
-    <mergeCell ref="C515:E515"/>
-    <mergeCell ref="C532:E532"/>
-    <mergeCell ref="C549:E549"/>
-    <mergeCell ref="C550:E550"/>
-    <mergeCell ref="C567:E567"/>
-    <mergeCell ref="C396:E396"/>
-    <mergeCell ref="C413:E413"/>
-    <mergeCell ref="C430:E430"/>
-    <mergeCell ref="C447:E447"/>
-    <mergeCell ref="C464:E464"/>
-    <mergeCell ref="C481:E481"/>
-    <mergeCell ref="C294:E294"/>
-    <mergeCell ref="C311:E311"/>
-    <mergeCell ref="C328:E328"/>
-    <mergeCell ref="C345:E345"/>
-    <mergeCell ref="C362:E362"/>
-    <mergeCell ref="C379:E379"/>
-    <mergeCell ref="C225:E225"/>
-    <mergeCell ref="C242:E242"/>
-    <mergeCell ref="C259:E259"/>
-    <mergeCell ref="C276:E276"/>
-    <mergeCell ref="C277:E277"/>
-    <mergeCell ref="C106:E106"/>
-    <mergeCell ref="C123:E123"/>
-    <mergeCell ref="C140:E140"/>
-    <mergeCell ref="C157:E157"/>
-    <mergeCell ref="C174:E174"/>
-    <mergeCell ref="C191:E191"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="C89:E89"/>
-    <mergeCell ref="C21:E21"/>
-    <mergeCell ref="C38:E38"/>
-    <mergeCell ref="C55:E55"/>
-    <mergeCell ref="C72:E72"/>
-    <mergeCell ref="C208:E208"/>
+    <mergeCell ref="C2034:E2034"/>
+    <mergeCell ref="C2051:E2051"/>
+    <mergeCell ref="C2068:E2068"/>
+    <mergeCell ref="C2085:E2085"/>
+    <mergeCell ref="C2170:E2170"/>
+    <mergeCell ref="C2102:E2102"/>
+    <mergeCell ref="C2119:E2119"/>
+    <mergeCell ref="C2136:E2136"/>
+    <mergeCell ref="C2153:E2153"/>
   </mergeCells>
   <phoneticPr fontId="14" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -25245,51 +25255,51 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="24" thickBot="1">
-      <c r="A1" s="200" t="s">
+      <c r="A1" s="201" t="s">
         <v>156</v>
       </c>
-      <c r="B1" s="200"/>
-      <c r="C1" s="200"/>
-      <c r="D1" s="200"/>
-      <c r="E1" s="200"/>
-      <c r="F1" s="200"/>
-      <c r="G1" s="200"/>
-      <c r="H1" s="200"/>
-      <c r="I1" s="200"/>
-      <c r="J1" s="200"/>
-      <c r="K1" s="200"/>
-      <c r="L1" s="200"/>
+      <c r="B1" s="201"/>
+      <c r="C1" s="201"/>
+      <c r="D1" s="201"/>
+      <c r="E1" s="201"/>
+      <c r="F1" s="201"/>
+      <c r="G1" s="201"/>
+      <c r="H1" s="201"/>
+      <c r="I1" s="201"/>
+      <c r="J1" s="201"/>
+      <c r="K1" s="201"/>
+      <c r="L1" s="201"/>
     </row>
     <row r="2" spans="1:12" ht="18.75" thickBot="1">
-      <c r="A2" s="197" t="s">
+      <c r="A2" s="198" t="s">
         <v>157</v>
       </c>
-      <c r="B2" s="198"/>
-      <c r="C2" s="198"/>
-      <c r="D2" s="198"/>
-      <c r="E2" s="198"/>
-      <c r="F2" s="198"/>
-      <c r="G2" s="198"/>
-      <c r="H2" s="198"/>
-      <c r="I2" s="198"/>
-      <c r="J2" s="198"/>
-      <c r="K2" s="198"/>
-      <c r="L2" s="199"/>
+      <c r="B2" s="199"/>
+      <c r="C2" s="199"/>
+      <c r="D2" s="199"/>
+      <c r="E2" s="199"/>
+      <c r="F2" s="199"/>
+      <c r="G2" s="199"/>
+      <c r="H2" s="199"/>
+      <c r="I2" s="199"/>
+      <c r="J2" s="199"/>
+      <c r="K2" s="199"/>
+      <c r="L2" s="200"/>
     </row>
     <row r="3" spans="1:12" s="31" customFormat="1" ht="16.5" customHeight="1" thickBot="1">
-      <c r="A3" s="194" t="s">
+      <c r="A3" s="195" t="s">
         <v>158</v>
       </c>
-      <c r="B3" s="195"/>
-      <c r="C3" s="195"/>
-      <c r="D3" s="195"/>
-      <c r="E3" s="195"/>
-      <c r="F3" s="195"/>
-      <c r="G3" s="195"/>
-      <c r="H3" s="195"/>
-      <c r="I3" s="195"/>
-      <c r="J3" s="195"/>
-      <c r="K3" s="196"/>
+      <c r="B3" s="196"/>
+      <c r="C3" s="196"/>
+      <c r="D3" s="196"/>
+      <c r="E3" s="196"/>
+      <c r="F3" s="196"/>
+      <c r="G3" s="196"/>
+      <c r="H3" s="196"/>
+      <c r="I3" s="196"/>
+      <c r="J3" s="196"/>
+      <c r="K3" s="197"/>
     </row>
     <row r="4" spans="1:12" s="27" customFormat="1">
       <c r="A4" s="28" t="s">
@@ -25506,19 +25516,19 @@
       <c r="K19" s="2"/>
     </row>
     <row r="20" spans="1:11" ht="18" customHeight="1" thickBot="1">
-      <c r="A20" s="194" t="s">
+      <c r="A20" s="195" t="s">
         <v>166</v>
       </c>
-      <c r="B20" s="195"/>
-      <c r="C20" s="195"/>
-      <c r="D20" s="195"/>
-      <c r="E20" s="195"/>
-      <c r="F20" s="195"/>
-      <c r="G20" s="195"/>
-      <c r="H20" s="195"/>
-      <c r="I20" s="195"/>
-      <c r="J20" s="195"/>
-      <c r="K20" s="196"/>
+      <c r="B20" s="196"/>
+      <c r="C20" s="196"/>
+      <c r="D20" s="196"/>
+      <c r="E20" s="196"/>
+      <c r="F20" s="196"/>
+      <c r="G20" s="196"/>
+      <c r="H20" s="196"/>
+      <c r="I20" s="196"/>
+      <c r="J20" s="196"/>
+      <c r="K20" s="197"/>
     </row>
     <row r="21" spans="1:11">
       <c r="A21" s="28" t="s">
@@ -25735,19 +25745,19 @@
       <c r="K36" s="2"/>
     </row>
     <row r="37" spans="1:11" ht="18" customHeight="1" thickBot="1">
-      <c r="A37" s="194" t="s">
+      <c r="A37" s="195" t="s">
         <v>167</v>
       </c>
-      <c r="B37" s="195"/>
-      <c r="C37" s="195"/>
-      <c r="D37" s="195"/>
-      <c r="E37" s="195"/>
-      <c r="F37" s="195"/>
-      <c r="G37" s="195"/>
-      <c r="H37" s="195"/>
-      <c r="I37" s="195"/>
-      <c r="J37" s="195"/>
-      <c r="K37" s="196"/>
+      <c r="B37" s="196"/>
+      <c r="C37" s="196"/>
+      <c r="D37" s="196"/>
+      <c r="E37" s="196"/>
+      <c r="F37" s="196"/>
+      <c r="G37" s="196"/>
+      <c r="H37" s="196"/>
+      <c r="I37" s="196"/>
+      <c r="J37" s="196"/>
+      <c r="K37" s="197"/>
     </row>
     <row r="38" spans="1:11">
       <c r="A38" s="28" t="s">
@@ -26005,28 +26015,28 @@
       </c>
     </row>
     <row r="3" spans="1:1">
-      <c r="A3" s="201"/>
+      <c r="A3" s="202"/>
     </row>
     <row r="4" spans="1:1">
-      <c r="A4" s="202"/>
+      <c r="A4" s="203"/>
     </row>
     <row r="5" spans="1:1">
-      <c r="A5" s="202"/>
+      <c r="A5" s="203"/>
     </row>
     <row r="6" spans="1:1">
-      <c r="A6" s="202"/>
+      <c r="A6" s="203"/>
     </row>
     <row r="7" spans="1:1">
-      <c r="A7" s="202"/>
+      <c r="A7" s="203"/>
     </row>
     <row r="8" spans="1:1">
-      <c r="A8" s="202"/>
+      <c r="A8" s="203"/>
     </row>
     <row r="9" spans="1:1">
-      <c r="A9" s="202"/>
+      <c r="A9" s="203"/>
     </row>
     <row r="10" spans="1:1" ht="13.5" thickBot="1">
-      <c r="A10" s="203"/>
+      <c r="A10" s="204"/>
     </row>
     <row r="11" spans="1:1" ht="27" customHeight="1">
       <c r="A11" s="22" t="s">
@@ -26209,10 +26219,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="4" customFormat="1" ht="25.5" customHeight="1" thickBot="1">
-      <c r="B1" s="204" t="s">
+      <c r="B1" s="205" t="s">
         <v>162</v>
       </c>
-      <c r="C1" s="205"/>
+      <c r="C1" s="206"/>
       <c r="D1" s="92"/>
       <c r="E1" s="32"/>
     </row>
@@ -26223,7 +26233,7 @@
       <c r="E2" s="119"/>
     </row>
     <row r="3" spans="1:5" ht="12.75" customHeight="1">
-      <c r="A3" s="206" t="s">
+      <c r="A3" s="207" t="s">
         <v>202</v>
       </c>
       <c r="B3" s="131" t="s">
@@ -26237,7 +26247,7 @@
       <c r="E3" s="5"/>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="207"/>
+      <c r="A4" s="208"/>
       <c r="B4" s="128" t="s">
         <v>159</v>
       </c>
@@ -26249,7 +26259,7 @@
       <c r="E4" s="5"/>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="207"/>
+      <c r="A5" s="208"/>
       <c r="B5" s="128" t="s">
         <v>160</v>
       </c>
@@ -26258,7 +26268,7 @@
       <c r="E5" s="5"/>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="207"/>
+      <c r="A6" s="208"/>
       <c r="B6" s="139" t="s">
         <v>204</v>
       </c>
@@ -26270,7 +26280,7 @@
       <c r="E6" s="5"/>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="207"/>
+      <c r="A7" s="208"/>
       <c r="B7" s="128" t="s">
         <v>171</v>
       </c>
@@ -26282,7 +26292,7 @@
       <c r="E7" s="5"/>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="207"/>
+      <c r="A8" s="208"/>
       <c r="B8" s="128" t="s">
         <v>172</v>
       </c>
@@ -26291,7 +26301,7 @@
       <c r="E8" s="5"/>
     </row>
     <row r="9" spans="1:5" ht="13.5" thickBot="1">
-      <c r="A9" s="208"/>
+      <c r="A9" s="209"/>
       <c r="B9" s="136" t="s">
         <v>161</v>
       </c>
@@ -26306,7 +26316,7 @@
       <c r="E10" s="94"/>
     </row>
     <row r="11" spans="1:5" ht="19.5" customHeight="1">
-      <c r="A11" s="206" t="s">
+      <c r="A11" s="207" t="s">
         <v>203</v>
       </c>
       <c r="B11" s="131" t="s">
@@ -26320,7 +26330,7 @@
       <c r="E11" s="5"/>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="207"/>
+      <c r="A12" s="208"/>
       <c r="B12" s="128" t="s">
         <v>159</v>
       </c>
@@ -26332,7 +26342,7 @@
       <c r="E12" s="5"/>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" s="207"/>
+      <c r="A13" s="208"/>
       <c r="B13" s="128" t="s">
         <v>160</v>
       </c>
@@ -26341,7 +26351,7 @@
       <c r="E13" s="5"/>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="207"/>
+      <c r="A14" s="208"/>
       <c r="B14" s="139" t="s">
         <v>204</v>
       </c>
@@ -26353,7 +26363,7 @@
       <c r="E14" s="5"/>
     </row>
     <row r="15" spans="1:5">
-      <c r="A15" s="207"/>
+      <c r="A15" s="208"/>
       <c r="B15" s="128" t="s">
         <v>171</v>
       </c>
@@ -26365,7 +26375,7 @@
       <c r="E15" s="5"/>
     </row>
     <row r="16" spans="1:5">
-      <c r="A16" s="207"/>
+      <c r="A16" s="208"/>
       <c r="B16" s="128" t="s">
         <v>172</v>
       </c>
@@ -26374,7 +26384,7 @@
       <c r="E16" s="5"/>
     </row>
     <row r="17" spans="1:5" ht="13.5" thickBot="1">
-      <c r="A17" s="208"/>
+      <c r="A17" s="209"/>
       <c r="B17" s="136" t="s">
         <v>161</v>
       </c>
@@ -26389,7 +26399,7 @@
       <c r="E18" s="94"/>
     </row>
     <row r="19" spans="1:5" collapsed="1">
-      <c r="A19" s="206" t="s">
+      <c r="A19" s="207" t="s">
         <v>203</v>
       </c>
       <c r="B19" s="131" t="s">
@@ -26398,7 +26408,7 @@
       <c r="C19" s="130"/>
     </row>
     <row r="20" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A20" s="207"/>
+      <c r="A20" s="208"/>
       <c r="B20" s="128" t="s">
         <v>159</v>
       </c>
@@ -26408,14 +26418,14 @@
       </c>
     </row>
     <row r="21" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A21" s="207"/>
+      <c r="A21" s="208"/>
       <c r="B21" s="128" t="s">
         <v>160</v>
       </c>
       <c r="C21" s="133"/>
     </row>
     <row r="22" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A22" s="207"/>
+      <c r="A22" s="208"/>
       <c r="B22" s="139" t="s">
         <v>204</v>
       </c>
@@ -26425,7 +26435,7 @@
       </c>
     </row>
     <row r="23" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A23" s="207"/>
+      <c r="A23" s="208"/>
       <c r="B23" s="128" t="s">
         <v>171</v>
       </c>
@@ -26435,14 +26445,14 @@
       </c>
     </row>
     <row r="24" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A24" s="207"/>
+      <c r="A24" s="208"/>
       <c r="B24" s="128" t="s">
         <v>172</v>
       </c>
       <c r="C24" s="132"/>
     </row>
     <row r="25" spans="1:5" ht="13.5" thickBot="1">
-      <c r="A25" s="208"/>
+      <c r="A25" s="209"/>
       <c r="B25" s="136" t="s">
         <v>161</v>
       </c>
@@ -26486,17 +26496,17 @@
       <c r="E1" s="5"/>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="225" t="s">
+      <c r="A2" s="216" t="s">
         <v>183</v>
       </c>
-      <c r="B2" s="226"/>
+      <c r="B2" s="217"/>
       <c r="C2" s="120"/>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="227" t="s">
+      <c r="A3" s="218" t="s">
         <v>185</v>
       </c>
-      <c r="B3" s="226"/>
+      <c r="B3" s="217"/>
       <c r="C3" s="120"/>
     </row>
     <row r="4" spans="1:5">
@@ -26512,115 +26522,128 @@
       <c r="C5" s="120"/>
     </row>
     <row r="7" spans="1:5" ht="18.75">
-      <c r="A7" s="213" t="s">
+      <c r="A7" s="227" t="s">
         <v>186</v>
       </c>
-      <c r="B7" s="214"/>
+      <c r="B7" s="228"/>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="120"/>
       <c r="B8" s="9"/>
     </row>
     <row r="9" spans="1:5" ht="39" customHeight="1">
-      <c r="A9" s="215" t="s">
+      <c r="A9" s="225" t="s">
         <v>187</v>
       </c>
-      <c r="B9" s="216"/>
+      <c r="B9" s="226"/>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="217"/>
-      <c r="B10" s="218"/>
+      <c r="A10" s="212"/>
+      <c r="B10" s="213"/>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="209" t="s">
+      <c r="A11" s="214" t="s">
         <v>188</v>
       </c>
-      <c r="B11" s="210"/>
+      <c r="B11" s="215"/>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="209" t="s">
+      <c r="A12" s="214" t="s">
         <v>189</v>
       </c>
-      <c r="B12" s="210"/>
+      <c r="B12" s="215"/>
     </row>
     <row r="13" spans="1:5" ht="43.5" customHeight="1">
-      <c r="A13" s="209" t="s">
+      <c r="A13" s="214" t="s">
         <v>190</v>
       </c>
-      <c r="B13" s="210"/>
+      <c r="B13" s="215"/>
     </row>
     <row r="14" spans="1:5" ht="19.5" customHeight="1">
-      <c r="A14" s="209" t="s">
+      <c r="A14" s="214" t="s">
         <v>191</v>
       </c>
-      <c r="B14" s="210"/>
+      <c r="B14" s="215"/>
     </row>
     <row r="15" spans="1:5" ht="18" customHeight="1">
-      <c r="A15" s="209" t="s">
+      <c r="A15" s="214" t="s">
         <v>192</v>
       </c>
-      <c r="B15" s="210"/>
+      <c r="B15" s="215"/>
     </row>
     <row r="16" spans="1:5" ht="21" customHeight="1">
-      <c r="A16" s="209" t="s">
+      <c r="A16" s="214" t="s">
         <v>193</v>
       </c>
-      <c r="B16" s="210"/>
+      <c r="B16" s="215"/>
     </row>
     <row r="17" spans="1:2" ht="48.75" customHeight="1">
-      <c r="A17" s="211" t="s">
+      <c r="A17" s="210" t="s">
         <v>195</v>
       </c>
-      <c r="B17" s="212"/>
+      <c r="B17" s="211"/>
     </row>
     <row r="19" spans="1:2" ht="18.75">
-      <c r="A19" s="213" t="s">
+      <c r="A19" s="227" t="s">
         <v>197</v>
       </c>
-      <c r="B19" s="214"/>
+      <c r="B19" s="228"/>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="120"/>
       <c r="B20" s="9"/>
     </row>
     <row r="21" spans="1:2">
-      <c r="A21" s="215" t="s">
+      <c r="A21" s="225" t="s">
         <v>198</v>
       </c>
-      <c r="B21" s="216"/>
+      <c r="B21" s="226"/>
     </row>
     <row r="22" spans="1:2">
-      <c r="A22" s="217"/>
-      <c r="B22" s="218"/>
+      <c r="A22" s="212"/>
+      <c r="B22" s="213"/>
     </row>
     <row r="23" spans="1:2">
-      <c r="A23" s="209" t="s">
+      <c r="A23" s="214" t="s">
         <v>199</v>
       </c>
-      <c r="B23" s="210"/>
+      <c r="B23" s="215"/>
     </row>
     <row r="24" spans="1:2">
-      <c r="A24" s="209"/>
-      <c r="B24" s="210"/>
+      <c r="A24" s="214"/>
+      <c r="B24" s="215"/>
     </row>
     <row r="25" spans="1:2">
-      <c r="A25" s="209" t="s">
+      <c r="A25" s="214" t="s">
         <v>200</v>
       </c>
-      <c r="B25" s="210"/>
+      <c r="B25" s="215"/>
     </row>
     <row r="26" spans="1:2">
-      <c r="A26" s="209" t="s">
+      <c r="A26" s="214" t="s">
         <v>201</v>
       </c>
-      <c r="B26" s="210"/>
+      <c r="B26" s="215"/>
     </row>
     <row r="27" spans="1:2">
-      <c r="A27" s="211"/>
-      <c r="B27" s="212"/>
+      <c r="A27" s="210"/>
+      <c r="B27" s="211"/>
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A7:B7"/>
     <mergeCell ref="A17:B17"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
@@ -26631,19 +26654,6 @@
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="A14:B14"/>
     <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A24:B24"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A3" r:id="rId1"/>

</xml_diff>

<commit_message>
Tempo - Jungle Stages 1 & 2 done.  Time for the boss fight!
</commit_message>
<xml_diff>
--- a/trunk/Tempo/Tempo.xlsx
+++ b/trunk/Tempo/Tempo.xlsx
@@ -2264,29 +2264,29 @@
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="26" fillId="13" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="27" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="26" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="27" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="24" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="25" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="22" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="23" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="15" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="22" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="23" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="24" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="25" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="26" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="27" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="26" fillId="13" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="27" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="17" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="17" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="17" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -2322,20 +2322,34 @@
     <xf numFmtId="0" fontId="56" fillId="22" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="53" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="54" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="54" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="50" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="4"/>
     </xf>
@@ -2345,20 +2359,6 @@
     <xf numFmtId="0" fontId="51" fillId="0" borderId="33" xfId="3" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" indent="4"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="52" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="52" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="54" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="54" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="53" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Accent1" xfId="2" builtinId="29"/>
@@ -2669,8 +2669,8 @@
   <dimension ref="A1:K167"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A96" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C112" sqref="C112"/>
+      <pane ySplit="6" topLeftCell="A102" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C116" sqref="C116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" outlineLevelRow="2"/>
@@ -4616,20 +4616,24 @@
       <c r="B113" s="152" t="s">
         <v>253</v>
       </c>
-      <c r="C113" s="101"/>
+      <c r="C113" s="101">
+        <v>41008</v>
+      </c>
       <c r="D113" s="101">
         <v>52785</v>
       </c>
       <c r="E113" s="123">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>11777</v>
       </c>
       <c r="F113" s="105"/>
     </row>
     <row r="114" spans="1:9" ht="15" outlineLevel="1">
       <c r="A114" s="165"/>
       <c r="B114" s="100"/>
-      <c r="C114" s="101"/>
+      <c r="C114" s="101">
+        <v>41008</v>
+      </c>
       <c r="D114" s="101"/>
       <c r="E114" s="123">
         <f t="shared" si="8"/>
@@ -4642,13 +4646,15 @@
       <c r="B115" s="152" t="s">
         <v>254</v>
       </c>
-      <c r="C115" s="101"/>
+      <c r="C115" s="101">
+        <v>41570</v>
+      </c>
       <c r="D115" s="101">
         <v>53409</v>
       </c>
       <c r="E115" s="123">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>11839</v>
       </c>
       <c r="F115" s="105"/>
     </row>
@@ -5357,6 +5363,11 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="A152:A166"/>
+    <mergeCell ref="A123:A132"/>
+    <mergeCell ref="A93:A107"/>
+    <mergeCell ref="A135:A149"/>
+    <mergeCell ref="A110:A120"/>
     <mergeCell ref="A43:A70"/>
     <mergeCell ref="A73:A90"/>
     <mergeCell ref="C5:D5"/>
@@ -5366,11 +5377,6 @@
     <mergeCell ref="A8:A18"/>
     <mergeCell ref="A21:A40"/>
     <mergeCell ref="C4:E4"/>
-    <mergeCell ref="A152:A166"/>
-    <mergeCell ref="A123:A132"/>
-    <mergeCell ref="A93:A107"/>
-    <mergeCell ref="A135:A149"/>
-    <mergeCell ref="A110:A120"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -5402,13 +5408,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="26.25" customHeight="1">
-      <c r="A1" s="192" t="s">
+      <c r="A1" s="174" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="192"/>
-      <c r="C1" s="192"/>
-      <c r="D1" s="192"/>
-      <c r="E1" s="192"/>
+      <c r="B1" s="174"/>
+      <c r="C1" s="174"/>
+      <c r="D1" s="174"/>
+      <c r="E1" s="174"/>
       <c r="F1" s="7"/>
       <c r="G1" s="5"/>
       <c r="H1" s="5"/>
@@ -5438,18 +5444,18 @@
         <v>8</v>
       </c>
       <c r="B3" s="36"/>
-      <c r="C3" s="193"/>
-      <c r="D3" s="194"/>
-      <c r="E3" s="194"/>
+      <c r="C3" s="175"/>
+      <c r="D3" s="176"/>
+      <c r="E3" s="176"/>
     </row>
     <row r="4" spans="1:8" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A4" s="46" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="87"/>
-      <c r="C4" s="174"/>
-      <c r="D4" s="175"/>
-      <c r="E4" s="175"/>
+      <c r="C4" s="177"/>
+      <c r="D4" s="178"/>
+      <c r="E4" s="178"/>
       <c r="F4" s="6"/>
     </row>
     <row r="5" spans="1:8" hidden="1" outlineLevel="2">
@@ -5601,9 +5607,9 @@
         <v>9</v>
       </c>
       <c r="B21" s="90"/>
-      <c r="C21" s="176"/>
-      <c r="D21" s="177"/>
-      <c r="E21" s="177"/>
+      <c r="C21" s="179"/>
+      <c r="D21" s="180"/>
+      <c r="E21" s="180"/>
     </row>
     <row r="22" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A22" s="47">
@@ -5754,9 +5760,9 @@
         <v>10</v>
       </c>
       <c r="B38" s="87"/>
-      <c r="C38" s="174"/>
-      <c r="D38" s="175"/>
-      <c r="E38" s="175"/>
+      <c r="C38" s="177"/>
+      <c r="D38" s="178"/>
+      <c r="E38" s="178"/>
     </row>
     <row r="39" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A39" s="47">
@@ -5907,9 +5913,9 @@
         <v>11</v>
       </c>
       <c r="B55" s="87"/>
-      <c r="C55" s="174"/>
-      <c r="D55" s="175"/>
-      <c r="E55" s="175"/>
+      <c r="C55" s="177"/>
+      <c r="D55" s="178"/>
+      <c r="E55" s="178"/>
     </row>
     <row r="56" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A56" s="47">
@@ -6060,9 +6066,9 @@
         <v>12</v>
       </c>
       <c r="B72" s="87"/>
-      <c r="C72" s="174"/>
-      <c r="D72" s="175"/>
-      <c r="E72" s="175"/>
+      <c r="C72" s="177"/>
+      <c r="D72" s="178"/>
+      <c r="E72" s="178"/>
     </row>
     <row r="73" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A73" s="47">
@@ -6213,9 +6219,9 @@
         <v>13</v>
       </c>
       <c r="B89" s="87"/>
-      <c r="C89" s="174"/>
-      <c r="D89" s="175"/>
-      <c r="E89" s="175"/>
+      <c r="C89" s="177"/>
+      <c r="D89" s="178"/>
+      <c r="E89" s="178"/>
     </row>
     <row r="90" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A90" s="47">
@@ -6366,9 +6372,9 @@
         <v>14</v>
       </c>
       <c r="B106" s="87"/>
-      <c r="C106" s="174"/>
-      <c r="D106" s="175"/>
-      <c r="E106" s="175"/>
+      <c r="C106" s="177"/>
+      <c r="D106" s="178"/>
+      <c r="E106" s="178"/>
     </row>
     <row r="107" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A107" s="47">
@@ -6519,9 +6525,9 @@
         <v>15</v>
       </c>
       <c r="B123" s="87"/>
-      <c r="C123" s="174"/>
-      <c r="D123" s="175"/>
-      <c r="E123" s="175"/>
+      <c r="C123" s="177"/>
+      <c r="D123" s="178"/>
+      <c r="E123" s="178"/>
     </row>
     <row r="124" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A124" s="47">
@@ -6672,9 +6678,9 @@
         <v>16</v>
       </c>
       <c r="B140" s="87"/>
-      <c r="C140" s="174"/>
-      <c r="D140" s="175"/>
-      <c r="E140" s="175"/>
+      <c r="C140" s="177"/>
+      <c r="D140" s="178"/>
+      <c r="E140" s="178"/>
     </row>
     <row r="141" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A141" s="47">
@@ -6825,9 +6831,9 @@
         <v>17</v>
       </c>
       <c r="B157" s="87"/>
-      <c r="C157" s="174"/>
-      <c r="D157" s="175"/>
-      <c r="E157" s="175"/>
+      <c r="C157" s="177"/>
+      <c r="D157" s="178"/>
+      <c r="E157" s="178"/>
     </row>
     <row r="158" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A158" s="47">
@@ -6978,9 +6984,9 @@
         <v>18</v>
       </c>
       <c r="B174" s="87"/>
-      <c r="C174" s="174"/>
-      <c r="D174" s="175"/>
-      <c r="E174" s="175"/>
+      <c r="C174" s="177"/>
+      <c r="D174" s="178"/>
+      <c r="E174" s="178"/>
     </row>
     <row r="175" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A175" s="47">
@@ -7131,9 +7137,9 @@
         <v>19</v>
       </c>
       <c r="B191" s="87"/>
-      <c r="C191" s="174"/>
-      <c r="D191" s="175"/>
-      <c r="E191" s="175"/>
+      <c r="C191" s="177"/>
+      <c r="D191" s="178"/>
+      <c r="E191" s="178"/>
     </row>
     <row r="192" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A192" s="47">
@@ -7284,9 +7290,9 @@
         <v>20</v>
       </c>
       <c r="B208" s="87"/>
-      <c r="C208" s="174"/>
-      <c r="D208" s="175"/>
-      <c r="E208" s="175"/>
+      <c r="C208" s="177"/>
+      <c r="D208" s="178"/>
+      <c r="E208" s="178"/>
     </row>
     <row r="209" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A209" s="47">
@@ -7437,9 +7443,9 @@
         <v>21</v>
       </c>
       <c r="B225" s="87"/>
-      <c r="C225" s="174"/>
-      <c r="D225" s="175"/>
-      <c r="E225" s="175"/>
+      <c r="C225" s="177"/>
+      <c r="D225" s="178"/>
+      <c r="E225" s="178"/>
     </row>
     <row r="226" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A226" s="47">
@@ -7590,9 +7596,9 @@
         <v>22</v>
       </c>
       <c r="B242" s="87"/>
-      <c r="C242" s="174"/>
-      <c r="D242" s="175"/>
-      <c r="E242" s="175"/>
+      <c r="C242" s="177"/>
+      <c r="D242" s="178"/>
+      <c r="E242" s="178"/>
     </row>
     <row r="243" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A243" s="47">
@@ -7743,9 +7749,9 @@
         <v>23</v>
       </c>
       <c r="B259" s="87"/>
-      <c r="C259" s="174"/>
-      <c r="D259" s="175"/>
-      <c r="E259" s="175"/>
+      <c r="C259" s="177"/>
+      <c r="D259" s="178"/>
+      <c r="E259" s="178"/>
     </row>
     <row r="260" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A260" s="47">
@@ -7896,18 +7902,18 @@
         <v>24</v>
       </c>
       <c r="B276" s="37"/>
-      <c r="C276" s="190"/>
-      <c r="D276" s="191"/>
-      <c r="E276" s="191"/>
+      <c r="C276" s="181"/>
+      <c r="D276" s="182"/>
+      <c r="E276" s="182"/>
     </row>
     <row r="277" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A277" s="51" t="s">
         <v>25</v>
       </c>
       <c r="B277" s="87"/>
-      <c r="C277" s="174"/>
-      <c r="D277" s="175"/>
-      <c r="E277" s="175"/>
+      <c r="C277" s="177"/>
+      <c r="D277" s="178"/>
+      <c r="E277" s="178"/>
     </row>
     <row r="278" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A278" s="52">
@@ -8058,9 +8064,9 @@
         <v>26</v>
       </c>
       <c r="B294" s="90"/>
-      <c r="C294" s="176"/>
-      <c r="D294" s="177"/>
-      <c r="E294" s="177"/>
+      <c r="C294" s="179"/>
+      <c r="D294" s="180"/>
+      <c r="E294" s="180"/>
     </row>
     <row r="295" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A295" s="52">
@@ -8211,9 +8217,9 @@
         <v>27</v>
       </c>
       <c r="B311" s="87"/>
-      <c r="C311" s="174"/>
-      <c r="D311" s="175"/>
-      <c r="E311" s="175"/>
+      <c r="C311" s="177"/>
+      <c r="D311" s="178"/>
+      <c r="E311" s="178"/>
     </row>
     <row r="312" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A312" s="52">
@@ -8364,9 +8370,9 @@
         <v>28</v>
       </c>
       <c r="B328" s="87"/>
-      <c r="C328" s="174"/>
-      <c r="D328" s="175"/>
-      <c r="E328" s="175"/>
+      <c r="C328" s="177"/>
+      <c r="D328" s="178"/>
+      <c r="E328" s="178"/>
     </row>
     <row r="329" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A329" s="52">
@@ -8517,9 +8523,9 @@
         <v>29</v>
       </c>
       <c r="B345" s="87"/>
-      <c r="C345" s="174"/>
-      <c r="D345" s="175"/>
-      <c r="E345" s="175"/>
+      <c r="C345" s="177"/>
+      <c r="D345" s="178"/>
+      <c r="E345" s="178"/>
     </row>
     <row r="346" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A346" s="52">
@@ -8670,9 +8676,9 @@
         <v>30</v>
       </c>
       <c r="B362" s="87"/>
-      <c r="C362" s="174"/>
-      <c r="D362" s="175"/>
-      <c r="E362" s="175"/>
+      <c r="C362" s="177"/>
+      <c r="D362" s="178"/>
+      <c r="E362" s="178"/>
     </row>
     <row r="363" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A363" s="52">
@@ -8823,9 +8829,9 @@
         <v>31</v>
       </c>
       <c r="B379" s="87"/>
-      <c r="C379" s="174"/>
-      <c r="D379" s="175"/>
-      <c r="E379" s="175"/>
+      <c r="C379" s="177"/>
+      <c r="D379" s="178"/>
+      <c r="E379" s="178"/>
     </row>
     <row r="380" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A380" s="52">
@@ -8976,9 +8982,9 @@
         <v>32</v>
       </c>
       <c r="B396" s="87"/>
-      <c r="C396" s="174"/>
-      <c r="D396" s="175"/>
-      <c r="E396" s="175"/>
+      <c r="C396" s="177"/>
+      <c r="D396" s="178"/>
+      <c r="E396" s="178"/>
     </row>
     <row r="397" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A397" s="52">
@@ -9129,9 +9135,9 @@
         <v>33</v>
       </c>
       <c r="B413" s="87"/>
-      <c r="C413" s="174"/>
-      <c r="D413" s="175"/>
-      <c r="E413" s="175"/>
+      <c r="C413" s="177"/>
+      <c r="D413" s="178"/>
+      <c r="E413" s="178"/>
     </row>
     <row r="414" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A414" s="52">
@@ -9282,9 +9288,9 @@
         <v>34</v>
       </c>
       <c r="B430" s="87"/>
-      <c r="C430" s="174"/>
-      <c r="D430" s="175"/>
-      <c r="E430" s="175"/>
+      <c r="C430" s="177"/>
+      <c r="D430" s="178"/>
+      <c r="E430" s="178"/>
     </row>
     <row r="431" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A431" s="52">
@@ -9435,9 +9441,9 @@
         <v>35</v>
       </c>
       <c r="B447" s="87"/>
-      <c r="C447" s="174"/>
-      <c r="D447" s="175"/>
-      <c r="E447" s="175"/>
+      <c r="C447" s="177"/>
+      <c r="D447" s="178"/>
+      <c r="E447" s="178"/>
     </row>
     <row r="448" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A448" s="52">
@@ -9588,9 +9594,9 @@
         <v>36</v>
       </c>
       <c r="B464" s="87"/>
-      <c r="C464" s="174"/>
-      <c r="D464" s="175"/>
-      <c r="E464" s="175"/>
+      <c r="C464" s="177"/>
+      <c r="D464" s="178"/>
+      <c r="E464" s="178"/>
     </row>
     <row r="465" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A465" s="52">
@@ -9741,9 +9747,9 @@
         <v>37</v>
       </c>
       <c r="B481" s="87"/>
-      <c r="C481" s="174"/>
-      <c r="D481" s="175"/>
-      <c r="E481" s="175"/>
+      <c r="C481" s="177"/>
+      <c r="D481" s="178"/>
+      <c r="E481" s="178"/>
     </row>
     <row r="482" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A482" s="52">
@@ -9894,9 +9900,9 @@
         <v>38</v>
       </c>
       <c r="B498" s="87"/>
-      <c r="C498" s="174"/>
-      <c r="D498" s="175"/>
-      <c r="E498" s="175"/>
+      <c r="C498" s="177"/>
+      <c r="D498" s="178"/>
+      <c r="E498" s="178"/>
     </row>
     <row r="499" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A499" s="52">
@@ -10047,9 +10053,9 @@
         <v>39</v>
       </c>
       <c r="B515" s="87"/>
-      <c r="C515" s="174"/>
-      <c r="D515" s="175"/>
-      <c r="E515" s="175"/>
+      <c r="C515" s="177"/>
+      <c r="D515" s="178"/>
+      <c r="E515" s="178"/>
     </row>
     <row r="516" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A516" s="52">
@@ -10200,9 +10206,9 @@
         <v>40</v>
       </c>
       <c r="B532" s="87"/>
-      <c r="C532" s="174"/>
-      <c r="D532" s="175"/>
-      <c r="E532" s="175"/>
+      <c r="C532" s="177"/>
+      <c r="D532" s="178"/>
+      <c r="E532" s="178"/>
     </row>
     <row r="533" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A533" s="55">
@@ -10353,18 +10359,18 @@
         <v>50</v>
       </c>
       <c r="B549" s="38"/>
-      <c r="C549" s="188"/>
-      <c r="D549" s="189"/>
-      <c r="E549" s="189"/>
+      <c r="C549" s="183"/>
+      <c r="D549" s="184"/>
+      <c r="E549" s="184"/>
     </row>
     <row r="550" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A550" s="58" t="s">
         <v>51</v>
       </c>
       <c r="B550" s="87"/>
-      <c r="C550" s="174"/>
-      <c r="D550" s="175"/>
-      <c r="E550" s="175"/>
+      <c r="C550" s="177"/>
+      <c r="D550" s="178"/>
+      <c r="E550" s="178"/>
     </row>
     <row r="551" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A551" s="59">
@@ -10515,9 +10521,9 @@
         <v>52</v>
       </c>
       <c r="B567" s="90"/>
-      <c r="C567" s="176"/>
-      <c r="D567" s="177"/>
-      <c r="E567" s="177"/>
+      <c r="C567" s="179"/>
+      <c r="D567" s="180"/>
+      <c r="E567" s="180"/>
     </row>
     <row r="568" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A568" s="59">
@@ -10668,9 +10674,9 @@
         <v>53</v>
       </c>
       <c r="B584" s="87"/>
-      <c r="C584" s="174"/>
-      <c r="D584" s="175"/>
-      <c r="E584" s="175"/>
+      <c r="C584" s="177"/>
+      <c r="D584" s="178"/>
+      <c r="E584" s="178"/>
     </row>
     <row r="585" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A585" s="59">
@@ -10821,9 +10827,9 @@
         <v>54</v>
       </c>
       <c r="B601" s="87"/>
-      <c r="C601" s="174"/>
-      <c r="D601" s="175"/>
-      <c r="E601" s="175"/>
+      <c r="C601" s="177"/>
+      <c r="D601" s="178"/>
+      <c r="E601" s="178"/>
     </row>
     <row r="602" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A602" s="59">
@@ -10974,9 +10980,9 @@
         <v>55</v>
       </c>
       <c r="B618" s="87"/>
-      <c r="C618" s="174"/>
-      <c r="D618" s="175"/>
-      <c r="E618" s="175"/>
+      <c r="C618" s="177"/>
+      <c r="D618" s="178"/>
+      <c r="E618" s="178"/>
     </row>
     <row r="619" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A619" s="59">
@@ -11127,9 +11133,9 @@
         <v>56</v>
       </c>
       <c r="B635" s="87"/>
-      <c r="C635" s="174"/>
-      <c r="D635" s="175"/>
-      <c r="E635" s="175"/>
+      <c r="C635" s="177"/>
+      <c r="D635" s="178"/>
+      <c r="E635" s="178"/>
     </row>
     <row r="636" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A636" s="59">
@@ -11280,9 +11286,9 @@
         <v>57</v>
       </c>
       <c r="B652" s="87"/>
-      <c r="C652" s="174"/>
-      <c r="D652" s="175"/>
-      <c r="E652" s="175"/>
+      <c r="C652" s="177"/>
+      <c r="D652" s="178"/>
+      <c r="E652" s="178"/>
     </row>
     <row r="653" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A653" s="59">
@@ -11433,9 +11439,9 @@
         <v>58</v>
       </c>
       <c r="B669" s="87"/>
-      <c r="C669" s="174"/>
-      <c r="D669" s="175"/>
-      <c r="E669" s="175"/>
+      <c r="C669" s="177"/>
+      <c r="D669" s="178"/>
+      <c r="E669" s="178"/>
     </row>
     <row r="670" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A670" s="59">
@@ -11586,9 +11592,9 @@
         <v>59</v>
       </c>
       <c r="B686" s="87"/>
-      <c r="C686" s="174"/>
-      <c r="D686" s="175"/>
-      <c r="E686" s="175"/>
+      <c r="C686" s="177"/>
+      <c r="D686" s="178"/>
+      <c r="E686" s="178"/>
     </row>
     <row r="687" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A687" s="59">
@@ -11739,9 +11745,9 @@
         <v>60</v>
       </c>
       <c r="B703" s="87"/>
-      <c r="C703" s="174"/>
-      <c r="D703" s="175"/>
-      <c r="E703" s="175"/>
+      <c r="C703" s="177"/>
+      <c r="D703" s="178"/>
+      <c r="E703" s="178"/>
     </row>
     <row r="704" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A704" s="59">
@@ -11892,9 +11898,9 @@
         <v>61</v>
       </c>
       <c r="B720" s="87"/>
-      <c r="C720" s="174"/>
-      <c r="D720" s="175"/>
-      <c r="E720" s="175"/>
+      <c r="C720" s="177"/>
+      <c r="D720" s="178"/>
+      <c r="E720" s="178"/>
     </row>
     <row r="721" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A721" s="59">
@@ -12045,9 +12051,9 @@
         <v>62</v>
       </c>
       <c r="B737" s="87"/>
-      <c r="C737" s="174"/>
-      <c r="D737" s="175"/>
-      <c r="E737" s="175"/>
+      <c r="C737" s="177"/>
+      <c r="D737" s="178"/>
+      <c r="E737" s="178"/>
     </row>
     <row r="738" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A738" s="59">
@@ -12198,9 +12204,9 @@
         <v>63</v>
       </c>
       <c r="B754" s="87"/>
-      <c r="C754" s="174"/>
-      <c r="D754" s="175"/>
-      <c r="E754" s="175"/>
+      <c r="C754" s="177"/>
+      <c r="D754" s="178"/>
+      <c r="E754" s="178"/>
     </row>
     <row r="755" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A755" s="59">
@@ -12351,9 +12357,9 @@
         <v>64</v>
       </c>
       <c r="B771" s="87"/>
-      <c r="C771" s="174"/>
-      <c r="D771" s="175"/>
-      <c r="E771" s="175"/>
+      <c r="C771" s="177"/>
+      <c r="D771" s="178"/>
+      <c r="E771" s="178"/>
     </row>
     <row r="772" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A772" s="59">
@@ -12504,9 +12510,9 @@
         <v>65</v>
       </c>
       <c r="B788" s="87"/>
-      <c r="C788" s="174"/>
-      <c r="D788" s="175"/>
-      <c r="E788" s="175"/>
+      <c r="C788" s="177"/>
+      <c r="D788" s="178"/>
+      <c r="E788" s="178"/>
     </row>
     <row r="789" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A789" s="59">
@@ -12657,9 +12663,9 @@
         <v>66</v>
       </c>
       <c r="B805" s="87"/>
-      <c r="C805" s="174"/>
-      <c r="D805" s="175"/>
-      <c r="E805" s="175"/>
+      <c r="C805" s="177"/>
+      <c r="D805" s="178"/>
+      <c r="E805" s="178"/>
     </row>
     <row r="806" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A806" s="59">
@@ -12810,18 +12816,18 @@
         <v>67</v>
       </c>
       <c r="B822" s="39"/>
-      <c r="C822" s="186"/>
-      <c r="D822" s="187"/>
-      <c r="E822" s="187"/>
+      <c r="C822" s="185"/>
+      <c r="D822" s="186"/>
+      <c r="E822" s="186"/>
     </row>
     <row r="823" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A823" s="63" t="s">
         <v>68</v>
       </c>
       <c r="B823" s="87"/>
-      <c r="C823" s="174"/>
-      <c r="D823" s="175"/>
-      <c r="E823" s="175"/>
+      <c r="C823" s="177"/>
+      <c r="D823" s="178"/>
+      <c r="E823" s="178"/>
     </row>
     <row r="824" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A824" s="64">
@@ -12972,9 +12978,9 @@
         <v>69</v>
       </c>
       <c r="B840" s="90"/>
-      <c r="C840" s="176"/>
-      <c r="D840" s="177"/>
-      <c r="E840" s="177"/>
+      <c r="C840" s="179"/>
+      <c r="D840" s="180"/>
+      <c r="E840" s="180"/>
     </row>
     <row r="841" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A841" s="64">
@@ -13125,9 +13131,9 @@
         <v>70</v>
       </c>
       <c r="B857" s="87"/>
-      <c r="C857" s="174"/>
-      <c r="D857" s="175"/>
-      <c r="E857" s="175"/>
+      <c r="C857" s="177"/>
+      <c r="D857" s="178"/>
+      <c r="E857" s="178"/>
     </row>
     <row r="858" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A858" s="64">
@@ -13278,9 +13284,9 @@
         <v>71</v>
       </c>
       <c r="B874" s="87"/>
-      <c r="C874" s="174"/>
-      <c r="D874" s="175"/>
-      <c r="E874" s="175"/>
+      <c r="C874" s="177"/>
+      <c r="D874" s="178"/>
+      <c r="E874" s="178"/>
     </row>
     <row r="875" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A875" s="64">
@@ -13431,9 +13437,9 @@
         <v>72</v>
       </c>
       <c r="B891" s="87"/>
-      <c r="C891" s="174"/>
-      <c r="D891" s="175"/>
-      <c r="E891" s="175"/>
+      <c r="C891" s="177"/>
+      <c r="D891" s="178"/>
+      <c r="E891" s="178"/>
     </row>
     <row r="892" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A892" s="64">
@@ -13584,9 +13590,9 @@
         <v>73</v>
       </c>
       <c r="B908" s="87"/>
-      <c r="C908" s="174"/>
-      <c r="D908" s="175"/>
-      <c r="E908" s="175"/>
+      <c r="C908" s="177"/>
+      <c r="D908" s="178"/>
+      <c r="E908" s="178"/>
     </row>
     <row r="909" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A909" s="64">
@@ -13737,9 +13743,9 @@
         <v>74</v>
       </c>
       <c r="B925" s="87"/>
-      <c r="C925" s="174"/>
-      <c r="D925" s="175"/>
-      <c r="E925" s="175"/>
+      <c r="C925" s="177"/>
+      <c r="D925" s="178"/>
+      <c r="E925" s="178"/>
     </row>
     <row r="926" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A926" s="64">
@@ -13890,9 +13896,9 @@
         <v>75</v>
       </c>
       <c r="B942" s="87"/>
-      <c r="C942" s="174"/>
-      <c r="D942" s="175"/>
-      <c r="E942" s="175"/>
+      <c r="C942" s="177"/>
+      <c r="D942" s="178"/>
+      <c r="E942" s="178"/>
     </row>
     <row r="943" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A943" s="64">
@@ -14043,9 +14049,9 @@
         <v>76</v>
       </c>
       <c r="B959" s="87"/>
-      <c r="C959" s="174"/>
-      <c r="D959" s="175"/>
-      <c r="E959" s="175"/>
+      <c r="C959" s="177"/>
+      <c r="D959" s="178"/>
+      <c r="E959" s="178"/>
     </row>
     <row r="960" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A960" s="64">
@@ -14196,9 +14202,9 @@
         <v>77</v>
       </c>
       <c r="B976" s="87"/>
-      <c r="C976" s="174"/>
-      <c r="D976" s="175"/>
-      <c r="E976" s="175"/>
+      <c r="C976" s="177"/>
+      <c r="D976" s="178"/>
+      <c r="E976" s="178"/>
     </row>
     <row r="977" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A977" s="64">
@@ -14349,9 +14355,9 @@
         <v>78</v>
       </c>
       <c r="B993" s="87"/>
-      <c r="C993" s="174"/>
-      <c r="D993" s="175"/>
-      <c r="E993" s="175"/>
+      <c r="C993" s="177"/>
+      <c r="D993" s="178"/>
+      <c r="E993" s="178"/>
     </row>
     <row r="994" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A994" s="64">
@@ -14502,9 +14508,9 @@
         <v>79</v>
       </c>
       <c r="B1010" s="87"/>
-      <c r="C1010" s="174"/>
-      <c r="D1010" s="175"/>
-      <c r="E1010" s="175"/>
+      <c r="C1010" s="177"/>
+      <c r="D1010" s="178"/>
+      <c r="E1010" s="178"/>
     </row>
     <row r="1011" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1011" s="64">
@@ -14655,9 +14661,9 @@
         <v>80</v>
       </c>
       <c r="B1027" s="87"/>
-      <c r="C1027" s="174"/>
-      <c r="D1027" s="175"/>
-      <c r="E1027" s="175"/>
+      <c r="C1027" s="177"/>
+      <c r="D1027" s="178"/>
+      <c r="E1027" s="178"/>
     </row>
     <row r="1028" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1028" s="64">
@@ -14808,9 +14814,9 @@
         <v>83</v>
       </c>
       <c r="B1044" s="87"/>
-      <c r="C1044" s="174"/>
-      <c r="D1044" s="175"/>
-      <c r="E1044" s="175"/>
+      <c r="C1044" s="177"/>
+      <c r="D1044" s="178"/>
+      <c r="E1044" s="178"/>
     </row>
     <row r="1045" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1045" s="64">
@@ -14961,9 +14967,9 @@
         <v>82</v>
       </c>
       <c r="B1061" s="87"/>
-      <c r="C1061" s="174"/>
-      <c r="D1061" s="175"/>
-      <c r="E1061" s="175"/>
+      <c r="C1061" s="177"/>
+      <c r="D1061" s="178"/>
+      <c r="E1061" s="178"/>
     </row>
     <row r="1062" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1062" s="64">
@@ -15114,9 +15120,9 @@
         <v>84</v>
       </c>
       <c r="B1078" s="87"/>
-      <c r="C1078" s="174"/>
-      <c r="D1078" s="175"/>
-      <c r="E1078" s="175"/>
+      <c r="C1078" s="177"/>
+      <c r="D1078" s="178"/>
+      <c r="E1078" s="178"/>
     </row>
     <row r="1079" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1079" s="64">
@@ -15267,18 +15273,18 @@
         <v>104</v>
       </c>
       <c r="B1095" s="40"/>
-      <c r="C1095" s="184"/>
-      <c r="D1095" s="185"/>
-      <c r="E1095" s="185"/>
+      <c r="C1095" s="187"/>
+      <c r="D1095" s="188"/>
+      <c r="E1095" s="188"/>
     </row>
     <row r="1096" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A1096" s="68" t="s">
         <v>85</v>
       </c>
       <c r="B1096" s="87"/>
-      <c r="C1096" s="174"/>
-      <c r="D1096" s="175"/>
-      <c r="E1096" s="175"/>
+      <c r="C1096" s="177"/>
+      <c r="D1096" s="178"/>
+      <c r="E1096" s="178"/>
     </row>
     <row r="1097" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1097" s="69">
@@ -15429,9 +15435,9 @@
         <v>86</v>
       </c>
       <c r="B1113" s="90"/>
-      <c r="C1113" s="176"/>
-      <c r="D1113" s="177"/>
-      <c r="E1113" s="177"/>
+      <c r="C1113" s="179"/>
+      <c r="D1113" s="180"/>
+      <c r="E1113" s="180"/>
     </row>
     <row r="1114" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1114" s="69">
@@ -15582,9 +15588,9 @@
         <v>87</v>
       </c>
       <c r="B1130" s="87"/>
-      <c r="C1130" s="174"/>
-      <c r="D1130" s="175"/>
-      <c r="E1130" s="175"/>
+      <c r="C1130" s="177"/>
+      <c r="D1130" s="178"/>
+      <c r="E1130" s="178"/>
     </row>
     <row r="1131" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1131" s="69">
@@ -15735,9 +15741,9 @@
         <v>88</v>
       </c>
       <c r="B1147" s="87"/>
-      <c r="C1147" s="174"/>
-      <c r="D1147" s="175"/>
-      <c r="E1147" s="175"/>
+      <c r="C1147" s="177"/>
+      <c r="D1147" s="178"/>
+      <c r="E1147" s="178"/>
     </row>
     <row r="1148" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1148" s="69">
@@ -15888,9 +15894,9 @@
         <v>89</v>
       </c>
       <c r="B1164" s="87"/>
-      <c r="C1164" s="174"/>
-      <c r="D1164" s="175"/>
-      <c r="E1164" s="175"/>
+      <c r="C1164" s="177"/>
+      <c r="D1164" s="178"/>
+      <c r="E1164" s="178"/>
     </row>
     <row r="1165" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1165" s="69">
@@ -16041,9 +16047,9 @@
         <v>90</v>
       </c>
       <c r="B1181" s="87"/>
-      <c r="C1181" s="174"/>
-      <c r="D1181" s="175"/>
-      <c r="E1181" s="175"/>
+      <c r="C1181" s="177"/>
+      <c r="D1181" s="178"/>
+      <c r="E1181" s="178"/>
     </row>
     <row r="1182" spans="1:5" hidden="1" outlineLevel="3">
       <c r="A1182" s="69">
@@ -16194,9 +16200,9 @@
         <v>91</v>
       </c>
       <c r="B1198" s="87"/>
-      <c r="C1198" s="174"/>
-      <c r="D1198" s="175"/>
-      <c r="E1198" s="175"/>
+      <c r="C1198" s="177"/>
+      <c r="D1198" s="178"/>
+      <c r="E1198" s="178"/>
     </row>
     <row r="1199" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1199" s="69">
@@ -16347,9 +16353,9 @@
         <v>92</v>
       </c>
       <c r="B1215" s="87"/>
-      <c r="C1215" s="174"/>
-      <c r="D1215" s="175"/>
-      <c r="E1215" s="175"/>
+      <c r="C1215" s="177"/>
+      <c r="D1215" s="178"/>
+      <c r="E1215" s="178"/>
     </row>
     <row r="1216" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1216" s="69">
@@ -16500,9 +16506,9 @@
         <v>93</v>
       </c>
       <c r="B1232" s="87"/>
-      <c r="C1232" s="174"/>
-      <c r="D1232" s="175"/>
-      <c r="E1232" s="175"/>
+      <c r="C1232" s="177"/>
+      <c r="D1232" s="178"/>
+      <c r="E1232" s="178"/>
     </row>
     <row r="1233" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1233" s="69">
@@ -16653,9 +16659,9 @@
         <v>94</v>
       </c>
       <c r="B1249" s="87"/>
-      <c r="C1249" s="174"/>
-      <c r="D1249" s="175"/>
-      <c r="E1249" s="175"/>
+      <c r="C1249" s="177"/>
+      <c r="D1249" s="178"/>
+      <c r="E1249" s="178"/>
     </row>
     <row r="1250" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1250" s="69">
@@ -16806,9 +16812,9 @@
         <v>99</v>
       </c>
       <c r="B1266" s="87"/>
-      <c r="C1266" s="174"/>
-      <c r="D1266" s="175"/>
-      <c r="E1266" s="175"/>
+      <c r="C1266" s="177"/>
+      <c r="D1266" s="178"/>
+      <c r="E1266" s="178"/>
     </row>
     <row r="1267" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1267" s="69">
@@ -16959,9 +16965,9 @@
         <v>100</v>
       </c>
       <c r="B1283" s="87"/>
-      <c r="C1283" s="174"/>
-      <c r="D1283" s="175"/>
-      <c r="E1283" s="175"/>
+      <c r="C1283" s="177"/>
+      <c r="D1283" s="178"/>
+      <c r="E1283" s="178"/>
     </row>
     <row r="1284" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1284" s="69">
@@ -17112,9 +17118,9 @@
         <v>101</v>
       </c>
       <c r="B1300" s="87"/>
-      <c r="C1300" s="174"/>
-      <c r="D1300" s="175"/>
-      <c r="E1300" s="175"/>
+      <c r="C1300" s="177"/>
+      <c r="D1300" s="178"/>
+      <c r="E1300" s="178"/>
     </row>
     <row r="1301" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1301" s="69">
@@ -17265,9 +17271,9 @@
         <v>81</v>
       </c>
       <c r="B1317" s="87"/>
-      <c r="C1317" s="174"/>
-      <c r="D1317" s="175"/>
-      <c r="E1317" s="175"/>
+      <c r="C1317" s="177"/>
+      <c r="D1317" s="178"/>
+      <c r="E1317" s="178"/>
     </row>
     <row r="1318" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1318" s="69">
@@ -17418,9 +17424,9 @@
         <v>102</v>
       </c>
       <c r="B1334" s="87"/>
-      <c r="C1334" s="174"/>
-      <c r="D1334" s="175"/>
-      <c r="E1334" s="175"/>
+      <c r="C1334" s="177"/>
+      <c r="D1334" s="178"/>
+      <c r="E1334" s="178"/>
     </row>
     <row r="1335" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1335" s="69">
@@ -17571,9 +17577,9 @@
         <v>98</v>
       </c>
       <c r="B1351" s="87"/>
-      <c r="C1351" s="174"/>
-      <c r="D1351" s="175"/>
-      <c r="E1351" s="175"/>
+      <c r="C1351" s="177"/>
+      <c r="D1351" s="178"/>
+      <c r="E1351" s="178"/>
     </row>
     <row r="1352" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1352" s="69">
@@ -17724,18 +17730,18 @@
         <v>103</v>
       </c>
       <c r="B1368" s="41"/>
-      <c r="C1368" s="182"/>
-      <c r="D1368" s="183"/>
-      <c r="E1368" s="183"/>
+      <c r="C1368" s="189"/>
+      <c r="D1368" s="190"/>
+      <c r="E1368" s="190"/>
     </row>
     <row r="1369" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A1369" s="73" t="s">
         <v>105</v>
       </c>
       <c r="B1369" s="87"/>
-      <c r="C1369" s="174"/>
-      <c r="D1369" s="175"/>
-      <c r="E1369" s="175"/>
+      <c r="C1369" s="177"/>
+      <c r="D1369" s="178"/>
+      <c r="E1369" s="178"/>
     </row>
     <row r="1370" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1370" s="74">
@@ -17886,9 +17892,9 @@
         <v>106</v>
       </c>
       <c r="B1386" s="90"/>
-      <c r="C1386" s="176"/>
-      <c r="D1386" s="177"/>
-      <c r="E1386" s="177"/>
+      <c r="C1386" s="179"/>
+      <c r="D1386" s="180"/>
+      <c r="E1386" s="180"/>
     </row>
     <row r="1387" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1387" s="74">
@@ -18039,9 +18045,9 @@
         <v>107</v>
       </c>
       <c r="B1403" s="87"/>
-      <c r="C1403" s="174"/>
-      <c r="D1403" s="175"/>
-      <c r="E1403" s="175"/>
+      <c r="C1403" s="177"/>
+      <c r="D1403" s="178"/>
+      <c r="E1403" s="178"/>
     </row>
     <row r="1404" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1404" s="74">
@@ -18192,9 +18198,9 @@
         <v>108</v>
       </c>
       <c r="B1420" s="87"/>
-      <c r="C1420" s="174"/>
-      <c r="D1420" s="175"/>
-      <c r="E1420" s="175"/>
+      <c r="C1420" s="177"/>
+      <c r="D1420" s="178"/>
+      <c r="E1420" s="178"/>
     </row>
     <row r="1421" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1421" s="74">
@@ -18345,9 +18351,9 @@
         <v>109</v>
       </c>
       <c r="B1437" s="87"/>
-      <c r="C1437" s="174"/>
-      <c r="D1437" s="175"/>
-      <c r="E1437" s="175"/>
+      <c r="C1437" s="177"/>
+      <c r="D1437" s="178"/>
+      <c r="E1437" s="178"/>
     </row>
     <row r="1438" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1438" s="74">
@@ -18498,9 +18504,9 @@
         <v>110</v>
       </c>
       <c r="B1454" s="87"/>
-      <c r="C1454" s="174"/>
-      <c r="D1454" s="175"/>
-      <c r="E1454" s="175"/>
+      <c r="C1454" s="177"/>
+      <c r="D1454" s="178"/>
+      <c r="E1454" s="178"/>
     </row>
     <row r="1455" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1455" s="74">
@@ -18651,9 +18657,9 @@
         <v>111</v>
       </c>
       <c r="B1471" s="87"/>
-      <c r="C1471" s="174"/>
-      <c r="D1471" s="175"/>
-      <c r="E1471" s="175"/>
+      <c r="C1471" s="177"/>
+      <c r="D1471" s="178"/>
+      <c r="E1471" s="178"/>
     </row>
     <row r="1472" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1472" s="74">
@@ -18804,9 +18810,9 @@
         <v>112</v>
       </c>
       <c r="B1488" s="87"/>
-      <c r="C1488" s="174"/>
-      <c r="D1488" s="175"/>
-      <c r="E1488" s="175"/>
+      <c r="C1488" s="177"/>
+      <c r="D1488" s="178"/>
+      <c r="E1488" s="178"/>
     </row>
     <row r="1489" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1489" s="74">
@@ -18957,9 +18963,9 @@
         <v>113</v>
       </c>
       <c r="B1505" s="87"/>
-      <c r="C1505" s="174"/>
-      <c r="D1505" s="175"/>
-      <c r="E1505" s="175"/>
+      <c r="C1505" s="177"/>
+      <c r="D1505" s="178"/>
+      <c r="E1505" s="178"/>
     </row>
     <row r="1506" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1506" s="74">
@@ -19110,9 +19116,9 @@
         <v>114</v>
       </c>
       <c r="B1522" s="87"/>
-      <c r="C1522" s="174"/>
-      <c r="D1522" s="175"/>
-      <c r="E1522" s="175"/>
+      <c r="C1522" s="177"/>
+      <c r="D1522" s="178"/>
+      <c r="E1522" s="178"/>
     </row>
     <row r="1523" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1523" s="74">
@@ -19263,9 +19269,9 @@
         <v>95</v>
       </c>
       <c r="B1539" s="87"/>
-      <c r="C1539" s="174"/>
-      <c r="D1539" s="175"/>
-      <c r="E1539" s="175"/>
+      <c r="C1539" s="177"/>
+      <c r="D1539" s="178"/>
+      <c r="E1539" s="178"/>
     </row>
     <row r="1540" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1540" s="74">
@@ -19416,9 +19422,9 @@
         <v>115</v>
       </c>
       <c r="B1556" s="87"/>
-      <c r="C1556" s="174"/>
-      <c r="D1556" s="175"/>
-      <c r="E1556" s="175"/>
+      <c r="C1556" s="177"/>
+      <c r="D1556" s="178"/>
+      <c r="E1556" s="178"/>
     </row>
     <row r="1557" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1557" s="74">
@@ -19569,9 +19575,9 @@
         <v>116</v>
       </c>
       <c r="B1573" s="87"/>
-      <c r="C1573" s="174"/>
-      <c r="D1573" s="175"/>
-      <c r="E1573" s="175"/>
+      <c r="C1573" s="177"/>
+      <c r="D1573" s="178"/>
+      <c r="E1573" s="178"/>
     </row>
     <row r="1574" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1574" s="74">
@@ -19722,9 +19728,9 @@
         <v>117</v>
       </c>
       <c r="B1590" s="87"/>
-      <c r="C1590" s="174"/>
-      <c r="D1590" s="175"/>
-      <c r="E1590" s="175"/>
+      <c r="C1590" s="177"/>
+      <c r="D1590" s="178"/>
+      <c r="E1590" s="178"/>
     </row>
     <row r="1591" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1591" s="74">
@@ -19875,9 +19881,9 @@
         <v>118</v>
       </c>
       <c r="B1607" s="87"/>
-      <c r="C1607" s="174"/>
-      <c r="D1607" s="175"/>
-      <c r="E1607" s="175"/>
+      <c r="C1607" s="177"/>
+      <c r="D1607" s="178"/>
+      <c r="E1607" s="178"/>
     </row>
     <row r="1608" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1608" s="74">
@@ -20028,9 +20034,9 @@
         <v>119</v>
       </c>
       <c r="B1624" s="87"/>
-      <c r="C1624" s="174"/>
-      <c r="D1624" s="175"/>
-      <c r="E1624" s="175"/>
+      <c r="C1624" s="177"/>
+      <c r="D1624" s="178"/>
+      <c r="E1624" s="178"/>
     </row>
     <row r="1625" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1625" s="74">
@@ -20181,18 +20187,18 @@
         <v>120</v>
       </c>
       <c r="B1641" s="42"/>
-      <c r="C1641" s="180"/>
-      <c r="D1641" s="181"/>
-      <c r="E1641" s="181"/>
+      <c r="C1641" s="191"/>
+      <c r="D1641" s="192"/>
+      <c r="E1641" s="192"/>
     </row>
     <row r="1642" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A1642" s="78" t="s">
         <v>121</v>
       </c>
       <c r="B1642" s="87"/>
-      <c r="C1642" s="174"/>
-      <c r="D1642" s="175"/>
-      <c r="E1642" s="175"/>
+      <c r="C1642" s="177"/>
+      <c r="D1642" s="178"/>
+      <c r="E1642" s="178"/>
     </row>
     <row r="1643" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1643" s="79">
@@ -20343,9 +20349,9 @@
         <v>122</v>
       </c>
       <c r="B1659" s="90"/>
-      <c r="C1659" s="176"/>
-      <c r="D1659" s="177"/>
-      <c r="E1659" s="177"/>
+      <c r="C1659" s="179"/>
+      <c r="D1659" s="180"/>
+      <c r="E1659" s="180"/>
     </row>
     <row r="1660" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1660" s="79">
@@ -20496,9 +20502,9 @@
         <v>123</v>
       </c>
       <c r="B1676" s="87"/>
-      <c r="C1676" s="174"/>
-      <c r="D1676" s="175"/>
-      <c r="E1676" s="175"/>
+      <c r="C1676" s="177"/>
+      <c r="D1676" s="178"/>
+      <c r="E1676" s="178"/>
     </row>
     <row r="1677" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1677" s="79">
@@ -20649,9 +20655,9 @@
         <v>124</v>
       </c>
       <c r="B1693" s="87"/>
-      <c r="C1693" s="174"/>
-      <c r="D1693" s="175"/>
-      <c r="E1693" s="175"/>
+      <c r="C1693" s="177"/>
+      <c r="D1693" s="178"/>
+      <c r="E1693" s="178"/>
     </row>
     <row r="1694" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1694" s="79">
@@ -20802,9 +20808,9 @@
         <v>125</v>
       </c>
       <c r="B1710" s="87"/>
-      <c r="C1710" s="174"/>
-      <c r="D1710" s="175"/>
-      <c r="E1710" s="175"/>
+      <c r="C1710" s="177"/>
+      <c r="D1710" s="178"/>
+      <c r="E1710" s="178"/>
     </row>
     <row r="1711" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1711" s="79">
@@ -20955,9 +20961,9 @@
         <v>126</v>
       </c>
       <c r="B1727" s="87"/>
-      <c r="C1727" s="174"/>
-      <c r="D1727" s="175"/>
-      <c r="E1727" s="175"/>
+      <c r="C1727" s="177"/>
+      <c r="D1727" s="178"/>
+      <c r="E1727" s="178"/>
     </row>
     <row r="1728" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1728" s="79">
@@ -21108,9 +21114,9 @@
         <v>127</v>
       </c>
       <c r="B1744" s="87"/>
-      <c r="C1744" s="174"/>
-      <c r="D1744" s="175"/>
-      <c r="E1744" s="175"/>
+      <c r="C1744" s="177"/>
+      <c r="D1744" s="178"/>
+      <c r="E1744" s="178"/>
     </row>
     <row r="1745" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1745" s="79">
@@ -21261,9 +21267,9 @@
         <v>128</v>
       </c>
       <c r="B1761" s="87"/>
-      <c r="C1761" s="174"/>
-      <c r="D1761" s="175"/>
-      <c r="E1761" s="175"/>
+      <c r="C1761" s="177"/>
+      <c r="D1761" s="178"/>
+      <c r="E1761" s="178"/>
     </row>
     <row r="1762" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1762" s="79">
@@ -21414,9 +21420,9 @@
         <v>129</v>
       </c>
       <c r="B1778" s="87"/>
-      <c r="C1778" s="174"/>
-      <c r="D1778" s="175"/>
-      <c r="E1778" s="175"/>
+      <c r="C1778" s="177"/>
+      <c r="D1778" s="178"/>
+      <c r="E1778" s="178"/>
     </row>
     <row r="1779" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1779" s="79">
@@ -21567,9 +21573,9 @@
         <v>130</v>
       </c>
       <c r="B1795" s="87"/>
-      <c r="C1795" s="174"/>
-      <c r="D1795" s="175"/>
-      <c r="E1795" s="175"/>
+      <c r="C1795" s="177"/>
+      <c r="D1795" s="178"/>
+      <c r="E1795" s="178"/>
     </row>
     <row r="1796" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1796" s="79">
@@ -21720,9 +21726,9 @@
         <v>131</v>
       </c>
       <c r="B1812" s="87"/>
-      <c r="C1812" s="174"/>
-      <c r="D1812" s="175"/>
-      <c r="E1812" s="175"/>
+      <c r="C1812" s="177"/>
+      <c r="D1812" s="178"/>
+      <c r="E1812" s="178"/>
     </row>
     <row r="1813" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1813" s="79">
@@ -21873,9 +21879,9 @@
         <v>96</v>
       </c>
       <c r="B1829" s="87"/>
-      <c r="C1829" s="174"/>
-      <c r="D1829" s="175"/>
-      <c r="E1829" s="175"/>
+      <c r="C1829" s="177"/>
+      <c r="D1829" s="178"/>
+      <c r="E1829" s="178"/>
     </row>
     <row r="1830" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1830" s="79">
@@ -22026,9 +22032,9 @@
         <v>132</v>
       </c>
       <c r="B1846" s="87"/>
-      <c r="C1846" s="174"/>
-      <c r="D1846" s="175"/>
-      <c r="E1846" s="175"/>
+      <c r="C1846" s="177"/>
+      <c r="D1846" s="178"/>
+      <c r="E1846" s="178"/>
     </row>
     <row r="1847" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1847" s="79">
@@ -22179,9 +22185,9 @@
         <v>133</v>
       </c>
       <c r="B1863" s="87"/>
-      <c r="C1863" s="174"/>
-      <c r="D1863" s="175"/>
-      <c r="E1863" s="175"/>
+      <c r="C1863" s="177"/>
+      <c r="D1863" s="178"/>
+      <c r="E1863" s="178"/>
     </row>
     <row r="1864" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1864" s="79">
@@ -22332,9 +22338,9 @@
         <v>134</v>
       </c>
       <c r="B1880" s="87"/>
-      <c r="C1880" s="174"/>
-      <c r="D1880" s="175"/>
-      <c r="E1880" s="175"/>
+      <c r="C1880" s="177"/>
+      <c r="D1880" s="178"/>
+      <c r="E1880" s="178"/>
     </row>
     <row r="1881" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1881" s="79">
@@ -22485,9 +22491,9 @@
         <v>135</v>
       </c>
       <c r="B1897" s="87"/>
-      <c r="C1897" s="174"/>
-      <c r="D1897" s="175"/>
-      <c r="E1897" s="175"/>
+      <c r="C1897" s="177"/>
+      <c r="D1897" s="178"/>
+      <c r="E1897" s="178"/>
     </row>
     <row r="1898" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1898" s="79">
@@ -22638,18 +22644,18 @@
         <v>136</v>
       </c>
       <c r="B1914" s="43"/>
-      <c r="C1914" s="178"/>
-      <c r="D1914" s="179"/>
-      <c r="E1914" s="179"/>
+      <c r="C1914" s="193"/>
+      <c r="D1914" s="194"/>
+      <c r="E1914" s="194"/>
     </row>
     <row r="1915" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A1915" s="83" t="s">
         <v>137</v>
       </c>
       <c r="B1915" s="87"/>
-      <c r="C1915" s="174"/>
-      <c r="D1915" s="175"/>
-      <c r="E1915" s="175"/>
+      <c r="C1915" s="177"/>
+      <c r="D1915" s="178"/>
+      <c r="E1915" s="178"/>
     </row>
     <row r="1916" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1916" s="84">
@@ -22800,9 +22806,9 @@
         <v>138</v>
       </c>
       <c r="B1932" s="90"/>
-      <c r="C1932" s="176"/>
-      <c r="D1932" s="177"/>
-      <c r="E1932" s="177"/>
+      <c r="C1932" s="179"/>
+      <c r="D1932" s="180"/>
+      <c r="E1932" s="180"/>
     </row>
     <row r="1933" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1933" s="84">
@@ -22953,9 +22959,9 @@
         <v>139</v>
       </c>
       <c r="B1949" s="87"/>
-      <c r="C1949" s="174"/>
-      <c r="D1949" s="175"/>
-      <c r="E1949" s="175"/>
+      <c r="C1949" s="177"/>
+      <c r="D1949" s="178"/>
+      <c r="E1949" s="178"/>
     </row>
     <row r="1950" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1950" s="84">
@@ -23106,9 +23112,9 @@
         <v>140</v>
       </c>
       <c r="B1966" s="87"/>
-      <c r="C1966" s="174"/>
-      <c r="D1966" s="175"/>
-      <c r="E1966" s="175"/>
+      <c r="C1966" s="177"/>
+      <c r="D1966" s="178"/>
+      <c r="E1966" s="178"/>
     </row>
     <row r="1967" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1967" s="84">
@@ -23259,9 +23265,9 @@
         <v>141</v>
       </c>
       <c r="B1983" s="87"/>
-      <c r="C1983" s="174"/>
-      <c r="D1983" s="175"/>
-      <c r="E1983" s="175"/>
+      <c r="C1983" s="177"/>
+      <c r="D1983" s="178"/>
+      <c r="E1983" s="178"/>
     </row>
     <row r="1984" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1984" s="84">
@@ -23412,9 +23418,9 @@
         <v>142</v>
       </c>
       <c r="B2000" s="87"/>
-      <c r="C2000" s="174"/>
-      <c r="D2000" s="175"/>
-      <c r="E2000" s="175"/>
+      <c r="C2000" s="177"/>
+      <c r="D2000" s="178"/>
+      <c r="E2000" s="178"/>
     </row>
     <row r="2001" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2001" s="84">
@@ -23565,9 +23571,9 @@
         <v>143</v>
       </c>
       <c r="B2017" s="87"/>
-      <c r="C2017" s="174"/>
-      <c r="D2017" s="175"/>
-      <c r="E2017" s="175"/>
+      <c r="C2017" s="177"/>
+      <c r="D2017" s="178"/>
+      <c r="E2017" s="178"/>
     </row>
     <row r="2018" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2018" s="84">
@@ -23718,9 +23724,9 @@
         <v>144</v>
       </c>
       <c r="B2034" s="87"/>
-      <c r="C2034" s="174"/>
-      <c r="D2034" s="175"/>
-      <c r="E2034" s="175"/>
+      <c r="C2034" s="177"/>
+      <c r="D2034" s="178"/>
+      <c r="E2034" s="178"/>
     </row>
     <row r="2035" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2035" s="84">
@@ -23871,9 +23877,9 @@
         <v>145</v>
       </c>
       <c r="B2051" s="87"/>
-      <c r="C2051" s="174"/>
-      <c r="D2051" s="175"/>
-      <c r="E2051" s="175"/>
+      <c r="C2051" s="177"/>
+      <c r="D2051" s="178"/>
+      <c r="E2051" s="178"/>
     </row>
     <row r="2052" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2052" s="84">
@@ -24024,9 +24030,9 @@
         <v>146</v>
       </c>
       <c r="B2068" s="87"/>
-      <c r="C2068" s="174"/>
-      <c r="D2068" s="175"/>
-      <c r="E2068" s="175"/>
+      <c r="C2068" s="177"/>
+      <c r="D2068" s="178"/>
+      <c r="E2068" s="178"/>
     </row>
     <row r="2069" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2069" s="84">
@@ -24177,9 +24183,9 @@
         <v>147</v>
       </c>
       <c r="B2085" s="87"/>
-      <c r="C2085" s="174"/>
-      <c r="D2085" s="175"/>
-      <c r="E2085" s="175"/>
+      <c r="C2085" s="177"/>
+      <c r="D2085" s="178"/>
+      <c r="E2085" s="178"/>
     </row>
     <row r="2086" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2086" s="84">
@@ -24330,9 +24336,9 @@
         <v>148</v>
       </c>
       <c r="B2102" s="87"/>
-      <c r="C2102" s="174"/>
-      <c r="D2102" s="175"/>
-      <c r="E2102" s="175"/>
+      <c r="C2102" s="177"/>
+      <c r="D2102" s="178"/>
+      <c r="E2102" s="178"/>
     </row>
     <row r="2103" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2103" s="84">
@@ -24483,9 +24489,9 @@
         <v>97</v>
       </c>
       <c r="B2119" s="87"/>
-      <c r="C2119" s="174"/>
-      <c r="D2119" s="175"/>
-      <c r="E2119" s="175"/>
+      <c r="C2119" s="177"/>
+      <c r="D2119" s="178"/>
+      <c r="E2119" s="178"/>
     </row>
     <row r="2120" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2120" s="84">
@@ -24636,9 +24642,9 @@
         <v>149</v>
       </c>
       <c r="B2136" s="87"/>
-      <c r="C2136" s="174"/>
-      <c r="D2136" s="175"/>
-      <c r="E2136" s="175"/>
+      <c r="C2136" s="177"/>
+      <c r="D2136" s="178"/>
+      <c r="E2136" s="178"/>
     </row>
     <row r="2137" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2137" s="84">
@@ -24789,9 +24795,9 @@
         <v>150</v>
       </c>
       <c r="B2153" s="87"/>
-      <c r="C2153" s="174"/>
-      <c r="D2153" s="175"/>
-      <c r="E2153" s="175"/>
+      <c r="C2153" s="177"/>
+      <c r="D2153" s="178"/>
+      <c r="E2153" s="178"/>
     </row>
     <row r="2154" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2154" s="84">
@@ -24942,9 +24948,9 @@
         <v>151</v>
       </c>
       <c r="B2170" s="87"/>
-      <c r="C2170" s="174"/>
-      <c r="D2170" s="175"/>
-      <c r="E2170" s="175"/>
+      <c r="C2170" s="177"/>
+      <c r="D2170" s="178"/>
+      <c r="E2170" s="178"/>
     </row>
     <row r="2171" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2171" s="84">
@@ -25092,26 +25098,111 @@
     </row>
   </sheetData>
   <mergeCells count="137">
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="C89:E89"/>
-    <mergeCell ref="C21:E21"/>
-    <mergeCell ref="C38:E38"/>
-    <mergeCell ref="C55:E55"/>
-    <mergeCell ref="C72:E72"/>
-    <mergeCell ref="C208:E208"/>
-    <mergeCell ref="C225:E225"/>
-    <mergeCell ref="C242:E242"/>
-    <mergeCell ref="C259:E259"/>
-    <mergeCell ref="C276:E276"/>
-    <mergeCell ref="C277:E277"/>
-    <mergeCell ref="C106:E106"/>
-    <mergeCell ref="C123:E123"/>
-    <mergeCell ref="C140:E140"/>
-    <mergeCell ref="C157:E157"/>
-    <mergeCell ref="C174:E174"/>
-    <mergeCell ref="C191:E191"/>
+    <mergeCell ref="C2034:E2034"/>
+    <mergeCell ref="C2051:E2051"/>
+    <mergeCell ref="C2068:E2068"/>
+    <mergeCell ref="C2085:E2085"/>
+    <mergeCell ref="C2170:E2170"/>
+    <mergeCell ref="C2102:E2102"/>
+    <mergeCell ref="C2119:E2119"/>
+    <mergeCell ref="C2136:E2136"/>
+    <mergeCell ref="C2153:E2153"/>
+    <mergeCell ref="C1932:E1932"/>
+    <mergeCell ref="C1949:E1949"/>
+    <mergeCell ref="C1966:E1966"/>
+    <mergeCell ref="C1983:E1983"/>
+    <mergeCell ref="C2000:E2000"/>
+    <mergeCell ref="C2017:E2017"/>
+    <mergeCell ref="C1846:E1846"/>
+    <mergeCell ref="C1863:E1863"/>
+    <mergeCell ref="C1880:E1880"/>
+    <mergeCell ref="C1897:E1897"/>
+    <mergeCell ref="C1914:E1914"/>
+    <mergeCell ref="C1915:E1915"/>
+    <mergeCell ref="C1744:E1744"/>
+    <mergeCell ref="C1761:E1761"/>
+    <mergeCell ref="C1778:E1778"/>
+    <mergeCell ref="C1795:E1795"/>
+    <mergeCell ref="C1812:E1812"/>
+    <mergeCell ref="C1829:E1829"/>
+    <mergeCell ref="C1642:E1642"/>
+    <mergeCell ref="C1659:E1659"/>
+    <mergeCell ref="C1676:E1676"/>
+    <mergeCell ref="C1693:E1693"/>
+    <mergeCell ref="C1710:E1710"/>
+    <mergeCell ref="C1727:E1727"/>
+    <mergeCell ref="C1556:E1556"/>
+    <mergeCell ref="C1573:E1573"/>
+    <mergeCell ref="C1590:E1590"/>
+    <mergeCell ref="C1607:E1607"/>
+    <mergeCell ref="C1624:E1624"/>
+    <mergeCell ref="C1641:E1641"/>
+    <mergeCell ref="C1454:E1454"/>
+    <mergeCell ref="C1471:E1471"/>
+    <mergeCell ref="C1488:E1488"/>
+    <mergeCell ref="C1505:E1505"/>
+    <mergeCell ref="C1522:E1522"/>
+    <mergeCell ref="C1539:E1539"/>
+    <mergeCell ref="C1368:E1368"/>
+    <mergeCell ref="C1369:E1369"/>
+    <mergeCell ref="C1386:E1386"/>
+    <mergeCell ref="C1403:E1403"/>
+    <mergeCell ref="C1420:E1420"/>
+    <mergeCell ref="C1437:E1437"/>
+    <mergeCell ref="C1266:E1266"/>
+    <mergeCell ref="C1283:E1283"/>
+    <mergeCell ref="C1300:E1300"/>
+    <mergeCell ref="C1317:E1317"/>
+    <mergeCell ref="C1334:E1334"/>
+    <mergeCell ref="C1351:E1351"/>
+    <mergeCell ref="C1164:E1164"/>
+    <mergeCell ref="C1181:E1181"/>
+    <mergeCell ref="C1198:E1198"/>
+    <mergeCell ref="C1215:E1215"/>
+    <mergeCell ref="C1232:E1232"/>
+    <mergeCell ref="C1249:E1249"/>
+    <mergeCell ref="C1078:E1078"/>
+    <mergeCell ref="C1095:E1095"/>
+    <mergeCell ref="C1096:E1096"/>
+    <mergeCell ref="C1113:E1113"/>
+    <mergeCell ref="C1130:E1130"/>
+    <mergeCell ref="C1147:E1147"/>
+    <mergeCell ref="C976:E976"/>
+    <mergeCell ref="C993:E993"/>
+    <mergeCell ref="C1010:E1010"/>
+    <mergeCell ref="C1027:E1027"/>
+    <mergeCell ref="C1044:E1044"/>
+    <mergeCell ref="C1061:E1061"/>
+    <mergeCell ref="C874:E874"/>
+    <mergeCell ref="C891:E891"/>
+    <mergeCell ref="C908:E908"/>
+    <mergeCell ref="C925:E925"/>
+    <mergeCell ref="C942:E942"/>
+    <mergeCell ref="C959:E959"/>
+    <mergeCell ref="C788:E788"/>
+    <mergeCell ref="C805:E805"/>
+    <mergeCell ref="C822:E822"/>
+    <mergeCell ref="C823:E823"/>
+    <mergeCell ref="C840:E840"/>
+    <mergeCell ref="C857:E857"/>
+    <mergeCell ref="C686:E686"/>
+    <mergeCell ref="C703:E703"/>
+    <mergeCell ref="C720:E720"/>
+    <mergeCell ref="C737:E737"/>
+    <mergeCell ref="C754:E754"/>
+    <mergeCell ref="C771:E771"/>
+    <mergeCell ref="C584:E584"/>
+    <mergeCell ref="C601:E601"/>
+    <mergeCell ref="C618:E618"/>
+    <mergeCell ref="C635:E635"/>
+    <mergeCell ref="C652:E652"/>
+    <mergeCell ref="C669:E669"/>
+    <mergeCell ref="C498:E498"/>
+    <mergeCell ref="C515:E515"/>
+    <mergeCell ref="C532:E532"/>
+    <mergeCell ref="C549:E549"/>
+    <mergeCell ref="C550:E550"/>
+    <mergeCell ref="C567:E567"/>
     <mergeCell ref="C396:E396"/>
     <mergeCell ref="C413:E413"/>
     <mergeCell ref="C430:E430"/>
@@ -25124,111 +25215,26 @@
     <mergeCell ref="C345:E345"/>
     <mergeCell ref="C362:E362"/>
     <mergeCell ref="C379:E379"/>
-    <mergeCell ref="C584:E584"/>
-    <mergeCell ref="C601:E601"/>
-    <mergeCell ref="C618:E618"/>
-    <mergeCell ref="C635:E635"/>
-    <mergeCell ref="C652:E652"/>
-    <mergeCell ref="C669:E669"/>
-    <mergeCell ref="C498:E498"/>
-    <mergeCell ref="C515:E515"/>
-    <mergeCell ref="C532:E532"/>
-    <mergeCell ref="C549:E549"/>
-    <mergeCell ref="C550:E550"/>
-    <mergeCell ref="C567:E567"/>
-    <mergeCell ref="C788:E788"/>
-    <mergeCell ref="C805:E805"/>
-    <mergeCell ref="C822:E822"/>
-    <mergeCell ref="C823:E823"/>
-    <mergeCell ref="C840:E840"/>
-    <mergeCell ref="C857:E857"/>
-    <mergeCell ref="C686:E686"/>
-    <mergeCell ref="C703:E703"/>
-    <mergeCell ref="C720:E720"/>
-    <mergeCell ref="C737:E737"/>
-    <mergeCell ref="C754:E754"/>
-    <mergeCell ref="C771:E771"/>
-    <mergeCell ref="C976:E976"/>
-    <mergeCell ref="C993:E993"/>
-    <mergeCell ref="C1010:E1010"/>
-    <mergeCell ref="C1027:E1027"/>
-    <mergeCell ref="C1044:E1044"/>
-    <mergeCell ref="C1061:E1061"/>
-    <mergeCell ref="C874:E874"/>
-    <mergeCell ref="C891:E891"/>
-    <mergeCell ref="C908:E908"/>
-    <mergeCell ref="C925:E925"/>
-    <mergeCell ref="C942:E942"/>
-    <mergeCell ref="C959:E959"/>
-    <mergeCell ref="C1164:E1164"/>
-    <mergeCell ref="C1181:E1181"/>
-    <mergeCell ref="C1198:E1198"/>
-    <mergeCell ref="C1215:E1215"/>
-    <mergeCell ref="C1232:E1232"/>
-    <mergeCell ref="C1249:E1249"/>
-    <mergeCell ref="C1078:E1078"/>
-    <mergeCell ref="C1095:E1095"/>
-    <mergeCell ref="C1096:E1096"/>
-    <mergeCell ref="C1113:E1113"/>
-    <mergeCell ref="C1130:E1130"/>
-    <mergeCell ref="C1147:E1147"/>
-    <mergeCell ref="C1368:E1368"/>
-    <mergeCell ref="C1369:E1369"/>
-    <mergeCell ref="C1386:E1386"/>
-    <mergeCell ref="C1403:E1403"/>
-    <mergeCell ref="C1420:E1420"/>
-    <mergeCell ref="C1437:E1437"/>
-    <mergeCell ref="C1266:E1266"/>
-    <mergeCell ref="C1283:E1283"/>
-    <mergeCell ref="C1300:E1300"/>
-    <mergeCell ref="C1317:E1317"/>
-    <mergeCell ref="C1334:E1334"/>
-    <mergeCell ref="C1351:E1351"/>
-    <mergeCell ref="C1556:E1556"/>
-    <mergeCell ref="C1573:E1573"/>
-    <mergeCell ref="C1590:E1590"/>
-    <mergeCell ref="C1607:E1607"/>
-    <mergeCell ref="C1624:E1624"/>
-    <mergeCell ref="C1641:E1641"/>
-    <mergeCell ref="C1454:E1454"/>
-    <mergeCell ref="C1471:E1471"/>
-    <mergeCell ref="C1488:E1488"/>
-    <mergeCell ref="C1505:E1505"/>
-    <mergeCell ref="C1522:E1522"/>
-    <mergeCell ref="C1539:E1539"/>
-    <mergeCell ref="C1744:E1744"/>
-    <mergeCell ref="C1761:E1761"/>
-    <mergeCell ref="C1778:E1778"/>
-    <mergeCell ref="C1795:E1795"/>
-    <mergeCell ref="C1812:E1812"/>
-    <mergeCell ref="C1829:E1829"/>
-    <mergeCell ref="C1642:E1642"/>
-    <mergeCell ref="C1659:E1659"/>
-    <mergeCell ref="C1676:E1676"/>
-    <mergeCell ref="C1693:E1693"/>
-    <mergeCell ref="C1710:E1710"/>
-    <mergeCell ref="C1727:E1727"/>
-    <mergeCell ref="C1932:E1932"/>
-    <mergeCell ref="C1949:E1949"/>
-    <mergeCell ref="C1966:E1966"/>
-    <mergeCell ref="C1983:E1983"/>
-    <mergeCell ref="C2000:E2000"/>
-    <mergeCell ref="C2017:E2017"/>
-    <mergeCell ref="C1846:E1846"/>
-    <mergeCell ref="C1863:E1863"/>
-    <mergeCell ref="C1880:E1880"/>
-    <mergeCell ref="C1897:E1897"/>
-    <mergeCell ref="C1914:E1914"/>
-    <mergeCell ref="C1915:E1915"/>
-    <mergeCell ref="C2034:E2034"/>
-    <mergeCell ref="C2051:E2051"/>
-    <mergeCell ref="C2068:E2068"/>
-    <mergeCell ref="C2085:E2085"/>
-    <mergeCell ref="C2170:E2170"/>
-    <mergeCell ref="C2102:E2102"/>
-    <mergeCell ref="C2119:E2119"/>
-    <mergeCell ref="C2136:E2136"/>
-    <mergeCell ref="C2153:E2153"/>
+    <mergeCell ref="C225:E225"/>
+    <mergeCell ref="C242:E242"/>
+    <mergeCell ref="C259:E259"/>
+    <mergeCell ref="C276:E276"/>
+    <mergeCell ref="C277:E277"/>
+    <mergeCell ref="C106:E106"/>
+    <mergeCell ref="C123:E123"/>
+    <mergeCell ref="C140:E140"/>
+    <mergeCell ref="C157:E157"/>
+    <mergeCell ref="C174:E174"/>
+    <mergeCell ref="C191:E191"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="C89:E89"/>
+    <mergeCell ref="C21:E21"/>
+    <mergeCell ref="C38:E38"/>
+    <mergeCell ref="C55:E55"/>
+    <mergeCell ref="C72:E72"/>
+    <mergeCell ref="C208:E208"/>
   </mergeCells>
   <phoneticPr fontId="14" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -26487,163 +26493,150 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="33">
-      <c r="A1" s="219" t="s">
+      <c r="A1" s="220" t="s">
         <v>184</v>
       </c>
-      <c r="B1" s="220"/>
+      <c r="B1" s="221"/>
       <c r="C1" s="118"/>
       <c r="D1" s="5"/>
       <c r="E1" s="5"/>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="216" t="s">
+      <c r="A2" s="226" t="s">
         <v>183</v>
       </c>
-      <